<commit_message>
two dfs for forces at permeation, with and without ions - 3000:6799
</commit_message>
<xml_diff>
--- a/results/forces/force_results.xlsx
+++ b/results/forces/force_results.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{3185: {'frame': 3185, 'ionic_force': [1.3455531299114227, -1.2103240936994553, -9.767556190490723], 'ionic_force_magnitude': 9.93380851293186, 'motion_vector': [3.3021926879882812, 1.7625465393066406, 0.34154510498046875], 'cosine_ionic_motion': -0.027479692611883776, 'ionic_motion_component': -0.27297800440068176, 'ionic_force_x': 1.3455531299114227, 'ionic_force_y': -1.2103240936994553, 'ionic_force_z': -9.767556190490723, 'radial_force': 1.8098059667278792, 'axial_force': -9.767556190490723, 'contributions': [{'ion': 1313, 'force': [1.0481852293014526, -0.9845649600028992, -6.827840805053711], 'magnitude': 6.9776411056518555, 'distance': 6.8978657722473145, 'directional_contribution': -0.1612393407807282}, {'ion': 1460, 'force': [0.2973679006099701, -0.2257591336965561, -2.9397153854370117], 'magnitude': 2.963329553604126, 'distance': 10.584712982177734, 'directional_contribution': -0.11173867455445308}]}, 3186: {'frame': 3186, 'ionic_force': [3.8716278672218323, 0.9531629383563995, -6.351068735122681], 'ionic_force_magnitude': 7.498939658882293, 'motion_vector': [-1.120147705078125, -0.510986328125, 0.8818283081054688], 'cosine_ionic_motion': -0.917921914123857, 'ionic_motion_component': -6.883441045580538, 'ionic_force_x': 3.8716278672218323, 'ionic_force_y': 0.9531629383563995, 'ionic_force_z': -6.351068735122681, 'radial_force': 3.987232364598893, 'axial_force': -6.351068735122681, 'contributions': [{'ion': 1313, 'force': [2.8922908306121826, 0.682626485824585, -4.142235279083252], 'magnitude': 5.0979838371276855, 'distance': 8.069931030273438, 'directional_contribution': -4.781606164194734}, {'ion': 1460, 'force': [0.9793370366096497, 0.2705364525318146, -2.2088334560394287], 'magnitude': 2.4313035011291504, 'distance': 11.685558319091797, 'directional_contribution': -2.101834725921859}]}, 3187: {'frame': 3187, 'ionic_force': [4.825020015239716, 1.0010420382022858, -9.05678677558899], 'ionic_force_magnitude': 10.31059115706736, 'motion_vector': [-4.467868804931641, 3.94091796875, -0.4804229736328125], 'cosine_ionic_motion': -0.2151940520558242, 'ionic_motion_component': -2.218777890180274, 'ionic_force_x': 4.825020015239716, 'ionic_force_y': 1.0010420382022858, 'ionic_force_z': -9.05678677558899, 'radial_force': 4.927768593360696, 'axial_force': -9.05678677558899, 'contributions': [{'ion': 1313, 'force': [3.834963321685791, 0.7111164927482605, -6.247584819793701], 'magnitude': 7.365116596221924, 'distance': 6.713967323303223, 'directional_contribution': -1.8956571041124768}, {'ion': 1460, 'force': [0.9900566935539246, 0.28992554545402527, -2.809201955795288], 'magnitude': 2.992638349533081, 'distance': 10.532752990722656, 'directional_contribution': -0.32312089049107406}]}, 3188: {'frame': 3188, 'ionic_force': [-0.7788635641336441, 4.744892954826355, -7.823496103286743], 'ionic_force_magnitude': 9.183013061214636, 'motion_vector': [2.9478530883789062, -1.2035942077636719, 0.8451919555664062], 'cosine_ionic_motion': -0.48324645421477935, 'ionic_motion_component': -4.437658500839979, 'ionic_force_x': -0.7788635641336441, 'ionic_force_y': 4.744892954826355, 'ionic_force_z': -7.823496103286743, 'radial_force': 4.808392413717472, 'axial_force': -7.823496103286743, 'contributions': [{'ion': 1313, 'force': [-0.5623465180397034, 3.5319478511810303, -5.200526714324951], 'magnitude': 6.311605930328369, 'distance': 7.252689838409424, 'directional_contribution': -3.127825041783648}, {'ion': 1460, 'force': [-0.21651704609394073, 1.2129451036453247, -2.622969388961792], 'magnitude': 2.897944688796997, 'distance': 10.703454971313477, 'directional_contribution': -1.3098335379862371}]}, 3189: {'frame': 3189, 'ionic_force': [2.2279635965824127, 3.7496649622917175, -8.675254344940186], 'ionic_force_magnitude': 9.70998697561115, 'motion_vector': [2.050933837890625, -1.666748046875, -0.683929443359375], 'cosine_ionic_motion': 0.16044574791098273, 'ionic_motion_component': 1.5579261225078322, 'ionic_force_x': 2.2279635965824127, 'ionic_force_y': 3.7496649622917175, 'ionic_force_z': -8.675254344940186, 'radial_force': 4.361629181525475, 'axial_force': -8.675254344940186, 'contributions': [{'ion': 1313, 'force': [1.8297994136810303, 3.0413978099823, -6.2925825119018555], 'magnitude': 7.2246012687683105, 'distance': 6.778944969177246, 'directional_contribution': 1.0942816903629335}, {'ion': 1460, 'force': [0.39816418290138245, 0.7082671523094177, -2.38267183303833], 'magnitude': 2.517399787902832, 'distance': 11.483993530273438, 'directional_contribution': 0.4636445661517268}]}, 3190: {'frame': 3190, 'ionic_force': [3.4962931871414185, 1.3681584894657135, -6.685306072235107], 'ionic_force_magnitude': 7.667414230509018, 'motion_vector': [-0.8215522766113281, -0.8835487365722656, -0.6362762451171875], 'cosine_ionic_motion': 0.016492182069415995, 'ionic_motion_component': 0.12645239149118587, 'ionic_force_x': 3.4962931871414185, 'ionic_force_y': 1.3681584894657135, 'ionic_force_z': -6.685306072235107, 'radial_force': 3.7544538487972656, 'axial_force': -6.685306072235107, 'contributions': [{'ion': 1313, 'force': [2.741168975830078, 1.0629887580871582, -4.5104899406433105], 'magnitude': 5.38409423828125, 'distance': 7.852586269378662, 'directional_contribution': -0.23555877116258728}, {'ion': 1460, 'force': [0.7551242113113403, 0.3051697313785553, -2.174816131591797], 'magnitude': 2.3223190307617188, 'distance': 11.956610679626465, 'directional_contribution': 0.3620110105470804}]}, 3191: {'frame': 3191, 'ionic_force': [3.8587116599082947, 0.6158474087715149, -7.850509166717529], 'ionic_force_magnitude': 8.769231316479157, 'motion_vector': [1.4482460021972656, 0.2650604248046875, 0.5260162353515625], 'cosine_ionic_motion': 0.11831350931893483, 'ionic_motion_component': 1.037518531082152, 'ionic_force_x': 3.8587116599082947, 'ionic_force_y': 0.6158474087715149, 'ionic_force_z': -7.850509166717529, 'radial_force': 3.9075470189369206, 'axial_force': -7.850509166717529, 'contributions': [{'ion': 1313, 'force': [2.9662954807281494, 0.4142634868621826, -5.240616798400879], 'magnitude': 6.036106586456299, 'distance': 7.416356086730957, 'directional_contribution': 1.0547725824270096}, {'ion': 1460, 'force': [0.8924161791801453, 0.20158392190933228, -2.6098923683166504], 'magnitude': 2.7656068801879883, 'distance': 10.956549644470215, 'directional_contribution': -0.01725393739331782}]}, 3192: {'frame': 3192, 'ionic_force': [4.3233126401901245, 0.8234727382659912, -6.483328104019165], 'ionic_force_magnitude': 7.835986398652038, 'motion_vector': [-1.4279060363769531, -0.3152008056640625, 0.24273681640625], 'cosine_ionic_motion': -0.6893186884874044, 'ionic_motion_component': -5.401491867323962, 'ionic_force_x': 4.3233126401901245, 'ionic_force_y': 0.8234727382659912, 'ionic_force_z': -6.483328104019165, 'radial_force': 4.401038461033372, 'axial_force': -6.483328104019165, 'contributions': [{'ion': 1313, 'force': [3.2284295558929443, 0.5756868124008179, -4.195573329925537], 'magnitude': 5.325129985809326, 'distance': 7.895941734313965, 'directional_contribution': -3.919452270043964}, {'ion': 1460, 'force': [1.0948830842971802, 0.24778592586517334, -2.287754774093628], 'magnitude': 2.548330545425415, 'distance': 11.41408634185791, 'directional_contribution': -1.4820395787670382}]}, 3193: {'frame': 3193, 'ionic_force': [4.54551488161087, 0.7150068581104279, -9.185447692871094], 'ionic_force_magnitude': 10.273528588783979, 'motion_vector': [-1.265380859375, 0.5024642944335938, 1.421234130859375], 'cosine_ionic_motion': -0.9123378360158684, 'ionic_motion_component': -9.372928840938334, 'ionic_force_x': 4.54551488161087, 'ionic_force_y': 0.7150068581104279, 'ionic_force_z': -9.185447692871094, 'radial_force': 4.6014063443789475, 'axial_force': -9.185447692871094, 'contributions': [{'ion': 1313, 'force': [3.558159112930298, 0.47408899664878845, -6.336966037750244], 'magnitude': 7.283020973205566, 'distance': 6.751701831817627, 'directional_contribution': -6.74268190178226}, {'ion': 1460, 'force': [0.9873557686805725, 0.2409178614616394, -2.8484816551208496], 'magnitude': 3.0243611335754395, 'distance': 10.477368354797363, 'directional_contribution': -2.630246830321605}]}, 3194: {'frame': 3194, 'ionic_force': [7.131795823574066, 3.0327844619750977, -18.466155529022217], 'ionic_force_magnitude': 20.026462325732517, 'motion_vector': [1.2636222839355469, 1.3273963928222656, -1.654449462890625], 'cosine_ionic_motion': 0.8815604678031085, 'ionic_motion_component': 17.654537496314084, 'ionic_force_x': 7.131795823574066, 'ionic_force_y': 3.0327844619750977, 'ionic_force_z': -18.466155529022217, 'radial_force': 7.749857628495254, 'axial_force': -18.466155529022217, 'contributions': [{'ion': 1313, 'force': [5.728073596954346, 2.3258800506591797, -12.010092735290527], 'magnitude': 13.507882118225098, 'distance': 4.957644939422607, 'directional_contribution': 12.229917716004195}, {'ion': 1387, 'force': [0.3024868369102478, 0.18391072750091553, -1.7984228134155273], 'magnitude': 1.832933783531189, 'distance': 13.45846939086914, 'directional_contribution': 1.4587937625408287}, {'ion': 1460, 'force': [1.1012353897094727, 0.5229936838150024, -4.657639980316162], 'magnitude': 4.814545631408691, 'distance': 8.3040771484375, 'directional_contribution': 3.965825965203912}]}, 3195: {'frame': 3195, 'ionic_force': [4.266230762004852, 2.5804542303085327, -8.203031539916992], 'ionic_force_magnitude': 9.599437243623537, 'motion_vector': [-2.6438636779785156, 0.3204536437988281, -0.75738525390625], 'cosine_ionic_motion': -0.15950752621456848, 'ionic_motion_component': -1.5311824877823865, 'ionic_force_x': 4.266230762004852, 'ionic_force_y': 2.5804542303085327, 'ionic_force_z': -8.203031539916992, 'radial_force': 4.985927090260517, 'axial_force': -8.203031539916992, 'contributions': [{'ion': 1313, 'force': [3.318345785140991, 1.9544174671173096, -5.576297760009766], 'magnitude': 6.776891708374023, 'distance': 6.99928617477417, 'directional_contribution': -1.4170494408500325}, {'ion': 1460, 'force': [0.9478849768638611, 0.6260367631912231, -2.6267337799072266], 'magnitude': 2.8618416786193848, 'distance': 10.770756721496582, 'directional_contribution': -0.11413311435657825}]}, 3196: {'frame': 3196, 'ionic_force': [0.6016596853733063, 2.649301290512085, -8.311489343643188], 'ionic_force_magnitude': 8.744235061708187, 'motion_vector': [2.318988800048828, -2.4310836791992188, 0.22534942626953125], 'cosine_ionic_motion': -0.2349655890604089, 'ionic_motion_component': -2.0545943421569453, 'ionic_force_x': 0.6016596853733063, 'ionic_force_y': 2.649301290512085, 'ionic_force_z': -8.311489343643188, 'radial_force': 2.716761252836271, 'axial_force': -8.311489343643188, 'contributions': [{'ion': 1313, 'force': [0.49341556429862976, 2.0448687076568604, -5.6436381340026855], 'magnitude': 6.022922515869141, 'distance': 7.424468994140625, 'directional_contribution': -1.5142172100840625}, {'ion': 1460, 'force': [0.10824412107467651, 0.6044325828552246, -2.667851209640503], 'magnitude': 2.7376058101654053, 'distance': 11.01244068145752, 'directional_contribution': -0.5403771640603434}]}, 3197: {'frame': 3197, 'ionic_force': [2.8209893107414246, 0.17508456483483315, -8.191557884216309], 'ionic_force_magnitude': 8.665463395954491, 'motion_vector': [-2.359294891357422, 1.4584197998046875, 2.7145614624023438], 'cosine_ionic_motion': -0.8515068024527294, 'ionic_motion_component': -7.378701028060378, 'ionic_force_x': 2.8209893107414246, 'ionic_force_y': 0.17508456483483315, 'ionic_force_z': -8.191557884216309, 'radial_force': 2.8264173959556613, 'axial_force': -8.191557884216309, 'contributions': [{'ion': 1313, 'force': [2.2362687587738037, 0.05940436199307442, -5.672110557556152], 'magnitude': 6.097315788269043, 'distance': 7.379036903381348, 'directional_contribution': -5.304486381330342}, {'ion': 1460, 'force': [0.5847205519676208, 0.11568020284175873, -2.5194473266601562], 'magnitude': 2.5889949798583984, 'distance': 11.32409381866455, 'directional_contribution': -2.074214723975322}]}, 3198: {'frame': 3198, 'ionic_force': [4.809750139713287, 10.997350573539734, -26.898103833198547], 'ionic_force_magnitude': 29.45476881364607, 'motion_vector': [0.19825363159179688, 0.10056686401367188, -2.5326690673828125], 'cosine_ionic_motion': 0.9372048718855969, 'ionic_motion_component': 27.605152832413037, 'ionic_force_x': 4.809750139713287, 'ionic_force_y': 10.997350573539734, 'ionic_force_z': -26.898103833198547, 'radial_force': 12.003141923838388, 'axial_force': -26.898103833198547, 'contributions': [{'ion': 1313, 'force': [3.9049830436706543, 9.421380996704102, -19.212223052978516], 'magnitude': 21.751340866088867, 'distance': 3.906843662261963, 'directional_contribution': 19.815816810828306}, {'ion': 1387, 'force': [0.15719091892242432, 0.2684478759765625, -1.947790265083313], 'magnitude': 1.9724756479263306, 'distance': 12.973681449890137, 'directional_contribution': 1.9632065286741396}, {'ion': 1460, 'force': [0.7475761771202087, 1.3075217008590698, -5.738090515136719], 'magnitude': 5.932466983795166, 'distance': 7.4808573722839355, 'directional_contribution': 5.8261289687319895}]}, 3199: {'frame': 3199, 'ionic_force': [0.9833395779132843, 3.1130231618881226, -10.068522930145264], 'ionic_force_magnitude': 10.58456536315042, 'motion_vector': [-0.02933502197265625, -3.176746368408203, 1.2943191528320312], 'cosine_ionic_motion': -0.6320647076797856, 'ionic_motion_component': -6.6901302121772535, 'ionic_force_x': 0.9833395779132843, 'ionic_force_y': 3.1130231618881226, 'ionic_force_z': -10.068522930145264, 'radial_force': 3.264639326471241, 'axial_force': -10.068522930145264, 'contributions': [{'ion': 1313, 'force': [0.8440772891044617, 2.4483911991119385, -7.0417280197143555], 'magnitude': 7.502867221832275, 'distance': 6.652048587799072, 'directional_contribution': -4.931431210428519}, {'ion': 1460, 'force': [0.13926228880882263, 0.6646319627761841, -3.026794910430908], 'magnitude': 3.102034330368042, 'distance': 10.345362663269043, 'directional_contribution': -1.7586989570614022}]}, 3200: {'frame': 3200, 'ionic_force': [1.5398932620882988, -3.925731360912323, -14.942134141921997], 'ionic_force_magnitude': 15.525785348634267, 'motion_vector': [-0.7101936340332031, -1.3734970092773438, -0.6399917602539062], 'cosine_ionic_motion': 0.5334978917055188, 'ionic_motion_component': 8.282973750568814, 'ionic_force_x': 1.5398932620882988, 'ionic_force_y': -3.925731360912323, 'ionic_force_z': -14.942134141921997, 'radial_force': 4.21694652286171, 'axial_force': -14.942134141921997, 'contributions': [{'ion': 1313, 'force': [1.2463655471801758, -3.3982043266296387, -10.489591598510742], 'magnitude': 11.096519470214844, 'distance': 5.469852924346924, 'directional_contribution': 6.2717565039260705}, {'ion': 1387, 'force': [0.09594348818063736, -0.13932183384895325, -1.5808546543121338], 'magnitude': 1.5898796319961548, 'distance': 14.450634956359863, 'directional_contribution': 0.6782090140143298}, {'ion': 1460, 'force': [0.19758422672748566, -0.3882052004337311, -2.871687889099121], 'magnitude': 2.9045369625091553, 'distance': 10.691302299499512, 'directional_contribution': 1.3330083846379597}]}, 3201: {'frame': 3201, 'ionic_force': [0.3855626368895173, -4.750433802604675, -10.51581072807312], 'ionic_force_magnitude': 11.54545603813691, 'motion_vector': [-0.7017936706542969, -0.01294708251953125, -0.8671646118164062], 'cosine_ionic_motion': 0.6917273308343146, 'ionic_motion_component': 7.986307488525365, 'ionic_force_x': 0.3855626368895173, 'ionic_force_y': -4.750433802604675, 'ionic_force_z': -10.51581072807312, 'radial_force': 4.766054957708137, 'axial_force': -10.51581072807312, 'contributions': [{'ion': 1313, 'force': [0.3916058838367462, -3.7393531799316406, -7.343410015106201], 'magnitude': 8.249957084655762, 'distance': 6.343708038330078, 'directional_contribution': 5.504932773013024}, {'ion': 1460, 'force': [-0.0060432469472289085, -1.0110806226730347, -3.172400712966919], 'magnitude': 3.3296315670013428, 'distance': 9.985526084899902, 'directional_contribution': 2.4813749044541478}]}, 3202: {'frame': 3202, 'ionic_force': [-0.8432059288024902, -2.719889461994171, -7.3930346965789795], 'ionic_force_magnitude': 7.9224842662295805, 'motion_vector': [-0.6875076293945312, -0.4496726989746094, -0.5331268310546875], 'cosine_ionic_motion': 0.7403493413536228, 'ionic_motion_component': 5.8654060083875095, 'ionic_force_x': -0.8432059288024902, 'ionic_force_y': -2.719889461994171, 'ionic_force_z': -7.3930346965789795, 'radial_force': 2.8475945855817697, 'axial_force': -7.3930346965789795, 'contributions': [{'ion': 1313, 'force': [-0.6528485417366028, -2.2744596004486084, -5.246335506439209], 'magnitude': 5.755294322967529, 'distance': 7.595130920410156, 'directional_contribution': 4.358635548107902}, {'ion': 1460, 'force': [-0.19035738706588745, -0.44542986154556274, -2.1466991901397705], 'magnitude': 2.2006728649139404, 'distance': 12.282628059387207, 'directional_contribution': 1.506770640505895}]}, 3203: {'frame': 3203, 'ionic_force': [-0.9554902762174606, -3.667130023241043, -8.258195757865906], 'ionic_force_magnitude': 9.086176393320592, 'motion_vector': [-1.41168212890625, -0.13762283325195312, 1.837890625], 'cosine_ionic_motion': -0.6316526643237212, 'ionic_motion_component': -5.739307527356252, 'ionic_force_x': -0.9554902762174606, 'ionic_force_y': -3.667130023241043, 'ionic_force_z': -8.258195757865906, 'radial_force': 3.7895651828807444, 'axial_force': -8.258195757865906, 'contributions': [{'ion': 1313, 'force': [-0.582251787185669, -2.546912908554077, -4.254993915557861], 'magnitude': 4.993070602416992, 'distance': 8.154272079467773, 'directional_contribution': -2.863485398333836}, {'ion': 1387, 'force': [-0.14848487079143524, -0.3223477303981781, -1.5331422090530396], 'magnitude': 1.5736838579177856, 'distance': 14.52480411529541, 'directional_contribution': -1.1043327598431159}, {'ion': 1460, 'force': [-0.22475361824035645, -0.7978693842887878, -2.470059633255005], 'magnitude': 2.6054375171661377, 'distance': 11.288304328918457, 'directional_contribution': -1.7714891742978693}]}, 3204: {'frame': 3204, 'ionic_force': [-4.891388177871704, -6.8576348423957825, -12.308661103248596], 'ionic_force_magnitude': 14.914957998361531, 'motion_vector': [2.0974998474121094, 3.643840789794922, -4.29998779296875], 'cosine_ionic_motion': 0.19709987365095533, 'ionic_motion_component': 2.9397363369863636, 'ionic_force_x': -4.891388177871704, 'ionic_force_y': -6.8576348423957825, 'ionic_force_z': -12.308661103248596, 'radial_force': 8.423350517357312, 'axial_force': -12.308661103248596, 'contributions': [{'ion': 1313, 'force': [-3.5466692447662354, -5.008401393890381, -7.102478504180908], 'magnitude': 9.386594772338867, 'distance': 5.947234153747559, 'directional_contribution': 0.8067335028722198}, {'ion': 1387, 'force': [-0.37983453273773193, -0.5484148859977722, -1.9710179567337036], 'magnitude': 2.0808520317077637, 'distance': 12.631312370300293, 'directional_contribution': 0.9445309271792581}, {'ion': 1460, 'force': [-0.9648844003677368, -1.3008185625076294, -3.2351646423339844], 'magnitude': 3.6179304122924805, 'distance': 9.579413414001465, 'directional_contribution': 1.1884714828583895}]}, 3205: {'frame': 3205, 'ionic_force': [-0.6016021221876144, 0.16618561744689941, -6.180601716041565], 'ionic_force_magnitude': 6.21203512105355, 'motion_vector': [-2.4292831420898438, -0.1877899169921875, 1.3914337158203125], 'cosine_ionic_motion': -0.41133902842181963, 'ionic_motion_component': -2.555252491216388, 'ionic_force_x': -0.6016021221876144, 'ionic_force_y': 0.16618561744689941, 'ionic_force_z': -6.180601716041565, 'radial_force': 0.6241336177989842, 'axial_force': -6.180601716041565, 'contributions': [{'ion': 1313, 'force': [-0.47208482027053833, 0.13534782826900482, -4.1929497718811035], 'magnitude': 4.221612453460693, 'distance': 8.868085861206055, 'directional_contribution': -1.679636592081345}, {'ion': 1460, 'force': [-0.1295173019170761, 0.030837789177894592, -1.9876519441604614], 'magnitude': 1.9921059608459473, 'distance': 12.909601211547852, 'directional_contribution': -0.8756158111541572}]}, 3206: {'frame': 3206, 'ionic_force': [-2.3814292550086975, -0.07051205262541771, -6.440298318862915], 'ionic_force_magnitude': 6.866849327175107, 'motion_vector': [4.136890411376953, -0.5502357482910156, -0.2530059814453125], 'cosine_ionic_motion': -0.2850374206019799, 'ionic_motion_component': -1.9573090198804335, 'ionic_force_x': -2.3814292550086975, 'ionic_force_y': -0.07051205262541771, 'ionic_force_z': -6.440298318862915, 'radial_force': 2.3824729266408737, 'axial_force': -6.440298318862915, 'contributions': [{'ion': 1313, 'force': [-1.8158272504806519, -0.09443157911300659, -4.377440452575684], 'magnitude': 4.740056037902832, 'distance': 8.369071960449219, 'directional_contribution': -1.5193549276856588}, {'ion': 1460, 'force': [-0.5656020045280457, 0.023919526487588882, -2.0628578662872314], 'magnitude': 2.1391260623931885, 'distance': 12.458072662353516, 'directional_contribution': -0.4379541001504612}]}, 3207: {'frame': 3207, 'ionic_force': [0.5504616945981979, -0.20011846721172333, -6.7197370529174805], 'ionic_force_magnitude': 6.7452147140392205, 'motion_vector': [-0.4560203552246094, -0.9889564514160156, 2.2855987548828125], 'cosine_ionic_motion': -0.9024609612745147, 'ionic_motion_component': -6.087292954834836, 'ionic_force_x': 0.5504616945981979, 'ionic_force_y': -0.20011846721172333, 'ionic_force_z': -6.7197370529174805, 'radial_force': 0.5857093802724089, 'axial_force': -6.7197370529174805, 'contributions': [{'ion': 1313, 'force': [0.4108598530292511, -0.13039463758468628, -4.540388107299805], 'magnitude': 4.5608038902282715, 'distance': 8.531950950622559, 'directional_contribution': -4.1219528871178355}, {'ion': 1460, 'force': [0.13960184156894684, -0.06972382962703705, -2.179348945617676], 'magnitude': 2.1849284172058105, 'distance': 12.326803207397461, 'directional_contribution': -1.9653401082788329}]}, 3208: {'frame': 3208, 'ionic_force': [0.6337229162454605, -2.9306737780570984, -10.785738706588745], 'ionic_force_magnitude': 11.194758281212362, 'motion_vector': [0.30518341064453125, 1.3927268981933594, -1.3763351440429688], 'cosine_ionic_motion': 0.49388111416975305, 'ionic_motion_component': 5.528879692786231, 'ionic_force_x': 0.6337229162454605, 'ionic_force_y': -2.9306737780570984, 'ionic_force_z': -10.785738706588745, 'radial_force': 2.998408499181877, 'axial_force': -10.785738706588745, 'contributions': [{'ion': 1313, 'force': [0.44283202290534973, -2.438164234161377, -7.620040416717529], 'magnitude': 8.012849807739258, 'distance': 6.436882019042969, 'directional_contribution': 3.6469636778250076}, {'ion': 1460, 'force': [0.19089089334011078, -0.49250954389572144, -3.165698289871216], 'magnitude': 3.2094626426696777, 'distance': 10.170747756958008, 'directional_contribution': 1.881915847192219}]}, 3209: {'frame': 3209, 'ionic_force': [0.43650949746370316, -0.5205679461359978, -6.388556241989136], 'ionic_force_magnitude': 6.424576436231311, 'motion_vector': [-2.8515777587890625, -0.7392349243164062, -1.9197006225585938], 'cosine_ionic_motion': 0.5048408404249863, 'ionic_motion_component': 3.2433885674415786, 'ionic_force_x': 0.43650949746370316, 'ionic_force_y': -0.5205679461359978, 'ionic_force_z': -6.388556241989136, 'radial_force': 0.6793611174627716, 'axial_force': -6.388556241989136, 'contributions': [{'ion': 1313, 'force': [0.33712059259414673, -0.4496636390686035, -4.658642292022705], 'magnitude': 4.692419052124023, 'distance': 8.411445617675781, 'directional_contribution': 2.3646068414033508}, {'ion': 1460, 'force': [0.09938890486955643, -0.07090430706739426, -1.7299139499664307], 'magnitude': 1.7342168092727661, 'distance': 13.836216926574707, 'directional_contribution': 0.8787818106888906}]}, 3210: {'frame': 3210, 'ionic_force': [-1.0865365266799927, -0.4411945790052414, -5.631094336509705], 'ionic_force_magnitude': 5.751907310364546, 'motion_vector': [-0.060733795166015625, -0.4639701843261719, -0.5265655517578125], 'cosine_ionic_motion': 0.7986072361519804, 'ionic_motion_component': 4.593514799732601, 'ionic_force_x': -1.0865365266799927, 'ionic_force_y': -0.4411945790052414, 'ionic_force_z': -5.631094336509705, 'radial_force': 1.1726953058460814, 'axial_force': -5.631094336509705, 'contributions': [{'ion': 1313, 'force': [-0.8106954097747803, -0.30610916018486023, -3.7750306129455566], 'magnitude': 3.87321400642395, 'distance': 9.258343696594238, 'directional_contribution': 3.093350535334695}, {'ion': 1460, 'force': [-0.2758411169052124, -0.13508541882038116, -1.856063723564148], 'magnitude': 1.8813050985336304, 'distance': 13.284322738647461, 'directional_contribution': 1.500164348614363}]}, 3211: {'frame': 3211, 'ionic_force': [-1.4129315614700317, -1.1412988752126694, -6.022145748138428], 'ionic_force_magnitude': 6.290085701465569, 'motion_vector': [0.17093276977539062, 2.88043212890625, 2.7339096069335938], 'cosine_ionic_motion': -0.7996257345609912, 'ionic_motion_component': -5.029714399485993, 'ionic_force_x': -1.4129315614700317, 'ionic_force_y': -1.1412988752126694, 'ionic_force_z': -6.022145748138428, 'radial_force': 1.816298081252041, 'axial_force': -6.022145748138428, 'contributions': [{'ion': 1313, 'force': [-1.1177146434783936, -0.9046632647514343, -4.136012077331543], 'magnitude': 4.378846645355225, 'distance': 8.707413673400879, 'directional_contribution': -3.54829498140504}, {'ion': 1460, 'force': [-0.2952169179916382, -0.23663561046123505, -1.8861336708068848], 'magnitude': 1.9237072467803955, 'distance': 13.137101173400879, 'directional_contribution': -1.4814192978902772}]}, 3212: {'frame': 3212, 'ionic_force': [-2.1320821791887283, 1.880209058523178, -9.907267928123474], 'ionic_force_magnitude': 10.307032469250826, 'motion_vector': [-0.551544189453125, -2.786346435546875, -0.7046661376953125], 'cosine_ionic_motion': 0.09675015725847247, 'ionic_motion_component': 0.9972070122681992, 'ionic_force_x': -2.1320821791887283, 'ionic_force_y': 1.880209058523178, 'ionic_force_z': -9.907267928123474, 'radial_force': 2.8427030310193806, 'axial_force': -9.907267928123474, 'contributions': [{'ion': 1313, 'force': [-1.564578652381897, 1.3044873476028442, -5.753448963165283], 'magnitude': 6.10342264175415, 'distance': 7.375344753265381, 'directional_contribution': 0.43821464403485066}, {'ion': 1387, 'force': [-0.18752484023571014, 0.17749661207199097, -1.5429457426071167], 'magnitude': 1.5644015073776245, 'distance': 14.567831993103027, 'directional_contribution': 0.23786760187487754}, {'ion': 1460, 'force': [-0.3799786865711212, 0.3982250988483429, -2.610873222351074], 'magnitude': 2.6682627201080322, 'distance': 11.154619216918945, 'directional_contribution': 0.32112471648709473}]}, 3213: {'frame': 3213, 'ionic_force': [-3.1511535048484802, -1.7650651186704636, -9.942092418670654], 'ionic_force_magnitude': 10.57782704271792, 'motion_vector': [-0.14082717895507812, -0.13962173461914062, -1.2342300415039062], 'cosine_ionic_motion': 0.9801949420071061, 'ionic_motion_component': 10.368332564698092, 'ionic_force_x': -3.1511535048484802, 'ionic_force_y': -1.7650651186704636, 'ionic_force_z': -9.942092418670654, 'radial_force': 3.611817172043186, 'axial_force': -9.942092418670654, 'contributions': [{'ion': 1313, 'force': [-2.6584701538085938, -1.5168129205703735, -7.454015254974365], 'magnitude': 8.057948112487793, 'distance': 6.418843746185303, 'directional_contribution': 7.82853127435799}, {'ion': 1460, 'force': [-0.4926833510398865, -0.24825219810009003, -2.488077163696289], 'magnitude': 2.5485081672668457, 'distance': 11.413688659667969, 'directional_contribution': 2.5398012725363297}]}, 3214: {'frame': 3214, 'ionic_force': [-1.5444872081279755, -1.1262651979923248, -6.004039764404297], 'ionic_force_magnitude': 6.300984647245829, 'motion_vector': [0.7136573791503906, -0.08641815185546875, -0.5668869018554688], 'cosine_ionic_motion': 0.4158258844145278, 'ionic_motion_component': 2.6201125136233583, 'ionic_force_x': -1.5444872081279755, 'ionic_force_y': -1.1262651979923248, 'ionic_force_z': -6.004039764404297, 'radial_force': 1.9115213920538894, 'axial_force': -6.004039764404297, 'contributions': [{'ion': 1313, 'force': [-1.1439869403839111, -0.8971394300460815, -3.885117769241333], 'magnitude': 4.14821720123291, 'distance': 8.94619369506836, 'directional_contribution': 1.5986245614389398}, {'ion': 1460, 'force': [-0.40050026774406433, -0.2291257679462433, -2.118921995162964], 'magnitude': 2.1685779094696045, 'distance': 12.373186111450195, 'directional_contribution': 1.0214880782956504}]}, 3215: {'frame': 3215, 'ionic_force': [-0.8170889019966125, -0.7826167792081833, -5.666041016578674], 'ionic_force_magnitude': 5.777901357622516, 'motion_vector': [-0.340850830078125, 0.852874755859375, 0.39165496826171875], 'cosine_ionic_motion': -0.4520783780553534, 'ionic_motion_component': -2.6120642743178117, 'ionic_force_x': -0.8170889019966125, 'ionic_force_y': -0.7826167792081833, 'ionic_force_z': -5.666041016578674, 'radial_force': 1.1314253386168351, 'axial_force': -5.666041016578674, 'contributions': [{'ion': 1313, 'force': [-0.5830154418945312, -0.575762152671814, -3.7722537517547607], 'magnitude': 3.8602211475372314, 'distance': 9.273911476135254, 'directional_contribution': -1.772442377020944}, {'ion': 1460, 'force': [-0.2340734601020813, -0.20685462653636932, -1.8937872648239136], 'magnitude': 1.919377326965332, 'distance': 13.151910781860352, 'directional_contribution': -0.8396218303850214}]}, 3216: {'frame': 3216, 'ionic_force': [-1.1128128170967102, -0.3707253783941269, -5.447134375572205], 'ionic_force_magnitude': 5.571989104226656, 'motion_vector': [-0.07701492309570312, 0.34079742431640625, -0.7521133422851562], 'cosine_ionic_motion': 0.8778023359725989, 'ionic_motion_component': 4.891105051704027, 'ionic_force_x': -1.1128128170967102, 'ionic_force_y': -0.3707253783941269, 'ionic_force_z': -5.447134375572205, 'radial_force': 1.172940608931324, 'axial_force': -5.447134375572205, 'contributions': [{'ion': 1313, 'force': [-0.8524911999702454, -0.24588410556316376, -3.6285605430603027], 'magnitude': 3.7354586124420166, 'distance': 9.427511215209961, 'directional_contribution': 3.268933585247774}, {'ion': 1460, 'force': [-0.26032161712646484, -0.12484127283096313, -1.8185738325119019], 'magnitude': 1.8413482904434204, 'distance': 13.427682876586914, 'directional_contribution': 1.62217142084992}]}, 3217: {'frame': 3217, 'ionic_force': [-1.4508692920207977, -0.46767644584178925, -6.193138003349304], 'ionic_force_magnitude': 6.377985676454091, 'motion_vector': [0.3350868225097656, -0.818328857421875, 1.3462371826171875], 'cosine_ionic_motion': -0.8216643914566963, 'ionic_motion_component': -5.240563719563176, 'ionic_force_x': -1.4508692920207977, 'ionic_force_y': -0.46767644584178925, 'ionic_force_z': -6.193138003349304, 'radial_force': 1.5243828129850252, 'axial_force': -6.193138003349304, 'contributions': [{'ion': 1313, 'force': [-1.1386771202087402, -0.4060887098312378, -4.431575775146484], 'magnitude': 4.593512535095215, 'distance': 8.501520156860352, 'directional_contribution': -3.7345610560322555}, {'ion': 1460, 'force': [-0.3121921718120575, -0.06158773601055145, -1.7615622282028198], 'magnitude': 1.7900722026824951, 'distance': 13.618640899658203, 'directional_contribution': -1.5060028340960763}]}, 3218: {'frame': 3218, 'ionic_force': [-1.4466897547245026, -1.0704763382673264, -6.978714466094971], 'ionic_force_magnitude': 7.207030347965677, 'motion_vector': [-0.02951812744140625, -1.8394279479980469, 2.84552001953125], 'cosine_ionic_motion': -0.7307948046456053, 'ionic_motion_component': -5.266860335216526, 'ionic_force_x': -1.4466897547245026, 'ionic_force_y': -1.0704763382673264, 'ionic_force_z': -6.978714466094971, 'radial_force': 1.7996752032561498, 'axial_force': -6.978714466094971, 'contributions': [{'ion': 1313, 'force': [-1.0941110849380493, -0.8335011601448059, -4.779510498046875], 'magnitude': 4.973482131958008, 'distance': 8.170313835144043, 'directional_contribution': -3.5517299026190443}, {'ion': 1460, 'force': [-0.35257866978645325, -0.23697517812252045, -2.1992039680480957], 'magnitude': 2.239858865737915, 'distance': 12.174713134765625, 'directional_contribution': -1.7151306360939262}]}, 3219: {'frame': 3219, 'ionic_force': [-3.3365544825792313, -6.55618155002594, -12.028961539268494], 'ionic_force_magnitude': 14.100071916317333, 'motion_vector': [1.9461097717285156, 0.4013671875, -0.7011947631835938], 'cosine_ionic_motion': -0.02322678217601994, 'ionic_motion_component': -0.32749929906651876, 'ionic_force_x': -3.3365544825792313, 'ionic_force_y': -6.55618155002594, 'ionic_force_z': -12</t>
+          <t>{3185: {'frame': 3185, 'ionic_force': [1.3455531299114227, -1.2103240936994553, -9.767556190490723], 'ionic_force_magnitude': 9.93380851293186, 'motion_vector': [3.3021926879882812, 1.7625465393066406, 0.34154510498046875], 'cosine_ionic_motion': -0.027479692611883776, 'ionic_motion_component': -0.27297800440068176, 'ionic_force_x': 1.3455531299114227, 'ionic_force_y': -1.2103240936994553, 'ionic_force_z': -9.767556190490723, 'radial_force': 1.8098059667278792, 'axial_force': -9.767556190490723, 'contributions': [{'ion': 1313, 'force': [1.0481852293014526, -0.9845649600028992, -6.827840805053711], 'magnitude': 6.9776411056518555, 'distance': 6.8978657722473145, 'cosine_with_motion': -0.023108002613043896, 'motion_component': -0.1612393407807282}, {'ion': 1460, 'force': [0.2973679006099701, -0.2257591336965561, -2.9397153854370117], 'magnitude': 2.963329553604126, 'distance': 10.584712982177734, 'cosine_with_motion': -0.03770713874789775, 'motion_component': -0.11173867455445306}]}, 3186: {'frame': 3186, 'ionic_force': [3.8716278672218323, 0.9531629383563995, -6.351068735122681], 'ionic_force_magnitude': 7.498939658882293, 'motion_vector': [-1.120147705078125, -0.510986328125, 0.8818283081054688], 'cosine_ionic_motion': -0.917921914123857, 'ionic_motion_component': -6.883441045580538, 'ionic_force_x': 3.8716278672218323, 'ionic_force_y': 0.9531629383563995, 'ionic_force_z': -6.351068735122681, 'radial_force': 3.987232364598893, 'axial_force': -6.351068735122681, 'contributions': [{'ion': 1313, 'force': [2.8922908306121826, 0.682626485824585, -4.142235279083252], 'magnitude': 5.0979838371276855, 'distance': 8.069931030273438, 'cosine_with_motion': -0.9379406452351742, 'motion_component': -4.781606164194734}, {'ion': 1460, 'force': [0.9793370366096497, 0.2705364525318146, -2.2088334560394287], 'magnitude': 2.4313035011291504, 'distance': 11.685558319091797, 'cosine_with_motion': -0.8644888675281329, 'motion_component': -2.101834725921859}]}, 3187: {'frame': 3187, 'ionic_force': [4.825020015239716, 1.0010420382022858, -9.05678677558899], 'ionic_force_magnitude': 10.31059115706736, 'motion_vector': [-4.467868804931641, 3.94091796875, -0.4804229736328125], 'cosine_ionic_motion': -0.2151940520558242, 'ionic_motion_component': -2.218777890180274, 'ionic_force_x': 4.825020015239716, 'ionic_force_y': 1.0010420382022858, 'ionic_force_z': -9.05678677558899, 'radial_force': 4.927768593360696, 'axial_force': -9.05678677558899, 'contributions': [{'ion': 1313, 'force': [3.834963321685791, 0.7111164927482605, -6.247584819793701], 'magnitude': 7.365116596221924, 'distance': 6.713967323303223, 'cosine_with_motion': -0.257383167032912, 'motion_component': -1.8956571041124768}, {'ion': 1460, 'force': [0.9900566935539246, 0.28992554545402527, -2.809201955795288], 'magnitude': 2.992638349533081, 'distance': 10.532752990722656, 'cosine_with_motion': -0.1079719114881787, 'motion_component': -0.32312089049107406}]}, 3188: {'frame': 3188, 'ionic_force': [-0.7788635641336441, 4.744892954826355, -7.823496103286743], 'ionic_force_magnitude': 9.183013061214636, 'motion_vector': [2.9478530883789062, -1.2035942077636719, 0.8451919555664062], 'cosine_ionic_motion': -0.48324645421477935, 'ionic_motion_component': -4.437658500839979, 'ionic_force_x': -0.7788635641336441, 'ionic_force_y': 4.744892954826355, 'ionic_force_z': -7.823496103286743, 'radial_force': 4.808392413717472, 'axial_force': -7.823496103286743, 'contributions': [{'ion': 1313, 'force': [-0.5623465180397034, 3.5319478511810303, -5.200526714324951], 'magnitude': 6.311605930328369, 'distance': 7.252689838409424, 'cosine_with_motion': -0.49556723884648435, 'motion_component': -3.127825041783648}, {'ion': 1460, 'force': [-0.21651704609394073, 1.2129451036453247, -2.622969388961792], 'magnitude': 2.897944688796997, 'distance': 10.703454971313477, 'cosine_with_motion': -0.45198706097319374, 'motion_component': -1.3098335379862371}]}, 3189: {'frame': 3189, 'ionic_force': [2.2279635965824127, 3.7496649622917175, -8.675254344940186], 'ionic_force_magnitude': 9.70998697561115, 'motion_vector': [2.050933837890625, -1.666748046875, -0.683929443359375], 'cosine_ionic_motion': 0.16044574791098273, 'ionic_motion_component': 1.5579261225078322, 'ionic_force_x': 2.2279635965824127, 'ionic_force_y': 3.7496649622917175, 'ionic_force_z': -8.675254344940186, 'radial_force': 4.361629181525475, 'axial_force': -8.675254344940186, 'contributions': [{'ion': 1313, 'force': [1.8297994136810303, 3.0413978099823, -6.2925825119018555], 'magnitude': 7.2246012687683105, 'distance': 6.778944969177246, 'cosine_with_motion': 0.15146603579443732, 'motion_component': 1.0942816903629335}, {'ion': 1460, 'force': [0.39816418290138245, 0.7082671523094177, -2.38267183303833], 'magnitude': 2.517399787902832, 'distance': 11.483993530273438, 'cosine_with_motion': 0.1841759707827572, 'motion_component': 0.4636445661517268}]}, 3190: {'frame': 3190, 'ionic_force': [3.4962931871414185, 1.3681584894657135, -6.685306072235107], 'ionic_force_magnitude': 7.667414230509018, 'motion_vector': [-0.8215522766113281, -0.8835487365722656, -0.6362762451171875], 'cosine_ionic_motion': 0.016492182069415995, 'ionic_motion_component': 0.12645239149118587, 'ionic_force_x': 3.4962931871414185, 'ionic_force_y': 1.3681584894657135, 'ionic_force_z': -6.685306072235107, 'radial_force': 3.7544538487972656, 'axial_force': -6.685306072235107, 'contributions': [{'ion': 1313, 'force': [2.741168975830078, 1.0629887580871582, -4.5104899406433105], 'magnitude': 5.38409423828125, 'distance': 7.852586269378662, 'cosine_with_motion': -0.04375086242833566, 'motion_component': -0.23555877116258728}, {'ion': 1460, 'force': [0.7551242113113403, 0.3051697313785553, -2.174816131591797], 'magnitude': 2.3223190307617188, 'distance': 11.956610679626465, 'cosine_with_motion': 0.15588340078660728, 'motion_component': 0.36201101054708035}]}, 3191: {'frame': 3191, 'ionic_force': [3.8587116599082947, 0.6158474087715149, -7.850509166717529], 'ionic_force_magnitude': 8.769231316479157, 'motion_vector': [1.4482460021972656, 0.2650604248046875, 0.5260162353515625], 'cosine_ionic_motion': 0.11831350931893483, 'ionic_motion_component': 1.037518531082152, 'ionic_force_x': 3.8587116599082947, 'ionic_force_y': 0.6158474087715149, 'ionic_force_z': -7.850509166717529, 'radial_force': 3.9075470189369206, 'axial_force': -7.850509166717529, 'contributions': [{'ion': 1313, 'force': [2.9662954807281494, 0.4142634868621826, -5.240616798400879], 'magnitude': 6.036106586456299, 'distance': 7.416356086730957, 'cosine_with_motion': 0.17474385144598134, 'motion_component': 1.0547725824270096}, {'ion': 1460, 'force': [0.8924161791801453, 0.20158392190933228, -2.6098923683166504], 'magnitude': 2.7656068801879883, 'distance': 10.956549644470215, 'cosine_with_motion': -0.006238752915845556, 'motion_component': -0.01725393739331782}]}, 3192: {'frame': 3192, 'ionic_force': [4.3233126401901245, 0.8234727382659912, -6.483328104019165], 'ionic_force_magnitude': 7.835986398652038, 'motion_vector': [-1.4279060363769531, -0.3152008056640625, 0.24273681640625], 'cosine_ionic_motion': -0.6893186884874044, 'ionic_motion_component': -5.401491867323962, 'ionic_force_x': 4.3233126401901245, 'ionic_force_y': 0.8234727382659912, 'ionic_force_z': -6.483328104019165, 'radial_force': 4.401038461033372, 'axial_force': -6.483328104019165, 'contributions': [{'ion': 1313, 'force': [3.2284295558929443, 0.5756868124008179, -4.195573329925537], 'magnitude': 5.325129985809326, 'distance': 7.895941734313965, 'cosine_with_motion': -0.7360294220437638, 'motion_component': -3.919452270043964}, {'ion': 1460, 'force': [1.0948830842971802, 0.24778592586517334, -2.287754774093628], 'magnitude': 2.548330545425415, 'distance': 11.41408634185791, 'cosine_with_motion': -0.5815727327514694, 'motion_component': -1.4820395787670382}]}, 3193: {'frame': 3193, 'ionic_force': [4.54551488161087, 0.7150068581104279, -9.185447692871094], 'ionic_force_magnitude': 10.273528588783979, 'motion_vector': [-1.265380859375, 0.5024642944335938, 1.421234130859375], 'cosine_ionic_motion': -0.9123378360158684, 'ionic_motion_component': -9.372928840938334, 'ionic_force_x': 4.54551488161087, 'ionic_force_y': 0.7150068581104279, 'ionic_force_z': -9.185447692871094, 'radial_force': 4.6014063443789475, 'axial_force': -9.185447692871094, 'contributions': [{'ion': 1313, 'force': [3.558159112930298, 0.47408899664878845, -6.336966037750244], 'magnitude': 7.283020973205566, 'distance': 6.751701831817627, 'cosine_with_motion': -0.9258083810288427, 'motion_component': -6.74268190178226}, {'ion': 1460, 'force': [0.9873557686805725, 0.2409178614616394, -2.8484816551208496], 'magnitude': 3.0243611335754395, 'distance': 10.477368354797363, 'cosine_with_motion': -0.8696867439300969, 'motion_component': -2.630246830321605}]}, 3194: {'frame': 3194, 'ionic_force': [7.131795823574066, 3.0327844619750977, -18.466155529022217], 'ionic_force_magnitude': 20.026462325732517, 'motion_vector': [1.2636222839355469, 1.3273963928222656, -1.654449462890625], 'cosine_ionic_motion': 0.8815604678031085, 'ionic_motion_component': 17.654537496314084, 'ionic_force_x': 7.131795823574066, 'ionic_force_y': 3.0327844619750977, 'ionic_force_z': -18.466155529022217, 'radial_force': 7.749857628495254, 'axial_force': -18.466155529022217, 'contributions': [{'ion': 1313, 'force': [5.728073596954346, 2.3258800506591797, -12.010092735290527], 'magnitude': 13.507882118225098, 'distance': 4.957644939422607, 'cosine_with_motion': 0.9053912250945034, 'motion_component': 12.229917716004195}, {'ion': 1387, 'force': [0.3024868369102478, 0.18391072750091553, -1.7984228134155273], 'magnitude': 1.832933783531189, 'distance': 13.45846939086914, 'cosine_with_motion': 0.7958791628889741, 'motion_component': 1.4587937625408287}, {'ion': 1460, 'force': [1.1012353897094727, 0.5229936838150024, -4.657639980316162], 'magnitude': 4.814545631408691, 'distance': 8.3040771484375, 'cosine_with_motion': 0.8237175571334348, 'motion_component': 3.965825965203912}]}, 3195: {'frame': 3195, 'ionic_force': [4.266230762004852, 2.5804542303085327, -8.203031539916992], 'ionic_force_magnitude': 9.599437243623537, 'motion_vector': [-2.6438636779785156, 0.3204536437988281, -0.75738525390625], 'cosine_ionic_motion': -0.15950752621456848, 'ionic_motion_component': -1.5311824877823865, 'ionic_force_x': 4.266230762004852, 'ionic_force_y': 2.5804542303085327, 'ionic_force_z': -8.203031539916992, 'radial_force': 4.985927090260517, 'axial_force': -8.203031539916992, 'contributions': [{'ion': 1313, 'force': [3.318345785140991, 1.9544174671173096, -5.576297760009766], 'magnitude': 6.776891708374023, 'distance': 6.99928617477417, 'cosine_with_motion': -0.20910020006651614, 'motion_component': -1.4170494408500325}, {'ion': 1460, 'force': [0.9478849768638611, 0.6260367631912231, -2.6267337799072266], 'magnitude': 2.8618416786193848, 'distance': 10.770756721496582, 'cosine_with_motion': -0.039881000971897285, 'motion_component': -0.11413311435657825}]}, 3196: {'frame': 3196, 'ionic_force': [0.6016596853733063, 2.649301290512085, -8.311489343643188], 'ionic_force_magnitude': 8.744235061708187, 'motion_vector': [2.318988800048828, -2.4310836791992188, 0.22534942626953125], 'cosine_ionic_motion': -0.2349655890604089, 'ionic_motion_component': -2.0545943421569453, 'ionic_force_x': 0.6016596853733063, 'ionic_force_y': 2.649301290512085, 'ionic_force_z': -8.311489343643188, 'radial_force': 2.716761252836271, 'axial_force': -8.311489343643188, 'contributions': [{'ion': 1313, 'force': [0.49341556429862976, 2.0448687076568604, -5.6436381340026855], 'magnitude': 6.022922515869141, 'distance': 7.424468994140625, 'cosine_with_motion': -0.25140903765843836, 'motion_component': -1.5142172100840625}, {'ion': 1460, 'force': [0.10824412107467651, 0.6044325828552246, -2.667851209640503], 'magnitude': 2.7376058101654053, 'distance': 11.01244068145752, 'cosine_with_motion': -0.19739042068930143, 'motion_component': -0.5403771640603434}]}, 3197: {'frame': 3197, 'ionic_force': [2.8209893107414246, 0.17508456483483315, -8.191557884216309], 'ionic_force_magnitude': 8.665463395954491, 'motion_vector': [-2.359294891357422, 1.4584197998046875, 2.7145614624023438], 'cosine_ionic_motion': -0.8515068024527294, 'ionic_motion_component': -7.378701028060378, 'ionic_force_x': 2.8209893107414246, 'ionic_force_y': 0.17508456483483315, 'ionic_force_z': -8.191557884216309, 'radial_force': 2.8264173959556613, 'axial_force': -8.191557884216309, 'contributions': [{'ion': 1313, 'force': [2.2362687587738037, 0.05940436199307442, -5.672110557556152], 'magnitude': 6.097315788269043, 'distance': 7.379036903381348, 'cosine_with_motion': -0.8699706879091497, 'motion_component': -5.304486381330342}, {'ion': 1460, 'force': [0.5847205519676208, 0.11568020284175873, -2.5194473266601562], 'magnitude': 2.5889949798583984, 'distance': 11.32409381866455, 'cosine_with_motion': -0.8011659975708844, 'motion_component': -2.074214723975322}]}, 3198: {'frame': 3198, 'ionic_force': [4.809750139713287, 10.997350573539734, -26.898103833198547], 'ionic_force_magnitude': 29.45476881364607, 'motion_vector': [0.19825363159179688, 0.10056686401367188, -2.5326690673828125], 'cosine_ionic_motion': 0.9372048718855969, 'ionic_motion_component': 27.605152832413037, 'ionic_force_x': 4.809750139713287, 'ionic_force_y': 10.997350573539734, 'ionic_force_z': -26.898103833198547, 'radial_force': 12.003141923838388, 'axial_force': -26.898103833198547, 'contributions': [{'ion': 1313, 'force': [3.9049830436706543, 9.421380996704102, -19.212223052978516], 'magnitude': 21.751340866088867, 'distance': 3.906843662261963, 'cosine_with_motion': 0.9110158763380631, 'motion_component': 19.815816810828306}, {'ion': 1387, 'force': [0.15719091892242432, 0.2684478759765625, -1.947790265083313], 'magnitude': 1.9724756479263306, 'distance': 12.973681449890137, 'cosine_with_motion': 0.995300771002789, 'motion_component': 1.9632065286741396}, {'ion': 1460, 'force': [0.7475761771202087, 1.3075217008590698, -5.738090515136719], 'magnitude': 5.932466983795166, 'distance': 7.4808573722839355, 'cosine_with_motion': 0.9820752260428413, 'motion_component': 5.8261289687319895}]}, 3199: {'frame': 3199, 'ionic_force': [0.9833395779132843, 3.1130231618881226, -10.068522930145264], 'ionic_force_magnitude': 10.58456536315042, 'motion_vector': [-0.02933502197265625, -3.176746368408203, 1.2943191528320312], 'cosine_ionic_motion': -0.6320647076797856, 'ionic_motion_component': -6.6901302121772535, 'ionic_force_x': 0.9833395779132843, 'ionic_force_y': 3.1130231618881226, 'ionic_force_z': -10.068522930145264, 'radial_force': 3.264639326471241, 'axial_force': -10.068522930145264, 'contributions': [{'ion': 1313, 'force': [0.8440772891044617, 2.4483911991119385, -7.0417280197143555], 'magnitude': 7.502867221832275, 'distance': 6.652048587799072, 'cosine_with_motion': -0.6572728715675435, 'motion_component': -4.931431210428519}, {'ion': 1460, 'force': [0.13926228880882263, 0.6646319627761841, -3.026794910430908], 'magnitude': 3.102034330368042, 'distance': 10.345362663269043, 'cosine_with_motion': -0.5669501891312683, 'motion_component': -1.7586989570614022}]}, 3200: {'frame': 3200, 'ionic_force': [1.5398932620882988, -3.925731360912323, -14.942134141921997], 'ionic_force_magnitude': 15.525785348634267, 'motion_vector': [-0.7101936340332031, -1.3734970092773438, -0.6399917602539062], 'cosine_ionic_motion': 0.5334978917055188, 'ionic_motion_component': 8.282973750568814, 'ionic_force_x': 1.5398932620882988, 'ionic_force_y': -3.925731360912323, 'ionic_force_z': -14.942134141921997, 'radial_force': 4.21694652286171, 'axial_force': -14.942134141921997, 'contributions': [{'ion': 1313, 'force': [1.2463655471801758, -3.3982043266296387, -10.489591598510742], 'magnitude': 11.096519470214844, 'distance': 5.469852924346924, 'cosine_with_motion': 0.5652003166871671, 'motion_component': 6.2717565039260705}, {'ion': 1387, 'force': [0.09594348818063736, -0.13932183384895325, -1.5808546543121338], 'magnitude': 1.5898796319961548, 'distance': 14.450634956359863, 'cosine_with_motion': 0.4265788497944352, 'motion_component': 0.6782090140143298}, {'ion': 1460, 'force': [0.19758422672748566, -0.3882052004337311, -2.871687889099121], 'magnitude': 2.9045369625091553, 'distance': 10.691302299499512, 'cosine_with_motion': 0.45894008835435396, 'motion_component': 1.3330083846379597}]}, 3201: {'frame': 3201, 'ionic_force': [0.3855626368895173, -4.750433802604675, -10.51581072807312], 'ionic_force_magnitude': 11.54545603813691, 'motion_vector': [-0.7017936706542969, -0.01294708251953125, -0.8671646118164062], 'cosine_ionic_motion': 0.6917273308343146, 'ionic_motion_component': 7.986307488525365, 'ionic_force_x': 0.3855626368895173, 'ionic_force_y': -4.750433802604675, 'ionic_force_z': -10.51581072807312, 'radial_force': 4.766054957708137, 'axial_force': -10.51581072807312, 'contributions': [{'ion': 1313, 'force': [0.3916058838367462, -3.7393531799316406, -7.343410015106201], 'magnitude': 8.249957084655762, 'distance': 6.343708038330078, 'cosine_with_motion': 0.6672680685827019, 'motion_component': 5.504932773013024}, {'ion': 1460, 'force': [-0.0060432469472289085, -1.0110806226730347, -3.172400712966919], 'magnitude': 3.3296315670013428, 'distance': 9.985526084899902, 'cosine_with_motion': 0.74524006733559, 'motion_component': 2.4813749044541478}]}, 3202: {'frame': 3202, 'ionic_force': [-0.8432059288024902, -2.719889461994171, -7.3930346965789795], 'ionic_force_magnitude': 7.9224842662295805, 'motion_vector': [-0.6875076293945312, -0.4496726989746094, -0.5331268310546875], 'cosine_ionic_motion': 0.7403493413536228, 'ionic_motion_component': 5.8654060083875095, 'ionic_force_x': -0.8432059288024902, 'ionic_force_y': -2.719889461994171, 'ionic_force_z': -7.3930346965789795, 'radial_force': 2.8475945855817697, 'axial_force': -7.3930346965789795, 'contributions': [{'ion': 1313, 'force': [-0.6528485417366028, -2.2744596004486084, -5.246335506439209], 'magnitude': 5.755294322967529, 'distance': 7.595130920410156, 'cosine_with_motion': 0.7573262503904421, 'motion_component': 4.358635548107902}, {'ion': 1460, 'force': [-0.19035738706588745, -0.44542986154556274, -2.1466991901397705], 'magnitude': 2.2006728649139404, 'distance': 12.282628059387207, 'cosine_with_motion': 0.6846863323502752, 'motion_component': 1.5067706405058947}]}, 3203: {'frame': 3203, 'ionic_force': [-0.9554902762174606, -3.667130023241043, -8.258195757865906], 'ionic_force_magnitude': 9.086176393320592, 'motion_vector': [-1.41168212890625, -0.13762283325195312, 1.837890625], 'cosine_ionic_motion': -0.6316526643237212, 'ionic_motion_component': -5.739307527356252, 'ionic_force_x': -0.9554902762174606, 'ionic_force_y': -3.667130023241043, 'ionic_force_z': -8.258195757865906, 'radial_force': 3.7895651828807444, 'axial_force': -8.258195757865906, 'contributions': [{'ion': 1313, 'force': [-0.582251787185669, -2.546912908554077, -4.254993915557861], 'magnitude': 4.993070602416992, 'distance': 8.154272079467773, 'cosine_with_motion': -0.5734918508861262, 'motion_component': -2.863485398333836}, {'ion': 1387, 'force': [-0.14848487079143524, -0.3223477303981781, -1.5331422090530396], 'magnitude': 1.5736838579177856, 'distance': 14.52480411529541, 'cosine_with_motion': -0.7017500765273089, 'motion_component': -1.1043327598431159}, {'ion': 1460, 'force': [-0.22475361824035645, -0.7978693842887878, -2.470059633255005], 'magnitude': 2.6054375171661377, 'distance': 11.288304328918457, 'cosine_with_motion': -0.6799200535321163, 'motion_component': -1.7714891742978691}]}, 3204: {'frame': 3204, 'ionic_force': [-4.891388177871704, -6.8576348423957825, -12.308661103248596], 'ionic_force_magnitude': 14.914957998361531, 'motion_vector': [2.0974998474121094, 3.643840789794922, -4.29998779296875], 'cosine_ionic_motion': 0.19709987365095533, 'ionic_motion_component': 2.9397363369863636, 'ionic_force_x': -4.891388177871704, 'ionic_force_y': -6.8576348423957825, 'ionic_force_z': -12.308661103248596, 'radial_force': 8.423350517357312, 'axial_force': -12.308661103248596, 'contributions': [{'ion': 1313, 'force': [-3.5466692447662354, -5.008401393890381, -7.102478504180908], 'magnitude': 9.386594772338867, 'distance': 5.947234153747559, 'cosine_with_motion': 0.0859452850752351, 'motion_component': 0.8067335028722198}, {'ion': 1387, 'force': [-0.37983453273773193, -0.5484148859977722, -1.9710179567337036], 'magnitude': 2.0808520317077637, 'distance': 12.631312370300293, 'cosine_with_motion': 0.45391548181313884, 'motion_component': 0.9445309271792581}, {'ion': 1460, 'force': [-0.9648844003677368, -1.3008185625076294, -3.2351646423339844], 'magnitude': 3.6179304122924805, 'distance': 9.579413414001465, 'cosine_with_motion': 0.32849483507551613, 'motion_component': 1.1884714828583895}]}, 3205: {'frame': 3205, 'ionic_force': [-0.6016021221876144, 0.16618561744689941, -6.180601716041565], 'ionic_force_magnitude': 6.21203512105355, 'motion_vector': [-2.4292831420898438, -0.1877899169921875, 1.3914337158203125], 'cosine_ionic_motion': -0.41133902842181963, 'ionic_motion_component': -2.555252491216388, 'ionic_force_x': -0.6016021221876144, 'ionic_force_y': 0.16618561744689941, 'ionic_force_z': -6.180601716041565, 'radial_force': 0.6241336177989842, 'axial_force': -6.180601716041565, 'contributions': [{'ion': 1313, 'force': [-0.47208482027053833, 0.13534782826900482, -4.1929497718811035], 'magnitude': 4.221612453460693, 'distance': 8.868085861206055, 'cosine_with_motion': -0.39786613493239775, 'motion_component': -1.679636592081345}, {'ion': 1460, 'force': [-0.1295173019170761, 0.030837789177894592, -1.9876519441604614], 'magnitude': 1.9921059608459473, 'distance': 12.909601211547852, 'cosine_with_motion': -0.43954280105675997, 'motion_component': -0.8756158111541572}]}, 3206: {'frame': 3206, 'ionic_force': [-2.3814292550086975, -0.07051205262541771, -6.440298318862915], 'ionic_force_magnitude': 6.866849327175107, 'motion_vector': [4.136890411376953, -0.5502357482910156, -0.2530059814453125], 'cosine_ionic_motion': -0.2850374206019799, 'ionic_motion_component': -1.9573090198804335, 'ionic_force_x': -2.3814292550086975, 'ionic_force_y': -0.07051205262541771, 'ionic_force_z': -6.440298318862915, 'radial_force': 2.3824729266408737, 'axial_force': -6.440298318862915, 'contributions': [{'ion': 1313, 'force': [-1.8158272504806519, -0.09443157911300659, -4.377440452575684], 'magnitude': 4.740056037902832, 'distance': 8.369071960449219, 'cosine_with_motion': -0.3205352276549729, 'motion_component': -1.5193549276856588}, {'ion': 1460, 'force': [-0.5656020045280457, 0.023919526487588882, -2.0628578662872314], 'magnitude': 2.1391260623931885, 'distance': 12.458072662353516, 'cosine_with_motion': -0.20473505796635882, 'motion_component': -0.4379541001504612}]}, 3207: {'frame': 3207, 'ionic_force': [0.5504616945981979, -0.20011846721172333, -6.7197370529174805], 'ionic_force_magnitude': 6.7452147140392205, 'motion_vector': [-0.4560203552246094, -0.9889564514160156, 2.2855987548828125], 'cosine_ionic_motion': -0.9024609612745147, 'ionic_motion_component': -6.087292954834836, 'ionic_force_x': 0.5504616945981979, 'ionic_force_y': -0.20011846721172333, 'ionic_force_z': -6.7197370529174805, 'radial_force': 0.5857093802724089, 'axial_force': -6.7197370529174805, 'contributions': [{'ion': 1313, 'force': [0.4108598530292511, -0.13039463758468628, -4.540388107299805], 'magnitude': 4.5608038902282715, 'distance': 8.531950950622559, 'cosine_with_motion': -0.9037776946529549, 'motion_component': -4.1219528871178355}, {'ion': 1460, 'force': [0.13960184156894684, -0.06972382962703705, -2.179348945617676], 'magnitude': 2.1849284172058105, 'distance': 12.326803207397461, 'cosine_with_motion': -0.8994986514893245, 'motion_component': -1.9653401082788329}]}, 3208: {'frame': 3208, 'ionic_force': [0.6337229162454605, -2.9306737780570984, -10.785738706588745], 'ionic_force_magnitude': 11.194758281212362, 'motion_vector': [0.30518341064453125, 1.3927268981933594, -1.3763351440429688], 'cosine_ionic_motion': 0.49388111416975305, 'ionic_motion_component': 5.528879692786231, 'ionic_force_x': 0.6337229162454605, 'ionic_force_y': -2.9306737780570984, 'ionic_force_z': -10.785738706588745, 'radial_force': 2.998408499181877, 'axial_force': -10.785738706588745, 'contributions': [{'ion': 1313, 'force': [0.44283202290534973, -2.438164234161377, -7.620040416717529], 'magnitude': 8.012849807739258, 'distance': 6.436882019042969, 'cosine_with_motion': 0.45513940674212605, 'motion_component': 3.6469636778250076}, {'ion': 1460, 'force': [0.19089089334011078, -0.49250954389572144, -3.165698289871216], 'magnitude': 3.2094626426696777, 'distance': 10.170747756958008, 'cosine_with_motion': 0.5863647716762116, 'motion_component': 1.8819158471922193}]}, 3209: {'frame': 3209, 'ionic_force': [0.43650949746370316, -0.5205679461359978, -6.388556241989136], 'ionic_force_magnitude': 6.424576436231311, 'motion_vector': [-2.8515777587890625, -0.7392349243164062, -1.9197006225585938], 'cosine_ionic_motion': 0.5048408404249863, 'ionic_motion_component': 3.2433885674415786, 'ionic_force_x': 0.43650949746370316, 'ionic_force_y': -0.5205679461359978, 'ionic_force_z': -6.388556241989136, 'radial_force': 0.6793611174627716, 'axial_force': -6.388556241989136, 'contributions': [{'ion': 1313, 'force': [0.33712059259414673, -0.4496636390686035, -4.658642292022705], 'magnitude': 4.692419052124023, 'distance': 8.411445617675781, 'cosine_with_motion': 0.5039206562836169, 'motion_component': 2.3646068414033508}, {'ion': 1460, 'force': [0.09938890486955643, -0.07090430706739426, -1.7299139499664307], 'magnitude': 1.7342168092727661, 'distance': 13.836216926574707, 'cosine_with_motion': 0.5067312342068669, 'motion_component': 0.8787818106888905}]}, 3210: {'frame': 3210, 'ionic_force': [-1.0865365266799927, -0.4411945790052414, -5.631094336509705], 'ionic_force_magnitude': 5.751907310364546, 'motion_vector': [-0.060733795166015625, -0.4639701843261719, -0.5265655517578125], 'cosine_ionic_motion': 0.7986072361519804, 'ionic_motion_component': 4.593514799732601, 'ionic_force_x': -1.0865365266799927, 'ionic_force_y': -0.4411945790052414, 'ionic_force_z': -5.631094336509705, 'radial_force': 1.1726953058460814, 'axial_force': -5.631094336509705, 'contributions': [{'ion': 1313, 'force': [-0.8106954097747803, -0.30610916018486023, -3.7750306129455566], 'magnitude': 3.87321400642395, 'distance': 9.258343696594238, 'cosine_with_motion': 0.7986521289722621, 'motion_component': 3.093350535334695}, {'ion': 1460, 'force': [-0.2758411169052124, -0.13508541882038116, -1.856063723564148], 'magnitude': 1.8813050985336304, 'distance': 13.284322738647461, 'cosine_with_motion': 0.7974061921978106, 'motion_component': 1.500164348614363}]}, 3211: {'frame': 3211, 'ionic_force': [-1.4129315614700317, -1.1412988752126694, -6.022145748138428], 'ionic_force_magnitude': 6.290085701465569, 'motion_vector': [0.17093276977539062, 2.88043212890625, 2.7339096069335938], 'cosine_ionic_motion': -0.7996257345609912, 'ionic_motion_component': -5.029714399485993, 'ionic_force_x': -1.4129315614700317, 'ionic_force_y': -1.1412988752126694, 'ionic_force_z': -6.022145748138428, 'radial_force': 1.816298081252041, 'axial_force': -6.022145748138428, 'contributions': [{'ion': 1313, 'force': [-1.1177146434783936, -0.9046632647514343, -4.136012077331543], 'magnitude': 4.378846645355225, 'distance': 8.707413673400879, 'cosine_with_motion': -0.8103263953123397, 'motion_component': -3.54829498140504}, {'ion': 1460, 'force': [-0.2952169179916382, -0.23663561046123505, -1.8861336708068848], 'magnitude': 1.9237072467803955, 'distance': 13.137101173400879, 'cosine_with_motion': -0.7700856154835416, 'motion_component': -1.4814192978902772}]}, 3212: {'frame': 3212, 'ionic_force': [-2.1320821791887283, 1.880209058523178, -9.907267928123474], 'ionic_force_magnitude': 10.307032469250826, 'motion_vector': [-0.551544189453125, -2.786346435546875, -0.7046661376953125], 'cosine_ionic_motion': 0.09675015725847247, 'ionic_motion_component': 0.9972070122681992, 'ionic_force_x': -2.1320821791887283, 'ionic_force_y': 1.880209058523178, 'ionic_force_z': -9.907267928123474, 'radial_force': 2.8427030310193806, 'axial_force': -9.907267928123474, 'contributions': [{'ion': 1313, 'force': [-1.564578652381897, 1.3044873476028442, -5.753448963165283], 'magnitude': 6.10342264175415, 'distance': 7.375344753265381, 'cosine_with_motion': 0.07179818047445186, 'motion_component': 0.4382146440348506}, {'ion': 1387, 'force': [-0.18752484023571014, 0.17749661207199097, -1.5429457426071167], 'magnitude': 1.5644015073776245, 'distance': 14.567831993103027, 'cosine_with_motion': 0.15205022229138687, 'motion_component': 0.23786760187487757}, {'ion': 1460, 'force': [-0.3799786865711212, 0.3982250988483429, -2.610873222351074], 'magnitude': 2.6682627201080322, 'distance': 11.154619216918945, 'cosine_with_motion': 0.1203497363508293, 'motion_component': 0.32112471648709473}]}, 3213: {'frame': 3213, 'ionic_force': [-3.1511535048484802, -1.7650651186704636, -9.942092418670654], 'ionic_force_magnitude': 10.57782704271792, 'motion_vector': [-0.14082717895507812, -0.13962173461914062, -1.2342300415039062], 'cosine_ionic_motion': 0.9801949420071061, 'ionic_motion_component': 10.368332564698092, 'ionic_force_x': -3.1511535048484802, 'ionic_force_y': -1.7650651186704636, 'ionic_force_z': -9.942092418670654, 'radial_force': 3.611817172043186, 'axial_force': -9.942092418670654, 'contributions': [{'ion': 1313, 'force': [-2.6584701538085938, -1.5168129205703735, -7.454015254974365], 'magnitude': 8.057948112487793, 'distance': 6.418843746185303, 'cosine_with_motion': 0.9715291196890977, 'motion_component': 7.82853127435799}, {'ion': 1460, 'force': [-0.4926833510398865, -0.24825219810009003, -2.488077163696289], 'magnitude': 2.5485081672668457, 'distance': 11.413688659667969, 'cosine_with_motion': 0.9965835225965978, 'motion_component': 2.5398012725363297}]}, 3214: {'frame': 3214, 'ionic_force': [-1.5444872081279755, -1.1262651979923248, -6.004039764404297], 'ionic_force_magnitude': 6.300984647245829, 'motion_vector': [0.7136573791503906, -0.08641815185546875, -0.5668869018554688], 'cosine_ionic_motion': 0.4158258844145278, 'ionic_motion_component': 2.6201125136233583, 'ionic_force_x': -1.5444872081279755, 'ionic_force_y': -1.1262651979923248, 'ionic_force_z': -6.004039764404297, 'radial_force': 1.9115213920538894, 'axial_force': -6.004039764404297, 'contributions': [{'ion': 1313, 'force': [-1.1439869403839111, -0.8971394300460815, -3.885117769241333], 'magnitude': 4.14821720123291, 'distance': 8.94619369506836, 'cosine_with_motion': 0.3853762981400929, 'motion_component': 1.5986245614389398}, {'ion': 1460, 'force': [-0.40050026774406433, -0.2291257679462433, -2.118921995162964], 'magnitude': 2.1685779094696045, 'distance': 12.373186111450195, 'cosine_with_motion': 0.4710405579521181, 'motion_component': 1.0214880782956504}]}, 3215: {'frame': 3215, 'ionic_force': [-0.8170889019966125, -0.7826167792081833, -5.666041016578674], 'ionic_force_magnitude': 5.777901357622516, 'motion_vector': [-0.340850830078125, 0.852874755859375, 0.39165496826171875], 'cosine_ionic_motion': -0.4520783780553534, 'ionic_motion_component': -2.6120642743178117, 'ionic_force_x': -0.8170889019966125, 'ionic_force_y': -0.7826167792081833, 'ionic_force_z': -5.666041016578674, 'radial_force': 1.1314253386168351, 'axial_force': -5.666041016578674, 'contributions': [{'ion': 1313, 'force': [-0.5830154418945312, -0.575762152671814, -3.7722537517547607], 'magnitude': 3.8602211475372314, 'distance': 9.273911476135254, 'cosine_with_motion': -0.4591556550887339, 'motion_component': -1.772442377020944}, {'ion': 1460, 'force': [-0.2340734601020813, -0.20685462653636932, -1.8937872648239136], 'magnitude': 1.919377326965332, 'distance': 13.151910781860352, 'cosine_with_motion': -0.43744489784368085, 'motion_component': -0.8396218303850214}]}, 3216: {'frame': 3216, 'ionic_force': [-1.1128128170967102, -0.3707253783941269, -5.447134375572205], 'ionic_force_magnitude': 5.571989104226656, 'motion_vector': [-0.07701492309570312, 0.34079742431640625, -0.7521133422851562], 'cosine_ionic_motion': 0.8778023359725989, 'ionic_motion_component': 4.891105051704027, 'ionic_force_x': -1.1128128170967102, 'ionic_force_y': -0.3707253783941269, 'ionic_force_z': -5.447134375572205, 'radial_force': 1.172940608931324, 'axial_force': -5.447134375572205, 'contributions': [{'ion': 1313, 'force': [-0.8524911999702454, -0.24588410556316376, -3.6285605430603027], 'magnitude': 3.7354586124420166, 'distance': 9.427511215209961, 'cosine_with_motion': 0.8751090106105364, 'motion_component': 3.268933585247774}, {'ion': 1460, 'force': [-0.26032161712646484, -0.124</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{3320: {'frame': 3320, 'ionic_force': [4.8733450174331665, 3.184350647032261, -8.640591382980347], 'ionic_force_magnitude': 10.418704341223512, 'motion_vector': [-0.18167495727539062, 0.760711669921875, 0.7443389892578125], 'cosine_ionic_motion': -0.4351086894470255, 'ionic_motion_component': -4.533268791645797, 'ionic_force_x': 4.8733450174331665, 'ionic_force_y': 3.184350647032261, 'ionic_force_z': -8.640591382980347, 'radial_force': 5.821475818226461, 'axial_force': -8.640591382980347, 'contributions': [{'ion': 1387, 'force': [0.3318135738372803, -0.0069795772433280945, -1.9514002799987793], 'magnitude': 1.9794220924377441, 'distance': 12.950896263122559, 'directional_contribution': -1.4060482193826478}, {'ion': 1460, 'force': [1.624815821647644, -0.2846843898296356, -5.312528133392334], 'magnitude': 5.562735557556152, 'distance': 7.725468635559082, 'directional_contribution': -4.1364433416914}, {'ion': 2433, 'force': [2.916715621948242, 3.4760146141052246, -1.3766629695892334], 'magnitude': 4.741846561431885, 'distance': 8.367491722106934, 'directional_contribution': 1.0092227157837357}]}, 3321: {'frame': 3321, 'ionic_force': [4.962071061134338, 4.828094765543938, -10.522126078605652], 'ionic_force_magnitude': 12.595546256311902, 'motion_vector': [3.44659423828125, 0.5642127990722656, -0.29720306396484375], 'cosine_ionic_motion': 0.5199156061735278, 'ionic_motion_component': 6.548621066937112, 'ionic_force_x': 4.962071061134338, 'ionic_force_y': 4.828094765543938, 'ionic_force_z': -10.522126078605652, 'radial_force': 6.9233408323452945, 'axial_force': -10.522126078605652, 'contributions': [{'ion': 1387, 'force': [0.4181758165359497, 0.16234956681728363, -2.319929599761963], 'magnitude': 2.362901210784912, 'distance': 11.853490829467773, 'directional_contribution': 0.6340408627544847}, {'ion': 1460, 'force': [2.362652540206909, 0.5963982939720154, -7.155970096588135], 'magnitude': 7.559479236602783, 'distance': 6.62709379196167, 'directional_contribution': 3.0259899505259265}, {'ion': 2433, 'force': [2.1812427043914795, 4.069346904754639, -1.0462263822555542], 'magnitude': 4.734130859375, 'distance': 8.374307632446289, 'directional_contribution': 2.8885903144106857}]}, 3322: {'frame': 3322, 'ionic_force': [5.101867258548737, 2.400673806667328, -5.333805024623871], 'ionic_force_magnitude': 7.761556563639349, 'motion_vector': [-1.1910209655761719, 1.1273345947265625, 1.091339111328125], 'cosine_ionic_motion': -0.6011411421058467, 'ionic_motion_component': -4.665790977185289, 'ionic_force_x': 5.101867258548737, 'ionic_force_y': 2.400673806667328, 'ionic_force_z': -5.333805024623871, 'radial_force': 5.638464706803635, 'axial_force': -5.333805024623871, 'contributions': [{'ion': 1387, 'force': [0.8166144490242004, 0.16744935512542725, -1.7120360136032104], 'magnitude': 1.904196858406067, 'distance': 13.204231262207031, 'directional_contribution': -1.3463980228761798}, {'ion': 1460, 'force': [2.6996209621429443, 0.5092499852180481, -3.1144349575042725], 'magnitude': 4.152949810028076, 'distance': 8.941094398498535, 'directional_contribution': -3.066231583865708}, {'ion': 2433, 'force': [1.5856318473815918, 1.7239744663238525, -0.5073340535163879], 'magnitude': 2.3966026306152344, 'distance': 11.769852638244629, 'directional_contribution': -0.2531614541572438}]}, 3323: {'frame': 3323, 'ionic_force': [5.707005620002747, 4.04939991235733, -7.091884225606918], 'ionic_force_magnitude': 9.963050469929113, 'motion_vector': [-0.09119033813476562, -1.4596443176269531, 0.58355712890625], 'cosine_ionic_motion': -0.6737404389098686, 'ionic_motion_component': -6.712509996491213, 'ionic_force_x': 5.707005620002747, 'ionic_force_y': 4.04939991235733, 'ionic_force_z': -7.091884225606918, 'radial_force': 6.997681958830545, 'axial_force': -7.091884225606918, 'contributions': [{'ion': 1387, 'force': [0.8393199443817139, 0.3989105820655823, -2.18998122215271], 'magnitude': 2.3789925575256348, 'distance': 11.813334465026855, 'directional_contribution': -1.2300042650106304}, {'ion': 1460, 'force': [3.4794766902923584, 1.5985596179962158, -4.6523637771606445], 'magnitude': 6.02549934387207, 'distance': 7.422881603240967, 'directional_contribution': -3.4075245058578423}, {'ion': 2433, 'force': [1.3882089853286743, 2.0519297122955322, -0.24953922629356384], 'magnitude': 2.4899415969848633, 'distance': 11.547141075134277, 'directional_contribution': -2.0749813240573336}]}, 3324: {'frame': 3324, 'ionic_force': [9.42669403553009, 3.5997143760323524, -10.327790841460228], 'ionic_force_magnitude': 14.438966988447003, 'motion_vector': [1.4581718444824219, 0.5040359497070312, -1.6050872802734375], 'cosine_ionic_motion': 0.9997192109901553, 'ionic_motion_component': 14.434912685203136, 'ionic_force_x': 9.42669403553009, 'ionic_force_y': 3.5997143760323524, 'ionic_force_z': -10.327790841460228, 'radial_force': 10.090614650679738, 'axial_force': -10.327790841460228, 'contributions': [{'ion': 1316, 'force': [0.5152910947799683, 0.09902171045541763, -1.5304564237594604], 'magnitude': 1.617908239364624, 'distance': 14.32491683959961, 'directional_contribution': 1.4632979506664054}, {'ion': 1387, 'force': [1.6848300695419312, 0.3395357131958008, -3.116074562072754], 'magnitude': 3.558631420135498, 'distance': 9.658897399902344, 'directional_contribution': 3.4269052191387033}, {'ion': 1460, 'force': [5.295093536376953, 0.8498631119728088, -5.482320308685303], 'magnitude': 7.6691670417785645, 'distance': 6.579531192779541, 'directional_contribution': 7.612971853423932}, {'ion': 2433, 'force': [1.9314793348312378, 2.311293840408325, -0.19893954694271088], 'magnitude': 3.018653392791748, 'distance': 10.487269401550293, 'directional_contribution': 1.9317376565473428}]}, 3325: {'frame': 3325, 'ionic_force': [6.025220155715942, 3.329250246286392, -5.533735513687134], 'ionic_force_magnitude': 8.832293805274247, 'motion_vector': [-1.0484428405761719, -1.0520210266113281, -0.158599853515625], 'cosine_ionic_motion': -0.6777865381816526, 'ionic_motion_component': -5.986409842480087, 'ionic_force_x': 6.025220155715942, 'ionic_force_y': 3.329250246286392, 'ionic_force_z': -5.533735513687134, 'radial_force': 6.883835059561178, 'axial_force': -5.533735513687134, 'contributions': [{'ion': 1387, 'force': [1.0765461921691895, 0.23434945940971375, -2.0206117630004883], 'magnitude': 2.3014655113220215, 'distance': 12.010658264160156, 'directional_contribution': -0.7061458862244105}, {'ion': 1460, 'force': [2.5632970333099365, 0.5630773901939392, -3.0066704750061035], 'magnitude': 3.9909415245056152, 'distance': 9.120766639709473, 'directional_contribution': -1.8765382588053043}, {'ion': 2433, 'force': [2.3853769302368164, 2.5318233966827393, -0.506453275680542], 'magnitude': 3.515202283859253, 'distance': 9.718379974365234, 'directional_contribution': -3.403725551910478}]}, 3326: {'frame': 3326, 'ionic_force': [5.521149039268494, 2.2750196903944016, -6.492782413959503], 'ionic_force_magnitude': 8.821282490688043, 'motion_vector': [0.80645751953125, 0.5555877685546875, -0.410614013671875], 'cosine_ionic_motion': 0.8948647231467417, 'ionic_motion_component': 7.893854513828756, 'ionic_force_x': 5.521149039268494, 'ionic_force_y': 2.2750196903944016, 'ionic_force_z': -6.492782413959503, 'radial_force': 5.971499083605192, 'axial_force': -6.492782413959503, 'contributions': [{'ion': 1387, 'force': [0.7306075096130371, 0.05163702368736267, -1.8644970655441284], 'magnitude': 2.0031981468200684, 'distance': 12.873809814453125, 'directional_contribution': 1.3028221533939597}, {'ion': 1460, 'force': [2.9076755046844482, 0.214521124958992, -4.017284393310547], 'magnitude': 4.963785648345947, 'distance': 8.178290367126465, 'directional_contribution': 3.873822364127798}, {'ion': 2433, 'force': [1.8828660249710083, 2.008861541748047, -0.6110009551048279], 'magnitude': 2.820289134979248, 'distance': 10.849812507629395, 'directional_contribution': 2.7172101317688018}]}, 3327: {'frame': 3327, 'ionic_force': [4.962403953075409, 2.0606805086135864, -5.490831732749939], 'ionic_force_magnitude': 7.682518484810309, 'motion_vector': [-0.40179443359375, 0.5124359130859375, 0.6054840087890625], 'cosine_ionic_motion': -0.6239824605969704, 'ionic_motion_component': -4.7937567877336456, 'ionic_force_x': 4.962403953075409, 'ionic_force_y': 2.0606805086135864, 'ionic_force_z': -5.490831732749939, 'radial_force': 5.373253870056615, 'axial_force': -5.490831732749939, 'contributions': [{'ion': 1387, 'force': [0.7123898863792419, 0.10276107490062714, -1.644201397895813], 'magnitude': 1.7948418855667114, 'distance': 13.600533485412598, 'directional_contribution': -1.382300725170892}, {'ion': 1460, 'force': [2.544466972351074, 0.2279723435640335, -3.2194597721099854], 'magnitude': 4.109890937805176, 'distance': 8.987810134887695, 'directional_contribution': -3.2106709714302584}, {'ion': 2433, 'force': [1.7055470943450928, 1.7299470901489258, -0.6271705627441406], 'magnitude': 2.508974075317383, 'distance': 11.503260612487793, 'directional_contribution': -0.20078512136664983}]}, 3328: {'frame': 3328, 'ionic_force': [5.662827789783478, 2.698476254940033, -6.413617879152298], 'ionic_force_magnitude': 8.971281233748122, 'motion_vector': [-1.1094818115234375, 0.8973617553710938, 1.1634902954101562], 'cosine_ionic_motion': -0.6855367750310243, 'ionic_motion_component': -6.150143204880036, 'ionic_force_x': 5.662827789783478, 'ionic_force_y': 2.698476254940033, 'ionic_force_z': -6.413617879152298, 'radial_force': 6.272909426671105, 'axial_force': -6.413617879152298, 'contributions': [{'ion': 1387, 'force': [0.7809037566184998, 0.18411484360694885, -1.7854108810424805], 'magnitude': 1.9573965072631836, 'distance': 13.023557662963867, 'directional_contribution': -1.5090864508773922}, {'ion': 1460, 'force': [3.093663454055786, 0.4853256046772003, -4.167239665985107], 'magnitude': 5.21269416809082, 'distance': 7.9806437492370605, 'directional_contribution': -4.261084555910353}, {'ion': 2433, 'force': [1.788260579109192, 2.029035806655884, -0.4609673321247101], 'magnitude': 2.7436022758483887, 'distance': 11.000399589538574, 'directional_contribution': -0.3799721065212349}]}, 3329: {'frame': 3329, 'ionic_force': [6.12342631816864, 5.340087965130806, -8.698342144489288], 'ionic_force_magnitude': 11.90269067950494, 'motion_vector': [0.8754844665527344, -1.0129776000976562, 0.6521530151367188], 'cosine_ionic_motion': -0.3227464606590609, 'ionic_motion_component': -3.8415512891298116, 'ionic_force_x': 6.12342631816864, 'ionic_force_y': 5.340087965130806, 'ionic_force_z': -8.698342144489288, 'radial_force': 8.12483165052515, 'axial_force': -8.698342144489288, 'contributions': [{'ion': 1316, 'force': [0.37819957733154297, 0.24994249641895294, -1.4104505777359009], 'magnitude': 1.4815117120742798, 'distance': 14.969817161560059, 'directional_contribution': -0.5653190013484792}, {'ion': 1387, 'force': [0.9713860750198364, 0.7008095979690552, -2.4578428268432617], 'magnitude': 2.734175682067871, 'distance': 11.019346237182617, 'directional_contribution': -0.9819366955576072}, {'ion': 1460, 'force': [3.2983713150024414, 2.064893960952759, -4.52915096282959], 'magnitude': 5.971285343170166, 'distance': 7.456501483917236, 'directional_contribution': -1.4488509092765014}, {'ion': 2433, 'force': [1.4754693508148193, 2.324441909790039, -0.3008977770805359], 'magnitude': 2.7695810794830322, 'distance': 10.948685646057129, 'directional_contribution': -0.8454448625147428}]}, 3330: {'frame': 3330, 'ionic_force': [8.562611877918243, 3.4708504751324654, -9.022035978734493], 'ionic_force_magnitude': 12.913646208339978, 'motion_vector': [1.0237197875976562, -1.2902107238769531, 0.8571853637695312], 'cosine_ionic_motion': -0.14371961245459278, 'ionic_motion_component': -1.8559442284383432, 'ionic_force_x': 8.562611877918243, 'ionic_force_y': 3.4708504751324654, 'ionic_force_z': -9.022035978734493, 'radial_force': 9.239324931649165, 'axial_force': -9.022035978734493, 'contributions': [{'ion': 1316, 'force': [0.5562570691108704, 0.11473546177148819, -1.4796452522277832], 'magnitude': 1.5849088430404663, 'distance': 14.47327709197998, 'directional_contribution': -0.45613305128550374}, {'ion': 1387, 'force': [1.3070932626724243, 0.29501739144325256, -2.6750640869140625], 'magnitude': 2.9919052124023438, 'distance': 10.53404426574707, 'directional_contribution': -0.7193127855523347}, {'ion': 1460, 'force': [4.905503273010254, 1.0822356939315796, -4.953392505645752], 'magnitude': 7.054877281188965, 'distance': 6.8600029945373535, 'directional_contribution': -0.33415189509761234}, {'ion': 2433, 'force': [1.7937582731246948, 1.978861927986145, 0.0860658660531044], 'magnitude': 2.672240734100342, 'distance': 11.146313667297363, 'directional_contribution': -0.3463464546020445}]}, 3331: {'frame': 3331, 'ionic_force': [12.735351324081421, 2.3743116538971663, -6.971976637840271], 'ionic_force_magnitude': 14.711729586156919, 'motion_vector': [-1.5520782470703125, 0.7276382446289062, -2.8383560180664062], 'cosine_ionic_motion': 0.035881050304702455, 'ionic_motion_component': 0.5278723093500758, 'ionic_force_x': 12.735351324081421, 'ionic_force_y': 2.3743116538971663, 'ionic_force_z': -6.971976637840271, 'radial_force': 12.954787886245544, 'axial_force': -6.971976637840271, 'contributions': [{'ion': 1316, 'force': [0.7236177921295166, -0.01991807110607624, -1.514197587966919], 'magnitude': 1.6783366203308105, 'distance': 14.064668655395508, 'directional_contribution': 0.9530753588752279}, {'ion': 1387, 'force': [2.3421452045440674, -0.13869722187519073, -2.969356060028076], 'magnitude': 3.784435987472534, 'distance': 9.366308212280273, 'directional_contribution': 1.4150268355639988}, {'ion': 1460, 'force': [6.530500888824463, -0.4096313416957855, -3.7830898761749268], 'magnitude': 7.558241367340088, 'distance': 6.627636432647705, 'directional_contribution': 0.09163469545941672}, {'ion': 2433, 'force': [3.139087438583374, 2.9425582885742188, 1.2946668863296509], 'magnitude': 4.4931817054748535, 'distance': 8.595913887023926, 'directional_contribution': -1.931864480817218}]}, 3332: {'frame': 3332, 'ionic_force': [5.920918166637421, 3.972064346075058, -6.426218777894974], 'ionic_force_magnitude': 9.598481905319595, 'motion_vector': [0.7343177795410156, 1.0062751770019531, 2.0959930419921875], 'cosine_ionic_motion': -0.21896350382145063, 'ionic_motion_component': -2.1017172293555717, 'ionic_force_x': 5.920918166637421, 'ionic_force_y': 3.972064346075058, 'ionic_force_z': -6.426218777894974, 'radial_force': 7.12983640102476, 'axial_force': -6.426218777894974, 'contributions': [{'ion': 1387, 'force': [0.6480094790458679, 0.07161861658096313, -1.956294298171997], 'magnitude': 2.06207013130188, 'distance': 12.688705444335938, 'directional_contribution': -1.4569816124307788}, {'ion': 1460, 'force': [2.506962299346924, 0.3197813332080841, -4.0640716552734375], 'magnitude': 4.785791397094727, 'distance': 8.328987121582031, 'directional_contribution': -2.606625695022325}, {'ion': 2433, 'force': [2.765946388244629, 3.5806643962860107, -0.4058528244495392], 'magnitude': 4.542723178863525, 'distance': 8.54891300201416, 'directional_contribution': 1.9618899948423572}]}, 3333: {'frame': 3333, 'ionic_force': [11.138619840145111, 7.894609674811363, -10.194625984877348], 'ionic_force_magnitude': 17.038899988920527, 'motion_vector': [-0.58197021484375, -0.06623077392578125, -0.9650726318359375], 'cosine_ionic_motion': 0.1472983279094927, 'ionic_motion_component': 2.5098014777850675, 'ionic_force_x': 11.138619840145111, 'ionic_force_y': 7.894609674811363, 'ionic_force_z': -10.194625984877348, 'radial_force': 13.652608317127518, 'axial_force': -10.194625984877348, 'contributions': [{'ion': 1316, 'force': [0.6237956881523132, 0.15656648576259613, -1.627447485923767], 'magnitude': 1.7499197721481323, 'distance': 13.773996353149414, 'directional_contribution': 1.06049509096636}, {'ion': 1387, 'force': [1.9665889739990234, 0.6323477029800415, -3.3439724445343018], 'magnitude': 3.9305837154388428, 'distance': 9.190528869628906, 'directional_contribution': 1.8077584950588932}, {'ion': 1460, 'force': [5.7677435874938965, 2.1759836673736572, -5.206416130065918], 'magnitude': 8.068985939025879, 'distance': 6.414451599121094, 'directional_contribution': 1.3497937077936975}, {'ion': 2433, 'force': [2.780491590499878, 4.929711818695068, -0.01678992435336113], 'magnitude': 5.659811973571777, 'distance': 7.658928871154785, 'directional_contribution': -1.7082461370083915}]}, 3334: {'frame': 3334, 'ionic_force': [8.556934595108032, 6.820997595787048, -7.33417646586895], 'ionic_force_magnitude': 13.173355013025168, 'motion_vector': [0.17787933349609375, -0.084075927734375, 0.6251068115234375], 'cosine_ionic_motion': -0.42117706074107514, 'ionic_motion_component': -5.548314944484647, 'ionic_force_x': 8.556934595108032, 'ionic_force_y': 6.820997595787048, 'ionic_force_z': -7.33417646586895, 'radial_force': 10.942903539129336, 'axial_force': -7.33417646586895, 'contributions': [{'ion': 1387, 'force': [1.4384901523590088, 0.4807847738265991, -2.7401866912841797], 'magnitude': 3.131937265396118, 'distance': 10.295857429504395, 'directional_contribution': -2.2850091222240625}, {'ion': 1460, 'force': [4.045209884643555, 1.0065531730651855, -4.721059799194336], 'magnitude': 6.298037528991699, 'distance': 7.260498046875, 'directional_contribution': -3.534409758359267}, {'ion': 2433, 'force': [3.0732345581054688, 5.333659648895264, 0.12707002460956573], 'magnitude': 6.157015800476074, 'distance': 7.343175411224365, 'directional_contribution': 0.2711040889088734}]}, 3335: {'frame': 3335, 'ionic_force': [10.957434237003326, 7.65510667860508, -10.461147874593735], 'ionic_force_magnitude': 16.973557027717963, 'motion_vector': [0.046604156494140625, 0.275848388671875, -0.0363616943359375], 'cosine_ionic_motion': 0.627074144131308, 'ionic_motion_component': 10.64367874602019, 'ionic_force_x': 10.957434237003326, 'ionic_force_y': 7.65510667860508, 'ionic_force_z': -10.461147874593735, 'radial_force': 13.366601038374593, 'axial_force': -10.461147874593735, 'contributions': [{'ion': 1316, 'force': [0.5002949833869934, 0.06886790692806244, -1.5100455284118652], 'magnitude': 1.5922547578811646, 'distance': 14.439852714538574, 'directional_contribution': 0.344619091924816}, {'ion': 1387, 'force': [1.7298309803009033, 0.3097245991230011, -3.301562786102295], 'magnitude': 3.740128517150879, 'distance': 9.421624183654785, 'directional_contribution': 1.0141577034043774}, {'ion': 1460, 'force': [5.743025779724121, 1.7341681718826294, -5.573688983917236], 'magnitude': 8.188754081726074, 'distance': 6.36737060546875, 'directional_contribution': 3.3628113618595847}, {'ion': 2433, 'force': [2.9842824935913086, 5.542346000671387, -0.07585057616233826], 'magnitude': 6.295180320739746, 'distance': 7.262145519256592, 'directional_contribution': 5.922090530346958}]}, 3336: {'frame': 3336, 'ionic_force': [9.11018654704094, 6.392471864819527, -9.55652368068695], 'ionic_force_magnitude': 14.669231074733448, 'motion_vector': [-4.241512298583984, -1.3926010131835938, -0.917877197265625], 'cosine_ionic_motion': -0.5799124377910689, 'ionic_motion_component': -8.506869553069176, 'ionic_force_x': 9.11018654704094, 'ionic_force_y': 6.392471864819527, 'ionic_force_z': -9.55652368068695, 'radial_force': 11.129204619576143, 'axial_force': -9.55652368068695, 'contributions': [{'ion': 1316, 'force': [0.46599122881889343, 0.17207498848438263, -1.45326566696167], 'magnitude': 1.5358186960220337, 'distance': 14.702767372131348, 'directional_contribution': -0.19356862820591125}, {'ion': 1387, 'force': [1.0968544483184814, 0.3437471389770508, -2.457841634750366], 'magnitude': 2.7133443355560303, 'distance': 11.061565399169922, 'directional_contribution': -0.6308122367540214}, {'ion': 1460, 'force': [5.049988269805908, 1.1790555715560913, -5.30512809753418], 'magnitude': 7.4186882972717285, 'distance': 6.6896820068359375, 'directional_contribution': -3.991540987216098}, {'ion': 2433, 'force': [2.4973526000976562, 4.697594165802002, -0.34028828144073486], 'magnitude': 5.3310370445251465, 'distance': 7.891565799713135, 'directional_contribution': -3.6909476351492234}]}, 3337: {'frame': 3337, 'ionic_force': [-1.0386495990678668, 10.650418624281883, -13.788317680358887], 'ionic_force_magnitude': 17.45359316348905, 'motion_vector': [0.44036865234375, 2.80010986328125, -1.7934036254882812], 'cosine_ionic_motion': 0.9239821916649363, 'ionic_motion_component': 16.12680926362876, 'ionic_force_x': -1.0386495990678668, 'ionic_force_y': 10.650418624281883, 'ionic_force_z': -13.788317680358887, 'radial_force': 10.70094434440691, 'axial_force': -13.788317680358887, 'contributions': [{'ion': 1387, 'force': [-0.007922927848994732, 0.10124565660953522, -2.5693626403808594], 'magnitude': 2.571368932723999, 'distance': 11.362838745117188, 'directional_contribution': 1.4572403853948068}, {'ion': 1460, 'force': [0.24486219882965088, 0.3454366624355316, -9.121464729309082], 'magnitude': 9.13128662109375, 'distance': 6.029801845550537, 'directional_contribution': 5.197489938044287}, {'ion': 2433, 'force': [-1.275588870048523, 10.203736305236816, -2.0974903106689453], 'magnitude': 10.494894981384277, 'distance': 5.624449253082275, 'directional_contribution': 9.472079013835085}]}, 3338: {'frame': 3338, 'ionic_force': [0.4838514244183898, 6.611688911914825, -7.909306526184082], 'ionic_force_magnitude': 10.320158535312686, 'motion_vector': [0.3501434326171875, -1.3354682922363281, -0.2438507080078125], 'cosine_ionic_motion': -0.4652546041033829, 'ionic_motion_component': -4.801501273631051, 'ionic_force_x': 0.4838514244183898, 'ionic_force_y': 6.611688911914825, 'ionic_force_z': -7.909306526184082, 'radial_force': 6.629369688654355, 'axial_force': -7.909306526184082, 'contributions': [{'ion': 1387, 'force': [0.04897297918796539, 0.46202152967453003, -1.8418389558792114], 'magnitude': 1.8995349407196045, 'distance': 13.22042465209961, 'directional_contribution': -0.10751520117704749}, {'ion': 1460, 'force': [0.4208226501941681, 1.4192343950271606, -4.18621301651001], 'magnitude': 4.4402360916137695, 'distance': 8.647010803222656, 'directional_contribution': -0.5186842424025317}, {'ion': 2433, 'force': [0.014055795036256313, 4.730432987213135, -1.8812545537948608], 'magnitude': 5.09080696105957, 'distance': 8.075617790222168, 'directional_contribution': -4.175301935356039}]}, 3339: {'frame': 3339, 'ionic_force': [1.6150415539741516, 6.130378037691116, -9.246256113052368], 'ionic_force_magnitude': 11.21084948673503, 'motion_vector': [3.524639129638672, 0.14524078369140625, 2.0793838500976562], 'cosine_ionic_motion': -0.27541953448901435, 'ionic_motion_component': -3.0876869468629677, 'ionic_force_x': 1.6150415539741516, 'ionic_force_y': 6.130378037691116, 'ionic_force_z': -9.246256113052368, 'radial_force': 6.339549992394478, 'axial_force': -9.246256113052368, 'contributions': [{'ion': 1387, 'force': [0.22951126098632812, 0.4398341476917267, -2.3072080612182617], 'magnitude': 2.3599445819854736, 'distance': 11.860913276672363, 'directional_contribution': -0.9584526927085806}, {'ion': 1460, 'force': [0.8212767243385315, 1.1787450313568115, -4.737607955932617], 'magnitude': 4.950643062591553, 'distance': 8.189139366149902, 'directional_contribution': -1.6570464033133092}, {'ion': 2433, 'force': [0.564253568649292, 4.511798858642578, -2.2014400959014893], 'magnitude': 5.051836013793945, 'distance': 8.106705665588379, 'directional_contribution': -0.47218808329276385}]}, 3340: {'frame': 3340, 'ionic_force': [7.662343084812164, 5.0752958953380585, -9.21539893746376], 'ionic_force_magnitude': 13.01513378921678, 'motion_vector': [-0.8464088439941406, -2.9289093017578125, 0.38051605224609375], 'cosine_ionic_motion': -0.6216180445886148, 'ionic_motion_component': -8.090442016112144, 'ionic_force_x': 7.662343084812164, 'ionic_force_y': 5.0752958953380585, 'ionic_force_z': -9.21539893746376, 'radial_force': 9.19076329662581, 'axial_force': -9.21539893746376, 'contributions': [{'ion': 1316, 'force': [0.6508142352104187, 0.245817631483078, -1.7105921506881714], 'magnitude': 1.8466485738754272, 'distance': 13.408398628234863, 'directional_contribution': -0.6254827999084984}, {'ion': 1387, 'force': [1.4326162338256836, 0.5672101974487305, -2.7843194007873535], 'magnitude': 3.1822242736816406, 'distance': 10.214183807373047, 'directional_contribution': -1.2802208037761034}, {'ion': 1460, 'force': [4.253185749053955, 1.8484575748443604, -4.438457012176514], 'magnitude': 6.4192118644714355, 'distance': 7.191643714904785, 'directional_contribution': -3.483519195765453}, {'ion': 2433, 'force': [1.325726866722107, 2.4138104915618896, -0.2820303738117218], 'magnitude': 2.7683160305023193, 'distance': 10.951187133789062, 'directional_contribution': -2.701219314438271}]}, 3341: {'frame': 3341, 'ionic_force': [14.888546645641327, 3.9325586408376694, -6.769061803817749], 'ionic_force_magnitude': 16.821237659190512, 'motion_vector': [0.7330703735351562, 1.167449951171875, -0.67529296875], 'cosine_ionic_motion': 0.7775177842387024, 'ionic_motion_component': 13.078811432926425, 'ionic_force_x': 14.888546645641327, 'ionic_force_y': 3.9325586408376694, 'ionic_force_z': -6.769061803817749, 'radial_force': 15.399150583167392, 'axial_force': -6.769061803817749, 'contributions': [{'ion': 1316, 'force': [0.40359848737716675, -0.08952778577804565, -1.4260478019714355], 'magnitude': 1.4847623109817505, 'distance': 14.953420639038086, 'directional_contribution': 0.7519972570620421}, {'ion': 1387, 'force': [0.9169735908508301, -0.240996316075325, -2.4629430770874023], 'magnitude': 2.639130115509033, 'distance': 11.216015815734863, 'directional_contribution': 1.338115802175614}, {'ion': 1460, 'force': [4.683155536651611, -1.4487550258636475, -5.592735767364502], 'magnitude': 7.437037944793701, 'distance': 6.681424140930176, 'directional_contribution': 3.5949966741954995}, {'ion': 2433, 'force': [8.884819030761719, 5.7118377685546875, 2.712664842605591], 'magnitude': 10.90521240234375, 'distance': 5.517622470855713, 'directional_contribution': 7.3937018143221}]}, 3342: {'frame': 3342, 'ionic_force': [9.231768727302551, 6.486842645332217, -8.162149548530579], 'ionic_force_magnitude': 13.925708836259645, 'motion_vector': [-1.4764938354492188, 1.4851150512695312, 0.42453765869140625], 'cosine_ionic_motion': -0.2507741042712223, 'ionic_motion_component': -3.4922071597548583, 'ionic_force_x': 9.231768727302551, 'ionic_force_y': 6.486842645332217, 'ionic_force_z': -8.162149548530579, 'radial_force': 11.282937620128104, 'axial_force': -8.162149548530579, 'contributions': [{'ion': 1387, 'force': [0.796237587928772, 0.016238732263445854, -1.9542186260223389], 'magnitude': 2.110267400741577, 'distance': 12.542967796325684, 'directional_contribution': -0.9271717172143745}, {'ion': 1460, 'force': [3.3354697227478027, 0.10465142130851746, -4.341390609741211], 'magnitude': 5.475763320922852, 'distance': 7.786579132080078, 'directional_contribution': -3.094591785827248}, {'ion': 2433, 'force': [5.100061416625977, 6.365952491760254, -1.8665403127670288], 'magnitude': 8.367792129516602, 'distance': 6.29888391494751, 'directional_contribution': 0.5295565281574355}]}, 3343: {'frame': 3343, 'ionic_force': [6.78049048781395, 6.935463041067123, -10.414144240319729], 'ionic_force_magnitude': 14.231307006298756, 'motion_vector': [-1.2784309387207031, -1.8371505737304688, -1.54437255859375], 'cosine_ionic_motion': -0.13764005680158262, 'ionic_motion_component': -1.9587979047077215, 'ionic_force_x': 6.78049048781395, 'ionic_force_y': 6.935463041067123, 'ionic_force_z': -10.414144240319729, 'radial_force': 9.699262799272091, 'axial_force': -10.414144240319729, 'contributions': [{'ion': 1316, 'force': [0.30228039622306824, 0.15748772025108337, -1.4446684122085571], 'magnitude': 1.4843324422836304, 'distance': 14.955586433410645, 'directional_contribution': 0.5719607082213471}, {'ion': 1387, 'force': [0.6677933931350708, 0.4127635955810547, -2.39450740814209], 'magnitude': 2.519918203353882, 'distance': 11.478253364562988, 'directional_contribution': 0.7670998458948546}, {'ion': 1460, 'force': [3.6871559619903564, 1.7069761753082275, -6.695205211639404], 'magnitude': 7.831644535064697, 'distance': 6.510922908782959, 'directional_contribution': 0.91572990354382}, {'ion': 2433, 'force': [2.123260736465454, 4.658235549926758, 0.12023679167032242], 'magnitude': 5.1207275390625, 'distance': 8.051989555358887, 'directional_contribution': -4.21358843681035}]}, 3344: {'frame': 3344, 'ionic_force': [4.965911656618118, 8.838596478104591, -13.473165035247803], 'ionic_force_magnitude': 16.861412821917458, 'motion_vector': [3.2638702392578125, 0.03415679931640625, 2.7843475341796875], 'cosine_ionic_motion': -0.29034934299537596, 'ionic_motion_component': -4.895700134817542, 'ionic_force_x': 4.965911656618118, 'ionic_force_y': 8.838596478104591, 'ionic_force_z': -13.473165035247803, 'radial_force': 10.138099737332366, 'axial_force': -13.473165035247803, 'contributions': [{'ion': 1387, 'force': [0.446129709482193, -0.06396286189556122, -2.735747814178467], 'magnitude': 2.772623062133789, 'distance': 10.94267749786377, 'directional_contribution': -1.4365799324708046}, {'ion': 1460, 'force': [1.9232772588729858, -0.41003602743148804, -6.321849346160889], 'magnitude': 6.620642185211182, 'distance': 7.081397533416748, 'directional_contribution': -2.642920945873833}, {'ion': 2433, 'force': [2.5965046882629395, 9.31259536743164, -4.415567874908447], 'magnitude': 10.628429412841797, 'distance': 5.589004993438721, 'directional_contribution': -0.8161990217935475}]}, 3345: {'frame': 3345, 'ionic_force': [11.459057569503784, 4.5299258679151535, -9.10696730017662], 'ionic_force_magnitude': 15.322110891012866, 'motion_vector': [1.4095878601074219, 1.650238037109375, -2.3775634765625], 'cosine_ionic_motion': 0.9180117022436276, 'ionic_motion_component': 14.065877101024347, 'ionic_force_x': 11.459057569503784, 'ionic_force_y': 4.5299258679151535, 'ionic_force_z': -9.10696730017662, 'radial_force': 12.321940948974266, 'axial_force': -9.10696730017662, 'contributions': [{'ion': 1316, 'force': [0.602062463760376, -0.06746698170900345, -1.5646878480911255], 'magnitude': 1.6778793334960938, 'distance': 14.066584587097168, 'directional_contribution': 1.3846653387323933}, {'ion': 1387, 'force': [1.3200268745422363, -0.06782228499650955, -2.4617674350738525], 'magnitude': 2.7941670417785645, 'distance': 10.900410652160645, 'directional_contribution': 2.3614123977009704}, {'ion': 1460, 'force': [5.418282985687256, -0.2359398603439331, -4.656142711639404], 'magnitude': 7.147945404052734, 'distance': 6.815197467803955, 'directional_contribution': 5.690437196735175}, {'ion': 2433, 'force': [4.118685245513916, 4.9011549949646, -0.42436930537223816], 'magnitude': 6.415993690490723, 'distance': 7.193447113037109, 'directional_contribution': 4.629362064755696}]}, 3346: {'frame': 3346, 'ionic_force': [7.0407936573028564, 4.407854497432709, -5.5570178627967834], 'ionic_force_magnitude': 9.994118476518898, 'motion_vector': [-3.005786895751953, -0.8942451477050781, 2.5088882446289062], 'cosine_ionic_motion': -0.9728312076224561, 'ionic_motion_component': -9.72259034663378, 'ionic_force_x': 7.0407936573028564, 'ionic_force_y': 4.407854497432709, 'ionic_force_z': -5.5570178627967834, 'radial_force': 8.30674163527757, 'axial_force': -5.5570178627967834, 'contributions': [{'ion': 1387, 'force': [1.2626168727874756, 0.2959780693054199, -1.982247233390808], 'magnitude': 2.3687777519226074, 'distance': 11.838778495788574, 'directional_contribution': -2.249222186355972}, {'ion': 1460, 'force': [3.078824758529663, 0.8143443465232849, -2.7305893898010254], 'magnitude': 4.195049285888672, 'distance': 8.896117210388184, 'directional_contribution': -4.191457977518737}, {'ion': 2433, 'force': [2.6993520259857178, 3.297532081604004, -0.84418123960495], 'magnitude': 4.344290733337402, 'distance': 8.741975784301758, 'directional_contribution': -3.281910109448056}]}, 3347: {'frame': 3347, 'ionic_force': [12.897669553756714, 7.732845552265644, -13.545651823282242], 'ionic_force_magnitude': 20.23935432692177, 'motion_vector': [1.4391937255859375, -0.04620361328125, -0.0015106201171875], 'cosine_ionic_motion': 0.6253710512073722, 'ionic_motion_component': 12.657106291185546, 'ionic_force_x': 12.897669553756714, 'ionic_force_y': 7.732845552265644, 'ionic_force_z': -13.545651823282242, 'radial_force': 15.038177424578334, 'axial_force': -13.545651823282242, 'contributions': [{'ion': 1316, 'force': [0.4173687696456909, 0.10308853536844254, -1.7034296989440918], 'magnitude': 1.756842851638794, 'distance': 13.746830940246582, 'directional_contributio</t>
+          <t>{3320: {'frame': 3320, 'ionic_force': [4.8733450174331665, 3.184350647032261, -8.640591382980347], 'ionic_force_magnitude': 10.418704341223512, 'motion_vector': [-0.18167495727539062, 0.760711669921875, 0.7443389892578125], 'cosine_ionic_motion': -0.4351086894470255, 'ionic_motion_component': -4.533268791645797, 'ionic_force_x': 4.8733450174331665, 'ionic_force_y': 3.184350647032261, 'ionic_force_z': -8.640591382980347, 'radial_force': 5.821475818226461, 'axial_force': -8.640591382980347, 'contributions': [{'ion': 1387, 'force': [0.3318135738372803, -0.0069795772433280945, -1.9514002799987793], 'magnitude': 1.9794220924377441, 'distance': 12.950896263122559, 'cosine_with_motion': -0.7103326722280674, 'motion_component': -1.4060482193826478}, {'ion': 1460, 'force': [1.624815821647644, -0.2846843898296356, -5.312528133392334], 'magnitude': 5.562735557556152, 'distance': 7.725468635559082, 'cosine_with_motion': -0.7435987748913293, 'motion_component': -4.1364433416914}, {'ion': 2433, 'force': [2.916715621948242, 3.4760146141052246, -1.3766629695892334], 'magnitude': 4.741846561431885, 'distance': 8.367491722106934, 'cosine_with_motion': 0.21283327257076928, 'motion_component': 1.0092227157837357}]}, 3321: {'frame': 3321, 'ionic_force': [4.962071061134338, 4.828094765543938, -10.522126078605652], 'ionic_force_magnitude': 12.595546256311902, 'motion_vector': [3.44659423828125, 0.5642127990722656, -0.29720306396484375], 'cosine_ionic_motion': 0.5199156061735278, 'ionic_motion_component': 6.548621066937112, 'ionic_force_x': 4.962071061134338, 'ionic_force_y': 4.828094765543938, 'ionic_force_z': -10.522126078605652, 'radial_force': 6.9233408323452945, 'axial_force': -10.522126078605652, 'contributions': [{'ion': 1387, 'force': [0.4181758165359497, 0.16234956681728363, -2.319929599761963], 'magnitude': 2.362901210784912, 'distance': 11.853490829467773, 'cosine_with_motion': 0.26833152479280165, 'motion_component': 0.6340408627544847}, {'ion': 1460, 'force': [2.362652540206909, 0.5963982939720154, -7.155970096588135], 'magnitude': 7.559479236602783, 'distance': 6.62709379196167, 'cosine_with_motion': 0.40029079586086974, 'motion_component': 3.0259899505259265}, {'ion': 2433, 'force': [2.1812427043914795, 4.069346904754639, -1.0462263822555542], 'magnitude': 4.734130859375, 'distance': 8.374307632446289, 'cosine_with_motion': 0.6101627710360925, 'motion_component': 2.8885903144106857}]}, 3322: {'frame': 3322, 'ionic_force': [5.101867258548737, 2.400673806667328, -5.333805024623871], 'ionic_force_magnitude': 7.761556563639349, 'motion_vector': [-1.1910209655761719, 1.1273345947265625, 1.091339111328125], 'cosine_ionic_motion': -0.6011411421058467, 'ionic_motion_component': -4.665790977185289, 'ionic_force_x': 5.101867258548737, 'ionic_force_y': 2.400673806667328, 'ionic_force_z': -5.333805024623871, 'radial_force': 5.638464706803635, 'axial_force': -5.333805024623871, 'contributions': [{'ion': 1387, 'force': [0.8166144490242004, 0.16744935512542725, -1.7120360136032104], 'magnitude': 1.904196858406067, 'distance': 13.204231262207031, 'cosine_with_motion': -0.7070687055580778, 'motion_component': -1.3463980228761798}, {'ion': 1460, 'force': [2.6996209621429443, 0.5092499852180481, -3.1144349575042725], 'magnitude': 4.152949810028076, 'distance': 8.941094398498535, 'cosine_with_motion': -0.7383261436332469, 'motion_component': -3.066231583865708}, {'ion': 2433, 'force': [1.5856318473815918, 1.7239744663238525, -0.5073340535163879], 'magnitude': 2.3966026306152344, 'distance': 11.769852638244629, 'cosine_with_motion': -0.10563347096891086, 'motion_component': -0.2531614541572438}]}, 3323: {'frame': 3323, 'ionic_force': [5.707005620002747, 4.04939991235733, -7.091884225606918], 'ionic_force_magnitude': 9.963050469929113, 'motion_vector': [-0.09119033813476562, -1.4596443176269531, 0.58355712890625], 'cosine_ionic_motion': -0.6737404389098686, 'ionic_motion_component': -6.712509996491213, 'ionic_force_x': 5.707005620002747, 'ionic_force_y': 4.04939991235733, 'ionic_force_z': -7.091884225606918, 'radial_force': 6.997681958830545, 'axial_force': -7.091884225606918, 'contributions': [{'ion': 1387, 'force': [0.8393199443817139, 0.3989105820655823, -2.18998122215271], 'magnitude': 2.3789925575256348, 'distance': 11.813334465026855, 'cosine_with_motion': -0.5170273796606956, 'motion_component': -1.2300042650106304}, {'ion': 1460, 'force': [3.4794766902923584, 1.5985596179962158, -4.6523637771606445], 'magnitude': 6.02549934387207, 'distance': 7.422881603240967, 'cosine_with_motion': -0.5655173853401619, 'motion_component': -3.4075245058578427}, {'ion': 2433, 'force': [1.3882089853286743, 2.0519297122955322, -0.24953922629356384], 'magnitude': 2.4899415969848633, 'distance': 11.547141075134277, 'cosine_with_motion': -0.8333453521952254, 'motion_component': -2.0749813240573336}]}, 3324: {'frame': 3324, 'ionic_force': [9.42669403553009, 3.5997143760323524, -10.327790841460228], 'ionic_force_magnitude': 14.438966988447003, 'motion_vector': [1.4581718444824219, 0.5040359497070312, -1.6050872802734375], 'cosine_ionic_motion': 0.9997192109901553, 'ionic_motion_component': 14.434912685203136, 'ionic_force_x': 9.42669403553009, 'ionic_force_y': 3.5997143760323524, 'ionic_force_z': -10.327790841460228, 'radial_force': 10.090614650679738, 'axial_force': -10.327790841460228, 'contributions': [{'ion': 1316, 'force': [0.5152910947799683, 0.09902171045541763, -1.5304564237594604], 'magnitude': 1.617908239364624, 'distance': 14.32491683959961, 'cosine_with_motion': 0.9044381588025899, 'motion_component': 1.4632979506664054}, {'ion': 1387, 'force': [1.6848300695419312, 0.3395357131958008, -3.116074562072754], 'magnitude': 3.558631420135498, 'distance': 9.658897399902344, 'cosine_with_motion': 0.9629840296835332, 'motion_component': 3.4269052191387033}, {'ion': 1460, 'force': [5.295093536376953, 0.8498631119728088, -5.482320308685303], 'magnitude': 7.6691670417785645, 'distance': 6.579531192779541, 'cosine_with_motion': 0.9926726186717297, 'motion_component': 7.612971853423932}, {'ion': 2433, 'force': [1.9314793348312378, 2.311293840408325, -0.19893954694271088], 'magnitude': 3.018653392791748, 'distance': 10.487269401550293, 'cosine_with_motion': 0.6399335650787177, 'motion_component': 1.9317376565473425}]}, 3325: {'frame': 3325, 'ionic_force': [6.025220155715942, 3.329250246286392, -5.533735513687134], 'ionic_force_magnitude': 8.832293805274247, 'motion_vector': [-1.0484428405761719, -1.0520210266113281, -0.158599853515625], 'cosine_ionic_motion': -0.6777865381816526, 'ionic_motion_component': -5.986409842480087, 'ionic_force_x': 6.025220155715942, 'ionic_force_y': 3.329250246286392, 'ionic_force_z': -5.533735513687134, 'radial_force': 6.883835059561178, 'axial_force': -5.533735513687134, 'contributions': [{'ion': 1387, 'force': [1.0765461921691895, 0.23434945940971375, -2.0206117630004883], 'magnitude': 2.3014655113220215, 'distance': 12.010658264160156, 'cosine_with_motion': -0.3068244551499629, 'motion_component': -0.7061458862244105}, {'ion': 1460, 'force': [2.5632970333099365, 0.5630773901939392, -3.0066704750061035], 'magnitude': 3.9909415245056152, 'distance': 9.120766639709473, 'cosine_with_motion': -0.47019937350483226, 'motion_component': -1.8765382588053043}, {'ion': 2433, 'force': [2.3853769302368164, 2.5318233966827393, -0.506453275680542], 'magnitude': 3.515202283859253, 'distance': 9.718379974365234, 'cosine_with_motion': -0.9682872249034437, 'motion_component': -3.403725551910478}]}, 3326: {'frame': 3326, 'ionic_force': [5.521149039268494, 2.2750196903944016, -6.492782413959503], 'ionic_force_magnitude': 8.821282490688043, 'motion_vector': [0.80645751953125, 0.5555877685546875, -0.410614013671875], 'cosine_ionic_motion': 0.8948647231467417, 'ionic_motion_component': 7.893854513828756, 'ionic_force_x': 5.521149039268494, 'ionic_force_y': 2.2750196903944016, 'ionic_force_z': -6.492782413959503, 'radial_force': 5.971499083605192, 'axial_force': -6.492782413959503, 'contributions': [{'ion': 1387, 'force': [0.7306075096130371, 0.05163702368736267, -1.8644970655441284], 'magnitude': 2.0031981468200684, 'distance': 12.873809814453125, 'cosine_with_motion': 0.6503710687869672, 'motion_component': 1.3028221533939597}, {'ion': 1460, 'force': [2.9076755046844482, 0.214521124958992, -4.017284393310547], 'magnitude': 4.963785648345947, 'distance': 8.178290367126465, 'cosine_with_motion': 0.7804168984028671, 'motion_component': 3.873822364127798}, {'ion': 2433, 'force': [1.8828660249710083, 2.008861541748047, -0.6110009551048279], 'magnitude': 2.820289134979248, 'distance': 10.849812507629395, 'cosine_with_motion': 0.9634508776201375, 'motion_component': 2.7172101317688018}]}, 3327: {'frame': 3327, 'ionic_force': [4.962403953075409, 2.0606805086135864, -5.490831732749939], 'ionic_force_magnitude': 7.682518484810309, 'motion_vector': [-0.40179443359375, 0.5124359130859375, 0.6054840087890625], 'cosine_ionic_motion': -0.6239824605969704, 'ionic_motion_component': -4.7937567877336456, 'ionic_force_x': 4.962403953075409, 'ionic_force_y': 2.0606805086135864, 'ionic_force_z': -5.490831732749939, 'radial_force': 5.373253870056615, 'axial_force': -5.490831732749939, 'contributions': [{'ion': 1387, 'force': [0.7123898863792419, 0.10276107490062714, -1.644201397895813], 'magnitude': 1.7948418855667114, 'distance': 13.600533485412598, 'cosine_with_motion': -0.7701518053219849, 'motion_component': -1.382300725170892}, {'ion': 1460, 'force': [2.544466972351074, 0.2279723435640335, -3.2194597721099854], 'magnitude': 4.109890937805176, 'distance': 8.987810134887695, 'cosine_with_motion': -0.7812058518484315, 'motion_component': -3.2106709714302584}, {'ion': 2433, 'force': [1.7055470943450928, 1.7299470901489258, -0.6271705627441406], 'magnitude': 2.508974075317383, 'distance': 11.503260612487793, 'cosine_with_motion': -0.0800267830802497, 'motion_component': -0.20078512136664983}]}, 3328: {'frame': 3328, 'ionic_force': [5.662827789783478, 2.698476254940033, -6.413617879152298], 'ionic_force_magnitude': 8.971281233748122, 'motion_vector': [-1.1094818115234375, 0.8973617553710938, 1.1634902954101562], 'cosine_ionic_motion': -0.6855367750310243, 'ionic_motion_component': -6.150143204880036, 'ionic_force_x': 5.662827789783478, 'ionic_force_y': 2.698476254940033, 'ionic_force_z': -6.413617879152298, 'radial_force': 6.272909426671105, 'axial_force': -6.413617879152298, 'contributions': [{'ion': 1387, 'force': [0.7809037566184998, 0.18411484360694885, -1.7854108810424805], 'magnitude': 1.9573965072631836, 'distance': 13.023557662963867, 'cosine_with_motion': -0.7709661628922033, 'motion_component': -1.5090864508773922}, {'ion': 1460, 'force': [3.093663454055786, 0.4853256046772003, -4.167239665985107], 'magnitude': 5.21269416809082, 'distance': 7.9806437492370605, 'cosine_with_motion': -0.8174437983446711, 'motion_component': -4.261084555910353}, {'ion': 2433, 'force': [1.788260579109192, 2.029035806655884, -0.4609673321247101], 'magnitude': 2.7436022758483887, 'distance': 11.000399589538574, 'cosine_with_motion': -0.1384938768402133, 'motion_component': -0.3799721065212349}]}, 3329: {'frame': 3329, 'ionic_force': [6.12342631816864, 5.340087965130806, -8.698342144489288], 'ionic_force_magnitude': 11.90269067950494, 'motion_vector': [0.8754844665527344, -1.0129776000976562, 0.6521530151367188], 'cosine_ionic_motion': -0.3227464606590609, 'ionic_motion_component': -3.8415512891298116, 'ionic_force_x': 6.12342631816864, 'ionic_force_y': 5.340087965130806, 'ionic_force_z': -8.698342144489288, 'radial_force': 8.12483165052515, 'axial_force': -8.698342144489288, 'contributions': [{'ion': 1316, 'force': [0.37819957733154297, 0.24994249641895294, -1.4104505777359009], 'magnitude': 1.4815117120742798, 'distance': 14.969817161560059, 'cosine_with_motion': -0.38158253503441575, 'motion_component': -0.5653190013484792}, {'ion': 1387, 'force': [0.9713860750198364, 0.7008095979690552, -2.4578428268432617], 'magnitude': 2.734175682067871, 'distance': 11.019346237182617, 'cosine_with_motion': -0.35913446296586105, 'motion_component': -0.9819366955576072}, {'ion': 1460, 'force': [3.2983713150024414, 2.064893960952759, -4.52915096282959], 'magnitude': 5.971285343170166, 'distance': 7.456501483917236, 'cosine_with_motion': -0.2426363541558891, 'motion_component': -1.4488509092765014}, {'ion': 2433, 'force': [1.4754693508148193, 2.324441909790039, -0.3008977770805359], 'magnitude': 2.7695810794830322, 'distance': 10.948685646057129, 'cosine_with_motion': -0.3052609156370647, 'motion_component': -0.8454448625147428}]}, 3330: {'frame': 3330, 'ionic_force': [8.562611877918243, 3.4708504751324654, -9.022035978734493], 'ionic_force_magnitude': 12.913646208339978, 'motion_vector': [1.0237197875976562, -1.2902107238769531, 0.8571853637695312], 'cosine_ionic_motion': -0.14371961245459278, 'ionic_motion_component': -1.8559442284383432, 'ionic_force_x': 8.562611877918243, 'ionic_force_y': 3.4708504751324654, 'ionic_force_z': -9.022035978734493, 'radial_force': 9.239324931649165, 'axial_force': -9.022035978734493, 'contributions': [{'ion': 1316, 'force': [0.5562570691108704, 0.11473546177148819, -1.4796452522277832], 'magnitude': 1.5849088430404663, 'distance': 14.47327709197998, 'cosine_with_motion': -0.28779764622325893, 'motion_component': -0.4561330512855037}, {'ion': 1387, 'force': [1.3070932626724243, 0.29501739144325256, -2.6750640869140625], 'magnitude': 2.9919052124023438, 'distance': 10.53404426574707, 'cosine_with_motion': -0.24041965554896735, 'motion_component': -0.7193127855523347}, {'ion': 1460, 'force': [4.905503273010254, 1.0822356939315796, -4.953392505645752], 'magnitude': 7.054877281188965, 'distance': 6.8600029945373535, 'cosine_with_motion': -0.04736466428845592, 'motion_component': -0.33415189509761234}, {'ion': 2433, 'force': [1.7937582731246948, 1.978861927986145, 0.0860658660531044], 'magnitude': 2.672240734100342, 'distance': 11.146313667297363, 'cosine_with_motion': -0.12960900139424755, 'motion_component': -0.3463464546020445}]}, 3331: {'frame': 3331, 'ionic_force': [12.735351324081421, 2.3743116538971663, -6.971976637840271], 'ionic_force_magnitude': 14.711729586156919, 'motion_vector': [-1.5520782470703125, 0.7276382446289062, -2.8383560180664062], 'cosine_ionic_motion': 0.035881050304702455, 'ionic_motion_component': 0.5278723093500758, 'ionic_force_x': 12.735351324081421, 'ionic_force_y': 2.3743116538971663, 'ionic_force_z': -6.971976637840271, 'radial_force': 12.954787886245544, 'axial_force': -6.971976637840271, 'contributions': [{'ion': 1316, 'force': [0.7236177921295166, -0.01991807110607624, -1.514197587966919], 'magnitude': 1.6783366203308105, 'distance': 14.064668655395508, 'cosine_with_motion': 0.5678690160279444, 'motion_component': 0.9530753588752279}, {'ion': 1387, 'force': [2.3421452045440674, -0.13869722187519073, -2.969356060028076], 'magnitude': 3.784435987472534, 'distance': 9.366308212280273, 'cosine_with_motion': 0.3739069185928592, 'motion_component': 1.4150268355639988}, {'ion': 1460, 'force': [6.530500888824463, -0.4096313416957855, -3.7830898761749268], 'magnitude': 7.558241367340088, 'distance': 6.627636432647705, 'cosine_with_motion': 0.01212381215447484, 'motion_component': 0.09163469545941672}, {'ion': 2433, 'force': [3.139087438583374, 2.9425582885742188, 1.2946668863296509], 'magnitude': 4.4931817054748535, 'distance': 8.595913887023926, 'cosine_with_motion': -0.42995467800748755, 'motion_component': -1.931864480817218}]}, 3332: {'frame': 3332, 'ionic_force': [5.920918166637421, 3.972064346075058, -6.426218777894974], 'ionic_force_magnitude': 9.598481905319595, 'motion_vector': [0.7343177795410156, 1.0062751770019531, 2.0959930419921875], 'cosine_ionic_motion': -0.21896350382145063, 'ionic_motion_component': -2.1017172293555717, 'ionic_force_x': 5.920918166637421, 'ionic_force_y': 3.972064346075058, 'ionic_force_z': -6.426218777894974, 'radial_force': 7.12983640102476, 'axial_force': -6.426218777894974, 'contributions': [{'ion': 1387, 'force': [0.6480094790458679, 0.07161861658096313, -1.956294298171997], 'magnitude': 2.06207013130188, 'distance': 12.688705444335938, 'cosine_with_motion': -0.7065626176169941, 'motion_component': -1.4569816124307788}, {'ion': 1460, 'force': [2.506962299346924, 0.3197813332080841, -4.0640716552734375], 'magnitude': 4.785791397094727, 'distance': 8.328987121582031, 'cosine_with_motion': -0.5446592892584318, 'motion_component': -2.606625695022325}, {'ion': 2433, 'force': [2.765946388244629, 3.5806643962860107, -0.4058528244495392], 'magnitude': 4.542723178863525, 'distance': 8.54891300201416, 'cosine_with_motion': 0.43187531744995167, 'motion_component': 1.9618899948423572}]}, 3333: {'frame': 3333, 'ionic_force': [11.138619840145111, 7.894609674811363, -10.194625984877348], 'ionic_force_magnitude': 17.038899988920527, 'motion_vector': [-0.58197021484375, -0.06623077392578125, -0.9650726318359375], 'cosine_ionic_motion': 0.1472983279094927, 'ionic_motion_component': 2.5098014777850675, 'ionic_force_x': 11.138619840145111, 'ionic_force_y': 7.894609674811363, 'ionic_force_z': -10.194625984877348, 'radial_force': 13.652608317127518, 'axial_force': -10.194625984877348, 'contributions': [{'ion': 1316, 'force': [0.6237956881523132, 0.15656648576259613, -1.627447485923767], 'magnitude': 1.7499197721481323, 'distance': 13.773996353149414, 'cosine_with_motion': 0.6060249544382219, 'motion_component': 1.06049509096636}, {'ion': 1387, 'force': [1.9665889739990234, 0.6323477029800415, -3.3439724445343018], 'magnitude': 3.9305837154388428, 'distance': 9.190528869628906, 'cosine_with_motion': 0.4599211400015446, 'motion_component': 1.8077584950588932}, {'ion': 1460, 'force': [5.7677435874938965, 2.1759836673736572, -5.206416130065918], 'magnitude': 8.068985939025879, 'distance': 6.414451599121094, 'cosine_with_motion': 0.16728169529424516, 'motion_component': 1.3497937077936975}, {'ion': 2433, 'force': [2.780491590499878, 4.929711818695068, -0.01678992435336113], 'magnitude': 5.659811973571777, 'distance': 7.658928871154785, 'cosine_with_motion': -0.30182028666503474, 'motion_component': -1.7082461370083915}]}, 3334: {'frame': 3334, 'ionic_force': [8.556934595108032, 6.820997595787048, -7.33417646586895], 'ionic_force_magnitude': 13.173355013025168, 'motion_vector': [0.17787933349609375, -0.084075927734375, 0.6251068115234375], 'cosine_ionic_motion': -0.42117706074107514, 'ionic_motion_component': -5.548314944484647, 'ionic_force_x': 8.556934595108032, 'ionic_force_y': 6.820997595787048, 'ionic_force_z': -7.33417646586895, 'radial_force': 10.942903539129336, 'axial_force': -7.33417646586895, 'contributions': [{'ion': 1387, 'force': [1.4384901523590088, 0.4807847738265991, -2.7401866912841797], 'magnitude': 3.131937265396118, 'distance': 10.295857429504395, 'cosine_with_motion': -0.7295832994848833, 'motion_component': -2.2850091222240625}, {'ion': 1460, 'force': [4.045209884643555, 1.0065531730651855, -4.721059799194336], 'magnitude': 6.298037528991699, 'distance': 7.260498046875, 'cosine_with_motion': -0.5611922266405833, 'motion_component': -3.534409758359267}, {'ion': 2433, 'force': [3.0732345581054688, 5.333659648895264, 0.12707002460956573], 'magnitude': 6.157015800476074, 'distance': 7.343175411224365, 'cosine_with_motion': 0.04403173563774378, 'motion_component': 0.2711040889088734}]}, 3335: {'frame': 3335, 'ionic_force': [10.957434237003326, 7.65510667860508, -10.461147874593735], 'ionic_force_magnitude': 16.973557027717963, 'motion_vector': [0.046604156494140625, 0.275848388671875, -0.0363616943359375], 'cosine_ionic_motion': 0.627074144131308, 'ionic_motion_component': 10.64367874602019, 'ionic_force_x': 10.957434237003326, 'ionic_force_y': 7.65510667860508, 'ionic_force_z': -10.461147874593735, 'radial_force': 13.366601038374593, 'axial_force': -10.461147874593735, 'contributions': [{'ion': 1316, 'force': [0.5002949833869934, 0.06886790692806244, -1.5100455284118652], 'magnitude': 1.5922547578811646, 'distance': 14.439852714538574, 'cosine_with_motion': 0.21643463805504745, 'motion_component': 0.344619091924816}, {'ion': 1387, 'force': [1.7298309803009033, 0.3097245991230011, -3.301562786102295], 'magnitude': 3.740128517150879, 'distance': 9.421624183654785, 'cosine_with_motion': 0.27115584312548485, 'motion_component': 1.0141577034043774}, {'ion': 1460, 'force': [5.743025779724121, 1.7341681718826294, -5.573688983917236], 'magnitude': 8.188754081726074, 'distance': 6.36737060546875, 'cosine_with_motion': 0.41066215110078985, 'motion_component': 3.3628113618595847}, {'ion': 2433, 'force': [2.9842824935913086, 5.542346000671387, -0.07585057616233826], 'magnitude': 6.295180320739746, 'distance': 7.262145519256592, 'cosine_with_motion': 0.9407340673341933, 'motion_component': 5.922090530346958}]}, 3336: {'frame': 3336, 'ionic_force': [9.11018654704094, 6.392471864819527, -9.55652368068695], 'ionic_force_magnitude': 14.669231074733448, 'motion_vector': [-4.241512298583984, -1.3926010131835938, -0.917877197265625], 'cosine_ionic_motion': -0.5799124377910689, 'ionic_motion_component': -8.506869553069176, 'ionic_force_x': 9.11018654704094, 'ionic_force_y': 6.392471864819527, 'ionic_force_z': -9.55652368068695, 'radial_force': 11.129204619576143, 'axial_force': -9.55652368068695, 'contributions': [{'ion': 1316, 'force': [0.46599122881889343, 0.17207498848438263, -1.45326566696167], 'magnitude': 1.5358186960220337, 'distance': 14.702767372131348, 'cosine_with_motion': -0.12603612829488975, 'motion_component': -0.19356862820591123}, {'ion': 1387, 'force': [1.0968544483184814, 0.3437471389770508, -2.457841634750366], 'magnitude': 2.7133443355560303, 'distance': 11.061565399169922, 'cosine_with_motion': -0.2324851428875588, 'motion_component': -0.6308122367540214}, {'ion': 1460, 'force': [5.049988269805908, 1.1790555715560913, -5.30512809753418], 'magnitude': 7.4186882972717285, 'distance': 6.6896820068359375, 'cosine_with_motion': -0.538038635350998, 'motion_component': -3.991540987216098}, {'ion': 2433, 'force': [2.4973526000976562, 4.697594165802002, -0.34028828144073486], 'magnitude': 5.3310370445251465, 'distance': 7.891565799713135, 'cosine_with_motion': -0.6923507626904895, 'motion_component': -3.6909476351492234}]}, 3337: {'frame': 3337, 'ionic_force': [-1.0386495990678668, 10.650418624281883, -13.788317680358887], 'ionic_force_magnitude': 17.45359316348905, 'motion_vector': [0.44036865234375, 2.80010986328125, -1.7934036254882812], 'cosine_ionic_motion': 0.9239821916649363, 'ionic_motion_component': 16.12680926362876, 'ionic_force_x': -1.0386495990678668, 'ionic_force_y': 10.650418624281883, 'ionic_force_z': -13.788317680358887, 'radial_force': 10.70094434440691, 'axial_force': -13.788317680358887, 'contributions': [{'ion': 1387, 'force': [-0.007922927848994732, 0.10124565660953522, -2.5693626403808594], 'magnitude': 2.571368932723999, 'distance': 11.362838745117188, 'cosine_with_motion': 0.5667177533058034, 'motion_component': 1.4572403853948068}, {'ion': 1460, 'force': [0.24486219882965088, 0.3454366624355316, -9.121464729309082], 'magnitude': 9.13128662109375, 'distance': 6.029801845550537, 'cosine_with_motion': 0.5691957685666009, 'motion_component': 5.197489938044287}, {'ion': 2433, 'force': [-1.275588870048523, 10.203736305236816, -2.0974903106689453], 'magnitude': 10.494894981384277, 'distance': 5.624449253082275, 'cosine_with_motion': 0.9025415453681213, 'motion_component': 9.472079013835085}]}, 3338: {'frame': 3338, 'ionic_force': [0.4838514244183898, 6.611688911914825, -7.909306526184082], 'ionic_force_magnitude': 10.320158535312686, 'motion_vector': [0.3501434326171875, -1.3354682922363281, -0.2438507080078125], 'cosine_ionic_motion': -0.4652546041033829, 'ionic_motion_component': -4.801501273631051, 'ionic_force_x': 0.4838514244183898, 'ionic_force_y': 6.611688911914825, 'ionic_force_z': -7.909306526184082, 'radial_force': 6.629369688654355, 'axial_force': -7.909306526184082, 'contributions': [{'ion': 1387, 'force': [0.04897297918796539, 0.46202152967453003, -1.8418389558792114], 'magnitude': 1.8995349407196045, 'distance': 13.22042465209961, 'cosine_with_motion': -0.056600802095017826, 'motion_component': -0.10751520117704749}, {'ion': 1460, 'force': [0.4208226501941681, 1.4192343950271606, -4.18621301651001], 'magnitude': 4.4402360916137695, 'distance': 8.647010803222656, 'cosine_with_motion': -0.1168145613509119, 'motion_component': -0.5186842424025317}, {'ion': 2433, 'force': [0.014055795036256313, 4.730432987213135, -1.8812545537948608], 'magnitude': 5.09080696105957, 'distance': 8.075617790222168, 'cosine_with_motion': -0.8201650955329496, 'motion_component': -4.175301935356039}]}, 3339: {'frame': 3339, 'ionic_force': [1.6150415539741516, 6.130378037691116, -9.246256113052368], 'ionic_force_magnitude': 11.21084948673503, 'motion_vector': [3.524639129638672, 0.14524078369140625, 2.0793838500976562], 'cosine_ionic_motion': -0.27541953448901435, 'ionic_motion_component': -3.0876869468629677, 'ionic_force_x': 1.6150415539741516, 'ionic_force_y': 6.130378037691116, 'ionic_force_z': -9.246256113052368, 'radial_force': 6.339549992394478, 'axial_force': -9.246256113052368, 'contributions': [{'ion': 1387, 'force': [0.22951126098632812, 0.4398341476917267, -2.3072080612182617], 'magnitude': 2.3599445819854736, 'distance': 11.860913276672363, 'cosine_with_motion': -0.4061335554517213, 'motion_component': -0.9584526927085806}, {'ion': 1460, 'force': [0.8212767243385315, 1.1787450313568115, -4.737607955932617], 'magnitude': 4.950643062591553, 'distance': 8.189139366149902, 'cosine_with_motion': -0.3347133815773649, 'motion_component': -1.6570464033133092}, {'ion': 2433, 'force': [0.564253568649292, 4.511798858642578, -2.2014400959014893], 'magnitude': 5.051836013793945, 'distance': 8.106705665588379, 'cosine_with_motion': -0.09346860421670186, 'motion_component': -0.47218808329276385}]}, 3340: {'frame': 3340, 'ionic_force': [7.662343084812164, 5.0752958953380585, -9.21539893746376], 'ionic_force_magnitude': 13.01513378921678, 'motion_vector': [-0.8464088439941406, -2.9289093017578125, 0.38051605224609375], 'cosine_ionic_motion': -0.6216180445886148, 'ionic_motion_component': -8.090442016112144, 'ionic_force_x': 7.662343084812164, 'ionic_force_y': 5.0752958953380585, 'ionic_force_z': -9.21539893746376, 'radial_force': 9.19076329662581, 'axial_force': -9.21539893746376, 'contributions': [{'ion': 1316, 'force': [0.6508142352104187, 0.245817631483078, -1.7105921506881714], 'magnitude': 1.8466485738754272, 'distance': 13.408398628234863, 'cosine_with_motion': -0.338712414616134, 'motion_component': -0.6254827999084984}, {'ion': 1387, 'force': [1.4326162338256836, 0.5672101974487305, -2.7843194007873535], 'magnitude': 3.1822242736816406, 'distance': 10.214183807373047, 'cosine_with_motion': -0.4023037665843089, 'motion_component': -1.2802208037761034}, {'ion': 1460, 'force': [4.253185749053955, 1.8484575748443604, -4.438457012176514], 'magnitude': 6.4192118644714355, 'distance': 7.191643714904785, 'cosine_with_motion': -0.5426708286919631, 'motion_component': -3.483519195765453}, {'ion': 2433, 'force': [1.325726866722107, 2.4138104915618896, -0.2820303738117218], 'magnitude': 2.7683160305023193, 'distance': 10.951187133789062, 'cosine_with_motion': -0.9757626049800445, 'motion_component': -2.701219314438271}]}, 3341: {'frame': 3341, 'ionic_force': [14.888546645641327, 3.9325586408376694, -6.769061803817749], 'ionic_force_magnitude': 16.821237659190512, 'motion_vector': [0.7330703735351562, 1.167449951171875, -0.67529296875], 'cosine_ionic_motion': 0.7775177842387024, 'ionic_motion_component': 13.078811432926425, 'ionic_force_x': 14.888546645641327, 'ionic_force_y': 3.9325586408376694, 'ionic_force_z': -6.769061803817749, 'radial_force': 15.399150583167392, 'axial_force': -6.769061803817749, 'contributions': [{'ion': 1316, 'force': [0.40359848737716675, -0.08952778577804565, -1.4260478019714355], 'magnitude': 1.4847623109817505, 'distance': 14.953420639038086, 'cosine_with_motion': 0.5064765055924272, 'motion_component': 0.751997257062042}, {'ion': 1387, 'force': [0.9169735908508301, -0.240996316075325, -2.4629430770874023], 'magnitude': 2.639130115509033, 'distance': 11.216015815734863, 'cosine_with_motion': 0.507029090482631, 'motion_component': 1.338115802175614}, {'ion': 1460, 'force': [4.683155536651611, -1.4487550258636475, -5.592735767364502], 'magnitude': 7.437037944793701, 'distance': 6.681424140930176, 'cosine_with_motion': 0.4833909417143953, 'motion_component': 3.5949966741954995}, {'ion': 2433, 'force': [8.884819030761719, 5.7118377685546875, 2.712664842605591], 'magnitude': 10.90521240234375, 'distance': 5.517622470855713, 'cosine_with_motion': 0.6779970679963836, 'motion_component': 7.393701814322099}]}, 3342: {'frame': 3342, 'ionic_force': [9.231768727302551, 6.486842645332217, -8.162149548530579], 'ionic_force_magnitude': 13.925708836259645, 'motion_vector': [-1.4764938354492188, 1.4851150512695312, 0.42453765869140625], 'cosine_ionic_motion': -0.2507741042712223, 'ionic_motion_component': -3.4922071597548583, 'ionic_force_x': 9.231768727302551, 'ionic_force_y': 6.486842645332217, 'ionic_force_z': -8.162149548530579, 'radial_force': 11.282937620128104, 'axial_force': -8.162149548530579, 'contributions': [{'ion': 1387, 'force': [0.796237587928772, 0.016238732263445854, -1.9542186260223389], 'magnitude': 2.110267400741577, 'distance': 12.542967796325684, 'cosine_with_motion': -0.4393621985204794, 'motion_component': -0.9271717172143745}, {'ion': 1460, 'force': [3.3354697227478027, 0.10465142130851746, -4.341390609741211], 'magnitude': 5.475763320922852, 'distance': 7.786579132080078, 'cosine_with_motion': -0.5651434645811022, 'motion_component': -3.094591785827248}, {'ion': 2433, 'force': [5.100061416625977, 6.365952491760254, -1.8665403127670288], 'magnitude': 8.367792129516602, 'distance': 6.29888391494751, 'cosine_with_motion': 0.06328509364338056, 'motion_component': 0.5295565281574355}]}, 3343: {'frame': 3343, 'ionic_force': [6.78049048781395, 6.935463041067123, -10.414144240319729], 'ionic_force_magnitude': 14.231307006298756, 'motion_vector': [-1.2784309387207031, -1.8371505737304688, -1.54437255859375], 'cosine_ionic_motion': -0.13764005680158262, 'ionic_motion_component': -1.9587979047077215, 'ionic_force_x': 6.78049048781395, 'ionic_force_y': 6.935463041067123, 'ionic_force_z': -10.414144240319729, 'radial_force': 9.699262799272091, 'axial_force': -10.414144240319729, 'contributions': [{'ion': 1316, 'force': [0.30228039622306824, 0.15748772025108337, -1.4446684122085571], 'magnitude': 1.4843324422836304, 'distance': 14.955586433410645, 'cosine_with_motion': 0.3853319596324988, 'motion_component': 0.5719607082213471}, {'ion': 1387, 'force': [0.6677933931350708, 0.4127635955810547, -2.39450740814209], 'magnitude': 2.519918203353882, 'distance': 11.478253364562988, 'cosine_with_motion': 0.30441458706669083, 'motion_component': 0.7670998458948546}, {'ion': 1460, 'force': [3.6871559619903564, 1.7069761753082275, -6.695205211639404], 'magnitude': 7.831644535064697, 'distance': 6.510922908782959, 'cosine_with_motion': 0.11692689494059591, 'motion_component': 0.91572990354382}, {'ion': 2433, 'force': [2.123260736465454, 4.658235549926758, 0.12023679167032242], 'magnitude': 5.1207275390625, 'distance': 8.051989555358887, 'cosine_with_motion': -0.8228495518087805, 'motion_component': -4.21358843681035}]}, 3344: {'frame': 3344, 'ionic_force': [4.965911656618118, 8.838596478104591, -13.473165035247803], 'ionic_force_magnitude': 16.861412821917458, 'motion_vector': [3.2638702392578125, 0.03415679931640625, 2.7843475341796875], 'cosine_ionic_motion': -0.29034934299537596, 'ionic_motion_component': -4.895700134817542, 'ionic_force_x': 4.965911656618118, 'ionic_force_y': 8.838596478104591, 'ionic_force_z': -13.473165035247803, 'radial_force': 10.138099737332366, 'axial_force': -13.473165035247803, 'contributions': [{'ion': 1387, 'force': [0.446129709482193, -0.06396286189556122, -2.735747814178467], 'magnitude': 2.772623062133789, 'distance': 10.94267749786377, 'cosine_with_motion': -0.5181302545307397, 'motion_component': -1.4365799324708046}, {'ion': 1460, 'force': [1.9232772588729858, -0.41003602743148804, -6.321849346160889], 'magnitude': 6.620642185211182, 'distance': 7.081397533416748, 'cosine_with_motion': -0.3991940414069441, 'motion_component': -2.642920945873833}, {'ion': 2433, 'force': [2.5965046882629395, 9.31259536743164, -4.415567874908447], 'magnitude': 10.628429412841797, 'distance': 5.589004993438721, 'cosine_with_motion': -0.07679394585184894, 'motion_component': -0.8161990217935475}]}, 3345: {'frame': 3345, 'ionic_force': [11.459057569503784, 4.5299258679151535, -9.10696730017662], 'ionic_force_magnitude': 15.</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{4333: {'frame': 4333, 'ionic_force': [5.670064628124237, -0.11623673886060715, -16.053759455680847], 'ionic_force_magnitude': 17.02604876439125, 'motion_vector': [-1.0914764404296875, 2.8184471130371094, 0.5848388671875], 'cosine_ionic_motion': -0.30345207696552395, 'ionic_motion_component': -5.166589860070817, 'ionic_force_x': 5.670064628124237, 'ionic_force_y': -0.11623673886060715, 'ionic_force_z': -16.053759455680847, 'radial_force': 5.671255933791614, 'axial_force': -16.053759455680847, 'contributions': [{'ion': 1308, 'force': [0.17358297109603882, -0.07655664533376694, -1.6345635652542114], 'magnitude': 1.6455363035202026, 'distance': 14.20415210723877, 'directional_contribution': -0.4421635449013346}, {'ion': 1316, 'force': [0.8972761631011963, -0.14553450047969818, -3.8930156230926514], 'magnitude': 3.9977312088012695, 'distance': 9.113018035888672, 'directional_contribution': -1.190955063856654}, {'ion': 1387, 'force': [4.599205493927002, 0.10585440695285797, -10.526180267333984], 'magnitude': 11.487574577331543, 'distance': 5.375945568084717, 'directional_contribution': -3.5334713216154103}]}, 4334: {'frame': 4334, 'ionic_force': [3.895419254899025, 7.656647235155106, -16.01752197742462], 'ionic_force_magnitude': 18.175795673156294, 'motion_vector': [0.5448684692382812, -2.2713394165039062, -1.4224014282226562], 'cosine_ionic_motion': 0.15118571210621812, 'ionic_motion_component': 2.747920611943252, 'ionic_force_x': 3.895419254899025, 'ionic_force_y': 7.656647235155106, 'ionic_force_z': -16.01752197742462, 'radial_force': 8.59060754865722, 'axial_force': -16.01752197742462, 'contributions': [{'ion': 1308, 'force': [0.18028856813907623, 0.2747263014316559, -1.6901415586471558], 'magnitude': 1.721789002418518, 'distance': 13.886061668395996, 'directional_contribution': 0.6868150546000797}, {'ion': 1316, 'force': [0.8013342618942261, 1.1461530923843384, -3.9313461780548096], 'magnitude': 4.172683238983154, 'distance': 8.919927597045898, 'directional_contribution': 1.2524794981272755}, {'ion': 1387, 'force': [2.9137964248657227, 6.235767841339111, -10.396034240722656], 'magnitude': 12.468061447143555, 'distance': 5.160236358642578, 'directional_contribution': 0.8086261068832243}]}, 4335: {'frame': 4335, 'ionic_force': [7.201493963599205, 1.6286407187581062, -22.629054307937622], 'ionic_force_magnitude': 23.803110821280125, 'motion_vector': [-2.4897499084472656, -1.9592094421386719, -2.6416397094726562], 'cosine_ionic_motion': 0.3937050990196898, 'ionic_motion_component': 9.371406102868741, 'ionic_force_x': 7.201493963599205, 'ionic_force_y': 1.6286407187581062, 'ionic_force_z': -22.629054307937622, 'radial_force': 7.383358713929096, 'axial_force': -22.629054307937622, 'contributions': [{'ion': 1308, 'force': [0.17067889869213104, -0.07447502017021179, -1.5542986392974854], 'magnitude': 1.565414309501648, 'distance': 14.563118934631348, 'directional_contribution': 0.9277242097333298}, {'ion': 1316, 'force': [0.7298926711082458, 0.04116610437631607, -3.5585622787475586], 'magnitude': 3.632878065109253, 'distance': 9.559685707092285, 'directional_contribution': 1.81879711751787}, {'ion': 1387, 'force': [6.300922393798828, 1.661949634552002, -17.516193389892578], 'magnitude': 18.68905258178711, 'distance': 4.214784622192383, 'directional_contribution': 6.624885037317597}]}, 4336: {'frame': 4336, 'ionic_force': [-0.5388405174016953, -1.7428620159626007, -9.03514313697815], 'ionic_force_magnitude': 9.217468666372689, 'motion_vector': [0.6896553039550781, 0.1011199951171875, 0.940399169921875], 'cosine_ionic_motion': -0.8382634653281991, 'ionic_motion_component': -7.726667225827664, 'ionic_force_x': -0.5388405174016953, 'ionic_force_y': -1.7428620159626007, 'ionic_force_z': -9.03514313697815, 'radial_force': 1.8242579614404721, 'axial_force': -9.03514313697815, 'contributions': [{'ion': 1316, 'force': [-0.19560758769512177, -0.3452792465686798, -2.427891969680786], 'magnitude': 2.4601097106933594, 'distance': 11.616941452026367, 'directional_contribution': -2.0955894897212177}, {'ion': 1387, 'force': [-0.3432329297065735, -1.397582769393921, -6.607251167297363], 'magnitude': 6.762160301208496, 'distance': 7.006906032562256, 'directional_contribution': -5.631077594624198}]}, 4337: {'frame': 4337, 'ionic_force': [-0.16387367993593216, -1.5002783238887787, -8.31986379623413], 'ionic_force_magnitude': 8.455638545964089, 'motion_vector': [-1.2149238586425781, 0.8994140625, 1.17535400390625], 'cosine_ionic_motion': -0.6750159695501066, 'ionic_motion_component': -5.707691051269203, 'ionic_force_x': -0.16387367993593216, 'ionic_force_y': -1.5002783238887787, 'ionic_force_z': -8.31986379623413, 'radial_force': 1.509201653890648, 'axial_force': -8.31986379623413, 'contributions': [{'ion': 1316, 'force': [-0.0917414203286171, -0.38027724623680115, -2.686659812927246], 'magnitude': 2.714989423751831, 'distance': 11.058213233947754, 'directional_contribution': -1.7695590827597387}, {'ion': 1387, 'force': [-0.07213225960731506, -1.1200010776519775, -5.633203983306885], 'magnitude': 5.743917942047119, 'distance': 7.602648735046387, 'directional_contribution': -3.9381319494534495}]}, 4338: {'frame': 4338, 'ionic_force': [-2.4280003905296326, -1.0742815136909485, -10.110801935195923], 'ionic_force_magnitude': 10.453591843946834, 'motion_vector': [1.5186386108398438, 5.265224456787109, -0.11255645751953125], 'cosine_ionic_motion': -0.1432126280334982, 'ionic_motion_component': -1.4970863603611686, 'ionic_force_x': -2.4280003905296326, 'ionic_force_y': -1.0742815136909485, 'ionic_force_z': -10.110801935195923, 'radial_force': 2.655045511299225, 'axial_force': -10.110801935195923, 'contributions': [{'ion': 1316, 'force': [-0.5445583462715149, -0.3111899495124817, -2.85630202293396], 'magnitude': 2.92435359954834, 'distance': 10.65501594543457, 'directional_contribution': -0.39116425460121373}, {'ion': 1387, 'force': [-1.8834420442581177, -0.7630915641784668, -7.254499912261963], 'magnitude': 7.533752918243408, 'distance': 6.638399124145508, 'directional_contribution': -1.10592210987212}]}, 4339: {'frame': 4339, 'ionic_force': [-0.01052268361672759, 7.317051321268082, -8.848112106323242], 'ionic_force_magnitude': 11.48165661440044, 'motion_vector': [-0.3119239807128906, 0.11574172973632812, 2.2965164184570312], 'cosine_ionic_motion': -0.7307586444093754, 'ionic_motion_component': -8.390319823113206, 'ionic_force_x': -0.01052268361672759, 'ionic_force_y': 7.317051321268082, 'ionic_force_z': -8.848112106323242, 'radial_force': 7.317058887622914, 'axial_force': -8.848112106323242, 'contributions': [{'ion': 1308, 'force': [0.015117759816348553, 0.40834537148475647, -1.4295883178710938], 'magnitude': 1.4868414402008057, 'distance': 14.942962646484375, 'directional_contribution': -1.3964827394725436}, {'ion': 1316, 'force': [-0.007704783696681261, 1.2880055904388428, -2.648350715637207], 'magnitude': 2.944958209991455, 'distance': 10.61767578125, 'directional_contribution': -2.5557094833582963}, {'ion': 1387, 'force': [-0.017935659736394882, 5.620700359344482, -4.770173072814941], 'magnitude': 7.37205171585083, 'distance': 6.710808753967285, 'directional_contribution': -4.438127686965383}]}, 4340: {'frame': 4340, 'ionic_force': [-0.6614977717399597, 11.020213901996613, -11.043931484222412], 'ionic_force_magnitude': 15.615732975943697, 'motion_vector': [0.09852218627929688, -2.540813446044922, -1.569000244140625], 'cosine_ionic_motion': -0.23013628428245336, 'ionic_motion_component': -3.59374676343066, 'ionic_force_x': -0.6614977717399597, 'ionic_force_y': 11.020213901996613, 'ionic_force_z': -11.043931484222412, 'radial_force': 11.040049535567144, 'axial_force': -11.043931484222412, 'contributions': [{'ion': 1308, 'force': [-0.11230937391519547, 0.5389495491981506, -1.9288716316223145], 'magnitude': 2.0058977603912354, 'distance': 12.865143775939941, 'directional_contribution': 0.5508874269489278}, {'ion': 1316, 'force': [-0.09320607036352158, 2.1498072147369385, -3.7819480895996094], 'magnitude': 4.351263046264648, 'distance': 8.734969139099121, 'directional_contribution': 0.15477234838873555}, {'ion': 1387, 'force': [-0.4559823274612427, 8.331457138061523, -5.333111763000488], 'magnitude': 9.902685165405273, 'distance': 5.790186405181885, 'directional_contribution': -4.299406738489893}]}, 4341: {'frame': 4341, 'ionic_force': [-1.1659248024225235, 9.977354973554611, -17.802505493164062], 'ionic_force_magnitude': 20.441041919318973, 'motion_vector': [-0.7720985412597656, -0.6841316223144531, -3.7374649047851562], 'cosine_ionic_motion': 0.7647606975638053, 'ionic_motion_component': 15.632505477149364, 'ionic_force_x': -1.1659248024225235, 'ionic_force_y': 9.977354973554611, 'ionic_force_z': -17.802505493164062, 'radial_force': 10.045247279844283, 'axial_force': -17.802505493164062, 'contributions': [{'ion': 1308, 'force': [-0.09177793562412262, 0.24030449986457825, -1.6979613304138184], 'magnitude': 1.717335820198059, 'distance': 13.904053688049316, 'directional_contribution': 1.6126339887252703}, {'ion': 1316, 'force': [-0.13407957553863525, 0.977773129940033, -3.8091092109680176], 'magnitude': 3.9348864555358887, 'distance': 9.185503005981445, 'directional_contribution': 3.5259846615014645}, {'ion': 1387, 'force': [-0.9400672912597656, 8.75927734375, -12.295434951782227], 'magnitude': 15.125685691833496, 'distance': 4.685020446777344, 'directional_contribution': 10.493887334066017}]}, 4342: {'frame': 4342, 'ionic_force': [-1.3840811252593994, 1.351293995976448, -7.411204814910889], 'ionic_force_magnitude': 7.659479932307392, 'motion_vector': [-2.657154083251953, -1.6822662353515625, 5.648590087890625], 'cosine_ionic_motion': -0.8170268253809583, 'ionic_motion_component': -6.258000573162266, 'ionic_force_x': -1.3840811252593994, 'ionic_force_y': 1.351293995976448, 'ionic_force_z': -7.411204814910889, 'radial_force': 1.9343412379570781, 'axial_force': -7.411204814910889, 'contributions': [{'ion': 1316, 'force': [-0.2974294424057007, 0.23622436821460724, -2.1497864723205566], 'magnitude': 2.183082342147827, 'distance': 12.332013130187988, 'directional_contribution': -1.8175130650926032}, {'ion': 1387, 'force': [-1.0866516828536987, 1.1150696277618408, -5.261418342590332], 'magnitude': 5.4869585037231445, 'distance': 7.778631687164307, 'directional_contribution': -4.440487642549986}]}, 4343: {'frame': 4343, 'ionic_force': [-16.709574282169342, -0.8938723057508469, -13.62956953048706], 'ionic_force_magnitude': 21.58179895135493, 'motion_vector': [2.1892776489257812, 5.375339508056641, -3.4262237548828125], 'cosine_ionic_motion': 0.036513285370066664, 'ionic_motion_component': 0.788022383910228, 'ionic_force_x': -16.709574282169342, 'ionic_force_y': -0.8938723057508469, 'ionic_force_z': -13.62956953048706, 'radial_force': 16.733465880992004, 'axial_force': -13.62956953048706, 'contributions': [{'ion': 1308, 'force': [-0.6828966736793518, -0.1254197210073471, -2.168544292449951], 'magnitude': 2.2769854068756104, 'distance': 12.07504940032959, 'directional_contribution': 0.7805302860302321}, {'ion': 1316, 'force': [-2.210134983062744, -0.2589053511619568, -4.237045764923096], 'magnitude': 4.785842418670654, 'distance': 8.32894229888916, 'directional_contribution': 1.2295089090269506}, {'ion': 1387, 'force': [-13.816542625427246, -0.509547233581543, -7.223979473114014], 'magnitude': 15.599434852600098, 'distance': 4.613330841064453, 'directional_contribution': -1.2220163395787154}]}, 4344: {'frame': 4344, 'ionic_force': [-1.153914988040924, 3.170382857322693, -5.203489422798157], 'ionic_force_magnitude': 6.201544116976302, 'motion_vector': [1.4634857177734375, -1.2306327819824219, 0.8022537231445312], 'cosine_ionic_motion': -0.7593428919930103, 'ionic_motion_component': -4.709098444607024, 'ionic_force_x': -1.153914988040924, 'ionic_force_y': 3.170382857322693, 'ionic_force_z': -5.203489422798157, 'radial_force': 3.373847545700767, 'axial_force': -5.203489422798157, 'contributions': [{'ion': 1316, 'force': [-0.2957773804664612, 0.846617579460144, -1.985202670097351], 'magnitude': 2.1783652305603027, 'distance': 12.345357894897461, 'directional_contribution': -1.4792451065752275}, {'ion': 1387, 'force': [-0.8581376075744629, 2.323765277862549, -3.2182867527008057], 'magnitude': 4.061237812042236, 'distance': 9.041485786437988, 'directional_contribution': -3.2298533141553847}]}, 4345: {'frame': 4345, 'ionic_force': [0.08994757011532784, 5.610477715730667, -9.722934126853943], 'ionic_force_magnitude': 11.225907482213682, 'motion_vector': [-1.1395187377929688, 0.0416717529296875, -1.0085220336914062], 'cosine_ionic_motion': 0.5814891324386149, 'ionic_motion_component': 6.5277432026685895, 'ionic_force_x': 0.08994757011532784, 'ionic_force_y': 5.610477715730667, 'ionic_force_z': -9.722934126853943, 'radial_force': 5.611198692265321, 'axial_force': -9.722934126853943, 'contributions': [{'ion': 1308, 'force': [-0.04955724999308586, 0.3378300964832306, -1.4625250101089478], 'magnitude': 1.5018537044525146, 'distance': 14.868091583251953, 'directional_contribution': 1.0152741867035733}, {'ion': 1316, 'force': [-0.044318169355392456, 1.0932285785675049, -2.809373140335083], 'magnitude': 3.014911413192749, 'distance': 10.493775367736816, 'directional_contribution': 1.9243243929068639}, {'ion': 1387, 'force': [0.18382298946380615, 4.179419040679932, -5.451035976409912], 'magnitude': 6.871326446533203, 'distance': 6.951023101806641, 'directional_contribution': 3.5881446979568086}]}, 4346: {'frame': 4346, 'ionic_force': [-0.9703720510005951, 4.194342374801636, -6.858072519302368], 'ionic_force_magnitude': 8.097363061789316, 'motion_vector': [-4.582515716552734, 0.4224891662597656, 2.309173583984375], 'cosine_ionic_motion': -0.23068510028921504, 'ionic_motion_component': -1.867941009987054, 'ionic_force_x': -0.9703720510005951, 'ionic_force_y': 4.194342374801636, 'ionic_force_z': -6.858072519302368, 'radial_force': 4.305128322642628, 'axial_force': -6.858072519302368, 'contributions': [{'ion': 1316, 'force': [-0.26130351424217224, 0.9197101593017578, -2.4406163692474365], 'magnitude': 2.6212124824523926, 'distance': 11.25428581237793, 'directional_contribution': -0.7865532102811734}, {'ion': 1387, 'force': [-0.7090685367584229, 3.274632215499878, -4.417456150054932], 'magnitude': 5.544358730316162, 'distance': 7.7382612228393555, 'directional_contribution': -1.0813878190443305}]}, 4347: {'frame': 4347, 'ionic_force': [-5.324795186519623, 4.4520832896232605, -5.531670093536377], 'ionic_force_magnitude': 8.87546412419373, 'motion_vector': [-0.36487579345703125, -0.39484405517578125, 1.3642425537109375], 'cosine_ionic_motion': -0.5656374441017312, 'ionic_motion_component': -5.020294842425552, 'ionic_force_x': -5.324795186519623, 'ionic_force_y': 4.4520832896232605, 'ionic_force_z': -5.531670093536377, 'radial_force': 6.940784494286306, 'axial_force': -5.531670093536377, 'contributions': [{'ion': 1308, 'force': [-0.5734414458274841, 0.4193485379219055, -1.335965633392334], 'magnitude': 1.5131069421768188, 'distance': 14.812700271606445, 'directional_contribution': -1.213161044334834}, {'ion': 1316, 'force': [-1.3264715671539307, 1.0629514455795288, -2.074846029281616], 'magnitude': 2.6822338104248047, 'distance': 11.125530242919922, 'directional_contribution': -1.886513049774802}, {'ion': 1387, 'force': [-3.424882173538208, 2.969783306121826, -2.1208584308624268], 'magnitude': 5.004745006561279, 'distance': 8.144756317138672, 'directional_contribution': -1.9206208369105298}]}, 4348: {'frame': 4348, 'ionic_force': [-4.811583518981934, 3.2644795179367065, -4.231451034545898], 'ionic_force_magnitude': 7.191198811111148, 'motion_vector': [1.2287940979003906, -3.6073760986328125, -4.4157257080078125], 'cosine_ionic_motion': 0.023752005658367503, 'ionic_motion_component': 0.17080539485195764, 'ionic_force_x': -4.811583518981934, 'ionic_force_y': 3.2644795179367065, 'ionic_force_z': -4.231451034545898, 'radial_force': 5.8144786940160715, 'axial_force': -4.231451034545898, 'contributions': [{'ion': 1316, 'force': [-1.6572506427764893, 1.0221670866012573, -2.0923280715942383], 'magnitude': 2.858170986175537, 'distance': 10.777670860290527, 'directional_contribution': 0.602691103493072}, {'ion': 1387, 'force': [-3.1543328762054443, 2.242312431335449, -2.13912296295166], 'magnitude': 4.421948432922363, 'distance': 8.664873123168945, 'directional_contribution': -0.4318857455830667}]}, 4349: {'frame': 4349, 'ionic_force': [-2.8148942589759827, 0.3423163443803787, -5.1887286901474], 'ionic_force_magnitude': 5.913012395455015, 'motion_vector': [3.6558074951171875, 0.5428085327148438, 1.3375320434570312], 'cosine_ionic_motion': -0.7334051060764676, 'ionic_motion_component': -4.336633483120153, 'ionic_force_x': -2.8148942589759827, 'ionic_force_y': 0.3423163443803787, 'ionic_force_z': -5.1887286901474, 'radial_force': 2.835632234413675, 'axial_force': -5.1887286901474, 'contributions': [{'ion': 1316, 'force': [-0.7681282162666321, 0.059397414326667786, -1.9104300737380981], 'magnitude': 2.0599253177642822, 'distance': 12.69530963897705, 'directional_contribution': -1.356365627793785}, {'ion': 1387, 'force': [-2.0467660427093506, 0.28291893005371094, -3.2782986164093018], 'magnitude': 3.875117540359497, 'distance': 9.25606918334961, 'directional_contribution': -2.9802678535875486}]}, 4350: {'frame': 4350, 'ionic_force': [-1.14635768532753, 1.0225782543420792, -9.443222522735596], 'ionic_force_magnitude': 9.567353544364483, 'motion_vector': [-3.0155258178710938, -3.347362518310547, 1.5890350341796875], 'cosine_ionic_motion': -0.3275592344848105, 'ionic_motion_component': -3.1338750030375686, 'ionic_force_x': -1.14635768532753, 'ionic_force_y': 1.0225782543420792, 'ionic_force_z': -9.443222522735596, 'radial_force': 1.536164779235218, 'axial_force': -9.443222522735596, 'contributions': [{'ion': 1316, 'force': [-0.2180737555027008, 0.12293900549411774, -2.9367432594299316], 'magnitude': 2.9473938941955566, 'distance': 10.613287925720215, 'directional_contribution': -0.9253003451579866}, {'ion': 1387, 'force': [-0.9282839298248291, 0.8996392488479614, -6.506479263305664], 'magnitude': 6.6336517333984375, 'distance': 7.074450492858887, 'directional_contribution': -2.2085744950483175}]}, 4351: {'frame': 4351, 'ionic_force': [-5.821552753448486, -2.9807128310203552, -7.226513624191284], 'ionic_force_magnitude': 9.746672488742774, 'motion_vector': [0.9067535400390625, 2.27435302734375, -1.0322418212890625], 'cosine_ionic_motion': -0.17755595543049107, 'ionic_motion_component': -1.7305797460068055, 'ionic_force_x': -5.821552753448486, 'ionic_force_y': -2.9807128310203552, 'ionic_force_z': -7.226513624191284, 'radial_force': 6.540269523665904, 'axial_force': -7.226513624191284, 'contributions': [{'ion': 1316, 'force': [-1.437971591949463, -0.7615723013877869, -2.7652251720428467], 'magnitude': 3.2084615230560303, 'distance': 10.172334671020508, 'directional_contribution': -0.06834000613675784}, {'ion': 1387, 'force': [-4.383581161499023, -2.2191405296325684, -4.4612884521484375], 'magnitude': 6.6365251541137695, 'distance': 7.07291841506958, 'directional_contribution': -1.6622398829874783}]}, 4352: {'frame': 4352, 'ionic_force': [-3.8882360458374023, 0.07716289162635803, -8.414870738983154], 'ionic_force_magnitude': 9.270080000398504, 'motion_vector': [-1.1390266418457031, -0.5661506652832031, -1.0862197875976562], 'cosine_ionic_motion': 0.8722952131855376, 'ionic_motion_component': 8.086246410194603, 'ionic_force_x': -3.8882360458374023, 'ionic_force_y': 0.07716289162635803, 'ionic_force_z': -8.414870738983154, 'radial_force': 3.889001627666594, 'axial_force': -8.414870738983154, 'contributions': [{'ion': 1316, 'force': [-0.9431006908416748, -0.052728161215782166, -2.691154956817627], 'magnitude': 2.8521103858947754, 'distance': 10.789115905761719, 'directional_contribution': 2.4076987968412804}, {'ion': 1387, 'force': [-2.9451353549957275, 0.1298910528421402, -5.723715782165527], 'magnitude': 6.438292980194092, 'distance': 7.180979251861572, 'directional_contribution': 5.678547440850384}]}, 4353: {'frame': 4353, 'ionic_force': [-6.081224143505096, -0.8584663271903992, -9.448819756507874], 'ionic_force_magnitude': 11.269358735502326, 'motion_vector': [1.2044410705566406, -1.20880126953125, 0.8453292846679688], 'cosine_ionic_motion': -0.6651334853126875, 'ionic_motion_component': -7.495627852983643, 'ionic_force_x': -6.081224143505096, 'ionic_force_y': -0.8584663271903992, 'ionic_force_z': -9.448819756507874, 'radial_force': 6.141518665482428, 'axial_force': -9.448819756507874, 'contributions': [{'ion': 1308, 'force': [-0.4175664782524109, -0.13317164778709412, -1.4587963819503784], 'magnitude': 1.5232148170471191, 'distance': 14.763470649719238, 'directional_contribution': -0.827126651667454}, {'ion': 1316, 'force': [-1.1213693618774414, -0.22113272547721863, -2.5067636966705322], 'magnitude': 2.755037784576416, 'distance': 10.977545738220215, 'directional_contribution': -1.6816223630058307}, {'ion': 1387, 'force': [-4.542288303375244, -0.5041619539260864, -5.483259677886963], 'magnitude': 7.138115882873535, 'distance': 6.819888114929199, 'directional_contribution': -4.986878762952777}]}, 4354: {'frame': 4354, 'ionic_force': [-3.467491030693054, -1.7887528538703918, -8.15508508682251], 'ionic_force_magnitude': 9.040384040154553, 'motion_vector': [-1.2567825317382812, 0.8124618530273438, 0.4911346435546875], 'cosine_ionic_motion': -0.077297958681048, 'ionic_motion_component': -0.6988032319966724, 'ionic_force_x': -3.467491030693054, 'ionic_force_y': -1.7887528538703918, 'ionic_force_z': -8.15508508682251, 'radial_force': 3.901683075310737, 'axial_force': -8.15508508682251, 'contributions': [{'ion': 1316, 'force': [-0.8548189401626587, -0.5112813115119934, -2.679126739501953], 'magnitude': 2.8582937717437744, 'distance': 10.777440071105957, 'directional_contribution': -0.4170555891222918}, {'ion': 1387, 'force': [-2.6126720905303955, -1.2774715423583984, -5.475958347320557], 'magnitude': 6.200331687927246, 'distance': 7.317480564117432, 'directional_contribution': -0.2817476814382047}]}, 4355: {'frame': 4355, 'ionic_force': [-4.742857813835144, -1.030191957950592, -6.752213716506958], 'ionic_force_magnitude': 8.315550840796288, 'motion_vector': [-0.8599281311035156, 1.072509765625, 0.5235366821289062], 'cosine_ionic_motion': -0.04589578220628883, 'ionic_motion_component': -0.38164871031450837, 'ionic_force_x': -4.742857813835144, 'ionic_force_y': -1.030191957950592, 'ionic_force_z': -6.752213716506958, 'radial_force': 4.853451937794703, 'axial_force': -6.752213716506958, 'contributions': [{'ion': 1316, 'force': [-1.2849539518356323, -0.36015647649765015, -2.5392329692840576], 'magnitude': 2.8685402870178223, 'distance': 10.758173942565918, 'directional_contribution': -0.4151492194617141}, {'ion': 1387, 'force': [-3.4579038619995117, -0.6700354814529419, -4.2129807472229], 'magnitude': 5.491379737854004, 'distance': 7.77549934387207, 'directional_contribution': 0.033500446055334976}]}, 4356: {'frame': 4356, 'ionic_force': [-8.145591795444489, 0.5536623261868954, -8.388230919837952], 'ionic_force_magnitude': 11.705538246231, 'motion_vector': [-0.17728042602539062, -5.445198059082031, 0.5759963989257812], 'cosine_ionic_motion': -0.09983658107924243, 'ionic_motion_component': -1.1686409181960145, 'ionic_force_x': -8.145591795444489, 'ionic_force_y': 0.5536623261868954, 'ionic_force_z': -8.388230919837952, 'radial_force': 8.164386545812935, 'axial_force': -8.388230919837952, 'contributions': [{'ion': 1308, 'force': [-0.6154080033302307, -0.04097851738333702, -1.5266047716140747], 'magnitude': 1.6464896202087402, 'distance': 14.20003890991211, 'directional_contribution': -0.09986094493453779}, {'ion': 1316, 'force': [-1.5749125480651855, -0.061273880302906036, -2.6270933151245117], 'magnitude': 3.063612699508667, 'distance': 10.410033226013184, 'directional_contribution': -0.16434341226880056}, {'ion': 1387, 'force': [-5.955271244049072, 0.6559147238731384, -4.234532833099365], 'magnitude': 7.336671352386475, 'distance': 6.726970195770264, 'directional_contribution': -0.904436581779466}]}, 4357: {'frame': 4357, 'ionic_force': [-5.270969092845917, -5.013264775276184, -4.879510402679443], 'ionic_force_magnitude': 8.759312795797326, 'motion_vector': [0.0101470947265625, 0.001705169677734375, 0.09522247314453125], 'cosine_ionic_motion': -0.6277842758580351, 'ionic_motion_component': -5.498958840523645, 'ionic_force_x': -5.270969092845917, 'ionic_force_y': -5.013264775276184, 'ionic_force_z': -4.879510402679443, 'radial_force': 7.274334257151088, 'axial_force': -4.879510402679443, 'contributions': [{'ion': 1308, 'force': [-0.6041297316551208, -0.6097363233566284, -1.3066514730453491], 'magnitude': 1.5633583068847656, 'distance': 14.572691917419434, 'directional_contribution': -1.3739494831185086}, {'ion': 1316, 'force': [-1.375537633895874, -1.3294124603271484, -1.9107221364974976], 'magnitude': 2.703756809234619, 'distance': 11.081160545349121, 'directional_contribution': -2.069063945781279}, {'ion': 1387, 'force': [-3.291301727294922, -3.0741159915924072, -1.6621367931365967], 'magnitude': 4.800578594207764, 'distance': 8.31614875793457, 'directional_contribution': -2.055945354053961}]}, 4358: {'frame': 4358, 'ionic_force': [-4.603870153427124, -3.909831404685974, -3.866476058959961], 'ionic_force_magnitude': 7.171613424969053, 'motion_vector': [1.1465644836425781, -0.06743621826171875, 0.3713531494140625], 'cosine_ionic_motion': -0.7451740365570843, 'ionic_motion_component': -5.344100124511165, 'ionic_force_x': -4.603870153427124, 'ionic_force_y': -3.909831404685974, 'ionic_force_z': -3.866476058959961, 'radial_force': 6.040066390585934, 'axial_force': -3.866476058959961, 'contributions': [{'ion': 1316, 'force': [-1.2709743976593018, -1.2347279787063599, -1.9208208322525024], 'magnitude': 2.613327741622925, 'distance': 11.27125072479248, 'directional_contribution': -1.7291962063176305}, {'ion': 1387, 'force': [-3.3328957557678223, -2.6751034259796143, -1.9456552267074585], 'magnitude': 4.695737361907959, 'distance': 8.408473014831543, 'directional_contribution': -3.6149038997023144}]}, 4359: {'frame': 4359, 'ionic_force': [-6.097867250442505, -7.210108399391174, -5.836791396141052], 'ionic_force_magnitude': 11.101251368069125, 'motion_vector': [-1.8090705871582031, 0.6514205932617188, -0.31896209716796875], 'cosine_ionic_motion': 0.3788134547827392, 'ionic_motion_component': 4.205303383149875, 'ionic_force_x': -6.097867250442505, 'ionic_force_y': -7.210108399391174, 'ionic_force_z': -5.836791396141052, 'radial_force': 9.442968184580016, 'axial_force': -5.836791396141052, 'contributions': [{'ion': 1308, 'force': [-0.5732018947601318, -0.8108179569244385, -1.6454930305480957], 'magnitude': 1.9218828678131104, 'distance': 13.143335342407227, 'directional_contribution': 0.5303227369907617}, {'ion': 1316, 'force': [-1.4675121307373047, -1.8761595487594604, -2.2478926181793213], 'magnitude': 3.275146961212158, 'distance': 10.068242073059082, 'directional_contribution': 1.1029215441539115}, {'ion': 1387, 'force': [-4.057153224945068, -4.523130893707275, -1.9434057474136353], 'magnitude': 6.379344463348389, 'distance': 7.214081287384033, 'directional_contribution': 2.572058988408134}]}, 4360: {'frame': 4360, 'ionic_force': [-5.140026926994324, -3.9340438842773438, -3.686625123023987], 'ionic_force_magnitude': 7.449012209102514, 'motion_vector': [-0.8460655212402344, 0.20500564575195312, 0.1761016845703125], 'cosine_ionic_motion': 0.4372801521611261, 'ionic_motion_component': 3.257305192246433, 'ionic_force_x': -5.140026926994324, 'ionic_force_y': -3.9340438842773438, 'ionic_force_z': -3.686625123023987, 'radial_force': 6.472756607014254, 'axial_force': -3.686625123023987, 'contributions': [{'ion': 1316, 'force': [-1.4018090963363647, -1.172297477722168, -1.9389605522155762], 'magnitude': 2.664379358291626, 'distance': 11.162744522094727, 'directional_contribution': 0.6803122125233401}, {'ion': 1387, 'force': [-3.738217830657959, -2.761746406555176, -1.7476645708084106], 'magnitude': 4.965465545654297, 'distance': 8.17690658569336, 'directional_contribution': 2.5769931313869705}]}, 4361: {'frame': 4361, 'ionic_force': [-5.4141963720321655, -3.7038130164146423, -4.313818573951721], 'ionic_force_magnitude': 7.851164493529584, 'motion_vector': [1.1817245483398438, -0.8403396606445312, -0.4484710693359375], 'cosine_ionic_motion': -0.11337134838642916, 'ionic_motion_component': -0.8900971050351052, 'ionic_force_x': -5.4141963720321655, 'ionic_force_y': -3.7038130164146423, 'ionic_force_z': -4.313818573951721, 'radial_force': 6.559859237475206, 'axial_force': -4.313818573951721, 'contributions': [{'ion': 1308, 'force': [-0.7086317539215088, -0.5181094408035278, -1.3205690383911133], 'magnitude': 1.5857172012329102, 'distance': 14.469588279724121, 'directional_contribution': 0.1253229768646662}, {'ion': 1316, 'force': [-1.3960002660751343, -0.9637919068336487, -1.544816255569458], 'magnitude': 2.294377565383911, 'distance': 12.029195785522461, 'directional_contribution': -0.09682967574426726}, {'ion': 1387, 'force': [-3.3095643520355225, -2.221911668777466, -1.44843327999115], 'magnitude': 4.241234302520752, 'distance': 8.84754753112793, 'directional_contribution': -0.9185902935916275}]}, 4362: {'frame': 4362, 'ionic_force': [-4.9034892320632935, -4.803059756755829, -4.693336129188538], 'ionic_force_magnitude': 8.315106355151116, 'motion_vector': [0.7227058410644531, -0.5454826354980469, 0.70068359375], 'cosine_ionic_motion': -0.4424713221093263, 'ionic_motion_component': -3.6791961024433757, 'ionic_force_x': -4.9034892320632935, 'ionic_force_y': -4.803059756755829, 'ionic_force_z': -4.693336129188538, 'radial_force': 6.863933979572358, 'axial_force': -4.693336129188538, 'contributions': [{'ion': 1308, 'force': [-0.5720486640930176, -0.5742262005805969, -1.2654268741607666], 'magnitude': 1.5027576684951782, 'distance': 14.863618850708008, 'directional_contribution': -0.8619531518802397}, {'ion': 1316, 'force': [-1.2409831285476685, -1.17379891872406, -1.7205088138580322], 'magnitude': 2.424457311630249, 'distance': 11.702045440673828, 'directional_contribution': -1.2770564991251376}, {'ion': 1387, 'force': [-3.0904574394226074, -3.055034637451172, -1.7074004411697388], 'magnitude': 4.668980598449707, 'distance': 8.43253231048584, 'directional_contribution': -1.5401867417355248}]}, 4363: {'frame': 4363, 'ionic_force': [-5.15885055065155, -6.060519695281982, -4.759960770606995], 'ionic_force_magnitude': 9.273665107096338, 'motion_vector': [0.15148544311523438, 0.16559600830078125, -0.0403900146484375], 'cosine_ionic_motion': -0.7532033054635574, 'ionic_motion_component': -6.984955212427017, 'ionic_force_x': -5.15885055065155, 'ionic_force_y': -6.060519695281982, 'ionic_force_z': -4.759960770606995, 'radial_force': 7.958871652493123, 'axial_force': -4.759960770606995, 'contributions': [{'ion': 1308, 'force': [-0.6784613132476807, -0.7572453022003174, -1.4538769721984863], 'magnitude': 1.7741162776947021, 'distance': 13.6797456741333, 'directional_contribution': -0.7430860403188788}, {'ion': 1316, 'force': [-1.3555282354354858, -1.692523717880249, -1.860271692276001], 'magnitude': 2.8570446968078613, 'distance': 10.77979564666748, 'directional_contribution': -1.8000593899340664}, {'ion': 1387, 'force': [-3.124861001968384, -3.610750675201416, -1.4458121061325073], 'magnitude': 4.989253520965576, 'distance': 8.157390594482422, 'directional_contribution': -4.441809759552326}]}, 4364: {'frame': 4364, 'ionic_force': [-5.2863510847091675, -6.0709163546562195, -5.215934872627258], 'ionic_force_magnitude': 9.59205451253939, 'motion_vector': [-0.5905914306640625, 0.47576904296875, -0.7368392944335938], 'cosine_ionic_motion': 0.4019703684568437, 'ionic_motion_component': 3.8557216866635886, 'ionic_force_x': -5.2863510847091675, 'ionic_force_y': -6.0709163546562195, 'ionic_force_z': -5.215934872627258, 'radial_force': 8.04993994859826, 'axial_force': -5.215934872627258, 'contributions': [{'ion': 1308, 'force': [-0.5430638790130615, -0.7677804827690125, -1.5132291316986084], 'magnitude': 1.7816474437713623, 'distance': 13.650801658630371, 'directional_contribution': 1.0123446301502295}, {'ion': 1316, 'force': [-1.3232744932174683, -1.5703063011169434, -1.9702478647232056], 'magnitude': 2.8458380699157715, 'distance': 10.800999641418457, 'directional_contribution': 1.405497277112012}, {'ion': 1387, 'force': [-3.4200127124786377, -3.7328295707702637, -1.7324578762054443], 'magnitude': 5.350879669189453, 'distance': 7.876920223236084, 'directional_contribution': 1.4378796202559556}]}, 4365: {'frame': 4365, 'ionic_force': [-5.281224012374878, -4.7340929</t>
+          <t>{4333: {'frame': 4333, 'ionic_force': [5.670064628124237, -0.11623673886060715, -16.053759455680847], 'ionic_force_magnitude': 17.02604876439125, 'motion_vector': [-1.0914764404296875, 2.8184471130371094, 0.5848388671875], 'cosine_ionic_motion': -0.30345207696552395, 'ionic_motion_component': -5.166589860070817, 'ionic_force_x': 5.670064628124237, 'ionic_force_y': -0.11623673886060715, 'ionic_force_z': -16.053759455680847, 'radial_force': 5.671255933791614, 'axial_force': -16.053759455680847, 'contributions': [{'ion': 1308, 'force': [0.17358297109603882, -0.07655664533376694, -1.6345635652542114], 'magnitude': 1.6455363035202026, 'distance': 14.20415210723877, 'cosine_with_motion': -0.2687048108516073, 'motion_component': -0.4421635449013345}, {'ion': 1316, 'force': [0.8972761631011963, -0.14553450047969818, -3.8930156230926514], 'magnitude': 3.9977312088012695, 'distance': 9.113018035888672, 'cosine_with_motion': -0.2979077327293967, 'motion_component': -1.190955063856654}, {'ion': 1387, 'force': [4.599205493927002, 0.10585440695285797, -10.526180267333984], 'magnitude': 11.487574577331543, 'distance': 5.375945568084717, 'cosine_with_motion': -0.30759072151122985, 'motion_component': -3.5334713216154103}]}, 4334: {'frame': 4334, 'ionic_force': [3.895419254899025, 7.656647235155106, -16.01752197742462], 'ionic_force_magnitude': 18.175795673156294, 'motion_vector': [0.5448684692382812, -2.2713394165039062, -1.4224014282226562], 'cosine_ionic_motion': 0.15118571210621812, 'ionic_motion_component': 2.747920611943252, 'ionic_force_x': 3.895419254899025, 'ionic_force_y': 7.656647235155106, 'ionic_force_z': -16.01752197742462, 'radial_force': 8.59060754865722, 'axial_force': -16.01752197742462, 'contributions': [{'ion': 1308, 'force': [0.18028856813907623, 0.2747263014316559, -1.6901415586471558], 'magnitude': 1.721789002418518, 'distance': 13.886061668395996, 'cosine_with_motion': 0.39889620431807066, 'motion_component': 0.6868150546000797}, {'ion': 1316, 'force': [0.8013342618942261, 1.1461530923843384, -3.9313461780548096], 'magnitude': 4.172683238983154, 'distance': 8.919927597045898, 'cosine_with_motion': 0.3001616454276057, 'motion_component': 1.2524794981272755}, {'ion': 1387, 'force': [2.9137964248657227, 6.235767841339111, -10.396034240722656], 'magnitude': 12.468061447143555, 'distance': 5.160236358642578, 'cosine_with_motion': 0.06485580436767582, 'motion_component': 0.8086261068832242}]}, 4335: {'frame': 4335, 'ionic_force': [7.201493963599205, 1.6286407187581062, -22.629054307937622], 'ionic_force_magnitude': 23.803110821280125, 'motion_vector': [-2.4897499084472656, -1.9592094421386719, -2.6416397094726562], 'cosine_ionic_motion': 0.3937050990196898, 'ionic_motion_component': 9.371406102868741, 'ionic_force_x': 7.201493963599205, 'ionic_force_y': 1.6286407187581062, 'ionic_force_z': -22.629054307937622, 'radial_force': 7.383358713929096, 'axial_force': -22.629054307937622, 'contributions': [{'ion': 1308, 'force': [0.17067889869213104, -0.07447502017021179, -1.5542986392974854], 'magnitude': 1.565414309501648, 'distance': 14.563118934631348, 'cosine_with_motion': 0.5926381165473805, 'motion_component': 0.9277242097333298}, {'ion': 1316, 'force': [0.7298926711082458, 0.04116610437631607, -3.5585622787475586], 'magnitude': 3.632878065109253, 'distance': 9.559685707092285, 'cosine_with_motion': 0.5006490876675077, 'motion_component': 1.8187971175178699}, {'ion': 1387, 'force': [6.300922393798828, 1.661949634552002, -17.516193389892578], 'magnitude': 18.68905258178711, 'distance': 4.214784622192383, 'cosine_with_motion': 0.3544794253429433, 'motion_component': 6.624885037317597}]}, 4336: {'frame': 4336, 'ionic_force': [-0.5388405174016953, -1.7428620159626007, -9.03514313697815], 'ionic_force_magnitude': 9.217468666372689, 'motion_vector': [0.6896553039550781, 0.1011199951171875, 0.940399169921875], 'cosine_ionic_motion': -0.8382634653281991, 'ionic_motion_component': -7.726667225827664, 'ionic_force_x': -0.5388405174016953, 'ionic_force_y': -1.7428620159626007, 'ionic_force_z': -9.03514313697815, 'radial_force': 1.8242579614404721, 'axial_force': -9.03514313697815, 'contributions': [{'ion': 1316, 'force': [-0.19560758769512177, -0.3452792465686798, -2.427891969680786], 'magnitude': 2.4601097106933594, 'distance': 11.616941452026367, 'cosine_with_motion': -0.8518276766603495, 'motion_component': -2.0955894897212177}, {'ion': 1387, 'force': [-0.3432329297065735, -1.397582769393921, -6.607251167297363], 'magnitude': 6.762160301208496, 'distance': 7.006906032562256, 'cosine_with_motion': -0.8327335038641387, 'motion_component': -5.631077594624198}]}, 4337: {'frame': 4337, 'ionic_force': [-0.16387367993593216, -1.5002783238887787, -8.31986379623413], 'ionic_force_magnitude': 8.455638545964089, 'motion_vector': [-1.2149238586425781, 0.8994140625, 1.17535400390625], 'cosine_ionic_motion': -0.6750159695501066, 'ionic_motion_component': -5.707691051269203, 'ionic_force_x': -0.16387367993593216, 'ionic_force_y': -1.5002783238887787, 'ionic_force_z': -8.31986379623413, 'radial_force': 1.509201653890648, 'axial_force': -8.31986379623413, 'contributions': [{'ion': 1316, 'force': [-0.0917414203286171, -0.38027724623680115, -2.686659812927246], 'magnitude': 2.714989423751831, 'distance': 11.058213233947754, 'cosine_with_motion': -0.6517738113728772, 'motion_component': -1.7695590827597387}, {'ion': 1387, 'force': [-0.07213225960731506, -1.1200010776519775, -5.633203983306885], 'magnitude': 5.743917942047119, 'distance': 7.602648735046387, 'cosine_with_motion': -0.6856177321457585, 'motion_component': -3.9381319494534495}]}, 4338: {'frame': 4338, 'ionic_force': [-2.4280003905296326, -1.0742815136909485, -10.110801935195923], 'ionic_force_magnitude': 10.453591843946834, 'motion_vector': [1.5186386108398438, 5.265224456787109, -0.11255645751953125], 'cosine_ionic_motion': -0.1432126280334982, 'ionic_motion_component': -1.4970863603611686, 'ionic_force_x': -2.4280003905296326, 'ionic_force_y': -1.0742815136909485, 'ionic_force_z': -10.110801935195923, 'radial_force': 2.655045511299225, 'axial_force': -10.110801935195923, 'contributions': [{'ion': 1316, 'force': [-0.5445583462715149, -0.3111899495124817, -2.85630202293396], 'magnitude': 2.92435359954834, 'distance': 10.65501594543457, 'cosine_with_motion': -0.13376092719612437, 'motion_component': -0.39116425460121373}, {'ion': 1387, 'force': [-1.8834420442581177, -0.7630915641784668, -7.254499912261963], 'magnitude': 7.533752918243408, 'distance': 6.638399124145508, 'cosine_with_motion': -0.14679564559442262, 'motion_component': -1.10592210987212}]}, 4339: {'frame': 4339, 'ionic_force': [-0.01052268361672759, 7.317051321268082, -8.848112106323242], 'ionic_force_magnitude': 11.48165661440044, 'motion_vector': [-0.3119239807128906, 0.11574172973632812, 2.2965164184570312], 'cosine_ionic_motion': -0.7307586444093754, 'ionic_motion_component': -8.390319823113206, 'ionic_force_x': -0.01052268361672759, 'ionic_force_y': 7.317051321268082, 'ionic_force_z': -8.848112106323242, 'radial_force': 7.317058887622914, 'axial_force': -8.848112106323242, 'contributions': [{'ion': 1308, 'force': [0.015117759816348553, 0.40834537148475647, -1.4295883178710938], 'magnitude': 1.4868414402008057, 'distance': 14.942962646484375, 'cosine_with_motion': -0.9392277961859843, 'motion_component': -1.3964827394725436}, {'ion': 1316, 'force': [-0.007704783696681261, 1.2880055904388428, -2.648350715637207], 'magnitude': 2.944958209991455, 'distance': 10.61767578125, 'cosine_with_motion': -0.8678253609626467, 'motion_component': -2.5557094833582963}, {'ion': 1387, 'force': [-0.017935659736394882, 5.620700359344482, -4.770173072814941], 'magnitude': 7.37205171585083, 'distance': 6.710808753967285, 'cosine_with_motion': -0.6020206998732269, 'motion_component': -4.438127686965383}]}, 4340: {'frame': 4340, 'ionic_force': [-0.6614977717399597, 11.020213901996613, -11.043931484222412], 'ionic_force_magnitude': 15.615732975943697, 'motion_vector': [0.09852218627929688, -2.540813446044922, -1.569000244140625], 'cosine_ionic_motion': -0.23013628428245336, 'ionic_motion_component': -3.59374676343066, 'ionic_force_x': -0.6614977717399597, 'ionic_force_y': 11.020213901996613, 'ionic_force_z': -11.043931484222412, 'radial_force': 11.040049535567144, 'axial_force': -11.043931484222412, 'contributions': [{'ion': 1308, 'force': [-0.11230937391519547, 0.5389495491981506, -1.9288716316223145], 'magnitude': 2.0058977603912354, 'distance': 12.865143775939941, 'cosine_with_motion': 0.27463385257681466, 'motion_component': 0.5508874269489278}, {'ion': 1316, 'force': [-0.09320607036352158, 2.1498072147369385, -3.7819480895996094], 'magnitude': 4.351263046264648, 'distance': 8.734969139099121, 'cosine_with_motion': 0.03556952269342487, 'motion_component': 0.15477234838873555}, {'ion': 1387, 'force': [-0.4559823274612427, 8.331457138061523, -5.333111763000488], 'magnitude': 9.902685165405273, 'distance': 5.790186405181885, 'cosine_with_motion': -0.43416573845546347, 'motion_component': -4.299406738489893}]}, 4341: {'frame': 4341, 'ionic_force': [-1.1659248024225235, 9.977354973554611, -17.802505493164062], 'ionic_force_magnitude': 20.441041919318973, 'motion_vector': [-0.7720985412597656, -0.6841316223144531, -3.7374649047851562], 'cosine_ionic_motion': 0.7647606975638053, 'ionic_motion_component': 15.632505477149364, 'ionic_force_x': -1.1659248024225235, 'ionic_force_y': 9.977354973554611, 'ionic_force_z': -17.802505493164062, 'radial_force': 10.045247279844283, 'axial_force': -17.802505493164062, 'contributions': [{'ion': 1308, 'force': [-0.09177793562412262, 0.24030449986457825, -1.6979613304138184], 'magnitude': 1.717335820198059, 'distance': 13.904053688049316, 'cosine_with_motion': 0.9390324383797626, 'motion_component': 1.6126339887252703}, {'ion': 1316, 'force': [-0.13407957553863525, 0.977773129940033, -3.8091092109680176], 'magnitude': 3.9348864555358887, 'distance': 9.185503005981445, 'cosine_with_motion': 0.8960829730796381, 'motion_component': 3.5259846615014645}, {'ion': 1387, 'force': [-0.9400672912597656, 8.75927734375, -12.295434951782227], 'magnitude': 15.125685691833496, 'distance': 4.685020446777344, 'cosine_with_motion': 0.6937792513859733, 'motion_component': 10.493887334066017}]}, 4342: {'frame': 4342, 'ionic_force': [-1.3840811252593994, 1.351293995976448, -7.411204814910889], 'ionic_force_magnitude': 7.659479932307392, 'motion_vector': [-2.657154083251953, -1.6822662353515625, 5.648590087890625], 'cosine_ionic_motion': -0.8170268253809583, 'ionic_motion_component': -6.258000573162266, 'ionic_force_x': -1.3840811252593994, 'ionic_force_y': 1.351293995976448, 'ionic_force_z': -7.411204814910889, 'radial_force': 1.9343412379570781, 'axial_force': -7.411204814910889, 'contributions': [{'ion': 1316, 'force': [-0.2974294424057007, 0.23622436821460724, -2.1497864723205566], 'magnitude': 2.183082342147827, 'distance': 12.332013130187988, 'cosine_with_motion': -0.832544475446919, 'motion_component': -1.8175130650926032}, {'ion': 1387, 'force': [-1.0866516828536987, 1.1150696277618408, -5.261418342590332], 'magnitude': 5.4869585037231445, 'distance': 7.778631687164307, 'cosine_with_motion': -0.8092803195561473, 'motion_component': -4.440487642549986}]}, 4343: {'frame': 4343, 'ionic_force': [-16.709574282169342, -0.8938723057508469, -13.62956953048706], 'ionic_force_magnitude': 21.58179895135493, 'motion_vector': [2.1892776489257812, 5.375339508056641, -3.4262237548828125], 'cosine_ionic_motion': 0.036513285370066664, 'ionic_motion_component': 0.788022383910228, 'ionic_force_x': -16.709574282169342, 'ionic_force_y': -0.8938723057508469, 'ionic_force_z': -13.62956953048706, 'radial_force': 16.733465880992004, 'axial_force': -13.62956953048706, 'contributions': [{'ion': 1308, 'force': [-0.6828966736793518, -0.1254197210073471, -2.168544292449951], 'magnitude': 2.2769854068756104, 'distance': 12.07504940032959, 'cosine_with_motion': 0.34279108699768035, 'motion_component': 0.7805302860302322}, {'ion': 1316, 'force': [-2.210134983062744, -0.2589053511619568, -4.237045764923096], 'magnitude': 4.785842418670654, 'distance': 8.32894229888916, 'cosine_with_motion': 0.2569054433894155, 'motion_component': 1.2295089090269506}, {'ion': 1387, 'force': [-13.816542625427246, -0.509547233581543, -7.223979473114014], 'magnitude': 15.599434852600098, 'distance': 4.613330841064453, 'cosine_with_motion': -0.07833721866182479, 'motion_component': -1.2220163395787154}]}, 4344: {'frame': 4344, 'ionic_force': [-1.153914988040924, 3.170382857322693, -5.203489422798157], 'ionic_force_magnitude': 6.201544116976302, 'motion_vector': [1.4634857177734375, -1.2306327819824219, 0.8022537231445312], 'cosine_ionic_motion': -0.7593428919930103, 'ionic_motion_component': -4.709098444607024, 'ionic_force_x': -1.153914988040924, 'ionic_force_y': 3.170382857322693, 'ionic_force_z': -5.203489422798157, 'radial_force': 3.373847545700767, 'axial_force': -5.203489422798157, 'contributions': [{'ion': 1316, 'force': [-0.2957773804664612, 0.846617579460144, -1.985202670097351], 'magnitude': 2.1783652305603027, 'distance': 12.345357894897461, 'cosine_with_motion': -0.6790620152713646, 'motion_component': -1.4792451065752275}, {'ion': 1387, 'force': [-0.8581376075744629, 2.323765277862549, -3.2182867527008057], 'magnitude': 4.061237812042236, 'distance': 9.041485786437988, 'cosine_with_motion': -0.7952878508257138, 'motion_component': -3.2298533141553847}]}, 4345: {'frame': 4345, 'ionic_force': [0.08994757011532784, 5.610477715730667, -9.722934126853943], 'ionic_force_magnitude': 11.225907482213682, 'motion_vector': [-1.1395187377929688, 0.0416717529296875, -1.0085220336914062], 'cosine_ionic_motion': 0.5814891324386149, 'ionic_motion_component': 6.5277432026685895, 'ionic_force_x': 0.08994757011532784, 'ionic_force_y': 5.610477715730667, 'ionic_force_z': -9.722934126853943, 'radial_force': 5.611198692265321, 'axial_force': -9.722934126853943, 'contributions': [{'ion': 1308, 'force': [-0.04955724999308586, 0.3378300964832306, -1.4625250101089478], 'magnitude': 1.5018537044525146, 'distance': 14.868091583251953, 'cosine_with_motion': 0.6760140450308809, 'motion_component': 1.0152741867035733}, {'ion': 1316, 'force': [-0.044318169355392456, 1.0932285785675049, -2.809373140335083], 'magnitude': 3.014911413192749, 'distance': 10.493775367736816, 'cosine_with_motion': 0.6382689866249723, 'motion_component': 1.9243243929068639}, {'ion': 1387, 'force': [0.18382298946380615, 4.179419040679932, -5.451035976409912], 'magnitude': 6.871326446533203, 'distance': 6.951023101806641, 'cosine_with_motion': 0.5221909782986967, 'motion_component': 3.5881446979568086}]}, 4346: {'frame': 4346, 'ionic_force': [-0.9703720510005951, 4.194342374801636, -6.858072519302368], 'ionic_force_magnitude': 8.097363061789316, 'motion_vector': [-4.582515716552734, 0.4224891662597656, 2.309173583984375], 'cosine_ionic_motion': -0.23068510028921504, 'ionic_motion_component': -1.867941009987054, 'ionic_force_x': -0.9703720510005951, 'ionic_force_y': 4.194342374801636, 'ionic_force_z': -6.858072519302368, 'radial_force': 4.305128322642628, 'axial_force': -6.858072519302368, 'contributions': [{'ion': 1316, 'force': [-0.26130351424217224, 0.9197101593017578, -2.4406163692474365], 'magnitude': 2.6212124824523926, 'distance': 11.25428581237793, 'cosine_with_motion': -0.30007228847047807, 'motion_component': -0.7865532102811734}, {'ion': 1387, 'force': [-0.7090685367584229, 3.274632215499878, -4.417456150054932], 'magnitude': 5.544358730316162, 'distance': 7.7382612228393555, 'cosine_with_motion': -0.1950429042251414, 'motion_component': -1.0813878190443305}]}, 4347: {'frame': 4347, 'ionic_force': [-5.324795186519623, 4.4520832896232605, -5.531670093536377], 'ionic_force_magnitude': 8.87546412419373, 'motion_vector': [-0.36487579345703125, -0.39484405517578125, 1.3642425537109375], 'cosine_ionic_motion': -0.5656374441017312, 'ionic_motion_component': -5.020294842425552, 'ionic_force_x': -5.324795186519623, 'ionic_force_y': 4.4520832896232605, 'ionic_force_z': -5.531670093536377, 'radial_force': 6.940784494286306, 'axial_force': -5.531670093536377, 'contributions': [{'ion': 1308, 'force': [-0.5734414458274841, 0.4193485379219055, -1.335965633392334], 'magnitude': 1.5131069421768188, 'distance': 14.812700271606445, 'cosine_with_motion': -0.8017682373028415, 'motion_component': -1.213161044334834}, {'ion': 1316, 'force': [-1.3264715671539307, 1.0629514455795288, -2.074846029281616], 'magnitude': 2.6822338104248047, 'distance': 11.125530242919922, 'cosine_with_motion': -0.7033365199731868, 'motion_component': -1.8865130497748017}, {'ion': 1387, 'force': [-3.424882173538208, 2.969783306121826, -2.1208584308624268], 'magnitude': 5.004745006561279, 'distance': 8.144756317138672, 'cosine_with_motion': -0.3837599886865634, 'motion_component': -1.9206208369105298}]}, 4348: {'frame': 4348, 'ionic_force': [-4.811583518981934, 3.2644795179367065, -4.231451034545898], 'ionic_force_magnitude': 7.191198811111148, 'motion_vector': [1.2287940979003906, -3.6073760986328125, -4.4157257080078125], 'cosine_ionic_motion': 0.023752005658367503, 'ionic_motion_component': 0.17080539485195764, 'ionic_force_x': -4.811583518981934, 'ionic_force_y': 3.2644795179367065, 'ionic_force_z': -4.231451034545898, 'radial_force': 5.8144786940160715, 'axial_force': -4.231451034545898, 'contributions': [{'ion': 1316, 'force': [-1.6572506427764893, 1.0221670866012573, -2.0923280715942383], 'magnitude': 2.858170986175537, 'distance': 10.777670860290527, 'cosine_with_motion': 0.2108659991227886, 'motion_component': 0.602691103493072}, {'ion': 1387, 'force': [-3.1543328762054443, 2.242312431335449, -2.13912296295166], 'magnitude': 4.421948432922363, 'distance': 8.664873123168945, 'cosine_with_motion': -0.09766865255972287, 'motion_component': -0.43188574558306664}]}, 4349: {'frame': 4349, 'ionic_force': [-2.8148942589759827, 0.3423163443803787, -5.1887286901474], 'ionic_force_magnitude': 5.913012395455015, 'motion_vector': [3.6558074951171875, 0.5428085327148438, 1.3375320434570312], 'cosine_ionic_motion': -0.7334051060764676, 'ionic_motion_component': -4.336633483120153, 'ionic_force_x': -2.8148942589759827, 'ionic_force_y': 0.3423163443803787, 'ionic_force_z': -5.1887286901474, 'radial_force': 2.835632234413675, 'axial_force': -5.1887286901474, 'contributions': [{'ion': 1316, 'force': [-0.7681282162666321, 0.059397414326667786, -1.9104300737380981], 'magnitude': 2.0599253177642822, 'distance': 12.69530963897705, 'cosine_with_motion': -0.658453806185171, 'motion_component': -1.356365627793785}, {'ion': 1387, 'force': [-2.0467660427093506, 0.28291893005371094, -3.2782986164093018], 'magnitude': 3.875117540359497, 'distance': 9.25606918334961, 'cosine_with_motion': -0.769078047461971, 'motion_component': -2.9802678535875486}]}, 4350: {'frame': 4350, 'ionic_force': [-1.14635768532753, 1.0225782543420792, -9.443222522735596], 'ionic_force_magnitude': 9.567353544364483, 'motion_vector': [-3.0155258178710938, -3.347362518310547, 1.5890350341796875], 'cosine_ionic_motion': -0.3275592344848105, 'ionic_motion_component': -3.1338750030375686, 'ionic_force_x': -1.14635768532753, 'ionic_force_y': 1.0225782543420792, 'ionic_force_z': -9.443222522735596, 'radial_force': 1.536164779235218, 'axial_force': -9.443222522735596, 'contributions': [{'ion': 1316, 'force': [-0.2180737555027008, 0.12293900549411774, -2.9367432594299316], 'magnitude': 2.9473938941955566, 'distance': 10.613287925720215, 'cosine_with_motion': -0.31393846865149616, 'motion_component': -0.9253003451579868}, {'ion': 1387, 'force': [-0.9282839298248291, 0.8996392488479614, -6.506479263305664], 'magnitude': 6.6336517333984375, 'distance': 7.074450492858887, 'cosine_with_motion': -0.33293495212071195, 'motion_component': -2.2085744950483175}]}, 4351: {'frame': 4351, 'ionic_force': [-5.821552753448486, -2.9807128310203552, -7.226513624191284], 'ionic_force_magnitude': 9.746672488742774, 'motion_vector': [0.9067535400390625, 2.27435302734375, -1.0322418212890625], 'cosine_ionic_motion': -0.17755595543049107, 'ionic_motion_component': -1.7305797460068055, 'ionic_force_x': -5.821552753448486, 'ionic_force_y': -2.9807128310203552, 'ionic_force_z': -7.226513624191284, 'radial_force': 6.540269523665904, 'axial_force': -7.226513624191284, 'contributions': [{'ion': 1316, 'force': [-1.437971591949463, -0.7615723013877869, -2.7652251720428467], 'magnitude': 3.2084615230560303, 'distance': 10.172334671020508, 'cosine_with_motion': -0.021299930527719835, 'motion_component': -0.06834000613675784}, {'ion': 1387, 'force': [-4.383581161499023, -2.2191405296325684, -4.4612884521484375], 'magnitude': 6.6365251541137695, 'distance': 7.07291841506958, 'cosine_with_motion': -0.2504684154112141, 'motion_component': -1.6622398829874785}]}, 4352: {'frame': 4352, 'ionic_force': [-3.8882360458374023, 0.07716289162635803, -8.414870738983154], 'ionic_force_magnitude': 9.270080000398504, 'motion_vector': [-1.1390266418457031, -0.5661506652832031, -1.0862197875976562], 'cosine_ionic_motion': 0.8722952131855376, 'ionic_motion_component': 8.086246410194603, 'ionic_force_x': -3.8882360458374023, 'ionic_force_y': 0.07716289162635803, 'ionic_force_z': -8.414870738983154, 'radial_force': 3.889001627666594, 'axial_force': -8.414870738983154, 'contributions': [{'ion': 1316, 'force': [-0.9431006908416748, -0.052728161215782166, -2.691154956817627], 'magnitude': 2.8521103858947754, 'distance': 10.789115905761719, 'cosine_with_motion': 0.8441814635731749, 'motion_component': 2.4076987968412804}, {'ion': 1387, 'force': [-2.9451353549957275, 0.1298910528421402, -5.723715782165527], 'magnitude': 6.438292980194092, 'distance': 7.180979251861572, 'cosine_with_motion': 0.8819958134782798, 'motion_component': 5.678547440850384}]}, 4353: {'frame': 4353, 'ionic_force': [-6.081224143505096, -0.8584663271903992, -9.448819756507874], 'ionic_force_magnitude': 11.269358735502326, 'motion_vector': [1.2044410705566406, -1.20880126953125, 0.8453292846679688], 'cosine_ionic_motion': -0.6651334853126875, 'ionic_motion_component': -7.495627852983643, 'ionic_force_x': -6.081224143505096, 'ionic_force_y': -0.8584663271903992, 'ionic_force_z': -9.448819756507874, 'radial_force': 6.141518665482428, 'axial_force': -9.448819756507874, 'contributions': [{'ion': 1308, 'force': [-0.4175664782524109, -0.13317164778709412, -1.4587963819503784], 'magnitude': 1.5232148170471191, 'distance': 14.763470649719238, 'cosine_with_motion': -0.5430137956490898, 'motion_component': -0.827126651667454}, {'ion': 1316, 'force': [-1.1213693618774414, -0.22113272547721863, -2.5067636966705322], 'magnitude': 2.755037784576416, 'distance': 10.977545738220215, 'cosine_with_motion': -0.6103808725777308, 'motion_component': -1.6816223630058307}, {'ion': 1387, 'force': [-4.542288303375244, -0.5041619539260864, -5.483259677886963], 'magnitude': 7.138115882873535, 'distance': 6.819888114929199, 'cosine_with_motion': -0.6986267543476838, 'motion_component': -4.986878762952777}]}, 4354: {'frame': 4354, 'ionic_force': [-3.467491030693054, -1.7887528538703918, -8.15508508682251], 'ionic_force_magnitude': 9.040384040154553, 'motion_vector': [-1.2567825317382812, 0.8124618530273438, 0.4911346435546875], 'cosine_ionic_motion': -0.077297958681048, 'ionic_motion_component': -0.6988032319966724, 'ionic_force_x': -3.467491030693054, 'ionic_force_y': -1.7887528538703918, 'ionic_force_z': -8.15508508682251, 'radial_force': 3.901683075310737, 'axial_force': -8.15508508682251, 'contributions': [{'ion': 1316, 'force': [-0.8548189401626587, -0.5112813115119934, -2.679126739501953], 'magnitude': 2.8582937717437744, 'distance': 10.777440071105957, 'cosine_with_motion': -0.14591067328640753, 'motion_component': -0.4170555891222918}, {'ion': 1387, 'force': [-2.6126720905303955, -1.2774715423583984, -5.475958347320557], 'magnitude': 6.200331687927246, 'distance': 7.317480564117432, 'cosine_with_motion': -0.045440745930926375, 'motion_component': -0.2817476814382047}]}, 4355: {'frame': 4355, 'ionic_force': [-4.742857813835144, -1.030191957950592, -6.752213716506958], 'ionic_force_magnitude': 8.315550840796288, 'motion_vector': [-0.8599281311035156, 1.072509765625, 0.5235366821289062], 'cosine_ionic_motion': -0.04589578220628883, 'ionic_motion_component': -0.38164871031450837, 'ionic_force_x': -4.742857813835144, 'ionic_force_y': -1.030191957950592, 'ionic_force_z': -6.752213716506958, 'radial_force': 4.853451937794703, 'axial_force': -6.752213716506958, 'contributions': [{'ion': 1316, 'force': [-1.2849539518356323, -0.36015647649765015, -2.5392329692840576], 'magnitude': 2.8685402870178223, 'distance': 10.758173942565918, 'cosine_with_motion': -0.14472490427713985, 'motion_component': -0.4151492194617141}, {'ion': 1387, 'force': [-3.4579038619995117, -0.6700354814529419, -4.2129807472229], 'magnitude': 5.491379737854004, 'distance': 7.77549934387207, 'cosine_with_motion': 0.006100551507003937, 'motion_component': 0.033500446055334976}]}, 4356: {'frame': 4356, 'ionic_force': [-8.145591795444489, 0.5536623261868954, -8.388230919837952], 'ionic_force_magnitude': 11.705538246231, 'motion_vector': [-0.17728042602539062, -5.445198059082031, 0.5759963989257812], 'cosine_ionic_motion': -0.09983658107924243, 'ionic_motion_component': -1.1686409181960145, 'ionic_force_x': -8.145591795444489, 'ionic_force_y': 0.5536623261868954, 'ionic_force_z': -8.388230919837952, 'radial_force': 8.164386545812935, 'axial_force': -8.388230919837952, 'contributions': [{'ion': 1308, 'force': [-0.6154080033302307, -0.04097851738333702, -1.5266047716140747], 'magnitude': 1.6464896202087402, 'distance': 14.20003890991211, 'cosine_with_motion': -0.06065081615029968, 'motion_component': -0.09986094493453779}, {'ion': 1316, 'force': [-1.5749125480651855, -0.061273880302906036, -2.6270933151245117], 'magnitude': 3.063612699508667, 'distance': 10.410033226013184, 'cosine_with_motion': -0.05364366311720108, 'motion_component': -0.16434341226880056}, {'ion': 1387, 'force': [-5.955271244049072, 0.6559147238731384, -4.234532833099365], 'magnitude': 7.336671352386475, 'distance': 6.726970195770264, 'cosine_with_motion': -0.12327614605629073, 'motion_component': -0.904436581779466}]}, 4357: {'frame': 4357, 'ionic_force': [-5.270969092845917, -5.013264775276184, -4.879510402679443], 'ionic_force_magnitude': 8.759312795797326, 'motion_vector': [0.0101470947265625, 0.001705169677734375, 0.09522247314453125], 'cosine_ionic_motion': -0.6277842758580351, 'ionic_motion_component': -5.498958840523645, 'ionic_force_x': -5.270969092845917, 'ionic_force_y': -5.013264775276184, 'ionic_force_z': -4.879510402679443, 'radial_force': 7.274334257151088, 'axial_force': -4.879510402679443, 'contributions': [{'ion': 1308, 'force': [-0.6041297316551208, -0.6097363233566284, -1.3066514730453491], 'magnitude': 1.5633583068847656, 'distance': 14.572691917419434, 'cosine_with_motion': -0.8788449065300563, 'motion_component': -1.3739494831185086}, {'ion': 1316, 'force': [-1.375537633895874, -1.3294124603271484, -1.9107221364974976], 'magnitude': 2.703756809234619, 'distance': 11.081160545349121, 'cosine_with_motion': -0.7652552232236913, 'motion_component': -2.069063945781279}, {'ion': 1387, 'force': [-3.291301727294922, -3.0741159915924072, -1.6621367931365967], 'magnitude': 4.800578594207764, 'distance': 8.31614875793457, 'cosine_with_motion': -0.4282703242108116, 'motion_component': -2.055945354053961}]}, 4358: {'frame': 4358, 'ionic_force': [-4.603870153427124, -3.909831404685974, -3.866476058959961], 'ionic_force_magnitude': 7.171613424969053, 'motion_vector': [1.1465644836425781, -0.06743621826171875, 0.3713531494140625], 'cosine_ionic_motion': -0.7451740365570843, 'ionic_motion_component': -5.344100124511165, 'ionic_force_x': -4.603870153427124, 'ionic_force_y': -3.909831404685974, 'ionic_force_z': -3.866476058959961, 'radial_force': 6.040066390585934, 'axial_force': -3.866476058959961, 'contributions': [{'ion': 1316, 'force': [-1.2709743976593018, -1.2347279787063599, -1.9208208322525024], 'magnitude': 2.613327741622925, 'distance': 11.27125072479248, 'cosine_with_motion': -0.6616836431521577, 'motion_component': -1.7291962063176305}, {'ion': 1387, 'force': [-3.3328957557678223, -2.6751034259796143, -1.9456552267074585], 'magnitude': 4.695737361907959, 'distance': 8.408473014831543, 'cosine_with_motion': -0.7698267254974382, 'motion_component': -3.6149038997023144}]}, 4359: {'frame': 4359, 'ionic_force': [-6.097867250442505, -7.210108399391174, -5.836791396141052], 'ionic_force_magnitude': 11.101251368069125, 'motion_vector': [-1.8090705871582031, 0.6514205932617188, -0.31896209716796875], 'cosine_ionic_motion': 0.3788134547827392, 'ionic_motion_component': 4.205303383149875, 'ionic_force_x': -6.097867250442505, 'ionic_force_y': -7.210108399391174, 'ionic_force_z': -5.836791396141052, 'radial_force': 9.442968184580016, 'axial_force': -5.836791396141052, 'contributions': [{'ion': 1308, 'force': [-0.5732018947601318, -0.8108179569244385, -1.6454930305480957], 'magnitude': 1.9218828678131104, 'distance': 13.143335342407227, 'cosine_with_motion': 0.2759391664501587, 'motion_component': 0.5303227369907617}, {'ion': 1316, 'force': [-1.4675121307373047, -1.8761595487594604, -2.2478926181793213], 'magnitude': 3.275146961212158, 'distance': 10.068242073059082, 'cosine_with_motion': 0.33675482397552703, 'motion_component': 1.1029215441539115}, {'ion': 1387, 'force': [-4.057153224945068, -4.523130893707275, -1.9434057474136353], 'magnitude': 6.379344463348389, 'distance': 7.214081287384033, 'cosine_with_motion': 0.4031854911937974, 'motion_component': 2.572058988408134}]}, 4360: {'frame': 4360, 'ionic_force': [-5.140026926994324, -3.9340438842773438, -3.686625123023987], 'ionic_force_magnitude': 7.449012209102514, 'motion_vector': [-0.8460655212402344, 0.20500564575195312, 0.1761016845703125], 'cosine_ionic_motion': 0.4372801521611261, 'ionic_motion_component': 3.257305192246433, 'ionic_force_x': -5.140026926994324, 'ionic_force_y': -3.9340438842773438, 'ionic_force_z': -3.686625123023987, 'radial_force': 6.472756607014254, 'axial_force': -3.686625123023987, 'contributions': [{'ion': 1316, 'force': [-1.4018090963363647, -1.172297477722168, -1.9389605522155762], 'magnitude': 2.664379358291626, 'distance': 11.162744522094727, 'cosine_with_motion': 0.25533607786550655, 'motion_component': 0.6803122125233402}, {'ion': 1387, 'force': [-3.738217830657959, -2.761746406555176, -1.7476645708084106], 'magnitude': 4.965465545654297, 'distance': 8.17690658569336, 'cosine_with_motion': 0.518983195660116, 'motion_component': 2.576993131386971}]}, 4361: {'frame': 4361, 'ionic_force': [-5.4141963720321655, -3.7038130164146423, -4.313818573951721], 'ionic_force_magnitude': 7.851164493529584, 'motion_vector': [1.1817245483398438, -0.8403396606445312, -0.4484710693359375], 'cosine_ionic_motion': -0.11337134838642916, 'ionic_motion_component': -0.8900971050351052, 'ionic_force_x': -5.4141963720321655, 'ionic_force_y': -3.7038130164146423, 'ionic_force_z': -4.313818573951721, 'radial_force': 6.559859237475206, 'axial_force': -4.313818573951721, 'contributions': [{'ion': 1308, 'force': [-0.7086317539215088, -0.5181094408035278, -1.3205690383911133], 'magnitude': 1.5857172012329102, 'distance': 14.469588279724121, 'cosine_with_motion': 0.07903236422258367, 'motion_component': 0.1253229768646662}, {'ion': 1316, 'force': [-1.3960002660751343, -0.9637919068336487, -1.544816255569458], 'magnitude': 2.294377565383911, 'distance': 12.029195785522461, 'cosine_with_motion': -0.04220302413094465, 'motion_component': -0.09682967574426726}, {'ion': 1387, 'force': [-3.3095643520355225, -2.221911668777466, -1.44843327999115], 'magnitude': 4.241234302520752, 'distance': 8.84754753112793, 'cosine_with_motion': -0.21658561481700964, 'motion_component': -0.9185902935916275}]}, 4362: {'frame': 4362, 'ionic_force': [-4.9034892320632935, -4.803059756755829, -4.693336129188538], 'ionic_force_magnitude': 8.315106355151116, 'motion_vector': [0.7227058410644531, -0.5454826354980469, 0.70068359375], 'cosine_ionic_motion': -0.4424713221093263, 'ionic_motion_component': -3.6791961024433757, 'ionic_force_x': -4.9034892320632935, 'ionic_force_y': -4.803059756755829, 'ionic_force_z': -4.693336129188538, 'radial_force': 6.863933979572358, 'axial_force': -4.693336129188538, 'contributions': [{'ion': 1308, 'force': [-0.5720486640930176, -0.5742262005805969, -1.2654268741607666], 'magnitude': 1.5027576684951782, 'distance': 14.863618850708008, 'cosine_with_motion': -0.573580941371845, 'motion_component': -0.8619531518802396}, {'ion': 1316, 'force': [-1.2409831285476685, -1.17379891872406, -1.7205088138580322], 'magnitude': 2.424457311630249, 'distance': 11.702045440</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{4408: {'frame': 4408, 'ionic_force': [9.28405300155282, -3.821890950202942, -9.041797399520874], 'ionic_force_magnitude': 13.51127643062888, 'motion_vector': [0.9472541809082031, 6.171745300292969, -2.0280227661132812], 'cosine_ionic_motion': 0.03994897088398283, 'ionic_motion_component': 0.5397615887326366, 'ionic_force_x': 9.28405300155282, 'ionic_force_y': -3.821890950202942, 'ionic_force_z': -9.041797399520874, 'radial_force': 10.039944749394046, 'axial_force': -9.041797399520874, 'contributions': [{'ion': 1308, 'force': [0.0392477847635746, -0.5659531354904175, -1.739326000213623], 'magnitude': 1.8295077085494995, 'distance': 13.471064567565918, 'directional_contribution': 0.010914022006728752}, {'ion': 1316, 'force': [0.1305760145187378, -2.5276927947998047, -4.4630842208862305], 'magnitude': 5.130828380584717, 'distance': 8.044059753417969, 'directional_contribution': -0.9787126361579297}, {'ion': 1460, 'force': [9.114229202270508, -0.7282450199127197, -2.8393871784210205], 'magnitude': 9.574007987976074, 'distance': 5.888736724853516, 'directional_contribution': 1.5075601164077739}]}, 4409: {'frame': 4409, 'ionic_force': [2.3813661485910416, 3.48429112136364, -6.0583014488220215], 'ionic_force_magnitude': 7.383373605396644, 'motion_vector': [1.2028884887695312, 0.22224044799804688, -0.367950439453125], 'cosine_ionic_motion': 0.6221774438388844, 'ionic_motion_component': 4.593768516713172, 'ionic_force_x': 2.3813661485910416, 'ionic_force_y': 3.48429112136364, 'ionic_force_z': -6.0583014488220215, 'radial_force': 4.220330479010953, 'axial_force': -6.0583014488220215, 'contributions': [{'ion': 1308, 'force': [0.11879675090312958, 0.2119782418012619, -1.456363558769226], 'magnitude': 1.4764965772628784, 'distance': 14.995219230651855, 'directional_contribution': 0.5682527165054461}, {'ion': 1316, 'force': [0.3882765471935272, 1.0418009757995605, -3.5045788288116455], 'magnitude': 3.6767079830169678, 'distance': 9.502534866333008, 'directional_contribution': 1.5563756601938152}, {'ion': 1460, 'force': [1.8742928504943848, 2.2305119037628174, -1.09735906124115], 'magnitude': 3.1132545471191406, 'distance': 10.326704025268555, 'directional_contribution': 2.469140102033048}]}, 4410: {'frame': 4410, 'ionic_force': [2.7379980981349945, 3.005010947585106, -6.075490713119507], 'ionic_force_magnitude': 7.310151283366067, 'motion_vector': [-0.20865249633789062, -4.049587249755859, 2.408935546875], 'cosine_ionic_motion': -0.7939953037108676, 'ionic_motion_component': -5.804225788408629, 'ionic_force_x': 2.7379980981349945, 'ionic_force_y': 3.005010947585106, 'ionic_force_z': -6.075490713119507, 'radial_force': 4.065307415251297, 'axial_force': -6.075490713119507, 'contributions': [{'ion': 1308, 'force': [0.2570955455303192, 0.21237300336360931, -1.531499981880188], 'magnitude': 1.5673840045928955, 'distance': 14.55396556854248, 'directional_contribution': -0.9759188427346959}, {'ion': 1316, 'force': [1.0977156162261963, 1.1136078834533691, -3.712677240371704], 'magnitude': 4.0285325050354, 'distance': 9.078113555908203, 'directional_contribution': -2.900923142959339}, {'ion': 1460, 'force': [1.383186936378479, 1.6790300607681274, -0.8313134908676147], 'magnitude': 2.3288259506225586, 'distance': 11.939895629882812, 'directional_contribution': -1.9273837390999855}]}, 4411: {'frame': 4411, 'ionic_force': [6.368192136287689, 0.6474573612213135, -10.474817991256714], 'ionic_force_magnitude': 12.275784458405555, 'motion_vector': [-2.447307586669922, -1.137054443359375, 2.16204833984375], 'cosine_ionic_motion': -0.918028029918748, 'ionic_motion_component': -11.269514222057236, 'ionic_force_x': 6.368192136287689, 'ionic_force_y': 0.6474573612213135, 'ionic_force_z': -10.474817991256714, 'radial_force': 6.401021177849362, 'axial_force': -10.474817991256714, 'contributions': [{'ion': 1308, 'force': [0.3361741900444031, -0.34610939025878906, -2.0818889141082764], 'magnitude': 2.1370694637298584, 'distance': 12.464065551757812, 'directional_contribution': -1.4258381357650443}, {'ion': 1316, 'force': [2.108905553817749, -1.8903121948242188, -7.310626983642578], 'magnitude': 7.840027332305908, 'distance': 6.50744104385376, 'directional_contribution': -5.442032838588133}, {'ion': 1460, 'force': [3.923112392425537, 2.8838789463043213, -1.0823020935058594], 'magnitude': 4.987879753112793, 'distance': 8.158514022827148, 'directional_contribution': -4.401643196460441}]}, 4412: {'frame': 4412, 'ionic_force': [6.665052300319076, -3.4289957880973816, -16.710674703121185], 'ionic_force_magnitude': 18.314682178905333, 'motion_vector': [-1.1050071716308594, 3.6569137573242188, -0.751708984375], 'cosine_ionic_motion': -0.10297495998403897, 'ionic_motion_component': -1.8859536644931683, 'ionic_force_x': 6.665052300319076, 'ionic_force_y': -3.4289957880973816, 'ionic_force_z': -16.710674703121185, 'radial_force': 7.495394204495064, 'axial_force': -16.710674703121185, 'contributions': [{'ion': 1308, 'force': [0.019204726442694664, -0.8384458422660828, -2.92292857170105], 'magnitude': 3.0408670902252197, 'distance': 10.448894500732422, 'directional_contribution': -0.2286272422142609}, {'ion': 1316, 'force': [0.2137768417596817, -8.213178634643555, -14.422178268432617], 'magnitude': 16.598230361938477, 'distance': 4.472374439239502, 'directional_contribution': -4.990360527573039}, {'ion': 1460, 'force': [6.432070732116699, 5.622628688812256, 0.6344321370124817], 'magnitude': 8.566679000854492, 'distance': 6.225336074829102, 'directional_contribution': 3.3330342370915735}]}, 4413: {'frame': 4413, 'ionic_force': [-2.547465205192566, 7.662760257720947, -13.662325963377953], 'ionic_force_magnitude': 15.870306376014476, 'motion_vector': [-0.39898681640625, 0.20450210571289062, -7.287322998046875], 'cosine_ionic_motion': 0.8815448570321193, 'ionic_motion_component': 13.990386965299612, 'ionic_force_x': -2.547465205192566, 'ionic_force_y': 7.662760257720947, 'ionic_force_z': -13.662325963377953, 'radial_force': 8.075114472190124, 'axial_force': -13.662325963377953, 'contributions': [{'ion': 1308, 'force': [-0.4219435453414917, 0.12968969345092773, -2.742938280105591], 'magnitude': 2.778230667114258, 'distance': 10.931629180908203, 'directional_contribution': 2.764452530560943}, {'ion': 1316, 'force': [-4.159623622894287, 3.1517434120178223, -10.773609161376953], 'magnitude': 11.971074104309082, 'distance': 5.266262531280518, 'directional_contribution': 11.068869716949145}, {'ion': 1460, 'force': [2.034101963043213, 4.381327152252197, -0.14577852189540863], 'magnitude': 4.832685470581055, 'distance': 8.288477897644043, 'directional_contribution': 0.1570647748159848}]}, 4414: {'frame': 4414, 'ionic_force': [0.45747989416122437, 1.9616330564022064, -3.9405404329299927], 'ionic_force_magnitude': 4.425511383454767, 'motion_vector': [-0.04938507080078125, -0.9767036437988281, 0.471405029296875], 'cosine_ionic_motion': -0.7901159574218629, 'ionic_motion_component': -3.496667163819716, 'ionic_force_x': 0.45747989416122437, 'ionic_force_y': 1.9616330564022064, 'ionic_force_z': -3.9405404329299927, 'radial_force': 2.0142721021579053, 'axial_force': -3.9405404329299927, 'contributions': [{'ion': 1316, 'force': [-0.3398584723472595, 0.2946309745311737, -2.221829891204834], 'magnitude': 2.2669007778167725, 'distance': 12.10187816619873, 'directional_contribution': -1.2143680491908286}, {'ion': 1460, 'force': [0.7973383665084839, 1.6670020818710327, -1.7187105417251587], 'magnitude': 2.5236105918884277, 'distance': 11.469853401184082, 'directional_contribution': -2.2822991356094935}]}, 4415: {'frame': 4415, 'ionic_force': [0.11436110734939575, 1.6295432336628437, -4.317601203918457], 'ionic_force_magnitude': 4.6162939431245755, 'motion_vector': [-1.1576690673828125, 0.13907241821289062, -4.969749450683594], 'cosine_ionic_motion': 0.9145691038902696, 'ionic_motion_component': 4.2219198148575225, 'ionic_force_x': 0.11436110734939575, 'ionic_force_y': 1.6295432336628437, 'ionic_force_z': -4.317601203918457, 'radial_force': 1.6335512276174682, 'axial_force': -4.317601203918457, 'contributions': [{'ion': 1316, 'force': [-0.3461155891418457, 0.052372146397829056, -2.328737497329712], 'magnitude': 2.35490083694458, 'distance': 11.873608589172363, 'directional_contribution': 2.3470950127604313}, {'ion': 1460, 'force': [0.46047669649124146, 1.5771710872650146, -1.9888637065887451], 'magnitude': 2.5797455310821533, 'distance': 11.344376564025879, 'directional_contribution': 1.874824819083032}]}}</t>
+          <t>{4408: {'frame': 4408, 'ionic_force': [9.28405300155282, -3.821890950202942, -9.041797399520874], 'ionic_force_magnitude': 13.51127643062888, 'motion_vector': [0.9472541809082031, 6.171745300292969, -2.0280227661132812], 'cosine_ionic_motion': 0.03994897088398283, 'ionic_motion_component': 0.5397615887326366, 'ionic_force_x': 9.28405300155282, 'ionic_force_y': -3.821890950202942, 'ionic_force_z': -9.041797399520874, 'radial_force': 10.039944749394046, 'axial_force': -9.041797399520874, 'contributions': [{'ion': 1308, 'force': [0.0392477847635746, -0.5659531354904175, -1.739326000213623], 'magnitude': 1.8295077085494995, 'distance': 13.471064567565918, 'cosine_with_motion': 0.00596555141577959, 'motion_component': 0.010914022006728752}, {'ion': 1316, 'force': [0.1305760145187378, -2.5276927947998047, -4.4630842208862305], 'magnitude': 5.130828380584717, 'distance': 8.044059753417969, 'cosine_with_motion': -0.190751381479075, 'motion_component': -0.9787126361579297}, {'ion': 1460, 'force': [9.114229202270508, -0.7282450199127197, -2.8393871784210205], 'magnitude': 9.574007987976074, 'distance': 5.888736724853516, 'cosine_with_motion': 0.157463841084995, 'motion_component': 1.5075601164077739}]}, 4409: {'frame': 4409, 'ionic_force': [2.3813661485910416, 3.48429112136364, -6.0583014488220215], 'ionic_force_magnitude': 7.383373605396644, 'motion_vector': [1.2028884887695312, 0.22224044799804688, -0.367950439453125], 'cosine_ionic_motion': 0.6221774438388844, 'ionic_motion_component': 4.593768516713172, 'ionic_force_x': 2.3813661485910416, 'ionic_force_y': 3.48429112136364, 'ionic_force_z': -6.0583014488220215, 'radial_force': 4.220330479010953, 'axial_force': -6.0583014488220215, 'contributions': [{'ion': 1308, 'force': [0.11879675090312958, 0.2119782418012619, -1.456363558769226], 'magnitude': 1.4764965772628784, 'distance': 14.995219230651855, 'cosine_with_motion': 0.38486557312870256, 'motion_component': 0.5682527165054461}, {'ion': 1316, 'force': [0.3882765471935272, 1.0418009757995605, -3.5045788288116455], 'magnitude': 3.6767079830169678, 'distance': 9.502534866333008, 'cosine_with_motion': 0.4233068597611323, 'motion_component': 1.5563756601938152}, {'ion': 1460, 'force': [1.8742928504943848, 2.2305119037628174, -1.09735906124115], 'magnitude': 3.1132545471191406, 'distance': 10.326704025268555, 'cosine_with_motion': 0.7931057531386033, 'motion_component': 2.469140102033048}]}, 4410: {'frame': 4410, 'ionic_force': [2.7379980981349945, 3.005010947585106, -6.075490713119507], 'ionic_force_magnitude': 7.310151283366067, 'motion_vector': [-0.20865249633789062, -4.049587249755859, 2.408935546875], 'cosine_ionic_motion': -0.7939953037108676, 'ionic_motion_component': -5.804225788408629, 'ionic_force_x': 2.7379980981349945, 'ionic_force_y': 3.005010947585106, 'ionic_force_z': -6.075490713119507, 'radial_force': 4.065307415251297, 'axial_force': -6.075490713119507, 'contributions': [{'ion': 1308, 'force': [0.2570955455303192, 0.21237300336360931, -1.531499981880188], 'magnitude': 1.5673840045928955, 'distance': 14.55396556854248, 'cosine_with_motion': -0.6226418300254172, 'motion_component': -0.9759188427346958}, {'ion': 1316, 'force': [1.0977156162261963, 1.1136078834533691, -3.712677240371704], 'magnitude': 4.0285325050354, 'distance': 9.078113555908203, 'cosine_with_motion': -0.7200942571398282, 'motion_component': -2.900923142959339}, {'ion': 1460, 'force': [1.383186936378479, 1.6790300607681274, -0.8313134908676147], 'magnitude': 2.3288259506225586, 'distance': 11.939895629882812, 'cosine_with_motion': -0.8276203568856679, 'motion_component': -1.9273837390999855}]}, 4411: {'frame': 4411, 'ionic_force': [6.368192136287689, 0.6474573612213135, -10.474817991256714], 'ionic_force_magnitude': 12.275784458405555, 'motion_vector': [-2.447307586669922, -1.137054443359375, 2.16204833984375], 'cosine_ionic_motion': -0.918028029918748, 'ionic_motion_component': -11.269514222057236, 'ionic_force_x': 6.368192136287689, 'ionic_force_y': 0.6474573612213135, 'ionic_force_z': -10.474817991256714, 'radial_force': 6.401021177849362, 'axial_force': -10.474817991256714, 'contributions': [{'ion': 1308, 'force': [0.3361741900444031, -0.34610939025878906, -2.0818889141082764], 'magnitude': 2.1370694637298584, 'distance': 12.464065551757812, 'cosine_with_motion': -0.6671931374770188, 'motion_component': -1.4258381357650443}, {'ion': 1316, 'force': [2.108905553817749, -1.8903121948242188, -7.310626983642578], 'magnitude': 7.840027332305908, 'distance': 6.50744104385376, 'cosine_with_motion': -0.6941344152193054, 'motion_component': -5.442032838588133}, {'ion': 1460, 'force': [3.923112392425537, 2.8838789463043213, -1.0823020935058594], 'magnitude': 4.987879753112793, 'distance': 8.158514022827148, 'cosine_with_motion': -0.8824677491173122, 'motion_component': -4.401643196460441}]}, 4412: {'frame': 4412, 'ionic_force': [6.665052300319076, -3.4289957880973816, -16.710674703121185], 'ionic_force_magnitude': 18.314682178905333, 'motion_vector': [-1.1050071716308594, 3.6569137573242188, -0.751708984375], 'cosine_ionic_motion': -0.10297495998403897, 'ionic_motion_component': -1.8859536644931683, 'ionic_force_x': 6.665052300319076, 'ionic_force_y': -3.4289957880973816, 'ionic_force_z': -16.710674703121185, 'radial_force': 7.495394204495064, 'axial_force': -16.710674703121185, 'contributions': [{'ion': 1308, 'force': [0.019204726442694664, -0.8384458422660828, -2.92292857170105], 'magnitude': 3.0408670902252197, 'distance': 10.448894500732422, 'cosine_with_motion': -0.07518488886952328, 'motion_component': -0.2286272422142609}, {'ion': 1316, 'force': [0.2137768417596817, -8.213178634643555, -14.422178268432617], 'magnitude': 16.598230361938477, 'distance': 4.472374439239502, 'cosine_with_motion': -0.3006561911623409, 'motion_component': -4.990360527573039}, {'ion': 1460, 'force': [6.432070732116699, 5.622628688812256, 0.6344321370124817], 'magnitude': 8.566679000854492, 'distance': 6.225336074829102, 'cosine_with_motion': 0.38906957811169834, 'motion_component': 3.3330342370915735}]}, 4413: {'frame': 4413, 'ionic_force': [-2.547465205192566, 7.662760257720947, -13.662325963377953], 'ionic_force_magnitude': 15.870306376014476, 'motion_vector': [-0.39898681640625, 0.20450210571289062, -7.287322998046875], 'cosine_ionic_motion': 0.8815448570321193, 'ionic_motion_component': 13.990386965299612, 'ionic_force_x': -2.547465205192566, 'ionic_force_y': 7.662760257720947, 'ionic_force_z': -13.662325963377953, 'radial_force': 8.075114472190124, 'axial_force': -13.662325963377953, 'contributions': [{'ion': 1308, 'force': [-0.4219435453414917, 0.12968969345092773, -2.742938280105591], 'magnitude': 2.778230667114258, 'distance': 10.931629180908203, 'cosine_with_motion': 0.9950406445494476, 'motion_component': 2.764452530560943}, {'ion': 1316, 'force': [-4.159623622894287, 3.1517434120178223, -10.773609161376953], 'magnitude': 11.971074104309082, 'distance': 5.266262531280518, 'cosine_with_motion': 0.9246346516533765, 'motion_component': 11.068869716949145}, {'ion': 1460, 'force': [2.034101963043213, 4.381327152252197, -0.14577852189540863], 'magnitude': 4.832685470581055, 'distance': 8.288477897644043, 'cosine_with_motion': 0.032500516046732666, 'motion_component': 0.1570647748159848}]}, 4414: {'frame': 4414, 'ionic_force': [0.45747989416122437, 1.9616330564022064, -3.9405404329299927], 'ionic_force_magnitude': 4.425511383454767, 'motion_vector': [-0.04938507080078125, -0.9767036437988281, 0.471405029296875], 'cosine_ionic_motion': -0.7901159574218629, 'ionic_motion_component': -3.496667163819716, 'ionic_force_x': 0.45747989416122437, 'ionic_force_y': 1.9616330564022064, 'ionic_force_z': -3.9405404329299927, 'radial_force': 2.0142721021579053, 'axial_force': -3.9405404329299927, 'contributions': [{'ion': 1316, 'force': [-0.3398584723472595, 0.2946309745311737, -2.221829891204834], 'magnitude': 2.2669007778167725, 'distance': 12.10187816619873, 'cosine_with_motion': -0.5356952746826692, 'motion_component': -1.2143680491908284}, {'ion': 1460, 'force': [0.7973383665084839, 1.6670020818710327, -1.7187105417251587], 'magnitude': 2.5236105918884277, 'distance': 11.469853401184082, 'cosine_with_motion': -0.9043784954636804, 'motion_component': -2.2822991356094935}]}, 4415: {'frame': 4415, 'ionic_force': [0.11436110734939575, 1.6295432336628437, -4.317601203918457], 'ionic_force_magnitude': 4.6162939431245755, 'motion_vector': [-1.1576690673828125, 0.13907241821289062, -4.969749450683594], 'cosine_ionic_motion': 0.9145691038902696, 'ionic_motion_component': 4.2219198148575225, 'ionic_force_x': 0.11436110734939575, 'ionic_force_y': 1.6295432336628437, 'ionic_force_z': -4.317601203918457, 'radial_force': 1.6335512276174682, 'axial_force': -4.317601203918457, 'contributions': [{'ion': 1316, 'force': [-0.3461155891418457, 0.052372146397829056, -2.328737497329712], 'magnitude': 2.35490083694458, 'distance': 11.873608589172363, 'cosine_with_motion': 0.9966853552791446, 'motion_component': 2.3470950127604313}, {'ion': 1460, 'force': [0.46047669649124146, 1.5771710872650146, -1.9888637065887451], 'magnitude': 2.5797455310821533, 'distance': 11.344376564025879, 'cosine_with_motion': 0.7267480067537534, 'motion_component': 1.874824819083032}]}}</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{4857: {'frame': 4857, 'ionic_force': [-23.60623151063919, 0.16038507223129272, 2.653203248977661], 'ionic_force_magnitude': 23.755407320980098, 'motion_vector': [0.9804725646972656, -0.3909263610839844, 0.2857513427734375], 'cosine_ionic_motion': -0.8642116533491877, 'ionic_motion_component': -20.52969983684761, 'ionic_force_x': -23.60623151063919, 'ionic_force_y': 0.16038507223129272, 'ionic_force_z': 2.653203248977661, 'radial_force': 23.606776347169667, 'axial_force': 2.653203248977661, 'contributions': [{'ion': 1308, 'force': [-1.2521235942840576, 1.593077540397644, -2.4381844997406006], 'magnitude': 3.1702449321746826, 'distance': 10.233463287353516, 'directional_contribution': -2.329307494535591}, {'ion': 1320, 'force': [-0.6172628998756409, 0.6778424382209778, -1.6455979347229004], 'magnitude': 1.8837400674819946, 'distance': 13.275734901428223, 'directional_contribution': -1.2257824654629097}, {'ion': 1460, 'force': [-21.736845016479492, -2.110534906387329, 6.736985683441162], 'magnitude': 22.854578018188477, 'distance': 3.8113815784454346, 'directional_contribution': -16.9746092376122}]}, 4858: {'frame': 4858, 'ionic_force': [-8.50262776017189, 3.199307382106781, 3.651916027069092], 'ionic_force_magnitude': 9.791156071782979, 'motion_vector': [-0.14766693115234375, 1.5113677978515625, -0.5906982421875], 'cosine_ionic_motion': 0.24656918258421606, 'ionic_motion_component': 2.414197349174013, 'ionic_force_x': -8.50262776017189, 'ionic_force_y': 3.199307382106781, 'ionic_force_z': 3.651916027069092, 'radial_force': 9.084615927668523, 'axial_force': 3.651916027069092, 'contributions': [{'ion': 1308, 'force': [-1.0608267784118652, 1.5705699920654297, -2.8913075923919678], 'magnitude': 3.4571235179901123, 'distance': 9.799673080444336, 'directional_contribution': 2.6011008640142848}, {'ion': 1320, 'force': [-0.4662999212741852, 0.6704815030097961, -1.7270715236663818], 'magnitude': 1.9104337692260742, 'distance': 13.182660102844238, 'directional_contribution': 1.2902738108900658}, {'ion': 1460, 'force': [-6.97550106048584, 0.9582558870315552, 8.270295143127441], 'magnitude': 10.861567497253418, 'distance': 5.5286970138549805, 'directional_contribution': -1.4771773018897036}]}, 4859: {'frame': 4859, 'ionic_force': [-9.53341594338417, 13.158035159111023, 4.4725987911224365], 'ionic_force_magnitude': 16.85301304646511, 'motion_vector': [-0.5728759765625, -0.2980232238769531, -0.14586639404296875], 'cosine_ionic_motion': 0.07955984094930431, 'ionic_motion_component': 1.3408230374933148, 'ionic_force_x': -9.53341594338417, 'ionic_force_y': 13.158035159111023, 'ionic_force_z': 4.4725987911224365, 'radial_force': 16.248689448628568, 'axial_force': 4.4725987911224365, 'contributions': [{'ion': 1308, 'force': [-0.8318650126457214, 1.5506973266601562, -2.159569263458252], 'magnitude': 2.785749673843384, 'distance': 10.916866302490234, 'directional_contribution': 0.49759226274005286}, {'ion': 1320, 'force': [-0.4241594970226288, 0.7252730131149292, -1.4648845195770264], 'magnitude': 1.6887328624725342, 'distance': 14.021308898925781, 'directional_contribution': 0.36330764449495057}, {'ion': 1460, 'force': [-8.27739143371582, 10.882064819335938, 8.097052574157715], 'magnitude': 15.890148162841797, 'distance': 4.570935249328613, 'directional_contribution': 0.47992324150436616}]}, 4860: {'frame': 4860, 'ionic_force': [-2.976147174835205, 6.678335726261139, -2.335963726043701], 'ionic_force_magnitude': 7.675568161923092, 'motion_vector': [0.6911888122558594, -0.11594009399414062, 0.5926361083984375], 'cosine_ionic_motion': -0.598417063639624, 'ionic_motion_component': -4.593190961223803, 'ionic_force_x': -2.976147174835205, 'ionic_force_y': 6.678335726261139, 'ionic_force_z': -2.335963726043701, 'radial_force': 7.311471813454215, 'axial_force': -2.335963726043701, 'contributions': [{'ion': 1308, 'force': [-0.9280287027359009, 1.4536443948745728, -2.190319776535034], 'magnitude': 2.7877984046936035, 'distance': 10.912854194641113, 'directional_contribution': -2.2967804955902}, {'ion': 1320, 'force': [-0.4511340856552124, 0.7071818709373474, -1.4634768962860107], 'magnitude': 1.6868292093276978, 'distance': 14.029218673706055, 'directional_contribution': -1.3740305233741053}, {'ion': 1460, 'force': [-1.5969843864440918, 4.517509460449219, 1.3178329467773438], 'magnitude': 4.969399929046631, 'distance': 8.173669815063477, 'directional_contribution': -0.9223798648451975}]}, 4861: {'frame': 4861, 'ionic_force': [-2.949042022228241, 8.77355444431305, -2.55695903301239], 'ionic_force_magnitude': 9.60261141214706, 'motion_vector': [0.4648017883300781, 0.24734878540039062, -0.2841033935546875], 'cosine_ionic_motion': 0.2655944164048997, 'ionic_motion_component': 2.5503999739722283, 'ionic_force_x': -2.949042022228241, 'ionic_force_y': 8.77355444431305, 'ionic_force_z': -2.55695903301239, 'radial_force': 9.255922776049577, 'axial_force': -2.55695903301239, 'contributions': [{'ion': 1308, 'force': [-0.8082016706466675, 1.8407821655273438, -2.506990909576416], 'magnitude': 3.2135140895843506, 'distance': 10.164334297180176, 'directional_contribution': 1.3236421976845847}, {'ion': 1320, 'force': [-0.4184555411338806, 0.7065335512161255, -1.485287070274353], 'magnitude': 1.6971659660339355, 'distance': 13.986430168151855, 'directional_contribution': 0.672323388035597}, {'ion': 1460, 'force': [-1.7223848104476929, 6.22623872756958, 1.435318946838379], 'magnitude': 6.617612838745117, 'distance': 7.0830183029174805, 'directional_contribution': 0.554434531374163}]}, 4862: {'frame': 4862, 'ionic_force': [-2.821112185716629, 16.71923440694809, -1.5727373361587524], 'ionic_force_magnitude': 17.02835799034726, 'motion_vector': [-0.7869873046875, 0.3434638977050781, -0.23621368408203125], 'cosine_ionic_motion': 0.5495663586687077, 'ionic_motion_component': 9.358212694862338, 'ionic_force_x': -2.821112185716629, 'ionic_force_y': 16.71923440694809, 'ionic_force_z': -1.5727373361587524, 'radial_force': 16.955573511942195, 'axial_force': -1.5727373361587524, 'contributions': [{'ion': 1308, 'force': [-0.5865727663040161, 1.652468204498291, -2.294264078140259], 'magnitude': 2.8876230716705322, 'distance': 10.722567558288574, 'directional_contribution': 1.7641810025489164}, {'ion': 1320, 'force': [-0.32260993123054504, 0.7156185507774353, -1.465861201286316], 'magnitude': 1.6628097295761108, 'distance': 14.130182266235352, 'directional_contribution': 0.9498819854370506}, {'ion': 1460, 'force': [-1.9119294881820679, 14.351147651672363, 2.1873879432678223], 'magnitude': 14.642252922058105, 'distance': 4.761733531951904, 'directional_contribution': 6.644149834145949}]}, 4863: {'frame': 4863, 'ionic_force': [-3.69932222366333, 9.218546092510223, -2.963527649641037], 'ionic_force_magnitude': 10.36576447274449, 'motion_vector': [1.4510307312011719, -0.018299102783203125, -1.9164810180664062], 'cosine_ionic_motion': 0.005739696896891008, 'ionic_motion_component': 0.059496346178114605, 'ionic_force_x': -3.69932222366333, 'ionic_force_y': 9.218546092510223, 'ionic_force_z': -2.963527649641037, 'radial_force': 9.93310510234463, 'axial_force': -2.963527649641037, 'contributions': [{'ion': 1308, 'force': [-0.7104681134223938, 1.5558724403381348, -1.9979960918426514], 'magnitude': 2.630112648010254, 'distance': 11.235227584838867, 'directional_contribution': 1.1521869135222806}, {'ion': 1320, 'force': [-0.3768095374107361, 0.7196657061576843, -1.397373080253601], 'magnitude': 1.6163402795791626, 'distance': 14.331863403320312, 'directional_contribution': 0.8811138419875748}, {'ion': 1460, 'force': [-2.6120445728302, 6.943007946014404, 0.43184152245521545], 'magnitude': 7.430654048919678, 'distance': 6.684293746948242, 'directional_contribution': -1.9738043384000463}]}, 4864: {'frame': 4864, 'ionic_force': [-3.9271629452705383, 6.102272391319275, -2.3661776781082153], 'ionic_force_magnitude': 7.63276712214784, 'motion_vector': [-1.0789031982421875, -0.15365219116210938, 2.0991592407226562], 'cosine_ionic_motion': -0.09237188980147616, 'ionic_motion_component': -0.7050531234873706, 'ionic_force_x': -3.9271629452705383, 'ionic_force_y': 6.102272391319275, 'ionic_force_z': -2.3661776781082153, 'radial_force': 7.256744251836593, 'axial_force': -2.3661776781082153, 'contributions': [{'ion': 1308, 'force': [-0.32004624605178833, 1.0951236486434937, -1.809603214263916], 'magnitude': 2.139249563217163, 'distance': 12.457712173461914, 'directional_contribution': -1.5312169138518108}, {'ion': 1460, 'force': [-3.60711669921875, 5.007148742675781, -0.5565744638442993], 'magnitude': 6.196176528930664, 'distance': 7.319933891296387, 'directional_contribution': 0.8261637182101396}]}, 4865: {'frame': 4865, 'ionic_force': [-3.168602854013443, 5.503656804561615, -3.0944536328315735], 'ionic_force_magnitude': 7.064412612142925, 'motion_vector': [3.705402374267578, -1.9471969604492188, -2.8583602905273438], 'cosine_ionic_motion': -0.3801608278025133, 'ionic_motion_component': -2.6856129465707697, 'ionic_force_x': -3.168602854013443, 'ionic_force_y': 5.503656804561615, 'ionic_force_z': -3.0944536328315735, 'radial_force': 6.350612747511811, 'axial_force': -3.0944536328315735, 'contributions': [{'ion': 1308, 'force': [-0.8212441205978394, 1.7357362508773804, -2.2392847537994385], 'magnitude': 2.949850559234619, 'distance': 10.608867645263672, 'directional_contribution': -0.004375345063333924}, {'ion': 1320, 'force': [-0.41535165905952454, 0.8550887703895569, -1.5833065509796143], 'magnitude': 1.8467683792114258, 'distance': 13.407963752746582, 'directional_contribution': 0.26073495759911935}, {'ion': 1460, 'force': [-1.932007074356079, 2.9128317832946777, 0.7281376719474792], 'magnitude': 3.5703535079956055, 'distance': 9.643028259277344, 'directional_contribution': -2.9419724204515667}]}, 4866: {'frame': 4866, 'ionic_force': [-7.758470341563225, 11.393471777439117, -3.07043993473053], 'ionic_force_magnitude': 14.122062971712237, 'motion_vector': [-0.006435394287109375, 0.24068450927734375, 0.5570297241210938], 'cosine_ionic_motion': 0.12623792979283582, 'ionic_motion_component': 1.782739993953016, 'ionic_force_x': -7.758470341563225, 'ionic_force_y': 11.393471777439117, 'ionic_force_z': -3.07043993473053, 'radial_force': 13.784232339315013, 'axial_force': -3.07043993473053, 'contributions': [{'ion': 1308, 'force': [0.049068644642829895, 0.7890864014625549, -2.0871825218200684], 'magnitude': 2.2319042682647705, 'distance': 12.196389198303223, 'directional_contribution': -1.603421891308001}, {'ion': 1460, 'force': [-7.807538986206055, 10.604385375976562, -0.9832574129104614], 'magnitude': 13.205204963684082, 'distance': 5.0141401290893555, 'directional_contribution': 3.386161754441588}]}, 4867: {'frame': 4867, 'ionic_force': [0.12337589636445045, 4.056435167789459, -4.2135396003723145], 'ionic_force_magnitude': 5.850111438783753, 'motion_vector': [-0.9177093505859375, 0.6418495178222656, 2.0229339599609375], 'cosine_ionic_motion': -0.44602597766328916, 'ionic_motion_component': -2.609301673922715, 'ionic_force_x': 0.12337589636445045, 'ionic_force_y': 4.056435167789459, 'ionic_force_z': -4.2135396003723145, 'radial_force': 4.058310964216866, 'axial_force': -4.2135396003723145, 'contributions': [{'ion': 1308, 'force': [0.09774009138345718, 0.9288542866706848, -2.069882869720459], 'magnitude': 2.270845413208008, 'distance': 12.091362953186035, 'directional_contribution': -1.5918586226891804}, {'ion': 1460, 'force': [0.02563580498099327, 3.1275808811187744, -2.1436567306518555], 'magnitude': 3.7917916774749756, 'distance': 9.357219696044922, 'directional_contribution': -1.0174431206508086}]}, 4868: {'frame': 4868, 'ionic_force': [-1.2063874416053295, 6.333217084407806, -5.534350037574768], 'ionic_force_magnitude': 8.496707576226324, 'motion_vector': [0.3851051330566406, 2.4810562133789062, 0.2808074951171875], 'cosine_ionic_motion': 0.6379499331499946, 'ionic_motion_component': 5.420474030248636, 'ionic_force_x': -1.2063874416053295, 'ionic_force_y': 6.333217084407806, 'ionic_force_z': -5.534350037574768, 'radial_force': 6.447093088943107, 'axial_force': -5.534350037574768, 'contributions': [{'ion': 1308, 'force': [-0.13308840990066528, 1.483996033668518, -2.676917314529419], 'magnitude': 3.0636322498321533, 'distance': 10.40999984741211, 'directional_contribution': 1.1395278843755534}, {'ion': 1320, 'force': [-0.05506179854273796, 0.6272523999214172, -1.598051905632019], 'magnitude': 1.7176283597946167, 'distance': 13.90286922454834, 'directional_contribution': 0.4299755799140038}, {'ion': 1460, 'force': [-1.0182372331619263, 4.221968650817871, -1.25938081741333], 'magnitude': 4.5219316482543945, 'distance': 8.568544387817383, 'directional_contribution': 3.8509706902766823}]}, 4869: {'frame': 4869, 'ionic_force': [0.0542104747146368, 5.165193021297455, -3.881076753139496], 'ionic_force_magnitude': 6.461030450832787, 'motion_vector': [-0.0664825439453125, -0.035305023193359375, -0.05754852294921875], 'cosine_ionic_motion': 0.06107260201521054, 'ionic_motion_component': 0.39459194133186715, 'ionic_force_x': 0.0542104747146368, 'ionic_force_y': 5.165193021297455, 'ionic_force_z': -3.881076753139496, 'radial_force': 5.165477492239098, 'axial_force': -3.881076753139496, 'contributions': [{'ion': 1308, 'force': [-0.011133236810564995, 1.6809277534484863, -1.8282040357589722], 'magnitude': 2.4835402965545654, 'distance': 11.562012672424316, 'directional_contribution': 0.49186012500856546}, {'ion': 1320, 'force': [0.029794860631227493, 0.8571366667747498, -1.3412694931030273], 'magnitude': 1.5920348167419434, 'distance': 14.440850257873535, 'directional_contribution': 0.47434724454418253}, {'ion': 1460, 'force': [0.035548850893974304, 2.6271286010742188, -0.7116032242774963], 'magnitude': 2.7220301628112793, 'distance': 11.043903350830078, 'directional_contribution': -0.5716154000736449}]}, 4870: {'frame': 4870, 'ionic_force': [-0.09000088274478912, 4.857101559638977, -3.782764494419098], 'ionic_force_magnitude': 6.157015749515344, 'motion_vector': [-0.150634765625, -2.8217086791992188, -4.534019470214844], 'cosine_ionic_motion': 0.10516778943237615, 'ionic_motion_component': 0.6475197358768533, 'ionic_force_x': -0.09000088274478912, 'ionic_force_y': 4.857101559638977, 'ionic_force_z': -3.782764494419098, 'radial_force': 4.85793533505153, 'axial_force': -3.782764494419098, 'contributions': [{'ion': 1308, 'force': [-0.0317416787147522, 1.5285658836364746, -1.7929517030715942], 'magnitude': 2.3563101291656494, 'distance': 11.870057106018066, 'directional_contribution': 0.7151909310539509}, {'ion': 1320, 'force': [-0.024010654538869858, 0.8109053373336792, -1.3013789653778076], 'magnitude': 1.5335354804992676, 'distance': 14.71370792388916, 'directional_contribution': 0.6768312379802743}, {'ion': 1460, 'force': [-0.03424854949116707, 2.5176303386688232, -0.688433825969696], 'magnitude': 2.6102828979492188, 'distance': 11.277822494506836, 'directional_contribution': -0.7445026222250652}]}, 4871: {'frame': 4871, 'ionic_force': [-1.4377694465219975, 2.7718199491500854, -5.007754564285278], 'ionic_force_magnitude': 5.901505959327551, 'motion_vector': [-0.12489700317382812, -0.5373611450195312, 0.7347412109375], 'cosine_ionic_motion': -0.9201397059694539, 'ionic_motion_component': -5.430209958192633, 'ionic_force_x': -1.4377694465219975, 'ionic_force_y': 2.7718199491500854, 'ionic_force_z': -5.007754564285278, 'radial_force': 3.122525710359893, 'axial_force': -5.007754564285278, 'contributions': [{'ion': 1308, 'force': [-0.03414252772927284, 0.5607947111129761, -1.570929765701294], 'magnitude': 1.6683754920959473, 'distance': 14.106593132019043, 'directional_contribution': -1.579566219617024}, {'ion': 1460, 'force': [-1.4036269187927246, 2.2110252380371094, -3.4368247985839844], 'magnitude': 4.3209452629089355, 'distance': 8.765560150146484, 'directional_contribution': -3.8506437663609603}]}, 4872: {'frame': 4872, 'ionic_force': [-1.5672330230518128, 3.253392219543457, -6.297172904014587], 'ionic_force_magnitude': 7.259143673036479, 'motion_vector': [1.6905479431152344, -0.46477508544921875, 1.652435302734375], 'cosine_ionic_motion': -0.8329315936526057, 'ionic_motion_component': -6.046370108135505, 'ionic_force_x': -1.5672330230518128, 'ionic_force_y': 3.253392219543457, 'ionic_force_z': -6.297172904014587, 'radial_force': 3.6112020550960624, 'axial_force': -6.297172904014587, 'contributions': [{'ion': 1308, 'force': [2.390443842159584e-05, 0.5934185981750488, -1.8552712202072144], 'magnitude': 1.9478647708892822, 'distance': 13.055383682250977, 'directional_contribution': -1.3869354112101064}, {'ion': 1460, 'force': [-1.5672569274902344, 2.659973621368408, -4.441901683807373], 'magnitude': 5.409458637237549, 'distance': 7.8341546058654785, 'directional_contribution': -4.659434702269067}]}, 4873: {'frame': 4873, 'ionic_force': [-1.6994890123605728, 6.724162369966507, -11.125696539878845], 'ionic_force_magnitude': 13.110444156407517, 'motion_vector': [-1.8945083618164062, 4.309528350830078, 0.9468460083007812], 'cosine_ionic_motion': 0.34411208913073765, 'ionic_motion_component': 4.511462328093263, 'ionic_force_x': -1.6994890123605728, 'ionic_force_y': 6.724162369966507, 'ionic_force_z': -11.125696539878845, 'radial_force': 6.935605415593358, 'axial_force': -11.125696539878845, 'contributions': [{'ion': 1308, 'force': [0.2984895706176758, 0.8108097314834595, -2.3136789798736572], 'magnitude': 2.469740629196167, 'distance': 11.594268798828125, 'directional_contribution': 0.153694867391323}, {'ion': 1320, 'force': [0.10234962403774261, 0.38926997780799866, -1.4215017557144165], 'magnitude': 1.477387547492981, 'distance': 14.990696907043457, 'directional_contribution': 0.028681596305214274}, {'ion': 1460, 'force': [-2.100328207015991, 5.524082660675049, -7.3905158042907715], 'magnitude': 9.462905883789062, 'distance': 5.923205375671387, 'directional_contribution': 4.329086093616461}]}, 4874: {'frame': 4874, 'ionic_force': [-1.8247650638222694, 5.6435387134552, -3.796484112739563], 'ionic_force_magnitude': 7.0422005343995835, 'motion_vector': [1.5041236877441406, -3.0937538146972656, -1.0170440673828125], 'cosine_ionic_motion': -0.6469517009967339, 'ionic_motion_component': -4.55596361448992, 'ionic_force_x': -1.8247650638222694, 'ionic_force_y': 5.6435387134552, 'ionic_force_z': -3.796484112739563, 'radial_force': 5.931213766878907, 'axial_force': -3.796484112739563, 'contributions': [{'ion': 1308, 'force': [-0.06882379204034805, 1.2181742191314697, -1.544019103050232], 'magnitude': 1.9679126739501953, 'distance': 12.988713264465332, 'directional_contribution': -0.641700611758041}, {'ion': 1460, 'force': [-1.7559412717819214, 4.4253644943237305, -2.252465009689331], 'magnitude': 5.266951560974121, 'distance': 7.939431190490723, 'directional_contribution': -3.9142629071584913}]}, 4875: {'frame': 4875, 'ionic_force': [-1.1494073271751404, 5.382365703582764, -6.437063932418823], 'ionic_force_magnitude': 8.469167009860838, 'motion_vector': [-4.102687835693359, -0.4046134948730469, 2.7181549072265625], 'cosine_ionic_motion': -0.35769251277853253, 'ionic_motion_component': -3.029357628898174, 'ionic_force_x': -1.1494073271751404, 'ionic_force_y': 5.382365703582764, 'ionic_force_z': -6.437063932418823, 'radial_force': 5.5037258081110725, 'axial_force': -6.437063932418823, 'contributions': [{'ion': 1308, 'force': [0.1549651026725769, 0.9382805824279785, -2.0105345249176025], 'magnitude': 2.2241029739379883, 'distance': 12.21776008605957, 'directional_contribution': -1.3123371483160682}, {'ion': 1460, 'force': [-1.3043724298477173, 4.444085121154785, -4.426529407501221], 'magnitude': 6.406671524047852, 'distance': 7.198678970336914, 'directional_contribution': -1.71702038868942}]}, 4876: {'frame': 4876, 'ionic_force': [-5.890000581741333, 6.048319339752197, -6.3055113554000854], 'ionic_force_magnitude': 10.537255199605498, 'motion_vector': [5.018623352050781, -2.8053436279296875, -2.0750503540039062], 'cosine_ionic_motion': -0.519231764832483, 'ionic_motion_component': -5.471277613781421, 'ionic_force_x': -5.890000581741333, 'ionic_force_y': 6.048319339752197, 'ionic_force_z': -6.3055113554000854, 'radial_force': 8.442409234841302, 'axial_force': -6.3055113554000854, 'contributions': [{'ion': 1308, 'force': [-1.146353840827942, 1.7300130128860474, -2.72662091255188], 'magnitude': 3.4265921115875244, 'distance': 9.84323501586914, 'directional_contribution': -0.8095775295885126}, {'ion': 1320, 'force': [-0.5717068910598755, 0.7419012784957886, -1.8075217008590698], 'magnitude': 2.035780191421509, 'distance': 12.770373344421387, 'directional_contribution': -0.19628231660630036}, {'ion': 1460, 'force': [-4.171939849853516, 3.5764050483703613, -1.7713687419891357], 'magnitude': 5.773517608642578, 'distance': 7.58313512802124, 'directional_contribution': -4.465417884486193}]}, 4877: {'frame': 4877, 'ionic_force': [-1.2858441323041916, 6.905015721917152, -19.02397847175598], 'ionic_force_magnitude': 20.27916157404786, 'motion_vector': [-1.6677970886230469, 2.3718338012695312, 1.7540283203125], 'cosine_ionic_motion': -0.2160392511374309, 'ionic_motion_component': -4.381094880152263, 'ionic_force_x': -1.2858441323041916, 'ionic_force_y': 6.905015721917152, 'ionic_force_z': -19.02397847175598, 'radial_force': 7.023719616592349, 'axial_force': -19.02397847175598, 'contributions': [{'ion': 1308, 'force': [0.548943817615509, 0.45097389817237854, -2.8554723262786865], 'magnitude': 2.9425225257873535, 'distance': 10.622069358825684, 'directional_contribution': -1.4325173471264652}, {'ion': 1320, 'force': [0.22946275770664215, 0.1839812844991684, -1.6267189979553223], 'magnitude': 1.6530932188034058, 'distance': 14.171648979187012, 'directional_contribution': -0.826151048322767}, {'ion': 1460, 'force': [-2.0642507076263428, 6.2700605392456055, -14.541787147521973], 'magnitude': 15.96992015838623, 'distance': 4.559504508972168, 'directional_contribution': -2.122426196693901}]}, 4878: {'frame': 4878, 'ionic_force': [-4.718822101131082, 12.355452835559845, -11.77543318271637], 'ionic_force_magnitude': 17.70834050481537, 'motion_vector': [3.3215065002441406, -4.6515045166015625, -1.365631103515625], 'cosine_ionic_motion': -0.5483564622691216, 'ionic_motion_component': -9.710482951877548, 'ionic_force_x': -4.718822101131082, 'ionic_force_y': 12.355452835559845, 'ionic_force_z': -11.77543318271637, 'radial_force': 13.225902494494164, 'axial_force': -11.77543318271637, 'contributions': [{'ion': 1308, 'force': [0.08313600718975067, 1.643194556236267, -3.1667728424072266], 'magnitude': 3.568676233291626, 'distance': 9.645294189453125, 'directional_contribution': -0.5177435774466472}, {'ion': 1320, 'force': [-0.023140454664826393, 0.592434823513031, -1.7460500001907349], 'magnitude': 1.8439644575119019, 'distance': 13.418153762817383, 'directional_contribution': -0.07625461900061781}, {'ion': 1460, 'force': [-4.778817653656006, 10.119823455810547, -6.862610340118408], 'magnitude': 13.127961158752441, 'distance': 5.028870105743408, 'directional_contribution': -9.11648447082684}]}, 4879: {'frame': 4879, 'ionic_force': [16.751477003097534, -3.802208073437214, -9.315209746360779], 'ionic_force_magnitude': 19.540775333586726, 'motion_vector': [1.0792694091796875, 2.2563400268554688, 0.31360626220703125], 'cosine_ionic_motion': 0.13356250676512846, 'ionic_motion_component': 2.6099149376880324, 'ionic_force_x': 16.751477003097534, 'ionic_force_y': -3.802208073437214, 'ionic_force_z': -9.315209746360779, 'radial_force': 17.177565835094814, 'axial_force': -9.315209746360779, 'contributions': [{'ion': 1308, 'force': [0.9992598295211792, -0.08213885873556137, -2.9084274768829346], 'magnitude': 3.0763967037200928, 'distance': 10.388381004333496, 'directional_contribution': -0.007522996143335625}, {'ion': 1320, 'force': [0.36823737621307373, -0.04548029601573944, -1.686635136604309], 'magnitude': 1.7269641160964966, 'distance': 13.865239143371582, 'directional_contribution': -0.09288104654053786}, {'ion': 1460, 'force': [15.383979797363281, -3.674588918685913, -4.720147132873535], 'magnitude': 16.50603675842285, 'distance': 4.484847068786621, 'directional_contribution': 2.7103190141106452}]}, 4880: {'frame': 4880, 'ionic_force': [11.858177244663239, 6.56685571372509, -19.13987958431244], 'ionic_force_magnitude': 23.453676727385687, 'motion_vector': [-0.8839454650878906, 1.5736312866210938, 0.37496185302734375], 'cosine_ionic_motion': -0.169418778362439, 'ionic_motion_component': -3.9734932592612493, 'ionic_force_x': 11.858177244663239, 'ionic_force_y': 6.56685571372509, 'ionic_force_z': -19.13987958431244, 'radial_force': 13.555071432151617, 'axial_force': -19.13987958431244, 'contributions': [{'ion': 1308, 'force': [1.1822991371154785, 0.5047712326049805, -2.458538770675659], 'magnitude': 2.7743537425994873, 'distance': 10.939264297485352, 'directional_contribution': -0.6361054945617823}, {'ion': 1320, 'force': [0.4902520775794983, 0.22216300666332245, -1.5701862573623657], 'magnitude': 1.6598759889602661, 'distance': 14.142663955688477, 'directional_contribution': -0.36481433416091846}, {'ion': 1460, 'force': [10.185626029968262, 5.839921474456787, -15.111154556274414], 'magnitude': 19.13631820678711, 'distance': 4.165238380432129, 'directional_contribution': -2.9725734479425796}]}, 4881: {'frame': 4881, 'ionic_force': [3.114603340625763, 12.471758097410202, -14.59370231628418], 'ionic_force_magnitude': 19.447921516349048, 'motion_vector': [0.3200035095214844, -2.01806640625, -2.126708984375], 'cosine_ionic_motion': 0.11968036629602533, 'ionic_motion_component': 2.3275343707730065, 'ionic_force_x': 3.114603340625763, 'ionic_force_y': 12.471758097410202, 'ionic_force_z': -14.59370231628418, 'radial_force': 12.854785257239971, 'axial_force': -14.59370231628418, 'contributions': [{'ion': 1308, 'force': [1.0287961959838867, 0.8844953179359436, -2.4416749477386475], 'magnitude': 2.7933008670806885, 'distance': 10.902100563049316, 'directional_contribution': 1.2671089138537504}, {'ion': 1320, 'force': [0.4618956446647644, 0.41249433159828186, -1.5808985233306885], 'magnitude': 1.6978631019592285, 'distance': 13.983558654785156, 'directional_contribution': 0.9078605109345066}, {'ion': 1460, 'force': [1.6239114999771118, 11.174768447875977, -10.571128845214844], 'magnitude': 15.468073844909668, 'distance': 4.63287878036499, 'directional_contribution': 0.15256490293600677}]}, 4882: {'frame': 4882, 'ionic_force': [2.9245057702064514, 1.4519258439540863, -13.961868047714233], 'ionic_force_magnitude': 14.33856973474329, 'motion_vector': [-5.703945159912109, -0.015411376953125, -1.0719757080078125], 'cosine_ionic_motion': -0.02087051426507955, 'ionic_motion_component': -0.2992533241897977, 'ionic_force_x': 2.9245057702064514, 'ionic_force_y': 1.4519258439540863, 'ionic_force_z': -13.961868047714233, 'radial_force': 3.2650915234205327, 'axial_force': -13.961868047714233, 'contributions': [{'ion': 1308, 'force': [0.6743703484535217, 0.30599769949913025, -2.060572385787964], 'magnitude': 2.1896045207977295, 'distance': 12.31363296508789, 'directional_contribution': -0.28298653249725403}, {'ion': 1460, 'force': [2.2501354217529297, 1.145928144454956, -11.90129566192627], 'magnitude': 12.166228294372559, 'distance': 5.2238545417785645, 'directional_contribution': -0.016266773147486813}]}, 4883: {'frame': 4883, 'ionic_force': [-3.27836936712265, 0.9993527233600616, -6.624387979507446], 'ionic_force_magnitude': 7.458480252438702, 'motion_vector': [1.4264259338378906, 0.6671638488769531, 5.739585876464844], 'cosine_ionic_motion': -0.9468419034633856, 'ionic_motion_component': -7.062001639163133, 'ionic_force_x': -3.27836936712265, 'ionic_force_y': 0.9993527233600616, 'ionic_force_z': -6.624387979507446, 'radial_force': 3.4273038343536655, 'axial_force': -6.624387979507446, 'contributions': [{'ion': 1308, 'force': [-0.274458110332489, 0.2523268163204193, -2.2293708324432373], 'magnitude': 2.2603297233581543, 'distance': 12.11945629119873, 'directional_contribution': -2.18741411319553}, {'ion': 1460, 'force': [-3.003911256790161, 0.7470259070396423, -4.395017147064209], 'magnitude': 5.3756585121154785, 'distance': 7.858745098114014, 'directional_contribution': -4.874587594102056}]}, 4884: {'frame': 4884, 'ionic_force': [-6.833262346684933, 17.534541964530945, -3.9410240650177], 'ionic_force_magnitude': 19.227202263604745, 'motion_vector': [0.24680328369140625, -1.6334991455078125, 0.6660842895507812], 'cosine_ionic_motion': -0.9622021441283682, 'ionic_motion_component': -18.500455243630302, 'ionic_force_x': -6.833262346684933, 'ionic_force_y': 17.534541964530945, 'ionic_force_z': -3.9410240650177, 'radial_force': 18.818970115405325, 'axial_force': -3.9410240650177, 'contributions': [{'ion': 1308, 'force': [-0.2761423885822296, 2.3214807510375977, -6.306930065155029], 'magnitude': 6.726283550262451, 'distance': 7.025568008422852, 'directional_contribution': -4.525572306611302}, {'ion': 1320, 'force': [-0.03301822394132614, 0.6696442365646362, -2.9598124027252197], 'magnitude': 3.0347986221313477, 'distance': 10.459335327148438, 'directional_contribution': -1.7254588325924702}, {'ion': 1460, 'force': [-6.524101734161377, 14.543416976928711, 5.325718402862549], 'magnitude': 16.805896759033203, 'distance': 4.4446563720703125, 'directional_contribution': -12.24942439985157}]}, 4885: {'frame': 4885, 'ionic_force': [8.870568364858627, 13.079958885908127, -2.2769949436187744], 'ionic_force_magnitude': 15.967373407857131, 'motion_vector': [-0.5143928527832031, -0.7691268920898438, 0.460906982421875], 'cosine_ionic_motion': -0.9495140680693623, 'ionic_motion_component': -15.161245680876982, 'ionic_force_x': 8.870568364858627, 'ionic_force_y': 13.079958885908127, 'ionic_force_z': -2.2769949436187744, 'radial_force': 15.804186393885566, 'axial_force': -2.2769949436187744, 'contributions': [{'ion': 1308, 'force': [-0.0231691375374794, 0.9201945662498474, -9.202110290527344], 'magnitude': 9.24803352355957, 'distance': 5.991621017456055, 'directional_contribution': -4.776063202192125}, {'ion': 1320, 'force': [-0.06408911198377609, 0.3074703514575958, -3.724951982498169], 'magnitude': 3.7381696701049805, 'distance': 9.424092292785645, 'directional_contribution': -1.857717956996175}, {'ion': 1460, 'force': [8.957826614379883, 11.852293968200684, 10.650067329406738], 'magnitude': 18.279590606689453, 'distance': 4.261728763580322, 'directional_contribution': -8.527464247766517}]}, 4886: {'frame': 4886, 'ionic_force': [-0.7766930758953094, 3.442865401506424, -11.02680230140686], 'ionic_force_magnitude': 11.5778643670301, 'motion_vector': [-0.024410247802734375, -0.002422332763671875, -0.506988525390625], 'cosine_ionic_motion': 0.9530979581087893, 'ionic_motion_component': 11.0348388874769, 'ionic_force_x': -0.7766930758953094, 'ionic_force_y': 3.442865401506424, 'ionic_force_z': -11.02680230140686, 'radial_force': 3.529387242430859, 'axial_force': -11.02680230140686, 'contributions': [{'ion': 1308, 'force': [-0.7440503835678101, -0.3250575363636017, -10.203084945678711], 'magnitude': 10.23534107208252, 'distance': 5.695316791534424, 'directional_contribution': 10.228495743685466}, {'ion': 1320, 'force': [-0.10336621850728989, -0.08003968000411987, -4.072631359100342], 'magnitude': 4.0747294425964355, 'distance': 9.026505470275879, 'directional_contribution': 4.073225276167847}, {'ion': 1460, 'force': [0.0707235261797905, 3.8479626178741455, 3.2489140033721924], 'magnitude': 5.03659200668335, 'distance': 8.118965148925781, 'directional_contribution': -3.2668823112096597}]}, 4887: {'frame': 4887, 'ionic_force': [-1.0733441188931465, 4.621083882637322, -10.55761456489563], 'ionic_force_magnitude': 11.574528463346974, 'motion_vector': [0.034473419189453125, 2.0418128967285156, 0.23172760009765625], 'cosine_ionic_motion': 0.29224284745935736, 'ionic_motion_component': 3.3825731561278998, 'ionic_force_x': -1.0733441188931465, 'ionic_force_y': 4.621083882637322, 'ionic_force_z': -10.55761456489563, 'radial_force': 4.744099898603837, 'axial_force': -10.55761456489563, 'contributions': [{'ion': 1308, 'force': [-0.7732217311859131, -0.015549938194453716, -10.2127685546875], 'magnitude': 10.242009162902832, 'distance': 5.693462371826172, 'directional_contribution': -1.179921637769379}, {'ion': 1320, 'force': [-0.3980359137058258, -0.11241107434034348, -3.6412546634674072], 'magnitude': 3.6646697521209717, 'distance': 9.518129348754883, 'directional_contribution': -0.5289111944347624}, {'ion': 1460, 'force': [0.09791352599859238, 4.749044895172119, 3.2964086532592773], 'magnitude': 5.7818098068237305, 'distance': 7.577695369720459, 'directional_contribution': 5.091406021042593}]}, 4888: {'frame': 4888, 'ionic_force': [-1.2431</t>
+          <t>{4857: {'frame': 4857, 'ionic_force': [-23.60623151063919, 0.16038507223129272, 2.653203248977661], 'ionic_force_magnitude': 23.755407320980098, 'motion_vector': [0.9804725646972656, -0.3909263610839844, 0.2857513427734375], 'cosine_ionic_motion': -0.8642116533491877, 'ionic_motion_component': -20.52969983684761, 'ionic_force_x': -23.60623151063919, 'ionic_force_y': 0.16038507223129272, 'ionic_force_z': 2.653203248977661, 'radial_force': 23.606776347169667, 'axial_force': 2.653203248977661, 'contributions': [{'ion': 1308, 'force': [-1.2521235942840576, 1.593077540397644, -2.4381844997406006], 'magnitude': 3.1702449321746826, 'distance': 10.233463287353516, 'cosine_with_motion': -0.7347405368026476, 'motion_component': -2.329307494535591}, {'ion': 1320, 'force': [-0.6172628998756409, 0.6778424382209778, -1.6455979347229004], 'magnitude': 1.8837400674819946, 'distance': 13.275734901428223, 'cosine_with_motion': -0.6507174342681865, 'motion_component': -1.2257824654629097}, {'ion': 1460, 'force': [-21.736845016479492, -2.110534906387329, 6.736985683441162], 'magnitude': 22.854578018188477, 'distance': 3.8113815784454346, 'cosine_with_motion': -0.7427224759895918, 'motion_component': -16.9746092376122}]}, 4858: {'frame': 4858, 'ionic_force': [-8.50262776017189, 3.199307382106781, 3.651916027069092], 'ionic_force_magnitude': 9.791156071782979, 'motion_vector': [-0.14766693115234375, 1.5113677978515625, -0.5906982421875], 'cosine_ionic_motion': 0.24656918258421606, 'ionic_motion_component': 2.414197349174013, 'ionic_force_x': -8.50262776017189, 'ionic_force_y': 3.199307382106781, 'ionic_force_z': 3.651916027069092, 'radial_force': 9.084615927668523, 'axial_force': 3.651916027069092, 'contributions': [{'ion': 1308, 'force': [-1.0608267784118652, 1.5705699920654297, -2.8913075923919678], 'magnitude': 3.4571235179901123, 'distance': 9.799673080444336, 'cosine_with_motion': 0.7523887522231089, 'motion_component': 2.6011008640142848}, {'ion': 1320, 'force': [-0.4662999212741852, 0.6704815030097961, -1.7270715236663818], 'magnitude': 1.9104337692260742, 'distance': 13.182660102844238, 'cosine_with_motion': 0.6753826513946052, 'motion_component': 1.2902738108900658}, {'ion': 1460, 'force': [-6.97550106048584, 0.9582558870315552, 8.270295143127441], 'magnitude': 10.861567497253418, 'distance': 5.5286970138549805, 'cosine_with_motion': -0.1360003780017847, 'motion_component': -1.4771773018897036}]}, 4859: {'frame': 4859, 'ionic_force': [-9.53341594338417, 13.158035159111023, 4.4725987911224365], 'ionic_force_magnitude': 16.85301304646511, 'motion_vector': [-0.5728759765625, -0.2980232238769531, -0.14586639404296875], 'cosine_ionic_motion': 0.07955984094930431, 'ionic_motion_component': 1.3408230374933148, 'ionic_force_x': -9.53341594338417, 'ionic_force_y': 13.158035159111023, 'ionic_force_z': 4.4725987911224365, 'radial_force': 16.248689448628568, 'axial_force': 4.4725987911224365, 'contributions': [{'ion': 1308, 'force': [-0.8318650126457214, 1.5506973266601562, -2.159569263458252], 'magnitude': 2.785749673843384, 'distance': 10.916866302490234, 'cosine_with_motion': 0.1786205972552863, 'motion_component': 0.49759226274005286}, {'ion': 1320, 'force': [-0.4241594970226288, 0.7252730131149292, -1.4648845195770264], 'magnitude': 1.6887328624725342, 'distance': 14.021308898925781, 'cosine_with_motion': 0.2151362361665056, 'motion_component': 0.36330764449495057}, {'ion': 1460, 'force': [-8.27739143371582, 10.882064819335938, 8.097052574157715], 'magnitude': 15.890148162841797, 'distance': 4.570935249328613, 'cosine_with_motion': 0.030202565824339556, 'motion_component': 0.47992324150436616}]}, 4860: {'frame': 4860, 'ionic_force': [-2.976147174835205, 6.678335726261139, -2.335963726043701], 'ionic_force_magnitude': 7.675568161923092, 'motion_vector': [0.6911888122558594, -0.11594009399414062, 0.5926361083984375], 'cosine_ionic_motion': -0.598417063639624, 'ionic_motion_component': -4.593190961223803, 'ionic_force_x': -2.976147174835205, 'ionic_force_y': 6.678335726261139, 'ionic_force_z': -2.335963726043701, 'radial_force': 7.311471813454215, 'axial_force': -2.335963726043701, 'contributions': [{'ion': 1308, 'force': [-0.9280287027359009, 1.4536443948745728, -2.190319776535034], 'magnitude': 2.7877984046936035, 'distance': 10.912854194641113, 'cosine_with_motion': -0.8238689283199169, 'motion_component': -2.2967804955902}, {'ion': 1320, 'force': [-0.4511340856552124, 0.7071818709373474, -1.4634768962860107], 'magnitude': 1.6868292093276978, 'distance': 14.029218673706055, 'cosine_with_motion': -0.8145641030190202, 'motion_component': -1.3740305233741053}, {'ion': 1460, 'force': [-1.5969843864440918, 4.517509460449219, 1.3178329467773438], 'magnitude': 4.969399929046631, 'distance': 8.173669815063477, 'cosine_with_motion': -0.18561192477866056, 'motion_component': -0.9223798648451975}]}, 4861: {'frame': 4861, 'ionic_force': [-2.949042022228241, 8.77355444431305, -2.55695903301239], 'ionic_force_magnitude': 9.60261141214706, 'motion_vector': [0.4648017883300781, 0.24734878540039062, -0.2841033935546875], 'cosine_ionic_motion': 0.2655944164048997, 'ionic_motion_component': 2.5503999739722283, 'ionic_force_x': -2.949042022228241, 'ionic_force_y': 8.77355444431305, 'ionic_force_z': -2.55695903301239, 'radial_force': 9.255922776049577, 'axial_force': -2.55695903301239, 'contributions': [{'ion': 1308, 'force': [-0.8082016706466675, 1.8407821655273438, -2.506990909576416], 'magnitude': 3.2135140895843506, 'distance': 10.164334297180176, 'cosine_with_motion': 0.41189868486252534, 'motion_component': 1.3236421976845847}, {'ion': 1320, 'force': [-0.4184555411338806, 0.7065335512161255, -1.485287070274353], 'magnitude': 1.6971659660339355, 'distance': 13.986430168151855, 'cosine_with_motion': 0.39614474603532723, 'motion_component': 0.672323388035597}, {'ion': 1460, 'force': [-1.7223848104476929, 6.22623872756958, 1.435318946838379], 'magnitude': 6.617612838745117, 'distance': 7.0830183029174805, 'cosine_with_motion': 0.0837816523417639, 'motion_component': 0.554434531374163}]}, 4862: {'frame': 4862, 'ionic_force': [-2.821112185716629, 16.71923440694809, -1.5727373361587524], 'ionic_force_magnitude': 17.02835799034726, 'motion_vector': [-0.7869873046875, 0.3434638977050781, -0.23621368408203125], 'cosine_ionic_motion': 0.5495663586687077, 'ionic_motion_component': 9.358212694862338, 'ionic_force_x': -2.821112185716629, 'ionic_force_y': 16.71923440694809, 'ionic_force_z': -1.5727373361587524, 'radial_force': 16.955573511942195, 'axial_force': -1.5727373361587524, 'contributions': [{'ion': 1308, 'force': [-0.5865727663040161, 1.652468204498291, -2.294264078140259], 'magnitude': 2.8876230716705322, 'distance': 10.722567558288574, 'cosine_with_motion': 0.6109457566715136, 'motion_component': 1.7641810025489164}, {'ion': 1320, 'force': [-0.32260993123054504, 0.7156185507774353, -1.465861201286316], 'magnitude': 1.6628097295761108, 'distance': 14.130182266235352, 'cosine_with_motion': 0.5712511650610931, 'motion_component': 0.9498819854370506}, {'ion': 1460, 'force': [-1.9119294881820679, 14.351147651672363, 2.1873879432678223], 'magnitude': 14.642252922058105, 'distance': 4.761733531951904, 'cosine_with_motion': 0.45376553288560995, 'motion_component': 6.644149834145949}]}, 4863: {'frame': 4863, 'ionic_force': [-3.69932222366333, 9.218546092510223, -2.963527649641037], 'ionic_force_magnitude': 10.36576447274449, 'motion_vector': [1.4510307312011719, -0.018299102783203125, -1.9164810180664062], 'cosine_ionic_motion': 0.005739696896891008, 'ionic_motion_component': 0.059496346178114605, 'ionic_force_x': -3.69932222366333, 'ionic_force_y': 9.218546092510223, 'ionic_force_z': -2.963527649641037, 'radial_force': 9.93310510234463, 'axial_force': -2.963527649641037, 'contributions': [{'ion': 1308, 'force': [-0.7104681134223938, 1.5558724403381348, -1.9979960918426514], 'magnitude': 2.630112648010254, 'distance': 11.235227584838867, 'cosine_with_motion': 0.4380751251609181, 'motion_component': 1.1521869135222806}, {'ion': 1320, 'force': [-0.3768095374107361, 0.7196657061576843, -1.397373080253601], 'magnitude': 1.6163402795791626, 'distance': 14.331863403320312, 'cosine_with_motion': 0.5451289495529077, 'motion_component': 0.8811138419875748}, {'ion': 1460, 'force': [-2.6120445728302, 6.943007946014404, 0.43184152245521545], 'magnitude': 7.430654048919678, 'distance': 6.684293746948242, 'cosine_with_motion': -0.2656299511950648, 'motion_component': -1.9738043384000463}]}, 4864: {'frame': 4864, 'ionic_force': [-3.9271629452705383, 6.102272391319275, -2.3661776781082153], 'ionic_force_magnitude': 7.63276712214784, 'motion_vector': [-1.0789031982421875, -0.15365219116210938, 2.0991592407226562], 'cosine_ionic_motion': -0.09237188980147616, 'ionic_motion_component': -0.7050531234873706, 'ionic_force_x': -3.9271629452705383, 'ionic_force_y': 6.102272391319275, 'ionic_force_z': -2.3661776781082153, 'radial_force': 7.256744251836593, 'axial_force': -2.3661776781082153, 'contributions': [{'ion': 1308, 'force': [-0.32004624605178833, 1.0951236486434937, -1.809603214263916], 'magnitude': 2.139249563217163, 'distance': 12.457712173461914, 'cosine_with_motion': -0.7157728839742278, 'motion_component': -1.5312169138518108}, {'ion': 1460, 'force': [-3.60711669921875, 5.007148742675781, -0.5565744638442993], 'magnitude': 6.196176528930664, 'distance': 7.319933891296387, 'cosine_with_motion': 0.13333443679738946, 'motion_component': 0.8261637182101396}]}, 4865: {'frame': 4865, 'ionic_force': [-3.168602854013443, 5.503656804561615, -3.0944536328315735], 'ionic_force_magnitude': 7.064412612142925, 'motion_vector': [3.705402374267578, -1.9471969604492188, -2.8583602905273438], 'cosine_ionic_motion': -0.3801608278025133, 'ionic_motion_component': -2.6856129465707697, 'ionic_force_x': -3.168602854013443, 'ionic_force_y': 5.503656804561615, 'ionic_force_z': -3.0944536328315735, 'radial_force': 6.350612747511811, 'axial_force': -3.0944536328315735, 'contributions': [{'ion': 1308, 'force': [-0.8212441205978394, 1.7357362508773804, -2.2392847537994385], 'magnitude': 2.949850559234619, 'distance': 10.608867645263672, 'cosine_with_motion': -0.0014832429453785205, 'motion_component': -0.004375345063333924}, {'ion': 1320, 'force': [-0.41535165905952454, 0.8550887703895569, -1.5833065509796143], 'magnitude': 1.8467683792114258, 'distance': 13.407963752746582, 'cosine_with_motion': 0.14118443913662393, 'motion_component': 0.26073495759911935}, {'ion': 1460, 'force': [-1.932007074356079, 2.9128317832946777, 0.7281376719474792], 'magnitude': 3.5703535079956055, 'distance': 9.643028259277344, 'cosine_with_motion': -0.8240002960827033, 'motion_component': -2.9419724204515667}]}, 4866: {'frame': 4866, 'ionic_force': [-7.758470341563225, 11.393471777439117, -3.07043993473053], 'ionic_force_magnitude': 14.122062971712237, 'motion_vector': [-0.006435394287109375, 0.24068450927734375, 0.5570297241210938], 'cosine_ionic_motion': 0.12623792979283582, 'ionic_motion_component': 1.782739993953016, 'ionic_force_x': -7.758470341563225, 'ionic_force_y': 11.393471777439117, 'ionic_force_z': -3.07043993473053, 'radial_force': 13.784232339315013, 'axial_force': -3.07043993473053, 'contributions': [{'ion': 1308, 'force': [0.049068644642829895, 0.7890864014625549, -2.0871825218200684], 'magnitude': 2.2319042682647705, 'distance': 12.196389198303223, 'cosine_with_motion': -0.7184098472140821, 'motion_component': -1.603421891308001}, {'ion': 1460, 'force': [-7.807538986206055, 10.604385375976562, -0.9832574129104614], 'magnitude': 13.205204963684082, 'distance': 5.0141401290893555, 'cosine_with_motion': 0.25642628453809563, 'motion_component': 3.386161754441588}]}, 4867: {'frame': 4867, 'ionic_force': [0.12337589636445045, 4.056435167789459, -4.2135396003723145], 'ionic_force_magnitude': 5.850111438783753, 'motion_vector': [-0.9177093505859375, 0.6418495178222656, 2.0229339599609375], 'cosine_ionic_motion': -0.44602597766328916, 'ionic_motion_component': -2.609301673922715, 'ionic_force_x': 0.12337589636445045, 'ionic_force_y': 4.056435167789459, 'ionic_force_z': -4.2135396003723145, 'radial_force': 4.058310964216866, 'axial_force': -4.2135396003723145, 'contributions': [{'ion': 1308, 'force': [0.09774009138345718, 0.9288542866706848, -2.069882869720459], 'magnitude': 2.270845413208008, 'distance': 12.091362953186035, 'cosine_with_motion': -0.7009982594382919, 'motion_component': -1.5918586226891804}, {'ion': 1460, 'force': [0.02563580498099327, 3.1275808811187744, -2.1436567306518555], 'magnitude': 3.7917916774749756, 'distance': 9.357219696044922, 'cosine_with_motion': -0.2683278059184076, 'motion_component': -1.0174431206508086}]}, 4868: {'frame': 4868, 'ionic_force': [-1.2063874416053295, 6.333217084407806, -5.534350037574768], 'ionic_force_magnitude': 8.496707576226324, 'motion_vector': [0.3851051330566406, 2.4810562133789062, 0.2808074951171875], 'cosine_ionic_motion': 0.6379499331499946, 'ionic_motion_component': 5.420474030248636, 'ionic_force_x': -1.2063874416053295, 'ionic_force_y': 6.333217084407806, 'ionic_force_z': -5.534350037574768, 'radial_force': 6.447093088943107, 'axial_force': -5.534350037574768, 'contributions': [{'ion': 1308, 'force': [-0.13308840990066528, 1.483996033668518, -2.676917314529419], 'magnitude': 3.0636322498321533, 'distance': 10.40999984741211, 'cosine_with_motion': 0.37195321146052107, 'motion_component': 1.1395278843755534}, {'ion': 1320, 'force': [-0.05506179854273796, 0.6272523999214172, -1.598051905632019], 'magnitude': 1.7176283597946167, 'distance': 13.90286922454834, 'cosine_with_motion': 0.25033097015726313, 'motion_component': 0.4299755799140038}, {'ion': 1460, 'force': [-1.0182372331619263, 4.221968650817871, -1.25938081741333], 'magnitude': 4.5219316482543945, 'distance': 8.568544387817383, 'cosine_with_motion': 0.851620709199047, 'motion_component': 3.8509706902766823}]}, 4869: {'frame': 4869, 'ionic_force': [0.0542104747146368, 5.165193021297455, -3.881076753139496], 'ionic_force_magnitude': 6.461030450832787, 'motion_vector': [-0.0664825439453125, -0.035305023193359375, -0.05754852294921875], 'cosine_ionic_motion': 0.06107260201521054, 'ionic_motion_component': 0.39459194133186715, 'ionic_force_x': 0.0542104747146368, 'ionic_force_y': 5.165193021297455, 'ionic_force_z': -3.881076753139496, 'radial_force': 5.165477492239098, 'axial_force': -3.881076753139496, 'contributions': [{'ion': 1308, 'force': [-0.011133236810564995, 1.6809277534484863, -1.8282040357589722], 'magnitude': 2.4835402965545654, 'distance': 11.562012672424316, 'cosine_with_motion': 0.19804797994433204, 'motion_component': 0.49186012500856546}, {'ion': 1320, 'force': [0.029794860631227493, 0.8571366667747498, -1.3412694931030273], 'magnitude': 1.5920348167419434, 'distance': 14.440850257873535, 'cosine_with_motion': 0.2979502960962926, 'motion_component': 0.47434724454418253}, {'ion': 1460, 'force': [0.035548850893974304, 2.6271286010742188, -0.7116032242774963], 'magnitude': 2.7220301628112793, 'distance': 11.043903350830078, 'cosine_with_motion': -0.20999599232849375, 'motion_component': -0.5716154000736449}]}, 4870: {'frame': 4870, 'ionic_force': [-0.09000088274478912, 4.857101559638977, -3.782764494419098], 'ionic_force_magnitude': 6.157015749515344, 'motion_vector': [-0.150634765625, -2.8217086791992188, -4.534019470214844], 'cosine_ionic_motion': 0.10516778943237615, 'ionic_motion_component': 0.6475197358768533, 'ionic_force_x': -0.09000088274478912, 'ionic_force_y': 4.857101559638977, 'ionic_force_z': -3.782764494419098, 'radial_force': 4.85793533505153, 'axial_force': -3.782764494419098, 'contributions': [{'ion': 1308, 'force': [-0.0317416787147522, 1.5285658836364746, -1.7929517030715942], 'magnitude': 2.3563101291656494, 'distance': 11.870057106018066, 'cosine_with_motion': 0.30352157353261566, 'motion_component': 0.7151909310539509}, {'ion': 1320, 'force': [-0.024010654538869858, 0.8109053373336792, -1.3013789653778076], 'magnitude': 1.5335354804992676, 'distance': 14.71370792388916, 'cosine_with_motion': 0.44135347987078855, 'motion_component': 0.6768312379802743}, {'ion': 1460, 'force': [-0.03424854949116707, 2.5176303386688232, -0.688433825969696], 'magnitude': 2.6102828979492188, 'distance': 11.277822494506836, 'cosine_with_motion': -0.28521913588366826, 'motion_component': -0.7445026222250654}]}, 4871: {'frame': 4871, 'ionic_force': [-1.4377694465219975, 2.7718199491500854, -5.007754564285278], 'ionic_force_magnitude': 5.901505959327551, 'motion_vector': [-0.12489700317382812, -0.5373611450195312, 0.7347412109375], 'cosine_ionic_motion': -0.9201397059694539, 'ionic_motion_component': -5.430209958192633, 'ionic_force_x': -1.4377694465219975, 'ionic_force_y': 2.7718199491500854, 'ionic_force_z': -5.007754564285278, 'radial_force': 3.122525710359893, 'axial_force': -5.007754564285278, 'contributions': [{'ion': 1308, 'force': [-0.03414252772927284, 0.5607947111129761, -1.570929765701294], 'magnitude': 1.6683754920959473, 'distance': 14.106593132019043, 'cosine_with_motion': -0.9467690197126633, 'motion_component': -1.579566219617024}, {'ion': 1460, 'force': [-1.4036269187927246, 2.2110252380371094, -3.4368247985839844], 'magnitude': 4.3209452629089355, 'distance': 8.765560150146484, 'cosine_with_motion': -0.8911577797428331, 'motion_component': -3.8506437663609603}]}, 4872: {'frame': 4872, 'ionic_force': [-1.5672330230518128, 3.253392219543457, -6.297172904014587], 'ionic_force_magnitude': 7.259143673036479, 'motion_vector': [1.6905479431152344, -0.46477508544921875, 1.652435302734375], 'cosine_ionic_motion': -0.8329315936526057, 'ionic_motion_component': -6.046370108135505, 'ionic_force_x': -1.5672330230518128, 'ionic_force_y': 3.253392219543457, 'ionic_force_z': -6.297172904014587, 'radial_force': 3.6112020550960624, 'axial_force': -6.297172904014587, 'contributions': [{'ion': 1308, 'force': [2.390443842159584e-05, 0.5934185981750488, -1.8552712202072144], 'magnitude': 1.9478647708892822, 'distance': 13.055383682250977, 'cosine_with_motion': -0.7120286142675283, 'motion_component': -1.3869354112101064}, {'ion': 1460, 'force': [-1.5672569274902344, 2.659973621368408, -4.441901683807373], 'magnitude': 5.409458637237549, 'distance': 7.8341546058654785, 'cosine_with_motion': -0.861349512827743, 'motion_component': -4.659434702269067}]}, 4873: {'frame': 4873, 'ionic_force': [-1.6994890123605728, 6.724162369966507, -11.125696539878845], 'ionic_force_magnitude': 13.110444156407517, 'motion_vector': [-1.8945083618164062, 4.309528350830078, 0.9468460083007812], 'cosine_ionic_motion': 0.34411208913073765, 'ionic_motion_component': 4.511462328093263, 'ionic_force_x': -1.6994890123605728, 'ionic_force_y': 6.724162369966507, 'ionic_force_z': -11.125696539878845, 'radial_force': 6.935605415593358, 'axial_force': -11.125696539878845, 'contributions': [{'ion': 1308, 'force': [0.2984895706176758, 0.8108097314834595, -2.3136789798736572], 'magnitude': 2.469740629196167, 'distance': 11.594268798828125, 'cosine_with_motion': 0.06223117700292426, 'motion_component': 0.153694867391323}, {'ion': 1320, 'force': [0.10234962403774261, 0.38926997780799866, -1.4215017557144165], 'magnitude': 1.477387547492981, 'distance': 14.990696907043457, 'cosine_with_motion': 0.019413726224842758, 'motion_component': 0.028681596305214274}, {'ion': 1460, 'force': [-2.100328207015991, 5.524082660675049, -7.3905158042907715], 'magnitude': 9.462905883789062, 'distance': 5.923205375671387, 'cosine_with_motion': 0.4574795577949567, 'motion_component': 4.329086093616461}]}, 4874: {'frame': 4874, 'ionic_force': [-1.8247650638222694, 5.6435387134552, -3.796484112739563], 'ionic_force_magnitude': 7.0422005343995835, 'motion_vector': [1.5041236877441406, -3.0937538146972656, -1.0170440673828125], 'cosine_ionic_motion': -0.6469517009967339, 'ionic_motion_component': -4.55596361448992, 'ionic_force_x': -1.8247650638222694, 'ionic_force_y': 5.6435387134552, 'ionic_force_z': -3.796484112739563, 'radial_force': 5.931213766878907, 'axial_force': -3.796484112739563, 'contributions': [{'ion': 1308, 'force': [-0.06882379204034805, 1.2181742191314697, -1.544019103050232], 'magnitude': 1.9679126739501953, 'distance': 12.988713264465332, 'cosine_with_motion': -0.3260818599535824, 'motion_component': -0.641700611758041}, {'ion': 1460, 'force': [-1.7559412717819214, 4.4253644943237305, -2.252465009689331], 'magnitude': 5.266951560974121, 'distance': 7.939431190490723, 'cosine_with_motion': -0.7431742677572718, 'motion_component': -3.9142629071584913}]}, 4875: {'frame': 4875, 'ionic_force': [-1.1494073271751404, 5.382365703582764, -6.437063932418823], 'ionic_force_magnitude': 8.469167009860838, 'motion_vector': [-4.102687835693359, -0.4046134948730469, 2.7181549072265625], 'cosine_ionic_motion': -0.35769251277853253, 'ionic_motion_component': -3.029357628898174, 'ionic_force_x': -1.1494073271751404, 'ionic_force_y': 5.382365703582764, 'ionic_force_z': -6.437063932418823, 'radial_force': 5.5037258081110725, 'axial_force': -6.437063932418823, 'contributions': [{'ion': 1308, 'force': [0.1549651026725769, 0.9382805824279785, -2.0105345249176025], 'magnitude': 2.2241029739379883, 'distance': 12.21776008605957, 'cosine_with_motion': -0.5900523524559439, 'motion_component': -1.3123371483160682}, {'ion': 1460, 'force': [-1.3043724298477173, 4.444085121154785, -4.426529407501221], 'magnitude': 6.406671524047852, 'distance': 7.198678970336914, 'cosine_with_motion': -0.26800505197085495, 'motion_component': -1.7170203886894198}]}, 4876: {'frame': 4876, 'ionic_force': [-5.890000581741333, 6.048319339752197, -6.3055113554000854], 'ionic_force_magnitude': 10.537255199605498, 'motion_vector': [5.018623352050781, -2.8053436279296875, -2.0750503540039062], 'cosine_ionic_motion': -0.519231764832483, 'ionic_motion_component': -5.471277613781421, 'ionic_force_x': -5.890000581741333, 'ionic_force_y': 6.048319339752197, 'ionic_force_z': -6.3055113554000854, 'radial_force': 8.442409234841302, 'axial_force': -6.3055113554000854, 'contributions': [{'ion': 1308, 'force': [-1.146353840827942, 1.7300130128860474, -2.72662091255188], 'magnitude': 3.4265921115875244, 'distance': 9.84323501586914, 'cosine_with_motion': -0.23626317181720632, 'motion_component': -0.8095775295885126}, {'ion': 1320, 'force': [-0.5717068910598755, 0.7419012784957886, -1.8075217008590698], 'magnitude': 2.035780191421509, 'distance': 12.770373344421387, 'cosine_with_motion': -0.09641626228940431, 'motion_component': -0.19628231660630036}, {'ion': 1460, 'force': [-4.171939849853516, 3.5764050483703613, -1.7713687419891357], 'magnitude': 5.773517608642578, 'distance': 7.58313512802124, 'cosine_with_motion': -0.7734311038664372, 'motion_component': -4.465417884486193}]}, 4877: {'frame': 4877, 'ionic_force': [-1.2858441323041916, 6.905015721917152, -19.02397847175598], 'ionic_force_magnitude': 20.27916157404786, 'motion_vector': [-1.6677970886230469, 2.3718338012695312, 1.7540283203125], 'cosine_ionic_motion': -0.2160392511374309, 'ionic_motion_component': -4.381094880152263, 'ionic_force_x': -1.2858441323041916, 'ionic_force_y': 6.905015721917152, 'ionic_force_z': -19.02397847175598, 'radial_force': 7.023719616592349, 'axial_force': -19.02397847175598, 'contributions': [{'ion': 1308, 'force': [0.548943817615509, 0.45097389817237854, -2.8554723262786865], 'magnitude': 2.9425225257873535, 'distance': 10.622069358825684, 'cosine_with_motion': -0.48683309000334857, 'motion_component': -1.4325173471264652}, {'ion': 1320, 'force': [0.22946275770664215, 0.1839812844991684, -1.6267189979553223], 'magnitude': 1.6530932188034058, 'distance': 14.171648979187012, 'cosine_with_motion': -0.49976073485214356, 'motion_component': -0.826151048322767}, {'ion': 1460, 'force': [-2.0642507076263428, 6.2700605392456055, -14.541787147521973], 'magnitude': 15.96992015838623, 'distance': 4.559504508972168, 'cosine_with_motion': -0.13290148720347839, 'motion_component': -2.122426196693901}]}, 4878: {'frame': 4878, 'ionic_force': [-4.718822101131082, 12.355452835559845, -11.77543318271637], 'ionic_force_magnitude': 17.70834050481537, 'motion_vector': [3.3215065002441406, -4.6515045166015625, -1.365631103515625], 'cosine_ionic_motion': -0.5483564622691216, 'ionic_motion_component': -9.710482951877548, 'ionic_force_x': -4.718822101131082, 'ionic_force_y': 12.355452835559845, 'ionic_force_z': -11.77543318271637, 'radial_force': 13.225902494494164, 'axial_force': -11.77543318271637, 'contributions': [{'ion': 1308, 'force': [0.08313600718975067, 1.643194556236267, -3.1667728424072266], 'magnitude': 3.568676233291626, 'distance': 9.645294189453125, 'cosine_with_motion': -0.14508000757337663, 'motion_component': -0.5177435774466472}, {'ion': 1320, 'force': [-0.023140454664826393, 0.592434823513031, -1.7460500001907349], 'magnitude': 1.8439644575119019, 'distance': 13.418153762817383, 'cosine_with_motion': -0.04135362622311115, 'motion_component': -0.07625461900061781}, {'ion': 1460, 'force': [-4.778817653656006, 10.119823455810547, -6.862610340118408], 'magnitude': 13.127961158752441, 'distance': 5.028870105743408, 'cosine_with_motion': -0.6944326580126445, 'motion_component': -9.11648447082684}]}, 4879: {'frame': 4879, 'ionic_force': [16.751477003097534, -3.802208073437214, -9.315209746360779], 'ionic_force_magnitude': 19.540775333586726, 'motion_vector': [1.0792694091796875, 2.2563400268554688, 0.31360626220703125], 'cosine_ionic_motion': 0.13356250676512846, 'ionic_motion_component': 2.6099149376880324, 'ionic_force_x': 16.751477003097534, 'ionic_force_y': -3.802208073437214, 'ionic_force_z': -9.315209746360779, 'radial_force': 17.177565835094814, 'axial_force': -9.315209746360779, 'contributions': [{'ion': 1308, 'force': [0.9992598295211792, -0.08213885873556137, -2.9084274768829346], 'magnitude': 3.0763967037200928, 'distance': 10.388381004333496, 'cosine_with_motion': -0.0024453919914148078, 'motion_component': -0.007522996143335624}, {'ion': 1320, 'force': [0.36823737621307373, -0.04548029601573944, -1.686635136604309], 'magnitude': 1.7269641160964966, 'distance': 13.865239143371582, 'cosine_with_motion': -0.05378284459316496, 'motion_component': -0.09288104654053786}, {'ion': 1460, 'force': [15.383979797363281, -3.674588918685913, -4.720147132873535], 'magnitude': 16.50603675842285, 'distance': 4.484847068786621, 'cosine_with_motion': 0.16420168966862303, 'motion_component': 2.7103190141106452}]}, 4880: {'frame': 4880, 'ionic_force': [11.858177244663239, 6.56685571372509, -19.13987958431244], 'ionic_force_magnitude': 23.453676727385687, 'motion_vector': [-0.8839454650878906, 1.5736312866210938, 0.37496185302734375], 'cosine_ionic_motion': -0.169418778362439, 'ionic_motion_component': -3.9734932592612493, 'ionic_force_x': 11.858177244663239, 'ionic_force_y': 6.56685571372509, 'ionic_force_z': -19.13987958431244, 'radial_force': 13.555071432151617, 'axial_force': -19.13987958431244, 'contributions': [{'ion': 1308, 'force': [1.1822991371154785, 0.5047712326049805, -2.458538770675659], 'magnitude': 2.7743537425994873, 'distance': 10.939264297485352, 'cosine_with_motion': -0.22928060965663458, 'motion_component': -0.6361054945617823}, {'ion': 1320, 'force': [0.4902520775794983, 0.22216300666332245, -1.5701862573623657], 'magnitude': 1.6598759889602661, 'distance': 14.142663955688477, 'cosine_with_motion': -0.2197840868520927, 'motion_component': -0.36481433416091846}, {'ion': 1460, 'force': [10.185626029968262, 5.839921474456787, -15.111154556274414], 'magnitude': 19.13631820678711, 'distance': 4.165238380432129, 'cosine_with_motion': -0.15533675314471485, 'motion_component': -2.972573447942579}]}, 4881: {'frame': 4881, 'ionic_force': [3.114603340625763, 12.471758097410202, -14.59370231628418], 'ionic_force_magnitude': 19.447921516349048, 'motion_vector': [0.3200035095214844, -2.01806640625, -2.126708984375], 'cosine_ionic_motion': 0.11968036629602533, 'ionic_motion_component': 2.3275343707730065, 'ionic_force_x': 3.114603340625763, 'ionic_force_y': 12.471758097410202, 'ionic_force_z': -14.59370231628418, 'radial_force': 12.854785257239971, 'axial_force': -14.59370231628418, 'contributions': [{'ion': 1308, 'force': [1.0287961959838867, 0.8844953179359436, -2.4416749477386475], 'magnitude': 2.7933008670806885, 'distance': 10.902100563049316, 'cosine_with_motion': 0.45362420374227375, 'motion_component': 1.2671089138537504}, {'ion': 1320, 'force': [0.4618956446647644, 0.41249433159828186, -1.5808985233306885], 'magnitude': 1.6978631019592285, 'distance': 13.983558654785156, 'cosine_with_motion': 0.53470770419971, 'motion_component': 0.9078605109345066}, {'ion': 1460, 'force': [1.6239114999771118, 11.174768447875977, -10.571128845214844], 'magnitude': 15.468073844909668, 'distance': 4.63287878036499, 'cosine_with_motion': 0.009863212837963545, 'motion_component': 0.15256490293600677}]}, 4882: {'frame': 4882, 'ionic_force': [2.9245057702064514, 1.4519258439540863, -13.961868047714233], 'ionic_force_magnitude': 14.33856973474329, 'motion_vector': [-5.703945159912109, -0.015411376953125, -1.0719757080078125], 'cosine_ionic_motion': -0.02087051426507955, 'ionic_motion_component': -0.2992533241897977, 'ionic_force_x': 2.9245057702064514, 'ionic_force_y': 1.4519258439540863, 'ionic_force_z': -13.961868047714233, 'radial_force': 3.2650915234205327, 'axial_force': -13.961868047714233, 'contributions': [{'ion': 1308, 'force': [0.6743703484535217, 0.30599769949913025, -2.060572385787964], 'magnitude': 2.1896045207977295, 'distance': 12.31363296508789, 'cosine_with_motion': -0.12924092607834214, 'motion_component': -0.28298653249725403}, {'ion': 1460, 'force': [2.2501354217529297, 1.145928144454956, -11.90129566192627], 'magnitude': 12.166228294372559, 'distance': 5.2238545417785645, 'cosine_with_motion': -0.0013370432807549883, 'motion_component': -0.016266773147486813}]}, 4883: {'frame': 4883, 'ionic_force': [-3.27836936712265, 0.9993527233600616, -6.624387979507446], 'ionic_force_magnitude': 7.458480252438702, 'motion_vector': [1.4264259338378906, 0.6671638488769531, 5.739585876464844], 'cosine_ionic_motion': -0.9468419034633856, 'ionic_motion_component': -7.062001639163133, 'ionic_force_x': -3.27836936712265, 'ionic_force_y': 0.9993527233600616, 'ionic_force_z': -6.624387979507446, 'radial_force': 3.4273038343536655, 'axial_force': -6.624387979507446, 'contributions': [{'ion': 1308, 'force': [-0.274458110332489, 0.2523268163204193, -2.2293708324432373], 'magnitude': 2.2603297233581543, 'distance': 12.11945629119873, 'cosine_with_motion': -0.9677411690240902, 'motion_component': -2.18741411319553}, {'ion': 1460, 'force': [-3.003911256790161, 0.7470259070396423, -4.395017147064209], 'magnitude': 5.3756585121154785, 'distance': 7.858745098114014, 'cosine_with_motion': -0.9067888945866973, 'motion_component': -4.874587594102056}]}, 4884: {'frame': 4884, 'ionic_force': [-6.833262346684933, 17.534541964530945, -3.9410240650177], 'ionic_force_magnitude': 19.227202263604745, 'motion_vector': [0.24680328369140625, -1.6334991455078125, 0.6660842895507812], 'cosine_ionic_motion': -0.9622021441283682, 'ionic_motion_component': -18.500455243630302, 'ionic_force_x': -6.833262346684933, 'ionic_force_y': 17.534541964530945, 'ionic_force_z': -3.9410240650177, 'radial_force': 18.818970115405325, 'axial_force': -3.9410240650177, 'contributions': [{'ion': 1308, 'force': [-0.2761423885822296, 2.3214807510375977, -6.306930065155029], 'magnitude': 6.726283550262451, 'distance': 7.025568008422852, 'cosine_with_motion': -0.6728191096191648, 'motion_component': -4.525572306611302}, {'ion': 1320, 'force': [-0.03301822394132614, 0.6696442365646362, -2.9598124027252197], 'magnitude': 3.0347986221313477, 'distance': 10.459335327148438, 'cosine_with_motion': -0.5685579212934188, 'motion_component': -1.7254588325924702}, {'ion': 1460, 'force': [-6.524101734161377, 14.543416976928711, 5.325718402862549], 'magnitude': 16.805896759033203, 'distance': 4.4446563720703125, 'cosine_with_motion': -0.7288765819072703, 'motion_component': -12.24942439985157}]}, 4885: {'frame': 4885, 'ionic_force': [8.870568364858627, 13.079958885908127, -2.2769949436187744], 'ionic_force_magnitude': 15.967373407857131, 'motion_vector': [-0.5143928527832031, -0.7691268920898438, 0.460906982421875], 'cosine_ionic_motion': -0.9495140680693623, 'ionic_motion_component': -15.161245680876982, 'ionic_force_x': 8.870568364858627, 'ionic_force_y': 13.079958885908127, 'ionic_force_z': -2.2769949436187744, 'radial_force': 15.804186393885566, 'axial_force': -2.2769949436187744, 'contributions': [{'ion': 1308, 'force': [-0.0231691375374794, 0.9201945662498474, -9.202110290527344], 'magnitude': 9.24803352355957, 'distance': 5.991621017456055, 'cosine_with_motion': -0.5164409343596666, 'motion_component': -4.776063202192125}, {'io</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{4992: {'frame': 4992, 'ionic_force': [-9.90977567434311, -3.2852199375629425, -0.025440236553549767], 'ionic_force_magnitude': 10.440161452755383, 'motion_vector': [1.30914306640625, -2.567424774169922, 0.49839019775390625], 'cosine_ionic_motion': -0.14905922879596165, 'ionic_motion_component': -1.556202414653044, 'ionic_force_x': -9.90977567434311, 'ionic_force_y': -3.2852199375629425, 'ionic_force_z': -0.025440236553549767, 'radial_force': 10.440130456750216, 'axial_force': -0.025440236553549767, 'contributions': [{'ion': 1309, 'force': [-0.8666126132011414, -0.2845568358898163, -1.5572242736816406], 'magnitude': 1.8046987056732178, 'distance': 13.56334114074707, 'directional_contribution': -0.4034750869979291}, {'ion': 1316, 'force': [-3.8274505138397217, -1.5964282751083374, 4.4594645500183105], 'magnitude': 6.089727878570557, 'distance': 7.383633136749268, 'directional_contribution': 0.44810709179433417}, {'ion': 1320, 'force': [-3.069931983947754, -1.0022555589675903, -2.9554810523986816], 'magnitude': 4.377655506134033, 'distance': 8.708598136901855, 'directional_contribution': -0.9979618179615599}, {'ion': 1460, 'force': [-2.145780563354492, -0.4019792675971985, 0.027800539508461952], 'magnitude': 2.1832852363586426, 'distance': 12.331439971923828, 'directional_contribution': -0.602872663331882}]}, 4993: {'frame': 4993, 'ionic_force': [-6.721731662750244, -7.0382163524627686, 0.02508533000946045], 'ionic_force_magnitude': 9.732358154315692, 'motion_vector': [-1.2147407531738281, 0.47171783447265625, 0.3584442138671875], 'cosine_ionic_motion': 0.3690367022768285, 'ionic_motion_component': 3.5915973586456644, 'ionic_force_x': -6.721731662750244, 'ionic_force_y': -7.0382163524627686, 'ionic_force_z': 0.02508533000946045, 'radial_force': 9.732325825315009, 'axial_force': 0.02508533000946045, 'contributions': [{'ion': 1309, 'force': [-0.767593502998352, -0.664334774017334, -1.574743628501892], 'magnitude': 1.873594880104065, 'distance': 13.311628341674805, 'directional_contribution': 0.040392239910257643}, {'ion': 1316, 'force': [-0.9619420766830444, -1.5705485343933105, 2.251835346221924], 'magnitude': 2.9090750217437744, 'distance': 10.68295955657959, 'directional_contribution': 0.9136495223597336}, {'ion': 1320, 'force': [-2.390256643295288, -2.211256742477417, -2.6654586791992188], 'magnitude': 4.2080464363098145, 'distance': 8.882369041442871, 'directional_contribution': 0.6696440311311278}, {'ion': 1460, 'force': [-2.6019394397735596, -2.592076301574707, 2.0134522914886475], 'magnitude': 4.18842887878418, 'distance': 8.903144836425781, 'directional_contribution': 1.9679114067019796}]}, 4994: {'frame': 4994, 'ionic_force': [-8.510059118270874, -4.980317711830139, -0.8486621975898743], 'ionic_force_magnitude': 9.89671148578417, 'motion_vector': [0.4574928283691406, 1.3063774108886719, 0.06430816650390625], 'cosine_ionic_motion': -0.762318113348161, 'ionic_motion_component': -7.544442428194064, 'ionic_force_x': -8.510059118270874, 'ionic_force_y': -4.980317711830139, 'ionic_force_z': -0.8486621975898743, 'radial_force': 9.860257131902506, 'axial_force': -0.8486621975898743, 'contributions': [{'ion': 1309, 'force': [-0.9202994108200073, -0.567900538444519, -1.5354427099227905], 'magnitude': 1.8780431747436523, 'distance': 13.295854568481445, 'directional_contribution': -0.9105142778132502}, {'ion': 1316, 'force': [-1.8541682958602905, -1.3925756216049194, 2.6088037490844727], 'magnitude': 3.490424633026123, 'distance': 9.752813339233398, 'directional_contribution': -1.8039984403479075}, {'ion': 1320, 'force': [-2.610811948776245, -1.7711108922958374, -2.3384480476379395], 'magnitude': 3.927023410797119, 'distance': 9.194694519042969, 'directional_contribution': -2.640290627803788}, {'ion': 1460, 'force': [-3.124779462814331, -1.2487306594848633, 0.41642481088638306], 'magnitude': 3.3907203674316406, 'distance': 9.89516544342041, 'directional_contribution': -2.189639274119873}]}, 4995: {'frame': 4995, 'ionic_force': [-7.9496631026268005, -3.4401994943618774, -2.7620067689567804], 'ionic_force_magnitude': 9.091798358852705, 'motion_vector': [0.29911041259765625, -1.0097732543945312, -0.8112640380859375], 'cosine_ionic_motion': 0.2760697449015972, 'ionic_motion_component': 2.5099704536252263, 'ionic_force_x': -7.9496631026268005, 'ionic_force_y': -3.4401994943618774, 'ionic_force_z': -2.7620067689567804, 'radial_force': 8.662108057873308, 'axial_force': -2.7620067689567804, 'contributions': [{'ion': 1309, 'force': [-0.9697037935256958, -0.4882330298423767, -1.6673376560211182], 'magnitude': 1.989651083946228, 'distance': 12.917562484741211, 'directional_contribution': 1.1701726210799208}, {'ion': 1316, 'force': [-0.7669690251350403, -0.3876888155937195, 1.759548544883728], 'magnitude': 1.9582020044326782, 'distance': 13.020878791809082, 'directional_contribution': -0.9518621296608849}, {'ion': 1320, 'force': [-3.7609140872955322, -1.9077779054641724, -2.8672845363616943], 'magnitude': 5.099550247192383, 'distance': 8.06869125366211, 'directional_contribution': 2.3526855188822395}, {'ion': 1460, 'force': [-2.4520761966705322, -0.6564997434616089, 0.013066878542304039], 'magnitude': 2.5384721755981445, 'distance': 11.43622875213623, 'directional_contribution': -0.061025553861092874}]}, 4996: {'frame': 4996, 'ionic_force': [-5.756140172481537, -3.3770331740379333, -4.165502771735191], 'ionic_force_magnitude': 7.866950875983785, 'motion_vector': [-0.20244598388671875, 1.0721435546875, 1.0912857055664062], 'cosine_ionic_motion': -0.5766948765207079, 'ionic_motion_component': -4.536830264019944, 'ionic_force_x': -5.756140172481537, 'ionic_force_y': -3.3770331740379333, 'ionic_force_z': -4.165502771735191, 'radial_force': 6.673642389565723, 'axial_force': -4.165502771735191, 'contributions': [{'ion': 1309, 'force': [-0.8596774935722351, -0.5392806529998779, -1.5933207273483276], 'magnitude': 1.889057993888855, 'distance': 13.257035255432129, 'directional_contribution': -1.3886435159335724}, {'ion': 1320, 'force': [-2.712550401687622, -1.9728121757507324, -2.712400197982788], 'magnitude': 4.313587188720703, 'distance': 8.773033142089844, 'directional_contribution': -2.9329172369528784}, {'ion': 1460, 'force': [-2.1839122772216797, -0.864940345287323, 0.14021815359592438], 'magnitude': 2.353137493133545, 'distance': 11.878056526184082, 'directional_contribution': -0.21526948954107716}]}, 4997: {'frame': 4997, 'ionic_force': [-6.240003228187561, -2.746828645467758, -4.2932528257369995], 'ionic_force_magnitude': 8.056967650490607, 'motion_vector': [-0.3025016784667969, -0.6528167724609375, -0.76025390625], 'cosine_ionic_motion': 0.8234675078649084, 'ionic_motion_component': 6.634651072097687, 'ionic_force_x': -6.240003228187561, 'ionic_force_y': -2.746828645467758, 'ionic_force_z': -4.2932528257369995, 'radial_force': 6.817822811965226, 'axial_force': -4.2932528257369995, 'contributions': [{'ion': 1309, 'force': [-1.0400985479354858, -0.5203492045402527, -1.7408907413482666], 'magnitude': 2.093625783920288, 'distance': 12.592719078063965, 'directional_contribution': 1.889528208024867}, {'ion': 1320, 'force': [-3.253243923187256, -1.7816591262817383, -2.824697256088257], 'magnitude': 4.662276268005371, 'distance': 8.438592910766602, 'directional_contribution': 4.102928252537652}, {'ion': 1460, 'force': [-1.9466607570648193, -0.4448203146457672, 0.2723351716995239], 'magnitude': 2.0153212547302246, 'distance': 12.835030555725098, 'directional_contribution': 0.6421947467171396}]}, 4998: {'frame': 4998, 'ionic_force': [-5.917741358280182, -2.6335960030555725, -4.115299761295319], 'ionic_force_magnitude': 7.67405908343996, 'motion_vector': [1.2956390380859375, -1.7068977355957031, 0.36876678466796875], 'cosine_ionic_motion': -0.28103523912743056, 'ionic_motion_component': -2.15668102959258, 'ionic_force_x': -5.917741358280182, 'ionic_force_y': -2.6335960030555725, 'ionic_force_z': -4.115299761295319, 'radial_force': 6.477305820386286, 'axial_force': -4.115299761295319, 'contributions': [{'ion': 1309, 'force': [-0.8881041407585144, -0.46092355251312256, -1.5887774229049683], 'magnitude': 1.8776030540466309, 'distance': 13.297412872314453, 'directional_contribution': -0.4368036629911547}, {'ion': 1320, 'force': [-3.2808942794799805, -1.594046950340271, -2.6922800540924072], 'magnitude': 4.533610820770264, 'distance': 8.557500839233398, 'directional_contribution': -1.160210559338669}, {'ion': 1460, 'force': [-1.748742938041687, -0.578625500202179, 0.16575771570205688], 'magnitude': 1.8494282960891724, 'distance': 13.39831829071045, 'directional_contribution': -0.5596666774590444}]}, 4999: {'frame': 4999, 'ionic_force': [-11.94784277677536, -6.789508700370789, -1.4325785636901855], 'ionic_force_magnitude': 13.816680381050233, 'motion_vector': [-0.551971435546875, 1.3257789611816406, 0.19469451904296875], 'cosine_ionic_motion': -0.13411382016327142, 'ionic_motion_component': -1.8530077878775715, 'ionic_force_x': -11.94784277677536, 'ionic_force_y': -6.789508700370789, 'ionic_force_z': -1.4325785636901855, 'radial_force': 13.742211445431693, 'axial_force': -1.4325785636901855, 'contributions': [{'ion': 1309, 'force': [-0.7131099104881287, -0.7815901041030884, -1.624629020690918], 'magnitude': 1.938769817352295, 'distance': 13.085969924926758, 'directional_contribution': -0.6616655531706854}, {'ion': 1320, 'force': [-2.2887518405914307, -2.6869468688964844, -2.5399811267852783], 'magnitude': 4.348513603210449, 'distance': 8.737730026245117, 'directional_contribution': -1.9275696379600227}, {'ion': 1460, 'force': [-8.9459810256958, -3.320971727371216, 2.7320315837860107], 'magnitude': 9.925896644592285, 'distance': 5.783412456512451, 'directional_contribution': 0.7362275165773262}]}, 5000: {'frame': 5000, 'ionic_force': [-9.01192718744278, -4.783424496650696, -3.6936601996421814], 'ionic_force_magnitude': 10.850765282566433, 'motion_vector': [-0.7812538146972656, 0.4613761901855469, -0.36583709716796875], 'cosine_ionic_motion': 0.5826446516183137, 'ionic_motion_component': 6.322140357853013, 'ionic_force_x': -9.01192718744278, 'ionic_force_y': -4.783424496650696, 'ionic_force_z': -3.6936601996421814, 'radial_force': 10.202743824429206, 'axial_force': -3.6936601996421814, 'contributions': [{'ion': 1309, 'force': [-0.9397225975990295, -0.6545020341873169, -1.707296371459961], 'magnitude': 2.055799722671509, 'distance': 12.70804214477539, 'directional_contribution': 1.080228253059616}, {'ion': 1320, 'force': [-3.7437233924865723, -2.7520456314086914, -2.9792110919952393], 'magnitude': 5.519503593444824, 'distance': 7.755664825439453, 'directional_contribution': 2.8058756448791513}, {'ion': 1460, 'force': [-4.328481197357178, -1.3768768310546875, 0.9928472638130188], 'magnitude': 4.649439334869385, 'distance': 8.450234413146973, 'directional_contribution': 2.436036667233086}]}, 5001: {'frame': 5001, 'ionic_force': [-6.330652832984924, -3.146571785211563, -2.4073009490966797], 'ionic_force_magnitude': 7.468144157070839, 'motion_vector': [-0.016719818115234375, -0.3343772888183594, 0.31487274169921875], 'cosine_ionic_motion': 0.11653666175395425, 'ionic_motion_component': 0.870312589562334, 'ionic_force_x': -6.330652832984924, 'ionic_force_y': -3.146571785211563, 'ionic_force_z': -2.4073009490966797, 'radial_force': 7.06951761376047, 'axial_force': -2.4073009490966797, 'contributions': [{'ion': 1309, 'force': [-0.9957014322280884, -0.4937232434749603, -1.515923261642456], 'magnitude': 1.8796827793121338, 'distance': 13.290054321289062, 'directional_contribution': -0.6431349952876526}, {'ion': 1320, 'force': [-2.770164966583252, -1.6772152185440063, -2.3731327056884766], 'magnitude': 4.014800548553467, 'distance': 9.09362506866455, 'directional_contribution': -0.3048201694466055}, {'ion': 1460, 'force': [-2.564786434173584, -0.9756333231925964, 1.481755018234253], 'magnitude': 3.1185874938964844, 'distance': 10.317870140075684, 'directional_contribution': 1.8182676836329943}]}, 5002: {'frame': 5002, 'ionic_force': [-7.864047288894653, -3.612726092338562, -1.8392441272735596], 'ionic_force_magnitude': 8.847476958994891, 'motion_vector': [1.8620643615722656, -2.09149169921875, 0.0738525390625], 'cosine_ionic_motion': -0.2914451320352368, 'ionic_motion_component': -2.5785540904929816, 'ionic_force_x': -7.864047288894653, 'ionic_force_y': -3.612726092338562, 'ionic_force_z': -1.8392441272735596, 'radial_force': 8.654191445781356, 'axial_force': -1.8392441272735596, 'contributions': [{'ion': 1309, 'force': [-1.0093481540679932, -0.5549268126487732, -1.643075942993164], 'magnitude': 2.0065956115722656, 'distance': 12.862906455993652, 'directional_contribution': -0.299933138318341}, {'ion': 1320, 'force': [-3.4694180488586426, -2.0770719051361084, -2.471514940261841], 'magnitude': 4.739142894744873, 'distance': 8.369877815246582, 'directional_contribution': -0.8205685344170597}, {'ion': 1460, 'force': [-3.3852810859680176, -0.9807273745536804, 2.2753467559814453], 'magnitude': 4.195135116577148, 'distance': 8.896026611328125, 'directional_contribution': -1.4580521448367172}]}, 5003: {'frame': 5003, 'ionic_force': [-5.132673859596252, -6.734123051166534, -1.4360578060150146], 'ionic_force_magnitude': 8.58807407044512, 'motion_vector': [-0.707275390625, -0.40502166748046875, -0.429779052734375], 'cosine_ionic_motion': 0.8814315808209459, 'ionic_motion_component': 7.569799704119818, 'ionic_force_x': -5.132673859596252, 'ionic_force_y': -6.734123051166534, 'ionic_force_z': -1.4360578060150146, 'radial_force': 8.467157387059435, 'axial_force': -1.4360578060150146, 'contributions': [{'ion': 1309, 'force': [-0.6637636423110962, -0.8726678490638733, -1.511733055114746], 'magnitude': 1.8674763441085815, 'distance': 13.333417892456055, 'directional_contribution': 1.5982341395508683}, {'ion': 1320, 'force': [-2.242825746536255, -3.0832972526550293, -2.36020565032959], 'magnitude': 4.484145164489746, 'distance': 8.604570388793945, 'directional_contribution': 4.17781086980186}, {'ion': 1460, 'force': [-2.2260844707489014, -2.778157949447632, 2.4358808994293213], 'magnitude': 4.313598155975342, 'distance': 8.773021697998047, 'directional_contribution': 1.793754685761428}]}, 5004: {'frame': 5004, 'ionic_force': [-4.717077851295471, -4.595800518989563, -2.3284347653388977], 'ionic_force_magnitude': 6.985256925981022, 'motion_vector': [-0.6747245788574219, 2.4837417602539062, -0.2197113037109375], 'cosine_ionic_motion': -0.42787515374866464, 'ionic_motion_component': -2.9888178811780546, 'ionic_force_x': -4.717077851295471, 'ionic_force_y': -4.595800518989563, 'ionic_force_z': -2.3284347653388977, 'radial_force': 6.585757804955102, 'axial_force': -2.3284347653388977, 'contributions': [{'ion': 1309, 'force': [-0.6875178813934326, -0.8340977430343628, -1.441748857498169], 'magnitude': 1.8019543886184692, 'distance': 13.573665618896484, 'directional_contribution': -0.4997950258276198}, {'ion': 1320, 'force': [-2.1348366737365723, -2.760021209716797, -1.877365231513977], 'magnitude': 3.9622902870178223, 'distance': 9.15368366241455, 'directional_contribution': -1.936525656408099}, {'ion': 1460, 'force': [-1.8947232961654663, -1.0016815662384033, 0.9906793236732483], 'magnitude': 2.3610990047454834, 'distance': 11.858014106750488, 'directional_contribution': -0.552497107667592}]}, 5005: {'frame': 5005, 'ionic_force': [-5.8636956214904785, -3.0404764115810394, -2.9966933727264404], 'ionic_force_magnitude': 7.253109286437775, 'motion_vector': [1.9760818481445312, -2.551136016845703, 1.67626953125], 'cosine_ionic_motion': -0.33568837728081463, 'ionic_motion_component': -2.434784486604704, 'ionic_force_x': -5.8636956214904785, 'ionic_force_y': -3.0404764115810394, 'ionic_force_z': -2.9966933727264404, 'radial_force': 6.605105839490183, 'axial_force': -2.9966933727264404, 'contributions': [{'ion': 1309, 'force': [-0.8727691173553467, -0.5728297829627991, -1.483247995376587], 'magnitude': 1.8138039112091064, 'distance': 13.529254913330078, 'directional_contribution': -0.7561473993155872}, {'ion': 1320, 'force': [-3.1719272136688232, -2.036134958267212, -2.4662981033325195], 'magnitude': 4.504396915435791, 'distance': 8.585206031799316, 'directional_contribution': -1.4321241320576235}, {'ion': 1460, 'force': [-1.8189992904663086, -0.43151167035102844, 0.952852725982666], 'magnitude': 2.098306179046631, 'distance': 12.578666687011719, 'directional_contribution': -0.24651297452992438}]}, 5006: {'frame': 5006, 'ionic_force': [-4.633662641048431, -6.107035517692566, -2.5804152488708496], 'ionic_force_magnitude': 8.088587957240227, 'motion_vector': [-2.692249298095703, 2.7754745483398438, -1.560882568359375], 'cosine_ionic_motion': -0.013259507049575554, 'ionic_motion_component': -0.10725068904013872, 'ionic_force_x': -4.633662641048431, 'ionic_force_y': -6.107035517692566, 'ionic_force_z': -2.5804152488708496, 'radial_force': 7.665944970152501, 'axial_force': -2.5804152488708496, 'contributions': [{'ion': 1309, 'force': [-0.7836499810218811, -1.1199933290481567, -1.7357754707336426], 'magnitude': 2.2093911170959473, 'distance': 12.258370399475098, 'directional_contribution': 0.41023095682033883}, {'ion': 1320, 'force': [-2.376492977142334, -4.063398838043213, -2.111187219619751], 'magnitude': 5.159073352813721, 'distance': 8.02200984954834, 'directional_contribution': -0.37997168201967924}, {'ion': 1460, 'force': [-1.4735196828842163, -0.9236433506011963, 1.266547441482544], 'magnitude': 2.151399612426758, 'distance': 12.422486305236816, 'directional_contribution': -0.1375097622119199}]}, 5007: {'frame': 5007, 'ionic_force': [-5.718433976173401, -2.855208694934845, -3.147172212600708], 'ionic_force_magnitude': 7.124422556758681, 'motion_vector': [0.5759010314941406, -0.5521697998046875, 0.14435577392578125], 'cosine_ionic_motion': -0.37583636937022347, 'ionic_motion_component': -2.6776171075915074, 'ionic_force_x': -5.718433976173401, 'ionic_force_y': -2.855208694934845, 'ionic_force_z': -3.147172212600708, 'radial_force': 6.391611990060556, 'axial_force': -3.147172212600708, 'contributions': [{'ion': 1309, 'force': [-0.9638186693191528, -0.5711681842803955, -1.511455774307251], 'magnitude': 1.8814032077789307, 'distance': 13.283976554870605, 'directional_contribution': -0.5647154217011554}, {'ion': 1320, 'force': [-3.205503225326538, -1.8640981912612915, -2.3779666423797607], 'magnitude': 4.405092239379883, 'distance': 8.681435585021973, 'directional_contribution': -1.4307240068059563}, {'ion': 1460, 'force': [-1.54911208152771, -0.41994231939315796, 0.7422502040863037], 'magnitude': 1.7683424949645996, 'distance': 13.702059745788574, 'directional_contribution': -0.682177547541098}]}, 5008: {'frame': 5008, 'ionic_force': [-5.75127911567688, -3.5837172269821167, -3.116843521595001], 'ionic_force_magnitude': 7.45888424414122, 'motion_vector': [0.1088409423828125, -0.9409523010253906, -0.1216583251953125], 'cosine_ionic_motion': 0.4387472499987256, 'ionic_motion_component': 3.2725649501757834, 'ionic_force_x': -5.75127911567688, 'ionic_force_y': -3.5837172269821167, 'ionic_force_z': -3.116843521595001, 'radial_force': 6.776447493295394, 'axial_force': -3.116843521595001, 'contributions': [{'ion': 1309, 'force': [-0.929062008857727, -0.6301071643829346, -1.557762622833252], 'magnitude': 1.9201081991195679, 'distance': 13.149407386779785, 'directional_contribution': 0.7133933226855955}, {'ion': 1320, 'force': [-3.084425449371338, -2.398221731185913, -2.444641351699829], 'magnitude': 4.608841419219971, 'distance': 8.487370491027832, 'directional_contribution': 2.3228222934584686}, {'ion': 1460, 'force': [-1.737791657447815, -0.555388331413269, 0.8855604529380798], 'magnitude': 2.0279529094696045, 'distance': 12.794994354248047, 'directional_contribution': 0.23634932566563815}]}, 5009: {'frame': 5009, 'ionic_force': [-4.791661620140076, -3.3943287134170532, -3.0958730578422546], 'ionic_force_magnitude': 6.638216514013718, 'motion_vector': [-0.2537117004394531, 1.1904716491699219, 0.37801361083984375], 'cosine_ionic_motion': -0.4722309263117984, 'ionic_motion_component': -3.1347711334709754, 'ionic_force_x': -4.791661620140076, 'ionic_force_y': -3.3943287134170532, 'ionic_force_z': -3.0958730578422546, 'radial_force': 5.87209404698621, 'axial_force': -3.0958730578422546, 'contributions': [{'ion': 1309, 'force': [-0.8100695610046387, -0.6891690492630005, -1.492370843887329], 'magnitude': 1.8325767517089844, 'distance': 13.459779739379883, 'directional_contribution': -0.9250678833166077}, {'ion': 1320, 'force': [-2.5722618103027344, -2.1343741416931152, -2.2908530235290527], 'magnitude': 4.052171230316162, 'distance': 9.051595687866211, 'directional_contribution': -2.1609704321776206}, {'ion': 1460, 'force': [-1.4093302488327026, -0.5707855224609375, 0.6873508095741272], 'magnitude': 1.6686698198318481, 'distance': 14.10534954071045, 'directional_contribution': -0.048732690720088456}]}, 5010: {'frame': 5010, 'ionic_force': [-6.056791543960571, -3.679370939731598, -3.146594524383545], 'ionic_force_magnitude': 7.753937800886345, 'motion_vector': [0.18355178833007812, 0.16788864135742188, -0.24420166015625], 'cosine_ionic_motion': -0.3555627191622645, 'ionic_motion_component': -2.7570112086982186, 'ionic_force_x': -6.056791543960571, 'ionic_force_y': -3.679370939731598, 'ionic_force_z': -3.146594524383545, 'radial_force': 7.086783072673642, 'axial_force': -3.146594524383545, 'contributions': [{'ion': 1309, 'force': [-1.0071114301681519, -0.6563244462013245, -1.6691867113113403], 'magnitude': 2.056992769241333, 'distance': 12.70435619354248, 'directional_contribution': 0.3229377694326381}, {'ion': 1320, 'force': [-3.5231919288635254, -2.5213658809661865, -2.321716070175171], 'magnitude': 4.915336608886719, 'distance': 8.218497276306152, 'directional_contribution': -1.4430578597423107}, {'ion': 1460, 'force': [-1.526488184928894, -0.5016806125640869, 0.8443082571029663], 'magnitude': 1.81513249874115, 'distance': 13.52430248260498, 'directional_contribution': -1.6368912062349423}]}, 5011: {'frame': 5011, 'ionic_force': [-5.516871929168701, -3.2253422141075134, -3.525465488433838], 'ionic_force_magnitude': 7.2984666328682755, 'motion_vector': [0.9372367858886719, -0.7911605834960938, -0.0274505615234375], 'cosine_ionic_motion': -0.2816719609338294, 'ionic_motion_component': -2.0557734082901304, 'ionic_force_x': -5.516871929168701, 'ionic_force_y': -3.2253422141075134, 'ionic_force_z': -3.525465488433838, 'radial_force': 6.390517058967415, 'axial_force': -3.525465488433838, 'contributions': [{'ion': 1309, 'force': [-0.9378553628921509, -0.546708881855011, -1.6660550832748413], 'magnitude': 1.9885177612304688, 'distance': 12.921243667602539, 'directional_contribution': -0.3266347355442112}, {'ion': 1320, 'force': [-3.1024675369262695, -2.091669797897339, -2.5550997257232666], 'magnitude': 4.530885696411133, 'distance': 8.560073852539062, 'directional_contribution': -0.9640824441874996}, {'ion': 1460, 'force': [-1.4765490293502808, -0.5869635343551636, 0.69568932056427], 'magnitude': 1.7345623970031738, 'distance': 13.834837913513184, 'directional_contribution': -0.7650562903700497}]}, 5012: {'frame': 5012, 'ionic_force': [-5.650092005729675, -4.366848289966583, -3.620231330394745], 'ionic_force_magnitude': 8.006183769210281, 'motion_vector': [-0.8405380249023438, -0.2687263488769531, 0.18675994873046875], 'cosine_ionic_motion': 0.7265048948557896, 'ionic_motion_component': 5.816531697446245, 'ionic_force_x': -5.650092005729675, 'ionic_force_y': -4.366848289966583, 'ionic_force_z': -3.620231330394745, 'radial_force': 7.140931568135523, 'axial_force': -3.620231330394745, 'contributions': [{'ion': 1309, 'force': [-0.7837142944335938, -0.6856822371482849, -1.6732805967330933], 'magnitude': 1.9708465337753296, 'distance': 12.979042053222656, 'directional_contribution': 0.5881407195424284}, {'ion': 1320, 'force': [-3.166684865951538, -2.999635934829712, -2.8368637561798096], 'magnitude': 5.203220844268799, 'distance': 7.987905502319336, 'directional_contribution': 3.257205947883776}, {'ion': 1460, 'force': [-1.6996928453445435, -0.6815301179885864, 0.889913022518158], 'magnitude': 2.0360217094421387, 'distance': 12.76961612701416, 'directional_contribution': 1.9711850814531946}]}, 5013: {'frame': 5013, 'ionic_force': [-5.9465718269348145, -4.000038325786591, -3.3016263842582703], 'ionic_force_magnitude': 7.8906755022549735, 'motion_vector': [-0.21096038818359375, 1.4655113220214844, 0.278533935546875], 'cosine_ionic_motion': -0.4649415414172259, 'ionic_motion_component': -3.6687028308415703, 'ionic_force_x': -5.9465718269348145, 'ionic_force_y': -4.000038325786591, 'ionic_force_z': -3.3016263842582703, 'radial_force': 7.166730293561803, 'axial_force': -3.3016263842582703, 'contributions': [{'ion': 1309, 'force': [-0.7687656879425049, -0.6304101347923279, -1.5830514430999756], 'magnitude': 1.8693499565124512, 'distance': 13.326733589172363, 'directional_contribution': -0.7982455958570078}, {'ion': 1320, 'force': [-2.5553226470947266, -2.115832567214966, -2.6662724018096924], 'magnitude': 4.256222248077393, 'distance': 8.831955909729004, 'directional_contribution': -2.193267829759243}, {'ion': 1460, 'force': [-2.622483491897583, -1.2537956237792969, 0.9476974606513977], 'magnitude': 3.0573768615722656, 'distance': 10.42064380645752, 'directional_contribution': -0.6771893240015832}]}, 5014: {'frame': 5014, 'ionic_force': [-6.269465744495392, -3.210474908351898, -4.206337511539459], 'ionic_force_magnitude': 8.204061501448063, 'motion_vector': [-0.07615280151367188, 0.12347412109375, -0.5725250244140625], 'cosine_ionic_motion': 0.5137294905108934, 'ionic_motion_component': 4.214668335258949, 'ionic_force_x': -6.269465744495392, 'ionic_force_y': -3.210474908351898, 'ionic_force_z': -4.206337511539459, 'radial_force': 7.043674457167814, 'axial_force': -4.206337511539459, 'contributions': [{'ion': 1309, 'force': [-0.9814146161079407, -0.5977436304092407, -1.782705545425415], 'magnitude': 2.120969533920288, 'distance': 12.511282920837402, 'directional_contribution': 1.7296706601974083}, {'ion': 1320, 'force': [-3.2142367362976074, -2.007704019546509, -2.7193706035614014], 'magnitude': 4.664458274841309, 'distance': 8.43661880493164, 'directional_contribution': 2.6307708040646354}, {'ion': 1460, 'force': [-2.0738143920898438, -0.6050272583961487, 0.2957386374473572], 'magnitude': 2.1804184913635254, 'distance': 12.339544296264648, 'directional_contribution': -0.14577299787865972}]}, 5015: {'frame': 5015, 'ionic_force': [-6.003054678440094, -2.8174749612808228, -4.174112513661385], 'ionic_force_magnitude': 7.8356905188049915, 'motion_vector': [-0.7897682189941406, -0.2777671813964844, 0.30731964111328125], 'cosine_ionic_motion': 0.6068754930825757, 'ionic_motion_component': 4.755288547242243, 'ionic_force_x': -6.003054678440094, 'ionic_force_y': -2.8174749612808228, 'ionic_force_z': -4.174112513661385, 'radial_force': 6.631352096653131, 'axial_force': -4.174112513661385, 'contributions': [{'ion': 1309, 'force': [-0.8658602833747864, -0.46252405643463135, -1.602197527885437], 'magnitude': 1.8790102005004883, 'distance': 13.29243278503418, 'directional_contribution': 0.35872485650961394}, {'ion': 1320, 'force': [-3.3091530799865723, -1.7206918001174927, -2.800626277923584], 'magnitude': 4.6642022132873535, 'distance': 8.436850547790527, 'directional_contribution': 2.5013354411892053}, {'ion': 1460, 'force': [-1.8280413150787354, -0.6342591047286987, 0.2287112921476364], 'magnitude': 1.9484169483184814, 'distance': 13.053533554077148, 'directional_contribution': 1.8952282556125608}]}, 5016: {'frame': 5016, 'ionic_force': [-4.904240369796753, -2.443116396665573, -3.3296403288841248], 'ionic_force_magnitude': 6.411465983075317, 'motion_vector': [1.1025390625, 0.10252761840820312, 0.24944305419921875], 'cosine_ionic_motion': -0.8915613515141652, 'ionic_motion_component': -5.716215277057725, 'ionic_force_x': -4.904240369796753, 'ionic_force_y': -2.443116396665573, 'ionic_force_z': -3.3296403288841248, 'radial_force': 5.479086724299988, 'axial_force': -3.3296403288841248, 'contributions': [{'ion': 1309, 'force': [-1.0098766088485718, -0.4893936812877655, -1.7097877264022827], 'magnitude': 2.045172691345215, 'distance': 12.741015434265137, 'directional_contribution': -1.4009137019063496}, {'ion': 1320, 'force': [-2.484668016433716, -1.4379808902740479, -2.1973519325256348], 'magnitude': 3.615206718444824, 'distance': 9.583022117614746, 'directional_contribution': -3.0263045629930083}, {'ion': 1460, 'force': [-1.4096957445144653, -0.5157418251037598, 0.5774993300437927], 'magnitude': 1.608333706855774, 'distance': 14.367491722106934, 'directional_contribution': -1.288997173785691}]}, 5017: {'frame': 5017, 'ionic_force': [-5.9368895292282104, -3.2834761142730713, -4.590190887451172], 'ionic_force_magnitude': 8.191320104751195, 'motion_vector': [0.5471343994140625, -1.6718521118164062, -0.3502349853515625], 'cosine_ionic_motion': 0.2619658768360037, 'ionic_motion_component': 2.1458463536855326, 'ionic_force_x': -5.9368895292282104, 'ionic_force_y': -3.2834761142730713, 'ionic_force_z': -4.590190887451172, 'radial_force': 6.784384472836232, 'axial_force': -4.590190887451172, 'contributions': [{'ion': 1309, 'force': [-0.9971057176589966, -0.5652839541435242, -2.227571964263916], 'magnitude': 2.5051631927490234, 'distance': 11.512006759643555, 'directional_contribution': 0.6577129548394858}, {'ion': 1320, 'force': [-3.1286773681640625, -1.8227983713150024, -2.7695655822753906], 'magnitude': 4.558696269989014, 'distance': 8.533923149108887, 'directional_contribution': 1.2854605198777804}, {'ion': 1460, 'force': [-1.8111064434051514, -0.8953937888145447, 0.40694665908813477], 'magnitude': 2.0609323978424072, 'distance': 12.692207336425781, 'directional_contribution': 0.20267299659885296}]}, 5018: {'frame': 5018, 'ionic_force': [-5.112821400165558, -4.175246596336365, -3.6171252131462097], 'ionic_force_magnitude': 7.52709915025618, 'motion_vector': [-0.7775535583496094, 0.9555816650390625, -0.4134063720703125], 'cosine_ionic_motion': 0.15141662162349226, 'ionic_motion_component': 1.13972792395685, 'ionic_force_x': -5.112821400165558, 'ionic_force_y': -4.175246596336365, 'ionic_force_z': -3.6171252131462097, 'radial_force': 6.6010322533835035, 'axial_force': -3.6171252131462097, 'contributions': [{'ion': 1309, 'force': [-0.8273432850837708, -0.6951525807380676, -1.5980772972106934], 'magnitude': 1.9291410446166992, 'distance': 13.118586540222168, 'directional_contribution': 0.4922640614733851}, {'ion': 1320, 'force': [-2.6921701431274414, -2.517709493637085, -2.5012779235839844], 'magnitude': 4.454551696777344, 'distance': 8.633105278015137, 'directional_contribution': 0.555204709857918}, {'ion': 1460, 'force': [-1.5933079719543457, -0.9623845219612122, 0.482230007648468], 'magnitude': 1.9228520393371582, 'distance': 13.140022277832031, 'directional_contribution': 0.09225915488240055}]}, 5019: {'frame': 5019, 'ionic_force': [-5.461706221103668, -3.557756721973419, -4.075013521593064], 'ionic_force_magnitude': 7.687236365531885, 'motion_vector': [-0.7913475036621094, 1.0461807250976562, 0.7367630004882812], 'cosine_ionic_motion': -0.20770966272884678, 'ionic_motion_component': -1.5967132728015538, 'ionic_force_x': -5.461706221103668, 'ionic_force_y': -3.557756721973419, 'ionic_force_z': -4.075013521593064, 'radial_force': 6.518271836797662, 'axial_force': -4.075013521593064, 'contributions': [{'ion': 1309, 'force': [-0.8766928315162659, -0.5472941994667053, -1.570601463317871], 'magnitude': 1.8801356554031372, 'distance': 13.288454055786133, 'directional_contribution': -0.6885712376992821}, {'ion': 1320, 'force': [-2.96341609954834, -2.007153272628784, -2.510063886642456], 'magnitude': 4.371603965759277, 'distance': 8.71462345123291, 'directional_contribution': -1.066179289497434}, {'ion': 1460, 'force': [-1.6215972900390625, -1.0033092498779297, 0.005651828367263079], 'magnitude': 1.9068925380706787, 'distance': 13.194894790649414, 'directional_contribution': 0.15803715018454773}]}, 5020: {'frame': 5020, 'ionic_force': [-6.23261284828186, -3.1551178693771362, -3.0239685773849487], 'ionic_force_magnitude': 7.612136207612328, 'motion_vector': [1.7669715881347656, -2.7974472045898438, -1.122650146484375], 'cosine_ionic_motion': 0.04542930806501695, 'ionic_motion_component': 0.3458140808084903, 'ionic_force_x': -6.23261284828186, 'ionic_force_y': -3.1551178693771362, 'ionic_force_z': -3.0239685773849487, 'radial_force': 6.985716261503257, 'axial_force': -3.0239685773849487, 'contributions': [{'ion': 1309, 'force': [-1.063096284866333, -0.41905951499938965, -1.6496542692184448], 'magnitude': 2.006774425506592, 'distance': 12.862333297729492, 'directiona</t>
+          <t>{4992: {'frame': 4992, 'ionic_force': [-9.90977567434311, -3.2852199375629425, -0.025440236553549767], 'ionic_force_magnitude': 10.440161452755383, 'motion_vector': [1.30914306640625, -2.567424774169922, 0.49839019775390625], 'cosine_ionic_motion': -0.14905922879596165, 'ionic_motion_component': -1.556202414653044, 'ionic_force_x': -9.90977567434311, 'ionic_force_y': -3.2852199375629425, 'ionic_force_z': -0.025440236553549767, 'radial_force': 10.440130456750216, 'axial_force': -0.025440236553549767, 'contributions': [{'ion': 1309, 'force': [-0.8666126132011414, -0.2845568358898163, -1.5572242736816406], 'magnitude': 1.8046987056732178, 'distance': 13.56334114074707, 'cosine_with_motion': -0.2235692216062886, 'motion_component': -0.4034750869979291}, {'ion': 1316, 'force': [-3.8274505138397217, -1.5964282751083374, 4.4594645500183105], 'magnitude': 6.089727878570557, 'distance': 7.383633136749268, 'cosine_with_motion': 0.073584092113622, 'motion_component': 0.44810709179433417}, {'ion': 1320, 'force': [-3.069931983947754, -1.0022555589675903, -2.9554810523986816], 'magnitude': 4.377655506134033, 'distance': 8.708598136901855, 'cosine_with_motion': -0.22796719378171773, 'motion_component': -0.9979618179615599}, {'ion': 1460, 'force': [-2.145780563354492, -0.4019792675971985, 0.027800539508461952], 'magnitude': 2.1832852363586426, 'distance': 12.331439971923828, 'cosine_with_motion': -0.27613096677313564, 'motion_component': -0.602872663331882}]}, 4993: {'frame': 4993, 'ionic_force': [-6.721731662750244, -7.0382163524627686, 0.02508533000946045], 'ionic_force_magnitude': 9.732358154315692, 'motion_vector': [-1.2147407531738281, 0.47171783447265625, 0.3584442138671875], 'cosine_ionic_motion': 0.3690367022768285, 'ionic_motion_component': 3.5915973586456644, 'ionic_force_x': -6.721731662750244, 'ionic_force_y': -7.0382163524627686, 'ionic_force_z': 0.02508533000946045, 'radial_force': 9.732325825315009, 'axial_force': 0.02508533000946045, 'contributions': [{'ion': 1309, 'force': [-0.767593502998352, -0.664334774017334, -1.574743628501892], 'magnitude': 1.873594880104065, 'distance': 13.311628341674805, 'cosine_with_motion': 0.02155868336146814, 'motion_component': 0.040392239910257643}, {'ion': 1316, 'force': [-0.9619420766830444, -1.5705485343933105, 2.251835346221924], 'magnitude': 2.9090750217437744, 'distance': 10.68295955657959, 'cosine_with_motion': 0.31406873477619174, 'motion_component': 0.9136495223597336}, {'ion': 1320, 'force': [-2.390256643295288, -2.211256742477417, -2.6654586791992188], 'magnitude': 4.2080464363098145, 'distance': 8.882369041442871, 'cosine_with_motion': 0.15913419023094658, 'motion_component': 0.6696440311311278}, {'ion': 1460, 'force': [-2.6019394397735596, -2.592076301574707, 2.0134522914886475], 'magnitude': 4.18842887878418, 'distance': 8.903144836425781, 'cosine_with_motion': 0.46984474326150344, 'motion_component': 1.9679114067019796}]}, 4994: {'frame': 4994, 'ionic_force': [-8.510059118270874, -4.980317711830139, -0.8486621975898743], 'ionic_force_magnitude': 9.89671148578417, 'motion_vector': [0.4574928283691406, 1.3063774108886719, 0.06430816650390625], 'cosine_ionic_motion': -0.762318113348161, 'ionic_motion_component': -7.544442428194064, 'ionic_force_x': -8.510059118270874, 'ionic_force_y': -4.980317711830139, 'ionic_force_z': -0.8486621975898743, 'radial_force': 9.860257131902506, 'axial_force': -0.8486621975898743, 'contributions': [{'ion': 1309, 'force': [-0.9202994108200073, -0.567900538444519, -1.5354427099227905], 'magnitude': 1.8780431747436523, 'distance': 13.295854568481445, 'cosine_with_motion': -0.4848207257917492, 'motion_component': -0.9105142778132502}, {'ion': 1316, 'force': [-1.8541682958602905, -1.3925756216049194, 2.6088037490844727], 'magnitude': 3.490424633026123, 'distance': 9.752813339233398, 'cosine_with_motion': -0.5168421163071228, 'motion_component': -1.8039984403479077}, {'ion': 1320, 'force': [-2.610811948776245, -1.7711108922958374, -2.3384480476379395], 'magnitude': 3.927023410797119, 'distance': 9.194694519042969, 'cosine_with_motion': -0.6723389238516795, 'motion_component': -2.640290627803788}, {'ion': 1460, 'force': [-3.124779462814331, -1.2487306594848633, 0.41642481088638306], 'magnitude': 3.3907203674316406, 'distance': 9.89516544342041, 'cosine_with_motion': -0.6457740657600884, 'motion_component': -2.189639274119873}]}, 4995: {'frame': 4995, 'ionic_force': [-7.9496631026268005, -3.4401994943618774, -2.7620067689567804], 'ionic_force_magnitude': 9.091798358852705, 'motion_vector': [0.29911041259765625, -1.0097732543945312, -0.8112640380859375], 'cosine_ionic_motion': 0.2760697449015972, 'ionic_motion_component': 2.5099704536252263, 'ionic_force_x': -7.9496631026268005, 'ionic_force_y': -3.4401994943618774, 'ionic_force_z': -2.7620067689567804, 'radial_force': 8.662108057873308, 'axial_force': -2.7620067689567804, 'contributions': [{'ion': 1309, 'force': [-0.9697037935256958, -0.4882330298423767, -1.6673376560211182], 'magnitude': 1.989651083946228, 'distance': 12.917562484741211, 'cosine_with_motion': 0.5881295353879933, 'motion_component': 1.1701726210799208}, {'ion': 1316, 'force': [-0.7669690251350403, -0.3876888155937195, 1.759548544883728], 'magnitude': 1.9582020044326782, 'distance': 13.020878791809082, 'cosine_with_motion': -0.48608984963177254, 'motion_component': -0.9518621296608849}, {'ion': 1320, 'force': [-3.7609140872955322, -1.9077779054641724, -2.8672845363616943], 'magnitude': 5.099550247192383, 'distance': 8.06869125366211, 'cosine_with_motion': 0.461351578304799, 'motion_component': 2.3526855188822395}, {'ion': 1460, 'force': [-2.4520761966705322, -0.6564997434616089, 0.013066878542304039], 'magnitude': 2.5384721755981445, 'distance': 11.43622875213623, 'cosine_with_motion': -0.02404027018762123, 'motion_component': -0.061025553861092874}]}, 4996: {'frame': 4996, 'ionic_force': [-5.756140172481537, -3.3770331740379333, -4.165502771735191], 'ionic_force_magnitude': 7.866950875983785, 'motion_vector': [-0.20244598388671875, 1.0721435546875, 1.0912857055664062], 'cosine_ionic_motion': -0.5766948765207079, 'ionic_motion_component': -4.536830264019944, 'ionic_force_x': -5.756140172481537, 'ionic_force_y': -3.3770331740379333, 'ionic_force_z': -4.165502771735191, 'radial_force': 6.673642389565723, 'axial_force': -4.165502771735191, 'contributions': [{'ion': 1309, 'force': [-0.8596774935722351, -0.5392806529998779, -1.5933207273483276], 'magnitude': 1.889057993888855, 'distance': 13.257035255432129, 'cosine_with_motion': -0.7350984190555, 'motion_component': -1.3886435159335724}, {'ion': 1320, 'force': [-2.712550401687622, -1.9728121757507324, -2.712400197982788], 'magnitude': 4.313587188720703, 'distance': 8.773033142089844, 'cosine_with_motion': -0.6799253774807416, 'motion_component': -2.9329172369528784}, {'ion': 1460, 'force': [-2.1839122772216797, -0.864940345287323, 0.14021815359592438], 'magnitude': 2.353137493133545, 'distance': 11.878056526184082, 'cosine_with_motion': -0.09148190274176744, 'motion_component': -0.21526948954107716}]}, 4997: {'frame': 4997, 'ionic_force': [-6.240003228187561, -2.746828645467758, -4.2932528257369995], 'ionic_force_magnitude': 8.056967650490607, 'motion_vector': [-0.3025016784667969, -0.6528167724609375, -0.76025390625], 'cosine_ionic_motion': 0.8234675078649084, 'ionic_motion_component': 6.634651072097687, 'ionic_force_x': -6.240003228187561, 'ionic_force_y': -2.746828645467758, 'ionic_force_z': -4.2932528257369995, 'radial_force': 6.817822811965226, 'axial_force': -4.2932528257369995, 'contributions': [{'ion': 1309, 'force': [-1.0400985479354858, -0.5203492045402527, -1.7408907413482666], 'magnitude': 2.093625783920288, 'distance': 12.592719078063965, 'cosine_with_motion': 0.9025147840163484, 'motion_component': 1.889528208024867}, {'ion': 1320, 'force': [-3.253243923187256, -1.7816591262817383, -2.824697256088257], 'magnitude': 4.662276268005371, 'distance': 8.438592910766602, 'cosine_with_motion': 0.8800268431847608, 'motion_component': 4.102928252537652}, {'ion': 1460, 'force': [-1.9466607570648193, -0.4448203146457672, 0.2723351716995239], 'magnitude': 2.0153212547302246, 'distance': 12.835030555725098, 'cosine_with_motion': 0.31865627031193433, 'motion_component': 0.6421947467171396}]}, 4998: {'frame': 4998, 'ionic_force': [-5.917741358280182, -2.6335960030555725, -4.115299761295319], 'ionic_force_magnitude': 7.67405908343996, 'motion_vector': [1.2956390380859375, -1.7068977355957031, 0.36876678466796875], 'cosine_ionic_motion': -0.28103523912743056, 'ionic_motion_component': -2.15668102959258, 'ionic_force_x': -5.917741358280182, 'ionic_force_y': -2.6335960030555725, 'ionic_force_z': -4.115299761295319, 'radial_force': 6.477305820386286, 'axial_force': -4.115299761295319, 'contributions': [{'ion': 1309, 'force': [-0.8881041407585144, -0.46092355251312256, -1.5887774229049683], 'magnitude': 1.8776030540466309, 'distance': 13.297412872314453, 'cosine_with_motion': -0.23263898336225206, 'motion_component': -0.4368036629911547}, {'ion': 1320, 'force': [-3.2808942794799805, -1.594046950340271, -2.6922800540924072], 'magnitude': 4.533610820770264, 'distance': 8.557500839233398, 'cosine_with_motion': -0.2559131491847294, 'motion_component': -1.160210559338669}, {'ion': 1460, 'force': [-1.748742938041687, -0.578625500202179, 0.16575771570205688], 'magnitude': 1.8494282960891724, 'distance': 13.39831829071045, 'cosine_with_motion': -0.3026160485951843, 'motion_component': -0.5596666774590444}]}, 4999: {'frame': 4999, 'ionic_force': [-11.94784277677536, -6.789508700370789, -1.4325785636901855], 'ionic_force_magnitude': 13.816680381050233, 'motion_vector': [-0.551971435546875, 1.3257789611816406, 0.19469451904296875], 'cosine_ionic_motion': -0.13411382016327142, 'ionic_motion_component': -1.8530077878775715, 'ionic_force_x': -11.94784277677536, 'ionic_force_y': -6.789508700370789, 'ionic_force_z': -1.4325785636901855, 'radial_force': 13.742211445431693, 'axial_force': -1.4325785636901855, 'contributions': [{'ion': 1309, 'force': [-0.7131099104881287, -0.7815901041030884, -1.624629020690918], 'magnitude': 1.938769817352295, 'distance': 13.085969924926758, 'cosine_with_motion': -0.34128113473276755, 'motion_component': -0.6616655531706854}, {'ion': 1320, 'force': [-2.2887518405914307, -2.6869468688964844, -2.5399811267852783], 'magnitude': 4.348513603210449, 'distance': 8.737730026245117, 'cosine_with_motion': -0.44327089905166983, 'motion_component': -1.9275696379600227}, {'ion': 1460, 'force': [-8.9459810256958, -3.320971727371216, 2.7320315837860107], 'magnitude': 9.925896644592285, 'distance': 5.783412456512451, 'cosine_with_motion': 0.07417239319387016, 'motion_component': 0.7362275165773262}]}, 5000: {'frame': 5000, 'ionic_force': [-9.01192718744278, -4.783424496650696, -3.6936601996421814], 'ionic_force_magnitude': 10.850765282566433, 'motion_vector': [-0.7812538146972656, 0.4613761901855469, -0.36583709716796875], 'cosine_ionic_motion': 0.5826446516183137, 'ionic_motion_component': 6.322140357853013, 'ionic_force_x': -9.01192718744278, 'ionic_force_y': -4.783424496650696, 'ionic_force_z': -3.6936601996421814, 'radial_force': 10.202743824429206, 'axial_force': -3.6936601996421814, 'contributions': [{'ion': 1309, 'force': [-0.9397225975990295, -0.6545020341873169, -1.707296371459961], 'magnitude': 2.055799722671509, 'distance': 12.70804214477539, 'cosine_with_motion': 0.525454039767896, 'motion_component': 1.080228253059616}, {'ion': 1320, 'force': [-3.7437233924865723, -2.7520456314086914, -2.9792110919952393], 'magnitude': 5.519503593444824, 'distance': 7.755664825439453, 'cosine_with_motion': 0.5083565310182332, 'motion_component': 2.805875644879151}, {'ion': 1460, 'force': [-4.328481197357178, -1.3768768310546875, 0.9928472638130188], 'magnitude': 4.649439334869385, 'distance': 8.450234413146973, 'cosine_with_motion': 0.523942040511297, 'motion_component': 2.436036667233086}]}, 5001: {'frame': 5001, 'ionic_force': [-6.330652832984924, -3.146571785211563, -2.4073009490966797], 'ionic_force_magnitude': 7.468144157070839, 'motion_vector': [-0.016719818115234375, -0.3343772888183594, 0.31487274169921875], 'cosine_ionic_motion': 0.11653666175395425, 'ionic_motion_component': 0.870312589562334, 'ionic_force_x': -6.330652832984924, 'ionic_force_y': -3.146571785211563, 'ionic_force_z': -2.4073009490966797, 'radial_force': 7.06951761376047, 'axial_force': -2.4073009490966797, 'contributions': [{'ion': 1309, 'force': [-0.9957014322280884, -0.4937232434749603, -1.515923261642456], 'magnitude': 1.8796827793121338, 'distance': 13.290054321289062, 'cosine_with_motion': -0.3421508167823267, 'motion_component': -0.6431349952876526}, {'ion': 1320, 'force': [-2.770164966583252, -1.6772152185440063, -2.3731327056884766], 'magnitude': 4.014800548553467, 'distance': 9.09362506866455, 'cosine_with_motion': -0.07592411220123893, 'motion_component': -0.3048201694466055}, {'ion': 1460, 'force': [-2.564786434173584, -0.9756333231925964, 1.481755018234253], 'magnitude': 3.1185874938964844, 'distance': 10.317870140075684, 'cosine_with_motion': 0.5830420678716011, 'motion_component': 1.8182676836329943}]}, 5002: {'frame': 5002, 'ionic_force': [-7.864047288894653, -3.612726092338562, -1.8392441272735596], 'ionic_force_magnitude': 8.847476958994891, 'motion_vector': [1.8620643615722656, -2.09149169921875, 0.0738525390625], 'cosine_ionic_motion': -0.2914451320352368, 'ionic_motion_component': -2.5785540904929816, 'ionic_force_x': -7.864047288894653, 'ionic_force_y': -3.612726092338562, 'ionic_force_z': -1.8392441272735596, 'radial_force': 8.654191445781356, 'axial_force': -1.8392441272735596, 'contributions': [{'ion': 1309, 'force': [-1.0093481540679932, -0.5549268126487732, -1.643075942993164], 'magnitude': 2.0065956115722656, 'distance': 12.862906455993652, 'cosine_with_motion': -0.14947363285212528, 'motion_component': -0.299933138318341}, {'ion': 1320, 'force': [-3.4694180488586426, -2.0770719051361084, -2.471514940261841], 'magnitude': 4.739142894744873, 'distance': 8.369877815246582, 'cosine_with_motion': -0.17314703360432673, 'motion_component': -0.8205685344170597}, {'ion': 1460, 'force': [-3.3852810859680176, -0.9807273745536804, 2.2753467559814453], 'magnitude': 4.195135116577148, 'distance': 8.896026611328125, 'cosine_with_motion': -0.34755786630106694, 'motion_component': -1.4580521448367174}]}, 5003: {'frame': 5003, 'ionic_force': [-5.132673859596252, -6.734123051166534, -1.4360578060150146], 'ionic_force_magnitude': 8.58807407044512, 'motion_vector': [-0.707275390625, -0.40502166748046875, -0.429779052734375], 'cosine_ionic_motion': 0.8814315808209459, 'ionic_motion_component': 7.569799704119818, 'ionic_force_x': -5.132673859596252, 'ionic_force_y': -6.734123051166534, 'ionic_force_z': -1.4360578060150146, 'radial_force': 8.467157387059435, 'axial_force': -1.4360578060150146, 'contributions': [{'ion': 1309, 'force': [-0.6637636423110962, -0.8726678490638733, -1.511733055114746], 'magnitude': 1.8674763441085815, 'distance': 13.333417892456055, 'cosine_with_motion': 0.8558256065889733, 'motion_component': 1.5982341395508683}, {'ion': 1320, 'force': [-2.242825746536255, -3.0832972526550293, -2.36020565032959], 'magnitude': 4.484145164489746, 'distance': 8.604570388793945, 'cosine_with_motion': 0.9316849689159826, 'motion_component': 4.17781086980186}, {'ion': 1460, 'force': [-2.2260844707489014, -2.778157949447632, 2.4358808994293213], 'magnitude': 4.313598155975342, 'distance': 8.773021697998047, 'cosine_with_motion': 0.41583722061378225, 'motion_component': 1.793754685761428}]}, 5004: {'frame': 5004, 'ionic_force': [-4.717077851295471, -4.595800518989563, -2.3284347653388977], 'ionic_force_magnitude': 6.985256925981022, 'motion_vector': [-0.6747245788574219, 2.4837417602539062, -0.2197113037109375], 'cosine_ionic_motion': -0.42787515374866464, 'ionic_motion_component': -2.9888178811780546, 'ionic_force_x': -4.717077851295471, 'ionic_force_y': -4.595800518989563, 'ionic_force_z': -2.3284347653388977, 'radial_force': 6.585757804955102, 'axial_force': -2.3284347653388977, 'contributions': [{'ion': 1309, 'force': [-0.6875178813934326, -0.8340977430343628, -1.441748857498169], 'magnitude': 1.8019543886184692, 'distance': 13.573665618896484, 'cosine_with_motion': -0.27736274933035654, 'motion_component': -0.4997950258276198}, {'ion': 1320, 'force': [-2.1348366737365723, -2.760021209716797, -1.877365231513977], 'magnitude': 3.9622902870178223, 'distance': 9.15368366241455, 'cosine_with_motion': -0.48873895636195097, 'motion_component': -1.936525656408099}, {'ion': 1460, 'force': [-1.8947232961654663, -1.0016815662384033, 0.9906793236732483], 'magnitude': 2.3610990047454834, 'distance': 11.858014106750488, 'cosine_with_motion': -0.23399998864807015, 'motion_component': -0.552497107667592}]}, 5005: {'frame': 5005, 'ionic_force': [-5.8636956214904785, -3.0404764115810394, -2.9966933727264404], 'ionic_force_magnitude': 7.253109286437775, 'motion_vector': [1.9760818481445312, -2.551136016845703, 1.67626953125], 'cosine_ionic_motion': -0.33568837728081463, 'ionic_motion_component': -2.434784486604704, 'ionic_force_x': -5.8636956214904785, 'ionic_force_y': -3.0404764115810394, 'ionic_force_z': -2.9966933727264404, 'radial_force': 6.605105839490183, 'axial_force': -2.9966933727264404, 'contributions': [{'ion': 1309, 'force': [-0.8727691173553467, -0.5728297829627991, -1.483247995376587], 'magnitude': 1.8138039112091064, 'distance': 13.529254913330078, 'cosine_with_motion': -0.4168848729684455, 'motion_component': -0.7561473993155872}, {'ion': 1320, 'force': [-3.1719272136688232, -2.036134958267212, -2.4662981033325195], 'magnitude': 4.504396915435791, 'distance': 8.585206031799316, 'cosine_with_motion': -0.31793913100847976, 'motion_component': -1.4321241320576232}, {'ion': 1460, 'force': [-1.8189992904663086, -0.43151167035102844, 0.952852725982666], 'magnitude': 2.098306179046631, 'distance': 12.578666687011719, 'cosine_with_motion': -0.11748188627750467, 'motion_component': -0.24651297452992438}]}, 5006: {'frame': 5006, 'ionic_force': [-4.633662641048431, -6.107035517692566, -2.5804152488708496], 'ionic_force_magnitude': 8.088587957240227, 'motion_vector': [-2.692249298095703, 2.7754745483398438, -1.560882568359375], 'cosine_ionic_motion': -0.013259507049575554, 'ionic_motion_component': -0.10725068904013872, 'ionic_force_x': -4.633662641048431, 'ionic_force_y': -6.107035517692566, 'ionic_force_z': -2.5804152488708496, 'radial_force': 7.665944970152501, 'axial_force': -2.5804152488708496, 'contributions': [{'ion': 1309, 'force': [-0.7836499810218811, -1.1199933290481567, -1.7357754707336426], 'magnitude': 2.2093911170959473, 'distance': 12.258370399475098, 'cosine_with_motion': 0.18567602863252866, 'motion_component': 0.41023095682033883}, {'ion': 1320, 'force': [-2.376492977142334, -4.063398838043213, -2.111187219619751], 'magnitude': 5.159073352813721, 'distance': 8.02200984954834, 'cosine_with_motion': -0.07365114574792865, 'motion_component': -0.3799716820196793}, {'ion': 1460, 'force': [-1.4735196828842163, -0.9236433506011963, 1.266547441482544], 'magnitude': 2.151399612426758, 'distance': 12.422486305236816, 'cosine_with_motion': -0.06391642443920177, 'motion_component': -0.1375097622119199}]}, 5007: {'frame': 5007, 'ionic_force': [-5.718433976173401, -2.855208694934845, -3.147172212600708], 'ionic_force_magnitude': 7.124422556758681, 'motion_vector': [0.5759010314941406, -0.5521697998046875, 0.14435577392578125], 'cosine_ionic_motion': -0.37583636937022347, 'ionic_motion_component': -2.6776171075915074, 'ionic_force_x': -5.718433976173401, 'ionic_force_y': -2.855208694934845, 'ionic_force_z': -3.147172212600708, 'radial_force': 6.391611990060556, 'axial_force': -3.147172212600708, 'contributions': [{'ion': 1309, 'force': [-0.9638186693191528, -0.5711681842803955, -1.511455774307251], 'magnitude': 1.8814032077789307, 'distance': 13.283976554870605, 'cosine_with_motion': -0.3001565084066107, 'motion_component': -0.5647154217011554}, {'ion': 1320, 'force': [-3.205503225326538, -1.8640981912612915, -2.3779666423797607], 'magnitude': 4.405092239379883, 'distance': 8.681435585021973, 'cosine_with_motion': -0.32478865433870185, 'motion_component': -1.4307240068059563}, {'ion': 1460, 'force': [-1.54911208152771, -0.41994231939315796, 0.7422502040863037], 'magnitude': 1.7683424949645996, 'distance': 13.702059745788574, 'cosine_with_motion': -0.38577229909063343, 'motion_component': -0.682177547541098}]}, 5008: {'frame': 5008, 'ionic_force': [-5.75127911567688, -3.5837172269821167, -3.116843521595001], 'ionic_force_magnitude': 7.45888424414122, 'motion_vector': [0.1088409423828125, -0.9409523010253906, -0.1216583251953125], 'cosine_ionic_motion': 0.4387472499987256, 'ionic_motion_component': 3.2725649501757834, 'ionic_force_x': -5.75127911567688, 'ionic_force_y': -3.5837172269821167, 'ionic_force_z': -3.116843521595001, 'radial_force': 6.776447493295394, 'axial_force': -3.116843521595001, 'contributions': [{'ion': 1309, 'force': [-0.929062008857727, -0.6301071643829346, -1.557762622833252], 'magnitude': 1.9201081991195679, 'distance': 13.149407386779785, 'cosine_with_motion': 0.37153807724211496, 'motion_component': 0.7133933226855955}, {'ion': 1320, 'force': [-3.084425449371338, -2.398221731185913, -2.444641351699829], 'magnitude': 4.608841419219971, 'distance': 8.487370491027832, 'cosine_with_motion': 0.5039926709766444, 'motion_component': 2.3228222934584686}, {'ion': 1460, 'force': [-1.737791657447815, -0.555388331413269, 0.8855604529380798], 'magnitude': 2.0279529094696045, 'distance': 12.794994354248047, 'cosine_with_motion': 0.11654576116051595, 'motion_component': 0.23634932566563815}]}, 5009: {'frame': 5009, 'ionic_force': [-4.791661620140076, -3.3943287134170532, -3.0958730578422546], 'ionic_force_magnitude': 6.638216514013718, 'motion_vector': [-0.2537117004394531, 1.1904716491699219, 0.37801361083984375], 'cosine_ionic_motion': -0.4722309263117984, 'ionic_motion_component': -3.1347711334709754, 'ionic_force_x': -4.791661620140076, 'ionic_force_y': -3.3943287134170532, 'ionic_force_z': -3.0958730578422546, 'radial_force': 5.87209404698621, 'axial_force': -3.0958730578422546, 'contributions': [{'ion': 1309, 'force': [-0.8100695610046387, -0.6891690492630005, -1.492370843887329], 'magnitude': 1.8325767517089844, 'distance': 13.459779739379883, 'cosine_with_motion': -0.5047908100773542, 'motion_component': -0.9250678833166076}, {'ion': 1320, 'force': [-2.5722618103027344, -2.1343741416931152, -2.2908530235290527], 'magnitude': 4.052171230316162, 'distance': 9.051595687866211, 'cosine_with_motion': -0.5332870526809247, 'motion_component': -2.1609704321776206}, {'ion': 1460, 'force': [-1.4093302488327026, -0.5707855224609375, 0.6873508095741272], 'magnitude': 1.6686698198318481, 'distance': 14.10534954071045, 'cosine_with_motion': -0.02920451360238688, 'motion_component': -0.048732690720088456}]}, 5010: {'frame': 5010, 'ionic_force': [-6.056791543960571, -3.679370939731598, -3.146594524383545], 'ionic_force_magnitude': 7.753937800886345, 'motion_vector': [0.18355178833007812, 0.16788864135742188, -0.24420166015625], 'cosine_ionic_motion': -0.3555627191622645, 'ionic_motion_component': -2.7570112086982186, 'ionic_force_x': -6.056791543960571, 'ionic_force_y': -3.679370939731598, 'ionic_force_z': -3.146594524383545, 'radial_force': 7.086783072673642, 'axial_force': -3.146594524383545, 'contributions': [{'ion': 1309, 'force': [-1.0071114301681519, -0.6563244462013245, -1.6691867113113403], 'magnitude': 2.056992769241333, 'distance': 12.70435619354248, 'cosine_with_motion': 0.15699508780823138, 'motion_component': 0.3229377694326381}, {'ion': 1320, 'force': [-3.5231919288635254, -2.5213658809661865, -2.321716070175171], 'magnitude': 4.915336608886719, 'distance': 8.218497276306152, 'cosine_with_motion': -0.2935827208285289, 'motion_component': -1.4430578597423107}, {'ion': 1460, 'force': [-1.526488184928894, -0.5016806125640869, 0.8443082571029663], 'magnitude': 1.81513249874115, 'distance': 13.52430248260498, 'cosine_with_motion': -0.9018025914210851, 'motion_component': -1.6368912062349423}]}, 5011: {'frame': 5011, 'ionic_force': [-5.516871929168701, -3.2253422141075134, -3.525465488433838], 'ionic_force_magnitude': 7.2984666328682755, 'motion_vector': [0.9372367858886719, -0.7911605834960938, -0.0274505615234375], 'cosine_ionic_motion': -0.2816719609338294, 'ionic_motion_component': -2.0557734082901304, 'ionic_force_x': -5.516871929168701, 'ionic_force_y': -3.2253422141075134, 'ionic_force_z': -3.525465488433838, 'radial_force': 6.390517058967415, 'axial_force': -3.525465488433838, 'contributions': [{'ion': 1309, 'force': [-0.9378553628921509, -0.546708881855011, -1.6660550832748413], 'magnitude': 1.9885177612304688, 'distance': 12.921243667602539, 'cosine_with_motion': -0.16426040768421035, 'motion_component': -0.3266347355442112}, {'ion': 1320, 'force': [-3.1024675369262695, -2.091669797897339, -2.5550997257232666], 'magnitude': 4.530885696411133, 'distance': 8.560073852539062, 'cosine_with_motion': -0.21278014597992131, 'motion_component': -0.9640824441874996}, {'ion': 1460, 'force': [-1.4765490293502808, -0.5869635343551636, 0.69568932056427], 'magnitude': 1.7345623970031738, 'distance': 13.834837913513184, 'cosine_with_motion': -0.44106586930846237, 'motion_component': -0.7650562903700497}]}, 5012: {'frame': 5012, 'ionic_force': [-5.650092005729675, -4.366848289966583, -3.620231330394745], 'ionic_force_magnitude': 8.006183769210281, 'motion_vector': [-0.8405380249023438, -0.2687263488769531, 0.18675994873046875], 'cosine_ionic_motion': 0.7265048948557896, 'ionic_motion_component': 5.816531697446245, 'ionic_force_x': -5.650092005729675, 'ionic_force_y': -4.366848289966583, 'ionic_force_z': -3.620231330394745, 'radial_force': 7.140931568135523, 'axial_force': -3.620231330394745, 'contributions': [{'ion': 1309, 'force': [-0.7837142944335938, -0.6856822371482849, -1.6732805967330933], 'magnitude': 1.9708465337753296, 'distance': 12.979042053222656, 'cosine_with_motion': 0.2984203489596868, 'motion_component': 0.5881407195424284}, {'ion': 1320, 'force': [-3.166684865951538, -2.999635934829712, -2.8368637561798096], 'magnitude': 5.203220844268799, 'distance': 7.987905502319336, 'cosine_with_motion': 0.625998048098166, 'motion_component': 3.257205947883776}, {'ion': 1460, 'force': [-1.6996928453445435, -0.6815301179885864, 0.889913022518158], 'magnitude': 2.0360217094421387, 'distance': 12.76961612701416, 'cosine_with_motion': 0.9681552541475777, 'motion_component': 1.9711850814531946}]}, 5013: {'frame': 5013, 'ionic_force': [-5.9465718269348145, -4.000038325786591, -3.3016263842582703], 'ionic_force_magnitude': 7.8906755022549735, 'motion_vector': [-0.21096038818359375, 1.4655113220214844, 0.278533935546875], 'cosine_ionic_motion': -0.4649415414172259, 'ionic_motion_component': -3.6687028308415703, 'ionic_force_x': -5.9465718269348145, 'ionic_force_y': -4.000038325786591, 'ionic_force_z': -3.3016263842582703, 'radial_force': 7.166730293561803, 'axial_force': -3.3016263842582703, 'contributions': [{'ion': 1309, 'force': [-0.7687656879425049, -0.6304101347923279, -1.5830514430999756], 'magnitude': 1.8693499565124512, 'distance': 13.326733589172363, 'cosine_with_motion': -0.4270177269430876, 'motion_component': -0.7982455958570078}, {'ion': 1320, 'force': [-2.5553226470947266, -2.115832567214966, -2.6662724018096924], 'magnitude': 4.256222248077393, 'distance': 8.831955909729004, 'cosine_with_motion': -0.5153085487858513, 'motion_component': -2.193267829759243}, {'ion': 1460, 'force': [-2.622483491897583, -1.2537956237792969, 0.9476974606513977], 'magnitude': 3.0573768615722656, 'distance': 10.42064380645752, 'cosine_with_motion': -0.22149356868241477, 'motion_component': -0.6771893240015832}]}, 5014: {'frame': 5014, 'ionic_force': [-6.269465744495392, -3.210474908351898, -4.206337511539459], 'ionic_force_magnitude': 8.204061501448063, 'motion_vector': [-0.07615280151367188, 0.12347412109375, -0.5725250244140625], 'cosine_ionic_motion': 0.5137294905108934, 'ionic_motion_component': 4.214668335258949, 'ionic_force_x': -6.269465744495392, 'ionic_force_y': -3.210474908351898, 'ionic_force_z': -4.206337511539459, 'radial_force': 7.043674457167814, 'axial_force': -4.206337511539459, 'contributions': [{'ion': 1309, 'force': [-0.9814146161079407, -0.5977436304092407, -1.782705545425415], 'magnitude': 2.120969533920288, 'distance': 12.511282920837402, 'cosine_with_motion': 0.8155094870457856, 'motion_component': 1.7296706601974083}, {'ion': 1320, 'force': [-3.2142367362976074, -2.007704019546509, -2.7193706035614014], 'magnitude': 4.664458274841309, 'distance': 8.43661880493164, 'cosine_with_motion': 0.5640035191898288, 'motion_component': 2.6307708040646354}, {'ion': 1460, 'force': [-2.0738143920898438, -0.6050272583961487, 0.2957386374473572], 'magnitude': 2.1804184913635254, 'distance': 12.339544296264648, 'cosine_with_motion': -0.06685550885342192, 'motion_component': -0.14577299787865972}]}, 5015: {'frame': 5015, 'ionic_force': [-6.003054678440094, -2.8174749612808228, -4.174112513661385], 'ionic_force_magnitude': 7.8356905188049915, 'motion_vector': [-0.7897682189941406, -0.2777671813964844, 0.30731964111328125], 'cosine_ionic_motion': 0.6068754930825757, 'ionic_motion_component': 4.755288547242243, 'ionic_force_x': -6.003054678440094, 'ionic_force_y': -2.8174749612808228, 'ionic_force_z': -4.174112513661385, 'radial_force': 6.631352096653131, 'axial_force': -4.174112513661385, 'contributions': [{'ion': 1309, 'force': [-0.8658602833747864, -0.46252405643463135, -1.602197527885437], 'magnitude': 1.8790102005004883, 'distance': 13.29243278503418, 'cosine_with_motion': 0.19091160358013518, 'motion_component': 0.35872485650961394}, {'ion': 1320, 'force': [-3.3091530799865723, -1.7206918001174927, -2.800626277923584], 'magnitude': 4.6642022132873535, 'distance': 8.436850547790527, 'cosine_with_motion': 0.5362836659961173, 'motion_component': 2.5013354411892053}, {'ion': 1460, 'force': [-1.8280413150787354, -0.6342591047286987, 0.2287112921476364], 'magnitude': 1.9484169483184814, 'distance': 13.053533554077148, 'cosine_with_motion': 0.9727015971388674, 'motion_component': 1.8952282556125608}]}, 5016: {'frame': 5016, 'ionic_force': [-4.904240369796753, -2.443116396665573, -3.3296403288841248], 'ionic_force_magnitude': 6.411465983075317, 'motion_vector': [1.1025390625, 0.10252761840820312, 0.24944305419921875], 'cosine_ionic_motion': -0.8915613515141652, 'ionic_motion_component': -5.716215277057725, 'ionic_force_x': -4.904240369796753, 'ionic_force_y': -2.443116396665573, 'ionic_force_z': -3.3296403288841248, 'radial_force': 5.479086724299988, 'axial_force': -3.3296403288841248, 'contributions': [{'ion': 1309, 'force': [-1.0098766088485718, -0.4893936812877655, -1.7097877264022827], 'magnitude': 2.045172691345215, 'distance': 12.741015434265137, 'cosine_with_motion': -0.6849855578015981, 'motion_component': -1.4009137019063496}, {'ion': 1320, 'force': [-2.484668016433716, -1.4379808902740479, -2.1973519325256348], 'magnitude': 3.615206718444824, 'distance': 9.583022117614746, 'cosine_with_motion': -0.8371041514779677, 'motion_component': -3.0263045629930083}, {'ion': 1460, 'force': [-1.4096957445144653, -0.5157418251037598, 0.5774993300437927], 'magnitude': 1.608333706855774, 'distance': 14.367491722106934, 'cosine_with_motion': -0.8014488515229483, 'motion_component': -1.288997173785691}]}, 5017: {'frame': 5017, 'ionic_force': [-5.9368895292282104, -3.2834761142730713, -4.590190887451172], 'ionic_force_magnitude': 8.191320104751195, 'motion_vector': [0.5471343994140625, -1.6718521118164062, -0.3502349853515625], 'cosine_ionic_motion': 0.2619658768360037, 'ionic_motion_component': 2.1458463536855326, 'ionic_force_x': -5.9368895292282104, 'ionic_force_y': -3.2834761142730713, 'ionic_force_z': -4.590190887451172, 'radial_force': 6.784384472836232, 'axial_force': -4.590190887451172, 'contributions': [{'ion': 1309, 'force': [-0.9971057176589966, -0.5652839541435242, -2.227571964263916], 'magnitude': 2.5051631927490234, 'distance': 11.512006759643555, 'cosine_with_motion': 0.2625429580884971, 'motion_component': 0.6577129548394858}, {'ion': 1320, 'force': [-3.1286773681640625, -1.8227983713150024, -2.7695655822753906], 'magnitude': 4.558696269989014, 'distance': 8.533923149108887, 'cosine_with_motion': 0.2819798713288931, 'motion_component': 1.2854605198777804}, {'ion': 1460, 'force': [-1.8111064434051514, -0.8953937888145447, 0.40694665908813477], 'magnitude': 2.0609323978424072, 'distance': 12.692207336425781, 'cosine_with_motion': 0.09834044099433077, 'motion_component': 0.20267299659885296}]}, 5018: {'frame': 5018, 'ionic_force': [-5.11282</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{5173: {'frame': 5173, 'ionic_force': [0.15724579244852066, 4.5542712807655334, -5.197363078594208], 'ionic_force_magnitude': 6.912213546237034, 'motion_vector': [-0.32863616943359375, 0.4364585876464844, -0.3377685546875], 'cosine_ionic_motion': 0.8314539168547679, 'ionic_motion_component': 5.747187027155367, 'ionic_force_x': 0.15724579244852066, 'ionic_force_y': 4.5542712807655334, 'ionic_force_z': -5.197363078594208, 'radial_force': 4.5569850930246085, 'axial_force': -5.197363078594208, 'contributions': [{'ion': 1308, 'force': [0.7354629039764404, 2.4643869400024414, -0.565873920917511], 'magnitude': 2.633310079574585, 'distance': 11.22840404510498, 'directional_contribution': 1.595816040795068}, {'ion': 1309, 'force': [-0.48083266615867615, 1.5299593210220337, -3.0795645713806152], 'magnitude': 3.4721310138702393, 'distance': 9.778471946716309, 'directional_contribution': 2.904999593045128}, {'ion': 1403, 'force': [-0.09738444536924362, 0.5599250197410583, -1.5519245862960815], 'magnitude': 1.652715802192688, 'distance': 14.173266410827637, 'directional_contribution': 1.246371467798952}]}, 5174: {'frame': 5174, 'ionic_force': [-0.5605248957872391, 5.194657146930695, -6.168241083621979], 'ionic_force_magnitude': 8.083677943772715, 'motion_vector': [-2.1065216064453125, -0.9170722961425781, 2.1868057250976562], 'cosine_ionic_motion': -0.6658256553908883, 'ionic_motion_component': -5.382320164881336, 'ionic_force_x': -0.5605248957872391, 'ionic_force_y': 5.194657146930695, 'ionic_force_z': -6.168241083621979, 'radial_force': 5.224811100217446, 'axial_force': -6.168241083621979, 'contributions': [{'ion': 1308, 'force': [0.4955497980117798, 2.235003709793091, -0.6512793898582458], 'magnitude': 2.3801209926605225, 'distance': 11.81053352355957, 'directional_contribution': -1.4243362059982232}, {'ion': 1309, 'force': [-0.8381993174552917, 2.3942766189575195, -3.879767417907715], 'magnitude': 4.635486602783203, 'distance': 8.462942123413086, 'directional_contribution': -2.810461728992255}, {'ion': 1403, 'force': [-0.2178753763437271, 0.5653768181800842, -1.637194275856018], 'magnitude': 1.7457164525985718, 'distance': 13.790569305419922, 'directional_contribution': -1.147522273230206}]}, 5175: {'frame': 5175, 'ionic_force': [-3.0609599202871323, 6.934767544269562, -6.165554910898209], 'ionic_force_magnitude': 9.771107607940857, 'motion_vector': [0.8205947875976562, 1.4489250183105469, -0.349456787109375], 'cosine_ionic_motion': 0.5829055047166817, 'ionic_motion_component': 5.6956324118477735, 'ionic_force_x': -3.0609599202871323, 'ionic_force_y': 6.934767544269562, 'ionic_force_z': -6.165554910898209, 'radial_force': 7.580268895405934, 'axial_force': -6.165554910898209, 'contributions': [{'ion': 1308, 'force': [0.23377586901187897, 3.548218250274658, -0.4093410074710846], 'magnitude': 3.5793943405151367, 'distance': 9.630842208862305, 'directional_contribution': 3.218451420795778}, {'ion': 1309, 'force': [-2.680544376373291, 2.8133533000946045, -3.845205307006836], 'magnitude': 5.466797828674316, 'distance': 7.792961597442627, 'directional_contribution': 1.892773534790706}, {'ion': 1403, 'force': [-0.6141914129257202, 0.5731959939002991, -1.911008596420288], 'magnitude': 2.087519645690918, 'distance': 12.611123085021973, 'directional_contribution': 0.5844072358015922}]}, 5176: {'frame': 5176, 'ionic_force': [-0.9744367897510529, 5.9303571581840515, -4.997504740953445], 'ionic_force_magnitude': 7.816246971321807, 'motion_vector': [-0.2884254455566406, 1.5469932556152344, -1.362060546875], 'cosine_ionic_motion': 0.9996707091622106, 'ionic_motion_component': 7.813673152808251, 'ionic_force_x': -0.9744367897510529, 'ionic_force_y': 5.9303571581840515, 'ionic_force_z': -4.997504740953445, 'radial_force': 6.0098804547881945, 'axial_force': -4.997504740953445, 'contributions': [{'ion': 1308, 'force': [0.5721141695976257, 2.9097232818603516, -0.24224546551704407], 'magnitude': 2.9753129482269287, 'distance': 10.563375473022461, 'directional_contribution': 2.242052118813529}, {'ion': 1309, 'force': [-1.1644694805145264, 2.285262107849121, -3.060650587081909], 'magnitude': 3.99324369430542, 'distance': 9.11813735961914, 'directional_contribution': 3.863040438722315}, {'ion': 1403, 'force': [-0.3820814788341522, 0.7353717684745789, -1.6946086883544922], 'magnitude': 1.8863871097564697, 'distance': 13.266416549682617, 'directional_contribution': 1.708580390070872}]}, 5177: {'frame': 5177, 'ionic_force': [-0.9265254437923431, 5.745557546615601, -3.907246023416519], 'ionic_force_magnitude': 7.0097398244849485, 'motion_vector': [1.0473556518554688, -0.16293716430664062, -0.0436553955078125], 'cosine_ionic_motion': -0.23344863634489804, 'ionic_motion_component': -1.6364142031585363, 'ionic_force_x': -0.9265254437923431, 'ionic_force_y': 5.745557546615601, 'ionic_force_z': -3.907246023416519, 'radial_force': 5.819783580122724, 'axial_force': -3.907246023416519, 'contributions': [{'ion': 1308, 'force': [0.689740777015686, 2.4730772972106934, -0.39926019310951233], 'magnitude': 2.5983190536499023, 'distance': 11.303756713867188, 'directional_contribution': 0.3175536045510019}, {'ion': 1309, 'force': [-1.2035044431686401, 2.5528600215911865, -2.146219491958618], 'magnitude': 3.5456700325012207, 'distance': 9.676535606384277, 'directional_contribution': -1.4919688284648274}, {'ion': 1403, 'force': [-0.41276177763938904, 0.7196202278137207, -1.3617663383483887], 'magnitude': 1.594563603401184, 'distance': 14.429394721984863, 'directional_contribution': -0.4619990058729666}]}, 5178: {'frame': 5178, 'ionic_force': [-0.6896159946918488, 5.541051208972931, -4.2868136167526245], 'ionic_force_magnitude': 7.039573119541477, 'motion_vector': [-0.499969482421875, -1.2579994201660156, 0.6877059936523438], 'cosine_ionic_motion': -0.8957020063259677, 'ionic_motion_component': -6.305359766851653, 'ionic_force_x': -0.6896159946918488, 'ionic_force_y': 5.541051208972931, 'ionic_force_z': -4.2868136167526245, 'radial_force': 5.583799666946801, 'axial_force': -4.2868136167526245, 'contributions': [{'ion': 1308, 'force': [0.52821284532547, 2.203639030456543, -0.34880292415618896], 'magnitude': 2.2927489280700684, 'distance': 12.033468246459961, 'directional_contribution': -2.1576581707824296}, {'ion': 1309, 'force': [-0.9532740116119385, 2.5756494998931885, -2.5336785316467285], 'magnitude': 3.7366065979003906, 'distance': 9.426063537597656, 'directional_contribution': -2.9676295725849258}, {'ion': 1403, 'force': [-0.26455482840538025, 0.7617626786231995, -1.404332160949707], 'magnitude': 1.6193888187408447, 'distance': 14.318366050720215, 'directional_contribution': -1.1800719301357088}]}, 5179: {'frame': 5179, 'ionic_force': [-2.030127376317978, 6.3477553725242615, -5.428711324930191], 'ionic_force_magnitude': 8.595715332822024, 'motion_vector': [0.006259918212890625, 2.1265487670898438, -1.1589584350585938], 'cosine_ionic_motion': 0.9500465456928359, 'ionic_motion_component': 8.16632965970651, 'ionic_force_x': -2.030127376317978, 'ionic_force_y': 6.3477553725242615, 'ionic_force_z': -5.428711324930191, 'radial_force': 6.66448913522157, 'axial_force': -5.428711324930191, 'contributions': [{'ion': 1308, 'force': [0.29383471608161926, 2.3622288703918457, -0.319489985704422], 'magnitude': 2.401777982711792, 'distance': 11.75716495513916, 'directional_contribution': 2.2278319278088166}, {'ion': 1309, 'force': [-1.8343040943145752, 3.2689404487609863, -3.492114543914795], 'magnitude': 5.123036861419678, 'distance': 8.050174713134766, 'directional_contribution': 4.53670662706779}, {'ion': 1403, 'force': [-0.489657998085022, 0.7165860533714294, -1.6171067953109741], 'magnitude': 1.8352915048599243, 'distance': 13.449821472167969, 'directional_contribution': 1.4017909947725329}]}, 5180: {'frame': 5180, 'ionic_force': [-0.47080206871032715, 4.05627167224884, -2.3710789382457733], 'ionic_force_magnitude': 4.721970965432023, 'motion_vector': [0.3277015686035156, -0.06797409057617188, 1.3685455322265625], 'cosine_ionic_motion': -0.552400466844324, 'ionic_motion_component': -2.6084189657299928, 'ionic_force_x': -0.47080206871032715, 'ionic_force_y': 4.05627167224884, 'ionic_force_z': -2.3710789382457733, 'radial_force': 4.083502720335855, 'axial_force': -2.3710789382457733, 'contributions': [{'ion': 1308, 'force': [0.32464051246643066, 1.7187424898147583, -0.2759523093700409], 'magnitude': 1.770767331123352, 'distance': 13.69267463684082, 'directional_contribution': -0.27546685084777156}, {'ion': 1309, 'force': [-0.7954425811767578, 2.337529182434082, -2.0951266288757324], 'magnitude': 3.238259792327881, 'distance': 10.125423431396484, 'directional_contribution': -2.332952148085589}]}, 5181: {'frame': 5181, 'ionic_force': [-0.6866850852966309, 5.2680962681770325, -3.737524628639221], 'ionic_force_magnitude': 6.4956497016722174, 'motion_vector': [-0.3796195983886719, -1.8383750915527344, -0.54205322265625], 'cosine_ionic_motion': -0.5829162005149764, 'ionic_motion_component': -3.7864194439750087, 'ionic_force_x': -0.6866850852966309, 'ionic_force_y': 5.2680962681770325, 'ionic_force_z': -3.737524628639221, 'radial_force': 5.312661733740406, 'axial_force': -3.737524628639221, 'contributions': [{'ion': 1308, 'force': [0.3693566620349884, 1.7314714193344116, -0.16969358921051025], 'magnitude': 1.7785425186157227, 'distance': 13.662712097167969, 'directional_contribution': -1.6538194403953677}, {'ion': 1309, 'force': [-0.789997935295105, 2.699798583984375, -2.170147180557251], 'magnitude': 3.5528225898742676, 'distance': 9.666790008544922, 'directional_contribution': -1.7846798437849252}, {'ion': 1403, 'force': [-0.2660438120365143, 0.8368262648582458, -1.39768385887146], 'magnitude': 1.6506295204162598, 'distance': 14.182221412658691, 'directional_contribution': -0.3479201363469171}]}, 5182: {'frame': 5182, 'ionic_force': [-1.5095845460891724, 5.511749029159546, -4.918577492237091], 'ionic_force_magnitude': 7.53993550432454, 'motion_vector': [3.399822235107422, 1.0570564270019531, -0.6069412231445312], 'cosine_ionic_motion': 0.1351049295348629, 'ionic_motion_component': 1.018682455009178, 'ionic_force_x': -1.5095845460891724, 'ionic_force_y': 5.511749029159546, 'ionic_force_z': -4.918577492237091, 'radial_force': 5.714737339741211, 'axial_force': -4.918577492237091, 'contributions': [{'ion': 1308, 'force': [0.24988240003585815, 2.1664843559265137, -0.3289939761161804], 'magnitude': 2.2055232524871826, 'distance': 12.26911449432373, 'directional_contribution': 0.9245816354512906}, {'ion': 1309, 'force': [-1.407989263534546, 2.6396069526672363, -3.090088129043579], 'magnitude': 4.301000118255615, 'distance': 8.785860061645508, 'directional_contribution': -0.033556814397886825}, {'ion': 1403, 'force': [-0.3514776825904846, 0.7056577205657959, -1.4994953870773315], 'magnitude': 1.694100260734558, 'distance': 13.999079704284668, 'directional_contribution': 0.12765764161992088}]}, 5183: {'frame': 5183, 'ionic_force': [0.906077116727829, 3.351901054382324, -2.439151182770729], 'ionic_force_magnitude': 4.243309429235511, 'motion_vector': [-0.3704338073730469, 0.2990570068359375, 0.07714080810546875], 'cosine_ionic_motion': 0.23386514195069716, 'ionic_motion_component': 0.9923621620088946, 'ionic_force_x': 0.906077116727829, 'ionic_force_y': 3.351901054382324, 'ionic_force_z': -2.439151182770729, 'radial_force': 3.472206275529602, 'axial_force': -2.439151182770729, 'contributions': [{'ion': 1308, 'force': [0.6261655688285828, 1.4340345859527588, -0.20961131155490875], 'magnitude': 1.5787575244903564, 'distance': 14.501446723937988, 'directional_contribution': 0.37474197496300743}, {'ion': 1309, 'force': [0.2799115478992462, 1.9178664684295654, -2.2295398712158203], 'magnitude': 2.954219102859497, 'distance': 10.601020812988281, 'directional_contribution': 0.6176201873585594}]}, 5184: {'frame': 5184, 'ionic_force': [0.7254925360903144, 4.958870887756348, -4.047217309474945], 'ionic_force_magnitude': 6.441793838013896, 'motion_vector': [-0.18041229248046875, 0.4036216735839844, 0.16362762451171875], 'cosine_ionic_motion': 0.3979180144561937, 'ionic_motion_component': 2.563305813558633, 'ionic_force_x': 0.7254925360903144, 'ionic_force_y': 4.958870887756348, 'ionic_force_z': -4.047217309474945, 'radial_force': 5.011660393657992, 'axial_force': -4.047217309474945, 'contributions': [{'ion': 1308, 'force': [0.5973078608512878, 1.5048673152923584, -0.26393312215805054], 'magnitude': 1.6404459476470947, 'distance': 14.22617244720459, 'directional_contribution': 0.9682501389175826}, {'ion': 1309, 'force': [0.1381777822971344, 2.6733298301696777, -2.3793797492980957], 'magnitude': 3.581512689590454, 'distance': 9.6279935836792, 'directional_contribution': 1.410118846732325}, {'ion': 1403, 'force': [-0.009993107058107853, 0.7806737422943115, -1.4039044380187988], 'magnitude': 1.6063930988311768, 'distance': 14.376167297363281, 'directional_contribution': 0.18493679439559696}]}, 5185: {'frame': 5185, 'ionic_force': [0.7339238412678242, 5.119778215885162, -3.856375366449356], 'ionic_force_magnitude': 6.45154277298004, 'motion_vector': [-0.11819076538085938, -0.16250991821289062, 0.146270751953125], 'cosine_ionic_motion': -0.924755423083406, 'ionic_motion_component': -5.966099166567847, 'ionic_force_x': 0.7339238412678242, 'ionic_force_y': 5.119778215885162, 'ionic_force_z': -3.856375366449356, 'radial_force': 5.172114962433992, 'axial_force': -3.856375366449356, 'contributions': [{'ion': 1308, 'force': [0.8244546055793762, 1.679525375366211, -0.2533508837223053], 'magnitude': 1.8880459070205688, 'distance': 13.260587692260742, 'directional_contribution': -1.6393144610569834}, {'ion': 1309, 'force': [-0.028522875159978867, 2.627678871154785, -2.242663860321045], 'magnitude': 3.454714298248291, 'distance': 9.803089141845703, 'directional_contribution': -3.024380502198848}, {'ion': 1403, 'force': [-0.06200788915157318, 0.8125739693641663, -1.3603606224060059], 'magnitude': 1.5857813358306885, 'distance': 14.469295501708984, 'directional_contribution': -1.302404121518519}]}, 5186: {'frame': 5186, 'ionic_force': [0.6085753031075001, 5.361973226070404, -3.9645311534404755], 'ionic_force_magnitude': 6.696165174429937, 'motion_vector': [0.29323577880859375, 0.5634040832519531, 0.6587371826171875], 'cosine_ionic_motion': 0.09593404861098064, 'ionic_motion_component': 0.6423902353509172, 'ionic_force_x': 0.6085753031075001, 'ionic_force_y': 5.361973226070404, 'ionic_force_z': -3.9645311534404755, 'radial_force': 5.396398871159196, 'axial_force': -3.9645311534404755, 'contributions': [{'ion': 1308, 'force': [0.7067315578460693, 1.7726627588272095, -0.21329709887504578], 'magnitude': 1.920233964920044, 'distance': 13.148977279663086, 'directional_contribution': 1.1643503887190967}, {'ion': 1309, 'force': [-0.05736168473958969, 2.774033784866333, -2.3771002292633057], 'magnitude': 3.6536500453948975, 'distance': 9.532472610473633, 'directional_contribution': -0.021640899696546034}, {'ion': 1403, 'force': [-0.04079456999897957, 0.8152766823768616, -1.374133825302124], 'magnitude': 1.598306655883789, 'distance': 14.41248893737793, 'directional_contribution': -0.5003192851393142}]}, 5187: {'frame': 5187, 'ionic_force': [0.44809454679489136, 5.63523006439209, -3.661033511161804], 'ionic_force_magnitude': 6.7349664417386315, 'motion_vector': [-0.44336700439453125, -0.58660888671875, -0.7073516845703125], 'cosine_ionic_motion': -0.1331114322693107, 'ionic_motion_component': -0.8965010293455722, 'ionic_force_x': 0.44809454679489136, 'ionic_force_y': 5.63523006439209, 'ionic_force_z': -3.661033511161804, 'radial_force': 5.653017477550887, 'axial_force': -3.661033511161804, 'contributions': [{'ion': 1308, 'force': [0.5526303648948669, 1.42279052734375, -0.1382688283920288], 'magnitude': 1.5325963497161865, 'distance': 14.718214988708496, 'directional_contribution': -0.962291660716259}, {'ion': 1309, 'force': [-0.0501912422478199, 3.1493821144104004, -2.052255630493164], 'magnitude': 3.7593722343444824, 'distance': 9.397479057312012, 'directional_contribution': -0.36610075432767797}, {'ion': 1403, 'force': [-0.054344575852155685, 1.0630574226379395, -1.4705090522766113], 'magnitude': 1.8153350353240967, 'distance': 13.523548126220703, 'directional_contribution': 0.43189137043733694}]}, 5188: {'frame': 5188, 'ionic_force': [0.6004464058205485, 5.34605211019516, -4.232802301645279], 'ionic_force_magnitude': 6.845248306380018, 'motion_vector': [0.09778976440429688, 0.3133354187011719, -0.27387237548828125], 'cosine_ionic_motion': 0.9886528166637947, 'ionic_motion_component': 6.767574018865675, 'ionic_force_x': 0.6004464058205485, 'ionic_force_y': 5.34605211019516, 'ionic_force_z': -4.232802301645279, 'radial_force': 5.37966625834586, 'axial_force': -4.232802301645279, 'contributions': [{'ion': 1308, 'force': [0.7558067440986633, 2.0558364391326904, -0.4618763029575348], 'magnitude': 2.238534450531006, 'distance': 12.178313255310059, 'directional_contribution': 1.975650853246151}, {'ion': 1309, 'force': [-0.012659800238907337, 2.442432165145874, -2.3873846530914307], 'magnitude': 3.4154415130615234, 'distance': 9.859289169311523, 'directional_contribution': 3.3168027721633653}, {'ion': 1403, 'force': [-0.14270053803920746, 0.8477835059165955, -1.3835413455963135], 'magnitude': 1.6288913488388062, 'distance': 14.276540756225586, 'directional_contribution': 1.4751202866299886}]}, 5189: {'frame': 5189, 'ionic_force': [0.32750216871500015, 4.727729856967926, -3.834524780511856], 'ionic_force_magnitude': 6.096086249663672, 'motion_vector': [-0.000904083251953125, -0.1085205078125, 0.5684127807617188], 'cosine_ionic_motion': -0.7633747994882957, 'ionic_motion_component': -4.653598618500362, 'ionic_force_x': 0.32750216871500015, 'ionic_force_y': 4.727729856967926, 'ionic_force_z': -3.834524780511856, 'radial_force': 4.739059745453627, 'axial_force': -3.834524780511856, 'contributions': [{'ion': 1308, 'force': [0.5216655135154724, 1.448395848274231, -0.2568974792957306], 'magnitude': 1.5607632398605347, 'distance': 14.58480167388916, 'directional_contribution': -0.5247737514062334}, {'ion': 1309, 'force': [-0.11025428026914597, 2.4549198150634766, -2.214020013809204], 'magnitude': 3.307668685913086, 'distance': 10.018623352050781, 'directional_contribution': -2.6349391937450988}, {'ion': 1403, 'force': [-0.0839090645313263, 0.8244141936302185, -1.3636072874069214], 'magnitude': 1.5956579446792603, 'distance': 14.424446105957031, 'directional_contribution': -1.4938856029452705}]}, 5190: {'frame': 5190, 'ionic_force': [0.34706735610961914, 4.918230354785919, -3.804109513759613], 'ionic_force_magnitude': 6.227414773811919, 'motion_vector': [0.3770256042480469, -0.35123443603515625, -0.49456024169921875], 'cosine_ionic_motion': 0.06402448857565023, 'ionic_motion_component': 0.39870704604175666, 'ionic_force_x': 0.34706735610961914, 'ionic_force_y': 4.918230354785919, 'ionic_force_z': -3.804109513759613, 'radial_force': 4.930460989848165, 'axial_force': -3.804109513759613, 'contributions': [{'ion': 1308, 'force': [0.5309812426567078, 1.4431406259536743, -0.21502536535263062], 'magnitude': 1.5526853799819946, 'distance': 14.62269115447998, 'directional_contribution': -0.28050943300189246}, {'ion': 1309, 'force': [-0.07559871673583984, 2.564948797225952, -2.245485782623291], 'magnitude': 3.4098215103149414, 'distance': 9.867410659790039, 'directional_contribution': 0.25360268929463814}, {'ion': 1403, 'force': [-0.10831516981124878, 0.9101409316062927, -1.3435983657836914], 'magnitude': 1.6264517307281494, 'distance': 14.287243843078613, 'directional_contribution': 0.4256137020260162}]}, 5191: {'frame': 5191, 'ionic_force': [0.657955770380795, 5.201777338981628, -4.198868662118912], 'ionic_force_magnitude': 6.717283031244436, 'motion_vector': [-0.9679679870605469, 0.518524169921875, 1.3073348999023438], 'cosine_ionic_motion': -0.2989874499026258, 'ionic_motion_component': -2.0083833237859543, 'ionic_force_x': 0.657955770380795, 'ionic_force_y': 5.201777338981628, 'ionic_force_z': -4.198868662118912, 'radial_force': 5.243223558090975, 'axial_force': -4.198868662118912, 'contributions': [{'ion': 1308, 'force': [0.6094868183135986, 1.5151386260986328, -0.26498427987098694], 'magnitude': 1.6544896364212036, 'distance': 14.165666580200195, 'directional_contribution': -0.08829664447299024}, {'ion': 1309, 'force': [0.05508818104863167, 2.8828670978546143, -2.548942804336548], 'magnitude': 3.8485147953033447, 'distance': 9.288005828857422, 'directional_contribution': -1.1074697614626865}, {'ion': 1403, 'force': [-0.006619228981435299, 0.8037716150283813, -1.384941577911377], 'magnitude': 1.601298213005066, 'distance': 14.399020195007324, 'directional_contribution': -0.8126170453461972}]}, 5192: {'frame': 5192, 'ionic_force': [0.1945376694202423, 5.99289608001709, -3.5691631473600864], 'ionic_force_magnitude': 6.977934787828059, 'motion_vector': [-2.582378387451172, -1.3664169311523438, 0.01790618896484375], 'cosine_ionic_motion': -0.4294408475329646, 'ionic_motion_component': -2.996610229314639, 'ionic_force_x': 0.1945376694202423, 'ionic_force_y': 5.99289608001709, 'ionic_force_z': -3.5691631473600864, 'radial_force': 5.996052729146706, 'axial_force': -3.5691631473600864, 'contributions': [{'ion': 1308, 'force': [0.6152461171150208, 1.7376521825790405, -0.03967398777604103], 'magnitude': 1.8437833786010742, 'distance': 13.41881275177002, 'directional_contribution': -1.356717336705017}, {'ion': 1309, 'force': [-0.2750970125198364, 3.165602922439575, -1.957560658454895], 'magnitude': 3.732125997543335, 'distance': 9.431719779968262, 'directional_contribution': -1.2493521061189088}, {'ion': 1403, 'force': [-0.14561143517494202, 1.0896409749984741, -1.5719285011291504], 'magnitude': 1.9181969165802002, 'distance': 13.155957221984863, 'directional_contribution': -0.39054084032030834}]}, 5193: {'frame': 5193, 'ionic_force': [-1.93711456656456, 6.59854257106781, -4.372821029275656], 'ionic_force_magnitude': 8.149523952984381, 'motion_vector': [0.4185295104980469, 1.0166091918945312, -0.2987213134765625], 'cosine_ionic_motion': 0.7758910631739562, 'ionic_motion_component': 6.323142804242674, 'ionic_force_x': -1.93711456656456, 'ionic_force_y': 6.59854257106781, 'ionic_force_z': -4.372821029275656, 'radial_force': 6.877003483072463, 'axial_force': -4.372821029275656, 'contributions': [{'ion': 1308, 'force': [0.4174995720386505, 2.2765603065490723, -0.059432800859212875], 'magnitude': 2.3152894973754883, 'distance': 11.974748611450195, 'directional_contribution': 2.2004450859416735}, {'ion': 1309, 'force': [-1.7871077060699463, 3.376755714416504, -2.6929991245269775], 'magnitude': 4.674235820770264, 'distance': 8.427790641784668, 'directional_contribution': 3.062833615510769}, {'ion': 1403, 'force': [-0.5675064325332642, 0.9452265501022339, -1.6203891038894653], 'magnitude': 1.9598922729492188, 'distance': 13.015262603759766, 'directional_contribution': 1.0598641965006337}]}, 5194: {'frame': 5194, 'ionic_force': [-0.9560555219650269, 5.772682011127472, -3.487354025244713], 'ionic_force_magnitude': 6.811720624046837, 'motion_vector': [-0.6451492309570312, -1.4054031372070312, -0.01318359375], 'cosine_ionic_motion': -0.7072447724738669, 'ionic_motion_component': -4.8175538029095515, 'ionic_force_x': -0.9560555219650269, 'ionic_force_y': 5.772682011127472, 'ionic_force_z': -3.487354025244713, 'radial_force': 5.8513160709941605, 'axial_force': -3.487354025244713, 'contributions': [{'ion': 1308, 'force': [0.6240898370742798, 2.3083484172821045, -0.197579488158226], 'magnitude': 2.3993747234344482, 'distance': 11.763051986694336, 'directional_contribution': -2.3564645829506077}, {'ion': 1309, 'force': [-1.1822179555892944, 2.5775022506713867, -1.9253954887390137], 'magnitude': 3.4275801181793213, 'distance': 9.841815948486328, 'directional_contribution': -1.832787666237321}, {'ion': 1403, 'force': [-0.3979274034500122, 0.8868313431739807, -1.3643790483474731], 'magnitude': 1.675215244293213, 'distance': 14.077766418457031, 'directional_contribution': -0.6283016794686191}]}, 5195: {'frame': 5195, 'ionic_force': [-2.697285771369934, 7.435713529586792, -4.3827709555625916], 'ionic_force_magnitude': 9.042890438097643, 'motion_vector': [0.4557342529296875, 0.3656768798828125, 0.8678741455078125], 'cosine_ionic_motion': -0.24456839884992476, 'ionic_motion_component': -2.2116052354208353, 'ionic_force_x': -2.697285771369934, 'ionic_force_y': 7.435713529586792, 'ionic_force_z': -4.3827709555625916, 'radial_force': 7.90981581495516, 'axial_force': -4.3827709555625916, 'contributions': [{'ion': 1308, 'force': [-0.6983073353767395, 3.93900203704834, -0.37639325857162476], 'magnitude': 4.018089294433594, 'distance': 9.089902877807617, 'directional_contribution': 0.760339042032788}, {'ion': 1309, 'force': [-1.4922806024551392, 2.734032154083252, -2.6263973712921143], 'magnitude': 4.074284553527832, 'distance': 9.026997566223145, 'directional_contribution': -1.8730815485615615}, {'ion': 1403, 'force': [-0.5066978335380554, 0.7626793384552002, -1.3799803256988525], 'magnitude': 1.6561305522918701, 'distance': 14.158647537231445, 'directional_contribution': -1.0988628374351261}]}, 5196: {'frame': 5196, 'ionic_force': [-2.689316511154175, 6.572674095630646, -2.8800116777420044], 'ionic_force_magnitude': 7.66335013740537, 'motion_vector': [0.2856636047363281, 0.22528839111328125, 0.144744873046875], 'cosine_ionic_motion': 0.09852816387166814, 'ionic_motion_component': 0.7550558181442468, 'ionic_force_x': -2.689316511154175, 'ionic_force_y': 6.572674095630646, 'ionic_force_z': -2.8800116777420044, 'radial_force': 7.101582081799843, 'axial_force': -2.8800116777420044, 'contributions': [{'ion': 1308, 'force': [-0.6410857439041138, 2.2917823791503906, 1.5949033498764038], 'magnitude': 2.864781618118286, 'distance': 10.765229225158691, 'directional_contribution': 1.4405170996993455}, {'ion': 1309, 'force': [-1.6070647239685059, 3.372495651245117, -2.893615961074829], 'magnitude': 4.725399017333984, 'distance': 8.382040977478027, 'directional_contribution': -0.30170480085153173}, {'ion': 1403, 'force': [-0.4411660432815552, 0.9083960652351379, -1.581299066543579], 'magnitude': 1.876250982284546, 'distance': 13.302203178405762, 'directional_contribution': -0.3837563310297796}]}, 5197: {'frame': 5197, 'ionic_force': [-2.394786536693573, 9.815348863601685, -3.377447187900543], 'ionic_force_magnitude': 10.652850575202534, 'motion_vector': [-0.7711677551269531, -0.23419952392578125, -1.1207962036132812], 'cosine_ionic_motion': 0.22667240517304837, 'ionic_motion_component': 2.4147072618302503, 'ionic_force_x': -2.394786536693573, 'ionic_force_y': 9.815348863601685, 'ionic_force_z': -3.377447187900543, 'radial_force': 10.10327055316919, 'axial_force': -3.377447187900543, 'contributions': [{'ion': 1308, 'force': [-0.5111057162284851, 5.275302886962891, 0.6245482563972473], 'magnitude': 5.336676120758057, 'distance': 7.88739538192749, 'directional_contribution': -1.1165053118480337}, {'ion': 1309, 'force': [-1.4601268768310547, 3.5319414138793945, -2.432771682739258], 'magnitude': 4.530447959899902, 'distance': 8.560486793518066, 'directional_contribution': 2.191598932025954}, {'ion': 1403, 'force': [-0.4235539436340332, 1.0081045627593994, -1.5692237615585327], 'magnitude': 1.9126254320144653, 'distance': 13.175105094909668, 'directional_contribution': 1.3396134605632426}]}, 5198: {'frame': 5198, 'ionic_force': [-2.4582442939281464, 7.281810879707336, -3.801115170121193], 'ionic_force_magnitude': 8.574159505921259, 'motion_vector': [1.0001983642578125, 2.0919723510742188, -0.8253173828125], 'cosine_ionic_motion': 0.7539895480987615, 'ionic_motion_component': 6.46482665119627, 'ionic_force_x': -2.4582442939281464, 'ionic_force_y': 7.281810879707336, 'ionic_force_z': -3.801115170121193, 'radial_force': 7.685553636300668, 'axial_force': -3.801115170121193, 'contributions': [{'ion': 1308, 'force': [-0.5375314950942993, 3.8752388954162598, -0.03662027418613434], 'magnitude': 3.912513017654419, 'distance': 9.211729049682617, 'directional_contribution': 3.087613531795399}, {'ion': 1309, 'force': [-1.4404795169830322, 2.623394727706909, -2.3200292587280273], 'magnitude': 3.7867817878723145, 'distance': 9.363407135009766, 'directional_contribution': 2.4223441302027737}, {'ion': 1403, 'force': [-0.4802332818508148, 0.7831772565841675, -1.4444656372070312], 'magnitude': 1.7118620872497559, 'distance': 13.926264762878418, 'directional_contribution': 0.954869117280472}]}, 5199: {'frame': 5199, 'ionic_force': [-1.14464071393013, 4.792068958282471, -1.1551509499549866], 'ionic_force_magnitude': 5.060484263596008, 'motion_vector': [0.4618873596191406, -1.79718017578125, 1.5188522338867188], 'cosine_ionic_motion': -0.8978699993094448, 'ionic_motion_component': -4.543657002260404, 'ionic_force_x': -1.14464071393013, 'ionic_force_y': 4.792068958282471, 'ionic_force_z': -1.1551509499549866, 'radial_force': 4.926878044453802, 'axial_force': -1.1551509499549866, 'contributions': [{'ion': 1308, 'force': [-0.3644380271434784, 2.3148305416107178, 0.5557435154914856], 'magnitude': 2.4083409309387207, 'distance': 11.741133689880371, 'directional_contribution': -1.4530834354263638}, {'ion': 1309, 'force': [-0.7802026867866516, 2.477238416671753, -1.7108944654464722], 'magnitude': 3.1100780963897705, 'distance': 10.331975936889648, 'directional_contribution': -3.0905737117048435}]}, 5200: {'frame': 5200, 'ionic_force': [-1.6555381119251251, 7.148874580860138, -3.147367298603058], 'ionic_force_magnitude': 7.984556038078806, 'motion_vector': [-1.8232803344726562, -0.8938713073730469, -0.5885772705078125], 'cosine_ionic_motion': -0.08999526784902638, 'ionic_motion_component': -0.718572259302463, 'ionic_force_x': -1.6555381119251251, 'ionic_force_y': 7.148874580860138, 'ionic_force_z': -3.147367298603058, 'radial_force': 7.338066108512844, 'axial_force': -3.147367298603058, 'contributions': [{'ion': 1308, 'force': [-0.19619184732437134, 2.808659076690674, 0.9512656331062317], 'magnitude': 2.9718620777130127, 'distance': 10.569506645202637, 'directional_contribution': -1.2831232899199367}, {'ion': 1309, 'force': [-1.1075390577316284, 3.3808846473693848, -2.5640246868133545], 'magnitude': 4.385344505310059, 'distance': 8.700960159301758, 'directional_contribution': 0.23952728061865258}, {'ion': 1403, 'force': [-0.35180720686912537, 0.9593308568000793, -1.534608244895935], 'magnitude': 1.8436665534973145, 'distance': 13.419238090515137, 'directional_contribution': 0.3250237242425431}]}, 5201: {'frame': 5201, 'ionic_force': [-4.156924664974213, 6.935702562332153, -3.2922180891036987], 'ionic_force_magnitude': 8.73056084393399, 'motion_vector': [1.1770477294921875, 1.5356216430664062, -0.2644500732421875], 'cosine_ionic_motion': 0.38877692353487286, 'ionic_motion_component': 3.3942405856386797, 'ionic_force_x': -4.156924664974213, 'ionic_force_y': 6.935702562332153, 'ionic_force_z': -3.2922180891036987, 'radial_force': 8.086036897232894, 'axial_force': -3.2922180891036987, 'contributions': [{'ion': 1308, 'force': [-1.71828031539917, 3.6425421237945557, 1.0551244020462036], 'magnitude': 4.163398265838623, 'distance': 8.929868698120117, 'directional_contribution': 1.6857874149521965}, {'ion': 1309, 'force': [-1.858840823173523, 2.5847413539886475, -2.804428815841675], 'magnitude': 4.242758274078369, 'distance': 8.845958709716797, 'directional_contribution': 1.2919115454045773}, {'ion': 1403, 'force': [-0.5798035264015198, 0.7084190845489502, -1.5429136753082275], 'magnitude': 1.7940491437911987, 'distance': 13.603537559509277, 'directional_contribution': 0.41654148549958236}]}, 5202: {'frame': 5202, 'ionic_force': [-4.524553209543228, 6.495882093906403, -3.208431661128998], 'ionic_force_magnitude': 8.541785507027013, 'motion_vector': [-0.5452957153320312, -2.3845901489257812, 0.18315887451171875], 'cosine_ionic_motion': -0.6495728386876835, 'ionic_motion_component': -5.54851185926085, 'ionic_force_x': -4.524553209543228, 'ionic_force_y': 6.495882093906403, 'ionic_force_z': -3.208431661128998, 'radial_force': 7.916316436570847, 'axial_force': -3.208431661128998, 'contributions': [{'ion': 1308, 'force': [-3.1942861080169678, 3.2119216918945312, 0.43542641401290894], 'magnitude': 4.550769329071045, 'distance': 8.541352272033691, 'directional_contribution': -2.379761757023173}, {'ion': 1309, 'force': [-0.9592924118041992, 2.4764177799224854, -2.2959697246551514], 'magnitude': 3.5106072425842285, 'distance': 9.724738121032715, 'directional_contribution': -2.365549109757348}, {'ion': 1403, 'force': [-0.37097468972206116, 0.807542622089386, -1.3478883504867554], 'magnitude': 1.6144814491271973, 'distance': 14.340110778808594, 'directional_contribution</t>
+          <t>{5173: {'frame': 5173, 'ionic_force': [0.15724579244852066, 4.5542712807655334, -5.197363078594208], 'ionic_force_magnitude': 6.912213546237034, 'motion_vector': [-0.32863616943359375, 0.4364585876464844, -0.3377685546875], 'cosine_ionic_motion': 0.8314539168547679, 'ionic_motion_component': 5.747187027155367, 'ionic_force_x': 0.15724579244852066, 'ionic_force_y': 4.5542712807655334, 'ionic_force_z': -5.197363078594208, 'radial_force': 4.5569850930246085, 'axial_force': -5.197363078594208, 'contributions': [{'ion': 1308, 'force': [0.7354629039764404, 2.4643869400024414, -0.565873920917511], 'magnitude': 2.633310079574585, 'distance': 11.22840404510498, 'cosine_with_motion': 0.6060114431838383, 'motion_component': 1.5958160407950677}, {'ion': 1309, 'force': [-0.48083266615867615, 1.5299593210220337, -3.0795645713806152], 'magnitude': 3.4721310138702393, 'distance': 9.778471946716309, 'cosine_with_motion': 0.8366618689570267, 'motion_component': 2.904999593045128}, {'ion': 1403, 'force': [-0.09738444536924362, 0.5599250197410583, -1.5519245862960815], 'magnitude': 1.652715802192688, 'distance': 14.173266410827637, 'cosine_with_motion': 0.7541353633832589, 'motion_component': 1.246371467798952}]}, 5174: {'frame': 5174, 'ionic_force': [-0.5605248957872391, 5.194657146930695, -6.168241083621979], 'ionic_force_magnitude': 8.083677943772715, 'motion_vector': [-2.1065216064453125, -0.9170722961425781, 2.1868057250976562], 'cosine_ionic_motion': -0.6658256553908883, 'ionic_motion_component': -5.382320164881336, 'ionic_force_x': -0.5605248957872391, 'ionic_force_y': 5.194657146930695, 'ionic_force_z': -6.168241083621979, 'radial_force': 5.224811100217446, 'axial_force': -6.168241083621979, 'contributions': [{'ion': 1308, 'force': [0.4955497980117798, 2.235003709793091, -0.6512793898582458], 'magnitude': 2.3801209926605225, 'distance': 11.81053352355957, 'cosine_with_motion': -0.5984301635066598, 'motion_component': -1.4243362059982232}, {'ion': 1309, 'force': [-0.8381993174552917, 2.3942766189575195, -3.879767417907715], 'magnitude': 4.635486602783203, 'distance': 8.462942123413086, 'cosine_with_motion': -0.6062927398856023, 'motion_component': -2.8104617289922547}, {'ion': 1403, 'force': [-0.2178753763437271, 0.5653768181800842, -1.637194275856018], 'magnitude': 1.7457164525985718, 'distance': 13.790569305419922, 'cosine_with_motion': -0.6573360244306076, 'motion_component': -1.147522273230206}]}, 5175: {'frame': 5175, 'ionic_force': [-3.0609599202871323, 6.934767544269562, -6.165554910898209], 'ionic_force_magnitude': 9.771107607940857, 'motion_vector': [0.8205947875976562, 1.4489250183105469, -0.349456787109375], 'cosine_ionic_motion': 0.5829055047166817, 'ionic_motion_component': 5.6956324118477735, 'ionic_force_x': -3.0609599202871323, 'ionic_force_y': 6.934767544269562, 'ionic_force_z': -6.165554910898209, 'radial_force': 7.580268895405934, 'axial_force': -6.165554910898209, 'contributions': [{'ion': 1308, 'force': [0.23377586901187897, 3.548218250274658, -0.4093410074710846], 'magnitude': 3.5793943405151367, 'distance': 9.630842208862305, 'cosine_with_motion': 0.8991608912132001, 'motion_component': 3.218451420795778}, {'ion': 1309, 'force': [-2.680544376373291, 2.8133533000946045, -3.845205307006836], 'magnitude': 5.466797828674316, 'distance': 7.792961597442627, 'cosine_with_motion': 0.34623075238245715, 'motion_component': 1.892773534790706}, {'ion': 1403, 'force': [-0.6141914129257202, 0.5731959939002991, -1.911008596420288], 'magnitude': 2.087519645690918, 'distance': 12.611123085021973, 'cosine_with_motion': 0.2799529169991263, 'motion_component': 0.5844072358015922}]}, 5176: {'frame': 5176, 'ionic_force': [-0.9744367897510529, 5.9303571581840515, -4.997504740953445], 'ionic_force_magnitude': 7.816246971321807, 'motion_vector': [-0.2884254455566406, 1.5469932556152344, -1.362060546875], 'cosine_ionic_motion': 0.9996707091622106, 'ionic_motion_component': 7.813673152808251, 'ionic_force_x': -0.9744367897510529, 'ionic_force_y': 5.9303571581840515, 'ionic_force_z': -4.997504740953445, 'radial_force': 6.0098804547881945, 'axial_force': -4.997504740953445, 'contributions': [{'ion': 1308, 'force': [0.5721141695976257, 2.9097232818603516, -0.24224546551704407], 'magnitude': 2.9753129482269287, 'distance': 10.563375473022461, 'cosine_with_motion': 0.7535516993446264, 'motion_component': 2.242052118813529}, {'ion': 1309, 'force': [-1.1644694805145264, 2.285262107849121, -3.060650587081909], 'magnitude': 3.99324369430542, 'distance': 9.11813735961914, 'cosine_with_motion': 0.9673941460377422, 'motion_component': 3.863040438722315}, {'ion': 1403, 'force': [-0.3820814788341522, 0.7353717684745789, -1.6946086883544922], 'magnitude': 1.8863871097564697, 'distance': 13.266416549682617, 'cosine_with_motion': 0.905742166955266, 'motion_component': 1.708580390070872}]}, 5177: {'frame': 5177, 'ionic_force': [-0.9265254437923431, 5.745557546615601, -3.907246023416519], 'ionic_force_magnitude': 7.0097398244849485, 'motion_vector': [1.0473556518554688, -0.16293716430664062, -0.0436553955078125], 'cosine_ionic_motion': -0.23344863634489804, 'ionic_motion_component': -1.6364142031585363, 'ionic_force_x': -0.9265254437923431, 'ionic_force_y': 5.745557546615601, 'ionic_force_z': -3.907246023416519, 'radial_force': 5.819783580122724, 'axial_force': -3.907246023416519, 'contributions': [{'ion': 1308, 'force': [0.689740777015686, 2.4730772972106934, -0.39926019310951233], 'magnitude': 2.5983190536499023, 'distance': 11.303756713867188, 'cosine_with_motion': 0.12221501182130788, 'motion_component': 0.3175536045510019}, {'ion': 1309, 'force': [-1.2035044431686401, 2.5528600215911865, -2.146219491958618], 'magnitude': 3.5456700325012207, 'distance': 9.676535606384277, 'cosine_with_motion': -0.42078615680419346, 'motion_component': -1.4919688284648274}, {'ion': 1403, 'force': [-0.41276177763938904, 0.7196202278137207, -1.3617663383483887], 'magnitude': 1.594563603401184, 'distance': 14.429394721984863, 'cosine_with_motion': -0.2897338193037402, 'motion_component': -0.46199900587296655}]}, 5178: {'frame': 5178, 'ionic_force': [-0.6896159946918488, 5.541051208972931, -4.2868136167526245], 'ionic_force_magnitude': 7.039573119541477, 'motion_vector': [-0.499969482421875, -1.2579994201660156, 0.6877059936523438], 'cosine_ionic_motion': -0.8957020063259677, 'ionic_motion_component': -6.305359766851653, 'ionic_force_x': -0.6896159946918488, 'ionic_force_y': 5.541051208972931, 'ionic_force_z': -4.2868136167526245, 'radial_force': 5.583799666946801, 'axial_force': -4.2868136167526245, 'contributions': [{'ion': 1308, 'force': [0.52821284532547, 2.203639030456543, -0.34880292415618896], 'magnitude': 2.2927489280700684, 'distance': 12.033468246459961, 'cosine_with_motion': -0.9410791659335338, 'motion_component': -2.1576581707824296}, {'ion': 1309, 'force': [-0.9532740116119385, 2.5756494998931885, -2.5336785316467285], 'magnitude': 3.7366065979003906, 'distance': 9.426063537597656, 'cosine_with_motion': -0.794204453800667, 'motion_component': -2.9676295725849258}, {'ion': 1403, 'force': [-0.26455482840538025, 0.7617626786231995, -1.404332160949707], 'magnitude': 1.6193888187408447, 'distance': 14.318366050720215, 'cosine_with_motion': -0.7287143440952004, 'motion_component': -1.1800719301357088}]}, 5179: {'frame': 5179, 'ionic_force': [-2.030127376317978, 6.3477553725242615, -5.428711324930191], 'ionic_force_magnitude': 8.595715332822024, 'motion_vector': [0.006259918212890625, 2.1265487670898438, -1.1589584350585938], 'cosine_ionic_motion': 0.9500465456928359, 'ionic_motion_component': 8.16632965970651, 'ionic_force_x': -2.030127376317978, 'ionic_force_y': 6.3477553725242615, 'ionic_force_z': -5.428711324930191, 'radial_force': 6.66448913522157, 'axial_force': -5.428711324930191, 'contributions': [{'ion': 1308, 'force': [0.29383471608161926, 2.3622288703918457, -0.319489985704422], 'magnitude': 2.401777982711792, 'distance': 11.75716495513916, 'cosine_with_motion': 0.9275760945020237, 'motion_component': 2.2278319278088166}, {'ion': 1309, 'force': [-1.8343040943145752, 3.2689404487609863, -3.492114543914795], 'magnitude': 5.123036861419678, 'distance': 8.050174713134766, 'cosine_with_motion': 0.885550252509541, 'motion_component': 4.53670662706779}, {'ion': 1403, 'force': [-0.489657998085022, 0.7165860533714294, -1.6171067953109741], 'magnitude': 1.8352915048599243, 'distance': 13.449821472167969, 'cosine_with_motion': 0.7637974619760005, 'motion_component': 1.4017909947725329}]}, 5180: {'frame': 5180, 'ionic_force': [-0.47080206871032715, 4.05627167224884, -2.3710789382457733], 'ionic_force_magnitude': 4.721970965432023, 'motion_vector': [0.3277015686035156, -0.06797409057617188, 1.3685455322265625], 'cosine_ionic_motion': -0.552400466844324, 'ionic_motion_component': -2.6084189657299928, 'ionic_force_x': -0.47080206871032715, 'ionic_force_y': 4.05627167224884, 'ionic_force_z': -2.3710789382457733, 'radial_force': 4.083502720335855, 'axial_force': -2.3710789382457733, 'contributions': [{'ion': 1308, 'force': [0.32464051246643066, 1.7187424898147583, -0.2759523093700409], 'magnitude': 1.770767331123352, 'distance': 13.69267463684082, 'cosine_with_motion': -0.15556355057782062, 'motion_component': -0.27546685084777156}, {'ion': 1309, 'force': [-0.7954425811767578, 2.337529182434082, -2.0951266288757324], 'magnitude': 3.238259792327881, 'distance': 10.125423431396484, 'cosine_with_motion': -0.7204338815501123, 'motion_component': -2.332952148085589}]}, 5181: {'frame': 5181, 'ionic_force': [-0.6866850852966309, 5.2680962681770325, -3.737524628639221], 'ionic_force_magnitude': 6.4956497016722174, 'motion_vector': [-0.3796195983886719, -1.8383750915527344, -0.54205322265625], 'cosine_ionic_motion': -0.5829162005149764, 'ionic_motion_component': -3.7864194439750087, 'ionic_force_x': -0.6866850852966309, 'ionic_force_y': 5.2680962681770325, 'ionic_force_z': -3.737524628639221, 'radial_force': 5.312661733740406, 'axial_force': -3.737524628639221, 'contributions': [{'ion': 1308, 'force': [0.3693566620349884, 1.7314714193344116, -0.16969358921051025], 'magnitude': 1.7785425186157227, 'distance': 13.662712097167969, 'cosine_with_motion': -0.9298734282283851, 'motion_component': -1.6538194403953677}, {'ion': 1309, 'force': [-0.789997935295105, 2.699798583984375, -2.170147180557251], 'magnitude': 3.5528225898742676, 'distance': 9.666790008544922, 'cosine_with_motion': -0.5023273269637426, 'motion_component': -1.7846798437849252}, {'ion': 1403, 'force': [-0.2660438120365143, 0.8368262648582458, -1.39768385887146], 'magnitude': 1.6506295204162598, 'distance': 14.182221412658691, 'cosine_with_motion': -0.21078027551344006, 'motion_component': -0.3479201363469171}]}, 5182: {'frame': 5182, 'ionic_force': [-1.5095845460891724, 5.511749029159546, -4.918577492237091], 'ionic_force_magnitude': 7.53993550432454, 'motion_vector': [3.399822235107422, 1.0570564270019531, -0.6069412231445312], 'cosine_ionic_motion': 0.1351049295348629, 'ionic_motion_component': 1.018682455009178, 'ionic_force_x': -1.5095845460891724, 'ionic_force_y': 5.511749029159546, 'ionic_force_z': -4.918577492237091, 'radial_force': 5.714737339741211, 'axial_force': -4.918577492237091, 'contributions': [{'ion': 1308, 'force': [0.24988240003585815, 2.1664843559265137, -0.3289939761161804], 'magnitude': 2.2055232524871826, 'distance': 12.26911449432373, 'cosine_with_motion': 0.4192119235928302, 'motion_component': 0.9245816354512906}, {'ion': 1309, 'force': [-1.407989263534546, 2.6396069526672363, -3.090088129043579], 'magnitude': 4.301000118255615, 'distance': 8.785860061645508, 'cosine_with_motion': -0.00780209540420473, 'motion_component': -0.033556814397886825}, {'ion': 1403, 'force': [-0.3514776825904846, 0.7056577205657959, -1.4994953870773315], 'magnitude': 1.694100260734558, 'distance': 13.999079704284668, 'cosine_with_motion': 0.07535424101003572, 'motion_component': 0.12765764161992088}]}, 5183: {'frame': 5183, 'ionic_force': [0.906077116727829, 3.351901054382324, -2.439151182770729], 'ionic_force_magnitude': 4.243309429235511, 'motion_vector': [-0.3704338073730469, 0.2990570068359375, 0.07714080810546875], 'cosine_ionic_motion': 0.23386514195069716, 'ionic_motion_component': 0.9923621620088946, 'ionic_force_x': 0.906077116727829, 'ionic_force_y': 3.351901054382324, 'ionic_force_z': -2.439151182770729, 'radial_force': 3.472206275529602, 'axial_force': -2.439151182770729, 'contributions': [{'ion': 1308, 'force': [0.6261655688285828, 1.4340345859527588, -0.20961131155490875], 'magnitude': 1.5787575244903564, 'distance': 14.501446723937988, 'cosine_with_motion': 0.23736511913737168, 'motion_component': 0.37474197496300743}, {'ion': 1309, 'force': [0.2799115478992462, 1.9178664684295654, -2.2295398712158203], 'magnitude': 2.954219102859497, 'distance': 10.601020812988281, 'cosine_with_motion': 0.20906377391369516, 'motion_component': 0.6176201873585594}]}, 5184: {'frame': 5184, 'ionic_force': [0.7254925360903144, 4.958870887756348, -4.047217309474945], 'ionic_force_magnitude': 6.441793838013896, 'motion_vector': [-0.18041229248046875, 0.4036216735839844, 0.16362762451171875], 'cosine_ionic_motion': 0.3979180144561937, 'ionic_motion_component': 2.563305813558633, 'ionic_force_x': 0.7254925360903144, 'ionic_force_y': 4.958870887756348, 'ionic_force_z': -4.047217309474945, 'radial_force': 5.011660393657992, 'axial_force': -4.047217309474945, 'contributions': [{'ion': 1308, 'force': [0.5973078608512878, 1.5048673152923584, -0.26393312215805054], 'magnitude': 1.6404459476470947, 'distance': 14.22617244720459, 'cosine_with_motion': 0.5902359183247087, 'motion_component': 0.9682501389175825}, {'ion': 1309, 'force': [0.1381777822971344, 2.6733298301696777, -2.3793797492980957], 'magnitude': 3.581512689590454, 'distance': 9.6279935836792, 'cosine_with_motion': 0.3937215782895846, 'motion_component': 1.410118846732325}, {'ion': 1403, 'force': [-0.009993107058107853, 0.7806737422943115, -1.4039044380187988], 'magnitude': 1.6063930988311768, 'distance': 14.376167297363281, 'cosine_with_motion': 0.1151254858041788, 'motion_component': 0.18493679439559696}]}, 5185: {'frame': 5185, 'ionic_force': [0.7339238412678242, 5.119778215885162, -3.856375366449356], 'ionic_force_magnitude': 6.45154277298004, 'motion_vector': [-0.11819076538085938, -0.16250991821289062, 0.146270751953125], 'cosine_ionic_motion': -0.924755423083406, 'ionic_motion_component': -5.966099166567847, 'ionic_force_x': 0.7339238412678242, 'ionic_force_y': 5.119778215885162, 'ionic_force_z': -3.856375366449356, 'radial_force': 5.172114962433992, 'axial_force': -3.856375366449356, 'contributions': [{'ion': 1308, 'force': [0.8244546055793762, 1.679525375366211, -0.2533508837223053], 'magnitude': 1.8880459070205688, 'distance': 13.260587692260742, 'cosine_with_motion': -0.8682598275267359, 'motion_component': -1.6393144610569834}, {'ion': 1309, 'force': [-0.028522875159978867, 2.627678871154785, -2.242663860321045], 'magnitude': 3.454714298248291, 'distance': 9.803089141845703, 'cosine_with_motion': -0.8754357746797629, 'motion_component': -3.024380502198848}, {'ion': 1403, 'force': [-0.06200788915157318, 0.8125739693641663, -1.3603606224060059], 'magnitude': 1.5857813358306885, 'distance': 14.469295501708984, 'cosine_with_motion': -0.8213012027582747, 'motion_component': -1.302404121518519}]}, 5186: {'frame': 5186, 'ionic_force': [0.6085753031075001, 5.361973226070404, -3.9645311534404755], 'ionic_force_magnitude': 6.696165174429937, 'motion_vector': [0.29323577880859375, 0.5634040832519531, 0.6587371826171875], 'cosine_ionic_motion': 0.09593404861098064, 'ionic_motion_component': 0.6423902353509172, 'ionic_force_x': 0.6085753031075001, 'ionic_force_y': 5.361973226070404, 'ionic_force_z': -3.9645311534404755, 'radial_force': 5.396398871159196, 'axial_force': -3.9645311534404755, 'contributions': [{'ion': 1308, 'force': [0.7067315578460693, 1.7726627588272095, -0.21329709887504578], 'magnitude': 1.920233964920044, 'distance': 13.148977279663086, 'cosine_with_motion': 0.6063586115181139, 'motion_component': 1.1643503887190967}, {'ion': 1309, 'force': [-0.05736168473958969, 2.774033784866333, -2.3771002292633057], 'magnitude': 3.6536500453948975, 'distance': 9.532472610473633, 'cosine_with_motion': -0.005923090307569401, 'motion_component': -0.021640899696546034}, {'ion': 1403, 'force': [-0.04079456999897957, 0.8152766823768616, -1.374133825302124], 'magnitude': 1.598306655883789, 'distance': 14.41248893737793, 'cosine_with_motion': -0.31303085430443395, 'motion_component': -0.5003192851393142}]}, 5187: {'frame': 5187, 'ionic_force': [0.44809454679489136, 5.63523006439209, -3.661033511161804], 'ionic_force_magnitude': 6.7349664417386315, 'motion_vector': [-0.44336700439453125, -0.58660888671875, -0.7073516845703125], 'cosine_ionic_motion': -0.1331114322693107, 'ionic_motion_component': -0.8965010293455722, 'ionic_force_x': 0.44809454679489136, 'ionic_force_y': 5.63523006439209, 'ionic_force_z': -3.661033511161804, 'radial_force': 5.653017477550887, 'axial_force': -3.661033511161804, 'contributions': [{'ion': 1308, 'force': [0.5526303648948669, 1.42279052734375, -0.1382688283920288], 'magnitude': 1.5325963497161865, 'distance': 14.718214988708496, 'cosine_with_motion': -0.6278833176374604, 'motion_component': -0.962291660716259}, {'ion': 1309, 'force': [-0.0501912422478199, 3.1493821144104004, -2.052255630493164], 'magnitude': 3.7593722343444824, 'distance': 9.397479057312012, 'cosine_with_motion': -0.09738347942390585, 'motion_component': -0.36610075432767797}, {'ion': 1403, 'force': [-0.054344575852155685, 1.0630574226379395, -1.4705090522766113], 'magnitude': 1.8153350353240967, 'distance': 13.523548126220703, 'cosine_with_motion': 0.23791276105627682, 'motion_component': 0.43189137043733694}]}, 5188: {'frame': 5188, 'ionic_force': [0.6004464058205485, 5.34605211019516, -4.232802301645279], 'ionic_force_magnitude': 6.845248306380018, 'motion_vector': [0.09778976440429688, 0.3133354187011719, -0.27387237548828125], 'cosine_ionic_motion': 0.9886528166637947, 'ionic_motion_component': 6.767574018865675, 'ionic_force_x': 0.6004464058205485, 'ionic_force_y': 5.34605211019516, 'ionic_force_z': -4.232802301645279, 'radial_force': 5.37966625834586, 'axial_force': -4.232802301645279, 'contributions': [{'ion': 1308, 'force': [0.7558067440986633, 2.0558364391326904, -0.4618763029575348], 'magnitude': 2.238534450531006, 'distance': 12.178313255310059, 'cosine_with_motion': 0.8825643705961469, 'motion_component': 1.975650853246151}, {'ion': 1309, 'force': [-0.012659800238907337, 2.442432165145874, -2.3873846530914307], 'magnitude': 3.4154415130615234, 'distance': 9.859289169311523, 'cosine_with_motion': 0.9711197726701742, 'motion_component': 3.3168027721633653}, {'ion': 1403, 'force': [-0.14270053803920746, 0.8477835059165955, -1.3835413455963135], 'magnitude': 1.6288913488388062, 'distance': 14.276540756225586, 'cosine_with_motion': 0.9055977262933529, 'motion_component': 1.4751202866299886}]}, 5189: {'frame': 5189, 'ionic_force': [0.32750216871500015, 4.727729856967926, -3.834524780511856], 'ionic_force_magnitude': 6.096086249663672, 'motion_vector': [-0.000904083251953125, -0.1085205078125, 0.5684127807617188], 'cosine_ionic_motion': -0.7633747994882957, 'ionic_motion_component': -4.653598618500362, 'ionic_force_x': 0.32750216871500015, 'ionic_force_y': 4.727729856967926, 'ionic_force_z': -3.834524780511856, 'radial_force': 4.739059745453627, 'axial_force': -3.834524780511856, 'contributions': [{'ion': 1308, 'force': [0.5216655135154724, 1.448395848274231, -0.2568974792957306], 'magnitude': 1.5607632398605347, 'distance': 14.58480167388916, 'cosine_with_motion': -0.33622893755916217, 'motion_component': -0.5247737514062334}, {'ion': 1309, 'force': [-0.11025428026914597, 2.4549198150634766, -2.214020013809204], 'magnitude': 3.307668685913086, 'distance': 10.018623352050781, 'cosine_with_motion': -0.7966152203201085, 'motion_component': -2.6349391937450988}, {'ion': 1403, 'force': [-0.0839090645313263, 0.8244141936302185, -1.3636072874069214], 'magnitude': 1.5956579446792603, 'distance': 14.424446105957031, 'cosine_with_motion': -0.9362191895719004, 'motion_component': -1.4938856029452705}]}, 5190: {'frame': 5190, 'ionic_force': [0.34706735610961914, 4.918230354785919, -3.804109513759613], 'ionic_force_magnitude': 6.227414773811919, 'motion_vector': [0.3770256042480469, -0.35123443603515625, -0.49456024169921875], 'cosine_ionic_motion': 0.06402448857565023, 'ionic_motion_component': 0.39870704604175666, 'ionic_force_x': 0.34706735610961914, 'ionic_force_y': 4.918230354785919, 'ionic_force_z': -3.804109513759613, 'radial_force': 4.930460989848165, 'axial_force': -3.804109513759613, 'contributions': [{'ion': 1308, 'force': [0.5309812426567078, 1.4431406259536743, -0.21502536535263062], 'magnitude': 1.5526853799819946, 'distance': 14.62269115447998, 'cosine_with_motion': -0.1806608335869741, 'motion_component': -0.28050943300189246}, {'ion': 1309, 'force': [-0.07559871673583984, 2.564948797225952, -2.245485782623291], 'magnitude': 3.4098215103149414, 'distance': 9.867410659790039, 'cosine_with_motion': 0.07437417935511147, 'motion_component': 0.25360268929463814}, {'ion': 1403, 'force': [-0.10831516981124878, 0.9101409316062927, -1.3435983657836914], 'magnitude': 1.6264517307281494, 'distance': 14.287243843078613, 'cosine_with_motion': 0.26168234308413185, 'motion_component': 0.42561370202601617}]}, 5191: {'frame': 5191, 'ionic_force': [0.657955770380795, 5.201777338981628, -4.198868662118912], 'ionic_force_magnitude': 6.717283031244436, 'motion_vector': [-0.9679679870605469, 0.518524169921875, 1.3073348999023438], 'cosine_ionic_motion': -0.2989874499026258, 'ionic_motion_component': -2.0083833237859543, 'ionic_force_x': 0.657955770380795, 'ionic_force_y': 5.201777338981628, 'ionic_force_z': -4.198868662118912, 'radial_force': 5.243223558090975, 'axial_force': -4.198868662118912, 'contributions': [{'ion': 1308, 'force': [0.6094868183135986, 1.5151386260986328, -0.26498427987098694], 'magnitude': 1.6544896364212036, 'distance': 14.165666580200195, 'cosine_with_motion': -0.05336790472600894, 'motion_component': -0.08829664447299024}, {'ion': 1309, 'force': [0.05508818104863167, 2.8828670978546143, -2.548942804336548], 'magnitude': 3.8485147953033447, 'distance': 9.288005828857422, 'cosine_with_motion': -0.2877654872420616, 'motion_component': -1.1074697614626865}, {'ion': 1403, 'force': [-0.006619228981435299, 0.8037716150283813, -1.384941577911377], 'magnitude': 1.601298213005066, 'distance': 14.399020195007324, 'cosine_with_motion': -0.5074739143486897, 'motion_component': -0.8126170453461972}]}, 5192: {'frame': 5192, 'ionic_force': [0.1945376694202423, 5.99289608001709, -3.5691631473600864], 'ionic_force_magnitude': 6.977934787828059, 'motion_vector': [-2.582378387451172, -1.3664169311523438, 0.01790618896484375], 'cosine_ionic_motion': -0.4294408475329646, 'ionic_motion_component': -2.996610229314639, 'ionic_force_x': 0.1945376694202423, 'ionic_force_y': 5.99289608001709, 'ionic_force_z': -3.5691631473600864, 'radial_force': 5.996052729146706, 'axial_force': -3.5691631473600864, 'contributions': [{'ion': 1308, 'force': [0.6152461171150208, 1.7376521825790405, -0.03967398777604103], 'magnitude': 1.8437833786010742, 'distance': 13.41881275177002, 'cosine_with_motion': -0.7358333946801904, 'motion_component': -1.356717336705017}, {'ion': 1309, 'force': [-0.2750970125198364, 3.165602922439575, -1.957560658454895], 'magnitude': 3.732125997543335, 'distance': 9.431719779968262, 'cosine_with_motion': -0.3347561495557672, 'motion_component': -1.2493521061189088}, {'ion': 1403, 'force': [-0.14561143517494202, 1.0896409749984741, -1.5719285011291504], 'magnitude': 1.9181969165802002, 'distance': 13.155957221984863, 'cosine_with_motion': -0.20359788913885363, 'motion_component': -0.39054084032030834}]}, 5193: {'frame': 5193, 'ionic_force': [-1.93711456656456, 6.59854257106781, -4.372821029275656], 'ionic_force_magnitude': 8.149523952984381, 'motion_vector': [0.4185295104980469, 1.0166091918945312, -0.2987213134765625], 'cosine_ionic_motion': 0.7758910631739562, 'ionic_motion_component': 6.323142804242674, 'ionic_force_x': -1.93711456656456, 'ionic_force_y': 6.59854257106781, 'ionic_force_z': -4.372821029275656, 'radial_force': 6.877003483072463, 'axial_force': -4.372821029275656, 'contributions': [{'ion': 1308, 'force': [0.4174995720386505, 2.2765603065490723, -0.059432800859212875], 'magnitude': 2.3152894973754883, 'distance': 11.974748611450195, 'cosine_with_motion': 0.9503974281845952, 'motion_component': 2.2004450859416735}, {'ion': 1309, 'force': [-1.7871077060699463, 3.376755714416504, -2.6929991245269775], 'magnitude': 4.674235820770264, 'distance': 8.427790641784668, 'cosine_with_motion': 0.655258731336676, 'motion_component': 3.062833615510769}, {'ion': 1403, 'force': [-0.5675064325332642, 0.9452265501022339, -1.6203891038894653], 'magnitude': 1.9598922729492188, 'distance': 13.015262603759766, 'cosine_with_motion': 0.540776768071992, 'motion_component': 1.0598641965006337}]}, 5194: {'frame': 5194, 'ionic_force': [-0.9560555219650269, 5.772682011127472, -3.487354025244713], 'ionic_force_magnitude': 6.811720624046837, 'motion_vector': [-0.6451492309570312, -1.4054031372070312, -0.01318359375], 'cosine_ionic_motion': -0.7072447724738669, 'ionic_motion_component': -4.8175538029095515, 'ionic_force_x': -0.9560555219650269, 'ionic_force_y': 5.772682011127472, 'ionic_force_z': -3.487354025244713, 'radial_force': 5.8513160709941605, 'axial_force': -3.487354025244713, 'contributions': [{'ion': 1308, 'force': [0.6240898370742798, 2.3083484172821045, -0.197579488158226], 'magnitude': 2.3993747234344482, 'distance': 11.763051986694336, 'cosine_with_motion': -0.9821161896001479, 'motion_component': -2.3564645829506077}, {'ion': 1309, 'force': [-1.1822179555892944, 2.5775022506713867, -1.9253954887390137], 'magnitude': 3.4275801181793213, 'distance': 9.841815948486328, 'cosine_with_motion': -0.5347176855163869, 'motion_component': -1.8327876662373213}, {'ion': 1403, 'force': [-0.3979274034500122, 0.8868313431739807, -1.3643790483474731], 'magnitude': 1.675215244293213, 'distance': 14.077766418457031, 'cosine_with_motion': -0.3750572757112363, 'motion_component': -0.6283016794686191}]}, 5195: {'frame': 5195, 'ionic_force': [-2.697285771369934, 7.435713529586792, -4.3827709555625916], 'ionic_force_magnitude': 9.042890438097643, 'motion_vector': [0.4557342529296875, 0.3656768798828125, 0.8678741455078125], 'cosine_ionic_motion': -0.24456839884992476, 'ionic_motion_component': -2.2116052354208353, 'ionic_force_x': -2.697285771369934, 'ionic_force_y': 7.435713529586792, 'ionic_force_z': -4.3827709555625916, 'radial_force': 7.90981581495516, 'axial_force': -4.3827709555625916, 'contributions': [{'ion': 1308, 'force': [-0.6983073353767395, 3.93900203704834, -0.37639325857162476], 'magnitude': 4.018089294433594, 'distance': 9.089902877807617, 'cosine_with_motion': 0.18922900283928057, 'motion_component': 0.760339042032788}, {'ion': 1309, 'force': [-1.4922806024551392, 2.734032154083252, -2.6263973712921143], 'magnitude': 4.074284553527832, 'distance': 9.026997566223145, 'cosine_with_motion': -0.4597326047091931, 'motion_component': -1.8730815485615615}, {'ion': 1403, 'force': [-0.5066978335380554, 0.7626793384552002, -1.3799803256988525], 'magnitude': 1.6561305522918701, 'distance': 14.158647537231445, 'cosine_with_motion': -0.6635122356815232, 'motion_component': -1.0988628374351261}]}, 5196: {'frame': 5196, 'ionic_force': [-2.689316511154175, 6.572674095630646, -2.8800116777420044], 'ionic_force_magnitude': 7.66335013740537, 'motion_vector': [0.2856636047363281, 0.22528839111328125, 0.144744873046875], 'cosine_ionic_motion': 0.09852816387166814, 'ionic_motion_component': 0.7550558181442468, 'ionic_force_x': -2.689316511154175, 'ionic_force_y': 6.572674095630646, 'ionic_force_z': -2.8800116777420044, 'radial_force': 7.101582081799843, 'axial_force': -2.8800116777420044, 'contributions': [{'ion': 1308, 'force': [-0.6410857439041138, 2.2917823791503906, 1.5949033498764038], 'magnitude': 2.864781618118286, 'distance': 10.765229225158691, 'cosine_with_motion': 0.5028366061858794, 'motion_component': 1.4405170996993453}, {'ion': 1309, 'force': [-1.6070647239685059, 3.372495651245117, -2.893615961074829], 'magnitude': 4.725399017333984, 'distance': 8.382040977478027, 'cosine_with_motion': -0.06384747410201075, 'motion_component': -0.30170480085153173}, {'ion': 1403, 'force': [-0.4411660432815552, 0.9083960652351379, -1.581299066543579], 'magnitude': 1.876250982284546, 'distance': 13.302203178405762, 'cosine_with_motion': -0.20453358387588322, 'motion_component': -0.3837563310297796}]}, 5197: {'frame': 5197, 'ionic_force': [-2.394786536693573, 9.815348863601685, -3.377447187900543], 'ionic_force_magnitude': 10.652850575202534, 'motion_vector': [-0.7711677551269531, -0.23419952392578125, -1.1207962036132812], 'cosine_ionic_motion': 0.22667240517304837, 'ionic_motion_component': 2.4147072618302503, 'ionic_force_x': -2.394786536693573, 'ionic_force_y': 9.815348863601685, 'ionic_force_z': -3.377447187900543, 'radial_force': 10.10327055316919, 'axial_force': -3.377447187900543, 'contributions': [{'ion': 1308, 'force': [-0.5111057162284851, 5.275302886962891, 0.6245482563972473], 'magnitude': 5.336676120758057, 'distance': 7.88739538192749, 'cosine_with_motion': -0.2092136235456392, 'motion_component': -1.1165053118480337}, {'ion': 1309, 'force': [-1.4601268768310547, 3.5319414138793945, -2.432771682739258], 'magnitude': 4.530447959899902, 'distance': 8.560486793518066, 'cosine_with_motion': 0.48374883718600237, 'motion_component': 2.191598932025954}, {'ion': 1403, 'force': [-0.4235539436340332, 1.0081045627593994, -1.5692237615585327], 'magnitude': 1.9126254320144653, 'distance': 13.175105094909668, 'cosine_with_motion': 0.7004055536376355, 'motion_component': 1.3396134605632426}]}, 5198: {'frame': 5198, 'ionic_force': [-2.4582442939281464, 7.281810879707336, -3.801115170121193], 'ionic_force_magnitude': 8.574159505921259, 'motion_vector': [1.0001983642578125, 2.0919723510742188, -0.8253173828125], 'cosine_ionic_motion': 0.7539895480987615, 'ionic_motion_component': 6.46482665119627, 'ionic_force_x': -2.4582442939281464, 'ionic_force_y': 7.281810879707336, 'ionic_force_z': -3.801115170121193, 'radial_force': 7.685553636300668, 'axial_force': -3.801115170121193, 'contributions': [{'ion': 1308, 'force': [-0.5375314950942993, 3.8752388954162598, -0.03662027418613434], 'magnitude': 3.912513017654419, 'distance': 9.211729049682617, 'cosine_with_motion': 0.7891637841625229, 'motion_component': 3.087613531795399}, {'ion': 1309, 'force': [-1.4404795169830322, 2.623394727706909, -2.3200292587280273], 'magnitude': 3.7867817878723145, 'distance': 9.363407135009766, 'cosine_with_motion': 0.6396840948812568, 'motion_component': 2.4223441302027737}, {'ion': 1403, 'force': [-0.4802332818508148, 0.7831772565841675, -1.4444656372070312], 'magnitude': 1.7118620872497559, 'distance': 13.926264762878418, 'cosine_with_motion': 0.5577956065243156, 'motion_component': 0.954869117280472}]}, 5199: {'frame': 5199, 'ionic_force': [-1.14464071393013, 4.792068958282471, -1.1551509499549866], 'ionic_force_magnitude': 5.060484263596008, 'motion_vector': [0.4618873596191406, -1.79718017578125, 1.5188522338867188], 'cosine_ionic_motion': -0.8978699993094448, 'ionic_motion_component': -4.543657002260404, 'ionic_force_x': -1.14464071393013, 'ionic_force_y': 4.792068958282471, 'ionic_force_z': -1.1551509499549866, 'radial_force': 4.926878044453802, 'axial_force': -1.1551509499549866, 'contributions': [{'ion': 1308, 'force': [-0.3644380271434784, 2.3148305416107178, 0.5557435154914856], 'magnitude': 2.4083409309387207, 'distance': 11.741133689880371, 'cosine_with_motion': -0.6033545233363018, 'motion_component': -1.4530834354263635}, {'ion': 1309, 'force': [-0.7802026867866516, 2.477238416671753, -1.7108944654464722], 'magnitude': 3.1100780963897705, 'distance': 10.331975936889648, 'cosine_with_motion': -0.9937286248646539, 'motion_component': -3.0905737117048435}]}, 5200: {'frame': 5200, 'ionic_force': [-1.6555381119251251, 7.148874580860138, -3.147367298603058], 'ionic_force_magnitude': 7.984556038078806, 'motion_vector': [-1.8232803344726562, -0.8938713073730469, -0.5885772705078125], 'cosine_ionic_motion': -0.08999526784902638, 'ionic_motion_component': -0.718572259302463, 'ionic_force_x': -1.6555381119251251, 'ionic_force_y': 7.148874580860138, 'ionic_force_z': -3.147367298603058, 'radial_force': 7.338066108512844, 'axial_force': -3.147367298603058, 'contributions': [{'ion': 1308, 'force': [-0.19619184732437134, 2.808659076690674, 0.9512656331062317]</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>{5213: {'frame': 5213, 'ionic_force': [9.059208557009697, 6.910908341407776, -17.690110206604004], 'ionic_force_magnitude': 21.042098586037763, 'motion_vector': [-0.08104324340820312, -3.535572052001953, 0.40856170654296875], 'cosine_ionic_motion': -0.43245966970827554, 'ionic_motion_component': -9.099859004486863, 'ionic_force_x': 9.059208557009697, 'ionic_force_y': 6.910908341407776, 'ionic_force_z': -17.690110206604004, 'radial_force': 11.394293035670852, 'axial_force': -17.690110206604004, 'contributions': [{'ion': 1308, 'force': [4.778199672698975, 9.435524940490723, -10.170702934265137], 'magnitude': 14.673224449157715, 'distance': 4.756705284118652, 'directional_contribution': -10.646724441459995}, {'ion': 1320, 'force': [4.232130527496338, -3.0712902545928955, -4.9525957107543945], 'magnitude': 7.202219009399414, 'distance': 6.789470195770264, 'directional_contribution': 2.3854740970482444}, {'ion': 1403, 'force': [0.04887835681438446, 0.5466736555099487, -2.5668115615844727], 'magnitude': 2.624835729598999, 'distance': 11.246515274047852, 'directional_contribution': -0.8386088114752297}]}, 5214: {'frame': 5214, 'ionic_force': [0.876273438334465, -7.065377295017242, -7.964790105819702], 'ionic_force_magnitude': 10.682944017893153, 'motion_vector': [-2.800647735595703, -0.17963790893554688, 2.6386032104492188], 'cosine_ionic_motion': -0.5394970021714701, 'ionic_motion_component': -5.763416272018996, 'ionic_force_x': 0.876273438334465, 'ionic_force_y': -7.065377295017242, 'ionic_force_z': -7.964790105819702, 'radial_force': 7.119509214803761, 'axial_force': -7.964790105819702, 'contributions': [{'ion': 1308, 'force': [-1.3250770568847656, -3.1238503456115723, -2.5353305339813232], 'magnitude': 4.2358198165893555, 'distance': 8.85319995880127, 'directional_contribution': -0.6275900945759094}, {'ion': 1320, 'force': [2.0835518836975098, -3.640300989151001, -2.173349618911743], 'magnitude': 4.724026679992676, 'distance': 8.383258819580078, 'directional_contribution': -2.833822626494336}, {'ion': 1403, 'force': [0.11779861152172089, -0.3012259602546692, -3.2561099529266357], 'magnitude': 3.272134780883789, 'distance': 10.072875022888184, 'directional_contribution': -2.302003315099296}]}, 5215: {'frame': 5215, 'ionic_force': [-3.1574587523937225, -9.676621198654175, -7.118128061294556], 'ionic_force_magnitude': 12.42072021632804, 'motion_vector': [0.9844284057617188, -0.2884941101074219, -5.571617126464844], 'cosine_ionic_motion': 0.5591117071431897, 'ionic_motion_component': 6.944570084099098, 'ionic_force_x': -3.1574587523937225, 'ionic_force_y': -9.676621198654175, 'ionic_force_z': -7.118128061294556, 'radial_force': 10.178729959838362, 'axial_force': -7.118128061294556, 'contributions': [{'ion': 1308, 'force': [-2.1365599632263184, -3.032615900039673, -0.8023586273193359], 'magnitude': 3.7954483032226562, 'distance': 9.352710723876953, 'directional_contribution': 0.5722654804066467}, {'ion': 1320, 'force': [0.5601136684417725, -6.005922317504883, -0.8906189203262329], 'magnitude': 6.097379207611084, 'distance': 7.378998756408691, 'directional_contribution': 1.2790664955624322}, {'ion': 1403, 'force': [-1.2336101531982422, -0.5227363109588623, -3.747150182723999], 'magnitude': 3.9794700145721436, 'distance': 9.133903503417969, 'directional_contribution': 3.4974685416808162}, {'ion': 1469, 'force': [-0.34740230441093445, -0.11534667015075684, -1.6780003309249878], 'magnitude': 1.7174626588821411, 'distance': 13.903539657592773, 'directional_contribution': 1.5957694874407418}]}, 5216: {'frame': 5216, 'ionic_force': [0.3360389769077301, -3.4986054599285126, -5.366488456726074], 'ionic_force_magnitude': 6.415010577888161, 'motion_vector': [0.49591064453125, 1.3578147888183594, -0.21898651123046875], 'cosine_ionic_motion': -0.3634329471769188, 'ionic_motion_component': -2.3314262004930035, 'ionic_force_x': 0.3360389769077301, 'ionic_force_y': -3.4986054599285126, 'ionic_force_z': -5.366488456726074, 'radial_force': 3.51470658209797, 'axial_force': -5.366488456726074, 'contributions': [{'ion': 1308, 'force': [-0.5920225381851196, -1.5384231805801392, -1.2295265197753906], 'magnitude': 2.0564465522766113, 'distance': 12.706043243408203, 'directional_contribution': -1.4454071028631574}, {'ion': 1320, 'force': [1.186414122581482, -1.7023833990097046, -2.2223496437072754], 'magnitude': 3.0404810905456543, 'distance': 10.449557304382324, 'directional_contribution': -0.8457405365038682}, {'ion': 1403, 'force': [-0.2583526074886322, -0.2577988803386688, -1.9146122932434082], 'magnitude': 1.9490886926651, 'distance': 13.051283836364746, 'directional_contribution': -0.04027859703741399}]}, 5217: {'frame': 5217, 'ionic_force': [-0.5696889609098434, -2.4908271618187428, -6.695563793182373], 'ionic_force_magnitude': 7.166543097673472, 'motion_vector': [1.0223388671875, -0.4985237121582031, 2.0433120727539062], 'cosine_ionic_motion': -0.7769881557830077, 'ionic_motion_component': -5.5683191048007545, 'ionic_force_x': -0.5696889609098434, 'ionic_force_y': -2.4908271618187428, 'ionic_force_z': -6.695563793182373, 'radial_force': 2.555144900438437, 'axial_force': -6.695563793182373, 'contributions': [{'ion': 1308, 'force': [-1.6062496900558472, -1.6342322826385498, -2.415165901184082], 'magnitude': 3.329231023788452, 'distance': 9.986126899719238, 'directional_contribution': -2.4640738930936728}, {'ion': 1320, 'force': [1.2217909097671509, -0.8660487532615662, -2.349320888519287], 'magnitude': 2.7860584259033203, 'distance': 10.916261672973633, 'directional_contribution': -1.333972960252149}, {'ion': 1403, 'force': [-0.18523018062114716, 0.009453874081373215, -1.931077003479004], 'magnitude': 1.939963459968567, 'distance': 13.08194351196289, 'directional_contribution': -1.7702721473163905}]}, 5218: {'frame': 5218, 'ionic_force': [4.206250421702862, -4.269712045788765, -7.6996800899505615], 'ionic_force_magnitude': 9.757461609025693, 'motion_vector': [-0.7376747131347656, 0.12036895751953125, 5.263938903808594], 'cosine_ionic_motion': -0.8509877619478586, 'ionic_motion_component': -8.303480416956926, 'ionic_force_x': 4.206250421702862, 'ionic_force_y': -4.269712045788765, 'ionic_force_z': -7.6996800899505615, 'radial_force': 5.993578527393228, 'axial_force': -7.6996800899505615, 'contributions': [{'ion': 1308, 'force': [-1.0178943872451782, -2.646784543991089, -2.161548376083374], 'magnitude': 3.5656511783599854, 'distance': 9.649384498596191, 'directional_contribution': -2.0587763371135157}, {'ion': 1320, 'force': [5.3220672607421875, -1.4583486318588257, -2.8955790996551514], 'magnitude': 6.231818199157715, 'distance': 7.298971652984619, 'directional_contribution': -3.638254433041088}, {'ion': 1403, 'force': [-0.09792245179414749, -0.1645788699388504, -2.642552614212036], 'magnitude': 2.6494827270507812, 'distance': 11.194082260131836, 'directional_contribution': -2.606449820321628}]}, 5219: {'frame': 5219, 'ionic_force': [-0.8370766043663025, 7.505206935107708, 4.665254652500153], 'ionic_force_magnitude': 8.876566304210236, 'motion_vector': [-1.3892173767089844, -0.5494041442871094, 1.6649017333984375], 'cosine_ionic_motion': 0.24207837425350287, 'ionic_motion_component': 2.1488247398766385, 'ionic_force_x': -0.8370766043663025, 'ionic_force_y': 7.505206935107708, 'ionic_force_z': 4.665254652500153, 'radial_force': 7.551743400061091, 'axial_force': 4.665254652500153, 'contributions': [{'ion': 1308, 'force': [-1.2311298847198486, -4.110632419586182, -0.6271311640739441], 'magnitude': 4.336619853973389, 'distance': 8.749703407287598, 'directional_contribution': 1.3074386645678935}, {'ion': 1320, 'force': [1.5758368968963623, 11.999844551086426, 15.897293090820312], 'magnitude': 19.98007583618164, 'distance': 4.076340675354004, 'directional_contribution': 7.906290618905373}, {'ion': 1403, 'force': [-1.0520174503326416, -0.32890668511390686, -8.382981300354004], 'magnitude': 8.455134391784668, 'distance': 6.266265392303467, 'directional_contribution': -5.505262943493138}, {'ion': 1469, 'force': [-0.12976616621017456, -0.0550985112786293, -2.221925973892212], 'magnitude': 2.226393938064575, 'distance': 12.211472511291504, 'directional_contribution': -1.5596416475744035}]}, 5220: {'frame': 5220, 'ionic_force': [-7.989065766334534, -10.187750428915024, -5.366817504167557], 'ionic_force_magnitude': 14.01492635527265, 'motion_vector': [-0.5346794128417969, -1.1390304565429688, -0.756134033203125], 'cosine_ionic_motion': 0.9688891272673253, 'ionic_motion_component': 13.578909765075954, 'ionic_force_x': -7.989065766334534, 'ionic_force_y': -10.187750428915024, 'ionic_force_z': -5.366817504167557, 'radial_force': 12.946637811442654, 'axial_force': -5.366817504167557, 'contributions': [{'ion': 1308, 'force': [-1.290416955947876, -3.383082866668701, 0.44074055552482605], 'magnitude': 3.6475577354431152, 'distance': 9.540430068969727, 'directional_contribution': 2.867947724152115}, {'ion': 1320, 'force': [-1.2900820970535278, -3.8637619018554688, 8.199496269226074], 'magnitude': 9.155583381652832, 'distance': 6.021795749664307, 'directional_contribution': -0.7555849354875583}, {'ion': 1403, 'force': [-4.87747859954834, -2.6918888092041016, -11.338939666748047], 'magnitude': 12.633590698242188, 'distance': 5.126319408416748, 'directional_contribution': 9.705606906917723}, {'ion': 1469, 'force': [-0.53108811378479, -0.24901685118675232, -2.66811466217041], 'magnitude': 2.7318308353424072, 'distance': 11.02407455444336, 'directional_contribution': 1.7609397736349202}]}, 5221: {'frame': 5221, 'ionic_force': [-10.496177196502686, -8.205937772989273, 0.1122767822816968], 'ionic_force_magnitude': 13.32365402396785, 'motion_vector': [0.09583663940429688, 4.582389831542969, -4.5017547607421875], 'cosine_ionic_motion': -0.4569579844587636, 'ionic_motion_component': -6.0883500884182435, 'ionic_force_x': -10.496177196502686, 'ionic_force_y': -8.205937772989273, 'ionic_force_z': 0.1122767822816968, 'radial_force': 13.32318094429987, 'axial_force': 0.1122767822816968, 'contributions': [{'ion': 1308, 'force': [-0.9717339277267456, -2.528850793838501, 0.010465134866535664], 'magnitude': 2.709144353866577, 'distance': 11.070137023925781, 'directional_contribution': -1.825597403703803}, {'ion': 1320, 'force': [-6.512366771697998, -3.0620293617248535, 8.233292579650879], 'magnitude': 10.934991836547852, 'distance': 5.510104179382324, 'directional_contribution': -8.050490911518978}, {'ion': 1403, 'force': [-2.5566587448120117, -2.16740083694458, -6.0023908615112305], 'magnitude': 6.874796390533447, 'distance': 6.9492692947387695, 'directional_contribution': 2.6219290923979797}, {'ion': 1469, 'force': [-0.4554177522659302, -0.4476567804813385, -2.1290900707244873], 'magnitude': 2.22279691696167, 'distance': 12.221348762512207, 'directional_contribution': 1.1658092836760385}]}, 5222: {'frame': 5222, 'ionic_force': [-10.679179668426514, 1.4521918892860413, -9.871692180633545], 'ionic_force_magnitude': 14.615199149618997, 'motion_vector': [-3.9730682373046875, -1.5599021911621094, 2.0731430053710938], 'cosine_ionic_motion': 0.2840376600251383, 'ionic_motion_component': 4.151266967259171, 'ionic_force_x': -10.679179668426514, 'ionic_force_y': 1.4521918892860413, 'ionic_force_z': -9.871692180633545, 'radial_force': 10.777464436213297, 'axial_force': -9.871692180633545, 'contributions': [{'ion': 1308, 'force': [-2.3145053386688232, -2.909573793411255, -2.4544501304626465], 'magnitude': 4.454983711242676, 'distance': 8.632686614990234, 'directional_contribution': 1.822050778624856}, {'ion': 1320, 'force': [-7.233617305755615, 3.4570906162261963, -3.964205026626587], 'magnitude': 8.943802833557129, 'distance': 6.0926737785339355, 'directional_contribution': 3.1882140577431386}, {'ion': 1403, 'force': [-1.1310570240020752, 0.9046750664710999, -3.4530370235443115], 'magnitude': 3.74448823928833, 'distance': 9.4161376953125, 'directional_contribution': -0.8589978912641101}]}, 5223: {'frame': 5223, 'ionic_force': [-9.0616614818573, -0.7365338355302811, -3.7814049124717712], 'ionic_force_magnitude': 9.846583875371337, 'motion_vector': [1.1881523132324219, 0.9744796752929688, 2.5615386962890625], 'cosine_ionic_motion': -0.7197750582208821, 'ionic_motion_component': -7.0873254821722025, 'ionic_force_x': -9.0616614818573, 'ionic_force_y': -0.7365338355302811, 'ionic_force_z': -3.7814049124717712, 'radial_force': 9.09154502285817, 'axial_force': -3.7814049124717712, 'contributions': [{'ion': 1308, 'force': [-2.0935752391815186, -1.8744561672210693, -0.5705388188362122], 'magnitude': 2.8674304485321045, 'distance': 10.760255813598633, 'directional_contribution': -1.933498388602409}, {'ion': 1320, 'force': [-4.028995990753174, 0.7997772693634033, 0.7936450242996216], 'magnitude': 4.183578014373779, 'distance': 8.908306121826172, 'directional_contribution': -0.6610887659741991}, {'ion': 1403, 'force': [-2.2542738914489746, 0.2554945647716522, -2.6964259147644043], 'magnitude': 3.523881435394287, 'distance': 9.706404685974121, 'directional_contribution': -3.125583209489937}, {'ion': 1469, 'force': [-0.6848163604736328, 0.08265049755573273, -1.3080852031707764], 'magnitude': 1.4788141250610352, 'distance': 14.983464241027832, 'directional_contribution': -1.367155000136628}]}, 5224: {'frame': 5224, 'ionic_force': [-11.852895140647888, 1.5224820375442505, -2.5712924543768167], 'ionic_force_magnitude': 12.223772725953896, 'motion_vector': [0.0398406982421875, 2.6087303161621094, -0.5442276000976562], 'cosine_ionic_motion': 0.1503708447138321, 'ionic_motion_component': 1.8380990303915896, 'ionic_force_x': -11.852895140647888, 'ionic_force_y': 1.5224820375442505, 'ionic_force_z': -2.5712924543768167, 'radial_force': 11.950275091806015, 'axial_force': -2.5712924543768167, 'contributions': [{'ion': 1308, 'force': [-3.0808727741241455, -2.469778537750244, 0.02193385921418667], 'magnitude': 3.948678731918335, 'distance': 9.16944694519043, 'directional_contribution': -2.4679905922540377}, {'ion': 1320, 'force': [-3.7092082500457764, 2.256039619445801, 2.863736867904663], 'magnitude': 5.2008585929870605, 'distance': 7.989719390869141, 'directional_contribution': 1.56802880677661}, {'ion': 1403, 'force': [-4.130849361419678, 1.4701601266860962, -3.665073871612549], 'magnitude': 5.714722633361816, 'distance': 7.622044086456299, 'directional_contribution': 2.125667116136732}, {'ion': 1469, 'force': [-0.9319647550582886, 0.26606082916259766, -1.7918893098831177], 'magnitude': 2.0372073650360107, 'distance': 12.765899658203125, 'directional_contribution': 0.6123937048573254}]}, 5225: {'frame': 5225, 'ionic_force': [-12.727189838886261, 4.494718790054321, -5.815616488456726], 'ionic_force_magnitude': 14.697117177784452, 'motion_vector': [1.9323806762695312, 0.8050422668457031, -0.5858154296875], 'cosine_ionic_motion': -0.5498999726922859, 'ionic_motion_component': -8.081944334718996, 'ionic_force_x': -12.727189838886261, 'ionic_force_y': 4.494718790054321, 'ionic_force_z': -5.815616488456726, 'radial_force': 13.49755008128205, 'axial_force': -5.815616488456726, 'contributions': [{'ion': 1308, 'force': [-5.498988151550293, -1.1754382848739624, 0.6942658424377441], 'magnitude': 5.665909767150879, 'distance': 7.654806613922119, 'directional_contribution': -5.510707500471813}, {'ion': 1320, 'force': [-4.546165466308594, 3.720468282699585, -2.5248541831970215], 'magnitude': 6.394090175628662, 'distance': 7.2057576179504395, 'directional_contribution': -1.983028263270576}, {'ion': 1403, 'force': [-2.0169267654418945, 1.4461729526519775, -2.5027101039886475], 'magnitude': 3.524623155593872, 'distance': 9.70538330078125, 'directional_contribution': -0.5829049549384706}, {'ion': 1469, 'force': [-0.6651094555854797, 0.5035158395767212, -1.4823180437088013], 'magnitude': 1.7009308338165283, 'distance': 13.970943450927734, 'directional_contribution': -0.005303314350566524}]}, 5226: {'frame': 5226, 'ionic_force': [-8.63455793261528, 10.306835412979126, -8.068451166152954], 'ionic_force_magnitude': 15.680763729567671, 'motion_vector': [-0.0262298583984375, 0.5780372619628906, 0.1553192138671875], 'cosine_ionic_motion': 0.5248802706088915, 'ionic_motion_component': 8.23052350972957, 'ionic_force_x': -8.63455793261528, 'ionic_force_y': 10.306835412979126, 'ionic_force_z': -8.068451166152954, 'radial_force': 13.445685067036564, 'axial_force': -8.068451166152954, 'contributions': [{'ion': 1308, 'force': [-3.372286558151245, 1.1184394359588623, 0.5709807872772217], 'magnitude': 3.5985054969787598, 'distance': 9.605234146118164, 'directional_contribution': 1.374757997942818}, {'ion': 1320, 'force': [-3.445181369781494, 6.423120021820068, -3.7658469676971436], 'magnitude': 8.204105377197266, 'distance': 6.361410617828369, 'directional_contribution': 5.371688847001147}, {'ion': 1403, 'force': [-1.4268732070922852, 2.1184980869293213, -3.1947760581970215], 'magnitude': 4.090305328369141, 'distance': 9.009303092956543, 'directional_contribution': 1.278197102482256}, {'ion': 1469, 'force': [-0.39021679759025574, 0.646777868270874, -1.6788089275360107], 'magnitude': 1.8409210443496704, 'distance': 13.429241180419922, 'directional_contribution': 0.20587985755624938}]}, 5227: {'frame': 5227, 'ionic_force': [-7.94691988825798, 10.216525435447693, -6.894068896770477], 'ionic_force_magnitude': 14.66489391836702, 'motion_vector': [-1.3651809692382812, -0.9860496520996094, 0.14288330078125], 'cosine_ionic_motion': -0.008475451243119256, 'ionic_motion_component': -0.12429159339063578, 'ionic_force_x': -7.94691988825798, 'ionic_force_y': 10.216525435447693, 'ionic_force_z': -6.894068896770477, 'radial_force': 12.94337389105097, 'axial_force': -6.894068896770477, 'contributions': [{'ion': 1308, 'force': [-3.113513946533203, 1.471713900566101, 0.5079912543296814], 'magnitude': 3.4810869693756104, 'distance': 9.765885353088379, 'directional_contribution': 1.6992574855999774}, {'ion': 1320, 'force': [-3.006080389022827, 5.83809232711792, -2.921882152557373], 'magnitude': 7.1872968673706055, 'distance': 6.796514511108398, 'directional_contribution': -1.2249553237593886}, {'ion': 1403, 'force': [-1.393346905708313, 2.2208824157714844, -2.820758104324341], 'magnitude': 3.851027250289917, 'distance': 9.284975051879883, 'directional_contribution': -0.40871553483142975}, {'ion': 1469, 'force': [-0.4339786469936371, 0.6858367919921875, -1.6594198942184448], 'magnitude': 1.8472638130187988, 'distance': 13.40616512298584, 'directional_contribution': -0.1898785247648629}]}, 5228: {'frame': 5228, 'ionic_force': [-9.87448799610138, 7.389701664447784, -6.990283265709877], 'ionic_force_magnitude': 14.176645019522642, 'motion_vector': [0.7691383361816406, -0.3768424987792969, -0.10305023193359375], 'cosine_ionic_motion': -0.789812787166785, 'ionic_motion_component': -11.1968955155433, 'ionic_force_x': -9.87448799610138, 'ionic_force_y': 7.389701664447784, 'ionic_force_z': -6.990283265709877, 'radial_force': 12.333418174808337, 'axial_force': -6.990283265709877, 'contributions': [{'ion': 1308, 'force': [-2.4451513290405273, 0.9452031254768372, 0.08026061952114105], 'magnitude': 2.622711658477783, 'distance': 11.251069068908691, 'directional_contribution': -2.6025218019028573}, {'ion': 1320, 'force': [-5.125226974487305, 4.3977861404418945, -2.9678163528442383], 'magnitude': 7.3767476081848145, 'distance': 6.708672046661377, 'directional_contribution': -6.136104879864973}, {'ion': 1403, 'force': [-1.7134193181991577, 1.530916690826416, -2.4926624298095703], 'magnitude': 3.3901147842407227, 'distance': 9.896049499511719, 'directional_contribution': -1.8986371754413724}, {'ion': 1469, 'force': [-0.5906903743743896, 0.5157957077026367, -1.6100651025772095], 'magnitude': 1.790885329246521, 'distance': 13.615549087524414, 'directional_contribution': -0.5596317703114053}]}, 5229: {'frame': 5229, 'ionic_force': [-9.413652211427689, 7.915450572967529, -7.1453061401844025], 'ionic_force_magnitude': 14.224155706676102, 'motion_vector': [-2.0034332275390625, -4.632930755615234, 0.2904510498046875], 'cosine_ionic_motion': -0.2765377108802912, 'ionic_motion_component': -3.9335154583290404, 'ionic_force_x': -9.413652211427689, 'ionic_force_y': 7.915450572967529, 'ionic_force_z': -7.1453061401844025, 'radial_force': 12.299235981588833, 'axial_force': -7.1453061401844025, 'contributions': [{'ion': 1308, 'force': [-3.0030407905578613, 0.9390349388122559, 0.19887909293174744], 'magnitude': 3.152712106704712, 'distance': 10.261878967285156, 'directional_contribution': 0.3409227587045228}, {'ion': 1320, 'force': [-4.218984603881836, 4.771722316741943, -2.8418822288513184], 'magnitude': 6.974629878997803, 'distance': 6.899354457855225, 'directional_contribution': -2.8639856380834434}, {'ion': 1403, 'force': [-1.7074979543685913, 1.6937834024429321, -2.7924537658691406], 'magnitude': 3.685410261154175, 'distance': 9.49130916595459, 'directional_contribution': -1.0358969432865663}, {'ion': 1469, 'force': [-0.4841288626194, 0.510909914970398, -1.709849238395691], 'magnitude': 1.8490521907806396, 'distance': 13.399681091308594, 'directional_contribution': -0.37455583836772854}]}, 5230: {'frame': 5230, 'ionic_force': [-13.472239375114441, -2.136018753051758, -5.8683589696884155], 'ionic_force_magnitude': 14.849291124188225, 'motion_vector': [5.115959167480469, 0.8695487976074219, -4.300270080566406], 'cosine_ionic_motion': -0.4551001034999545, 'ionic_motion_component': -6.7579139275190165, 'ionic_force_x': -13.472239375114441, 'ionic_force_y': -2.136018753051758, 'ionic_force_z': -5.8683589696884155, 'radial_force': 13.64052088058857, 'axial_force': -5.8683589696884155, 'contributions': [{'ion': 1308, 'force': [-3.4431419372558594, -1.4593416452407837, 1.5944634675979614], 'magnitude': 4.065368175506592, 'distance': 9.03689193725586, 'directional_contribution': -3.819332482993259}, {'ion': 1320, 'force': [-6.761546611785889, -0.46857988834381104, -2.9621737003326416], 'magnitude': 7.396793365478516, 'distance': 6.699575424194336, 'directional_contribution': -3.3030568067030313}, {'ion': 1403, 'force': [-2.4797613620758057, -0.12971417605876923, -2.8303792476654053], 'magnitude': 3.7652475833892822, 'distance': 9.390144348144531, 'directional_contribution': -0.0931450562886138}, {'ion': 1469, 'force': [-0.7877894639968872, -0.07838304340839386, -1.67026948928833], 'magnitude': 1.8483929634094238, 'distance': 13.402070045471191, 'directional_contribution': 0.4576203640856893}]}, 5231: {'frame': 5231, 'ionic_force': [-4.702645644545555, -10.708216772880405, -12.202762365341187], 'ionic_force_magnitude': 16.902313210272368, 'motion_vector': [-1.9342155456542969, 1.1726150512695312, 1.3013763427734375], 'cosine_ionic_motion': -0.43849772857207303, 'ionic_motion_component': -7.411625950318177, 'ionic_force_x': -4.702645644545555, 'ionic_force_y': -10.708216772880405, 'ionic_force_z': -12.202762365341187, 'radial_force': 11.695331654688571, 'axial_force': -12.202762365341187, 'contributions': [{'ion': 1308, 'force': [-4.075906753540039, -10.616989135742188, -3.460934638977051], 'magnitude': 11.887453079223633, 'distance': 5.284752368927002, 'directional_contribution': -3.4756596741904104}, {'ion': 1320, 'force': [-0.42284056544303894, -0.09886391460895538, -6.389946937561035], 'magnitude': 6.404685020446777, 'distance': 7.199795246124268, 'directional_contribution': -2.9176545042145263}, {'ion': 1403, 'force': [-0.2038983255624771, 0.007636277470737696, -2.3518807888031006], 'magnitude': 2.36071515083313, 'distance': 11.858977317810059, 'directional_contribution': -1.0183118087160872}]}, 5232: {'frame': 5232, 'ionic_force': [-15.006769359111786, -7.3863255977630615, -12.328855037689209], 'ionic_force_magnitude': 20.778873862028732, 'motion_vector': [-2.0798912048339844, 0.45478057861328125, 1.3255767822265625], 'cosine_ionic_motion': 0.2208754185682539, 'ionic_motion_component': 4.589542461652547, 'ionic_force_x': -15.006769359111786, 'ionic_force_y': -7.3863255977630615, 'ionic_force_z': -12.328855037689209, 'radial_force': 16.726055495356526, 'axial_force': -12.328855037689209, 'contributions': [{'ion': 1308, 'force': [-10.581357955932617, -10.495577812194824, -2.068549871444702], 'magnitude': 15.04663372039795, 'distance': 4.6973114013671875, 'directional_contribution': 5.778718101797736}, {'ion': 1320, 'force': [-3.4290311336517334, 2.5227065086364746, -7.157139778137207], 'magnitude': 8.327482223510742, 'distance': 6.31411075592041, 'directional_contribution': -0.48168358166323344}, {'ion': 1403, 'force': [-0.9963802695274353, 0.5865457057952881, -3.1031653881073], 'magnitude': 3.3115622997283936, 'distance': 10.012731552124023, 'directional_contribution': -0.7074926152914962}]}, 5233: {'frame': 5233, 'ionic_force': [-14.879006922245026, 1.6513826549053192, -8.93515632301569], 'ionic_force_magnitude': 17.434131185174234, 'motion_vector': [-1.1857566833496094, -2.693035125732422, 0.8188629150390625], 'cosine_ionic_motion': 0.11040390686238014, 'ionic_motion_component': 1.9247961955944932, 'ionic_force_x': -14.879006922245026, 'ionic_force_y': 1.6513826549053192, 'ionic_force_z': -8.93515632301569, 'radial_force': 14.970367786568824, 'axial_force': -8.93515632301569, 'contributions': [{'ion': 1308, 'force': [-8.045933723449707, -1.5553702116012573, 0.07402922958135605], 'magnitude': 8.19522476196289, 'distance': 6.364856243133545, 'directional_contribution': 4.514823348282454}, {'ion': 1320, 'force': [-4.9024658203125, 2.3702609539031982, -4.955585479736328], 'magnitude': 7.362753391265869, 'distance': 6.715044975280762, 'directional_contribution': -1.5152240276781868}, {'ion': 1403, 'force': [-1.4236538410186768, 0.6275284290313721, -2.5825090408325195], 'magnitude': 3.0149519443511963, 'distance': 10.493704795837402, 'directional_contribution': -0.6929712621797393}, {'ion': 1469, 'force': [-0.5069535374641418, 0.20896348357200623, -1.4710910320281982], 'magnitude': 1.569960594177246, 'distance': 14.542016983032227, 'directional_contribution': -0.3818318543778467}]}, 5234: {'frame': 5234, 'ionic_force': [-12.36766916513443, -6.169648960232735, -5.632678389549255], 'ionic_force_magnitude': 14.924840860485348, 'motion_vector': [-0.7371978759765625, 0.9959373474121094, -1.500885009765625], 'cosine_ionic_motion': 0.39337879102866113, 'ionic_motion_component': 5.8711158539928885, 'ionic_force_x': -12.36766916513443, 'ionic_force_y': -6.169648960232735, 'ionic_force_z': -5.632678389549255, 'radial_force': 13.82113630895513, 'axial_force': -5.632678389549255, 'contributions': [{'ion': 1308, 'force': [-4.263079643249512, -5.226989269256592, 1.3957465887069702], 'magnitude': 6.887914657592773, 'distance': 6.942647933959961, 'directional_contribution': -2.1363187537023762}, {'ion': 1320, 'force': [-5.668378829956055, -0.6114987134933472, -3.2219982147216797], 'magnitude': 6.54871940612793, 'distance': 7.12017822265625, 'directional_contribution': 4.318776847613336}, {'ion': 1403, 'force': [-1.7518445253372192, -0.24626709520816803, -2.2820186614990234], 'magnitude': 2.8874237537384033, 'distance': 10.72293758392334, 'directional_contribution': 2.2973240529196257}, {'ion': 1469, 'force': [-0.6843661665916443, -0.08489388227462769, -1.5244081020355225], 'magnitude': 1.6731359958648682, 'distance': 14.086509704589844, 'directional_contribution': 1.3913336358783646}]}, 5235: {'frame': 5235, 'ionic_force': [-9.108755230903625, -5.003531493246555, -4.880807518959045], 'ionic_force_magnitude': 11.481595328940635, 'motion_vector': [0.478057861328125, 0.5345573425292969, -0.0841217041015625], 'cosine_ionic_motion': -0.7983481136190297, 'ionic_motion_component': -9.166309972196819, 'ionic_force_x': -9.108755230903625, 'ionic_force_y': -5.003531493246555, 'ionic_force_z': -4.880807518959045, 'radial_force': 10.39253334179998, 'axial_force': -4.880807518959045, 'contributions': [{'ion': 1308, 'force': [-4.102746486663818, -5.535513401031494, -1.0437307357788086], 'magnitude': 6.968774318695068, 'distance': 6.902252674102783, 'directional_contribution': -6.692815687143749}, {'ion': 1320, 'force': [-3.311994791030884, 0.44610047340393066, -1.7596060037612915], 'magnitude': 3.776841163635254, 'distance': 9.375720977783203, 'directional_contribution': -1.6575375503540872}, {'ion': 1403, 'force': [-1.6940139532089233, 0.08588143438100815, -2.0774707794189453], 'magnitude': 2.681966543197632, 'distance': 11.12608528137207, 'directional_contribution': -0.8159565702947376}]}, 5236: {'frame': 5236, 'ionic_force': [-8.572914719581604, -3.368498131632805, -3.489031046628952], 'ionic_force_magnitude': 9.849618474660495, 'motion_vector': [-1.1881294250488281, -1.5159759521484375, -0.36592864990234375], 'cosine_ionic_motion': 0.8580266738193267, 'ionic_motion_component': 8.451235378202336, 'ionic_force_x': -8.572914719581604, 'ionic_force_y': -3.368498131632805, 'ionic_force_z': -3.489031046628952, 'radial_force': 9.210952526858046, 'axial_force': -3.489031046628952, 'contributions': [{'ion': 1308, 'force': [-4.18311882019043, -3.761627435684204, -0.9836950898170471], 'magnitude': 5.711040496826172, 'distance': 7.6245012283325195, 'directional_contribution': 5.62730424929216}, {'ion': 1320, 'force': [-2.6477365493774414, 0.20306988060474396, -0.23778191208839417], 'magnitude': 2.6661369800567627, 'distance': 11.159065246582031, 'directional_contribution': 1.4919398983652878}, {'ion': 1403, 'force': [-1.742059350013733, 0.19005942344665527, -2.2675540447235107], 'magnitude': 2.8657801151275635, 'distance': 10.763354301452637, 'directional_contribution': 1.3319913392970584}]}, 5237: {'frame': 5237, 'ionic_force': [-6.391249179840088, -5.777417056262493, -3.9080119132995605], 'ionic_force_magnitude': 9.460400151964539, 'motion_vector': [0.7070693969726562, -0.0630950927734375, -0.1740264892578125], 'cosine_ionic_motion': -0.5024779128737921, 'ionic_motion_component': -4.753642123310047, 'ionic_force_x': -6.391249179840088, 'ionic_force_y': -5.777417056262493, 'ionic_force_z': -3.9080119132995605, 'radial_force': 8.61548686498908, 'axial_force': -3.9080119132995605, 'contributions': [{'ion': 1308, 'force': [-2.8145735263824463, -5.6946563720703125, -2.4584314823150635], 'magnitude': 6.811374187469482, 'distance': 6.981546878814697, 'directional_contribution': -1.6458657787542137}, {'ion': 1320, 'force': [-2.0174343585968018, 0.07914838939905167, 0.4097496271133423], 'magnitude': 2.060145616531372, 'distance': 12.69463062286377, 'directional_contribution': -2.056053109547623}, {'ion': 1403, 'force': [-1.5592412948608398, -0.1619090735912323, -1.8593300580978394], 'magnitude': 2.431986093521118, 'distance': 11.683917999267578, 'directional_contribution': -1.0517231484963974}]}, 5238: {'frame': 5238, 'ionic_force': [-7.0983967781066895, -5.104644980281591, -4.2284344136714935], 'ionic_force_magnitude': 9.712069541805745, 'motion_vector': [0.08398056030273438, 0.23592376708984375, -0.195953369140625], 'cosine_ionic_motion': -0.3146973925458533, 'ionic_motion_component': -3.0563629610302683, 'ionic_force_x': -7.0983967781066895, 'ionic_force_y': -5.104644980281591, 'ionic_force_z': -4.2284344136714935, 'radial_force': 8.74326238849947, 'axial_force': -4.2284344136714935, 'contributions': [{'ion': 1308, 'force': [-3.053865671157837, -5.131225109100342, -2.3726069927215576], 'magnitude': 6.425327301025391, 'distance': 7.188220977783203, 'directional_contribution': -3.151540825804503}, {'ion': 1320, 'force': [-2.2170028686523438, 0.06498879194259644, 0.2705501616001129], 'magnitude': 2.2343952655792236, 'distance': 12.189587593078613, 'directional_contribution': -0.7040343494075945}, {'ion': 1403, 'force': [-1.8275282382965088, -0.038408663123846054, -2.126377582550049], 'magnitude': 2.8040714263916016, 'distance': 10.881142616271973, 'directional_contribution': 0.7992122036876315}]}, 5239: {'frame': 5239, 'ionic_force': [-8.07841670513153, -6.338533233851194, -6.204916596412659], 'ionic_force_magnitude': 11.99745014521092, 'motion_vector': [0.3502960205078125, -0.14125442504882812, 0.9509506225585938], 'cosine_ionic_motion': -0.6382442224773681, 'ionic_motion_component': -7.657303239641131, 'ionic_force_x': -8.07841670513153, 'ionic_force_y': -6.338533233851194, 'ionic_force_z': -6.204916596412659, 'radial_force': 10.268291971812268, 'axial_force': -6.204916596412659, 'contributions': [{'ion': 1308, 'force': [-4.299147605895996, -6.337735652923584, -4.5308661460876465], 'magnitude': 8.89822006225586, 'distance': 6.108259677886963, 'directional_contribution': -4.807763211573729}, {'ion': 1320, 'force': [-2.1025471687316895, 0.04053327441215515, 0.4063223600387573], 'magnitude': 2.141832113265991, 'distance': 12.450199127197266, 'directional_contribution': -0.3477736340537625}, {'ion': 1403, 'force': [-1.6767219305038452, -0.04133085533976555, -2.080</t>
+          <t>{5213: {'frame': 5213, 'ionic_force': [9.059208557009697, 6.910908341407776, -17.690110206604004], 'ionic_force_magnitude': 21.042098586037763, 'motion_vector': [-0.08104324340820312, -3.535572052001953, 0.40856170654296875], 'cosine_ionic_motion': -0.43245966970827554, 'ionic_motion_component': -9.099859004486863, 'ionic_force_x': 9.059208557009697, 'ionic_force_y': 6.910908341407776, 'ionic_force_z': -17.690110206604004, 'radial_force': 11.394293035670852, 'axial_force': -17.690110206604004, 'contributions': [{'ion': 1308, 'force': [4.778199672698975, 9.435524940490723, -10.170702934265137], 'magnitude': 14.673224449157715, 'distance': 4.756705284118652, 'cosine_with_motion': -0.7255885946159099, 'motion_component': -10.646724441459995}, {'ion': 1320, 'force': [4.232130527496338, -3.0712902545928955, -4.9525957107543945], 'magnitude': 7.202219009399414, 'distance': 6.789470195770264, 'cosine_with_motion': 0.33121377374106037, 'motion_component': 2.3854740970482444}, {'ion': 1403, 'force': [0.04887835681438446, 0.5466736555099487, -2.5668115615844727], 'magnitude': 2.624835729598999, 'distance': 11.246515274047852, 'cosine_with_motion': -0.31949001303026325, 'motion_component': -0.8386088114752297}]}, 5214: {'frame': 5214, 'ionic_force': [0.876273438334465, -7.065377295017242, -7.964790105819702], 'ionic_force_magnitude': 10.682944017893153, 'motion_vector': [-2.800647735595703, -0.17963790893554688, 2.6386032104492188], 'cosine_ionic_motion': -0.5394970021714701, 'ionic_motion_component': -5.763416272018996, 'ionic_force_x': 0.876273438334465, 'ionic_force_y': -7.065377295017242, 'ionic_force_z': -7.964790105819702, 'radial_force': 7.119509214803761, 'axial_force': -7.964790105819702, 'contributions': [{'ion': 1308, 'force': [-1.3250770568847656, -3.1238503456115723, -2.5353305339813232], 'magnitude': 4.2358198165893555, 'distance': 8.85319995880127, 'cosine_with_motion': -0.14816259756217112, 'motion_component': -0.6275900945759094}, {'ion': 1320, 'force': [2.0835518836975098, -3.640300989151001, -2.173349618911743], 'magnitude': 4.724026679992676, 'distance': 8.383258819580078, 'cosine_with_motion': -0.5998743875613214, 'motion_component': -2.8338226264943356}, {'ion': 1403, 'force': [0.11779861152172089, -0.3012259602546692, -3.2561099529266357], 'magnitude': 3.272134780883789, 'distance': 10.072875022888184, 'cosine_with_motion': -0.7035172793829035, 'motion_component': -2.302003315099296}]}, 5215: {'frame': 5215, 'ionic_force': [-3.1574587523937225, -9.676621198654175, -7.118128061294556], 'ionic_force_magnitude': 12.42072021632804, 'motion_vector': [0.9844284057617188, -0.2884941101074219, -5.571617126464844], 'cosine_ionic_motion': 0.5591117071431897, 'ionic_motion_component': 6.944570084099098, 'ionic_force_x': -3.1574587523937225, 'ionic_force_y': -9.676621198654175, 'ionic_force_z': -7.118128061294556, 'radial_force': 10.178729959838362, 'axial_force': -7.118128061294556, 'contributions': [{'ion': 1308, 'force': [-2.1365599632263184, -3.032615900039673, -0.8023586273193359], 'magnitude': 3.7954483032226562, 'distance': 9.352710723876953, 'cosine_with_motion': 0.15077678582865442, 'motion_component': 0.5722654804066467}, {'ion': 1320, 'force': [0.5601136684417725, -6.005922317504883, -0.8906189203262329], 'magnitude': 6.097379207611084, 'distance': 7.378998756408691, 'cosine_with_motion': 0.20977316123691703, 'motion_component': 1.2790664955624322}, {'ion': 1403, 'force': [-1.2336101531982422, -0.5227363109588623, -3.747150182723999], 'magnitude': 3.9794700145721436, 'distance': 9.133903503417969, 'cosine_with_motion': 0.8788779690915066, 'motion_component': 3.4974685416808162}, {'ion': 1469, 'force': [-0.34740230441093445, -0.11534667015075684, -1.6780003309249878], 'magnitude': 1.7174626588821411, 'distance': 13.903539657592773, 'cosine_with_motion': 0.9291435751757805, 'motion_component': 1.5957694874407418}]}, 5216: {'frame': 5216, 'ionic_force': [0.3360389769077301, -3.4986054599285126, -5.366488456726074], 'ionic_force_magnitude': 6.415010577888161, 'motion_vector': [0.49591064453125, 1.3578147888183594, -0.21898651123046875], 'cosine_ionic_motion': -0.3634329471769188, 'ionic_motion_component': -2.3314262004930035, 'ionic_force_x': 0.3360389769077301, 'ionic_force_y': -3.4986054599285126, 'ionic_force_z': -5.366488456726074, 'radial_force': 3.51470658209797, 'axial_force': -5.366488456726074, 'contributions': [{'ion': 1308, 'force': [-0.5920225381851196, -1.5384231805801392, -1.2295265197753906], 'magnitude': 2.0564465522766113, 'distance': 12.706043243408203, 'cosine_with_motion': -0.7028663925785696, 'motion_component': -1.4454071028631574}, {'ion': 1320, 'force': [1.186414122581482, -1.7023833990097046, -2.2223496437072754], 'magnitude': 3.0404810905456543, 'distance': 10.449557304382324, 'cosine_with_motion': -0.2781600982653527, 'motion_component': -0.8457405365038682}, {'ion': 1403, 'force': [-0.2583526074886322, -0.2577988803386688, -1.9146122932434082], 'magnitude': 1.9490886926651, 'distance': 13.051283836364746, 'cosine_with_motion': -0.020665348923662074, 'motion_component': -0.04027859703741399}]}, 5217: {'frame': 5217, 'ionic_force': [-0.5696889609098434, -2.4908271618187428, -6.695563793182373], 'ionic_force_magnitude': 7.166543097673472, 'motion_vector': [1.0223388671875, -0.4985237121582031, 2.0433120727539062], 'cosine_ionic_motion': -0.7769881557830077, 'ionic_motion_component': -5.5683191048007545, 'ionic_force_x': -0.5696889609098434, 'ionic_force_y': -2.4908271618187428, 'ionic_force_z': -6.695563793182373, 'radial_force': 2.555144900438437, 'axial_force': -6.695563793182373, 'contributions': [{'ion': 1308, 'force': [-1.6062496900558472, -1.6342322826385498, -2.415165901184082], 'magnitude': 3.329231023788452, 'distance': 9.986126899719238, 'cosine_with_motion': -0.7401330330015188, 'motion_component': -2.4640738930936728}, {'ion': 1320, 'force': [1.2217909097671509, -0.8660487532615662, -2.349320888519287], 'magnitude': 2.7860584259033203, 'distance': 10.916261672973633, 'cosine_with_motion': -0.47880292106144073, 'motion_component': -1.333972960252149}, {'ion': 1403, 'force': [-0.18523018062114716, 0.009453874081373215, -1.931077003479004], 'magnitude': 1.939963459968567, 'distance': 13.08194351196289, 'cosine_with_motion': -0.912528632425414, 'motion_component': -1.7702721473163905}]}, 5218: {'frame': 5218, 'ionic_force': [4.206250421702862, -4.269712045788765, -7.6996800899505615], 'ionic_force_magnitude': 9.757461609025693, 'motion_vector': [-0.7376747131347656, 0.12036895751953125, 5.263938903808594], 'cosine_ionic_motion': -0.8509877619478586, 'ionic_motion_component': -8.303480416956926, 'ionic_force_x': 4.206250421702862, 'ionic_force_y': -4.269712045788765, 'ionic_force_z': -7.6996800899505615, 'radial_force': 5.993578527393228, 'axial_force': -7.6996800899505615, 'contributions': [{'ion': 1308, 'force': [-1.0178943872451782, -2.646784543991089, -2.161548376083374], 'magnitude': 3.5656511783599854, 'distance': 9.649384498596191, 'cosine_with_motion': -0.5773913926795388, 'motion_component': -2.0587763371135157}, {'ion': 1320, 'force': [5.3220672607421875, -1.4583486318588257, -2.8955790996551514], 'magnitude': 6.231818199157715, 'distance': 7.298971652984619, 'cosine_with_motion': -0.5838190835985204, 'motion_component': -3.6382544330410886}, {'ion': 1403, 'force': [-0.09792245179414749, -0.1645788699388504, -2.642552614212036], 'magnitude': 2.6494827270507812, 'distance': 11.194082260131836, 'cosine_with_motion': -0.9837579542078188, 'motion_component': -2.606449820321628}]}, 5219: {'frame': 5219, 'ionic_force': [-0.8370766043663025, 7.505206935107708, 4.665254652500153], 'ionic_force_magnitude': 8.876566304210236, 'motion_vector': [-1.3892173767089844, -0.5494041442871094, 1.6649017333984375], 'cosine_ionic_motion': 0.24207837425350287, 'ionic_motion_component': 2.1488247398766385, 'ionic_force_x': -0.8370766043663025, 'ionic_force_y': 7.505206935107708, 'ionic_force_z': 4.665254652500153, 'radial_force': 7.551743400061091, 'axial_force': 4.665254652500153, 'contributions': [{'ion': 1308, 'force': [-1.2311298847198486, -4.110632419586182, -0.6271311640739441], 'magnitude': 4.336619853973389, 'distance': 8.749703407287598, 'cosine_with_motion': 0.30148794664863837, 'motion_component': 1.3074386645678937}, {'ion': 1320, 'force': [1.5758368968963623, 11.999844551086426, 15.897293090820312], 'magnitude': 19.98007583618164, 'distance': 4.076340675354004, 'cosine_with_motion': 0.3957087251708299, 'motion_component': 7.906290618905373}, {'ion': 1403, 'force': [-1.0520174503326416, -0.32890668511390686, -8.382981300354004], 'magnitude': 8.455134391784668, 'distance': 6.266265392303467, 'cosine_with_motion': -0.6511147850343424, 'motion_component': -5.505262943493138}, {'ion': 1469, 'force': [-0.12976616621017456, -0.0550985112786293, -2.221925973892212], 'magnitude': 2.226393938064575, 'distance': 12.211472511291504, 'cosine_with_motion': -0.7005236558494705, 'motion_component': -1.5596416475744035}]}, 5220: {'frame': 5220, 'ionic_force': [-7.989065766334534, -10.187750428915024, -5.366817504167557], 'ionic_force_magnitude': 14.01492635527265, 'motion_vector': [-0.5346794128417969, -1.1390304565429688, -0.756134033203125], 'cosine_ionic_motion': 0.9688891272673253, 'ionic_motion_component': 13.578909765075954, 'ionic_force_x': -7.989065766334534, 'ionic_force_y': -10.187750428915024, 'ionic_force_z': -5.366817504167557, 'radial_force': 12.946637811442654, 'axial_force': -5.366817504167557, 'contributions': [{'ion': 1308, 'force': [-1.290416955947876, -3.383082866668701, 0.44074055552482605], 'magnitude': 3.6475577354431152, 'distance': 9.540430068969727, 'cosine_with_motion': 0.7862651912087649, 'motion_component': 2.867947724152115}, {'ion': 1320, 'force': [-1.2900820970535278, -3.8637619018554688, 8.199496269226074], 'magnitude': 9.155583381652832, 'distance': 6.021795749664307, 'cosine_with_motion': -0.0825272300641764, 'motion_component': -0.7555849354875583}, {'ion': 1403, 'force': [-4.87747859954834, -2.6918888092041016, -11.338939666748047], 'magnitude': 12.633590698242188, 'distance': 5.126319408416748, 'cosine_with_motion': 0.7682381903521565, 'motion_component': 9.705606906917723}, {'ion': 1469, 'force': [-0.53108811378479, -0.24901685118675232, -2.66811466217041], 'magnitude': 2.7318308353424072, 'distance': 11.02407455444336, 'cosine_with_motion': 0.6446005870361542, 'motion_component': 1.7609397736349202}]}, 5221: {'frame': 5221, 'ionic_force': [-10.496177196502686, -8.205937772989273, 0.1122767822816968], 'ionic_force_magnitude': 13.32365402396785, 'motion_vector': [0.09583663940429688, 4.582389831542969, -4.5017547607421875], 'cosine_ionic_motion': -0.4569579844587636, 'ionic_motion_component': -6.0883500884182435, 'ionic_force_x': -10.496177196502686, 'ionic_force_y': -8.205937772989273, 'ionic_force_z': 0.1122767822816968, 'radial_force': 13.32318094429987, 'axial_force': 0.1122767822816968, 'contributions': [{'ion': 1308, 'force': [-0.9717339277267456, -2.528850793838501, 0.010465134866535664], 'magnitude': 2.709144353866577, 'distance': 11.070137023925781, 'cosine_with_motion': -0.6738649628328864, 'motion_component': -1.825597403703803}, {'ion': 1320, 'force': [-6.512366771697998, -3.0620293617248535, 8.233292579650879], 'magnitude': 10.934991836547852, 'distance': 5.510104179382324, 'cosine_with_motion': -0.7362136948005549, 'motion_component': -8.050490911518978}, {'ion': 1403, 'force': [-2.5566587448120117, -2.16740083694458, -6.0023908615112305], 'magnitude': 6.874796390533447, 'distance': 6.9492692947387695, 'cosine_with_motion': 0.3813827954446882, 'motion_component': 2.6219290923979797}, {'ion': 1469, 'force': [-0.4554177522659302, -0.4476567804813385, -2.1290900707244873], 'magnitude': 2.22279691696167, 'distance': 12.221348762512207, 'cosine_with_motion': 0.5244785240319814, 'motion_component': 1.1658092836760383}]}, 5222: {'frame': 5222, 'ionic_force': [-10.679179668426514, 1.4521918892860413, -9.871692180633545], 'ionic_force_magnitude': 14.615199149618997, 'motion_vector': [-3.9730682373046875, -1.5599021911621094, 2.0731430053710938], 'cosine_ionic_motion': 0.2840376600251383, 'ionic_motion_component': 4.151266967259171, 'ionic_force_x': -10.679179668426514, 'ionic_force_y': 1.4521918892860413, 'ionic_force_z': -9.871692180633545, 'radial_force': 10.777464436213297, 'axial_force': -9.871692180633545, 'contributions': [{'ion': 1308, 'force': [-2.3145053386688232, -2.909573793411255, -2.4544501304626465], 'magnitude': 4.454983711242676, 'distance': 8.632686614990234, 'cosine_with_motion': 0.4089915671206331, 'motion_component': 1.822050778624856}, {'ion': 1320, 'force': [-7.233617305755615, 3.4570906162261963, -3.964205026626587], 'magnitude': 8.943802833557129, 'distance': 6.0926737785339355, 'cosine_with_motion': 0.356471846835402, 'motion_component': 3.1882140577431386}, {'ion': 1403, 'force': [-1.1310570240020752, 0.9046750664710999, -3.4530370235443115], 'magnitude': 3.74448823928833, 'distance': 9.4161376953125, 'cosine_with_motion': -0.22940328619630437, 'motion_component': -0.8589978912641101}]}, 5223: {'frame': 5223, 'ionic_force': [-9.0616614818573, -0.7365338355302811, -3.7814049124717712], 'ionic_force_magnitude': 9.846583875371337, 'motion_vector': [1.1881523132324219, 0.9744796752929688, 2.5615386962890625], 'cosine_ionic_motion': -0.7197750582208821, 'ionic_motion_component': -7.0873254821722025, 'ionic_force_x': -9.0616614818573, 'ionic_force_y': -0.7365338355302811, 'ionic_force_z': -3.7814049124717712, 'radial_force': 9.09154502285817, 'axial_force': -3.7814049124717712, 'contributions': [{'ion': 1308, 'force': [-2.0935752391815186, -1.8744561672210693, -0.5705388188362122], 'magnitude': 2.8674304485321045, 'distance': 10.760255813598633, 'cosine_with_motion': -0.6742965102789934, 'motion_component': -1.933498388602409}, {'ion': 1320, 'force': [-4.028995990753174, 0.7997772693634033, 0.7936450242996216], 'magnitude': 4.183578014373779, 'distance': 8.908306121826172, 'cosine_with_motion': -0.15801994549859863, 'motion_component': -0.6610887659741991}, {'ion': 1403, 'force': [-2.2542738914489746, 0.2554945647716522, -2.6964259147644043], 'magnitude': 3.523881435394287, 'distance': 9.706404685974121, 'cosine_with_motion': -0.886971707792664, 'motion_component': -3.125583209489937}, {'ion': 1469, 'force': [-0.6848163604736328, 0.08265049755573273, -1.3080852031707764], 'magnitude': 1.4788141250610352, 'distance': 14.983464241027832, 'cosine_with_motion': -0.9244940953963866, 'motion_component': -1.367155000136628}]}, 5224: {'frame': 5224, 'ionic_force': [-11.852895140647888, 1.5224820375442505, -2.5712924543768167], 'ionic_force_magnitude': 12.223772725953896, 'motion_vector': [0.0398406982421875, 2.6087303161621094, -0.5442276000976562], 'cosine_ionic_motion': 0.1503708447138321, 'ionic_motion_component': 1.8380990303915896, 'ionic_force_x': -11.852895140647888, 'ionic_force_y': 1.5224820375442505, 'ionic_force_z': -2.5712924543768167, 'radial_force': 11.950275091806015, 'axial_force': -2.5712924543768167, 'contributions': [{'ion': 1308, 'force': [-3.0808727741241455, -2.469778537750244, 0.02193385921418667], 'magnitude': 3.948678731918335, 'distance': 9.16944694519043, 'cosine_with_motion': -0.6250168030414615, 'motion_component': -2.4679905922540377}, {'ion': 1320, 'force': [-3.7092082500457764, 2.256039619445801, 2.863736867904663], 'magnitude': 5.2008585929870605, 'distance': 7.989719390869141, 'cosine_with_motion': 0.3014942239922375, 'motion_component': 1.5680288067766102}, {'ion': 1403, 'force': [-4.130849361419678, 1.4701601266860962, -3.665073871612549], 'magnitude': 5.714722633361816, 'distance': 7.622044086456299, 'cosine_with_motion': 0.3719633106605391, 'motion_component': 2.125667116136732}, {'ion': 1469, 'force': [-0.9319647550582886, 0.26606082916259766, -1.7918893098831177], 'magnitude': 2.0372073650360107, 'distance': 12.765899658203125, 'cosine_with_motion': 0.3006044973620889, 'motion_component': 0.6123937048573254}]}, 5225: {'frame': 5225, 'ionic_force': [-12.727189838886261, 4.494718790054321, -5.815616488456726], 'ionic_force_magnitude': 14.697117177784452, 'motion_vector': [1.9323806762695312, 0.8050422668457031, -0.5858154296875], 'cosine_ionic_motion': -0.5498999726922859, 'ionic_motion_component': -8.081944334718996, 'ionic_force_x': -12.727189838886261, 'ionic_force_y': 4.494718790054321, 'ionic_force_z': -5.815616488456726, 'radial_force': 13.49755008128205, 'axial_force': -5.815616488456726, 'contributions': [{'ion': 1308, 'force': [-5.498988151550293, -1.1754382848739624, 0.6942658424377441], 'magnitude': 5.665909767150879, 'distance': 7.654806613922119, 'cosine_with_motion': -0.9726077449400174, 'motion_component': -5.510707500471813}, {'ion': 1320, 'force': [-4.546165466308594, 3.720468282699585, -2.5248541831970215], 'magnitude': 6.394090175628662, 'distance': 7.2057576179504395, 'cosine_with_motion': -0.3101345317109207, 'motion_component': -1.983028263270576}, {'ion': 1403, 'force': [-2.0169267654418945, 1.4461729526519775, -2.5027101039886475], 'magnitude': 3.524623155593872, 'distance': 9.70538330078125, 'cosine_with_motion': -0.16538079293163058, 'motion_component': -0.5829049549384706}, {'ion': 1469, 'force': [-0.6651094555854797, 0.5035158395767212, -1.4823180437088013], 'magnitude': 1.7009308338165283, 'distance': 13.970943450927734, 'cosine_with_motion': -0.0031178895486980596, 'motion_component': -0.005303314350566524}]}, 5226: {'frame': 5226, 'ionic_force': [-8.63455793261528, 10.306835412979126, -8.068451166152954], 'ionic_force_magnitude': 15.680763729567671, 'motion_vector': [-0.0262298583984375, 0.5780372619628906, 0.1553192138671875], 'cosine_ionic_motion': 0.5248802706088915, 'ionic_motion_component': 8.23052350972957, 'ionic_force_x': -8.63455793261528, 'ionic_force_y': 10.306835412979126, 'ionic_force_z': -8.068451166152954, 'radial_force': 13.445685067036564, 'axial_force': -8.068451166152954, 'contributions': [{'ion': 1308, 'force': [-3.372286558151245, 1.1184394359588623, 0.5709807872772217], 'magnitude': 3.5985054969787598, 'distance': 9.605234146118164, 'cosine_with_motion': 0.382035810311084, 'motion_component': 1.374757997942818}, {'ion': 1320, 'force': [-3.445181369781494, 6.423120021820068, -3.7658469676971436], 'magnitude': 8.204105377197266, 'distance': 6.361410617828369, 'cosine_with_motion': 0.6547561796468672, 'motion_component': 5.371688847001148}, {'ion': 1403, 'force': [-1.4268732070922852, 2.1184980869293213, -3.1947760581970215], 'magnitude': 4.090305328369141, 'distance': 9.009303092956543, 'cosine_with_motion': 0.31249432221731166, 'motion_component': 1.278197102482256}, {'ion': 1469, 'force': [-0.39021679759025574, 0.646777868270874, -1.6788089275360107], 'magnitude': 1.8409210443496704, 'distance': 13.429241180419922, 'cosine_with_motion': 0.11183524775394986, 'motion_component': 0.20587985755624938}]}, 5227: {'frame': 5227, 'ionic_force': [-7.94691988825798, 10.216525435447693, -6.894068896770477], 'ionic_force_magnitude': 14.66489391836702, 'motion_vector': [-1.3651809692382812, -0.9860496520996094, 0.14288330078125], 'cosine_ionic_motion': -0.008475451243119256, 'ionic_motion_component': -0.12429159339063578, 'ionic_force_x': -7.94691988825798, 'ionic_force_y': 10.216525435447693, 'ionic_force_z': -6.894068896770477, 'radial_force': 12.94337389105097, 'axial_force': -6.894068896770477, 'contributions': [{'ion': 1308, 'force': [-3.113513946533203, 1.471713900566101, 0.5079912543296814], 'magnitude': 3.4810869693756104, 'distance': 9.765885353088379, 'cosine_with_motion': 0.4881399211648226, 'motion_component': 1.6992574855999774}, {'ion': 1320, 'force': [-3.006080389022827, 5.83809232711792, -2.921882152557373], 'magnitude': 7.1872968673706055, 'distance': 6.796514511108398, 'cosine_with_motion': -0.17043338293533036, 'motion_component': -1.2249553237593886}, {'ion': 1403, 'force': [-1.393346905708313, 2.2208824157714844, -2.820758104324341], 'magnitude': 3.851027250289917, 'distance': 9.284975051879883, 'cosine_with_motion': -0.10613156239445612, 'motion_component': -0.40871553483142975}, {'ion': 1469, 'force': [-0.4339786469936371, 0.6858367919921875, -1.6594198942184448], 'magnitude': 1.8472638130187988, 'distance': 13.40616512298584, 'cosine_with_motion': -0.10278906205083915, 'motion_component': -0.1898785247648629}]}, 5228: {'frame': 5228, 'ionic_force': [-9.87448799610138, 7.389701664447784, -6.990283265709877], 'ionic_force_magnitude': 14.176645019522642, 'motion_vector': [0.7691383361816406, -0.3768424987792969, -0.10305023193359375], 'cosine_ionic_motion': -0.789812787166785, 'ionic_motion_component': -11.1968955155433, 'ionic_force_x': -9.87448799610138, 'ionic_force_y': 7.389701664447784, 'ionic_force_z': -6.990283265709877, 'radial_force': 12.333418174808337, 'axial_force': -6.990283265709877, 'contributions': [{'ion': 1308, 'force': [-2.4451513290405273, 0.9452031254768372, 0.08026061952114105], 'magnitude': 2.622711658477783, 'distance': 11.251069068908691, 'cosine_with_motion': -0.9923019662020579, 'motion_component': -2.6025218019028573}, {'ion': 1320, 'force': [-5.125226974487305, 4.3977861404418945, -2.9678163528442383], 'magnitude': 7.3767476081848145, 'distance': 6.708672046661377, 'cosine_with_motion': -0.8318170866945936, 'motion_component': -6.136104879864973}, {'ion': 1403, 'force': [-1.7134193181991577, 1.530916690826416, -2.4926624298095703], 'magnitude': 3.3901147842407227, 'distance': 9.896049499511719, 'cosine_with_motion': -0.560051014426819, 'motion_component': -1.8986371754413724}, {'ion': 1469, 'force': [-0.5906903743743896, 0.5157957077026367, -1.6100651025772095], 'magnitude': 1.790885329246521, 'distance': 13.615549087524414, 'cosine_with_motion': -0.3124889054191626, 'motion_component': -0.5596317703114053}]}, 5229: {'frame': 5229, 'ionic_force': [-9.413652211427689, 7.915450572967529, -7.1453061401844025], 'ionic_force_magnitude': 14.224155706676102, 'motion_vector': [-2.0034332275390625, -4.632930755615234, 0.2904510498046875], 'cosine_ionic_motion': -0.2765377108802912, 'ionic_motion_component': -3.9335154583290404, 'ionic_force_x': -9.413652211427689, 'ionic_force_y': 7.915450572967529, 'ionic_force_z': -7.1453061401844025, 'radial_force': 12.299235981588833, 'axial_force': -7.1453061401844025, 'contributions': [{'ion': 1308, 'force': [-3.0030407905578613, 0.9390349388122559, 0.19887909293174744], 'magnitude': 3.152712106704712, 'distance': 10.261878967285156, 'cosine_with_motion': 0.10813634399926765, 'motion_component': 0.3409227587045228}, {'ion': 1320, 'force': [-4.218984603881836, 4.771722316741943, -2.8418822288513184], 'magnitude': 6.974629878997803, 'distance': 6.899354457855225, 'cosine_with_motion': -0.41062905962600516, 'motion_component': -2.8639856380834434}, {'ion': 1403, 'force': [-1.7074979543685913, 1.6937834024429321, -2.7924537658691406], 'magnitude': 3.685410261154175, 'distance': 9.49130916595459, 'cosine_with_motion': -0.28108048830992605, 'motion_component': -1.0358969432865663}, {'ion': 1469, 'force': [-0.4841288626194, 0.510909914970398, -1.709849238395691], 'magnitude': 1.8490521907806396, 'distance': 13.399681091308594, 'cosine_with_motion': -0.20256639275756702, 'motion_component': -0.37455583836772854}]}, 5230: {'frame': 5230, 'ionic_force': [-13.472239375114441, -2.136018753051758, -5.8683589696884155], 'ionic_force_magnitude': 14.849291124188225, 'motion_vector': [5.115959167480469, 0.8695487976074219, -4.300270080566406], 'cosine_ionic_motion': -0.4551001034999545, 'ionic_motion_component': -6.7579139275190165, 'ionic_force_x': -13.472239375114441, 'ionic_force_y': -2.136018753051758, 'ionic_force_z': -5.8683589696884155, 'radial_force': 13.64052088058857, 'axial_force': -5.8683589696884155, 'contributions': [{'ion': 1308, 'force': [-3.4431419372558594, -1.4593416452407837, 1.5944634675979614], 'magnitude': 4.065368175506592, 'distance': 9.03689193725586, 'cosine_with_motion': -0.9394801019205968, 'motion_component': -3.819332482993259}, {'ion': 1320, 'force': [-6.761546611785889, -0.46857988834381104, -2.9621737003326416], 'magnitude': 7.396793365478516, 'distance': 6.699575424194336, 'cosine_with_motion': -0.44655252950108015, 'motion_component': -3.3030568067030313}, {'ion': 1403, 'force': [-2.4797613620758057, -0.12971417605876923, -2.8303792476654053], 'magnitude': 3.7652475833892822, 'distance': 9.390144348144531, 'cosine_with_motion': -0.024738096463148694, 'motion_component': -0.0931450562886138}, {'ion': 1469, 'force': [-0.7877894639968872, -0.07838304340839386, -1.67026948928833], 'magnitude': 1.8483929634094238, 'distance': 13.402070045471191, 'cosine_with_motion': 0.2475774303234592, 'motion_component': 0.4576203640856893}]}, 5231: {'frame': 5231, 'ionic_force': [-4.702645644545555, -10.708216772880405, -12.202762365341187], 'ionic_force_magnitude': 16.902313210272368, 'motion_vector': [-1.9342155456542969, 1.1726150512695312, 1.3013763427734375], 'cosine_ionic_motion': -0.43849772857207303, 'ionic_motion_component': -7.411625950318177, 'ionic_force_x': -4.702645644545555, 'ionic_force_y': -10.708216772880405, 'ionic_force_z': -12.202762365341187, 'radial_force': 11.695331654688571, 'axial_force': -12.202762365341187, 'contributions': [{'ion': 1308, 'force': [-4.075906753540039, -10.616989135742188, -3.460934638977051], 'magnitude': 11.887453079223633, 'distance': 5.284752368927002, 'cosine_with_motion': -0.29238051464697856, 'motion_component': -3.475659674190411}, {'ion': 1320, 'force': [-0.42284056544303894, -0.09886391460895538, -6.389946937561035], 'magnitude': 6.404685020446777, 'distance': 7.199795246124268, 'cosine_with_motion': -0.4555500386801142, 'motion_component': -2.9176545042145263}, {'ion': 1403, 'force': [-0.2038983255624771, 0.007636277470737696, -2.3518807888031006], 'magnitude': 2.36071515083313, 'distance': 11.858977317810059, 'cosine_with_motion': -0.43135733794867037, 'motion_component': -1.0183118087160872}]}, 5232: {'frame': 5232, 'ionic_force': [-15.006769359111786, -7.3863255977630615, -12.328855037689209], 'ionic_force_magnitude': 20.778873862028732, 'motion_vector': [-2.0798912048339844, 0.45478057861328125, 1.3255767822265625], 'cosine_ionic_motion': 0.2208754185682539, 'ionic_motion_component': 4.589542461652547, 'ionic_force_x': -15.006769359111786, 'ionic_force_y': -7.3863255977630615, 'ionic_force_z': -12.328855037689209, 'radial_force': 16.726055495356526, 'axial_force': -12.328855037689209, 'contributions': [{'ion': 1308, 'force': [-10.581357955932617, -10.495577812194824, -2.068549871444702], 'magnitude': 15.04663372039795, 'distance': 4.6973114013671875, 'cosine_with_motion': 0.38405388094854503, 'motion_component': 5.778718101797736}, {'ion': 1320, 'force': [-3.4290311336517334, 2.5227065086364746, -7.157139778137207], 'magnitude': 8.327482223510742, 'distance': 6.31411075592041, 'cosine_with_motion': -0.057842646264237296, 'motion_component': -0.48168358166323344}, {'ion': 1403, 'force': [-0.9963802695274353, 0.5865457057952881, -3.1031653881073], 'magnitude': 3.3115622997283936, 'distance': 10.012731552124023, 'cosine_with_motion': -0.21364315361773834, 'motion_component': -0.7074926152914962}]}, 5233: {'frame': 5233, 'ionic_force': [-14.879006922245026, 1.6513826549053192, -8.93515632301569], 'ionic_force_magnitude': 17.434131185174234, 'motion_vector': [-1.1857566833496094, -2.693035125732422, 0.8188629150390625], 'cosine_ionic_motion': 0.11040390686238014, 'ionic_motion_component': 1.9247961955944932, 'ionic_force_x': -14.879006922245026, 'ionic_force_y': 1.6513826549053192, 'ionic_force_z': -8.93515632301569, 'radial_force': 14.970367786568824, 'axial_force': -8.93515632301569, 'contributions': [{'ion': 1308, 'force': [-8.045933723449707, -1.5553702116012573, 0.07402922958135605], 'magnitude': 8.19522476196289, 'distance': 6.364856243133545, 'cosine_with_motion': 0.5509090435760458, 'motion_component': 4.514823348282454}, {'ion': 1320, 'force': [-4.9024658203125, 2.3702609539031982, -4.955585479736328], 'magnitude': 7.362753391265869, 'distance': 6.715044975280762, 'cosine_with_motion': -0.20579584488781474, 'motion_component': -1.5152240276781868}, {'ion': 1403, 'force': [-1.4236538410186768, 0.6275284290313721, -2.5825090408325195], 'magnitude': 3.0149519443511963, 'distance': 10.493704795837402, 'cosine_with_motion': -0.22984487928672453, 'motion_component': -0.6929712621797393}, {'ion': 1469, 'force': [-0.5069535374641418, 0.20896348357200623, -1.4710910320281982], 'magnitude': 1.569960594177246, 'distance': 14.542016983032227, 'cosine_with_motion': -0.24321109813377306, 'motion_component': -0.3818318543778467}]}, 5234: {'frame': 5234, 'ionic_force': [-12.36766916513443, -6.169648960232735, -5.632678389549255], 'ionic_force_magnitude': 14.924840860485348, 'motion_vector': [-0.7371978759765625, 0.9959373474121094, -1.500885009765625], 'cosine_ionic_motion': 0.39337879102866113, 'ionic_motion_component': 5.8711158539928885, 'ionic_force_x': -12.36766916513443, 'ionic_force_y': -6.169648960232735, 'ionic_force_z': -5.632678389549255, 'radial_force': 13.82113630895513, 'axial_force': -5.632678389549255, 'contributions': [{'ion': 1308, 'force': [-4.263079643249512, -5.226989269256592, 1.3957465887069702], 'magnitude': 6.887914657592773, 'distance': 6.942647933959961, 'cosine_with_motion': -0.3101546325173943, 'motion_component': -2.1363187537023762}, {'ion': 1320, 'force': [-5.668378829956055, -0.6114987134933472, -3.2219982147216797], 'magnitude': 6.54871940612793, 'distance': 7.12017822265625, 'cosine_with_motion': 0.6594842117417947, 'motion_component': 4.318776847613336}, {'ion': 1403, 'force': [-1.7518445253372192, -0.24626709520816803, -2.2820186614990234], 'magnitude': 2.8874237537384033, 'distance': 10.72293758392334, 'cosine_with_motion': 0.7956310726232749, 'motion_component': 2.2973240529196257}, {'ion': 1469, 'force': [-0.6843661665916443, -0.08489388227462769, -1.5244081020355225], 'magnitude': 1.6731359958648682, 'distance': 14.086509704589844, 'cosine_with_motion': 0.8315723490625314, 'motion_component': 1.3913336358783646}]}, 5235: {'frame': 5235, 'ionic_force': [-9.108755230903625, -5.003531493246555, -4.880807518959045], 'ionic_force_magnitude': 11.481595328940635, 'motion_vector': [0.478057861328125, 0.5345573425292969, -0.0841217041015625], 'cosine_ionic_motion': -0.7983481136190297, 'ionic_motion_component': -9.166309972196819, 'ionic_force_x': -9.108755230903625, 'ionic_force_y': -5.003531493246555, 'ionic_force_z': -4.880807518959045, 'radial_force': 10.39253334179998, 'axial_force': -4.880807518959045, 'contributions': [{'ion': 1308, 'force': [-4.102746486663818, -5.535513401031494, -1.0437307357788086], 'magnitude': 6.968774318695068, 'distance': 6.902252674102783, 'cosine_with_motion': -0.960400735912664, 'motion_component': -6.692815687143749}, {'ion': 1320, 'force': [-3.311994791030884, 0.44610047340393066, -1.7596060037612915], 'magnitude': 3.776841163635254, 'distance': 9.375720977783203, 'cosine_with_motion': -0.4388687590021384, 'motion_component': -1.6575375503540872}, {'ion': 1403, 'force': [-1.6940139532089233, 0.08588143438100815, -2.0774707794189453], 'magnitude': 2.681966543197632, 'distance': 11.12608528137207, 'cosine_with_motion': -0.30423817852102863, 'motion_component': -0.8159565702947376}]}, 5236: {'frame': 5236, 'ionic_force': [-8.572914719581604, -3.368498131632805, -3.489031046628952], 'ionic_force_magnitude': 9.849618474660495, 'motion_vector': [-1.1881294250488281, -1.5159759521484375, -0.36592864990234375], 'cosine_ionic_motion': 0.8580266738193267, 'ionic_motion_component': 8.451235378202336, 'ionic_force_x': -8.572914719581604, 'ionic_force_y': -3.368498131632805, 'ionic_force_z': -3.489031046628952, 'radial_force': 9.210952526858046, 'axial_force': -3.489031046628952, 'contributions': [{'ion': 1308, 'force': [-4.18311882019043, -3.761627435684204, -0.9836950898170471], 'magnitude': 5.711040496826172, 'distance': 7.6245012283325195, 'cosine_with_motion': 0.9853378826804866, 'motion_component': 5.62730424929216}, {'ion': 1320, 'force': [-2.6477365493774414, 0.20306988060474396, -0.23778191208839417], 'magnitude': 2.6661369800567627, 'distance': 11.159065246582031, 'cosine_with_motion': 0.5595886122897646, 'motion_component': 1.4919398983652878}, {'ion': 1403, 'force': [-1.742059350013733, 0.19005942344665527, -2.2675540447235107], 'magnitude': 2.8657801151275635, 'distance': 10.763354301452637, 'cosine_with_motion': 0.4647919112995481, 'motion_component': 1.3319913392970584}]}, 5237: {'frame': 5237, 'ionic_force': [-6.391249179840088, -5.777417056262493, -3.9080119132995605], 'ionic_force_magnitude': 9.460400151964539, 'motion_vector': [0.7070693969726562, -0.0630950927734375, -0.1740264</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{5293: {'frame': 5293, 'ionic_force': [-4.439165145158768, -11.485485851764679, -5.509422957897186], 'ionic_force_magnitude': 13.489859664432528, 'motion_vector': [3.6029815673828125, -0.9414405822753906, -2.305633544921875], 'cosine_ionic_motion': 0.12729862041329584, 'ionic_motion_component': 1.7172405248512268, 'ionic_force_x': -4.439165145158768, 'ionic_force_y': -11.485485851764679, 'ionic_force_z': -5.509422957897186, 'radial_force': 12.31351178328421, 'axial_force': -5.509422957897186, 'contributions': [{'ion': 1309, 'force': [-0.4600997269153595, -6.4237165451049805, -1.8560487031936646], 'magnitude': 6.702293872833252, 'distance': 7.038130283355713, 'directional_contribution': 1.9793003634343176}, {'ion': 1320, 'force': [-2.2913060188293457, -4.553028583526611, 0.9146720767021179], 'magnitude': 5.178492069244385, 'distance': 8.00695514678955, 'directional_contribution': -1.387701281697467}, {'ion': 1469, 'force': [-1.280375599861145, -0.43071743845939636, -2.963862419128418], 'magnitude': 3.2572009563446045, 'distance': 10.095939636230469, 'directional_contribution': 0.5995323182463634}, {'ion': 2436, 'force': [-0.4073837995529175, -0.0780232846736908, -1.6041839122772217], 'magnitude': 1.656941533088684, 'distance': 14.155181884765625, 'directional_contribution': 0.5261092018864266}]}, 5294: {'frame': 5294, 'ionic_force': [0.1658477745950222, -6.8131378293037415, -5.872682213783264], 'ionic_force_magnitude': 8.99637421128724, 'motion_vector': [-1.1986160278320312, 0.10608673095703125, 0.8895950317382812], 'cosine_ionic_motion': -0.4565192458823854, 'ionic_motion_component': -4.10701797061259, 'ionic_force_x': 0.1658477745950222, 'ionic_force_y': -6.8131378293037415, 'ionic_force_z': -5.872682213783264, 'radial_force': 6.815156092521126, 'axial_force': -5.872682213783264, 'contributions': [{'ion': 1309, 'force': [1.4283074140548706, -3.2946081161499023, -1.909952163696289], 'magnitude': 4.067237377166748, 'distance': 9.034814834594727, 'directional_contribution': -2.5130349266499294}, {'ion': 1320, 'force': [-1.2332184314727783, -2.8408944606781006, -1.2032557725906372], 'magnitude': 3.3225491046905518, 'distance': 9.996163368225098, 'directional_contribution': 0.0710782469366329}, {'ion': 1469, 'force': [-0.029241207987070084, -0.6776352524757385, -2.759474277496338], 'magnitude': 2.841609239578247, 'distance': 10.809033393859863, 'directional_contribution': -1.6650611084765343}]}, 5295: {'frame': 5295, 'ionic_force': [-0.8948521912097931, -8.003737807273865, -7.197145462036133], 'ionic_force_magnitude': 10.800901912961034, 'motion_vector': [1.4610366821289062, 0.4837226867675781, -0.33788299560546875], 'cosine_ionic_motion': -0.16142186763286107, 'ionic_motion_component': -1.7435017589095119, 'ionic_force_x': -0.8948521912097931, 'ionic_force_y': -8.003737807273865, 'ionic_force_z': -7.197145462036133, 'radial_force': 8.053606603981724, 'axial_force': -7.197145462036133, 'contributions': [{'ion': 1309, 'force': [1.2909294366836548, -4.2322163581848145, -2.066220760345459], 'magnitude': 4.883382320404053, 'distance': 8.245342254638672, 'directional_contribution': 0.340815084300246}, {'ion': 1320, 'force': [-1.8195945024490356, -3.148383855819702, -1.8783209323883057], 'magnitude': 4.09283971786499, 'distance': 9.006513595581055, 'directional_contribution': -2.2509498785102373}, {'ion': 1469, 'force': [-0.36618712544441223, -0.6231375932693481, -3.252603769302368], 'magnitude': 3.331940174102783, 'distance': 9.98206615447998, 'directional_contribution': 0.16663289920801638}]}, 5296: {'frame': 5296, 'ionic_force': [0.31867482099914923, -8.267817586660385, -7.231484055519104], 'ionic_force_magnitude': 10.988754384963595, 'motion_vector': [-0.4652824401855469, 0.103912353515625, -2.422882080078125], 'cosine_ionic_motion': 0.6085736128030453, 'ionic_motion_component': 6.687465956262602, 'ionic_force_x': 0.31867482099914923, 'ionic_force_y': -8.267817586660385, 'ionic_force_z': -7.231484055519104, 'radial_force': 8.273956809642506, 'axial_force': -7.231484055519104, 'contributions': [{'ion': 1309, 'force': [2.060899019241333, -4.070521354675293, -2.4136157035827637], 'magnitude': 5.161587715148926, 'distance': 8.020055770874023, 'directional_contribution': 1.808591562717023}, {'ion': 1320, 'force': [-1.741642713546753, -3.7549068927764893, -1.5699185132980347], 'magnitude': 4.426882743835449, 'distance': 8.660042762756348, 'directional_contribution': 1.7105384314382377}, {'ion': 1469, 'force': [-0.000581484695430845, -0.4423893392086029, -3.2479498386383057], 'magnitude': 3.2779393196105957, 'distance': 10.063952445983887, 'directional_contribution': 3.1683358083492243}]}, 5297: {'frame': 5297, 'ionic_force': [2.0586469620466232, -4.025961697101593, -6.761675596237183], 'ionic_force_magnitude': 8.134288645580657, 'motion_vector': [0.11940383911132812, -0.8824501037597656, 1.4705276489257812], 'cosine_ionic_motion': -0.439411799823159, 'ionic_motion_component': -3.5743024140356825, 'ionic_force_x': 2.0586469620466232, 'ionic_force_y': -4.025961697101593, 'ionic_force_z': -6.761675596237183, 'radial_force': 4.521769001272945, 'axial_force': -6.761675596237183, 'contributions': [{'ion': 1309, 'force': [2.703697919845581, -1.9296005964279175, -3.2435293197631836], 'magnitude': 4.642609596252441, 'distance': 8.45644760131836, 'directional_contribution': -1.5962042757614867}, {'ion': 1320, 'force': [-0.5463349223136902, -1.8209863901138306, -1.1804895401000977], 'magnitude': 2.2378625869750977, 'distance': 12.18014144897461, 'directional_contribution': -0.1129913241681777}, {'ion': 1469, 'force': [-0.09871603548526764, -0.27537471055984497, -2.3376567363739014], 'magnitude': 2.3558895587921143, 'distance': 11.871116638183594, 'directional_contribution': -1.8651069085584862}]}, 5298: {'frame': 5298, 'ionic_force': [2.64043165743351, -8.706450581550598, -7.226660072803497], 'ionic_force_magnitude': 11.618897403558226, 'motion_vector': [-0.8501853942871094, 0.7801551818847656, 2.5111923217773438], 'cosine_ionic_motion': -0.8466110490409935, 'ionic_motion_component': -9.836686919526105, 'ionic_force_x': 2.64043165743351, 'ionic_force_y': -8.706450581550598, 'ionic_force_z': -7.226660072803497, 'radial_force': 9.098030614729751, 'axial_force': -7.226660072803497, 'contributions': [{'ion': 1309, 'force': [3.2287416458129883, -6.1072096824646, -3.8306076526641846], 'magnitude': 7.899135589599609, 'distance': 6.483048439025879, 'directional_contribution': -6.19804851018975}, {'ion': 1320, 'force': [-0.4978197515010834, -2.0856738090515137, -0.9577496647834778], 'magnitude': 2.3484344482421875, 'distance': 11.889945030212402, 'directional_contribution': -1.3059016451634013}, {'ion': 1469, 'force': [-0.09049023687839508, -0.5135670900344849, -2.438302755355835], 'magnitude': 2.493443489074707, 'distance': 11.539029121398926, 'directional_contribution': -2.3327365935457256}]}, 5299: {'frame': 5299, 'ionic_force': [8.148396573960781, -5.8599869310855865, -10.365723192691803], 'ionic_force_magnitude': 14.428583813615887, 'motion_vector': [-0.3539390563964844, 2.2585983276367188, 2.1390380859375], 'cosine_ionic_motion': -0.84767086277239, 'ionic_motion_component': -12.230690089871521, 'ionic_force_x': 8.148396573960781, 'ionic_force_y': -5.8599869310855865, 'ionic_force_z': -10.365723192691803, 'radial_force': 10.036723248103918, 'axial_force': -10.365723192691803, 'contributions': [{'ion': 1309, 'force': [9.771367073059082, -2.351778030395508, -4.5568013191223145], 'magnitude': 11.03516674041748, 'distance': 5.485037326812744, 'directional_contribution': -5.914543591356164}, {'ion': 1320, 'force': [-1.1783761978149414, -2.824215888977051, -0.5681673884391785], 'magnitude': 3.11248779296875, 'distance': 10.32797622680664, 'directional_contribution': -2.2923807326295993}, {'ion': 1469, 'force': [-0.3746396005153656, -0.5283625721931458, -3.711301326751709], 'magnitude': 3.767396926879883, 'distance': 9.387465476989746, 'directional_contribution': -2.8744477578251457}, {'ion': 2436, 'force': [-0.06995470076799393, -0.1556304395198822, -1.529453158378601], 'magnitude': 1.5389416217803955, 'distance': 14.687841415405273, 'directional_contribution': -1.1493178342881796}]}, 5300: {'frame': 5300, 'ionic_force': [11.58044770359993, 2.511912077665329, -5.298129674047232], 'ionic_force_magnitude': 12.98024072753482, 'motion_vector': [2.946308135986328, -2.5934295654296875, 0.6218948364257812], 'cosine_ionic_motion': 0.47126898983142484, 'ionic_motion_component': 6.117184935434054, 'ionic_force_x': 11.58044770359993, 'ionic_force_y': 2.511912077665329, 'ionic_force_z': -5.298129674047232, 'radial_force': 11.849745621815426, 'axial_force': -5.298129674047232, 'contributions': [{'ion': 1309, 'force': [15.33890438079834, 5.875173568725586, 3.291243076324463], 'magnitude': 16.752071380615234, 'distance': 4.451791286468506, 'directional_contribution': 8.052945245231506}, {'ion': 1320, 'force': [-2.06095027923584, -3.7897627353668213, -0.05836188420653343], 'magnitude': 4.314304351806641, 'distance': 8.772303581237793, 'directional_contribution': 0.9360623548549916}, {'ion': 1469, 'force': [-1.4913935661315918, 0.3887030780315399, -6.317618370056152], 'magnitude': 6.502894878387451, 'distance': 7.145220756530762, 'directional_contribution': -2.347979613803373}, {'ion': 2436, 'force': [-0.2061128318309784, 0.037798166275024414, -2.213392496109009], 'magnitude': 2.223289728164673, 'distance': 12.21999454498291, 'directional_contribution': -0.5238427378697725}]}, 5301: {'frame': 5301, 'ionic_force': [11.182874098420143, -8.029923260211945, -7.2750024273991585], 'ionic_force_magnitude': 15.571191379745887, 'motion_vector': [-1.3564949035644531, -1.4149208068847656, -1.5110244750976562], 'cosine_ionic_motion': 0.18643873805724717, 'ionic_motion_component': 2.9030732708877087, 'ionic_force_x': 11.182874098420143, 'ionic_force_y': -8.029923260211945, 'ionic_force_z': -7.2750024273991585, 'radial_force': 13.767219787088784, 'axial_force': -7.2750024273991585, 'contributions': [{'ion': 1309, 'force': [8.657218933105469, -1.525900959968567, 3.219957113265991], 'magnitude': 9.361833572387695, 'distance': 5.9550933837890625, 'directional_contribution': -5.838501907603842}, {'ion': 1320, 'force': [-0.21056003868579865, -2.90226411819458, -0.06113452464342117], 'magnitude': 2.910534143447876, 'distance': 10.680280685424805, 'directional_contribution': 1.8119602242220658}, {'ion': 1469, 'force': [2.363967180252075, -3.182705879211426, -7.91904354095459], 'magnitude': 8.856026649475098, 'distance': 6.122793197631836, 'directional_contribution': 5.35871319760362}, {'ion': 2436, 'force': [0.3722480237483978, -0.4190523028373718, -2.5147814750671387], 'magnitude': 2.5764896869659424, 'distance': 11.351541519165039, 'directional_contribution': 1.570901341876704}]}, 5302: {'frame': 5302, 'ionic_force': [9.384686825796962, -10.808709025382996, -6.232582181692123], 'ionic_force_magnitude': 15.612354667545477, 'motion_vector': [-1.703094482421875, 1.6502799987792969, -1.0469818115234375], 'cosine_ionic_motion': -0.6744132230711771, 'ionic_motion_component': -10.529178431069681, 'ionic_force_x': 9.384686825796962, 'ionic_force_y': -10.808709025382996, 'ionic_force_z': -6.232582181692123, 'radial_force': 14.314347264674101, 'axial_force': -6.232582181692123, 'contributions': [{'ion': 1309, 'force': [9.655634880065918, -6.011810302734375, 0.029120855033397675], 'magnitude': 11.374268531799316, 'distance': 5.402655601501465, 'directional_contribution': -10.182428538158979}, {'ion': 1320, 'force': [-0.391956627368927, -2.144749641418457, -0.11846282333135605], 'magnitude': 2.1834867000579834, 'distance': 12.33087158203125, 'directional_contribution': -1.0600039710206126}, {'ion': 1469, 'force': [0.1119040995836258, -2.1314122676849365, -4.249485492706299], 'magnitude': 4.755372524261475, 'distance': 8.355583190917969, 'directional_contribution': 0.2858920014635995}, {'ion': 2436, 'force': [0.009104473516345024, -0.520736813545227, -1.8937547206878662], 'magnitude': 1.9640663862228394, 'distance': 13.001425743103027, 'directional_contribution': 0.42736206507377106}]}, 5303: {'frame': 5303, 'ionic_force': [4.634013906121254, -7.393165856599808, -18.30676108598709], 'ionic_force_magnitude': 20.279804923241485, 'motion_vector': [2.9986648559570312, -0.3383674621582031, -0.0259552001953125], 'cosine_ionic_motion': 0.2756939581042625, 'ionic_motion_component': 5.591019688870754, 'ionic_force_x': 4.634013906121254, 'ionic_force_y': -7.393165856599808, 'ionic_force_z': -18.30676108598709, 'radial_force': 8.725421838817784, 'axial_force': -18.30676108598709, 'contributions': [{'ion': 1309, 'force': [6.351526737213135, -4.161134243011475, -12.593794822692871], 'magnitude': 14.705801963806152, 'distance': 4.751433849334717, 'directional_contribution': 6.886115674686596}, {'ion': 1320, 'force': [-0.7893285751342773, -2.2547266483306885, -0.49746209383010864], 'magnitude': 2.440143585205078, 'distance': 11.664371490478516, 'directional_contribution': -0.5272352060481691}, {'ion': 1469, 'force': [-0.7389268279075623, -0.7736309766769409, -3.6220219135284424], 'magnitude': 3.7767128944396973, 'distance': 9.375880241394043, 'directional_contribution': -0.6163456335657835}, {'ion': 2436, 'force': [-0.1892574280500412, -0.20367398858070374, -1.593482255935669], 'magnitude': 1.6175559759140015, 'distance': 14.326476097106934, 'directional_contribution': -0.15151526404247218}]}, 5304: {'frame': 5304, 'ionic_force': [11.509692594408989, -10.579159915447235, -10.748389482498169], 'ionic_force_magnitude': 18.971545129532174, 'motion_vector': [-1.4822731018066406, 2.659027099609375, -2.7203369140625], 'cosine_ionic_motion': -0.20594956949000837, 'ionic_motion_component': -3.9071815519874162, 'ionic_force_x': 11.509692594408989, 'ionic_force_y': -10.579159915447235, 'ionic_force_z': -10.748389482498169, 'radial_force': 15.633030676564243, 'axial_force': -10.748389482498169, 'contributions': [{'ion': 1309, 'force': [10.475059509277344, -6.060859680175781, -4.418924331665039], 'magnitude': 12.883625030517578, 'distance': 5.076332092285156, 'directional_contribution': -4.806208557360378}, {'ion': 1320, 'force': [-0.10482928156852722, -3.094301462173462, -0.409082293510437], 'magnitude': 3.122985601425171, 'distance': 10.310602188110352, 'directional_contribution': -1.7046904380766525}, {'ion': 1469, 'force': [0.9543324708938599, -1.1745716333389282, -4.332919597625732], 'magnitude': 4.589614391326904, 'distance': 8.50512981414795, 'directional_contribution': 1.7756247490290527}, {'ion': 2436, 'force': [0.18512989580631256, -0.24942713975906372, -1.5874632596969604], 'magnitude': 1.6175681352615356, 'distance': 14.326422691345215, 'directional_contribution': 0.8280927206379407}]}, 5305: {'frame': 5305, 'ionic_force': [-7.564083315432072, 10.154234908521175, -16.6937335729599], 'ionic_force_magnitude': 20.952436220764316, 'motion_vector': [3.7210350036621094, 0.5313720703125, 4.7978057861328125], 'cosine_ionic_motion': -0.80534045139699, 'ionic_motion_component': -16.873844443896978, 'ionic_force_x': -7.564083315432072, 'ionic_force_y': 10.154234908521175, 'ionic_force_z': -16.6937335729599, 'radial_force': 12.66190518761801, 'axial_force': -16.6937335729599, 'contributions': [{'ion': 1309, 'force': [-6.675297737121582, 13.578149795532227, -11.790082931518555], 'magnitude': 19.181549072265625, 'distance': 4.160324573516846, 'directional_contribution': -12.17262015225235}, {'ion': 1320, 'force': [-0.9775453209877014, -3.548858880996704, -1.993395209312439], 'magnitude': 4.186121940612793, 'distance': 8.905597686767578, 'directional_contribution': -2.4753893727261147}, {'ion': 1469, 'force': [0.08875974267721176, 0.12494399398565292, -2.9102554321289062], 'magnitude': 2.91428804397583, 'distance': 10.673399925231934, 'directional_contribution': -2.2258355180118463}]}, 5306: {'frame': 5306, 'ionic_force': [17.47581458091736, -4.5736775398254395, -4.979289084672928], 'ionic_force_magnitude': 18.738087983933962, 'motion_vector': [-1.9650535583496094, -1.8321075439453125, -0.7120208740234375], 'cosine_ionic_motion': -0.4304121236027933, 'ionic_motion_component': -8.065100241421, 'ionic_force_x': 17.47581458091736, 'ionic_force_y': -4.5736775398254395, 'ionic_force_z': -4.979289084672928, 'radial_force': 18.064402052238194, 'axial_force': -4.979289084672928, 'contributions': [{'ion': 1309, 'force': [4.468284606933594, 4.662998676300049, 3.70725679397583], 'magnitude': 7.44666862487793, 'distance': 6.677102088928223, 'directional_contribution': -7.182567102252463}, {'ion': 1320, 'force': [7.873488903045654, -10.533976554870605, 0.34959670901298523], 'magnitude': 13.155938148498535, 'distance': 5.023519992828369, 'directional_contribution': 1.2875583823797827}, {'ion': 1469, 'force': [4.469884872436523, 1.055068850517273, -6.895050525665283], 'magnitude': 8.2846097946167, 'distance': 6.330427169799805, 'directional_contribution': -2.0893564481400375}, {'ion': 2436, 'force': [0.6641561985015869, 0.24223148822784424, -2.14109206199646], 'magnitude': 2.2547848224639893, 'distance': 12.13434886932373, 'directional_contribution': -0.08073505180798435}]}, 5307: {'frame': 5307, 'ionic_force': [6.0052439123392105, 2.971535697579384, -1.2920927703380585], 'ionic_force_magnitude': 6.823670755233991, 'motion_vector': [-1.8429718017578125, 0.5340690612792969, 3.6442413330078125], 'cosine_ionic_motion': -0.5048908635908108, 'ionic_motion_component': -3.44520902046945, 'ionic_force_x': 6.0052439123392105, 'ionic_force_y': 2.971535697579384, 'ionic_force_z': -1.2920927703380585, 'radial_force': 6.700222298452175, 'axial_force': -1.2920927703380585, 'contributions': [{'ion': 1309, 'force': [5.069587707519531, 8.484151840209961, 7.271227836608887], 'magnitude': 12.269975662231445, 'distance': 5.201722621917725, 'directional_contribution': 5.265504527085966}, {'ion': 1320, 'force': [-0.18250830471515656, -4.807651519775391, -0.49011465907096863], 'magnitude': 4.836014270782471, 'distance': 8.285624504089355, 'directional_contribution': -0.975435141621853}, {'ion': 1469, 'force': [0.850151538848877, -0.5294232368469238, -5.994930744171143], 'magnitude': 6.078012943267822, 'distance': 7.390745162963867, 'directional_contribution': -5.753640939993872}, {'ion': 2436, 'force': [0.26801297068595886, -0.17554138600826263, -2.078275203704834], 'magnitude': 2.102825164794922, 'distance': 12.565143585205078, 'directional_contribution': -1.9816373740599276}]}, 5308: {'frame': 5308, 'ionic_force': [-3.9245860427618027, -5.353306509554386, -11.027286529541016], 'ionic_force_magnitude': 12.870948465318119, 'motion_vector': [-0.12729644775390625, 0.5117263793945312, -0.26439666748046875], 'cosine_ionic_motion': 0.08900058775676298, 'ionic_motion_component': 1.145521978400319, 'ionic_force_x': -3.9245860427618027, 'ionic_force_y': -5.353306509554386, 'ionic_force_z': -11.027286529541016, 'radial_force': 6.637790761411368, 'axial_force': -11.027286529541016, 'contributions': [{'ion': 1309, 'force': [0.1623639464378357, 0.4300653338432312, 3.4034218788146973], 'magnitude': 3.434326410293579, 'distance': 9.832144737243652, 'directional_contribution': -1.1874117610608668}, {'ion': 1320, 'force': [-3.1859545707702637, -5.096459865570068, 2.4922938346862793], 'magnitude': 6.506591796875, 'distance': 7.143190860748291, 'directional_contribution': -4.850686286735993}, {'ion': 1469, 'force': [-1.04063880443573, -0.7825348973274231, -12.82127857208252], 'magnitude': 12.887221336364746, 'distance': 5.075623512268066, 'directional_contribution': 5.292364458409139}, {'ion': 2436, 'force': [0.13964338600635529, 0.09562291949987411, -4.101723670959473], 'magnitude': 4.1052141189575195, 'distance': 8.992928504943848, 'directional_contribution': 1.891255809716336}]}, 5309: {'frame': 5309, 'ionic_force': [-6.100982252508402, -3.1015712544322014, -15.906369686126709], 'ionic_force_magnitude': 17.31630229822387, 'motion_vector': [0.6568450927734375, -0.14005661010742188, -0.313629150390625], 'cosine_ionic_motion': 0.11029630434347097, 'ionic_motion_component': 1.909924148388446, 'ionic_force_x': -6.100982252508402, 'ionic_force_y': -3.1015712544322014, 'ionic_force_z': -15.906369686126709, 'radial_force': 6.844101744695401, 'axial_force': -15.906369686126709, 'contributions': [{'ion': 1309, 'force': [0.20207388699054718, 0.08543962985277176, 2.6796698570251465], 'magnitude': 2.688636302947998, 'distance': 11.112276077270508, 'directional_contribution': -0.970894309377176}, {'ion': 1320, 'force': [-3.724456787109375, -3.0685253143310547, 2.46171236038208], 'magnitude': 5.417328834533691, 'distance': 7.828461647033691, 'directional_contribution': -3.7622355398655856}, {'ion': 1469, 'force': [-2.5375022888183594, -0.4666903018951416, -17.041349411010742], 'magnitude': 17.235553741455078, 'distance': 4.388907432556152, 'directional_contribution': 5.050081723024142}, {'ion': 2436, 'force': [-0.041097063571214676, 0.34820473194122314, -4.006402492523193], 'magnitude': 4.0217156410217285, 'distance': 9.085803985595703, 'directional_contribution': 1.59297246126204}]}, 5310: {'frame': 5310, 'ionic_force': [-2.138845317065716, -6.399635553359985, -14.446752071380615], 'ionic_force_magnitude': 15.944862492919254, 'motion_vector': [-0.4894981384277344, 0.20468902587890625, 0.37158966064453125], 'cosine_ionic_motion': -0.5452217807443366, 'ionic_motion_component': -8.693486322113017, 'ionic_force_x': -2.138845317065716, 'ionic_force_y': -6.399635553359985, 'ionic_force_z': -14.446752071380615, 'radial_force': 6.747591756038824, 'axial_force': -14.446752071380615, 'contributions': [{'ion': 1309, 'force': [-0.425532728433609, 0.4280744194984436, 4.451706409454346], 'magnitude': 4.4924397468566895, 'distance': 8.596623420715332, 'directional_contribution': 3.0106006276943322}, {'ion': 1320, 'force': [-2.6733267307281494, -4.865641117095947, 5.675074100494385], 'magnitude': 7.938992977142334, 'distance': 6.466753959655762, 'directional_contribution': 3.7382171379287144}, {'ion': 1469, 'force': [0.8352939486503601, -1.7298543453216553, -20.9677677154541], 'magnitude': 21.055578231811523, 'distance': 3.970867872238159, 'directional_contribution': -13.206196705608171}, {'ion': 2436, 'force': [0.12472019344568253, -0.23221451044082642, -3.605764865875244], 'magnitude': 3.615386486053467, 'distance': 9.582783699035645, 'directional_contribution': -2.2361076710314904}]}, 5311: {'frame': 5311, 'ionic_force': [-1.5457566678524017, -3.735124170780182, -10.29975938796997], 'ionic_force_magnitude': 11.064608429466993, 'motion_vector': [0.5821189880371094, -0.71893310546875, 0.33875274658203125], 'cosine_ionic_motion': -0.15629080861675848, 'ionic_motion_component': -1.7292965984691986, 'ionic_force_x': -1.5457566678524017, 'ionic_force_y': -3.735124170780182, 'ionic_force_z': -10.29975938796997, 'radial_force': 4.042340441793158, 'axial_force': -10.29975938796997, 'contributions': [{'ion': 1309, 'force': [0.2618166506290436, 0.38895392417907715, 3.28230881690979], 'magnitude': 3.315627336502075, 'distance': 10.006591796875, 'directional_contribution': 0.9995308598941133}, {'ion': 1320, 'force': [-0.6014491319656372, -3.967463493347168, 2.3787336349487305], 'magnitude': 4.66485595703125, 'distance': 8.436259269714355, 'directional_contribution': 3.3579619209873}, {'ion': 1469, 'force': [-1.1576669216156006, -0.06768996268510818, -12.637163162231445], 'magnitude': 12.690258979797363, 'distance': 5.114860534667969, 'directional_contribution': -4.980164781043792}, {'ion': 2436, 'force': [-0.04845726490020752, -0.08892463892698288, -3.323638677597046], 'magnitude': 3.325181007385254, 'distance': 9.992206573486328, 'directional_contribution': -1.1066244041700855}]}, 5312: {'frame': 5312, 'ionic_force': [-0.6932454779744148, -6.2057766020298, -20.55894696712494], 'ionic_force_magnitude': 21.486334096911186, 'motion_vector': [-0.3184471130371094, 0.7150497436523438, -0.7793121337890625], 'cosine_ionic_motion': 0.49742079003617534, 'ionic_motion_component': 10.687749281466774, 'ionic_force_x': -0.6932454779744148, 'ionic_force_y': -6.2057766020298, 'ionic_force_z': -20.55894696712494, 'radial_force': 6.244377673318016, 'axial_force': -20.55894696712494, 'contributions': [{'ion': 1309, 'force': [0.08076175302267075, 0.06683516502380371, 2.8113584518432617], 'magnitude': 2.81331205368042, 'distance': 10.86325740814209, 'directional_contribution': -1.9635620526184647}, {'ion': 1320, 'force': [-0.7783627510070801, -3.133505344390869, 1.1805278062820435], 'magnitude': 3.4377827644348145, 'distance': 9.827200889587402, 'directional_contribution': -2.6370403123848902}, {'ion': 1469, 'force': [-0.06458400189876556, -2.735037326812744, -20.452817916870117], 'magnitude': 20.634979248046875, 'distance': 4.011132717132568, 'directional_contribution': 12.678466790651052}, {'ion': 2436, 'force': [0.06893952190876007, -0.40406909584999084, -4.098015308380127], 'magnitude': 4.118464946746826, 'distance': 8.978449821472168, 'directional_contribution': 2.6098849380748117}]}, 5313: {'frame': 5313, 'ionic_force': [-6.034946657717228, -5.350842729210854, -16.52107262611389], 'ionic_force_magnitude': 18.384720280482124, 'motion_vector': [-0.3755340576171875, -0.5339927673339844, 0.46227264404296875], 'cosine_ionic_motion': -0.17092017347635274, 'ionic_motion_component': -3.142319579654225, 'ionic_force_x': -6.034946657717228, 'ionic_force_y': -5.350842729210854, 'ionic_force_z': -16.52107262611389, 'radial_force': 8.065488148540112, 'axial_force': -16.52107262611389, 'contributions': [{'ion': 1309, 'force': [-0.11181335151195526, -3.108283758163452, 3.290030002593994], 'magnitude': 4.527496814727783, 'distance': 8.563276290893555, 'directional_contribution': 4.028760797518868}, {'ion': 1320, 'force': [-4.065372467041016, -4.175497531890869, 2.469059705734253], 'magnitude': 6.329161643981934, 'distance': 7.242623805999756, 'directional_contribution': 6.1228087225875925}, {'ion': 1469, 'force': [-1.8919004201889038, 1.7885223627090454, -18.668319702148438], 'magnitude': 18.84898567199707, 'distance': 4.196865558624268, 'directional_contribution': -11.094174008723336}, {'ion': 2436, 'force': [0.03413958102464676, 0.1444161981344223, -3.611842632293701], 'magnitude': 3.6148898601531982, 'distance': 9.583441734313965, 'directional_contribution': -2.1997155227084764}]}, 5314: {'frame': 5314, 'ionic_force': [-5.211430847644806, -8.442669451236725, -17.771475553512573], 'ionic_force_magnitude': 20.35345234331819, 'motion_vector': [-0.15516281127929688, 0.3010063171386719, -0.0225677490234375], 'cosine_ionic_motion': -0.19276747009609363, 'ionic_motion_component': -3.9234835159428556, 'ionic_force_x': -5.211430847644806, 'ionic_force_y': -8.442669451236725, 'ionic_force_z': -17.771475553512573, 'radial_force': 9.921576434349014, 'axial_force': -17.771475553512573, 'contributions': [{'ion': 1309, 'force': [-0.48251619935035706, -3.664240598678589, 1.9041845798492432], 'magnitude': 4.157571315765381, 'distance': 8.936123847961426, 'directional_contribution': -3.155795436619493}, {'ion': 1320, 'force': [-3.720808982849121, -2.3928604125976562, 4.966029167175293], 'magnitude': 6.6506876945495605, 'distance': 7.0653839111328125, 'directional_contribution': -0.7513555677998909}, {'ion': 1469, 'force': [-1.2004474401474, -2.1353933811187744, -20.877975463867188], 'magnitude': 21.02120018005371, 'distance': 3.974113702774048, 'directional_contribution': 0.043214457157265684}, {'ion': 2436, 'force': [0.19234177470207214, -0.2501750588417053, -3.763713836669922], 'magnitude': 3.7769198417663574, 'distance': 9.37562370300293, 'directional_contribution': -0.059547009893312186}]}, 5315: {'frame': 5315, 'ionic_force': [-4.354976288974285, -2.9413586780428886, -13.101229906082153], 'ionic_force_magnitude': 14.115935477411613, 'motion_vector': [0.5261955261230469, -0.461700439453125, -0.2435302734375], 'cosine_ionic_motion': 0.21572260525693082, 'ionic_motion_component': 3.0451263768259706, 'ionic_force_x': -4.354976288974285, 'ionic_force_y': -2.9413586780428886, 'ionic_force_z': -13.101229906082153, 'radial_force': 5.2552268600343455, 'axial_force': -13.101229906082153, 'contributions': [{'ion': 1309, 'force': [-1.3679094314575195, -3.2166194915771484, 1.7919011116027832], 'magnitude': 3.9279417991638184, 'distance': 9.193619728088379, 'directional_contribution': 0.44380874123271497}, {'ion': 1320, 'force': [-0.15094943344593048, 0.24601347744464874, 6.12855863571167], 'magnitude': 6.135351657867432, 'distance': 7.356128692626953, 'directional_contribution': -2.2740635689315685}, {'ion': 1469, 'force': [-2.7265963554382324, 0.12713120877742767, -17.374311447143555], 'magnitude': 17.58741569519043, 'distance': 4.34478235244751, 'directional_contribution': 3.6937466750015853}, {'ion': 2436, 'force': [-0.10952106863260269, -0.09788387268781662, -3.6473782062530518], 'magnitude': 3.6503348350524902, 'distance': 9.536800384521484, 'directional_contribution': 1.1816347130642422}]}, 5316: {'frame': 5316, 'ionic_force': [1.7553037405014038, -11.83569049090147, -15.618502497673035], 'ionic_force_magnitude': 19.6749150160211, 'motion_vector': [-0.0081329345703125, -0.06674957275390625, -0.1145172119140625], 'cosine_ionic_motion': 0.9814416458058247, 'ionic_motion_component': 19.30978097441348, 'ionic_force_x': 1.7553037405014038, 'ionic_force_y': -11.83569049090147, 'ionic_force_z': -15.618502497673035, 'radial_force': 11.965143568626067, 'axial_force': -15.618502497673035, 'contributions': [{'ion': 1309, 'force': [-1.1511693000793457, -4.0106306076049805, 0.9726828336715698], 'magnitude': 4.2844438552856445, 'distance': 8.80281925201416, 'directional_contribution': 1.2476004088355062}, {'ion': 1320, 'force': [5.6856689453125, -1.988126516342163, 10.163335800170898], 'magnitude': 11.814096450805664, 'distance': 5.30113410949707, 'directional_contribution': -8.113038165455393}, {'ion': 1469, 'force': [-2.813703775405884, -5.7387566566467285, -22.967845916748047], 'magnitude': 23.840559005737305, 'distance': 3.7317354679107666, 'directional_contribution': 22.86262740742002}, {'ion': 2436, 'force': [0.0345078706741333, -0.09817671030759811, -3.786675214767456], 'magnitude': 3.788105010986328, 'distance': 9.361771583557129, 'directional_contribution': 3.3125910751450642}]}, 5317: {'frame': 5317, 'ionic_force': [0.3822760283946991, -7.415548861026764, -9.089471697807312], 'ionic_force_magnitude': 11.736907412832425, 'motion_vector': [0.2352142333984375, 0.3178596496582031, 0.7380828857421875], 'cosine_ionic_motion': -0.913333580340876, 'ionic_motion_component': -10.719711669491605, 'ionic_force_x': 0.3822760283946991, 'ionic_force_y': -7.415548861026764, 'ionic_force_z': -9.089471697807312, 'radial_force': 7.425395603748029, 'axial_force': -9.089471697807312, 'contributions': [{'ion': 1309, 'force': [-1.128919005393982, -3.293989896774292, 1.7603298425674438], 'magnitude': 3.9017417430877686, 'distance': 9.224434852600098, 'directional_contribution': -0.01587781602301419}, {'ion': 1320, 'force': [0.5020703673362732, -1.9142985343933105, 6.496671676635742], 'magnitude': 6.791417598724365, 'distance': 6.991796970367432, 'directional_contribution': 5.140961670027668}, {'ion': 1469, 'force': [0.5732925534248352, -1.7882095575332642, -13.811469078063965], 'magnitude': 13.938545227050781, 'distance': 4.880455017089844, 'directional_contribution': -12.692153885959268}, {'ion': 2436, 'force': [0.43583211302757263, -0.4190508723258972, -3.535004138946533], 'magnitude': 3.586336135864258, 'distance': 9.621517181396484, 'directional_contribution': -3.1526415604566598}]}, 5318: {'frame': 5318, 'ionic_force': [1.0821340382099152, -5.015195339918137, -10.96111798286438], 'ionic_force_magnitude': 12.102450405123005, 'motion_vector': [-0.9112663269042969, -3.5516128540039062, -7.006256103515625], 'cosine_ionic_motion': 0.9782615430679917, 'ionic_motion_component': 11.839361808219472, 'ionic_force_x': 1.0821340382099152, 'ionic_force_y': -5.015195339918137, 'ionic_force_z': -10.96111798286438, 'radial_force': 5.130613839901526, 'axial_force': -10.96111798286438, 'contributions': [{'ion': 1309, 'force': [-0.9033969044685364, -3.438693046569824, 1.1628429889678955], 'magnitude': 3.7407138347625732, 'distance': 9.420886993408203, 'directional_contribution': 0.6182525025727679}, {'ion': 1320, 'force': [0.8172289729118347, 0.9615076184272766, 7.869882106781006], 'magnitude': 7.970407962799072, 'distance': 6.4539971351623535, 'directional_contribution': -7.498754460052293}, {'ion': 1469, 'force': [0.9927124381065369, -2.2097842693328857, -16.332483291625977], 'magnitude': 16.511167526245117, 'distance': 4.484150409698486, 'directional_contribution': 15.348707947360236}, {'ion': 2436, 'force': [0.175</t>
+          <t>{5293: {'frame': 5293, 'ionic_force': [-4.439165145158768, -11.485485851764679, -5.509422957897186], 'ionic_force_magnitude': 13.489859664432528, 'motion_vector': [3.6029815673828125, -0.9414405822753906, -2.305633544921875], 'cosine_ionic_motion': 0.12729862041329584, 'ionic_motion_component': 1.7172405248512268, 'ionic_force_x': -4.439165145158768, 'ionic_force_y': -11.485485851764679, 'ionic_force_z': -5.509422957897186, 'radial_force': 12.31351178328421, 'axial_force': -5.509422957897186, 'contributions': [{'ion': 1309, 'force': [-0.4600997269153595, -6.4237165451049805, -1.8560487031936646], 'magnitude': 6.702293872833252, 'distance': 7.038130283355713, 'cosine_with_motion': 0.2953168585098998, 'motion_component': 1.9793003634343174}, {'ion': 1320, 'force': [-2.2913060188293457, -4.553028583526611, 0.9146720767021179], 'magnitude': 5.178492069244385, 'distance': 8.00695514678955, 'cosine_with_motion': -0.26797402199208176, 'motion_component': -1.387701281697467}, {'ion': 1469, 'force': [-1.280375599861145, -0.43071743845939636, -2.963862419128418], 'magnitude': 3.2572009563446045, 'distance': 10.095939636230469, 'cosine_with_motion': 0.18406364306654752, 'motion_component': 0.5995323182463634}, {'ion': 2436, 'force': [-0.4073837995529175, -0.0780232846736908, -1.6041839122772217], 'magnitude': 1.656941533088684, 'distance': 14.155181884765625, 'cosine_with_motion': 0.3175182671968274, 'motion_component': 0.5261092018864266}]}, 5294: {'frame': 5294, 'ionic_force': [0.1658477745950222, -6.8131378293037415, -5.872682213783264], 'ionic_force_magnitude': 8.99637421128724, 'motion_vector': [-1.1986160278320312, 0.10608673095703125, 0.8895950317382812], 'cosine_ionic_motion': -0.4565192458823854, 'ionic_motion_component': -4.10701797061259, 'ionic_force_x': 0.1658477745950222, 'ionic_force_y': -6.8131378293037415, 'ionic_force_z': -5.872682213783264, 'radial_force': 6.815156092521126, 'axial_force': -5.872682213783264, 'contributions': [{'ion': 1309, 'force': [1.4283074140548706, -3.2946081161499023, -1.909952163696289], 'magnitude': 4.067237377166748, 'distance': 9.034814834594727, 'cosine_with_motion': -0.6178726576783165, 'motion_component': -2.5130349266499294}, {'ion': 1320, 'force': [-1.2332184314727783, -2.8408944606781006, -1.2032557725906372], 'magnitude': 3.3225491046905518, 'distance': 9.996163368225098, 'cosine_with_motion': 0.021392684254919057, 'motion_component': 0.0710782469366329}, {'ion': 1469, 'force': [-0.029241207987070084, -0.6776352524757385, -2.759474277496338], 'magnitude': 2.841609239578247, 'distance': 10.809033393859863, 'cosine_with_motion': -0.585957106898025, 'motion_component': -1.665061108476534}]}, 5295: {'frame': 5295, 'ionic_force': [-0.8948521912097931, -8.003737807273865, -7.197145462036133], 'ionic_force_magnitude': 10.800901912961034, 'motion_vector': [1.4610366821289062, 0.4837226867675781, -0.33788299560546875], 'cosine_ionic_motion': -0.16142186763286107, 'ionic_motion_component': -1.7435017589095119, 'ionic_force_x': -0.8948521912097931, 'ionic_force_y': -8.003737807273865, 'ionic_force_z': -7.197145462036133, 'radial_force': 8.053606603981724, 'axial_force': -7.197145462036133, 'contributions': [{'ion': 1309, 'force': [1.2909294366836548, -4.2322163581848145, -2.066220760345459], 'magnitude': 4.883382320404053, 'distance': 8.245342254638672, 'cosine_with_motion': 0.06979078553032043, 'motion_component': 0.340815084300246}, {'ion': 1320, 'force': [-1.8195945024490356, -3.148383855819702, -1.8783209323883057], 'magnitude': 4.09283971786499, 'distance': 9.006513595581055, 'cosine_with_motion': -0.5499726823402922, 'motion_component': -2.2509498785102373}, {'ion': 1469, 'force': [-0.36618712544441223, -0.6231375932693481, -3.252603769302368], 'magnitude': 3.331940174102783, 'distance': 9.98206615447998, 'cosine_with_motion': 0.05001077294285725, 'motion_component': 0.16663289920801638}]}, 5296: {'frame': 5296, 'ionic_force': [0.31867482099914923, -8.267817586660385, -7.231484055519104], 'ionic_force_magnitude': 10.988754384963595, 'motion_vector': [-0.4652824401855469, 0.103912353515625, -2.422882080078125], 'cosine_ionic_motion': 0.6085736128030453, 'ionic_motion_component': 6.687465956262602, 'ionic_force_x': 0.31867482099914923, 'ionic_force_y': -8.267817586660385, 'ionic_force_z': -7.231484055519104, 'radial_force': 8.273956809642506, 'axial_force': -7.231484055519104, 'contributions': [{'ion': 1309, 'force': [2.060899019241333, -4.070521354675293, -2.4136157035827637], 'magnitude': 5.161587715148926, 'distance': 8.020055770874023, 'cosine_with_motion': 0.350394413188984, 'motion_component': 1.808591562717023}, {'ion': 1320, 'force': [-1.741642713546753, -3.7549068927764893, -1.5699185132980347], 'magnitude': 4.426882743835449, 'distance': 8.660042762756348, 'cosine_with_motion': 0.3863979687561965, 'motion_component': 1.7105384314382377}, {'ion': 1469, 'force': [-0.000581484695430845, -0.4423893392086029, -3.2479498386383057], 'magnitude': 3.2779393196105957, 'distance': 10.063952445983887, 'cosine_with_motion': 0.9665632598820196, 'motion_component': 3.1683358083492243}]}, 5297: {'frame': 5297, 'ionic_force': [2.0586469620466232, -4.025961697101593, -6.761675596237183], 'ionic_force_magnitude': 8.134288645580657, 'motion_vector': [0.11940383911132812, -0.8824501037597656, 1.4705276489257812], 'cosine_ionic_motion': -0.439411799823159, 'ionic_motion_component': -3.5743024140356825, 'ionic_force_x': 2.0586469620466232, 'ionic_force_y': -4.025961697101593, 'ionic_force_z': -6.761675596237183, 'radial_force': 4.521769001272945, 'axial_force': -6.761675596237183, 'contributions': [{'ion': 1309, 'force': [2.703697919845581, -1.9296005964279175, -3.2435293197631836], 'magnitude': 4.642609596252441, 'distance': 8.45644760131836, 'cosine_with_motion': -0.34381617958818117, 'motion_component': -1.5962042757614867}, {'ion': 1320, 'force': [-0.5463349223136902, -1.8209863901138306, -1.1804895401000977], 'magnitude': 2.2378625869750977, 'distance': 12.18014144897461, 'cosine_with_motion': -0.050490734426634716, 'motion_component': -0.1129913241681777}, {'ion': 1469, 'force': [-0.09871603548526764, -0.27537471055984497, -2.3376567363739014], 'magnitude': 2.3558895587921143, 'distance': 11.871116638183594, 'cosine_with_motion': -0.7916784499341073, 'motion_component': -1.8651069085584862}]}, 5298: {'frame': 5298, 'ionic_force': [2.64043165743351, -8.706450581550598, -7.226660072803497], 'ionic_force_magnitude': 11.618897403558226, 'motion_vector': [-0.8501853942871094, 0.7801551818847656, 2.5111923217773438], 'cosine_ionic_motion': -0.8466110490409935, 'ionic_motion_component': -9.836686919526105, 'ionic_force_x': 2.64043165743351, 'ionic_force_y': -8.706450581550598, 'ionic_force_z': -7.226660072803497, 'radial_force': 9.098030614729751, 'axial_force': -7.226660072803497, 'contributions': [{'ion': 1309, 'force': [3.2287416458129883, -6.1072096824646, -3.8306076526641846], 'magnitude': 7.899135589599609, 'distance': 6.483048439025879, 'cosine_with_motion': -0.7846489917489425, 'motion_component': -6.19804851018975}, {'ion': 1320, 'force': [-0.4978197515010834, -2.0856738090515137, -0.9577496647834778], 'magnitude': 2.3484344482421875, 'distance': 11.889945030212402, 'cosine_with_motion': -0.5560732892391631, 'motion_component': -1.3059016451634013}, {'ion': 1469, 'force': [-0.09049023687839508, -0.5135670900344849, -2.438302755355835], 'magnitude': 2.493443489074707, 'distance': 11.539029121398926, 'cosine_with_motion': -0.9355482454164143, 'motion_component': -2.3327365935457256}]}, 5299: {'frame': 5299, 'ionic_force': [8.148396573960781, -5.8599869310855865, -10.365723192691803], 'ionic_force_magnitude': 14.428583813615887, 'motion_vector': [-0.3539390563964844, 2.2585983276367188, 2.1390380859375], 'cosine_ionic_motion': -0.84767086277239, 'ionic_motion_component': -12.230690089871521, 'ionic_force_x': 8.148396573960781, 'ionic_force_y': -5.8599869310855865, 'ionic_force_z': -10.365723192691803, 'radial_force': 10.036723248103918, 'axial_force': -10.365723192691803, 'contributions': [{'ion': 1309, 'force': [9.771367073059082, -2.351778030395508, -4.5568013191223145], 'magnitude': 11.03516674041748, 'distance': 5.485037326812744, 'cosine_with_motion': -0.5359722734248957, 'motion_component': -5.914543591356164}, {'ion': 1320, 'force': [-1.1783761978149414, -2.824215888977051, -0.5681673884391785], 'magnitude': 3.11248779296875, 'distance': 10.32797622680664, 'cosine_with_motion': -0.7365107631581589, 'motion_component': -2.2923807326295993}, {'ion': 1469, 'force': [-0.3746396005153656, -0.5283625721931458, -3.711301326751709], 'magnitude': 3.767396926879883, 'distance': 9.387465476989746, 'cosine_with_motion': -0.7629798072189766, 'motion_component': -2.8744477578251457}, {'ion': 2436, 'force': [-0.06995470076799393, -0.1556304395198822, -1.529453158378601], 'magnitude': 1.5389416217803955, 'distance': 14.687841415405273, 'cosine_with_motion': -0.7468235204612907, 'motion_component': -1.1493178342881796}]}, 5300: {'frame': 5300, 'ionic_force': [11.58044770359993, 2.511912077665329, -5.298129674047232], 'ionic_force_magnitude': 12.98024072753482, 'motion_vector': [2.946308135986328, -2.5934295654296875, 0.6218948364257812], 'cosine_ionic_motion': 0.47126898983142484, 'ionic_motion_component': 6.117184935434054, 'ionic_force_x': 11.58044770359993, 'ionic_force_y': 2.511912077665329, 'ionic_force_z': -5.298129674047232, 'radial_force': 11.849745621815426, 'axial_force': -5.298129674047232, 'contributions': [{'ion': 1309, 'force': [15.33890438079834, 5.875173568725586, 3.291243076324463], 'magnitude': 16.752071380615234, 'distance': 4.451791286468506, 'cosine_with_motion': 0.48071337114347773, 'motion_component': 8.052945245231506}, {'ion': 1320, 'force': [-2.06095027923584, -3.7897627353668213, -0.05836188420653343], 'magnitude': 4.314304351806641, 'distance': 8.772303581237793, 'cosine_with_motion': 0.21696714822175778, 'motion_component': 0.9360623548549916}, {'ion': 1469, 'force': [-1.4913935661315918, 0.3887030780315399, -6.317618370056152], 'magnitude': 6.502894878387451, 'distance': 7.145220756530762, 'cosine_with_motion': -0.36106680502471306, 'motion_component': -2.347979613803373}, {'ion': 2436, 'force': [-0.2061128318309784, 0.037798166275024414, -2.213392496109009], 'magnitude': 2.223289728164673, 'distance': 12.21999454498291, 'cosine_with_motion': -0.23561603955225588, 'motion_component': -0.5238427378697725}]}, 5301: {'frame': 5301, 'ionic_force': [11.182874098420143, -8.029923260211945, -7.2750024273991585], 'ionic_force_magnitude': 15.571191379745887, 'motion_vector': [-1.3564949035644531, -1.4149208068847656, -1.5110244750976562], 'cosine_ionic_motion': 0.18643873805724717, 'ionic_motion_component': 2.9030732708877087, 'ionic_force_x': 11.182874098420143, 'ionic_force_y': -8.029923260211945, 'ionic_force_z': -7.2750024273991585, 'radial_force': 13.767219787088784, 'axial_force': -7.2750024273991585, 'contributions': [{'ion': 1309, 'force': [8.657218933105469, -1.525900959968567, 3.219957113265991], 'magnitude': 9.361833572387695, 'distance': 5.9550933837890625, 'cosine_with_motion': -0.6236493685107676, 'motion_component': -5.838501907603841}, {'ion': 1320, 'force': [-0.21056003868579865, -2.90226411819458, -0.06113452464342117], 'magnitude': 2.910534143447876, 'distance': 10.680280685424805, 'cosine_with_motion': 0.6225524357419339, 'motion_component': 1.811960224222066}, {'ion': 1469, 'force': [2.363967180252075, -3.182705879211426, -7.91904354095459], 'magnitude': 8.856026649475098, 'distance': 6.122793197631836, 'cosine_with_motion': 0.6050922614910305, 'motion_component': 5.3587131976036195}, {'ion': 2436, 'force': [0.3722480237483978, -0.4190523028373718, -2.5147814750671387], 'magnitude': 2.5764896869659424, 'distance': 11.351541519165039, 'cosine_with_motion': 0.6097060384339743, 'motion_component': 1.570901341876704}]}, 5302: {'frame': 5302, 'ionic_force': [9.384686825796962, -10.808709025382996, -6.232582181692123], 'ionic_force_magnitude': 15.612354667545477, 'motion_vector': [-1.703094482421875, 1.6502799987792969, -1.0469818115234375], 'cosine_ionic_motion': -0.6744132230711771, 'ionic_motion_component': -10.529178431069681, 'ionic_force_x': 9.384686825796962, 'ionic_force_y': -10.808709025382996, 'ionic_force_z': -6.232582181692123, 'radial_force': 14.314347264674101, 'axial_force': -6.232582181692123, 'contributions': [{'ion': 1309, 'force': [9.655634880065918, -6.011810302734375, 0.029120855033397675], 'magnitude': 11.374268531799316, 'distance': 5.402655601501465, 'cosine_with_motion': -0.8952160799916463, 'motion_component': -10.182428538158979}, {'ion': 1320, 'force': [-0.391956627368927, -2.144749641418457, -0.11846282333135605], 'magnitude': 2.1834867000579834, 'distance': 12.33087158203125, 'cosine_with_motion': -0.4854638859897166, 'motion_component': -1.0600039710206126}, {'ion': 1469, 'force': [0.1119040995836258, -2.1314122676849365, -4.249485492706299], 'magnitude': 4.755372524261475, 'distance': 8.355583190917969, 'cosine_with_motion': 0.06011979097258749, 'motion_component': 0.2858920014635995}, {'ion': 2436, 'force': [0.009104473516345024, -0.520736813545227, -1.8937547206878662], 'magnitude': 1.9640663862228394, 'distance': 13.001425743103027, 'cosine_with_motion': 0.21759044093186494, 'motion_component': 0.42736206507377106}]}, 5303: {'frame': 5303, 'ionic_force': [4.634013906121254, -7.393165856599808, -18.30676108598709], 'ionic_force_magnitude': 20.279804923241485, 'motion_vector': [2.9986648559570312, -0.3383674621582031, -0.0259552001953125], 'cosine_ionic_motion': 0.2756939581042625, 'ionic_motion_component': 5.591019688870754, 'ionic_force_x': 4.634013906121254, 'ionic_force_y': -7.393165856599808, 'ionic_force_z': -18.30676108598709, 'radial_force': 8.725421838817784, 'axial_force': -18.30676108598709, 'contributions': [{'ion': 1309, 'force': [6.351526737213135, -4.161134243011475, -12.593794822692871], 'magnitude': 14.705801963806152, 'distance': 4.751433849334717, 'cosine_with_motion': 0.46825843997322103, 'motion_component': 6.886115674686596}, {'ion': 1320, 'force': [-0.7893285751342773, -2.2547266483306885, -0.49746209383010864], 'magnitude': 2.440143585205078, 'distance': 11.664371490478516, 'cosine_with_motion': -0.21606729356545698, 'motion_component': -0.5272352060481691}, {'ion': 1469, 'force': [-0.7389268279075623, -0.7736309766769409, -3.6220219135284424], 'magnitude': 3.7767128944396973, 'distance': 9.375880241394043, 'cosine_with_motion': -0.16319631554447808, 'motion_component': -0.6163456335657835}, {'ion': 2436, 'force': [-0.1892574280500412, -0.20367398858070374, -1.593482255935669], 'magnitude': 1.6175559759140015, 'distance': 14.326476097106934, 'cosine_with_motion': -0.093669258529189, 'motion_component': -0.15151526404247218}]}, 5304: {'frame': 5304, 'ionic_force': [11.509692594408989, -10.579159915447235, -10.748389482498169], 'ionic_force_magnitude': 18.971545129532174, 'motion_vector': [-1.4822731018066406, 2.659027099609375, -2.7203369140625], 'cosine_ionic_motion': -0.20594956949000837, 'ionic_motion_component': -3.9071815519874162, 'ionic_force_x': 11.509692594408989, 'ionic_force_y': -10.579159915447235, 'ionic_force_z': -10.748389482498169, 'radial_force': 15.633030676564243, 'axial_force': -10.748389482498169, 'contributions': [{'ion': 1309, 'force': [10.475059509277344, -6.060859680175781, -4.418924331665039], 'magnitude': 12.883625030517578, 'distance': 5.076332092285156, 'cosine_with_motion': -0.3730478564218393, 'motion_component': -4.806208557360378}, {'ion': 1320, 'force': [-0.10482928156852722, -3.094301462173462, -0.409082293510437], 'magnitude': 3.122985601425171, 'distance': 10.310602188110352, 'cosine_with_motion': -0.5458528017668542, 'motion_component': -1.7046904380766525}, {'ion': 1469, 'force': [0.9543324708938599, -1.1745716333389282, -4.332919597625732], 'magnitude': 4.589614391326904, 'distance': 8.50512981414795, 'cosine_with_motion': 0.3868788436129706, 'motion_component': 1.7756247490290527}, {'ion': 2436, 'force': [0.18512989580631256, -0.24942713975906372, -1.5874632596969604], 'magnitude': 1.6175681352615356, 'distance': 14.326422691345215, 'cosine_with_motion': 0.5119368498997857, 'motion_component': 0.8280927206379406}]}, 5305: {'frame': 5305, 'ionic_force': [-7.564083315432072, 10.154234908521175, -16.6937335729599], 'ionic_force_magnitude': 20.952436220764316, 'motion_vector': [3.7210350036621094, 0.5313720703125, 4.7978057861328125], 'cosine_ionic_motion': -0.80534045139699, 'ionic_motion_component': -16.873844443896978, 'ionic_force_x': -7.564083315432072, 'ionic_force_y': 10.154234908521175, 'ionic_force_z': -16.6937335729599, 'radial_force': 12.66190518761801, 'axial_force': -16.6937335729599, 'contributions': [{'ion': 1309, 'force': [-6.675297737121582, 13.578149795532227, -11.790082931518555], 'magnitude': 19.181549072265625, 'distance': 4.160324573516846, 'cosine_with_motion': -0.6346004901054394, 'motion_component': -12.17262015225235}, {'ion': 1320, 'force': [-0.9775453209877014, -3.548858880996704, -1.993395209312439], 'magnitude': 4.186121940612793, 'distance': 8.905597686767578, 'cosine_with_motion': -0.5913323316384337, 'motion_component': -2.4753893727261147}, {'ion': 1469, 'force': [0.08875974267721176, 0.12494399398565292, -2.9102554321289062], 'magnitude': 2.91428804397583, 'distance': 10.673399925231934, 'cosine_with_motion': -0.7637664263245683, 'motion_component': -2.2258355180118463}]}, 5306: {'frame': 5306, 'ionic_force': [17.47581458091736, -4.5736775398254395, -4.979289084672928], 'ionic_force_magnitude': 18.738087983933962, 'motion_vector': [-1.9650535583496094, -1.8321075439453125, -0.7120208740234375], 'cosine_ionic_motion': -0.4304121236027933, 'ionic_motion_component': -8.065100241421, 'ionic_force_x': 17.47581458091736, 'ionic_force_y': -4.5736775398254395, 'ionic_force_z': -4.979289084672928, 'radial_force': 18.064402052238194, 'axial_force': -4.979289084672928, 'contributions': [{'ion': 1309, 'force': [4.468284606933594, 4.662998676300049, 3.70725679397583], 'magnitude': 7.44666862487793, 'distance': 6.677102088928223, 'cosine_with_motion': -0.9645342433791801, 'motion_component': -7.182567102252463}, {'ion': 1320, 'force': [7.873488903045654, -10.533976554870605, 0.34959670901298523], 'magnitude': 13.155938148498535, 'distance': 5.023519992828369, 'cosine_with_motion': 0.09786899057282514, 'motion_component': 1.2875583823797827}, {'ion': 1469, 'force': [4.469884872436523, 1.055068850517273, -6.895050525665283], 'magnitude': 8.2846097946167, 'distance': 6.330427169799805, 'cosine_with_motion': -0.25219732116268007, 'motion_component': -2.0893564481400375}, {'ion': 2436, 'force': [0.6641561985015869, 0.24223148822784424, -2.14109206199646], 'magnitude': 2.2547848224639893, 'distance': 12.13434886932373, 'cosine_with_motion': -0.03580609982653162, 'motion_component': -0.08073505180798435}]}, 5307: {'frame': 5307, 'ionic_force': [6.0052439123392105, 2.971535697579384, -1.2920927703380585], 'ionic_force_magnitude': 6.823670755233991, 'motion_vector': [-1.8429718017578125, 0.5340690612792969, 3.6442413330078125], 'cosine_ionic_motion': -0.5048908635908108, 'ionic_motion_component': -3.44520902046945, 'ionic_force_x': 6.0052439123392105, 'ionic_force_y': 2.971535697579384, 'ionic_force_z': -1.2920927703380585, 'radial_force': 6.700222298452175, 'axial_force': -1.2920927703380585, 'contributions': [{'ion': 1309, 'force': [5.069587707519531, 8.484151840209961, 7.271227836608887], 'magnitude': 12.269975662231445, 'distance': 5.201722621917725, 'cosine_with_motion': 0.4291373195283767, 'motion_component': 5.265504527085966}, {'ion': 1320, 'force': [-0.18250830471515656, -4.807651519775391, -0.49011465907096863], 'magnitude': 4.836014270782471, 'distance': 8.285624504089355, 'cosine_with_motion': -0.2017022843551575, 'motion_component': -0.975435141621853}, {'ion': 1469, 'force': [0.850151538848877, -0.5294232368469238, -5.994930744171143], 'magnitude': 6.078012943267822, 'distance': 7.390745162963867, 'cosine_with_motion': -0.9466319012710269, 'motion_component': -5.753640939993872}, {'ion': 2436, 'force': [0.26801297068595886, -0.17554138600826263, -2.078275203704834], 'magnitude': 2.102825164794922, 'distance': 12.565143585205078, 'cosine_with_motion': -0.942369072941603, 'motion_component': -1.9816373740599276}]}, 5308: {'frame': 5308, 'ionic_force': [-3.9245860427618027, -5.353306509554386, -11.027286529541016], 'ionic_force_magnitude': 12.870948465318119, 'motion_vector': [-0.12729644775390625, 0.5117263793945312, -0.26439666748046875], 'cosine_ionic_motion': 0.08900058775676298, 'ionic_motion_component': 1.145521978400319, 'ionic_force_x': -3.9245860427618027, 'ionic_force_y': -5.353306509554386, 'ionic_force_z': -11.027286529541016, 'radial_force': 6.637790761411368, 'axial_force': -11.027286529541016, 'contributions': [{'ion': 1309, 'force': [0.1623639464378357, 0.4300653338432312, 3.4034218788146973], 'magnitude': 3.434326410293579, 'distance': 9.832144737243652, 'cosine_with_motion': -0.3457480673528202, 'motion_component': -1.1874117610608668}, {'ion': 1320, 'force': [-3.1859545707702637, -5.096459865570068, 2.4922938346862793], 'magnitude': 6.506591796875, 'distance': 7.143190860748291, 'cosine_with_motion': -0.7455033842480661, 'motion_component': -4.850686286735993}, {'ion': 1469, 'force': [-1.04063880443573, -0.7825348973274231, -12.82127857208252], 'magnitude': 12.887221336364746, 'distance': 5.075623512268066, 'cosine_with_motion': 0.4106676150977118, 'motion_component': 5.292364458409139}, {'ion': 2436, 'force': [0.13964338600635529, 0.09562291949987411, -4.101723670959473], 'magnitude': 4.1052141189575195, 'distance': 8.992928504943848, 'cosine_with_motion': 0.4606960465227934, 'motion_component': 1.891255809716336}]}, 5309: {'frame': 5309, 'ionic_force': [-6.100982252508402, -3.1015712544322014, -15.906369686126709], 'ionic_force_magnitude': 17.31630229822387, 'motion_vector': [0.6568450927734375, -0.14005661010742188, -0.313629150390625], 'cosine_ionic_motion': 0.11029630434347097, 'ionic_motion_component': 1.909924148388446, 'ionic_force_x': -6.100982252508402, 'ionic_force_y': -3.1015712544322014, 'ionic_force_z': -15.906369686126709, 'radial_force': 6.844101744695401, 'axial_force': -15.906369686126709, 'contributions': [{'ion': 1309, 'force': [0.20207388699054718, 0.08543962985277176, 2.6796698570251465], 'magnitude': 2.688636302947998, 'distance': 11.112276077270508, 'cosine_with_motion': -0.3611103386395704, 'motion_component': -0.970894309377176}, {'ion': 1320, 'force': [-3.724456787109375, -3.0685253143310547, 2.46171236038208], 'magnitude': 5.417328834533691, 'distance': 7.828461647033691, 'cosine_with_motion': -0.6944816395866571, 'motion_component': -3.7622355398655856}, {'ion': 1469, 'force': [-2.5375022888183594, -0.4666903018951416, -17.041349411010742], 'magnitude': 17.235553741455078, 'distance': 4.388907432556152, 'cosine_with_motion': 0.29300374354212066, 'motion_component': 5.050081723024142}, {'ion': 2436, 'force': [-0.041097063571214676, 0.34820473194122314, -4.006402492523193], 'magnitude': 4.0217156410217285, 'distance': 9.085803985595703, 'cosine_with_motion': 0.39609276644881936, 'motion_component': 1.59297246126204}]}, 5310: {'frame': 5310, 'ionic_force': [-2.138845317065716, -6.399635553359985, -14.446752071380615], 'ionic_force_magnitude': 15.944862492919254, 'motion_vector': [-0.4894981384277344, 0.20468902587890625, 0.37158966064453125], 'cosine_ionic_motion': -0.5452217807443366, 'ionic_motion_component': -8.693486322113017, 'ionic_force_x': -2.138845317065716, 'ionic_force_y': -6.399635553359985, 'ionic_force_z': -14.446752071380615, 'radial_force': 6.747591756038824, 'axial_force': -14.446752071380615, 'contributions': [{'ion': 1309, 'force': [-0.425532728433609, 0.4280744194984436, 4.451706409454346], 'magnitude': 4.4924397468566895, 'distance': 8.596623420715332, 'cosine_with_motion': 0.6701482337154809, 'motion_component': 3.0106006276943322}, {'ion': 1320, 'force': [-2.6733267307281494, -4.865641117095947, 5.675074100494385], 'magnitude': 7.938992977142334, 'distance': 6.466753959655762, 'cosine_with_motion': 0.4708679390348454, 'motion_component': 3.7382171379287144}, {'ion': 1469, 'force': [0.8352939486503601, -1.7298543453216553, -20.9677677154541], 'magnitude': 21.055578231811523, 'distance': 3.970867872238159, 'cosine_with_motion': -0.6272065415358462, 'motion_component': -13.206196705608171}, {'ion': 2436, 'force': [0.12472019344568253, -0.23221451044082642, -3.605764865875244], 'magnitude': 3.615386486053467, 'distance': 9.582783699035645, 'cosine_with_motion': -0.6184975575539667, 'motion_component': -2.2361076710314904}]}, 5311: {'frame': 5311, 'ionic_force': [-1.5457566678524017, -3.735124170780182, -10.29975938796997], 'ionic_force_magnitude': 11.064608429466993, 'motion_vector': [0.5821189880371094, -0.71893310546875, 0.33875274658203125], 'cosine_ionic_motion': -0.15629080861675848, 'ionic_motion_component': -1.7292965984691986, 'ionic_force_x': -1.5457566678524017, 'ionic_force_y': -3.735124170780182, 'ionic_force_z': -10.29975938796997, 'radial_force': 4.042340441793158, 'axial_force': -10.29975938796997, 'contributions': [{'ion': 1309, 'force': [0.2618166506290436, 0.38895392417907715, 3.28230881690979], 'magnitude': 3.315627336502075, 'distance': 10.006591796875, 'cosine_with_motion': 0.30146056067917015, 'motion_component': 0.9995308598941133}, {'ion': 1320, 'force': [-0.6014491319656372, -3.967463493347168, 2.3787336349487305], 'magnitude': 4.66485595703125, 'distance': 8.436259269714355, 'cosine_with_motion': 0.71984257043354, 'motion_component': 3.3579619209873}, {'ion': 1469, 'force': [-1.1576669216156006, -0.06768996268510818, -12.637163162231445], 'magnitude': 12.690258979797363, 'distance': 5.114860534667969, 'cosine_with_motion': -0.3924399710702723, 'motion_component': -4.980164781043792}, {'ion': 2436, 'force': [-0.04845726490020752, -0.08892463892698288, -3.323638677597046], 'magnitude': 3.325181007385254, 'distance': 9.992206573486328, 'cosine_with_motion': -0.33280123710707715, 'motion_component': -1.1066244041700855}]}, 5312: {'frame': 5312, 'ionic_force': [-0.6932454779744148, -6.2057766020298, -20.55894696712494], 'ionic_force_magnitude': 21.486334096911186, 'motion_vector': [-0.3184471130371094, 0.7150497436523438, -0.7793121337890625], 'cosine_ionic_motion': 0.49742079003617534, 'ionic_motion_component': 10.687749281466774, 'ionic_force_x': -0.6932454779744148, 'ionic_force_y': -6.2057766020298, 'ionic_force_z': -20.55894696712494, 'radial_force': 6.244377673318016, 'axial_force': -20.55894696712494, 'contributions': [{'ion': 1309, 'force': [0.08076175302267075, 0.06683516502380371, 2.8113584518432617], 'magnitude': 2.81331205368042, 'distance': 10.86325740814209, 'cosine_with_motion': -0.6979538305612016, 'motion_component': -1.9635620526184647}, {'ion': 1320, 'force': [-0.7783627510070801, -3.133505344390869, 1.1805278062820435], 'magnitude': 3.4377827644348145, 'distance': 9.827200889587402, 'cosine_with_motion': -0.7670759051133565, 'motion_component': -2.6370403123848902}, {'ion': 1469, 'force': [-0.06458400189876556, -2.735037326812744, -20.452817916870117], 'magnitude': 20.634979248046875, 'distance': 4.011132717132568, 'cosine_with_motion': 0.6144162662202742, 'motion_component': 12.678466790651052}, {'ion': 2436, 'force': [0.06893952190876007, -0.40406909584999084, -4.098015308380127], 'magnitude': 4.118464946746826, 'distance': 8.978449821472168, 'cosine_with_motion': 0.6337033185455325, 'motion_component': 2.6098849380748117}]}, 5313: {'frame': 5313, 'ionic_force': [-6.034946657717228, -5.350842729210854, -16.52107262611389], 'ionic_force_magnitude': 18.384720280482124, 'motion_vector': [-0.3755340576171875, -0.5339927673339844, 0.46227264404296875], 'cosine_ionic_motion': -0.17092017347635274, 'ionic_motion_component': -3.142319579654225, 'ionic_force_x': -6.034946657717228, 'ionic_force_y': -5.350842729210854, 'ionic_force_z': -16.52107262611389, 'radial_force': 8.065488148540112, 'axial_force': -16.52107262611389, 'contributions': [{'ion': 1309, 'force': [-0.11181335151195526, -3.108283758163452, 3.290030002593994], 'magnitude': 4.527496814727783, 'distance': 8.563276290893555, 'cosine_with_motion': 0.8898428749727498, 'motion_component': 4.028760797518868}, {'ion': 1320, 'force': [-4.065372467041016, -4.175497531890869, 2.469059705734253], 'magnitude': 6.329161643981934, 'distance': 7.242623805999756, 'cosine_with_motion': 0.9673964643253833, 'motion_component': 6.1228087225875925}, {'ion': 1469, 'force': [-1.8919004201889038, 1.7885223627090454, -18.668319702148438], 'magnitude': 18.84898567199707, 'distance': 4.196865558624268, 'cosine_with_motion': -0.5885820179472476, 'motion_component': -11.094174008723336}, {'ion': 2436, 'force': [0.03413958102464676, 0.1444161981344223, -3.611842632293701], 'magnitude': 3.6148898601531982, 'distance': 9.583441734313965, 'cosine_with_motion': -0.6085152255557099, 'motion_component': -2.1997155227084764}]}, 5314: {'frame': 5314, 'ionic_force': [-5.211430847644806, -8.442669451236725, -17.771475553512573], 'ionic_force_magnitude': 20.35345234331819, 'motion_vector': [-0.15516281127929688, 0.3010063171386719, -0.0225677490234375], 'cosine_ionic_motion': -0.19276747009609363, 'ionic_motion_component': -3.9234835159428556, 'ionic_force_x': -5.211430847644806, 'ionic_force_y': -8.442669451236725, 'ionic_force_z': -17.771475553512573, 'radial_force': 9.921576434349014, 'axial_force': -17.771475553512573, 'contributions': [{'ion': 1309, 'force': [-0.48251619935035706, -3.664240598678589, 1.9041845798492432], 'magnitude': 4.157571315765381, 'distance': 8.936123847961426, 'cosine_with_motion': -0.759047802567711, 'motion_component': -3.155795436619493}, {'ion': 1320, 'force': [-3.720808982849121, -2.3928604125976562, 4.966029167175293], 'magnitude': 6.6506876945495605, 'distance': 7.0653839111328125, 'cosine_with_motion': -0.11297411757773741, 'motion_component': -0.7513555677998909}, {'ion': 1469, 'force': [-1.2004474401474, -2.1353933811187744, -20.877975463867188], 'magnitude': 21.02120018005371, 'distance': 3.974113702774048, 'cosine_with_motion': 0.002055755984253285, 'motion_component': 0.04321445715726568}, {'ion': 2436, 'force': [0.19234177470207214, -0.2501750588417053, -3.763713836669922], 'magnitude': 3.7769198417663574, 'distance': 9.37562370300293, 'cosine_with_motion': -0.015766023567895776, 'motion_component': -0.059547009893312186}]}, 5315: {'frame': 5315, 'ionic_force': [-4.354976288974285, -2.9413586780428886, -13.101229906082153], 'ionic_force_magnitude': 14.115935477411613, 'motion_vector': [0.5261955261230469, -0.461700439453125, -0.2435302734375], 'cosine_ionic_motion': 0.21572260525693082, 'ionic_motion_component': 3.0451263768259706, 'ionic_force_x': -4.354976288974285, 'ionic_force_y': -2.9413586780428886, 'ionic_force_z': -13.101229906082153, 'radial_force': 5.2552268600343455, 'axial_force': -13.101229906082153, 'contributions': [{'ion': 1309, 'force': [-1.3679094314575195, -3.2166194915771484, 1.7919011116027832], 'magnitude': 3.9279417991638184, 'distance': 9.193619728088379, 'cosine_with_motion': 0.11298760627771773, 'motion_component': 0.44380874123271497}, {'ion': 1320, 'force': [-0.15094943344593048, 0.24601347744464874, 6.12855863571167], 'magnitude': 6.135351657867432, 'distance': 7.356128692626953, 'cosine_with_motion': -0.37064926599663733, 'motion_component': -2.2740635689315685}, {'ion': 1469, 'force': [-2.7265963554382324, 0.12713120877742767, -17.374311447143555], 'magnitude': 17.58741569519043, 'distance': 4.34478235244751, 'cosine_with_motion': 0.21002214050115225, 'motion_component': 3.6937466750015853}, {'ion': 2436, 'force': [-0.10952106863260269, -0.09788387268781662, -3.6473782062530518], 'magnitude': 3.6503348350524902, 'distance': 9.536800384521484, 'cosine_with_motion': 0.32370584867965324, 'motion_component': 1.1816347130642422}]}, 5316: {'frame': 5316, 'ionic_force': [1.7553037405014038, -11.83569049090147, -15.618502497673035], 'ionic_force_magnitude': 19.6749150160211, 'motion_vector': [-0.0081329345703125, -0.06674957275390625, -0.1145172119140625], 'cosine_ionic_motion': 0.9814416458058247, 'ionic_motion_component': 19.30978097441348, 'ionic_force_x': 1.7553037405014038, 'ionic_force_y': -11.83569049090147, 'ionic_force_z': -15.618502497673035, 'radial_force': 11.965143568626067, 'axial_force': -15.618502497673035, 'contributions': [{'ion': 1309, 'force': [-1.1511693000793457, -4.0106306076049805, 0.9726828336715698], 'magnitude': 4.2844438552856445, 'distance': 8.80281925201416, 'cosine_with_motion': 0.29119307062612976, 'motion_component': 1.2476004088355062}, {'ion': 13</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{5347: {'frame': 5347, 'ionic_force': [0.6853100061416626, -9.129887342453003, -11.733562916517258], 'ionic_force_magnitude': 14.88290937304499, 'motion_vector': [3.316211700439453, -1.65020751953125, -0.9902801513671875], 'cosine_ionic_motion': 0.5074709139954511, 'ionic_motion_component': 7.552643622450607, 'ionic_force_x': 0.6853100061416626, 'ionic_force_y': -9.129887342453003, 'ionic_force_z': -11.733562916517258, 'radial_force': 9.15557167469085, 'axial_force': -11.733562916517258, 'contributions': [{'ion': 1309, 'force': [-3.900376081466675, -0.4288240671157837, -0.44240328669548035], 'magnitude': 3.948739528656006, 'distance': 9.169376373291016, 'directional_contribution': -3.0746222669723364}, {'ion': 1320, 'force': [5.2017621994018555, -9.052448272705078, -8.116565704345703], 'magnitude': 13.224363327026367, 'distance': 5.010506629943848, 'directional_contribution': 10.491425302286757}, {'ion': 2436, 'force': [-0.6160761117935181, 0.3513849973678589, -3.174593925476074], 'magnitude': 3.2528553009033203, 'distance': 10.102682113647461, 'directional_contribution': 0.13584067736087846}]}, 5348: {'frame': 5348, 'ionic_force': [-2.9597952365875244, -4.185118928551674, -6.418415784835815], 'ionic_force_magnitude': 8.21411404082493, 'motion_vector': [1.4751319885253906, 0.6213607788085938, -1.0232925415039062], 'cosine_ionic_motion': -0.02554542998862456, 'ionic_motion_component': -0.20983307514847122, 'ionic_force_x': -2.9597952365875244, 'ionic_force_y': -4.185118928551674, 'ionic_force_z': -6.418415784835815, 'radial_force': 5.125973886848011, 'axial_force': -6.418415784835815, 'contributions': [{'ion': 1309, 'force': [-6.009511947631836, -2.5683140754699707, -1.4689178466796875], 'magnitude': 6.6983723640441895, 'distance': 7.04019021987915, 'directional_contribution': -4.714996792595642}, {'ion': 1320, 'force': [2.708761215209961, -1.4557560682296753, -2.3566243648529053], 'magnitude': 3.874311685562134, 'distance': 9.25703239440918, 'directional_contribution': 2.8964909137275363}, {'ion': 2436, 'force': [0.3409554958343506, -0.1610487848520279, -2.5928735733032227], 'magnitude': 2.6201491355895996, 'distance': 11.256568908691406, 'directional_contribution': 1.6086729895284697}]}, 5349: {'frame': 5349, 'ionic_force': [-7.378105878829956, -6.646641850471497, -10.801924467086792], 'ionic_force_magnitude': 14.672963791964886, 'motion_vector': [-0.10723876953125, -1.5981407165527344, 3.5609359741210938], 'cosine_ionic_motion': -0.47216925748123195, 'ionic_motion_component': -6.9281224187010615, 'ionic_force_x': -7.378105878829956, 'ionic_force_y': -6.646641850471497, 'ionic_force_z': -10.801924467086792, 'radial_force': 9.93047301228216, 'axial_force': -10.801924467086792, 'contributions': [{'ion': 1309, 'force': [-10.252406120300293, -4.798220634460449, -6.5559773445129395], 'magnitude': 13.08111572265625, 'distance': 5.037866592407227, 'directional_contribution': -3.7334855442888415}, {'ion': 1320, 'force': [2.3740317821502686, -1.7368981838226318, -2.094464063644409], 'magnitude': 3.61104154586792, 'distance': 9.588546752929688, 'directional_contribution': -1.2644179383602139}, {'ion': 2436, 'force': [0.5002684593200684, -0.11152303218841553, -2.1514830589294434], 'magnitude': 2.2116928100585938, 'distance': 12.25199031829834, 'directional_contribution': -1.9302188522429757}]}, 5350: {'frame': 5350, 'ionic_force': [-0.14506256580352783, -16.753881365060806, -3.0993531867861748], 'ionic_force_magnitude': 17.038766801590157, 'motion_vector': [2.5827255249023438, 0.7509269714355469, 2.464935302734375], 'cosine_ionic_motion': -0.33131159151419914, 'ionic_motion_component': -5.645140946474135, 'ionic_force_x': -0.14506256580352783, 'ionic_force_y': -16.753881365060806, 'ionic_force_z': -3.0993531867861748, 'radial_force': 16.754509361438465, 'axial_force': -3.0993531867861748, 'contributions': [{'ion': 1309, 'force': [-7.1796159744262695, -10.836474418640137, 3.318307876586914], 'magnitude': 13.415931701660156, 'distance': 4.974605083465576, 'directional_contribution': -5.07108568105761}, {'ion': 1320, 'force': [5.264742851257324, -4.707367897033691, -0.06457030028104782], 'magnitude': 7.062648296356201, 'distance': 6.856228351593018, 'directional_contribution': 2.714488781801923}, {'ion': 2434, 'force': [0.3296545743942261, -0.23305991291999817, -1.7742886543273926], 'magnitude': 1.8196399211883545, 'distance': 13.50754165649414, 'directional_contribution': -1.0133722924457365}, {'ion': 2436, 'force': [1.4401559829711914, -0.97697913646698, -4.578802108764648], 'magnitude': 4.8983635902404785, 'distance': 8.232723236083984, 'directional_contribution': -2.2751716672537476}]}, 5351: {'frame': 5351, 'ionic_force': [6.5781702399253845, -10.670942857861519, 6.412924081087112], 'ionic_force_magnitude': 14.080729400530808, 'motion_vector': [-4.924442291259766, -0.13016128540039062, 1.0756683349609375], 'cosine_ionic_motion': -0.3395388214293875, 'ionic_motion_component': -4.7809542655223565, 'ionic_force_x': 6.5781702399253845, 'ionic_force_y': -10.670942857861519, 'ionic_force_z': 6.412924081087112, 'radial_force': 12.535603104006832, 'axial_force': 6.412924081087112, 'contributions': [{'ion': 1309, 'force': [-0.7276131510734558, -8.576908111572266, 12.734542846679688], 'magnitude': 15.370795249938965, 'distance': 4.647515773773193, 'directional_contribution': 3.648702129922416}, {'ion': 1320, 'force': [2.105349540710449, -1.2945811748504639, 0.18129947781562805], 'magnitude': 2.478165864944458, 'distance': 11.574542999267578, 'directional_contribution': -1.9840704163505523}, {'ion': 2434, 'force': [1.0735446214675903, -0.11892910301685333, -2.175081729888916], 'magnitude': 2.428502082824707, 'distance': 11.692296028137207, 'directional_contribution': -1.5094089525808843}, {'ion': 2436, 'force': [4.126889228820801, -0.680524468421936, -4.327836513519287], 'magnitude': 6.018678665161133, 'distance': 7.427085876464844, 'directional_contribution': -4.93617713739299}]}, 5352: {'frame': 5352, 'ionic_force': [9.924710154533386, -10.801763534545898, -9.8836290538311], 'ionic_force_magnitude': 17.687964562986828, 'motion_vector': [1.6225547790527344, 0.3573951721191406, -0.7139053344726562], 'cosine_ionic_motion': 0.6033578075989015, 'ionic_motion_component': 10.672171519610794, 'ionic_force_x': 9.924710154533386, 'ionic_force_y': -10.801763534545898, 'ionic_force_z': -9.8836290538311, 'radial_force': 14.668945671306565, 'axial_force': -9.8836290538311, 'contributions': [{'ion': 1309, 'force': [5.455544471740723, -4.775212287902832, 4.03164005279541], 'magnitude': 8.295766830444336, 'distance': 6.326169013977051, 'directional_contribution': 2.359669156171975}, {'ion': 1320, 'force': [3.4328699111938477, -2.7567880153656006, 0.24743130803108215], 'magnitude': 4.409727573394775, 'distance': 8.676871299743652, 'directional_contribution': 2.437664444258087}, {'ion': 2434, 'force': [0.07548081874847412, -0.4966468811035156, -2.923949956893921], 'magnitude': 2.9667892456054688, 'distance': 10.57853889465332, 'directional_contribution': 1.1239045384416073}, {'ion': 2436, 'force': [0.9608149528503418, -2.77311635017395, -11.238750457763672], 'magnitude': 11.615629196166992, 'distance': 5.346230506896973, 'directional_contribution': 4.750933804418082}]}, 5353: {'frame': 5353, 'ionic_force': [11.046917110681534, -10.955666691064835, -16.785257935523987], 'ionic_force_magnitude': 22.88680611745656, 'motion_vector': [-1.0786094665527344, -0.3579292297363281, -0.06634521484375], 'cosine_ionic_motion': -0.2640805144456472, 'ionic_motion_component': -6.043959533515713, 'ionic_force_x': 11.046917110681534, 'ionic_force_y': -10.955666691064835, 'ionic_force_z': -16.785257935523987, 'radial_force': 15.558310007708934, 'axial_force': -16.785257935523987, 'contributions': [{'ion': 1309, 'force': [0.8205000758171082, -5.329401016235352, 1.1785228252410889], 'magnitude': 5.519479274749756, 'distance': 7.755681991577148, 'directional_contribution': 0.8295632579359236}, {'ion': 1320, 'force': [3.7472195625305176, -2.678145170211792, 0.29563629627227783], 'magnitude': 4.615356922149658, 'distance': 8.481377601623535, 'directional_contribution': -2.7256354706602135}, {'ion': 2434, 'force': [0.39906546473503113, -0.3938721716403961, -2.652449131011963], 'magnitude': 2.7110652923583984, 'distance': 11.066213607788086, 'directional_contribution': -0.09968546798403999}, {'ion': 2436, 'force': [6.080132007598877, -2.554248332977295, -15.60696792602539], 'magnitude': 16.943130493164062, 'distance': 4.426620006561279, 'directional_contribution': -4.0482022507508475}]}, 5354: {'frame': 5354, 'ionic_force': [-0.8884754180908203, -10.587919175624847, -4.579100914299488], 'ionic_force_magnitude': 11.569856793472182, 'motion_vector': [-1.3265037536621094, 1.3291473388671875, 1.2285842895507812], 'cosine_ionic_motion': -0.7133261353379372, 'ionic_motion_component': -8.25308123290089, 'ionic_force_x': -0.8884754180908203, 'ionic_force_y': -10.587919175624847, 'ionic_force_z': -4.579100914299488, 'radial_force': 10.62513157744957, 'axial_force': -4.579100914299488, 'contributions': [{'ion': 1309, 'force': [-6.627227306365967, -5.314355373382568, 7.1092095375061035], 'magnitude': 11.077156066894531, 'distance': 5.4746317863464355, 'directional_contribution': 4.662036524869421}, {'ion': 1320, 'force': [3.325421094894409, -3.054407835006714, 0.12004440277814865], 'magnitude': 4.5168843269348145, 'distance': 8.573330879211426, 'directional_contribution': -3.709158100849936}, {'ion': 2434, 'force': [0.26523327827453613, -0.28264373540878296, -2.6325316429138184], 'magnitude': 2.6609132289886475, 'distance': 11.170013427734375, 'directional_contribution': -1.7654833460838617}, {'ion': 2436, 'force': [2.148097515106201, -1.9365122318267822, -9.175823211669922], 'magnitude': 9.620818138122559, 'distance': 5.874393939971924, 'directional_contribution': -7.440476332000287}]}, 5355: {'frame': 5355, 'ionic_force': [-1.0782689899206161, -3.377299338579178, -19.434728145599365], 'ionic_force_magnitude': 19.755441603020266, 'motion_vector': [-0.3754844665527344, 2.017047882080078, -2.8304595947265625], 'cosine_ionic_motion': 0.7037424023399148, 'ionic_motion_component': 13.90274193299538, 'ionic_force_x': -1.0782689899206161, 'ionic_force_y': -3.377299338579178, 'ionic_force_z': -19.434728145599365, 'radial_force': 3.5452524362859945, 'axial_force': -19.434728145599365, 'contributions': [{'ion': 1309, 'force': [-4.155211925506592, -0.5779337286949158, 3.243894577026367], 'magnitude': 5.303078651428223, 'distance': 7.912341117858887, 'directional_contribution': -2.5136126988026177}, {'ion': 1320, 'force': [5.40611457824707, -3.8656556606292725, 1.663935661315918], 'magnitude': 6.851134777069092, 'distance': 6.961258888244629, 'directional_contribution': -4.15830878571586}, {'ion': 2434, 'force': [-0.2116548866033554, 0.1417645514011383, -3.8158822059631348], 'magnitude': 3.824375867843628, 'distance': 9.31727123260498, 'directional_contribution': 3.1941063817137327}, {'ion': 2436, 'force': [-2.1175167560577393, 0.9245254993438721, -20.526676177978516], 'magnitude': 20.656307220458984, 'distance': 4.009061336517334, 'directional_contribution': 17.380556983894365}]}, 5356: {'frame': 5356, 'ionic_force': [9.193988606333733, -9.341656267642975, -8.68997049331665], 'ionic_force_magnitude': 15.726142422441105, 'motion_vector': [-5.566600799560547, -5.137775421142578, 0.14322662353515625], 'cosine_ionic_motion': -0.03716797145292092, 'ionic_motion_component': -0.5845088126218596, 'ionic_force_x': 9.193988606333733, 'ionic_force_y': -9.341656267642975, 'ionic_force_z': -8.68997049331665, 'radial_force': 13.107096105399846, 'axial_force': -8.68997049331665, 'contributions': [{'ion': 1309, 'force': [-5.083637714385986, 1.7815605401992798, 4.272593021392822], 'magnitude': 6.875491142272949, 'distance': 6.948917865753174, 'directional_contribution': 2.6076830443856958}, {'ion': 1320, 'force': [15.738530158996582, -14.13753890991211, -3.5142836570739746], 'magnitude': 21.44577980041504, 'distance': 3.934577465057373, 'directional_contribution': -2.042873198654397}, {'ion': 2434, 'force': [-0.2095593959093094, 0.4638260006904602, -2.334017753601074], 'magnitude': 2.3888676166534424, 'distance': 11.788891792297363, 'directional_contribution': -0.2046830264040187}, {'ion': 2436, 'force': [-1.2513444423675537, 2.5504961013793945, -7.114262104034424], 'magnitude': 7.660523414611816, 'distance': 6.583241939544678, 'directional_contribution': -0.9446358543236686}]}, 5357: {'frame': 5357, 'ionic_force': [-6.36072164773941, -7.776129573583603, -3.584123432636261], 'ionic_force_magnitude': 10.666438571779926, 'motion_vector': [1.0815353393554688, -1.1651802062988281, 1.2048263549804688], 'cosine_ionic_motion': -0.10043836085855601, 'ionic_motion_component': -1.071319606348053, 'ionic_force_x': -6.36072164773941, 'ionic_force_y': -7.776129573583603, 'ionic_force_z': -3.584123432636261, 'radial_force': 10.046241636810368, 'axial_force': -3.584123432636261, 'contributions': [{'ion': 1309, 'force': [-1.7606245279312134, -0.44900551438331604, 1.1280972957611084], 'magnitude': 2.13869309425354, 'distance': 12.459333419799805, 'directional_contribution': -0.010950832851939651}, {'ion': 1320, 'force': [-1.3347965478897095, -6.032811641693115, -0.6402768492698669], 'magnitude': 6.211799621582031, 'distance': 7.310723304748535, 'directional_contribution': 2.4134832243306086}, {'ion': 2434, 'force': [-0.9485629200935364, -0.36116552352905273, -1.7239831686019897], 'magnitude': 2.000582456588745, 'distance': 12.882223129272461, 'directional_contribution': -1.344630176815933}, {'ion': 2436, 'force': [-2.316737651824951, -0.9331468939781189, -2.3479607105255127], 'magnitude': 3.427966594696045, 'distance': 9.84126091003418, 'directional_contribution': -2.129221633842434}]}, 5358: {'frame': 5358, 'ionic_force': [-8.373949587345123, -10.114233255386353, -2.16071218252182], 'ionic_force_magnitude': 13.307494999866014, 'motion_vector': [-0.13986587524414062, 0.56707763671875, 0.13983154296875], 'cosine_ionic_motion': -0.6089035342787845, 'ionic_motion_component': -8.102980737815669, 'ionic_force_x': -8.373949587345123, 'ionic_force_y': -10.114233255386353, 'ionic_force_z': -2.16071218252182, 'radial_force': 13.130908043077628, 'axial_force': -2.16071218252182, 'contributions': [{'ion': 1309, 'force': [-2.585419178009033, -2.5263538360595703, 2.679021120071411], 'magnitude': 4.499334335327148, 'distance': 8.590034484863281, 'directional_contribution': -1.1595774628844175}, {'ion': 1320, 'force': [-1.769490361213684, -4.937245845794678, 0.018840014934539795], 'magnitude': 5.244792461395264, 'distance': 7.956185340881348, 'directional_contribution': -4.245379473738665}, {'ion': 2434, 'force': [-0.9104146361351013, -0.6412608623504639, -1.7891393899917603], 'magnitude': 2.107389450073242, 'distance': 12.551528930664062, 'directional_contribution': -0.8100328801187882}, {'ion': 2436, 'force': [-3.1086254119873047, -2.0093727111816406, -3.0694339275360107], 'magnitude': 4.808591842651367, 'distance': 8.309216499328613, 'directional_contribution': -1.887990983593486}]}, 5359: {'frame': 5359, 'ionic_force': [-7.488657891750336, -9.668851613998413, -3.8453208655118942], 'ionic_force_magnitude': 12.82003046454787, 'motion_vector': [-0.3754844665527344, 0.34723663330078125, 0.0055084228515625], 'cosine_ionic_motion': -0.08642539269380385, 'ionic_motion_component': -1.1079761672450783, 'ionic_force_x': -7.488657891750336, 'ionic_force_y': -9.668851613998413, 'ionic_force_z': -3.8453208655118942, 'radial_force': 12.229746054321582, 'axial_force': -3.8453208655118942, 'contributions': [{'ion': 1309, 'force': [-3.55322265625, -1.968692660331726, 0.8038131594657898], 'magnitude': 4.140924453735352, 'distance': 8.95406723022461, 'directional_contribution': 1.2806561095230804}, {'ion': 1320, 'force': [-0.5556600689888, -5.521777629852295, -0.23913930356502533], 'magnitude': 5.554815292358398, 'distance': 7.730974197387695, 'directional_contribution': -3.3434406354042325}, {'ion': 2434, 'force': [-0.9361525774002075, -0.5566215515136719, -1.8760818243026733], 'magnitude': 2.169306993484497, 'distance': 12.37110710144043, 'directional_contribution': 0.2891660423462572}, {'ion': 2436, 'force': [-2.443622589111328, -1.6217597723007202, -2.5339128971099854], 'magnitude': 3.8758368492126465, 'distance': 9.255210876464844, 'directional_contribution': 0.6656424831540266}]}, 5360: {'frame': 5360, 'ionic_force': [-5.99063166975975, -12.09947857260704, -4.111779734492302], 'ionic_force_magnitude': 14.113531879607137, 'motion_vector': [0.4962959289550781, -1.1936683654785156, -0.0410003662109375], 'cosine_ionic_motion': 0.637564935265345, 'ionic_motion_component': 8.998293039187107, 'ionic_force_x': -5.99063166975975, 'ionic_force_y': -12.09947857260704, 'ionic_force_z': -4.111779734492302, 'radial_force': 13.50129806839718, 'axial_force': -4.111779734492302, 'contributions': [{'ion': 1309, 'force': [-1.7648735046386719, -0.8681292533874512, 0.4014160633087158], 'magnitude': 2.0073769092559814, 'distance': 12.860404014587402, 'directional_contribution': 0.11125925468247111}, {'ion': 1320, 'force': [-0.222377210855484, -9.145050048828125, 0.049248531460762024], 'magnitude': 9.147886276245117, 'distance': 6.024328708648682, 'directional_contribution': 8.35312313240585}, {'ion': 2434, 'force': [-0.8280560374259949, -0.4974512755870819, -1.6552377939224243], 'magnitude': 1.91649329662323, 'distance': 13.161803245544434, 'directional_contribution': 0.1938302006527346}, {'ion': 2436, 'force': [-3.1753249168395996, -1.5888479948043823, -2.9072065353393555], 'magnitude': 4.589005947113037, 'distance': 8.505693435668945, 'directional_contribution': 0.340080087499274}]}, 5361: {'frame': 5361, 'ionic_force': [-5.120174393057823, -19.02680516242981, -0.25727808475494385], 'ionic_force_magnitude': 19.705372174036345, 'motion_vector': [-0.574737548828125, 0.9560508728027344, -0.38732147216796875], 'cosine_ionic_motion': -0.6510080193920725, 'ionic_motion_component': -12.82835531040306, 'ionic_force_x': -5.120174393057823, 'ionic_force_y': -19.02680516242981, 'ionic_force_z': -0.25727808475494385, 'radial_force': 19.703692560136812, 'axial_force': -0.25727808475494385, 'contributions': [{'ion': 1309, 'force': [-1.4405096769332886, -0.9803712368011475, 0.35021817684173584], 'magnitude': 1.7773150205612183, 'distance': 13.667428970336914, 'directional_contribution': -0.2074942939315676}, {'ion': 1320, 'force': [0.1950037032365799, -15.115640640258789, 4.1602349281311035], 'magnitude': 15.678908348083496, 'distance': 4.601624011993408, 'directional_contribution': -13.69770373827267}, {'ion': 2434, 'force': [-0.9663851857185364, -0.6437287330627441, -2.0172598361968994], 'magnitude': 2.3275790214538574, 'distance': 11.943093299865723, 'directional_contribution': 0.6108454331708923}, {'ion': 2436, 'force': [-2.908283233642578, -2.287064552307129, -2.750471353530884], 'magnitude': 4.610191822052002, 'distance': 8.486127853393555, 'directional_contribution': 0.4659969298493891}]}, 5362: {'frame': 5362, 'ionic_force': [-2.3333985209465027, -17.115698158740997, 4.077326849102974], 'ionic_force_magnitude': 17.748703230182798, 'motion_vector': [0.4037361145019531, -0.2184600830078125, -0.226226806640625], 'cosine_ionic_motion': 0.2063827837405274, 'ionic_motion_component': 3.6630267804296164, 'ionic_force_x': -2.3333985209465027, 'ionic_force_y': -17.115698158740997, 'ionic_force_z': 4.077326849102974, 'radial_force': 17.274023043827555, 'axial_force': 4.077326849102974, 'contributions': [{'ion': 1309, 'force': [-1.5750622749328613, -0.9575368165969849, 0.24507339298725128], 'magnitude': 1.8595050573349, 'distance': 13.361966133117676, 'directional_contribution': -0.9421620101963057}, {'ion': 1320, 'force': [3.2834606170654297, -13.994690895080566, 8.046475410461426], 'magnitude': 16.473562240600586, 'distance': 4.489265441894531, 'directional_contribution': 5.007358344099799}, {'ion': 2434, 'force': [-0.9333657622337341, -0.5060002207756042, -1.6682040691375732], 'magnitude': 1.977400541305542, 'distance': 12.957514762878418, 'directional_contribution': 0.2170903667758015}, {'ion': 2436, 'force': [-3.108431100845337, -1.6574702262878418, -2.54601788520813], 'magnitude': 4.346465110778809, 'distance': 8.739789009094238, 'directional_contribution': -0.6192601042226045}]}, 5363: {'frame': 5363, 'ionic_force': [-4.615044325590134, -13.802704691886902, 2.612096294760704], 'ionic_force_magnitude': 14.786356481287097, 'motion_vector': [-0.16725540161132812, -0.3708457946777344, 0.30941009521484375], 'cosine_ionic_motion': 0.8863761547181133, 'ionic_motion_component': 13.106273800174508, 'ionic_force_x': -4.615044325590134, 'ionic_force_y': -13.802704691886902, 'ionic_force_z': 2.612096294760704, 'radial_force': 14.553806750764501, 'axial_force': 2.612096294760704, 'contributions': [{'ion': 1309, 'force': [-1.4222971200942993, -1.290872573852539, 0.12278829514980316], 'magnitude': 1.924670934677124, 'distance': 13.133811950683594, 'directional_contribution': 1.476375688362606}, {'ion': 1320, 'force': [0.3337534964084625, -10.261008262634277, 7.174679279327393], 'magnitude': 12.525003433227539, 'distance': 5.148492813110352, 'directional_contribution': 11.679136241201018}, {'ion': 2434, 'force': [-0.8723053932189941, -0.5652945041656494, -1.9188066720962524], 'magnitude': 2.182267904281616, 'distance': 12.334314346313477, 'directional_contribution': -0.4659707309890351}, {'ion': 2436, 'force': [-2.6541953086853027, -1.685529351234436, -2.7665646076202393], 'magnitude': 4.188035488128662, 'distance': 8.903563499450684, 'directional_contribution': 0.41673236184657725}]}, 5364: {'frame': 5364, 'ionic_force': [-5.364780865609646, -11.734835743904114, 1.9194905273616314], 'ionic_force_magnitude': 13.044987066189526, 'motion_vector': [0.7199592590332031, 0.047824859619140625, -0.00384521484375], 'cosine_ionic_motion': -0.47074968515216353, 'ionic_motion_component': -6.1409235542227645, 'ionic_force_x': -5.364780865609646, 'ionic_force_y': -11.734835743904114, 'ionic_force_z': 1.9194905273616314, 'radial_force': 12.90299359344261, 'axial_force': 1.9194905273616314, 'contributions': [{'ion': 1309, 'force': [-1.2786661386489868, -1.378605604171753, 0.06221873685717583], 'magnitude': 1.8813323974609375, 'distance': 13.284226417541504, 'directional_contribution': -1.3675419927947812}, {'ion': 1320, 'force': [-0.05913498252630234, -7.958459854125977, 6.173501968383789], 'magnitude': 10.072373390197754, 'distance': 5.741206169128418, 'directional_contribution': -0.6193910793836221}, {'ion': 2434, 'force': [-0.9266603589057922, -0.606224775314331, -1.7449246644973755], 'magnitude': 2.0666325092315674, 'distance': 12.674692153930664, 'directional_contribution': -0.9554913652822146}, {'ion': 2436, 'force': [-3.1003193855285645, -1.7915455102920532, -2.571305513381958], 'magnitude': 4.408313274383545, 'distance': 8.678262710571289, 'directional_contribution': -3.198499114070995}]}, 5365: {'frame': 5365, 'ionic_force': [-4.773198127746582, -14.88428270816803, 1.0287406668066978], 'ionic_force_magnitude': 15.664724685194285, 'motion_vector': [-0.7137031555175781, 0.053272247314453125, -0.5380477905273438], 'cosine_ionic_motion': 0.14688671051438024, 'ionic_motion_component': 2.3009398801215992, 'ionic_force_x': -4.773198127746582, 'ionic_force_y': -14.88428270816803, 'ionic_force_z': 1.0287406668066978, 'radial_force': 15.630908230278665, 'axial_force': 1.0287406668066978, 'contributions': [{'ion': 1309, 'force': [-0.9053996205329895, -1.410875916481018, 0.084062360227108], 'magnitude': 1.6785070896148682, 'distance': 14.06395435333252, 'directional_contribution': 0.5872326946989048}, {'ion': 1320, 'force': [0.3944142460823059, -10.42065715789795, 5.925753593444824], 'magnitude': 11.994174003601074, 'distance': 5.261188507080078, 'directional_contribution': -4.495258911100009}, {'ion': 2434, 'force': [-0.8353512287139893, -0.7200510501861572, -1.9241082668304443], 'magnitude': 2.217764139175415, 'distance': 12.235208511352539, 'directional_contribution': 1.7792402857389131}, {'ion': 2436, 'force': [-3.426861524581909, -2.3326985836029053, -3.05696702003479], 'magnitude': 5.150719165802002, 'distance': 8.028512954711914, 'directional_contribution': 4.429725728516766}]}, 5366: {'frame': 5366, 'ionic_force': [-7.155528903007507, -14.01739877462387, 7.555211916565895], 'ionic_force_magnitude': 17.457671362264268, 'motion_vector': [0.0323638916015625, -0.11964035034179688, 0.4410858154296875], 'cosine_ionic_motion': 0.5973538208346165, 'ionic_motion_component': 10.428406691123625, 'ionic_force_x': -7.155528903007507, 'ionic_force_y': -14.01739877462387, 'ionic_force_z': 7.555211916565895, 'radial_force': 15.738140369452886, 'axial_force': 7.555211916565895, 'contributions': [{'ion': 1309, 'force': [-1.2609608173370361, -1.393578290939331, -0.11961029469966888], 'magnitude': 1.8831859827041626, 'distance': 13.277687072753906, 'directional_contribution': 0.15967983512905182}, {'ion': 1320, 'force': [-2.2902896404266357, -10.353372573852539, 11.880364418029785], 'magnitude': 15.924220085144043, 'distance': 4.566042423248291, 'directional_contribution': 13.97919184290714}, {'ion': 2434, 'force': [-0.7939726114273071, -0.5141727328300476, -1.6001249551773071], 'magnitude': 1.8588076829910278, 'distance': 13.364472389221191, 'directional_contribution': -1.462285938092987}, {'ion': 2436, 'force': [-2.8103058338165283, -1.7562751770019531, -2.605417251586914], 'magnitude': 4.215509414672852, 'distance': 8.874502182006836, 'directional_contribution': -2.248178821084748}]}, 5367: {'frame': 5367, 'ionic_force': [-10.474521219730377, -7.64684385061264, -1.9239774346351624], 'ionic_force_magnitude': 13.110740056427767, 'motion_vector': [0.06612777709960938, -0.14238357543945312, 0.14096832275390625], 'cosine_ionic_motion': 0.045153985928468254, 'ionic_motion_component': 0.5920021720197445, 'ionic_force_x': -10.474521219730377, 'ionic_force_y': -7.64684385061264, 'ionic_force_z': -1.9239774346351624, 'radial_force': 12.968801627684583, 'axial_force': -1.9239774346351624, 'contributions': [{'ion': 1309, 'force': [-2.1570794582366943, -3.1891884803771973, 1.5716099739074707], 'magnitude': 4.158590316772461, 'distance': 8.935029029846191, 'directional_contribution': 2.5261146834102277}, {'ion': 1320, 'force': [-4.7571210861206055, -2.028890371322632, 0.9322972893714905], 'magnitude': 5.255071640014648, 'distance': 7.948400020599365, 'directional_contribution': 0.5010935265026362}, {'ion': 2434, 'force': [-0.8019500374794006, -0.6224215626716614, -1.7185429334640503], 'magnitude': 1.9959765672683716, 'distance': 12.897078514099121, 'directional_contribution': -0.9795050759979063}, {'ion': 2436, 'force': [-2.7583706378936768, -1.80634343624115, -2.7093417644500732], 'magnitude': 4.267553806304932, 'distance': 8.820221900939941, 'directional_contribution': -1.4557008757963885}]}, 5368: {'frame': 5368, 'ionic_force': [-7.8661617040634155, -5.908215522766113, -2.403372425585985], 'ionic_force_magnitude': 10.127176784968029, 'motion_vector': [-0.2716789245605469, 1.168243408203125, -0.486358642578125], 'cosine_ionic_motion': -0.27436994724357705, 'ionic_motion_component': -2.7785929602180564, 'ionic_force_x': -7.8661617040634155, 'ionic_force_y': -5.908215522766113, 'ionic_force_z': -2.403372425585985, 'radial_force': 9.837861079418042, 'axial_force': -2.403372425585985, 'contributions': [{'ion': 1309, 'force': [-1.2717992067337036, -1.4661600589752197, -0.025815505534410477], 'magnitude': 1.9410731792449951, 'distance': 13.078203201293945, 'directional_contribution': -1.0467292586320212}, {'ion': 1320, 'force': [-2.6795947551727295, -1.736313819885254, 2.1068739891052246], 'magnitude': 3.825432300567627, 'distance': 9.315985679626465, 'directional_contribution': -1.7964842439859154}, {'ion': 2434, 'force': [-0.9058058261871338, -0.6099779605865479, -1.7394031286239624], 'magnitude': 2.0537965297698975, 'distance': 12.714237213134766, 'directional_contribution': 0.29318300798421504}, {'ion': 2436, 'force': [-3.0089619159698486, -2.095763683319092, -2.745027780532837], 'magnitude': 4.580530166625977, 'distance': 8.513559341430664, 'directional_contribution': -0.22856246161882865}]}, 5369: {'frame': 5369, 'ionic_force': [-6.711408376693726, -4.462401032447815, -3.780743934214115], 'ionic_force_magnitude': 8.90224971955083, 'motion_vector': [0.5668296813964844, -0.4966011047363281, 0.5632095336914062], 'cosine_ionic_motion': -0.4438709940897048, 'ionic_motion_component': -3.951450432651823, 'ionic_force_x': -6.711408376693726, 'ionic_force_y': -4.462401032447815, 'ionic_force_z': -3.780743934214115, 'radial_force': 8.059530096298793, 'axial_force': -3.780743934214115, 'contributions': [{'ion': 1309, 'force': [-1.5613667964935303, -1.5342515707015991, -0.11372516304254532], 'magnitude': 2.1919689178466797, 'distance': 12.306989669799805, 'directional_contribution': -0.19894579554980885}, {'ion': 1320, 'force': [-2.044916868209839, -1.249974012374878, 0.6413288116455078], 'magnitude': 2.4810123443603516, 'distance': 11.567900657653809, 'directional_contribution': -0.18832669687147074}, {'ion': 2434, 'force': [-0.7636282444000244, -0.5087323188781738, -1.6250380277633667], 'magnitude': 1.8661953210830688, 'distance': 13.337992668151855, 'directional_contribution': -1.1643723905510441}, {'ion': 2436, 'force': [-2.341496467590332, -1.169443130493164, -2.683309555053711], 'magnitude': 3.748379945755005, 'distance': 9.411248207092285, 'directional_contribution': -2.3998056755567063}]}, 5370: {'frame': 5370, 'ionic_force': [-6.235943615436554, -5.78334653377533, -3.747200697660446], 'ionic_force_magnitude': 9.293847587150436, 'motion_vector': [-1.1579437255859375, -0.5086555480957031, -0.5385818481445312], 'cosine_ionic_motion': 0.9534337552821666, 'ionic_motion_component': 8.861068006036943, 'ionic_force_x': -6.235943615436554, 'ionic_force_y': -5.78334653377533, 'ionic_force_z': -3.747200697660446, 'radial_force': 8.50494502654985, 'axial_force': -3.747200697660446, 'contributions': [{'ion': 1309, 'force': [-1.6968252658843994, -0.9753545522689819, 0.14005836844444275], 'magnitude': 1.9621795415878296, 'distance': 13.007674217224121, 'directional_contribution': 1.7353743509200008}, {'ion': 1320, 'force': [-1.1757864952087402, -2.343637466430664, 0.33124250173568726], 'magnitude': 2.64288330078125, 'distance': 11.208049774169922, 'directional_contribution': 1.7278689909980471}, {'ion': 2434, 'force': [-0.7862456440925598, -0.6258909702301025, -1.6082265377044678], 'magnitude': 1.8963950872421265, 'distance': 13.231364250183105, 'directional_contribution': 1.5240011332923693}, {'ion': 2436, 'force': [-2.5770862102508545, -1.838463544845581, -2.6102750301361084], 'magnitude': 4.103030204772949, 'distance': 8.995321273803711, 'directional_contribution': 3.8738234694952425}]}, 5371: {'frame': 5371, 'ionic_force': [-8.769533276557922, -4.900592505931854, -2.362326404079795], 'ionic_force_magnitude': 10.319937346576516, 'motion_vector': [0.7847366333007812, 0.39499664306640625, 0.34635162353515625], 'cosine_ionic_motion': -0.9887204635221369, 'ionic_motion_component': -10.203533236826544, 'ionic_force_x': -8.769533276557922, 'ionic_force_y': -4.900592505931854, 'ionic_force_z': -2.362326404079795, 'radial_force': 10.04592060479537, 'axial_force': -2.362326404079795, 'contributions': [{'ion': 1309, 'force': [-2.0226423740386963, -0.7244314551353455, 0.016752222552895546], 'magnitude': 2.1485259532928467, 'distance': 12.430789947509766, 'directional_contribution': -1.9776472324573502}, {'ion': 1320, 'force': [-2.832592248916626, -1.997374415397644, 1.3567837476730347], 'magnitude': 3.7220888137817383, 'distance': 9.444428443908691, 'directional_contribution': -2.691667231942535}, {'ion': 2434, 'force': [-0.9106048345565796, -0.5352990627288818, -1.525680661201477], 'magnitude': 1.855652928352356, 'distance': 13.37582778930664, 'directional_contribution': -1.540161184435771}, {'ion': 2436, 'force': [-3.0036938190460205, -1.643487572669983, -2.210181713104248], 'magnitude': 4.075307369232178, 'distance': 9.02586555480957, 'directional_contribution': -3.9940575840646773}]}, 5372: {'frame': 5372, 'ionic_force': [-9.854567110538483, -9.004291117191315, -0.6223315000534058], 'ionic_force_magnitude': 13.363272352054937, 'motion_vector': [-0.04046630859375, 0.151031494140625, -0.122314453125], 'cosine_ionic_motion': -0.3336183449458439, 'ionic_motion_component': -4.458232805153123, 'ionic_force_x': -9.854567110538483, 'ionic_force_y': -9.004291117191315, 'ionic_force_z': -0.6223315000534058, 'radial_force': 13.348773406543284, 'axial_force': -0.6223315000534058, 'contrib</t>
+          <t>{5347: {'frame': 5347, 'ionic_force': [0.6853100061416626, -9.129887342453003, -11.733562916517258], 'ionic_force_magnitude': 14.88290937304499, 'motion_vector': [3.316211700439453, -1.65020751953125, -0.9902801513671875], 'cosine_ionic_motion': 0.5074709139954511, 'ionic_motion_component': 7.552643622450607, 'ionic_force_x': 0.6853100061416626, 'ionic_force_y': -9.129887342453003, 'ionic_force_z': -11.733562916517258, 'radial_force': 9.15557167469085, 'axial_force': -11.733562916517258, 'contributions': [{'ion': 1309, 'force': [-3.900376081466675, -0.4288240671157837, -0.44240328669548035], 'magnitude': 3.948739528656006, 'distance': 9.169376373291016, 'cosine_with_motion': -0.7786338398051467, 'motion_component': -3.0746222669723364}, {'ion': 1320, 'force': [5.2017621994018555, -9.052448272705078, -8.116565704345703], 'magnitude': 13.224363327026367, 'distance': 5.010506629943848, 'cosine_with_motion': 0.793340665917229, 'motion_component': 10.491425302286757}, {'ion': 2436, 'force': [-0.6160761117935181, 0.3513849973678589, -3.174593925476074], 'magnitude': 3.2528553009033203, 'distance': 10.102682113647461, 'cosine_with_motion': 0.04176044234126463, 'motion_component': 0.13584067736087846}]}, 5348: {'frame': 5348, 'ionic_force': [-2.9597952365875244, -4.185118928551674, -6.418415784835815], 'ionic_force_magnitude': 8.21411404082493, 'motion_vector': [1.4751319885253906, 0.6213607788085938, -1.0232925415039062], 'cosine_ionic_motion': -0.02554542998862456, 'ionic_motion_component': -0.20983307514847122, 'ionic_force_x': -2.9597952365875244, 'ionic_force_y': -4.185118928551674, 'ionic_force_z': -6.418415784835815, 'radial_force': 5.125973886848011, 'axial_force': -6.418415784835815, 'contributions': [{'ion': 1309, 'force': [-6.009511947631836, -2.5683140754699707, -1.4689178466796875], 'magnitude': 6.6983723640441895, 'distance': 7.04019021987915, 'cosine_with_motion': -0.7039018768949364, 'motion_component': -4.714996792595642}, {'ion': 1320, 'force': [2.708761215209961, -1.4557560682296753, -2.3566243648529053], 'magnitude': 3.874311685562134, 'distance': 9.25703239440918, 'cosine_with_motion': 0.7476143142621089, 'motion_component': 2.8964909137275363}, {'ion': 2436, 'force': [0.3409554958343506, -0.1610487848520279, -2.5928735733032227], 'magnitude': 2.6201491355895996, 'distance': 11.256568908691406, 'cosine_with_motion': 0.6139624104715719, 'motion_component': 1.6086729895284697}]}, 5349: {'frame': 5349, 'ionic_force': [-7.378105878829956, -6.646641850471497, -10.801924467086792], 'ionic_force_magnitude': 14.672963791964886, 'motion_vector': [-0.10723876953125, -1.5981407165527344, 3.5609359741210938], 'cosine_ionic_motion': -0.47216925748123195, 'ionic_motion_component': -6.9281224187010615, 'ionic_force_x': -7.378105878829956, 'ionic_force_y': -6.646641850471497, 'ionic_force_z': -10.801924467086792, 'radial_force': 9.93047301228216, 'axial_force': -10.801924467086792, 'contributions': [{'ion': 1309, 'force': [-10.252406120300293, -4.798220634460449, -6.5559773445129395], 'magnitude': 13.08111572265625, 'distance': 5.037866592407227, 'cosine_with_motion': -0.28541032674556904, 'motion_component': -3.733485544288841}, {'ion': 1320, 'force': [2.3740317821502686, -1.7368981838226318, -2.094464063644409], 'magnitude': 3.61104154586792, 'distance': 9.588546752929688, 'cosine_with_motion': -0.35015323973539414, 'motion_component': -1.2644179383602139}, {'ion': 2436, 'force': [0.5002684593200684, -0.11152303218841553, -2.1514830589294434], 'magnitude': 2.2116928100585938, 'distance': 12.25199031829834, 'cosine_with_motion': -0.872733684797831, 'motion_component': -1.9302188522429757}]}, 5350: {'frame': 5350, 'ionic_force': [-0.14506256580352783, -16.753881365060806, -3.0993531867861748], 'ionic_force_magnitude': 17.038766801590157, 'motion_vector': [2.5827255249023438, 0.7509269714355469, 2.464935302734375], 'cosine_ionic_motion': -0.33131159151419914, 'ionic_motion_component': -5.645140946474135, 'ionic_force_x': -0.14506256580352783, 'ionic_force_y': -16.753881365060806, 'ionic_force_z': -3.0993531867861748, 'radial_force': 16.754509361438465, 'axial_force': -3.0993531867861748, 'contributions': [{'ion': 1309, 'force': [-7.1796159744262695, -10.836474418640137, 3.318307876586914], 'magnitude': 13.415931701660156, 'distance': 4.974605083465576, 'cosine_with_motion': -0.3779898179059257, 'motion_component': -5.07108568105761}, {'ion': 1320, 'force': [5.264742851257324, -4.707367897033691, -0.06457030028104782], 'magnitude': 7.062648296356201, 'distance': 6.856228351593018, 'cosine_with_motion': 0.3843443305678448, 'motion_component': 2.714488781801923}, {'ion': 2434, 'force': [0.3296545743942261, -0.23305991291999817, -1.7742886543273926], 'magnitude': 1.8196399211883545, 'distance': 13.50754165649414, 'cosine_with_motion': -0.5569081574761272, 'motion_component': -1.0133722924457365}, {'ion': 2436, 'force': [1.4401559829711914, -0.97697913646698, -4.578802108764648], 'magnitude': 4.8983635902404785, 'distance': 8.232723236083984, 'cosine_with_motion': -0.4644758616720765, 'motion_component': -2.2751716672537476}]}, 5351: {'frame': 5351, 'ionic_force': [6.5781702399253845, -10.670942857861519, 6.412924081087112], 'ionic_force_magnitude': 14.080729400530808, 'motion_vector': [-4.924442291259766, -0.13016128540039062, 1.0756683349609375], 'cosine_ionic_motion': -0.3395388214293875, 'ionic_motion_component': -4.7809542655223565, 'ionic_force_x': 6.5781702399253845, 'ionic_force_y': -10.670942857861519, 'ionic_force_z': 6.412924081087112, 'radial_force': 12.535603104006832, 'axial_force': 6.412924081087112, 'contributions': [{'ion': 1309, 'force': [-0.7276131510734558, -8.576908111572266, 12.734542846679688], 'magnitude': 15.370795249938965, 'distance': 4.647515773773193, 'cosine_with_motion': 0.23737887367365, 'motion_component': 3.648702129922416}, {'ion': 1320, 'force': [2.105349540710449, -1.2945811748504639, 0.18129947781562805], 'magnitude': 2.478165864944458, 'distance': 11.574542999267578, 'cosine_with_motion': -0.8006204730018646, 'motion_component': -1.984070416350552}, {'ion': 2434, 'force': [1.0735446214675903, -0.11892910301685333, -2.175081729888916], 'magnitude': 2.428502082824707, 'distance': 11.692296028137207, 'cosine_with_motion': -0.6215390624157976, 'motion_component': -1.5094089525808843}, {'ion': 2436, 'force': [4.126889228820801, -0.680524468421936, -4.327836513519287], 'magnitude': 6.018678665161133, 'distance': 7.427085876464844, 'cosine_with_motion': -0.8201429451411554, 'motion_component': -4.93617713739299}]}, 5352: {'frame': 5352, 'ionic_force': [9.924710154533386, -10.801763534545898, -9.8836290538311], 'ionic_force_magnitude': 17.687964562986828, 'motion_vector': [1.6225547790527344, 0.3573951721191406, -0.7139053344726562], 'cosine_ionic_motion': 0.6033578075989015, 'ionic_motion_component': 10.672171519610794, 'ionic_force_x': 9.924710154533386, 'ionic_force_y': -10.801763534545898, 'ionic_force_z': -9.8836290538311, 'radial_force': 14.668945671306565, 'axial_force': -9.8836290538311, 'contributions': [{'ion': 1309, 'force': [5.455544471740723, -4.775212287902832, 4.03164005279541], 'magnitude': 8.295766830444336, 'distance': 6.326169013977051, 'cosine_with_motion': 0.28444257656282923, 'motion_component': 2.359669156171975}, {'ion': 1320, 'force': [3.4328699111938477, -2.7567880153656006, 0.24743130803108215], 'magnitude': 4.409727573394775, 'distance': 8.676871299743652, 'cosine_with_motion': 0.5527925122176478, 'motion_component': 2.4376644442580866}, {'ion': 2434, 'force': [0.07548081874847412, -0.4966468811035156, -2.923949956893921], 'magnitude': 2.9667892456054688, 'distance': 10.57853889465332, 'cosine_with_motion': 0.37882856508898916, 'motion_component': 1.1239045384416073}, {'ion': 2436, 'force': [0.9608149528503418, -2.77311635017395, -11.238750457763672], 'magnitude': 11.615629196166992, 'distance': 5.346230506896973, 'cosine_with_motion': 0.4090121636963402, 'motion_component': 4.750933804418082}]}, 5353: {'frame': 5353, 'ionic_force': [11.046917110681534, -10.955666691064835, -16.785257935523987], 'ionic_force_magnitude': 22.88680611745656, 'motion_vector': [-1.0786094665527344, -0.3579292297363281, -0.06634521484375], 'cosine_ionic_motion': -0.2640805144456472, 'ionic_motion_component': -6.043959533515713, 'ionic_force_x': 11.046917110681534, 'ionic_force_y': -10.955666691064835, 'ionic_force_z': -16.785257935523987, 'radial_force': 15.558310007708934, 'axial_force': -16.785257935523987, 'contributions': [{'ion': 1309, 'force': [0.8205000758171082, -5.329401016235352, 1.1785228252410889], 'magnitude': 5.519479274749756, 'distance': 7.755681991577148, 'cosine_with_motion': 0.15029737672327664, 'motion_component': 0.8295632579359236}, {'ion': 1320, 'force': [3.7472195625305176, -2.678145170211792, 0.29563629627227783], 'magnitude': 4.615356922149658, 'distance': 8.481377601623535, 'cosine_with_motion': -0.5905579328226201, 'motion_component': -2.7256354706602135}, {'ion': 2434, 'force': [0.39906546473503113, -0.3938721716403961, -2.652449131011963], 'magnitude': 2.7110652923583984, 'distance': 11.066213607788086, 'cosine_with_motion': -0.0367698516531741, 'motion_component': -0.09968546798404}, {'ion': 2436, 'force': [6.080132007598877, -2.554248332977295, -15.60696792602539], 'magnitude': 16.943130493164062, 'distance': 4.426620006561279, 'cosine_with_motion': -0.23892883827431421, 'motion_component': -4.0482022507508475}]}, 5354: {'frame': 5354, 'ionic_force': [-0.8884754180908203, -10.587919175624847, -4.579100914299488], 'ionic_force_magnitude': 11.569856793472182, 'motion_vector': [-1.3265037536621094, 1.3291473388671875, 1.2285842895507812], 'cosine_ionic_motion': -0.7133261353379372, 'ionic_motion_component': -8.25308123290089, 'ionic_force_x': -0.8884754180908203, 'ionic_force_y': -10.587919175624847, 'ionic_force_z': -4.579100914299488, 'radial_force': 10.62513157744957, 'axial_force': -4.579100914299488, 'contributions': [{'ion': 1309, 'force': [-6.627227306365967, -5.314355373382568, 7.1092095375061035], 'magnitude': 11.077156066894531, 'distance': 5.4746317863464355, 'cosine_with_motion': 0.4208694645766861, 'motion_component': 4.662036524869421}, {'ion': 1320, 'force': [3.325421094894409, -3.054407835006714, 0.12004440277814865], 'magnitude': 4.5168843269348145, 'distance': 8.573330879211426, 'cosine_with_motion': -0.8211762565733415, 'motion_component': -3.709158100849936}, {'ion': 2434, 'force': [0.26523327827453613, -0.28264373540878296, -2.6325316429138184], 'magnitude': 2.6609132289886475, 'distance': 11.170013427734375, 'cosine_with_motion': -0.6634877643934309, 'motion_component': -1.7654833460838617}, {'ion': 2436, 'force': [2.148097515106201, -1.9365122318267822, -9.175823211669922], 'magnitude': 9.620818138122559, 'distance': 5.874393939971924, 'cosine_with_motion': -0.773372547498979, 'motion_component': -7.440476332000287}]}, 5355: {'frame': 5355, 'ionic_force': [-1.0782689899206161, -3.377299338579178, -19.434728145599365], 'ionic_force_magnitude': 19.755441603020266, 'motion_vector': [-0.3754844665527344, 2.017047882080078, -2.8304595947265625], 'cosine_ionic_motion': 0.7037424023399148, 'ionic_motion_component': 13.90274193299538, 'ionic_force_x': -1.0782689899206161, 'ionic_force_y': -3.377299338579178, 'ionic_force_z': -19.434728145599365, 'radial_force': 3.5452524362859945, 'axial_force': -19.434728145599365, 'contributions': [{'ion': 1309, 'force': [-4.155211925506592, -0.5779337286949158, 3.243894577026367], 'magnitude': 5.303078651428223, 'distance': 7.912341117858887, 'cosine_with_motion': -0.4739911959579365, 'motion_component': -2.5136126988026177}, {'ion': 1320, 'force': [5.40611457824707, -3.8656556606292725, 1.663935661315918], 'magnitude': 6.851134777069092, 'distance': 6.961258888244629, 'cosine_with_motion': -0.6069518120289323, 'motion_component': -4.15830878571586}, {'ion': 2434, 'force': [-0.2116548866033554, 0.1417645514011383, -3.8158822059631348], 'magnitude': 3.824375867843628, 'distance': 9.31727123260498, 'cosine_with_motion': 0.835196737960166, 'motion_component': 3.1941063817137327}, {'ion': 2436, 'force': [-2.1175167560577393, 0.9245254993438721, -20.526676177978516], 'magnitude': 20.656307220458984, 'distance': 4.009061336517334, 'cosine_with_motion': 0.8414164330538239, 'motion_component': 17.380556983894365}]}, 5356: {'frame': 5356, 'ionic_force': [9.193988606333733, -9.341656267642975, -8.68997049331665], 'ionic_force_magnitude': 15.726142422441105, 'motion_vector': [-5.566600799560547, -5.137775421142578, 0.14322662353515625], 'cosine_ionic_motion': -0.03716797145292092, 'ionic_motion_component': -0.5845088126218596, 'ionic_force_x': 9.193988606333733, 'ionic_force_y': -9.341656267642975, 'ionic_force_z': -8.68997049331665, 'radial_force': 13.107096105399846, 'axial_force': -8.68997049331665, 'contributions': [{'ion': 1309, 'force': [-5.083637714385986, 1.7815605401992798, 4.272593021392822], 'magnitude': 6.875491142272949, 'distance': 6.948917865753174, 'cosine_with_motion': 0.37927224489761086, 'motion_component': 2.6076830443856958}, {'ion': 1320, 'force': [15.738530158996582, -14.13753890991211, -3.5142836570739746], 'magnitude': 21.44577980041504, 'distance': 3.934577465057373, 'cosine_with_motion': -0.09525757946206342, 'motion_component': -2.042873198654397}, {'ion': 2434, 'force': [-0.2095593959093094, 0.4638260006904602, -2.334017753601074], 'magnitude': 2.3888676166534424, 'distance': 11.788891792297363, 'cosine_with_motion': -0.08568202920856213, 'motion_component': -0.20468302640401867}, {'ion': 2436, 'force': [-1.2513444423675537, 2.5504961013793945, -7.114262104034424], 'magnitude': 7.660523414611816, 'distance': 6.583241939544678, 'cosine_with_motion': -0.12331218202884321, 'motion_component': -0.9446358543236686}]}, 5357: {'frame': 5357, 'ionic_force': [-6.36072164773941, -7.776129573583603, -3.584123432636261], 'ionic_force_magnitude': 10.666438571779926, 'motion_vector': [1.0815353393554688, -1.1651802062988281, 1.2048263549804688], 'cosine_ionic_motion': -0.10043836085855601, 'ionic_motion_component': -1.071319606348053, 'ionic_force_x': -6.36072164773941, 'ionic_force_y': -7.776129573583603, 'ionic_force_z': -3.584123432636261, 'radial_force': 10.046241636810368, 'axial_force': -3.584123432636261, 'contributions': [{'ion': 1309, 'force': [-1.7606245279312134, -0.44900551438331604, 1.1280972957611084], 'magnitude': 2.13869309425354, 'distance': 12.459333419799805, 'cosine_with_motion': -0.005120338601344486, 'motion_component': -0.010950832851939651}, {'ion': 1320, 'force': [-1.3347965478897095, -6.032811641693115, -0.6402768492698669], 'magnitude': 6.211799621582031, 'distance': 7.310723304748535, 'cosine_with_motion': 0.38853205719115985, 'motion_component': 2.4134832243306086}, {'ion': 2434, 'force': [-0.9485629200935364, -0.36116552352905273, -1.7239831686019897], 'magnitude': 2.000582456588745, 'distance': 12.882223129272461, 'cosine_with_motion': -0.6721193525377495, 'motion_component': -1.344630176815933}, {'ion': 2436, 'force': [-2.316737651824951, -0.9331468939781189, -2.3479607105255127], 'magnitude': 3.427966594696045, 'distance': 9.84126091003418, 'cosine_with_motion': -0.6211325241080135, 'motion_component': -2.129221633842434}]}, 5358: {'frame': 5358, 'ionic_force': [-8.373949587345123, -10.114233255386353, -2.16071218252182], 'ionic_force_magnitude': 13.307494999866014, 'motion_vector': [-0.13986587524414062, 0.56707763671875, 0.13983154296875], 'cosine_ionic_motion': -0.6089035342787845, 'ionic_motion_component': -8.102980737815669, 'ionic_force_x': -8.373949587345123, 'ionic_force_y': -10.114233255386353, 'ionic_force_z': -2.16071218252182, 'radial_force': 13.130908043077628, 'axial_force': -2.16071218252182, 'contributions': [{'ion': 1309, 'force': [-2.585419178009033, -2.5263538360595703, 2.679021120071411], 'magnitude': 4.499334335327148, 'distance': 8.590034484863281, 'cosine_with_motion': -0.2577219996351968, 'motion_component': -1.1595774628844175}, {'ion': 1320, 'force': [-1.769490361213684, -4.937245845794678, 0.018840014934539795], 'magnitude': 5.244792461395264, 'distance': 7.956185340881348, 'cosine_with_motion': -0.8094466141356852, 'motion_component': -4.245379473738665}, {'ion': 2434, 'force': [-0.9104146361351013, -0.6412608623504639, -1.7891393899917603], 'magnitude': 2.107389450073242, 'distance': 12.551528930664062, 'cosine_with_motion': -0.3843774113266263, 'motion_component': -0.8100328801187882}, {'ion': 2436, 'force': [-3.1086254119873047, -2.0093727111816406, -3.0694339275360107], 'magnitude': 4.808591842651367, 'distance': 8.309216499328613, 'cosine_with_motion': -0.39262866442624267, 'motion_component': -1.887990983593486}]}, 5359: {'frame': 5359, 'ionic_force': [-7.488657891750336, -9.668851613998413, -3.8453208655118942], 'ionic_force_magnitude': 12.82003046454787, 'motion_vector': [-0.3754844665527344, 0.34723663330078125, 0.0055084228515625], 'cosine_ionic_motion': -0.08642539269380385, 'ionic_motion_component': -1.1079761672450783, 'ionic_force_x': -7.488657891750336, 'ionic_force_y': -9.668851613998413, 'ionic_force_z': -3.8453208655118942, 'radial_force': 12.229746054321582, 'axial_force': -3.8453208655118942, 'contributions': [{'ion': 1309, 'force': [-3.55322265625, -1.968692660331726, 0.8038131594657898], 'magnitude': 4.140924453735352, 'distance': 8.95406723022461, 'cosine_with_motion': 0.3092681448214228, 'motion_component': 1.2806561095230804}, {'ion': 1320, 'force': [-0.5556600689888, -5.521777629852295, -0.23913930356502533], 'magnitude': 5.554815292358398, 'distance': 7.730974197387695, 'cosine_with_motion': -0.6018995063443169, 'motion_component': -3.3434406354042325}, {'ion': 2434, 'force': [-0.9361525774002075, -0.5566215515136719, -1.8760818243026733], 'magnitude': 2.169306993484497, 'distance': 12.37110710144043, 'cosine_with_motion': 0.133298819524226, 'motion_component': 0.2891660423462572}, {'ion': 2436, 'force': [-2.443622589111328, -1.6217597723007202, -2.5339128971099854], 'magnitude': 3.8758368492126465, 'distance': 9.255210876464844, 'cosine_with_motion': 0.1717416192223846, 'motion_component': 0.6656424831540266}]}, 5360: {'frame': 5360, 'ionic_force': [-5.99063166975975, -12.09947857260704, -4.111779734492302], 'ionic_force_magnitude': 14.113531879607137, 'motion_vector': [0.4962959289550781, -1.1936683654785156, -0.0410003662109375], 'cosine_ionic_motion': 0.637564935265345, 'ionic_motion_component': 8.998293039187107, 'ionic_force_x': -5.99063166975975, 'ionic_force_y': -12.09947857260704, 'ionic_force_z': -4.111779734492302, 'radial_force': 13.50129806839718, 'axial_force': -4.111779734492302, 'contributions': [{'ion': 1309, 'force': [-1.7648735046386719, -0.8681292533874512, 0.4014160633087158], 'magnitude': 2.0073769092559814, 'distance': 12.860404014587402, 'cosine_with_motion': 0.05542519617332915, 'motion_component': 0.11125925468247111}, {'ion': 1320, 'force': [-0.222377210855484, -9.145050048828125, 0.049248531460762024], 'magnitude': 9.147886276245117, 'distance': 6.024328708648682, 'cosine_with_motion': 0.9131206022804962, 'motion_component': 8.35312313240585}, {'ion': 2434, 'force': [-0.8280560374259949, -0.4974512755870819, -1.6552377939224243], 'magnitude': 1.91649329662323, 'distance': 13.161803245544434, 'cosine_with_motion': 0.10113794630997673, 'motion_component': 0.1938302006527346}, {'ion': 2436, 'force': [-3.1753249168395996, -1.5888479948043823, -2.9072065353393555], 'magnitude': 4.589005947113037, 'distance': 8.505693435668945, 'cosine_with_motion': 0.074107570812104, 'motion_component': 0.340080087499274}]}, 5361: {'frame': 5361, 'ionic_force': [-5.120174393057823, -19.02680516242981, -0.25727808475494385], 'ionic_force_magnitude': 19.705372174036345, 'motion_vector': [-0.574737548828125, 0.9560508728027344, -0.38732147216796875], 'cosine_ionic_motion': -0.6510080193920725, 'ionic_motion_component': -12.82835531040306, 'ionic_force_x': -5.120174393057823, 'ionic_force_y': -19.02680516242981, 'ionic_force_z': -0.25727808475494385, 'radial_force': 19.703692560136812, 'axial_force': -0.25727808475494385, 'contributions': [{'ion': 1309, 'force': [-1.4405096769332886, -0.9803712368011475, 0.35021817684173584], 'magnitude': 1.7773150205612183, 'distance': 13.667428970336914, 'cosine_with_motion': -0.1167459297738805, 'motion_component': -0.2074942939315676}, {'ion': 1320, 'force': [0.1950037032365799, -15.115640640258789, 4.1602349281311035], 'magnitude': 15.678908348083496, 'distance': 4.601624011993408, 'cosine_with_motion': -0.8736388570428829, 'motion_component': -13.69770373827267}, {'ion': 2434, 'force': [-0.9663851857185364, -0.6437287330627441, -2.0172598361968994], 'magnitude': 2.3275790214538574, 'distance': 11.943093299865723, 'cosine_with_motion': 0.2624381036375999, 'motion_component': 0.6108454331708925}, {'ion': 2436, 'force': [-2.908283233642578, -2.287064552307129, -2.750471353530884], 'magnitude': 4.610191822052002, 'distance': 8.486127853393555, 'cosine_with_motion': 0.10107972759484486, 'motion_component': 0.4659969298493891}]}, 5362: {'frame': 5362, 'ionic_force': [-2.3333985209465027, -17.115698158740997, 4.077326849102974], 'ionic_force_magnitude': 17.748703230182798, 'motion_vector': [0.4037361145019531, -0.2184600830078125, -0.226226806640625], 'cosine_ionic_motion': 0.2063827837405274, 'ionic_motion_component': 3.6630267804296164, 'ionic_force_x': -2.3333985209465027, 'ionic_force_y': -17.115698158740997, 'ionic_force_z': 4.077326849102974, 'radial_force': 17.274023043827555, 'axial_force': 4.077326849102974, 'contributions': [{'ion': 1309, 'force': [-1.5750622749328613, -0.9575368165969849, 0.24507339298725128], 'magnitude': 1.8595050573349, 'distance': 13.361966133117676, 'cosine_with_motion': -0.5066735521869951, 'motion_component': -0.9421620101963059}, {'ion': 1320, 'force': [3.2834606170654297, -13.994690895080566, 8.046475410461426], 'magnitude': 16.473562240600586, 'distance': 4.489265441894531, 'cosine_with_motion': 0.3039632998783835, 'motion_component': 5.007358344099799}, {'ion': 2434, 'force': [-0.9333657622337341, -0.5060002207756042, -1.6682040691375732], 'magnitude': 1.977400541305542, 'distance': 12.957514762878418, 'cosine_with_motion': 0.1097857354681624, 'motion_component': 0.2170903667758015}, {'ion': 2436, 'force': [-3.108431100845337, -1.6574702262878418, -2.54601788520813], 'magnitude': 4.346465110778809, 'distance': 8.739789009094238, 'cosine_with_motion': -0.14247442357158616, 'motion_component': -0.6192601042226045}]}, 5363: {'frame': 5363, 'ionic_force': [-4.615044325590134, -13.802704691886902, 2.612096294760704], 'ionic_force_magnitude': 14.786356481287097, 'motion_vector': [-0.16725540161132812, -0.3708457946777344, 0.30941009521484375], 'cosine_ionic_motion': 0.8863761547181133, 'ionic_motion_component': 13.106273800174508, 'ionic_force_x': -4.615044325590134, 'ionic_force_y': -13.802704691886902, 'ionic_force_z': 2.612096294760704, 'radial_force': 14.553806750764501, 'axial_force': 2.612096294760704, 'contributions': [{'ion': 1309, 'force': [-1.4222971200942993, -1.290872573852539, 0.12278829514980316], 'magnitude': 1.924670934677124, 'distance': 13.133811950683594, 'cosine_with_motion': 0.7670795510974251, 'motion_component': 1.476375688362606}, {'ion': 1320, 'force': [0.3337534964084625, -10.261008262634277, 7.174679279327393], 'magnitude': 12.525003433227539, 'distance': 5.148492813110352, 'cosine_with_motion': 0.9324657304241323, 'motion_component': 11.679136241201018}, {'ion': 2434, 'force': [-0.8723053932189941, -0.5652945041656494, -1.9188066720962524], 'magnitude': 2.182267904281616, 'distance': 12.334314346313477, 'cosine_with_motion': -0.2135258965253157, 'motion_component': -0.4659707309890351}, {'ion': 2436, 'force': [-2.6541953086853027, -1.685529351234436, -2.7665646076202393], 'magnitude': 4.188035488128662, 'distance': 8.903563499450684, 'cosine_with_motion': 0.09950545026923256, 'motion_component': 0.41673236184657725}]}, 5364: {'frame': 5364, 'ionic_force': [-5.364780865609646, -11.734835743904114, 1.9194905273616314], 'ionic_force_magnitude': 13.044987066189526, 'motion_vector': [0.7199592590332031, 0.047824859619140625, -0.00384521484375], 'cosine_ionic_motion': -0.47074968515216353, 'ionic_motion_component': -6.1409235542227645, 'ionic_force_x': -5.364780865609646, 'ionic_force_y': -11.734835743904114, 'ionic_force_z': 1.9194905273616314, 'radial_force': 12.90299359344261, 'axial_force': 1.9194905273616314, 'contributions': [{'ion': 1309, 'force': [-1.2786661386489868, -1.378605604171753, 0.06221873685717583], 'magnitude': 1.8813323974609375, 'distance': 13.284226417541504, 'cosine_with_motion': -0.7269007740173844, 'motion_component': -1.3675419927947812}, {'ion': 1320, 'force': [-0.05913498252630234, -7.958459854125977, 6.173501968383789], 'magnitude': 10.072373390197754, 'distance': 5.741206169128418, 'cosine_with_motion': -0.061494054302821094, 'motion_component': -0.6193910793836221}, {'ion': 2434, 'force': [-0.9266603589057922, -0.606224775314331, -1.7449246644973755], 'magnitude': 2.0666325092315674, 'distance': 12.674692153930664, 'cosine_with_motion': -0.462342170077388, 'motion_component': -0.9554913652822146}, {'ion': 2436, 'force': [-3.1003193855285645, -1.7915455102920532, -2.571305513381958], 'magnitude': 4.408313274383545, 'distance': 8.678262710571289, 'cosine_with_motion': -0.7255607242424008, 'motion_component': -3.198499114070995}]}, 5365: {'frame': 5365, 'ionic_force': [-4.773198127746582, -14.88428270816803, 1.0287406668066978], 'ionic_force_magnitude': 15.664724685194285, 'motion_vector': [-0.7137031555175781, 0.053272247314453125, -0.5380477905273438], 'cosine_ionic_motion': 0.14688671051438024, 'ionic_motion_component': 2.3009398801215992, 'ionic_force_x': -4.773198127746582, 'ionic_force_y': -14.88428270816803, 'ionic_force_z': 1.0287406668066978, 'radial_force': 15.630908230278665, 'axial_force': 1.0287406668066978, 'contributions': [{'ion': 1309, 'force': [-0.9053996205329895, -1.410875916481018, 0.084062360227108], 'magnitude': 1.6785070896148682, 'distance': 14.06395435333252, 'cosine_with_motion': 0.3498541792620414, 'motion_component': 0.5872326946989048}, {'ion': 1320, 'force': [0.3944142460823059, -10.42065715789795, 5.925753593444824], 'magnitude': 11.994174003601074, 'distance': 5.261188507080078, 'cosine_with_motion': -0.37478686319241056, 'motion_component': -4.495258911100009}, {'ion': 2434, 'force': [-0.8353512287139893, -0.7200510501861572, -1.9241082668304443], 'magnitude': 2.217764139175415, 'distance': 12.235208511352539, 'cosine_with_motion': 0.8022675846631492, 'motion_component': 1.7792402857389131}, {'ion': 2436, 'force': [-3.426861524581909, -2.3326985836029053, -3.05696702003479], 'magnitude': 5.150719165802002, 'distance': 8.028512954711914, 'cosine_with_motion': 0.8600207886859776, 'motion_component': 4.429725728516766}]}, 5366: {'frame': 5366, 'ionic_force': [-7.155528903007507, -14.01739877462387, 7.555211916565895], 'ionic_force_magnitude': 17.457671362264268, 'motion_vector': [0.0323638916015625, -0.11964035034179688, 0.4410858154296875], 'cosine_ionic_motion': 0.5973538208346165, 'ionic_motion_component': 10.428406691123625, 'ionic_force_x': -7.155528903007507, 'ionic_force_y': -14.01739877462387, 'ionic_force_z': 7.555211916565895, 'radial_force': 15.738140369452886, 'axial_force': 7.555211916565895, 'contributions': [{'ion': 1309, 'force': [-1.2609608173370361, -1.393578290939331, -0.11961029469966888], 'magnitude': 1.8831859827041626, 'distance': 13.277687072753906, 'cosine_with_motion': 0.08479238949629006, 'motion_component': 0.15967983512905182}, {'ion': 1320, 'force': [-2.2902896404266357, -10.353372573852539, 11.880364418029785], 'magnitude': 15.924220085144043, 'distance': 4.566042423248291, 'cosine_with_motion': 0.8778571958683916, 'motion_component': 13.97919184290714}, {'ion': 2434, 'force': [-0.7939726114273071, -0.5141727328300476, -1.6001249551773071], 'magnitude': 1.8588076829910278, 'distance': 13.364472389221191, 'cosine_with_motion': -0.7866795238692053, 'motion_component': -1.462285938092987}, {'ion': 2436, 'force': [-2.8103058338165283, -1.7562751770019531, -2.605417251586914], 'magnitude': 4.215509414672852, 'distance': 8.874502182006836, 'cosine_with_motion': -0.5333112914507774, 'motion_component': -2.248178821084748}]}, 5367: {'frame': 5367, 'ionic_force': [-10.474521219730377, -7.64684385061264, -1.9239774346351624], 'ionic_force_magnitude': 13.110740056427767, 'motion_vector': [0.06612777709960938, -0.14238357543945312, 0.14096832275390625], 'cosine_ionic_motion': 0.045153985928468254, 'ionic_motion_component': 0.5920021720197445, 'ionic_force_x': -10.474521219730377, 'ionic_force_y': -7.64684385061264, 'ionic_force_z': -1.9239774346351624, 'radial_force': 12.968801627684583, 'axial_force': -1.9239774346351624, 'contributions': [{'ion': 1309, 'force': [-2.1570794582366943, -3.1891884803771973, 1.5716099739074707], 'magnitude': 4.158590316772461, 'distance': 8.935029029846191, 'cosine_with_motion': 0.6074449589642145, 'motion_component': 2.5261146834102273}, {'ion': 1320, 'force': [-4.7571210861206055, -2.028890371322632, 0.9322972893714905], 'magnitude': 5.255071640014648, 'distance': 7.948400020599365, 'cosine_with_motion': 0.09535427561499123, 'motion_component': 0.5010935265026362}, {'ion': 2434, 'force': [-0.8019500374794006, -0.6224215626716614, -1.7185429334640503], 'magnitude': 1.9959765672683716, 'distance': 12.897078514099121, 'cosine_with_motion': -0.4907397782220592, 'motion_component': -0.9795050759979063}, {'ion': 2436, 'force': [-2.7583706378936768, -1.80634343624115, -2.7093417644500732], 'magnitude': 4.267553806304932, 'distance': 8.820221900939941, 'cosine_with_motion': -0.34110894490204924, 'motion_component': -1.4557008757963885}]}, 5368: {'frame': 5368, 'ionic_force': [-7.8661617040634155, -5.908215522766113, -2.403372425585985], 'ionic_force_magnitude': 10.127176784968029, 'motion_vector': [-0.2716789245605469, 1.168243408203125, -0.486358642578125], 'cosine_ionic_motion': -0.27436994724357705, 'ionic_motion_component': -2.7785929602180564, 'ionic_force_x': -7.8661617040634155, 'ionic_force_y': -5.908215522766113, 'ionic_force_z': -2.403372425585985, 'radial_force': 9.837861079418042, 'axial_force': -2.403372425585985, 'contributions': [{'ion': 1309, 'force': [-1.2717992067337036, -1.4661600589752197, -0.025815505534410477], 'magnitude': 1.9410731792449951, 'distance': 13.078203201293945, 'cosine_with_motion': -0.5392528651463202, 'motion_component': -1.0467292586320212}, {'ion': 1320, 'force': [-2.6795947551727295, -1.736313819885254, 2.1068739891052246], 'magnitude': 3.825432300567627, 'distance': 9.315985679626465, 'cosine_with_motion': -0.4696160162881312, 'motion_component': -1.7964842439859154}, {'ion': 2434, 'force': [-0.9058058261871338, -0.6099779605865479, -1.7394031286239624], 'magnitude': 2.0537965297698975, 'distance': 12.714237213134766, 'cosine_with_motion': 0.14275172396010247, 'motion_component': 0.29318300798421504}, {'ion': 2436, 'force': [-3.0089619159698486, -2.095763683319092, -2.745027780532837], 'magnitude': 4.580530166625977, 'distance': 8.513559341430664, 'cosine_with_motion': -0.049898693700076234, 'motion_component': -0.22856246161882865}]}, 5369: {'frame': 5369, 'ionic_force': [-6.711408376693726, -4.462401032447815, -3.780743934214115], 'ionic_force_magnitude': 8.90224971955083, 'motion_vector': [0.5668296813964844, -0.4966011047363281, 0.5632095336914062], 'cosine_ionic_motion': -0.4438709940897048, 'ionic_motion_component': -3.951450432651823, 'ionic_force_x': -6.711408376693726, 'ionic_force_y': -4.462401032447815, 'ionic_force_z': -3.780743934214115, 'radial_force': 8.059530096298793, 'axial_force': -3.780743934214115, 'contributions': [{'ion': 1309, 'force': [-1.5613667964935303, -1.5342515707015991, -0.11372516304254532], 'magnitude': 2.1919689178466797, 'distance': 12.306989669799805, 'cosine_with_motion': -0.09076123179609208, 'motion_component': -0.19894579554980885}, {'ion': 1320, 'force': [-2.044916868209839, -1.249974012374878, 0.6413288116455078], 'magnitude': 2.4810123443603516, 'distance': 11.567900657653809, 'cosine_with_motion': -0.07590719605042631, 'motion_component': -0.18832669687147074}, {'ion': 2434, 'force': [-0.7636282444000244, -0.5087323188781738, -1.6250380277633667], 'magnitude': 1.8661953210830688, 'distance': 13.337992668151855, 'cosine_with_motion': -0.623928444178269, 'motion_component': -1.1643723905510441}, {'ion': 2436, 'force': [-2.341496467590332, -1.169443130493164, -2.683309555053711], 'magnitude': 3.748379945755005, 'distance': 9.411248207092285, 'cosine_with_motion': -0.6402247461472825, 'motion_component': -2.3998056755567063}]}, 5370: {'frame': 5370, 'ionic_force'</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{5415: {'frame': 5415, 'ionic_force': [-0.86297807097435, 12.021617323160172, -7.310816407203674], 'ionic_force_magnitude': 14.096526194609996, 'motion_vector': [-0.3487205505371094, 3.4752159118652344, 0.6145477294921875], 'cosine_ionic_motion': 0.7518541705699963, 'ionic_motion_component': 10.598532009966725, 'ionic_force_x': -0.86297807097435, 'ionic_force_y': 12.021617323160172, 'ionic_force_z': -7.310816407203674, 'radial_force': 12.05255218679792, 'axial_force': -7.310816407203674, 'contributions': [{'ion': 1309, 'force': [-1.2417367696762085, 2.2549033164978027, 3.7121427059173584], 'magnitude': 4.517355442047119, 'distance': 8.572882652282715, 'directional_contribution': 2.9750776534110397}, {'ion': 1469, 'force': [3.919631004333496, 7.311126232147217, -1.3659437894821167], 'magnitude': 8.407251358032227, 'distance': 6.284084796905518, 'directional_contribution': 6.542397326645556}, {'ion': 2434, 'force': [-3.1615939140319824, 2.1154823303222656, -7.686925411224365], 'magnitude': 8.576698303222656, 'distance': 6.221698760986328, 'directional_contribution': 1.0518751575718213}, {'ion': 2444, 'force': [-0.37927839159965515, 0.34010544419288635, -1.9700899124145508], 'magnitude': 2.0348901748657227, 'distance': 12.773165702819824, 'directional_contribution': 0.0291817164848438}]}, 5416: {'frame': 5416, 'ionic_force': [-2.890625089406967, 9.539554595947266, -3.3671732246875763], 'ionic_force_magnitude': 10.52124853910507, 'motion_vector': [-2.1743736267089844, -0.24370956420898438, 0.42597198486328125], 'cosine_ionic_motion': 0.10771079835192808, 'ionic_motion_component': 1.1332520798060641, 'ionic_force_x': -2.890625089406967, 'ionic_force_y': 9.539554595947266, 'ionic_force_z': -3.3671732246875763, 'radial_force': 9.967889209685652, 'axial_force': -3.3671732246875763, 'contributions': [{'ion': 1309, 'force': [-1.7372729778289795, 1.9497443437576294, 1.9252551794052124], 'magnitude': 3.244414806365967, 'distance': 10.115814208984375, 'directional_contribution': 1.8493884414458872}, {'ion': 1469, 'force': [1.0098694562911987, 3.874903678894043, -0.12357929348945618], 'magnitude': 4.0062432289123535, 'distance': 9.103331565856934, 'directional_contribution': -1.432358656018975}, {'ion': 2434, 'force': [-1.7631807327270508, 3.0347986221313477, -3.503937005996704], 'magnitude': 4.959474086761475, 'distance': 8.181844711303711, 'directional_contribution': 0.7185176510370184}, {'ion': 2444, 'force': [-0.4000408351421356, 0.6801079511642456, -1.6649121046066284], 'magnitude': 1.8424201011657715, 'distance': 13.423776626586914, 'directional_contribution': -0.00229534554213906}]}, 5417: {'frame': 5417, 'ionic_force': [-4.601493835449219, 9.4010049700737, -1.1370874345302582], 'ionic_force_magnitude': 10.528324073602322, 'motion_vector': [0.7505950927734375, 1.0793838500976562, -1.4337081909179688], 'cosine_ionic_motion': 0.4064264224237802, 'ionic_motion_component': 4.278989087352351, 'ionic_force_x': -4.601493835449219, 'ionic_force_y': 9.4010049700737, 'ionic_force_z': -1.1370874345302582, 'radial_force': 10.46673970083462, 'axial_force': -1.1370874345302582, 'contributions': [{'ion': 1309, 'force': [-1.6386932134628296, 1.689590573310852, 3.3819234371185303], 'magnitude': 4.120368480682373, 'distance': 8.976375579833984, 'directional_contribution': -2.187368593057652}, {'ion': 1469, 'force': [0.2765955328941345, 4.555323600769043, -0.1436668336391449], 'magnitude': 4.56597375869751, 'distance': 8.527118682861328, 'directional_contribution': 2.7402861903056674}, {'ion': 2434, 'force': [-2.509505271911621, 2.4902234077453613, -2.8283956050872803], 'magnitude': 4.527543544769287, 'distance': 8.563232421875, 'directional_contribution': 2.4980793799438032}, {'ion': 2444, 'force': [-0.7298908829689026, 0.6658673882484436, -1.5469484329223633], 'magnitude': 1.8355298042297363, 'distance': 13.448948860168457, 'directional_contribution': 1.227992153000633}]}, 5418: {'frame': 5418, 'ionic_force': [-1.8272255063056946, 7.148484110832214, -0.753704845905304], 'ionic_force_magnitude': 7.416714173301805, 'motion_vector': [0.6279106140136719, 0.4439239501953125, -0.27136993408203125], 'cosine_ionic_motion': 0.3688091800561364, 'ionic_motion_component': 2.735352272966164, 'ionic_force_x': -1.8272255063056946, 'ionic_force_y': 7.148484110832214, 'ionic_force_z': -0.753704845905304, 'radial_force': 7.378318110092214, 'axial_force': -0.753704845905304, 'contributions': [{'ion': 1309, 'force': [-1.2601678371429443, 2.125608205795288, 2.1942358016967773], 'magnitude': 3.3046791553497314, 'distance': 10.023154258728027, 'directional_contribution': -0.5433886430388242}, {'ion': 1469, 'force': [0.4336826205253601, 3.54756498336792, -0.8087297081947327], 'magnitude': 3.6643335819244385, 'distance': 9.518566131591797, 'directional_contribution': 2.5342963743771456}, {'ion': 2434, 'force': [-1.0007402896881104, 1.4753109216690063, -2.1392109394073486], 'magnitude': 2.784644842147827, 'distance': 10.919032096862793, 'directional_contribution': 0.7444446326850809}]}, 5419: {'frame': 5419, 'ionic_force': [-2.556093394756317, 7.023166179656982, -1.4966426491737366], 'ionic_force_magnitude': 7.622231684298261, 'motion_vector': [-0.07321548461914062, -1.4095268249511719, 1.3923492431640625], 'cosine_ionic_motion': -0.7805771866631694, 'ionic_motion_component': -5.949740164224408, 'ionic_force_x': -2.556093394756317, 'ionic_force_y': 7.023166179656982, 'ionic_force_z': -1.4966426491737366, 'radial_force': 7.473852863804219, 'axial_force': -1.4966426491737366, 'contributions': [{'ion': 1309, 'force': [-2.2032456398010254, 2.115774631500244, 1.356068730354309], 'magnitude': 3.3421125411987305, 'distance': 9.966863632202148, 'directional_contribution': -0.4704937454166114}, {'ion': 1469, 'force': [0.5705264210700989, 3.1289117336273193, -0.7028989195823669], 'magnitude': 3.257246732711792, 'distance': 10.095869064331055, 'directional_contribution': -2.7391786691732083}, {'ion': 2434, 'force': [-0.9233741760253906, 1.778479814529419, -2.1498124599456787], 'magnitude': 2.9389290809631348, 'distance': 10.628561973571777, 'directional_contribution': -2.7400675900062055}]}, 5420: {'frame': 5420, 'ionic_force': [-4.017000198364258, 7.976373076438904, -4.721324697136879], 'ionic_force_magnitude': 10.101966389965497, 'motion_vector': [1.37384033203125, 0.6198310852050781, 1.271148681640625], 'cosine_ionic_motion': -0.33017035763647795, 'ionic_motion_component': -3.3353698558065883, 'ionic_force_x': -4.017000198364258, 'ionic_force_y': 7.976373076438904, 'ionic_force_z': -4.721324697136879, 'radial_force': 8.930779252013673, 'axial_force': -4.721324697136879, 'contributions': [{'ion': 1309, 'force': [-2.296131134033203, 1.0717114210128784, 0.202259823679924], 'magnitude': 2.5419859886169434, 'distance': 11.428321838378906, 'directional_contribution': -1.132616194223882}, {'ion': 1469, 'force': [0.5067126154899597, 4.24498176574707, -0.2817506194114685], 'magnitude': 4.2843918800354, 'distance': 8.802873611450195, 'directional_contribution': 1.505921613751351}, {'ion': 2434, 'force': [-1.693018913269043, 2.0171566009521484, -2.944333791732788], 'magnitude': 3.9502322673797607, 'distance': 9.167643547058105, 'directional_contribution': -2.4437910563266314}, {'ion': 2444, 'force': [-0.5345627665519714, 0.6425232887268066, -1.6975001096725464], 'magnitude': 1.8921153545379639, 'distance': 13.246319770812988, 'directional_contribution': -1.2648843400024923}]}, 5421: {'frame': 5421, 'ionic_force': [-4.36628919839859, 9.376880168914795, -2.967519700527191], 'ionic_force_magnitude': 10.76087990079142, 'motion_vector': [-0.43817138671875, 0.11849594116210938, -1.432342529296875], 'cosine_ionic_motion': 0.44993154895126, 'ionic_motion_component': 4.841659361841564, 'ionic_force_x': -4.36628919839859, 'ionic_force_y': 9.376880168914795, 'ionic_force_z': -2.967519700527191, 'radial_force': 10.343614603524232, 'axial_force': -2.967519700527191, 'contributions': [{'ion': 1309, 'force': [-3.586841344833374, 1.4117411375045776, 1.6100742816925049], 'magnitude': 4.177413463592529, 'distance': 8.914875984191895, 'directional_contribution': -0.377520252610303}, {'ion': 1469, 'force': [1.202595829963684, 3.48968505859375, 0.13294559717178345], 'magnitude': 3.6934826374053955, 'distance': 9.480932235717773, 'directional_contribution': -0.2022257049529017}, {'ion': 2434, 'force': [-1.507516622543335, 3.459397077560425, -2.9776651859283447], 'magnitude': 4.806924819946289, 'distance': 8.310657501220703, 'directional_contribution': 3.550983443186361}, {'ion': 2444, 'force': [-0.4745270609855652, 1.0160568952560425, -1.7328743934631348], 'magnitude': 2.0640740394592285, 'distance': 12.682544708251953, 'directional_contribution': 1.8704217850621294}]}, 5422: {'frame': 5422, 'ionic_force': [-3.337195932865143, 8.502465009689331, -4.2525006383657455], 'ionic_force_magnitude': 10.075343647470499, 'motion_vector': [0.1480560302734375, -0.8996047973632812, 0.5749053955078125], 'cosine_ionic_motion': -0.9749704271170396, 'ionic_motion_component': -9.823162099325264, 'ionic_force_x': -3.337195932865143, 'ionic_force_y': 8.502465009689331, 'ionic_force_z': -4.2525006383657455, 'radial_force': 9.133936059296838, 'axial_force': -4.2525006383657455, 'contributions': [{'ion': 1309, 'force': [-2.566864252090454, 1.8449293375015259, 0.5315044522285461], 'magnitude': 3.205472469329834, 'distance': 10.17707633972168, 'directional_contribution': -1.6089514764139317}, {'ion': 1469, 'force': [1.0937838554382324, 3.111398458480835, -0.23599140346050262], 'magnitude': 3.3064868450164795, 'distance': 10.020413398742676, 'directional_contribution': -2.572530709600221}, {'ion': 2434, 'force': [-1.3929810523986816, 2.763676643371582, -2.991767168045044], 'magnitude': 4.304529666900635, 'distance': 8.782258033752441, 'directional_contribution': -4.093803070234479}, {'ion': 2444, 'force': [-0.4711344838142395, 0.7824605703353882, -1.5562465190887451], 'magnitude': 1.8044710159301758, 'distance': 13.564197540283203, 'directional_contribution': -1.5478770422136625}]}, 5423: {'frame': 5423, 'ionic_force': [-7.194524526596069, 10.885988421738148, -3.873266875743866], 'ionic_force_magnitude': 13.611323351266917, 'motion_vector': [-0.2519950866699219, 0.5466041564941406, 0.0637054443359375], 'cosine_ionic_motion': 0.9123871441683606, 'ionic_motion_component': 12.418796440814543, 'ionic_force_x': -7.194524526596069, 'ionic_force_y': 10.885988421738148, 'ionic_force_z': -3.873266875743866, 'radial_force': 13.048598663535078, 'axial_force': -3.873266875743866, 'contributions': [{'ion': 1309, 'force': [-7.53367280960083, -0.03545748442411423, 1.090088963508606], 'magnitude': 7.612212181091309, 'distance': 6.604099273681641, 'directional_contribution': 3.219313426221046}, {'ion': 1469, 'force': [3.078547954559326, 6.243687152862549, 0.9668325781822205], 'magnitude': 7.0282182693481445, 'distance': 6.873001575469971, 'directional_contribution': 4.45866631981975}, {'ion': 2434, 'force': [-2.2350199222564697, 3.7992143630981445, -4.083253383636475], 'magnitude': 6.008519172668457, 'distance': 7.4333624839782715, 'directional_contribution': 3.9318091657978513}, {'ion': 2444, 'force': [-0.5043797492980957, 0.8785443902015686, -1.8469350337982178], 'magnitude': 2.106515645980835, 'distance': 12.554132461547852, 'directional_contribution': 0.8090074727170524}]}, 5424: {'frame': 5424, 'ionic_force': [-9.829724729061127, 8.064699590206146, -3.82029065862298], 'ionic_force_magnitude': 13.276200075539274, 'motion_vector': [-1.8115425109863281, -1.1403274536132812, 0.10491180419921875], 'cosine_ionic_motion': 0.2885408107742469, 'ionic_motion_component': 3.8307255337972204, 'ionic_force_x': -9.829724729061127, 'ionic_force_y': 8.064699590206146, 'ionic_force_z': -3.82029065862298, 'radial_force': 12.71467135750614, 'axial_force': -3.82029065862298, 'contributions': [{'ion': 1309, 'force': [-8.29712200164795, 0.1777876615524292, 0.9536499381065369], 'magnitude': 8.353639602661133, 'distance': 6.30421781539917, 'directional_contribution': 6.965442263992603}, {'ion': 1469, 'force': [0.7835202217102051, 3.773498058319092, -0.03277162089943886], 'magnitude': 3.854123115539551, 'distance': 9.281245231628418, 'directional_contribution': -2.671709695405911}, {'ion': 2434, 'force': [-1.8014920949935913, 3.1987240314483643, -3.0620651245117188], 'magnitude': 4.7805280685424805, 'distance': 8.33357048034668, 'directional_contribution': -0.3291250055472901}, {'ion': 2444, 'force': [-0.5146308541297913, 0.914689838886261, -1.6791038513183594], 'magnitude': 1.9801243543624878, 'distance': 12.948599815368652, 'directional_contribution': -0.13388225810879462}]}, 5425: {'frame': 5425, 'ionic_force': [-7.359991593286395, 3.306031584739685, -5.195836968719959], 'ionic_force_magnitude': 9.59666832281182, 'motion_vector': [0.7701644897460938, 1.122161865234375, -0.6427230834960938], 'cosine_ionic_motion': 0.09560626418969688, 'ionic_motion_component': 0.9175016070116421, 'ionic_force_x': -7.359991593286395, 'ionic_force_y': 3.306031584739685, 'ionic_force_z': -5.195836968719959, 'radial_force': 8.068415029765314, 'axial_force': -5.195836968719959, 'contributions': [{'ion': 1309, 'force': [-4.172080993652344, -2.511462926864624, -0.10490787774324417], 'magnitude': 4.87080192565918, 'distance': 8.255983352661133, 'directional_contribution': -3.96240076768688}, {'ion': 1469, 'force': [0.024452881887555122, 2.9648444652557373, -0.17231887578964233], 'magnitude': 2.9699485301971436, 'distance': 10.572911262512207, 'directional_contribution': 2.2965209036455843}, {'ion': 2434, 'force': [-2.4676637649536133, 2.1257126331329346, -3.127074718475342], 'magnitude': 4.515153884887695, 'distance': 8.574973106384277, 'directional_contribution': 1.657456226845511}, {'ion': 2444, 'force': [-0.7446997165679932, 0.7269374132156372, -1.791535496711731], 'magnitude': 2.0718626976013184, 'distance': 12.658683776855469, 'directional_contribution': 0.9259250504055956}]}, 5426: {'frame': 5426, 'ionic_force': [-5.71360582113266, 4.7653467655181885, -4.617043234407902], 'ionic_force_magnitude': 8.756192637402826, 'motion_vector': [0.9683570861816406, -1.1876640319824219, -1.7886962890625], 'cosine_ionic_motion': -0.14225960241465066, 'ionic_motion_component': -1.2456524832630174, 'ionic_force_x': -5.71360582113266, 'ionic_force_y': 4.7653467655181885, 'ionic_force_z': -4.617043234407902, 'radial_force': 7.440014870611193, 'axial_force': -4.617043234407902, 'contributions': [{'ion': 1309, 'force': [-3.82336688041687, -1.281545877456665, 0.038811035454273224], 'magnitude': 4.032617092132568, 'distance': 9.073514938354492, 'directional_contribution': -0.9551680765469284}, {'ion': 1469, 'force': [0.3030494451522827, 3.1069347858428955, -0.22176901996135712], 'magnitude': 3.129547119140625, 'distance': 10.299788475036621, 'directional_contribution': -1.2736328422891834}, {'ion': 2434, 'force': [-1.6431152820587158, 2.2570924758911133, -2.791811227798462], 'magnitude': 3.948227882385254, 'distance': 9.169970512390137, 'directional_contribution': 0.306498423729046}, {'ion': 2444, 'force': [-0.5501731038093567, 0.6828653812408447, -1.642274022102356], 'magnitude': 1.8617355823516846, 'distance': 13.353959083557129, 'directional_contribution': 0.6766499945516973}]}, 5427: {'frame': 5427, 'ionic_force': [-8.04122668504715, 2.214553475379944, -8.471194505691528], 'ionic_force_magnitude': 11.888091101976386, 'motion_vector': [1.9277992248535156, -0.47090911865234375, 1.2962722778320312], 'cosine_ionic_motion': -0.9768244492629804, 'ionic_motion_component': -11.612578043476221, 'ionic_force_x': -8.04122668504715, 'ionic_force_y': 2.214553475379944, 'ionic_force_z': -8.471194505691528, 'radial_force': 8.340597921949707, 'axial_force': -8.471194505691528, 'contributions': [{'ion': 1309, 'force': [-7.151926517486572, -4.424306392669678, -2.266660690307617], 'magnitude': 8.709896087646484, 'distance': 6.1739420890808105, 'directional_contribution': -6.17728795671141}, {'ion': 1469, 'force': [1.0913169384002686, 4.217013835906982, -1.362021803855896], 'magnitude': 4.563910484313965, 'distance': 8.529046058654785, 'directional_contribution': -0.6950669595563213}, {'ion': 2434, 'force': [-1.582262396812439, 1.9491033554077148, -3.3685457706451416], 'magnitude': 4.2011494636535645, 'distance': 8.889656066894531, 'directional_contribution': -3.516248744739322}, {'ion': 2444, 'force': [-0.398354709148407, 0.4727426767349243, -1.4739662408828735], 'magnitude': 1.5983580350875854, 'distance': 14.412257194519043, 'directional_contribution': -1.2239739834485697}]}, 5428: {'frame': 5428, 'ionic_force': [-4.013658359646797, 2.036353588104248, -10.628021240234375], 'ionic_force_magnitude': 11.541708055856407, 'motion_vector': [0.24727249145507812, -2.330799102783203, -4.778404235839844], 'cosine_ionic_motion': 0.733311095968307, 'ionic_motion_component': 8.4636625837863, 'ionic_force_x': -4.013658359646797, 'ionic_force_y': 2.036353588104248, 'ionic_force_z': -10.628021240234375, 'radial_force': 4.5006876545421, 'axial_force': -10.628021240234375, 'contributions': [{'ion': 1309, 'force': [-4.697807788848877, -6.503828525543213, -1.5563700199127197], 'magnitude': 8.172605514526367, 'distance': 6.373658657073975, 'directional_contribution': 4.027286881652531}, {'ion': 1469, 'force': [2.3175904750823975, 4.2220258712768555, -0.8517012596130371], 'magnitude': 4.891024589538574, 'distance': 8.238897323608398, 'directional_contribution': -0.9766156258850804}, {'ion': 2434, 'force': [-1.4328304529190063, 3.6519341468811035, -6.213566780090332], 'magnitude': 7.3483357429504395, 'distance': 6.7216291427612305, 'directional_contribution': 3.9127245672438407}, {'ion': 2444, 'force': [-0.20061059296131134, 0.666222095489502, -2.006383180618286], 'magnitude': 2.123598337173462, 'distance': 12.503536224365234, 'directional_contribution': 1.5002665511818145}]}, 5429: {'frame': 5429, 'ionic_force': [-0.07442072033882141, -0.02468770742416382, -7.9879608154296875], 'ionic_force_magnitude': 7.9883456306893565, 'motion_vector': [3.7690887451171875, -2.5068588256835938, -3.2027816772460938], 'cosine_ionic_motion': 0.572624250980996, 'ionic_motion_component': 4.574320433350805, 'ionic_force_x': -0.07442072033882141, 'ionic_force_y': -0.02468770742416382, 'ionic_force_z': -7.9879608154296875, 'radial_force': 0.0784087145259389, 'axial_force': -7.9879608154296875, 'contributions': [{'ion': 1309, 'force': [-1.8123735189437866, -2.4131195545196533, -2.5620484352111816], 'magnitude': 3.9587795734405518, 'distance': 9.15774154663086, 'directional_contribution': 1.3388449937113478}, {'ion': 1469, 'force': [1.9238256216049194, 2.0180952548980713, -2.4386179447174072], 'magnitude': 3.7041423320770264, 'distance': 9.467279434204102, 'directional_contribution': 1.803816336372222}, {'ion': 2434, 'force': [-0.18587282299995422, 0.3703365921974182, -2.9872944355010986], 'magnitude': 3.0158956050872803, 'distance': 10.492063522338867, 'directional_contribution': 1.431659057345513}]}, 5430: {'frame': 5430, 'ionic_force': [2.4746485874056816, -1.7678358405828476, -3.220875859260559], 'ionic_force_magnitude': 4.429804791541682, 'motion_vector': [-0.60418701171875, 0.23330307006835938, 2.4262313842773438], 'cosine_ionic_motion': -0.8739764423926943, 'ionic_motion_component': -3.87154503220571, 'ionic_force_x': 2.4746485874056816, 'ionic_force_y': -1.7678358405828476, 'ionic_force_z': -3.220875859260559, 'radial_force': 3.0412381015629473, 'axial_force': -3.220875859260559, 'contributions': [{'ion': 1309, 'force': [0.12402363866567612, -1.6623444557189941, -1.531604528427124], 'magnitude': 2.26375412940979, 'distance': 12.110285758972168, 'directional_contribution': -1.6640683471142115}, {'ion': 1320, 'force': [0.5745420455932617, -0.34557026624679565, 1.4239434003829956], 'magnitude': 1.5738908052444458, 'distance': 14.523849487304688, 'directional_contribution': 1.20542995909179}, {'ion': 1469, 'force': [1.4435352087020874, 0.3784688711166382, -1.497428059577942], 'magnitude': 2.11407732963562, 'distance': 12.531660079956055, 'directional_contribution': -1.7589173250676327}, {'ion': 2434, 'force': [0.33254769444465637, -0.13838998973369598, -1.6157866716384888], 'magnitude': 1.6554474830627441, 'distance': 14.161567687988281, 'directional_contribution': -1.6539893131995007}]}, 5431: {'frame': 5431, 'ionic_force': [3.104661077260971, -1.3943484723567963, -5.393718481063843], 'ionic_force_magnitude': 6.377721154142177, 'motion_vector': [-2.8593292236328125, 1.6220474243164062, -1.3614044189453125], 'cosine_ionic_motion': -0.1672747077358023, 'ionic_motion_component': -1.0668314420795766, 'ionic_force_x': 3.104661077260971, 'ionic_force_y': -1.3943484723567963, 'ionic_force_z': -5.393718481063843, 'radial_force': 3.4033994868400304, 'axial_force': -5.393718481063843, 'contributions': [{'ion': 1309, 'force': [0.6289064884185791, -2.2084546089172363, -1.3620975017547607], 'magnitude': 2.669851064682007, 'distance': 11.151300430297852, 'directional_contribution': -0.9910014747644809}, {'ion': 1469, 'force': [2.067415952682495, 1.0044293403625488, -1.9814109802246094], 'magnitude': 3.0346460342407227, 'distance': 10.459598541259766, 'directional_contribution': -0.44537244017870137}, {'ion': 2434, 'force': [0.40833863615989685, -0.19032320380210876, -2.0502099990844727], 'magnitude': 2.0991246700286865, 'distance': 12.576213836669922, 'directional_contribution': 0.3695425753775714}]}, 5432: {'frame': 5432, 'ionic_force': [1.1073409914970398, -2.299594771116972, -5.362725257873535], 'ionic_force_magnitude': 5.939121346986686, 'motion_vector': [-2.0052490234375, -1.7602043151855469, -0.211578369140625], 'cosine_ionic_motion': 0.18632320852044088, 'ionic_motion_component': 1.106596145162802, 'ionic_force_x': 1.1073409914970398, 'ionic_force_y': -2.299594771116972, 'ionic_force_z': -5.362725257873535, 'radial_force': 2.5523205485985034, 'axial_force': -5.362725257873535, 'contributions': [{'ion': 1309, 'force': [-0.5481927990913391, -3.5546693801879883, -2.8332223892211914], 'magnitude': 4.578573703765869, 'distance': 8.51537799835205, 'directional_contribution': 2.972315746727638}, {'ion': 1320, 'force': [0.22608864307403564, -0.023177023977041245, 1.754052996635437], 'magnitude': 1.7687156200408936, 'distance': 13.700613975524902, 'directional_contribution': -0.29279375053671397}, {'ion': 1469, 'force': [1.5149571895599365, 1.144568681716919, -2.3458662033081055], 'magnitude': 3.0179829597473145, 'distance': 10.488433837890625, 'directional_contribution': -1.7022461345254385}, {'ion': 2434, 'force': [-0.08551204204559326, 0.1336829513311386, -1.9376896619796753], 'magnitude': 1.9441771507263184, 'distance': 13.06775951385498, 'directional_contribution': 0.12932031630161678}]}, 5433: {'frame': 5433, 'ionic_force': [-0.44162964820861816, -0.36573115549981594, -4.841521263122559], 'ionic_force_magnitude': 4.875358875564747, 'motion_vector': [1.0330657958984375, 1.6155204772949219, -5.069999694824219], 'cosine_ionic_motion': 0.889221364727531, 'ionic_motion_component': 4.335273272866165, 'ionic_force_x': -0.44162964820861816, 'ionic_force_y': -0.36573115549981594, 'ionic_force_z': -4.841521263122559, 'radial_force': 0.5734073807338883, 'axial_force': -4.841521263122559, 'contributions': [{'ion': 1309, 'force': [-0.640687882900238, -1.2333738803863525, -1.1129107475280762], 'magnitude': 1.7805230617523193, 'distance': 13.655111312866211, 'directional_contribution': 0.551246759031236}, {'ion': 1320, 'force': [-0.537470281124115, 0.01673593558371067, 1.5264745950698853], 'magnitude': 1.6184186935424805, 'distance': 14.322657585144043, 'directional_contribution': -1.525210077137657}, {'ion': 1469, 'force': [1.1431920528411865, 1.02493155002594, -3.420396089553833], 'magnitude': 3.749197483062744, 'distance': 9.410222053527832, 'directional_contribution': 3.722558026865098}, {'ion': 2434, 'force': [-0.40666353702545166, -0.174024760723114, -1.8346890211105347], 'magnitude': 1.8872582912445068, 'distance': 13.263354301452637, 'directional_contribution': 1.586678610431468}]}}</t>
+          <t>{5415: {'frame': 5415, 'ionic_force': [-0.86297807097435, 12.021617323160172, -7.310816407203674], 'ionic_force_magnitude': 14.096526194609996, 'motion_vector': [-0.3487205505371094, 3.4752159118652344, 0.6145477294921875], 'cosine_ionic_motion': 0.7518541705699963, 'ionic_motion_component': 10.598532009966725, 'ionic_force_x': -0.86297807097435, 'ionic_force_y': 12.021617323160172, 'ionic_force_z': -7.310816407203674, 'radial_force': 12.05255218679792, 'axial_force': -7.310816407203674, 'contributions': [{'ion': 1309, 'force': [-1.2417367696762085, 2.2549033164978027, 3.7121427059173584], 'magnitude': 4.517355442047119, 'distance': 8.572882652282715, 'cosine_with_motion': 0.6585883074501265, 'motion_component': 2.9750776534110397}, {'ion': 1469, 'force': [3.919631004333496, 7.311126232147217, -1.3659437894821167], 'magnitude': 8.407251358032227, 'distance': 6.284084796905518, 'cosine_with_motion': 0.7781850453014673, 'motion_component': 6.542397326645556}, {'ion': 2434, 'force': [-3.1615939140319824, 2.1154823303222656, -7.686925411224365], 'magnitude': 8.576698303222656, 'distance': 6.221698760986328, 'cosine_with_motion': 0.12264335860419856, 'motion_component': 1.0518751575718213}, {'ion': 2444, 'force': [-0.37927839159965515, 0.34010544419288635, -1.9700899124145508], 'magnitude': 2.0348901748657227, 'distance': 12.773165702819824, 'cosine_with_motion': 0.014340683672517583, 'motion_component': 0.0291817164848438}]}, 5416: {'frame': 5416, 'ionic_force': [-2.890625089406967, 9.539554595947266, -3.3671732246875763], 'ionic_force_magnitude': 10.52124853910507, 'motion_vector': [-2.1743736267089844, -0.24370956420898438, 0.42597198486328125], 'cosine_ionic_motion': 0.10771079835192808, 'ionic_motion_component': 1.1332520798060641, 'ionic_force_x': -2.890625089406967, 'ionic_force_y': 9.539554595947266, 'ionic_force_z': -3.3671732246875763, 'radial_force': 9.967889209685652, 'axial_force': -3.3671732246875763, 'contributions': [{'ion': 1309, 'force': [-1.7372729778289795, 1.9497443437576294, 1.9252551794052124], 'magnitude': 3.244414806365967, 'distance': 10.115814208984375, 'cosine_with_motion': 0.57002217966702, 'motion_component': 1.849388441445887}, {'ion': 1469, 'force': [1.0098694562911987, 3.874903678894043, -0.12357929348945618], 'magnitude': 4.0062432289123535, 'distance': 9.103331565856934, 'cosine_with_motion': -0.35753160520772975, 'motion_component': -1.432358656018975}, {'ion': 2434, 'force': [-1.7631807327270508, 3.0347986221313477, -3.503937005996704], 'magnitude': 4.959474086761475, 'distance': 8.181844711303711, 'cosine_with_motion': 0.14487779028910183, 'motion_component': 0.7185176510370184}, {'ion': 2444, 'force': [-0.4000408351421356, 0.6801079511642456, -1.6649121046066284], 'magnitude': 1.8424201011657715, 'distance': 13.423776626586914, 'cosine_with_motion': -0.0012458317985159255, 'motion_component': -0.00229534554213906}]}, 5417: {'frame': 5417, 'ionic_force': [-4.601493835449219, 9.4010049700737, -1.1370874345302582], 'ionic_force_magnitude': 10.528324073602322, 'motion_vector': [0.7505950927734375, 1.0793838500976562, -1.4337081909179688], 'cosine_ionic_motion': 0.4064264224237802, 'ionic_motion_component': 4.278989087352351, 'ionic_force_x': -4.601493835449219, 'ionic_force_y': 9.4010049700737, 'ionic_force_z': -1.1370874345302582, 'radial_force': 10.46673970083462, 'axial_force': -1.1370874345302582, 'contributions': [{'ion': 1309, 'force': [-1.6386932134628296, 1.689590573310852, 3.3819234371185303], 'magnitude': 4.120368480682373, 'distance': 8.976375579833984, 'cosine_with_motion': -0.5308672048478624, 'motion_component': -2.187368593057652}, {'ion': 1469, 'force': [0.2765955328941345, 4.555323600769043, -0.1436668336391449], 'magnitude': 4.56597375869751, 'distance': 8.527118682861328, 'cosine_with_motion': 0.6001537030888063, 'motion_component': 2.7402861903056674}, {'ion': 2434, 'force': [-2.509505271911621, 2.4902234077453613, -2.8283956050872803], 'magnitude': 4.527543544769287, 'distance': 8.563232421875, 'cosine_with_motion': 0.5517515902465349, 'motion_component': 2.4980793799438032}, {'ion': 2444, 'force': [-0.7298908829689026, 0.6658673882484436, -1.5469484329223633], 'magnitude': 1.8355298042297363, 'distance': 13.448948860168457, 'cosine_with_motion': 0.669012387353238, 'motion_component': 1.227992153000633}]}, 5418: {'frame': 5418, 'ionic_force': [-1.8272255063056946, 7.148484110832214, -0.753704845905304], 'ionic_force_magnitude': 7.416714173301805, 'motion_vector': [0.6279106140136719, 0.4439239501953125, -0.27136993408203125], 'cosine_ionic_motion': 0.3688091800561364, 'ionic_motion_component': 2.735352272966164, 'ionic_force_x': -1.8272255063056946, 'ionic_force_y': 7.148484110832214, 'ionic_force_z': -0.753704845905304, 'radial_force': 7.378318110092214, 'axial_force': -0.753704845905304, 'contributions': [{'ion': 1309, 'force': [-1.2601678371429443, 2.125608205795288, 2.1942358016967773], 'magnitude': 3.3046791553497314, 'distance': 10.023154258728027, 'cosine_with_motion': -0.1644300780964941, 'motion_component': -0.5433886430388242}, {'ion': 1469, 'force': [0.4336826205253601, 3.54756498336792, -0.8087297081947327], 'magnitude': 3.6643335819244385, 'distance': 9.518566131591797, 'cosine_with_motion': 0.6916117806805393, 'motion_component': 2.5342963743771456}, {'ion': 2434, 'force': [-1.0007402896881104, 1.4753109216690063, -2.1392109394073486], 'magnitude': 2.784644842147827, 'distance': 10.919032096862793, 'cosine_with_motion': 0.26733916725288576, 'motion_component': 0.7444446326850809}]}, 5419: {'frame': 5419, 'ionic_force': [-2.556093394756317, 7.023166179656982, -1.4966426491737366], 'ionic_force_magnitude': 7.622231684298261, 'motion_vector': [-0.07321548461914062, -1.4095268249511719, 1.3923492431640625], 'cosine_ionic_motion': -0.7805771866631694, 'ionic_motion_component': -5.949740164224408, 'ionic_force_x': -2.556093394756317, 'ionic_force_y': 7.023166179656982, 'ionic_force_z': -1.4966426491737366, 'radial_force': 7.473852863804219, 'axial_force': -1.4966426491737366, 'contributions': [{'ion': 1309, 'force': [-2.2032456398010254, 2.115774631500244, 1.356068730354309], 'magnitude': 3.3421125411987305, 'distance': 9.966863632202148, 'cosine_with_motion': -0.14077735077576017, 'motion_component': -0.4704937454166113}, {'ion': 1469, 'force': [0.5705264210700989, 3.1289117336273193, -0.7028989195823669], 'magnitude': 3.257246732711792, 'distance': 10.095869064331055, 'cosine_with_motion': -0.8409491019474874, 'motion_component': -2.7391786691732083}, {'ion': 2434, 'force': [-0.9233741760253906, 1.778479814529419, -2.1498124599456787], 'magnitude': 2.9389290809631348, 'distance': 10.628561973571777, 'cosine_with_motion': -0.9323354010550714, 'motion_component': -2.7400675900062055}]}, 5420: {'frame': 5420, 'ionic_force': [-4.017000198364258, 7.976373076438904, -4.721324697136879], 'ionic_force_magnitude': 10.101966389965497, 'motion_vector': [1.37384033203125, 0.6198310852050781, 1.271148681640625], 'cosine_ionic_motion': -0.33017035763647795, 'ionic_motion_component': -3.3353698558065883, 'ionic_force_x': -4.017000198364258, 'ionic_force_y': 7.976373076438904, 'ionic_force_z': -4.721324697136879, 'radial_force': 8.930779252013673, 'axial_force': -4.721324697136879, 'contributions': [{'ion': 1309, 'force': [-2.296131134033203, 1.0717114210128784, 0.202259823679924], 'magnitude': 2.5419859886169434, 'distance': 11.428321838378906, 'cosine_with_motion': -0.44556351398937477, 'motion_component': -1.132616194223882}, {'ion': 1469, 'force': [0.5067126154899597, 4.24498176574707, -0.2817506194114685], 'magnitude': 4.2843918800354, 'distance': 8.802873611450195, 'cosine_with_motion': 0.3514901901202061, 'motion_component': 1.505921613751351}, {'ion': 2434, 'force': [-1.693018913269043, 2.0171566009521484, -2.944333791732788], 'magnitude': 3.9502322673797607, 'distance': 9.167643547058105, 'cosine_with_motion': -0.6186448965736641, 'motion_component': -2.4437910563266314}, {'ion': 2444, 'force': [-0.5345627665519714, 0.6425232887268066, -1.6975001096725464], 'magnitude': 1.8921153545379639, 'distance': 13.246319770812988, 'cosine_with_motion': -0.6685027957609565, 'motion_component': -1.2648843400024923}]}, 5421: {'frame': 5421, 'ionic_force': [-4.36628919839859, 9.376880168914795, -2.967519700527191], 'ionic_force_magnitude': 10.76087990079142, 'motion_vector': [-0.43817138671875, 0.11849594116210938, -1.432342529296875], 'cosine_ionic_motion': 0.44993154895126, 'ionic_motion_component': 4.841659361841564, 'ionic_force_x': -4.36628919839859, 'ionic_force_y': 9.376880168914795, 'ionic_force_z': -2.967519700527191, 'radial_force': 10.343614603524232, 'axial_force': -2.967519700527191, 'contributions': [{'ion': 1309, 'force': [-3.586841344833374, 1.4117411375045776, 1.6100742816925049], 'magnitude': 4.177413463592529, 'distance': 8.914875984191895, 'cosine_with_motion': -0.09037177139810013, 'motion_component': -0.377520252610303}, {'ion': 1469, 'force': [1.202595829963684, 3.48968505859375, 0.13294559717178345], 'magnitude': 3.6934826374053955, 'distance': 9.480932235717773, 'cosine_with_motion': -0.05475204072792799, 'motion_component': -0.2022257049529017}, {'ion': 2434, 'force': [-1.507516622543335, 3.459397077560425, -2.9776651859283447], 'magnitude': 4.806924819946289, 'distance': 8.310657501220703, 'cosine_with_motion': 0.7387225120534889, 'motion_component': 3.550983443186361}, {'ion': 2444, 'force': [-0.4745270609855652, 1.0160568952560425, -1.7328743934631348], 'magnitude': 2.0640740394592285, 'distance': 12.682544708251953, 'cosine_with_motion': 0.906179644664221, 'motion_component': 1.8704217850621294}]}, 5422: {'frame': 5422, 'ionic_force': [-3.337195932865143, 8.502465009689331, -4.2525006383657455], 'ionic_force_magnitude': 10.075343647470499, 'motion_vector': [0.1480560302734375, -0.8996047973632812, 0.5749053955078125], 'cosine_ionic_motion': -0.9749704271170396, 'ionic_motion_component': -9.823162099325264, 'ionic_force_x': -3.337195932865143, 'ionic_force_y': 8.502465009689331, 'ionic_force_z': -4.2525006383657455, 'radial_force': 9.133936059296838, 'axial_force': -4.2525006383657455, 'contributions': [{'ion': 1309, 'force': [-2.566864252090454, 1.8449293375015259, 0.5315044522285461], 'magnitude': 3.205472469329834, 'distance': 10.17707633972168, 'cosine_with_motion': -0.501938957417652, 'motion_component': -1.6089514764139317}, {'ion': 1469, 'force': [1.0937838554382324, 3.111398458480835, -0.23599140346050262], 'magnitude': 3.3064868450164795, 'distance': 10.020413398742676, 'cosine_with_motion': -0.7780253814588048, 'motion_component': -2.572530709600221}, {'ion': 2434, 'force': [-1.3929810523986816, 2.763676643371582, -2.991767168045044], 'magnitude': 4.304529666900635, 'distance': 8.782258033752441, 'cosine_with_motion': -0.9510453856970562, 'motion_component': -4.093803070234479}, {'ion': 2444, 'force': [-0.4711344838142395, 0.7824605703353882, -1.5562465190887451], 'magnitude': 1.8044710159301758, 'distance': 13.564197540283203, 'cosine_with_motion': -0.8578010229664738, 'motion_component': -1.5478770422136625}]}, 5423: {'frame': 5423, 'ionic_force': [-7.194524526596069, 10.885988421738148, -3.873266875743866], 'ionic_force_magnitude': 13.611323351266917, 'motion_vector': [-0.2519950866699219, 0.5466041564941406, 0.0637054443359375], 'cosine_ionic_motion': 0.9123871441683606, 'ionic_motion_component': 12.418796440814543, 'ionic_force_x': -7.194524526596069, 'ionic_force_y': 10.885988421738148, 'ionic_force_z': -3.873266875743866, 'radial_force': 13.048598663535078, 'axial_force': -3.873266875743866, 'contributions': [{'ion': 1309, 'force': [-7.53367280960083, -0.03545748442411423, 1.090088963508606], 'magnitude': 7.612212181091309, 'distance': 6.604099273681641, 'cosine_with_motion': 0.4229142947215601, 'motion_component': 3.219313426221046}, {'ion': 1469, 'force': [3.078547954559326, 6.243687152862549, 0.9668325781822205], 'magnitude': 7.0282182693481445, 'distance': 6.873001575469971, 'cosine_with_motion': 0.6343949704708078, 'motion_component': 4.45866631981975}, {'ion': 2434, 'force': [-2.2350199222564697, 3.7992143630981445, -4.083253383636475], 'magnitude': 6.008519172668457, 'distance': 7.4333624839782715, 'cosine_with_motion': 0.654372414694982, 'motion_component': 3.931809165797851}, {'ion': 2444, 'force': [-0.5043797492980957, 0.8785443902015686, -1.8469350337982178], 'magnitude': 2.106515645980835, 'distance': 12.554132461547852, 'cosine_with_motion': 0.3840500646571, 'motion_component': 0.8090074727170524}]}, 5424: {'frame': 5424, 'ionic_force': [-9.829724729061127, 8.064699590206146, -3.82029065862298], 'ionic_force_magnitude': 13.276200075539274, 'motion_vector': [-1.8115425109863281, -1.1403274536132812, 0.10491180419921875], 'cosine_ionic_motion': 0.2885408107742469, 'ionic_motion_component': 3.8307255337972204, 'ionic_force_x': -9.829724729061127, 'ionic_force_y': 8.064699590206146, 'ionic_force_z': -3.82029065862298, 'radial_force': 12.71467135750614, 'axial_force': -3.82029065862298, 'contributions': [{'ion': 1309, 'force': [-8.29712200164795, 0.1777876615524292, 0.9536499381065369], 'magnitude': 8.353639602661133, 'distance': 6.30421781539917, 'cosine_with_motion': 0.8338212823493995, 'motion_component': 6.965442263992603}, {'ion': 1469, 'force': [0.7835202217102051, 3.773498058319092, -0.03277162089943886], 'magnitude': 3.854123115539551, 'distance': 9.281245231628418, 'cosine_with_motion': -0.6932081742710833, 'motion_component': -2.671709695405911}, {'ion': 2434, 'force': [-1.8014920949935913, 3.1987240314483643, -3.0620651245117188], 'magnitude': 4.7805280685424805, 'distance': 8.33357048034668, 'cosine_with_motion': -0.06884699269022612, 'motion_component': -0.3291250055472901}, {'ion': 2444, 'force': [-0.5146308541297913, 0.914689838886261, -1.6791038513183594], 'magnitude': 1.9801243543624878, 'distance': 12.948599815368652, 'cosine_with_motion': -0.06761305818944655, 'motion_component': -0.13388225810879462}]}, 5425: {'frame': 5425, 'ionic_force': [-7.359991593286395, 3.306031584739685, -5.195836968719959], 'ionic_force_magnitude': 9.59666832281182, 'motion_vector': [0.7701644897460938, 1.122161865234375, -0.6427230834960938], 'cosine_ionic_motion': 0.09560626418969688, 'ionic_motion_component': 0.9175016070116421, 'ionic_force_x': -7.359991593286395, 'ionic_force_y': 3.306031584739685, 'ionic_force_z': -5.195836968719959, 'radial_force': 8.068415029765314, 'axial_force': -5.195836968719959, 'contributions': [{'ion': 1309, 'force': [-4.172080993652344, -2.511462926864624, -0.10490787774324417], 'magnitude': 4.87080192565918, 'distance': 8.255983352661133, 'cosine_with_motion': -0.8135006963141567, 'motion_component': -3.9624007676868804}, {'ion': 1469, 'force': [0.024452881887555122, 2.9648444652557373, -0.17231887578964233], 'magnitude': 2.9699485301971436, 'distance': 10.572911262512207, 'cosine_with_motion': 0.77325275445924, 'motion_component': 2.2965209036455843}, {'ion': 2434, 'force': [-2.4676637649536133, 2.1257126331329346, -3.127074718475342], 'magnitude': 4.515153884887695, 'distance': 8.574973106384277, 'cosine_with_motion': 0.36708742493103036, 'motion_component': 1.6574562268455113}, {'ion': 2444, 'force': [-0.7446997165679932, 0.7269374132156372, -1.791535496711731], 'magnitude': 2.0718626976013184, 'distance': 12.658683776855469, 'cosine_with_motion': 0.4469046351630615, 'motion_component': 0.9259250504055956}]}, 5426: {'frame': 5426, 'ionic_force': [-5.71360582113266, 4.7653467655181885, -4.617043234407902], 'ionic_force_magnitude': 8.756192637402826, 'motion_vector': [0.9683570861816406, -1.1876640319824219, -1.7886962890625], 'cosine_ionic_motion': -0.14225960241465066, 'ionic_motion_component': -1.2456524832630174, 'ionic_force_x': -5.71360582113266, 'ionic_force_y': 4.7653467655181885, 'ionic_force_z': -4.617043234407902, 'radial_force': 7.440014870611193, 'axial_force': -4.617043234407902, 'contributions': [{'ion': 1309, 'force': [-3.82336688041687, -1.281545877456665, 0.038811035454273224], 'magnitude': 4.032617092132568, 'distance': 9.073514938354492, 'cosine_with_motion': -0.23686059447804464, 'motion_component': -0.9551680765469284}, {'ion': 1469, 'force': [0.3030494451522827, 3.1069347858428955, -0.22176901996135712], 'magnitude': 3.129547119140625, 'distance': 10.299788475036621, 'cosine_with_motion': -0.40697035549176575, 'motion_component': -1.2736328422891834}, {'ion': 2434, 'force': [-1.6431152820587158, 2.2570924758911133, -2.791811227798462], 'magnitude': 3.948227882385254, 'distance': 9.169970512390137, 'cosine_with_motion': 0.07762936310697147, 'motion_component': 0.306498423729046}, {'ion': 2444, 'force': [-0.5501731038093567, 0.6828653812408447, -1.642274022102356], 'magnitude': 1.8617355823516846, 'distance': 13.353959083557129, 'cosine_with_motion': 0.3634511718692843, 'motion_component': 0.6766499945516973}]}, 5427: {'frame': 5427, 'ionic_force': [-8.04122668504715, 2.214553475379944, -8.471194505691528], 'ionic_force_magnitude': 11.888091101976386, 'motion_vector': [1.9277992248535156, -0.47090911865234375, 1.2962722778320312], 'cosine_ionic_motion': -0.9768244492629804, 'ionic_motion_component': -11.612578043476221, 'ionic_force_x': -8.04122668504715, 'ionic_force_y': 2.214553475379944, 'ionic_force_z': -8.471194505691528, 'radial_force': 8.340597921949707, 'axial_force': -8.471194505691528, 'contributions': [{'ion': 1309, 'force': [-7.151926517486572, -4.424306392669678, -2.266660690307617], 'magnitude': 8.709896087646484, 'distance': 6.1739420890808105, 'cosine_with_motion': -0.7092263629987502, 'motion_component': -6.17728795671141}, {'ion': 1469, 'force': [1.0913169384002686, 4.217013835906982, -1.362021803855896], 'magnitude': 4.563910484313965, 'distance': 8.529046058654785, 'cosine_with_motion': -0.1522963508158204, 'motion_component': -0.6950669595563213}, {'ion': 2434, 'force': [-1.582262396812439, 1.9491033554077148, -3.3685457706451416], 'magnitude': 4.2011494636535645, 'distance': 8.889656066894531, 'cosine_with_motion': -0.8369729709418179, 'motion_component': -3.516248744739322}, {'ion': 2444, 'force': [-0.398354709148407, 0.4727426767349243, -1.4739662408828735], 'magnitude': 1.5983580350875854, 'distance': 14.412257194519043, 'cosine_with_motion': -0.7657695663854323, 'motion_component': -1.2239739834485697}]}, 5428: {'frame': 5428, 'ionic_force': [-4.013658359646797, 2.036353588104248, -10.628021240234375], 'ionic_force_magnitude': 11.541708055856407, 'motion_vector': [0.24727249145507812, -2.330799102783203, -4.778404235839844], 'cosine_ionic_motion': 0.733311095968307, 'ionic_motion_component': 8.4636625837863, 'ionic_force_x': -4.013658359646797, 'ionic_force_y': 2.036353588104248, 'ionic_force_z': -10.628021240234375, 'radial_force': 4.5006876545421, 'axial_force': -10.628021240234375, 'contributions': [{'ion': 1309, 'force': [-4.697807788848877, -6.503828525543213, -1.5563700199127197], 'magnitude': 8.172605514526367, 'distance': 6.373658657073975, 'cosine_with_motion': 0.49277885349233314, 'motion_component': 4.027286881652531}, {'ion': 1469, 'force': [2.3175904750823975, 4.2220258712768555, -0.8517012596130371], 'magnitude': 4.891024589538574, 'distance': 8.238897323608398, 'cosine_with_motion': -0.19967505294610755, 'motion_component': -0.9766156258850804}, {'ion': 2434, 'force': [-1.4328304529190063, 3.6519341468811035, -6.213566780090332], 'magnitude': 7.3483357429504395, 'distance': 6.7216291427612305, 'cosine_with_motion': 0.5324640438268261, 'motion_component': 3.91272456724384}, {'ion': 2444, 'force': [-0.20061059296131134, 0.666222095489502, -2.006383180618286], 'magnitude': 2.123598337173462, 'distance': 12.503536224365234, 'cosine_with_motion': 0.7064737784360602, 'motion_component': 1.5002665511818145}]}, 5429: {'frame': 5429, 'ionic_force': [-0.07442072033882141, -0.02468770742416382, -7.9879608154296875], 'ionic_force_magnitude': 7.9883456306893565, 'motion_vector': [3.7690887451171875, -2.5068588256835938, -3.2027816772460938], 'cosine_ionic_motion': 0.572624250980996, 'ionic_motion_component': 4.574320433350805, 'ionic_force_x': -0.07442072033882141, 'ionic_force_y': -0.02468770742416382, 'ionic_force_z': -7.9879608154296875, 'radial_force': 0.0784087145259389, 'axial_force': -7.9879608154296875, 'contributions': [{'ion': 1309, 'force': [-1.8123735189437866, -2.4131195545196533, -2.5620484352111816], 'magnitude': 3.9587795734405518, 'distance': 9.15774154663086, 'cosine_with_motion': 0.3381963958982721, 'motion_component': 1.3388449937113478}, {'ion': 1469, 'force': [1.9238256216049194, 2.0180952548980713, -2.4386179447174072], 'magnitude': 3.7041423320770264, 'distance': 9.467279434204102, 'cosine_with_motion': 0.4869727291469073, 'motion_component': 1.803816336372222}, {'ion': 2434, 'force': [-0.18587282299995422, 0.3703365921974182, -2.9872944355010986], 'magnitude': 3.0158956050872803, 'distance': 10.492063522338867, 'cosine_with_motion': 0.4747044569942231, 'motion_component': 1.431659057345513}]}, 5430: {'frame': 5430, 'ionic_force': [2.4746485874056816, -1.7678358405828476, -3.220875859260559], 'ionic_force_magnitude': 4.429804791541682, 'motion_vector': [-0.60418701171875, 0.23330307006835938, 2.4262313842773438], 'cosine_ionic_motion': -0.8739764423926943, 'ionic_motion_component': -3.87154503220571, 'ionic_force_x': 2.4746485874056816, 'ionic_force_y': -1.7678358405828476, 'ionic_force_z': -3.220875859260559, 'radial_force': 3.0412381015629473, 'axial_force': -3.220875859260559, 'contributions': [{'ion': 1309, 'force': [0.12402363866567612, -1.6623444557189941, -1.531604528427124], 'magnitude': 2.26375412940979, 'distance': 12.110285758972168, 'cosine_with_motion': -0.7350923070401219, 'motion_component': -1.6640683471142113}, {'ion': 1320, 'force': [0.5745420455932617, -0.34557026624679565, 1.4239434003829956], 'magnitude': 1.5738908052444458, 'distance': 14.523849487304688, 'cosine_with_motion': 0.7658917483680011, 'motion_component': 1.20542995909179}, {'ion': 1469, 'force': [1.4435352087020874, 0.3784688711166382, -1.497428059577942], 'magnitude': 2.11407732963562, 'distance': 12.531660079956055, 'cosine_with_motion': -0.832002319477491, 'motion_component': -1.7589173250676327}, {'ion': 2434, 'force': [0.33254769444465637, -0.13838998973369598, -1.6157866716384888], 'magnitude': 1.6554474830627441, 'distance': 14.161567687988281, 'cosine_with_motion': -0.9991191765221671, 'motion_component': -1.6539893131995007}]}, 5431: {'frame': 5431, 'ionic_force': [3.104661077260971, -1.3943484723567963, -5.393718481063843], 'ionic_force_magnitude': 6.377721154142177, 'motion_vector': [-2.8593292236328125, 1.6220474243164062, -1.3614044189453125], 'cosine_ionic_motion': -0.1672747077358023, 'ionic_motion_component': -1.0668314420795766, 'ionic_force_x': 3.104661077260971, 'ionic_force_y': -1.3943484723567963, 'ionic_force_z': -5.393718481063843, 'radial_force': 3.4033994868400304, 'axial_force': -5.393718481063843, 'contributions': [{'ion': 1309, 'force': [0.6289064884185791, -2.2084546089172363, -1.3620975017547607], 'magnitude': 2.669851064682007, 'distance': 11.151300430297852, 'cosine_with_motion': -0.3711823052455934, 'motion_component': -0.9910014747644809}, {'ion': 1469, 'force': [2.067415952682495, 1.0044293403625488, -1.9814109802246094], 'magnitude': 3.0346460342407227, 'distance': 10.459598541259766, 'cosine_with_motion': -0.14676256689893674, 'motion_component': -0.44537244017870137}, {'ion': 2434, 'force': [0.40833863615989685, -0.19032320380210876, -2.0502099990844727], 'magnitude': 2.0991246700286865, 'distance': 12.576213836669922, 'cosine_with_motion': 0.17604603464467547, 'motion_component': 0.3695425753775714}]}, 5432: {'frame': 5432, 'ionic_force': [1.1073409914970398, -2.299594771116972, -5.362725257873535], 'ionic_force_magnitude': 5.939121346986686, 'motion_vector': [-2.0052490234375, -1.7602043151855469, -0.211578369140625], 'cosine_ionic_motion': 0.18632320852044088, 'ionic_motion_component': 1.106596145162802, 'ionic_force_x': 1.1073409914970398, 'ionic_force_y': -2.299594771116972, 'ionic_force_z': -5.362725257873535, 'radial_force': 2.5523205485985034, 'axial_force': -5.362725257873535, 'contributions': [{'ion': 1309, 'force': [-0.5481927990913391, -3.5546693801879883, -2.8332223892211914], 'magnitude': 4.578573703765869, 'distance': 8.51537799835205, 'cosine_with_motion': 0.6491793774627083, 'motion_component': 2.972315746727638}, {'ion': 1320, 'force': [0.22608864307403564, -0.023177023977041245, 1.754052996635437], 'magnitude': 1.7687156200408936, 'distance': 13.700613975524902, 'cosine_with_motion': -0.1655403146509752, 'motion_component': -0.29279375053671397}, {'ion': 1469, 'force': [1.5149571895599365, 1.144568681716919, -2.3458662033081055], 'magnitude': 3.0179829597473145, 'distance': 10.488433837890625, 'cosine_with_motion': -0.5640343802705116, 'motion_component': -1.7022461345254385}, {'ion': 2434, 'force': [-0.08551204204559326, 0.1336829513311386, -1.9376896619796753], 'magnitude': 1.9441771507263184, 'distance': 13.06775951385498, 'cosine_with_motion': 0.06651673609911267, 'motion_component': 0.12932031630161678}]}, 5433: {'frame': 5433, 'ionic_force': [-0.44162964820861816, -0.36573115549981594, -4.841521263122559], 'ionic_force_magnitude': 4.875358875564747, 'motion_vector': [1.0330657958984375, 1.6155204772949219, -5.069999694824219], 'cosine_ionic_motion': 0.889221364727531, 'ionic_motion_component': 4.335273272866165, 'ionic_force_x': -0.44162964820861816, 'ionic_force_y': -0.36573115549981594, 'ionic_force_z': -4.841521263122559, 'radial_force': 0.5734073807338883, 'axial_force': -4.841521263122559, 'contributions': [{'ion': 1309, 'force': [-0.640687882900238, -1.2333738803863525, -1.1129107475280762], 'magnitude': 1.7805230617523193, 'distance': 13.655111312866211, 'cosine_with_motion': 0.30959821103666846, 'motion_component': 0.551246759031236}, {'ion': 1320, 'force': [-0.537470281124115, 0.01673593558371067, 1.5264745950698853], 'magnitude': 1.6184186935424805, 'distance': 14.322657585144043, 'cosine_with_motion': -0.9424075972696683, 'motion_component': -1.525210077137657}, {'ion': 1469, 'force': [1.1431920528411865, 1.02493155002594, -3.420396089553833], 'magnitude': 3.749197483062744, 'distance': 9.410222053527832, 'cosine_with_motion': 0.9928946105038673, 'motion_component': 3.722558026865098}, {'ion': 2434, 'force': [-0.40666353702545166, -0.174024760723114, -1.8346890211105347], 'magnitude': 1.8872582912445068, 'distance': 13.263354301452637, 'cosine_with_motion': 0.8407321155935801, 'motion_component': 1.586678610431468}]}}</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{5477: {'frame': 5477, 'ionic_force': [1.4224569201469421, -4.641303360462189, -9.415545463562012], 'ionic_force_magnitude': 10.59327980136061, 'motion_vector': [-0.5623664855957031, 0.9072761535644531, 0.3484649658203125], 'cosine_ionic_motion': -0.6970970980387372, 'ionic_motion_component': -7.384544608240852, 'ionic_force_x': 1.4224569201469421, 'ionic_force_y': -4.641303360462189, 'ionic_force_z': -9.415545463562012, 'radial_force': 4.854387765054573, 'axial_force': -9.415545463562012, 'contributions': [{'ion': 1309, 'force': [-0.14590446650981903, -7.744018077850342, -4.193130970001221], 'magnitude': 8.807579040527344, 'distance': 6.1396098136901855, 'directional_contribution': -7.485354932675172}, {'ion': 1469, 'force': [1.5043941736221313, 2.458629608154297, -1.5455207824707031], 'magnitude': 3.270580291748047, 'distance': 10.075268745422363, 'directional_contribution': 0.753494470362682}, {'ion': 2444, 'force': [0.06396721303462982, 0.6440851092338562, -3.676893711090088], 'magnitude': 3.7334280014038086, 'distance': 9.430074691772461, 'directional_contribution': -0.6526841261401124}]}, 5478: {'frame': 5478, 'ionic_force': [3.782637048512697, -4.220937579870224, -11.806665897369385], 'ionic_force_magnitude': 13.096641428474966, 'motion_vector': [5.6822967529296875, -1.4546623229980469, 1.581939697265625], 'cosine_ionic_motion': 0.112572399553655, 'ionic_motion_component': 1.4743203516972347, 'ionic_force_x': 3.782637048512697, 'ionic_force_y': -4.220937579870224, 'ionic_force_z': -11.806665897369385, 'radial_force': 5.667861774420893, 'axial_force': -11.806665897369385, 'contributions': [{'ion': 1309, 'force': [2.848625421524048, -7.680440902709961, -5.491806507110596], 'magnitude': 9.862239837646484, 'distance': 5.802047252655029, 'directional_contribution': 3.0734338476905663}, {'ion': 1469, 'force': [1.1187093257904053, 2.1294939517974854, -1.1434855461120605], 'magnitude': 2.663421392440796, 'distance': 11.164752006530762, 'directional_contribution': 0.23871443615680477}, {'ion': 2443, 'force': [-0.03920864686369896, 0.29816392064094543, -1.4478132724761963], 'magnitude': 1.478716492652893, 'distance': 14.983959197998047, 'directional_contribution': -0.48507299002336723}, {'ion': 2444, 'force': [-0.14548905193805695, 1.0318454504013062, -3.7235605716705322], 'magnitude': 3.8666231632232666, 'distance': 9.266230583190918, 'directional_contribution': -1.3527548319276432}]}, 5479: {'frame': 5479, 'ionic_force': [7.66579008102417, -0.03574265539646149, -6.5100264847278595], 'ionic_force_magnitude': 10.057139749232956, 'motion_vector': [-0.8315162658691406, 0.4536933898925781, 0.4904327392578125], 'cosine_ionic_motion': -0.8933169575861272, 'ionic_motion_component': -8.98421348280329, 'ionic_force_x': 7.66579008102417, 'ionic_force_y': -0.03574265539646149, 'ionic_force_z': -6.5100264847278595, 'radial_force': 7.665873407756179, 'axial_force': -6.5100264847278595, 'contributions': [{'ion': 1309, 'force': [2.8427734375, -2.1192972660064697, -0.8717526197433472], 'magnitude': 3.6514017581939697, 'distance': 9.535407066345215, 'directional_contribution': -3.518300505546865}, {'ion': 1469, 'force': [1.5580865144729614, 1.1739774942398071, -0.4098491966724396], 'magnitude': 1.9934475421905518, 'distance': 12.905256271362305, 'directional_contribution': -0.9037035172938319}, {'ion': 2443, 'force': [0.5962351560592651, 0.1816510409116745, -1.6120604276657104], 'magnitude': 1.7283612489700317, 'distance': 13.859634399414062, 'directional_contribution': -1.1287225779949241}, {'ion': 2444, 'force': [2.6686949729919434, 0.7279260754585266, -3.6163642406463623], 'magnitude': 4.553009986877441, 'distance': 8.539250373840332, 'directional_contribution': -3.433486780340937}]}, 5480: {'frame': 5480, 'ionic_force': [8.63328468799591, 0.006521552801132202, -5.980384021997452], 'ionic_force_magnitude': 10.502315939124951, 'motion_vector': [-2.4467201232910156, 2.9426307678222656, 1.0514373779296875], 'cosine_ionic_motion': -0.6571806221442732, 'ionic_motion_component': -6.9019185228298525, 'ionic_force_x': 8.63328468799591, 'ionic_force_y': 0.006521552801132202, 'ionic_force_z': -5.980384021997452, 'radial_force': 8.633287151174551, 'axial_force': -5.980384021997452, 'contributions': [{'ion': 1309, 'force': [4.6044087409973145, -2.470323085784912, -0.8643374443054199], 'magnitude': 5.296239852905273, 'distance': 7.917448043823242, 'directional_contribution': -4.899202125768213}, {'ion': 1469, 'force': [1.6390438079833984, 1.4995357990264893, -0.4266315996646881], 'magnitude': 2.2620978355407715, 'distance': 12.11471939086914, 'directional_contribution': -0.011660503617133777}, {'ion': 2443, 'force': [0.6318773031234741, 0.20215561985969543, -1.57472562789917], 'magnitude': 1.708770513534546, 'distance': 13.938857078552246, 'directional_contribution': -0.6568511695921728}, {'ion': 2444, 'force': [1.7579548358917236, 0.7751532196998596, -3.114689350128174], 'magnitude': 3.6595845222473145, 'distance': 9.524741172790527, 'directional_contribution': -1.334204640375063}]}, 5481: {'frame': 5481, 'ionic_force': [10.722378462553024, 3.6098837852478027, -5.247070275247097], 'ionic_force_magnitude': 12.471263260415826, 'motion_vector': [1.9404220581054688, -4.451213836669922, 0.8924026489257812], 'cosine_ionic_motion': 0.0008944936529652115, 'ionic_motion_component': 0.011155465830900187, 'ionic_force_x': 10.722378462553024, 'ionic_force_y': 3.6098837852478027, 'ionic_force_z': -5.247070275247097, 'radial_force': 11.313737704101856, 'axial_force': -5.247070275247097, 'contributions': [{'ion': 1309, 'force': [8.690352439880371, -0.589633584022522, -0.05870877951383591], 'magnitude': 8.710530281066895, 'distance': 6.173717498779297, 'directional_contribution': 3.936553096417698}, {'ion': 1469, 'force': [0.9652875065803528, 1.5830146074295044, -0.20551034808158875], 'magnitude': 1.865462303161621, 'distance': 13.34061336517334, 'directional_contribution': -1.0849835709259943}, {'ion': 2443, 'force': [0.3752489387989044, 0.6354923248291016, -1.8373764753341675], 'magnitude': 1.9800541400909424, 'distance': 12.948829650878906, 'directional_contribution': -0.757580910428099}, {'ion': 2444, 'force': [0.691489577293396, 1.9810104370117188, -3.145474672317505], 'magnitude': 3.781080722808838, 'distance': 9.370463371276855, 'directional_contribution': -2.0828331023756945}]}, 5482: {'frame': 5482, 'ionic_force': [10.771212220191956, -0.8395132049918175, -7.971047785133123], 'ionic_force_magnitude': 13.426146055612676, 'motion_vector': [-3.371776580810547, 2.4830093383789062, -2.777191162109375], 'cosine_ionic_motion': -0.24110797819383406, 'ionic_motion_component': -3.2371509304038923, 'ionic_force_x': 10.771212220191956, 'ionic_force_y': -0.8395132049918175, 'ionic_force_z': -7.971047785133123, 'radial_force': 10.803878706916704, 'axial_force': -7.971047785133123, 'contributions': [{'ion': 1309, 'force': [2.8360345363616943, -2.8020989894866943, 0.3442707359790802], 'magnitude': 4.001671314239502, 'distance': 9.10853099822998, 'directional_contribution': -3.4781039011742347}, {'ion': 1469, 'force': [2.137364387512207, 1.547278881072998, -0.054249223321676254], 'magnitude': 2.639193296432495, 'distance': 11.215882301330566, 'directional_contribution': -0.6396771424608481}, {'ion': 2443, 'force': [0.930376410484314, 0.07820767909288406, -2.1504712104797363], 'magnitude': 2.344406843185425, 'distance': 11.900153160095215, 'directional_contribution': 0.6029166436709448}, {'ion': 2444, 'force': [4.86743688583374, 0.33709922432899475, -6.110598087310791], 'magnitude': 7.819525718688965, 'distance': 6.515966415405273, 'directional_contribution': 0.2777134832245567}]}, 5483: {'frame': 5483, 'ionic_force': [14.705014813691378, -4.830581963062286, -13.659503698348999], 'ionic_force_magnitude': 20.64349834834095, 'motion_vector': [-1.0512886047363281, -1.1198539733886719, -3.1050186157226562], 'cosine_ionic_motion': 0.45255552467683335, 'ionic_motion_component': 9.342329226198782, 'ionic_force_x': 14.705014813691378, 'ionic_force_y': -4.830581963062286, 'ionic_force_z': -13.659503698348999, 'radial_force': 15.478113023645536, 'axial_force': -13.659503698348999, 'contributions': [{'ion': 1309, 'force': [12.95172119140625, -9.656329154968262, -6.279929161071777], 'magnitude': 17.332895278930664, 'distance': 4.376565933227539, 'directional_contribution': 4.819917962997209}, {'ion': 1469, 'force': [1.47786545753479, 2.6548736095428467, -0.7496045827865601], 'magnitude': 3.129592180252075, 'distance': 10.299714088439941, 'directional_contribution': -0.6348425513631568}, {'ion': 2443, 'force': [0.023254413157701492, 0.36658936738967896, -1.7489255666732788], 'magnitude': 1.7870839834213257, 'distance': 13.630022048950195, 'directional_contribution': 1.4420434863079719}, {'ion': 2444, 'force': [0.2521737515926361, 1.8042842149734497, -4.881044387817383], 'magnitude': 5.209954738616943, 'distance': 7.982741832733154, 'directional_contribution': 3.7152102230572357}]}, 5484: {'frame': 5484, 'ionic_force': [3.3583530709147453, -1.8520203530788422, -9.582316398620605], 'ionic_force_magnitude': 10.32130332372875, 'motion_vector': [-1.2701416015625, -1.1113739013671875, -2.5788192749023438], 'cosine_ionic_motion': 0.7074375045446344, 'ionic_motion_component': 7.301677066986908, 'ionic_force_x': 3.3583530709147453, 'ionic_force_y': -1.8520203530788422, 'ionic_force_z': -9.582316398620605, 'radial_force': 3.8351681497870183, 'axial_force': -9.582316398620605, 'contributions': [{'ion': 1309, 'force': [2.1952145099639893, -4.486453056335449, -5.257387638092041], 'magnitude': 7.251713752746582, 'distance': 6.766260623931885, 'directional_contribution': 5.112183207305485}, {'ion': 1469, 'force': [1.2880535125732422, 2.27970814704895, -1.8271305561065674], 'magnitude': 3.1928915977478027, 'distance': 10.19710636138916, 'directional_contribution': 0.17593160856745982}, {'ion': 2444, 'force': [-0.12491495162248611, 0.35472455620765686, -2.497798204421997], 'magnitude': 2.5259511470794678, 'distance': 11.46453857421875, 'directional_contribution': 2.0135623682589534}]}, 5485: {'frame': 5485, 'ionic_force': [1.483163833618164, -0.4733795076608658, -5.7409727573394775], 'ionic_force_magnitude': 5.948330128375544, 'motion_vector': [4.385654449462891, -1.0877685546875, 2.3917007446289062], 'cosine_ionic_motion': -0.22068268473215408, 'ionic_motion_component': -1.312693462403074, 'ionic_force_x': 1.483163833618164, 'ionic_force_y': -0.4733795076608658, 'ionic_force_z': -5.7409727573394775, 'radial_force': 1.5568760758731481, 'axial_force': -5.7409727573394775, 'contributions': [{'ion': 1309, 'force': [0.5064878463745117, -2.087893009185791, -3.4851157665252686], 'magnitude': 4.094125270843506, 'distance': 9.005099296569824, 'directional_contribution': -0.7516762541344804}, {'ion': 1469, 'force': [0.7889192700386047, 1.6113115549087524, -1.897242546081543], 'magnitude': 2.611177444458008, 'distance': 11.275890350341797, 'directional_contribution': -0.5536342103565328}, {'ion': 2436, 'force': [0.3979494571685791, -0.12599879503250122, 1.4812759160995483], 'magnitude': 1.538966417312622, 'distance': 14.687723159790039, 'directional_contribution': 1.0611476762695622}, {'ion': 2444, 'force': [-0.2101927399635315, 0.129200741648674, -1.8398903608322144], 'magnitude': 1.8563593626022339, 'distance': 13.373282432556152, 'directional_contribution': -1.0685306575260782}]}, 5486: {'frame': 5486, 'ionic_force': [4.225400745868683, -1.113166643306613, -5.5725942850112915], 'ionic_force_magnitude': 7.081451722937793, 'motion_vector': [-1.728607177734375, 5.325992584228516, 4.6172027587890625], 'cosine_ionic_motion': -0.7581095044957695, 'ionic_motion_component': -5.368515856787083, 'ionic_force_x': 4.225400745868683, 'ionic_force_y': -1.113166643306613, 'ionic_force_z': -5.5725942850112915, 'radial_force': 4.369571081806329, 'axial_force': -5.5725942850112915, 'contributions': [{'ion': 1309, 'force': [2.1206986904144287, -2.4510836601257324, -1.6197460889816284], 'magnitude': 3.623361825942993, 'distance': 9.57223129272461, 'directional_contribution': -3.334295689758271}, {'ion': 1469, 'force': [1.5200526714324951, 1.3517338037490845, -1.3707325458526611], 'magnitude': 2.4528865814208984, 'distance': 11.634034156799316, 'directional_contribution': -0.24211843857373339}, {'ion': 2444, 'force': [0.584649384021759, -0.01381678692996502, -2.582115650177002], 'magnitude': 2.6475133895874023, 'distance': 11.19824504852295, 'directional_contribution': -1.7921018533477944}]}, 5487: {'frame': 5487, 'ionic_force': [15.482393935322762, 3.9336164593696594, -6.411904938519001], 'ionic_force_magnitude': 17.213087618395118, 'motion_vector': [0.3015022277832031, -3.9131088256835938, 0.8899307250976562], 'cosine_ionic_motion': -0.23719556888232954, 'ionic_motion_component': -4.082868109866613, 'ionic_force_x': 15.482393935322762, 'ionic_force_y': 3.9336164593696594, 'ionic_force_z': -6.411904938519001, 'radial_force': 15.974287477629257, 'axial_force': -6.411904938519001, 'contributions': [{'ion': 1309, 'force': [13.761055946350098, -2.1138620376586914, -0.08146259933710098], 'magnitude': 13.922704696655273, 'distance': 4.883230686187744, 'directional_contribution': 3.068396117715446}, {'ion': 1469, 'force': [0.9084755182266235, 1.9054216146469116, -0.2553384602069855], 'magnitude': 2.1263012886047363, 'distance': 12.495586395263672, 'directional_contribution': -1.8411592612795076}, {'ion': 2443, 'force': [0.1551320105791092, 0.6592459082603455, -1.8346444368362427], 'magnitude': 1.9556562900543213, 'distance': 13.029350280761719, 'directional_contribution': -1.0351104068303}, {'ion': 2444, 'force': [0.6577304601669312, 3.4828109741210938, -4.240459442138672], 'magnitude': 5.526669979095459, 'distance': 7.750635147094727, 'directional_contribution': -4.274994714874654}]}, 5488: {'frame': 5488, 'ionic_force': [10.131879150867462, -2.3410739302635193, 1.1676548570394516], 'ionic_force_magnitude': 10.464177948597303, 'motion_vector': [0.2902336120605469, 0.38472747802734375, 0.097137451171875], 'cosine_ionic_motion': 0.41858651573256284, 'ionic_motion_component': 4.380163787508862, 'ionic_force_x': 10.131879150867462, 'ionic_force_y': -2.3410739302635193, 'ionic_force_z': 1.1676548570394516, 'radial_force': 10.398826966285295, 'axial_force': 1.1676548570394516, 'contributions': [{'ion': 1309, 'force': [5.3689775466918945, -8.8337984085083, 14.100717544555664], 'magnitude': 17.484054565429688, 'distance': 4.357605934143066, 'directional_contribution': -0.9573313061794977}, {'ion': 1469, 'force': [2.2769510746002197, 3.038987398147583, 0.0664893239736557], 'magnitude': 3.797943115234375, 'distance': 9.349638938903809, 'directional_contribution': 3.735613939452394}, {'ion': 2443, 'force': [0.3027248978614807, 0.33519941568374634, -2.6992714405059814], 'magnitude': 2.7367987632751465, 'distance': 11.014063835144043, 'directional_contribution': -0.09230570945979721}, {'ion': 2444, 'force': [2.183225631713867, 3.118537664413452, -10.300280570983887], 'magnitude': 10.98123550415039, 'distance': 5.498489856719971, 'directional_contribution': 1.694186662448928}]}, 5489: {'frame': 5489, 'ionic_force': [11.221921682357788, -2.8993600010871887, -5.796612232923508], 'ionic_force_magnitude': 12.959109847507065, 'motion_vector': [-0.5663490295410156, 0.11797332763671875, -0.6750717163085938], 'cosine_ionic_motion': -0.24168081898249347, 'ionic_motion_component': -3.1319682812296037, 'ionic_force_x': 11.221921682357788, 'ionic_force_y': -2.8993600010871887, 'ionic_force_z': -5.796612232923508, 'radial_force': 11.590419089095793, 'axial_force': -5.796612232923508, 'contributions': [{'ion': 1309, 'force': [6.7409892082214355, -7.9767279624938965, 4.073198318481445], 'magnitude': 11.209820747375488, 'distance': 5.442140102386475, 'directional_contribution': -8.44562826709155}, {'ion': 1469, 'force': [2.320533037185669, 3.024193286895752, -0.05600830912590027], 'magnitude': 3.8123161792755127, 'distance': 9.33199691772461, 'directional_contribution': -1.0344288301227174}, {'ion': 2443, 'force': [0.43547987937927246, 0.21962839365005493, -2.5775437355041504], 'magnitude': 2.6232824325561523, 'distance': 11.249844551086426, 'directional_contribution': 1.7089275777366293}, {'ion': 2444, 'force': [1.7249195575714111, 1.8335462808609009, -7.236258506774902], 'magnitude': 7.661636829376221, 'distance': 6.582763671875, 'directional_contribution': 4.639161737269472}]}, 5490: {'frame': 5490, 'ionic_force': [4.6175917610526085, -3.9973922222852707, -10.50867223739624], 'ionic_force_magnitude': 12.154566649763792, 'motion_vector': [0.1108245849609375, -3.2973403930664062, -3.8913345336914062], 'cosine_ionic_motion': 0.8802824710280489, 'ionic_motion_component': 10.699451964729185, 'ionic_force_x': 4.6175917610526085, 'ionic_force_y': -3.9973922222852707, 'ionic_force_z': -10.50867223739624, 'radial_force': 6.107478878434842, 'axial_force': -10.50867223739624, 'contributions': [{'ion': 1309, 'force': [1.3767764568328857, -9.229324340820312, 0.24545180797576904], 'magnitude': 9.334676742553711, 'distance': 5.963749885559082, 'directional_contribution': 5.807817134494535}, {'ion': 1469, 'force': [2.126258611679077, 3.1915740966796875, -0.6759365797042847], 'magnitude': 3.894099473953247, 'distance': 9.233482360839844, 'directional_contribution': -1.5010266361122788}, {'ion': 2443, 'force': [0.12220724672079086, 0.23922725021839142, -2.3671770095825195], 'magnitude': 2.382370948791504, 'distance': 11.80495548248291, 'directional_contribution': 1.6536110358295508}, {'ion': 2444, 'force': [0.9923494458198547, 1.801130771636963, -7.711010456085205], 'magnitude': 7.980508327484131, 'distance': 6.449911594390869, 'directional_contribution': 4.7390504322573275}]}, 5491: {'frame': 5491, 'ionic_force': [3.531671144068241, -3.3812859058380127, -9.039488315582275], 'ionic_force_magnitude': 10.277068864925035, 'motion_vector': [0.054042816162109375, 6.2353515625, 0.45986175537109375], 'cosine_ionic_motion': -0.3898304601081398, 'ionic_motion_component': -4.006314484176764, 'ionic_force_x': 3.531671144068241, 'ionic_force_y': -3.3812859058380127, 'ionic_force_z': -9.039488315582275, 'radial_force': 4.8893553201688125, 'axial_force': -9.039488315582275, 'contributions': [{'ion': 1309, 'force': [0.08836428076028824, -4.612890720367432, -2.9233412742614746], 'magnitude': 5.461913108825684, 'distance': 7.796445369720459, 'directional_contribution': -4.814467416335644}, {'ion': 1469, 'force': [3.120267152786255, 1.8323882818222046, -2.4592511653900146], 'magnitude': 4.375114917755127, 'distance': 8.711126327514648, 'directional_contribution': 1.6734529448831683}, {'ion': 2444, 'force': [0.323039710521698, -0.6007834672927856, -3.656895875930786], 'magnitude': 3.719970941543579, 'distance': 9.44711685180664, 'directional_contribution': -0.865299891166011}]}, 5492: {'frame': 5492, 'ionic_force': [7.392548680305481, -1.4014756679534912, -11.69499546289444], 'ionic_force_magnitude': 13.906359297662114, 'motion_vector': [2.7979888916015625, 1.0762748718261719, 3.96209716796875], 'cosine_ionic_motion': -0.39310618776822775, 'ionic_motion_component': -5.466675889239203, 'ionic_force_x': 7.392548680305481, 'ionic_force_y': -1.4014756679534912, 'ionic_force_z': -11.69499546289444, 'radial_force': 7.524221556981957, 'axial_force': -11.69499546289444, 'contributions': [{'ion': 1309, 'force': [6.099052906036377, -4.69687557220459, -7.9687724113464355], 'magnitude': 11.079730033874512, 'distance': 5.473995685577393, 'directional_contribution': -3.9374786012320016}, {'ion': 1469, 'force': [1.0042378902435303, 1.8420790433883667, -0.7561507821083069], 'magnitude': 2.230137586593628, 'distance': 12.20121955871582, 'directional_contribution': 0.36158019590189205}, {'ion': 2444, 'force': [0.28925788402557373, 1.453320860862732, -2.9700722694396973], 'magnitude': 3.3192079067230225, 'distance': 10.001193046569824, 'directional_contribution': -1.8907777069422327}]}, 5493: {'frame': 5493, 'ionic_force': [10.50127774477005, 5.519231498241425, -3.8027787916362286], 'ionic_force_magnitude': 12.457924271005234, 'motion_vector': [-1.495269775390625, 1.0756874084472656, 0.23244476318359375], 'cosine_ionic_motion': -0.4604190596535929, 'ionic_motion_component': -5.7358657780919025, 'ionic_force_x': 10.50127774477005, 'ionic_force_y': 5.519231498241425, 'ionic_force_z': -3.8027787916362286, 'radial_force': 11.863336402715007, 'axial_force': -3.8027787916362286, 'contributions': [{'ion': 1309, 'force': [7.177574157714844, 0.5480061769485474, 0.4017539322376251], 'magnitude': 7.2096662521362305, 'distance': 6.7859625816345215, 'directional_contribution': -5.412871918936274}, {'ion': 1469, 'force': [0.9419129490852356, 1.280834674835205, -0.03194640204310417], 'magnitude': 1.5902068614959717, 'distance': 14.44914722442627, 'directional_contribution': -0.02050088629485819}, {'ion': 2443, 'force': [0.5624699592590332, 0.8197107911109924, -1.5806218385696411], 'magnitude': 1.8672609329223633, 'distance': 13.334186553955078, 'directional_contribution': -0.17596622429598163}, {'ion': 2444, 'force': [1.8193206787109375, 2.8706798553466797, -2.5919644832611084], 'magnitude': 4.274226188659668, 'distance': 8.813335418701172, 'directional_contribution': -0.1265266770110891}]}, 5494: {'frame': 5494, 'ionic_force': [7.604774683713913, 7.194220662117004, -4.560827128589153], 'ionic_force_magnitude': 11.418868289903429, 'motion_vector': [0.6881828308105469, 0.4589118957519531, 0.434112548828125], 'cosine_ionic_motion': 0.6145182648430363, 'ionic_motion_component': 7.017103127982624, 'ionic_force_x': 7.604774683713913, 'ionic_force_y': 7.194220662117004, 'ionic_force_z': -4.560827128589153, 'radial_force': 10.468496020216431, 'axial_force': -4.560827128589153, 'contributions': [{'ion': 1309, 'force': [5.270052433013916, 1.1801180839538574, -0.09136883914470673], 'magnitude': 5.401340484619141, 'distance': 7.8400397300720215, 'directional_contribution': 4.419669416924913}, {'ion': 1469, 'force': [0.786957323551178, 1.485055923461914, -0.08958549052476883], 'magnitude': 1.6830681562423706, 'distance': 14.04488468170166, 'directional_contribution': 1.2676563817786788}, {'ion': 2443, 'force': [0.3067300617694855, 1.0199345350265503, -1.5694105625152588], 'magnitude': 1.8966810703277588, 'distance': 13.230366706848145, 'directional_contribution': -0.0023062019846715742}, {'ion': 2444, 'force': [1.2410348653793335, 3.5091121196746826, -2.810462236404419], 'magnitude': 4.663982391357422, 'distance': 8.43704891204834, 'directional_contribution': 1.332083575267653}]}, 5495: {'frame': 5495, 'ionic_force': [7.7076713144779205, 6.843995451927185, -3.1370171401649714], 'ionic_force_magnitude': 10.774476663658175, 'motion_vector': [0.6293601989746094, -1.066162109375, -0.34174346923828125], 'cosine_ionic_motion': -0.09927879076110027, 'ionic_motion_component': -1.0696770142516778, 'ionic_force_x': 7.7076713144779205, 'ionic_force_y': 6.843995451927185, 'ionic_force_z': -3.1370171401649714, 'radial_force': 10.307689888526225, 'axial_force': -3.1370171401649714, 'contributions': [{'ion': 1309, 'force': [4.939149856567383, 1.1103832721710205, 0.3859111964702606], 'magnitude': 5.077113151550293, 'distance': 8.08650016784668, 'directional_contribution': 1.3958477346173073}, {'ion': 1469, 'force': [1.0719969272613525, 1.4649080038070679, 0.0071951355785131454], 'magnitude': 1.815264344215393, 'distance': 13.523811340332031, 'directional_contribution': -0.6926524235055304}, {'ion': 2443, 'force': [0.3923477232456207, 1.103355884552002, -1.5097792148590088], 'magnitude': 1.910697340965271, 'distance': 13.181750297546387, 'directional_contribution': -0.3219272821939594}, {'ion': 2444, 'force': [1.3041768074035645, 3.1653482913970947, -2.0203442573547363], 'magnitude': 3.9751853942871094, 'distance': 9.138824462890625, 'directional_contribution': -1.4509450661405054}]}, 5496: {'frame': 5496, 'ionic_force': [8.74626049399376, 6.5846357345581055, -4.182012894656509], 'ionic_force_magnitude': 11.71937422547334, 'motion_vector': [0.7211837768554688, -0.30852508544921875, -0.23809051513671875], 'cosine_ionic_motion': 0.5487553892618503, 'ionic_motion_component': 6.431069765004918, 'ionic_force_x': 8.74626049399376, 'ionic_force_y': 6.5846357345581055, 'ionic_force_z': -4.182012894656509, 'radial_force': 10.947808017389395, 'axial_force': -4.182012894656509, 'contributions': [{'ion': 1309, 'force': [5.159459590911865, 1.0115982294082642, -0.0068298703990876675], 'magnitude': 5.257699489593506, 'distance': 7.946413516998291, 'directional_contribution': 4.160371529084642}, {'ion': 1469, 'force': [1.318227767944336, 1.3875240087509155, 0.040635738521814346], 'magnitude': 1.9143141508102417, 'distance': 13.169292449951172, 'directional_contribution': 0.6257115470666249}, {'ion': 2443, 'force': [0.47910425066947937, 1.0934357643127441, -1.6458216905593872], 'magnitude': 2.0331923961639404, 'distance': 12.778497695922852, 'directional_contribution': 0.48798672728567816}, {'ion': 2444, 'force': [1.7894688844680786, 3.0920777320861816, -2.5699970722198486], 'magnitude': 4.400912284851074, 'distance': 8.68555736541748, 'directional_contribution': 1.1570000549089627}]}, 5497: {'frame': 5497, 'ionic_force': [6.961087644100189, 5.41208153963089, -4.26440330222249], 'ionic_force_magnitude': 9.794513939163284, 'motion_vector': [-1.509521484375, 1.9396095275878906, 0.17327117919921875], 'cosine_ionic_motion': -0.031056908057381913, 'ionic_motion_component': -0.3041873188753397, 'ionic_force_x': 6.961087644100189, 'ionic_force_y': 5.41208153963089, 'ionic_force_z': -4.26440330222249, 'radial_force': 8.81744678353421, 'axial_force': -4.26440330222249, 'contributions': [{'ion': 1309, 'force': [3.2068612575531006, 0.40660589933395386, -0.12844008207321167], 'magnitude': 3.235086441040039, 'distance': 10.130388259887695, 'directional_contribution': -1.6536538458867085}, {'ion': 1469, 'force': [1.2073882818222046, 1.2977768182754517, -0.038394588977098465], 'magnitude': 1.772987723350525, 'distance': 13.684098243713379, 'directional_contribution': 0.27921242850128447}, {'ion': 2443, 'force': [0.6200312972068787, 1.031477451324463, -1.5388377904891968], 'magnitude': 1.9535624980926514, 'distance': 13.036331176757812, 'directional_contribution': 0.32390903411250704}, {'ion': 2444, 'force': [1.9268068075180054, 2.6762213706970215, -2.5587308406829834], 'magnitude': 4.173948764801025, 'distance': 8.918575286865234, 'directional_contribution': 0.7463453587972211}]}, 5498: {'frame': 5498, 'ionic_force': [4.10741001367569, 5.098243832588196, -3.6214068830013275], 'ionic_force_magnitude': 7.481810944498417, 'motion_vector': [-0.3549995422363281, 0.2932014465332031, 0.5114364624023438], 'cosine_ionic_motion': -0.352603884698631, 'ionic_motion_component': -2.6381156036108755, 'ionic_force_x': 4.10741001367569, 'ionic_force_y': 5.098243832588196, 'ionic_force_z': -3.6214068830013275, 'radial_force': 6.54697695100318, 'axial_force': -3.6214068830013275, 'contributions': [{'ion': 1309, 'force': [2.7465009689331055, 1.1063706874847412, -0.25553974509239197], 'magnitude': 2.971973180770874, 'distance': 10.56930923461914, 'directional_contribution': -1.1353664041428075}, {'ion': 2443, 'force': [0.3203471302986145, 1.1662036180496216, -1.4032648801803589], 'magnitude': 1.852513313293457, 'distance': 13.387157440185547, 'directional_contribution': -0.71127933747524}, {'ion': 2444, 'force': [1.0405619144439697, 2.825669527053833, -1.9626022577285767], 'magnitude': 3.594299077987671, 'distance': 9.61085319519043, 'directional_contribution': -0.791469925361028}]}, 5499: {'frame': 5499, 'ionic_force': [4.963673681020737, 6.609779596328735, -3.376120550557971], 'ionic_force_magnitude': 8.9289099388224, 'motion_vector': [0.3253974914550781, -0.08216476440429688, -0.2378997802734375], 'cosine_ionic_motion': 0.5105307809870959, 'ionic_motion_component': 4.558483364430443, 'ionic_force_x': 4.963673681020737, 'ionic_force_y': 6.609779596328735, 'ionic_force_z': -3.376120550557971, 'radial_force': 8.266029441255434, 'axial_force': -3.376120550557971, 'contributions': [{'ion': 1309, 'force': [3.1469173431396484, 1.3124815225601196, -0.09989611059427261], 'magnitude': 3.4111106395721436, 'distance': 9.865546226501465, 'directional_contribution': 2.2848262464939917}, {'ion': 1469, 'force': [0.7330875396728516, 1.2971830368041992, -0.008259242400527], 'magnitude': 1.4900232553482056, 'distance': 14.92699909210205, 'directional_contribution': 0.3255579170800985}, {'ion': 2443, 'force': [0.2510865032672882, 1.1263843774795532, -1.4073807001113892], 'magnitude': 1.8200292587280273, 'distance': 13.506096839904785, 'directional_contribution': 0.787524601535635}, {'ion': 2444, 'force': [0.8325822949409485, 2.8737306594848633, -1.8605844974517822], 'magnitude': 3.5232508182525635, 'distance': 9.707273483276367, 'directional_contribution': 1.1605744432274108}]}, 5500: {'frame': 5500, 'ionic_force': [5.459194302558899, 5.718991637229919, -2.9895115792751312], 'ionic_force_magnitude': 8.45262369104513, 'motion_vector': [2.9813499450683594, -5.0980072021484375, -0.931304931640625], 'cosine_ionic_motion': -0.19976887581490052, 'ionic_motion_component': -1.6885711324464805, 'ionic_force_x': 5.459194302558899, 'ionic_force_y': 5.718991637229919, 'ionic_force_z': -2.9895115792751312, 'radial_force': 7.906305570859079, 'axial_force': -2.9895115792751312, 'contributions': [{'ion': 1309, 'force': [4.1073384284973145, 2.204691171646118, 0.19625237584114075], 'magnitude': 4.665769577026367, 'distance': 8.435433387756348, 'directional_contribution': 0.1376726661623504}, {'ion': 2443, 'force': [0.4238545298576355, 0.9974464178085327, -1.3428990840911865], 'magnitude': 1.725667953491211, 'distance': 13.870445251464844, 'directional_contribution': -0.4299697665107587}, {'ion': 2444, 'force': [0.928001344203949, 2.5168540477752686, -1.8428648710250854], 'magnitude': 3.254518508911133, 'distance': 10.100099563598633, 'directional_contribution': -1.396274131536721}]}, 5501: {'frame': 5501, 'ionic_force': [7.573021769523621, 1.5885308384895325, -4.311880387365818], 'ionic_force_magnitude': 8.858126292927919, 'motion_vector': [-1.8371849060058594, 3.13043212890625, 0.7911148071289062], 'cosine_ionic_motion': -0.3753402319335324, 'ionic_motion_component': -3.3248111772840865, 'ionic_force_x': 7.573021769523621, 'ionic_force_y': 1.5885308384895325, 'ionic_force_z': -4.311880387365818, 'radial_force': 7.737834900442818, 'axial_force': -4.311880387365818, 'contributions': [{'ion': 1309, 'force': [3.218261957168579, -0.9777354598045349, -0.12876777350902557], 'magnitude': 3.3659706115722656, 'distance': 9.931477546691895, 'directional_contribution': -2.442884056028147}, {'ion': 1469, 'force': [1.2849994897842407, 1.0848615169525146, -0.10196994990110397], 'magnitude': 1.6847984790802002, 'distance': 14.037671089172363, 'directional_contribution': 0.25697211549839205}, {'ion': 2443, 'force': [0.7342042922973633, 0.28474247455596924, -1.428147792816162], 'magnitude': 1.6308709383010864, 'distance': 14.26787281036377, 'directional_contribution': -0.42728404033350387}, {'ion': 2444, 'force': [2.3355560302734375, 1.1966623067855835, -2.6529948711395264], 'magnitude': 3.7316489219665527, 'distance': 9.43232250213623, 'directional_contribution': -0.7116151885375679}]}, 5502: {'frame': 5502, 'ionic_force': [9.961987733840942, 4.5200366377830505, -3.4055233784019947], 'ionic_force_magnitude': 11.457291141318747, 'motion_vector': [-0.2687187194824219, 0.6909828186035156, 1.2530059814453125], 'cosine_ionic_motion': -0.22905580256794522, 'ionic_motion_component': -2.6243590176293745, 'ionic_force_x': 9.961987733840942, 'ionic_force_y': 4.5200366377830505, 'ionic_force_z': -3.4055233784019947, 'radial_force': 10.939466660495771, 'axial_force': -3.4055233784019947, 'contributions': [{'ion': 1309, 'force': [6.560629367828369, -0.4574304223060608, 0.8440222144126892], 'magnitude': 6.630495548248291, 'distance': 7.076133728027344, 'directional_contribution': -0.7016034353266942}, {'ion': 1469, 'force': [0.9992931485176086, 1.4651027917861938, -0.03822602704167366], 'magnitude': 1.7738585472106934, 'distance': 13.68073844909668, 'directional_contribution': 0.47800466491294014}, {'ion': 2443, 'force': [0.5734100937843323, 0.882344126701355, -1.5693317651748657], 'magnitude': 1.889479398727417, 'distance': 13.255556106567383, 'directional_contribution': -1.037685989808983}, {'ion': 2444, 'force': [1.8286551237106323, 2.6300201416015625, -2.6419878005981445], 'magnitude': 4.152238368988037, 'distance': 8.94186019897461, 'directional_contribution': -1.3630744535531782}]}, 5503: {'frame': 5503, 'ionic_force': [10.119293808937073, 6.6088771522045135, -2.062005452811718</t>
+          <t>{5477: {'frame': 5477, 'ionic_force': [1.4224569201469421, -4.641303360462189, -9.415545463562012], 'ionic_force_magnitude': 10.59327980136061, 'motion_vector': [-0.5623664855957031, 0.9072761535644531, 0.3484649658203125], 'cosine_ionic_motion': -0.6970970980387372, 'ionic_motion_component': -7.384544608240852, 'ionic_force_x': 1.4224569201469421, 'ionic_force_y': -4.641303360462189, 'ionic_force_z': -9.415545463562012, 'radial_force': 4.854387765054573, 'axial_force': -9.415545463562012, 'contributions': [{'ion': 1309, 'force': [-0.14590446650981903, -7.744018077850342, -4.193130970001221], 'magnitude': 8.807579040527344, 'distance': 6.1396098136901855, 'cosine_with_motion': -0.8498765392041681, 'motion_component': -7.485354932675172}, {'ion': 1469, 'force': [1.5043941736221313, 2.458629608154297, -1.5455207824707031], 'magnitude': 3.270580291748047, 'distance': 10.075268745422363, 'cosine_with_motion': 0.23038555492130164, 'motion_component': 0.753494470362682}, {'ion': 2444, 'force': [0.06396721303462982, 0.6440851092338562, -3.676893711090088], 'magnitude': 3.7334280014038086, 'distance': 9.430074691772461, 'cosine_with_motion': -0.174821671211077, 'motion_component': -0.6526841261401124}]}, 5478: {'frame': 5478, 'ionic_force': [3.782637048512697, -4.220937579870224, -11.806665897369385], 'ionic_force_magnitude': 13.096641428474966, 'motion_vector': [5.6822967529296875, -1.4546623229980469, 1.581939697265625], 'cosine_ionic_motion': 0.112572399553655, 'ionic_motion_component': 1.4743203516972347, 'ionic_force_x': 3.782637048512697, 'ionic_force_y': -4.220937579870224, 'ionic_force_z': -11.806665897369385, 'radial_force': 5.667861774420893, 'axial_force': -11.806665897369385, 'contributions': [{'ion': 1309, 'force': [2.848625421524048, -7.680440902709961, -5.491806507110596], 'magnitude': 9.862239837646484, 'distance': 5.802047252655029, 'cosine_with_motion': 0.311636488808021, 'motion_component': 3.073433847690566}, {'ion': 1469, 'force': [1.1187093257904053, 2.1294939517974854, -1.1434855461120605], 'magnitude': 2.663421392440796, 'distance': 11.164752006530762, 'cosine_with_motion': 0.08962698302468124, 'motion_component': 0.23871443615680477}, {'ion': 2443, 'force': [-0.03920864686369896, 0.29816392064094543, -1.4478132724761963], 'magnitude': 1.478716492652893, 'distance': 14.983959197998047, 'cosine_with_motion': -0.3280365163349735, 'motion_component': -0.48507299002336723}, {'ion': 2444, 'force': [-0.14548905193805695, 1.0318454504013062, -3.7235605716705322], 'magnitude': 3.8666231632232666, 'distance': 9.266230583190918, 'cosine_with_motion': -0.34985431505545295, 'motion_component': -1.3527548319276432}]}, 5479: {'frame': 5479, 'ionic_force': [7.66579008102417, -0.03574265539646149, -6.5100264847278595], 'ionic_force_magnitude': 10.057139749232956, 'motion_vector': [-0.8315162658691406, 0.4536933898925781, 0.4904327392578125], 'cosine_ionic_motion': -0.8933169575861272, 'ionic_motion_component': -8.98421348280329, 'ionic_force_x': 7.66579008102417, 'ionic_force_y': -0.03574265539646149, 'ionic_force_z': -6.5100264847278595, 'radial_force': 7.665873407756179, 'axial_force': -6.5100264847278595, 'contributions': [{'ion': 1309, 'force': [2.8427734375, -2.1192972660064697, -0.8717526197433472], 'magnitude': 3.6514017581939697, 'distance': 9.535407066345215, 'cosine_with_motion': -0.963547918868339, 'motion_component': -3.518300505546865}, {'ion': 1469, 'force': [1.5580865144729614, 1.1739774942398071, -0.4098491966724396], 'magnitude': 1.9934475421905518, 'distance': 12.905256271362305, 'cosine_with_motion': -0.4533369941770629, 'motion_component': -0.9037035172938319}, {'ion': 2443, 'force': [0.5962351560592651, 0.1816510409116745, -1.6120604276657104], 'magnitude': 1.7283612489700317, 'distance': 13.859634399414062, 'cosine_with_motion': -0.6530594455283119, 'motion_component': -1.1287225779949241}, {'ion': 2444, 'force': [2.6686949729919434, 0.7279260754585266, -3.6163642406463623], 'magnitude': 4.553009986877441, 'distance': 8.539250373840332, 'cosine_with_motion': -0.7541136132982074, 'motion_component': -3.433486780340937}]}, 5480: {'frame': 5480, 'ionic_force': [8.63328468799591, 0.006521552801132202, -5.980384021997452], 'ionic_force_magnitude': 10.502315939124951, 'motion_vector': [-2.4467201232910156, 2.9426307678222656, 1.0514373779296875], 'cosine_ionic_motion': -0.6571806221442732, 'ionic_motion_component': -6.9019185228298525, 'ionic_force_x': 8.63328468799591, 'ionic_force_y': 0.006521552801132202, 'ionic_force_z': -5.980384021997452, 'radial_force': 8.633287151174551, 'axial_force': -5.980384021997452, 'contributions': [{'ion': 1309, 'force': [4.6044087409973145, -2.470323085784912, -0.8643374443054199], 'magnitude': 5.296239852905273, 'distance': 7.917448043823242, 'cosine_with_motion': -0.9250340582306482, 'motion_component': -4.899202125768213}, {'ion': 1469, 'force': [1.6390438079833984, 1.4995357990264893, -0.4266315996646881], 'magnitude': 2.2620978355407715, 'distance': 12.11471939086914, 'cosine_with_motion': -0.005154729957164885, 'motion_component': -0.011660503617133777}, {'ion': 2443, 'force': [0.6318773031234741, 0.20215561985969543, -1.57472562789917], 'magnitude': 1.708770513534546, 'distance': 13.938857078552246, 'cosine_with_motion': -0.38439987659516817, 'motion_component': -0.6568511695921728}, {'ion': 2444, 'force': [1.7579548358917236, 0.7751532196998596, -3.114689350128174], 'magnitude': 3.6595845222473145, 'distance': 9.524741172790527, 'cosine_with_motion': -0.36457819253244267, 'motion_component': -1.334204640375063}]}, 5481: {'frame': 5481, 'ionic_force': [10.722378462553024, 3.6098837852478027, -5.247070275247097], 'ionic_force_magnitude': 12.471263260415826, 'motion_vector': [1.9404220581054688, -4.451213836669922, 0.8924026489257812], 'cosine_ionic_motion': 0.0008944936529652115, 'ionic_motion_component': 0.011155465830900187, 'ionic_force_x': 10.722378462553024, 'ionic_force_y': 3.6098837852478027, 'ionic_force_z': -5.247070275247097, 'radial_force': 11.313737704101856, 'axial_force': -5.247070275247097, 'contributions': [{'ion': 1309, 'force': [8.690352439880371, -0.589633584022522, -0.05870877951383591], 'magnitude': 8.710530281066895, 'distance': 6.173717498779297, 'cosine_with_motion': 0.45193035456920416, 'motion_component': 3.9365530964176982}, {'ion': 1469, 'force': [0.9652875065803528, 1.5830146074295044, -0.20551034808158875], 'magnitude': 1.865462303161621, 'distance': 13.34061336517334, 'cosine_with_motion': -0.5816164448618182, 'motion_component': -1.0849835709259943}, {'ion': 2443, 'force': [0.3752489387989044, 0.6354923248291016, -1.8373764753341675], 'magnitude': 1.9800541400909424, 'distance': 12.948829650878906, 'cosine_with_motion': -0.3826061510855403, 'motion_component': -0.757580910428099}, {'ion': 2444, 'force': [0.691489577293396, 1.9810104370117188, -3.145474672317505], 'magnitude': 3.781080722808838, 'distance': 9.370463371276855, 'cosine_with_motion': -0.5508565617056489, 'motion_component': -2.0828331023756945}]}, 5482: {'frame': 5482, 'ionic_force': [10.771212220191956, -0.8395132049918175, -7.971047785133123], 'ionic_force_magnitude': 13.426146055612676, 'motion_vector': [-3.371776580810547, 2.4830093383789062, -2.777191162109375], 'cosine_ionic_motion': -0.24110797819383406, 'ionic_motion_component': -3.2371509304038923, 'ionic_force_x': 10.771212220191956, 'ionic_force_y': -0.8395132049918175, 'ionic_force_z': -7.971047785133123, 'radial_force': 10.803878706916704, 'axial_force': -7.971047785133123, 'contributions': [{'ion': 1309, 'force': [2.8360345363616943, -2.8020989894866943, 0.3442707359790802], 'magnitude': 4.001671314239502, 'distance': 9.10853099822998, 'cosine_with_motion': -0.8691628231816363, 'motion_component': -3.4781039011742347}, {'ion': 1469, 'force': [2.137364387512207, 1.547278881072998, -0.054249223321676254], 'magnitude': 2.639193296432495, 'distance': 11.215882301330566, 'cosine_with_motion': -0.24237600744025303, 'motion_component': -0.6396771424608481}, {'ion': 2443, 'force': [0.930376410484314, 0.07820767909288406, -2.1504712104797363], 'magnitude': 2.344406843185425, 'distance': 11.900153160095215, 'cosine_with_motion': 0.25717236860653303, 'motion_component': 0.6029166436709448}, {'ion': 2444, 'force': [4.86743688583374, 0.33709922432899475, -6.110598087310791], 'magnitude': 7.819525718688965, 'distance': 6.515966415405273, 'cosine_with_motion': 0.035515385916932506, 'motion_component': 0.2777134832245567}]}, 5483: {'frame': 5483, 'ionic_force': [14.705014813691378, -4.830581963062286, -13.659503698348999], 'ionic_force_magnitude': 20.64349834834095, 'motion_vector': [-1.0512886047363281, -1.1198539733886719, -3.1050186157226562], 'cosine_ionic_motion': 0.45255552467683335, 'ionic_motion_component': 9.342329226198782, 'ionic_force_x': 14.705014813691378, 'ionic_force_y': -4.830581963062286, 'ionic_force_z': -13.659503698348999, 'radial_force': 15.478113023645536, 'axial_force': -13.659503698348999, 'contributions': [{'ion': 1309, 'force': [12.95172119140625, -9.656329154968262, -6.279929161071777], 'magnitude': 17.332895278930664, 'distance': 4.376565933227539, 'cosine_with_motion': 0.27807920582061574, 'motion_component': 4.819917962997209}, {'ion': 1469, 'force': [1.47786545753479, 2.6548736095428467, -0.7496045827865601], 'magnitude': 3.129592180252075, 'distance': 10.299714088439941, 'cosine_with_motion': -0.20285152649453522, 'motion_component': -0.6348425513631568}, {'ion': 2443, 'force': [0.023254413157701492, 0.36658936738967896, -1.7489255666732788], 'magnitude': 1.7870839834213257, 'distance': 13.630022048950195, 'cosine_with_motion': 0.8069254149980343, 'motion_component': 1.4420434863079719}, {'ion': 2444, 'force': [0.2521737515926361, 1.8042842149734497, -4.881044387817383], 'magnitude': 5.209954738616943, 'distance': 7.982741832733154, 'cosine_with_motion': 0.7130983805644391, 'motion_component': 3.7152102230572357}]}, 5484: {'frame': 5484, 'ionic_force': [3.3583530709147453, -1.8520203530788422, -9.582316398620605], 'ionic_force_magnitude': 10.32130332372875, 'motion_vector': [-1.2701416015625, -1.1113739013671875, -2.5788192749023438], 'cosine_ionic_motion': 0.7074375045446344, 'ionic_motion_component': 7.301677066986908, 'ionic_force_x': 3.3583530709147453, 'ionic_force_y': -1.8520203530788422, 'ionic_force_z': -9.582316398620605, 'radial_force': 3.8351681497870183, 'axial_force': -9.582316398620605, 'contributions': [{'ion': 1309, 'force': [2.1952145099639893, -4.486453056335449, -5.257387638092041], 'magnitude': 7.251713752746582, 'distance': 6.766260623931885, 'cosine_with_motion': 0.7049620782123642, 'motion_component': 5.112183207305485}, {'ion': 1469, 'force': [1.2880535125732422, 2.27970814704895, -1.8271305561065674], 'magnitude': 3.1928915977478027, 'distance': 10.19710636138916, 'cosine_with_motion': 0.05510102667779303, 'motion_component': 0.17593160856745982}, {'ion': 2444, 'force': [-0.12491495162248611, 0.35472455620765686, -2.497798204421997], 'magnitude': 2.5259511470794678, 'distance': 11.46453857421875, 'cosine_with_motion': 0.7971501673219711, 'motion_component': 2.0135623682589534}]}, 5485: {'frame': 5485, 'ionic_force': [1.483163833618164, -0.4733795076608658, -5.7409727573394775], 'ionic_force_magnitude': 5.948330128375544, 'motion_vector': [4.385654449462891, -1.0877685546875, 2.3917007446289062], 'cosine_ionic_motion': -0.22068268473215408, 'ionic_motion_component': -1.312693462403074, 'ionic_force_x': 1.483163833618164, 'ionic_force_y': -0.4733795076608658, 'ionic_force_z': -5.7409727573394775, 'radial_force': 1.5568760758731481, 'axial_force': -5.7409727573394775, 'contributions': [{'ion': 1309, 'force': [0.5064878463745117, -2.087893009185791, -3.4851157665252686], 'magnitude': 4.094125270843506, 'distance': 9.005099296569824, 'cosine_with_motion': -0.18359875780452614, 'motion_component': -0.7516762541344804}, {'ion': 1469, 'force': [0.7889192700386047, 1.6113115549087524, -1.897242546081543], 'magnitude': 2.611177444458008, 'distance': 11.275890350341797, 'cosine_with_motion': -0.21202473408075306, 'motion_component': -0.5536342103565328}, {'ion': 2436, 'force': [0.3979494571685791, -0.12599879503250122, 1.4812759160995483], 'magnitude': 1.538966417312622, 'distance': 14.687723159790039, 'cosine_with_motion': 0.6895196838728914, 'motion_component': 1.0611476762695622}, {'ion': 2444, 'force': [-0.2101927399635315, 0.129200741648674, -1.8398903608322144], 'magnitude': 1.8563593626022339, 'distance': 13.373282432556152, 'cosine_with_motion': -0.5756054760786232, 'motion_component': -1.0685306575260782}]}, 5486: {'frame': 5486, 'ionic_force': [4.225400745868683, -1.113166643306613, -5.5725942850112915], 'ionic_force_magnitude': 7.081451722937793, 'motion_vector': [-1.728607177734375, 5.325992584228516, 4.6172027587890625], 'cosine_ionic_motion': -0.7581095044957695, 'ionic_motion_component': -5.368515856787083, 'ionic_force_x': 4.225400745868683, 'ionic_force_y': -1.113166643306613, 'ionic_force_z': -5.5725942850112915, 'radial_force': 4.369571081806329, 'axial_force': -5.5725942850112915, 'contributions': [{'ion': 1309, 'force': [2.1206986904144287, -2.4510836601257324, -1.6197460889816284], 'magnitude': 3.623361825942993, 'distance': 9.57223129272461, 'cosine_with_motion': -0.9202215468575357, 'motion_component': -3.334295689758271}, {'ion': 1469, 'force': [1.5200526714324951, 1.3517338037490845, -1.3707325458526611], 'magnitude': 2.4528865814208984, 'distance': 11.634034156799316, 'cosine_with_motion': -0.098707559429281, 'motion_component': -0.24211843857373339}, {'ion': 2444, 'force': [0.584649384021759, -0.01381678692996502, -2.582115650177002], 'magnitude': 2.6475133895874023, 'distance': 11.19824504852295, 'cosine_with_motion': -0.6769000204594124, 'motion_component': -1.7921018533477944}]}, 5487: {'frame': 5487, 'ionic_force': [15.482393935322762, 3.9336164593696594, -6.411904938519001], 'ionic_force_magnitude': 17.213087618395118, 'motion_vector': [0.3015022277832031, -3.9131088256835938, 0.8899307250976562], 'cosine_ionic_motion': -0.23719556888232954, 'ionic_motion_component': -4.082868109866613, 'ionic_force_x': 15.482393935322762, 'ionic_force_y': 3.9336164593696594, 'ionic_force_z': -6.411904938519001, 'radial_force': 15.974287477629257, 'axial_force': -6.411904938519001, 'contributions': [{'ion': 1309, 'force': [13.761055946350098, -2.1138620376586914, -0.08146259933710098], 'magnitude': 13.922704696655273, 'distance': 4.883230686187744, 'cosine_with_motion': 0.22038793154140668, 'motion_component': 3.068396117715446}, {'ion': 1469, 'force': [0.9084755182266235, 1.9054216146469116, -0.2553384602069855], 'magnitude': 2.1263012886047363, 'distance': 12.495586395263672, 'cosine_with_motion': -0.8658976507435727, 'motion_component': -1.8411592612795076}, {'ion': 2443, 'force': [0.1551320105791092, 0.6592459082603455, -1.8346444368362427], 'magnitude': 1.9556562900543213, 'distance': 13.029350280761719, 'cosine_with_motion': -0.5292905712008917, 'motion_component': -1.0351104068303}, {'ion': 2444, 'force': [0.6577304601669312, 3.4828109741210938, -4.240459442138672], 'magnitude': 5.526669979095459, 'distance': 7.750635147094727, 'cosine_with_motion': -0.7735209358664246, 'motion_component': -4.274994714874654}]}, 5488: {'frame': 5488, 'ionic_force': [10.131879150867462, -2.3410739302635193, 1.1676548570394516], 'ionic_force_magnitude': 10.464177948597303, 'motion_vector': [0.2902336120605469, 0.38472747802734375, 0.097137451171875], 'cosine_ionic_motion': 0.41858651573256284, 'ionic_motion_component': 4.380163787508862, 'ionic_force_x': 10.131879150867462, 'ionic_force_y': -2.3410739302635193, 'ionic_force_z': 1.1676548570394516, 'radial_force': 10.398826966285295, 'axial_force': 1.1676548570394516, 'contributions': [{'ion': 1309, 'force': [5.3689775466918945, -8.8337984085083, 14.100717544555664], 'magnitude': 17.484054565429688, 'distance': 4.357605934143066, 'cosine_with_motion': -0.054754537935703916, 'motion_component': -0.9573313061794977}, {'ion': 1469, 'force': [2.2769510746002197, 3.038987398147583, 0.0664893239736557], 'magnitude': 3.797943115234375, 'distance': 9.349638938903809, 'cosine_with_motion': 0.9835887182888736, 'motion_component': 3.735613939452394}, {'ion': 2443, 'force': [0.3027248978614807, 0.33519941568374634, -2.6992714405059814], 'magnitude': 2.7367987632751465, 'distance': 11.014063835144043, 'cosine_with_motion': -0.03372762061171953, 'motion_component': -0.09230570945979721}, {'ion': 2444, 'force': [2.183225631713867, 3.118537664413452, -10.300280570983887], 'magnitude': 10.98123550415039, 'distance': 5.498489856719971, 'cosine_with_motion': 0.15428015145398466, 'motion_component': 1.694186662448928}]}, 5489: {'frame': 5489, 'ionic_force': [11.221921682357788, -2.8993600010871887, -5.796612232923508], 'ionic_force_magnitude': 12.959109847507065, 'motion_vector': [-0.5663490295410156, 0.11797332763671875, -0.6750717163085938], 'cosine_ionic_motion': -0.24168081898249347, 'ionic_motion_component': -3.1319682812296037, 'ionic_force_x': 11.221921682357788, 'ionic_force_y': -2.8993600010871887, 'ionic_force_z': -5.796612232923508, 'radial_force': 11.590419089095793, 'axial_force': -5.796612232923508, 'contributions': [{'ion': 1309, 'force': [6.7409892082214355, -7.9767279624938965, 4.073198318481445], 'magnitude': 11.209820747375488, 'distance': 5.442140102386475, 'cosine_with_motion': -0.7534133565420311, 'motion_component': -8.44562826709155}, {'ion': 1469, 'force': [2.320533037185669, 3.024193286895752, -0.05600830912590027], 'magnitude': 3.8123161792755127, 'distance': 9.33199691772461, 'cosine_with_motion': -0.27133866911752824, 'motion_component': -1.0344288301227174}, {'ion': 2443, 'force': [0.43547987937927246, 0.21962839365005493, -2.5775437355041504], 'magnitude': 2.6232824325561523, 'distance': 11.249844551086426, 'cosine_with_motion': 0.6514462620569944, 'motion_component': 1.7089275777366293}, {'ion': 2444, 'force': [1.7249195575714111, 1.8335462808609009, -7.236258506774902], 'magnitude': 7.661636829376221, 'distance': 6.582763671875, 'cosine_with_motion': 0.6055053157498032, 'motion_component': 4.639161737269472}]}, 5490: {'frame': 5490, 'ionic_force': [4.6175917610526085, -3.9973922222852707, -10.50867223739624], 'ionic_force_magnitude': 12.154566649763792, 'motion_vector': [0.1108245849609375, -3.2973403930664062, -3.8913345336914062], 'cosine_ionic_motion': 0.8802824710280489, 'ionic_motion_component': 10.699451964729185, 'ionic_force_x': 4.6175917610526085, 'ionic_force_y': -3.9973922222852707, 'ionic_force_z': -10.50867223739624, 'radial_force': 6.107478878434842, 'axial_force': -10.50867223739624, 'contributions': [{'ion': 1309, 'force': [1.3767764568328857, -9.229324340820312, 0.24545180797576904], 'magnitude': 9.334676742553711, 'distance': 5.963749885559082, 'cosine_with_motion': 0.6221765749990734, 'motion_component': 5.807817134494535}, {'ion': 1469, 'force': [2.126258611679077, 3.1915740966796875, -0.6759365797042847], 'magnitude': 3.894099473953247, 'distance': 9.233482360839844, 'cosine_with_motion': -0.38546180551476794, 'motion_component': -1.5010266361122788}, {'ion': 2443, 'force': [0.12220724672079086, 0.23922725021839142, -2.3671770095825195], 'magnitude': 2.382370948791504, 'distance': 11.80495548248291, 'cosine_with_motion': 0.6941030928097753, 'motion_component': 1.6536110358295508}, {'ion': 2444, 'force': [0.9923494458198547, 1.801130771636963, -7.711010456085205], 'magnitude': 7.980508327484131, 'distance': 6.449911594390869, 'cosine_with_motion': 0.5938281486675583, 'motion_component': 4.7390504322573275}]}, 5491: {'frame': 5491, 'ionic_force': [3.531671144068241, -3.3812859058380127, -9.039488315582275], 'ionic_force_magnitude': 10.277068864925035, 'motion_vector': [0.054042816162109375, 6.2353515625, 0.45986175537109375], 'cosine_ionic_motion': -0.3898304601081398, 'ionic_motion_component': -4.006314484176764, 'ionic_force_x': 3.531671144068241, 'ionic_force_y': -3.3812859058380127, 'ionic_force_z': -9.039488315582275, 'radial_force': 4.8893553201688125, 'axial_force': -9.039488315582275, 'contributions': [{'ion': 1309, 'force': [0.08836428076028824, -4.612890720367432, -2.9233412742614746], 'magnitude': 5.461913108825684, 'distance': 7.796445369720459, 'cosine_with_motion': -0.8814617600389186, 'motion_component': -4.814467416335644}, {'ion': 1469, 'force': [3.120267152786255, 1.8323882818222046, -2.4592511653900146], 'magnitude': 4.375114917755127, 'distance': 8.711126327514648, 'cosine_with_motion': 0.3824934866218572, 'motion_component': 1.6734529448831683}, {'ion': 2444, 'force': [0.323039710521698, -0.6007834672927856, -3.656895875930786], 'magnitude': 3.719970941543579, 'distance': 9.44711685180664, 'cosine_with_motion': -0.23260932244380778, 'motion_component': -0.865299891166011}]}, 5492: {'frame': 5492, 'ionic_force': [7.392548680305481, -1.4014756679534912, -11.69499546289444], 'ionic_force_magnitude': 13.906359297662114, 'motion_vector': [2.7979888916015625, 1.0762748718261719, 3.96209716796875], 'cosine_ionic_motion': -0.39310618776822775, 'ionic_motion_component': -5.466675889239203, 'ionic_force_x': 7.392548680305481, 'ionic_force_y': -1.4014756679534912, 'ionic_force_z': -11.69499546289444, 'radial_force': 7.524221556981957, 'axial_force': -11.69499546289444, 'contributions': [{'ion': 1309, 'force': [6.099052906036377, -4.69687557220459, -7.9687724113464355], 'magnitude': 11.079730033874512, 'distance': 5.473995685577393, 'cosine_with_motion': -0.3553767598406582, 'motion_component': -3.9374786012320016}, {'ion': 1469, 'force': [1.0042378902435303, 1.8420790433883667, -0.7561507821083069], 'magnitude': 2.230137586593628, 'distance': 12.20121955871582, 'cosine_with_motion': 0.16213359381764256, 'motion_component': 0.36158019590189205}, {'ion': 2444, 'force': [0.28925788402557373, 1.453320860862732, -2.9700722694396973], 'magnitude': 3.3192079067230225, 'distance': 10.001193046569824, 'cosine_with_motion': -0.5696472702968612, 'motion_component': -1.8907777069422327}]}, 5493: {'frame': 5493, 'ionic_force': [10.50127774477005, 5.519231498241425, -3.8027787916362286], 'ionic_force_magnitude': 12.457924271005234, 'motion_vector': [-1.495269775390625, 1.0756874084472656, 0.23244476318359375], 'cosine_ionic_motion': -0.4604190596535929, 'ionic_motion_component': -5.7358657780919025, 'ionic_force_x': 10.50127774477005, 'ionic_force_y': 5.519231498241425, 'ionic_force_z': -3.8027787916362286, 'radial_force': 11.863336402715007, 'axial_force': -3.8027787916362286, 'contributions': [{'ion': 1309, 'force': [7.177574157714844, 0.5480061769485474, 0.4017539322376251], 'magnitude': 7.2096662521362305, 'distance': 6.7859625816345215, 'cosine_with_motion': -0.7507798160511517, 'motion_component': -5.412871918936274}, {'ion': 1469, 'force': [0.9419129490852356, 1.280834674835205, -0.03194640204310417], 'magnitude': 1.5902068614959717, 'distance': 14.44914722442627, 'cosine_with_motion': -0.012891961460507317, 'motion_component': -0.02050088629485819}, {'ion': 2443, 'force': [0.5624699592590332, 0.8197107911109924, -1.5806218385696411], 'magnitude': 1.8672609329223633, 'distance': 13.334186553955078, 'cosine_with_motion': -0.09423761570225872, 'motion_component': -0.17596622429598163}, {'ion': 2444, 'force': [1.8193206787109375, 2.8706798553466797, -2.5919644832611084], 'magnitude': 4.274226188659668, 'distance': 8.813335418701172, 'cosine_with_motion': -0.02960224101162135, 'motion_component': -0.1265266770110891}]}, 5494: {'frame': 5494, 'ionic_force': [7.604774683713913, 7.194220662117004, -4.560827128589153], 'ionic_force_magnitude': 11.418868289903429, 'motion_vector': [0.6881828308105469, 0.4589118957519531, 0.434112548828125], 'cosine_ionic_motion': 0.6145182648430363, 'ionic_motion_component': 7.017103127982624, 'ionic_force_x': 7.604774683713913, 'ionic_force_y': 7.194220662117004, 'ionic_force_z': -4.560827128589153, 'radial_force': 10.468496020216431, 'axial_force': -4.560827128589153, 'contributions': [{'ion': 1309, 'force': [5.270052433013916, 1.1801180839538574, -0.09136883914470673], 'magnitude': 5.401340484619141, 'distance': 7.8400397300720215, 'cosine_with_motion': 0.8182541697057424, 'motion_component': 4.419669416924913}, {'ion': 1469, 'force': [0.786957323551178, 1.485055923461914, -0.08958549052476883], 'magnitude': 1.6830681562423706, 'distance': 14.04488468170166, 'cosine_with_motion': 0.7531818377095537, 'motion_component': 1.2676563817786788}, {'ion': 2443, 'force': [0.3067300617694855, 1.0199345350265503, -1.5694105625152588], 'magnitude': 1.8966810703277588, 'distance': 13.230366706848145, 'cosine_with_motion': -0.0012159144470626063, 'motion_component': -0.0023062019846715742}, {'ion': 2444, 'force': [1.2410348653793335, 3.5091121196746826, -2.810462236404419], 'magnitude': 4.663982391357422, 'distance': 8.43704891204834, 'cosine_with_motion': 0.2856107534826452, 'motion_component': 1.332083575267653}]}, 5495: {'frame': 5495, 'ionic_force': [7.7076713144779205, 6.843995451927185, -3.1370171401649714], 'ionic_force_magnitude': 10.774476663658175, 'motion_vector': [0.6293601989746094, -1.066162109375, -0.34174346923828125], 'cosine_ionic_motion': -0.09927879076110027, 'ionic_motion_component': -1.0696770142516778, 'ionic_force_x': 7.7076713144779205, 'ionic_force_y': 6.843995451927185, 'ionic_force_z': -3.1370171401649714, 'radial_force': 10.307689888526225, 'axial_force': -3.1370171401649714, 'contributions': [{'ion': 1309, 'force': [4.939149856567383, 1.1103832721710205, 0.3859111964702606], 'magnitude': 5.077113151550293, 'distance': 8.08650016784668, 'cosine_with_motion': 0.2749294025598821, 'motion_component': 1.3958477346173073}, {'ion': 1469, 'force': [1.0719969272613525, 1.4649080038070679, 0.0071951355785131454], 'magnitude': 1.815264344215393, 'distance': 13.523811340332031, 'cosine_with_motion': -0.3815711058689474, 'motion_component': -0.6926524235055304}, {'ion': 2443, 'force': [0.3923477232456207, 1.103355884552002, -1.5097792148590088], 'magnitude': 1.910697340965271, 'distance': 13.181750297546387, 'cosine_with_motion': -0.16848680323152304, 'motion_component': -0.3219272821939594}, {'ion': 2444, 'force': [1.3041768074035645, 3.1653482913970947, -2.0203442573547363], 'magnitude': 3.9751853942871094, 'distance': 9.138824462890625, 'cosine_with_motion': -0.36500061517302956, 'motion_component': -1.4509450661405054}]}, 5496: {'frame': 5496, 'ionic_force': [8.74626049399376, 6.5846357345581055, -4.182012894656509], 'ionic_force_magnitude': 11.71937422547334, 'motion_vector': [0.7211837768554688, -0.30852508544921875, -0.23809051513671875], 'cosine_ionic_motion': 0.5487553892618503, 'ionic_motion_component': 6.431069765004918, 'ionic_force_x': 8.74626049399376, 'ionic_force_y': 6.5846357345581055, 'ionic_force_z': -4.182012894656509, 'radial_force': 10.947808017389395, 'axial_force': -4.182012894656509, 'contributions': [{'ion': 1309, 'force': [5.159459590911865, 1.0115982294082642, -0.0068298703990876675], 'magnitude': 5.257699489593506, 'distance': 7.946413516998291, 'cosine_with_motion': 0.7912912796099127, 'motion_component': 4.160371529084642}, {'ion': 1469, 'force': [1.318227767944336, 1.3875240087509155, 0.040635738521814346], 'magnitude': 1.9143141508102417, 'distance': 13.169292449951172, 'cosine_with_motion': 0.3268593891850779, 'motion_component': 0.6257115470666249}, {'ion': 2443, 'force': [0.47910425066947937, 1.0934357643127441, -1.6458216905593872], 'magnitude': 2.0331923961639404, 'distance': 12.778497695922852, 'cosine_with_motion': 0.2400100975735285, 'motion_component': 0.48798672728567816}, {'ion': 2444, 'force': [1.7894688844680786, 3.0920777320861816, -2.5699970722198486], 'magnitude': 4.400912284851074, 'distance': 8.68555736541748, 'cosine_with_motion': 0.26290005160501845, 'motion_component': 1.1570000549089627}]}, 5497: {'frame': 5497, 'ionic_force': [6.961087644100189, 5.41208153963089, -4.26440330222249], 'ionic_force_magnitude': 9.794513939163284, 'motion_vector': [-1.509521484375, 1.9396095275878906, 0.17327117919921875], 'cosine_ionic_motion': -0.031056908057381913, 'ionic_motion_component': -0.3041873188753397, 'ionic_force_x': 6.961087644100189, 'ionic_force_y': 5.41208153963089, 'ionic_force_z': -4.26440330222249, 'radial_force': 8.81744678353421, 'axial_force': -4.26440330222249, 'contributions': [{'ion': 1309, 'force': [3.2068612575531006, 0.40660589933395386, -0.12844008207321167], 'magnitude': 3.235086441040039, 'distance': 10.130388259887695, 'cosine_with_motion': -0.5111621811598831, 'motion_component': -1.6536538458867085}, {'ion': 1469, 'force': [1.2073882818222046, 1.2977768182754517, -0.038394588977098465], 'magnitude': 1.772987723350525, 'distance': 13.684098243713379, 'cosine_with_motion': 0.15748131430486484, 'motion_component': 0.27921242850128447}, {'ion': 2443, 'force': [0.6200312972068787, 1.031477451324463, -1.5388377904891968], 'magnitude': 1.9535624980926514, 'distance': 13.036331176757812, 'cosine_with_motion': 0.16580428864796673, 'motion_component': 0.32390903411250704}, {'ion': 2444, 'force': [1.9268068075180054, 2.6762213706970215, -2.5587308406829834], 'magnitude': 4.173948764801025, 'distance': 8.918575286865234, 'cosine_with_motion': 0.1788103758969193, 'motion_component': 0.7463453587972211}]}, 5498: {'frame': 5498, 'ionic_force': [4.10741001367569, 5.098243832588196, -3.6214068830013275], 'ionic_force_magnitude': 7.481810944498417, 'motion_vector': [-0.3549995422363281, 0.2932014465332031, 0.5114364624023438], 'cosine_ionic_motion': -0.352603884698631, 'ionic_motion_component': -2.6381156036108755, 'ionic_force_x': 4.10741001367569, 'ionic_force_y': 5.098243832588196, 'ionic_force_z': -3.6214068830013275, 'radial_force': 6.54697695100318, 'axial_force': -3.6214068830013275, 'contributions': [{'ion': 1309, 'force': [2.7465009689331055, 1.1063706874847412, -0.25553974509239197], 'magnitude': 2.971973180770874, 'distance': 10.56930923461914, 'cosine_with_motion': -0.38202445241844485, 'motion_component': -1.1353664041428075}, {'ion': 2443, 'force': [0.3203471302986145, 1.1662036180496216, -1.4032648801803589], 'magnitude': 1.852513313293457, 'distance': 13.387157440185547, 'cosine_with_motion': -0.3839537031283095, 'motion_component': -0.71127933747524}, {'ion': 2444, 'force': [1.0405619144439697, 2.825669527053833, -1.9626022577285767], 'magnitude': 3.594299077987671, 'distance': 9.61085319519043, 'cosine_with_motion': -0.22020147314330785, 'motion_component': -0.791469925361028}]}, 5499: {'frame': 5499, 'ionic_force': [4.963673681020737, 6.609779596328735, -3.376120550557971], 'ionic_force_magnitude': 8.9289099388224, 'motion_vector': [0.3253974914550781, -0.08216476440429688, -0.2378997802734375], 'cosine_ionic_motion': 0.5105307809870959, 'ionic_motion_component': 4.558483364430443, 'ionic_force_x': 4.963673681020737, 'ionic_force_y': 6.609779596328735, 'ionic_force_z': -3.376120550557971, 'radial_force': 8.266029441255434, 'axial_force': -3.376120550557971, 'contributions': [{'ion': 1309, 'force': [3.1469173431396484, 1.3124815225601196, -0.09989611059427261], 'magnitude': 3.4111106395721436, 'distance': 9.865546226501465, 'cosine_with_motion': 0.6698188633880374, 'motion_component': 2.2848262464939917}, {'ion': 1469, 'force': [0.7330875396728516, 1.2971830368041992, -0.008259242400527], 'magnitude': 1.4900232553482056, 'distance': 14.92699909210205, 'cosine_with_motion': 0.21849183202341296, 'motion_component': 0.3255579170800985}, {'ion': 2443, 'force': [0.2510865032672882, 1.1263843774795532, -1.4073807001113892], 'magnitude': 1.8200292587280273, 'distance': 13.506096839904785, 'cosine_with_motion': 0.4326988603405221, 'motion_component': 0.787524601535635}, {'ion': 2444, 'force': [0.8325822949409485, 2.8737306594848633, -1.8605844974517822], 'magnitude': 3.5232508182525635, 'distance': 9.707273483276367, 'cosine_with_motion': 0.3294044407574017, 'motion_component': 1.1605744432274108}]}, 5500: {'frame': 5500, 'ionic_force': [5.459194302558899, 5.718991637229919, -2.9895115792751312], 'ionic_force_magnitude': 8.45262369104513, 'motion_vector': [2.9813499450683594, -5.0980072021484375, -0.931304931640625], 'cosine_ionic_motion': -0.19976887581490052, 'ionic_motion_component': -1.6885711324464805, 'ionic_force_x': 5.459194302558899, 'ionic_force_y': 5.718991637229919, 'ionic_force_z': -2.9895115792751312, 'radial_force': 7.906305570859079, 'axial_force': -2.9895115792751312, 'contributions': [{'ion': 1309, 'force': [4.1073384284973145, 2.204691171646118, 0.19625237584114075], 'magnitude': 4.665769577026367, 'distance': 8.435433387756348, 'cosine_with_motion': 0.029506956898164696, 'motion_component': 0.1376726661623504}, {'ion': 2443, 'force': [0.4238545298576355, 0.9974464178085327, -1.34289908409</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>{5576: {'frame': 5576, 'ionic_force': [-5.12838389724493, -9.299570322036743, -7.61335426568985], 'ionic_force_magnitude': 13.066961878987996, 'motion_vector': [0.9404220581054688, -0.198822021484375, -0.6372222900390625], 'cosine_ionic_motion': 0.12459092668388769, 'ionic_motion_component': 1.6280248894461486, 'ionic_force_x': -5.12838389724493, 'ionic_force_y': -9.299570322036743, 'ionic_force_z': -7.61335426568985, 'radial_force': 10.619902521776162, 'axial_force': -7.61335426568985, 'contributions': [{'ion': 1309, 'force': [6.9591827392578125, -4.298310279846191, -0.8726447224617004], 'magnitude': 8.226007461547852, 'distance': 6.352936267852783, 'directional_contribution': 6.898126405392048}, {'ion': 1380, 'force': [-0.09576242417097092, -0.6451082229614258, -1.4218106269836426], 'magnitude': 1.5642507076263428, 'distance': 14.568533897399902, 'directional_contribution': 0.8187447342328955}, {'ion': 1469, 'force': [-11.656188011169434, -2.1556320190429688, -2.5449581146240234], 'magnitude': 12.123954772949219, 'distance': 5.2329535484313965, 'directional_contribution': -7.727271987372546}, {'ion': 2443, 'force': [-0.33561620116233826, -2.2005198001861572, -2.7739408016204834], 'magnitude': 3.55663800239563, 'distance': 9.661603927612305, 'directional_contribution': 1.6384257216959917}]}, 5577: {'frame': 5577, 'ionic_force': [-5.55037547647953, -9.919090867042542, -9.448231399059296], 'ionic_force_magnitude': 14.780531388577412, 'motion_vector': [1.2938232421875, 4.777435302734375, -1.3350448608398438], 'cosine_ionic_motion': -0.5537087550802853, 'ionic_motion_component': -8.184109634594279, 'ionic_force_x': -5.55037547647953, 'ionic_force_y': -9.919090867042542, 'ionic_force_z': -9.448231399059296, 'radial_force': 11.366399234522433, 'axial_force': -9.448231399059296, 'contributions': [{'ion': 1309, 'force': [4.450619697570801, -1.8525863885879517, -2.3408517837524414], 'magnitude': 5.359074592590332, 'distance': 7.8708953857421875, 'directional_contribution': 0.0064071201351936224}, {'ion': 1469, 'force': [-9.812492370605469, -4.156482219696045, -4.021743297576904], 'magnitude': 11.39016056060791, 'distance': 5.398885250091553, 'directional_contribution': -5.302673516991831}, {'ion': 2434, 'force': [-0.3545006811618805, -1.8371081352233887, -0.5042237639427185], 'magnitude': 1.9377509355545044, 'distance': 13.089409828186035, 'directional_contribution': -1.6702026260898677}, {'ion': 2443, 'force': [0.16599787771701813, -2.0729141235351562, -2.5814125537872314], 'magnitude': 3.3148481845855713, 'distance': 10.007767677307129, 'directional_contribution': -1.2176403718538467}]}, 5578: {'frame': 5578, 'ionic_force': [1.3535993099212646, 2.408291459083557, -11.13271152973175], 'ionic_force_magnitude': 11.470368993538804, 'motion_vector': [-3.8603553771972656, 0.4764251708984375, -2.4455490112304688], 'cosine_ionic_motion': 0.4392217845722206, 'ionic_motion_component': 5.038035939043979, 'ionic_force_x': 1.3535993099212646, 'ionic_force_y': 2.408291459083557, 'ionic_force_z': -11.13271152973175, 'radial_force': 2.762625353484278, 'axial_force': -11.13271152973175, 'contributions': [{'ion': 1309, 'force': [3.6393582820892334, 1.2222265005111694, -1.990733027458191], 'magnitude': 4.32455587387085, 'distance': 8.761899948120117, 'directional_contribution': -1.871445900624309}, {'ion': 1469, 'force': [-2.00545072555542, 5.622910022735596, -3.1680915355682373], 'magnitude': 6.7583842277526855, 'distance': 7.00886344909668, 'directional_contribution': 3.9543174027435413}, {'ion': 2434, 'force': [-1.0407629013061523, -3.8392817974090576, -2.276965618133545], 'magnitude': 4.583431720733643, 'distance': 8.5108642578125, 'directional_contribution': 1.6883021294440397}, {'ion': 2443, 'force': [0.7604546546936035, -0.5975632667541504, -3.6969213485717773], 'magnitude': 3.8213350772857666, 'distance': 9.320978164672852, 'directional_contribution': 1.2668625111317056}]}, 5579: {'frame': 5579, 'ionic_force': [-1.6814625263214111, 1.4262338280677795, -10.292737245559692], 'ionic_force_magnitude': 10.526248104898524, 'motion_vector': [2.0666732788085938, -1.3358840942382812, 0.7496261596679688], 'cosine_ionic_motion': -0.4836302150923508, 'ionic_motion_component': -5.090811635087523, 'ionic_force_x': -1.6814625263214111, 'ionic_force_y': 1.4262338280677795, 'ionic_force_z': -10.292737245559692, 'radial_force': 2.20487168781951, 'axial_force': -10.292737245559692, 'contributions': [{'ion': 1309, 'force': [2.5060808658599854, 1.78612220287323, -4.071807861328125], 'magnitude': 5.103948593139648, 'distance': 8.065214157104492, 'directional_contribution': -0.10073359671217474}, {'ion': 1469, 'force': [-2.498354911804199, 1.540704369544983, -2.071153163909912], 'magnitude': 3.592384099960327, 'distance': 9.613414764404297, 'directional_contribution': -3.4107434696653627}, {'ion': 2434, 'force': [-1.2354334592819214, -1.6161770820617676, -1.6747441291809082], 'magnitude': 2.634974718093872, 'distance': 11.22485637664795, 'directional_contribution': -0.6412655505220783}, {'ion': 2443, 'force': [-0.4537550210952759, -0.28441566228866577, -2.475032091140747], 'magnitude': 2.5323052406311035, 'distance': 11.450145721435547, 'directional_contribution': -0.9380690479944036}]}, 5580: {'frame': 5580, 'ionic_force': [-0.7721650202292949, 0.8433377742767334, -11.557860493659973], 'ionic_force_magnitude': 11.614284162654782, 'motion_vector': [-1.6046180725097656, 1.9312629699707031, -1.8199996948242188], 'cosine_ionic_motion': 0.6636535826097525, 'ionic_motion_component': 7.707861293993555, 'ionic_force_x': -0.7721650202292949, 'ionic_force_y': 0.8433377742767334, 'ionic_force_z': -11.557860493659973, 'radial_force': 1.1434410435119695, 'axial_force': -11.557860493659973, 'contributions': [{'ion': 1309, 'force': [3.384483575820923, 0.7182776927947998, -3.0355429649353027], 'magnitude': 4.60273551940918, 'distance': 8.492998123168945, 'directional_contribution': 0.4775900803784907}, {'ion': 1469, 'force': [-3.7529938220977783, 2.630032777786255, -4.193670749664307], 'magnitude': 6.211997032165527, 'distance': 7.310606479644775, 'directional_contribution': 6.040997223573072}, {'ion': 2434, 'force': [-0.40012770891189575, -1.974854826927185, -1.4709564447402954], 'magnitude': 2.494767904281616, 'distance': 11.535965919494629, 'directional_contribution': -0.15954582303928788}, {'ion': 2443, 'force': [-0.0035270650405436754, -0.5301178693771362, -2.8576903343200684], 'magnitude': 2.9064464569091797, 'distance': 10.687788963317871, 'directional_contribution': 1.3488196484509294}]}, 5581: {'frame': 5581, 'ionic_force': [-1.0563013553619385, 1.5127899050712585, -8.483844637870789], 'ionic_force_magnitude': 8.682161348981825, 'motion_vector': [0.801727294921875, 2.2831573486328125, -1.9393539428710938], 'cosine_ionic_motion': 0.7079269250678751, 'ionic_motion_component': 6.1463357867278585, 'ionic_force_x': -1.0563013553619385, 'ionic_force_y': 1.5127899050712585, 'ionic_force_z': -8.483844637870789, 'radial_force': 1.8450761096022505, 'axial_force': -8.483844637870789, 'contributions': [{'ion': 1309, 'force': [1.5847398042678833, 1.608560562133789, -3.1895318031311035], 'magnitude': 3.907938003540039, 'distance': 9.217119216918945, 'directional_contribution': 3.5886770553587723}, {'ion': 1469, 'force': [-1.8289650678634644, 1.3348606824874878, -1.9141175746917725], 'magnitude': 2.964930534362793, 'distance': 10.581854820251465, 'directional_contribution': 1.7069941852641577}, {'ion': 2434, 'force': [-0.5441734194755554, -1.361169457435608, -1.2634094953536987], 'magnitude': 1.9352288246154785, 'distance': 13.097936630249023, 'directional_contribution': -0.35273069138135327}, {'ion': 2443, 'force': [-0.267902672290802, -0.0694618821144104, -2.116785764694214], 'magnitude': 2.1348018646240234, 'distance': 12.470683097839355, 'directional_contribution': 1.203395432897583}]}, 5582: {'frame': 5582, 'ionic_force': [-0.4570380374789238, 0.5276380777359009, -7.061962246894836], 'ionic_force_magnitude': 7.096379110880942, 'motion_vector': [1.6045913696289062, -2.307353973388672, -3.4020919799804688], 'cosine_ionic_motion': 0.7049239596112777, 'ionic_motion_component': 5.002407661744953, 'ionic_force_x': -0.4570380374789238, 'ionic_force_y': 0.5276380777359009, 'ionic_force_z': -7.061962246894836, 'radial_force': 0.6980585281904539, 'axial_force': -7.061962246894836, 'contributions': [{'ion': 1309, 'force': [0.9512708783149719, 0.9681544303894043, -2.003573179244995], 'magnitude': 2.420029878616333, 'distance': 11.71274471282959, 'directional_contribution': 1.384350614990204}, {'ion': 1469, 'force': [-1.059220314025879, 0.999154806137085, -1.5712475776672363], 'magnitude': 2.1422131061553955, 'distance': 12.449092864990234, 'directional_contribution': 0.30377723401855405}, {'ion': 2434, 'force': [-0.2705686688423157, -1.578347086906433, -1.934159755706787], 'magnitude': 2.511047840118408, 'distance': 11.498509407043457, 'directional_contribution': 2.218055772580776}, {'ion': 2443, 'force': [-0.07851993292570114, 0.13867592811584473, -1.5529817342758179], 'magnitude': 1.5611369609832764, 'distance': 14.58305549621582, 'directional_contribution': 1.096223878320914}]}}</t>
+          <t>{5576: {'frame': 5576, 'ionic_force': [-5.12838389724493, -9.299570322036743, -7.61335426568985], 'ionic_force_magnitude': 13.066961878987996, 'motion_vector': [0.9404220581054688, -0.198822021484375, -0.6372222900390625], 'cosine_ionic_motion': 0.12459092668388769, 'ionic_motion_component': 1.6280248894461486, 'ionic_force_x': -5.12838389724493, 'ionic_force_y': -9.299570322036743, 'ionic_force_z': -7.61335426568985, 'radial_force': 10.619902521776162, 'axial_force': -7.61335426568985, 'contributions': [{'ion': 1309, 'force': [6.9591827392578125, -4.298310279846191, -0.8726447224617004], 'magnitude': 8.226007461547852, 'distance': 6.352936267852783, 'cosine_with_motion': 0.838575231832428, 'motion_component': 6.898126405392048}, {'ion': 1380, 'force': [-0.09576242417097092, -0.6451082229614258, -1.4218106269836426], 'magnitude': 1.5642507076263428, 'distance': 14.568533897399902, 'cosine_with_motion': 0.5234101473850589, 'motion_component': 0.8187447342328956}, {'ion': 1469, 'force': [-11.656188011169434, -2.1556320190429688, -2.5449581146240234], 'magnitude': 12.123954772949219, 'distance': 5.2329535484313965, 'cosine_with_motion': -0.6373557234813525, 'motion_component': -7.727271987372546}, {'ion': 2443, 'force': [-0.33561620116233826, -2.2005198001861572, -2.7739408016204834], 'magnitude': 3.55663800239563, 'distance': 9.661603927612305, 'cosine_with_motion': 0.46066700205914507, 'motion_component': 1.6384257216959917}]}, 5577: {'frame': 5577, 'ionic_force': [-5.55037547647953, -9.919090867042542, -9.448231399059296], 'ionic_force_magnitude': 14.780531388577412, 'motion_vector': [1.2938232421875, 4.777435302734375, -1.3350448608398438], 'cosine_ionic_motion': -0.5537087550802853, 'ionic_motion_component': -8.184109634594279, 'ionic_force_x': -5.55037547647953, 'ionic_force_y': -9.919090867042542, 'ionic_force_z': -9.448231399059296, 'radial_force': 11.366399234522433, 'axial_force': -9.448231399059296, 'contributions': [{'ion': 1309, 'force': [4.450619697570801, -1.8525863885879517, -2.3408517837524414], 'magnitude': 5.359074592590332, 'distance': 7.8708953857421875, 'cosine_with_motion': 0.001195564678229169, 'motion_component': 0.0064071201351936224}, {'ion': 1469, 'force': [-9.812492370605469, -4.156482219696045, -4.021743297576904], 'magnitude': 11.39016056060791, 'distance': 5.398885250091553, 'cosine_with_motion': -0.4655485963425134, 'motion_component': -5.302673516991831}, {'ion': 2434, 'force': [-0.3545006811618805, -1.8371081352233887, -0.5042237639427185], 'magnitude': 1.9377509355545044, 'distance': 13.089409828186035, 'cosine_with_motion': -0.8619284381256479, 'motion_component': -1.6702026260898677}, {'ion': 2443, 'force': [0.16599787771701813, -2.0729141235351562, -2.5814125537872314], 'magnitude': 3.3148481845855713, 'distance': 10.007767677307129, 'cosine_with_motion': -0.3673291426502491, 'motion_component': -1.2176403718538467}]}, 5578: {'frame': 5578, 'ionic_force': [1.3535993099212646, 2.408291459083557, -11.13271152973175], 'ionic_force_magnitude': 11.470368993538804, 'motion_vector': [-3.8603553771972656, 0.4764251708984375, -2.4455490112304688], 'cosine_ionic_motion': 0.4392217845722206, 'ionic_motion_component': 5.038035939043979, 'ionic_force_x': 1.3535993099212646, 'ionic_force_y': 2.408291459083557, 'ionic_force_z': -11.13271152973175, 'radial_force': 2.762625353484278, 'axial_force': -11.13271152973175, 'contributions': [{'ion': 1309, 'force': [3.6393582820892334, 1.2222265005111694, -1.990733027458191], 'magnitude': 4.32455587387085, 'distance': 8.761899948120117, 'cosine_with_motion': -0.4327486833242564, 'motion_component': -1.871445900624309}, {'ion': 1469, 'force': [-2.00545072555542, 5.622910022735596, -3.1680915355682373], 'magnitude': 6.7583842277526855, 'distance': 7.00886344909668, 'cosine_with_motion': 0.5850980689663797, 'motion_component': 3.9543174027435417}, {'ion': 2434, 'force': [-1.0407629013061523, -3.8392817974090576, -2.276965618133545], 'magnitude': 4.583431720733643, 'distance': 8.5108642578125, 'cosine_with_motion': 0.368348936706906, 'motion_component': 1.6883021294440397}, {'ion': 2443, 'force': [0.7604546546936035, -0.5975632667541504, -3.6969213485717773], 'magnitude': 3.8213350772857666, 'distance': 9.320978164672852, 'cosine_with_motion': 0.33152354779450083, 'motion_component': 1.2668625111317056}]}, 5579: {'frame': 5579, 'ionic_force': [-1.6814625263214111, 1.4262338280677795, -10.292737245559692], 'ionic_force_magnitude': 10.526248104898524, 'motion_vector': [2.0666732788085938, -1.3358840942382812, 0.7496261596679688], 'cosine_ionic_motion': -0.4836302150923508, 'ionic_motion_component': -5.090811635087523, 'ionic_force_x': -1.6814625263214111, 'ionic_force_y': 1.4262338280677795, 'ionic_force_z': -10.292737245559692, 'radial_force': 2.20487168781951, 'axial_force': -10.292737245559692, 'contributions': [{'ion': 1309, 'force': [2.5060808658599854, 1.78612220287323, -4.071807861328125], 'magnitude': 5.103948593139648, 'distance': 8.065214157104492, 'cosine_with_motion': -0.019736404334987183, 'motion_component': -0.10073359671217474}, {'ion': 1469, 'force': [-2.498354911804199, 1.540704369544983, -2.071153163909912], 'magnitude': 3.592384099960327, 'distance': 9.613414764404297, 'cosine_with_motion': -0.9494373347064944, 'motion_component': -3.4107434696653627}, {'ion': 2434, 'force': [-1.2354334592819214, -1.6161770820617676, -1.6747441291809082], 'magnitude': 2.634974718093872, 'distance': 11.22485637664795, 'cosine_with_motion': -0.2433668646071048, 'motion_component': -0.6412655505220783}, {'ion': 2443, 'force': [-0.4537550210952759, -0.28441566228866577, -2.475032091140747], 'magnitude': 2.5323052406311035, 'distance': 11.450145721435547, 'cosine_with_motion': -0.3704407508345466, 'motion_component': -0.9380690479944036}]}, 5580: {'frame': 5580, 'ionic_force': [-0.7721650202292949, 0.8433377742767334, -11.557860493659973], 'ionic_force_magnitude': 11.614284162654782, 'motion_vector': [-1.6046180725097656, 1.9312629699707031, -1.8199996948242188], 'cosine_ionic_motion': 0.6636535826097525, 'ionic_motion_component': 7.707861293993555, 'ionic_force_x': -0.7721650202292949, 'ionic_force_y': 0.8433377742767334, 'ionic_force_z': -11.557860493659973, 'radial_force': 1.1434410435119695, 'axial_force': -11.557860493659973, 'contributions': [{'ion': 1309, 'force': [3.384483575820923, 0.7182776927947998, -3.0355429649353027], 'magnitude': 4.60273551940918, 'distance': 8.492998123168945, 'cosine_with_motion': 0.10376222845352057, 'motion_component': 0.4775900803784907}, {'ion': 1469, 'force': [-3.7529938220977783, 2.630032777786255, -4.193670749664307], 'magnitude': 6.211997032165527, 'distance': 7.310606479644775, 'cosine_with_motion': 0.9724726226719216, 'motion_component': 6.040997223573072}, {'ion': 2434, 'force': [-0.40012770891189575, -1.974854826927185, -1.4709564447402954], 'magnitude': 2.494767904281616, 'distance': 11.535965919494629, 'cosine_with_motion': -0.06395217211863438, 'motion_component': -0.15954582303928788}, {'ion': 2443, 'force': [-0.0035270650405436754, -0.5301178693771362, -2.8576903343200684], 'magnitude': 2.9064464569091797, 'distance': 10.687788963317871, 'cosine_with_motion': 0.4640786037765659, 'motion_component': 1.3488196484509294}]}, 5581: {'frame': 5581, 'ionic_force': [-1.0563013553619385, 1.5127899050712585, -8.483844637870789], 'ionic_force_magnitude': 8.682161348981825, 'motion_vector': [0.801727294921875, 2.2831573486328125, -1.9393539428710938], 'cosine_ionic_motion': 0.7079269250678751, 'ionic_motion_component': 6.1463357867278585, 'ionic_force_x': -1.0563013553619385, 'ionic_force_y': 1.5127899050712585, 'ionic_force_z': -8.483844637870789, 'radial_force': 1.8450761096022505, 'axial_force': -8.483844637870789, 'contributions': [{'ion': 1309, 'force': [1.5847398042678833, 1.608560562133789, -3.1895318031311035], 'magnitude': 3.907938003540039, 'distance': 9.217119216918945, 'cosine_with_motion': 0.9183044697980314, 'motion_component': 3.5886770553587723}, {'ion': 1469, 'force': [-1.8289650678634644, 1.3348606824874878, -1.9141175746917725], 'magnitude': 2.964930534362793, 'distance': 10.581854820251465, 'cosine_with_motion': 0.5757282457888437, 'motion_component': 1.7069941852641575}, {'ion': 2434, 'force': [-0.5441734194755554, -1.361169457435608, -1.2634094953536987], 'magnitude': 1.9352288246154785, 'distance': 13.097936630249023, 'cosine_with_motion': -0.1822682099252567, 'motion_component': -0.35273069138135327}, {'ion': 2443, 'force': [-0.267902672290802, -0.0694618821144104, -2.116785764694214], 'magnitude': 2.1348018646240234, 'distance': 12.470683097839355, 'cosine_with_motion': 0.5637035846568351, 'motion_component': 1.203395432897583}]}, 5582: {'frame': 5582, 'ionic_force': [-0.4570380374789238, 0.5276380777359009, -7.061962246894836], 'ionic_force_magnitude': 7.096379110880942, 'motion_vector': [1.6045913696289062, -2.307353973388672, -3.4020919799804688], 'cosine_ionic_motion': 0.7049239596112777, 'ionic_motion_component': 5.002407661744953, 'ionic_force_x': -0.4570380374789238, 'ionic_force_y': 0.5276380777359009, 'ionic_force_z': -7.061962246894836, 'radial_force': 0.6980585281904539, 'axial_force': -7.061962246894836, 'contributions': [{'ion': 1309, 'force': [0.9512708783149719, 0.9681544303894043, -2.003573179244995], 'magnitude': 2.420029878616333, 'distance': 11.71274471282959, 'cosine_with_motion': 0.5720386383493259, 'motion_component': 1.384350614990204}, {'ion': 1469, 'force': [-1.059220314025879, 0.999154806137085, -1.5712475776672363], 'magnitude': 2.1422131061553955, 'distance': 12.449092864990234, 'cosine_with_motion': 0.1418053295081253, 'motion_component': 0.30377723401855405}, {'ion': 2434, 'force': [-0.2705686688423157, -1.578347086906433, -1.934159755706787], 'magnitude': 2.511047840118408, 'distance': 11.498509407043457, 'cosine_with_motion': 0.8833188285271076, 'motion_component': 2.218055772580776}, {'ion': 2443, 'force': [-0.07851993292570114, 0.13867592811584473, -1.5529817342758179], 'magnitude': 1.5611369609832764, 'distance': 14.58305549621582, 'cosine_with_motion': 0.702195832082078, 'motion_component': 1.096223878320914}]}}</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>{5594: {'frame': 5594, 'ionic_force': [-4.9196601659059525, 1.0488449931144714, -6.5911475121974945], 'ionic_force_magnitude': 8.291342321670859, 'motion_vector': [1.2472190856933594, -0.8786392211914062, 1.1838226318359375], 'cosine_ionic_motion': -0.9281191389561603, 'ionic_motion_component': -7.695353496379928, 'ionic_force_x': -4.9196601659059525, 'ionic_force_y': 1.0488449931144714, 'ionic_force_z': -6.5911475121974945, 'radial_force': 5.03022186067206, 'axial_force': -6.5911475121974945, 'contributions': [{'ion': 1309, 'force': [2.8878653049468994, 3.550973415374756, 0.24883276224136353], 'magnitude': 4.5837860107421875, 'distance': 8.51053524017334, 'directional_contribution': 0.4020327582711829}, {'ion': 1380, 'force': [-0.7073386907577515, 1.981725811958313, -4.544967174530029], 'magnitude': 5.008421897888184, 'distance': 8.141765594482422, 'directional_contribution': -4.144800091426141}, {'ion': 1469, 'force': [-1.5927733182907104, 2.366380214691162, 0.28326359391212463], 'magnitude': 2.8665170669555664, 'distance': 10.761969566345215, 'directional_contribution': -1.931786259787092}, {'ion': 1476, 'force': [-0.1692715436220169, 0.5136356949806213, -2.323270082473755], 'magnitude': 2.3853843212127686, 'distance': 11.797496795654297, 'directional_contribution': -1.7672969554629239}, {'ion': 2434, 'force': [-5.338141918182373, -7.363870143890381, -0.2550066113471985], 'magnitude': 9.098756790161133, 'distance': 6.040571212768555, 'directional_contribution': -0.2535029218473497}]}, 5595: {'frame': 5595, 'ionic_force': [-2.300809770822525, 3.5821394324302673, -8.520911037921906], 'ionic_force_magnitude': 9.525301750131783, 'motion_vector': [-0.8982429504394531, -0.04642486572265625, -0.12294769287109375], 'cosine_ionic_motion': 0.340923910951574, 'ionic_motion_component': 3.2474031256488, 'ionic_force_x': -2.300809770822525, 'ionic_force_y': 3.5821394324302673, 'ionic_force_z': -8.520911037921906, 'radial_force': 4.2573992665574885, 'axial_force': -8.520911037921906, 'contributions': [{'ion': 1309, 'force': [2.716885566711426, 2.478614091873169, 0.5846787095069885], 'magnitude': 3.7238211631774902, 'distance': 9.442231178283691, 'directional_contribution': -2.894205831901914}, {'ion': 1380, 'force': [-0.13194406032562256, 3.3571829795837402, -8.195930480957031], 'magnitude': 8.857842445373535, 'distance': 6.122165679931641, 'directional_contribution': 1.068875712637837}, {'ion': 1469, 'force': [-1.9954568147659302, 3.5336289405822754, 1.0472036600112915], 'magnitude': 4.19106388092041, 'distance': 8.900345802307129, 'directional_contribution': 1.6519007656536218}, {'ion': 1476, 'force': [0.18375858664512634, 0.6461936831474304, -3.1573736667633057], 'magnitude': 3.228055477142334, 'distance': 10.141414642333984, 'directional_contribution': 0.21274644695871148}, {'ion': 2434, 'force': [-3.0740530490875244, -6.433480262756348, 1.2005107402801514], 'magnitude': 7.230539321899414, 'distance': 6.776160717010498, 'directional_contribution': 3.2080860657232506}]}, 5596: {'frame': 5596, 'ionic_force': [-2.110570512712002, 4.475105106830597, -9.859978318214417], 'ionic_force_magnitude': 11.031783447927587, 'motion_vector': [0.0039520263671875, 1.0794944763183594, -1.8756179809570312], 'cosine_ionic_motion': 0.976641108636546, 'ionic_motion_component': 10.774093216822296, 'ionic_force_x': -2.110570512712002, 'ionic_force_y': 4.475105106830597, 'ionic_force_z': -9.859978318214417, 'radial_force': 4.947835244459004, 'axial_force': -9.859978318214417, 'contributions': [{'ion': 1309, 'force': [3.438979148864746, 2.82747483253479, 0.5633991956710815], 'magnitude': 4.487606525421143, 'distance': 8.601251602172852, 'directional_contribution': 0.9283886550210865}, {'ion': 1380, 'force': [-0.861777663230896, 4.213195323944092, -8.890606880187988], 'magnitude': 9.876060485839844, 'distance': 5.7979865074157715, 'directional_contribution': 9.805570931246908}, {'ion': 1469, 'force': [-1.7644017934799194, 2.603040933609009, 0.6845284700393677], 'magnitude': 3.2183094024658203, 'distance': 10.156759262084961, 'directional_contribution': 0.7019506439526788}, {'ion': 1476, 'force': [-0.06188376992940903, 0.5250032544136047, -3.2976949214935303], 'magnitude': 3.3397979736328125, 'distance': 9.970316886901855, 'directional_contribution': 3.119889807339182}, {'ion': 2434, 'force': [-2.8614864349365234, -5.693609237670898, 1.0803958177566528], 'magnitude': 6.463168144226074, 'distance': 7.167147159576416, 'directional_contribution': -3.7817068149310367}]}, 5597: {'frame': 5597, 'ionic_force': [-2.391743592917919, 3.8317089676856995, -11.019856214523315], 'ionic_force_magnitude': 11.909645755272281, 'motion_vector': [1.3422393798828125, -0.8549842834472656, -0.35398101806640625], 'cosine_ionic_motion': -0.13316181833832863, 'ionic_motion_component': -1.585910084537414, 'ionic_force_x': -2.391743592917919, 'ionic_force_y': 3.8317089676856995, 'ionic_force_z': -11.019856214523315, 'radial_force': 4.5169050274836335, 'axial_force': -11.019856214523315, 'contributions': [{'ion': 1309, 'force': [2.360955238342285, 3.685953378677368, -0.3692745864391327], 'magnitude': 4.392804145812988, 'distance': 8.69356918334961, 'directional_contribution': 0.09093444345478696}, {'ion': 1380, 'force': [-0.3367534875869751, 4.115484714508057, -6.502329349517822], 'magnitude': 7.702655792236328, 'distance': 6.565212726593018, 'directional_contribution': -1.0237184513445428}, {'ion': 1469, 'force': [-1.0739519596099854, 3.1200692653656006, -0.15641751885414124], 'magnitude': 3.3034331798553467, 'distance': 10.025043487548828, 'directional_contribution': -2.486486908028081}, {'ion': 1476, 'force': [-0.05223899334669113, 0.661562979221344, -2.2055890560150146], 'magnitude': 2.30326247215271, 'distance': 12.005972862243652, 'directional_contribution': 0.0889361842241847}, {'ion': 2434, 'force': [-3.2897543907165527, -7.75136137008667, -1.7862457036972046], 'magnitude': 8.60794734954834, 'distance': 6.210395336151123, 'directional_contribution': 1.7444245546876704}]}, 5598: {'frame': 5598, 'ionic_force': [3.7280571311712265, -0.048622846603393555, -10.82320636510849], 'ionic_force_magnitude': 11.44738267798423, 'motion_vector': [1.0442886352539062, 2.5621337890625, -0.08968353271484375], 'cosine_ionic_motion': 0.14955505651374204, 'ionic_motion_component': 1.7120139633403633, 'ionic_force_x': 3.7280571311712265, 'ionic_force_y': -0.048622846603393555, 'ionic_force_z': -10.82320636510849, 'radial_force': 3.728374197219004, 'axial_force': -10.82320636510849, 'contributions': [{'ion': 1309, 'force': [7.3780598640441895, 4.05808687210083, -3.189204216003418], 'magnitude': 9.004158020019531, 'distance': 6.0722198486328125, 'directional_contribution': 6.642579449055013}, {'ion': 1380, 'force': [0.361459881067276, 1.1916948556900024, -3.9953513145446777], 'magnitude': 4.184927940368652, 'distance': 8.906867980957031, 'directional_contribution': 1.3687677047499784}, {'ion': 1469, 'force': [-1.4546935558319092, 3.4690563678741455, -0.2319532036781311], 'magnitude': 3.768857717514038, 'distance': 9.385645866394043, 'directional_contribution': 2.669526086335598}, {'ion': 1476, 'force': [0.21506913006305695, 0.3528536558151245, -1.9371775388717651], 'magnitude': 1.9807617664337158, 'distance': 12.946516036987305, 'directional_contribution': 0.470475445232283}, {'ion': 2434, 'force': [-2.7718381881713867, -9.120314598083496, -1.469520092010498], 'magnitude': 9.644827842712402, 'distance': 5.867076873779297, 'directional_contribution': -9.439334723743546}]}, 5599: {'frame': 5599, 'ionic_force': [-1.9013180434703827, -9.60105836391449, -11.383936129510403], 'ionic_force_magnitude': 15.012972184430726, 'motion_vector': [-3.3165664672851562, 2.1229324340820312, -0.15932464599609375], 'cosine_ionic_motion': -0.20725825176288065, 'ionic_motion_component': -3.1115623687098677, 'ionic_force_x': -1.9013180434703827, 'ionic_force_y': -9.60105836391449, 'ionic_force_z': -11.383936129510403, 'radial_force': 9.787508978780986, 'axial_force': -11.383936129510403, 'contributions': [{'ion': 1309, 'force': [3.44903564453125, 3.2919468879699707, -1.7546262741088867], 'magnitude': 5.080499172210693, 'distance': 8.083805084228516, 'directional_contribution': -1.0583028704620006}, {'ion': 1380, 'force': [0.5980334877967834, 1.709892749786377, -2.676297664642334], 'magnitude': 3.2317094802856445, 'distance': 10.135680198669434, 'directional_contribution': 0.5259947179221207}, {'ion': 1469, 'force': [-0.6552402973175049, 2.634486198425293, -0.08947023004293442], 'magnitude': 2.716222047805786, 'distance': 11.055704116821289, 'directional_contribution': 1.9741560530515698}, {'ion': 1476, 'force': [0.27780506014823914, 0.6250635385513306, -1.5681666135787964], 'magnitude': 1.710855484008789, 'distance': 13.930360794067383, 'directional_contribution': 0.16631533363621465}, {'ion': 2434, 'force': [-5.57095193862915, -17.86244773864746, -5.295375347137451], 'magnitude': 19.445913314819336, 'distance': 4.131947994232178, 'directional_contribution': -4.719725562381129}]}, 5600: {'frame': 5600, 'ionic_force': [-18.553392615169287, 5.5990365743637085, -7.359938099980354], 'ionic_force_magnitude': 20.7303226441178, 'motion_vector': [-2.751720428466797, -2.4600486755371094, 0.600830078125], 'cosine_ionic_motion': 0.42384193582320084, 'ionic_motion_component': 8.786380079722424, 'ionic_force_x': -18.553392615169287, 'ionic_force_y': 5.5990365743637085, 'ionic_force_z': -7.359938099980354, 'radial_force': 19.379824253426055, 'axial_force': -7.359938099980354, 'contributions': [{'ion': 1309, 'force': [-0.036227066069841385, 5.730989933013916, -1.8837703466415405], 'magnitude': 6.032756328582764, 'distance': 7.418415546417236, 'directional_contribution': -4.046033798670543}, {'ion': 1380, 'force': [-0.34478411078453064, 1.6263123750686646, -1.8408604860305786], 'magnitude': 2.4804306030273438, 'distance': 11.569257736206055, 'directional_contribution': -1.1119032798557278}, {'ion': 1469, 'force': [-0.7819127440452576, 1.468832015991211, -0.126841738820076], 'magnitude': 1.6688151359558105, 'distance': 14.104735374450684, 'directional_contribution': -0.4112719219322474}, {'ion': 1476, 'force': [-0.10772905498743057, 0.7481944561004639, -1.3221204280853271], 'magnitude': 1.5229586362838745, 'distance': 14.7647123336792, 'directional_contribution': -0.6253363968497498}, {'ion': 2434, 'force': [-17.282739639282227, -3.975292205810547, -2.186345100402832], 'magnitude': 17.86829948425293, 'distance': 4.310497760772705, 'directional_contribution': 14.980925987625355}]}, 5601: {'frame': 5601, 'ionic_force': [-9.747690379619598, 9.922138929367065, -7.001989342272282], 'ionic_force_magnitude': 15.572224099976358, 'motion_vector': [-0.6682701110839844, -0.8040084838867188, 0.39972686767578125], 'cosine_ionic_motion': -0.24454050825740734, 'ionic_motion_component': -3.808039596106466, 'ionic_force_x': -9.747690379619598, 'ionic_force_y': 9.922138929367065, 'ionic_force_z': -7.001989342272282, 'radial_force': 13.909216680697368, 'axial_force': -7.001989342272282, 'contributions': [{'ion': 1309, 'force': [-1.464813470840454, 7.521646022796631, -2.570472478866577], 'magnitude': 8.082584381103516, 'distance': 6.409053802490234, 'directional_contribution': -5.446396251043808}, {'ion': 1380, 'force': [-1.123779535293579, 1.281681776046753, -2.1522297859191895], 'magnitude': 2.745483875274658, 'distance': 10.99662971496582, 'directional_contribution': -1.0183286977882204}, {'ion': 1469, 'force': [-1.2938627004623413, 1.2048321962356567, -0.07915589958429337], 'magnitude': 1.769736409187317, 'distance': 13.696661949157715, 'directional_contribution': -0.12122595433600791}, {'ion': 1476, 'force': [-0.5480816960334778, 0.5199006199836731, -1.4181257486343384], 'magnitude': 1.606788992881775, 'distance': 14.374396324157715, 'directional_contribution': -0.5526756114863964}, {'ion': 2434, 'force': [-5.317152976989746, -0.6059216856956482, -0.7820054292678833], 'magnitude': 5.408400058746338, 'distance': 7.834921360015869, 'directional_contribution': 3.3305870717415047}]}, 5602: {'frame': 5602, 'ionic_force': [-9.748128592967987, 11.87373073399067, -8.434279189445078], 'ionic_force_magnitude': 17.525654283189, 'motion_vector': [1.2005729675292969, 0.9844474792480469, -0.0977783203125], 'cosine_ionic_motion': 0.029724777835226476, 'ionic_motion_component': 0.5209461799847783, 'ionic_force_x': -9.748128592967987, 'ionic_force_y': 11.87373073399067, 'ionic_force_z': -8.434279189445078, 'radial_force': 15.362665543724976, 'axial_force': -8.434279189445078, 'contributions': [{'ion': 1309, 'force': [-2.806483507156372, 9.153647422790527, -4.609921932220459], 'magnitude': 10.626240730285645, 'distance': 5.589580535888672, 'directional_contribution': 3.916442934703298}, {'ion': 1380, 'force': [-1.2517857551574707, 1.1912050247192383, -2.192772626876831], 'magnitude': 2.7918074131011963, 'distance': 10.90501594543457, 'directional_contribution': -0.07442236424890325}, {'ion': 1469, 'force': [-1.356601595878601, 1.2908194065093994, -0.006111637689173222], 'magnitude': 1.872597098350525, 'distance': 13.315174102783203, 'directional_contribution': -0.22971479932318095}, {'ion': 1476, 'force': [-0.6084700226783752, 0.47949525713920593, -1.4761505126953125], 'magnitude': 1.667084813117981, 'distance': 14.112052917480469, 'directional_contribution': -0.07337039408029966}, {'ion': 2434, 'force': [-3.724787712097168, -0.24143637716770172, -0.1493224799633026], 'magnitude': 3.7355899810791016, 'distance': 9.427346229553223, 'directional_contribution': -3.017989412981734}]}, 5603: {'frame': 5603, 'ionic_force': [-17.560770630836487, 16.140983641147614, -9.764761259779334], 'ionic_force_magnitude': 25.773291999919827, 'motion_vector': [-1.2378005981445312, -0.32138824462890625, 0.05432891845703125], 'cosine_ionic_motion': 0.4855662067281127, 'ionic_motion_component': 12.514639631297083, 'ionic_force_x': -17.560770630836487, 'ionic_force_y': 16.140983641147614, 'ionic_force_z': -9.764761259779334, 'radial_force': 23.851876614904835, 'axial_force': -9.764761259779334, 'contributions': [{'ion': 1309, 'force': [-7.167101860046387, 12.286242485046387, -4.010806083679199], 'magnitude': 14.77855396270752, 'distance': 4.739724159240723, 'directional_contribution': 3.6757009343113474}, {'ion': 1380, 'force': [-1.6355546712875366, 2.433621406555176, -2.8497138023376465], 'magnitude': 4.0888166427612305, 'distance': 9.010942459106445, 'directional_contribution': 0.8496358498721843}, {'ion': 1469, 'force': [-1.2709964513778687, 1.487382173538208, -0.02657478116452694], 'magnitude': 1.9566409587860107, 'distance': 13.02607250213623, 'directional_contribution': 0.8545092104852909}, {'ion': 1476, 'force': [-0.5827058553695679, 0.6906329989433289, -1.6999109983444214], 'magnitude': 1.9251538515090942, 'distance': 13.13216495513916, 'directional_contribution': 0.3179366770997212}, {'ion': 2434, 'force': [-6.904411792755127, -0.7568954229354858, -1.17775559425354], 'magnitude': 7.044920444488525, 'distance': 6.864849090576172, 'directional_contribution': 6.816856713678004}]}, 5604: {'frame': 5604, 'ionic_force': [-14.2177032828331, 19.06482544541359, -2.1827616719529033], 'ionic_force_magnitude': 23.882527178238888, 'motion_vector': [0.9648094177246094, 0.07035064697265625, 0.3220977783203125], 'cosine_ionic_motion': -0.5371282190388663, 'ionic_motion_component': -12.827979289394776, 'ionic_force_x': -14.2177032828331, 'ionic_force_y': 19.06482544541359, 'ionic_force_z': -2.1827616719529033, 'radial_force': 23.782570422533652, 'axial_force': -2.1827616719529033, 'contributions': [{'ion': 1309, 'force': [-7.5053019523620605, 15.458601951599121, 1.4540939331054688], 'magnitude': 17.245647430419922, 'distance': 4.387622833251953, 'directional_contribution': -5.576095474802756}, {'ion': 1380, 'force': [-1.4976059198379517, 1.5437307357788086, -2.2601349353790283], 'magnitude': 3.1199581623077393, 'distance': 10.315604209899902, 'directional_contribution': -2.0246339891788097}, {'ion': 1469, 'force': [-1.2702255249023438, 1.183520793914795, 0.04746720567345619], 'magnitude': 1.7367923259735107, 'distance': 13.825953483581543, 'directional_contribution': -1.1053272624682102}, {'ion': 1476, 'force': [-0.6734047532081604, 0.5765787363052368, -1.429139256477356], 'magnitude': 1.6817716360092163, 'distance': 14.050297737121582, 'directional_contribution': -1.0489240501870594}, {'ion': 2434, 'force': [-3.271165132522583, 0.30239322781562805, 0.004951381124556065], 'magnitude': 3.285115957260132, 'distance': 10.052953720092773, 'directional_contribution': -3.0729981144680583}]}, 5605: {'frame': 5605, 'ionic_force': [-18.65671706199646, 11.948305934667587, -10.66128496825695], 'ionic_force_magnitude': 24.586543136727947, 'motion_vector': [-0.040676116943359375, 0.6826667785644531, -0.5590362548828125], 'cosine_ionic_motion': 0.6849713259002533, 'ionic_motion_component': 16.841077051668314, 'ionic_force_x': -18.65671706199646, 'ionic_force_y': 11.948305934667587, 'ionic_force_z': -10.66128496825695, 'radial_force': 22.154798718106253, 'axial_force': -10.66128496825695, 'contributions': [{'ion': 1309, 'force': [-11.117942810058594, 8.545702934265137, -6.663941860198975], 'magnitude': 15.525650024414062, 'distance': 4.6242804527282715, 'directional_contribution': 11.334251141633246}, {'ion': 1380, 'force': [-1.4706867933273315, 1.5739147663116455, -2.449951410293579], 'magnitude': 3.262267589569092, 'distance': 10.08809757232666, 'directional_contribution': 2.83471864706858}, {'ion': 1469, 'force': [-1.0578231811523438, 1.5526583194732666, 0.06499066203832626], 'magnitude': 1.8798832893371582, 'distance': 13.289344787597656, 'directional_contribution': 1.2075742205013205}, {'ion': 1476, 'force': [-0.48204028606414795, 0.6503790020942688, -1.660539984703064], 'magnitude': 1.8473626375198364, 'distance': 13.405807495117188, 'directional_contribution': 1.5758061713531215}, {'ion': 2434, 'force': [-4.528223991394043, -0.37434908747673035, 0.048157624900341034], 'magnitude': 4.54392671585083, 'distance': 8.547780990600586, 'directional_contribution': -0.11127310436116833}]}, 5606: {'frame': 5606, 'ionic_force': [-21.41411665081978, 2.977629542350769, -6.465997515246272], 'ionic_force_magnitude': 22.566342049467565, 'motion_vector': [-0.3365478515625, -0.6044425964355469, 0.14295196533203125], 'cosine_ionic_motion': 0.2811967488243754, 'ionic_motion_component': 6.345582017169072, 'ionic_force_x': -21.41411665081978, 'ionic_force_y': 2.977629542350769, 'ionic_force_z': -6.465997515246272, 'radial_force': 21.62014499549892, 'axial_force': -6.465997515246272, 'contributions': [{'ion': 1309, 'force': [-7.701904296875, 6.24114990234375, -5.068641662597656], 'magnitude': 11.133840560913086, 'distance': 5.460677623748779, 'directional_contribution': -2.6965391842246618}, {'ion': 1380, 'force': [-1.0523978471755981, 1.6155245304107666, -2.1546742916107178], 'magnitude': 2.891380786895752, 'distance': 10.715598106384277, 'directional_contribution': -1.3169285881203194}, {'ion': 1469, 'force': [-1.061071753501892, 1.283768892288208, -0.014648376032710075], 'magnitude': 1.6655781269073486, 'distance': 14.11843490600586, 'directional_contribution': -0.5958894575502764}, {'ion': 1476, 'force': [-0.44619205594062805, 0.6866577863693237, -1.5260471105575562], 'magnitude': 1.7318793535232544, 'distance': 13.845550537109375, 'directional_contribution': -0.6837594740408859}, {'ion': 2434, 'force': [-11.15255069732666, -6.849471569061279, 2.298013925552368], 'magnitude': 13.288171768188477, 'distance': 4.998462200164795, 'directional_contribution': 11.638698756338389}]}, 5607: {'frame': 5607, 'ionic_force': [-23.770193874835968, 13.231722950935364, -0.08699758723378181], 'ionic_force_magnitude': 27.204929290071377, 'motion_vector': [-0.3793296813964844, -0.6377906799316406, 0.31902313232421875], 'cosine_ionic_motion': 0.025025193227587485, 'ionic_motion_component': 0.6808086122268906, 'ionic_force_x': -23.770193874835968, 'ionic_force_y': 13.231722950935364, 'ionic_force_z': -0.08699758723378181, 'radial_force': 27.20479018661234, 'axial_force': -0.08699758723378181, 'contributions': [{'ion': 1309, 'force': [-8.924793243408203, 5.3618340492248535, -5.453948497772217], 'magnitude': 11.753583908081055, 'distance': 5.314762592315674, 'directional_contribution': -2.1965297723835135}, {'ion': 1380, 'force': [-1.5038363933563232, 1.5769492387771606, -2.552949905395508], 'magnitude': 3.3564634323120117, 'distance': 9.945533752441406, 'directional_contribution': -1.5472355919411385}, {'ion': 1469, 'force': [-1.4209312200546265, 1.4332846403121948, 0.041228216141462326], 'magnitude': 2.0186753273010254, 'distance': 12.824362754821777, 'directional_contribution': -0.44814113030013036}, {'ion': 1476, 'force': [-0.508072555065155, 0.625862717628479, -1.5353832244873047], 'magnitude': 1.7341405153274536, 'distance': 13.836520195007324, 'directional_contribution': -0.8619918711442516}, {'ion': 2434, 'force': [-11.41256046295166, 4.233792304992676, 9.414055824279785], 'magnitude': 15.388176918029785, 'distance': 4.644890308380127, 'directional_contribution': 5.7347067941715295}]}, 5608: {'frame': 5608, 'ionic_force': [-18.901110351085663, 10.239649832248688, -9.298373874276876], 'ionic_force_magnitude': 23.42140384129062, 'motion_vector': [-1.0680618286132812, 0.4606742858886719, 1.07733154296875], 'cosine_ionic_motion': 0.4009149166517778, 'ionic_motion_component': 9.389990168898658, 'ionic_force_x': -18.901110351085663, 'ionic_force_y': 10.239649832248688, 'ionic_force_z': -9.298373874276876, 'radial_force': 21.496567195507943, 'axial_force': -9.298373874276876, 'contributions': [{'ion': 1309, 'force': [-12.437792778015137, 5.437849521636963, -5.057575702667236], 'magnitude': 14.486129760742188, 'distance': 4.78732442855835, 'directional_contribution': 6.522305330380007}, {'ion': 1380, 'force': [-1.8392237424850464, 1.9834181070327759, -2.787628412246704], 'magnitude': 3.8842713832855225, 'distance': 9.245156288146973, 'directional_contribution': -0.07889636593342786}, {'ion': 1469, 'force': [-1.3467543125152588, 1.3719929456710815, 0.04987660422921181], 'magnitude': 1.9231743812561035, 'distance': 13.138921737670898, 'directional_contribution': 1.3398125508718068}, {'ion': 1476, 'force': [-0.6551981568336487, 0.6240441799163818, -1.8183751106262207], 'magnitude': 2.031059741973877, 'distance': 12.785204887390137, 'directional_contribution': -0.6129021072239702}, {'ion': 2434, 'force': [-2.6221413612365723, 0.8223450779914856, 0.3153287470340729], 'magnitude': 2.7660999298095703, 'distance': 10.955573081970215, 'directional_contribution': 2.2196714879421684}]}, 5609: {'frame': 5609, 'ionic_force': [-12.13606995344162, 7.872880041599274, 1.560283213853836], 'ionic_force_magnitude': 14.54994562779101, 'motion_vector': [1.0545501708984375, 1.109100341796875, -1.9637222290039062], 'cosine_ionic_motion': -0.19683564010415658, 'ionic_motion_component': -2.863947861126918, 'ionic_force_x': -12.13606995344162, 'ionic_force_y': 7.872880041599274, 'ionic_force_z': 1.560283213853836, 'radial_force': 14.466044174695467, 'axial_force': 1.560283213853836, 'contributions': [{'ion': 1309, 'force': [-4.694593906402588, 2.2950472831726074, 4.785083293914795], 'magnitude': 7.0854411125183105, 'distance': 6.845191478729248, 'directional_contribution': -4.740343296502999}, {'ion': 1380, 'force': [-2.6745073795318604, 2.1261026859283447, -2.479200601577759], 'magnitude': 4.221343040466309, 'distance': 8.868368148803711, 'directional_contribution': 1.769771147065427}, {'ion': 1469, 'force': [-1.283077597618103, 1.198951244354248, 0.1152741014957428], 'magnitude': 1.7598466873168945, 'distance': 13.73509407043457, 'directional_contribution': -0.10028648381809724}, {'ion': 1476, 'force': [-0.8566756844520569, 0.700995147228241, -1.6807165145874023], 'magnitude': 2.0124850273132324, 'distance': 12.844072341918945, 'directional_contribution': 1.2750868315675952}, {'ion': 2434, 'force': [-2.6272153854370117, 1.5517836809158325, 0.8198429346084595], 'magnitude': 3.159499406814575, 'distance': 10.250850677490234, 'directional_contribution': -1.0681760815864507}]}, 5610: {'frame': 5610, 'ionic_force': [-9.932288229465485, 6.841108322143555, -1.9635789394378662], 'ionic_force_magnitude': 12.219114321418077, 'motion_vector': [-1.6703529357910156, -1.2484626770019531, 1.5174026489257812], 'cosine_ionic_motion': 0.1608859926502964, 'ionic_motion_component': 1.9658843369088004, 'ionic_force_x': -9.932288229465485, 'ionic_force_y': 6.841108322143555, 'ionic_force_z': -1.9635789394378662, 'radial_force': 12.06031146150382, 'axial_force': -1.9635789394378662, 'contributions': [{'ion': 1309, 'force': [-3.3086962699890137, 1.7046713829040527, -0.6709098815917969], 'magnitude': 3.781996250152588, 'distance': 9.369329452514648, 'directional_contribution': 0.9230052034104261}, {'ion': 1380, 'force': [-1.2851455211639404, 1.4375178813934326, -2.0031657218933105], 'magnitude': 2.780418872833252, 'distance': 10.927326202392578, 'directional_contribution': -1.0421280538444577}, {'ion': 1476, 'force': [-0.5182755589485168, 0.6067698001861572, -1.3568806648254395], 'magnitude': 1.5741360187530518, 'distance': 14.52271842956543, 'directional_contribution': -0.7564015403241271}, {'ion': 2434, 'force': [-4.820170879364014, 3.092149257659912, 2.0673773288726807], 'magnitude': 6.088470935821533, 'distance': 7.384394645690918, 'directional_contribution': 2.8414090212096283}]}, 5611: {'frame': 5611, 'ionic_force': [-7.319891095161438, 3.427933633327484, -1.2991392612457275], 'ionic_force_magnitude': 8.186531466966432, 'motion_vector': [0.3722648620605469, 0.18717193603515625, -0.787353515625], 'cosine_ionic_motion': -0.14541296849198615, 'ionic_motion_component': -1.190427842264643, 'ionic_force_x': -7.319891095161438, 'ionic_force_y': 3.427933633327484, 'ionic_force_z': -1.2991392612457275, 'radial_force': 8.082792502565031, 'axial_force': -1.2991392612457275, 'contributions': [{'ion': 1309, 'force': [-3.486069440841675, 0.9354033470153809, -0.12702131271362305], 'magnitude': 3.611619472503662, 'distance': 9.587779998779297, 'directional_contribution': -1.1480010286185447}, {'ion': 1380, 'force': [-1.856589436531067, 1.3159931898117065, -1.8384387493133545], 'magnitude': 2.9255118370056152, 'distance': 10.65290641784668, 'directional_contribution': 1.1255786580515608}, {'ion': 1476, 'force': [-0.8016357421875, 0.5831083059310913, -1.5238325595855713], 'magnitude': 1.8178836107254028, 'distance': 13.51406478881836, 'directional_contribution': 1.134380122219527}, {'ion': 2434, 'force': [-1.1755964756011963, 0.5934287905693054, 2.1901533603668213], 'magnitude': 2.5555734634399414, 'distance': 11.397899627685547, 'directional_contribution': -2.3023856100099485}]}, 5612: {'frame': 5612, 'ionic_force': [-8.621939957141876, 5.55222961306572, -0.17053657211363316], 'ionic_force_magnitude': 10.256421648079403, 'motion_vector': [-0.15586090087890625, -0.2966651916503906, 0.673583984375], 'cosine_ionic_motion': -0.05419679783775443, 'ionic_motion_component': -0.5558652105997276, 'ionic_force_x': -8.621939957141876, 'ionic_force_y': 5.55222961306572, 'ionic_force_z': -0.17053657211363316, 'radial_force': 10.25500376892976, 'axial_force': -0.17053657211363316, 'contributions': [{'ion': 1309, 'force': [-1.8972725868225098, 0.33734628558158875, 0.2534988522529602], 'magnitude': 1.9436324834823608, 'distance': 13.069589614868164, 'directional_contribution': 0.4869920414607831}, {'ion': 1380, 'force': [-2.6392738819122314, 1.7558408975601196, -2.227714776992798], 'magnitude': 3.874462127685547, 'distance': 9.256852149963379, 'directional_contribution': -2.140104738595909}, {'ion': 1469, 'force': [-1.0927656888961792, 1.0563461780548096, 0.016937261447310448], 'magnitude': 1.5199642181396484, 'distance': 14.77924919128418, 'directional_contribution': -0.17499099365643833}, {'ion': 1476, 'force': [-0.7975227236747742, 0.5886553525924683, -1.336457371711731], 'magnitude': 1.6639338731765747, 'distance': 14.125408172607422, 'directional_contribution': -1.2634512787489198}, {'ion': 2434, 'force': [-2.1951050758361816, 1.8140408992767334, 3.123199462890625], 'magnitude': 4.226535797119141, 'distance': 8.862918853759766, 'directional_contribution': 2.535689673958629}]}, 5613: {'frame': 5613, 'ionic_force': [-8.001798212528229, 4.851924538612366, -1.1275118589401245], 'ionic_force_magnitude': 9.425562548434941, 'motion_vector': [0.5693893432617188, 0.08654403686523438, 0.20262908935546875], 'cosine_ionic_motion': -0.7584671333421469, 'ionic_motion_component': -7.14897940624855, 'ionic_force_x': -8.001798212528229, 'ionic_force_y': 4.851924538612366, 'ionic_force_z': -1.1275118589401245, 'radial_force': 9.357881510385177, 'axial_force': -1.1275118589401245, 'contributions': [{'ion': 1309, 'force': [-1.5278608798980713, 0.33984047174453735, 0.21905148029327393], 'magnitude': 1.5804537534713745, 'distance': 14.49366283416748, 'directional_contribution': -1.3040214101879046}, {'ion': 1380, 'force': [-2.67531681060791, 1.8371814489364624, -2.140955686569214], 'magnitude': 3.8879618644714355, 'distance': 9.240767478942871, 'directional_contribution': -2.945155512046922}, {'ion': 1469, 'force': [-1.2662698030471802, 1.0634814500808716, 0.1482248306274414], 'magnitude': 1.660241723060608, 'distance': 14.141105651855469, 'directional_contribution': -0.9809890908244032}, {'ion': 1476, 'force': [-0.8664065003395081, 0.5512539744377136, -1.658254623413086], 'magnitude': 1.9504741430282593, 'distance': 13.046648025512695, 'directional_contribution': -1.280231056313176}, {'ion': 2434, 'force': [-1.665944218635559, 1.0601671934127808, 2.30442214012146], 'magnitude': 3.0347464084625244, 'distance': 10.459425926208496, 'directional_contribution': -0.6385825097011715}]}, 5614: {'frame': 5614, 'ionic_force': [-8.395618259906769, 5.211301505565643, -1.0251549035310745], 'ionic_force_magnitude': 9.934536321551425, 'motion_vector': [0.22345352172851562, -0.025363922119140625, -0.6832504272460938], 'cosine_ionic_motion': -0.1830074353759896, 'ionic_motion_component': -1.8180940138567439, 'ionic_force_x': -8.395618259906769, 'ionic_force_y': 5.211301505565643, 'ionic_force_z': -1.0251549035310745, 'radial_force': 9.88150137114754, 'axial_force': -1.0251549035310745, 'contributions': [{'ion': 1309, 'force': [-2.1133174896240234, 0.614422619342804, 0.6714437007904053], 'magnitude': 2.3009698390960693, 'distance': 12.011951446533203, 'directional_contribution': -1.315952071765018}, {'ion': 1380, 'force': [-3.3152236938476562, 2.337308645248413, -2.591264247894287], 'magnitude': 4.813353538513184, 'distance': 8.305106163024902, 'directional_contribution': 1.349072856216412}, {'ion': 1469, 'force': [-1.176487684249878, 1.1284040212631226, 0.15199308097362518], 'magnitude': 1.637229561805725, 'distance': 14.240139961242676, 'directional_contribution': -0.5496389239860986}, {'ion': 1476, 'force': [-0.8708063960075378, 0.6309050917625427, -1.5651661157608032], 'magnitude': 1.8989708423614502, 'distance': 13.22238826751709, 'directional_contribution': 1.1939417513447441}, {'ion': 2434, 'force': [-0.9197829961776733, 0.500261127948761, 2.3078386783599854], 'magnitude': 2.5342416763305664, 'distance': 11.445770263671875, 'directional_contribution': -2.4955176217695687}]}, 5615: {'frame': 5615, 'ionic_force': [-9.628775656223297, 5.215168535709381, -1.9353300631046295], 'ionic_force_magnitude': 11.120108180538896, 'motion_vector': [0.29178619384765625, 0.19367218017578125, -0.18132781982421875], 'cosine_ionic_motion': -0.3303161578496842, 'ionic_motion_component': -3.6731514090684505, 'ionic_force_x': -9.628775656223297, 'ionic_force_y': 5.215168535709381, 'ionic_force_z': -1.9353300631046295, 'radial_force': 10.950401978636744, 'axial_force': -1.9353300631046295, 'contributions': [{'ion': 1309, 'force': [-2.8607401847839355, -0.19050782918930054, 0.09593595564365387], 'magnitude': 2.868680953979492, 'distance': 10.757909774780273, 'directional_contribution': -2.2542685123557153}, {'ion': 1380, 'force': [-2.6496500968933105, 1.8394922018051147, -2.5170533657073975], 'magnitude': 4.091446399688721, 'distance': 9.00804615020752, 'directional_contribution': 0.10025854441482451}, {'ion': 1469, 'force': [-1.1855692863464355, 1.2768100500106812, 0.0760083943605423], 'magnitude': 1.7440171241760254, 'distance': 13.797286033630371, 'directional_contribution': -0.2850940080080169}, {'ion': 1476, 'force': [-0.8022776246070862, 0.5966756343841553, -1.6538258790969849], 'magnitude': 1.9325660467147827, 'distance': 13.10695743560791, 'directional_contribution': 0.4598485895024709}, {'ion': 2434, 'force': [-2.1305384635925293, 1.6926984786987305, 2.0636048316955566], 'magnitu</t>
+          <t>{5594: {'frame': 5594, 'ionic_force': [-4.9196601659059525, 1.0488449931144714, -6.5911475121974945], 'ionic_force_magnitude': 8.291342321670859, 'motion_vector': [1.2472190856933594, -0.8786392211914062, 1.1838226318359375], 'cosine_ionic_motion': -0.9281191389561603, 'ionic_motion_component': -7.695353496379928, 'ionic_force_x': -4.9196601659059525, 'ionic_force_y': 1.0488449931144714, 'ionic_force_z': -6.5911475121974945, 'radial_force': 5.03022186067206, 'axial_force': -6.5911475121974945, 'contributions': [{'ion': 1309, 'force': [2.8878653049468994, 3.550973415374756, 0.24883276224136353], 'magnitude': 4.5837860107421875, 'distance': 8.51053524017334, 'cosine_with_motion': 0.08770757195450159, 'motion_component': 0.4020327582711829}, {'ion': 1380, 'force': [-0.7073386907577515, 1.981725811958313, -4.544967174530029], 'magnitude': 5.008421897888184, 'distance': 8.141765594482422, 'cosine_with_motion': -0.8275660510800515, 'motion_component': -4.144800091426141}, {'ion': 1469, 'force': [-1.5927733182907104, 2.366380214691162, 0.28326359391212463], 'magnitude': 2.8665170669555664, 'distance': 10.761969566345215, 'cosine_with_motion': -0.6739140830450312, 'motion_component': -1.9317862597870918}, {'ion': 1476, 'force': [-0.1692715436220169, 0.5136356949806213, -2.323270082473755], 'magnitude': 2.3853843212127686, 'distance': 11.797496795654297, 'cosine_with_motion': -0.7408856258182113, 'motion_component': -1.7672969554629239}, {'ion': 2434, 'force': [-5.338141918182373, -7.363870143890381, -0.2550066113471985], 'magnitude': 9.098756790161133, 'distance': 6.040571212768555, 'cosine_with_motion': -0.02786127094080532, 'motion_component': -0.2535029218473497}]}, 5595: {'frame': 5595, 'ionic_force': [-2.300809770822525, 3.5821394324302673, -8.520911037921906], 'ionic_force_magnitude': 9.525301750131783, 'motion_vector': [-0.8982429504394531, -0.04642486572265625, -0.12294769287109375], 'cosine_ionic_motion': 0.340923910951574, 'ionic_motion_component': 3.2474031256488, 'ionic_force_x': -2.300809770822525, 'ionic_force_y': 3.5821394324302673, 'ionic_force_z': -8.520911037921906, 'radial_force': 4.2573992665574885, 'axial_force': -8.520911037921906, 'contributions': [{'ion': 1309, 'force': [2.716885566711426, 2.478614091873169, 0.5846787095069885], 'magnitude': 3.7238211631774902, 'distance': 9.442231178283691, 'cosine_with_motion': -0.7772139667226173, 'motion_component': -2.894205831901914}, {'ion': 1380, 'force': [-0.13194406032562256, 3.3571829795837402, -8.195930480957031], 'magnitude': 8.857842445373535, 'distance': 6.122165679931641, 'cosine_with_motion': 0.12066999207138907, 'motion_component': 1.068875712637837}, {'ion': 1469, 'force': [-1.9954568147659302, 3.5336289405822754, 1.0472036600112915], 'magnitude': 4.19106388092041, 'distance': 8.900345802307129, 'cosine_with_motion': 0.394148309798264, 'motion_component': 1.6519007656536218}, {'ion': 1476, 'force': [0.18375858664512634, 0.6461936831474304, -3.1573736667633057], 'magnitude': 3.228055477142334, 'distance': 10.141414642333984, 'cosine_with_motion': 0.06590545004032208, 'motion_component': 0.2127464469587115}, {'ion': 2434, 'force': [-3.0740530490875244, -6.433480262756348, 1.2005107402801514], 'magnitude': 7.230539321899414, 'distance': 6.776160717010498, 'cosine_with_motion': 0.4436855947787157, 'motion_component': 3.2080860657232506}]}, 5596: {'frame': 5596, 'ionic_force': [-2.110570512712002, 4.475105106830597, -9.859978318214417], 'ionic_force_magnitude': 11.031783447927587, 'motion_vector': [0.0039520263671875, 1.0794944763183594, -1.8756179809570312], 'cosine_ionic_motion': 0.976641108636546, 'ionic_motion_component': 10.774093216822296, 'ionic_force_x': -2.110570512712002, 'ionic_force_y': 4.475105106830597, 'ionic_force_z': -9.859978318214417, 'radial_force': 4.947835244459004, 'axial_force': -9.859978318214417, 'contributions': [{'ion': 1309, 'force': [3.438979148864746, 2.82747483253479, 0.5633991956710815], 'magnitude': 4.487606525421143, 'distance': 8.601251602172852, 'cosine_with_motion': 0.20687836589783148, 'motion_component': 0.9283886550210865}, {'ion': 1380, 'force': [-0.861777663230896, 4.213195323944092, -8.890606880187988], 'magnitude': 9.876060485839844, 'distance': 5.7979865074157715, 'cosine_with_motion': 0.9928626063658836, 'motion_component': 9.805570931246908}, {'ion': 1469, 'force': [-1.7644017934799194, 2.603040933609009, 0.6845284700393677], 'magnitude': 3.2183094024658203, 'distance': 10.156759262084961, 'cosine_with_motion': 0.21811161373303217, 'motion_component': 0.7019506439526788}, {'ion': 1476, 'force': [-0.06188376992940903, 0.5250032544136047, -3.2976949214935303], 'magnitude': 3.3397979736328125, 'distance': 9.970316886901855, 'cosine_with_motion': 0.9341552778496334, 'motion_component': 3.119889807339182}, {'ion': 2434, 'force': [-2.8614864349365234, -5.693609237670898, 1.0803958177566528], 'magnitude': 6.463168144226074, 'distance': 7.167147159576416, 'cosine_with_motion': -0.5851165520115609, 'motion_component': -3.7817068149310367}]}, 5597: {'frame': 5597, 'ionic_force': [-2.391743592917919, 3.8317089676856995, -11.019856214523315], 'ionic_force_magnitude': 11.909645755272281, 'motion_vector': [1.3422393798828125, -0.8549842834472656, -0.35398101806640625], 'cosine_ionic_motion': -0.13316181833832863, 'ionic_motion_component': -1.585910084537414, 'ionic_force_x': -2.391743592917919, 'ionic_force_y': 3.8317089676856995, 'ionic_force_z': -11.019856214523315, 'radial_force': 4.5169050274836335, 'axial_force': -11.019856214523315, 'contributions': [{'ion': 1309, 'force': [2.360955238342285, 3.685953378677368, -0.3692745864391327], 'magnitude': 4.392804145812988, 'distance': 8.69356918334961, 'cosine_with_motion': 0.02070077484749574, 'motion_component': 0.09093444345478696}, {'ion': 1380, 'force': [-0.3367534875869751, 4.115484714508057, -6.502329349517822], 'magnitude': 7.702655792236328, 'distance': 6.565212726593018, 'cosine_with_motion': -0.13290461052277605, 'motion_component': -1.0237184513445428}, {'ion': 1469, 'force': [-1.0739519596099854, 3.1200692653656006, -0.15641751885414124], 'magnitude': 3.3034331798553467, 'distance': 10.025043487548828, 'cosine_with_motion': -0.7526977822934205, 'motion_component': -2.486486908028081}, {'ion': 1476, 'force': [-0.05223899334669113, 0.661562979221344, -2.2055890560150146], 'magnitude': 2.30326247215271, 'distance': 12.005972862243652, 'cosine_with_motion': 0.0386131363744981, 'motion_component': 0.0889361842241847}, {'ion': 2434, 'force': [-3.2897543907165527, -7.75136137008667, -1.7862457036972046], 'magnitude': 8.60794734954834, 'distance': 6.210395336151123, 'cosine_with_motion': 0.20265278659256922, 'motion_component': 1.7444245546876704}]}, 5598: {'frame': 5598, 'ionic_force': [3.7280571311712265, -0.048622846603393555, -10.82320636510849], 'ionic_force_magnitude': 11.44738267798423, 'motion_vector': [1.0442886352539062, 2.5621337890625, -0.08968353271484375], 'cosine_ionic_motion': 0.14955505651374204, 'ionic_motion_component': 1.7120139633403633, 'ionic_force_x': 3.7280571311712265, 'ionic_force_y': -0.048622846603393555, 'ionic_force_z': -10.82320636510849, 'radial_force': 3.728374197219004, 'axial_force': -10.82320636510849, 'contributions': [{'ion': 1309, 'force': [7.3780598640441895, 4.05808687210083, -3.189204216003418], 'magnitude': 9.004158020019531, 'distance': 6.0722198486328125, 'cosine_with_motion': 0.7377235610363455, 'motion_component': 6.642579449055013}, {'ion': 1380, 'force': [0.361459881067276, 1.1916948556900024, -3.9953513145446777], 'magnitude': 4.184927940368652, 'distance': 8.906867980957031, 'cosine_with_motion': 0.32707079284715657, 'motion_component': 1.3687677047499784}, {'ion': 1469, 'force': [-1.4546935558319092, 3.4690563678741455, -0.2319532036781311], 'magnitude': 3.768857717514038, 'distance': 9.385645866394043, 'cosine_with_motion': 0.708311737890327, 'motion_component': 2.669526086335598}, {'ion': 1476, 'force': [0.21506913006305695, 0.3528536558151245, -1.9371775388717651], 'magnitude': 1.9807617664337158, 'distance': 12.946516036987305, 'cosine_with_motion': 0.23752247681468455, 'motion_component': 0.470475445232283}, {'ion': 2434, 'force': [-2.7718381881713867, -9.120314598083496, -1.469520092010498], 'magnitude': 9.644827842712402, 'distance': 5.867076873779297, 'cosine_with_motion': -0.9786939015619761, 'motion_component': -9.439334723743546}]}, 5599: {'frame': 5599, 'ionic_force': [-1.9013180434703827, -9.60105836391449, -11.383936129510403], 'ionic_force_magnitude': 15.012972184430726, 'motion_vector': [-3.3165664672851562, 2.1229324340820312, -0.15932464599609375], 'cosine_ionic_motion': -0.20725825176288065, 'ionic_motion_component': -3.1115623687098677, 'ionic_force_x': -1.9013180434703827, 'ionic_force_y': -9.60105836391449, 'ionic_force_z': -11.383936129510403, 'radial_force': 9.787508978780986, 'axial_force': -11.383936129510403, 'contributions': [{'ion': 1309, 'force': [3.44903564453125, 3.2919468879699707, -1.7546262741088867], 'magnitude': 5.080499172210693, 'distance': 8.083805084228516, 'cosine_with_motion': -0.2083068570552768, 'motion_component': -1.0583028704620006}, {'ion': 1380, 'force': [0.5980334877967834, 1.709892749786377, -2.676297664642334], 'magnitude': 3.2317094802856445, 'distance': 10.135680198669434, 'cosine_with_motion': 0.16276051846555098, 'motion_component': 0.5259947179221207}, {'ion': 1469, 'force': [-0.6552402973175049, 2.634486198425293, -0.08947023004293442], 'magnitude': 2.716222047805786, 'distance': 11.055704116821289, 'cosine_with_motion': 0.7268021563776397, 'motion_component': 1.9741560530515698}, {'ion': 1476, 'force': [0.27780506014823914, 0.6250635385513306, -1.5681666135787964], 'magnitude': 1.710855484008789, 'distance': 13.930360794067383, 'cosine_with_motion': 0.09721179363021912, 'motion_component': 0.16631533363621465}, {'ion': 2434, 'force': [-5.57095193862915, -17.86244773864746, -5.295375347137451], 'magnitude': 19.445913314819336, 'distance': 4.131947994232178, 'cosine_with_motion': -0.24271040835726235, 'motion_component': -4.719725562381129}]}, 5600: {'frame': 5600, 'ionic_force': [-18.553392615169287, 5.5990365743637085, -7.359938099980354], 'ionic_force_magnitude': 20.7303226441178, 'motion_vector': [-2.751720428466797, -2.4600486755371094, 0.600830078125], 'cosine_ionic_motion': 0.42384193582320084, 'ionic_motion_component': 8.786380079722424, 'ionic_force_x': -18.553392615169287, 'ionic_force_y': 5.5990365743637085, 'ionic_force_z': -7.359938099980354, 'radial_force': 19.379824253426055, 'axial_force': -7.359938099980354, 'contributions': [{'ion': 1309, 'force': [-0.036227066069841385, 5.730989933013916, -1.8837703466415405], 'magnitude': 6.032756328582764, 'distance': 7.418415546417236, 'cosine_with_motion': -0.6706774795430298, 'motion_component': -4.046033798670543}, {'ion': 1380, 'force': [-0.34478411078453064, 1.6263123750686646, -1.8408604860305786], 'magnitude': 2.4804306030273438, 'distance': 11.569257736206055, 'cosine_with_motion': -0.44827028613449765, 'motion_component': -1.1119032798557278}, {'ion': 1469, 'force': [-0.7819127440452576, 1.468832015991211, -0.126841738820076], 'magnitude': 1.6688151359558105, 'distance': 14.104735374450684, 'cosine_with_motion': -0.24644546931116953, 'motion_component': -0.4112719219322474}, {'ion': 1476, 'force': [-0.10772905498743057, 0.7481944561004639, -1.3221204280853271], 'magnitude': 1.5229586362838745, 'distance': 14.7647123336792, 'cosine_with_motion': -0.41060629870047766, 'motion_component': -0.6253363968497498}, {'ion': 2434, 'force': [-17.282739639282227, -3.975292205810547, -2.186345100402832], 'magnitude': 17.86829948425293, 'distance': 4.310497760772705, 'cosine_with_motion': 0.8384080211694442, 'motion_component': 14.980925987625355}]}, 5601: {'frame': 5601, 'ionic_force': [-9.747690379619598, 9.922138929367065, -7.001989342272282], 'ionic_force_magnitude': 15.572224099976358, 'motion_vector': [-0.6682701110839844, -0.8040084838867188, 0.39972686767578125], 'cosine_ionic_motion': -0.24454050825740734, 'ionic_motion_component': -3.808039596106466, 'ionic_force_x': -9.747690379619598, 'ionic_force_y': 9.922138929367065, 'ionic_force_z': -7.001989342272282, 'radial_force': 13.909216680697368, 'axial_force': -7.001989342272282, 'contributions': [{'ion': 1309, 'force': [-1.464813470840454, 7.521646022796631, -2.570472478866577], 'magnitude': 8.082584381103516, 'distance': 6.409053802490234, 'cosine_with_motion': -0.6738434349501465, 'motion_component': -5.446396251043808}, {'ion': 1380, 'force': [-1.123779535293579, 1.281681776046753, -2.1522297859191895], 'magnitude': 2.745483875274658, 'distance': 10.99662971496582, 'cosine_with_motion': -0.3709104648523173, 'motion_component': -1.0183286977882204}, {'ion': 1469, 'force': [-1.2938627004623413, 1.2048321962356567, -0.07915589958429337], 'magnitude': 1.769736409187317, 'distance': 13.696661949157715, 'cosine_with_motion': -0.06849944068954568, 'motion_component': -0.1212259543360079}, {'ion': 1476, 'force': [-0.5480816960334778, 0.5199006199836731, -1.4181257486343384], 'magnitude': 1.606788992881775, 'distance': 14.374396324157715, 'cosine_with_motion': -0.3439627835312633, 'motion_component': -0.5526756114863964}, {'ion': 2434, 'force': [-5.317152976989746, -0.6059216856956482, -0.7820054292678833], 'magnitude': 5.408400058746338, 'distance': 7.834921360015869, 'cosine_with_motion': 0.6158174580254275, 'motion_component': 3.3305870717415047}]}, 5602: {'frame': 5602, 'ionic_force': [-9.748128592967987, 11.87373073399067, -8.434279189445078], 'ionic_force_magnitude': 17.525654283189, 'motion_vector': [1.2005729675292969, 0.9844474792480469, -0.0977783203125], 'cosine_ionic_motion': 0.029724777835226476, 'ionic_motion_component': 0.5209461799847783, 'ionic_force_x': -9.748128592967987, 'ionic_force_y': 11.87373073399067, 'ionic_force_z': -8.434279189445078, 'radial_force': 15.362665543724976, 'axial_force': -8.434279189445078, 'contributions': [{'ion': 1309, 'force': [-2.806483507156372, 9.153647422790527, -4.609921932220459], 'magnitude': 10.626240730285645, 'distance': 5.589580535888672, 'cosine_with_motion': 0.3685633566753359, 'motion_component': 3.916442934703298}, {'ion': 1380, 'force': [-1.2517857551574707, 1.1912050247192383, -2.192772626876831], 'magnitude': 2.7918074131011963, 'distance': 10.90501594543457, 'cosine_with_motion': -0.02665741311094373, 'motion_component': -0.07442236424890325}, {'ion': 1469, 'force': [-1.356601595878601, 1.2908194065093994, -0.006111637689173222], 'magnitude': 1.872597098350525, 'distance': 13.315174102783203, 'cosine_with_motion': -0.12267176777810217, 'motion_component': -0.22971479932318095}, {'ion': 1476, 'force': [-0.6084700226783752, 0.47949525713920593, -1.4761505126953125], 'magnitude': 1.667084813117981, 'distance': 14.112052917480469, 'cosine_with_motion': -0.04401119431896101, 'motion_component': -0.07337039408029966}, {'ion': 2434, 'force': [-3.724787712097168, -0.24143637716770172, -0.1493224799633026], 'magnitude': 3.7355899810791016, 'distance': 9.427346229553223, 'cosine_with_motion': -0.8079016858035686, 'motion_component': -3.017989412981734}]}, 5603: {'frame': 5603, 'ionic_force': [-17.560770630836487, 16.140983641147614, -9.764761259779334], 'ionic_force_magnitude': 25.773291999919827, 'motion_vector': [-1.2378005981445312, -0.32138824462890625, 0.05432891845703125], 'cosine_ionic_motion': 0.4855662067281127, 'ionic_motion_component': 12.514639631297083, 'ionic_force_x': -17.560770630836487, 'ionic_force_y': 16.140983641147614, 'ionic_force_z': -9.764761259779334, 'radial_force': 23.851876614904835, 'axial_force': -9.764761259779334, 'contributions': [{'ion': 1309, 'force': [-7.167101860046387, 12.286242485046387, -4.010806083679199], 'magnitude': 14.77855396270752, 'distance': 4.739724159240723, 'cosine_with_motion': 0.24871857187461996, 'motion_component': 3.6757009343113474}, {'ion': 1380, 'force': [-1.6355546712875366, 2.433621406555176, -2.8497138023376465], 'magnitude': 4.0888166427612305, 'distance': 9.010942459106445, 'cosine_with_motion': 0.20779505125123693, 'motion_component': 0.8496358498721843}, {'ion': 1469, 'force': [-1.2709964513778687, 1.487382173538208, -0.02657478116452694], 'magnitude': 1.9566409587860107, 'distance': 13.02607250213623, 'cosine_with_motion': 0.43672253559983204, 'motion_component': 0.8545092104852909}, {'ion': 1476, 'force': [-0.5827058553695679, 0.6906329989433289, -1.6999109983444214], 'magnitude': 1.9251538515090942, 'distance': 13.13216495513916, 'cosine_with_motion': 0.16514870871978457, 'motion_component': 0.3179366770997212}, {'ion': 2434, 'force': [-6.904411792755127, -0.7568954229354858, -1.17775559425354], 'magnitude': 7.044920444488525, 'distance': 6.864849090576172, 'cosine_with_motion': 0.9676272386019888, 'motion_component': 6.816856713678004}]}, 5604: {'frame': 5604, 'ionic_force': [-14.2177032828331, 19.06482544541359, -2.1827616719529033], 'ionic_force_magnitude': 23.882527178238888, 'motion_vector': [0.9648094177246094, 0.07035064697265625, 0.3220977783203125], 'cosine_ionic_motion': -0.5371282190388663, 'ionic_motion_component': -12.827979289394776, 'ionic_force_x': -14.2177032828331, 'ionic_force_y': 19.06482544541359, 'ionic_force_z': -2.1827616719529033, 'radial_force': 23.782570422533652, 'axial_force': -2.1827616719529033, 'contributions': [{'ion': 1309, 'force': [-7.5053019523620605, 15.458601951599121, 1.4540939331054688], 'magnitude': 17.245647430419922, 'distance': 4.387622833251953, 'cosine_with_motion': -0.3233335147373387, 'motion_component': -5.576095474802756}, {'ion': 1380, 'force': [-1.4976059198379517, 1.5437307357788086, -2.2601349353790283], 'magnitude': 3.1199581623077393, 'distance': 10.315604209899902, 'cosine_with_motion': -0.648929883303207, 'motion_component': -2.0246339891788097}, {'ion': 1469, 'force': [-1.2702255249023438, 1.183520793914795, 0.04746720567345619], 'magnitude': 1.7367923259735107, 'distance': 13.825953483581543, 'cosine_with_motion': -0.6364187952686731, 'motion_component': -1.1053272624682102}, {'ion': 1476, 'force': [-0.6734047532081604, 0.5765787363052368, -1.429139256477356], 'magnitude': 1.6817716360092163, 'distance': 14.050297737121582, 'cosine_with_motion': -0.6237018120886582, 'motion_component': -1.0489240501870594}, {'ion': 2434, 'force': [-3.271165132522583, 0.30239322781562805, 0.004951381124556065], 'magnitude': 3.285115957260132, 'distance': 10.052953720092773, 'cosine_with_motion': -0.9354306093367044, 'motion_component': -3.0729981144680583}]}, 5605: {'frame': 5605, 'ionic_force': [-18.65671706199646, 11.948305934667587, -10.66128496825695], 'ionic_force_magnitude': 24.586543136727947, 'motion_vector': [-0.040676116943359375, 0.6826667785644531, -0.5590362548828125], 'cosine_ionic_motion': 0.6849713259002533, 'ionic_motion_component': 16.841077051668314, 'ionic_force_x': -18.65671706199646, 'ionic_force_y': 11.948305934667587, 'ionic_force_z': -10.66128496825695, 'radial_force': 22.154798718106253, 'axial_force': -10.66128496825695, 'contributions': [{'ion': 1309, 'force': [-11.117942810058594, 8.545702934265137, -6.663941860198975], 'magnitude': 15.525650024414062, 'distance': 4.6242804527282715, 'cosine_with_motion': 0.7300339144435805, 'motion_component': 11.334251141633246}, {'ion': 1380, 'force': [-1.4706867933273315, 1.5739147663116455, -2.449951410293579], 'magnitude': 3.262267589569092, 'distance': 10.08809757232666, 'cosine_with_motion': 0.8689412030578023, 'motion_component': 2.83471864706858}, {'ion': 1469, 'force': [-1.0578231811523438, 1.5526583194732666, 0.06499066203832626], 'magnitude': 1.8798832893371582, 'distance': 13.289344787597656, 'cosine_with_motion': 0.6423665599546077, 'motion_component': 1.2075742205013205}, {'ion': 1476, 'force': [-0.48204028606414795, 0.6503790020942688, -1.660539984703064], 'magnitude': 1.8473626375198364, 'distance': 13.405807495117188, 'cosine_with_motion': 0.8530031608461415, 'motion_component': 1.5758061713531215}, {'ion': 2434, 'force': [-4.528223991394043, -0.37434908747673035, 0.048157624900341034], 'magnitude': 4.54392671585083, 'distance': 8.547780990600586, 'cosine_with_motion': -0.024488314677508453, 'motion_component': -0.11127310436116833}]}, 5606: {'frame': 5606, 'ionic_force': [-21.41411665081978, 2.977629542350769, -6.465997515246272], 'ionic_force_magnitude': 22.566342049467565, 'motion_vector': [-0.3365478515625, -0.6044425964355469, 0.14295196533203125], 'cosine_ionic_motion': 0.2811967488243754, 'ionic_motion_component': 6.345582017169072, 'ionic_force_x': -21.41411665081978, 'ionic_force_y': 2.977629542350769, 'ionic_force_z': -6.465997515246272, 'radial_force': 21.62014499549892, 'axial_force': -6.465997515246272, 'contributions': [{'ion': 1309, 'force': [-7.701904296875, 6.24114990234375, -5.068641662597656], 'magnitude': 11.133840560913086, 'distance': 5.460677623748779, 'cosine_with_motion': -0.24219307971669768, 'motion_component': -2.6965391842246618}, {'ion': 1380, 'force': [-1.0523978471755981, 1.6155245304107666, -2.1546742916107178], 'magnitude': 2.891380786895752, 'distance': 10.715598106384277, 'cosine_with_motion': -0.45546704130604865, 'motion_component': -1.3169285881203194}, {'ion': 1469, 'force': [-1.061071753501892, 1.283768892288208, -0.014648376032710075], 'magnitude': 1.6655781269073486, 'distance': 14.11843490600586, 'cosine_with_motion': -0.3577673465268641, 'motion_component': -0.5958894575502764}, {'ion': 1476, 'force': [-0.44619205594062805, 0.6866577863693237, -1.5260471105575562], 'magnitude': 1.7318793535232544, 'distance': 13.845550537109375, 'cosine_with_motion': -0.3948078010148448, 'motion_component': -0.6837594740408859}, {'ion': 2434, 'force': [-11.15255069732666, -6.849471569061279, 2.298013925552368], 'magnitude': 13.288171768188477, 'distance': 4.998462200164795, 'cosine_with_motion': 0.8758690610119446, 'motion_component': 11.638698756338389}]}, 5607: {'frame': 5607, 'ionic_force': [-23.770193874835968, 13.231722950935364, -0.08699758723378181], 'ionic_force_magnitude': 27.204929290071377, 'motion_vector': [-0.3793296813964844, -0.6377906799316406, 0.31902313232421875], 'cosine_ionic_motion': 0.025025193227587485, 'ionic_motion_component': 0.6808086122268906, 'ionic_force_x': -23.770193874835968, 'ionic_force_y': 13.231722950935364, 'ionic_force_z': -0.08699758723378181, 'radial_force': 27.20479018661234, 'axial_force': -0.08699758723378181, 'contributions': [{'ion': 1309, 'force': [-8.924793243408203, 5.3618340492248535, -5.453948497772217], 'magnitude': 11.753583908081055, 'distance': 5.314762592315674, 'cosine_with_motion': -0.1868816901934147, 'motion_component': -2.1965297723835135}, {'ion': 1380, 'force': [-1.5038363933563232, 1.5769492387771606, -2.552949905395508], 'magnitude': 3.3564634323120117, 'distance': 9.945533752441406, 'cosine_with_motion': -0.4609719947420178, 'motion_component': -1.5472355919411385}, {'ion': 1469, 'force': [-1.4209312200546265, 1.4332846403121948, 0.041228216141462326], 'magnitude': 2.0186753273010254, 'distance': 12.824362754821777, 'cosine_with_motion': -0.2219976237801517, 'motion_component': -0.44814113030013036}, {'ion': 1476, 'force': [-0.508072555065155, 0.625862717628479, -1.5353832244873047], 'magnitude': 1.7341405153274536, 'distance': 13.836520195007324, 'cosine_with_motion': -0.4970715103472714, 'motion_component': -0.8619918711442516}, {'ion': 2434, 'force': [-11.41256046295166, 4.233792304992676, 9.414055824279785], 'magnitude': 15.388176918029785, 'distance': 4.644890308380127, 'cosine_with_motion': 0.3726696751642105, 'motion_component': 5.7347067941715295}]}, 5608: {'frame': 5608, 'ionic_force': [-18.901110351085663, 10.239649832248688, -9.298373874276876], 'ionic_force_magnitude': 23.42140384129062, 'motion_vector': [-1.0680618286132812, 0.4606742858886719, 1.07733154296875], 'cosine_ionic_motion': 0.4009149166517778, 'ionic_motion_component': 9.389990168898658, 'ionic_force_x': -18.901110351085663, 'ionic_force_y': 10.239649832248688, 'ionic_force_z': -9.298373874276876, 'radial_force': 21.496567195507943, 'axial_force': -9.298373874276876, 'contributions': [{'ion': 1309, 'force': [-12.437792778015137, 5.437849521636963, -5.057575702667236], 'magnitude': 14.486129760742188, 'distance': 4.78732442855835, 'cosine_with_motion': 0.4502448365240324, 'motion_component': 6.522305330380007}, {'ion': 1380, 'force': [-1.8392237424850464, 1.9834181070327759, -2.787628412246704], 'magnitude': 3.8842713832855225, 'distance': 9.245156288146973, 'cosine_with_motion': -0.02031175472901016, 'motion_component': -0.07889636593342786}, {'ion': 1469, 'force': [-1.3467543125152588, 1.3719929456710815, 0.04987660422921181], 'magnitude': 1.9231743812561035, 'distance': 13.138921737670898, 'cosine_with_motion': 0.6966672397713636, 'motion_component': 1.3398125508718068}, {'ion': 1476, 'force': [-0.6551981568336487, 0.6240441799163818, -1.8183751106262207], 'magnitude': 2.031059741973877, 'distance': 12.785204887390137, 'cosine_with_motion': -0.30176468217530766, 'motion_component': -0.6129021072239702}, {'ion': 2434, 'force': [-2.6221413612365723, 0.8223450779914856, 0.3153287470340729], 'magnitude': 2.7660999298095703, 'distance': 10.955573081970215, 'cosine_with_motion': 0.802455270445704, 'motion_component': 2.2196714879421684}]}, 5609: {'frame': 5609, 'ionic_force': [-12.13606995344162, 7.872880041599274, 1.560283213853836], 'ionic_force_magnitude': 14.54994562779101, 'motion_vector': [1.0545501708984375, 1.109100341796875, -1.9637222290039062], 'cosine_ionic_motion': -0.19683564010415658, 'ionic_motion_component': -2.863947861126918, 'ionic_force_x': -12.13606995344162, 'ionic_force_y': 7.872880041599274, 'ionic_force_z': 1.560283213853836, 'radial_force': 14.466044174695467, 'axial_force': 1.560283213853836, 'contributions': [{'ion': 1309, 'force': [-4.694593906402588, 2.2950472831726074, 4.785083293914795], 'magnitude': 7.0854411125183105, 'distance': 6.845191478729248, 'cosine_with_motion': -0.6690258524147681, 'motion_component': -4.740343296502999}, {'ion': 1380, 'force': [-2.6745073795318604, 2.1261026859283447, -2.479200601577759], 'magnitude': 4.221343040466309, 'distance': 8.868368148803711, 'cosine_with_motion': 0.41924361152831724, 'motion_component': 1.769771147065427}, {'ion': 1469, 'force': [-1.283077597618103, 1.198951244354248, 0.1152741014957428], 'magnitude': 1.7598466873168945, 'distance': 13.73509407043457, 'cosine_with_motion': -0.05698592106483147, 'motion_component': -0.10028648381809724}, {'ion': 1476, 'force': [-0.8566756844520569, 0.700995147228241, -1.6807165145874023], 'magnitude': 2.0124850273132324, 'distance': 12.844072341918945, 'cosine_with_motion': 0.6335882762341097, 'motion_component': 1.2750868315675952}, {'ion': 2434, 'force': [-2.6272153854370117, 1.5517836809158325, 0.8198429346084595], 'magnitude': 3.159499406814575, 'distance': 10.250850677490234, 'cosine_with_motion': -0.3380839767120004, 'motion_component': -1.0681760815864507}]}, 5610: {'frame': 5610, 'ionic_force': [-9.932288229465485, 6.841108322143555, -1.9635789394378662], 'ionic_force_magnitude': 12.219114321418077, 'motion_vector': [-1.6703529357910156, -1.2484626770019531, 1.5174026489257812], 'cosine_ionic_motion': 0.1608859926502964, 'ionic_motion_component': 1.9658843369088004, 'ionic_force_x': -9.932288229465485, 'ionic_force_y': 6.841108322143555, 'ionic_force_z': -1.9635789394378662, 'radial_force': 12.06031146150382, 'axial_force': -1.9635789394378662, 'contributions': [{'ion': 1309, 'force': [-3.3086962699890137, 1.7046713829040527, -0.6709098815917969], 'magnitude': 3.781996250152588, 'distance': 9.369329452514648, 'cosine_with_motion': 0.24405238491228257, 'motion_component': 0.9230052034104261}, {'ion': 1380, 'force': [-1.2851455211639404, 1.4375178813934326, -2.0031657218933105], 'magnitude': 2.780418872833252, 'distance': 10.927326202392578, 'cosine_with_motion': -0.3748097210425503, 'motion_component': -1.0421280538444577}, {'ion': 1476, 'force': [-0.5182755589485168, 0.6067698001861572, -1.3568806648254395], 'magnitude': 1.5741360187530518, 'distance': 14.52271842956543, 'cosine_with_motion': -0.4805185316498841, 'motion_component': -0.7564015403241271}, {'ion': 2434, 'force': [-4.820170879364014, 3.092149257659912, 2.0673773288726807], 'magnitude': 6.088470935821533, 'distance': 7.384394645690918, 'cosine_with_motion': 0.4666867689292263, 'motion_component': 2.8414090212096283}]}, 5611: {'frame': 5611, 'ionic_force': [-7.319891095161438, 3.427933633327484, -1.2991392612457275], 'ionic_force_magnitude': 8.186531466966432, 'motion_vector': [0.3722648620605469, 0.18717193603515625, -0.787353515625], 'cosine_ionic_motion': -0.14541296849198615, 'ionic_motion_component': -1.190427842264643, 'ionic_force_x': -7.319891095161438, 'ionic_force_y': 3.427933633327484, 'ionic_force_z': -1.2991392612457275, 'radial_force': 8.082792502565031, 'axial_force': -1.2991392612457275, 'contributions': [{'ion': 1309, 'force': [-3.486069440841675, 0.9354033470153809, -0.12702131271362305], 'magnitude': 3.611619472503662, 'distance': 9.587779998779297, 'cosine_with_motion': -0.3178632443387379, 'motion_component': -1.1480010286185447}, {'ion': 1380, 'force': [-1.856589436531067, 1.3159931898117065, -1.8384387493133545], 'magnitude': 2.9255118370056152, 'distance': 10.65290641784668, 'cosine_with_motion': 0.3847458922885325, 'motion_component': 1.1255786580515608}, {'ion': 1476, 'force': [-0.8016357421875, 0.5831083059310913, -1.5238325595855713], 'magnitude': 1.8178836107254028, 'distance': 13.51406478881836, 'cosine_with_motion': 0.6240114132207905, 'motion_component': 1.134380122219527}, {'ion': 2434, 'force': [-1.1755964756011963, 0.5934287905693054, 2.1901533603668213], 'magnitude': 2.5555734634399414, 'distance': 11.397899627685547, 'cosine_with_motion': -0.9009271299748812, 'motion_component': -2.3023856100099485}]}, 5612: {'frame': 5612, 'ionic_force': [-8.621939957141876, 5.55222961306572, -0.17053657211363316], 'ionic_force_magnitude': 10.256421648079403, 'motion_vector': [-0.15586090087890625, -0.2966651916503906, 0.673583984375], 'cosine_ionic_motion': -0.05419679783775443, 'ionic_motion_component': -0.5558652105997276, 'ionic_force_x': -8.621939957141876, 'ionic_force_y': 5.55222961306572, 'ionic_force_z': -0.17053657211363316, 'radial_force': 10.25500376892976, 'axial_force': -0.17053657211363316, 'contributions': [{'ion': 1309, 'force': [-1.8972725868225098, 0.33734628558158875, 0.2534988522529602], 'magnitude': 1.9436324834823608, 'distance': 13.069589614868164, 'cosine_with_motion': 0.25055767037628246, 'motion_component': 0.4869920414607831}, {'ion': 1380, 'force': [-2.6392738819122314, 1.7558408975601196, -2.227714776992798], 'magnitude': 3.874462127685547, 'distance': 9.256852149963379, 'cosine_with_motion': -0.5523617605924889, 'motion_component': -2.140104738595909}, {'ion': 1469, 'force': [-1.0927656888961792, 1.0563461780548096, 0.016937261447310448], 'magnitude': 1.5199642181396484, 'distance': 14.77924919128418, 'cosine_with_motion': -0.1151283702740333, 'motion_component': -0.17499099365643833}, {'ion': 1476, 'force': [-0.7975227236747742, 0.5886553525924683, -1.336457371711731], 'magnitude': 1.6639338731765747, 'distance': 14.125408172607422, 'cosine_with_motion': -0.7593158004457016, 'motion_component': -1.2634512787489198}, {'ion': 2434, 'force': [-2.1951050758361816, 1.8140408992767334, 3.123199462890625], 'magnitude': 4.226535797119141, 'distance': 8.862918853759766, 'cosine_with_motion': 0.5999451429384265, 'motion_component': 2.535689673958629}]}, 5613: {'frame': 5613, 'ionic_force': [-8.001798212528229, 4.851924538612366, -1.1275118589401245], 'ionic_force_magnitude': 9.425562548434941, 'motion_vector': [0.5693893432617188, 0.08654403686523438, 0.20262908935546875], 'cosine_ionic_motion': -0.7584671333421469, 'ionic_motion_component': -7.14897940624855, 'ionic_force_x': -8.001798212528229, 'ionic_force_y': 4.851924538612366, 'ionic_force_z': -1.1275118589401245, 'radial_force': 9.357881510385177, 'axial_force': -1.1275118589401245, 'contributions': [{'ion': 1309, 'force': [-1.5278608798980713, 0.33984047174453735, 0.21905148029327393], 'magnitude': 1.5804537534713745, 'distance': 14.49366283416748, 'cosine_with_motion': -0.8250930682166862, 'motion_component': -1.3040214101879046}, {'ion': 1380, 'force': [-2.67531681060791, 1.8371814489364624, -2.140955686569214], 'magnitude': 3.8879618644714355, 'distance': 9.240767478942871, 'cosine_with_motion': -0.7575062880921174, 'motion_component': -2.945155512046922}, {'ion': 1469, 'force': [-1.2662698030471802, 1.0634814500808716, 0.1482248306274414], 'magnitude': 1.660241723060608, 'distance': 14.141105651855469, 'cosine_with_motion': -0.5908712399073002, 'motion_component': -0.980</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>{5689: {'frame': 5689, 'ionic_force': [-10.846781343221664, 1.6348312199115753, -4.6059174835681915], 'ionic_force_magnitude': 11.897050663534147, 'motion_vector': [1.6955833435058594, -2.072643280029297, 4.204833984375], 'cosine_ionic_motion': -0.6937842477004733, 'ionic_motion_component': -8.253986344454455, 'ionic_force_x': -10.846781343221664, 'ionic_force_y': 1.6348312199115753, 'ionic_force_z': -4.6059174835681915, 'radial_force': 10.969290707482374, 'axial_force': -4.6059174835681915, 'contributions': [{'ion': 1355, 'force': [-0.2695693075656891, 0.3014860451221466, -1.9719277620315552], 'magnitude': 2.0129730701446533, 'distance': 12.842514038085938, 'directional_contribution': -1.88030930318196}, {'ion': 1469, 'force': [-2.6125478744506836, 2.329728126525879, -0.3506489098072052], 'magnitude': 3.5179531574249268, 'distance': 9.714579582214355, 'directional_contribution': -2.1529863553754645}, {'ion': 1476, 'force': [-1.3893324136734009, 1.863111972808838, -5.913637638092041], 'magnitude': 6.353939056396484, 'distance': 7.228488922119141, 'directional_contribution': -6.235180191289949}, {'ion': 2434, 'force': [-0.631294310092926, -5.49688720703125, -1.0274757146835327], 'magnitude': 5.62761116027832, 'distance': 7.680809497833252, 'directional_contribution': 1.2040436448136056}, {'ion': 2443, 'force': [-5.944037437438965, 2.637392282485962, 4.657772541046143], 'magnitude': 7.998891353607178, 'distance': 6.442495822906494, 'directional_contribution': 0.8104460085251759}]}, 5690: {'frame': 5690, 'ionic_force': [-3.750170722603798, 1.514174997806549, -21.49210250377655], 'ionic_force_magnitude': 21.869315865053835, 'motion_vector': [-0.13861846923828125, -0.5360183715820312, -0.34649658203125], 'cosine_ionic_motion': 0.5009314964763403, 'ionic_motion_component': 10.955029123195187, 'ionic_force_x': -3.750170722603798, 'ionic_force_y': 1.514174997806549, 'ionic_force_z': -21.49210250377655, 'radial_force': 4.04431778828731, 'axial_force': -21.49210250377655, 'contributions': [{'ion': 1355, 'force': [0.17119938135147095, -0.25686579942703247, -4.116479396820068], 'magnitude': 4.128037452697754, 'distance': 8.968033790588379, 'directional_contribution': 2.3583023822572544}, {'ion': 1469, 'force': [-3.6085445880889893, 4.346920967102051, 2.5242862701416016], 'magnitude': 6.187838077545166, 'distance': 7.324864387512207, 'directional_contribution': -4.140733987203493}, {'ion': 1476, 'force': [0.4883006513118744, 1.3090105056762695, -24.288963317871094], 'magnitude': 24.329113006591797, 'distance': 3.6940767765045166, 'directional_contribution': 11.707616165324877}, {'ion': 2434, 'force': [-0.0496017187833786, -3.2350029945373535, 1.141748309135437], 'magnitude': 3.430931806564331, 'distance': 9.837007522583008, 'directional_contribution': 2.0597219802080753}, {'ion': 2443, 'force': [-0.7515244483947754, -0.6498876810073853, 3.2473056316375732], 'magnitude': 3.395899772644043, 'distance': 9.887616157531738, 'directional_contribution': -1.029877723230527}]}, 5691: {'frame': 5691, 'ionic_force': [-3.733049623668194, -2.4102413058280945, -3.200647473335266], 'ionic_force_magnitude': 5.476227432608747, 'motion_vector': [-1.1974220275878906, -3.1602745056152344, -3.7289962768554688], 'cosine_ionic_motion': 0.8716542732504011, 'ionic_motion_component': 4.773377042924487, 'ionic_force_x': -3.733049623668194, 'ionic_force_y': -2.4102413058280945, 'ionic_force_z': -3.200647473335266, 'radial_force': 4.443525924880957, 'axial_force': -3.200647473335266, 'contributions': [{'ion': 1355, 'force': [0.06907344609498978, -0.44401097297668457, -3.827573776245117], 'magnitude': 3.8538601398468018, 'distance': 9.281561851501465, 'directional_contribution': 3.0985270472823183}, {'ion': 1469, 'force': [-4.9462971687316895, 4.178884029388428, 2.458789587020874], 'magnitude': 6.926368236541748, 'distance': 6.923349380493164, 'directional_contribution': -3.2692035798063515}, {'ion': 1476, 'force': [-0.3097705841064453, -0.9671092629432678, -10.523290634155273], 'magnitude': 10.572175979614258, 'distance': 5.603854179382324, 'directional_contribution': 8.478517138465996}, {'ion': 2434, 'force': [0.13542890548706055, -3.8748512268066406, 1.5841094255447388], 'magnitude': 4.188342571258545, 'distance': 8.903237342834473, 'directional_contribution': 1.227268361060787}, {'ion': 2443, 'force': [1.3185157775878906, -1.3031538724899292, 7.107317924499512], 'magnitude': 7.34511137008667, 'distance': 6.723104000091553, 'directional_contribution': -4.76173187307522}]}, 5692: {'frame': 5692, 'ionic_force': [-2.2680077254772186, -15.304942309856415, -10.105775147676468], 'ionic_force_magnitude': 18.48003813541121, 'motion_vector': [5.063621520996094, 4.651702880859375, -0.6800384521484375], 'cosine_ionic_motion': -0.5936836240157243, 'ionic_motion_component': -10.971296012179716, 'ionic_force_x': -2.2680077254772186, 'ionic_force_y': -15.304942309856415, 'ionic_force_z': -10.105775147676468, 'radial_force': 15.472075431268339, 'axial_force': -10.105775147676468, 'contributions': [{'ion': 1355, 'force': [-0.16544833779335022, -0.5105010867118835, -1.7802817821502686], 'magnitude': 1.859405279159546, 'distance': 13.362324714660645, 'directional_contribution': -0.2897184830593833}, {'ion': 1469, 'force': [-8.14029312133789, 1.124986171722412, -1.0288584232330322], 'magnitude': 8.281818389892578, 'distance': 6.331493854522705, 'directional_contribution': -5.106975882015757}, {'ion': 1476, 'force': [-0.7527567744255066, -2.250356912612915, -4.554305553436279], 'magnitude': 5.135411262512207, 'distance': 8.040470123291016, 'directional_contribution': -1.618435477507159}, {'ion': 2434, 'force': [-0.9204217195510864, -2.4938366413116455, -0.17049100995063782], 'magnitude': 2.663731336593628, 'distance': 11.164103507995605, 'directional_contribution': -2.336686691254273}, {'ion': 2443, 'force': [7.710912227630615, -11.175233840942383, -2.57183837890625], 'magnitude': 13.818768501281738, 'distance': 4.901560306549072, 'directional_contribution': -1.6194791760610485}]}, 5693: {'frame': 5693, 'ionic_force': [14.037217020988464, 0.7251570634543896, -12.502707362174988], 'ionic_force_magnitude': 18.811884696786514, 'motion_vector': [0.5311241149902344, 0.9281234741210938, 2.3688735961914062], 'cosine_ionic_motion': -0.43950603727257137, 'ionic_motion_component': -8.267936896713168, 'ionic_force_x': 14.037217020988464, 'ionic_force_y': 0.7251570634543896, 'ionic_force_z': -12.502707362174988, 'radial_force': 14.055935204069705, 'axial_force': -12.502707362174988, 'contributions': [{'ion': 1355, 'force': [0.4393165409564972, 0.04694287106394768, -1.5332221984863281], 'magnitude': 1.595610499382019, 'distance': 14.424660682678223, 'directional_contribution': -1.2908975703916323}, {'ion': 1469, 'force': [-0.2973380386829376, 6.702067852020264, -1.863255262374878], 'magnitude': 6.9626030921936035, 'distance': 6.90531063079834, 'directional_contribution': 0.63431096597406}, {'ion': 1476, 'force': [1.3921409845352173, 0.3217581510543823, -3.227895498275757], 'magnitude': 3.529999256134033, 'distance': 9.697990417480469, 'directional_contribution': -2.5426374261861078}, {'ion': 2434, 'force': [2.518434524536133, -7.808837413787842, -1.8178147077560425], 'magnitude': 8.403862953186035, 'distance': 6.285351276397705, 'directional_contribution': -3.930717568695087}, {'ion': 2443, 'force': [9.984663009643555, 1.4632256031036377, -4.060519695281982], 'magnitude': 10.877607345581055, 'distance': 5.524619102478027, 'directional_contribution': -1.1379953539395444}]}, 5694: {'frame': 5694, 'ionic_force': [15.186673760414124, -2.523807108402252, -6.381444334983826], 'ionic_force_magnitude': 16.66515808584394, 'motion_vector': [-6.16156005859375, -6.210399627685547, -0.5569686889648438], 'cosine_ionic_motion': -0.5089087171859848, 'ionic_motion_component': -8.481044223168483, 'ionic_force_x': 15.186673760414124, 'ionic_force_y': -2.523807108402252, 'ionic_force_z': -6.381444334983826, 'radial_force': 15.39495573964643, 'axial_force': -6.381444334983826, 'contributions': [{'ion': 1355, 'force': [0.7672042846679688, 0.321216881275177, -2.13971209526062], 'magnitude': 2.2956807613372803, 'distance': 12.02578067779541, 'directional_contribution': -0.6308760194952647}, {'ion': 1469, 'force': [0.36691606044769287, 5.6577959060668945, 0.787419319152832], 'magnitude': 5.724099159240723, 'distance': 7.6157989501953125, 'directional_contribution': -4.316242741675154}, {'ion': 1476, 'force': [4.058429718017578, 1.9305769205093384, -4.828175067901611], 'magnitude': 6.596154689788818, 'distance': 7.09453010559082, 'directional_contribution': -3.9135829908792417}, {'ion': 2434, 'force': [3.7240912914276123, -11.90422248840332, -1.445675253868103], 'magnitude': 12.556645393371582, 'distance': 5.142002105712891, 'directional_contribution': 5.9078834976516035}, {'ion': 2443, 'force': [6.2700324058532715, 1.4708256721496582, 1.2446987628936768], 'magnitude': 6.559413909912109, 'distance': 7.114371299743652, 'directional_contribution': -5.528225916871648}]}, 5695: {'frame': 5695, 'ionic_force': [-17.885726302862167, -13.695586919784546, -6.164025843143463], 'ionic_force_magnitude': 23.35516048014249, 'motion_vector': [2.018024444580078, -2.0229759216308594, -1.58453369140625], 'cosine_ionic_motion': 0.01807265163752099, 'ionic_motion_component': 0.4220896792960127, 'ionic_force_x': -17.885726302862167, 'ionic_force_y': -13.695586919784546, 'ionic_force_z': -6.164025843143463, 'radial_force': 22.527057208127943, 'axial_force': -6.164025843143463, 'contributions': [{'ion': 1355, 'force': [-0.28277072310447693, -0.719104528427124, -1.999786376953125], 'magnitude': 2.143878698348999, 'distance': 12.444255828857422, 'directional_contribution': 1.240398856016542}, {'ion': 1469, 'force': [-9.842928886413574, 4.126557350158691, -0.23699882626533508], 'magnitude': 10.67557430267334, 'distance': 5.576650142669678, 'directional_contribution': -8.519330112078663}, {'ion': 1476, 'force': [-1.4224494695663452, -3.3690109252929688, -5.0304341316223145], 'magnitude': 6.219233512878418, 'distance': 7.306352615356445, 'directional_contribution': 3.646921530555055}, {'ion': 2434, 'force': [-1.0529464483261108, -2.425291061401367, -0.3027394115924835], 'magnitude': 2.6612749099731445, 'distance': 11.169254302978516, 'directional_contribution': 0.9980965971669695}, {'ion': 2443, 'force': [-5.28463077545166, -11.308737754821777, 1.405932903289795], 'magnitude': 12.561509132385254, 'distance': 5.141005992889404, 'directional_contribution': 3.0560029014484797}]}, 5696: {'frame': 5696, 'ionic_force': [-15.213935688138008, -14.176376223564148, -12.65572875738144], 'ionic_force_magnitude': 24.3433964831378, 'motion_vector': [-0.21909713745117188, -0.3765602111816406, 0.164337158203125], 'cosine_ionic_motion': 0.5815461614722945, 'ionic_motion_component': 14.15680878196694, 'ionic_force_x': -15.213935688138008, 'ionic_force_y': -14.176376223564148, 'ionic_force_z': -12.65572875738144, 'radial_force': 20.79503503134424, 'axial_force': -12.65572875738144, 'contributions': [{'ion': 1355, 'force': [0.09340129792690277, -0.6584328413009644, -1.331163763999939], 'magnitude': 1.4880372285842896, 'distance': 14.936958312988281, 'directional_contribution': 0.01871884341876351}, {'ion': 1469, 'force': [-16.17984390258789, -5.707157611846924, -8.072161674499512], 'magnitude': 18.960981369018555, 'distance': 4.184452533721924, 'directional_contribution': 9.379817903545728}, {'ion': 1476, 'force': [0.16498154401779175, -2.0770199298858643, -2.584268808364868], 'magnitude': 3.319589853286743, 'distance': 10.000617980957031, 'directional_contribution': 0.6900054763974506}, {'ion': 2434, 'force': [-0.31412482261657715, -3.6910321712493896, -0.3123330771923065], 'magnitude': 3.7175185680389404, 'distance': 9.450231552124023, 'directional_contribution': 3.0225779550752616}, {'ion': 2443, 'force': [1.0216501951217651, -2.042733669281006, -0.35580143332481384], 'magnitude': 2.3115200996398926, 'distance': 11.98450756072998, 'directional_contribution': 1.045688783874306}]}, 5697: {'frame': 5697, 'ionic_force': [-14.388794315978885, -13.769953429698944, -10.123002961277962], 'ionic_force_magnitude': 22.341087893781413, 'motion_vector': [-1.5983009338378906, 3.4348678588867188, 0.1610565185546875], 'cosine_ionic_motion': -0.30608964031464103, 'ionic_motion_component': -6.838375557645334, 'ionic_force_x': -14.388794315978885, 'ionic_force_y': -13.769953429698944, 'ionic_force_z': -10.123002961277962, 'radial_force': 19.916049290048065, 'axial_force': -10.123002961277962, 'contributions': [{'ion': 1355, 'force': [0.01840483583509922, -0.6926707625389099, -1.3557699918746948], 'magnitude': 1.5225780010223389, 'distance': 14.766557693481445, 'directional_contribution': -0.692786103021971}, {'ion': 1469, 'force': [-15.130455017089844, -6.483215808868408, -6.229846477508545], 'magnitude': 17.60038948059082, 'distance': 4.3431806564331055, 'directional_contribution': 0.24015990551625777}, {'ion': 1476, 'force': [0.08019865304231644, -2.2278919219970703, -2.5778114795684814], 'magnitude': 3.408085346221924, 'distance': 9.86992359161377, 'directional_contribution': -2.1613910932444793}, {'ion': 2434, 'force': [-0.08338899910449982, -2.282119035720825, 0.2655191719532013], 'magnitude': 2.2990262508392334, 'distance': 12.017027854919434, 'directional_contribution': -2.0207939367997354}, {'ion': 2443, 'force': [0.7264462113380432, -2.0840559005737305, -0.22509418427944183], 'magnitude': 2.2184860706329346, 'distance': 12.233217239379883, 'directional_contribution': -2.2035646993996467}]}, 5698: {'frame': 5698, 'ionic_force': [-9.738676965236664, -11.330120891332626, -6.976988285779953], 'ionic_force_magnitude': 16.48914291239402, 'motion_vector': [-2.993671417236328, -2.5537109375, 1.6241912841796875], 'cosine_ionic_motion': 0.6661082666101348, 'ionic_motion_component': 10.98355440326157, 'ionic_force_x': -9.738676965236664, 'ionic_force_y': -11.330120891332626, 'ionic_force_z': -6.976988285779953, 'radial_force': 14.940330265608027, 'axial_force': -6.976988285779953, 'contributions': [{'ion': 1355, 'force': [-0.1521759033203125, -0.4667292535305023, -1.7436898946762085], 'magnitude': 1.8114768266677856, 'distance': 13.537941932678223, 'directional_contribution': -0.2782822313194284}, {'ion': 1469, 'force': [-6.2060546875, 1.8714954853057861, -0.3370665907859802], 'magnitude': 6.490856647491455, 'distance': 7.151844024658203, 'directional_contribution': 3.1130770405235584}, {'ion': 1476, 'force': [-0.9171950221061707, -2.0580520629882812, -4.527716159820557], 'magnitude': 5.057374477386475, 'distance': 8.102265357971191, 'directional_contribution': 0.15212195803306727}, {'ion': 2434, 'force': [-3.975003957748413, -6.597219944000244, 0.32685384154319763], 'magnitude': 7.709137439727783, 'distance': 6.5624518394470215, 'directional_contribution': 6.877745132606193}, {'ion': 2443, 'force': [1.5117526054382324, -4.079615116119385, -0.6953694820404053], 'magnitude': 4.4059271812438965, 'distance': 8.680612564086914, 'directional_contribution': 1.1188924746078683}]}, 5699: {'frame': 5699, 'ionic_force': [-7.502817556262016, -9.551654130220413, -3.1742424368858337], 'ionic_force_magnitude': 12.553970804253016, 'motion_vector': [-0.2769050598144531, -0.16832733154296875, 0.20163726806640625], 'cosine_ionic_motion': 0.635580549251634, 'ionic_motion_component': 7.979059659056109, 'ionic_force_x': -7.502817556262016, 'ionic_force_y': -9.551654130220413, 'ionic_force_z': -3.1742424368858337, 'radial_force': 12.14604330248786, 'axial_force': -3.1742424368858337, 'contributions': [{'ion': 1355, 'force': [-0.6258348226547241, -0.9120814800262451, -1.6169955730438232], 'magnitude': 1.959141731262207, 'distance': 13.017755508422852, 'directional_contribution': 0.0020397527652349368}, {'ion': 1469, 'force': [-3.346435785293579, -0.3936164677143097, 0.2601182758808136], 'magnitude': 3.379530668258667, 'distance': 9.91153335571289, 'directional_contribution': 2.7389235418649394}, {'ion': 1476, 'force': [-2.058412790298462, -2.6242835521698, -2.340930461883545], 'magnitude': 4.074786186218262, 'distance': 9.026442527770996, 'directional_contribution': 1.414080129720439}, {'ion': 2434, 'force': [-1.4498467445373535, -2.6175620555877686, 0.3526051938533783], 'magnitude': 3.012974739074707, 'distance': 10.497147560119629, 'directional_contribution': 2.3926106197890356}, {'ion': 2443, 'force': [-0.022287413477897644, -3.00411057472229, 0.17096012830734253], 'magnitude': 3.0090537071228027, 'distance': 10.503984451293945, 'directional_contribution': 1.4314057776705322}]}, 5700: {'frame': 5700, 'ionic_force': [-7.085268452763557, -8.294093906879425, -2.452709883451462], 'ionic_force_magnitude': 11.180733811170061, 'motion_vector': [0.4935493469238281, -0.46282196044921875, 0.6883697509765625], 'cosine_ionic_motion': -0.12478037358923734, 'ionic_motion_component': -1.3951361419596175, 'ionic_force_x': -7.085268452763557, 'ionic_force_y': -8.294093906879425, 'ionic_force_z': -2.452709883451462, 'radial_force': 10.908392309770532, 'axial_force': -2.452709883451462, 'contributions': [{'ion': 1355, 'force': [-0.5744865536689758, -0.7606053352355957, -1.4772404432296753], 'magnitude': 1.7580655813217163, 'distance': 13.742049217224121, 'directional_contribution': -0.9825750645518134}, {'ion': 1469, 'force': [-3.6154754161834717, -0.5478944182395935, 0.3197089731693268], 'magnitude': 3.670703649520874, 'distance': 9.510303497314453, 'directional_contribution': -1.3579921723084798}, {'ion': 1476, 'force': [-1.7856495380401611, -2.236912727355957, -2.2723193168640137], 'magnitude': 3.654552936553955, 'distance': 9.531294822692871, 'directional_contribution': -1.4610254591911342}, {'ion': 2434, 'force': [-0.9666056632995605, -1.7378770112991333, 0.8489934206008911], 'magnitude': 2.1622519493103027, 'distance': 12.39127254486084, 'directional_contribution': 0.9445331170802014}, {'ion': 2443, 'force': [-0.14305128157138824, -3.0108044147491455, 0.12814748287200928], 'magnitude': 3.016923666000366, 'distance': 10.490275382995605, 'directional_contribution': 1.4619233628143808}]}, 5701: {'frame': 5701, 'ionic_force': [-7.92530158162117, -8.08792930841446, -1.2593768686056137], 'ionic_force_magnitude': 11.393464607165614, 'motion_vector': [0.5581855773925781, 0.4502677917480469, 0.15650177001953125], 'cosine_ionic_motion': -0.9879751759881211, 'ionic_motion_component': -11.256460200378877, 'ionic_force_x': -7.92530158162117, 'ionic_force_y': -8.08792930841446, 'ionic_force_z': -1.2593768686056137, 'radial_force': 11.323648071957933, 'axial_force': -1.2593768686056137, 'contributions': [{'ion': 1355, 'force': [-0.6315168142318726, -1.0191653966903687, -1.574242353439331], 'magnitude': 1.978825569152832, 'distance': 12.952848434448242, 'directional_contribution': -1.441041549650734}, {'ion': 1469, 'force': [-3.8441007137298584, -0.7395055890083313, 0.717881441116333], 'magnitude': 3.979865789413452, 'distance': 9.13344955444336, 'directional_contribution': -3.223759742268882}, {'ion': 1476, 'force': [-1.9888440370559692, -2.9822001457214355, -2.092775821685791], 'magnitude': 4.150750637054443, 'distance': 8.943463325500488, 'directional_contribution': -3.787914575494952}, {'ion': 2434, 'force': [-1.2842319011688232, -1.5509859323501587, 1.57150137424469], 'magnitude': 2.554295539855957, 'distance': 11.400751113891602, 'directional_contribution': -1.592919314496072}, {'ion': 2443, 'force': [-0.1766081154346466, -1.796072244644165, 0.11825849115848541], 'magnitude': 1.8086047172546387, 'distance': 13.548686981201172, 'directional_contribution': -1.2108249223917582}]}, 5702: {'frame': 5702, 'ionic_force': [-7.804108589887619, -8.228433191776276, -0.8812482059001923], 'ionic_force_magnitude': 11.37487679382443, 'motion_vector': [-0.39960479736328125, -0.060466766357421875, -0.1700592041015625], 'cosine_ionic_motion': 0.755066697342409, 'ionic_motion_component': 8.588790653389824, 'ionic_force_x': -7.804108589887619, 'ionic_force_y': -8.228433191776276, 'ionic_force_z': -0.8812482059001923, 'radial_force': 11.340688853605112, 'axial_force': -0.8812482059001923, 'contributions': [{'ion': 1355, 'force': [-0.5931767225265503, -0.9305346608161926, -1.5677777528762817], 'magnitude': 1.9172064065933228, 'distance': 13.159355163574219, 'directional_contribution': 1.276966028057073}, {'ion': 1469, 'force': [-4.320357799530029, -0.4477121829986572, 0.8675047755241394], 'magnitude': 4.4292778968811035, 'distance': 8.65770149230957, 'directional_contribution': 3.662649262649394}, {'ion': 1476, 'force': [-1.978808045387268, -2.9532740116119385, -2.4418883323669434], 'magnitude': 4.312809467315674, 'distance': 8.773823738098145, 'directional_contribution': 3.1577207300576404}, {'ion': 2434, 'force': [-0.7739160060882568, -1.956164002418518, 2.087541341781616], 'magnitude': 2.963671922683716, 'distance': 10.584100723266602, 'directional_contribution': 0.16543208727818737}, {'ion': 2443, 'force': [-0.13785001635551453, -1.9407483339309692, 0.17337176203727722], 'magnitude': 1.9533469676971436, 'distance': 13.037050247192383, 'directional_contribution': 0.3260227469765544}]}, 5703: {'frame': 5703, 'ionic_force': [-7.383249953389168, -8.355258643627167, -1.0149785578250885], 'ionic_force_magnitude': 11.196111304777759, 'motion_vector': [-0.3843231201171875, 0.9410591125488281, -0.6316909790039062], 'cosine_ionic_motion': -0.32718268002181145, 'ionic_motion_component': -3.6631737025196873, 'ionic_force_x': -7.383249953389168, 'ionic_force_y': -8.355258643627167, 'ionic_force_z': -1.0149785578250885, 'radial_force': 11.15001017381274, 'axial_force': -1.0149785578250885, 'contributions': [{'ion': 1355, 'force': [-0.60088050365448, -0.9079782366752625, -1.5684553384780884], 'magnitude': 1.9093282222747803, 'distance': 13.18647575378418, 'directional_contribution': 0.30686014280205853}, {'ion': 1469, 'force': [-3.552804470062256, -0.41763007640838623, 0.6142292618751526], 'magnitude': 3.6296157836914062, 'distance': 9.563981056213379, 'directional_contribution': 0.48830820908270667}, {'ion': 1476, 'force': [-2.070937156677246, -2.9030516147613525, -2.323512554168701], 'magnitude': 4.256195545196533, 'distance': 8.83198356628418, 'directional_contribution': -0.39128694689864574}, {'ion': 2434, 'force': [-1.004224419593811, -1.850171685218811, 2.136342763900757], 'magnitude': 2.999260425567627, 'distance': 10.521120071411133, 'directional_contribution': -2.2599289317871296}, {'ion': 2443, 'force': [-0.15440340340137482, -2.2764270305633545, 0.12641730904579163], 'magnitude': 2.285156726837158, 'distance': 12.05344009399414, 'directional_contribution': -1.8071260334216284}]}, 5704: {'frame': 5704, 'ionic_force': [-9.369131922721863, -6.612637624144554, -1.1421239897608757], 'ionic_force_magnitude': 11.524411331673532, 'motion_vector': [0.2603874206542969, -0.4796562194824219, 0.38088226318359375], 'cosine_ionic_motion': 0.03874520782907011, 'ionic_motion_component': 0.4465157121533816, 'ionic_force_x': -9.369131922721863, 'ionic_force_y': -6.612637624144554, 'ionic_force_z': -1.1421239897608757, 'radial_force': 11.467676719092582, 'axial_force': -1.1421239897608757, 'contributions': [{'ion': 1355, 'force': [-0.6172433495521545, -0.7568070888519287, -1.5594958066940308], 'magnitude': 1.8400471210479736, 'distance': 13.432429313659668, 'directional_contribution': -0.5885442069841993}, {'ion': 1469, 'force': [-3.870227813720703, 0.14175964891910553, 0.3387364447116852], 'magnitude': 3.887608766555786, 'distance': 9.24118709564209, 'directional_contribution': -1.4225086309504258}, {'ion': 1476, 'force': [-2.3841171264648438, -2.5097689628601074, -2.422724962234497], 'magnitude': 4.2252278327941895, 'distance': 8.864290237426758, 'directional_contribution': -0.5104742520899492}, {'ion': 2434, 'force': [-2.1380257606506348, -1.4192434549331665, 2.406752109527588], 'magnitude': 3.518218517303467, 'distance': 9.714213371276855, 'directional_contribution': 1.5637282455528023}, {'ion': 2443, 'force': [-0.3595178723335266, -2.068577766418457, 0.09460822492837906], 'magnitude': 2.101717710494995, 'distance': 12.568453788757324, 'directional_contribution': 1.4043143293516351}]}, 5705: {'frame': 5705, 'ionic_force': [-7.721536681056023, -8.126845806837082, -1.4946873784065247], 'ionic_force_magnitude': 11.309369648400695, 'motion_vector': [-0.3619537353515625, 0.5146217346191406, -0.38831329345703125], 'cosine_ionic_motion': -0.09651394143405095, 'ionic_motion_component': -1.091511839901778, 'ionic_force_x': -7.721536681056023, 'ionic_force_y': -8.126845806837082, 'ionic_force_z': -1.4946873784065247, 'radial_force': 11.210162866122825, 'axial_force': -1.4946873784065247, 'contributions': [{'ion': 1355, 'force': [-0.6187195181846619, -0.849595308303833, -1.482783317565918], 'magnitude': 1.8174906969070435, 'distance': 13.515525817871094, 'directional_contribution': 0.490314226479466}, {'ion': 1469, 'force': [-3.246384620666504, -0.28951355814933777, 0.4443724453449249], 'magnitude': 3.2894222736358643, 'distance': 10.046371459960938, 'directional_contribution': 1.1543915137098413}, {'ion': 1476, 'force': [-2.1111855506896973, -2.8807077407836914, -2.3419687747955322], 'magnitude': 4.270877838134766, 'distance': 8.816789627075195, 'directional_contribution': 0.2584637958280638}, {'ion': 2434, 'force': [-1.5408753156661987, -2.4781036376953125, 1.7578200101852417], 'magnitude': 3.406644344329834, 'distance': 9.872011184692383, 'directional_contribution': -1.89376061519296}, {'ion': 2443, 'force': [-0.20437167584896088, -1.6289255619049072, 0.1278722584247589], 'magnitude': 1.6466686725616455, 'distance': 14.199267387390137, 'directional_contribution': -1.1009207345678673}]}, 5706: {'frame': 5706, 'ionic_force': [-9.333332180976868, -9.798133179545403, -2.649417031556368], 'ionic_force_magnitude': 13.788905468225817, 'motion_vector': [0.46871185302734375, -0.7677764892578125, 0.569366455078125], 'cosine_ionic_motion': 0.11169603380458382, 'ionic_motion_component': 1.5401660513071616, 'ionic_force_x': -9.333332180976868, 'ionic_force_y': -9.798133179545403, 'ionic_force_z': -2.649417031556368, 'radial_force': 13.531980764269765, 'axial_force': -2.649417031556368, 'contributions': [{'ion': 1355, 'force': [-0.7529281377792358, -0.7786160707473755, -1.6140775680541992], 'magnitude': 1.9438081979751587, 'distance': 13.068999290466309, 'directional_contribution': -0.6332067072170027}, {'ion': 1469, 'force': [-3.3485147953033447, -0.18510238826274872, 0.3593425452709198], 'magnitude': 3.37282395362854, 'distance': 9.921382904052734, 'directional_contribution': -1.1485877339126427}, {'ion': 1476, 'force': [-2.198481321334839, -2.6305222511291504, -2.3725523948669434], 'magnitude': 4.1691694259643555, 'distance': 8.923686027526855, 'directional_contribution': -0.3397112611494819}, {'ion': 2434, 'force': [-2.7192623615264893, -3.5446817874908447, 0.9482372999191284], 'magnitude': 4.567090034484863, 'distance': 8.526077270507812, 'directional_contribution': 1.8663235327559207}, {'ion': 2443, 'force': [-0.314145565032959, -2.659210681915283, 0.029633086174726486], 'magnitude': 2.677866220474243, 'distance': 11.134599685668945, 'directional_contribution': 1.7953482110448467}]}, 5707: {'frame': 5707, 'ionic_force': [-9.118248001672328, -10.223654299974442, -2.7047302424907684], 'ionic_force_magnitude': 13.96356399885185, 'motion_vector': [-0.32656097412109375, 0.03221893310546875, -0.43898773193359375], 'cosine_ionic_motion': 0.5011819449497885, 'ionic_motion_component': 6.9982861633754165, 'ionic_force_x': -9.118248001672328, 'ionic_force_y': -10.223654299974442, 'ionic_force_z': -2.7047302424907684, 'radial_force': 13.699107776252703, 'axial_force': -2.7047302424907684, 'contributions': [{'ion': 1355, 'force': [-0.7430592179298401, -0.9873232841491699, -1.7624609470367432], 'magnitude': 2.1524899005889893, 'distance': 12.419339179992676, 'directional_contribution': 1.796351970501913}, {'ion': 1469, 'force': [-3.9833335876464844, -0.2822704613208771, 0.6409616470336914], 'magnitude': 4.044435024261475, 'distance': 9.060248374938965, 'directional_contribution': 1.843407514204464}, {'ion': 1476, 'force': [-2.176863431930542, -3.2478575706481934, -2.1858649253845215], 'magnitude': 4.479433059692383, 'distance': 8.609095573425293, 'directional_contribution': 2.856895963161545}, {'ion': 2434, 'force': [-2.212773084640503, -3.5199012756347656, 0.5018016695976257], 'magnitude': 4.187824726104736, 'distance': 8.903787612915039, 'directional_contribution': 0.7095934102755699}, {'ion': 2443, 'force': [-0.0022186795249581337, -2.1863017082214355, 0.10083231329917908], 'magnitude': 2.188626766204834, 'distance': 12.316383361816406, 'directional_contribution': -0.20796266539248132}]}, 5708: {'frame': 5708, 'ionic_force': [-7.562033966183662, -7.692690953612328, -1.67104172706604], 'ionic_force_magnitude': 10.915779049939598, 'motion_vector': [-1.0818023681640625, 2.732677459716797, -0.10074615478515625], 'cosine_ionic_motion': -0.3947808800753782, 'ionic_motion_component': -4.30934086004353, 'ionic_force_x': -7.562033966183662, 'ionic_force_y': -7.692690953612328, 'ionic_force_z': -1.67104172706604, 'radial_force': 10.787115082982305, 'axial_force': -1.67104172706604, 'contributions': [{'ion': 1355, 'force': [-0.5876579880714417, -0.8973038792610168, -1.4970914125442505], 'magnitude': 1.841678261756897, 'distance': 13.426480293273926, 'directional_contribution': -0.5663486421620689}, {'ion': 1469, 'force': [-3.555250406265259, -0.19343356788158417, 0.3396526575088501], 'magnitude': 3.5766725540161133, 'distance': 9.634506225585938, 'directional_contribution': 1.1164755088198905}, {'ion': 1476, 'force': [-1.8850804567337036, -2.6185390949249268, -2.144742488861084], 'magnitude': 3.8742992877960205, 'distance': 9.257046699523926, 'directional_contribution': -1.6663349729977135}, {'ion': 2434, 'force': [-1.4710770845413208, -2.029174327850342, 1.3063486814498901], 'magnitude': 2.82633376121521, 'distance': 10.838203430175781, 'directional_contribution': -1.3891976402875787}, {'ion': 2443, 'force': [-0.06296803057193756, -1.954240083694458, 0.3247908353805542], 'magnitude': 1.9820466041564941, 'distance': 12.942319869995117, 'directional_contribution': -1.8039350763789614}]}, 5709: {'frame': 5709, 'ionic_force': [-8.206216856837273, -7.025464236736298, -3.543524172157049], 'ionic_force_magnitude': 11.369067965394624, 'motion_vector': [1.6690330505371094, -2.759967803955078, 0.37714385986328125], 'cosine_ionic_motion': 0.118018876274731, 'ionic_motion_component': 1.3417646255669158, 'ionic_force_x': -8.206216856837273, 'ionic_force_y': -7.025464236736298, 'ionic_force_z': -3.543524172157049, 'radial_force': 10.802737747585143, 'axial_force': -3.543524172157049, 'contributions': [{'ion': 1355, 'force': [-0.8322591781616211, -0.49568411707878113, -1.5507534742355347], 'magnitude': 1.8284404277801514, 'distance': 13.474995613098145, 'directional_contribution': -0.18656799915738898}, {'ion': 1469, 'force': [-2.728053092956543, 0.3351321518421173, 0.03166264668107033], 'magnitude': 2.7487432956695557, 'distance': 10.990107536315918, 'directional_contribution': -1.6832834371799756}, {'ion': 1476, 'force': [-3.013021230697632, -1.691044807434082, -2.7624762058258057], 'magnitude': 4.423709392547607, 'distance': 8.663148880004883, 'directional_contribution': -0.4321832920748516}, {'ion': 2434, 'force': [-1.4870283603668213, -1.448777675628662, -0.17607536911964417], 'magnitude': 2.083557605743408, 'distance': 12.62310791015625, 'directional_contribution': 0.4466014159585072}, {'ion': 2443, 'force': [-0.14585499465465546, -3.7250897884368896, 0.914118230342865], 'magnitude': 3.8383824825286865, 'distance': 9.300256729125977, 'directional_contribution': 3.197197934532937}]}, 5710: {'frame': 5710, 'ionic_force': [-7.722934305667877, -6.871211111545563, -3.177142072468996], 'ionic_force_magnitude': 10.814411134118286, 'motion_vector': [-0.13116455078125, -0.18439483642578125, -0.395751953125], 'cosine_ionic_motion': 0.7175070979045479, 'ionic_motion_component': 7.759416748387842, 'ionic_force_x': -7.722934305667877, 'ionic_force_y': -6.871211111545563, 'ionic_force_z': -3.177142072468996, 'radial_force': 10.337178359160152, 'axial_force': -3.177142072468996, 'contributions': [{'ion': 1355, 'force': [-0.5726248025894165, -0.8952419757843018, -1.581054925918579], 'magnitude': 1.905017614364624, 'distance': 13.201386451721191, 'directional_contribution': 1.899391292036519}, {'ion': 1469, 'force': [-3.873427629470825, -0.260297954082489, 0.588064432144165], 'magnitude': 3.9264509677886963, 'distance': 9.195364952087402, 'directional_contribution': 0.7092380456100464}, {'ion': 1476, 'force': [-2.0810577869415283, -3</t>
+          <t>{5689: {'frame': 5689, 'ionic_force': [-10.846781343221664, 1.6348312199115753, -4.6059174835681915], 'ionic_force_magnitude': 11.897050663534147, 'motion_vector': [1.6955833435058594, -2.072643280029297, 4.204833984375], 'cosine_ionic_motion': -0.6937842477004733, 'ionic_motion_component': -8.253986344454455, 'ionic_force_x': -10.846781343221664, 'ionic_force_y': 1.6348312199115753, 'ionic_force_z': -4.6059174835681915, 'radial_force': 10.969290707482374, 'axial_force': -4.6059174835681915, 'contributions': [{'ion': 1355, 'force': [-0.2695693075656891, 0.3014860451221466, -1.9719277620315552], 'magnitude': 2.0129730701446533, 'distance': 12.842514038085938, 'cosine_with_motion': -0.9340956117594803, 'motion_component': -1.88030930318196}, {'ion': 1469, 'force': [-2.6125478744506836, 2.329728126525879, -0.3506489098072052], 'magnitude': 3.5179531574249268, 'distance': 9.714579582214355, 'cosine_with_motion': -0.6119997277317742, 'motion_component': -2.1529863553754645}, {'ion': 1476, 'force': [-1.3893324136734009, 1.863111972808838, -5.913637638092041], 'magnitude': 6.353939056396484, 'distance': 7.228488922119141, 'cosine_with_motion': -0.9813094185006677, 'motion_component': -6.235180191289949}, {'ion': 2434, 'force': [-0.631294310092926, -5.49688720703125, -1.0274757146835327], 'magnitude': 5.62761116027832, 'distance': 7.680809497833252, 'cosine_with_motion': 0.2139528837455448, 'motion_component': 1.2040436448136056}, {'ion': 2443, 'force': [-5.944037437438965, 2.637392282485962, 4.657772541046143], 'magnitude': 7.998891353607178, 'distance': 6.442495822906494, 'cosine_with_motion': 0.10131979104044181, 'motion_component': 0.8104460085251759}]}, 5690: {'frame': 5690, 'ionic_force': [-3.750170722603798, 1.514174997806549, -21.49210250377655], 'ionic_force_magnitude': 21.869315865053835, 'motion_vector': [-0.13861846923828125, -0.5360183715820312, -0.34649658203125], 'cosine_ionic_motion': 0.5009314964763403, 'ionic_motion_component': 10.955029123195187, 'ionic_force_x': -3.750170722603798, 'ionic_force_y': 1.514174997806549, 'ionic_force_z': -21.49210250377655, 'radial_force': 4.04431778828731, 'axial_force': -21.49210250377655, 'contributions': [{'ion': 1355, 'force': [0.17119938135147095, -0.25686579942703247, -4.116479396820068], 'magnitude': 4.128037452697754, 'distance': 8.968033790588379, 'cosine_with_motion': 0.5712890206481612, 'motion_component': 2.3583023822572544}, {'ion': 1469, 'force': [-3.6085445880889893, 4.346920967102051, 2.5242862701416016], 'magnitude': 6.187838077545166, 'distance': 7.324864387512207, 'cosine_with_motion': -0.669172996362154, 'motion_component': -4.140733987203493}, {'ion': 1476, 'force': [0.4883006513118744, 1.3090105056762695, -24.288963317871094], 'magnitude': 24.329113006591797, 'distance': 3.6940767765045166, 'cosine_with_motion': 0.48121839469197714, 'motion_component': 11.707616165324877}, {'ion': 2434, 'force': [-0.0496017187833786, -3.2350029945373535, 1.141748309135437], 'magnitude': 3.430931806564331, 'distance': 9.837007522583008, 'cosine_with_motion': 0.6003389231792499, 'motion_component': 2.0597219802080753}, {'ion': 2443, 'force': [-0.7515244483947754, -0.6498876810073853, 3.2473056316375732], 'magnitude': 3.395899772644043, 'distance': 9.887616157531738, 'cosine_with_motion': -0.3032709211137449, 'motion_component': -1.029877723230527}]}, 5691: {'frame': 5691, 'ionic_force': [-3.733049623668194, -2.4102413058280945, -3.200647473335266], 'ionic_force_magnitude': 5.476227432608747, 'motion_vector': [-1.1974220275878906, -3.1602745056152344, -3.7289962768554688], 'cosine_ionic_motion': 0.8716542732504011, 'ionic_motion_component': 4.773377042924487, 'ionic_force_x': -3.733049623668194, 'ionic_force_y': -2.4102413058280945, 'ionic_force_z': -3.200647473335266, 'radial_force': 4.443525924880957, 'axial_force': -3.200647473335266, 'contributions': [{'ion': 1355, 'force': [0.06907344609498978, -0.44401097297668457, -3.827573776245117], 'magnitude': 3.8538601398468018, 'distance': 9.281561851501465, 'cosine_with_motion': 0.8040060986052859, 'motion_component': 3.0985270472823183}, {'ion': 1469, 'force': [-4.9462971687316895, 4.178884029388428, 2.458789587020874], 'magnitude': 6.926368236541748, 'distance': 6.923349380493164, 'cosine_with_motion': -0.4719939195667975, 'motion_component': -3.2692035798063515}, {'ion': 1476, 'force': [-0.3097705841064453, -0.9671092629432678, -10.523290634155273], 'magnitude': 10.572175979614258, 'distance': 5.603854179382324, 'cosine_with_motion': 0.801965195618033, 'motion_component': 8.478517138465996}, {'ion': 2434, 'force': [0.13542890548706055, -3.8748512268066406, 1.5841094255447388], 'magnitude': 4.188342571258545, 'distance': 8.903237342834473, 'cosine_with_motion': 0.2930200343826377, 'motion_component': 1.227268361060787}, {'ion': 2443, 'force': [1.3185157775878906, -1.3031538724899292, 7.107317924499512], 'magnitude': 7.34511137008667, 'distance': 6.723104000091553, 'cosine_with_motion': -0.648285858839064, 'motion_component': -4.76173187307522}]}, 5692: {'frame': 5692, 'ionic_force': [-2.2680077254772186, -15.304942309856415, -10.105775147676468], 'ionic_force_magnitude': 18.48003813541121, 'motion_vector': [5.063621520996094, 4.651702880859375, -0.6800384521484375], 'cosine_ionic_motion': -0.5936836240157243, 'ionic_motion_component': -10.971296012179716, 'ionic_force_x': -2.2680077254772186, 'ionic_force_y': -15.304942309856415, 'ionic_force_z': -10.105775147676468, 'radial_force': 15.472075431268339, 'axial_force': -10.105775147676468, 'contributions': [{'ion': 1355, 'force': [-0.16544833779335022, -0.5105010867118835, -1.7802817821502686], 'magnitude': 1.859405279159546, 'distance': 13.362324714660645, 'cosine_with_motion': -0.1558124509191535, 'motion_component': -0.2897184830593833}, {'ion': 1469, 'force': [-8.14029312133789, 1.124986171722412, -1.0288584232330322], 'magnitude': 8.281818389892578, 'distance': 6.331493854522705, 'cosine_with_motion': -0.6166491039821831, 'motion_component': -5.106975882015757}, {'ion': 1476, 'force': [-0.7527567744255066, -2.250356912612915, -4.554305553436279], 'magnitude': 5.135411262512207, 'distance': 8.040470123291016, 'cosine_with_motion': -0.3151520722030431, 'motion_component': -1.618435477507159}, {'ion': 2434, 'force': [-0.9204217195510864, -2.4938366413116455, -0.17049100995063782], 'magnitude': 2.663731336593628, 'distance': 11.164103507995605, 'cosine_with_motion': -0.8772231185167029, 'motion_component': -2.336686691254273}, {'ion': 2443, 'force': [7.710912227630615, -11.175233840942383, -2.57183837890625], 'magnitude': 13.818768501281738, 'distance': 4.901560306549072, 'cosine_with_motion': -0.11719417252773648, 'motion_component': -1.6194791760610485}]}, 5693: {'frame': 5693, 'ionic_force': [14.037217020988464, 0.7251570634543896, -12.502707362174988], 'ionic_force_magnitude': 18.811884696786514, 'motion_vector': [0.5311241149902344, 0.9281234741210938, 2.3688735961914062], 'cosine_ionic_motion': -0.43950603727257137, 'ionic_motion_component': -8.267936896713168, 'ionic_force_x': 14.037217020988464, 'ionic_force_y': 0.7251570634543896, 'ionic_force_z': -12.502707362174988, 'radial_force': 14.055935204069705, 'axial_force': -12.502707362174988, 'contributions': [{'ion': 1355, 'force': [0.4393165409564972, 0.04694287106394768, -1.5332221984863281], 'magnitude': 1.595610499382019, 'distance': 14.424660682678223, 'cosine_with_motion': -0.8090304904701983, 'motion_component': -1.2908975703916323}, {'ion': 1469, 'force': [-0.2973380386829376, 6.702067852020264, -1.863255262374878], 'magnitude': 6.9626030921936035, 'distance': 6.90531063079834, 'cosine_with_motion': 0.09110255835193735, 'motion_component': 0.63431096597406}, {'ion': 1476, 'force': [1.3921409845352173, 0.3217581510543823, -3.227895498275757], 'magnitude': 3.529999256134033, 'distance': 9.697990417480469, 'cosine_with_motion': -0.7202940567532118, 'motion_component': -2.5426374261861078}, {'ion': 2434, 'force': [2.518434524536133, -7.808837413787842, -1.8178147077560425], 'magnitude': 8.403862953186035, 'distance': 6.285351276397705, 'cosine_with_motion': -0.4677274978934718, 'motion_component': -3.930717568695087}, {'ion': 2443, 'force': [9.984663009643555, 1.4632256031036377, -4.060519695281982], 'magnitude': 10.877607345581055, 'distance': 5.524619102478027, 'cosine_with_motion': -0.10461816669192547, 'motion_component': -1.1379953539395444}]}, 5694: {'frame': 5694, 'ionic_force': [15.186673760414124, -2.523807108402252, -6.381444334983826], 'ionic_force_magnitude': 16.66515808584394, 'motion_vector': [-6.16156005859375, -6.210399627685547, -0.5569686889648438], 'cosine_ionic_motion': -0.5089087171859848, 'ionic_motion_component': -8.481044223168483, 'ionic_force_x': 15.186673760414124, 'ionic_force_y': -2.523807108402252, 'ionic_force_z': -6.381444334983826, 'radial_force': 15.39495573964643, 'axial_force': -6.381444334983826, 'contributions': [{'ion': 1355, 'force': [0.7672042846679688, 0.321216881275177, -2.13971209526062], 'magnitude': 2.2956807613372803, 'distance': 12.02578067779541, 'cosine_with_motion': -0.2748099851973862, 'motion_component': -0.6308760194952647}, {'ion': 1469, 'force': [0.36691606044769287, 5.6577959060668945, 0.787419319152832], 'magnitude': 5.724099159240723, 'distance': 7.6157989501953125, 'cosine_with_motion': -0.7540475151744416, 'motion_component': -4.316242741675154}, {'ion': 1476, 'force': [4.058429718017578, 1.9305769205093384, -4.828175067901611], 'magnitude': 6.596154689788818, 'distance': 7.09453010559082, 'cosine_with_motion': -0.5933128190732816, 'motion_component': -3.9135829908792417}, {'ion': 2434, 'force': [3.7240912914276123, -11.90422248840332, -1.445675253868103], 'magnitude': 12.556645393371582, 'distance': 5.142002105712891, 'cosine_with_motion': 0.470498550170999, 'motion_component': 5.9078834976516035}, {'ion': 2443, 'force': [6.2700324058532715, 1.4708256721496582, 1.2446987628936768], 'magnitude': 6.559413909912109, 'distance': 7.114371299743652, 'cosine_with_motion': -0.8427926757632486, 'motion_component': -5.528225916871648}]}, 5695: {'frame': 5695, 'ionic_force': [-17.885726302862167, -13.695586919784546, -6.164025843143463], 'ionic_force_magnitude': 23.35516048014249, 'motion_vector': [2.018024444580078, -2.0229759216308594, -1.58453369140625], 'cosine_ionic_motion': 0.01807265163752099, 'ionic_motion_component': 0.4220896792960127, 'ionic_force_x': -17.885726302862167, 'ionic_force_y': -13.695586919784546, 'ionic_force_z': -6.164025843143463, 'radial_force': 22.527057208127943, 'axial_force': -6.164025843143463, 'contributions': [{'ion': 1355, 'force': [-0.28277072310447693, -0.719104528427124, -1.999786376953125], 'magnitude': 2.143878698348999, 'distance': 12.444255828857422, 'cosine_with_motion': 0.5785769589171919, 'motion_component': 1.240398856016542}, {'ion': 1469, 'force': [-9.842928886413574, 4.126557350158691, -0.23699882626533508], 'magnitude': 10.67557430267334, 'distance': 5.576650142669678, 'cosine_with_motion': -0.7980207558039879, 'motion_component': -8.519330112078663}, {'ion': 1476, 'force': [-1.4224494695663452, -3.3690109252929688, -5.0304341316223145], 'magnitude': 6.219233512878418, 'distance': 7.306352615356445, 'cosine_with_motion': 0.5863940567574065, 'motion_component': 3.646921530555055}, {'ion': 2434, 'force': [-1.0529464483261108, -2.425291061401367, -0.3027394115924835], 'magnitude': 2.6612749099731445, 'distance': 11.169254302978516, 'cosine_with_motion': 0.37504453080532796, 'motion_component': 0.9980965971669695}, {'ion': 2443, 'force': [-5.28463077545166, -11.308737754821777, 1.405932903289795], 'magnitude': 12.561509132385254, 'distance': 5.141005992889404, 'cosine_with_motion': 0.24328309559108077, 'motion_component': 3.0560029014484797}]}, 5696: {'frame': 5696, 'ionic_force': [-15.213935688138008, -14.176376223564148, -12.65572875738144], 'ionic_force_magnitude': 24.3433964831378, 'motion_vector': [-0.21909713745117188, -0.3765602111816406, 0.164337158203125], 'cosine_ionic_motion': 0.5815461614722945, 'ionic_motion_component': 14.15680878196694, 'ionic_force_x': -15.213935688138008, 'ionic_force_y': -14.176376223564148, 'ionic_force_z': -12.65572875738144, 'radial_force': 20.79503503134424, 'axial_force': -12.65572875738144, 'contributions': [{'ion': 1355, 'force': [0.09340129792690277, -0.6584328413009644, -1.331163763999939], 'magnitude': 1.4880372285842896, 'distance': 14.936958312988281, 'cosine_with_motion': 0.012579553778028203, 'motion_component': 0.01871884341876351}, {'ion': 1469, 'force': [-16.17984390258789, -5.707157611846924, -8.072161674499512], 'magnitude': 18.960981369018555, 'distance': 4.184452533721924, 'cosine_with_motion': 0.49469054526340944, 'motion_component': 9.379817903545728}, {'ion': 1476, 'force': [0.16498154401779175, -2.0770199298858643, -2.584268808364868], 'magnitude': 3.319589853286743, 'distance': 10.000617980957031, 'cosine_with_motion': 0.20785866103990283, 'motion_component': 0.6900054763974506}, {'ion': 2434, 'force': [-0.31412482261657715, -3.6910321712493896, -0.3123330771923065], 'magnitude': 3.7175185680389404, 'distance': 9.450231552124023, 'cosine_with_motion': 0.813063294942147, 'motion_component': 3.0225779550752616}, {'ion': 2443, 'force': [1.0216501951217651, -2.042733669281006, -0.35580143332481384], 'magnitude': 2.3115200996398926, 'distance': 11.98450756072998, 'cosine_with_motion': 0.45238145992863704, 'motion_component': 1.045688783874306}]}, 5697: {'frame': 5697, 'ionic_force': [-14.388794315978885, -13.769953429698944, -10.123002961277962], 'ionic_force_magnitude': 22.341087893781413, 'motion_vector': [-1.5983009338378906, 3.4348678588867188, 0.1610565185546875], 'cosine_ionic_motion': -0.30608964031464103, 'ionic_motion_component': -6.838375557645334, 'ionic_force_x': -14.388794315978885, 'ionic_force_y': -13.769953429698944, 'ionic_force_z': -10.123002961277962, 'radial_force': 19.916049290048065, 'axial_force': -10.123002961277962, 'contributions': [{'ion': 1355, 'force': [0.01840483583509922, -0.6926707625389099, -1.3557699918746948], 'magnitude': 1.5225780010223389, 'distance': 14.766557693481445, 'cosine_with_motion': -0.45500860962911804, 'motion_component': -0.692786103021971}, {'ion': 1469, 'force': [-15.130455017089844, -6.483215808868408, -6.229846477508545], 'magnitude': 17.60038948059082, 'distance': 4.3431806564331055, 'cosine_with_motion': 0.013645146477585305, 'motion_component': 0.24015990551625777}, {'ion': 1476, 'force': [0.08019865304231644, -2.2278919219970703, -2.5778114795684814], 'magnitude': 3.408085346221924, 'distance': 9.86992359161377, 'cosine_with_motion': -0.6341951047869588, 'motion_component': -2.1613910932444793}, {'ion': 2434, 'force': [-0.08338899910449982, -2.282119035720825, 0.2655191719532013], 'magnitude': 2.2990262508392334, 'distance': 12.017027854919434, 'cosine_with_motion': -0.8789782128093423, 'motion_component': -2.0207939367997354}, {'ion': 2443, 'force': [0.7264462113380432, -2.0840559005737305, -0.22509418427944183], 'magnitude': 2.2184860706329346, 'distance': 12.233217239379883, 'cosine_with_motion': -0.9932740707349745, 'motion_component': -2.2035646993996467}]}, 5698: {'frame': 5698, 'ionic_force': [-9.738676965236664, -11.330120891332626, -6.976988285779953], 'ionic_force_magnitude': 16.48914291239402, 'motion_vector': [-2.993671417236328, -2.5537109375, 1.6241912841796875], 'cosine_ionic_motion': 0.6661082666101348, 'ionic_motion_component': 10.98355440326157, 'ionic_force_x': -9.738676965236664, 'ionic_force_y': -11.330120891332626, 'ionic_force_z': -6.976988285779953, 'radial_force': 14.940330265608027, 'axial_force': -6.976988285779953, 'contributions': [{'ion': 1355, 'force': [-0.1521759033203125, -0.4667292535305023, -1.7436898946762085], 'magnitude': 1.8114768266677856, 'distance': 13.537941932678223, 'cosine_with_motion': -0.15362174844894844, 'motion_component': -0.2782822313194284}, {'ion': 1469, 'force': [-6.2060546875, 1.8714954853057861, -0.3370665907859802], 'magnitude': 6.490856647491455, 'distance': 7.151844024658203, 'cosine_with_motion': 0.4796095587467847, 'motion_component': 3.1130770405235584}, {'ion': 1476, 'force': [-0.9171950221061707, -2.0580520629882812, -4.527716159820557], 'magnitude': 5.057374477386475, 'distance': 8.102265357971191, 'cosine_with_motion': 0.030079234334032482, 'motion_component': 0.15212195803306727}, {'ion': 2434, 'force': [-3.975003957748413, -6.597219944000244, 0.32685384154319763], 'magnitude': 7.709137439727783, 'distance': 6.5624518394470215, 'cosine_with_motion': 0.8921549445409725, 'motion_component': 6.877745132606193}, {'ion': 2443, 'force': [1.5117526054382324, -4.079615116119385, -0.6953694820404053], 'magnitude': 4.4059271812438965, 'distance': 8.680612564086914, 'cosine_with_motion': 0.25395165049253243, 'motion_component': 1.1188924746078683}]}, 5699: {'frame': 5699, 'ionic_force': [-7.502817556262016, -9.551654130220413, -3.1742424368858337], 'ionic_force_magnitude': 12.553970804253016, 'motion_vector': [-0.2769050598144531, -0.16832733154296875, 0.20163726806640625], 'cosine_ionic_motion': 0.635580549251634, 'ionic_motion_component': 7.979059659056109, 'ionic_force_x': -7.502817556262016, 'ionic_force_y': -9.551654130220413, 'ionic_force_z': -3.1742424368858337, 'radial_force': 12.14604330248786, 'axial_force': -3.1742424368858337, 'contributions': [{'ion': 1355, 'force': [-0.6258348226547241, -0.9120814800262451, -1.6169955730438232], 'magnitude': 1.959141731262207, 'distance': 13.017755508422852, 'cosine_with_motion': 0.001041146067423937, 'motion_component': 0.0020397527652349368}, {'ion': 1469, 'force': [-3.346435785293579, -0.3936164677143097, 0.2601182758808136], 'magnitude': 3.379530668258667, 'distance': 9.91153335571289, 'cosine_with_motion': 0.8104449305357946, 'motion_component': 2.7389235418649394}, {'ion': 1476, 'force': [-2.058412790298462, -2.6242835521698, -2.340930461883545], 'magnitude': 4.074786186218262, 'distance': 9.026442527770996, 'cosine_with_motion': 0.3470317338278969, 'motion_component': 1.414080129720439}, {'ion': 2434, 'force': [-1.4498467445373535, -2.6175620555877686, 0.3526051938533783], 'magnitude': 3.012974739074707, 'distance': 10.497147560119629, 'cosine_with_motion': 0.7941024342820463, 'motion_component': 2.3926106197890356}, {'ion': 2443, 'force': [-0.022287413477897644, -3.00411057472229, 0.17096012830734253], 'magnitude': 3.0090537071228027, 'distance': 10.503984451293945, 'cosine_with_motion': 0.47569963817289296, 'motion_component': 1.4314057776705322}]}, 5700: {'frame': 5700, 'ionic_force': [-7.085268452763557, -8.294093906879425, -2.452709883451462], 'ionic_force_magnitude': 11.180733811170061, 'motion_vector': [0.4935493469238281, -0.46282196044921875, 0.6883697509765625], 'cosine_ionic_motion': -0.12478037358923734, 'ionic_motion_component': -1.3951361419596175, 'ionic_force_x': -7.085268452763557, 'ionic_force_y': -8.294093906879425, 'ionic_force_z': -2.452709883451462, 'radial_force': 10.908392309770532, 'axial_force': -2.452709883451462, 'contributions': [{'ion': 1355, 'force': [-0.5744865536689758, -0.7606053352355957, -1.4772404432296753], 'magnitude': 1.7580655813217163, 'distance': 13.742049217224121, 'cosine_with_motion': -0.5588955682721238, 'motion_component': -0.9825750645518134}, {'ion': 1469, 'force': [-3.6154754161834717, -0.5478944182395935, 0.3197089731693268], 'magnitude': 3.670703649520874, 'distance': 9.510303497314453, 'cosine_with_motion': -0.3699541929998266, 'motion_component': -1.3579921723084798}, {'ion': 1476, 'force': [-1.7856495380401611, -2.236912727355957, -2.2723193168640137], 'magnitude': 3.654552936553955, 'distance': 9.531294822692871, 'cosine_with_motion': -0.3997822563788361, 'motion_component': -1.4610254591911342}, {'ion': 2434, 'force': [-0.9666056632995605, -1.7378770112991333, 0.8489934206008911], 'magnitude': 2.1622519493103027, 'distance': 12.39127254486084, 'cosine_with_motion': 0.4368284570045849, 'motion_component': 0.9445331170802014}, {'ion': 2443, 'force': [-0.14305128157138824, -3.0108044147491455, 0.12814748287200928], 'magnitude': 3.016923666000366, 'distance': 10.490275382995605, 'cosine_with_motion': 0.48457418995848245, 'motion_component': 1.4619233628143808}]}, 5701: {'frame': 5701, 'ionic_force': [-7.92530158162117, -8.08792930841446, -1.2593768686056137], 'ionic_force_magnitude': 11.393464607165614, 'motion_vector': [0.5581855773925781, 0.4502677917480469, 0.15650177001953125], 'cosine_ionic_motion': -0.9879751759881211, 'ionic_motion_component': -11.256460200378877, 'ionic_force_x': -7.92530158162117, 'ionic_force_y': -8.08792930841446, 'ionic_force_z': -1.2593768686056137, 'radial_force': 11.323648071957933, 'axial_force': -1.2593768686056137, 'contributions': [{'ion': 1355, 'force': [-0.6315168142318726, -1.0191653966903687, -1.574242353439331], 'magnitude': 1.978825569152832, 'distance': 12.952848434448242, 'cosine_with_motion': -0.7282307151891029, 'motion_component': -1.441041549650734}, {'ion': 1469, 'force': [-3.8441007137298584, -0.7395055890083313, 0.717881441116333], 'magnitude': 3.979865789413452, 'distance': 9.13344955444336, 'cosine_with_motion': -0.8100171774076058, 'motion_component': -3.223759742268882}, {'ion': 1476, 'force': [-1.9888440370559692, -2.9822001457214355, -2.092775821685791], 'magnitude': 4.150750637054443, 'distance': 8.943463325500488, 'cosine_with_motion': -0.9125854852277061, 'motion_component': -3.787914575494952}, {'ion': 2434, 'force': [-1.2842319011688232, -1.5509859323501587, 1.57150137424469], 'magnitude': 2.554295539855957, 'distance': 11.400751113891602, 'cosine_with_motion': -0.623623740374531, 'motion_component': -1.592919314496072}, {'ion': 2443, 'force': [-0.1766081154346466, -1.796072244644165, 0.11825849115848541], 'magnitude': 1.8086047172546387, 'distance': 13.548686981201172, 'cosine_with_motion': -0.6694801324993472, 'motion_component': -1.2108249223917582}]}, 5702: {'frame': 5702, 'ionic_force': [-7.804108589887619, -8.228433191776276, -0.8812482059001923], 'ionic_force_magnitude': 11.37487679382443, 'motion_vector': [-0.39960479736328125, -0.060466766357421875, -0.1700592041015625], 'cosine_ionic_motion': 0.755066697342409, 'ionic_motion_component': 8.588790653389824, 'ionic_force_x': -7.804108589887619, 'ionic_force_y': -8.228433191776276, 'ionic_force_z': -0.8812482059001923, 'radial_force': 11.340688853605112, 'axial_force': -0.8812482059001923, 'contributions': [{'ion': 1355, 'force': [-0.5931767225265503, -0.9305346608161926, -1.5677777528762817], 'magnitude': 1.9172064065933228, 'distance': 13.159355163574219, 'cosine_with_motion': 0.6660555764511565, 'motion_component': 1.276966028057073}, {'ion': 1469, 'force': [-4.320357799530029, -0.4477121829986572, 0.8675047755241394], 'magnitude': 4.4292778968811035, 'distance': 8.65770149230957, 'cosine_with_motion': 0.8269179285556999, 'motion_component': 3.662649262649394}, {'ion': 1476, 'force': [-1.978808045387268, -2.9532740116119385, -2.4418883323669434], 'magnitude': 4.312809467315674, 'distance': 8.773823738098145, 'cosine_with_motion': 0.7321725204097072, 'motion_component': 3.1577207300576404}, {'ion': 2434, 'force': [-0.7739160060882568, -1.956164002418518, 2.087541341781616], 'magnitude': 2.963671922683716, 'distance': 10.584100723266602, 'cosine_with_motion': 0.05581996945277117, 'motion_component': 0.16543208727818737}, {'ion': 2443, 'force': [-0.13785001635551453, -1.9407483339309692, 0.17337176203727722], 'magnitude': 1.9533469676971436, 'distance': 13.037050247192383, 'cosine_with_motion': 0.16690467565863135, 'motion_component': 0.3260227469765544}]}, 5703: {'frame': 5703, 'ionic_force': [-7.383249953389168, -8.355258643627167, -1.0149785578250885], 'ionic_force_magnitude': 11.196111304777759, 'motion_vector': [-0.3843231201171875, 0.9410591125488281, -0.6316909790039062], 'cosine_ionic_motion': -0.32718268002181145, 'ionic_motion_component': -3.6631737025196873, 'ionic_force_x': -7.383249953389168, 'ionic_force_y': -8.355258643627167, 'ionic_force_z': -1.0149785578250885, 'radial_force': 11.15001017381274, 'axial_force': -1.0149785578250885, 'contributions': [{'ion': 1355, 'force': [-0.60088050365448, -0.9079782366752625, -1.5684553384780884], 'magnitude': 1.9093282222747803, 'distance': 13.18647575378418, 'cosine_with_motion': 0.16071629272356294, 'motion_component': 0.30686014280205853}, {'ion': 1469, 'force': [-3.552804470062256, -0.41763007640838623, 0.6142292618751526], 'magnitude': 3.6296157836914062, 'distance': 9.563981056213379, 'cosine_with_motion': 0.13453440074523831, 'motion_component': 0.48830820908270667}, {'ion': 1476, 'force': [-2.070937156677246, -2.9030516147613525, -2.323512554168701], 'magnitude': 4.256195545196533, 'distance': 8.83198356628418, 'cosine_with_motion': -0.09193349991236771, 'motion_component': -0.39128694689864574}, {'ion': 2434, 'force': [-1.004224419593811, -1.850171685218811, 2.136342763900757], 'magnitude': 2.999260425567627, 'distance': 10.521120071411133, 'cosine_with_motion': -0.7534954304754614, 'motion_component': -2.2599289317871296}, {'ion': 2443, 'force': [-0.15440340340137482, -2.2764270305633545, 0.12641730904579163], 'magnitude': 2.285156726837158, 'distance': 12.05344009399414, 'cosine_with_motion': -0.7908105052909971, 'motion_component': -1.8071260334216284}]}, 5704: {'frame': 5704, 'ionic_force': [-9.369131922721863, -6.612637624144554, -1.1421239897608757], 'ionic_force_magnitude': 11.524411331673532, 'motion_vector': [0.2603874206542969, -0.4796562194824219, 0.38088226318359375], 'cosine_ionic_motion': 0.03874520782907011, 'ionic_motion_component': 0.4465157121533816, 'ionic_force_x': -9.369131922721863, 'ionic_force_y': -6.612637624144554, 'ionic_force_z': -1.1421239897608757, 'radial_force': 11.467676719092582, 'axial_force': -1.1421239897608757, 'contributions': [{'ion': 1355, 'force': [-0.6172433495521545, -0.7568070888519287, -1.5594958066940308], 'magnitude': 1.8400471210479736, 'distance': 13.432429313659668, 'cosine_with_motion': -0.3198527868126092, 'motion_component': -0.5885442069841993}, {'ion': 1469, 'force': [-3.870227813720703, 0.14175964891910553, 0.3387364447116852], 'magnitude': 3.887608766555786, 'distance': 9.24118709564209, 'cosine_with_motion': -0.36590838633313716, 'motion_component': -1.4225086309504258}, {'ion': 1476, 'force': [-2.3841171264648438, -2.5097689628601074, -2.422724962234497], 'magnitude': 4.2252278327941895, 'distance': 8.864290237426758, 'cosine_with_motion': -0.12081579075749667, 'motion_component': -0.5104742520899492}, {'ion': 2434, 'force': [-2.1380257606506348, -1.4192434549331665, 2.406752109527588], 'magnitude': 3.518218517303467, 'distance': 9.714213371276855, 'cosine_with_motion': 0.444465918681543, 'motion_component': 1.5637282455528023}, {'ion': 2443, 'force': [-0.3595178723335266, -2.068577766418457, 0.09460822492837906], 'magnitude': 2.101717710494995, 'distance': 12.568453788757324, 'cosine_with_motion': 0.6681745362650324, 'motion_component': 1.4043143293516351}]}, 5705: {'frame': 5705, 'ionic_force': [-7.721536681056023, -8.126845806837082, -1.4946873784065247], 'ionic_force_magnitude': 11.309369648400695, 'motion_vector': [-0.3619537353515625, 0.5146217346191406, -0.38831329345703125], 'cosine_ionic_motion': -0.09651394143405095, 'ionic_motion_component': -1.091511839901778, 'ionic_force_x': -7.721536681056023, 'ionic_force_y': -8.126845806837082, 'ionic_force_z': -1.4946873784065247, 'radial_force': 11.210162866122825, 'axial_force': -1.4946873784065247, 'contributions': [{'ion': 1355, 'force': [-0.6187195181846619, -0.849595308303833, -1.482783317565918], 'magnitude': 1.8174906969070435, 'distance': 13.515525817871094, 'cosine_with_motion': 0.2697753721747423, 'motion_component': 0.49031422647946593}, {'ion': 1469, 'force': [-3.246384620666504, -0.28951355814933777, 0.4443724453449249], 'magnitude': 3.2894222736358643, 'distance': 10.046371459960938, 'cosine_with_motion': 0.35094051822464967, 'motion_component': 1.1543915137098413}, {'ion': 1476, 'force': [-2.1111855506896973, -2.8807077407836914, -2.3419687747955322], 'magnitude': 4.270877838134766, 'distance': 8.816789627075195, 'cosine_with_motion': 0.06051771865582957, 'motion_component': 0.2584637958280638}, {'ion': 2434, 'force': [-1.5408753156661987, -2.4781036376953125, 1.7578200101852417], 'magnitude': 3.406644344329834, 'distance': 9.872011184692383, 'cosine_with_motion': -0.5559020648508023, 'motion_component': -1.8937606151929602}, {'ion': 2443, 'force': [-0.20437167584896088, -1.6289255619049072, 0.1278722584247589], 'magnitude': 1.6466686725616455, 'distance': 14.199267387390137, 'cosine_with_motion': -0.6685745470466063, 'motion_component': -1.1009207345678673}]}, 5706: {'frame': 5706, 'ionic_force': [-9.333332180976868, -9.798133179545403, -2.649417031556368], 'ionic_force_magnitude': 13.788905468225817, 'motion_vector': [0.46871185302734375, -0.7677764892578125, 0.569366455078125], 'cosine_ionic_motion': 0.11169603380458382, 'ionic_motion_component': 1.5401660513071616, 'ionic_force_x': -9.333332180976868, 'ionic_force_y': -9.798133179545403, 'ionic_force_z': -2.649417031556368, 'radial_force': 13.531980764269765, 'axial_force': -2.649417031556368, 'contributions': [{'ion': 1355, 'force': [-0.7529281377792358, -0.7786160707473755, -1.6140775680541992], 'magnitude': 1.9438081979751587, 'distance': 13.068999290466309, 'cosine_with_motion': -0.32575576145976437, 'motion_component': -0.6332067072170027}, {'ion': 1469, 'force': [-3.3485147953033447, -0.18510238826274872, 0.3593425452709198], 'magnitude': 3.37282395362854, 'distance': 9.921382904052734, 'cosine_with_motion': -0.340541859346188, 'motion_component': -1.1485877339126427}, {'ion': 1476, 'force': [-2.198481321334839, -2.6305222511291504, -2.3725523948669434], 'magnitude': 4.1691694259643555, 'distance': 8.923686027526855, 'cosine_with_motion': -0.08148176294653371, 'motion_component': -0.3397112611494819}, {'ion': 2434, 'force': [-2.7192623615264893, -3.5446817874908447, 0.9482372999191284], 'magnitude': 4.567090034484863, 'distance': 8.526077270507812, 'cosine_with_motion': 0.408646106673994, 'motion_component': 1.8663235327559207}, {'ion': 2443, 'force': [-0.314145565032959, -2.659210681915283, 0.029633086174726486], 'magnitude': 2.677866220474243, 'distance': 11.134599685668945, 'cosine_with_motion': 0.6704398667945487, 'motion_component': 1.7953482110448467}]}, 5707: {'frame': 5707, 'ionic_force': [-9.118248001672328, -10.223654299974442, -2.7047302424907684], 'ionic_force_magnitude': 13.96356399885185, 'motion_vector': [-0.32656097412109375, 0.03221893310546875, -0.43898773193359375], 'cosine_ionic_motion': 0.5011819449497885, 'ionic_motion_component': 6.9982861633754165, 'ionic_force_x': -9.118248001672328, 'ionic_force_y': -10.223654299974442, 'ionic_force_z': -2.7047302424907684, 'radial_force': 13.699107776252703, 'axial_force': -2.7047302424907684, 'contributions': [{'ion': 1355, 'force': [-0.7430592179298401, -0.9873232841491699, -1.7624609470367432], 'magnitude': 2.1524899005889893, 'distance': 12.419339179992676, 'cosine_with_motion': 0.8345460544314233, 'motion_component': 1.796351970501913}, {'ion': 1469, 'force': [-3.9833335876464844, -0.2822704613208771, 0.6409616470336914], 'magnitude': 4.044435024261475, 'distance': 9.060248374938965, 'cosine_with_motion': 0.4557886302996786, 'motion_component': 1.843407514204464}, {'ion': 1476, 'force': [-2.176863431930542, -3.2478575706481934, -2.1858649253845215], 'magnitude': 4.479433059692383, 'distance': 8.609095573425293, 'cosine_with_motion': 0.6377807320191523, 'motion_component': 2.856895963161545}, {'ion': 2434, 'force': [-2.212773084640503, -3.5199012756347656, 0.5018016695976257], 'magnitude': 4.187824726104736, 'distance': 8.903787612915039, 'cosine_with_motion': 0.16944200942461562, 'motion_component': 0.7095934102755699}, {'ion': 2443, 'force': [-0.0022186795249581337, -2.1863017082214355, 0.10083231329917908], 'magnitude': 2.188626766204834, 'distance': 12.316383361816406, 'cosine_with_motion': -0.09501970189480759, 'motion_component': -0.20796266539248132}]}, 5708: {'frame': 5708, 'ionic_force': [-7.562033966183662, -7.692690953612328, -1.67104172706604], 'ionic_force_magnitude': 10.915779049939598, 'motion_vector': [-1.0818023681640625, 2.732677459716797, -0.10074615478515625], 'cosine_ionic_motion': -0.3947808800753782, 'ionic_motion_component': -4.30934086004353, 'ionic_force_x': -7.562033966183662, 'ionic_force_y': -7.692690953612328, 'ionic_force_z': -1.67104172706604, 'radial_force': 10.787115082982305, 'axial_force': -1.67104172706604, 'contributions': [{'ion': 1355, 'force': [-0.5876579880714417, -0.8973038792610168, -1.4970914125442505], 'magnitude': 1.841678261756897, 'distance': 13.426480293273926, 'cosine_with_moti</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>{5891: {'frame': 5891, 'ionic_force': [-1.5849148631095886, 7.950932557694614, -11.96000251173973], 'ionic_force_magnitude': 14.448908046670327, 'motion_vector': [-0.0869140625, 0.02236175537109375, -1.756866455078125], 'cosine_ionic_motion': 0.8390809281841389, 'ionic_motion_component': 12.123803175047412, 'ionic_force_x': -1.5849148631095886, 'ionic_force_y': 7.950932557694614, 'ionic_force_z': -11.96000251173973, 'radial_force': 8.10735984524641, 'axial_force': -11.96000251173973, 'contributions': [{'ion': 1355, 'force': [-1.7060837745666504, 0.8367077708244324, -5.490914821624756], 'magnitude': 5.810417175292969, 'distance': 7.559018135070801, 'directional_contribution': 5.578692453569913}, {'ion': 1380, 'force': [7.263280868530273, 6.749550819396973, -3.8440001010894775], 'magnitude': 10.634284973144531, 'distance': 5.587465763092041, 'directional_contribution': 3.5659379188627023}, {'ion': 1443, 'force': [-0.4787597060203552, 0.010035867802798748, -2.1720573902130127], 'magnitude': 2.2242178916931152, 'distance': 12.21744441986084, 'directional_contribution': 2.1930104608552266}, {'ion': 2434, 'force': [-3.879657030105591, -2.270467758178711, -0.30914631485939026], 'magnitude': 4.5058112144470215, 'distance': 8.583858489990234, 'directional_contribution': 0.47156326582191443}, {'ion': 2443, 'force': [-2.7836952209472656, 2.625105857849121, -0.14388388395309448], 'magnitude': 3.8289480209350586, 'distance': 9.311707496643066, 'directional_contribution': 0.3145989551665549}]}, 5892: {'frame': 5892, 'ionic_force': [-2.49815434217453, 7.7181031331419945, -11.375910818576813], 'ionic_force_magnitude': 13.972159390851319, 'motion_vector': [1.8442268371582031, 0.5494155883789062, -1.9481353759765625], 'cosine_ionic_motion': 0.5696590418762275, 'ionic_motion_component': 7.959366931534297, 'ionic_force_x': -2.49815434217453, 'ionic_force_y': 7.7181031331419945, 'ionic_force_z': -11.375910818576813, 'radial_force': 8.112329572394216, 'axial_force': -11.375910818576813, 'contributions': [{'ion': 1355, 'force': [-1.323460340499878, 0.5493678450584412, -3.9731087684631348], 'magnitude': 4.2236175537109375, 'distance': 8.86598014831543, 'directional_contribution': 2.045514847932078}, {'ion': 1380, 'force': [4.6296796798706055, 6.161921977996826, -3.7464330196380615], 'magnitude': 8.56965446472168, 'distance': 6.224255084991455, 'directional_contribution': 7.019766713293727}, {'ion': 1443, 'force': [-0.2683507800102234, 0.09991147369146347, -1.5568095445632935], 'magnitude': 1.582924723625183, 'distance': 14.482345581054688, 'directional_contribution': 0.9468916215238073}, {'ion': 2434, 'force': [-3.6428050994873047, -2.0931317806243896, -1.1591386795043945], 'magnitude': 4.358306407928467, 'distance': 8.72790813446045, 'directional_contribution': -2.048719607946321}, {'ion': 2443, 'force': [-1.8932178020477295, 3.0000336170196533, -0.9404208064079285], 'magnitude': 3.6699955463409424, 'distance': 9.511220932006836, 'directional_contribution': -0.004086816738126942}]}, 5893: {'frame': 5893, 'ionic_force': [-2.40166874229908, 3.821544498205185, -9.344871044158936], 'ionic_force_magnitude': 10.377804677842944, 'motion_vector': [1.5363502502441406, -0.806884765625, 5.4425048828125], 'cosine_ionic_motion': -0.9721669729770439, 'ionic_motion_component': -10.08895895980558, 'ionic_force_x': -2.40166874229908, 'ionic_force_y': 3.821544498205185, 'ionic_force_z': -9.344871044158936, 'radial_force': 4.513559028028632, 'axial_force': -9.344871044158936, 'contributions': [{'ion': 1355, 'force': [-0.15968115627765656, 0.468254417181015, -2.7393507957458496], 'magnitude': 2.7836670875549316, 'distance': 10.92094898223877, 'directional_contribution': -2.7189794345203118}, {'ion': 1380, 'force': [2.5271170139312744, 2.5101613998413086, -2.471982479095459], 'magnitude': 4.335657596588135, 'distance': 8.750675201416016, 'directional_contribution': -2.030059606386061}, {'ion': 2434, 'force': [-3.2794134616851807, -2.170670509338379, -2.4210591316223145], 'magnitude': 4.618212699890137, 'distance': 8.478754997253418, 'directional_contribution': -2.882024381575036}, {'ion': 2443, 'force': [-1.489691138267517, 3.0137991905212402, -1.7124786376953125], 'magnitude': 3.7728965282440186, 'distance': 9.380620956420898, 'directional_contribution': -2.457895387573828}]}, 5894: {'frame': 5894, 'ionic_force': [2.133852392435074, 4.722728848457336, -11.392761290073395], 'ionic_force_magnitude': 12.516089789600699, 'motion_vector': [-1.8502960205078125, -2.012805938720703, -7.103691101074219], 'cosine_ionic_motion': 0.708278545868222, 'ionic_motion_component': 8.864877876134484, 'ionic_force_x': 2.133852392435074, 'ionic_force_y': 4.722728848457336, 'ionic_force_z': -11.392761290073395, 'radial_force': 5.182421616267056, 'axial_force': -11.392761290073395, 'contributions': [{'ion': 1355, 'force': [2.837956190109253, 1.9178216457366943, -13.039620399475098], 'magnitude': 13.481978416442871, 'distance': 4.962405204772949, 'directional_contribution': 10.972395206762123}, {'ion': 1380, 'force': [3.910667657852173, 2.027388572692871, 0.4125763773918152], 'magnitude': 4.424233913421631, 'distance': 8.66263484954834, 'directional_contribution': -1.871791728097115}, {'ion': 1443, 'force': [0.15473537147045135, 0.442801833152771, -2.8794543743133545], 'magnitude': 2.9174089431762695, 'distance': 10.66769027709961, 'directional_contribution': 2.532583781260087}, {'ion': 2434, 'force': [-4.8726701736450195, -5.370229721069336, 1.624809980392456], 'magnitude': 7.4311699867248535, 'distance': 6.684061527252197, 'directional_contribution': 1.0881937725306159}, {'ion': 2443, 'force': [0.10316334664821625, 5.704946517944336, 2.488927125930786], 'magnitude': 6.225095748901367, 'distance': 7.302911281585693, 'directional_contribution': -3.8565031880570912}]}, 5895: {'frame': 5895, 'ionic_force': [5.1735977828502655, -3.9379420280456543, -22.839519739151], 'ionic_force_magnitude': 23.746940083935648, 'motion_vector': [-0.4307060241699219, 1.0893287658691406, 5.436920166015625], 'cosine_ionic_motion': -0.9895653006108213, 'ionic_motion_component': -23.49914790274694, 'ionic_force_x': 5.1735977828502655, 'ionic_force_y': -3.9379420280456543, 'ionic_force_z': -22.839519739151, 'radial_force': 6.5018075513630444, 'axial_force': -22.839519739151, 'contributions': [{'ion': 1355, 'force': [-0.23459890484809875, -0.226188063621521, -2.4711523056030273], 'magnitude': 2.4925472736358643, 'distance': 11.54110336303711, 'directional_contribution': -2.441855024673414}, {'ion': 1380, 'force': [2.8447628021240234, 1.016716718673706, -3.0548858642578125], 'magnitude': 4.296360492706299, 'distance': 8.790602684020996, 'directional_contribution': -3.0075262584837823}, {'ion': 2434, 'force': [-1.8455193042755127, -1.5154215097427368, -1.5823023319244385], 'magnitude': 2.864633321762085, 'distance': 10.765507698059082, 'directional_contribution': -1.700704341499744}, {'ion': 2443, 'force': [4.4089531898498535, -3.2130491733551025, -15.731179237365723], 'magnitude': 16.650300979614258, 'distance': 4.4653754234313965, 'directional_contribution': -16.349062107802858}]}, 5896: {'frame': 5896, 'ionic_force': [-0.017224013805389404, -9.5826591377554, 4.59900638461113], 'ionic_force_magnitude': 10.629135079711451, 'motion_vector': [-0.24406814575195312, -1.3061408996582031, -1.6460342407226562], 'cosine_ionic_motion': 0.22016303928493244, 'ionic_motion_component': 2.3401426841193658, 'ionic_force_x': -0.017224013805389404, 'ionic_force_y': -9.5826591377554, 'ionic_force_z': 4.59900638461113, 'radial_force': 9.582674617091964, 'axial_force': 4.59900638461113, 'contributions': [{'ion': 1355, 'force': [-1.8489515781402588, -0.00621435372158885, -7.483148097991943], 'magnitude': 7.708188056945801, 'distance': 6.562856197357178, 'directional_contribution': 6.039890199718068}, {'ion': 1380, 'force': [7.6192097663879395, 3.615647554397583, -0.6914269924163818], 'magnitude': 8.461874961853027, 'distance': 6.263769149780273, 'directional_contribution': -2.5735026015322013}, {'ion': 1443, 'force': [-0.3091173768043518, 0.00013788617798127234, -2.191742420196533], 'magnitude': 2.2134335041046143, 'distance': 12.247171401977539, 'directional_contribution': 1.7410010963815887}, {'ion': 2434, 'force': [-4.129177093505859, -3.6542301177978516, -0.2538600265979767], 'magnitude': 5.519777774810791, 'distance': 7.755472183227539, 'directional_contribution': 2.930199253874088}, {'ion': 2443, 'force': [-1.3491877317428589, -9.538000106811523, 15.219183921813965], 'magnitude': 18.01158905029297, 'distance': 4.293317794799805, 'directional_contribution': -5.797445201812349}]}, 5897: {'frame': 5897, 'ionic_force': [1.8552783280611038, -2.173237666487694, -12.846055001020432], 'ionic_force_magnitude': 13.160020847964342, 'motion_vector': [-2.82208251953125, 5.449005126953125, 2.03216552734375], 'cosine_ionic_motion': -0.5076259578248576, 'ionic_motion_component': -6.680368187942994, 'ionic_force_x': 1.8552783280611038, 'ionic_force_y': -2.173237666487694, 'ionic_force_z': -12.846055001020432, 'radial_force': 2.8574498472613796, 'axial_force': -12.846055001020432, 'contributions': [{'ion': 1355, 'force': [-0.9138748049736023, -0.6297469139099121, -4.202837944030762], 'magnitude': 4.346906661987305, 'distance': 8.73934555053711, 'directional_contribution': -1.4531370892927153}, {'ion': 1380, 'force': [9.447088241577148, 4.048842430114746, -5.9594407081604], 'magnitude': 11.880888938903809, 'distance': 5.286211967468262, 'directional_contribution': -2.584843313608019}, {'ion': 1443, 'force': [-0.18578504025936127, -0.21087370812892914, -1.5908935070037842], 'magnitude': 1.615526556968689, 'distance': 14.335472106933594, 'directional_contribution': -0.5967834414567519}, {'ion': 2434, 'force': [-1.8904106616973877, -2.4841415882110596, -0.7933556437492371], 'magnitude': 3.2208733558654785, 'distance': 10.152715682983398, 'directional_contribution': -1.51812747847017}, {'ion': 2443, 'force': [-4.601739406585693, -2.897317886352539, -0.29952719807624817], 'magnitude': 5.446115493774414, 'distance': 7.807744979858398, 'directional_contribution': -0.527476890051453}]}, 5898: {'frame': 5898, 'ionic_force': [-8.504436016082764, 11.964142084121704, -4.874931126832962], 'ionic_force_magnitude': 15.467096729899332, 'motion_vector': [1.28692626953125, 1.0255928039550781, -0.0074005126953125], 'cosine_ionic_motion': 0.053503810279040165, 'ionic_motion_component': 0.8275486090040964, 'ionic_force_x': -8.504436016082764, 'ionic_force_y': 11.964142084121704, 'ionic_force_z': -4.874931126832962, 'radial_force': 14.678764517516374, 'axial_force': -4.874931126832962, 'contributions': [{'ion': 1355, 'force': [-2.246494770050049, 1.9543259143829346, -3.1174850463867188], 'magnitude': 4.311013698577881, 'distance': 8.775650978088379, 'directional_contribution': -0.5248223988331979}, {'ion': 1380, 'force': [1.3024711608886719, 6.837247848510742, -1.0843136310577393], 'magnitude': 7.044155597686768, 'distance': 6.865221977233887, 'directional_contribution': 5.2845892541990045}, {'ion': 1443, 'force': [-0.6266984939575195, 0.5076103806495667, -1.6870962381362915], 'magnitude': 1.8699499368667603, 'distance': 13.32459545135498, 'directional_contribution': -0.16615464063826718}, {'ion': 2434, 'force': [-3.711239814758301, -0.4314489960670471, -0.2661377489566803], 'magnitude': 3.745701313018799, 'distance': 9.414612770080566, 'directional_contribution': -3.1699934160905885}, {'ion': 2443, 'force': [-3.2224740982055664, 3.096406936645508, 1.2801015377044678], 'magnitude': 4.6487345695495605, 'distance': 8.450874328613281, 'directional_contribution': -0.5960707047619812}]}, 5899: {'frame': 5899, 'ionic_force': [-6.799471914768219, 9.492137521505356, -5.600397616624832], 'ionic_force_magnitude': 12.949824188427762, 'motion_vector': [-1.2925643920898438, 0.4482421875, -0.7178955078125], 'cosine_ionic_motion': 0.8528839683401198, 'ionic_motion_component': 11.04469744313314, 'ionic_force_x': -6.799471914768219, 'ionic_force_y': 9.492137521505356, 'ionic_force_z': -5.600397616624832, 'radial_force': 11.676193431375298, 'axial_force': -5.600397616624832, 'contributions': [{'ion': 1355, 'force': [-1.5860280990600586, 2.484849214553833, -3.0621752738952637], 'magnitude': 4.250514984130859, 'distance': 8.837882995605469, 'directional_contribution': 3.4706716480274054}, {'ion': 1380, 'force': [1.502514123916626, 3.8119521141052246, -0.36482638120651245], 'magnitude': 4.113590717315674, 'distance': 8.98376750946045, 'directional_contribution': 0.01843933504465589}, {'ion': 1443, 'force': [-0.44899803400039673, 0.7380704879760742, -1.5459970235824585], 'magnitude': 1.7710037231445312, 'distance': 13.691761016845703, 'directional_contribution': 1.3081298281740104}, {'ion': 2434, 'force': [-5.232437610626221, -0.4004041254520416, -0.13199836015701294], 'magnitude': 5.249395370483398, 'distance': 7.952696323394775, 'directional_contribution': 4.322689741515248}, {'ion': 2443, 'force': [-1.034522294998169, 2.8576698303222656, -0.4954005777835846], 'magnitude': 3.079274892807007, 'distance': 10.383524894714355, 'directional_contribution': 1.9247671286365629}]}, 5900: {'frame': 5900, 'ionic_force': [-6.1381120681762695, 8.840319886803627, -5.065477430820465], 'ionic_force_magnitude': 11.894819757552376, 'motion_vector': [1.6382980346679688, 0.11060333251953125, 0.5860443115234375], 'cosine_ionic_motion': -0.5808999323825219, 'ionic_motion_component': -6.909699992864462, 'ionic_force_x': -6.1381120681762695, 'ionic_force_y': 8.840319886803627, 'ionic_force_z': -5.065477430820465, 'radial_force': 10.762326675143571, 'axial_force': -5.065477430820465, 'contributions': [{'ion': 1355, 'force': [-1.8010727167129517, 2.0751216411590576, -2.528494358062744], 'magnitude': 3.734069585800171, 'distance': 9.429265022277832, 'directional_contribution': -2.4106974082634594}, {'ion': 1380, 'force': [0.7935147881507874, 3.8666439056396484, -0.5172351598739624], 'magnitude': 3.980971336364746, 'distance': 9.132181167602539, 'directional_contribution': 0.8170782686594613}, {'ion': 1443, 'force': [-0.539768397808075, 0.6087048649787903, -1.3261784315109253], 'magnitude': 1.555834412574768, 'distance': 14.607885360717773, 'directional_contribution': -0.9143675408841645}, {'ion': 2434, 'force': [-3.400973320007324, 0.1036798506975174, -0.37451714277267456], 'magnitude': 3.423102617263794, 'distance': 9.848250389099121, 'directional_contribution': -3.315119277919867}, {'ion': 2443, 'force': [-1.189812421798706, 2.1861696243286133, -0.3190523386001587], 'magnitude': 2.5093395709991455, 'distance': 11.502422332763672, 'directional_contribution': -1.0865940833195076}]}, 5901: {'frame': 5901, 'ionic_force': [-7.439622104167938, 9.131087750196457, -4.992527484893799], 'ionic_force_magnitude': 12.792578756530364, 'motion_vector': [-0.2744865417480469, -0.7472152709960938, 0.6619415283203125], 'cosine_ionic_motion': -0.6105029271010953, 'ionic_motion_component': -7.809906776033078, 'ionic_force_x': -7.439622104167938, 'ionic_force_y': 9.131087750196457, 'ionic_force_z': -4.992527484893799, 'radial_force': 11.77814673684328, 'axial_force': -4.992527484893799, 'contributions': [{'ion': 1355, 'force': [-1.4037278890609741, 2.735112428665161, -2.956904888153076], 'magnitude': 4.265510082244873, 'distance': 8.822335243225098, 'directional_contribution': -3.4924388454826705}, {'ion': 1380, 'force': [1.2992652654647827, 3.4894778728485107, -0.26489782333374023], 'magnitude': 3.7329232692718506, 'distance': 9.430712699890137, 'directional_contribution': -3.032336416243023}, {'ion': 1443, 'force': [-0.41779905557632446, 0.741924524307251, -1.4480189085006714], 'magnitude': 1.6798115968704224, 'distance': 14.058492660522461, 'directional_contribution': -1.3505312414997288}, {'ion': 2434, 'force': [-5.164675235748291, 0.30420610308647156, -0.35055652260780334], 'magnitude': 5.185489654541016, 'distance': 8.001550674438477, 'directional_contribution': 0.9256072060184977}, {'ion': 2443, 'force': [-1.7526851892471313, 1.8603668212890625, 0.02785065770149231], 'magnitude': 2.5560996532440186, 'distance': 11.396726608276367, 'directional_contribution': -0.8602077719029388}]}, 5902: {'frame': 5902, 'ionic_force': [-7.47670590877533, 10.180595852434635, -5.091444402933121], 'ionic_force_magnitude': 13.618680892989754, 'motion_vector': [-0.6989402770996094, 0.07197189331054688, -0.5127105712890625], 'cosine_ionic_motion': 0.7233805888715068, 'ionic_motion_component': 9.851489404024067, 'ionic_force_x': -7.47670590877533, 'ionic_force_y': 10.180595852434635, 'ionic_force_z': -5.091444402933121, 'radial_force': 12.631138632638201, 'axial_force': -5.091444402933121, 'contributions': [{'ion': 1355, 'force': [-2.3436784744262695, 3.635133743286133, -3.490668773651123], 'magnitude': 5.558038711547852, 'distance': 7.728732109069824, 'directional_contribution': 4.241640120977877}, {'ion': 1380, 'force': [1.7799241542816162, 3.8899707794189453, -0.24371981620788574], 'magnitude': 4.284787178039551, 'distance': 8.802467346191406, 'directional_contribution': -0.9647328522041647}, {'ion': 1443, 'force': [-0.6318591833114624, 0.8132873177528381, -1.8050473928451538], 'magnitude': 2.078191041946411, 'distance': 12.639395713806152, 'directional_contribution': 1.6390157971740118}, {'ion': 2434, 'force': [-4.041162490844727, 0.0778370276093483, 0.15670618414878845], 'magnitude': 4.044948577880859, 'distance': 9.059673309326172, 'directional_contribution': 3.161366311019386}, {'ion': 2443, 'force': [-2.2399299144744873, 1.7643669843673706, 0.2912853956222534], 'magnitude': 2.866203784942627, 'distance': 10.762557983398438, 'directional_contribution': 1.7741998450811902}]}, 5903: {'frame': 5903, 'ionic_force': [-7.226976692676544, 9.150095321238041, -4.231179058551788], 'ionic_force_magnitude': 12.403882969850992, 'motion_vector': [-2.064189910888672, -0.9773674011230469, 0.5256500244140625], 'cosine_ionic_motion': 0.12902546839686596, 'ionic_motion_component': 1.600416810124933, 'ionic_force_x': -7.226976692676544, 'ionic_force_y': 9.150095321238041, 'ionic_force_z': -4.231179058551788, 'radial_force': 11.65990722536986, 'axial_force': -4.231179058551788, 'contributions': [{'ion': 1355, 'force': [-1.8546229600906372, 2.477461338043213, -2.9006059169769287], 'magnitude': 4.241574764251709, 'distance': 8.847192764282227, 'directional_contribution': -0.05026446999784895}, {'ion': 1380, 'force': [1.4170900583267212, 4.401101589202881, -0.24274271726608276], 'magnitude': 4.629985332489014, 'distance': 8.467968940734863, 'directional_contribution': -3.1380146253485997}, {'ion': 1443, 'force': [-0.5996553301811218, 0.7718545794487, -1.4985142946243286], 'magnitude': 1.7891035079956055, 'distance': 13.62232780456543, 'directional_contribution': -0.12983350805516558}, {'ion': 2434, 'force': [-4.2714080810546875, 0.0717788115143776, 0.005224108695983887], 'magnitude': 4.272014141082764, 'distance': 8.815616607666016, 'directional_contribution': 3.733405692233334}, {'ion': 2443, 'force': [-1.9183803796768188, 1.4278990030288696, 0.40545976161956787], 'magnitude': 2.4255878925323486, 'distance': 11.69931697845459, 'directional_contribution': 1.1851236810123673}]}, 5904: {'frame': 5904, 'ionic_force': [-9.568521454930305, 7.556034505367279, -3.6204235684126616], 'ionic_force_magnitude': 12.718401121779435, 'motion_vector': [0.26805877685546875, -0.65460205078125, 0.54949951171875], 'cosine_ionic_motion': -0.8339597165242312, 'ionic_motion_component': -10.606634194160641, 'ionic_force_x': -9.568521454930305, 'ionic_force_y': 7.556034505367279, 'ionic_force_z': -3.6204235684126616, 'radial_force': 12.192221302115644, 'axial_force': -3.6204235684126616, 'contributions': [{'ion': 1355, 'force': [-2.7520177364349365, 2.0397398471832275, -2.4019126892089844], 'magnitude': 4.183697700500488, 'distance': 8.908178329467773, 'directional_contribution': -3.787770130145411}, {'ion': 1380, 'force': [-0.21680445969104767, 5.097675800323486, -0.02414863370358944], 'magnitude': 5.102341175079346, 'distance': 8.066484451293945, 'directional_contribution': -3.8051470526533926}, {'ion': 1443, 'force': [-0.8819059133529663, 0.5921956896781921, -1.4838796854019165], 'magnitude': 1.8249253034591675, 'distance': 13.487966537475586, 'directional_contribution': -1.6070323817126706}, {'ion': 2434, 'force': [-3.755582809448242, -0.6733697652816772, -0.06396784633398056], 'magnitude': 3.8160085678100586, 'distance': 9.327481269836426, 'directional_contribution': -0.671057946384932}, {'ion': 2443, 'force': [-1.9622105360031128, 0.4997929334640503, 0.3534852862358093], 'magnitude': 2.0554840564727783, 'distance': 12.709017753601074, 'directional_contribution': -0.7356265858207962}]}, 5905: {'frame': 5905, 'ionic_force': [-9.992130100727081, 6.58165055513382, -3.931290879845619], 'ionic_force_magnitude': 12.594277905529433, 'motion_vector': [0.7903480529785156, -0.9876708984375, -0.41739654541015625], 'cosine_ionic_motion': -0.7604122752570438, 'ionic_motion_component': -9.576843517363152, 'ionic_force_x': -9.992130100727081, 'ionic_force_y': 6.58165055513382, 'ionic_force_z': -3.931290879845619, 'radial_force': 11.964981737543502, 'axial_force': -3.931290879845619, 'contributions': [{'ion': 1355, 'force': [-3.319589138031006, 2.096099615097046, -2.7997121810913086], 'magnitude': 4.822000980377197, 'distance': 8.29765510559082, 'directional_contribution': -2.6465153476760293}, {'ion': 1380, 'force': [-1.1027723550796509, 4.649133205413818, -0.03528514876961708], 'magnitude': 4.778262138366699, 'distance': 8.335545539855957, 'directional_contribution': -4.090424162976559}, {'ion': 1443, 'force': [-0.942359983921051, 0.5759227275848389, -1.6433050632476807], 'magnitude': 1.9799445867538452, 'distance': 12.949187278747559, 'directional_contribution': -0.47123119947199754}, {'ion': 2434, 'force': [-2.8171496391296387, -1.0690206289291382, 0.05009468272328377], 'magnitude': 3.0135769844055176, 'distance': 10.496098518371582, 'directional_contribution': -0.8945575505990111}, {'ion': 2443, 'force': [-1.8102589845657349, 0.32951563596725464, 0.49691683053970337], 'magnitude': 1.9059234857559204, 'distance': 13.198248863220215, 'directional_contribution': -1.4741154031700958}]}, 5906: {'frame': 5906, 'ionic_force': [-10.922582864761353, 10.523097217082977, -6.046317458152771], 'ionic_force_magnitude': 16.327778363345114, 'motion_vector': [1.9758110046386719, 3.4515724182128906, -0.8893280029296875], 'cosine_ionic_motion': 0.3023330582001712, 'ionic_motion_component': 4.936427166204714, 'ionic_force_x': -10.922582864761353, 'ionic_force_y': 10.523097217082977, 'ionic_force_z': -6.046317458152771, 'radial_force': 15.1670165648277, 'axial_force': -6.046317458152771, 'contributions': [{'ion': 1355, 'force': [-4.033276081085205, 1.9656189680099487, -3.9555554389953613], 'magnitude': 5.981420516967773, 'distance': 7.450181484222412, 'directional_contribution': 0.5725395255051566}, {'ion': 1380, 'force': [0.23750650882720947, 8.032539367675781, -0.7383502721786499], 'magnitude': 8.06989860534668, 'distance': 6.414089202880859, 'directional_contribution': 7.079424943052482}, {'ion': 1443, 'force': [-1.2005337476730347, 0.7920025587081909, -2.096895217895508], 'magnitude': 2.542738437652588, 'distance': 11.426630973815918, 'directional_contribution': 0.5463286174781139}, {'ion': 2434, 'force': [-3.1640639305114746, -0.9320102334022522, 0.2620435059070587], 'magnitude': 3.308868408203125, 'distance': 10.016806602478027, 'directional_contribution': -2.3805684658359643}, {'ion': 2443, 'force': [-2.7622156143188477, 0.6649465560913086, 0.48243996500968933], 'magnitude': 2.881793975830078, 'distance': 10.733406066894531, 'directional_contribution': -0.8812971210839531}]}, 5907: {'frame': 5907, 'ionic_force': [-9.553559362888336, 8.830352172255516, -5.354349387693219], 'ionic_force_magnitude': 14.068215002329891, 'motion_vector': [-1.1595115661621094, -0.7659034729003906, 0.1236724853515625], 'cosine_ionic_motion': 0.18607521899512322, 'ionic_motion_component': 2.6177461874290127, 'ionic_force_x': -9.553559362888336, 'ionic_force_y': 8.830352172255516, 'ionic_force_z': -5.354349387693219, 'radial_force': 13.009443338832337, 'axial_force': -5.354349387693219, 'contributions': [{'ion': 1355, 'force': [-1.5680482387542725, 3.1532657146453857, -3.071322202682495], 'magnitude': 4.672780513763428, 'distance': 8.429102897644043, 'directional_contribution': -0.7001279323548903}, {'ion': 1380, 'force': [0.9171464443206787, 3.123924732208252, -0.38423049449920654], 'magnitude': 3.278367757797241, 'distance': 10.063294410705566, 'directional_contribution': -2.5113081942758813}, {'ion': 1443, 'force': [-0.6362531781196594, 1.28103506565094, -1.8257994651794434], 'magnitude': 2.3193562030792236, 'distance': 11.964245796203613, 'directional_contribution': -0.3363195816363458}, {'ion': 2434, 'force': [-5.875592231750488, -0.22285892069339752, -0.07418480515480042], 'magnitude': 5.880284786224365, 'distance': 7.51397705078125, 'directional_contribution': 4.99907747936747}, {'ion': 2443, 'force': [-2.3908121585845947, 1.494985580444336, 0.0011875798227265477], 'magnitude': 2.8197457790374756, 'distance': 10.850857734680176, 'directional_contribution': 1.1664247125823328}]}, 5908: {'frame': 5908, 'ionic_force': [-11.456575185060501, 10.54627639055252, -7.669879510998726], 'ionic_force_magnitude': 17.35811373364363, 'motion_vector': [0.8431854248046875, 0.49897003173828125, 0.0274658203125], 'cosine_ionic_motion': -0.2708674020063873, 'ionic_motion_component': -4.701747170763442, 'ionic_force_x': -11.456575185060501, 'ionic_force_y': 10.54627639055252, 'ionic_force_z': -7.669879510998726, 'radial_force': 15.571674947701341, 'axial_force': -7.669879510998726, 'contributions': [{'ion': 1327, 'force': [-0.42327919602394104, 0.5680921673774719, -1.5069403648376465], 'magnitude': 1.6651616096496582, 'distance': 14.120200157165527, 'directional_contribution': -0.11715721735563278}, {'ion': 1355, 'force': [-3.401942491531372, 4.668416976928711, -2.9111828804016113], 'magnitude': 6.468563556671143, 'distance': 7.164157390594482, 'directional_contribution': -0.6315649612756662}, {'ion': 1380, 'force': [0.7152265310287476, 4.2912068367004395, -0.36868032813072205], 'magnitude': 4.365996837615967, 'distance': 8.72021770477295, 'directional_contribution': 2.7895076882816205}, {'ion': 1443, 'force': [-1.2062010765075684, 1.3956199884414673, -2.323375701904297], 'magnitude': 2.9666059017181396, 'distance': 10.578866004943848, 'directional_contribution': -0.3922801783022507}, {'ion': 2434, 'force': [-4.892893314361572, -1.0576077699661255, -0.7788661122322083], 'magnitude': 5.066120147705078, 'distance': 8.095269203186035, 'directional_contribution': -4.7694128038131645}, {'ion': 2443, 'force': [-2.247485637664795, 0.6805481910705566, 0.2191658765077591], 'magnitude': 2.3584680557250977, 'distance': 11.864625930786133, 'directional_contribution': -1.5808396584777453}]}, 5909: {'frame': 5909, 'ionic_force': [-11.318663328886032, 12.406723007559776, -6.972444713115692], 'ionic_force_magnitude': 18.183891239677976, 'motion_vector': [-2.2848129272460938, -0.2534599304199219, 0.33966064453125], 'cosine_ionic_motion': 0.4815507907179075, 'ionic_motion_component': 8.756467204795362, 'ionic_force_x': -11.318663328886032, 'ionic_force_y': 12.406723007559776, 'ionic_force_z': -6.972444713115692, 'radial_force': 16.794014271131918, 'axial_force': -6.972444713115692, 'contributions': [{'ion': 1327, 'force': [-0.33883413672447205, 0.5817093849182129, -1.368337631225586], 'magnitude': 1.5249727964401245, 'distance': 14.754958152770996, 'directional_contribution': 0.06969753108227472}, {'ion': 1355, 'force': [-2.4924542903900146, 5.4414496421813965, -2.8278679847717285], 'magnitude': 6.6195573806762695, 'distance': 7.081977844238281, 'directional_contribution': 1.443801974025039}, {'ion': 1380, 'force': [0.682213544845581, 3.278224229812622, -0.35480713844299316], 'magnitude': 3.3672032356262207, 'distance': 9.929659843444824, 'directional_contribution': -1.0801953509631037}, {'ion': 1443, 'force': [-0.9330054521560669, 1.539467692375183, -2.1729485988616943], 'magnitude': 2.821730852127075, 'distance': 10.847040176391602, 'directional_contribution': 0.43183167592455707}, {'ion': 2434, 'force': [-6.0750651359558105, -0.0652710348367691, -0.6163405776023865], 'magnitude': 6.1065993309021, 'distance': 7.3734259605407715, 'directional_contribution': 5.890208570060275}, {'ion': 2443, 'force': [-2.161517858505249, 1.6311430931091309, 0.3678572177886963], 'magnitude': 2.732783555984497, 'distance': 11.0221529006958, 'directional_contribution': 2.0011227836022023}]}, 5910: {'frame': 5910, 'ionic_force': [-10.408794045448303, 10.508824622258544, -5.274085454642773], 'ionic_force_magnitude': 15.703323399994726, 'motion_vector': [1.3806076049804688, -0.5164985656738281, -0.46323394775390625], 'cosine_ionic_motion': -0.7152705127165517, 'ionic_motion_component': -11.232124179668052, 'ionic_force_x': -10.408794045448303, 'ionic_force_y': 10.508824622258544, 'ionic_force_z': -5.274085454642773, 'radial_force': 14.791159130438272, 'axial_force': -5.274085454642773, 'contributions': [{'ion': 1327, 'force': [-0.6121020317077637, 0.6046913862228394, -1.447232961654663], 'magnitude': 1.683687448501587, 'distance': 14.042301177978516, 'directional_contribution': -0.3151752919328601}, {'ion': 1355, 'force': [-3.0769357681274414, 3.4389429092407227, -1.8768421411514282], 'magnitude': 4.9816060066223145, 'distance': 8.163649559020996, 'directional_contribution': -3.3361758323198316}, {'ion': 1380, 'force': [0.2949361801147461, 4.301926136016846, -0.4940275549888611], 'magnitude': 4.340232849121094, 'distance': 8.746061325073242, 'directional_contribution': -1.0263827729385078}, {'ion': 1443, 'force': [-1.3746557235717773, 1.4419944286346436, -1.9757091999053955], 'magnitude': 2.8057892322540283, 'distance': 10.877811431884766, 'directional_contribution': -1.1179836469762705}, {'ion': 2434, 'force': [-3.7204020023345947, -0.008718037977814674, 0.07665441185235977], 'magnitude': 3.7212016582489014, 'distance': 9.44555377960205, 'directional_contribution': -3.344322963905802}, {'ion': 2443, 'force': [-1.9196346998214722, 0.7299878001213074, 0.44307199120521545], 'magnitude': 2.1009979248046875, 'distance': 12.570606231689453, 'directional_contribution': -2.0920835913640463}]}, 5911: {'frame': 5911, 'ionic_force': [-10.766848921775818, 10.963305234909058, -7.595397055149078], 'ionic_force_magnitude': 17.140862107942432, 'motion_vector': [0.8972282409667969, 0.0338134765625, 0.5027389526367188], 'cosine_ionic_motion': -0.7431533102809617, 'ionic_motion_component': -12.73828841658692, 'ionic_force_x': -10.766848921775818, 'ionic_force_y': 10.963305234909058, 'ionic_force_z': -7.595397055149078, 'radial_force': 15.366167296308127, 'axial_force': -7.595397055149078, 'contributions': [{'ion': 1327, 'force': [-0.5103285312652588, 0.5325732827186584, -1.5038037300109863], 'magnitude': 1.6749613285064697, 'distance': 14.07883358001709, 'directional_contribution': -1.1621532902824823}, {'ion': 1355, 'force': [-3.0666186809539795, 4.69706916809082, -2.6569862365722656], 'magnitude': 6.20694637298584, 'distance': 7.313580513000488, 'directional_contribution': -3.8175687881888294}, {'ion': 1380, 'force': [1.1242055892944336, 4.820630073547363, -0.9092327952384949], 'magnitude': 5.032793998718262, 'distance': 8.122027397155762, 'directional_contribution': 0.694404081757682}, {'ion': 1443, 'force': [-1.2565020322799683, 1.390987515449524, -2.331714630126953], 'magnitude': 2.9917447566986084, 'distance': 10.534326553344727, 'directional_contribution': -2.1890254464942873}, {'ion': 2434, 'force': [-4.797569274902344, -1.150797963142395, -0.4690853953361511], 'magnitude': 4.9559102058410645, 'distance': 8.184785842895508, 'directional_contribution': -4.450057400890433}, {'ion': 2443, 'force': [-2.260035991668701, 0.6728431582450867, 0.2754257321357727], 'magnitude': 2.3740978240966797, 'distance': 11.825506210327148, 'directional_contribution': -1.8138876269042268}]}, 5912: {'frame': 5912, 'ionic_force': [-12.624213874340057, 11.033985555171967, -7.007168579846621], 'ionic_force_magnitude': 18.17195709556935, 'motion_vector': [-1.5638694763183594, 0.3469505310058594, -0.399810791015625], 'cosine_ionic_motion': 0.879006894420516, 'ionic_motion_component': 15.973275572119276, 'ionic_force_x': -12.624213874340057, 'ionic_force_y': 11.033985555171967, 'ionic_force_z': -7.007168579846621, 'radial_force': 16.766621996598587, 'axial_force': -7.007168579846621, 'contributions': [{'ion': 1327, 'force': [-0.41048890352249146, 0.6229236721992493, -1.6062426567077637], 'magnitude': 1.7710309028625488, 'distance': 13.6916</t>
+          <t>{5891: {'frame': 5891, 'ionic_force': [-1.5849148631095886, 7.950932557694614, -11.96000251173973], 'ionic_force_magnitude': 14.448908046670327, 'motion_vector': [-0.0869140625, 0.02236175537109375, -1.756866455078125], 'cosine_ionic_motion': 0.8390809281841389, 'ionic_motion_component': 12.123803175047412, 'ionic_force_x': -1.5849148631095886, 'ionic_force_y': 7.950932557694614, 'ionic_force_z': -11.96000251173973, 'radial_force': 8.10735984524641, 'axial_force': -11.96000251173973, 'contributions': [{'ion': 1355, 'force': [-1.7060837745666504, 0.8367077708244324, -5.490914821624756], 'magnitude': 5.810417175292969, 'distance': 7.559018135070801, 'cosine_with_motion': 0.9601190966229708, 'motion_component': 5.578692453569913}, {'ion': 1380, 'force': [7.263280868530273, 6.749550819396973, -3.8440001010894775], 'magnitude': 10.634284973144531, 'distance': 5.587465763092041, 'cosine_with_motion': 0.3353246454323799, 'motion_component': 3.5659379188627023}, {'ion': 1443, 'force': [-0.4787597060203552, 0.010035867802798748, -2.1720573902130127], 'magnitude': 2.2242178916931152, 'distance': 12.21744441986084, 'cosine_with_motion': 0.9859692911877616, 'motion_component': 2.1930104608552266}, {'ion': 2434, 'force': [-3.879657030105591, -2.270467758178711, -0.30914631485939026], 'magnitude': 4.5058112144470215, 'distance': 8.583858489990234, 'cosine_with_motion': 0.10465668711356463, 'motion_component': 0.47156326582191443}, {'ion': 2443, 'force': [-2.7836952209472656, 2.625105857849121, -0.14388388395309448], 'magnitude': 3.8289480209350586, 'distance': 9.311707496643066, 'cosine_with_motion': 0.08216328848026491, 'motion_component': 0.3145989551665549}]}, 5892: {'frame': 5892, 'ionic_force': [-2.49815434217453, 7.7181031331419945, -11.375910818576813], 'ionic_force_magnitude': 13.972159390851319, 'motion_vector': [1.8442268371582031, 0.5494155883789062, -1.9481353759765625], 'cosine_ionic_motion': 0.5696590418762275, 'ionic_motion_component': 7.959366931534297, 'ionic_force_x': -2.49815434217453, 'ionic_force_y': 7.7181031331419945, 'ionic_force_z': -11.375910818576813, 'radial_force': 8.112329572394216, 'axial_force': -11.375910818576813, 'contributions': [{'ion': 1355, 'force': [-1.323460340499878, 0.5493678450584412, -3.9731087684631348], 'magnitude': 4.2236175537109375, 'distance': 8.86598014831543, 'cosine_with_motion': 0.4843039886928752, 'motion_component': 2.045514847932078}, {'ion': 1380, 'force': [4.6296796798706055, 6.161921977996826, -3.7464330196380615], 'magnitude': 8.56965446472168, 'distance': 6.224255084991455, 'cosine_with_motion': 0.8191423334410239, 'motion_component': 7.019766713293727}, {'ion': 1443, 'force': [-0.2683507800102234, 0.09991147369146347, -1.5568095445632935], 'magnitude': 1.582924723625183, 'distance': 14.482345581054688, 'cosine_with_motion': 0.5981912216623002, 'motion_component': 0.9468916215238075}, {'ion': 2434, 'force': [-3.6428050994873047, -2.0931317806243896, -1.1591386795043945], 'magnitude': 4.358306407928467, 'distance': 8.72790813446045, 'cosine_with_motion': -0.4700724450400846, 'motion_component': -2.048719607946321}, {'ion': 2443, 'force': [-1.8932178020477295, 3.0000336170196533, -0.9404208064079285], 'magnitude': 3.6699955463409424, 'distance': 9.511220932006836, 'cosine_with_motion': -0.0011135754220507616, 'motion_component': -0.004086816738126942}]}, 5893: {'frame': 5893, 'ionic_force': [-2.40166874229908, 3.821544498205185, -9.344871044158936], 'ionic_force_magnitude': 10.377804677842944, 'motion_vector': [1.5363502502441406, -0.806884765625, 5.4425048828125], 'cosine_ionic_motion': -0.9721669729770439, 'ionic_motion_component': -10.08895895980558, 'ionic_force_x': -2.40166874229908, 'ionic_force_y': 3.821544498205185, 'ionic_force_z': -9.344871044158936, 'radial_force': 4.513559028028632, 'axial_force': -9.344871044158936, 'contributions': [{'ion': 1355, 'force': [-0.15968115627765656, 0.468254417181015, -2.7393507957458496], 'magnitude': 2.7836670875549316, 'distance': 10.92094898223877, 'cosine_with_motion': -0.9767616758619528, 'motion_component': -2.7189794345203118}, {'ion': 1380, 'force': [2.5271170139312744, 2.5101613998413086, -2.471982479095459], 'magnitude': 4.335657596588135, 'distance': 8.750675201416016, 'cosine_with_motion': -0.4682241377097566, 'motion_component': -2.030059606386061}, {'ion': 2434, 'force': [-3.2794134616851807, -2.170670509338379, -2.4210591316223145], 'magnitude': 4.618212699890137, 'distance': 8.478754997253418, 'cosine_with_motion': -0.6240561968776958, 'motion_component': -2.882024381575036}, {'ion': 2443, 'force': [-1.489691138267517, 3.0137991905212402, -1.7124786376953125], 'magnitude': 3.7728965282440186, 'distance': 9.380620956420898, 'cosine_with_motion': -0.6514611145093603, 'motion_component': -2.457895387573828}]}, 5894: {'frame': 5894, 'ionic_force': [2.133852392435074, 4.722728848457336, -11.392761290073395], 'ionic_force_magnitude': 12.516089789600699, 'motion_vector': [-1.8502960205078125, -2.012805938720703, -7.103691101074219], 'cosine_ionic_motion': 0.708278545868222, 'ionic_motion_component': 8.864877876134484, 'ionic_force_x': 2.133852392435074, 'ionic_force_y': 4.722728848457336, 'ionic_force_z': -11.392761290073395, 'radial_force': 5.182421616267056, 'axial_force': -11.392761290073395, 'contributions': [{'ion': 1355, 'force': [2.837956190109253, 1.9178216457366943, -13.039620399475098], 'magnitude': 13.481978416442871, 'distance': 4.962405204772949, 'cosine_with_motion': 0.8138564733433147, 'motion_component': 10.972395206762123}, {'ion': 1380, 'force': [3.910667657852173, 2.027388572692871, 0.4125763773918152], 'magnitude': 4.424233913421631, 'distance': 8.66263484954834, 'cosine_with_motion': -0.4230770317681675, 'motion_component': -1.871791728097115}, {'ion': 1443, 'force': [0.15473537147045135, 0.442801833152771, -2.8794543743133545], 'magnitude': 2.9174089431762695, 'distance': 10.66769027709961, 'cosine_with_motion': 0.8680935624145347, 'motion_component': 2.532583781260087}, {'ion': 2434, 'force': [-4.8726701736450195, -5.370229721069336, 1.624809980392456], 'magnitude': 7.4311699867248535, 'distance': 6.684061527252197, 'cosine_with_motion': 0.14643639628431301, 'motion_component': 1.0881937725306159}, {'ion': 2443, 'force': [0.10316334664821625, 5.704946517944336, 2.488927125930786], 'magnitude': 6.225095748901367, 'distance': 7.302911281585693, 'cosine_with_motion': -0.6195090667008921, 'motion_component': -3.8565031880570912}]}, 5895: {'frame': 5895, 'ionic_force': [5.1735977828502655, -3.9379420280456543, -22.839519739151], 'ionic_force_magnitude': 23.746940083935648, 'motion_vector': [-0.4307060241699219, 1.0893287658691406, 5.436920166015625], 'cosine_ionic_motion': -0.9895653006108213, 'ionic_motion_component': -23.49914790274694, 'ionic_force_x': 5.1735977828502655, 'ionic_force_y': -3.9379420280456543, 'ionic_force_z': -22.839519739151, 'radial_force': 6.5018075513630444, 'axial_force': -22.839519739151, 'contributions': [{'ion': 1355, 'force': [-0.23459890484809875, -0.226188063621521, -2.4711523056030273], 'magnitude': 2.4925472736358643, 'distance': 11.54110336303711, 'cosine_with_motion': -0.9796625124195689, 'motion_component': -2.441855024673414}, {'ion': 1380, 'force': [2.8447628021240234, 1.016716718673706, -3.0548858642578125], 'magnitude': 4.296360492706299, 'distance': 8.790602684020996, 'cosine_with_motion': -0.700017157373819, 'motion_component': -3.0075262584837823}, {'ion': 2434, 'force': [-1.8455193042755127, -1.5154215097427368, -1.5823023319244385], 'magnitude': 2.864633321762085, 'distance': 10.765507698059082, 'cosine_with_motion': -0.5936900479778674, 'motion_component': -1.700704341499744}, {'ion': 2443, 'force': [4.4089531898498535, -3.2130491733551025, -15.731179237365723], 'magnitude': 16.650300979614258, 'distance': 4.4653754234313965, 'cosine_with_motion': -0.9819078479353249, 'motion_component': -16.349062107802858}]}, 5896: {'frame': 5896, 'ionic_force': [-0.017224013805389404, -9.5826591377554, 4.59900638461113], 'ionic_force_magnitude': 10.629135079711451, 'motion_vector': [-0.24406814575195312, -1.3061408996582031, -1.6460342407226562], 'cosine_ionic_motion': 0.22016303928493244, 'ionic_motion_component': 2.3401426841193658, 'ionic_force_x': -0.017224013805389404, 'ionic_force_y': -9.5826591377554, 'ionic_force_z': 4.59900638461113, 'radial_force': 9.582674617091964, 'axial_force': 4.59900638461113, 'contributions': [{'ion': 1355, 'force': [-1.8489515781402588, -0.00621435372158885, -7.483148097991943], 'magnitude': 7.708188056945801, 'distance': 6.562856197357178, 'cosine_with_motion': 0.7835680717853275, 'motion_component': 6.039890199718068}, {'ion': 1380, 'force': [7.6192097663879395, 3.615647554397583, -0.6914269924163818], 'magnitude': 8.461874961853027, 'distance': 6.263769149780273, 'cosine_with_motion': -0.3041291046316781, 'motion_component': -2.5735026015322013}, {'ion': 1443, 'force': [-0.3091173768043518, 0.00013788617798127234, -2.191742420196533], 'magnitude': 2.2134335041046143, 'distance': 12.247171401977539, 'cosine_with_motion': 0.7865612401711798, 'motion_component': 1.7410010963815887}, {'ion': 2434, 'force': [-4.129177093505859, -3.6542301177978516, -0.2538600265979767], 'magnitude': 5.519777774810791, 'distance': 7.755472183227539, 'cosine_with_motion': 0.5308545741716985, 'motion_component': 2.930199253874088}, {'ion': 2443, 'force': [-1.3491877317428589, -9.538000106811523, 15.219183921813965], 'magnitude': 18.01158905029297, 'distance': 4.293317794799805, 'cosine_with_motion': -0.321873069029783, 'motion_component': -5.797445201812349}]}, 5897: {'frame': 5897, 'ionic_force': [1.8552783280611038, -2.173237666487694, -12.846055001020432], 'ionic_force_magnitude': 13.160020847964342, 'motion_vector': [-2.82208251953125, 5.449005126953125, 2.03216552734375], 'cosine_ionic_motion': -0.5076259578248576, 'ionic_motion_component': -6.680368187942994, 'ionic_force_x': 1.8552783280611038, 'ionic_force_y': -2.173237666487694, 'ionic_force_z': -12.846055001020432, 'radial_force': 2.8574498472613796, 'axial_force': -12.846055001020432, 'contributions': [{'ion': 1355, 'force': [-0.9138748049736023, -0.6297469139099121, -4.202837944030762], 'magnitude': 4.346906661987305, 'distance': 8.73934555053711, 'cosine_with_motion': -0.33429224387299245, 'motion_component': -1.4531370892927156}, {'ion': 1380, 'force': [9.447088241577148, 4.048842430114746, -5.9594407081604], 'magnitude': 11.880888938903809, 'distance': 5.286211967468262, 'cosine_with_motion': -0.21756311411583418, 'motion_component': -2.584843313608019}, {'ion': 1443, 'force': [-0.18578504025936127, -0.21087370812892914, -1.5908935070037842], 'magnitude': 1.615526556968689, 'distance': 14.335472106933594, 'cosine_with_motion': -0.36940491676610593, 'motion_component': -0.5967834414567519}, {'ion': 2434, 'force': [-1.8904106616973877, -2.4841415882110596, -0.7933556437492371], 'magnitude': 3.2208733558654785, 'distance': 10.152715682983398, 'cosine_with_motion': -0.47134032227528494, 'motion_component': -1.51812747847017}, {'ion': 2443, 'force': [-4.601739406585693, -2.897317886352539, -0.29952719807624817], 'magnitude': 5.446115493774414, 'distance': 7.807744979858398, 'cosine_with_motion': -0.09685378485089452, 'motion_component': -0.527476890051453}]}, 5898: {'frame': 5898, 'ionic_force': [-8.504436016082764, 11.964142084121704, -4.874931126832962], 'ionic_force_magnitude': 15.467096729899332, 'motion_vector': [1.28692626953125, 1.0255928039550781, -0.0074005126953125], 'cosine_ionic_motion': 0.053503810279040165, 'ionic_motion_component': 0.8275486090040964, 'ionic_force_x': -8.504436016082764, 'ionic_force_y': 11.964142084121704, 'ionic_force_z': -4.874931126832962, 'radial_force': 14.678764517516374, 'axial_force': -4.874931126832962, 'contributions': [{'ion': 1355, 'force': [-2.246494770050049, 1.9543259143829346, -3.1174850463867188], 'magnitude': 4.311013698577881, 'distance': 8.775650978088379, 'cosine_with_motion': -0.12173989718526873, 'motion_component': -0.5248223988331979}, {'ion': 1380, 'force': [1.3024711608886719, 6.837247848510742, -1.0843136310577393], 'magnitude': 7.044155597686768, 'distance': 6.865221977233887, 'cosine_with_motion': 0.7502090673975343, 'motion_component': 5.2845892541990045}, {'ion': 1443, 'force': [-0.6266984939575195, 0.5076103806495667, -1.6870962381362915], 'magnitude': 1.8699499368667603, 'distance': 13.32459545135498, 'cosine_with_motion': -0.08885512461797455, 'motion_component': -0.16615464063826718}, {'ion': 2434, 'force': [-3.711239814758301, -0.4314489960670471, -0.2661377489566803], 'magnitude': 3.745701313018799, 'distance': 9.414612770080566, 'cosine_with_motion': -0.8463017020136312, 'motion_component': -3.1699934160905885}, {'ion': 2443, 'force': [-3.2224740982055664, 3.096406936645508, 1.2801015377044678], 'magnitude': 4.6487345695495605, 'distance': 8.450874328613281, 'cosine_with_motion': -0.12822213597355978, 'motion_component': -0.5960707047619811}]}, 5899: {'frame': 5899, 'ionic_force': [-6.799471914768219, 9.492137521505356, -5.600397616624832], 'ionic_force_magnitude': 12.949824188427762, 'motion_vector': [-1.2925643920898438, 0.4482421875, -0.7178955078125], 'cosine_ionic_motion': 0.8528839683401198, 'ionic_motion_component': 11.04469744313314, 'ionic_force_x': -6.799471914768219, 'ionic_force_y': 9.492137521505356, 'ionic_force_z': -5.600397616624832, 'radial_force': 11.676193431375298, 'axial_force': -5.600397616624832, 'contributions': [{'ion': 1355, 'force': [-1.5860280990600586, 2.484849214553833, -3.0621752738952637], 'magnitude': 4.250514984130859, 'distance': 8.837882995605469, 'cosine_with_motion': 0.816529670001961, 'motion_component': 3.4706716480274054}, {'ion': 1380, 'force': [1.502514123916626, 3.8119521141052246, -0.36482638120651245], 'magnitude': 4.113590717315674, 'distance': 8.98376750946045, 'cosine_with_motion': 0.00448254038297453, 'motion_component': 0.01843933504465589}, {'ion': 1443, 'force': [-0.44899803400039673, 0.7380704879760742, -1.5459970235824585], 'magnitude': 1.7710037231445312, 'distance': 13.691761016845703, 'cosine_with_motion': 0.7386375500883181, 'motion_component': 1.3081298281740104}, {'ion': 2434, 'force': [-5.232437610626221, -0.4004041254520416, -0.13199836015701294], 'magnitude': 5.249395370483398, 'distance': 7.952696323394775, 'cosine_with_motion': 0.8234643314790869, 'motion_component': 4.322689741515248}, {'ion': 2443, 'force': [-1.034522294998169, 2.8576698303222656, -0.4954005777835846], 'magnitude': 3.079274892807007, 'distance': 10.383524894714355, 'cosine_with_motion': 0.6250715130958738, 'motion_component': 1.9247671286365629}]}, 5900: {'frame': 5900, 'ionic_force': [-6.1381120681762695, 8.840319886803627, -5.065477430820465], 'ionic_force_magnitude': 11.894819757552376, 'motion_vector': [1.6382980346679688, 0.11060333251953125, 0.5860443115234375], 'cosine_ionic_motion': -0.5808999323825219, 'ionic_motion_component': -6.909699992864462, 'ionic_force_x': -6.1381120681762695, 'ionic_force_y': 8.840319886803627, 'ionic_force_z': -5.065477430820465, 'radial_force': 10.762326675143571, 'axial_force': -5.065477430820465, 'contributions': [{'ion': 1355, 'force': [-1.8010727167129517, 2.0751216411590576, -2.528494358062744], 'magnitude': 3.734069585800171, 'distance': 9.429265022277832, 'cosine_with_motion': -0.6455951833243415, 'motion_component': -2.4106974082634594}, {'ion': 1380, 'force': [0.7935147881507874, 3.8666439056396484, -0.5172351598739624], 'magnitude': 3.980971336364746, 'distance': 9.132181167602539, 'cosine_with_motion': 0.20524595466575268, 'motion_component': 0.8170782686594613}, {'ion': 1443, 'force': [-0.539768397808075, 0.6087048649787903, -1.3261784315109253], 'magnitude': 1.555834412574768, 'distance': 14.607885360717773, 'cosine_with_motion': -0.5877023443381678, 'motion_component': -0.9143675408841645}, {'ion': 2434, 'force': [-3.400973320007324, 0.1036798506975174, -0.37451714277267456], 'magnitude': 3.423102617263794, 'distance': 9.848250389099121, 'cosine_with_motion': -0.9684545174849846, 'motion_component': -3.315119277919867}, {'ion': 2443, 'force': [-1.189812421798706, 2.1861696243286133, -0.3190523386001587], 'magnitude': 2.5093395709991455, 'distance': 11.502422332763672, 'cosine_with_motion': -0.4330199266346829, 'motion_component': -1.0865940833195076}]}, 5901: {'frame': 5901, 'ionic_force': [-7.439622104167938, 9.131087750196457, -4.992527484893799], 'ionic_force_magnitude': 12.792578756530364, 'motion_vector': [-0.2744865417480469, -0.7472152709960938, 0.6619415283203125], 'cosine_ionic_motion': -0.6105029271010953, 'ionic_motion_component': -7.809906776033078, 'ionic_force_x': -7.439622104167938, 'ionic_force_y': 9.131087750196457, 'ionic_force_z': -4.992527484893799, 'radial_force': 11.77814673684328, 'axial_force': -4.992527484893799, 'contributions': [{'ion': 1355, 'force': [-1.4037278890609741, 2.735112428665161, -2.956904888153076], 'magnitude': 4.265510082244873, 'distance': 8.822335243225098, 'cosine_with_motion': -0.8187622495734076, 'motion_component': -3.4924388454826705}, {'ion': 1380, 'force': [1.2992652654647827, 3.4894778728485107, -0.26489782333374023], 'magnitude': 3.7329232692718506, 'distance': 9.430712699890137, 'cosine_with_motion': -0.8123221702917955, 'motion_component': -3.032336416243023}, {'ion': 1443, 'force': [-0.41779905557632446, 0.741924524307251, -1.4480189085006714], 'magnitude': 1.6798115968704224, 'distance': 14.058492660522461, 'cosine_with_motion': -0.8039778328249968, 'motion_component': -1.3505312414997288}, {'ion': 2434, 'force': [-5.164675235748291, 0.30420610308647156, -0.35055652260780334], 'magnitude': 5.185489654541016, 'distance': 8.001550674438477, 'cosine_with_motion': 0.17849948460629902, 'motion_component': 0.9256072060184977}, {'ion': 2443, 'force': [-1.7526851892471313, 1.8603668212890625, 0.02785065770149231], 'magnitude': 2.5560996532440186, 'distance': 11.396726608276367, 'cosine_with_motion': -0.3365313831905415, 'motion_component': -0.8602077719029388}]}, 5902: {'frame': 5902, 'ionic_force': [-7.47670590877533, 10.180595852434635, -5.091444402933121], 'ionic_force_magnitude': 13.618680892989754, 'motion_vector': [-0.6989402770996094, 0.07197189331054688, -0.5127105712890625], 'cosine_ionic_motion': 0.7233805888715068, 'ionic_motion_component': 9.851489404024067, 'ionic_force_x': -7.47670590877533, 'ionic_force_y': 10.180595852434635, 'ionic_force_z': -5.091444402933121, 'radial_force': 12.631138632638201, 'axial_force': -5.091444402933121, 'contributions': [{'ion': 1355, 'force': [-2.3436784744262695, 3.635133743286133, -3.490668773651123], 'magnitude': 5.558038711547852, 'distance': 7.728732109069824, 'cosine_with_motion': 0.7631541126482841, 'motion_component': 4.241640120977877}, {'ion': 1380, 'force': [1.7799241542816162, 3.8899707794189453, -0.24371981620788574], 'magnitude': 4.284787178039551, 'distance': 8.802467346191406, 'cosine_with_motion': -0.2251530332435537, 'motion_component': -0.9647328522041647}, {'ion': 1443, 'force': [-0.6318591833114624, 0.8132873177528381, -1.8050473928451538], 'magnitude': 2.078191041946411, 'distance': 12.639395713806152, 'cosine_with_motion': 0.7886742332344485, 'motion_component': 1.6390157971740118}, {'ion': 2434, 'force': [-4.041162490844727, 0.0778370276093483, 0.15670618414878845], 'magnitude': 4.044948577880859, 'distance': 9.059673309326172, 'cosine_with_motion': 0.7815590684252294, 'motion_component': 3.161366311019386}, {'ion': 2443, 'force': [-2.2399299144744873, 1.7643669843673706, 0.2912853956222534], 'magnitude': 2.866203784942627, 'distance': 10.762557983398438, 'cosine_with_motion': 0.6190068769033602, 'motion_component': 1.7741998450811902}]}, 5903: {'frame': 5903, 'ionic_force': [-7.226976692676544, 9.150095321238041, -4.231179058551788], 'ionic_force_magnitude': 12.403882969850992, 'motion_vector': [-2.064189910888672, -0.9773674011230469, 0.5256500244140625], 'cosine_ionic_motion': 0.12902546839686596, 'ionic_motion_component': 1.600416810124933, 'ionic_force_x': -7.226976692676544, 'ionic_force_y': 9.150095321238041, 'ionic_force_z': -4.231179058551788, 'radial_force': 11.65990722536986, 'axial_force': -4.231179058551788, 'contributions': [{'ion': 1355, 'force': [-1.8546229600906372, 2.477461338043213, -2.9006059169769287], 'magnitude': 4.241574764251709, 'distance': 8.847192764282227, 'cosine_with_motion': -0.011850426762347991, 'motion_component': -0.05026446999784895}, {'ion': 1380, 'force': [1.4170900583267212, 4.401101589202881, -0.24274271726608276], 'magnitude': 4.629985332489014, 'distance': 8.467968940734863, 'cosine_with_motion': -0.6777590970009262, 'motion_component': -3.1380146253485997}, {'ion': 1443, 'force': [-0.5996553301811218, 0.7718545794487, -1.4985142946243286], 'magnitude': 1.7891035079956055, 'distance': 13.62232780456543, 'cosine_with_motion': -0.07256903406377582, 'motion_component': -0.12983350805516558}, {'ion': 2434, 'force': [-4.2714080810546875, 0.0717788115143776, 0.005224108695983887], 'magnitude': 4.272014141082764, 'distance': 8.815616607666016, 'cosine_with_motion': 0.8739216207863854, 'motion_component': 3.733405692233334}, {'ion': 2443, 'force': [-1.9183803796768188, 1.4278990030288696, 0.40545976161956787], 'magnitude': 2.4255878925323486, 'distance': 11.69931697845459, 'cosine_with_motion': 0.4885923536268643, 'motion_component': 1.1851236810123673}]}, 5904: {'frame': 5904, 'ionic_force': [-9.568521454930305, 7.556034505367279, -3.6204235684126616], 'ionic_force_magnitude': 12.718401121779435, 'motion_vector': [0.26805877685546875, -0.65460205078125, 0.54949951171875], 'cosine_ionic_motion': -0.8339597165242312, 'ionic_motion_component': -10.606634194160641, 'ionic_force_x': -9.568521454930305, 'ionic_force_y': 7.556034505367279, 'ionic_force_z': -3.6204235684126616, 'radial_force': 12.192221302115644, 'axial_force': -3.6204235684126616, 'contributions': [{'ion': 1355, 'force': [-2.7520177364349365, 2.0397398471832275, -2.4019126892089844], 'magnitude': 4.183697700500488, 'distance': 8.908178329467773, 'cosine_with_motion': -0.9053642438427174, 'motion_component': -3.787770130145411}, {'ion': 1380, 'force': [-0.21680445969104767, 5.097675800323486, -0.02414863370358944], 'magnitude': 5.102341175079346, 'distance': 8.066484451293945, 'cosine_with_motion': -0.7457649127659219, 'motion_component': -3.8051470526533926}, {'ion': 1443, 'force': [-0.8819059133529663, 0.5921956896781921, -1.4838796854019165], 'magnitude': 1.8249253034591675, 'distance': 13.487966537475586, 'cosine_with_motion': -0.8806016873471738, 'motion_component': -1.6070323817126706}, {'ion': 2434, 'force': [-3.755582809448242, -0.6733697652816772, -0.06396784633398056], 'magnitude': 3.8160085678100586, 'distance': 9.327481269836426, 'cosine_with_motion': -0.17585336726810966, 'motion_component': -0.671057946384932}, {'ion': 2443, 'force': [-1.9622105360031128, 0.4997929334640503, 0.3534852862358093], 'magnitude': 2.0554840564727783, 'distance': 12.709017753601074, 'cosine_with_motion': -0.3578848286087576, 'motion_component': -0.7356265858207962}]}, 5905: {'frame': 5905, 'ionic_force': [-9.992130100727081, 6.58165055513382, -3.931290879845619], 'ionic_force_magnitude': 12.594277905529433, 'motion_vector': [0.7903480529785156, -0.9876708984375, -0.41739654541015625], 'cosine_ionic_motion': -0.7604122752570438, 'ionic_motion_component': -9.576843517363152, 'ionic_force_x': -9.992130100727081, 'ionic_force_y': 6.58165055513382, 'ionic_force_z': -3.931290879845619, 'radial_force': 11.964981737543502, 'axial_force': -3.931290879845619, 'contributions': [{'ion': 1355, 'force': [-3.319589138031006, 2.096099615097046, -2.7997121810913086], 'magnitude': 4.822000980377197, 'distance': 8.29765510559082, 'cosine_with_motion': -0.5488417217053617, 'motion_component': -2.6465153476760293}, {'ion': 1380, 'force': [-1.1027723550796509, 4.649133205413818, -0.03528514876961708], 'magnitude': 4.778262138366699, 'distance': 8.335545539855957, 'cosine_with_motion': -0.8560484604784877, 'motion_component': -4.090424162976559}, {'ion': 1443, 'force': [-0.942359983921051, 0.5759227275848389, -1.6433050632476807], 'magnitude': 1.9799445867538452, 'distance': 12.949187278747559, 'cosine_with_motion': -0.23800220727946045, 'motion_component': -0.47123119947199754}, {'ion': 2434, 'force': [-2.8171496391296387, -1.0690206289291382, 0.05009468272328377], 'magnitude': 3.0135769844055176, 'distance': 10.496098518371582, 'cosine_with_motion': -0.29684243476094296, 'motion_component': -0.8945575505990111}, {'ion': 2443, 'force': [-1.8102589845657349, 0.32951563596725464, 0.49691683053970337], 'magnitude': 1.9059234857559204, 'distance': 13.198248863220215, 'cosine_with_motion': -0.7734389045849858, 'motion_component': -1.4741154031700958}]}, 5906: {'frame': 5906, 'ionic_force': [-10.922582864761353, 10.523097217082977, -6.046317458152771], 'ionic_force_magnitude': 16.327778363345114, 'motion_vector': [1.9758110046386719, 3.4515724182128906, -0.8893280029296875], 'cosine_ionic_motion': 0.3023330582001712, 'ionic_motion_component': 4.936427166204714, 'ionic_force_x': -10.922582864761353, 'ionic_force_y': 10.523097217082977, 'ionic_force_z': -6.046317458152771, 'radial_force': 15.1670165648277, 'axial_force': -6.046317458152771, 'contributions': [{'ion': 1355, 'force': [-4.033276081085205, 1.9656189680099487, -3.9555554389953613], 'magnitude': 5.981420516967773, 'distance': 7.450181484222412, 'cosine_with_motion': 0.09571965613329209, 'motion_component': 0.5725395255051566}, {'ion': 1380, 'force': [0.23750650882720947, 8.032539367675781, -0.7383502721786499], 'magnitude': 8.06989860534668, 'distance': 6.414089202880859, 'cosine_with_motion': 0.8772632129877416, 'motion_component': 7.079424943052482}, {'ion': 1443, 'force': [-1.2005337476730347, 0.7920025587081909, -2.096895217895508], 'magnitude': 2.542738437652588, 'distance': 11.426630973815918, 'cosine_with_motion': 0.2148583606219969, 'motion_component': 0.5463286174781139}, {'ion': 2434, 'force': [-3.1640639305114746, -0.9320102334022522, 0.2620435059070587], 'magnitude': 3.308868408203125, 'distance': 10.016806602478027, 'cosine_with_motion': -0.7194509242662153, 'motion_component': -2.3805684658359643}, {'ion': 2443, 'force': [-2.7622156143188477, 0.6649465560913086, 0.48243996500968933], 'magnitude': 2.881793975830078, 'distance': 10.733406066894531, 'cosine_with_motion': -0.30581543469071415, 'motion_component': -0.8812971210839531}]}, 5907: {'frame': 5907, 'ionic_force': [-9.553559362888336, 8.830352172255516, -5.354349387693219], 'ionic_force_magnitude': 14.068215002329891, 'motion_vector': [-1.1595115661621094, -0.7659034729003906, 0.1236724853515625], 'cosine_ionic_motion': 0.18607521899512322, 'ionic_motion_component': 2.6177461874290127, 'ionic_force_x': -9.553559362888336, 'ionic_force_y': 8.830352172255516, 'ionic_force_z': -5.354349387693219, 'radial_force': 13.009443338832337, 'axial_force': -5.354349387693219, 'contributions': [{'ion': 1355, 'force': [-1.5680482387542725, 3.1532657146453857, -3.071322202682495], 'magnitude': 4.672780513763428, 'distance': 8.429102897644043, 'cosine_with_motion': -0.14983111096125093, 'motion_component': -0.7001279323548903}, {'ion': 1380, 'force': [0.9171464443206787, 3.123924732208252, -0.38423049449920654], 'magnitude': 3.278367757797241, 'distance': 10.063294410705566, 'cosine_with_motion': -0.7660238977833006, 'motion_component': -2.5113081942758813}, {'ion': 1443, 'force': [-0.6362531781196594, 1.28103506565094, -1.8257994651794434], 'magnitude': 2.3193562030792236, 'distance': 11.964245796203613, 'cosine_with_motion': -0.14500558336337774, 'motion_component': -0.3363195816363458}, {'ion': 2434, 'force': [-5.875592231750488, -0.22285892069339752, -0.07418480515480042], 'magnitude': 5.880284786224365, 'distance': 7.51397705078125, 'cosine_with_motion': 0.8501420158589348, 'motion_component': 4.99907747936747}, {'ion': 2443, 'force': [-2.3908121585845947, 1.494985580444336, 0.0011875798227265477], 'magnitude': 2.8197457790374756, 'distance': 10.850857734680176, 'cosine_with_motion': 0.4136630808352814, 'motion_component': 1.1664247125823328}]}, 5908: {'frame': 5908, 'ionic_force': [-11.456575185060501, 10.54627639055252, -7.669879510998726], 'ionic_force_magnitude': 17.35811373364363, 'motion_vector': [0.8431854248046875, 0.49897003173828125, 0.0274658203125], 'cosine_ionic_motion': -0.2708674020063873, 'ionic_motion_component': -4.701747170763442, 'ionic_force_x': -11.456575185060501, 'ionic_force_y': 10.54627639055252, 'ionic_force_z': -7.669879510998726, 'radial_force': 15.571674947701341, 'axial_force': -7.669879510998726, 'contributions': [{'ion': 1327, 'force': [-0.42327919602394104, 0.5680921673774719, -1.5069403648376465], 'magnitude': 1.6651616096496582, 'distance': 14.120200157165527, 'cosine_with_motion': -0.070357865144216, 'motion_component': -0.11715721735563277}, {'ion': 1355, 'force': [-3.401942491531372, 4.668416976928711, -2.9111828804016113], 'magnitude': 6.468563556671143, 'distance': 7.164157390594482, 'cosine_with_motion': -0.0976360435702645, 'motion_component': -0.6315649612756662}, {'ion': 1380, 'force': [0.7152265310287476, 4.2912068367004395, -0.36868032813072205], 'magnitude': 4.365996837615967, 'distance': 8.72021770477295, 'cosine_with_motion': 0.6389165298771069, 'motion_component': 2.7895076882816205}, {'ion': 1443, 'force': [-1.2062010765075684, 1.3956199884414673, -2.323375701904297], 'magnitude': 2.9666059017181396, 'distance': 10.578866004943848, 'cosine_with_motion': -0.13223198004315548, 'motion_component': -0.3922801783022507}, {'ion': 2434, 'force': [-4.892893314361572, -1.0576077699661255, -0.7788661122322083], 'magnitude': 5.066120147705078, 'distance': 8.095269203186035, 'cosine_with_motion': -0.9414330547444434, 'motion_component': -4.7694128038131645}, {'ion': 2443, 'force': [-2.247485637664795, 0.6805481910705566, 0.2191658765077591], 'magnitude': 2.3584680557250977, 'distance': 11.864625930786133, 'cosine_with_motion': -0.670282434103589, 'motion_component': -1.5808396584777453}]}, 5909: {'frame': 5909, 'ionic_force': [-11.318663328886032, 12.406723007559776, -6.972444713115692], 'ionic_force_magnitude': 18.183891239677976, 'motion_vector': [-2.2848129272460938, -0.2534599304199219, 0.33966064453125], 'cosine_ionic_motion': 0.4815507907179075, 'ionic_motion_component': 8.756467204795362, 'ionic_force_x': -11.318663328886032, 'ionic_force_y': 12.406723007559776, 'ionic_force_z': -6.972444713115692, 'radial_force': 16.794014271131918, 'axial_force': -6.972444713115692, 'contributions': [{'ion': 1327, 'force': [-0.33883413672447205, 0.5817093849182129, -1.368337631225586], 'magnitude': 1.5249727964401245, 'distance': 14.754958152770996, 'cosine_with_motion': 0.04570411215886815, 'motion_component': 0.06969753108227472}, {'ion': 1355, 'force': [-2.4924542903900146, 5.4414496421813965, -2.8278679847717285], 'magnitude': 6.6195573806762695, 'distance': 7.081977844238281, 'cosine_with_motion': 0.21811155801574825, 'motion_component': 1.443801974025039}, {'ion': 1380, 'force': [0.682213544845581, 3.278224229812622, -0.35480713844299316], 'magnitude': 3.3672032356262207, 'distance': 9.929659843444824, 'cosine_with_motion': -0.3207989777487072, 'motion_component': -1.0801953509631037}, {'ion': 1443, 'force': [-0.9330054521560669, 1.539467692375183, -2.1729485988616943], 'magnitude': 2.821730852127075, 'distance': 10.847040176391602, 'cosine_with_motion': 0.1530378634036318, 'motion_component': 0.431831675924557}, {'ion': 2434, 'force': [-6.0750651359558105, -0.0652710348367691, -0.6163405776023865], 'magnitude': 6.1065993309021, 'distance': 7.3734259605407715, 'cosine_with_motion': 0.9645644793719439, 'motion_component': 5.890208570060275}, {'ion': 2443, 'force': [-2.161517858505249, 1.6311430931091309, 0.3678572177886963], 'magnitude': 2.732783555984497, 'distance': 11.0221529006958, 'cosine_with_motion': 0.732265367618633, 'motion_component': 2.0011227836022023}]}, 5910: {'frame': 5910, 'ionic_force': [-10.408794045448303, 10.508824622258544, -5.274085454642773], 'ionic_force_magnitude': 15.703323399994726, 'motion_vector': [1.3806076049804688, -0.5164985656738281, -0.46323394775390625], 'cosine_ionic_motion': -0.7152705127165517, 'ionic_motion_component': -11.232124179668052, 'ionic_force_x': -10.408794045448303, 'ionic_force_y': 10.508824622258544, 'ionic_force_z': -5.274085454642773, 'radial_force': 14.791159130438272, 'axial_force': -5.274085454642773, 'contributions': [{'ion': 1327, 'force': [-0.6121020317077637, 0.6046913862228394, -1.447232961654663], 'magnitude': 1.683687448501587, 'distance': 14.042301177978516, 'cosine_with_motion': -0.1871934547506613, 'motion_component': -0.3151752919328601}, {'ion': 1355, 'force': [</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>{5997: {'frame': 5997, 'ionic_force': [9.381639122962952, 3.428868383169174, -11.025252528488636], 'ionic_force_magnitude': 14.877112768933067, 'motion_vector': [0.7771873474121094, 0.3831329345703125, 0.82928466796875], 'cosine_ionic_motion': -0.03015511111987929, 'ionic_motion_component': -0.44862098869015166, 'ionic_force_x': 9.381639122962952, 'ionic_force_y': 3.428868383169174, 'ionic_force_z': -11.025252528488636, 'radial_force': 9.988608062318105, 'axial_force': -11.025252528488636, 'contributions': [{'ion': 1327, 'force': [0.5210571885108948, -0.15596595406532288, -1.7473162412643433], 'magnitude': 1.8300108909606934, 'distance': 13.469212532043457, 'directional_contribution': -0.9203210783935374}, {'ion': 1380, 'force': [3.0363898277282715, 0.8332290053367615, -0.6519385576248169], 'magnitude': 3.2154250144958496, 'distance': 10.161314010620117, 'directional_contribution': 1.7829460134996058}, {'ion': 1443, 'force': [2.586791753768921, -0.8877150416374207, -4.0297532081604], 'magnitude': 4.8701581954956055, 'distance': 8.256528854370117, 'directional_contribution': -1.3936340184841658}, {'ion': 1476, 'force': [1.3487483263015747, -1.712496280670166, -0.039044089615345], 'magnitude': 2.180204153060913, 'distance': 12.340150833129883, 'directional_contribution': 0.2999352078664286}, {'ion': 2434, 'force': [-0.48151785135269165, -7.0847249031066895, -1.291944980621338], 'magnitude': 7.217638969421387, 'distance': 6.7822136878967285, 'directional_contribution': -3.4684537373107496}, {'ion': 2443, 'force': [2.3701698780059814, 12.436541557312012, -3.2652554512023926], 'magnitude': 13.074676513671875, 'distance': 5.039106845855713, 'directional_contribution': 3.250906495401992}]}, 5998: {'frame': 5998, 'ionic_force': [10.780787527561188, 0.28440017998218536, -7.232492357492447], 'ionic_force_magnitude': 12.985191907629991, 'motion_vector': [-0.7672195434570312, 2.2775001525878906, -1.0481185913085938], 'cosine_ionic_motion': -0.001263009889529832, 'ionic_motion_component': -0.016400425796779423, 'ionic_force_x': 10.780787527561188, 'ionic_force_y': 0.28440017998218536, 'ionic_force_z': -7.232492357492447, 'radial_force': 10.784538153152075, 'axial_force': -7.232492357492447, 'contributions': [{'ion': 1327, 'force': [0.6711025238037109, -0.13265840709209442, -1.804991602897644], 'magnitude': 1.9302775859832764, 'distance': 13.114724159240723, 'directional_contribution': 0.40994944295757296}, {'ion': 1380, 'force': [2.8374791145324707, 0.6517823338508606, -0.4846545159816742], 'magnitude': 2.95143985748291, 'distance': 10.606010437011719, 'directional_contribution': -0.07039245638239944}, {'ion': 1443, 'force': [3.076692581176758, -0.8291545510292053, -3.541635036468506], 'magnitude': 4.764106750488281, 'distance': 8.347920417785645, 'directional_contribution': -0.20475667152368615}, {'ion': 1476, 'force': [1.263065218925476, -1.5566960573196411, 0.03140932321548462], 'magnitude': 2.004899740219116, 'distance': 12.868345260620117, 'directional_contribution': -1.7343919836517667}, {'ion': 2434, 'force': [-0.50923091173172, -8.268269538879395, -0.3708587884902954], 'magnitude': 8.29223346710205, 'distance': 6.327516555786133, 'directional_contribution': -6.88501421705325}, {'ion': 2443, 'force': [3.441679000854492, 10.41939640045166, -1.061761736869812], 'magnitude': 11.024351119995117, 'distance': 5.487727642059326, 'directional_contribution': 8.46820552903441}]}, 5999: {'frame': 5999, 'ionic_force': [6.903971970081329, -9.943094223737717, -11.683605313301086], 'ionic_force_magnitude': 16.8236911771107, 'motion_vector': [-1.3753700256347656, -4.601753234863281, -0.27584075927734375], 'cosine_ionic_motion': 0.48783230159410307, 'ionic_motion_component': 8.207139988238318, 'ionic_force_x': 6.903971970081329, 'ionic_force_y': -9.943094223737717, 'ionic_force_z': -11.683605313301086, 'radial_force': 12.104955667237903, 'axial_force': -11.683605313301086, 'contributions': [{'ion': 1327, 'force': [0.45604217052459717, 0.1768944263458252, -1.7557339668273926], 'magnitude': 1.822599172592163, 'distance': 13.49657154083252, 'directional_contribution': -0.19891637349124203}, {'ion': 1380, 'force': [2.0143558979034424, 1.382273554801941, -0.6717885732650757], 'magnitude': 2.5336947441101074, 'distance': 11.447005271911621, 'directional_contribution': -1.8595757916178344}, {'ion': 1443, 'force': [2.022075653076172, 0.4375012218952179, -3.6579012870788574], 'magnitude': 4.202432632446289, 'distance': 8.888298988342285, 'directional_contribution': -0.7868486203393044}, {'ion': 1476, 'force': [2.0586459636688232, -1.9142779111862183, -0.18536603450775146], 'magnitude': 2.8172404766082764, 'distance': 10.855681419372559, 'directional_contribution': 1.2531714830432583}, {'ion': 2434, 'force': [0.3335014283657074, -16.288362503051758, -3.843754291534424], 'magnitude': 16.73906898498535, 'distance': 4.453519821166992, 'directional_contribution': 15.705598484353184}, {'ion': 2443, 'force': [0.01935085654258728, 6.262876987457275, -1.5690611600875854], 'magnitude': 6.456466197967529, 'distance': 7.170866012573242, 'directional_contribution': -5.90628947647706}]}, 6000: {'frame': 6000, 'ionic_force': [5.517950534820557, 7.6139421463012695, -19.801055759191513], 'ionic_force_magnitude': 21.920349045819517, 'motion_vector': [-4.781524658203125, 2.4392776489257812, 0.5065383911132812], 'cosine_ionic_motion': -0.1509624024908215, 'ionic_motion_component': -3.3091485553943008, 'ionic_force_x': 5.517950534820557, 'ionic_force_y': 7.6139421463012695, 'ionic_force_z': -19.801055759191513, 'radial_force': 9.403185264151146, 'axial_force': -19.801055759191513, 'contributions': [{'ion': 1327, 'force': [0.27228718996047974, -0.34001588821411133, -1.6231095790863037], 'magnitude': 1.6805462837219238, 'distance': 14.055419921875, 'directional_contribution': -0.5477954425251834}, {'ion': 1380, 'force': [3.8357651233673096, 0.6248253583908081, -1.3770771026611328], 'magnitude': 4.123086452484131, 'distance': 8.973416328430176, 'directional_contribution': -3.248412278296371}, {'ion': 1443, 'force': [1.5023193359375, -1.549290657043457, -3.5091614723205566], 'magnitude': 4.119645595550537, 'distance': 8.977163314819336, 'directional_contribution': -2.362933013233306}, {'ion': 1476, 'force': [1.1409306526184082, -1.8393505811691284, -0.37553462386131287], 'magnitude': 2.1968066692352295, 'distance': 12.293431282043457, 'directional_contribution': -1.8792655123287687}, {'ion': 2434, 'force': [-0.8899776935577393, -4.16619348526001, -0.9849853515625], 'magnitude': 4.3725762367248535, 'distance': 8.713654518127441, 'directional_contribution': -1.1881359802195561}, {'ion': 2443, 'force': [-0.3433740735054016, 14.883967399597168, -11.931187629699707], 'magnitude': 19.07887840270996, 'distance': 4.17150354385376, 'directional_contribution': 5.917393768109569}]}, 6001: {'frame': 6001, 'ionic_force': [-5.739471256732941, 1.5717533826828003, -13.330579981207848], 'ionic_force_magnitude': 14.598503404055426, 'motion_vector': [1.7098503112792969, -0.131500244140625, 0.37758636474609375], 'cosine_ionic_motion': -0.5872436292990687, 'ionic_motion_component': -8.572878121332318, 'ionic_force_x': -5.739471256732941, 'ionic_force_y': 1.5717533826828003, 'ionic_force_z': -13.330579981207848, 'radial_force': 5.9507931406526335, 'axial_force': -13.330579981207848, 'contributions': [{'ion': 1327, 'force': [-0.37006884813308716, -0.10675269365310669, -1.939383625984192], 'magnitude': 1.9772597551345825, 'distance': 12.957976341247559, 'directional_contribution': -0.7693779149979432}, {'ion': 1380, 'force': [4.8833489418029785, 6.641224384307861, -3.6172406673431396], 'magnitude': 9.002077102661133, 'distance': 6.0729217529296875, 'directional_contribution': 3.479917939183366}, {'ion': 1443, 'force': [-1.8360635042190552, -0.6234139800071716, -6.40214204788208], 'magnitude': 6.689334392547607, 'distance': 7.044944763183594, 'directional_contribution': -3.1177967411055856}, {'ion': 1476, 'force': [-1.7837971448898315, -6.105370998382568, 0.018659725785255432], 'magnitude': 6.360647678375244, 'distance': 7.224676132202148, 'directional_contribution': -1.2757137265881193}, {'ion': 2434, 'force': [-2.968780040740967, -1.7256089448928833, -0.42890286445617676], 'magnitude': 3.460540294647217, 'distance': 9.79483413696289, 'directional_contribution': -2.853797203169603}, {'ion': 2443, 'force': [-3.6641106605529785, 3.491675615310669, -0.9615705013275146], 'magnitude': 5.151905059814453, 'distance': 8.027588844299316, 'directional_contribution': -4.036110359738709}]}, 6002: {'frame': 6002, 'ionic_force': [-2.454675856977701, -1.9141423031687737, -12.883132107555866], 'ionic_force_magnitude': 13.253847261091638, 'motion_vector': [-0.4403953552246094, 2.3236732482910156, 2.6926345825195312], 'cosine_ionic_motion': -0.801199510453789, 'ionic_motion_component': -10.618975937215913, 'ionic_force_x': -2.454675856977701, 'ionic_force_y': -1.9141423031687737, 'ionic_force_z': -12.883132107555866, 'radial_force': 3.1127759828823964, 'axial_force': -12.883132107555866, 'contributions': [{'ion': 1327, 'force': [-0.07753433287143707, -0.08069079369306564, -2.0556859970092773], 'magnitude': 2.058729648590088, 'distance': 12.698995590209961, 'directional_contribution': -1.587295673869313}, {'ion': 1380, 'force': [6.697790622711182, 2.4995415210723877, -1.7771592140197754], 'magnitude': 7.366573333740234, 'distance': 6.713303565979004, 'directional_contribution': -0.5376398875308581}, {'ion': 1443, 'force': [0.05283843353390694, -1.0870180130004883, -6.450309753417969], 'magnitude': 6.54147481918335, 'distance': 7.124119281768799, 'directional_contribution': -5.5576264474365935}, {'ion': 1476, 'force': [0.09511121362447739, -5.949183940887451, -0.06667114049196243], 'magnitude': 5.950317859649658, 'distance': 7.469627857208252, 'directional_contribution': -3.919117047338237}, {'ion': 2434, 'force': [-3.142949104309082, -4.085984230041504, -0.727785587310791], 'magnitude': 5.206060409545898, 'distance': 7.985726356506348, 'directional_contribution': -2.8098630678356358}, {'ion': 2443, 'force': [-6.079932689666748, 6.789193153381348, -1.8055204153060913], 'magnitude': 9.29078197479248, 'distance': 5.977820873260498, 'directional_contribution': 3.792566441006535}]}, 6003: {'frame': 6003, 'ionic_force': [-7.239282563328743, 3.985614240169525, -13.104669943451881], 'ionic_force_magnitude': 15.492730786726039, 'motion_vector': [-6.120677947998047, -2.7395401000976562, -2.5673294067382812], 'cosine_ionic_motion': 0.6025856708493228, 'ionic_motion_component': 9.335697574407266, 'ionic_force_x': -7.239282563328743, 'ionic_force_y': 3.985614240169525, 'ionic_force_z': -13.104669943451881, 'radial_force': 8.263917527611083, 'axial_force': -13.104669943451881, 'contributions': [{'ion': 1327, 'force': [-0.19644558429718018, 0.4891625642776489, -3.0373945236206055], 'magnitude': 3.082796812057495, 'distance': 10.377592086791992, 'directional_contribution': 1.0668251955116084}, {'ion': 1341, 'force': [-0.06385579705238342, 0.24247795343399048, -1.6175693273544312], 'magnitude': 1.6368883848190308, 'distance': 14.241623878479004, 'directional_contribution': 0.5402714950801091}, {'ion': 1380, 'force': [2.977800130844116, 4.4187140464782715, 0.1744322031736374], 'magnitude': 5.331299304962158, 'distance': 7.891371726989746, 'directional_contribution': -4.286527396978535}, {'ion': 1443, 'force': [-1.4516021013259888, 3.280688762664795, -14.232921600341797], 'magnitude': 14.678083419799805, 'distance': 4.755918025970459, 'directional_contribution': 5.074581030755816}, {'ion': 1476, 'force': [-0.12233380973339081, -6.026616096496582, 3.0402510166168213], 'magnitude': 6.751162528991699, 'distance': 7.012611389160156, 'directional_contribution': 1.3165731033157444}, {'ion': 2434, 'force': [-5.042224407196045, -2.669969320297241, 1.6620091199874878], 'magnitude': 5.94264554977417, 'distance': 7.474448204040527, 'directional_contribution': 4.722456452694576}, {'ion': 2443, 'force': [-3.340620994567871, 4.251156330108643, 0.9065231680870056], 'magnitude': 5.48214054107666, 'distance': 7.782049179077148, 'directional_contribution': 0.9015175947396639}]}, 6004: {'frame': 6004, 'ionic_force': [-13.262407958507538, 11.088155046105385, -8.382136479020119], 'ionic_force_magnitude': 19.2119457405354, 'motion_vector': [-0.223419189453125, 2.570514678955078, -0.7060775756835938], 'cosine_ionic_motion': 0.7274053216976897, 'ionic_motion_component': 13.974871571832711, 'ionic_force_x': -13.262407958507538, 'ionic_force_y': 11.088155046105385, 'ionic_force_z': -8.382136479020119, 'radial_force': 17.28695019904773, 'axial_force': -8.382136479020119, 'contributions': [{'ion': 1327, 'force': [-0.7501986622810364, -0.13029859960079193, -1.3091551065444946], 'magnitude': 1.5144842863082886, 'distance': 14.805962562561035, 'directional_contribution': 0.28299782470996293}, {'ion': 1380, 'force': [-4.599451065063477, 13.990073204040527, -4.257678985595703], 'magnitude': 15.329870223999023, 'distance': 4.653715133666992, 'directional_contribution': 14.95120619354374}, {'ion': 1443, 'force': [-2.4518744945526123, -0.6125720739364624, -2.5525479316711426], 'magnitude': 3.59199595451355, 'distance': 9.613933563232422, 'directional_contribution': 0.28988654720289553}, {'ion': 1476, 'force': [-1.4830362796783447, -2.197493553161621, 0.07560582458972931], 'magnitude': 2.652186155319214, 'distance': 11.188375473022461, 'directional_contribution': -2.0076974384426522}, {'ion': 2434, 'force': [-1.6397267580032349, -0.897940993309021, -0.09315349161624908], 'magnitude': 1.8718117475509644, 'distance': 13.317967414855957, 'directional_contribution': -0.7013085318627432}, {'ion': 2443, 'force': [-2.338120698928833, 0.9363870620727539, -0.2452067881822586], 'magnitude': 2.530564308166504, 'distance': 11.454083442687988, 'directional_contribution': 1.15978683758948}]}, 6005: {'frame': 6005, 'ionic_force': [-11.751091122627258, 3.513936460018158, -5.2574396431446075], 'ionic_force_magnitude': 13.344533098562968, 'motion_vector': [-0.2879486083984375, 0.21361923217773438, 0.6275177001953125], 'cosine_ionic_motion': 0.08660157332649941, 'ionic_motion_component': 1.1556575616430993, 'ionic_force_x': -11.751091122627258, 'ionic_force_y': 3.513936460018158, 'ionic_force_z': -5.2574396431446075, 'radial_force': 12.265231021767756, 'axial_force': -5.2574396431446075, 'contributions': [{'ion': 1380, 'force': [-1.5290939807891846, 5.18525505065918, -2.7910616397857666], 'magnitude': 6.0839972496032715, 'distance': 7.387109279632568, 'directional_contribution': -0.2815329896728045}, {'ion': 1443, 'force': [-2.1018567085266113, 0.29880401492118835, -2.3693599700927734], 'magnitude': 3.181344509124756, 'distance': 10.215596199035645, 'directional_contribution': -1.1314989344353963}, {'ion': 1476, 'force': [-1.9276835918426514, -2.4968819618225098, -0.44340747594833374], 'magnitude': 3.185434579849243, 'distance': 10.20903491973877, 'directional_contribution': -0.3549837172213053}, {'ion': 2434, 'force': [-4.488006591796875, -0.4852888882160187, 0.6003507971763611], 'magnitude': 4.553913593292236, 'distance': 8.538402557373047, 'directional_contribution': 2.165951055586958}, {'ion': 2443, 'force': [-1.704450249671936, 1.0120482444763184, -0.25396135449409485], 'magnitude': 1.9984716176986694, 'distance': 12.88902473449707, 'directional_contribution': 0.7577219696746003}]}, 6006: {'frame': 6006, 'ionic_force': [-11.669181168079376, 5.09692008793354, -6.636843234300613], 'ionic_force_magnitude': 14.35952894885207, 'motion_vector': [3.3086013793945312, -2.3047142028808594, -0.0504608154296875], 'cosine_ionic_motion': -0.8638428873633073, 'ionic_motion_component': -12.404376948353368, 'ionic_force_x': -11.669181168079376, 'ionic_force_y': 5.09692008793354, 'ionic_force_z': -6.636843234300613, 'radial_force': 12.733749782221999, 'axial_force': -6.636843234300613, 'contributions': [{'ion': 1327, 'force': [-0.7694267630577087, 0.20096524059772491, -1.2440012693405151], 'magnitude': 1.4764631986618042, 'distance': 14.995388984680176, 'directional_contribution': -0.7305931674763221}, {'ion': 1380, 'force': [-1.6209291219711304, 5.998019695281982, -2.354433298110962], 'magnitude': 6.644321918487549, 'distance': 7.06876802444458, 'directional_contribution': -4.7285551762152656}, {'ion': 1443, 'force': [-2.171865224838257, 0.4668664336204529, -2.2036139965057373], 'magnitude': 3.129037857055664, 'distance': 10.300626754760742, 'directional_contribution': -2.0212334267683243}, {'ion': 1476, 'force': [-3.098361015319824, -2.754167318344116, -0.36075103282928467], 'magnitude': 4.161180019378662, 'distance': 8.93224811553955, 'directional_contribution': -0.9635374656188068}, {'ion': 2434, 'force': [-2.578646183013916, 0.22548645734786987, -0.3415878117084503], 'magnitude': 2.6109275817871094, 'distance': 11.276430130004883, 'directional_contribution': -2.240333857713003}, {'ion': 2443, 'force': [-1.42995285987854, 0.9597495794296265, -0.13245582580566406], 'magnitude': 1.7272605895996094, 'distance': 13.864049911499023, 'directional_contribution': -1.7201240045553075}]}, 6007: {'frame': 6007, 'ionic_force': [-8.5225989818573, 11.005497053265572, -12.623888924717903], 'ionic_force_magnitude': 18.7914403486962, 'motion_vector': [2.3887977600097656, 0.3354644775390625, 2.6361465454101562], 'cosine_ionic_motion': -0.7438233596257194, 'ionic_motion_component': -13.977512292373508, 'ionic_force_x': -8.5225989818573, 'ionic_force_y': 11.005497053265572, 'ionic_force_z': -12.623888924717903, 'radial_force': 13.919614175507604, 'axial_force': -12.623888924717903, 'contributions': [{'ion': 1327, 'force': [-0.6066397428512573, -0.07653407752513885, -1.803540825843811], 'magnitude': 1.904370903968811, 'distance': 13.203627586364746, 'directional_contribution': -1.7432872690928678}, {'ion': 1380, 'force': [3.8302056789398193, 13.930157661437988, -4.655093669891357], 'magnitude': 15.178592681884766, 'distance': 4.676848411560059, 'directional_contribution': 0.434100132452798}, {'ion': 1443, 'force': [-2.181785821914673, -0.8094444274902344, -4.307274341583252], 'magnitude': 4.895712852478027, 'distance': 8.234951972961426, 'directional_contribution': -4.712226165570627}, {'ion': 1476, 'force': [-1.5309606790542603, -3.3161826133728027, -0.14249469339847565], 'magnitude': 3.655299186706543, 'distance': 9.530322074890137, 'directional_contribution': -1.43993422116767}, {'ion': 2434, 'force': [-4.577861785888672, -0.5349699258804321, -0.9441246390342712], 'magnitude': 4.704719066619873, 'distance': 8.400443077087402, 'directional_contribution': -3.807143908224935}, {'ion': 2443, 'force': [-3.455556631088257, 1.8124704360961914, -0.7713607549667358], 'magnitude': 3.9775516986846924, 'distance': 9.13610553741455, 'directional_contribution': -2.7090211738439223}]}, 6008: {'frame': 6008, 'ionic_force': [-13.272890001535416, -0.8764415849000216, -4.7812259793281555], 'ionic_force_magnitude': 14.134987821360276, 'motion_vector': [-3.128063201904297, -1.1513519287109375, -3.5046615600585938], 'cosine_ionic_motion': 0.8671605287776131, 'ionic_motion_component': 12.257303513435899, 'ionic_force_x': -13.272890001535416, 'ionic_force_y': -0.8764415849000216, 'ionic_force_z': -4.7812259793281555, 'radial_force': 13.30179532411324, 'axial_force': -4.7812259793281555, 'contributions': [{'ion': 1327, 'force': [-0.7063149809837341, -0.023201383650302887, -2.9974205493927], 'magnitude': 3.079602003097534, 'distance': 10.382973670959473, 'directional_contribution': 2.6342806923334523}, {'ion': 1341, 'force': [-0.16335004568099976, 0.015826871618628502, -1.473613977432251], 'magnitude': 1.4827244281768799, 'distance': 14.963693618774414, 'directional_contribution': 1.1696695558799857}, {'ion': 1380, 'force': [7.910303592681885, 9.88100528717041, 1.849670648574829], 'magnitude': 12.791733741760254, 'distance': 5.094532489776611, 'directional_contribution': -8.80837773022975}, {'ion': 1443, 'force': [-4.902888298034668, -1.712356448173523, -12.520059585571289], 'magnitude': 13.554422378540039, 'distance': 4.949126243591309, 'directional_contribution': 12.650661995358629}, {'ion': 1476, 'force': [0.212553471326828, -4.179253578186035, 1.9074146747589111], 'magnitude': 4.598865985870361, 'distance': 8.496570587158203, 'directional_contribution': -0.5247308855735806}, {'ion': 2434, 'force': [-11.429412841796875, -8.605399131774902, 7.497924327850342], 'magnitude': 16.15250015258789, 'distance': 4.53366231918335, 'directional_contribution': 4.007347459289264}, {'ion': 2443, 'force': [-4.193780899047852, 3.746936798095703, 0.9548584818840027], 'magnitude': 5.704304218292236, 'distance': 7.629001617431641, 'directional_contribution': 1.1284522554070335}]}, 6009: {'frame': 6009, 'ionic_force': [-7.961302757263184, 8.177349001169205, -15.085426807403564], 'ionic_force_magnitude': 18.916169808956028, 'motion_vector': [3.8805274963378906, 4.743255615234375, -1.0284576416015625], 'cosine_ionic_motion': 0.1991376659376658, 'ionic_motion_component': 3.7669219042360447, 'ionic_force_x': -7.961302757263184, 'ionic_force_y': 8.177349001169205, 'ionic_force_z': -15.085426807403564, 'radial_force': 11.41277259388486, 'axial_force': -15.085426807403564, 'contributions': [{'ion': 1327, 'force': [-0.591535210609436, -0.1539454162120819, -1.536857008934021], 'magnitude': 1.6539475917816162, 'distance': 14.167987823486328, 'directional_contribution': -0.23254940922222112}, {'ion': 1380, 'force': [0.541907787322998, 12.025218963623047, -9.050501823425293], 'magnitude': 15.060250282287598, 'distance': 4.695187568664551, 'directional_contribution': 11.015262292895684}, {'ion': 1443, 'force': [-2.206110715866089, -0.993217945098877, -3.5082154273986816], 'magnitude': 4.261570453643799, 'distance': 8.826412200927734, 'directional_contribution': -1.555165255618455}, {'ion': 1476, 'force': [-0.4248296022415161, -2.8931193351745605, -0.22868134081363678], 'magnitude': 2.933072566986084, 'distance': 10.639166831970215, 'directional_contribution': -2.4357906364350237}, {'ion': 2434, 'force': [-2.3827462196350098, -0.7271773219108582, -0.04096989333629608], 'magnitude': 2.491574764251709, 'distance': 11.543355941772461, 'directional_contribution': -2.0362435784710797}, {'ion': 2443, 'force': [-2.897988796234131, 0.9195900559425354, -0.720201313495636], 'magnitude': 3.124527931213379, 'distance': 10.30805778503418, 'directional_contribution': -0.9885913490203828}]}, 6010: {'frame': 6010, 'ionic_force': [-3.6213796138763428, 1.774631679058075, -10.690930426120758], 'ionic_force_magnitude': 11.426272414058323, 'motion_vector': [1.1203804016113281, -1.3056755065917969, -0.7982025146484375], 'cosine_ionic_motion': 0.09963000981851038, 'ionic_motion_component': 1.138399632801605, 'ionic_force_x': -3.6213796138763428, 'ionic_force_y': 1.774631679058075, 'ionic_force_z': -10.690930426120758, 'radial_force': 4.032828771980736, 'axial_force': -10.690930426120758, 'contributions': [{'ion': 1327, 'force': [-0.1575925350189209, 0.3570076823234558, -1.512939453125], 'magnitude': 1.5624581575393677, 'distance': 14.576889038085938, 'directional_contribution': 0.2978626321694442}, {'ion': 1380, 'force': [1.4782865047454834, 3.0387051105499268, -1.537086009979248], 'magnitude': 3.7123701572418213, 'distance': 9.456782341003418, 'directional_contribution': -0.5717612086865387}, {'ion': 1443, 'force': [-0.25140249729156494, 0.9879297614097595, -3.684279203414917], 'magnitude': 3.822711229324341, 'distance': 9.319299697875977, 'directional_contribution': 0.7219256417490847}, {'ion': 1476, 'force': [2.1201860904693604, -6.282724380493164, -2.145188093185425], 'magnitude': 6.969192981719971, 'distance': 6.902045249938965, 'directional_contribution': 6.4804272558418035}, {'ion': 2434, 'force': [-5.255415439605713, 0.688380777835846, -0.6865726113319397], 'magnitude': 5.344590187072754, 'distance': 7.881553649902344, 'directional_contribution': -3.289452726313776}, {'ion': 2443, 'force': [-1.5554417371749878, 2.985332727432251, -1.1248650550842285], 'magnitude': 3.54921555519104, 'distance': 9.671700477600098, 'directional_contribution': -2.5006020400647486}]}, 6011: {'frame': 6011, 'ionic_force': [-4.111999347805977, 4.2266088128089905, -12.676829218864441], 'ionic_force_magnitude': 13.981228835017564, 'motion_vector': [-0.2661705017089844, -1.283233642578125, 3.399566650390625], 'cosine_ionic_motion': -0.9310030034089785, 'ionic_motion_component': -13.016566036749564, 'ionic_force_x': -4.111999347805977, 'ionic_force_y': 4.2266088128089905, 'ionic_force_z': -12.676829218864441, 'radial_force': 5.89684328203416, 'axial_force': -12.676829218864441, 'contributions': [{'ion': 1380, 'force': [2.3445777893066406, 1.8577836751937866, -1.650367259979248], 'magnitude': 3.4164481163024902, 'distance': 9.857836723327637, 'directional_contribution': -2.3655069752017326}, {'ion': 1443, 'force': [0.19824711978435516, 0.7226526141166687, -3.8288686275482178], 'magnitude': 3.901508092880249, 'distance': 9.224711418151855, 'directional_contribution': -3.841597024019926}, {'ion': 1476, 'force': [1.8675719499588013, -4.334394454956055, -1.7466002702713013], 'magnitude': 5.032435894012451, 'distance': 8.122316360473633, 'directional_contribution': -0.23953675449160894}, {'ion': 2434, 'force': [-6.596822261810303, 2.5684547424316406, -3.428205728530884], 'magnitude': 7.865597248077393, 'distance': 6.49685525894165, 'directional_contribution': -3.6214386713071427}, {'ion': 2443, 'force': [-1.9255739450454712, 3.412112236022949, -2.02278733253479], 'magnitude': 4.4093098640441895, 'distance': 8.677282333374023, 'directional_contribution': -2.948486366220995}]}, 6012: {'frame': 6012, 'ionic_force': [-4.833177576772869, 11.546525403857231, 6.648796170949936], 'ionic_force_magnitude': 14.173508560458098, 'motion_vector': [3.3740692138671875, 0.3329048156738281, -0.6134490966796875], 'cosine_ionic_motion': -0.3387391465875492, 'ionic_motion_component': -4.801122193920899, 'ionic_force_x': -4.833177576772869, 'ionic_force_y': 11.546525403857231, 'ionic_force_z': 6.648796170949936, 'radial_force': 12.51726225620205, 'axial_force': 6.648796170949936, 'contributions': [{'ion': 1327, 'force': [-0.013671855442225933, 0.1790093630552292, -2.3655295372009277], 'magnitude': 2.3723323345184326, 'distance': 11.82990550994873, 'directional_contribution': 0.42507447806818743}, {'ion': 1380, 'force': [4.7871012687683105, 2.8894221782684326, -0.620657742023468], 'magnitude': 5.625861167907715, 'distance': 7.682003974914551, 'directional_contribution': 5.077533440530573}, {'ion': 1443, 'force': [0.34534260630607605, 0.6158301830291748, -8.505025863647461], 'magnitude': 8.534281730651855, 'distance': 6.237140655517578, 'directional_contribution': 1.911948331957884}, {'ion': 1476, 'force': [1.1810078620910645, -3.9667086601257324, 0.1162365972995758], 'magnitude': 4.140419006347656, 'distance': 8.954614639282227, 'directional_contribution': 0.7525637909667591}, {'ion': 2434, 'force': [-6.8852925300598145, 6.509122848510742, 18.551830291748047], 'magnitude': 20.831378936767578, 'distance': 3.9921791553497314, 'directional_contribution': -9.416663192693278}, {'ion': 2443, 'force': [-4.247664928436279, 5.319849491119385, -0.5280575752258301], 'magnitude': 6.828052520751953, 'distance': 6.973015308380127, 'directional_contribution': -3.551579070958546}]}, 6013: {'frame': 6013, 'ionic_force': [13.507776856422424, 12.524327024817467, -10.32847486436367], 'ionic_force_magnitude': 21.118622020654342, 'motion_vector': [-0.33412933349609375, -3.45306396484375, 0.26458740234375], 'cosine_ionic_motion': -0.6871974397232127, 'ionic_motion_component': -14.512662983075925, 'ionic_force_x': 13.507776856422424, 'ionic_force_y': 12.524327024817467, 'ionic_force_z': -10.32847486436367, 'radial_force': 18.420608106886004, 'axial_force': -10.32847486436367, 'contributions': [{'ion': 1327, 'force': [0.4487518072128296, 0.17691664397716522, -2.0343520641326904], 'magnitude': 2.090757369995117, 'distance': 12.601354598999023, 'directional_contribution': -0.37338597583429944}, {'ion': 1380, 'force': [2.8208999633789062, 1.3959943056106567, -0.5538100600242615], 'magnitude': 3.1957757472991943, 'distance': 10.192503929138184, 'directional_contribution': -1.6984997186537467}, {'ion': 1443, 'force': [2.2907891273498535, 0.40284377336502075, -4.769194602966309], 'magnitude': 5.306148529052734, 'distance': 7.9100518226623535, 'directional_contribution': -0.9824867792408725}, {'ion': 1476, 'force': [2.0120725631713867, -2.631169557571411, 0.06651456654071808], 'magnitude': 3.3129916191101074, 'distance': 10.010571479797363, 'directional_contribution': 2.4231836691692252}, {'ion': 2434, 'force': [7.2099080085754395, 4.52037239074707, -1.7856876850128174], 'magnitude': 8.695125579833984, 'distance': 6.179183483123779, 'directional_contribution': -5.314523608002732}, {'ion': 2443, 'force': [-1.2746446132659912, 8.659369468688965, -1.2519450187683105], 'magnitude': 8.84176254272461, 'distance': 6.127729892730713, 'directional_contribution': -8.566950580467749}]}, 6014: {'frame': 6014, 'ionic_force': [17.058067679405212, 13.762900233268738, -12.238668072968721], 'ionic_force_magnitude': 25.10338805791723, 'motion_vector': [-3.6916656494140625, 0.4512596130371094, -6.285575866699219], 'cosine_ionic_motion': 0.10998618155531045, 'ionic_motion_component': 2.761025796591497, 'ionic_force_x': 17.058067679405212, 'ionic_force_y': 13.762900233268738, 'ionic_force_z': -12.238668072968721, 'radial_force': 21.91791723193783, 'axial_force': -12.238668072968721, 'contributions': [{'ion': 1327, 'force': [0.44926393032073975, -0.36332571506500244, -2.013705015182495], 'magnitude': 2.094958543777466, 'distance': 12.588712692260742, 'directional_contribution': 1.4835177844258491}, {'ion': 1380, 'force': [4.343045234680176, 0.5186071395874023, -0.9668188691139221], 'magnitude': 4.4794793128967285, 'distance': 8.609050750732422, 'directional_contribution': -1.3311544996727882}, {'ion': 1443, 'force': [2.5901107788085938, -2.060776710510254, -4.672119617462158], 'magnitude': 5.7257466316223145, 'distance': 7.614703178405762, 'directional_contribution': 2.584418969917248}, {'ion': 1476, 'force': [1.0401111841201782, -2.099440574645996, -0.0368153341114521], 'magnitude': 2.3432536125183105, 'distance': 11.903080940246582, 'directional_contribution': -0.6237771116451376}, {'ion': 2434, 'force': [7.276932239532471, -2.6795096397399902, -2.861260414123535], 'magnitude': 8.265610694885254, 'distance': 6.337698459625244, 'directional_contribution': -1.381329949562966}, {'ion': 2443, 'force': [1.3586043119430542, 20.447345733642578, -1.6879488229751587], 'magnitude': 20.561830520629883, 'distance': 4.018260955810547, 'directional_contribution': 2.0293509431499572}]}, 6015: {'frame': 6015, 'ionic_force': [0.7399121336638927, -0.4049261808395386, -12.971693515777588], 'ionic_force_magnitude': 12.99908719275083, 'motion_vector': [5.720123291015625, 1.8185005187988281, 4.659736633300781], 'cosine_ionic_motion': -0.5765440841775743, 'ionic_motion_component': -7.494546820688963, 'ionic_force_x': 0.7399121336638927, 'ionic_force_y': -0.4049261808395386, 'ionic_force_z': -12.971693515777588, 'radial_force': 0.843466168540475, 'axial_force': -12.971693515777588, 'contributions': [{'ion': 1380, 'force': [1.9962375164031982, 0.9149305820465088, -3.438105583190918], 'magnitude': 4.079538345336914, 'distance': 9.021183967590332, 'directional_contribution': -0.38666464544393975}, {'ion': 1443, 'force': [-0.037719983607530594, -0.2460545301437378, -1.9342252016067505], 'magnitude': 1.9501776695251465, 'distance': 13.047639846801758, 'directional_contribution': -1.2734048735274763}, {'ion': 1476, 'force': [0.4504967927932739, -1.7856525182724, -0.9601248502731323], 'magnitude': 2.0768587589263916, 'distance': 12.643448829650879, 'directional_contribution': -0.676991713730386}, {'ion': 2434, 'force': [-0.5616505146026611, -1.280389428138733, -4.012508392333984], 'magnitude': 4.249125957489014, 'distance': 8.839327812194824, 'directional_contribution': -3.189809098028414}, {'ion': 2443, 'force': [-1.1074516773223877, 1.9922397136688232, -2.6267294883728027], 'magnitude': 3.4778120517730713, 'distance': 9.770482063293457, 'directional_contribution': -1.9676763714458225}]}, 6016: {'frame': 6016, 'ionic_force': [12.035094380378723, 6.451220761984587, -7.215009570121765], 'ionic_force_magnitude': 15.444031506100767, 'motion_vector': [-3.9956817626953125, -1.5027236938476562, -0.9187698364257812], 'cosine_ionic_motion': -0.7585211961422007, 'ionic_motion_component': -11.714625251265387, 'ionic_force_x': 12.035094380378723, 'ionic_force_y': 6.451220761984587, 'ionic_force_z': -7.215009570121765, 'radial_force': 13.6550996358</t>
+          <t>{5997: {'frame': 5997, 'ionic_force': [9.381639122962952, 3.428868383169174, -11.025252528488636], 'ionic_force_magnitude': 14.877112768933067, 'motion_vector': [0.7771873474121094, 0.3831329345703125, 0.82928466796875], 'cosine_ionic_motion': -0.03015511111987929, 'ionic_motion_component': -0.44862098869015166, 'ionic_force_x': 9.381639122962952, 'ionic_force_y': 3.428868383169174, 'ionic_force_z': -11.025252528488636, 'radial_force': 9.988608062318105, 'axial_force': -11.025252528488636, 'contributions': [{'ion': 1327, 'force': [0.5210571885108948, -0.15596595406532288, -1.7473162412643433], 'magnitude': 1.8300108909606934, 'distance': 13.469212532043457, 'cosine_with_motion': -0.5029046882528586, 'motion_component': -0.9203210783935373}, {'ion': 1380, 'force': [3.0363898277282715, 0.8332290053367615, -0.6519385576248169], 'magnitude': 3.2154250144958496, 'distance': 10.161314010620117, 'cosine_with_motion': 0.554497784335778, 'motion_component': 1.782946013499606}, {'ion': 1443, 'force': [2.586791753768921, -0.8877150416374207, -4.0297532081604], 'magnitude': 4.8701581954956055, 'distance': 8.256528854370117, 'cosine_with_motion': -0.28615785628677687, 'motion_component': -1.3936340184841656}, {'ion': 1476, 'force': [1.3487483263015747, -1.712496280670166, -0.039044089615345], 'magnitude': 2.180204153060913, 'distance': 12.340150833129883, 'cosine_with_motion': 0.13757207651808118, 'motion_component': 0.2999352078664286}, {'ion': 2434, 'force': [-0.48151785135269165, -7.0847249031066895, -1.291944980621338], 'magnitude': 7.217638969421387, 'distance': 6.7822136878967285, 'cosine_with_motion': -0.48055241989325803, 'motion_component': -3.4684537373107496}, {'ion': 2443, 'force': [2.3701698780059814, 12.436541557312012, -3.2652554512023926], 'magnitude': 13.074676513671875, 'distance': 5.039106845855713, 'cosine_with_motion': 0.24864144878760677, 'motion_component': 3.250906495401992}]}, 5998: {'frame': 5998, 'ionic_force': [10.780787527561188, 0.28440017998218536, -7.232492357492447], 'ionic_force_magnitude': 12.985191907629991, 'motion_vector': [-0.7672195434570312, 2.2775001525878906, -1.0481185913085938], 'cosine_ionic_motion': -0.001263009889529832, 'ionic_motion_component': -0.016400425796779423, 'ionic_force_x': 10.780787527561188, 'ionic_force_y': 0.28440017998218536, 'ionic_force_z': -7.232492357492447, 'radial_force': 10.784538153152075, 'axial_force': -7.232492357492447, 'contributions': [{'ion': 1327, 'force': [0.6711025238037109, -0.13265840709209442, -1.804991602897644], 'magnitude': 1.9302775859832764, 'distance': 13.114724159240723, 'cosine_with_motion': 0.21237849268114292, 'motion_component': 0.40994944295757296}, {'ion': 1380, 'force': [2.8374791145324707, 0.6517823338508606, -0.4846545159816742], 'magnitude': 2.95143985748291, 'distance': 10.606010437011719, 'cosine_with_motion': -0.02385020767435757, 'motion_component': -0.07039245638239944}, {'ion': 1443, 'force': [3.076692581176758, -0.8291545510292053, -3.541635036468506], 'magnitude': 4.764106750488281, 'distance': 8.347920417785645, 'cosine_with_motion': -0.04297902665725936, 'motion_component': -0.20475667152368615}, {'ion': 1476, 'force': [1.263065218925476, -1.5566960573196411, 0.03140932321548462], 'magnitude': 2.004899740219116, 'distance': 12.868345260620117, 'cosine_with_motion': -0.8650766728807576, 'motion_component': -1.7343919836517667}, {'ion': 2434, 'force': [-0.50923091173172, -8.268269538879395, -0.3708587884902954], 'magnitude': 8.29223346710205, 'distance': 6.327516555786133, 'cosine_with_motion': -0.8302967302675558, 'motion_component': -6.88501421705325}, {'ion': 2443, 'force': [3.441679000854492, 10.41939640045166, -1.061761736869812], 'magnitude': 11.024351119995117, 'distance': 5.487727642059326, 'cosine_with_motion': 0.7681364258085014, 'motion_component': 8.46820552903441}]}, 5999: {'frame': 5999, 'ionic_force': [6.903971970081329, -9.943094223737717, -11.683605313301086], 'ionic_force_magnitude': 16.8236911771107, 'motion_vector': [-1.3753700256347656, -4.601753234863281, -0.27584075927734375], 'cosine_ionic_motion': 0.48783230159410307, 'ionic_motion_component': 8.207139988238318, 'ionic_force_x': 6.903971970081329, 'ionic_force_y': -9.943094223737717, 'ionic_force_z': -11.683605313301086, 'radial_force': 12.104955667237903, 'axial_force': -11.683605313301086, 'contributions': [{'ion': 1327, 'force': [0.45604217052459717, 0.1768944263458252, -1.7557339668273926], 'magnitude': 1.822599172592163, 'distance': 13.49657154083252, 'cosine_with_motion': -0.10913884575298162, 'motion_component': -0.19891637349124203}, {'ion': 1380, 'force': [2.0143558979034424, 1.382273554801941, -0.6717885732650757], 'magnitude': 2.5336947441101074, 'distance': 11.447005271911621, 'cosine_with_motion': -0.7339383307098968, 'motion_component': -1.8595757916178342}, {'ion': 1443, 'force': [2.022075653076172, 0.4375012218952179, -3.6579012870788574], 'magnitude': 4.202432632446289, 'distance': 8.888298988342285, 'cosine_with_motion': -0.18723646755622428, 'motion_component': -0.7868486203393044}, {'ion': 1476, 'force': [2.0586459636688232, -1.9142779111862183, -0.18536603450775146], 'magnitude': 2.8172404766082764, 'distance': 10.855681419372559, 'cosine_with_motion': 0.44482233949506284, 'motion_component': 1.2531714830432583}, {'ion': 2434, 'force': [0.3335014283657074, -16.288362503051758, -3.843754291534424], 'magnitude': 16.73906898498535, 'distance': 4.453519821166992, 'cosine_with_motion': 0.9382599892586932, 'motion_component': 15.705598484353184}, {'ion': 2443, 'force': [0.01935085654258728, 6.262876987457275, -1.5690611600875854], 'magnitude': 6.456466197967529, 'distance': 7.170866012573242, 'cosine_with_motion': -0.9147867132530993, 'motion_component': -5.90628947647706}]}, 6000: {'frame': 6000, 'ionic_force': [5.517950534820557, 7.6139421463012695, -19.801055759191513], 'ionic_force_magnitude': 21.920349045819517, 'motion_vector': [-4.781524658203125, 2.4392776489257812, 0.5065383911132812], 'cosine_ionic_motion': -0.1509624024908215, 'ionic_motion_component': -3.3091485553943008, 'ionic_force_x': 5.517950534820557, 'ionic_force_y': 7.6139421463012695, 'ionic_force_z': -19.801055759191513, 'radial_force': 9.403185264151146, 'axial_force': -19.801055759191513, 'contributions': [{'ion': 1327, 'force': [0.27228718996047974, -0.34001588821411133, -1.6231095790863037], 'magnitude': 1.6805462837219238, 'distance': 14.055419921875, 'cosine_with_motion': -0.3259627221595233, 'motion_component': -0.5477954425251834}, {'ion': 1380, 'force': [3.8357651233673096, 0.6248253583908081, -1.3770771026611328], 'magnitude': 4.123086452484131, 'distance': 8.973416328430176, 'cosine_with_motion': -0.7878593598961018, 'motion_component': -3.2484122782963705}, {'ion': 1443, 'force': [1.5023193359375, -1.549290657043457, -3.5091614723205566], 'magnitude': 4.119645595550537, 'distance': 8.977163314819336, 'cosine_with_motion': -0.5735767810263909, 'motion_component': -2.362933013233306}, {'ion': 1476, 'force': [1.1409306526184082, -1.8393505811691284, -0.37553462386131287], 'magnitude': 2.1968066692352295, 'distance': 12.293431282043457, 'cosine_with_motion': -0.8554532966122542, 'motion_component': -1.8792655123287687}, {'ion': 2434, 'force': [-0.8899776935577393, -4.16619348526001, -0.9849853515625], 'magnitude': 4.3725762367248535, 'distance': 8.713654518127441, 'cosine_with_motion': -0.27172446280525053, 'motion_component': -1.1881359802195564}, {'ion': 2443, 'force': [-0.3433740735054016, 14.883967399597168, -11.931187629699707], 'magnitude': 19.07887840270996, 'distance': 4.17150354385376, 'cosine_with_motion': 0.31015416168122784, 'motion_component': 5.917393768109569}]}, 6001: {'frame': 6001, 'ionic_force': [-5.739471256732941, 1.5717533826828003, -13.330579981207848], 'ionic_force_magnitude': 14.598503404055426, 'motion_vector': [1.7098503112792969, -0.131500244140625, 0.37758636474609375], 'cosine_ionic_motion': -0.5872436292990687, 'ionic_motion_component': -8.572878121332318, 'ionic_force_x': -5.739471256732941, 'ionic_force_y': 1.5717533826828003, 'ionic_force_z': -13.330579981207848, 'radial_force': 5.9507931406526335, 'axial_force': -13.330579981207848, 'contributions': [{'ion': 1327, 'force': [-0.37006884813308716, -0.10675269365310669, -1.939383625984192], 'magnitude': 1.9772597551345825, 'distance': 12.957976341247559, 'cosine_with_motion': -0.3891132324604061, 'motion_component': -0.7693779149979432}, {'ion': 1380, 'force': [4.8833489418029785, 6.641224384307861, -3.6172406673431396], 'magnitude': 9.002077102661133, 'distance': 6.0729217529296875, 'cosine_with_motion': 0.38656834232561726, 'motion_component': 3.479917939183366}, {'ion': 1443, 'force': [-1.8360635042190552, -0.6234139800071716, -6.40214204788208], 'magnitude': 6.689334392547607, 'distance': 7.044944763183594, 'cosine_with_motion': -0.4660847366346669, 'motion_component': -3.1177967411055856}, {'ion': 1476, 'force': [-1.7837971448898315, -6.105370998382568, 0.018659725785255432], 'magnitude': 6.360647678375244, 'distance': 7.224676132202148, 'cosine_with_motion': -0.20056350312584506, 'motion_component': -1.2757137265881193}, {'ion': 2434, 'force': [-2.968780040740967, -1.7256089448928833, -0.42890286445617676], 'magnitude': 3.460540294647217, 'distance': 9.79483413696289, 'cosine_with_motion': -0.8246681142989506, 'motion_component': -2.853797203169603}, {'ion': 2443, 'force': [-3.6641106605529785, 3.491675615310669, -0.9615705013275146], 'magnitude': 5.151905059814453, 'distance': 8.027588844299316, 'cosine_with_motion': -0.7834209858121003, 'motion_component': -4.036110359738709}]}, 6002: {'frame': 6002, 'ionic_force': [-2.454675856977701, -1.9141423031687737, -12.883132107555866], 'ionic_force_magnitude': 13.253847261091638, 'motion_vector': [-0.4403953552246094, 2.3236732482910156, 2.6926345825195312], 'cosine_ionic_motion': -0.801199510453789, 'ionic_motion_component': -10.618975937215913, 'ionic_force_x': -2.454675856977701, 'ionic_force_y': -1.9141423031687737, 'ionic_force_z': -12.883132107555866, 'radial_force': 3.1127759828823964, 'axial_force': -12.883132107555866, 'contributions': [{'ion': 1327, 'force': [-0.07753433287143707, -0.08069079369306564, -2.0556859970092773], 'magnitude': 2.058729648590088, 'distance': 12.698995590209961, 'cosine_with_motion': -0.7710073664359711, 'motion_component': -1.587295673869313}, {'ion': 1380, 'force': [6.697790622711182, 2.4995415210723877, -1.7771592140197754], 'magnitude': 7.366573333740234, 'distance': 6.713303565979004, 'cosine_with_motion': -0.07298371535563009, 'motion_component': -0.5376398875308581}, {'ion': 1443, 'force': [0.05283843353390694, -1.0870180130004883, -6.450309753417969], 'magnitude': 6.54147481918335, 'distance': 7.124119281768799, 'cosine_with_motion': -0.8495983544202529, 'motion_component': -5.5576264474365935}, {'ion': 1476, 'force': [0.09511121362447739, -5.949183940887451, -0.06667114049196243], 'magnitude': 5.950317859649658, 'distance': 7.469627857208252, 'cosine_with_motion': -0.6586399658088433, 'motion_component': -3.919117047338237}, {'ion': 2434, 'force': [-3.142949104309082, -4.085984230041504, -0.727785587310791], 'magnitude': 5.206060409545898, 'distance': 7.985726356506348, 'cosine_with_motion': -0.5397292170014344, 'motion_component': -2.8098630678356358}, {'ion': 2443, 'force': [-6.079932689666748, 6.789193153381348, -1.8055204153060913], 'magnitude': 9.29078197479248, 'distance': 5.977820873260498, 'cosine_with_motion': 0.4082074537256893, 'motion_component': 3.792566441006535}]}, 6003: {'frame': 6003, 'ionic_force': [-7.239282563328743, 3.985614240169525, -13.104669943451881], 'ionic_force_magnitude': 15.492730786726039, 'motion_vector': [-6.120677947998047, -2.7395401000976562, -2.5673294067382812], 'cosine_ionic_motion': 0.6025856708493228, 'ionic_motion_component': 9.335697574407266, 'ionic_force_x': -7.239282563328743, 'ionic_force_y': 3.985614240169525, 'ionic_force_z': -13.104669943451881, 'radial_force': 8.263917527611083, 'axial_force': -13.104669943451881, 'contributions': [{'ion': 1327, 'force': [-0.19644558429718018, 0.4891625642776489, -3.0373945236206055], 'magnitude': 3.082796812057495, 'distance': 10.377592086791992, 'cosine_with_motion': 0.34605757366136947, 'motion_component': 1.0668251955116084}, {'ion': 1341, 'force': [-0.06385579705238342, 0.24247795343399048, -1.6175693273544312], 'magnitude': 1.6368883848190308, 'distance': 14.241623878479004, 'cosine_with_motion': 0.33006006611155425, 'motion_component': 0.5402714950801091}, {'ion': 1380, 'force': [2.977800130844116, 4.4187140464782715, 0.1744322031736374], 'magnitude': 5.331299304962158, 'distance': 7.891371726989746, 'cosine_with_motion': -0.8040305034849321, 'motion_component': -4.286527396978535}, {'ion': 1443, 'force': [-1.4516021013259888, 3.280688762664795, -14.232921600341797], 'magnitude': 14.678083419799805, 'distance': 4.755918025970459, 'cosine_with_motion': 0.3457250501952327, 'motion_component': 5.074581030755816}, {'ion': 1476, 'force': [-0.12233380973339081, -6.026616096496582, 3.0402510166168213], 'magnitude': 6.751162528991699, 'distance': 7.012611389160156, 'cosine_with_motion': 0.1950142850485213, 'motion_component': 1.3165731033157444}, {'ion': 2434, 'force': [-5.042224407196045, -2.669969320297241, 1.6620091199874878], 'magnitude': 5.94264554977417, 'distance': 7.474448204040527, 'cosine_with_motion': 0.7946723936861015, 'motion_component': 4.722456452694576}, {'ion': 2443, 'force': [-3.340620994567871, 4.251156330108643, 0.9065231680870056], 'magnitude': 5.48214054107666, 'distance': 7.782049179077148, 'cosine_with_motion': 0.16444628083933396, 'motion_component': 0.9015175947396638}]}, 6004: {'frame': 6004, 'ionic_force': [-13.262407958507538, 11.088155046105385, -8.382136479020119], 'ionic_force_magnitude': 19.2119457405354, 'motion_vector': [-0.223419189453125, 2.570514678955078, -0.7060775756835938], 'cosine_ionic_motion': 0.7274053216976897, 'ionic_motion_component': 13.974871571832711, 'ionic_force_x': -13.262407958507538, 'ionic_force_y': 11.088155046105385, 'ionic_force_z': -8.382136479020119, 'radial_force': 17.28695019904773, 'axial_force': -8.382136479020119, 'contributions': [{'ion': 1327, 'force': [-0.7501986622810364, -0.13029859960079193, -1.3091551065444946], 'magnitude': 1.5144842863082886, 'distance': 14.805962562561035, 'cosine_with_motion': 0.186860844372352, 'motion_component': 0.28299782470996293}, {'ion': 1380, 'force': [-4.599451065063477, 13.990073204040527, -4.257678985595703], 'magnitude': 15.329870223999023, 'distance': 4.653715133666992, 'cosine_with_motion': 0.9752989250966534, 'motion_component': 14.95120619354374}, {'ion': 1443, 'force': [-2.4518744945526123, -0.6125720739364624, -2.5525479316711426], 'magnitude': 3.59199595451355, 'distance': 9.613933563232422, 'cosine_with_motion': 0.08070347547918504, 'motion_component': 0.28988654720289553}, {'ion': 1476, 'force': [-1.4830362796783447, -2.197493553161621, 0.07560582458972931], 'magnitude': 2.652186155319214, 'distance': 11.188375473022461, 'cosine_with_motion': -0.7569972136268932, 'motion_component': -2.0076974384426522}, {'ion': 2434, 'force': [-1.6397267580032349, -0.897940993309021, -0.09315349161624908], 'magnitude': 1.8718117475509644, 'distance': 13.317967414855957, 'cosine_with_motion': -0.3746682915369973, 'motion_component': -0.7013085318627432}, {'ion': 2443, 'force': [-2.338120698928833, 0.9363870620727539, -0.2452067881822586], 'magnitude': 2.530564308166504, 'distance': 11.454083442687988, 'cosine_with_motion': 0.4583115526478856, 'motion_component': 1.15978683758948}]}, 6005: {'frame': 6005, 'ionic_force': [-11.751091122627258, 3.513936460018158, -5.2574396431446075], 'ionic_force_magnitude': 13.344533098562968, 'motion_vector': [-0.2879486083984375, 0.21361923217773438, 0.6275177001953125], 'cosine_ionic_motion': 0.08660157332649941, 'ionic_motion_component': 1.1556575616430993, 'ionic_force_x': -11.751091122627258, 'ionic_force_y': 3.513936460018158, 'ionic_force_z': -5.2574396431446075, 'radial_force': 12.265231021767756, 'axial_force': -5.2574396431446075, 'contributions': [{'ion': 1380, 'force': [-1.5290939807891846, 5.18525505065918, -2.7910616397857666], 'magnitude': 6.0839972496032715, 'distance': 7.387109279632568, 'cosine_with_motion': -0.046274344769027524, 'motion_component': -0.2815329896728045}, {'ion': 1443, 'force': [-2.1018567085266113, 0.29880401492118835, -2.3693599700927734], 'magnitude': 3.181344509124756, 'distance': 10.215596199035645, 'cosine_with_motion': -0.35566691171394543, 'motion_component': -1.1314989344353963}, {'ion': 1476, 'force': [-1.9276835918426514, -2.4968819618225098, -0.44340747594833374], 'magnitude': 3.185434579849243, 'distance': 10.20903491973877, 'cosine_with_motion': -0.1114396492132857, 'motion_component': -0.3549837172213053}, {'ion': 2434, 'force': [-4.488006591796875, -0.4852888882160187, 0.6003507971763611], 'magnitude': 4.553913593292236, 'distance': 8.538402557373047, 'cosine_with_motion': 0.475624094121237, 'motion_component': 2.165951055586958}, {'ion': 2443, 'force': [-1.704450249671936, 1.0120482444763184, -0.25396135449409485], 'magnitude': 1.9984716176986694, 'distance': 12.88902473449707, 'cosine_with_motion': 0.37915073484901873, 'motion_component': 0.7577219696746003}]}, 6006: {'frame': 6006, 'ionic_force': [-11.669181168079376, 5.09692008793354, -6.636843234300613], 'ionic_force_magnitude': 14.35952894885207, 'motion_vector': [3.3086013793945312, -2.3047142028808594, -0.0504608154296875], 'cosine_ionic_motion': -0.8638428873633073, 'ionic_motion_component': -12.404376948353368, 'ionic_force_x': -11.669181168079376, 'ionic_force_y': 5.09692008793354, 'ionic_force_z': -6.636843234300613, 'radial_force': 12.733749782221999, 'axial_force': -6.636843234300613, 'contributions': [{'ion': 1327, 'force': [-0.7694267630577087, 0.20096524059772491, -1.2440012693405151], 'magnitude': 1.4764631986618042, 'distance': 14.995388984680176, 'cosine_with_motion': -0.49482651686876605, 'motion_component': -0.7305931674763221}, {'ion': 1380, 'force': [-1.6209291219711304, 5.998019695281982, -2.354433298110962], 'magnitude': 6.644321918487549, 'distance': 7.06876802444458, 'cosine_with_motion': -0.7116686340399404, 'motion_component': -4.7285551762152656}, {'ion': 1443, 'force': [-2.171865224838257, 0.4668664336204529, -2.2036139965057373], 'magnitude': 3.129037857055664, 'distance': 10.300626754760742, 'cosine_with_motion': -0.6459600570181461, 'motion_component': -2.0212334267683243}, {'ion': 1476, 'force': [-3.098361015319824, -2.754167318344116, -0.36075103282928467], 'magnitude': 4.161180019378662, 'distance': 8.93224811553955, 'cosine_with_motion': -0.23155389581540803, 'motion_component': -0.9635374656188068}, {'ion': 2434, 'force': [-2.578646183013916, 0.22548645734786987, -0.3415878117084503], 'magnitude': 2.6109275817871094, 'distance': 11.276430130004883, 'cosine_with_motion': -0.858060532463983, 'motion_component': -2.240333857713003}, {'ion': 2443, 'force': [-1.42995285987854, 0.9597495794296265, -0.13245582580566406], 'magnitude': 1.7272605895996094, 'distance': 13.864049911499023, 'cosine_with_motion': -0.9958682908568361, 'motion_component': -1.7201240045553075}]}, 6007: {'frame': 6007, 'ionic_force': [-8.5225989818573, 11.005497053265572, -12.623888924717903], 'ionic_force_magnitude': 18.7914403486962, 'motion_vector': [2.3887977600097656, 0.3354644775390625, 2.6361465454101562], 'cosine_ionic_motion': -0.7438233596257194, 'ionic_motion_component': -13.977512292373508, 'ionic_force_x': -8.5225989818573, 'ionic_force_y': 11.005497053265572, 'ionic_force_z': -12.623888924717903, 'radial_force': 13.919614175507604, 'axial_force': -12.623888924717903, 'contributions': [{'ion': 1327, 'force': [-0.6066397428512573, -0.07653407752513885, -1.803540825843811], 'magnitude': 1.904370903968811, 'distance': 13.203627586364746, 'cosine_with_motion': -0.915413701296586, 'motion_component': -1.7432872690928678}, {'ion': 1380, 'force': [3.8302056789398193, 13.930157661437988, -4.655093669891357], 'magnitude': 15.178592681884766, 'distance': 4.676848411560059, 'cosine_with_motion': 0.02859949875737043, 'motion_component': 0.434100132452798}, {'ion': 1443, 'force': [-2.181785821914673, -0.8094444274902344, -4.307274341583252], 'magnitude': 4.895712852478027, 'distance': 8.234951972961426, 'cosine_with_motion': -0.9625209946089894, 'motion_component': -4.712226165570627}, {'ion': 1476, 'force': [-1.5309606790542603, -3.3161826133728027, -0.14249469339847565], 'magnitude': 3.655299186706543, 'distance': 9.530322074890137, 'cosine_with_motion': -0.39393060059103735, 'motion_component': -1.43993422116767}, {'ion': 2434, 'force': [-4.577861785888672, -0.5349699258804321, -0.9441246390342712], 'magnitude': 4.704719066619873, 'distance': 8.400443077087402, 'cosine_with_motion': -0.8092180961137404, 'motion_component': -3.8071439082249348}, {'ion': 2443, 'force': [-3.455556631088257, 1.8124704360961914, -0.7713607549667358], 'magnitude': 3.9775516986846924, 'distance': 9.13610553741455, 'cosine_with_motion': -0.6810775388365401, 'motion_component': -2.7090211738439223}]}, 6008: {'frame': 6008, 'ionic_force': [-13.272890001535416, -0.8764415849000216, -4.7812259793281555], 'ionic_force_magnitude': 14.134987821360276, 'motion_vector': [-3.128063201904297, -1.1513519287109375, -3.5046615600585938], 'cosine_ionic_motion': 0.8671605287776131, 'ionic_motion_component': 12.257303513435899, 'ionic_force_x': -13.272890001535416, 'ionic_force_y': -0.8764415849000216, 'ionic_force_z': -4.7812259793281555, 'radial_force': 13.30179532411324, 'axial_force': -4.7812259793281555, 'contributions': [{'ion': 1327, 'force': [-0.7063149809837341, -0.023201383650302887, -2.9974205493927], 'magnitude': 3.079602003097534, 'distance': 10.382973670959473, 'cosine_with_motion': 0.8553964457435272, 'motion_component': 2.6342806923334523}, {'ion': 1341, 'force': [-0.16335004568099976, 0.015826871618628502, -1.473613977432251], 'magnitude': 1.4827244281768799, 'distance': 14.963693618774414, 'cosine_with_motion': 0.7888650738158056, 'motion_component': 1.1696695558799857}, {'ion': 1380, 'force': [7.910303592681885, 9.88100528717041, 1.849670648574829], 'magnitude': 12.791733741760254, 'distance': 5.094532489776611, 'cosine_with_motion': -0.6885992131500849, 'motion_component': -8.80837773022975}, {'ion': 1443, 'force': [-4.902888298034668, -1.712356448173523, -12.520059585571289], 'magnitude': 13.554422378540039, 'distance': 4.949126243591309, 'cosine_with_motion': 0.9333235673743848, 'motion_component': 12.650661995358629}, {'ion': 1476, 'force': [0.212553471326828, -4.179253578186035, 1.9074146747589111], 'magnitude': 4.598865985870361, 'distance': 8.496570587158203, 'cosine_with_motion': -0.11410005519383634, 'motion_component': -0.5247308855735806}, {'ion': 2434, 'force': [-11.429412841796875, -8.605399131774902, 7.497924327850342], 'magnitude': 16.15250015258789, 'distance': 4.53366231918335, 'cosine_with_motion': 0.24809457196754212, 'motion_component': 4.007347459289264}, {'ion': 2443, 'force': [-4.193780899047852, 3.746936798095703, 0.9548584818840027], 'magnitude': 5.704304218292236, 'distance': 7.629001617431641, 'cosine_with_motion': 0.19782469214134593, 'motion_component': 1.1284522554070335}]}, 6009: {'frame': 6009, 'ionic_force': [-7.961302757263184, 8.177349001169205, -15.085426807403564], 'ionic_force_magnitude': 18.916169808956028, 'motion_vector': [3.8805274963378906, 4.743255615234375, -1.0284576416015625], 'cosine_ionic_motion': 0.1991376659376658, 'ionic_motion_component': 3.7669219042360447, 'ionic_force_x': -7.961302757263184, 'ionic_force_y': 8.177349001169205, 'ionic_force_z': -15.085426807403564, 'radial_force': 11.41277259388486, 'axial_force': -15.085426807403564, 'contributions': [{'ion': 1327, 'force': [-0.591535210609436, -0.1539454162120819, -1.536857008934021], 'magnitude': 1.6539475917816162, 'distance': 14.167987823486328, 'cosine_with_motion': -0.1406026487890743, 'motion_component': -0.23254940922222112}, {'ion': 1380, 'force': [0.541907787322998, 12.025218963623047, -9.050501823425293], 'magnitude': 15.060250282287598, 'distance': 4.695187568664551, 'cosine_with_motion': 0.7314129639106994, 'motion_component': 11.015262292895684}, {'ion': 1443, 'force': [-2.206110715866089, -0.993217945098877, -3.5082154273986816], 'magnitude': 4.261570453643799, 'distance': 8.826412200927734, 'cosine_with_motion': -0.3649277443025154, 'motion_component': -1.555165255618455}, {'ion': 1476, 'force': [-0.4248296022415161, -2.8931193351745605, -0.22868134081363678], 'magnitude': 2.933072566986084, 'distance': 10.639166831970215, 'cosine_with_motion': -0.8304569898762885, 'motion_component': -2.4357906364350237}, {'ion': 2434, 'force': [-2.3827462196350098, -0.7271773219108582, -0.04096989333629608], 'magnitude': 2.491574764251709, 'distance': 11.543355941772461, 'cosine_with_motion': -0.8172516378812329, 'motion_component': -2.0362435784710797}, {'ion': 2443, 'force': [-2.897988796234131, 0.9195900559425354, -0.720201313495636], 'magnitude': 3.124527931213379, 'distance': 10.30805778503418, 'cosine_with_motion': -0.3163970260731719, 'motion_component': -0.9885913490203828}]}, 6010: {'frame': 6010, 'ionic_force': [-3.6213796138763428, 1.774631679058075, -10.690930426120758], 'ionic_force_magnitude': 11.426272414058323, 'motion_vector': [1.1203804016113281, -1.3056755065917969, -0.7982025146484375], 'cosine_ionic_motion': 0.09963000981851038, 'ionic_motion_component': 1.138399632801605, 'ionic_force_x': -3.6213796138763428, 'ionic_force_y': 1.774631679058075, 'ionic_force_z': -10.690930426120758, 'radial_force': 4.032828771980736, 'axial_force': -10.690930426120758, 'contributions': [{'ion': 1327, 'force': [-0.1575925350189209, 0.3570076823234558, -1.512939453125], 'magnitude': 1.5624581575393677, 'distance': 14.576889038085938, 'cosine_with_motion': 0.19063718239012178, 'motion_component': 0.2978626321694442}, {'ion': 1380, 'force': [1.4782865047454834, 3.0387051105499268, -1.537086009979248], 'magnitude': 3.7123701572418213, 'distance': 9.456782341003418, 'cosine_with_motion': -0.15401513443536977, 'motion_component': -0.5717612086865387}, {'ion': 1443, 'force': [-0.25140249729156494, 0.9879297614097595, -3.684279203414917], 'magnitude': 3.822711229324341, 'distance': 9.319299697875977, 'cosine_with_motion': 0.1888517298913497, 'motion_component': 0.7219256417490847}, {'ion': 1476, 'force': [2.1201860904693604, -6.282724380493164, -2.145188093185425], 'magnitude': 6.969192981719971, 'distance': 6.902045249938965, 'cosine_with_motion': 0.92986771215663, 'motion_component': 6.4804272558418035}, {'ion': 2434, 'force': [-5.255415439605713, 0.688380777835846, -0.6865726113319397], 'magnitude': 5.344590187072754, 'distance': 7.881553649902344, 'cosine_with_motion': -0.6154733611346858, 'motion_component': -3.289452726313776}, {'ion': 2443, 'force': [-1.5554417371749878, 2.985332727432251, -1.1248650550842285], 'magnitude': 3.54921555519104, 'distance': 9.671700477600098, 'cosine_with_motion': -0.7045506025710427, 'motion_component': -2.5006020400647486}]}, 6011: {'frame': 6011, 'ionic_force': [-4.111999347805977, 4.2266088128089905, -12.676829218864441], 'ionic_force_magnitude': 13.981228835017564, 'motion_vector': [-0.2661705017089844, -1.283233642578125, 3.399566650390625], 'cosine_ionic_motion': -0.9310030034089785, 'ionic_motion_component': -13.016566036749564, 'ionic_force_x': -4.111999347805977, 'ionic_force_y': 4.2266088128089905, 'ionic_force_z': -12.676829218864441, 'radial_force': 5.89684328203416, 'axial_force': -12.676829218864441, 'contributions': [{'ion': 1380, 'force': [2.3445777893066406, 1.8577836751937866, -1.650367259979248], 'magnitude': 3.4164481163024902, 'distance': 9.857836723327637, 'cosine_with_motion': -0.6923878073754544, 'motion_component': -2.3655069752017326}, {'ion': 1443, 'force': [0.19824711978435516, 0.7226526141166687, -3.8288686275482178], 'magnitude': 3.901508092880249, 'distance': 9.224711418151855, 'cosine_with_motion': -0.984644180768522, 'motion_component': -3.841597024019926}, {'ion': 1476, 'force': [1.8675719499588013, -4.334394454956055, -1.7466002702713013], 'magnitude': 5.032435894012451, 'distance': 8.122316360473633, 'cosine_with_motion': -0.04759856881063422, 'motion_component': -0.2395367544916089}, {'ion': 2434, 'force': [-6.596822261810303, 2.5684547424316406, -3.428205728530884], 'magnitude': 7.865597248077393, 'distance': 6.49685525894165, 'cosine_with_motion': -0.46041497050577473, 'motion_component': -3.6214386713071427}, {'ion': 2443, 'force': [-1.9255739450454712, 3.412112236022949, -2.02278733253479], 'magnitude': 4.4093098640441895, 'distance': 8.677282333374023, 'cosine_with_motion': -0.6686956584488439, 'motion_component': -2.948486366220995}]}, 6012: {'frame': 6012, 'ionic_force': [-4.833177576772869, 11.546525403857231, 6.648796170949936], 'ionic_force_magnitude': 14.173508560458098, 'motion_vector': [3.3740692138671875, 0.3329048156738281, -0.6134490966796875], 'cosine_ionic_motion': -0.3387391465875492, 'ionic_motion_component': -4.801122193920899, 'ionic_force_x': -4.833177576772869, 'ionic_force_y': 11.546525403857231, 'ionic_force_z': 6.648796170949936, 'radial_force': 12.51726225620205, 'axial_force': 6.648796170949936, 'contributions': [{'ion': 1327, 'force': [-0.013671855442225933, 0.1790093630552292, -2.3655295372009277], 'magnitude': 2.3723323345184326, 'distance': 11.82990550994873, 'cosine_with_motion': 0.1791799786325783, 'motion_component': 0.42507447806818743}, {'ion': 1380, 'force': [4.7871012687683105, 2.8894221782684326, -0.620657742023468], 'magnitude': 5.625861167907715, 'distance': 7.682003974914551, 'cosine_with_motion': 0.9025344191787381, 'motion_component': 5.077533440530573}, {'ion': 1443, 'force': [0.34534260630607605, 0.6158301830291748, -8.505025863647461], 'magnitude': 8.534281730651855, 'distance': 6.237140655517578, 'cosine_with_motion': 0.2240315329688328, 'motion_component': 1.911948331957884}, {'ion': 1476, 'force': [1.1810078620910645, -3.9667086601257324, 0.1162365972995758], 'magnitude': 4.140419006347656, 'distance': 8.954614639282227, 'cosine_with_motion': 0.18176030526210937, 'motion_component': 0.7525637909667591}, {'ion': 2434, 'force': [-6.8852925300598145, 6.509122848510742, 18.551830291748047], 'magnitude': 20.831378936767578, 'distance': 3.9921791553497314, 'cosine_with_motion': -0.45204224383729774, 'motion_component': -9.416663192693278}, {'ion': 2443, 'force': [-4.247664928436279, 5.319849491119385, -0.5280575752258301], 'magnitude': 6.828052520751953, 'distance': 6.973015308380127, 'cosine_with_motion': -0.5201452505092705, 'motion_component': -3.5515790709585464}]}, 6013: {'frame': 6013, 'ionic_force': [13.507776856422424, 12.524327024817467, -10.32847486436367], 'ionic_force_magnitude': 21.118622020654342, 'motion_vector': [-0.33412933349609375, -3.45306396484375, 0.26458740234375], 'cosine_ionic_motion': -0.6871974397232127, 'ionic_motion_component': -14.512662983075925, 'ionic_force_x': 13.507776856422424, 'ionic_force_y': 12.524327024817467, 'ionic_force_z': -10.32847486436367, 'radial_force': 18.420608106886004, 'axial_force': -10.32847486436367, 'contributions': [{'ion': 1327, 'force': [0.4487518072128296, 0.17691664397716522, -2.0343520641326904], 'magnitude': 2.090757369995117, 'distance': 12.601354598999023, 'cosine_with_motion': -0.17858886796218035, 'motion_component': -0.37338597583429944}, {'ion': 1380, 'force': [2.8208999633789062, 1.3959943056106567, -0.5538100600242615], 'magnitude': 3.1957757472991943, 'distance': 10.192503929138184, 'cosine_with_motion': -0.5314827701352313, 'motion_component': -1.6984997186537467}, {'ion': 1443, 'force': [2.2907891273498535, 0.40284377336502075, -4.769194602966309], 'magnitude': 5.306148529052734, 'distance': 7.9100518226623535, 'cosine_with_motion': -0.18516005038430078, 'motion_component': -0.9824867792408724}, {'ion': 1476, 'force': [2.0120725631713867, -2.631169557571411, 0.06651456654071808], 'magnitude': 3.3129916191101074, 'distance': 10.010571479797363, 'cosine_with_motion': 0.7314185945024936, 'motion_component': 2.4231836691692252}, {'ion': 2434, 'force': [7.2099080085754395, 4.52037239074707, -1.7856876850128174], 'magnitude': 8.695125579833984, 'distance': 6.179183483123779, 'cosine_with_motion': -0.6112071813001704, 'motion_component': -5.314523608002732}, {'ion': 2443, 'force': [-1.2746446132659912, 8.659369468688965, -1.2519450187683105], 'magnitude': 8.84176254272461, 'distance': 6.127729892730713, 'cosine_with_motion': -0.9689188712793316, 'motion_component': -8.566950580467749}]}, 6014: {'frame': 6014, 'ionic_force': [17.058067679405212, 13.762900233268738, -12.238668072968721], 'ionic_force_magni</t>
         </is>
       </c>
     </row>
@@ -739,7 +739,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>{6160: {'frame': 6160, 'ionic_force': [3.740715362073388, 2.176445934921503, -12.598692059516907], 'ionic_force_magnitude': 13.321295355115527, 'motion_vector': [2.4038047790527344, -0.042205810546875, -2.1078033447265625], 'cosine_ionic_motion': 0.8324384974001108, 'ionic_motion_component': 11.089159088835444, 'ionic_force_x': 3.740715362073388, 'ionic_force_y': 2.176445934921503, 'ionic_force_z': -12.598692059516907, 'radial_force': 4.327801789325404, 'axial_force': -12.598692059516907, 'contributions': [{'ion': 1327, 'force': [-0.22856654226779938, 0.7065204977989197, -8.549403190612793], 'magnitude': 8.581591606140137, 'distance': 6.219924449920654, 'directional_contribution': 5.454936947654412}, {'ion': 1341, 'force': [-0.0005797222838737071, 0.04265621677041054, -2.332738161087036], 'magnitude': 2.3331282138824463, 'distance': 11.928881645202637, 'directional_contribution': 1.5368340101219817}, {'ion': 1355, 'force': [-1.527624487876892, -3.6898083686828613, -0.8481869697570801], 'magnitude': 4.082614898681641, 'distance': 9.017784118652344, 'directional_contribution': -0.5406293782664431}, {'ion': 1380, 'force': [5.1329145431518555, 4.496638774871826, -0.7909724116325378], 'magnitude': 6.869658946990967, 'distance': 6.95186710357666, 'directional_contribution': 4.321096572897298}, {'ion': 1476, 'force': [-4.47384786605835, 4.564768314361572, -0.8368766903877258], 'magnitude': 6.446145057678223, 'distance': 7.176604270935059, 'directional_contribution': -2.872070320188927}, {'ion': 2443, 'force': [4.838419437408447, -3.9443295001983643, 0.7594853639602661], 'magnitude': 6.288470268249512, 'distance': 7.266019344329834, 'directional_contribution': 3.1889909130123657}]}, 6161: {'frame': 6161, 'ionic_force': [2.045816570520401, 2.513314615935087, -12.963244438171387], 'ionic_force_magnitude': 13.362178795491031, 'motion_vector': [4.460853576660156, 2.02520751953125, 0.9477462768554688], 'cosine_ionic_motion': 0.02894916806440939, 'ionic_motion_component': 0.3868239596573573, 'ionic_force_x': 2.045816570520401, 'ionic_force_y': 2.513314615935087, 'ionic_force_z': -12.963244438171387, 'radial_force': 3.2406968076154223, 'axial_force': -12.963244438171387, 'contributions': [{'ion': 1327, 'force': [0.9507448077201843, 0.019289210438728333, -3.7588417530059814], 'magnitude': 3.8772642612457275, 'distance': 9.253506660461426, 'directional_contribution': 0.14384513881447392}, {'ion': 1341, 'force': [0.26577094197273254, -0.029373470693826675, -1.5081979036331177], 'magnitude': 1.531717300415039, 'distance': 14.722437858581543, 'directional_contribution': -0.06078522508307371}, {'ion': 1355, 'force': [-0.5799313187599182, -3.2436165809631348, -1.537106990814209], 'magnitude': 3.6359410285949707, 'distance': 9.555658340454102, 'directional_contribution': -2.1268592782617333}, {'ion': 1380, 'force': [2.139223337173462, 1.9624422788619995, -1.0930858850479126], 'magnitude': 3.1019821166992188, 'distance': 10.345450401306152, 'directional_contribution': 2.5012920002790526}, {'ion': 1476, 'force': [-4.092360019683838, 5.589524745941162, -4.061839580535889], 'magnitude': 8.030488014221191, 'distance': 6.429809093475342, 'directional_contribution': -2.161387671528992}, {'ion': 2443, 'force': [3.3623688220977783, -1.7849515676498413, -1.0041723251342773], 'magnitude': 3.9369959831237793, 'distance': 9.1830415725708, 'directional_contribution': 2.0907191092921558}]}, 6162: {'frame': 6162, 'ionic_force': [7.763323903083801, 2.8181435465812683, -6.318853139877319], 'ionic_force_magnitude': 10.398992070228124, 'motion_vector': [-1.7015113830566406, -2.5169944763183594, 0.5141983032226562], 'cosine_ionic_motion': -0.7350036857169278, 'ionic_motion_component': -7.643297499358775, 'ionic_force_x': 7.763323903083801, 'ionic_force_y': 2.8181435465812683, 'ionic_force_z': -6.318853139877319, 'radial_force': 8.259003031439688, 'axial_force': -6.318853139877319, 'contributions': [{'ion': 1327, 'force': [1.9486887454986572, 0.7575831413269043, -2.100437641143799], 'magnitude': 2.963639259338379, 'distance': 10.584158897399902, 'directional_contribution': -2.045389947290012}, {'ion': 1355, 'force': [1.829471230506897, -3.8013644218444824, -1.9934921264648438], 'magnitude': 4.665977478027344, 'distance': 8.435245513916016, 'directional_contribution': 1.7622382018976808}, {'ion': 1380, 'force': [1.3906784057617188, 0.7438085079193115, -0.29142385721206665], 'magnitude': 1.603797197341919, 'distance': 14.387797355651855, 'directional_contribution': -1.424131411579718}, {'ion': 1476, 'force': [0.6493955850601196, 5.551018238067627, -1.8384053707122803], 'magnitude': 5.883472919464111, 'distance': 7.511940956115723, 'directional_contribution': -5.199691748076372}, {'ion': 2443, 'force': [1.9450899362564087, -0.43290191888809204, -0.09509414434432983], 'magnitude': 1.9949489831924438, 'distance': 12.900399208068848, 'directional_contribution': -0.7363227905610161}]}, 6163: {'frame': 6163, 'ionic_force': [5.693150162696838, 11.41169948130846, -10.106098487973213], 'ionic_force_magnitude': 16.271818290385536, 'motion_vector': [-5.470054626464844, -0.9522628784179688, -5.482391357421875], 'cosine_ionic_motion': 0.10551406260941289, 'ionic_motion_component': 1.7169056538607292, 'ionic_force_x': 5.693150162696838, 'ionic_force_y': 11.41169948130846, 'ionic_force_z': -10.106098487973213, 'radial_force': 12.752993524138198, 'axial_force': -10.106098487973213, 'contributions': [{'ion': 1327, 'force': [2.395063638687134, 0.08514890819787979, -3.508793830871582], 'magnitude': 4.249142646789551, 'distance': 8.839310646057129, 'directional_contribution': 0.7759147168334264}, {'ion': 1341, 'force': [0.5789742469787598, -0.06532517075538635, -1.6003326177597046], 'magnitude': 1.7030980587005615, 'distance': 13.962050437927246, 'directional_contribution': 0.7265057019041103}, {'ion': 1355, 'force': [0.5200189352035522, -3.328923225402832, -0.7997344136238098], 'magnitude': 3.462907075881958, 'distance': 9.791486740112305, 'directional_contribution': 0.603615071780343}, {'ion': 1380, 'force': [2.3475747108459473, 0.65799880027771, -0.3588736653327942], 'magnitude': 2.4643173217773438, 'distance': 11.607020378112793, 'directional_contribution': -1.4738744496265603}, {'ion': 1476, 'force': [-2.214129686355591, 15.15945053100586, -3.8823859691619873], 'magnitude': 15.804563522338867, 'distance': 4.583294868469238, 'directional_contribution': 2.429922126119237}, {'ion': 2443, 'force': [2.065648317337036, -1.0966503620147705, 0.044022008776664734], 'magnitude': 2.3391201496124268, 'distance': 11.913593292236328, 'directional_contribution': -1.345177304391929}]}, 6164: {'frame': 6164, 'ionic_force': [0.7338058315217495, -0.6169207841157913, -9.97306752204895], 'ionic_force_magnitude': 10.019038778824891, 'motion_vector': [0.8026161193847656, -1.9557952880859375, 2.9555435180664062], 'cosine_ionic_motion': -0.7602959620299808, 'ionic_motion_component': -7.617434726962355, 'ionic_force_x': 0.7338058315217495, 'ionic_force_y': -0.6169207841157913, 'ionic_force_z': -9.97306752204895, 'radial_force': 0.9586773452258945, 'axial_force': -9.97306752204895, 'contributions': [{'ion': 1327, 'force': [-0.05467653647065163, -0.15348537266254425, -1.8620142936706543], 'magnitude': 1.8691293001174927, 'distance': 13.327520370483398, 'directional_contribution': -1.4439292905769412}, {'ion': 1355, 'force': [-0.5475013852119446, -1.3620316982269287, -1.0494215488433838], 'magnitude': 1.8044871091842651, 'distance': 13.564136505126953, 'directional_contribution': -0.24139666538441507}, {'ion': 1380, 'force': [1.875036597251892, 1.458633303642273, -2.697950601577759], 'magnitude': 3.594761610031128, 'distance': 9.610234260559082, 'directional_contribution': -2.565287626893147}, {'ion': 1476, 'force': [-2.0720303058624268, 1.2611353397369385, -2.7867367267608643], 'magnitude': 3.6945464611053467, 'distance': 9.47956657409668, 'directional_contribution': -3.403010647426644}, {'ion': 2443, 'force': [1.5329774618148804, -1.8211723566055298, -1.576944351196289], 'magnitude': 2.8554232120513916, 'distance': 10.782855987548828, 'directional_contribution': 0.036189325337053546}]}, 6165: {'frame': 6165, 'ionic_force': [0.8527390398085117, -2.051217794418335, -13.607491910457611], 'ionic_force_magnitude': 13.78762105670595, 'motion_vector': [-0.4117393493652344, 4.247417449951172, -2.2331161499023438], 'cosine_ionic_motion': 0.3211122018333723, 'ionic_motion_component': 4.427373355563015, 'ionic_force_x': 0.8527390398085117, 'ionic_force_y': -2.051217794418335, 'ionic_force_z': -13.607491910457611, 'radial_force': 2.221409082126019, 'axial_force': -13.607491910457611, 'contributions': [{'ion': 1327, 'force': [0.062102917581796646, -0.7361721992492676, -2.4836835861206055], 'magnitude': 2.591233491897583, 'distance': 11.319201469421387, 'directional_contribution': 0.49705077928710883}, {'ion': 1355, 'force': [-0.45634692907333374, -1.6045798063278198, -0.6252397894859314], 'magnitude': 1.7815312147140503, 'distance': 13.651247024536133, 'directional_contribution': -1.0861397009811737}, {'ion': 1380, 'force': [4.697567462921143, 1.9251720905303955, -4.4325270652771], 'magnitude': 6.739490032196045, 'distance': 7.018681526184082, 'directional_contribution': 3.351355452952653}, {'ion': 1476, 'force': [-5.758725166320801, 1.1061946153640747, -4.493953704833984], 'magnitude': 7.38797664642334, 'distance': 6.703571796417236, 'directional_contribution': 3.5514878332571698}, {'ion': 2443, 'force': [2.308140754699707, -2.7418324947357178, -1.5720877647399902], 'magnitude': 3.9136452674865723, 'distance': 9.210395812988281, 'directional_contribution': -1.88638086113815}]}, 6166: {'frame': 6166, 'ionic_force': [1.4523009806871414, 1.297539383172989, -11.587992548942566], 'ionic_force_magnitude': 11.750504580814315, 'motion_vector': [2.0425567626953125, -2.522167205810547, 0.7178115844726562], 'cosine_ionic_motion': -0.22080468377105897, 'ionic_motion_component': -2.5945664481170847, 'ionic_force_x': 1.4523009806871414, 'ionic_force_y': 1.297539383172989, 'ionic_force_z': -11.587992548942566, 'radial_force': 1.9475077893014379, 'axial_force': -11.587992548942566, 'contributions': [{'ion': 1327, 'force': [0.08723576366901398, 0.26207712292671204, -2.5743675231933594], 'magnitude': 2.5891432762145996, 'distance': 11.323769569396973, 'directional_contribution': -0.7011933863444675}, {'ion': 1355, 'force': [-0.8347313404083252, -2.0121395587921143, -1.8562531471252441], 'magnitude': 2.8620200157165527, 'distance': 10.770421981811523, 'directional_contribution': 0.6129840574588599}, {'ion': 1380, 'force': [1.436957836151123, 2.019728899002075, -1.8128858804702759], 'magnitude': 3.0709457397460938, 'distance': 10.39759635925293, 'directional_contribution': -1.041032571015542}, {'ion': 1476, 'force': [-1.8430176973342896, 1.9066798686981201, -2.2257046699523926], 'magnitude': 3.462066411972046, 'distance': 9.792675018310547, 'directional_contribution': -3.0599382305185827}, {'ion': 2443, 'force': [2.605856418609619, -0.8788069486618042, -3.118781328201294], 'magnitude': 4.158074855804443, 'distance': 8.935583114624023, 'directional_contribution': 1.5946137473633613}]}, 6167: {'frame': 6167, 'ionic_force': [1.0688188672065735, 1.0091578364372253, -11.419165134429932], 'ionic_force_magnitude': 11.513388105901736, 'motion_vector': [-0.13602447509765625, -1.4195594787597656, 3.152008056640625], 'cosine_ionic_motion': -0.9432504973964883, 'ionic_motion_component': -10.860009057610624, 'ionic_force_x': 1.0688188672065735, 'ionic_force_y': 1.0091578364372253, 'ionic_force_z': -11.419165134429932, 'radial_force': 1.4699569074430054, 'axial_force': -11.419165134429932, 'contributions': [{'ion': 1327, 'force': [0.37463992834091187, -0.28571516275405884, -2.148576259613037], 'magnitude': 2.199629068374634, 'distance': 12.285541534423828, 'directional_contribution': -1.8550431665611884}, {'ion': 1355, 'force': [-0.322290301322937, -1.734464168548584, -1.1195731163024902], 'magnitude': 2.089421033859253, 'distance': 12.605382919311523, 'directional_contribution': -0.2956671842401728}, {'ion': 1380, 'force': [2.3296315670013428, 1.3743340969085693, -2.2760865688323975], 'magnitude': 3.535045623779297, 'distance': 9.691065788269043, 'directional_contribution': -2.729243149966913}, {'ion': 1476, 'force': [-3.17857027053833, 2.7836079597473145, -4.389988899230957], 'magnitude': 6.092929363250732, 'distance': 7.381692886352539, 'directional_contribution': -5.016890211807125}, {'ion': 2443, 'force': [1.865407943725586, -1.1286048889160156, -1.4849402904510498], 'magnitude': 2.6379051208496094, 'distance': 11.218620300292969, 'directional_contribution': -0.9631653441107701}]}, 6168: {'frame': 6168, 'ionic_force': [-7.520926967263222, 6.472836136817932, -23.5761159658432], 'ionic_force_magnitude': 25.579194556042808, 'motion_vector': [-0.9997520446777344, 3.4777908325195312, -1.7257232666015625], 'cosine_ionic_motion': 0.6895845985397099, 'ionic_motion_component': 17.639018608897914, 'ionic_force_x': -7.520926967263222, 'ionic_force_y': 6.472836136817932, 'ionic_force_z': -23.5761159658432, 'radial_force': 9.922799509261651, 'axial_force': -23.5761159658432, 'contributions': [{'ion': 1327, 'force': [1.1435531377792358, -1.7503900527954102, -4.134721279144287], 'magnitude': 4.633303165435791, 'distance': 8.464936256408691, 'directional_contribution': -0.023789899881023757}, {'ion': 1341, 'force': [0.19866521656513214, -0.4084584712982178, -1.6042498350143433], 'magnitude': 1.667310357093811, 'distance': 14.111098289489746, 'directional_contribution': 0.2866853847935005}, {'ion': 1355, 'force': [-0.2531542479991913, -2.0059866905212402, -0.5837475061416626], 'magnitude': 2.104478597640991, 'distance': 12.560206413269043, 'directional_contribution': -1.4257476217592426}, {'ion': 1380, 'force': [4.757066249847412, 1.4454026222229004, -1.5462619066238403], 'magnitude': 5.206706523895264, 'distance': 7.985230922698975, 'directional_contribution': 0.7331725904093531}, {'ion': 1476, 'force': [-15.625587463378906, 11.02933120727539, -14.86202335357666], 'magnitude': 24.22157859802246, 'distance': 3.702267646789551, 'directional_contribution': 19.861746642845787}, {'ion': 2443, 'force': [2.2585301399230957, -1.8370624780654907, -0.8451120853424072], 'magnitude': 3.031496524810791, 'distance': 10.465030670166016, 'directional_contribution': -1.7930485609347073}]}, 6169: {'frame': 6169, 'ionic_force': [3.391502261161804, 2.702711671590805, -11.971076011657715], 'ionic_force_magnitude': 12.732383863366104, 'motion_vector': [0.38364410400390625, 1.7301025390625, 2.6249771118164062], 'cosine_ionic_motion': -0.631031291326958, 'ionic_motion_component': -8.034532630970435, 'ionic_force_x': 3.391502261161804, 'ionic_force_y': 2.702711671590805, 'ionic_force_z': -11.971076011657715, 'radial_force': 4.336696665345501, 'axial_force': -11.971076011657715, 'contributions': [{'ion': 1327, 'force': [0.43922919034957886, 0.3048649728298187, -4.18452787399292], 'magnitude': 4.2185468673706055, 'distance': 8.871306419372559, 'directional_contribution': -3.2484350091106715}, {'ion': 1355, 'force': [-1.1267592906951904, -3.0149948596954346, -1.965143084526062], 'magnitude': 3.7711493968963623, 'distance': 9.382793426513672, 'directional_contribution': -3.4121921389138965}, {'ion': 1380, 'force': [1.8862299919128418, 2.4746272563934326, -1.5418955087661743], 'magnitude': 3.4726195335388184, 'distance': 9.77778434753418, 'directional_contribution': 0.302339534481046}, {'ion': 1476, 'force': [-0.951141893863678, 4.275298595428467, -2.218920946121216], 'magnitude': 4.909832954406738, 'distance': 8.223102569580078, 'directional_contribution': 0.38115726637054026}, {'ion': 2443, 'force': [3.143944263458252, -1.3370842933654785, -2.0605885982513428], 'magnitude': 3.989762544631958, 'distance': 9.122114181518555, 'directional_contribution': -2.057402172322913}]}, 6170: {'frame': 6170, 'ionic_force': [5.667690142989159, 1.7710587978363037, -13.184255957603455], 'ionic_force_magnitude': 14.459736027256238, 'motion_vector': [3.7403221130371094, -1.5651435852050781, 1.4440078735351562], 'cosine_ionic_motion': -0.009819873621377127, 'ionic_motion_component': -0.14199278038613003, 'ionic_force_x': 5.667690142989159, 'ionic_force_y': 1.7710587978363037, 'ionic_force_z': -13.184255957603455, 'radial_force': 5.9379593146408345, 'axial_force': -13.184255957603455, 'contributions': [{'ion': 1327, 'force': [1.4770755767822266, 2.068378448486328, -6.052678108215332], 'magnitude': 6.564666748046875, 'distance': 7.1115241050720215, 'directional_contribution': -1.499212623473511}, {'ion': 1341, 'force': [0.2155987173318863, 0.3436358571052551, -2.0001230239868164], 'magnitude': 2.0408480167388916, 'distance': 12.754508018493652, 'directional_contribution': -0.6086417278985303}, {'ion': 1355, 'force': [-2.284257650375366, -6.364039421081543, -2.5249183177948], 'magnitude': 7.217620372772217, 'distance': 6.782222270965576, 'directional_contribution': -0.5179368895331322}, {'ion': 1380, 'force': [1.8270621299743652, 2.4519355297088623, -0.6305731534957886], 'magnitude': 3.1221413612365723, 'distance': 10.311996459960938, 'directional_contribution': 0.4845709438187029}, {'ion': 1476, 'force': [-0.3435497581958771, 4.183430194854736, -0.503319263458252], 'magnitude': 4.22758150100708, 'distance': 8.861822128295898, 'directional_contribution': -1.9886975530248403}, {'ion': 2443, 'force': [4.775761127471924, -0.9122818112373352, -1.4726440906524658], 'magnitude': 5.080239295959473, 'distance': 8.084012031555176, 'directional_contribution': 3.9879252955995987}]}, 6171: {'frame': 6171, 'ionic_force': [10.627623319625854, -0.529610387980938, -5.966325297951698], 'ionic_force_magnitude': 12.19934023412295, 'motion_vector': [-1.0708656311035156, 1.0283088684082031, -2.1849288940429688], 'cosine_ionic_motion': 0.0344641513177246, 'ionic_motion_component': 0.4204399078052192, 'ionic_force_x': 10.627623319625854, 'ionic_force_y': -0.529610387980938, 'ionic_force_z': -5.966325297951698, 'radial_force': 10.640811274847072, 'axial_force': -5.966325297951698, 'contributions': [{'ion': 1327, 'force': [3.3019585609436035, 0.4475037753582001, -3.7688305377960205], 'magnitude': 5.030633449554443, 'distance': 8.123771667480469, 'directional_contribution': 1.9529192173632346}, {'ion': 1341, 'force': [0.8308365941047668, 0.05887822061777115, -1.8445522785186768], 'magnitude': 2.0238895416259766, 'distance': 12.807832717895508, 'directional_contribution': 1.2117799274345193}, {'ion': 1355, 'force': [0.8886405825614929, -4.7136969566345215, -0.3486242890357971], 'magnitude': 4.809382438659668, 'distance': 8.308533668518066, 'directional_contribution': -1.9068059919821962}, {'ion': 1380, 'force': [2.0485944747924805, 1.2774423360824585, -0.12629811465740204], 'magnitude': 2.4175503253936768, 'distance': 11.71875, 'directional_contribution': -0.22872886755479094}, {'ion': 1476, 'force': [0.9028506278991699, 3.0675549507141113, 0.21530672907829285], 'magnitude': 3.2049007415771484, 'distance': 10.177983283996582, 'directional_contribution': 0.6500332783282765}, {'ion': 2443, 'force': [2.654742479324341, -0.6672927141189575, -0.09332680702209473], 'magnitude': 2.7389135360717773, 'distance': 11.009811401367188, 'directional_contribution': -1.2587577407312978}]}, 6172: {'frame': 6172, 'ionic_force': [7.3180464617908, 0.31938037276268005, -8.137867994606495], 'ionic_force_magnitude': 10.94900467335162, 'motion_vector': [0.2743377685546875, -2.2898902893066406, -0.9024124145507812], 'cosine_ionic_motion': 0.31789813815261664, 'ionic_motion_component': 3.4806682002827785, 'ionic_force_x': 7.3180464617908, 'ionic_force_y': 0.31938037276268005, 'ionic_force_z': -8.137867994606495, 'radial_force': 7.325012480496868, 'axial_force': -8.137867994606495, 'contributions': [{'ion': 1327, 'force': [1.9322783946990967, 0.7810750007629395, -3.4608781337738037], 'magnitude': 4.039981842041016, 'distance': 9.065240859985352, 'directional_contribution': 0.7529322689500795}, {'ion': 1341, 'force': [0.4868040978908539, 0.19157400727272034, -1.5694613456726074], 'magnitude': 1.654354214668274, 'distance': 14.16624641418457, 'directional_contribution': 0.4486786489014434}, {'ion': 1355, 'force': [0.41514936089515686, -4.178457260131836, -1.8555198907852173], 'magnitude': 4.590730667114258, 'distance': 8.504095077514648, 'directional_contribution': 4.585665498980331}, {'ion': 1380, 'force': [1.7028212547302246, 1.3459678888320923, -0.46063730120658875], 'magnitude': 2.2188773155212402, 'distance': 12.232138633728027, 'directional_contribution': -0.8880508790419137}, {'ion': 1476, 'force': [0.054844509810209274, 2.683497667312622, -0.06307730823755264], 'magnitude': 2.6847991943359375, 'distance': 11.120214462280273, 'directional_contribution': -2.4521990200139596}, {'ion': 2443, 'force': [2.726148843765259, -0.5042769312858582, -0.7282940149307251], 'magnitude': 2.8664603233337402, 'distance': 10.762076377868652, 'directional_contribution': 1.033641706957674}]}, 6173: {'frame': 6173, 'ionic_force': [6.784936279058456, 2.012464940547943, -7.050760209560394], 'ionic_force_magnitude': 9.989924673416631, 'motion_vector': [-1.894927978515625, 0.30248260498046875, -0.6227035522460938], 'cosine_ionic_motion': -0.3898840075180566, 'ionic_motion_component': -3.8949118664751885, 'ionic_force_x': 6.784936279058456, 'ionic_force_y': 2.012464940547943, 'ionic_force_z': -7.050760209560394, 'radial_force': 7.077102192834173, 'axial_force': -7.050760209560394, 'contributions': [{'ion': 1327, 'force': [1.4346952438354492, -0.13320499658584595, -2.9370408058166504], 'magnitude': 3.271437406539917, 'distance': 10.073948860168457, 'directional_contribution': -0.4609986571066518}, {'ion': 1355, 'force': [0.2875460088253021, -2.611074686050415, -1.1207534074783325], 'magnitude': 2.8559556007385254, 'distance': 10.781850814819336, 'directional_contribution': -0.31564307335446173}, {'ion': 1380, 'force': [2.0091943740844727, 1.0707746744155884, -0.7834347486495972], 'magnitude': 2.407735586166382, 'distance': 11.742610931396484, 'directional_contribution': -1.484832807733362}, {'ion': 1476, 'force': [0.7840487957000732, 4.45212459564209, -1.336418628692627], 'magnitude': 4.714038848876953, 'distance': 8.392135620117188, 'directional_contribution': 0.34358971695424145}, {'ion': 2443, 'force': [2.269451856613159, -0.7661546468734741, -0.8731126189231873], 'magnitude': 2.549456834793091, 'distance': 11.411564826965332, 'directional_contribution': -1.9770271258294603}]}, 6174: {'frame': 6174, 'ionic_force': [5.039700031280518, -0.18618684448301792, -7.465847820043564], 'ionic_force_magnitude': 9.009557459631223, 'motion_vector': [-4.1372528076171875, 1.9846878051757812, -0.39879608154296875], 'cosine_ionic_motion': -0.4396073734925297, 'ionic_motion_component': -3.96066789115851, 'ionic_force_x': 5.039700031280518, 'ionic_force_y': -0.18618684448301792, 'ionic_force_z': -7.465847820043564, 'radial_force': 5.043138105024231, 'axial_force': -7.465847820043564, 'contributions': [{'ion': 1327, 'force': [0.8549860119819641, -0.021522456780076027, -3.1400513648986816], 'magnitude': 3.254441022872925, 'distance': 10.1002197265625, 'directional_contribution': -0.5053815979560157}, {'ion': 1355, 'force': [-0.40528932213783264, -2.981875419616699, -1.5683804750442505], 'magnitude': 3.393472671508789, 'distance': 9.891151428222656, 'directional_contribution': -0.7850355044918764}, {'ion': 1380, 'force': [2.649775981903076, 1.5303508043289185, -1.275815725326538], 'magnitude': 3.3152663707733154, 'distance': 10.007136344909668, 'directional_contribution': -1.6102464920614352}, {'ion': 1476, 'force': [-0.39551082253456116, 2.728090524673462, -0.4340073764324188], 'magnitude': 2.7905678749084473, 'distance': 10.907437324523926, 'directional_contribution': 1.5683622750861201}, {'ion': 2443, 'force': [2.335738182067871, -1.441230297088623, -1.0475928783416748], 'magnitude': 2.9377317428588867, 'distance': 10.63072681427002, 'directional_contribution': -2.6283664235292683}]}, 6175: {'frame': 6175, 'ionic_force': [3.0340373516082764, 0.5058518648147583, -13.789096742868423], 'ionic_force_magnitude': 14.128002609862277, 'motion_vector': [1.6478233337402344, -1.9370346069335938, 6.6754608154296875], 'cosine_ionic_motion': -0.8722379391731214, 'ionic_motion_component': -12.322979881058753, 'ionic_force_x': 3.0340373516082764, 'ionic_force_y': 0.5058518648147583, 'ionic_force_z': -13.789096742868423, 'radial_force': 3.0759175476743086, 'axial_force': -13.789096742868423, 'contributions': [{'ion': 1327, 'force': [-0.6416452527046204, 0.5911756753921509, -3.6269683837890625], 'magnitude': 3.730428457260132, 'distance': 9.433865547180176, 'directional_contribution': -3.697659769813785}, {'ion': 1355, 'force': [-1.5452637672424316, -2.1077585220336914, -1.4997599124908447], 'magnitude': 3.0132648944854736, 'distance': 10.496642112731934, 'directional_contribution': -1.1864130704633098}, {'ion': 1380, 'force': [1.5424033403396606, 3.1613669395446777, -1.868808627128601], 'magnitude': 3.9831764698028564, 'distance': 9.129652976989746, 'directional_contribution': -2.247818183510285}, {'ion': 1476, 'force': [-0.9063621163368225, 1.9885385036468506, -0.29560258984565735], 'magnitude': 2.2052571773529053, 'distance': 12.269855499267578, 'directional_contribution': -1.0245263391440131}, {'ion': 2443, 'force': [4.58490514755249, -3.1274707317352295, -6.497957229614258], 'magnitude': 8.545517921447754, 'distance': 6.233038902282715, 'directional_contribution': -4.166562787615533}]}, 6176: {'frame': 6176, 'ionic_force': [5.311269089579582, -3.3787199184298515, -8.04486072063446], 'ionic_force_magnitude': 10.214945503698264, 'motion_vector': [-0.2370452880859375, -0.42974090576171875, -0.37250518798828125], 'cosine_ionic_motion': 0.5068002522900235, 'ionic_motion_component': 5.176936958403121, 'ionic_force_x': 5.311269089579582, 'ionic_force_y': -3.3787199184298515, 'ionic_force_z': -8.04486072063446, 'radial_force': 6.294865179582335, 'axial_force': -8.04486072063446, 'contributions': [{'ion': 1327, 'force': [-0.29267406463623047, 0.06538949906826019, -12.753213882446289], 'magnitude': 12.756739616394043, 'distance': 5.101515293121338, 'directional_contribution': 7.777321580484438}, {'ion': 1341, 'force': [-0.13413138687610626, 0.03554346412420273, -3.4107306003570557], 'magnitude': 3.4135520458221436, 'distance': 9.862017631530762, 'directional_contribution': 2.0888705206918945}, {'ion': 1355, 'force': [-1.3672962188720703, -3.3759875297546387, 0.6790082454681396], 'magnitude': 3.7051103115081787, 'distance': 9.466042518615723, 'directional_contribution': 2.4701824996911625}, {'ion': 1380, 'force': [3.2133100032806396, 3.5890440940856934, 1.645267367362976], 'magnitude': 5.090530872344971, 'distance': 8.075836181640625, 'directional_contribution': -4.734203521272185}, {'ion': 1476, 'force': [-0.8967666625976562, 2.297664165496826, 1.0266220569610596], 'magnitude': 2.6715919971466064, 'distance': 11.147665977478027, 'directional_contribution': -1.878224073124585}, {'ion': 2443, 'force': [4.788827419281006, -5.990373611450195, 4.768186092376709], 'magnitude': 9.030672073364258, 'distance': 6.063299179077148, 'directional_contribution': -0.5470101022199714}]}, 6177: {'frame': 6177, 'ionic_force': [5.809409823268652, -1.0547351241111755, -6.200492262840271], 'ionic_force_magnitude': 8.561998188405916, 'motion_vector': [0.2750663757324219, 0.47098541259765625, 0.6195907592773438], 'cosine_ionic_motion': -0.3877652637674757, 'ionic_motion_component': -3.320045485903869, 'ionic_force_x': 5.809409823268652, 'ionic_force_y': -1.0547351241111755, 'ionic_force_z': -6.200492262840271, 'radial_force': 5.904380465105897, 'axial_force': -6.200492262840271, 'contributions': [{'ion': 1327, 'force': [-0.6801349520683289, -1.2623990774154663, -10.40715503692627], 'magnitude': 10.50547981262207, 'distance': 5.621614933013916, 'directional_contribution': -8.7585651273188}, {'ion': 1341, 'force': [0.033730413764715195, -0.4598913788795471, -3.558413505554199], 'magnitude': 3.588167428970337, 'distance': 9.619061470031738, 'directional_contribution': -2.922114839486337}, {'ion': 1355, 'force': [-1.0431877374649048, -2.8463425636291504, 0.40366053581237793], 'magnitude': 3.0582427978515625, 'distance': 10.419168472290039, 'directional_contribution': -1.6686818151427971}, {'ion': 1380, 'force': [4.841607570648193, 4.804633617401123, 2.4913699626922607], 'magnitude': 7.261721134185791, 'distance': 6.7615966796875, 'directional_contribution': 6.2247907429244975}, {'ion': 1476, 'force': [-1.8445395231246948, 3.831808090209961, 1.4749726057052612], 'magnitude': 4.501180171966553, 'distance': 8.588273048400879, 'directional_contribution': 2.678795687712494}, {'ion': 2443, 'force': [4.501934051513672, -5.122543811798096, 3.395073175430298], 'magnitude': 7.618030071258545, 'distance': 6.601576805114746, 'directional_contribution': 1.1257299612341427}]}, 6178: {'frame': 6178, 'ionic_force': [3.472423955798149, -2.8070406317710876, -14.133636057376862], 'ionic_force_magnitude': 14.822175057649199, 'motion_vector': [-0.18217086791992188, -0.012928009033203125, -0.131744384765625], 'cosine_ionic_motion': 0.379216095936226, 'ionic_motion_component': 5.620807358645035, 'ionic_force_x': 3.472423955798149, 'ionic_force_y': -2.8070406317710876, 'ionic_force_z': -14.133636057376862, 'radial_force': 4.465109767655739, 'axial_force': -14.133636057376862, 'contributions': [{'ion': 1327, 'force': [-0.331557959318161, -0.4524635970592499, -16.043027877807617], 'magnitude': 16.052831649780273, 'distance': 4.547714710235596, 'directional_contribution': 9.68000976026046}, {'ion': 1341, 'force': [0.23961241543293, -0.10964533686637878, -4.009993553161621], 'magnitude': 4.018641948699951, 'distance': 9.089278221130371, 'directional_contribution': 2.158462228245467}, {'ion': 1355, 'force': [-1.1559723615646362, -2.685532808303833, 0.5706928372383118], 'magnitude': 2.9789342880249023, 'distance': 10.556953430175781, 'directional_contribution': 0.7554442795793159}, {'ion': 1380, 'force': [2.535071849822998, 2.90694260597229, 1.7361681461334229], 'magnitude': 4.22979736328125, 'distance': 8.859500885009766, 'directional_contribution': -3.23341136588978}, {'ion': 1476, 'force': [-0.7417896389961243, 2.057465076446533, 0.9261471033096313], 'magnitude': 2.3751132488250732, 'distance': 11.822978019714355, 'directional_contribution': -0.05986603743883556}, {'ion': 2443, 'force': [2.9270596504211426, -4.523806571960449, 2.6863772869110107], 'magnitude': 6.020724773406982, 'distance': 7.425824165344238, 'directional_contribution': -3.679831175497899}]}, 6179: {'frame': 6179, 'ionic_force': [5.215108044445515, -1.9847309440374374, -8.265763878822327], 'ionic_force_magnitude': 9.972931431424964, 'motion_vector': [0.3474769592285156, 0.08895492553710938, 0.16173553466796875], 'cosine_ionic_motion': 0.07612476863893897, 'ionic_motion_component': 0.7591870978692278, 'ionic_force_x': 5.215108044445515, 'ionic_force_y': -1.9847309440374374, 'ionic_force_z': -8.265763878822327, 'radial_force': 5.580009752272845, 'axial_force': -8.265763878822327, 'contributions': [{'ion': 1327, 'force': [-0.5457229614257812, -0.6229351162910461, -11.6111478805542], 'magnitude': 11.640645027160645, 'distance': 5.340482711791992, 'directional_contribution': -5.3956409530846985}, {'ion': 1341, 'force': [-0.025661997497081757, -0.12179915606975555, -3.3184821605682373], 'magnitude': 3.3208155632019043, 'distance': 9.998771667480469, 'directional_contribution': -1.4142901479638785}, {'ion': 1355, 'force': [-1.6094934940338135, -3.451591968536377, 0.6286934614181519], 'magnitude': 3.859949827194214, 'distance': 9.274237632751465, 'directional_contribution': -1.9433077951855147}, {'ion': 1380, 'force': [5.008050918579102, 3.347334384918213, 2.4847280979156494], 'magnitude': 6.516064167022705, 'distance': 7.137997150421143, 'directional_contribution': 6.200900971336765}, {'ion': 1476, 'force': [-0.9970760941505432, 2.8267033100128174, 1.0348708629608154], 'magnitude': 3.1710205078125, 'distance': 10.23221206665039, 'directional_contribution': 0.1839155470826519}, {'ion': 2443, 'force': [3.385011672973633, -3.962442398071289, 2.515573740005493], 'magnitude': 5.786827087402344, 'distance': 7.574409484863281, 'directional_contribution': 3.127609384171542}]}, 6180: {'frame': 6180, 'ionic_force': [0.31373659893870354, 2.3904974460601807, -6.461094975471497], 'ionic_force_magnitude': 6.8962784873580105, 'motion_vector': [-0.304931640625, -0.2544441223144531, 0.2266845703125], 'cosine_ionic_motion': -0.6876470124269158, 'ionic_motion_component': -4.742205298695747, 'ionic_force_x': 0.31373659893870354, 'ionic_force_y': 2.39</t>
+          <t>{6160: {'frame': 6160, 'ionic_force': [3.740715362073388, 2.176445934921503, -12.598692059516907], 'ionic_force_magnitude': 13.321295355115527, 'motion_vector': [2.4038047790527344, -0.042205810546875, -2.1078033447265625], 'cosine_ionic_motion': 0.8324384974001108, 'ionic_motion_component': 11.089159088835444, 'ionic_force_x': 3.740715362073388, 'ionic_force_y': 2.176445934921503, 'ionic_force_z': -12.598692059516907, 'radial_force': 4.327801789325404, 'axial_force': -12.598692059516907, 'contributions': [{'ion': 1327, 'force': [-0.22856654226779938, 0.7065204977989197, -8.549403190612793], 'magnitude': 8.581591606140137, 'distance': 6.219924449920654, 'cosine_with_motion': 0.6356556463125634, 'motion_component': 5.454936947654412}, {'ion': 1341, 'force': [-0.0005797222838737071, 0.04265621677041054, -2.332738161087036], 'magnitude': 2.3331282138824463, 'distance': 11.928881645202637, 'cosine_with_motion': 0.6587010552503938, 'motion_component': 1.5368340101219817}, {'ion': 1355, 'force': [-1.527624487876892, -3.6898083686828613, -0.8481869697570801], 'magnitude': 4.082614898681641, 'distance': 9.017784118652344, 'cosine_with_motion': -0.13242233380003088, 'motion_component': -0.5406293782664431}, {'ion': 1380, 'force': [5.1329145431518555, 4.496638774871826, -0.7909724116325378], 'magnitude': 6.869658946990967, 'distance': 6.95186710357666, 'cosine_with_motion': 0.6290118362515426, 'motion_component': 4.321096572897298}, {'ion': 1476, 'force': [-4.47384786605835, 4.564768314361572, -0.8368766903877258], 'magnitude': 6.446145057678223, 'distance': 7.176604270935059, 'cosine_with_motion': -0.4455485038776503, 'motion_component': -2.872070320188927}, {'ion': 2443, 'force': [4.838419437408447, -3.9443295001983643, 0.7594853639602661], 'magnitude': 6.288470268249512, 'distance': 7.266019344329834, 'cosine_with_motion': 0.507117132671062, 'motion_component': 3.1889909130123653}]}, 6161: {'frame': 6161, 'ionic_force': [2.045816570520401, 2.513314615935087, -12.963244438171387], 'ionic_force_magnitude': 13.362178795491031, 'motion_vector': [4.460853576660156, 2.02520751953125, 0.9477462768554688], 'cosine_ionic_motion': 0.02894916806440939, 'ionic_motion_component': 0.3868239596573573, 'ionic_force_x': 2.045816570520401, 'ionic_force_y': 2.513314615935087, 'ionic_force_z': -12.963244438171387, 'radial_force': 3.2406968076154223, 'axial_force': -12.963244438171387, 'contributions': [{'ion': 1327, 'force': [0.9507448077201843, 0.019289210438728333, -3.7588417530059814], 'magnitude': 3.8772642612457275, 'distance': 9.253506660461426, 'cosine_with_motion': 0.03709964672148767, 'motion_component': 0.14384513881447392}, {'ion': 1341, 'force': [0.26577094197273254, -0.029373470693826675, -1.5081979036331177], 'magnitude': 1.531717300415039, 'distance': 14.722437858581543, 'cosine_with_motion': -0.03968436262683752, 'motion_component': -0.06078522508307371}, {'ion': 1355, 'force': [-0.5799313187599182, -3.2436165809631348, -1.537106990814209], 'magnitude': 3.6359410285949707, 'distance': 9.555658340454102, 'cosine_with_motion': -0.5849542921591248, 'motion_component': -2.1268592782617333}, {'ion': 1380, 'force': [2.139223337173462, 1.9624422788619995, -1.0930858850479126], 'magnitude': 3.1019821166992188, 'distance': 10.345450401306152, 'cosine_with_motion': 0.8063528161229908, 'motion_component': 2.5012920002790526}, {'ion': 1476, 'force': [-4.092360019683838, 5.589524745941162, -4.061839580535889], 'magnitude': 8.030488014221191, 'distance': 6.429809093475342, 'cosine_with_motion': -0.2691477355049505, 'motion_component': -2.161387671528992}, {'ion': 2443, 'force': [3.3623688220977783, -1.7849515676498413, -1.0041723251342773], 'magnitude': 3.9369959831237793, 'distance': 9.1830415725708, 'cosine_with_motion': 0.5310442425551404, 'motion_component': 2.0907191092921558}]}, 6162: {'frame': 6162, 'ionic_force': [7.763323903083801, 2.8181435465812683, -6.318853139877319], 'ionic_force_magnitude': 10.398992070228124, 'motion_vector': [-1.7015113830566406, -2.5169944763183594, 0.5141983032226562], 'cosine_ionic_motion': -0.7350036857169278, 'ionic_motion_component': -7.643297499358775, 'ionic_force_x': 7.763323903083801, 'ionic_force_y': 2.8181435465812683, 'ionic_force_z': -6.318853139877319, 'radial_force': 8.259003031439688, 'axial_force': -6.318853139877319, 'contributions': [{'ion': 1327, 'force': [1.9486887454986572, 0.7575831413269043, -2.100437641143799], 'magnitude': 2.963639259338379, 'distance': 10.584158897399902, 'cosine_with_motion': -0.690161551578687, 'motion_component': -2.045389947290012}, {'ion': 1355, 'force': [1.829471230506897, -3.8013644218444824, -1.9934921264648438], 'magnitude': 4.665977478027344, 'distance': 8.435245513916016, 'cosine_with_motion': 0.3776782357281483, 'motion_component': 1.7622382018976808}, {'ion': 1380, 'force': [1.3906784057617188, 0.7438085079193115, -0.29142385721206665], 'magnitude': 1.603797197341919, 'distance': 14.387797355651855, 'cosine_with_motion': -0.8879747581624139, 'motion_component': -1.424131411579718}, {'ion': 1476, 'force': [0.6493955850601196, 5.551018238067627, -1.8384053707122803], 'magnitude': 5.883472919464111, 'distance': 7.511940956115723, 'cosine_with_motion': -0.8837793439367987, 'motion_component': -5.199691748076372}, {'ion': 2443, 'force': [1.9450899362564087, -0.43290191888809204, -0.09509414434432983], 'magnitude': 1.9949489831924438, 'distance': 12.900399208068848, 'cosine_with_motion': -0.369093526402772, 'motion_component': -0.7363227905610161}]}, 6163: {'frame': 6163, 'ionic_force': [5.693150162696838, 11.41169948130846, -10.106098487973213], 'ionic_force_magnitude': 16.271818290385536, 'motion_vector': [-5.470054626464844, -0.9522628784179688, -5.482391357421875], 'cosine_ionic_motion': 0.10551406260941289, 'ionic_motion_component': 1.7169056538607292, 'ionic_force_x': 5.693150162696838, 'ionic_force_y': 11.41169948130846, 'ionic_force_z': -10.106098487973213, 'radial_force': 12.752993524138198, 'axial_force': -10.106098487973213, 'contributions': [{'ion': 1327, 'force': [2.395063638687134, 0.08514890819787979, -3.508793830871582], 'magnitude': 4.249142646789551, 'distance': 8.839310646057129, 'cosine_with_motion': 0.18260500011970154, 'motion_component': 0.7759147168334264}, {'ion': 1341, 'force': [0.5789742469787598, -0.06532517075538635, -1.6003326177597046], 'magnitude': 1.7030980587005615, 'distance': 13.962050437927246, 'cosine_with_motion': 0.4265788997687441, 'motion_component': 0.7265057019041103}, {'ion': 1355, 'force': [0.5200189352035522, -3.328923225402832, -0.7997344136238098], 'magnitude': 3.462907075881958, 'distance': 9.791486740112305, 'cosine_with_motion': 0.1743087750944642, 'motion_component': 0.603615071780343}, {'ion': 1380, 'force': [2.3475747108459473, 0.65799880027771, -0.3588736653327942], 'magnitude': 2.4643173217773438, 'distance': 11.607020378112793, 'cosine_with_motion': -0.5980863138118124, 'motion_component': -1.4738744496265603}, {'ion': 1476, 'force': [-2.214129686355591, 15.15945053100586, -3.8823859691619873], 'magnitude': 15.804563522338867, 'distance': 4.583294868469238, 'cosine_with_motion': 0.15374813144196073, 'motion_component': 2.429922126119237}, {'ion': 2443, 'force': [2.065648317337036, -1.0966503620147705, 0.044022008776664734], 'magnitude': 2.3391201496124268, 'distance': 11.913593292236328, 'cosine_with_motion': -0.5750783357621444, 'motion_component': -1.345177304391929}]}, 6164: {'frame': 6164, 'ionic_force': [0.7338058315217495, -0.6169207841157913, -9.97306752204895], 'ionic_force_magnitude': 10.019038778824891, 'motion_vector': [0.8026161193847656, -1.9557952880859375, 2.9555435180664062], 'cosine_ionic_motion': -0.7602959620299808, 'ionic_motion_component': -7.617434726962355, 'ionic_force_x': 0.7338058315217495, 'ionic_force_y': -0.6169207841157913, 'ionic_force_z': -9.97306752204895, 'radial_force': 0.9586773452258945, 'axial_force': -9.97306752204895, 'contributions': [{'ion': 1327, 'force': [-0.05467653647065163, -0.15348537266254425, -1.8620142936706543], 'magnitude': 1.8691293001174927, 'distance': 13.327520370483398, 'cosine_with_motion': -0.772514375988365, 'motion_component': -1.4439292905769412}, {'ion': 1355, 'force': [-0.5475013852119446, -1.3620316982269287, -1.0494215488433838], 'magnitude': 1.8044871091842651, 'distance': 13.564136505126953, 'cosine_with_motion': -0.13377577768711005, 'motion_component': -0.24139666538441507}, {'ion': 1380, 'force': [1.875036597251892, 1.458633303642273, -2.697950601577759], 'magnitude': 3.594761610031128, 'distance': 9.610234260559082, 'cosine_with_motion': -0.7136182945906884, 'motion_component': -2.565287626893147}, {'ion': 1476, 'force': [-2.0720303058624268, 1.2611353397369385, -2.7867367267608643], 'magnitude': 3.6945464611053467, 'distance': 9.47956657409668, 'cosine_with_motion': -0.9210902306061706, 'motion_component': -3.403010647426644}, {'ion': 2443, 'force': [1.5329774618148804, -1.8211723566055298, -1.576944351196289], 'magnitude': 2.8554232120513916, 'distance': 10.782855987548828, 'cosine_with_motion': 0.01267389165193761, 'motion_component': 0.036189325337053546}]}, 6165: {'frame': 6165, 'ionic_force': [0.8527390398085117, -2.051217794418335, -13.607491910457611], 'ionic_force_magnitude': 13.78762105670595, 'motion_vector': [-0.4117393493652344, 4.247417449951172, -2.2331161499023438], 'cosine_ionic_motion': 0.3211122018333723, 'ionic_motion_component': 4.427373355563015, 'ionic_force_x': 0.8527390398085117, 'ionic_force_y': -2.051217794418335, 'ionic_force_z': -13.607491910457611, 'radial_force': 2.221409082126019, 'axial_force': -13.607491910457611, 'contributions': [{'ion': 1327, 'force': [0.062102917581796646, -0.7361721992492676, -2.4836835861206055], 'magnitude': 2.591233491897583, 'distance': 11.319201469421387, 'cosine_with_motion': 0.191820151327965, 'motion_component': 0.49705077928710883}, {'ion': 1355, 'force': [-0.45634692907333374, -1.6045798063278198, -0.6252397894859314], 'magnitude': 1.7815312147140503, 'distance': 13.651247024536133, 'cosine_with_motion': -0.6096663689107369, 'motion_component': -1.0861397009811737}, {'ion': 1380, 'force': [4.697567462921143, 1.9251720905303955, -4.4325270652771], 'magnitude': 6.739490032196045, 'distance': 7.018681526184082, 'cosine_with_motion': 0.4972713830043761, 'motion_component': 3.351355452952653}, {'ion': 1476, 'force': [-5.758725166320801, 1.1061946153640747, -4.493953704833984], 'magnitude': 7.38797664642334, 'distance': 6.703571796417236, 'cosine_with_motion': 0.4807118246685845, 'motion_component': 3.5514878332571698}, {'ion': 2443, 'force': [2.308140754699707, -2.7418324947357178, -1.5720877647399902], 'magnitude': 3.9136452674865723, 'distance': 9.210395812988281, 'cosine_with_motion': -0.48200098437439737, 'motion_component': -1.88638086113815}]}, 6166: {'frame': 6166, 'ionic_force': [1.4523009806871414, 1.297539383172989, -11.587992548942566], 'ionic_force_magnitude': 11.750504580814315, 'motion_vector': [2.0425567626953125, -2.522167205810547, 0.7178115844726562], 'cosine_ionic_motion': -0.22080468377105897, 'ionic_motion_component': -2.5945664481170847, 'ionic_force_x': 1.4523009806871414, 'ionic_force_y': 1.297539383172989, 'ionic_force_z': -11.587992548942566, 'radial_force': 1.9475077893014379, 'axial_force': -11.587992548942566, 'contributions': [{'ion': 1327, 'force': [0.08723576366901398, 0.26207712292671204, -2.5743675231933594], 'magnitude': 2.5891432762145996, 'distance': 11.323769569396973, 'cosine_with_motion': -0.2708206249400485, 'motion_component': -0.7011933863444675}, {'ion': 1355, 'force': [-0.8347313404083252, -2.0121395587921143, -1.8562531471252441], 'magnitude': 2.8620200157165527, 'distance': 10.770421981811523, 'cosine_with_motion': 0.21417882627641824, 'motion_component': 0.6129840574588599}, {'ion': 1380, 'force': [1.436957836151123, 2.019728899002075, -1.8128858804702759], 'magnitude': 3.0709457397460938, 'distance': 10.39759635925293, 'cosine_with_motion': -0.33899412500374865, 'motion_component': -1.041032571015542}, {'ion': 1476, 'force': [-1.8430176973342896, 1.9066798686981201, -2.2257046699523926], 'magnitude': 3.462066411972046, 'distance': 9.792675018310547, 'cosine_with_motion': -0.8838473596501303, 'motion_component': -3.0599382305185827}, {'ion': 2443, 'force': [2.605856418609619, -0.8788069486618042, -3.118781328201294], 'magnitude': 4.158074855804443, 'distance': 8.935583114624023, 'cosine_with_motion': 0.3834980879752371, 'motion_component': 1.5946137473633613}]}, 6167: {'frame': 6167, 'ionic_force': [1.0688188672065735, 1.0091578364372253, -11.419165134429932], 'ionic_force_magnitude': 11.513388105901736, 'motion_vector': [-0.13602447509765625, -1.4195594787597656, 3.152008056640625], 'cosine_ionic_motion': -0.9432504973964883, 'ionic_motion_component': -10.860009057610624, 'ionic_force_x': 1.0688188672065735, 'ionic_force_y': 1.0091578364372253, 'ionic_force_z': -11.419165134429932, 'radial_force': 1.4699569074430054, 'axial_force': -11.419165134429932, 'contributions': [{'ion': 1327, 'force': [0.37463992834091187, -0.28571516275405884, -2.148576259613037], 'magnitude': 2.199629068374634, 'distance': 12.285541534423828, 'cosine_with_motion': -0.8433436197672336, 'motion_component': -1.8550431665611884}, {'ion': 1355, 'force': [-0.322290301322937, -1.734464168548584, -1.1195731163024902], 'magnitude': 2.089421033859253, 'distance': 12.605382919311523, 'cosine_with_motion': -0.14150674080026152, 'motion_component': -0.2956671842401728}, {'ion': 1380, 'force': [2.3296315670013428, 1.3743340969085693, -2.2760865688323975], 'magnitude': 3.535045623779297, 'distance': 9.691065788269043, 'cosine_with_motion': -0.7720531629281498, 'motion_component': -2.729243149966913}, {'ion': 1476, 'force': [-3.17857027053833, 2.7836079597473145, -4.389988899230957], 'magnitude': 6.092929363250732, 'distance': 7.381692886352539, 'cosine_with_motion': -0.8233954713653064, 'motion_component': -5.016890211807125}, {'ion': 2443, 'force': [1.865407943725586, -1.1286048889160156, -1.4849402904510498], 'magnitude': 2.6379051208496094, 'distance': 11.218620300292969, 'cosine_with_motion': -0.36512508896735857, 'motion_component': -0.9631653441107701}]}, 6168: {'frame': 6168, 'ionic_force': [-7.520926967263222, 6.472836136817932, -23.5761159658432], 'ionic_force_magnitude': 25.579194556042808, 'motion_vector': [-0.9997520446777344, 3.4777908325195312, -1.7257232666015625], 'cosine_ionic_motion': 0.6895845985397099, 'ionic_motion_component': 17.639018608897914, 'ionic_force_x': -7.520926967263222, 'ionic_force_y': 6.472836136817932, 'ionic_force_z': -23.5761159658432, 'radial_force': 9.922799509261651, 'axial_force': -23.5761159658432, 'contributions': [{'ion': 1327, 'force': [1.1435531377792358, -1.7503900527954102, -4.134721279144287], 'magnitude': 4.633303165435791, 'distance': 8.464936256408691, 'cosine_with_motion': -0.005134544083482439, 'motion_component': -0.023789899881023757}, {'ion': 1341, 'force': [0.19866521656513214, -0.4084584712982178, -1.6042498350143433], 'magnitude': 1.667310357093811, 'distance': 14.111098289489746, 'cosine_with_motion': 0.1719448265095522, 'motion_component': 0.2866853847935005}, {'ion': 1355, 'force': [-0.2531542479991913, -2.0059866905212402, -0.5837475061416626], 'magnitude': 2.104478597640991, 'distance': 12.560206413269043, 'cosine_with_motion': -0.6774825447554669, 'motion_component': -1.4257476217592426}, {'ion': 1380, 'force': [4.757066249847412, 1.4454026222229004, -1.5462619066238403], 'magnitude': 5.206706523895264, 'distance': 7.985230922698975, 'cosine_with_motion': 0.14081311710588393, 'motion_component': 0.7331725904093531}, {'ion': 1476, 'force': [-15.625587463378906, 11.02933120727539, -14.86202335357666], 'magnitude': 24.22157859802246, 'distance': 3.702267646789551, 'cosine_with_motion': 0.820002155604511, 'motion_component': 19.861746642845787}, {'ion': 2443, 'force': [2.2585301399230957, -1.8370624780654907, -0.8451120853424072], 'magnitude': 3.031496524810791, 'distance': 10.465030670166016, 'cosine_with_motion': -0.591473065178646, 'motion_component': -1.7930485609347073}]}, 6169: {'frame': 6169, 'ionic_force': [3.391502261161804, 2.702711671590805, -11.971076011657715], 'ionic_force_magnitude': 12.732383863366104, 'motion_vector': [0.38364410400390625, 1.7301025390625, 2.6249771118164062], 'cosine_ionic_motion': -0.631031291326958, 'ionic_motion_component': -8.034532630970435, 'ionic_force_x': 3.391502261161804, 'ionic_force_y': 2.702711671590805, 'ionic_force_z': -11.971076011657715, 'radial_force': 4.336696665345501, 'axial_force': -11.971076011657715, 'contributions': [{'ion': 1327, 'force': [0.43922919034957886, 0.3048649728298187, -4.18452787399292], 'magnitude': 4.2185468673706055, 'distance': 8.871306419372559, 'cosine_with_motion': -0.7700364697131815, 'motion_component': -3.2484350091106715}, {'ion': 1355, 'force': [-1.1267592906951904, -3.0149948596954346, -1.965143084526062], 'magnitude': 3.7711493968963623, 'distance': 9.382793426513672, 'cosine_with_motion': -0.904814890937976, 'motion_component': -3.4121921389138965}, {'ion': 1380, 'force': [1.8862299919128418, 2.4746272563934326, -1.5418955087661743], 'magnitude': 3.4726195335388184, 'distance': 9.77778434753418, 'cosine_with_motion': 0.08706382729268759, 'motion_component': 0.302339534481046}, {'ion': 1476, 'force': [-0.951141893863678, 4.275298595428467, -2.218920946121216], 'magnitude': 4.909832954406738, 'distance': 8.223102569580078, 'cosine_with_motion': 0.0776314130857838, 'motion_component': 0.3811572663705402}, {'ion': 2443, 'force': [3.143944263458252, -1.3370842933654785, -2.0605885982513428], 'magnitude': 3.989762544631958, 'distance': 9.122114181518555, 'cosine_with_motion': -0.5156703286833915, 'motion_component': -2.057402172322913}]}, 6170: {'frame': 6170, 'ionic_force': [5.667690142989159, 1.7710587978363037, -13.184255957603455], 'ionic_force_magnitude': 14.459736027256238, 'motion_vector': [3.7403221130371094, -1.5651435852050781, 1.4440078735351562], 'cosine_ionic_motion': -0.009819873621377127, 'ionic_motion_component': -0.14199278038613003, 'ionic_force_x': 5.667690142989159, 'ionic_force_y': 1.7710587978363037, 'ionic_force_z': -13.184255957603455, 'radial_force': 5.9379593146408345, 'axial_force': -13.184255957603455, 'contributions': [{'ion': 1327, 'force': [1.4770755767822266, 2.068378448486328, -6.052678108215332], 'magnitude': 6.564666748046875, 'distance': 7.1115241050720215, 'cosine_with_motion': -0.22837603245973107, 'motion_component': -1.499212623473511}, {'ion': 1341, 'force': [0.2155987173318863, 0.3436358571052551, -2.0001230239868164], 'magnitude': 2.0408480167388916, 'distance': 12.754508018493652, 'cosine_with_motion': -0.2982298195332479, 'motion_component': -0.6086417278985303}, {'ion': 1355, 'force': [-2.284257650375366, -6.364039421081543, -2.5249183177948], 'magnitude': 7.217620372772217, 'distance': 6.782222270965576, 'cosine_with_motion': -0.0717600629576406, 'motion_component': -0.5179368895331322}, {'ion': 1380, 'force': [1.8270621299743652, 2.4519355297088623, -0.6305731534957886], 'magnitude': 3.1221413612365723, 'distance': 10.311996459960938, 'cosine_with_motion': 0.1552046801965146, 'motion_component': 0.4845709438187029}, {'ion': 1476, 'force': [-0.3435497581958771, 4.183430194854736, -0.503319263458252], 'magnitude': 4.22758150100708, 'distance': 8.861822128295898, 'cosine_with_motion': -0.47041022787114467, 'motion_component': -1.9886975530248403}, {'ion': 2443, 'force': [4.775761127471924, -0.9122818112373352, -1.4726440906524658], 'magnitude': 5.080239295959473, 'distance': 8.084012031555176, 'cosine_with_motion': 0.7849876604316632, 'motion_component': 3.9879252955995987}]}, 6171: {'frame': 6171, 'ionic_force': [10.627623319625854, -0.529610387980938, -5.966325297951698], 'ionic_force_magnitude': 12.19934023412295, 'motion_vector': [-1.0708656311035156, 1.0283088684082031, -2.1849288940429688], 'cosine_ionic_motion': 0.0344641513177246, 'ionic_motion_component': 0.4204399078052192, 'ionic_force_x': 10.627623319625854, 'ionic_force_y': -0.529610387980938, 'ionic_force_z': -5.966325297951698, 'radial_force': 10.640811274847072, 'axial_force': -5.966325297951698, 'contributions': [{'ion': 1327, 'force': [3.3019585609436035, 0.4475037753582001, -3.7688305377960205], 'magnitude': 5.030633449554443, 'distance': 8.123771667480469, 'cosine_with_motion': 0.38820542392481705, 'motion_component': 1.9529192173632346}, {'ion': 1341, 'force': [0.8308365941047668, 0.05887822061777115, -1.8445522785186768], 'magnitude': 2.0238895416259766, 'distance': 12.807832717895508, 'cosine_with_motion': 0.5987381498916219, 'motion_component': 1.2117799274345193}, {'ion': 1355, 'force': [0.8886405825614929, -4.7136969566345215, -0.3486242890357971], 'magnitude': 4.809382438659668, 'distance': 8.308533668518066, 'cosine_with_motion': -0.39647626158736854, 'motion_component': -1.9068059919821962}, {'ion': 1380, 'force': [2.0485944747924805, 1.2774423360824585, -0.12629811465740204], 'magnitude': 2.4175503253936768, 'distance': 11.71875, 'cosine_with_motion': -0.09461183391256422, 'motion_component': -0.22872886755479094}, {'ion': 1476, 'force': [0.9028506278991699, 3.0675549507141113, 0.21530672907829285], 'magnitude': 3.2049007415771484, 'distance': 10.177983283996582, 'cosine_with_motion': 0.2028247685813136, 'motion_component': 0.6500332783282765}, {'ion': 2443, 'force': [2.654742479324341, -0.6672927141189575, -0.09332680702209473], 'magnitude': 2.7389135360717773, 'distance': 11.009811401367188, 'cosine_with_motion': -0.45958287714503704, 'motion_component': -1.2587577407312978}]}, 6172: {'frame': 6172, 'ionic_force': [7.3180464617908, 0.31938037276268005, -8.137867994606495], 'ionic_force_magnitude': 10.94900467335162, 'motion_vector': [0.2743377685546875, -2.2898902893066406, -0.9024124145507812], 'cosine_ionic_motion': 0.31789813815261664, 'ionic_motion_component': 3.4806682002827785, 'ionic_force_x': 7.3180464617908, 'ionic_force_y': 0.31938037276268005, 'ionic_force_z': -8.137867994606495, 'radial_force': 7.325012480496868, 'axial_force': -8.137867994606495, 'contributions': [{'ion': 1327, 'force': [1.9322783946990967, 0.7810750007629395, -3.4608781337738037], 'magnitude': 4.039981842041016, 'distance': 9.065240859985352, 'cosine_with_motion': 0.18637019902355048, 'motion_component': 0.7529322689500795}, {'ion': 1341, 'force': [0.4868040978908539, 0.19157400727272034, -1.5694613456726074], 'magnitude': 1.654354214668274, 'distance': 14.16624641418457, 'cosine_with_motion': 0.27121075699936276, 'motion_component': 0.4486786489014434}, {'ion': 1355, 'force': [0.41514936089515686, -4.178457260131836, -1.8555198907852173], 'magnitude': 4.590730667114258, 'distance': 8.504095077514648, 'cosine_with_motion': 0.998896651421923, 'motion_component': 4.585665498980331}, {'ion': 1380, 'force': [1.7028212547302246, 1.3459678888320923, -0.46063730120658875], 'magnitude': 2.2188773155212402, 'distance': 12.232138633728027, 'cosine_with_motion': -0.4002253193375465, 'motion_component': -0.8880508790419137}, {'ion': 1476, 'force': [0.054844509810209274, 2.683497667312622, -0.06307730823755264], 'magnitude': 2.6847991943359375, 'distance': 11.120214462280273, 'cosine_with_motion': -0.9133640530735111, 'motion_component': -2.4521990200139596}, {'ion': 2443, 'force': [2.726148843765259, -0.5042769312858582, -0.7282940149307251], 'magnitude': 2.8664603233337402, 'distance': 10.762076377868652, 'cosine_with_motion': 0.3605986416231447, 'motion_component': 1.033641706957674}]}, 6173: {'frame': 6173, 'ionic_force': [6.784936279058456, 2.012464940547943, -7.050760209560394], 'ionic_force_magnitude': 9.989924673416631, 'motion_vector': [-1.894927978515625, 0.30248260498046875, -0.6227035522460938], 'cosine_ionic_motion': -0.3898840075180566, 'ionic_motion_component': -3.8949118664751885, 'ionic_force_x': 6.784936279058456, 'ionic_force_y': 2.012464940547943, 'ionic_force_z': -7.050760209560394, 'radial_force': 7.077102192834173, 'axial_force': -7.050760209560394, 'contributions': [{'ion': 1327, 'force': [1.4346952438354492, -0.13320499658584595, -2.9370408058166504], 'magnitude': 3.271437406539917, 'distance': 10.073948860168457, 'cosine_with_motion': -0.1409162394794962, 'motion_component': -0.46099865710665183}, {'ion': 1355, 'force': [0.2875460088253021, -2.611074686050415, -1.1207534074783325], 'magnitude': 2.8559556007385254, 'distance': 10.781850814819336, 'cosine_with_motion': -0.11052100472464929, 'motion_component': -0.31564307335446173}, {'ion': 1380, 'force': [2.0091943740844727, 1.0707746744155884, -0.7834347486495972], 'magnitude': 2.407735586166382, 'distance': 11.742610931396484, 'cosine_with_motion': -0.616692648196802, 'motion_component': -1.484832807733362}, {'ion': 1476, 'force': [0.7840487957000732, 4.45212459564209, -1.336418628692627], 'magnitude': 4.714038848876953, 'distance': 8.392135620117188, 'cosine_with_motion': 0.07288648656682731, 'motion_component': 0.34358971695424145}, {'ion': 2443, 'force': [2.269451856613159, -0.7661546468734741, -0.8731126189231873], 'magnitude': 2.549456834793091, 'distance': 11.411564826965332, 'cosine_with_motion': -0.7754699250894459, 'motion_component': -1.9770271258294603}]}, 6174: {'frame': 6174, 'ionic_force': [5.039700031280518, -0.18618684448301792, -7.465847820043564], 'ionic_force_magnitude': 9.009557459631223, 'motion_vector': [-4.1372528076171875, 1.9846878051757812, -0.39879608154296875], 'cosine_ionic_motion': -0.4396073734925297, 'ionic_motion_component': -3.96066789115851, 'ionic_force_x': 5.039700031280518, 'ionic_force_y': -0.18618684448301792, 'ionic_force_z': -7.465847820043564, 'radial_force': 5.043138105024231, 'axial_force': -7.465847820043564, 'contributions': [{'ion': 1327, 'force': [0.8549860119819641, -0.021522456780076027, -3.1400513648986816], 'magnitude': 3.254441022872925, 'distance': 10.1002197265625, 'cosine_with_motion': -0.1552898278023097, 'motion_component': -0.5053815979560157}, {'ion': 1355, 'force': [-0.40528932213783264, -2.981875419616699, -1.5683804750442505], 'magnitude': 3.393472671508789, 'distance': 9.891151428222656, 'cosine_with_motion': -0.23133690663508583, 'motion_component': -0.7850355044918764}, {'ion': 1380, 'force': [2.649775981903076, 1.5303508043289185, -1.275815725326538], 'magnitude': 3.3152663707733154, 'distance': 10.007136344909668, 'cosine_with_motion': -0.485706498100702, 'motion_component': -1.6102464920614352}, {'ion': 1476, 'force': [-0.39551082253456116, 2.728090524673462, -0.4340073764324188], 'magnitude': 2.7905678749084473, 'distance': 10.907437324523926, 'cosine_with_motion': 0.5620226202551888, 'motion_component': 1.5683622750861204}, {'ion': 2443, 'force': [2.335738182067871, -1.441230297088623, -1.0475928783416748], 'magnitude': 2.9377317428588867, 'distance': 10.63072681427002, 'cosine_with_motion': -0.8946924197105217, 'motion_component': -2.6283664235292683}]}, 6175: {'frame': 6175, 'ionic_force': [3.0340373516082764, 0.5058518648147583, -13.789096742868423], 'ionic_force_magnitude': 14.128002609862277, 'motion_vector': [1.6478233337402344, -1.9370346069335938, 6.6754608154296875], 'cosine_ionic_motion': -0.8722379391731214, 'ionic_motion_component': -12.322979881058753, 'ionic_force_x': 3.0340373516082764, 'ionic_force_y': 0.5058518648147583, 'ionic_force_z': -13.789096742868423, 'radial_force': 3.0759175476743086, 'axial_force': -13.789096742868423, 'contributions': [{'ion': 1327, 'force': [-0.6416452527046204, 0.5911756753921509, -3.6269683837890625], 'magnitude': 3.730428457260132, 'distance': 9.433865547180176, 'cosine_with_motion': -0.9912158206074198, 'motion_component': -3.697659769813785}, {'ion': 1355, 'force': [-1.5452637672424316, -2.1077585220336914, -1.4997599124908447], 'magnitude': 3.0132648944854736, 'distance': 10.496642112731934, 'cosine_with_motion': -0.39373008178062857, 'motion_component': -1.1864130704633098}, {'ion': 1380, 'force': [1.5424033403396606, 3.1613669395446777, -1.868808627128601], 'magnitude': 3.9831764698028564, 'distance': 9.129652976989746, 'cosine_with_motion': -0.5643280453750187, 'motion_component': -2.247818183510285}, {'ion': 1476, 'force': [-0.9063621163368225, 1.9885385036468506, -0.29560258984565735], 'magnitude': 2.2052571773529053, 'distance': 12.269855499267578, 'cosine_with_motion': -0.46458364097549226, 'motion_component': -1.0245263391440131}, {'ion': 2443, 'force': [4.58490514755249, -3.1274707317352295, -6.497957229614258], 'magnitude': 8.545517921447754, 'distance': 6.233038902282715, 'cosine_with_motion': -0.48757288041025726, 'motion_component': -4.166562787615533}]}, 6176: {'frame': 6176, 'ionic_force': [5.311269089579582, -3.3787199184298515, -8.04486072063446], 'ionic_force_magnitude': 10.214945503698264, 'motion_vector': [-0.2370452880859375, -0.42974090576171875, -0.37250518798828125], 'cosine_ionic_motion': 0.5068002522900235, 'ionic_motion_component': 5.176936958403121, 'ionic_force_x': 5.311269089579582, 'ionic_force_y': -3.3787199184298515, 'ionic_force_z': -8.04486072063446, 'radial_force': 6.294865179582335, 'axial_force': -8.04486072063446, 'contributions': [{'ion': 1327, 'force': [-0.29267406463623047, 0.06538949906826019, -12.753213882446289], 'magnitude': 12.756739616394043, 'distance': 5.101515293121338, 'cosine_with_motion': 0.6096637535551188, 'motion_component': 7.777321580484437}, {'ion': 1341, 'force': [-0.13413138687610626, 0.03554346412420273, -3.4107306003570557], 'magnitude': 3.4135520458221436, 'distance': 9.862017631530762, 'cosine_with_motion': 0.6119345691651443, 'motion_component': 2.0888705206918945}, {'ion': 1355, 'force': [-1.3672962188720703, -3.3759875297546387, 0.6790082454681396], 'magnitude': 3.7051103115081787, 'distance': 9.466042518615723, 'cosine_with_motion': 0.6666960615178826, 'motion_component': 2.4701824996911625}, {'ion': 1380, 'force': [3.2133100032806396, 3.5890440940856934, 1.645267367362976], 'magnitude': 5.090530872344971, 'distance': 8.075836181640625, 'cosine_with_motion': -0.9300019480237196, 'motion_component': -4.734203521272185}, {'ion': 1476, 'force': [-0.8967666625976562, 2.297664165496826, 1.0266220569610596], 'magnitude': 2.6715919971466064, 'distance': 11.147665977478027, 'cosine_with_motion': -0.7030355159917272, 'motion_component': -1.8782240731245852}, {'ion': 2443, 'force': [4.788827419281006, -5.990373611450195, 4.768186092376709], 'magnitude': 9.030672073364258, 'distance': 6.063299179077148, 'cosine_with_motion': -0.0605724670816613, 'motion_component': -0.5470101022199714}]}, 6177: {'frame': 6177, 'ionic_force': [5.809409823268652, -1.0547351241111755, -6.200492262840271], 'ionic_force_magnitude': 8.561998188405916, 'motion_vector': [0.2750663757324219, 0.47098541259765625, 0.6195907592773438], 'cosine_ionic_motion': -0.3877652637674757, 'ionic_motion_component': -3.320045485903869, 'ionic_force_x': 5.809409823268652, 'ionic_force_y': -1.0547351241111755, 'ionic_force_z': -6.200492262840271, 'radial_force': 5.904380465105897, 'axial_force': -6.200492262840271, 'contributions': [{'ion': 1327, 'force': [-0.6801349520683289, -1.2623990774154663, -10.40715503692627], 'magnitude': 10.50547981262207, 'distance': 5.621614933013916, 'cosine_with_motion': -0.8337139370096142, 'motion_component': -8.7585651273188}, {'ion': 1341, 'force': [0.033730413764715195, -0.4598913788795471, -3.558413505554199], 'magnitude': 3.588167428970337, 'distance': 9.619061470031738, 'cosine_with_motion': -0.8143753074190666, 'motion_component': -2.922114839486337}, {'ion': 1355, 'force': [-1.0431877374649048, -2.8463425636291504, 0.40366053581237793], 'magnitude': 3.0582427978515625, 'distance': 10.419168472290039, 'cosine_with_motion': -0.5456342002169842, 'motion_component': -1.6686818151427971}, {'ion': 1380, 'force': [4.841607570648193, 4.804633617401123, 2.4913699626922607], 'magnitude': 7.261721134185791, 'distance': 6.7615966796875, 'cosine_with_motion': 0.8572059866940269, 'motion_component': 6.2247907429244975}, {'ion': 1476, 'force': [-1.8445395231246948, 3.831808090209961, 1.4749726057052612], 'magnitude': 4.501180171966553, 'distance': 8.588273048400879, 'cosine_with_motion': 0.5951318431377391, 'motion_component': 2.678795687712494}, {'ion': 2443, 'force': [4.501934051513672, -5.122543811798096, 3.395073175430298], 'magnitude': 7.618030071258545, 'distance': 6.601576805114746, 'cosine_with_motion': 0.1477717864242414, 'motion_component': 1.1257299612341427}]}, 6178: {'frame': 6178, 'ionic_force': [3.472423955798149, -2.8070406317710876, -14.133636057376862], 'ionic_force_magnitude': 14.822175057649199, 'motion_vector': [-0.18217086791992188, -0.012928009033203125, -0.131744384765625], 'cosine_ionic_motion': 0.379216095936226, 'ionic_motion_component': 5.620807358645035, 'ionic_force_</t>
         </is>
       </c>
     </row>
@@ -755,7 +755,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>{6449: {'frame': 6449, 'ionic_force': [11.088144078850746, 3.661605954170227, -9.956974852830172], 'ionic_force_magnitude': 15.345867375188023, 'motion_vector': [4.9669189453125, 1.6391181945800781, 0.8033828735351562], 'cosine_ionic_motion': 0.6536010129993487, 'ionic_motion_component': 10.030074461776548, 'ionic_force_x': 11.088144078850746, 'ionic_force_y': 3.661605954170227, 'ionic_force_z': -9.956974852830172, 'radial_force': 11.67708427977497, 'axial_force': -9.956974852830172, 'contributions': [{'ion': 1327, 'force': [3.5316085815429688, 2.2948412895202637, -0.9144463539123535], 'magnitude': 4.309845447540283, 'distance': 8.776840209960938, 'directional_contribution': 3.8868339045883573}, {'ion': 1330, 'force': [0.982691764831543, 1.5302084684371948, -6.489742279052734], 'magnitude': 6.739731311798096, 'distance': 7.018555641174316, 'directional_contribution': 0.41109328010102075}, {'ion': 1355, 'force': [4.765550136566162, -4.245543003082275, 0.05606735870242119], 'magnitude': 6.3826518058776855, 'distance': 7.212211608886719, 'directional_contribution': 3.1664871931964558}, {'ion': 1465, 'force': [0.14122642576694489, 0.30911684036254883, -1.894454836845398], 'magnitude': 1.924696683883667, 'distance': 13.133724212646484, 'directional_contribution': -0.0593063682007644}, {'ion': 1476, 'force': [1.6670671701431274, 3.772982358932495, -0.7143987417221069], 'magnitude': 4.186272144317627, 'distance': 8.905438423156738, 'directional_contribution': 2.624966385042324}]}, 6450: {'frame': 6450, 'ionic_force': [11.005028426647186, 3.282705068588257, -4.414879508316517], 'ionic_force_magnitude': 12.303575265409675, 'motion_vector': [1.8098068237304688, -1.3127899169921875, -0.8244171142578125], 'cosine_ionic_motion': 0.6564770741103358, 'ionic_motion_component': 8.077015091332441, 'ionic_force_x': 11.005028426647186, 'ionic_force_y': 3.282705068588257, 'ionic_force_z': -4.414879508316517, 'radial_force': 11.484197979774107, 'axial_force': -4.414879508316517, 'contributions': [{'ion': 1327, 'force': [1.6276063919067383, 0.8470562100410461, -0.08977655321359634], 'magnitude': 1.8370264768600464, 'distance': 13.44346809387207, 'directional_contribution': 0.8005432095816627}, {'ion': 1330, 'force': [3.048281192779541, 1.3634477853775024, -2.819413661956787], 'magnitude': 4.370366096496582, 'distance': 8.71585750579834, 'directional_contribution': 2.5393885799464826}, {'ion': 1355, 'force': [2.8688948154449463, -1.2304490804672241, 0.45329388976097107], 'magnitude': 3.1543681621551514, 'distance': 10.259184837341309, 'directional_contribution': 2.699907953572965}, {'ion': 1465, 'force': [0.7390469908714294, 0.3952198624610901, -1.5287773609161377], 'magnitude': 1.7434303760528564, 'distance': 13.79960823059082, 'directional_contribution': 0.8724632119970934}, {'ion': 1476, 'force': [2.7211990356445312, 1.9074302911758423, -0.4302058219909668], 'magnitude': 3.3508644104003906, 'distance': 9.953839302062988, 'directional_contribution': 1.164712165083948}]}, 6451: {'frame': 6451, 'ionic_force': [8.739684104919434, 0.469412237405777, -2.0718104019761086], 'ionic_force_magnitude': 8.994155015572286, 'motion_vector': [-1.5418739318847656, -2.056304931640625, -0.31626129150390625], 'cosine_ionic_motion': -0.5918854713098048, 'ionic_motion_component': -5.323509680425447, 'ionic_force_x': 8.739684104919434, 'ionic_force_y': 0.469412237405777, 'ionic_force_z': -2.0718104019761086, 'radial_force': 8.75228119420347, 'axial_force': -2.0718104019761086, 'contributions': [{'ion': 1327, 'force': [1.4240713119506836, 0.4835692346096039, -0.21571895480155945], 'magnitude': 1.5193264484405518, 'distance': 14.782349586486816, 'directional_contribution': -1.2055671890198612}, {'ion': 1330, 'force': [2.4229938983917236, 0.5128621459007263, -2.0453357696533203], 'magnitude': 3.212059259414673, 'distance': 10.166635513305664, 'directional_contribution': -1.6001567804949488}, {'ion': 1355, 'force': [2.7083451747894287, -1.8824938535690308, -0.10277257114648819], 'magnitude': 3.2999210357666016, 'distance': 10.030377388000488, 'directional_contribution': -0.10520826545217404}, {'ion': 1476, 'force': [2.1842737197875977, 1.3554747104644775, 0.2920168936252594], 'magnitude': 2.5872063636779785, 'distance': 11.328006744384766, 'directional_contribution': -2.4125772285907994}]}, 6452: {'frame': 6452, 'ionic_force': [10.327910542488098, 1.1043216735124588, -5.13695291057229], 'ionic_force_magnitude': 11.58764634158565, 'motion_vector': [-0.060070037841796875, 3.2151107788085938, 1.4912796020507812], 'cosine_ionic_motion': -0.11517049748322489, 'ionic_motion_component': -1.3345549938200902, 'ionic_force_x': 10.327910542488098, 'ionic_force_y': 1.1043216735124588, 'ionic_force_z': -5.13695291057229, 'radial_force': 10.386783069469882, 'axial_force': -5.13695291057229, 'contributions': [{'ion': 1327, 'force': [1.7840296030044556, 0.277847021818161, -0.3307577669620514], 'magnitude': 1.8355820178985596, 'distance': 13.44875717163086, 'directional_contribution': 0.08262900902508541}, {'ion': 1330, 'force': [2.474438190460205, -0.39485305547714233, -2.829497814178467], 'magnitude': 3.7795252799987793, 'distance': 9.372391700744629, 'directional_contribution': -1.590489089812813}, {'ion': 1355, 'force': [2.0291547775268555, -1.468042254447937, -0.032318416982889175], 'magnitude': 2.504727840423584, 'distance': 11.513007164001465, 'directional_contribution': -1.379550057396542}, {'ion': 1465, 'force': [0.6779139041900635, -0.06925506889820099, -1.4678304195404053], 'magnitude': 1.6182984113693237, 'distance': 14.323189735412598, 'directional_contribution': -0.6918422968968603}, {'ion': 1476, 'force': [3.3623740673065186, 2.758625030517578, -0.4765484929084778], 'magnitude': 4.3752336502075195, 'distance': 8.711008071899414, 'directional_contribution': 2.2446974624236695}]}, 6453: {'frame': 6453, 'ionic_force': [9.139528214931488, 2.8800260424613953, -3.7206843197345734], 'ionic_force_magnitude': 10.279543657376202, 'motion_vector': [-0.720062255859375, 0.6362991333007812, 0.15360260009765625], 'cosine_ionic_motion': -0.5318267452065297, 'ionic_motion_component': -5.466936245510812, 'ionic_force_x': 9.139528214931488, 'ionic_force_y': 2.8800260424613953, 'ionic_force_z': -3.7206843197345734, 'radial_force': 9.582563644285624, 'axial_force': -3.7206843197345734, 'contributions': [{'ion': 1327, 'force': [1.5509934425354004, 0.7286680340766907, -0.15393760800361633], 'magnitude': 1.7205332517623901, 'distance': 13.891127586364746, 'directional_contribution': -0.695502212911935}, {'ion': 1330, 'force': [2.758227825164795, 1.1968661546707153, -2.8668406009674072], 'magnitude': 4.15440559387207, 'distance': 8.939528465270996, 'directional_contribution': -1.7108755555546544}, {'ion': 1355, 'force': [3.0123891830444336, -1.6359062194824219, 0.6324722766876221], 'magnitude': 3.4857852458953857, 'distance': 9.75930118560791, 'directional_contribution': -3.1988739910453567}, {'ion': 1465, 'force': [0.8180946707725525, 0.47484707832336426, -1.7255505323410034], 'magnitude': 1.9678118228912354, 'distance': 12.989046096801758, 'directional_contribution': -0.5672312566884852}, {'ion': 1476, 'force': [0.9998230934143066, 2.115550994873047, 0.39317214488983154], 'magnitude': 2.3727171421051025, 'distance': 11.828947067260742, 'directional_contribution': 0.7055466857160209}]}, 6454: {'frame': 6454, 'ionic_force': [11.519911527633667, 2.6967788338661194, -4.047921255230904], 'ionic_force_magnitude': 12.504664896423474, 'motion_vector': [1.3884010314941406, -1.9174156188964844, -1.4060287475585938], 'cosine_ionic_motion': 0.4796662185340068, 'ionic_motion_component': 5.998065324902385, 'ionic_force_x': 11.519911527633667, 'ionic_force_y': 2.6967788338661194, 'ionic_force_z': -4.047921255230904, 'radial_force': 11.831355699297328, 'axial_force': -4.047921255230904, 'contributions': [{'ion': 1327, 'force': [1.6504477262496948, 0.7416374683380127, -0.09881125390529633], 'magnitude': 1.8121168613433838, 'distance': 13.535551071166992, 'directional_contribution': 0.36623730695197043}, {'ion': 1330, 'force': [3.0074729919433594, 1.765475869178772, -3.316441059112549], 'magnitude': 4.812543869018555, 'distance': 8.305804252624512, 'directional_contribution': 1.980640093093207}, {'ion': 1355, 'force': [3.105611801147461, -2.121004343032837, 0.69764643907547], 'magnitude': 3.824943780899048, 'distance': 9.316579818725586, 'directional_contribution': 2.686804031990011}, {'ion': 1465, 'force': [0.7477613687515259, 0.573081910610199, -1.774617314338684], 'magnitude': 2.009187936782837, 'distance': 12.854605674743652, 'directional_contribution': 0.884195577283851}, {'ion': 1476, 'force': [3.008617639541626, 1.7375879287719727, 0.44430193305015564], 'magnitude': 3.502626895904541, 'distance': 9.735810279846191, 'directional_contribution': 0.08018833834593231}]}, 6455: {'frame': 6455, 'ionic_force': [12.358292996883392, 6.324190944433212, -5.279603046365082], 'ionic_force_magnitude': 14.852508381605297, 'motion_vector': [-0.5884780883789062, -1.5783882141113281, 0.5686721801757812], 'cosine_ionic_motion': -0.7671182394454574, 'ionic_motion_component': -11.393630081045956, 'ionic_force_x': 12.358292996883392, 'ionic_force_y': 6.324190944433212, 'ionic_force_z': -5.279603046365082, 'radial_force': 13.882463646574701, 'axial_force': -5.279603046365082, 'contributions': [{'ion': 1327, 'force': [1.4005006551742554, 0.43182238936424255, -0.22161030769348145], 'magnitude': 1.482222557067871, 'distance': 14.966226577758789, 'directional_contribution': -0.917797096281614}, {'ion': 1330, 'force': [2.4547295570373535, 0.45704543590545654, -2.393592596054077], 'magnitude': 3.458883285522461, 'distance': 9.79718017578125, 'directional_contribution': -1.9838444846666334}, {'ion': 1355, 'force': [2.053807497024536, -1.2260771989822388, 0.0074832020327448845], 'magnitude': 2.3919544219970703, 'distance': 11.781282424926758, 'directional_contribution': 0.4110758833959836}, {'ion': 1465, 'force': [0.7318766713142395, 0.13336181640625, -1.374646544456482], 'magnitude': 1.5630360841751099, 'distance': 14.574193954467773, 'directional_contribution': -0.8003241841063371}, {'ion': 1476, 'force': [5.717378616333008, 6.528038501739502, -1.2972368001937866], 'magnitude': 8.77419662475586, 'distance': 6.151278018951416, 'directional_contribution': -8.102740021611602}]}, 6456: {'frame': 6456, 'ionic_force': [9.233830749988556, 1.1224905923008919, -4.864724556449801], 'ionic_force_magnitude': 10.497102479225585, 'motion_vector': [0.4046783447265625, 0.90826416015625, -0.1713714599609375], 'cosine_ionic_motion': 0.5277719062348334, 'ionic_motion_component': 5.540075785403283, 'ionic_force_x': 9.233830749988556, 'ionic_force_y': 1.1224905923008919, 'ionic_force_z': -4.864724556449801, 'radial_force': 9.301807106645365, 'axial_force': -4.864724556449801, 'contributions': [{'ion': 1327, 'force': [1.8978043794631958, 0.4435109794139862, -0.23132824897766113], 'magnitude': 1.9626197814941406, 'distance': 13.006216049194336, 'directional_contribution': 1.1996741161612672}, {'ion': 1330, 'force': [2.841651201248169, -0.0774279534816742, -3.014273166656494], 'magnitude': 4.143286228179932, 'distance': 8.951516151428223, 'directional_contribution': 1.5819559606615972}, {'ion': 1355, 'force': [1.5171762704849243, -1.7436965703964233, -0.024102753028273582], 'magnitude': 2.3114676475524902, 'distance': 11.984643936157227, 'directional_contribution': -0.9570270502468217}, {'ion': 1465, 'force': [0.7945194840431213, 0.04755014926195145, -1.6000595092773438], 'magnitude': 1.7870961427688599, 'distance': 13.629975318908691, 'directional_contribution': 0.6332198785321617}, {'ion': 1476, 'force': [2.1826794147491455, 2.4525539875030518, 0.005039121489971876], 'magnitude': 3.2831594944000244, 'distance': 10.055949211120605, 'directional_contribution': 3.082252959352908}]}, 6457: {'frame': 6457, 'ionic_force': [9.096073269844055, 2.163865104317665, -4.737605880945921], 'ionic_force_magnitude': 10.481687392935767, 'motion_vector': [-0.11692047119140625, 0.4889183044433594, -0.9179763793945312], 'cosine_ionic_motion': 0.39593006496444544, 'ionic_motion_component': 4.1500151704220665, 'ionic_force_x': 9.096073269844055, 'ionic_force_y': 2.163865104317665, 'ionic_force_z': -4.737605880945921, 'radial_force': 9.349912358950496, 'axial_force': -4.737605880945921, 'contributions': [{'ion': 1327, 'force': [1.7632050514221191, 0.5160462856292725, -0.29753151535987854], 'magnitude': 1.8611074686050415, 'distance': 13.356212615966797, 'directional_contribution': 0.3050579272681855}, {'ion': 1330, 'force': [2.496544122695923, 0.2790150046348572, -2.758460760116577], 'magnitude': 3.730909824371338, 'distance': 9.433257102966309, 'directional_contribution': 2.270875241323065}, {'ion': 1355, 'force': [1.7096211910247803, -1.5737277269363403, -0.002807583659887314], 'magnitude': 2.3236677646636963, 'distance': 11.953140258789062, 'directional_contribution': -0.9236840021138677}, {'ion': 1465, 'force': [0.7106510400772095, 0.08507032692432404, -1.5122408866882324], 'magnitude': 1.6730613708496094, 'distance': 14.086824417114258, 'directional_contribution': 1.2867299912699872}, {'ion': 1476, 'force': [2.4160518646240234, 2.8574612140655518, -0.16656513512134552], 'magnitude': 3.7456822395324707, 'distance': 9.414636611938477, 'directional_contribution': 1.211035906255364}]}, 6458: {'frame': 6458, 'ionic_force': [7.916607975959778, 2.0578590631484985, -4.374101959168911], 'ionic_force_magnitude': 9.27578749853713, 'motion_vector': [1.0696640014648438, -0.24401092529296875, -0.6402435302734375], 'cosine_ionic_motion': 0.9137336519254561, 'ionic_motion_component': 8.475599185522823, 'ionic_force_x': 7.916607975959778, 'ionic_force_y': 2.0578590631484985, 'ionic_force_z': -4.374101959168911, 'radial_force': 8.179698391066285, 'axial_force': -4.374101959168911, 'contributions': [{'ion': 1327, 'force': [1.6573450565338135, 0.6732655763626099, -0.3442486822605133], 'magnitude': 1.821698784828186, 'distance': 13.499906539916992, 'directional_contribution': 1.4397677682584291}, {'ion': 1330, 'force': [2.1297972202301025, 0.3772757053375244, -2.3562591075897217], 'magnitude': 3.198488712310791, 'distance': 10.188179969787598, 'directional_contribution': 2.9085410090015955}, {'ion': 1355, 'force': [1.8750309944152832, -1.692273497581482, -0.19635580480098724], 'magnitude': 2.5333943367004395, 'distance': 11.447684288024902, 'directional_contribution': 2.002931512535695}, {'ion': 1465, 'force': [0.6408071517944336, 0.15025389194488525, -1.3914772272109985], 'magnitude': 1.5392916202545166, 'distance': 14.686171531677246, 'directional_contribution': 1.212062011077471}, {'ion': 1476, 'force': [1.613627552986145, 2.549337387084961, -0.08576113730669022], 'magnitude': 3.018322229385376, 'distance': 10.487844467163086, 'directional_contribution': 0.9122972296447824}]}, 6459: {'frame': 6459, 'ionic_force': [10.070922791957855, -0.5866779759526253, -2.2287999242544174], 'ionic_force_magnitude': 10.33127417269528, 'motion_vector': [-1.1145095825195312, -2.0631027221679688, 1.3752975463867188], 'cosine_ionic_motion': -0.46569356277561985, 'ionic_motion_component': -4.81120787749421, 'ionic_force_x': 10.070922791957855, 'ionic_force_y': -0.5866779759526253, 'ionic_force_z': -2.2287999242544174, 'radial_force': 10.087996675705444, 'axial_force': -2.2287999242544174, 'contributions': [{'ion': 1327, 'force': [1.3782541751861572, 0.488964319229126, -0.2811233103275299], 'magnitude': 1.4891947507858276, 'distance': 14.931151390075684, 'directional_contribution': -1.0783680709431334}, {'ion': 1330, 'force': [1.798455834388733, 0.22501133382320404, -1.8021730184555054], 'magnitude': 2.5559539794921875, 'distance': 11.397051811218262, 'directional_contribution': -1.8198394788149406}, {'ion': 1355, 'force': [1.6811152696609497, -1.412225365638733, -0.18546278774738312], 'magnitude': 2.2033896446228027, 'distance': 12.275053977966309, 'directional_contribution': 0.28872352276321767}, {'ion': 1465, 'force': [0.7065557837486267, 0.13394781947135925, -1.2894666194915771], 'magnitude': 1.476444125175476, 'distance': 14.995485305786133, 'directional_contribution': -1.0436874044938556}, {'ion': 1476, 'force': [4.506541728973389, -0.022376082837581635, 1.3294258117675781], 'magnitude': 4.698594570159912, 'distance': 8.405916213989258, 'directional_contribution': -1.1580363934527225}]}, 6460: {'frame': 6460, 'ionic_force': [10.501655519008636, -0.10368964076042175, -3.4797102883458138], 'ionic_force_magnitude': 11.063629778347849, 'motion_vector': [-4.040958404541016, 4.321376800537109, 0.48625946044921875], 'cosine_ionic_motion': -0.6787244499052771, 'ionic_motion_component': -7.5091560352647875, 'ionic_force_x': 10.501655519008636, 'ionic_force_y': -0.10368964076042175, 'ionic_force_z': -3.4797102883458138, 'radial_force': 10.502167403994548, 'axial_force': -3.4797102883458138, 'contributions': [{'ion': 1327, 'force': [1.7326629161834717, 0.26751768589019775, -0.18968352675437927], 'magnitude': 1.7634246349334717, 'distance': 13.721152305603027, 'directional_contribution': -1.000248120969888}, {'ion': 1330, 'force': [2.9949021339416504, -0.2766885459423065, -2.8809821605682373], 'magnitude': 4.164859294891357, 'distance': 8.928301811218262, 'directional_contribution': -2.476081887604808}, {'ion': 1355, 'force': [1.500700831413269, -1.4485684633255005, -0.06197259575128555], 'magnitude': 2.0866944789886475, 'distance': 12.613615989685059, 'directional_contribution': -2.0811176520772103}, {'ion': 1465, 'force': [0.7845519185066223, -0.08523333072662354, -1.5313416719436646], 'magnitude': 1.7227286100387573, 'distance': 13.88227367401123, 'directional_contribution': -0.7215386801651054}, {'ion': 1476, 'force': [3.488837718963623, 1.439283013343811, 1.184269666671753], 'magnitude': 3.955504894256592, 'distance': 9.161531448364258, 'directional_contribution': -1.2301697156885645}]}, 6461: {'frame': 6461, 'ionic_force': [9.932420074939728, 2.0168667435646057, -6.994688577950001], 'ionic_force_magnitude': 12.314478807845129, 'motion_vector': [1.1206817626953125, -1.6179962158203125, -0.19561004638671875], 'cosine_ionic_motion': 0.3791964013859275, 'ionic_motion_component': 4.669606048878139, 'ionic_force_x': 9.932420074939728, 'ionic_force_y': 2.0168667435646057, 'ionic_force_z': -6.994688577950001, 'radial_force': 10.135123087874296, 'axial_force': -6.994688577950001, 'contributions': [{'ion': 1327, 'force': [2.1432230472564697, 1.4571622610092163, -0.19045372307300568], 'magnitude': 2.598653554916382, 'distance': 11.30302906036377, 'directional_contribution': 0.041176191507181326}, {'ion': 1330, 'force': [2.3041412830352783, 2.8984789848327637, -5.283723831176758], 'magnitude': 6.451975345611572, 'distance': 7.173360824584961, 'directional_contribution': -0.5429837928883217}, {'ion': 1355, 'force': [4.2389912605285645, -5.536309242248535, 0.24877865612506866], 'magnitude': 6.977224349975586, 'distance': 6.898071765899658, 'directional_contribution': 6.906112256101975}, {'ion': 1465, 'force': [0.33492982387542725, 0.5356461405754089, -1.8747485876083374], 'magnitude': 1.9783267974853516, 'distance': 12.95448112487793, 'directional_contribution': -0.06299803976510887}, {'ion': 1476, 'force': [0.911134660243988, 2.661888599395752, 0.10545890778303146], 'magnitude': 2.8154821395874023, 'distance': 10.859070777893066, 'directional_contribution': -1.6717006091549076}]}, 6462: {'frame': 6462, 'ionic_force': [17.567132353782654, 1.7452539205551147, -1.5626121181994677], 'ionic_force_magnitude': 17.72263544212525, 'motion_vector': [4.015556335449219, -1.5489654541015625, -0.00579833984375], 'cosine_ionic_motion': 0.8894839537147118, 'ionic_motion_component': 15.763999843306046, 'ionic_force_x': 17.567132353782654, 'ionic_force_y': 1.7452539205551147, 'ionic_force_z': -1.5626121181994677, 'radial_force': 17.653612955498097, 'axial_force': -1.5626121181994677, 'contributions': [{'ion': 1327, 'force': [2.2711713314056396, 1.3109850883483887, -0.3511980175971985], 'magnitude': 2.64579701423645, 'distance': 11.201876640319824, 'directional_contribution': 1.6476434611698196}, {'ion': 1330, 'force': [3.1668646335601807, 2.0477538108825684, -5.296675682067871], 'magnitude': 6.502084255218506, 'distance': 7.145666599273682, 'directional_contribution': 2.224822717614096}, {'ion': 1355, 'force': [5.7192840576171875, -7.260217189788818, 0.016965268179774284], 'magnitude': 9.242362022399902, 'distance': 5.993459224700928, 'directional_contribution': 7.948930985423409}, {'ion': 1465, 'force': [0.5201071500778198, 0.3467801809310913, -1.9481827020645142], 'magnitude': 2.0460166931152344, 'distance': 12.738388061523438, 'directional_contribution': 0.36307663779865335}, {'ion': 1476, 'force': [5.889705181121826, 5.299952030181885, 6.016479015350342], 'magnitude': 9.948675155639648, 'distance': 5.776787757873535, 'directional_contribution': 3.5795255754979527}]}, 6463: {'frame': 6463, 'ionic_force': [15.515380442142487, 2.0406659450381994, -1.9564794301986694], 'ionic_force_magnitude': 15.770832556477377, 'motion_vector': [-1.9192962646484375, 4.6290435791015625, 0.8290939331054688], 'cosine_ionic_motion': -0.2740715950300907, 'ionic_motion_component': -4.322337233706238, 'ionic_force_x': 15.515380442142487, 'ionic_force_y': 2.0406659450381994, 'ionic_force_z': -1.9564794301986694, 'radial_force': 15.649004689233633, 'axial_force': -1.9564794301986694, 'contributions': [{'ion': 1327, 'force': [1.7279499769210815, 0.4192473888397217, -0.20830027759075165], 'magnitude': 1.7902426719665527, 'distance': 13.617992401123047, 'directional_contribution': -0.3048527198939759}, {'ion': 1330, 'force': [2.942939281463623, -0.07083207368850708, -2.4105186462402344], 'magnitude': 3.8048007488250732, 'distance': 9.341208457946777, 'directional_contribution': -1.570064019902123}, {'ion': 1355, 'force': [1.4266270399093628, -1.3901089429855347, 0.13944165408611298], 'magnitude': 1.9967752695083618, 'distance': 12.894497871398926, 'directional_contribution': -1.783200516420262}, {'ion': 1465, 'force': [0.8499615788459778, -0.021102407947182655, -1.4299547672271729], 'magnitude': 1.6636258363723755, 'distance': 14.126716613769531, 'directional_contribution': -0.5738166950758564}, {'ion': 1476, 'force': [8.567902565002441, 3.103461980819702, 1.9528526067733765], 'magnitude': 9.319552421569824, 'distance': 5.968586444854736, 'directional_contribution': -0.09040337073399485}]}, 6464: {'frame': 6464, 'ionic_force': [11.33767420053482, 4.5525089502334595, -1.6449899077415466], 'ionic_force_magnitude': 12.32778105808179, 'motion_vector': [1.3007926940917969, 0.5302505493164062, -0.1978912353515625], 'cosine_ionic_motion': 0.9999677833017746, 'ionic_motion_component': 12.327383897679653, 'ionic_force_x': 11.33767420053482, 'ionic_force_y': 4.5525089502334595, 'ionic_force_z': -1.6449899077415466, 'radial_force': 12.217536331823558, 'axial_force': -1.6449899077415466, 'contributions': [{'ion': 1327, 'force': [1.3779038190841675, 0.8388940691947937, -0.07618868350982666], 'magnitude': 1.614982008934021, 'distance': 14.337888717651367, 'directional_contribution': 1.587684638690158}, {'ion': 1330, 'force': [2.354668617248535, 1.9901186227798462, -2.5000572204589844], 'magnitude': 3.969297409057617, 'distance': 9.145600318908691, 'directional_contribution': 3.2517833314099853}, {'ion': 1355, 'force': [4.407364845275879, -3.357234239578247, -0.0832318663597107], 'magnitude': 5.541012287139893, 'distance': 7.740597724914551, 'directional_contribution': 2.7981112671611026}, {'ion': 1465, 'force': [0.7337548136711121, 0.5983582139015198, -1.5410960912704468], 'magnitude': 1.8087027072906494, 'distance': 13.548319816589355, 'directional_contribution': 1.1114668271117534}, {'ion': 1476, 'force': [2.463982105255127, 4.482372283935547, 2.555583953857422], 'magnitude': 5.717855930328369, 'distance': 7.619955539703369, 'directional_contribution': 3.578337952453353}]}, 6465: {'frame': 6465, 'ionic_force': [8.181056916713715, 1.5846307277679443, -2.695624351501465], 'ionic_force_magnitude': 8.75826109808924, 'motion_vector': [-4.231575012207031, 1.0118560791015625, 0.7423019409179688], 'cosine_ionic_motion': -0.9058280390134024, 'ionic_motion_component': -7.933478475649545, 'ionic_force_x': 8.181056916713715, 'ionic_force_y': 1.5846307277679443, 'ionic_force_z': -2.695624351501465, 'radial_force': 8.333111472787081, 'axial_force': -2.695624351501465, 'contributions': [{'ion': 1330, 'force': [1.9253636598587036, 1.5511382818222046, -1.7075893878936768], 'magnitude': 3.0048155784606934, 'distance': 10.51138973236084, 'directional_contribution': -1.777481269368515}, {'ion': 1355, 'force': [4.2340264320373535, -2.2788944244384766, 0.1942572146654129], 'magnitude': 4.812283992767334, 'distance': 8.306028366088867, 'directional_contribution': -4.549048944747952}, {'ion': 1465, 'force': [0.7398064732551575, 0.5602544546127319, -1.3368399143218994], 'magnitude': 1.6273720264434814, 'distance': 14.283203125, 'directional_contribution': -0.8056634834863594}, {'ion': 1476, 'force': [1.2818603515625, 1.7521324157714844, 0.15454773604869843], 'magnitude': 2.176469326019287, 'distance': 12.350733757019043, 'directional_contribution': -0.8012845776051729}]}, 6466: {'frame': 6466, 'ionic_force': [11.095829159021378, 11.397284507751465, -0.1161981022451073], 'ionic_force_magnitude': 15.906885957841842, 'motion_vector': [0.9455223083496094, 0.129486083984375, 0.086578369140625], 'cosine_ionic_motion': 0.7844291716732834, 'ionic_motion_component': 12.47782537581126, 'ionic_force_x': 11.095829159021378, 'ionic_force_y': 11.397284507751465, 'ionic_force_z': -0.1161981022451073, 'radial_force': 15.90646154481947, 'axial_force': -0.1161981022451073, 'contributions': [{'ion': 1327, 'force': [1.3715285062789917, 1.3724462985992432, -0.0012606775853782892], 'magnitude': 1.9402836561203003, 'distance': 13.080863952636719, 'directional_contribution': 1.5386264242361243}, {'ion': 1330, 'force': [1.4224761724472046, 3.4153378009796143, -2.5442066192626953], 'magnitude': 4.490095615386963, 'distance': 8.598867416381836, 'directional_contribution': 1.6351904344812702}, {'ion': 1355, 'force': [8.620282173156738, 1.4189844131469727, 1.5286056995391846], 'magnitude': 8.869014739990234, 'distance': 6.1183085441589355, 'directional_contribution': 8.835486686398186}, {'ion': 1465, 'force': [0.39631184935569763, 0.9951281547546387, -1.7195919752120972], 'magnitude': 2.0259170532226562, 'distance': 12.801422119140625, 'directional_contribution': 0.37014486904502863}, {'ion': 1476, 'force': [-0.7147695422172546, 4.195387840270996, 2.620255470275879], 'magnitude': 4.997790813446045, 'distance': 8.150420188903809, 'directional_contribution': 0.09837686238682863}]}, 6467: {'frame': 6467, 'ionic_force': [12.646102666854858, 8.711197972297668, -0.6976607432588935], 'ionic_force_magnitude': 15.371909877626823, 'motion_vector': [0.10419082641601562, -0.588623046875, 0.0458831787109375], 'cosine_ionic_motion': -0.41688779993381503, 'ionic_motion_component': -6.408361689664726, 'ionic_force_x': 12.646102666854858, 'ionic_force_y': 8.711197972297668, 'ionic_force_z': -0.6976607432588935, 'radial_force': 15.356069899984064, 'axial_force': -0.6976607432588935, 'contributions': [{'ion': 1327, 'force': [1.3215492963790894, 1.1881389617919922, 0.007228554226458073], 'magnitude': 1.7771378755569458, 'distance': 13.668110847473145, 'directional_contribution': -0.9362993373103939}, {'ion': 1330, 'force': [1.6552062034606934, 3.0671751499176025, -2.4254350662231445], 'magnitude': 4.246175289154053, 'distance': 8.842398643493652, 'directional_contribution': -2.9093370633845126}, {'ion': 1355, 'force': [8.693068504333496, 0.9444934129714966, 1.355777382850647], 'magnitude': 8.848709106445312, 'distance': 6.125324249267578, 'directional_contribution': 0.6871945697992645}, {'ion': 1465, 'force': [0.44038158655166626, 0.90205979347229, -1.5275148153305054], 'magnitude': 1.8278263807296753, 'distance': 13.477258682250977, 'directional_contribution': -0.9260174886346118}, {'ion': 1476, 'force': [0.5358970761299133, 2.609330654144287, 1.8922832012176514], 'magnitude': 3.267495632171631, 'distance': 10.080023765563965, 'directional_contribution': -2.323902132714779}]}, 6468: {'frame': 6468, 'ionic_force': [10.11287471652031, 10.04846477508545, -1.8506518509238958], 'ionic_force_magnitude': 14.37591011524129, 'motion_vector': [0.8352851867675781, 0.31511688232421875, 0.6468658447265625], 'cosine_ionic_motion': 0.6572317138478422, 'ionic_motion_component': 9.448304043162564, 'ionic_force_x': 10.11287471652031, 'ionic_force_y': 10.04846477508545, 'ionic_force_z': -1.8506518509238958, 'radial_force': 14.256292623545884, 'axial_force': -1.8506518509238958, 'contributions': [{'ion': 1327, 'force': [1.2898728847503662, 1.1364672183990479, -0.002380242571234703], 'magnitude': 1.7191089391708374, 'distance': 13.896881103515625, 'directional_contribution': 1.300710940442879}, {'ion': 1330, 'force': [1.9785761833190918, 2.999788999557495, -2.8233442306518555], 'magnitude': 4.569985866546631, 'distance': 8.523375511169434, 'directional_contribution': 0.6999157363938693}, {'ion': 1355, 'force': [5.315892219543457, 0.6447122097015381, 0.9586648941040039], 'magnitude': 5.439981937408447, 'distance': 7.812145709991455, 'directional_contribution': 4.774355307240334}, {'ion': 1465, 'force': [0.4987102448940277, 1.092886209487915, -1.8225653171539307], 'magnitude': 2.1828551292419434, 'distance': 12.33265495300293, 'directional_contribution': -0.37915214425949983}, {'ion': 1476, 'force': [1.0298231840133667, 4.174610137939453, 1.838973045349121], 'magnitude': 4.676507949829102, 'distance': 8.425743103027344, 'directional_contribution': 3.0524744107422066}]}, 6469: {'frame': 6469, 'ionic_force': [8.540325462818146, 8.121571838855743, -2.91854739934206], 'ionic_force_magnitude': 12.141458193592767, 'motion_vector': [-1.8116302490234375, -0.09438705444335938, -1.70416259765625], 'cosine_ionic_motion': -0.37275991687732457, 'ionic_motion_component': -4.525848947013151, 'ionic_force_x': 8.540325462818146, 'ionic_force_y': 8.121571838855743, 'ionic_force_z': -2.91854739934206, 'radial_force': 11.785460879598839, 'axial_force': -2.91854739934206, 'contributions': [{'ion': 1327, 'force': [1.1899250745773315, 1.021255373954773, 0.046343736350536346], 'magnitude': 1.5687676668167114, 'distance': 14.547545433044434, 'directional_contribution': -0.9365535961967288}, {'ion': 1330, 'force': [2.148881435394287, 2.901750087738037, -2.2233831882476807], 'magnitude': 4.240433692932129, 'distance': 8.848382949829102, 'directional_contribution': -0.15181238806897213}, {'ion': 1355, 'force': [3.58331298828125, 0.43657469749450684, 0.7156945466995239], 'magnitude': 3.680074453353882, 'distance': 9.498187065124512, 'directional_contribution': -3.1147162057607485}, {'ion': 1465, 'force': [0.6569304466247559, 0.9727057814598083, -1.5981245040893555], 'magnitude': 1.9828555583953857, 'distance': 12.939679145812988, 'directional_contribution': 0.5791652956295583}, {'ion': 1476, 'force': [0.9612755179405212, 2.789285898208618, 0.14092200994491577], 'magnitude': 2.953645944595337, 'distance': 10.602048873901367, 'directional_contribution': -0.901932156218967}]}, 6470: {'frame': 6470, 'ionic_force': [13.34115818142891, 9.546042263507843, -2.8391531258821487], 'ionic_force_magnitude': 16.648549936579816, 'motion_vector': [2.0888595581054688, -2.345661163330078, -0.346221923828125], 'cosine_ionic_motion': 0.12277440150635764, 'ionic_motion_component': 2.044015754412295, 'ionic_force_x': 13.34115818142891, 'ionic_force_y': 9.546042263507843, 'ionic_force_z': -2.8391531258821487, 'radial_force': 16.404676909911558, 'axial_force': -2.8391531258821487, 'contributions': [{'ion': 1327, 'force': [1.3334004878997803, 1.314848780632019, -0.10057435929775238], 'magnitude': 1.8753397464752197, 'distance': 13.305434226989746, 'directional_contribution': -0.08357146552605876}, {'ion': 1330, 'force': [1.4859381914138794, 3.3300931453704834, -2.836979389190674], 'magnitude': 4.620171546936035, 'distance': 8.476957321166992, 'directional_contribution': -1.1788544134336725}, {'ion': 1355, 'force': [9.047292709350586, 0.544345498085022, 0.4811491072177887], 'magnitude': 9.076416015625, 'distance': 6.048000812530518, 'directional_contribution': 5.523837508334666}, {'ion': 1465, 'force': [0.33565405011177063, 0.9165986180305481, -1.638068675994873], 'magnitude': 1.9068523645401, 'distance': 13.19503402709961, 'directional_contribution': -0.2790418558865593}, {'ion': 1476, 'force': [1.138872742652893, 3.4401562213897705, 1.2553201913833618], 'magnitude': 3.835040330886841, 'distance': 9.30430793762207, 'directional_contribu</t>
+          <t>{6449: {'frame': 6449, 'ionic_force': [11.088144078850746, 3.661605954170227, -9.956974852830172], 'ionic_force_magnitude': 15.345867375188023, 'motion_vector': [4.9669189453125, 1.6391181945800781, 0.8033828735351562], 'cosine_ionic_motion': 0.6536010129993487, 'ionic_motion_component': 10.030074461776548, 'ionic_force_x': 11.088144078850746, 'ionic_force_y': 3.661605954170227, 'ionic_force_z': -9.956974852830172, 'radial_force': 11.67708427977497, 'axial_force': -9.956974852830172, 'contributions': [{'ion': 1327, 'force': [3.5316085815429688, 2.2948412895202637, -0.9144463539123535], 'magnitude': 4.309845447540283, 'distance': 8.776840209960938, 'cosine_with_motion': 0.9018499490514568, 'motion_component': 3.886833904588357}, {'ion': 1330, 'force': [0.982691764831543, 1.5302084684371948, -6.489742279052734], 'magnitude': 6.739731311798096, 'distance': 7.018555641174316, 'cosine_with_motion': 0.060995501340076516, 'motion_component': 0.41109328010102075}, {'ion': 1355, 'force': [4.765550136566162, -4.245543003082275, 0.05606735870242119], 'magnitude': 6.3826518058776855, 'distance': 7.212211608886719, 'cosine_with_motion': 0.49610838474725943, 'motion_component': 3.1664871931964558}, {'ion': 1465, 'force': [0.14122642576694489, 0.30911684036254883, -1.894454836845398], 'magnitude': 1.924696683883667, 'distance': 13.133724212646484, 'cosine_with_motion': -0.030813358422604537, 'motion_component': -0.0593063682007644}, {'ion': 1476, 'force': [1.6670671701431274, 3.772982358932495, -0.7143987417221069], 'magnitude': 4.186272144317627, 'distance': 8.905438423156738, 'cosine_with_motion': 0.6270415061553786, 'motion_component': 2.6249663850423235}]}, 6450: {'frame': 6450, 'ionic_force': [11.005028426647186, 3.282705068588257, -4.414879508316517], 'ionic_force_magnitude': 12.303575265409675, 'motion_vector': [1.8098068237304688, -1.3127899169921875, -0.8244171142578125], 'cosine_ionic_motion': 0.6564770741103358, 'ionic_motion_component': 8.077015091332441, 'ionic_force_x': 11.005028426647186, 'ionic_force_y': 3.282705068588257, 'ionic_force_z': -4.414879508316517, 'radial_force': 11.484197979774107, 'axial_force': -4.414879508316517, 'contributions': [{'ion': 1327, 'force': [1.6276063919067383, 0.8470562100410461, -0.08977655321359634], 'magnitude': 1.8370264768600464, 'distance': 13.44346809387207, 'cosine_with_motion': 0.4357820526866752, 'motion_component': 0.8005432095816627}, {'ion': 1330, 'force': [3.048281192779541, 1.3634477853775024, -2.819413661956787], 'magnitude': 4.370366096496582, 'distance': 8.71585750579834, 'cosine_with_motion': 0.5810470822417294, 'motion_component': 2.5393885799464826}, {'ion': 1355, 'force': [2.8688948154449463, -1.2304490804672241, 0.45329388976097107], 'magnitude': 3.1543681621551514, 'distance': 10.259184837341309, 'cosine_with_motion': 0.855926739227634, 'motion_component': 2.699907953572965}, {'ion': 1465, 'force': [0.7390469908714294, 0.3952198624610901, -1.5287773609161377], 'magnitude': 1.7434303760528564, 'distance': 13.79960823059082, 'cosine_with_motion': 0.5004290581086671, 'motion_component': 0.8724632119970935}, {'ion': 1476, 'force': [2.7211990356445312, 1.9074302911758423, -0.4302058219909668], 'magnitude': 3.3508644104003906, 'distance': 9.953839302062988, 'cosine_with_motion': 0.34758559608259115, 'motion_component': 1.164712165083948}]}, 6451: {'frame': 6451, 'ionic_force': [8.739684104919434, 0.469412237405777, -2.0718104019761086], 'ionic_force_magnitude': 8.994155015572286, 'motion_vector': [-1.5418739318847656, -2.056304931640625, -0.31626129150390625], 'cosine_ionic_motion': -0.5918854713098048, 'ionic_motion_component': -5.323509680425447, 'ionic_force_x': 8.739684104919434, 'ionic_force_y': 0.469412237405777, 'ionic_force_z': -2.0718104019761086, 'radial_force': 8.75228119420347, 'axial_force': -2.0718104019761086, 'contributions': [{'ion': 1327, 'force': [1.4240713119506836, 0.4835692346096039, -0.21571895480155945], 'magnitude': 1.5193264484405518, 'distance': 14.782349586486816, 'cosine_with_motion': -0.7934879036563897, 'motion_component': -1.2055671890198612}, {'ion': 1330, 'force': [2.4229938983917236, 0.5128621459007263, -2.0453357696533203], 'magnitude': 3.212059259414673, 'distance': 10.166635513305664, 'cosine_with_motion': -0.49817160709433006, 'motion_component': -1.6001567804949488}, {'ion': 1355, 'force': [2.7083451747894287, -1.8824938535690308, -0.10277257114648819], 'magnitude': 3.2999210357666016, 'distance': 10.030377388000488, 'cosine_with_motion': -0.03188205537431328, 'motion_component': -0.10520826545217403}, {'ion': 1476, 'force': [2.1842737197875977, 1.3554747104644775, 0.2920168936252594], 'magnitude': 2.5872063636779785, 'distance': 11.328006744384766, 'cosine_with_motion': -0.932502786587697, 'motion_component': -2.4125772285907994}]}, 6452: {'frame': 6452, 'ionic_force': [10.327910542488098, 1.1043216735124588, -5.13695291057229], 'ionic_force_magnitude': 11.58764634158565, 'motion_vector': [-0.060070037841796875, 3.2151107788085938, 1.4912796020507812], 'cosine_ionic_motion': -0.11517049748322489, 'ionic_motion_component': -1.3345549938200902, 'ionic_force_x': 10.327910542488098, 'ionic_force_y': 1.1043216735124588, 'ionic_force_z': -5.13695291057229, 'radial_force': 10.386783069469882, 'axial_force': -5.13695291057229, 'contributions': [{'ion': 1327, 'force': [1.7840296030044556, 0.277847021818161, -0.3307577669620514], 'magnitude': 1.8355820178985596, 'distance': 13.44875717163086, 'cosine_with_motion': 0.045015155333941806, 'motion_component': 0.08262900902508541}, {'ion': 1330, 'force': [2.474438190460205, -0.39485305547714233, -2.829497814178467], 'magnitude': 3.7795252799987793, 'distance': 9.372391700744629, 'cosine_with_motion': -0.4208171612386723, 'motion_component': -1.590489089812813}, {'ion': 1355, 'force': [2.0291547775268555, -1.468042254447937, -0.032318416982889175], 'magnitude': 2.504727840423584, 'distance': 11.513007164001465, 'cosine_with_motion': -0.5507784216766087, 'motion_component': -1.379550057396542}, {'ion': 1465, 'force': [0.6779139041900635, -0.06925506889820099, -1.4678304195404053], 'magnitude': 1.6182984113693237, 'distance': 14.323189735412598, 'cosine_with_motion': -0.4275121960333371, 'motion_component': -0.6918422968968603}, {'ion': 1476, 'force': [3.3623740673065186, 2.758625030517578, -0.4765484929084778], 'magnitude': 4.3752336502075195, 'distance': 8.711008071899414, 'cosine_with_motion': 0.5130463007121352, 'motion_component': 2.2446974624236695}]}, 6453: {'frame': 6453, 'ionic_force': [9.139528214931488, 2.8800260424613953, -3.7206843197345734], 'ionic_force_magnitude': 10.279543657376202, 'motion_vector': [-0.720062255859375, 0.6362991333007812, 0.15360260009765625], 'cosine_ionic_motion': -0.5318267452065297, 'ionic_motion_component': -5.466936245510812, 'ionic_force_x': 9.139528214931488, 'ionic_force_y': 2.8800260424613953, 'ionic_force_z': -3.7206843197345734, 'radial_force': 9.582563644285624, 'axial_force': -3.7206843197345734, 'contributions': [{'ion': 1327, 'force': [1.5509934425354004, 0.7286680340766907, -0.15393760800361633], 'magnitude': 1.7205332517623901, 'distance': 13.891127586364746, 'cosine_with_motion': -0.40423643446915525, 'motion_component': -0.695502212911935}, {'ion': 1330, 'force': [2.758227825164795, 1.1968661546707153, -2.8668406009674072], 'magnitude': 4.15440559387207, 'distance': 8.939528465270996, 'cosine_with_motion': -0.41182200202131236, 'motion_component': -1.7108755555546544}, {'ion': 1355, 'force': [3.0123891830444336, -1.6359062194824219, 0.6324722766876221], 'magnitude': 3.4857852458953857, 'distance': 9.75930118560791, 'cosine_with_motion': -0.9176910640590641, 'motion_component': -3.1988739910453567}, {'ion': 1465, 'force': [0.8180946707725525, 0.47484707832336426, -1.7255505323410034], 'magnitude': 1.9678118228912354, 'distance': 12.989046096801758, 'cosine_with_motion': -0.2882548305003571, 'motion_component': -0.5672312566884852}, {'ion': 1476, 'force': [0.9998230934143066, 2.115550994873047, 0.39317214488983154], 'magnitude': 2.3727171421051025, 'distance': 11.828947067260742, 'cosine_with_motion': 0.29735811219878866, 'motion_component': 0.7055466857160209}]}, 6454: {'frame': 6454, 'ionic_force': [11.519911527633667, 2.6967788338661194, -4.047921255230904], 'ionic_force_magnitude': 12.504664896423474, 'motion_vector': [1.3884010314941406, -1.9174156188964844, -1.4060287475585938], 'cosine_ionic_motion': 0.4796662185340068, 'ionic_motion_component': 5.998065324902385, 'ionic_force_x': 11.519911527633667, 'ionic_force_y': 2.6967788338661194, 'ionic_force_z': -4.047921255230904, 'radial_force': 11.831355699297328, 'axial_force': -4.047921255230904, 'contributions': [{'ion': 1327, 'force': [1.6504477262496948, 0.7416374683380127, -0.09881125390529633], 'magnitude': 1.8121168613433838, 'distance': 13.535551071166992, 'cosine_with_motion': 0.20210468545852037, 'motion_component': 0.36623730695197043}, {'ion': 1330, 'force': [3.0074729919433594, 1.765475869178772, -3.316441059112549], 'magnitude': 4.812543869018555, 'distance': 8.305804252624512, 'cosine_with_motion': 0.41155781151904886, 'motion_component': 1.980640093093207}, {'ion': 1355, 'force': [3.105611801147461, -2.121004343032837, 0.69764643907547], 'magnitude': 3.824943780899048, 'distance': 9.316579818725586, 'cosine_with_motion': 0.7024427580038051, 'motion_component': 2.686804031990011}, {'ion': 1465, 'force': [0.7477613687515259, 0.573081910610199, -1.774617314338684], 'magnitude': 2.009187936782837, 'distance': 12.854605674743652, 'cosine_with_motion': 0.44007607183732467, 'motion_component': 0.884195577283851}, {'ion': 1476, 'force': [3.008617639541626, 1.7375879287719727, 0.44430193305015564], 'magnitude': 3.502626895904541, 'distance': 9.735810279846191, 'cosine_with_motion': 0.022893770199989852, 'motion_component': 0.08018833834593231}]}, 6455: {'frame': 6455, 'ionic_force': [12.358292996883392, 6.324190944433212, -5.279603046365082], 'ionic_force_magnitude': 14.852508381605297, 'motion_vector': [-0.5884780883789062, -1.5783882141113281, 0.5686721801757812], 'cosine_ionic_motion': -0.7671182394454574, 'ionic_motion_component': -11.393630081045956, 'ionic_force_x': 12.358292996883392, 'ionic_force_y': 6.324190944433212, 'ionic_force_z': -5.279603046365082, 'radial_force': 13.882463646574701, 'axial_force': -5.279603046365082, 'contributions': [{'ion': 1327, 'force': [1.4005006551742554, 0.43182238936424255, -0.22161030769348145], 'magnitude': 1.482222557067871, 'distance': 14.966226577758789, 'cosine_with_motion': -0.6192032869882479, 'motion_component': -0.9177970962816141}, {'ion': 1330, 'force': [2.4547295570373535, 0.45704543590545654, -2.393592596054077], 'magnitude': 3.458883285522461, 'distance': 9.79718017578125, 'cosine_with_motion': -0.5735505794656885, 'motion_component': -1.9838444846666337}, {'ion': 1355, 'force': [2.053807497024536, -1.2260771989822388, 0.0074832020327448845], 'magnitude': 2.3919544219970703, 'distance': 11.781282424926758, 'cosine_with_motion': 0.17185773231780294, 'motion_component': 0.4110758833959836}, {'ion': 1465, 'force': [0.7318766713142395, 0.13336181640625, -1.374646544456482], 'magnitude': 1.5630360841751099, 'distance': 14.574193954467773, 'cosine_with_motion': -0.5120317863135961, 'motion_component': -0.800324184106337}, {'ion': 1476, 'force': [5.717378616333008, 6.528038501739502, -1.2972368001937866], 'magnitude': 8.77419662475586, 'distance': 6.151278018951416, 'cosine_with_motion': -0.923473711829239, 'motion_component': -8.102740021611602}]}, 6456: {'frame': 6456, 'ionic_force': [9.233830749988556, 1.1224905923008919, -4.864724556449801], 'ionic_force_magnitude': 10.497102479225585, 'motion_vector': [0.4046783447265625, 0.90826416015625, -0.1713714599609375], 'cosine_ionic_motion': 0.5277719062348334, 'ionic_motion_component': 5.540075785403283, 'ionic_force_x': 9.233830749988556, 'ionic_force_y': 1.1224905923008919, 'ionic_force_z': -4.864724556449801, 'radial_force': 9.301807106645365, 'axial_force': -4.864724556449801, 'contributions': [{'ion': 1327, 'force': [1.8978043794631958, 0.4435109794139862, -0.23132824897766113], 'magnitude': 1.9626197814941406, 'distance': 13.006216049194336, 'cosine_with_motion': 0.6112616198270099, 'motion_component': 1.1996741161612672}, {'ion': 1330, 'force': [2.841651201248169, -0.0774279534816742, -3.014273166656494], 'magnitude': 4.143286228179932, 'distance': 8.951516151428223, 'cosine_with_motion': 0.3818119092933767, 'motion_component': 1.5819559606615972}, {'ion': 1355, 'force': [1.5171762704849243, -1.7436965703964233, -0.024102753028273582], 'magnitude': 2.3114676475524902, 'distance': 11.984643936157227, 'cosine_with_motion': -0.41403437645778535, 'motion_component': -0.9570270502468217}, {'ion': 1465, 'force': [0.7945194840431213, 0.04755014926195145, -1.6000595092773438], 'magnitude': 1.7870961427688599, 'distance': 13.629975318908691, 'cosine_with_motion': 0.3543289360404364, 'motion_component': 0.6332198785321617}, {'ion': 1476, 'force': [2.1826794147491455, 2.4525539875030518, 0.005039121489971876], 'magnitude': 3.2831594944000244, 'distance': 10.055949211120605, 'cosine_with_motion': 0.9388069691631643, 'motion_component': 3.082252959352908}]}, 6457: {'frame': 6457, 'ionic_force': [9.096073269844055, 2.163865104317665, -4.737605880945921], 'ionic_force_magnitude': 10.481687392935767, 'motion_vector': [-0.11692047119140625, 0.4889183044433594, -0.9179763793945312], 'cosine_ionic_motion': 0.39593006496444544, 'ionic_motion_component': 4.1500151704220665, 'ionic_force_x': 9.096073269844055, 'ionic_force_y': 2.163865104317665, 'ionic_force_z': -4.737605880945921, 'radial_force': 9.349912358950496, 'axial_force': -4.737605880945921, 'contributions': [{'ion': 1327, 'force': [1.7632050514221191, 0.5160462856292725, -0.29753151535987854], 'magnitude': 1.8611074686050415, 'distance': 13.356212615966797, 'cosine_with_motion': 0.16391204728999575, 'motion_component': 0.3050579272681855}, {'ion': 1330, 'force': [2.496544122695923, 0.2790150046348572, -2.758460760116577], 'magnitude': 3.730909824371338, 'distance': 9.433257102966309, 'cosine_with_motion': 0.6086652807854851, 'motion_component': 2.270875241323065}, {'ion': 1355, 'force': [1.7096211910247803, -1.5737277269363403, -0.002807583659887314], 'magnitude': 2.3236677646636963, 'distance': 11.953140258789062, 'cosine_with_motion': -0.39751123302335817, 'motion_component': -0.9236840021138677}, {'ion': 1465, 'force': [0.7106510400772095, 0.08507032692432404, -1.5122408866882324], 'magnitude': 1.6730613708496094, 'distance': 14.086824417114258, 'cosine_with_motion': 0.7690871425186415, 'motion_component': 1.2867299912699872}, {'ion': 1476, 'force': [2.4160518646240234, 2.8574612140655518, -0.16656513512134552], 'magnitude': 3.7456822395324707, 'distance': 9.414636611938477, 'cosine_with_motion': 0.32331517770345275, 'motion_component': 1.211035906255364}]}, 6458: {'frame': 6458, 'ionic_force': [7.916607975959778, 2.0578590631484985, -4.374101959168911], 'ionic_force_magnitude': 9.27578749853713, 'motion_vector': [1.0696640014648438, -0.24401092529296875, -0.6402435302734375], 'cosine_ionic_motion': 0.9137336519254561, 'ionic_motion_component': 8.475599185522823, 'ionic_force_x': 7.916607975959778, 'ionic_force_y': 2.0578590631484985, 'ionic_force_z': -4.374101959168911, 'radial_force': 8.179698391066285, 'axial_force': -4.374101959168911, 'contributions': [{'ion': 1327, 'force': [1.6573450565338135, 0.6732655763626099, -0.3442486822605133], 'magnitude': 1.821698784828186, 'distance': 13.499906539916992, 'cosine_with_motion': 0.7903435021550261, 'motion_component': 1.4397677682584291}, {'ion': 1330, 'force': [2.1297972202301025, 0.3772757053375244, -2.3562591075897217], 'magnitude': 3.198488712310791, 'distance': 10.188179969787598, 'cosine_with_motion': 0.909348525788148, 'motion_component': 2.9085410090015955}, {'ion': 1355, 'force': [1.8750309944152832, -1.692273497581482, -0.19635580480098724], 'magnitude': 2.5333943367004395, 'distance': 11.447684288024902, 'cosine_with_motion': 0.7906118493156139, 'motion_component': 2.002931512535695}, {'ion': 1465, 'force': [0.6408071517944336, 0.15025389194488525, -1.3914772272109985], 'magnitude': 1.5392916202545166, 'distance': 14.686171531677246, 'cosine_with_motion': 0.7874154182272478, 'motion_component': 1.212062011077471}, {'ion': 1476, 'force': [1.613627552986145, 2.549337387084961, -0.08576113730669022], 'magnitude': 3.018322229385376, 'distance': 10.487844467163086, 'cosine_with_motion': 0.30225307836269955, 'motion_component': 0.9122972296447824}]}, 6459: {'frame': 6459, 'ionic_force': [10.070922791957855, -0.5866779759526253, -2.2287999242544174], 'ionic_force_magnitude': 10.33127417269528, 'motion_vector': [-1.1145095825195312, -2.0631027221679688, 1.3752975463867188], 'cosine_ionic_motion': -0.46569356277561985, 'ionic_motion_component': -4.81120787749421, 'ionic_force_x': 10.070922791957855, 'ionic_force_y': -0.5866779759526253, 'ionic_force_z': -2.2287999242544174, 'radial_force': 10.087996675705444, 'axial_force': -2.2287999242544174, 'contributions': [{'ion': 1327, 'force': [1.3782541751861572, 0.488964319229126, -0.2811233103275299], 'magnitude': 1.4891947507858276, 'distance': 14.931151390075684, 'cosine_with_motion': -0.7241283073273487, 'motion_component': -1.0783680709431334}, {'ion': 1330, 'force': [1.798455834388733, 0.22501133382320404, -1.8021730184555054], 'magnitude': 2.5559539794921875, 'distance': 11.397051811218262, 'cosine_with_motion': -0.7120000779386864, 'motion_component': -1.8198394788149406}, {'ion': 1355, 'force': [1.6811152696609497, -1.412225365638733, -0.18546278774738312], 'magnitude': 2.2033896446228027, 'distance': 12.275053977966309, 'cosine_with_motion': 0.131036077420042, 'motion_component': 0.2887235227632176}, {'ion': 1465, 'force': [0.7065557837486267, 0.13394781947135925, -1.2894666194915771], 'magnitude': 1.476444125175476, 'distance': 14.995485305786133, 'cosine_with_motion': -0.7068925848535891, 'motion_component': -1.0436874044938556}, {'ion': 1476, 'force': [4.506541728973389, -0.022376082837581635, 1.3294258117675781], 'magnitude': 4.698594570159912, 'distance': 8.405916213989258, 'cosine_with_motion': -0.24646441555121948, 'motion_component': -1.1580363934527225}]}, 6460: {'frame': 6460, 'ionic_force': [10.501655519008636, -0.10368964076042175, -3.4797102883458138], 'ionic_force_magnitude': 11.063629778347849, 'motion_vector': [-4.040958404541016, 4.321376800537109, 0.48625946044921875], 'cosine_ionic_motion': -0.6787244499052771, 'ionic_motion_component': -7.5091560352647875, 'ionic_force_x': 10.501655519008636, 'ionic_force_y': -0.10368964076042175, 'ionic_force_z': -3.4797102883458138, 'radial_force': 10.502167403994548, 'axial_force': -3.4797102883458138, 'contributions': [{'ion': 1327, 'force': [1.7326629161834717, 0.26751768589019775, -0.18968352675437927], 'magnitude': 1.7634246349334717, 'distance': 13.721152305603027, 'cosine_with_motion': -0.5672191023917383, 'motion_component': -1.000248120969888}, {'ion': 1330, 'force': [2.9949021339416504, -0.2766885459423065, -2.8809821605682373], 'magnitude': 4.164859294891357, 'distance': 8.928301811218262, 'cosine_with_motion': -0.5945175260413068, 'motion_component': -2.476081887604808}, {'ion': 1355, 'force': [1.500700831413269, -1.4485684633255005, -0.06197259575128555], 'magnitude': 2.0866944789886475, 'distance': 12.613615989685059, 'cosine_with_motion': -0.9973273968062647, 'motion_component': -2.0811176520772103}, {'ion': 1465, 'force': [0.7845519185066223, -0.08523333072662354, -1.5313416719436646], 'magnitude': 1.7227286100387573, 'distance': 13.88227367401123, 'cosine_with_motion': -0.4188348006950093, 'motion_component': -0.7215386801651054}, {'ion': 1476, 'force': [3.488837718963623, 1.439283013343811, 1.184269666671753], 'magnitude': 3.955504894256592, 'distance': 9.161531448364258, 'cosine_with_motion': -0.3110019460566897, 'motion_component': -1.2301697156885645}]}, 6461: {'frame': 6461, 'ionic_force': [9.932420074939728, 2.0168667435646057, -6.994688577950001], 'ionic_force_magnitude': 12.314478807845129, 'motion_vector': [1.1206817626953125, -1.6179962158203125, -0.19561004638671875], 'cosine_ionic_motion': 0.3791964013859275, 'ionic_motion_component': 4.669606048878139, 'ionic_force_x': 9.932420074939728, 'ionic_force_y': 2.0168667435646057, 'ionic_force_z': -6.994688577950001, 'radial_force': 10.135123087874296, 'axial_force': -6.994688577950001, 'contributions': [{'ion': 1327, 'force': [2.1432230472564697, 1.4571622610092163, -0.19045372307300568], 'magnitude': 2.598653554916382, 'distance': 11.30302906036377, 'cosine_with_motion': 0.01584520331532757, 'motion_component': 0.041176191507181326}, {'ion': 1330, 'force': [2.3041412830352783, 2.8984789848327637, -5.283723831176758], 'magnitude': 6.451975345611572, 'distance': 7.173360824584961, 'cosine_with_motion': -0.08415776090292298, 'motion_component': -0.5429837928883217}, {'ion': 1355, 'force': [4.2389912605285645, -5.536309242248535, 0.24877865612506866], 'magnitude': 6.977224349975586, 'distance': 6.898071765899658, 'cosine_with_motion': 0.9898079870830155, 'motion_component': 6.906112256101975}, {'ion': 1465, 'force': [0.33492982387542725, 0.5356461405754089, -1.8747485876083374], 'magnitude': 1.9783267974853516, 'distance': 12.95448112487793, 'cosine_with_motion': -0.031844101211086266, 'motion_component': -0.06299803976510887}, {'ion': 1476, 'force': [0.911134660243988, 2.661888599395752, 0.10545890778303146], 'magnitude': 2.8154821395874023, 'distance': 10.859070777893066, 'cosine_with_motion': -0.5937529033887871, 'motion_component': -1.6717006091549076}]}, 6462: {'frame': 6462, 'ionic_force': [17.567132353782654, 1.7452539205551147, -1.5626121181994677], 'ionic_force_magnitude': 17.72263544212525, 'motion_vector': [4.015556335449219, -1.5489654541015625, -0.00579833984375], 'cosine_ionic_motion': 0.8894839537147118, 'ionic_motion_component': 15.763999843306046, 'ionic_force_x': 17.567132353782654, 'ionic_force_y': 1.7452539205551147, 'ionic_force_z': -1.5626121181994677, 'radial_force': 17.653612955498097, 'axial_force': -1.5626121181994677, 'contributions': [{'ion': 1327, 'force': [2.2711713314056396, 1.3109850883483887, -0.3511980175971985], 'magnitude': 2.64579701423645, 'distance': 11.201876640319824, 'cosine_with_motion': 0.6227399651913887, 'motion_component': 1.6476434611698196}, {'ion': 1330, 'force': [3.1668646335601807, 2.0477538108825684, -5.296675682067871], 'magnitude': 6.502084255218506, 'distance': 7.145666599273682, 'cosine_with_motion': 0.34217069584171755, 'motion_component': 2.224822717614096}, {'ion': 1355, 'force': [5.7192840576171875, -7.260217189788818, 0.016965268179774284], 'magnitude': 9.242362022399902, 'distance': 5.993459224700928, 'cosine_with_motion': 0.860054081373168, 'motion_component': 7.948930985423409}, {'ion': 1465, 'force': [0.5201071500778198, 0.3467801809310913, -1.9481827020645142], 'magnitude': 2.0460166931152344, 'distance': 12.738388061523438, 'cosine_with_motion': 0.1774553755351891, 'motion_component': 0.36307663779865335}, {'ion': 1476, 'force': [5.889705181121826, 5.299952030181885, 6.016479015350342], 'magnitude': 9.948675155639648, 'distance': 5.776787757873535, 'cosine_with_motion': 0.3597992195773787, 'motion_component': 3.5795255754979527}]}, 6463: {'frame': 6463, 'ionic_force': [15.515380442142487, 2.0406659450381994, -1.9564794301986694], 'ionic_force_magnitude': 15.770832556477377, 'motion_vector': [-1.9192962646484375, 4.6290435791015625, 0.8290939331054688], 'cosine_ionic_motion': -0.2740715950300907, 'ionic_motion_component': -4.322337233706238, 'ionic_force_x': 15.515380442142487, 'ionic_force_y': 2.0406659450381994, 'ionic_force_z': -1.9564794301986694, 'radial_force': 15.649004689233633, 'axial_force': -1.9564794301986694, 'contributions': [{'ion': 1327, 'force': [1.7279499769210815, 0.4192473888397217, -0.20830027759075165], 'magnitude': 1.7902426719665527, 'distance': 13.617992401123047, 'cosine_with_motion': -0.17028570485659653, 'motion_component': -0.3048527198939759}, {'ion': 1330, 'force': [2.942939281463623, -0.07083207368850708, -2.4105186462402344], 'magnitude': 3.8048007488250732, 'distance': 9.341208457946777, 'cosine_with_motion': -0.4126534114558553, 'motion_component': -1.570064019902123}, {'ion': 1355, 'force': [1.4266270399093628, -1.3901089429855347, 0.13944165408611298], 'magnitude': 1.9967752695083618, 'distance': 12.894497871398926, 'cosine_with_motion': -0.893040155913853, 'motion_component': -1.783200516420262}, {'ion': 1465, 'force': [0.8499615788459778, -0.021102407947182655, -1.4299547672271729], 'magnitude': 1.6636258363723755, 'distance': 14.126716613769531, 'cosine_with_motion': -0.34491933978937955, 'motion_component': -0.5738166950758564}, {'ion': 1476, 'force': [8.567902565002441, 3.103461980819702, 1.9528526067733765], 'magnitude': 9.319552421569824, 'distance': 5.968586444854736, 'cosine_with_motion': -0.009700397960359285, 'motion_component': -0.09040337073399485}]}, 6464: {'frame': 6464, 'ionic_force': [11.33767420053482, 4.5525089502334595, -1.6449899077415466], 'ionic_force_magnitude': 12.32778105808179, 'motion_vector': [1.3007926940917969, 0.5302505493164062, -0.1978912353515625], 'cosine_ionic_motion': 0.9999677833017746, 'ionic_motion_component': 12.327383897679653, 'ionic_force_x': 11.33767420053482, 'ionic_force_y': 4.5525089502334595, 'ionic_force_z': -1.6449899077415466, 'radial_force': 12.217536331823558, 'axial_force': -1.6449899077415466, 'contributions': [{'ion': 1327, 'force': [1.3779038190841675, 0.8388940691947937, -0.07618868350982666], 'magnitude': 1.614982008934021, 'distance': 14.337888717651367, 'cosine_with_motion': 0.9830974114455244, 'motion_component': 1.587684638690158}, {'ion': 1330, 'force': [2.354668617248535, 1.9901186227798462, -2.5000572204589844], 'magnitude': 3.969297409057617, 'distance': 9.145600318908691, 'cosine_with_motion': 0.8192339683710648, 'motion_component': 3.2517833314099853}, {'ion': 1355, 'force': [4.407364845275879, -3.357234239578247, -0.0832318663597107], 'magnitude': 5.541012287139893, 'distance': 7.740597724914551, 'cosine_with_motion': 0.5049819886765748, 'motion_component': 2.7981112671611026}, {'ion': 1465, 'force': [0.7337548136711121, 0.5983582139015198, -1.5410960912704468], 'magnitude': 1.8087027072906494, 'distance': 13.548319816589355, 'cosine_with_motion': 0.6145104786062255, 'motion_component': 1.1114668271117534}, {'ion': 1476, 'force': [2.463982105255127, 4.482372283935547, 2.555583953857422], 'magnitude': 5.717855930328369, 'distance': 7.619955539703369, 'cosine_with_motion': 0.6258181188800164, 'motion_component': 3.578337952453353}]}, 6465: {'frame': 6465, 'ionic_force': [8.181056916713715, 1.5846307277679443, -2.695624351501465], 'ionic_force_magnitude': 8.75826109808924, 'motion_vector': [-4.231575012207031, 1.0118560791015625, 0.7423019409179688], 'cosine_ionic_motion': -0.9058280390134024, 'ionic_motion_component': -7.933478475649545, 'ionic_force_x': 8.181056916713715, 'ionic_force_y': 1.5846307277679443, 'ionic_force_z': -2.695624351501465, 'radial_force': 8.333111472787081, 'axial_force': -2.695624351501465, 'contributions': [{'ion': 1330, 'force': [1.9253636598587036, 1.5511382818222046, -1.7075893878936768], 'magnitude': 3.0048155784606934, 'distance': 10.51138973236084, 'cosine_with_motion': -0.5915442123218393, 'motion_component': -1.777481269368515}, {'ion': 1355, 'force': [4.2340264320373535, -2.2788944244384766, 0.1942572146654129], 'magnitude': 4.812283992767334, 'distance': 8.306028366088867, 'cosine_with_motion': -0.945299388430905, 'motion_component': -4.549048944747952}, {'ion': 1465, 'force': [0.7398064732551575, 0.5602544546127319, -1.3368399143218994], 'magnitude': 1.6273720264434814, 'distance': 14.283203125, 'cosine_with_motion': -0.49507026248069363, 'motion_component': -0.8056634834863594}, {'ion': 1476, 'force': [1.2818603515625, 1.7521324157714844, 0.15454773604869843], 'magnitude': 2.176469326019287, 'distance': 12.350733757019043, 'cosine_with_motion': -0.36815798312379094, 'motion_component': -0.8012845776051729}]}, 6466: {'frame': 6466, 'ionic_force': [11.095829159021378, 11.397284507751465, -0.1161981022451073], 'ionic_force_magnitude': 15.906885957841842, 'motion_vector': [0.9455223083496094, 0.129486083984375, 0.086578369140625], 'cosine_ionic_motion': 0.7844291716732834, 'ionic_motion_component': 12.47782537581126, 'ionic_force_x': 11.095829159021378, 'ionic_force_y': 11.397284507751465, 'ionic_force_z': -0.1161981022451073, 'radial_force': 15.90646154481947, 'axial_force': -0.1161981022451073, 'contributions': [{'ion': 1327, 'force': [1.3715285062789917, 1.3724462985992432, -0.0012606775853782892], 'magnitude': 1.9402836561203003, 'distance': 13.080863952636719, 'cosine_with_motion': 0.7929904355159877, 'motion_component': 1.5386264242361243}, {'ion': 1330, 'force': [1.4224761724472046, 3.4153378009796143, -2.5442066192626953], 'magnitude': 4.490095615386963, 'distance': 8.598867416381836, 'cosine_with_motion': 0.36417720181723146, 'motion_component': 1.6351904344812702}, {'ion': 1355, 'force': [8.620282173156738, 1.4189844131469727, 1.5286056995391846], 'magnitude': 8.869014739990234, 'distance': 6.1183085441589355, 'cosine_with_motion': 0.9962196769212918, 'motion_component': 8.835486686398186}, {'ion': 1465, 'force': [0.39631184935569763, 0.9951281547546387, -1.7195919752120972], 'magnitude': 2.0259170532226562, 'distance': 12.801422119140625, 'cosine_with_motion': 0.1827048537507158, 'motion_component': 0.37014486904502863}, {'ion': 1476, 'force': [-0.7147695422172546, 4.195387840270996, 2.620255470275879], 'magnitude': 4.997790813446045, 'distance': 8.150420188903809, 'cosine_with_motion': 0.019684069498479846, 'motion_component': 0.09837686238682863}]}, 6467: {'frame': 6467, 'ionic_force': [12.646102666854858, 8.711197972297668, -0.6976607432588935], 'ionic_force_magnitude': 15.371909877626823, 'motion_vector': [0.10419082641601562, -0.588623046875, 0.0458831787109375], 'cosine_ionic_motion': -0.41688779993381503, 'ionic_motion_component': -6.408361689664726, 'ionic_force_x': 12.646102666854858, 'ionic_force_y': 8.711197972297668, 'ionic_force_z': -0.6976607432588935, 'radial_force': 15.356069899984064, 'axial_force': -0.6976607432588935, 'contributions': [{'ion': 1327, 'force': [1.3215492963790894, 1.1881389617919922, 0.007228554226458073], 'magnitude': 1.7771378755569458, 'distance': 13.668110847473145, 'cosine_with_motion': -0.5268580206034226, 'motion_component': -0.9362993373103939}, {'ion': 1330, 'force': [1.6552062034606934, 3.0671751499176025, -2.4254350662231445], 'magnitude': 4.246175289154053, 'distance': 8.842398643493652, 'cosine_with_motion': -0.68516646914074, 'motion_component': -2.9093370633845126}, {'ion': 1355, 'force': [8.693068504333496, 0.9444934129714966, 1.355777382850647], 'magnitude': 8.848709106445312, 'distance': 6.125324249267578, 'cosine_with_motion': 0.07766043807171832, 'motion_component': 0.6871945697992645}, {'ion': 1465, 'force': [0.44038158655166626, 0.90205979347229, -1.5275148153305054], 'magnitude': 1.8278263807296753, 'distance': 13.477258682250977, 'cosine_with_motion': -0.5066222328657881, 'motion_component': -0.9260174886346118}, {'ion': 1476, 'force': [0.5358970761299133, 2.609330654144287, 1.8922832012176514], 'magnitude': 3.267495632171631, 'distance': 10.080023765563965, 'cosine_with_motion': -0.7112181249520889, 'motion_component': -2.323902132714779}]}, 6468: {'frame': 6468, 'ionic_force': [10.11287471652031, 10.04846477508545, -1.8506518509238958], 'ionic_force_magnitude': 14.37591011524129, 'motion_vector': [0.8352851867675781, 0.31511688232421875, 0.6468658447265625], 'cosine_ionic_motion': 0.6572317138478422, 'ionic_motion_component': 9.448304043162564, 'ionic_force_x': 10.11287471652031, 'ionic_force_y': 10.04846477508545, 'ionic_force_z': -1.8506518509238958, 'radial_force': 14.256292623545884, 'axial_force': -1.8506518509238958, 'contributions': [{'ion': 1327, 'force': [1.2898728847503662, 1.1364672183990479, -0.002380242571234703], 'magnitude': 1.7191089391708374, 'distance': 13.896881103515625, 'cosine_with_motion': 0.7566192745686137, 'motion_component': 1.300710940442879}, {'ion': 1330, 'force': [1.9785761833190918, 2.999788999557495, -2.8233442306518555], 'magnitude': 4.569985866546631, 'distance': 8.523375511169434, 'cosine_with_motion': 0.15315490329314418, 'motion_component': 0.6999157363938693}, {'ion': 1355, 'force': [5.315892219543457, 0.6447122097015381, 0.9586648941040039], 'magnitude': 5.439981937408447, 'distance': 7.812145709991455, 'cosine_with_motion': 0.8776417747553531, 'motion_component': 4.774355307240334}, {'ion': 1465, 'force': [0.49871</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>{6569: {'frame': 6569, 'ionic_force': [8.93659296631813, 4.198592029511929, -11.964962244033813], 'ionic_force_magnitude': 15.51293622681027, 'motion_vector': [0.9375572204589844, 4.542621612548828, 3.9090347290039062], 'cosine_ionic_motion': -0.20531702194883455, 'ionic_motion_component': -3.185069867770875, 'ionic_force_x': 8.93659296631813, 'ionic_force_y': 4.198592029511929, 'ionic_force_z': -11.964962244033813, 'radial_force': 9.87374644579897, 'axial_force': -11.964962244033813, 'contributions': [{'ion': 1327, 'force': [2.5776994228363037, 1.23420250415802, -1.3029985427856445], 'magnitude': 3.1409544944763184, 'distance': 10.281067848205566, 'directional_contribution': 0.4829944183947106}, {'ion': 1330, 'force': [3.5478971004486084, -3.1198573112487793, -2.1965181827545166], 'magnitude': 5.210160732269287, 'distance': 7.982583522796631, 'directional_contribution': -3.20352882053065}, {'ion': 1341, 'force': [1.5748634338378906, 5.740958213806152, -3.378621816635132], 'magnitude': 6.844989776611328, 'distance': 6.964383125305176, 'directional_contribution': 2.365421161972364}, {'ion': 1359, 'force': [1.0105098485946655, 0.24263377487659454, -3.6123909950256348], 'magnitude': 3.7589054107666016, 'distance': 9.398062705993652, 'directional_contribution': -1.990040356360307}, {'ion': 1374, 'force': [0.22562316060066223, 0.10065484791994095, -1.4744327068328857], 'magnitude': 1.494987964630127, 'distance': 14.902193069458008, 'directional_contribution': -0.8399164247898128}]}, 6570: {'frame': 6570, 'ionic_force': [12.369088254868984, 9.554802000522614, -1.3525469191372395], 'ionic_force_magnitude': 15.688147395227915, 'motion_vector': [0.08165740966796875, 0.8572654724121094, 0.46636962890625], 'cosine_ionic_motion': 0.5578220875076787, 'ionic_motion_component': 8.751195129134187, 'ionic_force_x': 12.369088254868984, 'ionic_force_y': 9.554802000522614, 'ionic_force_z': -1.3525469191372395, 'radial_force': 15.629734019679567, 'axial_force': -1.3525469191372395, 'contributions': [{'ion': 1327, 'force': [1.5750917196273804, 1.453436017036438, -0.059865642338991165], 'magnitude': 2.1440553665161133, 'distance': 12.443742752075195, 'directional_contribution': 1.3751127123759574}, {'ion': 1330, 'force': [8.851373672485352, -0.5448993444442749, 0.612082302570343], 'magnitude': 8.889227867126465, 'distance': 6.1113481521606445, 'directional_contribution': 0.5525385419218214}, {'ion': 1341, 'force': [-0.1118030920624733, 4.923777103424072, 3.27870774269104], 'magnitude': 5.9165873527526855, 'distance': 7.490889549255371, 'directional_contribution': 5.862158742332892}, {'ion': 1359, 'force': [1.5930393934249878, 2.9040167331695557, -3.243910789489746], 'magnitude': 4.636167049407959, 'distance': 8.462321281433105, 'directional_contribution': 1.130102852027684}, {'ion': 1374, 'force': [0.4613865613937378, 0.8184714913368225, -1.9395605325698853], 'magnitude': 2.155149221420288, 'distance': 12.411674499511719, 'directional_contribution': -0.1687178298596086}]}, 6571: {'frame': 6571, 'ionic_force': [10.874882519245148, 11.021745204925537, -1.5739329904317856], 'ionic_force_magnitude': 15.563393017849684, 'motion_vector': [-0.7143974304199219, 2.6378211975097656, 0.46242523193359375], 'cosine_ionic_motion': 0.4770052911616335, 'ionic_motion_component': 7.423820817942322, 'ionic_force_x': 10.874882519245148, 'ionic_force_y': 11.021745204925537, 'ionic_force_z': -1.5739329904317856, 'radial_force': 15.483602202642729, 'axial_force': -1.5739329904317856, 'contributions': [{'ion': 1327, 'force': [0.9435466527938843, 1.3866626024246216, -0.0861724466085434], 'magnitude': 1.6794461011886597, 'distance': 14.060022354125977, 'directional_contribution': 1.0621120842852612}, {'ion': 1330, 'force': [7.051734924316406, 1.6229393482208252, 0.9881018400192261], 'magnitude': 7.3032355308532715, 'distance': 6.742351531982422, 'directional_contribution': -0.10816276256291779}, {'ion': 1341, 'force': [0.5937607288360596, 3.663236141204834, 2.101393938064575], 'magnitude': 4.264704704284668, 'distance': 8.82316780090332, 'directional_contribution': 3.683851482704153}, {'ion': 1359, 'force': [1.727158784866333, 3.3323826789855957, -2.602457046508789], 'magnitude': 4.5673441886901855, 'distance': 8.525839805603027, 'directional_contribution': 2.29206552316883}, {'ion': 1374, 'force': [0.5586814284324646, 1.0165244340896606, -1.9747992753982544], 'magnitude': 2.290257453918457, 'distance': 12.040011405944824, 'directional_contribution': 0.49395454936455074}]}, 6572: {'frame': 6572, 'ionic_force': [4.297864839434624, 8.788159370422363, -1.320813924074173], 'ionic_force_magnitude': 9.871572150372959, 'motion_vector': [0.8923988342285156, -0.882781982421875, -0.6154251098632812], 'cosine_ionic_motion': -0.2253358781914698, 'ionic_motion_component': -2.224419379634747, 'ionic_force_x': 4.297864839434624, 'ionic_force_y': 8.788159370422363, 'ionic_force_z': -1.320813924074173, 'radial_force': 9.782810807635544, 'axial_force': -1.320813924074173, 'contributions': [{'ion': 1330, 'force': [3.4389588832855225, 2.7700512409210205, 0.2946772277355194], 'magnitude': 4.425658702850342, 'distance': 8.661239624023438, 'directional_contribution': 0.3163212673156721}, {'ion': 1341, 'force': [-0.10774736106395721, 2.0299341678619385, 1.3322513103485107], 'magnitude': 2.430459976196289, 'distance': 11.687585830688477, 'directional_contribution': -1.9370725058540001}, {'ion': 1359, 'force': [0.6919946074485779, 2.870731830596924, -1.4831961393356323], 'magnitude': 3.304516315460205, 'distance': 10.02340030670166, 'directional_contribution': -0.718092146719588}, {'ion': 1374, 'force': [0.2746587097644806, 1.1174421310424805, -1.4645463228225708], 'magnitude': 1.8625279664993286, 'distance': 13.351118087768555, 'directional_contribution': 0.11442417383104164}]}, 6573: {'frame': 6573, 'ionic_force': [6.707516588270664, 9.176944971084595, -0.1950500402599573], 'ionic_force_magnitude': 11.368603357600545, 'motion_vector': [-0.3231239318847656, -0.48430633544921875, 0.06146240234375], 'cosine_ionic_motion': -0.995217753560235, 'ionic_motion_component': -11.31423589466856, 'ionic_force_x': 6.707516588270664, 'ionic_force_y': 9.176944971084595, 'ionic_force_z': -0.1950500402599573, 'radial_force': 11.366930007008971, 'axial_force': -0.1950500402599573, 'contributions': [{'ion': 1327, 'force': [0.9881269335746765, 1.1771571636199951, 0.006705602630972862], 'magnitude': 1.5369250774383545, 'distance': 14.697473526000977, 'directional_contribution': -1.5184832920336617}, {'ion': 1330, 'force': [4.258534908294678, 1.36393404006958, 1.1857856512069702], 'magnitude': 4.62617826461792, 'distance': 8.471452713012695, 'directional_contribution': -3.354258527189531}, {'ion': 1341, 'force': [-0.05445399135351181, 2.8371944427490234, 1.6453436613082886], 'magnitude': 3.28021240234375, 'distance': 10.060464859008789, 'directional_contribution': -2.144285189327313}, {'ion': 1359, 'force': [1.1280900239944458, 2.8237078189849854, -1.7318087816238403], 'magnitude': 3.499296188354492, 'distance': 9.740442276000977, 'directional_contribution': -3.14036519314781}, {'ion': 1374, 'force': [0.387218713760376, 0.9749515056610107, -1.3010761737823486], 'magnitude': 1.6713072061538696, 'distance': 14.094215393066406, 'directional_contribution': -1.1568440041993604}]}, 6574: {'frame': 6574, 'ionic_force': [9.922765612602234, 10.655503034591675, -1.8789064027369022], 'ionic_force_magnitude': 14.680984694259426, 'motion_vector': [0.2715606689453125, -0.07678985595703125, -0.05289459228515625], 'cosine_ionic_motion': 0.4687223494525201, 'ionic_motion_component': 6.881305638169765, 'ionic_force_x': 9.922765612602234, 'ionic_force_y': 10.655503034591675, 'ionic_force_z': -1.8789064027369022, 'radial_force': 14.560254885228959, 'axial_force': -1.8789064027369022, 'contributions': [{'ion': 1327, 'force': [0.8655595183372498, 1.3287378549575806, -0.03194442763924599], 'magnitude': 1.5861141681671143, 'distance': 14.467777252197266, 'directional_contribution': 0.4691645916303158}, {'ion': 1330, 'force': [6.645339488983154, 1.9468575716018677, 1.6377795934677124], 'magnitude': 7.115694999694824, 'distance': 6.830624103546143, 'directional_contribution': 5.462757472369846}, {'ion': 1341, 'force': [0.7769212126731873, 3.7414112091064453, 0.19452917575836182], 'magnitude': 3.826173782348633, 'distance': 9.315082550048828, 'directional_contribution': -0.3016500287318795}, {'ion': 1359, 'force': [1.2521162033081055, 2.632829427719116, -2.2195000648498535], 'magnitude': 3.664118766784668, 'distance': 9.518845558166504, 'directional_contribution': 0.8889929729182668}, {'ion': 1374, 'force': [0.3828291893005371, 1.005666971206665, -1.459770679473877], 'magnitude': 1.8135199546813965, 'distance': 13.530313491821289, 'directional_contribution': 0.3620408168458269}]}, 6575: {'frame': 6575, 'ionic_force': [6.102406769990921, 8.403478920459747, -1.6997588761150837], 'ionic_force_magnitude': 10.52364036776126, 'motion_vector': [-0.7413291931152344, 0.8488311767578125, 0.4405517578125], 'cosine_ionic_motion': 0.14609900437198084, 'ionic_motion_component': 1.5374933800987063, 'ionic_force_x': 6.102406769990921, 'ionic_force_y': 8.403478920459747, 'ionic_force_z': -1.6997588761150837, 'radial_force': 10.385462259959464, 'axial_force': -1.6997588761150837, 'contributions': [{'ion': 1330, 'force': [3.698859691619873, 1.877339243888855, -0.03207122161984444], 'magnitude': 4.148131370544434, 'distance': 8.94628620147705, 'directional_contribution': -0.9608514648929098}, {'ion': 1341, 'force': [0.6937668323516846, 2.8005433082580566, 1.644039273262024], 'magnitude': 3.320725917816162, 'distance': 9.998907089233398, 'directional_contribution': 2.1381010385898946}, {'ion': 1359, 'force': [1.2716120481491089, 2.7411482334136963, -1.8873075246810913], 'magnitude': 3.5626986026763916, 'distance': 9.653382301330566, 'directional_contribution': 0.45671016417391286}, {'ion': 1374, 'force': [0.4381681978702545, 0.9844481348991394, -1.4244194030761719], 'magnitude': 1.7860851287841797, 'distance': 13.633832931518555, 'directional_contribution': -0.09646636963300992}]}, 6576: {'frame': 6576, 'ionic_force': [5.697530130855739, 9.966541528701782, -1.1423418633639812], 'ionic_force_magnitude': 11.536842920320106, 'motion_vector': [0.1239013671875, -0.14241409301757812, -0.3520050048828125], 'cosine_ionic_motion': -0.06756220567549721, 'ionic_motion_component': -0.7794545542285709, 'ionic_force_x': 5.697530130855739, 'ionic_force_y': 9.966541528701782, 'ionic_force_z': -1.1423418633639812, 'radial_force': 11.480148066786693, 'axial_force': -1.1423418633639812, 'contributions': [{'ion': 1327, 'force': [0.8476411700248718, 1.4078731536865234, 0.05625929310917854], 'magnitude': 1.6443136930465698, 'distance': 14.209431648254395, 'directional_contribution': -0.28861598567276614}, {'ion': 1330, 'force': [3.670255661010742, 1.709186315536499, 0.31133517622947693], 'magnitude': 4.060667991638184, 'distance': 9.042120933532715, 'directional_contribution': 0.25473058028006434}, {'ion': 1341, 'force': [0.002328316681087017, 2.6095755100250244, 1.5804171562194824], 'magnitude': 3.050837278366089, 'distance': 10.431806564331055, 'directional_contribution': -2.322501282066058}, {'ion': 1359, 'force': [0.9095866680145264, 3.105701446533203, -1.6332862377166748], 'magnitude': 3.624962568283081, 'distance': 9.570117950439453, 'directional_contribution': 0.6142027188966424}, {'ion': 1374, 'force': [0.2677183151245117, 1.1342051029205322, -1.4570672512054443], 'magnitude': 1.8657810688018799, 'distance': 13.339473724365234, 'directional_contribution': 0.9627294710664245}]}, 6577: {'frame': 6577, 'ionic_force': [10.770041853189468, 11.033284544944763, -1.4359604306519032], 'ionic_force_magnitude': 15.48512679081343, 'motion_vector': [2.2769126892089844, -2.477092742919922, -0.91888427734375], 'cosine_ionic_motion': -0.027561089715659084, 'ionic_motion_component': -0.42678696873996497, 'ionic_force_x': 10.770041853189468, 'ionic_force_y': 11.033284544944763, 'ionic_force_z': -1.4359604306519032, 'radial_force': 15.41840359340648, 'axial_force': -1.4359604306519032, 'contributions': [{'ion': 1327, 'force': [1.0223180055618286, 1.2306550741195679, 0.052624136209487915], 'magnitude': 1.6007546186447144, 'distance': 14.401464462280273, 'directional_contribution': -0.22050455002434877}, {'ion': 1330, 'force': [7.852027416229248, 3.727412223815918, 1.5429376363754272], 'magnitude': 8.827717781066895, 'distance': 6.132602691650391, 'directional_contribution': 2.0722171355634664}, {'ion': 1341, 'force': [0.4523809254169464, 1.9864200353622437, 0.05863363668322563], 'magnitude': 2.0381243228912354, 'distance': 12.76302719116211, 'directional_contribution': -1.1309149590530434}, {'ion': 1359, 'force': [1.0853403806686401, 2.987722158432007, -1.669343113899231], 'magnitude': 3.5904252529144287, 'distance': 9.616036415100098, 'directional_contribution': -0.9735986645634576}, {'ion': 1374, 'force': [0.3579751253128052, 1.1010750532150269, -1.420812726020813], 'magnitude': 1.832817792892456, 'distance': 13.458894729614258, 'directional_contribution': -0.17398542697419472}]}, 6578: {'frame': 6578, 'ionic_force': [11.297083020210266, 8.097006931900978, -3.776877298951149], 'ionic_force_magnitude': 14.403138829856085, 'motion_vector': [-1.2792587280273438, 0.96728515625, 1.4186248779296875], 'cosine_ionic_motion': -0.38838770659146066, 'ionic_motion_component': -5.594002057846219, 'ionic_force_x': 11.297083020210266, 'ionic_force_y': 8.097006931900978, 'ionic_force_z': -3.776877298951149, 'radial_force': 13.899122491034303, 'axial_force': -3.776877298951149, 'contributions': [{'ion': 1327, 'force': [1.3949049711227417, 1.2103792428970337, -0.1234259232878685], 'magnitude': 1.8509489297866821, 'distance': 13.392813682556152, 'directional_contribution': -0.36837565457455934}, {'ion': 1330, 'force': [4.5826263427734375, 0.2037651091814041, 0.11392490565776825], 'magnitude': 4.588568687438965, 'distance': 8.506098747253418, 'directional_contribution': -2.57038469530253}, {'ion': 1341, 'force': [2.695676326751709, 3.7334976196289062, 0.10549106448888779], 'magnitude': 4.606170177459717, 'distance': 8.48983097076416, 'directional_contribution': 0.1459672195302515}, {'ion': 1359, 'force': [2.0399694442749023, 2.267669677734375, -2.4146974086761475], 'magnitude': 3.8903167247772217, 'distance': 9.237970352172852, 'directional_contribution': -1.7942070947055129}, {'ion': 1374, 'force': [0.5839059352874756, 0.681695282459259, -1.458169937133789], 'magnitude': 1.7122832536697388, 'distance': 13.924551963806152, 'directional_contribution': -1.0070017571075702}]}, 6579: {'frame': 6579, 'ionic_force': [9.608516097068787, 8.373697221279144, -1.9300379157066345], 'ionic_force_magnitude': 12.89059475343761, 'motion_vector': [2.924358367919922, -6.608238220214844, -2.4186172485351562], 'cosine_ionic_motion': -0.22974953235812362, 'ionic_motion_component': -2.9616081164203725, 'ionic_force_x': 9.608516097068787, 'ionic_force_y': 8.373697221279144, 'ionic_force_z': -1.9300379157066345, 'radial_force': 12.745288805723, 'axial_force': -1.9300379157066345, 'contributions': [{'ion': 1327, 'force': [1.3253157138824463, 1.562822699546814, 0.09811156988143921], 'magnitude': 2.0514633655548096, 'distance': 12.721465110778809, 'directional_contribution': -0.8777894316682975}, {'ion': 1330, 'force': [5.451991558074951, 0.6885251402854919, 1.5081236362457275], 'magnitude': 5.698483943939209, 'distance': 7.632896900177002, 'directional_contribution': 1.0164915061803086}, {'ion': 1341, 'force': [0.3505029082298279, 1.43211030960083, 0.5435124635696411], 'magnitude': 1.5713682174682617, 'distance': 14.535503387451172, 'directional_contribution': -1.2798917314959368}, {'ion': 1359, 'force': [1.873288631439209, 3.515359878540039, -2.291175127029419], 'magnitude': 4.595263957977295, 'distance': 8.499899864196777, 'directional_contribution': -1.6023703007219012}, {'ion': 1374, 'force': [0.6074172854423523, 1.1748791933059692, -1.7886104583740234], 'magnitude': 2.2245054244995117, 'distance': 12.216654777526855, 'directional_contribution': -0.21804798582489582}]}, 6580: {'frame': 6580, 'ionic_force': [9.401102185249329, 2.19012341927737, -3.330233727581799], 'ionic_force_magnitude': 10.211161519116729, 'motion_vector': [0.0558624267578125, 1.9655532836914062, -0.0980682373046875], 'cosine_ionic_motion': 0.2564989404926745, 'ionic_motion_component': 2.6191521108530096, 'ionic_force_x': 9.401102185249329, 'ionic_force_y': 2.19012341927737, 'ionic_force_z': -3.330233727581799, 'radial_force': 9.652842218184595, 'axial_force': -3.330233727581799, 'contributions': [{'ion': 1327, 'force': [1.994491696357727, 0.5432167649269104, -0.318158358335495], 'magnitude': 2.091484308242798, 'distance': 12.599164009094238, 'directional_contribution': 0.6147630256647435}, {'ion': 1330, 'force': [1.841148018836975, -1.1111570596694946, 0.003038342110812664], 'magnitude': 2.1504664421081543, 'distance': 12.425180435180664, 'directional_contribution': -1.0572404228431884}, {'ion': 1341, 'force': [3.1475207805633545, 2.842928171157837, 0.6421310901641846], 'magnitude': 4.289692401885986, 'distance': 8.797432899475098, 'directional_contribution': 2.89557522958656}, {'ion': 1359, 'force': [1.743165135383606, -0.0841091051697731, -2.3038322925567627], 'magnitude': 2.8902149200439453, 'distance': 10.717759132385254, 'directional_contribution': 0.08024686087711674}, {'ion': 1374, 'force': [0.674776554107666, -0.0007553519681096077, -1.3534125089645386], 'magnitude': 1.5122994184494019, 'distance': 14.816655158996582, 'directional_contribution': 0.08580736227417984}]}, 6581: {'frame': 6581, 'ionic_force': [8.237632095813751, 2.8010704964399338, -3.125244453549385], 'ionic_force_magnitude': 9.245092285447901, 'motion_vector': [-1.0904083251953125, 0.6786651611328125, -0.0248260498046875], 'cosine_ionic_motion': -0.5897330513000432, 'ionic_motion_component': -5.45213648304768, 'ionic_force_x': 8.237632095813751, 'ionic_force_y': 2.8010704964399338, 'ionic_force_z': -3.125244453549385, 'radial_force': 8.700837802878933, 'axial_force': -3.125244453549385, 'contributions': [{'ion': 1327, 'force': [1.5015419721603394, 0.9385555386543274, -0.21082422137260437], 'magnitude': 1.7832446098327637, 'distance': 13.644686698913574, 'directional_contribution': -0.7746350255753975}, {'ion': 1330, 'force': [2.607945680618286, -0.777786374092102, -0.1844618171453476], 'magnitude': 2.7277021408081055, 'distance': 11.032414436340332, 'directional_contribution': -2.621054553634242}, {'ion': 1341, 'force': [1.963555932044983, 2.088361978530884, 0.7296456098556519], 'magnitude': 2.9579031467437744, 'distance': 10.594417572021484, 'directional_contribution': -0.5775294285032408}, {'ion': 1359, 'force': [1.4981328248977661, 0.38405388593673706, -2.148705005645752], 'magnitude': 2.6474199295043945, 'distance': 11.198442459106445, 'directional_contribution': -1.0272382066311811}, {'ion': 1374, 'force': [0.6664556860923767, 0.16788546741008759, -1.310899019241333], 'magnitude': 1.480136752128601, 'distance': 14.976768493652344, 'directional_contribution': -0.45167915777951295}]}, 6582: {'frame': 6582, 'ionic_force': [13.439601302146912, 8.873756095767021, -5.538107238709927], 'ionic_force_magnitude': 17.030474514683455, 'motion_vector': [-3.5965843200683594, -4.00225830078125, 1.7977447509765625], 'cosine_ionic_motion': -0.9709190363327294, 'ionic_motion_component': -16.535211904085568, 'ionic_force_x': 13.439601302146912, 'ionic_force_y': 8.873756095767021, 'ionic_force_z': -5.538107238709927, 'radial_force': 16.104857354470152, 'axial_force': -5.538107238709927, 'contributions': [{'ion': 1327, 'force': [1.7381343841552734, 1.2546632289886475, -0.4241744577884674], 'magnitude': 2.1852266788482666, 'distance': 12.32596206665039, 'directional_contribution': -2.1214406083064645}, {'ion': 1330, 'force': [7.226673126220703, 3.71441388130188, -0.0353500172495842], 'magnitude': 8.125449180603027, 'distance': 6.392126560211182, 'directional_contribution': -7.21300471545702}, {'ion': 1341, 'force': [2.3823862075805664, 2.991396427154541, -1.2005852460861206], 'magnitude': 4.008194446563721, 'distance': 9.101116180419922, 'directional_contribution': -4.0011063288809225}, {'ion': 1359, 'force': [1.5048085451126099, 0.7228309512138367, -2.4776906967163086], 'magnitude': 2.987621784210205, 'distance': 10.541592597961426, 'directional_contribution': -2.249056399859022}, {'ion': 1374, 'force': [0.5875990390777588, 0.19045160710811615, -1.4003068208694458], 'magnitude': 1.5304913520812988, 'distance': 14.728333473205566, 'directional_contribution': -0.9506037495882076}]}, 6583: {'frame': 6583, 'ionic_force': [16.05817210674286, 6.1076273918151855, 3.6224589943885803], 'ionic_force_magnitude': 17.558195036308607, 'motion_vector': [-2.217937469482422, 1.4410781860351562, 1.8284072875976562], 'cosine_ionic_motion': -0.35763561505257213, 'ionic_motion_component': -6.279435881023248, 'ionic_force_x': 16.05817210674286, 'ionic_force_y': 6.1076273918151855, 'ionic_force_z': 3.6224589943885803, 'radial_force': 17.180454119930168, 'axial_force': 3.6224589943885803, 'contributions': [{'ion': 1327, 'force': [4.602260112762451, 2.496872901916504, -0.22734969854354858], 'magnitude': 5.2408833503723145, 'distance': 7.959151744842529, 'directional_contribution': -2.1847813997755807}, {'ion': 1330, 'force': [9.457734107971191, -11.10282039642334, 7.554731369018555], 'magnitude': 16.425447463989258, 'distance': 4.495835781097412, 'directional_contribution': -7.203866159760764}, {'ion': 1341, 'force': [-2.9511709213256836, 18.338525772094727, 8.4227876663208], 'magnitude': 20.394956588745117, 'distance': 4.034666538238525, 'directional_contribution': 15.044010246081825}, {'ion': 1359, 'force': [4.432460308074951, -3.265843629837036, -9.403403282165527], 'magnitude': 10.896624565124512, 'distance': 5.519796371459961, 'directional_contribution': -9.868182734805686}, {'ion': 1374, 'force': [0.5168884992599487, -0.35910725593566895, -2.724307060241699], 'magnitude': 2.796065092086792, 'distance': 10.896710395812988, 'directional_contribution': -2.066616029296412}]}, 6584: {'frame': 6584, 'ionic_force': [-2.7984437588602304, -2.5238340757787228, -6.624991416931152], 'ionic_force_magnitude': 7.621780447374292, 'motion_vector': [0.10931777954101562, -0.3145332336425781, 0.6563186645507812], 'cosine_ionic_motion': -0.688175507913837, 'ionic_motion_component': -5.245122630579555, 'ionic_force_x': -2.7984437588602304, 'ionic_force_y': -2.5238340757787228, 'ionic_force_z': -6.624991416931152, 'radial_force': 3.7684248584210374, 'axial_force': -6.624991416931152, 'contributions': [{'ion': 1327, 'force': [3.3435709476470947, 4.247110366821289, 1.7031737565994263], 'magnitude': 5.667293548583984, 'distance': 7.653872013092041, 'directional_contribution': 0.20039040457326607}, {'ion': 1330, 'force': [-2.1344544887542725, -9.71019172668457, 4.399707794189453], 'magnitude': 10.872035026550293, 'distance': 5.526034832000732, 'directional_contribution': 7.756483872724257}, {'ion': 1341, 'force': [-3.1538000106811523, 3.324544906616211, 1.762978434562683], 'magnitude': 4.909902572631836, 'distance': 8.223043441772461, 'directional_contribution': -0.3170972984109426}, {'ion': 1359, 'force': [-0.8428261280059814, -0.053758349269628525, -11.009814262390137], 'magnitude': 11.042158126831055, 'distance': 5.483300685882568, 'directional_contribution': -9.920624908005133}, {'ion': 1374, 'force': [-0.010934079065918922, -0.3315392732620239, -3.481037139892578], 'magnitude': 3.4968066215515137, 'distance': 9.743908882141113, 'directional_contribution': -2.9642747308761317}]}, 6585: {'frame': 6585, 'ionic_force': [0.19422585517168045, 0.5162233263254166, -7.085144519805908], 'ionic_force_magnitude': 7.1065802656408055, 'motion_vector': [-1.3601837158203125, -0.6397171020507812, -1.1410140991210938], 'cosine_ionic_motion': 0.558483083688465, 'ionic_motion_component': 3.968904861234668, 'ionic_force_x': 0.19422585517168045, 'ionic_force_y': 0.5162233263254166, 'ionic_force_z': -7.085144519805908, 'radial_force': 0.5515525409783261, 'axial_force': -7.085144519805908, 'contributions': [{'ion': 1327, 'force': [5.026834011077881, 4.280613899230957, 2.439513683319092], 'magnitude': 7.038745880126953, 'distance': 6.867859363555908, 'directional_contribution': -6.549275829282578}, {'ion': 1330, 'force': [-0.1826930046081543, -6.5750732421875, 4.005751609802246], 'magnitude': 7.701364040374756, 'distance': 6.565762996673584, 'directional_contribution': -0.06143517342584914}, {'ion': 1341, 'force': [-4.096582412719727, 4.5770263671875, 3.0861237049102783], 'magnitude': 6.874250411987305, 'distance': 6.949544906616211, 'directional_contribution': -0.4648376132503955}, {'ion': 1359, 'force': [-0.4727668762207031, -1.7130180597305298, -13.051497459411621], 'magnitude': 13.171921730041504, 'distance': 5.020471096038818, 'directional_contribution': 8.812779214975947}, {'ion': 1374, 'force': [-0.08056586235761642, -0.05332563817501068, -3.5650360584259033], 'magnitude': 3.566344976425171, 'distance': 9.648446083068848, 'directional_contribution': 2.2316741953015637}]}, 6586: {'frame': 6586, 'ionic_force': [-4.087879508733749, 1.6345014572143555, -16.545942544937134], 'ionic_force_magnitude': 17.121640359262365, 'motion_vector': [1.223419189453125, 0.5366973876953125, 1.0523300170898438], 'cosine_ionic_motion': -0.7396064486371673, 'ionic_motion_component': -12.663275620956831, 'ionic_force_x': -4.087879508733749, 'ionic_force_y': 1.6345014572143555, 'ionic_force_z': -16.545942544937134, 'radial_force': 4.402539482112696, 'axial_force': -16.545942544937134, 'contributions': [{'ion': 1327, 'force': [6.040377140045166, 7.853013038635254, 1.4087369441986084], 'magnitude': 10.007022857666016, 'distance': 5.759922027587891, 'directional_contribution': 7.695346888200817}, {'ion': 1330, 'force': [-0.9158151745796204, -3.5589420795440674, 1.8877583742141724], 'magnitude': 4.131394386291504, 'distance': 8.96438980102539, 'directional_contribution': -0.6138584619205041}, {'ion': 1341, 'force': [-4.4826340675354, 2.6424269676208496, 1.3166965246200562], 'magnitude': 5.3675055503845215, 'distance': 7.864711284637451, 'directional_contribution': -1.57608198749287}, {'ion': 1359, 'force': [-4.346304893493652, -4.65595006942749, -17.659698486328125], 'magnitude': 18.773204803466797, 'distance': 4.20532751083374, 'directional_contribution': -15.523524452550248}, {'ion': 1374, 'force': [-0.3835025131702423, -0.6460464000701904, -3.4994359016418457], 'magnitude': 3.579176187515259, 'distance': 9.631135940551758, 'directional_contribution': -2.645157889305745}]}, 6587: {'frame': 6587, 'ionic_force': [-1.3948394022881985, 2.136453092098236, -10.57060980796814], 'ionic_force_magnitude': 10.874180451198336, 'motion_vector': [0.24559402465820312, 0.056308746337890625, 0.05919647216796875], 'cosine_ionic_motion': -0.30129583505560287, 'ionic_motion_component': -3.276345279589115, 'ionic_force_x': -1.3948394022881985, 'ionic_force_y': 2.136453092098236, 'ionic_force_z': -10.57060980796814, 'radial_force': 2.5514718836216503, 'axial_force': -10.57060980796814, 'contributions': [{'ion': 1327, 'force': [3.978027582168579, 4.168118000030518, 1.4422818422317505], 'magnitude': 5.939536094665527, 'distance': 7.476404190063477, 'directional_contribution': 5.011301721015714}, {'ion': 1330, 'force': [-1.348442554473877, -4.446995735168457, 2.636247396469116], 'magnitude': 5.34264612197876, 'distance': 7.8829874992370605, 'directional_contribution': -1.6440245369487094}, {'ion': 1341, 'force': [-2.968979835510254, 3.28828763961792, 1.8167105913162231], 'magnitude': 4.788331031799316, 'distance': 8.326777458190918, 'directional_contribution': -1.6863070816566061}, {'ion': 1359, 'force': [-1.085584044456482, -0.44185957312583923, -12.848565101623535], 'magnitude': 12.9019136428833, 'distance': 5.072732925415039, 'directional_contribution': -4.064815264525501}, {'ion': 1374, 'force': [0.03013944998383522, -0.43109723925590515, -3.6172845363616943], 'magnitude': 3.6430070400238037, 'distance': 9.54638671875, 'directional_contribution': -0.8925000544187769}]}, 6588: {'frame': 6588, 'ionic_force': [2.170046664774418, 2.544392377138138, -12.059692144393921], 'ionic_force_magnitude': 12.514759674627943, 'motion_vector': [0.011474609375, 0.145538330078125, 0.04688262939453125], 'cosine_ionic_motion': -0.08868653371753571, 'ionic_motion_component': -1.1098906558507473, 'ionic_force_x': 2.170046664774418, 'ionic_force_y': 2.544392377138138, 'ionic_force_z': -12.059692144393921, 'radial_force': 3.3441045282911297, 'axial_force': -12.059692144393921, 'contributions': [{'ion': 1327, 'force': [5.032597064971924, 4.4192280769348145, 2.0241124629974365], 'magnitude': 6.996687889099121, 'distance': 6.88847017288208, 'directional_contribution': 5.190070898259815}, {'ion': 1330, 'force': [-0.6638263463973999, -3.996150016784668, 3.0800297260284424], 'magnitude': 5.0888566970825195, 'distance': 8.077164649963379, 'directional_contribution': -2.9009400990388547}, {'ion': 1341, 'force': [-1.5257741212844849, 3.4375202655792236, 1.539534568786621], 'magnitude': 4.063827991485596, 'distance': 9.038604736328125, 'directional_contribution': 3.619313609954143}, {'ion': 1359, 'force': [-0.7339341640472412, -0.867084801197052, -14.88182544708252], 'magnitude': 14.92512035369873, 'distance': 4.716394424438477, 'directional_contribution': -5.428146678758035}, {'ion': 1374, 'force': [0.060984231531620026, -0.4491211473941803, -3.8215434551239014], 'magnitude': 3.848327398300171, 'distance': 9.28823184967041, 'directional_contribution': -1.590188351621685}]}, 6589: {'frame': 6589, 'ionic_force': [1.487856362015009, 2.025739461183548, -13.677444696426392], 'ionic_force_magnitude': 13.90646721286133, 'motion_vector': [-0.4328804016113281, 0.26816558837890625, -0.0641326904296875], 'cosine_ionic_motion': 0.10877237261114421, 'ionic_motion_component': 1.5126394333820126, 'ionic_force_x': 1.487856362015009, 'ionic_force_y': 2.025739461183548, 'ionic_force_z': -13.677444696426392, 'radial_force': 2.5134313037329563, 'axial_force': -13.677444696426392, 'contributions': [{'ion': 1327, 'force': [5.244095802307129, 5.000150203704834, 2.211571216583252], 'magnitude': 7.575822830200195, 'distance': 6.619941234588623, 'directional_contribution': -2.0868218563574565}, {'ion': 1330, 'force': [-0.4646747410297394, -4.937812328338623, 4.85559606552124], 'magnitude': 6.940801620483398, 'distance': 6.916147232055664, 'directional_contribution': -2.7948254119333065}, {'ion': 1341, 'force': [-2.9041500091552734, 3.8647563457489014, 2.0955615043640137], 'magnitude': 5.268947601318359, 'distance': 7.93792724609375, 'directional_contribution': 4.2069342084578345}, {'ion': 1359, 'force': [-0.32860058546066284, -1.6061543226242065, -19.161134719848633], 'magnitude': 19.231142044067383, 'distance': 4.154956817626953, 'directional_contribution': 1.8322652544494318}, {'ion': 1374, 'force': [-0.05881410464644432, -0.2952004373073578, -3.6790387630462646], 'magnitude': 3.691331386566162, 'distance': 9.48369312286377, 'directional_contribution': 0.3550871634542645}]}, 6590: {'frame': 6590, 'ionic_force': [1.9864058825187385, 3.334870845079422, -7.872519016265869], 'ionic_force_magnitude': 8.777455641866469, 'motion_vector': [1.7067832946777344, -0.3767433166503906, -1.9141845703125], 'cosine_ionic_motion': 0.7561174737825332, 'ionic_motion_component': 6.636787586166318, 'ionic_force_x': 1.9864058825187385, 'ionic_force_y': 3.334870845079422, 'ionic_force_z': -7.872519016265869, 'radial_force': 3.8816455123395524, 'axial_force': -7.872519016265869, 'contributions': [{'ion': 1327, 'force': [6.007285118103027, 3.977473020553589, 3.4593403339385986], 'magnitude': 7.992171287536621, 'distance': 6.44520378112793, 'directional_contribution': 0.8228099331436773}, {'ion': 1330, 'force': [-0.007665280718356371, -2.9617135524749756, 3.247918128967285], 'magnitude': 4.395540714263916, 'distance': 8.690862655639648, 'directional_contribution': -1.9730447225018877}, {'ion': 1341, 'force': [-2.899707555770874, 3.2841711044311523, 2.0908212661743164], 'magnitude': 4.854443073272705, 'distance': 8.269882202148438, 'directional_contribution': -3.930617987100092}, {'ion': 1359, 'force': [-1.2136359214782715, -0.7365626692771912, -12.827872276306152], 'magnitude': 12.906189918518066, 'distance': 5.071892261505127, 'directional_contribution': 8.780802270129374}, {'ion': 1374, 'force': [0.10012952238321304, -0.22849705815315247, -3.842726469039917], 'magnitude': 3.850815773010254, 'distance': 9.285229682922363, 'directional_contribution': 2.9368382764187424}]}, 6591: {'frame': 6591, 'ionic_forc</t>
+          <t>{6569: {'frame': 6569, 'ionic_force': [8.93659296631813, 4.198592029511929, -11.964962244033813], 'ionic_force_magnitude': 15.51293622681027, 'motion_vector': [0.9375572204589844, 4.542621612548828, 3.9090347290039062], 'cosine_ionic_motion': -0.20531702194883455, 'ionic_motion_component': -3.185069867770875, 'ionic_force_x': 8.93659296631813, 'ionic_force_y': 4.198592029511929, 'ionic_force_z': -11.964962244033813, 'radial_force': 9.87374644579897, 'axial_force': -11.964962244033813, 'contributions': [{'ion': 1327, 'force': [2.5776994228363037, 1.23420250415802, -1.3029985427856445], 'magnitude': 3.1409544944763184, 'distance': 10.281067848205566, 'cosine_with_motion': 0.15377313307214993, 'motion_component': 0.4829944183947106}, {'ion': 1330, 'force': [3.5478971004486084, -3.1198573112487793, -2.1965181827545166], 'magnitude': 5.210160732269287, 'distance': 7.982583522796631, 'cosine_with_motion': -0.6148617942807654, 'motion_component': -3.20352882053065}, {'ion': 1341, 'force': [1.5748634338378906, 5.740958213806152, -3.378621816635132], 'magnitude': 6.844989776611328, 'distance': 6.964383125305176, 'cosine_with_motion': 0.3455697276985564, 'motion_component': 2.365421161972364}, {'ion': 1359, 'force': [1.0105098485946655, 0.24263377487659454, -3.6123909950256348], 'magnitude': 3.7589054107666016, 'distance': 9.398062705993652, 'cosine_with_motion': -0.5294201717457786, 'motion_component': -1.990040356360307}, {'ion': 1374, 'force': [0.22562316060066223, 0.10065484791994095, -1.4744327068328857], 'magnitude': 1.494987964630127, 'distance': 14.902193069458008, 'cosine_with_motion': -0.5618215292436758, 'motion_component': -0.8399164247898128}]}, 6570: {'frame': 6570, 'ionic_force': [12.369088254868984, 9.554802000522614, -1.3525469191372395], 'ionic_force_magnitude': 15.688147395227915, 'motion_vector': [0.08165740966796875, 0.8572654724121094, 0.46636962890625], 'cosine_ionic_motion': 0.5578220875076787, 'ionic_motion_component': 8.751195129134187, 'ionic_force_x': 12.369088254868984, 'ionic_force_y': 9.554802000522614, 'ionic_force_z': -1.3525469191372395, 'radial_force': 15.629734019679567, 'axial_force': -1.3525469191372395, 'contributions': [{'ion': 1327, 'force': [1.5750917196273804, 1.453436017036438, -0.059865642338991165], 'magnitude': 2.1440553665161133, 'distance': 12.443742752075195, 'cosine_with_motion': 0.6413605893494628, 'motion_component': 1.3751127123759574}, {'ion': 1330, 'force': [8.851373672485352, -0.5448993444442749, 0.612082302570343], 'magnitude': 8.889227867126465, 'distance': 6.1113481521606445, 'cosine_with_motion': 0.06215821404243742, 'motion_component': 0.5525385419218214}, {'ion': 1341, 'force': [-0.1118030920624733, 4.923777103424072, 3.27870774269104], 'magnitude': 5.9165873527526855, 'distance': 7.490889549255371, 'cosine_with_motion': 0.9908006826356204, 'motion_component': 5.862158742332892}, {'ion': 1359, 'force': [1.5930393934249878, 2.9040167331695557, -3.243910789489746], 'magnitude': 4.636167049407959, 'distance': 8.462321281433105, 'cosine_with_motion': 0.24375800960093685, 'motion_component': 1.130102852027684}, {'ion': 1374, 'force': [0.4613865613937378, 0.8184714913368225, -1.9395605325698853], 'magnitude': 2.155149221420288, 'distance': 12.411674499511719, 'cosine_with_motion': -0.07828591522281605, 'motion_component': -0.1687178298596086}]}, 6571: {'frame': 6571, 'ionic_force': [10.874882519245148, 11.021745204925537, -1.5739329904317856], 'ionic_force_magnitude': 15.563393017849684, 'motion_vector': [-0.7143974304199219, 2.6378211975097656, 0.46242523193359375], 'cosine_ionic_motion': 0.4770052911616335, 'ionic_motion_component': 7.423820817942322, 'ionic_force_x': 10.874882519245148, 'ionic_force_y': 11.021745204925537, 'ionic_force_z': -1.5739329904317856, 'radial_force': 15.483602202642729, 'axial_force': -1.5739329904317856, 'contributions': [{'ion': 1327, 'force': [0.9435466527938843, 1.3866626024246216, -0.0861724466085434], 'magnitude': 1.6794461011886597, 'distance': 14.060022354125977, 'cosine_with_motion': 0.6324180897014997, 'motion_component': 1.0621120842852612}, {'ion': 1330, 'force': [7.051734924316406, 1.6229393482208252, 0.9881018400192261], 'magnitude': 7.3032355308532715, 'distance': 6.742351531982422, 'cosine_with_motion': -0.014810253427721524, 'motion_component': -0.10816276256291779}, {'ion': 1341, 'force': [0.5937607288360596, 3.663236141204834, 2.101393938064575], 'magnitude': 4.264704704284668, 'distance': 8.82316780090332, 'cosine_with_motion': 0.8637998705639303, 'motion_component': 3.683851482704153}, {'ion': 1359, 'force': [1.727158784866333, 3.3323826789855957, -2.602457046508789], 'magnitude': 4.5673441886901855, 'distance': 8.525839805603027, 'cosine_with_motion': 0.501837686085301, 'motion_component': 2.29206552316883}, {'ion': 1374, 'force': [0.5586814284324646, 1.0165244340896606, -1.9747992753982544], 'magnitude': 2.290257453918457, 'distance': 12.040011405944824, 'cosine_with_motion': 0.21567643245512247, 'motion_component': 0.49395454936455074}]}, 6572: {'frame': 6572, 'ionic_force': [4.297864839434624, 8.788159370422363, -1.320813924074173], 'ionic_force_magnitude': 9.871572150372959, 'motion_vector': [0.8923988342285156, -0.882781982421875, -0.6154251098632812], 'cosine_ionic_motion': -0.2253358781914698, 'ionic_motion_component': -2.224419379634747, 'ionic_force_x': 4.297864839434624, 'ionic_force_y': 8.788159370422363, 'ionic_force_z': -1.320813924074173, 'radial_force': 9.782810807635544, 'axial_force': -1.320813924074173, 'contributions': [{'ion': 1330, 'force': [3.4389588832855225, 2.7700512409210205, 0.2946772277355194], 'magnitude': 4.425658702850342, 'distance': 8.661239624023438, 'cosine_with_motion': 0.07147438925554626, 'motion_component': 0.31632126731567206}, {'ion': 1341, 'force': [-0.10774736106395721, 2.0299341678619385, 1.3322513103485107], 'magnitude': 2.430459976196289, 'distance': 11.687585830688477, 'cosine_with_motion': -0.7969983098200872, 'motion_component': -1.9370725058540001}, {'ion': 1359, 'force': [0.6919946074485779, 2.870731830596924, -1.4831961393356323], 'magnitude': 3.304516315460205, 'distance': 10.02340030670166, 'cosine_with_motion': -0.21730627483870296, 'motion_component': -0.718092146719588}, {'ion': 1374, 'force': [0.2746587097644806, 1.1174421310424805, -1.4645463228225708], 'magnitude': 1.8625279664993286, 'distance': 13.351118087768555, 'cosine_with_motion': 0.061434877066536324, 'motion_component': 0.11442417383104164}]}, 6573: {'frame': 6573, 'ionic_force': [6.707516588270664, 9.176944971084595, -0.1950500402599573], 'ionic_force_magnitude': 11.368603357600545, 'motion_vector': [-0.3231239318847656, -0.48430633544921875, 0.06146240234375], 'cosine_ionic_motion': -0.995217753560235, 'ionic_motion_component': -11.31423589466856, 'ionic_force_x': 6.707516588270664, 'ionic_force_y': 9.176944971084595, 'ionic_force_z': -0.1950500402599573, 'radial_force': 11.366930007008971, 'axial_force': -0.1950500402599573, 'contributions': [{'ion': 1327, 'force': [0.9881269335746765, 1.1771571636199951, 0.006705602630972862], 'magnitude': 1.5369250774383545, 'distance': 14.697473526000977, 'cosine_with_motion': -0.9880008358344904, 'motion_component': -1.5184832920336617}, {'ion': 1330, 'force': [4.258534908294678, 1.36393404006958, 1.1857856512069702], 'magnitude': 4.62617826461792, 'distance': 8.471452713012695, 'cosine_with_motion': -0.7250604061209903, 'motion_component': -3.354258527189531}, {'ion': 1341, 'force': [-0.05445399135351181, 2.8371944427490234, 1.6453436613082886], 'magnitude': 3.28021240234375, 'distance': 10.060464859008789, 'cosine_with_motion': -0.6537031557818106, 'motion_component': -2.144285189327313}, {'ion': 1359, 'force': [1.1280900239944458, 2.8237078189849854, -1.7318087816238403], 'magnitude': 3.499296188354492, 'distance': 9.740442276000977, 'cosine_with_motion': -0.8974276319060125, 'motion_component': -3.14036519314781}, {'ion': 1374, 'force': [0.387218713760376, 0.9749515056610107, -1.3010761737823486], 'magnitude': 1.6713072061538696, 'distance': 14.094215393066406, 'cosine_with_motion': -0.6921791265166704, 'motion_component': -1.1568440041993604}]}, 6574: {'frame': 6574, 'ionic_force': [9.922765612602234, 10.655503034591675, -1.8789064027369022], 'ionic_force_magnitude': 14.680984694259426, 'motion_vector': [0.2715606689453125, -0.07678985595703125, -0.05289459228515625], 'cosine_ionic_motion': 0.4687223494525201, 'ionic_motion_component': 6.881305638169765, 'ionic_force_x': 9.922765612602234, 'ionic_force_y': 10.655503034591675, 'ionic_force_z': -1.8789064027369022, 'radial_force': 14.560254885228959, 'axial_force': -1.8789064027369022, 'contributions': [{'ion': 1327, 'force': [0.8655595183372498, 1.3287378549575806, -0.03194442763924599], 'magnitude': 1.5861141681671143, 'distance': 14.467777252197266, 'cosine_with_motion': 0.295794977559575, 'motion_component': 0.4691645916303158}, {'ion': 1330, 'force': [6.645339488983154, 1.9468575716018677, 1.6377795934677124], 'magnitude': 7.115694999694824, 'distance': 6.830624103546143, 'cosine_with_motion': 0.7677054146793523, 'motion_component': 5.462757472369846}, {'ion': 1341, 'force': [0.7769212126731873, 3.7414112091064453, 0.19452917575836182], 'magnitude': 3.826173782348633, 'distance': 9.315082550048828, 'cosine_with_motion': -0.07883855880427347, 'motion_component': -0.3016500287318795}, {'ion': 1359, 'force': [1.2521162033081055, 2.632829427719116, -2.2195000648498535], 'magnitude': 3.664118766784668, 'distance': 9.518845558166504, 'cosine_with_motion': 0.24262122220108004, 'motion_component': 0.8889929729182668}, {'ion': 1374, 'force': [0.3828291893005371, 1.005666971206665, -1.459770679473877], 'magnitude': 1.8135199546813965, 'distance': 13.530313491821289, 'cosine_with_motion': 0.19963431493602773, 'motion_component': 0.3620408168458269}]}, 6575: {'frame': 6575, 'ionic_force': [6.102406769990921, 8.403478920459747, -1.6997588761150837], 'ionic_force_magnitude': 10.52364036776126, 'motion_vector': [-0.7413291931152344, 0.8488311767578125, 0.4405517578125], 'cosine_ionic_motion': 0.14609900437198084, 'ionic_motion_component': 1.5374933800987063, 'ionic_force_x': 6.102406769990921, 'ionic_force_y': 8.403478920459747, 'ionic_force_z': -1.6997588761150837, 'radial_force': 10.385462259959464, 'axial_force': -1.6997588761150837, 'contributions': [{'ion': 1330, 'force': [3.698859691619873, 1.877339243888855, -0.03207122161984444], 'magnitude': 4.148131370544434, 'distance': 8.94628620147705, 'cosine_with_motion': -0.2316347697950632, 'motion_component': -0.96085146489291}, {'ion': 1341, 'force': [0.6937668323516846, 2.8005433082580566, 1.644039273262024], 'magnitude': 3.320725917816162, 'distance': 9.998907089233398, 'cosine_with_motion': 0.6438655630588777, 'motion_component': 2.1381010385898946}, {'ion': 1359, 'force': [1.2716120481491089, 2.7411482334136963, -1.8873075246810913], 'magnitude': 3.5626986026763916, 'distance': 9.653382301330566, 'cosine_with_motion': 0.12819220190672265, 'motion_component': 0.45671016417391286}, {'ion': 1374, 'force': [0.4381681978702545, 0.9844481348991394, -1.4244194030761719], 'magnitude': 1.7860851287841797, 'distance': 13.633832931518555, 'cosine_with_motion': -0.05400995022278874, 'motion_component': -0.09646636963300992}]}, 6576: {'frame': 6576, 'ionic_force': [5.697530130855739, 9.966541528701782, -1.1423418633639812], 'ionic_force_magnitude': 11.536842920320106, 'motion_vector': [0.1239013671875, -0.14241409301757812, -0.3520050048828125], 'cosine_ionic_motion': -0.06756220567549721, 'ionic_motion_component': -0.7794545542285709, 'ionic_force_x': 5.697530130855739, 'ionic_force_y': 9.966541528701782, 'ionic_force_z': -1.1423418633639812, 'radial_force': 11.480148066786693, 'axial_force': -1.1423418633639812, 'contributions': [{'ion': 1327, 'force': [0.8476411700248718, 1.4078731536865234, 0.05625929310917854], 'magnitude': 1.6443136930465698, 'distance': 14.209431648254395, 'cosine_with_motion': -0.17552367847627473, 'motion_component': -0.28861598567276614}, {'ion': 1330, 'force': [3.670255661010742, 1.709186315536499, 0.31133517622947693], 'magnitude': 4.060667991638184, 'distance': 9.042120933532715, 'cosine_with_motion': 0.06273120196461206, 'motion_component': 0.25473058028006434}, {'ion': 1341, 'force': [0.002328316681087017, 2.6095755100250244, 1.5804171562194824], 'magnitude': 3.050837278366089, 'distance': 10.431806564331055, 'cosine_with_motion': -0.7612668469814414, 'motion_component': -2.322501282066058}, {'ion': 1359, 'force': [0.9095866680145264, 3.105701446533203, -1.6332862377166748], 'magnitude': 3.624962568283081, 'distance': 9.570117950439453, 'cosine_with_motion': 0.16943698437349575, 'motion_component': 0.6142027188966424}, {'ion': 1374, 'force': [0.2677183151245117, 1.1342051029205322, -1.4570672512054443], 'magnitude': 1.8657810688018799, 'distance': 13.339473724365234, 'cosine_with_motion': 0.5159927105714089, 'motion_component': 0.9627294710664245}]}, 6577: {'frame': 6577, 'ionic_force': [10.770041853189468, 11.033284544944763, -1.4359604306519032], 'ionic_force_magnitude': 15.48512679081343, 'motion_vector': [2.2769126892089844, -2.477092742919922, -0.91888427734375], 'cosine_ionic_motion': -0.027561089715659084, 'ionic_motion_component': -0.42678696873996497, 'ionic_force_x': 10.770041853189468, 'ionic_force_y': 11.033284544944763, 'ionic_force_z': -1.4359604306519032, 'radial_force': 15.41840359340648, 'axial_force': -1.4359604306519032, 'contributions': [{'ion': 1327, 'force': [1.0223180055618286, 1.2306550741195679, 0.052624136209487915], 'magnitude': 1.6007546186447144, 'distance': 14.401464462280273, 'cosine_with_motion': -0.13775037653817027, 'motion_component': -0.22050455002434874}, {'ion': 1330, 'force': [7.852027416229248, 3.727412223815918, 1.5429376363754272], 'magnitude': 8.827717781066895, 'distance': 6.132602691650391, 'cosine_with_motion': 0.23473986102912722, 'motion_component': 2.0722171355634664}, {'ion': 1341, 'force': [0.4523809254169464, 1.9864200353622437, 0.05863363668322563], 'magnitude': 2.0381243228912354, 'distance': 12.76302719116211, 'cosine_with_motion': -0.5548802485993717, 'motion_component': -1.1309149590530434}, {'ion': 1359, 'force': [1.0853403806686401, 2.987722158432007, -1.669343113899231], 'magnitude': 3.5904252529144287, 'distance': 9.616036415100098, 'cosine_with_motion': -0.27116527483362757, 'motion_component': -0.9735986645634576}, {'ion': 1374, 'force': [0.3579751253128052, 1.1010750532150269, -1.420812726020813], 'magnitude': 1.832817792892456, 'distance': 13.458894729614258, 'cosine_with_motion': -0.09492783318420045, 'motion_component': -0.17398542697419472}]}, 6578: {'frame': 6578, 'ionic_force': [11.297083020210266, 8.097006931900978, -3.776877298951149], 'ionic_force_magnitude': 14.403138829856085, 'motion_vector': [-1.2792587280273438, 0.96728515625, 1.4186248779296875], 'cosine_ionic_motion': -0.38838770659146066, 'ionic_motion_component': -5.594002057846219, 'ionic_force_x': 11.297083020210266, 'ionic_force_y': 8.097006931900978, 'ionic_force_z': -3.776877298951149, 'radial_force': 13.899122491034303, 'axial_force': -3.776877298951149, 'contributions': [{'ion': 1327, 'force': [1.3949049711227417, 1.2103792428970337, -0.1234259232878685], 'magnitude': 1.8509489297866821, 'distance': 13.392813682556152, 'cosine_with_motion': -0.19901989675176637, 'motion_component': -0.36837565457455934}, {'ion': 1330, 'force': [4.5826263427734375, 0.2037651091814041, 0.11392490565776825], 'magnitude': 4.588568687438965, 'distance': 8.506098747253418, 'cosine_with_motion': -0.5601713361052677, 'motion_component': -2.57038469530253}, {'ion': 1341, 'force': [2.695676326751709, 3.7334976196289062, 0.10549106448888779], 'magnitude': 4.606170177459717, 'distance': 8.48983097076416, 'cosine_with_motion': 0.031689497765525536, 'motion_component': 0.1459672195302515}, {'ion': 1359, 'force': [2.0399694442749023, 2.267669677734375, -2.4146974086761475], 'magnitude': 3.8903167247772217, 'distance': 9.237970352172852, 'cosine_with_motion': -0.46119819915256116, 'motion_component': -1.7942070947055129}, {'ion': 1374, 'force': [0.5839059352874756, 0.681695282459259, -1.458169937133789], 'magnitude': 1.7122832536697388, 'distance': 13.924551963806152, 'cosine_with_motion': -0.5881046354072257, 'motion_component': -1.0070017571075702}]}, 6579: {'frame': 6579, 'ionic_force': [9.608516097068787, 8.373697221279144, -1.9300379157066345], 'ionic_force_magnitude': 12.89059475343761, 'motion_vector': [2.924358367919922, -6.608238220214844, -2.4186172485351562], 'cosine_ionic_motion': -0.22974953235812362, 'ionic_motion_component': -2.9616081164203725, 'ionic_force_x': 9.608516097068787, 'ionic_force_y': 8.373697221279144, 'ionic_force_z': -1.9300379157066345, 'radial_force': 12.745288805723, 'axial_force': -1.9300379157066345, 'contributions': [{'ion': 1327, 'force': [1.3253157138824463, 1.562822699546814, 0.09811156988143921], 'magnitude': 2.0514633655548096, 'distance': 12.721465110778809, 'cosine_with_motion': -0.4278845029472088, 'motion_component': -0.8777894316682975}, {'ion': 1330, 'force': [5.451991558074951, 0.6885251402854919, 1.5081236362457275], 'magnitude': 5.698483943939209, 'distance': 7.632896900177002, 'cosine_with_motion': 0.17837929729573904, 'motion_component': 1.0164915061803086}, {'ion': 1341, 'force': [0.3505029082298279, 1.43211030960083, 0.5435124635696411], 'magnitude': 1.5713682174682617, 'distance': 14.535503387451172, 'cosine_with_motion': -0.8145078473890567, 'motion_component': -1.2798917314959368}, {'ion': 1359, 'force': [1.873288631439209, 3.515359878540039, -2.291175127029419], 'magnitude': 4.595263957977295, 'distance': 8.499899864196777, 'cosine_with_motion': -0.3487003992758554, 'motion_component': -1.6023703007219012}, {'ion': 1374, 'force': [0.6074172854423523, 1.1748791933059692, -1.7886104583740234], 'magnitude': 2.2245054244995117, 'distance': 12.216654777526855, 'cosine_with_motion': -0.09802088427497478, 'motion_component': -0.21804798582489582}]}, 6580: {'frame': 6580, 'ionic_force': [9.401102185249329, 2.19012341927737, -3.330233727581799], 'ionic_force_magnitude': 10.211161519116729, 'motion_vector': [0.0558624267578125, 1.9655532836914062, -0.0980682373046875], 'cosine_ionic_motion': 0.2564989404926745, 'ionic_motion_component': 2.6191521108530096, 'ionic_force_x': 9.401102185249329, 'ionic_force_y': 2.19012341927737, 'ionic_force_z': -3.330233727581799, 'radial_force': 9.652842218184595, 'axial_force': -3.330233727581799, 'contributions': [{'ion': 1327, 'force': [1.994491696357727, 0.5432167649269104, -0.318158358335495], 'magnitude': 2.091484308242798, 'distance': 12.599164009094238, 'cosine_with_motion': 0.2939362459607358, 'motion_component': 0.6147630256647435}, {'ion': 1330, 'force': [1.841148018836975, -1.1111570596694946, 0.003038342110812664], 'magnitude': 2.1504664421081543, 'distance': 12.425180435180664, 'cosine_with_motion': -0.491633106325562, 'motion_component': -1.0572404228431884}, {'ion': 1341, 'force': [3.1475207805633545, 2.842928171157837, 0.6421310901641846], 'magnitude': 4.289692401885986, 'distance': 8.797432899475098, 'cosine_with_motion': 0.6750076766192781, 'motion_component': 2.89557522958656}, {'ion': 1359, 'force': [1.743165135383606, -0.0841091051697731, -2.3038322925567627], 'magnitude': 2.8902149200439453, 'distance': 10.717759132385254, 'cosine_with_motion': 0.0277650151279751, 'motion_component': 0.08024686087711674}, {'ion': 1374, 'force': [0.674776554107666, -0.0007553519681096077, -1.3534125089645386], 'magnitude': 1.5122994184494019, 'distance': 14.816655158996582, 'cosine_with_motion': 0.05673966670334128, 'motion_component': 0.08580736227417984}]}, 6581: {'frame': 6581, 'ionic_force': [8.237632095813751, 2.8010704964399338, -3.125244453549385], 'ionic_force_magnitude': 9.245092285447901, 'motion_vector': [-1.0904083251953125, 0.6786651611328125, -0.0248260498046875], 'cosine_ionic_motion': -0.5897330513000432, 'ionic_motion_component': -5.45213648304768, 'ionic_force_x': 8.237632095813751, 'ionic_force_y': 2.8010704964399338, 'ionic_force_z': -3.125244453549385, 'radial_force': 8.700837802878933, 'axial_force': -3.125244453549385, 'contributions': [{'ion': 1327, 'force': [1.5015419721603394, 0.9385555386543274, -0.21082422137260437], 'magnitude': 1.7832446098327637, 'distance': 13.644686698913574, 'cosine_with_motion': -0.434396371589925, 'motion_component': -0.7746350255753975}, {'ion': 1330, 'force': [2.607945680618286, -0.777786374092102, -0.1844618171453476], 'magnitude': 2.7277021408081055, 'distance': 11.032414436340332, 'cosine_with_motion': -0.9609020723946794, 'motion_component': -2.621054553634242}, {'ion': 1341, 'force': [1.963555932044983, 2.088361978530884, 0.7296456098556519], 'magnitude': 2.9579031467437744, 'distance': 10.594417572021484, 'cosine_with_motion': -0.1952496148674068, 'motion_component': -0.5775294285032408}, {'ion': 1359, 'force': [1.4981328248977661, 0.38405388593673706, -2.148705005645752], 'magnitude': 2.6474199295043945, 'distance': 11.198442459106445, 'cosine_with_motion': -0.38801482743793303, 'motion_component': -1.0272382066311811}, {'ion': 1374, 'force': [0.6664556860923767, 0.16788546741008759, -1.310899019241333], 'magnitude': 1.480136752128601, 'distance': 14.976768493652344, 'cosine_with_motion': -0.3051604131494634, 'motion_component': -0.45167915777951295}]}, 6582: {'frame': 6582, 'ionic_force': [13.439601302146912, 8.873756095767021, -5.538107238709927], 'ionic_force_magnitude': 17.030474514683455, 'motion_vector': [-3.5965843200683594, -4.00225830078125, 1.7977447509765625], 'cosine_ionic_motion': -0.9709190363327294, 'ionic_motion_component': -16.535211904085568, 'ionic_force_x': 13.439601302146912, 'ionic_force_y': 8.873756095767021, 'ionic_force_z': -5.538107238709927, 'radial_force': 16.104857354470152, 'axial_force': -5.538107238709927, 'contributions': [{'ion': 1327, 'force': [1.7381343841552734, 1.2546632289886475, -0.4241744577884674], 'magnitude': 2.1852266788482666, 'distance': 12.32596206665039, 'cosine_with_motion': -0.9708103909504258, 'motion_component': -2.1214406083064645}, {'ion': 1330, 'force': [7.226673126220703, 3.71441388130188, -0.0353500172495842], 'magnitude': 8.125449180603027, 'distance': 6.392126560211182, 'cosine_with_motion': -0.8877053495316299, 'motion_component': -7.21300471545702}, {'ion': 1341, 'force': [2.3823862075805664, 2.991396427154541, -1.2005852460861206], 'magnitude': 4.008194446563721, 'distance': 9.101116180419922, 'cosine_with_motion': -0.9982316294542771, 'motion_component': -4.0011063288809225}, {'ion': 1359, 'force': [1.5048085451126099, 0.7228309512138367, -2.4776906967163086], 'magnitude': 2.987621784210205, 'distance': 10.541592597961426, 'cosine_with_motion': -0.7527915131617094, 'motion_component': -2.249056399859022}, {'ion': 1374, 'force': [0.5875990390777588, 0.19045160710811615, -1.4003068208694458], 'magnitude': 1.5304913520812988, 'distance': 14.728333473205566, 'cosine_with_motion': -0.621110192406535, 'motion_component': -0.9506037495882076}]}, 6583: {'frame': 6583, 'ionic_force': [16.05817210674286, 6.1076273918151855, 3.6224589943885803], 'ionic_force_magnitude': 17.558195036308607, 'motion_vector': [-2.217937469482422, 1.4410781860351562, 1.8284072875976562], 'cosine_ionic_motion': -0.35763561505257213, 'ionic_motion_component': -6.279435881023248, 'ionic_force_x': 16.05817210674286, 'ionic_force_y': 6.1076273918151855, 'ionic_force_z': 3.6224589943885803, 'radial_force': 17.180454119930168, 'axial_force': 3.6224589943885803, 'contributions': [{'ion': 1327, 'force': [4.602260112762451, 2.496872901916504, -0.22734969854354858], 'magnitude': 5.2408833503723145, 'distance': 7.959151744842529, 'cosine_with_motion': -0.41687272413751025, 'motion_component': -2.1847813997755807}, {'ion': 1330, 'force': [9.457734107971191, -11.10282039642334, 7.554731369018555], 'magnitude': 16.425447463989258, 'distance': 4.495835781097412, 'cosine_with_motion': -0.43857960139192076, 'motion_component': -7.203866159760764}, {'ion': 1341, 'force': [-2.9511709213256836, 18.338525772094727, 8.4227876663208], 'magnitude': 20.394956588745117, 'distance': 4.034666538238525, 'cosine_with_motion': 0.7376338138105843, 'motion_component': 15.044010246081827}, {'ion': 1359, 'force': [4.432460308074951, -3.265843629837036, -9.403403282165527], 'magnitude': 10.896624565124512, 'distance': 5.519796371459961, 'cosine_with_motion': -0.9056182905666778, 'motion_component': -9.868182734805686}, {'ion': 1374, 'force': [0.5168884992599487, -0.35910725593566895, -2.724307060241699], 'magnitude': 2.796065092086792, 'distance': 10.896710395812988, 'cosine_with_motion': -0.7391158176049683, 'motion_component': -2.066616029296412}]}, 6584: {'frame': 6584, 'ionic_force': [-2.7984437588602304, -2.5238340757787228, -6.624991416931152], 'ionic_force_magnitude': 7.621780447374292, 'motion_vector': [0.10931777954101562, -0.3145332336425781, 0.6563186645507812], 'cosine_ionic_motion': -0.688175507913837, 'ionic_motion_component': -5.245122630579555, 'ionic_force_x': -2.7984437588602304, 'ionic_force_y': -2.5238340757787228, 'ionic_force_z': -6.624991416931152, 'radial_force': 3.7684248584210374, 'axial_force': -6.624991416931152, 'contributions': [{'ion': 1327, 'force': [3.3435709476470947, 4.247110366821289, 1.7031737565994263], 'magnitude': 5.667293548583984, 'distance': 7.653872013092041, 'cosine_with_motion': 0.03535910212294005, 'motion_component': 0.20039040457326607}, {'ion': 1330, 'force': [-2.1344544887542725, -9.71019172668457, 4.399707794189453], 'magnitude': 10.872035026550293, 'distance': 5.526034832000732, 'cosine_with_motion': 0.7134344007713144, 'motion_component': 7.7564838727242575}, {'ion': 1341, 'force': [-3.1538000106811523, 3.324544906616211, 1.762978434562683], 'magnitude': 4.909902572631836, 'distance': 8.223043441772461, 'cosine_with_motion': -0.06458321194415423, 'motion_component': -0.31709729841094264}, {'ion': 1359, 'force': [-0.8428261280059814, -0.053758349269628525, -11.009814262390137], 'magnitude': 11.042158126831055, 'distance': 5.483300685882568, 'cosine_with_motion': -0.8984317015483194, 'motion_component': -9.920624908005133}, {'ion': 1374, 'force': [-0.010934079065918922, -0.3315392732620239, -3.481037139892578], 'magnitude': 3.4968066215515137, 'distance': 9.743908882141113, 'cosine_with_motion': -0.8477090519700824, 'motion_component': -2.9642747308761317}]}, 6585: {'frame': 6585, 'ionic_force': [0.19422585517168045, 0.5162233263254166, -7.085144519805908], 'ionic_force_magnitude': 7.1065802656408055, 'motion_vector': [-1.3601837158203125, -0.6397171020507812, -1.1410140991210938], 'cosine_ionic_motion': 0.558483083688465, 'ionic_motion_component': 3.968904861234668, 'ionic_force_x': 0.19422585517168045, 'ionic_force_y': 0.5162233263254166, 'ionic_force_z': -7.085144519805908, 'radial_force': 0.5515525409783261, 'axial_force': -7.085144519805908, 'contributions': [{'ion': 1327, 'force': [5.026834011077881, 4.280613899230957, 2.439513683319092], 'magnitude': 7.038745880126953, 'distance': 6.867859363555908, 'cosine_with_motion': -0.9304606258766676, 'motion_component': -6.549275829282578}, {'ion': 1330, 'force': [-0.1826930046081543, -6.5750732421875, 4.005751609802246], 'magnitude': 7.701364040374756, 'distance': 6.565762996673584, 'cosine_with_motion': -0.007977180623971132, 'motion_component': -0.06143517342584914}, {'ion': 1341, 'force': [-4.096582412719727, 4.5770263671875, 3.0861237049102783], 'magnitude': 6.874250411987305, 'distance': 6.949544906616211, 'cosine_with_motion': -0.06762011741679047, 'motion_component': -0.4648376132503955}, {'ion': 1359, 'force': [-0.4727668762207031, -1.7130180597305298, -13.051497459411621], 'magnitude': 13.171921730041504, 'distance': 5.020471096038818, 'cosine_with_motion': 0.6690579638055455, 'motion_component': 8.812779214975947}, {'ion': 1374, 'force': [-0.08056586235761642, -0.05332563817501068, -3.5650360584259033], 'magnitude': 3.566344976425171, 'distance': 9.648446083068848, 'cosine_with_motion': 0.6257594826796723, 'motion_component': 2.2316741953015637}]}, 6586: {'frame': 6586, 'ionic_force': [-4.087879508733749, 1.6345014572143555, -16.545942544937134], 'ionic_force_magnitude': 17.121640359262365, 'motion_vector': [1.223419189453125, 0.5366973876953125, 1.0523300170898438], 'cosine_ionic_motion': -0.7396064486371673, 'ionic_motion_component': -12.663275620956831, 'ionic_force_x': -4.087879508733749, 'ionic_force_y': 1.6345014572143555, 'ionic_force_z': -16.545942544937134, 'radial_force': 4.402539482112696, 'axial_force': -16.545942544937134, 'contributions': [{'ion': 1327, 'force': [6.040377140045166, 7.853013038635254, 1.4087369441986084], 'magnitude': 10.007022857666016, 'distance': 5.759922027587891, 'cosine_with_motion': 0.7689946229958126, 'motion_component': 7.695346888200817}, {'ion': 1330, 'force': [-0.9158151745796204, -3.5589420795440674, 1.8877583742141724], 'magnitude': 4.131394386291504, 'distance': 8.96438980102539, 'cosine_with_motion': -0.14858385226471604, 'motion_component': -0.6138584619205041}, {'ion': 1341, 'force': [-4.4826340675354, 2.6424269676208496, 1.3166965246200562], 'magnitude': 5.3675055503845215, 'distance': 7.864711284637451, 'cosine_with_motion': -0.29363396235906114, 'motion_component': -1.5760819874928698}, {'ion': 1359, 'force': [-4.346304893493652, -4.65595006942749, -17.659698486328125], 'magnitude': 18.773204803466797, 'distance': 4.20532751083374, 'cosine_with_motion': -0.8268979799097133, 'motion_component': -15.523524452550248}, {'ion': 1374, 'force': [-0.3835025131702423, -0.6460464000701904, -3.4994359016418457], 'magnitude': 3.579176187515259, 'distance': 9.631135940551758, 'cosine_with_motion': -0.7390409955776951, 'motion_component': -2.645157889305745}]}, 6587: {'frame': 6587, 'ionic_force': [-1.3948394022881985, 2.136453092098236, -10.57060980796814], 'ionic_force_magnitude': 10.874180451198336, 'motion_vector': [0.24559402465820312, 0.056308746337890625, 0.05919647216796875], 'cosine_ionic_motion': -0.30129583505560287, 'ionic_motion_component': -3.276345279589115, 'ionic_force_x': -1.3948394022881985, 'ionic_force_y': 2.136453092098236, 'ionic_force_z': -10.57060980796814, 'radial_force': 2.5514718836216503, 'axial_force': -10.57060980796814, 'contributions': [{'ion': 1327, 'force': [3.978027582168579, 4.168118000030518, 1.4422818422317505], 'magnitude': 5.939536094665527, 'distance': 7.476404190063477, 'cosine_with_motion': 0.8437193936061972, 'motion_component': 5.011301721015714}, {'ion': 1330, 'force': [-1.348442554473877, -4.446995735168457, 2.636247396469116], 'magnitude': 5.34264612197876, 'distance': 7.8829874992370605, 'cosine_with_motion': -0.3077172746473687, 'motion_component': -1.6440245369487094}, {'ion': 1341, 'force': [-2.968979835510254, 3.28828763961792, 1.8167105913162231], 'magnitude': 4.788331031799316, 'distance': 8.326777458190918, 'cosine_with_motion': -0.35217011194823233, 'motion_component': -1.6863070816566061}, {'ion': 1359, 'force': [-1.085584044456482, -0.44185957312583923, -12.848565101623535], 'magnitude': 12.9019136428833, 'distance': 5.072732925415039, 'cosine_with_motion': -0.3150552387280355, 'motion_component': -4.064815264525501}, {'ion': 1374, 'force': [0.03013944998383522, -0.43109723925590515, -3.6172845363616943], 'magnitude': 3.6430070400238037, 'distance': 9.54638671875, 'cosine_with_motion': -0.24498993090008137, 'motion_component': -0.8925000544187769}]}, 6588: {'frame': 6588, 'ionic_force': [2.170046664774418, 2.544392377138138, -12.059692144393921], 'ionic_force_magnitude': 12.514759674627943, 'motion_vector': [0.011474609375, 0.145538330078125, 0.04688262939453125], 'cosine_ionic_motion': -0.08868653371753571, 'ionic_motion_component': -1.1098906558507473, 'ionic_force_x': 2.170046664774418, 'ionic_force_y': 2.544392377138138, 'ionic_force_z': -12.059692144393921, 'radial_force': 3.3441045282911297, 'axial_force': -12.059692144393921, 'contributions': [{'ion': 1327, 'force': [5.032597064971924, 4.4192280769348145, 2.0241124629974365], 'magnitude': 6.996687889099121, 'distance': 6.88847017288208, 'cosine_with_motion': 0.7417896850568094, 'motion_component': 5.190070898259815}, {'ion': 1330, 'force': [-0.6638263463973999, -3.996150016784668, 3.0800297260284424], 'magnitude': 5.0888566970825195, 'distance': 8.077164649963379, 'cosine_with_motion': -0.5700573263212879, 'motion_component': -2.9009400990388547}, {'ion': 1341, 'force': [-1.5257741212844849, 3.4375202655792236, 1.539534568786621], 'magnitude': 4.063827991485596, 'distance': 9.038604736328125, 'cosine_with_motion': 0.8906168049196592, 'motion_component': 3.619313609954143}, {'ion': 1359, 'force': [-0.7339341640472412, -0.867084801197052, -14.881825447</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>{6716: {'frame': 6716, 'ionic_force': [3.5372003354132175, 2.635218560695648, -13.300951480865479], 'ionic_force_magnitude': 14.013260625986366, 'motion_vector': [2.1366920471191406, 6.534908294677734, 0.9935302734375], 'cosine_ionic_motion': 0.1187908944309096, 'ionic_motion_component': 1.6646477636543684, 'ionic_force_x': 3.5372003354132175, 'ionic_force_y': 2.635218560695648, 'ionic_force_z': -13.300951480865479, 'radial_force': 4.4109140861597185, 'axial_force': -13.300951480865479, 'contributions': [{'ion': 1327, 'force': [1.9013433456420898, -1.8896634578704834, -1.5707390308380127], 'magnitude': 3.106952667236328, 'distance': 10.33717155456543, 'directional_contribution': -1.4174605754747915}, {'ion': 1330, 'force': [1.3640469312667847, -2.8642194271087646, -0.5391140580177307], 'magnitude': 3.217921733856201, 'distance': 10.157370567321777, 'directional_contribution': -2.3519556602151077}, {'ion': 1341, 'force': [3.074054718017578, 10.045456886291504, -7.949360370635986], 'magnitude': 13.173964500427246, 'distance': 5.020081996917725, 'directional_contribution': 9.258481228729863}, {'ion': 1359, 'force': [-2.778268337249756, -2.3256843090057373, -0.9613978266716003], 'magnitude': 3.748582124710083, 'distance': 9.410994529724121, 'directional_contribution': -3.179840794185729}, {'ion': 1400, 'force': [-0.023976322263479233, -0.33067113161087036, -2.2803401947021484], 'magnitude': 2.3043153285980225, 'distance': 12.003229141235352, 'directional_contribution': -0.6445764068267018}]}, 6717: {'frame': 6717, 'ionic_force': [0.5450510084629059, 4.748510509729385, -11.099060416221619], 'ionic_force_magnitude': 12.084476603716624, 'motion_vector': [-2.882415771484375, -8.947956085205078, 1.36480712890625], 'cosine_ionic_motion': -0.5157803651546883, 'ionic_motion_component': -6.232935755368247, 'ionic_force_x': 0.5450510084629059, 'ionic_force_y': 4.748510509729385, 'ionic_force_z': -11.099060416221619, 'radial_force': 4.779689599005029, 'axial_force': -11.099060416221619, 'contributions': [{'ion': 1327, 'force': [3.7785017490386963, 0.381460577249527, -2.1780126094818115], 'magnitude': 4.377936363220215, 'distance': 8.708318710327148, 'directional_contribution': -1.8187709444652604}, {'ion': 1330, 'force': [8.046460151672363, -2.481989860534668, -1.290306568145752], 'magnitude': 8.518842697143555, 'distance': 6.242790222167969, 'directional_contribution': -0.28902384491516386}, {'ion': 1341, 'force': [0.29557427763938904, 3.0619518756866455, -0.5244418382644653], 'magnitude': 3.1205694675445557, 'distance': 10.314593315124512, 'directional_contribution': -3.049267163667653}, {'ion': 1359, 'force': [-12.195097923278809, 2.7431704998016357, -4.48800802230835], 'magnitude': 13.281100273132324, 'distance': 4.99979305267334, 'directional_contribution': 0.47164561801915283}, {'ion': 1400, 'force': [0.6196127533912659, 1.0439174175262451, -2.6182913780212402], 'magnitude': 2.886023759841919, 'distance': 10.72553825378418, 'directional_contribution': -1.5475195795965124}]}, 6718: {'frame': 6718, 'ionic_force': [-15.74527932703495, -6.038105010986328, -8.724657155573368], 'ionic_force_magnitude': 18.986631499356328, 'motion_vector': [-0.8591651916503906, -0.15292739868164062, -0.16278839111328125], 'cosine_ionic_motion': 0.9416545980486678, 'ionic_motion_component': 17.878848852824557, 'ionic_force_x': -15.74527932703495, 'ionic_force_y': -6.038105010986328, 'ionic_force_z': -8.724657155573368, 'radial_force': 16.863348813626917, 'axial_force': -8.724657155573368, 'contributions': [{'ion': 1327, 'force': [1.6139215230941772, -3.2655608654022217, -0.8199719190597534], 'magnitude': 3.733762741088867, 'distance': 9.429652214050293, 'directional_contribution': -0.8490821403328379}, {'ion': 1330, 'force': [0.40082046389579773, -2.4494481086730957, 0.07108324021100998], 'magnitude': 2.483043670654297, 'distance': 11.5631685256958, 'directional_contribution': 0.021003429387131622}, {'ion': 1340, 'force': [-0.1447393149137497, -0.5571725368499756, -1.720524549484253], 'magnitude': 1.8142755031585693, 'distance': 13.527496337890625, 'directional_contribution': 0.5515723921234557}, {'ion': 1341, 'force': [-15.274748802185059, 4.401199817657471, -2.545541286468506], 'magnitude': 16.098703384399414, 'distance': 4.54123067855835, 'directional_contribution': 14.491971667476406}, {'ion': 1359, 'force': [-1.6921180486679077, -1.7458655834197998, -0.0793391764163971], 'magnitude': 2.432612895965576, 'distance': 11.682413101196289, 'directional_contribution': 1.9529916373492413}, {'ion': 1400, 'force': [-0.6484151482582092, -2.421257734298706, -3.6303634643554688], 'magnitude': 4.4116291999816895, 'distance': 8.67500114440918, 'directional_contribution': 1.7103914746028686}]}, 6719: {'frame': 6719, 'ionic_force': [-13.247648186981678, -7.324256241321564, -7.235395602881908], 'ionic_force_magnitude': 16.777838403822457, 'motion_vector': [3.021942138671875, 1.1164970397949219, -1.1178054809570312], 'cosine_ionic_motion': -0.7013024980662967, 'ionic_motion_component': -11.766339984753339, 'ionic_force_x': -13.247648186981678, 'ionic_force_y': -7.324256241321564, 'ionic_force_z': -7.235395602881908, 'radial_force': 15.13753321960275, 'axial_force': -7.235395602881908, 'contributions': [{'ion': 1327, 'force': [1.420046091079712, -3.122454881668091, -0.8165378570556641], 'magnitude': 3.5260443687438965, 'distance': 9.7034273147583, 'directional_contribution': 0.5037564096968339}, {'ion': 1330, 'force': [0.10633199661970139, -2.712059497833252, -0.04335900396108627], 'magnitude': 2.714489459991455, 'distance': 11.059231758117676, 'directional_contribution': -0.7795308899562283}, {'ion': 1340, 'force': [-0.22071534395217896, -0.5099888443946838, -1.6464329957962036], 'magnitude': 1.737683892250061, 'distance': 13.822405815124512, 'directional_contribution': 0.1771259648225083}, {'ion': 1341, 'force': [-12.584758758544922, 2.7286531925201416, -1.619233250617981], 'magnitude': 12.978583335876465, 'distance': 5.057727336883545, 'directional_contribution': -9.728376991680793}, {'ion': 1359, 'force': [-1.4268096685409546, -1.9060715436935425, -0.11701104044914246], 'magnitude': 2.383817672729492, 'distance': 11.801372528076172, 'directional_contribution': -1.8501583614498278}, {'ion': 1400, 'force': [-0.5417425036430359, -1.8023346662521362, -2.992821455001831], 'magnitude': 3.535374879837036, 'distance': 9.690614700317383, 'directional_contribution': -0.0891561282175708}]}, 6720: {'frame': 6720, 'ionic_force': [-13.875824749469757, -1.1168307960033417, -19.71669438481331], 'ionic_force_magnitude': 24.135738251999413, 'motion_vector': [-2.0362319946289062, -3.377918243408203, 1.4120712280273438], 'cosine_ionic_motion': 0.04139525447767722, 'ionic_motion_component': 0.999105026948124, 'ionic_force_x': -13.875824749469757, 'ionic_force_y': -1.1168307960033417, 'ionic_force_z': -19.71669438481331, 'radial_force': 13.920697665882228, 'axial_force': -19.71669438481331, 'contributions': [{'ion': 1327, 'force': [1.9507142305374146, -2.5765552520751953, -0.8716263175010681], 'magnitude': 3.3471860885620117, 'distance': 9.959306716918945, 'directional_contribution': 0.8355714608759257}, {'ion': 1330, 'force': [0.7414261698722839, -2.502897262573242, -0.2262757122516632], 'magnitude': 2.620192527770996, 'distance': 11.256476402282715, 'directional_contribution': 1.5814803630516323}, {'ion': 1340, 'force': [0.15693143010139465, -0.3897511661052704, -1.5432026386260986], 'magnitude': 1.5993773937225342, 'distance': 14.40766429901123, 'directional_contribution': -0.2821721389973071}, {'ion': 1341, 'force': [-16.80057144165039, 8.428204536437988, -13.408795356750488], 'magnitude': 23.088733673095703, 'distance': 3.792005777359009, 'directional_contribution': -3.1494503699860275}, {'ion': 1359, 'force': [-0.39115285873413086, -2.5806212425231934, -0.5263550877571106], 'magnitude': 2.6626408100128174, 'distance': 11.166389465332031, 'directional_contribution': 2.0934962423746057}, {'ion': 1400, 'force': [0.46682772040367126, -1.4952104091644287, -3.14043927192688], 'magnitude': 3.5094075202941895, 'distance': 9.726400375366211, 'directional_contribution': -0.0798205677429511}]}, 6721: {'frame': 6721, 'ionic_force': [-14.872823670506477, -15.005800008773804, -8.68900191783905], 'ionic_force_magnitude': 22.84455454075444, 'motion_vector': [-1.2706642150878906, 0.12684249877929688, -0.00298309326171875], 'cosine_ionic_motion': 0.5834653141139671, 'ionic_motion_component': 13.329005190914943, 'ionic_force_x': -14.872823670506477, 'ionic_force_y': -15.005800008773804, 'ionic_force_z': -8.68900191783905, 'radial_force': 21.127586654355333, 'axial_force': -8.68900191783905, 'contributions': [{'ion': 1327, 'force': [0.9067454934120178, -1.875288724899292, -0.39515984058380127], 'magnitude': 2.120152473449707, 'distance': 12.513692855834961, 'directional_contribution': -1.0876078009618537}, {'ion': 1340, 'force': [-0.07977347075939178, -0.7151584625244141, -1.4344524145126343], 'magnitude': 1.604826807975769, 'distance': 14.38318157196045, 'directional_contribution': 0.011693116688635014}, {'ion': 1341, 'force': [-14.652536392211914, -8.457913398742676, -4.700499534606934], 'magnitude': 17.55926513671875, 'distance': 4.348263740539551, 'directional_contribution': 13.75089103791261}, {'ion': 1359, 'force': [-0.839736819267273, -1.8682215213775635, -0.06597363948822021], 'magnitude': 2.0493321418762207, 'distance': 12.728078842163086, 'directional_contribution': 0.6501656636034504}, {'ion': 1400, 'force': [-0.20752248167991638, -2.0892179012298584, -2.092916488647461], 'magnitude': 2.964489221572876, 'distance': 10.5826416015625, 'directional_contribution': 0.0038631116715133196}]}, 6722: {'frame': 6722, 'ionic_force': [-6.684693541377783, -13.338738977909088, -3.4362437948584557], 'ionic_force_magnitude': 15.310612550797314, 'motion_vector': [1.3387413024902344, 0.14303207397460938, 0.6805572509765625], 'cosine_ionic_motion': -0.5712972196657156, 'ionic_motion_component': -8.746910381649515, 'ionic_force_x': -6.684693541377783, 'ionic_force_y': -13.338738977909088, 'ionic_force_z': -3.4362437948584557, 'radial_force': 14.920022964557695, 'axial_force': -3.4362437948584557, 'contributions': [{'ion': 1327, 'force': [0.81926029920578, -2.1865475177764893, -0.4886828362941742], 'magnitude': 2.3855793476104736, 'distance': 11.797014236450195, 'directional_contribution': 0.2992558764165798}, {'ion': 1330, 'force': [0.03506458178162575, -1.515844464302063, 0.15978533029556274], 'magnitude': 1.5246459245681763, 'distance': 14.756539344787598, 'directional_contribution': -0.04052054803409777}, {'ion': 1340, 'force': [-0.26287201046943665, -0.7818873524665833, -1.5102778673171997], 'magnitude': 1.7208685874938965, 'distance': 13.889774322509766, 'directional_contribution': -0.9887265207963449}, {'ion': 1341, 'force': [-5.845895767211914, -5.08392858505249, 0.5223320126533508], 'magnitude': 7.764898777008057, 'distance': 6.538846492767334, 'directional_contribution': -5.434099831997331}, {'ion': 1359, 'force': [-0.7654677033424377, -1.5446780920028687, -0.07922738045454025], 'magnitude': 1.7257601022720337, 'distance': 13.870075225830078, 'directional_contribution': -0.8614801146791009}, {'ion': 1400, 'force': [-0.6647829413414001, -2.2258529663085938, -2.040173053741455], 'magnitude': 3.0917088985443115, 'distance': 10.362624168395996, 'directional_contribution': -1.7213390931081953}]}, 6723: {'frame': 6723, 'ionic_force': [-0.5762564726173878, -13.915500342845917, 1.1806349530816078], 'ionic_force_magnitude': 13.977378874682344, 'motion_vector': [-0.162322998046875, 2.1346893310546875, 1.369384765625], 'cosine_ionic_motion': -0.7881157162106749, 'ionic_motion_component': -11.015791962568233, 'ionic_force_x': -0.5762564726173878, 'ionic_force_y': -13.915500342845917, 'ionic_force_z': 1.1806349530816078, 'radial_force': 13.92742694520342, 'axial_force': 1.1806349530816078, 'contributions': [{'ion': 1327, 'force': [0.9342626333236694, -2.013418436050415, -0.30056488513946533], 'magnitude': 2.239874839782715, 'distance': 12.17466926574707, 'directional_contribution': -1.9128666113018715}, {'ion': 1340, 'force': [-0.046403419226408005, -0.8943821787834167, -1.6315449476242065], 'magnitude': 1.8611855506896973, 'distance': 13.355932235717773, 'directional_contribution': -1.627445223510299}, {'ion': 1341, 'force': [-0.5979642868041992, -6.457273483276367, 5.619952201843262], 'magnitude': 8.581247329711914, 'distance': 6.2200493812561035, 'directional_contribution': -2.357539292708914}, {'ion': 1359, 'force': [-0.7437009215354919, -1.8613765239715576, 0.03603336960077286], 'magnitude': 2.004772424697876, 'distance': 12.868754386901855, 'directional_contribution': -1.4966049111608775}, {'ion': 1400, 'force': [-0.12245047837495804, -2.68904972076416, -2.543240785598755], 'magnitude': 3.703249454498291, 'distance': 9.46842098236084, 'directional_contribution': -3.6213363463983046}]}, 6724: {'frame': 6724, 'ionic_force': [-4.113540753722191, -15.694007277488708, 7.197184890508652], 'ionic_force_magnitude': 17.748874677189196, 'motion_vector': [-0.3926811218261719, -2.1882896423339844, -1.7566070556640625], 'cosine_ionic_motion': 0.4636191203107351, 'ionic_motion_component': 8.228717664343938, 'ionic_force_x': -4.113540753722191, 'ionic_force_y': -15.694007277488708, 'ionic_force_z': 7.197184890508652, 'radial_force': 16.224151193772876, 'axial_force': 7.197184890508652, 'contributions': [{'ion': 1327, 'force': [1.648600697517395, -2.8385839462280273, -0.17031431198120117], 'magnitude': 3.2870123386383057, 'distance': 10.050053596496582, 'directional_contribution': 2.0693608177461815}, {'ion': 1330, 'force': [0.29793596267700195, -1.9125956296920776, 0.4574536681175232], 'magnitude': 1.9889825582504272, 'distance': 12.919733047485352, 'directional_contribution': 1.1522155027986862}, {'ion': 1340, 'force': [-0.16771666705608368, -1.0057437419891357, -2.1990678310394287], 'magnitude': 2.423953056335449, 'distance': 11.703262329101562, 'directional_contribution': 2.163299418899779}, {'ion': 1341, 'force': [-4.0101213455200195, -2.7143781185150146, 13.681194305419922], 'magnitude': 14.512890815734863, 'distance': 4.7829084396362305, 'directional_contribution': -5.829606053067735}, {'ion': 1359, 'force': [-1.2397171258926392, -2.3678460121154785, 0.34243646264076233], 'magnitude': 2.6945974826812744, 'distance': 11.099977493286133, 'directional_contribution': 1.7882114083837166}, {'ion': 1400, 'force': [-0.6425222754478455, -4.854859828948975, -4.914517402648926], 'magnitude': 6.9379377365112305, 'distance': 6.917574405670166, 'directional_contribution': 6.885236625128063}]}, 6725: {'frame': 6725, 'ionic_force': [-2.6017091274261475, -10.550699710845947, -2.3864916190505028], 'ionic_force_magnitude': 11.125713326343421, 'motion_vector': [-0.458587646484375, 0.23482513427734375, -0.8922119140625], 'cosine_ionic_motion': 0.07370004659283276, 'ionic_motion_component': 0.8199655905300105, 'ionic_force_x': -2.6017091274261475, 'ionic_force_y': -10.550699710845947, 'ionic_force_z': -2.3864916190505028, 'radial_force': 10.866745362443039, 'axial_force': -2.3864916190505028, 'contributions': [{'ion': 1327, 'force': [1.0887424945831299, -2.387108087539673, -0.3622821271419525], 'magnitude': 2.648564338684082, 'distance': 11.196022987365723, 'directional_contribution': -0.7149519319481872}, {'ion': 1340, 'force': [-0.1545937955379486, -0.8115612268447876, -1.4531803131103516], 'magnitude': 1.671605110168457, 'distance': 14.0929594039917, 'directional_contribution': 1.1422706635808932}, {'ion': 1341, 'force': [-2.5049638748168945, -3.5627336502075195, 1.4722782373428345], 'magnitude': 4.5973381996154785, 'distance': 8.497982025146484, 'directional_contribution': -0.9720202514220446}, {'ion': 1359, 'force': [-0.7145503759384155, -1.7946149110794067, 0.0394371822476387], 'magnitude': 1.9320404529571533, 'distance': 13.108739852905273, 'directional_contribution': -0.1251333539189594}, {'ion': 1400, 'force': [-0.3163435757160187, -1.9946818351745605, -2.082744598388672], 'magnitude': 2.9011471271514893, 'distance': 10.697546005249023, 'directional_contribution': 1.489800382213538}]}, 6726: {'frame': 6726, 'ionic_force': [-10.6773931235075, -23.184772670269012, 0.8381237238645554], 'ionic_force_magnitude': 25.539045774313546, 'motion_vector': [1.3153266906738281, 2.5401535034179688, 0.22161865234375], 'cosine_ionic_motion': -0.9928761766499101, 'ionic_motion_component': -25.357110123687477, 'ionic_force_x': -10.6773931235075, 'ionic_force_y': -23.184772670269012, 'ionic_force_z': 0.8381237238645554, 'radial_force': 25.525289571050475, 'axial_force': 0.8381237238645554, 'contributions': [{'ion': 1327, 'force': [0.9742769598960876, -2.260103225708008, -0.6310176849365234], 'magnitude': 2.5407607555389404, 'distance': 11.431077003479004, 'directional_contribution': -1.6030829678477687}, {'ion': 1330, 'force': [0.2411656379699707, -1.9719339609146118, -0.08398731797933578], 'magnitude': 1.988400936126709, 'distance': 12.921623229980469, 'directional_contribution': -1.6417904545858815}, {'ion': 1340, 'force': [-0.16953469812870026, -0.6895309090614319, -1.4364378452301025], 'magnitude': 1.602357268333435, 'distance': 14.394261360168457, 'directional_contribution': -0.7991603382369856}, {'ion': 1341, 'force': [-10.608416557312012, -15.084050178527832, 5.144473552703857], 'magnitude': 19.145042419433594, 'distance': 4.1642889976501465, 'directional_contribution': -17.82081769047824}, {'ion': 1359, 'force': [-0.709636926651001, -1.48970365524292, -0.056744806468486786], 'magnitude': 1.651066780090332, 'distance': 14.180342674255371, 'directional_contribution': -1.6486357150974915}, {'ion': 1400, 'force': [-0.4052475392818451, -1.689450740814209, -2.0981621742248535], 'magnitude': 2.7241060733795166, 'distance': 11.039693832397461, 'directional_contribution': -1.8436230626847667}]}, 6727: {'frame': 6727, 'ionic_force': [0.19401593878865242, -14.893805980682373, -1.1919869855046272], 'ionic_force_magnitude': 14.942688237004964, 'motion_vector': [1.3554725646972656, -0.12535858154296875, 0.22263336181640625], 'cosine_ionic_motion': 0.09046944261007141, 'ionic_motion_component': 1.3518566758979096, 'ionic_force_x': 0.19401593878865242, 'ionic_force_y': -14.893805980682373, 'ionic_force_z': -1.1919869855046272, 'radial_force': 14.895069612952941, 'axial_force': -1.1919869855046272, 'contributions': [{'ion': 1327, 'force': [1.8957453966140747, -2.660691499710083, -0.9064189195632935], 'magnitude': 3.3903872966766357, 'distance': 9.895651817321777, 'directional_contribution': 1.958448986402642}, {'ion': 1330, 'force': [0.34051114320755005, -2.0693624019622803, 0.12192656844854355], 'magnitude': 2.1007320880889893, 'distance': 12.571402549743652, 'directional_contribution': 0.5423675841303569}, {'ion': 1340, 'force': [-0.058663200587034225, -0.5451574325561523, -1.6288467645645142], 'magnitude': 1.7186564207077026, 'distance': 13.898711204528809, 'directional_contribution': -0.2710072166161883}, {'ion': 1341, 'force': [0.5644397139549255, -4.903802871704102, 4.149296760559082], 'magnitude': 6.448452472686768, 'distance': 7.175320148468018, 'directional_contribution': 1.670062261776156}, {'ion': 1359, 'force': [-2.4074673652648926, -2.86397123336792, 0.0936751663684845], 'magnitude': 3.74259352684021, 'distance': 9.4185209274292, 'directional_contribution': -2.0903995876372625}, {'ion': 1400, 'force': [-0.14054974913597107, -1.850820541381836, -3.0216197967529297], 'magnitude': 3.546191930770874, 'distance': 9.675823211669922, 'directional_contribution': -0.45761540201143625}]}, 6728: {'frame': 6728, 'ionic_force': [2.4772856384515762, -9.180882215499878, -5.546252489089966], 'ionic_force_magnitude': 11.008472149308323, 'motion_vector': [-2.3235855102539062, 0.4115257263183594, -0.305999755859375], 'cosine_ionic_motion': -0.2991903473440756, 'ionic_motion_component': -3.2936286060791398, 'ionic_force_x': 2.4772856384515762, 'ionic_force_y': -9.180882215499878, 'ionic_force_z': -5.546252489089966, 'radial_force': 9.509234584831756, 'axial_force': -5.546252489089966, 'contributions': [{'ion': 1327, 'force': [1.678908109664917, -2.0583689212799072, -0.4516320526599884], 'magnitude': 2.694361925125122, 'distance': 11.100461959838867, 'directional_contribution': -1.9373614066475815}, {'ion': 1330, 'force': [0.7343488931655884, -2.256716251373291, 0.1098492443561554], 'magnitude': 2.375732183456421, 'distance': 11.82143783569336, 'directional_contribution': -1.121508178453884}, {'ion': 1340, 'force': [0.15440182387828827, -0.5537362098693848, -1.7548797130584717], 'magnitude': 1.8466365337371826, 'distance': 13.408442497253418, 'directional_contribution': -0.020865612699471292}, {'ion': 1359, 'force': [-0.4944912791252136, -2.2753615379333496, -0.14022064208984375], 'magnitude': 2.3326923847198486, 'distance': 11.929996490478516, 'directional_contribution': 0.10738810882518735}, {'ion': 1400, 'force': [0.4041180908679962, -2.0366992950439453, -3.3093693256378174], 'magnitude': 3.9068377017974854, 'distance': 9.218417167663574, 'directional_contribution': -0.3212816582897684}]}, 6729: {'frame': 6729, 'ionic_force': [-0.1381404548883438, -10.870651245117188, -5.780998591333628], 'ionic_force_magnitude': 12.313004750719704, 'motion_vector': [6.845603942871094, -0.24485015869140625, 2.0646591186523438], 'cosine_ionic_motion': -0.1160126295562164, 'ionic_motion_component': -1.4284640588691777, 'ionic_force_x': -0.1381404548883438, 'ionic_force_y': -10.870651245117188, 'ionic_force_z': -5.780998591333628, 'radial_force': 10.871528930111193, 'axial_force': -5.780998591333628, 'contributions': [{'ion': 1327, 'force': [1.820922613143921, -3.5445034503936768, -0.7323452830314636], 'magnitude': 4.051616191864014, 'distance': 9.052215576171875, 'directional_contribution': 1.652296140602055}, {'ion': 1330, 'force': [0.3618646562099457, -3.046487808227539, -0.05099794641137123], 'magnitude': 3.0683276653289795, 'distance': 10.402031898498535, 'directional_contribution': 0.43579241709412253}, {'ion': 1340, 'force': [-0.1966351717710495, -0.5052287578582764, -1.6221227645874023], 'magnitude': 1.7103227376937866, 'distance': 13.932531356811523, 'directional_contribution': -0.638981387348994}, {'ion': 1359, 'force': [-1.4620943069458008, -2.0969743728637695, -0.17865630984306335], 'magnitude': 2.5626041889190674, 'distance': 11.382254600524902, 'directional_contribution': -1.3787843484740705}, {'ion': 1400, 'force': [-0.6621982455253601, -1.6774568557739258, -3.196876287460327], 'magnitude': 3.6704750061035156, 'distance': 9.510600090026855, 'directional_contribution': -1.4987868125388708}]}, 6730: {'frame': 6730, 'ionic_force': [6.242489993572235, -8.63433450460434, -3.8057007491588593], 'ionic_force_magnitude': 11.313875191524735, 'motion_vector': [-1.2953071594238281, -0.1076507568359375, -0.698211669921875], 'cosine_ionic_motion': -0.2695318144968619, 'ionic_motion_component': -3.049449309362693, 'ionic_force_x': 6.242489993572235, 'ionic_force_y': -8.63433450460434, 'ionic_force_z': -3.8057007491588593, 'radial_force': 10.654595893662535, 'axial_force': -3.8057007491588593, 'contributions': [{'ion': 1327, 'force': [1.3685665130615234, -0.9375486373901367, -0.15849584341049194], 'magnitude': 1.6664611101150513, 'distance': 14.114693641662598, 'directional_contribution': -1.0580760571043282}, {'ion': 1330, 'force': [0.8389440178871155, -1.265562891960144, 0.2689129412174225], 'magnitude': 1.542008638381958, 'distance': 14.673227310180664, 'directional_contribution': -0.7714399357565522}, {'ion': 1340, 'force': [0.9004942774772644, -0.6039507985115051, -1.6845875978469849], 'magnitude': 2.0033676624298096, 'distance': 12.873265266418457, 'directional_contribution': 0.050695409994739205}, {'ion': 1359, 'force': [0.5381330847740173, -3.9731650352478027, 0.3912965655326843], 'magnitude': 4.028491020202637, 'distance': 9.078160285949707, 'directional_contribution': -0.3677161184567961}, {'ion': 1400, 'force': [2.5963521003723145, -1.854107141494751, -2.6228268146514893], 'magnitude': 4.130130290985107, 'distance': 8.965761184692383, 'directional_contribution': -0.902912752183548}]}, 6731: {'frame': 6731, 'ionic_force': [5.921286433935165, -8.68039095401764, -5.1164384491276], 'ionic_force_magnitude': 11.68711951470537, 'motion_vector': [-3.020660400390625, -1.9799308776855469, -1.5014266967773438], 'cosine_ionic_motion': 0.1527441594740681, 'ionic_motion_component': 1.7851392469466507, 'ionic_force_x': 5.921286433935165, 'ionic_force_y': -8.68039095401764, 'ionic_force_z': -5.1164384491276, 'radial_force': 10.50765531159525, 'axial_force': -5.1164384491276, 'contributions': [{'ion': 1327, 'force': [1.439094066619873, -1.194361925125122, -0.3095908463001251], 'magnitude': 1.8956103324890137, 'distance': 13.234103202819824, 'directional_contribution': -0.387954457184696}, {'ion': 1330, 'force': [1.0320136547088623, -1.5697842836380005, 0.09940695017576218], 'magnitude': 1.8812646865844727, 'distance': 13.284465789794922, 'directional_contribution': -0.040535871168225324}, {'ion': 1340, 'force': [0.6513602137565613, -0.6999785900115967, -1.7290127277374268], 'magnitude': 1.9757846593856812, 'distance': 12.962812423706055, 'directional_contribution': 0.5150006740955995}, {'ion': 1359, 'force': [0.184901624917984, -2.459430694580078, -0.0029063455294817686], 'magnitude': 2.4663732051849365, 'distance': 11.602181434631348, 'directional_contribution': 1.1032819666116813}, {'ion': 1400, 'force': [2.6139168739318848, -2.756835460662842, -3.174335479736328], 'magnitude': 4.950667381286621, 'distance': 8.189118385314941, 'directional_contribution': 0.5953468048874413}]}, 6732: {'frame': 6732, 'ionic_force': [1.955627828836441, -8.962807416915894, -4.607766941189766], 'ionic_force_magnitude': 10.265861541145165, 'motion_vector': [-0.6335678100585938, -1.2690963745117188, -0.14817047119140625], 'cosine_ionic_motion': 0.7389153337148393, 'ionic_motion_component': 7.585602506545614, 'ionic_force_x': 1.955627828836441, 'ionic_force_y': -8.962807416915894, 'ionic_force_z': -4.607766941189766, 'radial_force': 9.17367957788161, 'axial_force': -4.607766941189766, 'contributions': [{'ion': 1327, 'force': [1.5830357074737549, -2.1781046390533447, -0.5918393135070801], 'magnitude': 2.756885051727295, 'distance': 10.973867416381836, 'directional_contribution': 1.2964471163952993}, {'ion': 1330, 'force': [0.6768920421600342, -1.9366462230682373, -0.07332560420036316], 'magnitude': 2.0528414249420166, 'distance': 12.717195510864258, 'directional_contribution': 1.430260537403739}, {'ion': 1340, 'force': [0.1329919695854187, -0.6499176025390625, -1.403283953666687], 'magnitude': 1.5521873235702515, 'distance': 14.62503719329834, 'directional_contribution': 0.6650484593941961}, {'ion': 1359, 'force': [-0.771047830581665, -2.4881412982940674, -0.2284836620092392], 'magnitude': 2.6148741245269775, 'distance': 11.26791763305664, 'directional_contribution': 2.580372619434264}, {'ion': 1400, 'force': [0.3337559401988983, -1.7099976539611816, -2.3108344078063965], 'magnitude': 2.8940353393554688, 'distance': 10.710681915283203, 'directional_contribution': 1.613473877311847}]}, 6733: {'frame': 6733, 'ionic_force': [0.8487526476383209, -7.318961501121521, -2.883708417415619], 'ionic_force_magnitude': 7.912228052100479, 'motion_vector': [-0.7289466857910156, 5.138896942138672, 0.6813125610351562], 'cosine_ionic_motion': -0.9704328231613482, 'ionic_motion_component': -7.678285806096283, 'ionic_force_x': 0.8487526476383209, 'ionic_force_y': -7.318961501121521, 'ionic_force_z': -2.883708417415619, 'radial_force': 7.36801048531909, 'axial_force': -2.883708417415619, 'contributions': [{'ion': 1327, 'force': [0.8806033730506897, -1.7291022539138794, -0.42690375447273254], 'magnitude': 1.9868324995040894, 'distance': 12.926721572875977, 'directional_contribution': -1.875587146663626}, {'ion': 1330, 'force': [0.2919199466705322, -1.480368733406067, -0.12091124057769775], 'magnitude': 1.5137134790420532, 'distance': 14.809732437133789, 'directional_contribution': -1.5096156827237035}, {'ion': 1359, 'force': [-0.5403475761413574, -1.8719149827957153, -0.2762165367603302], 'magnitude': 1.9678254127502441, 'distance': 12.989001274108887, 'directional_contribution': -1.79830479272086}, {'ion': 1400, 'force': [0.21657690405845642, -2.2375755310058594, -2.0596768856048584], 'magnitude': 3.0489211082458496, 'distance': 10.435084342956543, 'directional_contribution': -2.4947780084346047}]}, 6734: {'frame': 6734, 'ionic_force': [1.6988947242498398, -13.474987864494324, -9.640124574303627], 'ionic_force_magnitude': 16.655135635606392, 'motion_vector': [-1.3968544006347656, -1.8214874267578125, 0.22377777099609375], 'cosine_ionic_motion': 0.5210392723071953, 'ionic_motion_component': 8.677979751753991, 'ionic_force_x': 1.6988947242498398, 'ionic_force_y': -13.474987864494324, 'ionic_force_z': -9.640124574303627, 'radial_force': 13.581661946623221, 'axial_force': -9.640124574303627, 'contributions': [{'ion': 1327, 'force': [2.9800620079040527, -3.1455931663513184, -1.373476266860962], 'magnitude': 4.545543193817139, 'distance': 8.546260833740234, 'directional_contribution': 0.54614896938042}, {'ion': 1330, 'force': [0.9229516983032227, -3.564603567123413, 0.016493961215019226], 'magnitude': 3.6821882724761963, 'distance': 9.495460510253906, 'directional_contribution': 2.2578612588795517}, {'ion': 1340, 'force': [-0.08694316446781158, -0.42748773097991943, -2.029315948486328], 'magnitude': 2.0756752490997314, 'distance': 12.647052764892578, 'directional_contribution': 0.19337965322766504}, {'ion': 1359, 'force': [-2.2848825454711914, -4.074965953826904, -0.5335938334465027], 'magnitude': 4.702207565307617, 'distance': 8.40268611907959, 'directional_contribution': 4.550434171515352}, {'ion': 1400, 'force': [0.16770672798156738, -2.2623374462127686, -5.7202324867248535], 'magnitude': 6.1536455154418945, 'distance': 7.345186233520508, 'directional_contribution': 1.1301556286647134}]}, 6735: {'frame': 6735, 'ionic_force': [0.1152866929769516, -11.250973999500275, -6.662376455962658], 'ionic_force_magnitude': 13.07612201686625, 'motion_vector': [4.712928771972656, -0.7217674255371094, 0.44530487060546875], 'cosine_ionic_motion': 0.09098434487215033, 'ionic_motion_component': 1.1897223951728768, 'ionic_force_x': 0.1152866929769516, 'ionic_force_y': -11.250973999500275, 'ionic_force_z': -6.662376455962658, 'radial_force': 11.251564644928667, 'axial_force': -6.662376455962658, 'contributions': [{'ion': 1327, 'force': [1.8394445180892944, -3.4707393646240234, -0.9118136167526245], 'magnitude': 4.032492160797119, 'distance': 9.073655128479004, 'directional_contribution': 2.248703950701711}, {'ion': 1330, 'force': [0.2747195065021515, -2.3483963012695312, 0.11314840614795685], 'magnitude': 2.3671159744262695, 'distance': 11.84293270111084, 'directional_contribution': 0.6348616172852385}, {'ion': 1340, 'force': [-0.17432545125484467, -0.5549548268318176, -1.7732774019241333], 'magnitude': 1.8662467002868652, 'distance': 13.337809562683105, 'directional_contribution': -0.25282494599125993}, {'ion': 1359, 'force': [-1.2591972351074219, -2.406722068786621, -0.10812569409608841], 'magnitude': 2.7183783054351807, 'distance': 11.051319122314453, 'directional_contribution': -0.8865929467409002}, {'ion': 1400, 'force': [-0.5653546452522278, -2.4701614379882812, -3.9823081493377686], 'magnitude': 4.720180034637451, 'distance': 8.386673927307129, 'directional_contribution': -0.5544252499863358}]}, 6736: {'frame': 6736, 'ionic_force': [3.921821415424347, -9.079240322113037, -5.114391982555389], 'ionic_force_magnitude': 11.13419477970415, 'motion_vector': [-2.3464584350585938, -0.8663825988769531, -0.7218017578125], 'cosine_ionic_motion': 0.08125496034866861, 'ionic_motion_component': 0.9047085553392137, 'ionic_force_x': 3.921821415424347, 'ionic_force_y': -9.079240322113037, 'ionic_force_z': -5.114391982555389, 'radial_force': 9.890060062566064, 'axial_force': -5.114391982555389, 'contributions': [{'ion': 1327, 'force': [1.412672996520996, -1.4278366565704346, -0.3714655935764313], 'magnitude': 2.042633056640625, 'distance': 12.748934745788574, 'directional_contribution': -0.6951021777302637}, {'ion': 1330, 'force': [0.909913957118988, -1.4062199592590332, 0.1630999743938446], 'magnitude': 1.6828545331954956, 'distance': 14.0457763671875, 'directional_contribution': -0.39736213453010993}, {'ion': 1340, 'force': [0.4152483642101288, -0.6940436363220215, -1.7204067707061768], 'magnitude': 1.9010332822799683, 'distance': 13.215213775634766, 'directional_contribution': 0.33369835997093844}, {'ion': 1359, 'force': [-0.3058496415615082, -3.166868209838867, -0.161498</t>
+          <t>{6716: {'frame': 6716, 'ionic_force': [3.5372003354132175, 2.635218560695648, -13.300951480865479], 'ionic_force_magnitude': 14.013260625986366, 'motion_vector': [2.1366920471191406, 6.534908294677734, 0.9935302734375], 'cosine_ionic_motion': 0.1187908944309096, 'ionic_motion_component': 1.6646477636543684, 'ionic_force_x': 3.5372003354132175, 'ionic_force_y': 2.635218560695648, 'ionic_force_z': -13.300951480865479, 'radial_force': 4.4109140861597185, 'axial_force': -13.300951480865479, 'contributions': [{'ion': 1327, 'force': [1.9013433456420898, -1.8896634578704834, -1.5707390308380127], 'magnitude': 3.106952667236328, 'distance': 10.33717155456543, 'cosine_with_motion': -0.4562221165872038, 'motion_component': -1.4174605754747915}, {'ion': 1330, 'force': [1.3640469312667847, -2.8642194271087646, -0.5391140580177307], 'magnitude': 3.217921733856201, 'distance': 10.157370567321777, 'cosine_with_motion': -0.7308927258320043, 'motion_component': -2.3519556602151077}, {'ion': 1341, 'force': [3.074054718017578, 10.045456886291504, -7.949360370635986], 'magnitude': 13.173964500427246, 'distance': 5.020081996917725, 'cosine_with_motion': 0.702786246731144, 'motion_component': 9.258481228729863}, {'ion': 1359, 'force': [-2.778268337249756, -2.3256843090057373, -0.9613978266716003], 'magnitude': 3.748582124710083, 'distance': 9.410994529724121, 'cosine_with_motion': -0.8482782703144434, 'motion_component': -3.179840794185729}, {'ion': 1400, 'force': [-0.023976322263479233, -0.33067113161087036, -2.2803401947021484], 'magnitude': 2.3043153285980225, 'distance': 12.003229141235352, 'cosine_with_motion': -0.2797257678152574, 'motion_component': -0.6445764068267018}]}, 6717: {'frame': 6717, 'ionic_force': [0.5450510084629059, 4.748510509729385, -11.099060416221619], 'ionic_force_magnitude': 12.084476603716624, 'motion_vector': [-2.882415771484375, -8.947956085205078, 1.36480712890625], 'cosine_ionic_motion': -0.5157803651546883, 'ionic_motion_component': -6.232935755368247, 'ionic_force_x': 0.5450510084629059, 'ionic_force_y': 4.748510509729385, 'ionic_force_z': -11.099060416221619, 'radial_force': 4.779689599005029, 'axial_force': -11.099060416221619, 'contributions': [{'ion': 1327, 'force': [3.7785017490386963, 0.381460577249527, -2.1780126094818115], 'magnitude': 4.377936363220215, 'distance': 8.708318710327148, 'cosine_with_motion': -0.41544024505267596, 'motion_component': -1.8187709444652604}, {'ion': 1330, 'force': [8.046460151672363, -2.481989860534668, -1.290306568145752], 'magnitude': 8.518842697143555, 'distance': 6.242790222167969, 'cosine_with_motion': -0.03392759388441384, 'motion_component': -0.28902384491516386}, {'ion': 1341, 'force': [0.29557427763938904, 3.0619518756866455, -0.5244418382644653], 'magnitude': 3.1205694675445557, 'distance': 10.314593315124512, 'cosine_with_motion': -0.9771509240004413, 'motion_component': -3.049267163667653}, {'ion': 1359, 'force': [-12.195097923278809, 2.7431704998016357, -4.48800802230835], 'magnitude': 13.281100273132324, 'distance': 4.99979305267334, 'cosine_with_motion': 0.035512542081213586, 'motion_component': 0.47164561801915283}, {'ion': 1400, 'force': [0.6196127533912659, 1.0439174175262451, -2.6182913780212402], 'magnitude': 2.886023759841919, 'distance': 10.72553825378418, 'cosine_with_motion': -0.5362116516285387, 'motion_component': -1.5475195795965124}]}, 6718: {'frame': 6718, 'ionic_force': [-15.74527932703495, -6.038105010986328, -8.724657155573368], 'ionic_force_magnitude': 18.986631499356328, 'motion_vector': [-0.8591651916503906, -0.15292739868164062, -0.16278839111328125], 'cosine_ionic_motion': 0.9416545980486678, 'ionic_motion_component': 17.878848852824557, 'ionic_force_x': -15.74527932703495, 'ionic_force_y': -6.038105010986328, 'ionic_force_z': -8.724657155573368, 'radial_force': 16.863348813626917, 'axial_force': -8.724657155573368, 'contributions': [{'ion': 1327, 'force': [1.6139215230941772, -3.2655608654022217, -0.8199719190597534], 'magnitude': 3.733762741088867, 'distance': 9.429652214050293, 'cosine_with_motion': -0.22740655832611156, 'motion_component': -0.8490821403328379}, {'ion': 1330, 'force': [0.40082046389579773, -2.4494481086730957, 0.07108324021100998], 'magnitude': 2.483043670654297, 'distance': 11.5631685256958, 'cosine_with_motion': 0.008458743424691165, 'motion_component': 0.021003429387131622}, {'ion': 1340, 'force': [-0.1447393149137497, -0.5571725368499756, -1.720524549484253], 'magnitude': 1.8142755031585693, 'distance': 13.527496337890625, 'cosine_with_motion': 0.3040179980827136, 'motion_component': 0.5515723921234557}, {'ion': 1341, 'force': [-15.274748802185059, 4.401199817657471, -2.545541286468506], 'magnitude': 16.098703384399414, 'distance': 4.54123067855835, 'cosine_with_motion': 0.900194890649546, 'motion_component': 14.491971667476406}, {'ion': 1359, 'force': [-1.6921180486679077, -1.7458655834197998, -0.0793391764163971], 'magnitude': 2.432612895965576, 'distance': 11.682413101196289, 'cosine_with_motion': 0.8028370445889909, 'motion_component': 1.9529916373492413}, {'ion': 1400, 'force': [-0.6484151482582092, -2.421257734298706, -3.6303634643554688], 'magnitude': 4.4116291999816895, 'distance': 8.67500114440918, 'cosine_with_motion': 0.3877006632017084, 'motion_component': 1.7103914746028686}]}, 6719: {'frame': 6719, 'ionic_force': [-13.247648186981678, -7.324256241321564, -7.235395602881908], 'ionic_force_magnitude': 16.777838403822457, 'motion_vector': [3.021942138671875, 1.1164970397949219, -1.1178054809570312], 'cosine_ionic_motion': -0.7013024980662967, 'ionic_motion_component': -11.766339984753339, 'ionic_force_x': -13.247648186981678, 'ionic_force_y': -7.324256241321564, 'ionic_force_z': -7.235395602881908, 'radial_force': 15.13753321960275, 'axial_force': -7.235395602881908, 'contributions': [{'ion': 1327, 'force': [1.420046091079712, -3.122454881668091, -0.8165378570556641], 'magnitude': 3.5260443687438965, 'distance': 9.7034273147583, 'cosine_with_motion': 0.14286728851306163, 'motion_component': 0.5037564096968339}, {'ion': 1330, 'force': [0.10633199661970139, -2.712059497833252, -0.04335900396108627], 'magnitude': 2.714489459991455, 'distance': 11.059231758117676, 'cosine_with_motion': -0.28717403087952637, 'motion_component': -0.7795308899562283}, {'ion': 1340, 'force': [-0.22071534395217896, -0.5099888443946838, -1.6464329957962036], 'magnitude': 1.737683892250061, 'distance': 13.822405815124512, 'cosine_with_motion': 0.10193220999201093, 'motion_component': 0.1771259648225083}, {'ion': 1341, 'force': [-12.584758758544922, 2.7286531925201416, -1.619233250617981], 'magnitude': 12.978583335876465, 'distance': 5.057727336883545, 'cosine_with_motion': -0.7495715800440138, 'motion_component': -9.728376991680793}, {'ion': 1359, 'force': [-1.4268096685409546, -1.9060715436935425, -0.11701104044914246], 'magnitude': 2.383817672729492, 'distance': 11.801372528076172, 'cosine_with_motion': -0.776132534249492, 'motion_component': -1.8501583614498278}, {'ion': 1400, 'force': [-0.5417425036430359, -1.8023346662521362, -2.992821455001831], 'magnitude': 3.535374879837036, 'distance': 9.690614700317383, 'cosine_with_motion': -0.025218295532721334, 'motion_component': -0.0891561282175708}]}, 6720: {'frame': 6720, 'ionic_force': [-13.875824749469757, -1.1168307960033417, -19.71669438481331], 'ionic_force_magnitude': 24.135738251999413, 'motion_vector': [-2.0362319946289062, -3.377918243408203, 1.4120712280273438], 'cosine_ionic_motion': 0.04139525447767722, 'ionic_motion_component': 0.999105026948124, 'ionic_force_x': -13.875824749469757, 'ionic_force_y': -1.1168307960033417, 'ionic_force_z': -19.71669438481331, 'radial_force': 13.920697665882228, 'axial_force': -19.71669438481331, 'contributions': [{'ion': 1327, 'force': [1.9507142305374146, -2.5765552520751953, -0.8716263175010681], 'magnitude': 3.3471860885620117, 'distance': 9.959306716918945, 'cosine_with_motion': 0.24963399482009194, 'motion_component': 0.8355714608759257}, {'ion': 1330, 'force': [0.7414261698722839, -2.502897262573242, -0.2262757122516632], 'magnitude': 2.620192527770996, 'distance': 11.256476402282715, 'cosine_with_motion': 0.6035741375210052, 'motion_component': 1.581480363051632}, {'ion': 1340, 'force': [0.15693143010139465, -0.3897511661052704, -1.5432026386260986], 'magnitude': 1.5993773937225342, 'distance': 14.40766429901123, 'cosine_with_motion': -0.17642624695933348, 'motion_component': -0.2821721389973071}, {'ion': 1341, 'force': [-16.80057144165039, 8.428204536437988, -13.408795356750488], 'magnitude': 23.088733673095703, 'distance': 3.792005777359009, 'cosine_with_motion': -0.13640637058778973, 'motion_component': -3.1494503699860275}, {'ion': 1359, 'force': [-0.39115285873413086, -2.5806212425231934, -0.5263550877571106], 'magnitude': 2.6626408100128174, 'distance': 11.166389465332031, 'cosine_with_motion': 0.7862480782728855, 'motion_component': 2.0934962423746057}, {'ion': 1400, 'force': [0.46682772040367126, -1.4952104091644287, -3.14043927192688], 'magnitude': 3.5094075202941895, 'distance': 9.726400375366211, 'cosine_with_motion': -0.022744741781503392, 'motion_component': -0.0798205677429511}]}, 6721: {'frame': 6721, 'ionic_force': [-14.872823670506477, -15.005800008773804, -8.68900191783905], 'ionic_force_magnitude': 22.84455454075444, 'motion_vector': [-1.2706642150878906, 0.12684249877929688, -0.00298309326171875], 'cosine_ionic_motion': 0.5834653141139671, 'ionic_motion_component': 13.329005190914943, 'ionic_force_x': -14.872823670506477, 'ionic_force_y': -15.005800008773804, 'ionic_force_z': -8.68900191783905, 'radial_force': 21.127586654355333, 'axial_force': -8.68900191783905, 'contributions': [{'ion': 1327, 'force': [0.9067454934120178, -1.875288724899292, -0.39515984058380127], 'magnitude': 2.120152473449707, 'distance': 12.513692855834961, 'cosine_with_motion': -0.5129856540705134, 'motion_component': -1.0876078009618537}, {'ion': 1340, 'force': [-0.07977347075939178, -0.7151584625244141, -1.4344524145126343], 'magnitude': 1.604826807975769, 'distance': 14.38318157196045, 'cosine_with_motion': 0.0072862170865083615, 'motion_component': 0.011693116688635014}, {'ion': 1341, 'force': [-14.652536392211914, -8.457913398742676, -4.700499534606934], 'magnitude': 17.55926513671875, 'distance': 4.348263740539551, 'cosine_with_motion': 0.7831130950979465, 'motion_component': 13.75089103791261}, {'ion': 1359, 'force': [-0.839736819267273, -1.8682215213775635, -0.06597363948822021], 'magnitude': 2.0493321418762207, 'distance': 12.728078842163086, 'cosine_with_motion': 0.3172573445902172, 'motion_component': 0.6501656636034504}, {'ion': 1400, 'force': [-0.20752248167991638, -2.0892179012298584, -2.092916488647461], 'magnitude': 2.964489221572876, 'distance': 10.5826416015625, 'cosine_with_motion': 0.0013031289237940694, 'motion_component': 0.0038631116715133196}]}, 6722: {'frame': 6722, 'ionic_force': [-6.684693541377783, -13.338738977909088, -3.4362437948584557], 'ionic_force_magnitude': 15.310612550797314, 'motion_vector': [1.3387413024902344, 0.14303207397460938, 0.6805572509765625], 'cosine_ionic_motion': -0.5712972196657156, 'ionic_motion_component': -8.746910381649515, 'ionic_force_x': -6.684693541377783, 'ionic_force_y': -13.338738977909088, 'ionic_force_z': -3.4362437948584557, 'radial_force': 14.920022964557695, 'axial_force': -3.4362437948584557, 'contributions': [{'ion': 1327, 'force': [0.81926029920578, -2.1865475177764893, -0.4886828362941742], 'magnitude': 2.3855793476104736, 'distance': 11.797014236450195, 'cosine_with_motion': 0.12544369478288375, 'motion_component': 0.2992558764165798}, {'ion': 1330, 'force': [0.03506458178162575, -1.515844464302063, 0.15978533029556274], 'magnitude': 1.5246459245681763, 'distance': 14.756539344787598, 'cosine_with_motion': -0.026577021145496933, 'motion_component': -0.04052054803409777}, {'ion': 1340, 'force': [-0.26287201046943665, -0.7818873524665833, -1.5102778673171997], 'magnitude': 1.7208685874938965, 'distance': 13.889774322509766, 'cosine_with_motion': -0.5745508499662869, 'motion_component': -0.9887265207963449}, {'ion': 1341, 'force': [-5.845895767211914, -5.08392858505249, 0.5223320126533508], 'magnitude': 7.764898777008057, 'distance': 6.538846492767334, 'cosine_with_motion': -0.699828776593821, 'motion_component': -5.434099831997331}, {'ion': 1359, 'force': [-0.7654677033424377, -1.5446780920028687, -0.07922738045454025], 'magnitude': 1.7257601022720337, 'distance': 13.870075225830078, 'cosine_with_motion': -0.49918877829101976, 'motion_component': -0.8614801146791009}, {'ion': 1400, 'force': [-0.6647829413414001, -2.2258529663085938, -2.040173053741455], 'magnitude': 3.0917088985443115, 'distance': 10.362624168395996, 'cosine_with_motion': -0.5567597574552943, 'motion_component': -1.7213390931081953}]}, 6723: {'frame': 6723, 'ionic_force': [-0.5762564726173878, -13.915500342845917, 1.1806349530816078], 'ionic_force_magnitude': 13.977378874682344, 'motion_vector': [-0.162322998046875, 2.1346893310546875, 1.369384765625], 'cosine_ionic_motion': -0.7881157162106749, 'ionic_motion_component': -11.015791962568233, 'ionic_force_x': -0.5762564726173878, 'ionic_force_y': -13.915500342845917, 'ionic_force_z': 1.1806349530816078, 'radial_force': 13.92742694520342, 'axial_force': 1.1806349530816078, 'contributions': [{'ion': 1327, 'force': [0.9342626333236694, -2.013418436050415, -0.30056488513946533], 'magnitude': 2.239874839782715, 'distance': 12.17466926574707, 'cosine_with_motion': -0.8540059906302656, 'motion_component': -1.9128666113018717}, {'ion': 1340, 'force': [-0.046403419226408005, -0.8943821787834167, -1.6315449476242065], 'magnitude': 1.8611855506896973, 'distance': 13.355932235717773, 'cosine_with_motion': -0.8744132028960275, 'motion_component': -1.627445223510299}, {'ion': 1341, 'force': [-0.5979642868041992, -6.457273483276367, 5.619952201843262], 'magnitude': 8.581247329711914, 'distance': 6.2200493812561035, 'cosine_with_motion': -0.27473154144593465, 'motion_component': -2.357539292708914}, {'ion': 1359, 'force': [-0.7437009215354919, -1.8613765239715576, 0.03603336960077286], 'magnitude': 2.004772424697876, 'distance': 12.868754386901855, 'cosine_with_motion': -0.7465211391778789, 'motion_component': -1.4966049111608775}, {'ion': 1400, 'force': [-0.12245047837495804, -2.68904972076416, -2.543240785598755], 'magnitude': 3.703249454498291, 'distance': 9.46842098236084, 'cosine_with_motion': -0.9778807589389066, 'motion_component': -3.6213363463983046}]}, 6724: {'frame': 6724, 'ionic_force': [-4.113540753722191, -15.694007277488708, 7.197184890508652], 'ionic_force_magnitude': 17.748874677189196, 'motion_vector': [-0.3926811218261719, -2.1882896423339844, -1.7566070556640625], 'cosine_ionic_motion': 0.4636191203107351, 'ionic_motion_component': 8.228717664343938, 'ionic_force_x': -4.113540753722191, 'ionic_force_y': -15.694007277488708, 'ionic_force_z': 7.197184890508652, 'radial_force': 16.224151193772876, 'axial_force': 7.197184890508652, 'contributions': [{'ion': 1327, 'force': [1.648600697517395, -2.8385839462280273, -0.17031431198120117], 'magnitude': 3.2870123386383057, 'distance': 10.050053596496582, 'cosine_with_motion': 0.6295567558755207, 'motion_component': 2.0693608177461815}, {'ion': 1330, 'force': [0.29793596267700195, -1.9125956296920776, 0.4574536681175232], 'magnitude': 1.9889825582504272, 'distance': 12.919733047485352, 'cosine_with_motion': 0.579298938670601, 'motion_component': 1.1522155027986862}, {'ion': 1340, 'force': [-0.16771666705608368, -1.0057437419891357, -2.1990678310394287], 'magnitude': 2.423953056335449, 'distance': 11.703262329101562, 'cosine_with_motion': 0.892467519191024, 'motion_component': 2.163299418899779}, {'ion': 1341, 'force': [-4.0101213455200195, -2.7143781185150146, 13.681194305419922], 'magnitude': 14.512890815734863, 'distance': 4.7829084396362305, 'cosine_with_motion': -0.40168469073769564, 'motion_component': -5.829606053067735}, {'ion': 1359, 'force': [-1.2397171258926392, -2.3678460121154785, 0.34243646264076233], 'magnitude': 2.6945974826812744, 'distance': 11.099977493286133, 'cosine_with_motion': 0.6636283776503213, 'motion_component': 1.7882114083837164}, {'ion': 1400, 'force': [-0.6425222754478455, -4.854859828948975, -4.914517402648926], 'magnitude': 6.9379377365112305, 'distance': 6.917574405670166, 'cosine_with_motion': 0.9924039216805082, 'motion_component': 6.885236625128063}]}, 6725: {'frame': 6725, 'ionic_force': [-2.6017091274261475, -10.550699710845947, -2.3864916190505028], 'ionic_force_magnitude': 11.125713326343421, 'motion_vector': [-0.458587646484375, 0.23482513427734375, -0.8922119140625], 'cosine_ionic_motion': 0.07370004659283276, 'ionic_motion_component': 0.8199655905300105, 'ionic_force_x': -2.6017091274261475, 'ionic_force_y': -10.550699710845947, 'ionic_force_z': -2.3864916190505028, 'radial_force': 10.866745362443039, 'axial_force': -2.3864916190505028, 'contributions': [{'ion': 1327, 'force': [1.0887424945831299, -2.387108087539673, -0.3622821271419525], 'magnitude': 2.648564338684082, 'distance': 11.196022987365723, 'cosine_with_motion': -0.2699394138825094, 'motion_component': -0.7149519319481872}, {'ion': 1340, 'force': [-0.1545937955379486, -0.8115612268447876, -1.4531803131103516], 'magnitude': 1.671605110168457, 'distance': 14.0929594039917, 'cosine_with_motion': 0.683337593691137, 'motion_component': 1.1422706635808932}, {'ion': 1341, 'force': [-2.5049638748168945, -3.5627336502075195, 1.4722782373428345], 'magnitude': 4.5973381996154785, 'distance': 8.497982025146484, 'cosine_with_motion': -0.21143109657537829, 'motion_component': -0.9720202514220446}, {'ion': 1359, 'force': [-0.7145503759384155, -1.7946149110794067, 0.0394371822476387], 'magnitude': 1.9320404529571533, 'distance': 13.108739852905273, 'cosine_with_motion': -0.06476746148457564, 'motion_component': -0.1251333539189594}, {'ion': 1400, 'force': [-0.3163435757160187, -1.9946818351745605, -2.082744598388672], 'magnitude': 2.9011471271514893, 'distance': 10.697546005249023, 'cosine_with_motion': 0.5135211624013504, 'motion_component': 1.489800382213538}]}, 6726: {'frame': 6726, 'ionic_force': [-10.6773931235075, -23.184772670269012, 0.8381237238645554], 'ionic_force_magnitude': 25.539045774313546, 'motion_vector': [1.3153266906738281, 2.5401535034179688, 0.22161865234375], 'cosine_ionic_motion': -0.9928761766499101, 'ionic_motion_component': -25.357110123687477, 'ionic_force_x': -10.6773931235075, 'ionic_force_y': -23.184772670269012, 'ionic_force_z': 0.8381237238645554, 'radial_force': 25.525289571050475, 'axial_force': 0.8381237238645554, 'contributions': [{'ion': 1327, 'force': [0.9742769598960876, -2.260103225708008, -0.6310176849365234], 'magnitude': 2.5407607555389404, 'distance': 11.431077003479004, 'cosine_with_motion': -0.6309460379872143, 'motion_component': -1.6030829678477687}, {'ion': 1330, 'force': [0.2411656379699707, -1.9719339609146118, -0.08398731797933578], 'magnitude': 1.988400936126709, 'distance': 12.921623229980469, 'cosine_with_motion': -0.8256838071159796, 'motion_component': -1.6417904545858815}, {'ion': 1340, 'force': [-0.16953469812870026, -0.6895309090614319, -1.4364378452301025], 'magnitude': 1.602357268333435, 'distance': 14.394261360168457, 'cosine_with_motion': -0.49874044444684573, 'motion_component': -0.7991603382369856}, {'ion': 1341, 'force': [-10.608416557312012, -15.084050178527832, 5.144473552703857], 'magnitude': 19.145042419433594, 'distance': 4.1642889976501465, 'cosine_with_motion': -0.9308319385126406, 'motion_component': -17.82081769047824}, {'ion': 1359, 'force': [-0.709636926651001, -1.48970365524292, -0.056744806468486786], 'magnitude': 1.651066780090332, 'distance': 14.180342674255371, 'cosine_with_motion': -0.9985275776246425, 'motion_component': -1.6486357150974915}, {'ion': 1400, 'force': [-0.4052475392818451, -1.689450740814209, -2.0981621742248535], 'magnitude': 2.7241060733795166, 'distance': 11.039693832397461, 'cosine_with_motion': -0.6767809384082066, 'motion_component': -1.8436230626847667}]}, 6727: {'frame': 6727, 'ionic_force': [0.19401593878865242, -14.893805980682373, -1.1919869855046272], 'ionic_force_magnitude': 14.942688237004964, 'motion_vector': [1.3554725646972656, -0.12535858154296875, 0.22263336181640625], 'cosine_ionic_motion': 0.09046944261007141, 'ionic_motion_component': 1.3518566758979096, 'ionic_force_x': 0.19401593878865242, 'ionic_force_y': -14.893805980682373, 'ionic_force_z': -1.1919869855046272, 'radial_force': 14.895069612952941, 'axial_force': -1.1919869855046272, 'contributions': [{'ion': 1327, 'force': [1.8957453966140747, -2.660691499710083, -0.9064189195632935], 'magnitude': 3.3903872966766357, 'distance': 9.895651817321777, 'cosine_with_motion': 0.5776475934913463, 'motion_component': 1.9584489864026418}, {'ion': 1330, 'force': [0.34051114320755005, -2.0693624019622803, 0.12192656844854355], 'magnitude': 2.1007320880889893, 'distance': 12.571402549743652, 'cosine_with_motion': 0.25818029144636306, 'motion_component': 0.5423675841303569}, {'ion': 1340, 'force': [-0.058663200587034225, -0.5451574325561523, -1.6288467645645142], 'magnitude': 1.7186564207077026, 'distance': 13.898711204528809, 'cosine_with_motion': -0.15768551440409598, 'motion_component': -0.2710072166161883}, {'ion': 1341, 'force': [0.5644397139549255, -4.903802871704102, 4.149296760559082], 'magnitude': 6.448452472686768, 'distance': 7.175320148468018, 'cosine_with_motion': 0.25898652222747937, 'motion_component': 1.670062261776156}, {'ion': 1359, 'force': [-2.4074673652648926, -2.86397123336792, 0.0936751663684845], 'magnitude': 3.74259352684021, 'distance': 9.4185209274292, 'cosine_with_motion': -0.5585430643324164, 'motion_component': -2.0903995876372625}, {'ion': 1400, 'force': [-0.14054974913597107, -1.850820541381836, -3.0216197967529297], 'magnitude': 3.546191930770874, 'distance': 9.675823211669922, 'cosine_with_motion': -0.12904417269620683, 'motion_component': -0.4576154020114362}]}, 6728: {'frame': 6728, 'ionic_force': [2.4772856384515762, -9.180882215499878, -5.546252489089966], 'ionic_force_magnitude': 11.008472149308323, 'motion_vector': [-2.3235855102539062, 0.4115257263183594, -0.305999755859375], 'cosine_ionic_motion': -0.2991903473440756, 'ionic_motion_component': -3.2936286060791398, 'ionic_force_x': 2.4772856384515762, 'ionic_force_y': -9.180882215499878, 'ionic_force_z': -5.546252489089966, 'radial_force': 9.509234584831756, 'axial_force': -5.546252489089966, 'contributions': [{'ion': 1327, 'force': [1.678908109664917, -2.0583689212799072, -0.4516320526599884], 'magnitude': 2.694361925125122, 'distance': 11.100461959838867, 'cosine_with_motion': -0.7190427304193472, 'motion_component': -1.9373614066475815}, {'ion': 1330, 'force': [0.7343488931655884, -2.256716251373291, 0.1098492443561554], 'magnitude': 2.375732183456421, 'distance': 11.82143783569336, 'cosine_with_motion': -0.47206843757298744, 'motion_component': -1.121508178453884}, {'ion': 1340, 'force': [0.15440182387828827, -0.5537362098693848, -1.7548797130584717], 'magnitude': 1.8466365337371826, 'distance': 13.408442497253418, 'cosine_with_motion': -0.011299252569514797, 'motion_component': -0.020865612699471292}, {'ion': 1359, 'force': [-0.4944912791252136, -2.2753615379333496, -0.14022064208984375], 'magnitude': 2.3326923847198486, 'distance': 11.929996490478516, 'cosine_with_motion': 0.046036121737723396, 'motion_component': 0.10738810882518735}, {'ion': 1400, 'force': [0.4041180908679962, -2.0366992950439453, -3.3093693256378174], 'magnitude': 3.9068377017974854, 'distance': 9.218417167663574, 'cosine_with_motion': -0.08223573214076878, 'motion_component': -0.3212816582897684}]}, 6729: {'frame': 6729, 'ionic_force': [-0.1381404548883438, -10.870651245117188, -5.780998591333628], 'ionic_force_magnitude': 12.313004750719704, 'motion_vector': [6.845603942871094, -0.24485015869140625, 2.0646591186523438], 'cosine_ionic_motion': -0.1160126295562164, 'ionic_motion_component': -1.4284640588691777, 'ionic_force_x': -0.1381404548883438, 'ionic_force_y': -10.870651245117188, 'ionic_force_z': -5.780998591333628, 'radial_force': 10.871528930111193, 'axial_force': -5.780998591333628, 'contributions': [{'ion': 1327, 'force': [1.820922613143921, -3.5445034503936768, -0.7323452830314636], 'magnitude': 4.051616191864014, 'distance': 9.052215576171875, 'cosine_with_motion': 0.40781161798980436, 'motion_component': 1.652296140602055}, {'ion': 1330, 'force': [0.3618646562099457, -3.046487808227539, -0.05099794641137123], 'magnitude': 3.0683276653289795, 'distance': 10.402031898498535, 'cosine_with_motion': 0.14202929470439557, 'motion_component': 0.43579241709412253}, {'ion': 1340, 'force': [-0.1966351717710495, -0.5052287578582764, -1.6221227645874023], 'magnitude': 1.7103227376937866, 'distance': 13.932531356811523, 'cosine_with_motion': -0.37360282117611954, 'motion_component': -0.638981387348994}, {'ion': 1359, 'force': [-1.4620943069458008, -2.0969743728637695, -0.17865630984306335], 'magnitude': 2.5626041889190674, 'distance': 11.382254600524902, 'cosine_with_motion': -0.5380403441470379, 'motion_component': -1.3787843484740705}, {'ion': 1400, 'force': [-0.6621982455253601, -1.6774568557739258, -3.196876287460327], 'magnitude': 3.6704750061035156, 'distance': 9.510600090026855, 'cosine_with_motion': -0.40833593798437023, 'motion_component': -1.4987868125388708}]}, 6730: {'frame': 6730, 'ionic_force': [6.242489993572235, -8.63433450460434, -3.8057007491588593], 'ionic_force_magnitude': 11.313875191524735, 'motion_vector': [-1.2953071594238281, -0.1076507568359375, -0.698211669921875], 'cosine_ionic_motion': -0.2695318144968619, 'ionic_motion_component': -3.049449309362693, 'ionic_force_x': 6.242489993572235, 'ionic_force_y': -8.63433450460434, 'ionic_force_z': -3.8057007491588593, 'radial_force': 10.654595893662535, 'axial_force': -3.8057007491588593, 'contributions': [{'ion': 1327, 'force': [1.3685665130615234, -0.9375486373901367, -0.15849584341049194], 'magnitude': 1.6664611101150513, 'distance': 14.114693641662598, 'cosine_with_motion': -0.63492393632704, 'motion_component': -1.0580760571043282}, {'ion': 1330, 'force': [0.8389440178871155, -1.265562891960144, 0.2689129412174225], 'magnitude': 1.542008638381958, 'distance': 14.673227310180664, 'cosine_with_motion': -0.5002824965118858, 'motion_component': -0.7714399357565522}, {'ion': 1340, 'force': [0.9004942774772644, -0.6039507985115051, -1.6845875978469849], 'magnitude': 2.0033676624298096, 'distance': 12.873265266418457, 'cosine_with_motion': 0.025305095819517134, 'motion_component': 0.050695409994739205}, {'ion': 1359, 'force': [0.5381330847740173, -3.9731650352478027, 0.3912965655326843], 'magnitude': 4.028491020202637, 'distance': 9.078160285949707, 'cosine_with_motion': -0.09127887054839494, 'motion_component': -0.3677161184567961}, {'ion': 1400, 'force': [2.5963521003723145, -1.854107141494751, -2.6228268146514893], 'magnitude': 4.130130290985107, 'distance': 8.965761184692383, 'cosine_with_motion': -0.21861603410071279, 'motion_component': -0.902912752183548}]}, 6731: {'frame': 6731, 'ionic_force': [5.921286433935165, -8.68039095401764, -5.1164384491276], 'ionic_force_magnitude': 11.68711951470537, 'motion_vector': [-3.020660400390625, -1.9799308776855469, -1.5014266967773438], 'cosine_ionic_motion': 0.1527441594740681, 'ionic_motion_component': 1.7851392469466507, 'ionic_force_x': 5.921286433935165, 'ionic_force_y': -8.68039095401764, 'ionic_force_z': -5.1164384491276, 'radial_force': 10.50765531159525, 'axial_force': -5.1164384491276, 'contributions': [{'ion': 1327, 'force': [1.439094066619873, -1.194361925125122, -0.3095908463001251], 'magnitude': 1.8956103324890137, 'distance': 13.234103202819824, 'cosine_with_motion': -0.20465938865396574, 'motion_component': -0.387954457184696}, {'ion': 1330, 'force': [1.0320136547088623, -1.5697842836380005, 0.09940695017576218], 'magnitude': 1.8812646865844727, 'distance': 13.284465789794922, 'cosine_with_motion': -0.021547139323103797, 'motion_component': -0.040535871168225324}, {'ion': 1340, 'force': [0.6513602137565613, -0.6999785900115967, -1.7290127277374268], 'magnitude': 1.9757846593856812, 'distance': 12.962812423706055, 'cosine_with_motion': 0.2606562724109064, 'motion_component': 0.5150006740955995}, {'ion': 1359, 'force': [0.184901624917984, -2.459430694580078, -0.0029063455294817686], 'magnitude': 2.4663732051849365, 'distance': 11.602181434631348, 'cosine_with_motion': 0.44732970642265735, 'motion_component': 1.1032819666116813}, {'ion': 1400, 'force': [2.6139168739318848, -2.756835460662842, -3.174335479736328], 'magnitude': 4.950667381286621, 'distance': 8.189118385314941, 'cosine_with_motion': 0.12025586492624583, 'motion_component': 0.5953468048874413}]}, 6732: {'frame': 6732, 'ionic_force': [1.955627828836441, -8.962807416915894, -4.607766941189766], 'ionic_force_magnitude': 10.265861541145165, 'motion_vector': [-0.6335678100585938, -1.2690963745117188, -0.14817047119140625], 'cosine_ionic_motion': 0.7389153337148393, 'ionic_motion_component': 7.585602506545614, 'ionic_force_x': 1.955627828836441, 'ionic_force_y': -8.962807416915894, 'ionic_force_z': -4.607766941189766, 'radial_force': 9.17367957788161, 'axial_force': -4.607766941189766, 'contributions': [{'ion': 1327, 'force': [1.5830357074737549, -2.1781046390533447, -0.5918393135070801], 'magnitude': 2.756885051727295, 'distance': 10.973867416381836, 'cosine_with_motion': 0.470257937243374, 'motion_component': 1.2964471163952993}, {'ion': 1330, 'force': [0.6768920421600342, -1.9366462230682373, -0.07332560420036316], 'magnitude': 2.0528414249420166, 'distance': 12.717195510864258, 'cosine_with_motion': 0.6967223542728048, 'motion_component': 1.430260537403739}, {'ion': 1340, 'force': [0.1329919695854187, -0.6499176025390625, -1.403283953666687], 'magnitude': 1.5521873235702515, 'distance': 14.62503719329834, 'cosine_with_motion': 0.4284588802932099, 'motion_component': 0.6650484593941961}, {'ion': 1359, 'force': [-0.771047830581665, -2.4881412982940674, -0.2284836620092392], 'magnitude': 2.6148741245269775, 'distance': 11.26791763305664, 'cosine_with_motion': 0.9868056745584073, 'motion_component': 2.580372619434264}, {'ion': 1400, 'force': [0.3337559401988983, -1.7099976539611816, -2.3108344078063965], 'magnitude': 2.8940353393554688, 'distance': 10.710681915283203, 'cosine_with_motion': 0.5575169880978661, 'motion_component': 1.6134738773118473}]}, 6733: {'frame': 6733, 'ionic_force': [0.8487526476383209, -7.318961501121521, -2.883708417415619], 'ionic_force_magnitude': 7.912228052100479, 'motion_vector': [-0.7289466857910156, 5.138896942138672, 0.6813125610351562], 'cosine_ionic_motion': -0.9704328231613482, 'ionic_motion_component': -7.678285806096283, 'ionic_force_x': 0.8487526476383209, 'ionic_force_y': -7.318961501121521, 'ionic_force_z': -2.883708417415619, 'radial_force': 7.36801048531909, 'axial_force': -2.883708417415619, 'contributions': [{'ion': 1327, 'force': [0.8806033730506897, -1.7291022539138794, -0.42690375447273254], 'magnitude': 1.9868324995040894, 'distance': 12.926721572875977, 'cosine_with_motion': -0.9440086501758859, 'motion_component': -1.875587146663626}, {'ion': 1330, 'force': [0.2919199466705322, -1.480368733406067, -0.12091124057769775], 'magnitude': 1.5137134790420532, 'distance': 14.809732437133789, 'cosine_with_motion': -0.9972929126098181, 'motion_component': -1.5096156827237035}, {'ion': 1359, 'force': [-0.5403475761413574, -1.8719149827957153, -0.2762165367603302], 'magnitude': 1.9678254127502441, 'distance': 12.989001274108887, 'cosine_with_motion': -0.9138538400095987, 'motion_component': -1.79830479272086}, {'ion': 1400, 'force': [0.21657690405845642, -2.2375755310058594, -2.0596768856048584], 'magnitude': 3.0489211082458496, 'distance': 10.435084342956543, 'cosine_with_motion': -0.8182495007592367, 'motion_component': -2.4947780084346047}]}, 6734: {'frame': 6734, 'ionic_force': [1.6988947242498398, -13.474987864494324, -9.640124574303627], 'ionic_force_magnitude': 16.655135635606392, 'motion_vector': [-1.3968544006347656, -1.8214874267578125, 0.22377777099609375], 'cosine_ionic_motion': 0.5210392723071953, 'ionic_motion_component': 8.677979751753991, 'ionic_force_x': 1.6988947242498398, 'ionic_force_y': -13.474987864494324, 'ionic_force_z': -9.640124574303627, 'radial_force': 13.581661946623221, 'axial_force': -9.640124574303627, 'contributions': [{'ion': 1327, 'force': [2.9800620079040527, -3.1455931663513184, -1.373476266860962], 'magnitude': 4.545543193817139, 'distance': 8.546260833740234, 'cosine_with_motion': 0.12015042981565179, 'motion_component': 0.54614896938042}, {'ion': 1330, 'force': [0.9229516983032227, -3.564603567123413, 0.016493961215019226], 'magnitude': 3.682188272</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add residues at force_results.json - 3000:6799
</commit_message>
<xml_diff>
--- a/results/forces/force_results.xlsx
+++ b/results/forces/force_results.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{3185: {'frame': 3185, 'ionic_force': [1.3455531299114227, -1.2103240936994553, -9.767556190490723], 'ionic_force_magnitude': 9.93380851293186, 'motion_vector': [3.3021926879882812, 1.7625465393066406, 0.34154510498046875], 'cosine_ionic_motion': -0.027479692611883776, 'ionic_motion_component': -0.27297800440068176, 'ionic_force_x': 1.3455531299114227, 'ionic_force_y': -1.2103240936994553, 'ionic_force_z': -9.767556190490723, 'radial_force': 1.8098059667278792, 'axial_force': -9.767556190490723, 'contributions': [{'ion': 1313, 'force': [1.0481852293014526, -0.9845649600028992, -6.827840805053711], 'magnitude': 6.9776411056518555, 'distance': 6.8978657722473145, 'cosine_with_motion': -0.023108002613043896, 'motion_component': -0.1612393407807282}, {'ion': 1460, 'force': [0.2973679006099701, -0.2257591336965561, -2.9397153854370117], 'magnitude': 2.963329553604126, 'distance': 10.584712982177734, 'cosine_with_motion': -0.03770713874789775, 'motion_component': -0.11173867455445306}]}, 3186: {'frame': 3186, 'ionic_force': [3.8716278672218323, 0.9531629383563995, -6.351068735122681], 'ionic_force_magnitude': 7.498939658882293, 'motion_vector': [-1.120147705078125, -0.510986328125, 0.8818283081054688], 'cosine_ionic_motion': -0.917921914123857, 'ionic_motion_component': -6.883441045580538, 'ionic_force_x': 3.8716278672218323, 'ionic_force_y': 0.9531629383563995, 'ionic_force_z': -6.351068735122681, 'radial_force': 3.987232364598893, 'axial_force': -6.351068735122681, 'contributions': [{'ion': 1313, 'force': [2.8922908306121826, 0.682626485824585, -4.142235279083252], 'magnitude': 5.0979838371276855, 'distance': 8.069931030273438, 'cosine_with_motion': -0.9379406452351742, 'motion_component': -4.781606164194734}, {'ion': 1460, 'force': [0.9793370366096497, 0.2705364525318146, -2.2088334560394287], 'magnitude': 2.4313035011291504, 'distance': 11.685558319091797, 'cosine_with_motion': -0.8644888675281329, 'motion_component': -2.101834725921859}]}, 3187: {'frame': 3187, 'ionic_force': [4.825020015239716, 1.0010420382022858, -9.05678677558899], 'ionic_force_magnitude': 10.31059115706736, 'motion_vector': [-4.467868804931641, 3.94091796875, -0.4804229736328125], 'cosine_ionic_motion': -0.2151940520558242, 'ionic_motion_component': -2.218777890180274, 'ionic_force_x': 4.825020015239716, 'ionic_force_y': 1.0010420382022858, 'ionic_force_z': -9.05678677558899, 'radial_force': 4.927768593360696, 'axial_force': -9.05678677558899, 'contributions': [{'ion': 1313, 'force': [3.834963321685791, 0.7111164927482605, -6.247584819793701], 'magnitude': 7.365116596221924, 'distance': 6.713967323303223, 'cosine_with_motion': -0.257383167032912, 'motion_component': -1.8956571041124768}, {'ion': 1460, 'force': [0.9900566935539246, 0.28992554545402527, -2.809201955795288], 'magnitude': 2.992638349533081, 'distance': 10.532752990722656, 'cosine_with_motion': -0.1079719114881787, 'motion_component': -0.32312089049107406}]}, 3188: {'frame': 3188, 'ionic_force': [-0.7788635641336441, 4.744892954826355, -7.823496103286743], 'ionic_force_magnitude': 9.183013061214636, 'motion_vector': [2.9478530883789062, -1.2035942077636719, 0.8451919555664062], 'cosine_ionic_motion': -0.48324645421477935, 'ionic_motion_component': -4.437658500839979, 'ionic_force_x': -0.7788635641336441, 'ionic_force_y': 4.744892954826355, 'ionic_force_z': -7.823496103286743, 'radial_force': 4.808392413717472, 'axial_force': -7.823496103286743, 'contributions': [{'ion': 1313, 'force': [-0.5623465180397034, 3.5319478511810303, -5.200526714324951], 'magnitude': 6.311605930328369, 'distance': 7.252689838409424, 'cosine_with_motion': -0.49556723884648435, 'motion_component': -3.127825041783648}, {'ion': 1460, 'force': [-0.21651704609394073, 1.2129451036453247, -2.622969388961792], 'magnitude': 2.897944688796997, 'distance': 10.703454971313477, 'cosine_with_motion': -0.45198706097319374, 'motion_component': -1.3098335379862371}]}, 3189: {'frame': 3189, 'ionic_force': [2.2279635965824127, 3.7496649622917175, -8.675254344940186], 'ionic_force_magnitude': 9.70998697561115, 'motion_vector': [2.050933837890625, -1.666748046875, -0.683929443359375], 'cosine_ionic_motion': 0.16044574791098273, 'ionic_motion_component': 1.5579261225078322, 'ionic_force_x': 2.2279635965824127, 'ionic_force_y': 3.7496649622917175, 'ionic_force_z': -8.675254344940186, 'radial_force': 4.361629181525475, 'axial_force': -8.675254344940186, 'contributions': [{'ion': 1313, 'force': [1.8297994136810303, 3.0413978099823, -6.2925825119018555], 'magnitude': 7.2246012687683105, 'distance': 6.778944969177246, 'cosine_with_motion': 0.15146603579443732, 'motion_component': 1.0942816903629335}, {'ion': 1460, 'force': [0.39816418290138245, 0.7082671523094177, -2.38267183303833], 'magnitude': 2.517399787902832, 'distance': 11.483993530273438, 'cosine_with_motion': 0.1841759707827572, 'motion_component': 0.4636445661517268}]}, 3190: {'frame': 3190, 'ionic_force': [3.4962931871414185, 1.3681584894657135, -6.685306072235107], 'ionic_force_magnitude': 7.667414230509018, 'motion_vector': [-0.8215522766113281, -0.8835487365722656, -0.6362762451171875], 'cosine_ionic_motion': 0.016492182069415995, 'ionic_motion_component': 0.12645239149118587, 'ionic_force_x': 3.4962931871414185, 'ionic_force_y': 1.3681584894657135, 'ionic_force_z': -6.685306072235107, 'radial_force': 3.7544538487972656, 'axial_force': -6.685306072235107, 'contributions': [{'ion': 1313, 'force': [2.741168975830078, 1.0629887580871582, -4.5104899406433105], 'magnitude': 5.38409423828125, 'distance': 7.852586269378662, 'cosine_with_motion': -0.04375086242833566, 'motion_component': -0.23555877116258728}, {'ion': 1460, 'force': [0.7551242113113403, 0.3051697313785553, -2.174816131591797], 'magnitude': 2.3223190307617188, 'distance': 11.956610679626465, 'cosine_with_motion': 0.15588340078660728, 'motion_component': 0.36201101054708035}]}, 3191: {'frame': 3191, 'ionic_force': [3.8587116599082947, 0.6158474087715149, -7.850509166717529], 'ionic_force_magnitude': 8.769231316479157, 'motion_vector': [1.4482460021972656, 0.2650604248046875, 0.5260162353515625], 'cosine_ionic_motion': 0.11831350931893483, 'ionic_motion_component': 1.037518531082152, 'ionic_force_x': 3.8587116599082947, 'ionic_force_y': 0.6158474087715149, 'ionic_force_z': -7.850509166717529, 'radial_force': 3.9075470189369206, 'axial_force': -7.850509166717529, 'contributions': [{'ion': 1313, 'force': [2.9662954807281494, 0.4142634868621826, -5.240616798400879], 'magnitude': 6.036106586456299, 'distance': 7.416356086730957, 'cosine_with_motion': 0.17474385144598134, 'motion_component': 1.0547725824270096}, {'ion': 1460, 'force': [0.8924161791801453, 0.20158392190933228, -2.6098923683166504], 'magnitude': 2.7656068801879883, 'distance': 10.956549644470215, 'cosine_with_motion': -0.006238752915845556, 'motion_component': -0.01725393739331782}]}, 3192: {'frame': 3192, 'ionic_force': [4.3233126401901245, 0.8234727382659912, -6.483328104019165], 'ionic_force_magnitude': 7.835986398652038, 'motion_vector': [-1.4279060363769531, -0.3152008056640625, 0.24273681640625], 'cosine_ionic_motion': -0.6893186884874044, 'ionic_motion_component': -5.401491867323962, 'ionic_force_x': 4.3233126401901245, 'ionic_force_y': 0.8234727382659912, 'ionic_force_z': -6.483328104019165, 'radial_force': 4.401038461033372, 'axial_force': -6.483328104019165, 'contributions': [{'ion': 1313, 'force': [3.2284295558929443, 0.5756868124008179, -4.195573329925537], 'magnitude': 5.325129985809326, 'distance': 7.895941734313965, 'cosine_with_motion': -0.7360294220437638, 'motion_component': -3.919452270043964}, {'ion': 1460, 'force': [1.0948830842971802, 0.24778592586517334, -2.287754774093628], 'magnitude': 2.548330545425415, 'distance': 11.41408634185791, 'cosine_with_motion': -0.5815727327514694, 'motion_component': -1.4820395787670382}]}, 3193: {'frame': 3193, 'ionic_force': [4.54551488161087, 0.7150068581104279, -9.185447692871094], 'ionic_force_magnitude': 10.273528588783979, 'motion_vector': [-1.265380859375, 0.5024642944335938, 1.421234130859375], 'cosine_ionic_motion': -0.9123378360158684, 'ionic_motion_component': -9.372928840938334, 'ionic_force_x': 4.54551488161087, 'ionic_force_y': 0.7150068581104279, 'ionic_force_z': -9.185447692871094, 'radial_force': 4.6014063443789475, 'axial_force': -9.185447692871094, 'contributions': [{'ion': 1313, 'force': [3.558159112930298, 0.47408899664878845, -6.336966037750244], 'magnitude': 7.283020973205566, 'distance': 6.751701831817627, 'cosine_with_motion': -0.9258083810288427, 'motion_component': -6.74268190178226}, {'ion': 1460, 'force': [0.9873557686805725, 0.2409178614616394, -2.8484816551208496], 'magnitude': 3.0243611335754395, 'distance': 10.477368354797363, 'cosine_with_motion': -0.8696867439300969, 'motion_component': -2.630246830321605}]}, 3194: {'frame': 3194, 'ionic_force': [7.131795823574066, 3.0327844619750977, -18.466155529022217], 'ionic_force_magnitude': 20.026462325732517, 'motion_vector': [1.2636222839355469, 1.3273963928222656, -1.654449462890625], 'cosine_ionic_motion': 0.8815604678031085, 'ionic_motion_component': 17.654537496314084, 'ionic_force_x': 7.131795823574066, 'ionic_force_y': 3.0327844619750977, 'ionic_force_z': -18.466155529022217, 'radial_force': 7.749857628495254, 'axial_force': -18.466155529022217, 'contributions': [{'ion': 1313, 'force': [5.728073596954346, 2.3258800506591797, -12.010092735290527], 'magnitude': 13.507882118225098, 'distance': 4.957644939422607, 'cosine_with_motion': 0.9053912250945034, 'motion_component': 12.229917716004195}, {'ion': 1387, 'force': [0.3024868369102478, 0.18391072750091553, -1.7984228134155273], 'magnitude': 1.832933783531189, 'distance': 13.45846939086914, 'cosine_with_motion': 0.7958791628889741, 'motion_component': 1.4587937625408287}, {'ion': 1460, 'force': [1.1012353897094727, 0.5229936838150024, -4.657639980316162], 'magnitude': 4.814545631408691, 'distance': 8.3040771484375, 'cosine_with_motion': 0.8237175571334348, 'motion_component': 3.965825965203912}]}, 3195: {'frame': 3195, 'ionic_force': [4.266230762004852, 2.5804542303085327, -8.203031539916992], 'ionic_force_magnitude': 9.599437243623537, 'motion_vector': [-2.6438636779785156, 0.3204536437988281, -0.75738525390625], 'cosine_ionic_motion': -0.15950752621456848, 'ionic_motion_component': -1.5311824877823865, 'ionic_force_x': 4.266230762004852, 'ionic_force_y': 2.5804542303085327, 'ionic_force_z': -8.203031539916992, 'radial_force': 4.985927090260517, 'axial_force': -8.203031539916992, 'contributions': [{'ion': 1313, 'force': [3.318345785140991, 1.9544174671173096, -5.576297760009766], 'magnitude': 6.776891708374023, 'distance': 6.99928617477417, 'cosine_with_motion': -0.20910020006651614, 'motion_component': -1.4170494408500325}, {'ion': 1460, 'force': [0.9478849768638611, 0.6260367631912231, -2.6267337799072266], 'magnitude': 2.8618416786193848, 'distance': 10.770756721496582, 'cosine_with_motion': -0.039881000971897285, 'motion_component': -0.11413311435657825}]}, 3196: {'frame': 3196, 'ionic_force': [0.6016596853733063, 2.649301290512085, -8.311489343643188], 'ionic_force_magnitude': 8.744235061708187, 'motion_vector': [2.318988800048828, -2.4310836791992188, 0.22534942626953125], 'cosine_ionic_motion': -0.2349655890604089, 'ionic_motion_component': -2.0545943421569453, 'ionic_force_x': 0.6016596853733063, 'ionic_force_y': 2.649301290512085, 'ionic_force_z': -8.311489343643188, 'radial_force': 2.716761252836271, 'axial_force': -8.311489343643188, 'contributions': [{'ion': 1313, 'force': [0.49341556429862976, 2.0448687076568604, -5.6436381340026855], 'magnitude': 6.022922515869141, 'distance': 7.424468994140625, 'cosine_with_motion': -0.25140903765843836, 'motion_component': -1.5142172100840625}, {'ion': 1460, 'force': [0.10824412107467651, 0.6044325828552246, -2.667851209640503], 'magnitude': 2.7376058101654053, 'distance': 11.01244068145752, 'cosine_with_motion': -0.19739042068930143, 'motion_component': -0.5403771640603434}]}, 3197: {'frame': 3197, 'ionic_force': [2.8209893107414246, 0.17508456483483315, -8.191557884216309], 'ionic_force_magnitude': 8.665463395954491, 'motion_vector': [-2.359294891357422, 1.4584197998046875, 2.7145614624023438], 'cosine_ionic_motion': -0.8515068024527294, 'ionic_motion_component': -7.378701028060378, 'ionic_force_x': 2.8209893107414246, 'ionic_force_y': 0.17508456483483315, 'ionic_force_z': -8.191557884216309, 'radial_force': 2.8264173959556613, 'axial_force': -8.191557884216309, 'contributions': [{'ion': 1313, 'force': [2.2362687587738037, 0.05940436199307442, -5.672110557556152], 'magnitude': 6.097315788269043, 'distance': 7.379036903381348, 'cosine_with_motion': -0.8699706879091497, 'motion_component': -5.304486381330342}, {'ion': 1460, 'force': [0.5847205519676208, 0.11568020284175873, -2.5194473266601562], 'magnitude': 2.5889949798583984, 'distance': 11.32409381866455, 'cosine_with_motion': -0.8011659975708844, 'motion_component': -2.074214723975322}]}, 3198: {'frame': 3198, 'ionic_force': [4.809750139713287, 10.997350573539734, -26.898103833198547], 'ionic_force_magnitude': 29.45476881364607, 'motion_vector': [0.19825363159179688, 0.10056686401367188, -2.5326690673828125], 'cosine_ionic_motion': 0.9372048718855969, 'ionic_motion_component': 27.605152832413037, 'ionic_force_x': 4.809750139713287, 'ionic_force_y': 10.997350573539734, 'ionic_force_z': -26.898103833198547, 'radial_force': 12.003141923838388, 'axial_force': -26.898103833198547, 'contributions': [{'ion': 1313, 'force': [3.9049830436706543, 9.421380996704102, -19.212223052978516], 'magnitude': 21.751340866088867, 'distance': 3.906843662261963, 'cosine_with_motion': 0.9110158763380631, 'motion_component': 19.815816810828306}, {'ion': 1387, 'force': [0.15719091892242432, 0.2684478759765625, -1.947790265083313], 'magnitude': 1.9724756479263306, 'distance': 12.973681449890137, 'cosine_with_motion': 0.995300771002789, 'motion_component': 1.9632065286741396}, {'ion': 1460, 'force': [0.7475761771202087, 1.3075217008590698, -5.738090515136719], 'magnitude': 5.932466983795166, 'distance': 7.4808573722839355, 'cosine_with_motion': 0.9820752260428413, 'motion_component': 5.8261289687319895}]}, 3199: {'frame': 3199, 'ionic_force': [0.9833395779132843, 3.1130231618881226, -10.068522930145264], 'ionic_force_magnitude': 10.58456536315042, 'motion_vector': [-0.02933502197265625, -3.176746368408203, 1.2943191528320312], 'cosine_ionic_motion': -0.6320647076797856, 'ionic_motion_component': -6.6901302121772535, 'ionic_force_x': 0.9833395779132843, 'ionic_force_y': 3.1130231618881226, 'ionic_force_z': -10.068522930145264, 'radial_force': 3.264639326471241, 'axial_force': -10.068522930145264, 'contributions': [{'ion': 1313, 'force': [0.8440772891044617, 2.4483911991119385, -7.0417280197143555], 'magnitude': 7.502867221832275, 'distance': 6.652048587799072, 'cosine_with_motion': -0.6572728715675435, 'motion_component': -4.931431210428519}, {'ion': 1460, 'force': [0.13926228880882263, 0.6646319627761841, -3.026794910430908], 'magnitude': 3.102034330368042, 'distance': 10.345362663269043, 'cosine_with_motion': -0.5669501891312683, 'motion_component': -1.7586989570614022}]}, 3200: {'frame': 3200, 'ionic_force': [1.5398932620882988, -3.925731360912323, -14.942134141921997], 'ionic_force_magnitude': 15.525785348634267, 'motion_vector': [-0.7101936340332031, -1.3734970092773438, -0.6399917602539062], 'cosine_ionic_motion': 0.5334978917055188, 'ionic_motion_component': 8.282973750568814, 'ionic_force_x': 1.5398932620882988, 'ionic_force_y': -3.925731360912323, 'ionic_force_z': -14.942134141921997, 'radial_force': 4.21694652286171, 'axial_force': -14.942134141921997, 'contributions': [{'ion': 1313, 'force': [1.2463655471801758, -3.3982043266296387, -10.489591598510742], 'magnitude': 11.096519470214844, 'distance': 5.469852924346924, 'cosine_with_motion': 0.5652003166871671, 'motion_component': 6.2717565039260705}, {'ion': 1387, 'force': [0.09594348818063736, -0.13932183384895325, -1.5808546543121338], 'magnitude': 1.5898796319961548, 'distance': 14.450634956359863, 'cosine_with_motion': 0.4265788497944352, 'motion_component': 0.6782090140143298}, {'ion': 1460, 'force': [0.19758422672748566, -0.3882052004337311, -2.871687889099121], 'magnitude': 2.9045369625091553, 'distance': 10.691302299499512, 'cosine_with_motion': 0.45894008835435396, 'motion_component': 1.3330083846379597}]}, 3201: {'frame': 3201, 'ionic_force': [0.3855626368895173, -4.750433802604675, -10.51581072807312], 'ionic_force_magnitude': 11.54545603813691, 'motion_vector': [-0.7017936706542969, -0.01294708251953125, -0.8671646118164062], 'cosine_ionic_motion': 0.6917273308343146, 'ionic_motion_component': 7.986307488525365, 'ionic_force_x': 0.3855626368895173, 'ionic_force_y': -4.750433802604675, 'ionic_force_z': -10.51581072807312, 'radial_force': 4.766054957708137, 'axial_force': -10.51581072807312, 'contributions': [{'ion': 1313, 'force': [0.3916058838367462, -3.7393531799316406, -7.343410015106201], 'magnitude': 8.249957084655762, 'distance': 6.343708038330078, 'cosine_with_motion': 0.6672680685827019, 'motion_component': 5.504932773013024}, {'ion': 1460, 'force': [-0.0060432469472289085, -1.0110806226730347, -3.172400712966919], 'magnitude': 3.3296315670013428, 'distance': 9.985526084899902, 'cosine_with_motion': 0.74524006733559, 'motion_component': 2.4813749044541478}]}, 3202: {'frame': 3202, 'ionic_force': [-0.8432059288024902, -2.719889461994171, -7.3930346965789795], 'ionic_force_magnitude': 7.9224842662295805, 'motion_vector': [-0.6875076293945312, -0.4496726989746094, -0.5331268310546875], 'cosine_ionic_motion': 0.7403493413536228, 'ionic_motion_component': 5.8654060083875095, 'ionic_force_x': -0.8432059288024902, 'ionic_force_y': -2.719889461994171, 'ionic_force_z': -7.3930346965789795, 'radial_force': 2.8475945855817697, 'axial_force': -7.3930346965789795, 'contributions': [{'ion': 1313, 'force': [-0.6528485417366028, -2.2744596004486084, -5.246335506439209], 'magnitude': 5.755294322967529, 'distance': 7.595130920410156, 'cosine_with_motion': 0.7573262503904421, 'motion_component': 4.358635548107902}, {'ion': 1460, 'force': [-0.19035738706588745, -0.44542986154556274, -2.1466991901397705], 'magnitude': 2.2006728649139404, 'distance': 12.282628059387207, 'cosine_with_motion': 0.6846863323502752, 'motion_component': 1.5067706405058947}]}, 3203: {'frame': 3203, 'ionic_force': [-0.9554902762174606, -3.667130023241043, -8.258195757865906], 'ionic_force_magnitude': 9.086176393320592, 'motion_vector': [-1.41168212890625, -0.13762283325195312, 1.837890625], 'cosine_ionic_motion': -0.6316526643237212, 'ionic_motion_component': -5.739307527356252, 'ionic_force_x': -0.9554902762174606, 'ionic_force_y': -3.667130023241043, 'ionic_force_z': -8.258195757865906, 'radial_force': 3.7895651828807444, 'axial_force': -8.258195757865906, 'contributions': [{'ion': 1313, 'force': [-0.582251787185669, -2.546912908554077, -4.254993915557861], 'magnitude': 4.993070602416992, 'distance': 8.154272079467773, 'cosine_with_motion': -0.5734918508861262, 'motion_component': -2.863485398333836}, {'ion': 1387, 'force': [-0.14848487079143524, -0.3223477303981781, -1.5331422090530396], 'magnitude': 1.5736838579177856, 'distance': 14.52480411529541, 'cosine_with_motion': -0.7017500765273089, 'motion_component': -1.1043327598431159}, {'ion': 1460, 'force': [-0.22475361824035645, -0.7978693842887878, -2.470059633255005], 'magnitude': 2.6054375171661377, 'distance': 11.288304328918457, 'cosine_with_motion': -0.6799200535321163, 'motion_component': -1.7714891742978691}]}, 3204: {'frame': 3204, 'ionic_force': [-4.891388177871704, -6.8576348423957825, -12.308661103248596], 'ionic_force_magnitude': 14.914957998361531, 'motion_vector': [2.0974998474121094, 3.643840789794922, -4.29998779296875], 'cosine_ionic_motion': 0.19709987365095533, 'ionic_motion_component': 2.9397363369863636, 'ionic_force_x': -4.891388177871704, 'ionic_force_y': -6.8576348423957825, 'ionic_force_z': -12.308661103248596, 'radial_force': 8.423350517357312, 'axial_force': -12.308661103248596, 'contributions': [{'ion': 1313, 'force': [-3.5466692447662354, -5.008401393890381, -7.102478504180908], 'magnitude': 9.386594772338867, 'distance': 5.947234153747559, 'cosine_with_motion': 0.0859452850752351, 'motion_component': 0.8067335028722198}, {'ion': 1387, 'force': [-0.37983453273773193, -0.5484148859977722, -1.9710179567337036], 'magnitude': 2.0808520317077637, 'distance': 12.631312370300293, 'cosine_with_motion': 0.45391548181313884, 'motion_component': 0.9445309271792581}, {'ion': 1460, 'force': [-0.9648844003677368, -1.3008185625076294, -3.2351646423339844], 'magnitude': 3.6179304122924805, 'distance': 9.579413414001465, 'cosine_with_motion': 0.32849483507551613, 'motion_component': 1.1884714828583895}]}, 3205: {'frame': 3205, 'ionic_force': [-0.6016021221876144, 0.16618561744689941, -6.180601716041565], 'ionic_force_magnitude': 6.21203512105355, 'motion_vector': [-2.4292831420898438, -0.1877899169921875, 1.3914337158203125], 'cosine_ionic_motion': -0.41133902842181963, 'ionic_motion_component': -2.555252491216388, 'ionic_force_x': -0.6016021221876144, 'ionic_force_y': 0.16618561744689941, 'ionic_force_z': -6.180601716041565, 'radial_force': 0.6241336177989842, 'axial_force': -6.180601716041565, 'contributions': [{'ion': 1313, 'force': [-0.47208482027053833, 0.13534782826900482, -4.1929497718811035], 'magnitude': 4.221612453460693, 'distance': 8.868085861206055, 'cosine_with_motion': -0.39786613493239775, 'motion_component': -1.679636592081345}, {'ion': 1460, 'force': [-0.1295173019170761, 0.030837789177894592, -1.9876519441604614], 'magnitude': 1.9921059608459473, 'distance': 12.909601211547852, 'cosine_with_motion': -0.43954280105675997, 'motion_component': -0.8756158111541572}]}, 3206: {'frame': 3206, 'ionic_force': [-2.3814292550086975, -0.07051205262541771, -6.440298318862915], 'ionic_force_magnitude': 6.866849327175107, 'motion_vector': [4.136890411376953, -0.5502357482910156, -0.2530059814453125], 'cosine_ionic_motion': -0.2850374206019799, 'ionic_motion_component': -1.9573090198804335, 'ionic_force_x': -2.3814292550086975, 'ionic_force_y': -0.07051205262541771, 'ionic_force_z': -6.440298318862915, 'radial_force': 2.3824729266408737, 'axial_force': -6.440298318862915, 'contributions': [{'ion': 1313, 'force': [-1.8158272504806519, -0.09443157911300659, -4.377440452575684], 'magnitude': 4.740056037902832, 'distance': 8.369071960449219, 'cosine_with_motion': -0.3205352276549729, 'motion_component': -1.5193549276856588}, {'ion': 1460, 'force': [-0.5656020045280457, 0.023919526487588882, -2.0628578662872314], 'magnitude': 2.1391260623931885, 'distance': 12.458072662353516, 'cosine_with_motion': -0.20473505796635882, 'motion_component': -0.4379541001504612}]}, 3207: {'frame': 3207, 'ionic_force': [0.5504616945981979, -0.20011846721172333, -6.7197370529174805], 'ionic_force_magnitude': 6.7452147140392205, 'motion_vector': [-0.4560203552246094, -0.9889564514160156, 2.2855987548828125], 'cosine_ionic_motion': -0.9024609612745147, 'ionic_motion_component': -6.087292954834836, 'ionic_force_x': 0.5504616945981979, 'ionic_force_y': -0.20011846721172333, 'ionic_force_z': -6.7197370529174805, 'radial_force': 0.5857093802724089, 'axial_force': -6.7197370529174805, 'contributions': [{'ion': 1313, 'force': [0.4108598530292511, -0.13039463758468628, -4.540388107299805], 'magnitude': 4.5608038902282715, 'distance': 8.531950950622559, 'cosine_with_motion': -0.9037776946529549, 'motion_component': -4.1219528871178355}, {'ion': 1460, 'force': [0.13960184156894684, -0.06972382962703705, -2.179348945617676], 'magnitude': 2.1849284172058105, 'distance': 12.326803207397461, 'cosine_with_motion': -0.8994986514893245, 'motion_component': -1.9653401082788329}]}, 3208: {'frame': 3208, 'ionic_force': [0.6337229162454605, -2.9306737780570984, -10.785738706588745], 'ionic_force_magnitude': 11.194758281212362, 'motion_vector': [0.30518341064453125, 1.3927268981933594, -1.3763351440429688], 'cosine_ionic_motion': 0.49388111416975305, 'ionic_motion_component': 5.528879692786231, 'ionic_force_x': 0.6337229162454605, 'ionic_force_y': -2.9306737780570984, 'ionic_force_z': -10.785738706588745, 'radial_force': 2.998408499181877, 'axial_force': -10.785738706588745, 'contributions': [{'ion': 1313, 'force': [0.44283202290534973, -2.438164234161377, -7.620040416717529], 'magnitude': 8.012849807739258, 'distance': 6.436882019042969, 'cosine_with_motion': 0.45513940674212605, 'motion_component': 3.6469636778250076}, {'ion': 1460, 'force': [0.19089089334011078, -0.49250954389572144, -3.165698289871216], 'magnitude': 3.2094626426696777, 'distance': 10.170747756958008, 'cosine_with_motion': 0.5863647716762116, 'motion_component': 1.8819158471922193}]}, 3209: {'frame': 3209, 'ionic_force': [0.43650949746370316, -0.5205679461359978, -6.388556241989136], 'ionic_force_magnitude': 6.424576436231311, 'motion_vector': [-2.8515777587890625, -0.7392349243164062, -1.9197006225585938], 'cosine_ionic_motion': 0.5048408404249863, 'ionic_motion_component': 3.2433885674415786, 'ionic_force_x': 0.43650949746370316, 'ionic_force_y': -0.5205679461359978, 'ionic_force_z': -6.388556241989136, 'radial_force': 0.6793611174627716, 'axial_force': -6.388556241989136, 'contributions': [{'ion': 1313, 'force': [0.33712059259414673, -0.4496636390686035, -4.658642292022705], 'magnitude': 4.692419052124023, 'distance': 8.411445617675781, 'cosine_with_motion': 0.5039206562836169, 'motion_component': 2.3646068414033508}, {'ion': 1460, 'force': [0.09938890486955643, -0.07090430706739426, -1.7299139499664307], 'magnitude': 1.7342168092727661, 'distance': 13.836216926574707, 'cosine_with_motion': 0.5067312342068669, 'motion_component': 0.8787818106888905}]}, 3210: {'frame': 3210, 'ionic_force': [-1.0865365266799927, -0.4411945790052414, -5.631094336509705], 'ionic_force_magnitude': 5.751907310364546, 'motion_vector': [-0.060733795166015625, -0.4639701843261719, -0.5265655517578125], 'cosine_ionic_motion': 0.7986072361519804, 'ionic_motion_component': 4.593514799732601, 'ionic_force_x': -1.0865365266799927, 'ionic_force_y': -0.4411945790052414, 'ionic_force_z': -5.631094336509705, 'radial_force': 1.1726953058460814, 'axial_force': -5.631094336509705, 'contributions': [{'ion': 1313, 'force': [-0.8106954097747803, -0.30610916018486023, -3.7750306129455566], 'magnitude': 3.87321400642395, 'distance': 9.258343696594238, 'cosine_with_motion': 0.7986521289722621, 'motion_component': 3.093350535334695}, {'ion': 1460, 'force': [-0.2758411169052124, -0.13508541882038116, -1.856063723564148], 'magnitude': 1.8813050985336304, 'distance': 13.284322738647461, 'cosine_with_motion': 0.7974061921978106, 'motion_component': 1.500164348614363}]}, 3211: {'frame': 3211, 'ionic_force': [-1.4129315614700317, -1.1412988752126694, -6.022145748138428], 'ionic_force_magnitude': 6.290085701465569, 'motion_vector': [0.17093276977539062, 2.88043212890625, 2.7339096069335938], 'cosine_ionic_motion': -0.7996257345609912, 'ionic_motion_component': -5.029714399485993, 'ionic_force_x': -1.4129315614700317, 'ionic_force_y': -1.1412988752126694, 'ionic_force_z': -6.022145748138428, 'radial_force': 1.816298081252041, 'axial_force': -6.022145748138428, 'contributions': [{'ion': 1313, 'force': [-1.1177146434783936, -0.9046632647514343, -4.136012077331543], 'magnitude': 4.378846645355225, 'distance': 8.707413673400879, 'cosine_with_motion': -0.8103263953123397, 'motion_component': -3.54829498140504}, {'ion': 1460, 'force': [-0.2952169179916382, -0.23663561046123505, -1.8861336708068848], 'magnitude': 1.9237072467803955, 'distance': 13.137101173400879, 'cosine_with_motion': -0.7700856154835416, 'motion_component': -1.4814192978902772}]}, 3212: {'frame': 3212, 'ionic_force': [-2.1320821791887283, 1.880209058523178, -9.907267928123474], 'ionic_force_magnitude': 10.307032469250826, 'motion_vector': [-0.551544189453125, -2.786346435546875, -0.7046661376953125], 'cosine_ionic_motion': 0.09675015725847247, 'ionic_motion_component': 0.9972070122681992, 'ionic_force_x': -2.1320821791887283, 'ionic_force_y': 1.880209058523178, 'ionic_force_z': -9.907267928123474, 'radial_force': 2.8427030310193806, 'axial_force': -9.907267928123474, 'contributions': [{'ion': 1313, 'force': [-1.564578652381897, 1.3044873476028442, -5.753448963165283], 'magnitude': 6.10342264175415, 'distance': 7.375344753265381, 'cosine_with_motion': 0.07179818047445186, 'motion_component': 0.4382146440348506}, {'ion': 1387, 'force': [-0.18752484023571014, 0.17749661207199097, -1.5429457426071167], 'magnitude': 1.5644015073776245, 'distance': 14.567831993103027, 'cosine_with_motion': 0.15205022229138687, 'motion_component': 0.23786760187487757}, {'ion': 1460, 'force': [-0.3799786865711212, 0.3982250988483429, -2.610873222351074], 'magnitude': 2.6682627201080322, 'distance': 11.154619216918945, 'cosine_with_motion': 0.1203497363508293, 'motion_component': 0.32112471648709473}]}, 3213: {'frame': 3213, 'ionic_force': [-3.1511535048484802, -1.7650651186704636, -9.942092418670654], 'ionic_force_magnitude': 10.57782704271792, 'motion_vector': [-0.14082717895507812, -0.13962173461914062, -1.2342300415039062], 'cosine_ionic_motion': 0.9801949420071061, 'ionic_motion_component': 10.368332564698092, 'ionic_force_x': -3.1511535048484802, 'ionic_force_y': -1.7650651186704636, 'ionic_force_z': -9.942092418670654, 'radial_force': 3.611817172043186, 'axial_force': -9.942092418670654, 'contributions': [{'ion': 1313, 'force': [-2.6584701538085938, -1.5168129205703735, -7.454015254974365], 'magnitude': 8.057948112487793, 'distance': 6.418843746185303, 'cosine_with_motion': 0.9715291196890977, 'motion_component': 7.82853127435799}, {'ion': 1460, 'force': [-0.4926833510398865, -0.24825219810009003, -2.488077163696289], 'magnitude': 2.5485081672668457, 'distance': 11.413688659667969, 'cosine_with_motion': 0.9965835225965978, 'motion_component': 2.5398012725363297}]}, 3214: {'frame': 3214, 'ionic_force': [-1.5444872081279755, -1.1262651979923248, -6.004039764404297], 'ionic_force_magnitude': 6.300984647245829, 'motion_vector': [0.7136573791503906, -0.08641815185546875, -0.5668869018554688], 'cosine_ionic_motion': 0.4158258844145278, 'ionic_motion_component': 2.6201125136233583, 'ionic_force_x': -1.5444872081279755, 'ionic_force_y': -1.1262651979923248, 'ionic_force_z': -6.004039764404297, 'radial_force': 1.9115213920538894, 'axial_force': -6.004039764404297, 'contributions': [{'ion': 1313, 'force': [-1.1439869403839111, -0.8971394300460815, -3.885117769241333], 'magnitude': 4.14821720123291, 'distance': 8.94619369506836, 'cosine_with_motion': 0.3853762981400929, 'motion_component': 1.5986245614389398}, {'ion': 1460, 'force': [-0.40050026774406433, -0.2291257679462433, -2.118921995162964], 'magnitude': 2.1685779094696045, 'distance': 12.373186111450195, 'cosine_with_motion': 0.4710405579521181, 'motion_component': 1.0214880782956504}]}, 3215: {'frame': 3215, 'ionic_force': [-0.8170889019966125, -0.7826167792081833, -5.666041016578674], 'ionic_force_magnitude': 5.777901357622516, 'motion_vector': [-0.340850830078125, 0.852874755859375, 0.39165496826171875], 'cosine_ionic_motion': -0.4520783780553534, 'ionic_motion_component': -2.6120642743178117, 'ionic_force_x': -0.8170889019966125, 'ionic_force_y': -0.7826167792081833, 'ionic_force_z': -5.666041016578674, 'radial_force': 1.1314253386168351, 'axial_force': -5.666041016578674, 'contributions': [{'ion': 1313, 'force': [-0.5830154418945312, -0.575762152671814, -3.7722537517547607], 'magnitude': 3.8602211475372314, 'distance': 9.273911476135254, 'cosine_with_motion': -0.4591556550887339, 'motion_component': -1.772442377020944}, {'ion': 1460, 'force': [-0.2340734601020813, -0.20685462653636932, -1.8937872648239136], 'magnitude': 1.919377326965332, 'distance': 13.151910781860352, 'cosine_with_motion': -0.43744489784368085, 'motion_component': -0.8396218303850214}]}, 3216: {'frame': 3216, 'ionic_force': [-1.1128128170967102, -0.3707253783941269, -5.447134375572205], 'ionic_force_magnitude': 5.571989104226656, 'motion_vector': [-0.07701492309570312, 0.34079742431640625, -0.7521133422851562], 'cosine_ionic_motion': 0.8778023359725989, 'ionic_motion_component': 4.891105051704027, 'ionic_force_x': -1.1128128170967102, 'ionic_force_y': -0.3707253783941269, 'ionic_force_z': -5.447134375572205, 'radial_force': 1.172940608931324, 'axial_force': -5.447134375572205, 'contributions': [{'ion': 1313, 'force': [-0.8524911999702454, -0.24588410556316376, -3.6285605430603027], 'magnitude': 3.7354586124420166, 'distance': 9.427511215209961, 'cosine_with_motion': 0.8751090106105364, 'motion_component': 3.268933585247774}, {'ion': 1460, 'force': [-0.26032161712646484, -0.124</t>
+          <t>{3185: {'frame': 3185, 'ionic_force': [1.3455531299114227, -1.2103240936994553, -9.767556190490723], 'ionic_force_magnitude': 9.93380851293186, 'motion_vector': [3.3021926879882812, 1.7625465393066406, 0.34154510498046875], 'cosine_ionic_motion': -0.027479692611883776, 'ionic_motion_component': -0.27297800440068176, 'ionic_force_x': 1.3455531299114227, 'ionic_force_y': -1.2103240936994553, 'ionic_force_z': -9.767556190490723, 'radial_force': 1.8098059667278792, 'axial_force': -9.767556190490723, 'before_closest_residue': None, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [1.0481852293014526, -0.9845649600028992, -6.827840805053711], 'magnitude': 6.9776411056518555, 'distance': 6.8978657722473145, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.023108002613043896, 'motion_component': -0.1612393407807282}, {'ion': 1460, 'force': [0.2973679006099701, -0.2257591336965561, -2.9397153854370117], 'magnitude': 2.963329553604126, 'distance': 10.584712982177734, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.03770713874789775, 'motion_component': -0.11173867455445306}]}, 3186: {'frame': 3186, 'ionic_force': [3.8716278672218323, 0.9531629383563995, -6.351068735122681], 'ionic_force_magnitude': 7.498939658882293, 'motion_vector': [-1.120147705078125, -0.510986328125, 0.8818283081054688], 'cosine_ionic_motion': -0.917921914123857, 'ionic_motion_component': -6.883441045580538, 'ionic_force_x': 3.8716278672218323, 'ionic_force_y': 0.9531629383563995, 'ionic_force_z': -6.351068735122681, 'radial_force': 3.987232364598893, 'axial_force': -6.351068735122681, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [2.8922908306121826, 0.682626485824585, -4.142235279083252], 'magnitude': 5.0979838371276855, 'distance': 8.069931030273438, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9379406452351742, 'motion_component': -4.781606164194734}, {'ion': 1460, 'force': [0.9793370366096497, 0.2705364525318146, -2.2088334560394287], 'magnitude': 2.4313035011291504, 'distance': 11.685558319091797, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8644888675281329, 'motion_component': -2.101834725921859}]}, 3187: {'frame': 3187, 'ionic_force': [4.825020015239716, 1.0010420382022858, -9.05678677558899], 'ionic_force_magnitude': 10.31059115706736, 'motion_vector': [-4.467868804931641, 3.94091796875, -0.4804229736328125], 'cosine_ionic_motion': -0.2151940520558242, 'ionic_motion_component': -2.218777890180274, 'ionic_force_x': 4.825020015239716, 'ionic_force_y': 1.0010420382022858, 'ionic_force_z': -9.05678677558899, 'radial_force': 4.927768593360696, 'axial_force': -9.05678677558899, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 130, 'contributions': [{'ion': 1313, 'force': [3.834963321685791, 0.7111164927482605, -6.247584819793701], 'magnitude': 7.365116596221924, 'distance': 6.713967323303223, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.257383167032912, 'motion_component': -1.8956571041124768}, {'ion': 1460, 'force': [0.9900566935539246, 0.28992554545402527, -2.809201955795288], 'magnitude': 2.992638349533081, 'distance': 10.532752990722656, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.1079719114881787, 'motion_component': -0.32312089049107406}]}, 3188: {'frame': 3188, 'ionic_force': [-0.7788635641336441, 4.744892954826355, -7.823496103286743], 'ionic_force_magnitude': 9.183013061214636, 'motion_vector': [2.9478530883789062, -1.2035942077636719, 0.8451919555664062], 'cosine_ionic_motion': -0.48324645421477935, 'ionic_motion_component': -4.437658500839979, 'ionic_force_x': -0.7788635641336441, 'ionic_force_y': 4.744892954826355, 'ionic_force_z': -7.823496103286743, 'radial_force': 4.808392413717472, 'axial_force': -7.823496103286743, 'before_closest_residue': 455, 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [-0.5623465180397034, 3.5319478511810303, -5.200526714324951], 'magnitude': 6.311605930328369, 'distance': 7.252689838409424, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.49556723884648435, 'motion_component': -3.127825041783648}, {'ion': 1460, 'force': [-0.21651704609394073, 1.2129451036453247, -2.622969388961792], 'magnitude': 2.897944688796997, 'distance': 10.703454971313477, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.45198706097319374, 'motion_component': -1.3098335379862371}]}, 3189: {'frame': 3189, 'ionic_force': [2.2279635965824127, 3.7496649622917175, -8.675254344940186], 'ionic_force_magnitude': 9.70998697561115, 'motion_vector': [2.050933837890625, -1.666748046875, -0.683929443359375], 'cosine_ionic_motion': 0.16044574791098273, 'ionic_motion_component': 1.5579261225078322, 'ionic_force_x': 2.2279635965824127, 'ionic_force_y': 3.7496649622917175, 'ionic_force_z': -8.675254344940186, 'radial_force': 4.361629181525475, 'axial_force': -8.675254344940186, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [1.8297994136810303, 3.0413978099823, -6.2925825119018555], 'magnitude': 7.2246012687683105, 'distance': 6.778944969177246, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.15146603579443732, 'motion_component': 1.0942816903629335}, {'ion': 1460, 'force': [0.39816418290138245, 0.7082671523094177, -2.38267183303833], 'magnitude': 2.517399787902832, 'distance': 11.483993530273438, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.1841759707827572, 'motion_component': 0.4636445661517268}]}, 3190: {'frame': 3190, 'ionic_force': [3.4962931871414185, 1.3681584894657135, -6.685306072235107], 'ionic_force_magnitude': 7.667414230509018, 'motion_vector': [-0.8215522766113281, -0.8835487365722656, -0.6362762451171875], 'cosine_ionic_motion': 0.016492182069415995, 'ionic_motion_component': 0.12645239149118587, 'ionic_force_x': 3.4962931871414185, 'ionic_force_y': 1.3681584894657135, 'ionic_force_z': -6.685306072235107, 'radial_force': 3.7544538487972656, 'axial_force': -6.685306072235107, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [2.741168975830078, 1.0629887580871582, -4.5104899406433105], 'magnitude': 5.38409423828125, 'distance': 7.852586269378662, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.04375086242833566, 'motion_component': -0.23555877116258728}, {'ion': 1460, 'force': [0.7551242113113403, 0.3051697313785553, -2.174816131591797], 'magnitude': 2.3223190307617188, 'distance': 11.956610679626465, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.15588340078660728, 'motion_component': 0.36201101054708035}]}, 3191: {'frame': 3191, 'ionic_force': [3.8587116599082947, 0.6158474087715149, -7.850509166717529], 'ionic_force_magnitude': 8.769231316479157, 'motion_vector': [1.4482460021972656, 0.2650604248046875, 0.5260162353515625], 'cosine_ionic_motion': 0.11831350931893483, 'ionic_motion_component': 1.037518531082152, 'ionic_force_x': 3.8587116599082947, 'ionic_force_y': 0.6158474087715149, 'ionic_force_z': -7.850509166717529, 'radial_force': 3.9075470189369206, 'axial_force': -7.850509166717529, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [2.9662954807281494, 0.4142634868621826, -5.240616798400879], 'magnitude': 6.036106586456299, 'distance': 7.416356086730957, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.17474385144598134, 'motion_component': 1.0547725824270096}, {'ion': 1460, 'force': [0.8924161791801453, 0.20158392190933228, -2.6098923683166504], 'magnitude': 2.7656068801879883, 'distance': 10.956549644470215, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.006238752915845556, 'motion_component': -0.01725393739331782}]}, 3192: {'frame': 3192, 'ionic_force': [4.3233126401901245, 0.8234727382659912, -6.483328104019165], 'ionic_force_magnitude': 7.835986398652038, 'motion_vector': [-1.4279060363769531, -0.3152008056640625, 0.24273681640625], 'cosine_ionic_motion': -0.6893186884874044, 'ionic_motion_component': -5.401491867323962, 'ionic_force_x': 4.3233126401901245, 'ionic_force_y': 0.8234727382659912, 'ionic_force_z': -6.483328104019165, 'radial_force': 4.401038461033372, 'axial_force': -6.483328104019165, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [3.2284295558929443, 0.5756868124008179, -4.195573329925537], 'magnitude': 5.325129985809326, 'distance': 7.895941734313965, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7360294220437638, 'motion_component': -3.919452270043964}, {'ion': 1460, 'force': [1.0948830842971802, 0.24778592586517334, -2.287754774093628], 'magnitude': 2.548330545425415, 'distance': 11.41408634185791, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5815727327514694, 'motion_component': -1.4820395787670382}]}, 3193: {'frame': 3193, 'ionic_force': [4.54551488161087, 0.7150068581104279, -9.185447692871094], 'ionic_force_magnitude': 10.273528588783979, 'motion_vector': [-1.265380859375, 0.5024642944335938, 1.421234130859375], 'cosine_ionic_motion': -0.9123378360158684, 'ionic_motion_component': -9.372928840938334, 'ionic_force_x': 4.54551488161087, 'ionic_force_y': 0.7150068581104279, 'ionic_force_z': -9.185447692871094, 'radial_force': 4.6014063443789475, 'axial_force': -9.185447692871094, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [3.558159112930298, 0.47408899664878845, -6.336966037750244], 'magnitude': 7.283020973205566, 'distance': 6.751701831817627, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9258083810288427, 'motion_component': -6.74268190178226}, {'ion': 1460, 'force': [0.9873557686805725, 0.2409178614616394, -2.8484816551208496], 'magnitude': 3.0243611335754395, 'distance': 10.477368354797363, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8696867439300969, 'motion_component': -2.630246830321605}]}, 3194: {'frame': 3194, 'ionic_force': [7.131795823574066, 3.0327844619750977, -18.466155529022217], 'ionic_force_magnitude': 20.026462325732517, 'motion_vector': [1.2636222839355469, 1.3273963928222656, -1.654449462890625], 'cosine_ionic_motion': 0.8815604678031085, 'ionic_motion_component': 17.654537496314084, 'ionic_force_x': 7.131795823574066, 'ionic_force_y': 3.0327844619750977, 'ionic_force_z': -18.466155529022217, 'radial_force': 7.749857628495254, 'axial_force': -18.466155529022217, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [5.728073596954346, 2.3258800506591797, -12.010092735290527], 'magnitude': 13.507882118225098, 'distance': 4.957644939422607, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9053912250945034, 'motion_component': 12.229917716004195}, {'ion': 1387, 'force': [0.3024868369102478, 0.18391072750091553, -1.7984228134155273], 'magnitude': 1.832933783531189, 'distance': 13.45846939086914, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7958791628889741, 'motion_component': 1.4587937625408287}, {'ion': 1460, 'force': [1.1012353897094727, 0.5229936838150024, -4.657639980316162], 'magnitude': 4.814545631408691, 'distance': 8.3040771484375, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8237175571334348, 'motion_component': 3.965825965203912}]}, 3195: {'frame': 3195, 'ionic_force': [4.266230762004852, 2.5804542303085327, -8.203031539916992], 'ionic_force_magnitude': 9.599437243623537, 'motion_vector': [-2.6438636779785156, 0.3204536437988281, -0.75738525390625], 'cosine_ionic_motion': -0.15950752621456848, 'ionic_motion_component': -1.5311824877823865, 'ionic_force_x': 4.266230762004852, 'ionic_force_y': 2.5804542303085327, 'ionic_force_z': -8.203031539916992, 'radial_force': 4.985927090260517, 'axial_force': -8.203031539916992, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 130, 'contributions': [{'ion': 1313, 'force': [3.318345785140991, 1.9544174671173096, -5.576297760009766], 'magnitude': 6.776891708374023, 'distance': 6.99928617477417, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.20910020006651614, 'motion_component': -1.4170494408500325}, {'ion': 1460, 'force': [0.9478849768638611, 0.6260367631912231, -2.6267337799072266], 'magnitude': 2.8618416786193848, 'distance': 10.770756721496582, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.039881000971897285, 'motion_component': -0.11413311435657825}]}, 3196: {'frame': 3196, 'ionic_force': [0.6016596853733063, 2.649301290512085, -8.311489343643188], 'ionic_force_magnitude': 8.744235061708187, 'motion_vector': [2.318988800048828, -2.4310836791992188, 0.22534942626953125], 'cosine_ionic_motion': -0.2349655890604089, 'ionic_motion_component': -2.0545943421569453, 'ionic_force_x': 0.6016596853733063, 'ionic_force_y': 2.649301290512085, 'ionic_force_z': -8.311489343643188, 'radial_force': 2.716761252836271, 'axial_force': -8.311489343643188, 'before_closest_residue': 455, 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [0.49341556429862976, 2.0448687076568604, -5.6436381340026855], 'magnitude': 6.022922515869141, 'distance': 7.424468994140625, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.25140903765843836, 'motion_component': -1.5142172100840625}, {'ion': 1460, 'force': [0.10824412107467651, 0.6044325828552246, -2.667851209640503], 'magnitude': 2.7376058101654053, 'distance': 11.01244068145752, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.19739042068930143, 'motion_component': -0.5403771640603434}]}, 3197: {'frame': 3197, 'ionic_force': [2.8209893107414246, 0.17508456483483315, -8.191557884216309], 'ionic_force_magnitude': 8.665463395954491, 'motion_vector': [-2.359294891357422, 1.4584197998046875, 2.7145614624023438], 'cosine_ionic_motion': -0.8515068024527294, 'ionic_motion_component': -7.378701028060378, 'ionic_force_x': 2.8209893107414246, 'ionic_force_y': 0.17508456483483315, 'ionic_force_z': -8.191557884216309, 'radial_force': 2.8264173959556613, 'axial_force': -8.191557884216309, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1313, 'force': [2.2362687587738037, 0.05940436199307442, -5.672110557556152], 'magnitude': 6.097315788269043, 'distance': 7.379036903381348, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8699706879091497, 'motion_component': -5.304486381330342}, {'ion': 1460, 'force': [0.5847205519676208, 0.11568020284175873, -2.5194473266601562], 'magnitude': 2.5889949798583984, 'distance': 11.32409381866455, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8011659975708844, 'motion_component': -2.074214723975322}]}, 3198: {'frame': 3198, 'ionic_force': [4.809750139713287, 10.997350573539734, -26.898103833198547], 'ionic_force_magnitude': 29.45476881364607, 'motion_vector': [0.19825363159179688, 0.10056686401367188, -2.5326690673828125], 'cosine_ionic_motion': 0.9372048718855969, 'ionic_motion_component': 27.605152832413037, 'ionic_force_x': 4.809750139713287, 'ionic_force_y': 10.997350573539734, 'ionic_force_z': -26.898103833198547, 'radial_force': 12.003141923838388, 'axial_force': -26.898103833198547, 'before_closest_residue': 455, 'closest_residue': 'SF', 'next_closest_residue': 455, 'contributions': [{'ion': 1313, 'force': [3.9049830436706543, 9.421380996704102, -19.212223052978516], 'magnitude': 21.751340866088867, 'distance': 3.906843662261963, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9110158763380631, 'motion_component': 19.815816810828306}, {'ion': 1387, 'force': [0.15719091892242432, 0.2684478759765625, -1.947790265083313], 'magnitude': 1.9724756479263306, 'distance': 12.973681449890137, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.995300771002789, 'motion_component': 1.9632065286741396}, {'ion': 1460, 'force': [0.7475761771202087, 1.3075217008590698, -5.738090515136719], 'magnitude': 5.932466983795166, 'distance': 7.4808573722839355, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9820752260428413, 'motion_component': 5.8261289687319895}]}, 3199: {'frame': 3199, 'ionic_force': [0.9833395779132843, 3.1130231618881226, -10.068522930145264], 'ionic_force_magnitude': 10.58456536315042, 'motion_vector': [-0.02933502197265625, -3.176746368408203, 1.2943191528320312], 'cosine_ionic_motion': -0.6320647076797856, 'ionic_motion_component': -6.6901302121772535, 'ionic_force_x': 0.9833395779132843, 'ionic_force_y': 3.1130231618881226, 'ionic_force_z': -10.068522930145264, 'radial_force': 3.264639326471241, 'axial_force': -10.068522930145264, 'before_closest_residue': 'SF', 'closest_residue': 455, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [0.8440772891044617, 2.4483911991119385, -7.0417280197143555], 'magnitude': 7.502867221832275, 'distance': 6.652048587799072, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6572728715675435, 'motion_component': -4.931431210428519}, {'ion': 1460, 'force': [0.13926228880882263, 0.6646319627761841, -3.026794910430908], 'magnitude': 3.102034330368042, 'distance': 10.345362663269043, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5669501891312683, 'motion_component': -1.7586989570614022}]}, 3200: {'frame': 3200, 'ionic_force': [1.5398932620882988, -3.925731360912323, -14.942134141921997], 'ionic_force_magnitude': 15.525785348634267, 'motion_vector': [-0.7101936340332031, -1.3734970092773438, -0.6399917602539062], 'cosine_ionic_motion': 0.5334978917055188, 'ionic_motion_component': 8.282973750568814, 'ionic_force_x': 1.5398932620882988, 'ionic_force_y': -3.925731360912323, 'ionic_force_z': -14.942134141921997, 'radial_force': 4.21694652286171, 'axial_force': -14.942134141921997, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [1.2463655471801758, -3.3982043266296387, -10.489591598510742], 'magnitude': 11.096519470214844, 'distance': 5.469852924346924, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5652003166871671, 'motion_component': 6.2717565039260705}, {'ion': 1387, 'force': [0.09594348818063736, -0.13932183384895325, -1.5808546543121338], 'magnitude': 1.5898796319961548, 'distance': 14.450634956359863, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4265788497944352, 'motion_component': 0.6782090140143298}, {'ion': 1460, 'force': [0.19758422672748566, -0.3882052004337311, -2.871687889099121], 'magnitude': 2.9045369625091553, 'distance': 10.691302299499512, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.45894008835435396, 'motion_component': 1.3330083846379597}]}, 3201: {'frame': 3201, 'ionic_force': [0.3855626368895173, -4.750433802604675, -10.51581072807312], 'ionic_force_magnitude': 11.54545603813691, 'motion_vector': [-0.7017936706542969, -0.01294708251953125, -0.8671646118164062], 'cosine_ionic_motion': 0.6917273308343146, 'ionic_motion_component': 7.986307488525365, 'ionic_force_x': 0.3855626368895173, 'ionic_force_y': -4.750433802604675, 'ionic_force_z': -10.51581072807312, 'radial_force': 4.766054957708137, 'axial_force': -10.51581072807312, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [0.3916058838367462, -3.7393531799316406, -7.343410015106201], 'magnitude': 8.249957084655762, 'distance': 6.343708038330078, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6672680685827019, 'motion_component': 5.504932773013024}, {'ion': 1460, 'force': [-0.0060432469472289085, -1.0110806226730347, -3.172400712966919], 'magnitude': 3.3296315670013428, 'distance': 9.985526084899902, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.74524006733559, 'motion_component': 2.4813749044541478}]}, 3202: {'frame': 3202, 'ionic_force': [-0.8432059288024902, -2.719889461994171, -7.3930346965789795], 'ionic_force_magnitude': 7.9224842662295805, 'motion_vector': [-0.6875076293945312, -0.4496726989746094, -0.5331268310546875], 'cosine_ionic_motion': 0.7403493413536228, 'ionic_motion_component': 5.8654060083875095, 'ionic_force_x': -0.8432059288024902, 'ionic_force_y': -2.719889461994171, 'ionic_force_z': -7.3930346965789795, 'radial_force': 2.8475945855817697, 'axial_force': -7.3930346965789795, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [-0.6528485417366028, -2.2744596004486084, -5.246335506439209], 'magnitude': 5.755294322967529, 'distance': 7.595130920410156, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7573262503904421, 'motion_component': 4.358635548107902}, {'ion': 1460, 'force': [-0.19035738706588745, -0.44542986154556274, -2.1466991901397705], 'magnitude': 2.2006728649139404, 'distance': 12.282628059387207, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6846863323502752, 'motion_component': 1.5067706405058947}]}, 3203: {'frame': 3203, 'ionic_force': [-0.9554902762174606, -3.667130023241043, -8.258195757865906], 'ionic_force_magnitude': 9.086176393320592, 'motion_vector': [-1.41168212890625, -0.13762283325195312, 1.837890625], 'cosine_ionic_motion': -0.6316526643237212, 'ionic_motion_component': -5.739307527356252, 'ionic_force_x': -0.9554902762174606, 'ionic_force_y': -3.667130023241043, 'ionic_force_z': -8.258195757865906, 'radial_force': 3.7895651828807444, 'axial_force': -8.258195757865906, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 1105, 'contributions': [{'ion': 1313, 'force': [-0.582251787185669, -2.546912908554077, -4.254993915557861], 'magnitude': 4.993070602416992, 'distance': 8.154272079467773, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5734918508861262, 'motion_component': -2.863485398333836}, {'ion': 1387, 'force': [-0.14848487079143524, -0.3223477303981781, -1.5331422090530396], 'magnitude': 1.5736838579177856, 'distance': 14.52480411529541, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7017500765273089, 'motion_component': -1.1043327598431159}, {'ion': 1460, 'force': [-0.22475361824035645, -0.7978693842887878, -2.470059633255005], 'magnitude': 2.6054375171661377, 'distance': 11.288304328918457, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6799200535321163, 'motion_component': -1.7714891742978691}]}, 3204: {'frame': 3204, 'ionic_force': [-4.891388177871704, -6.8576348423957825, -12.308661103248596], 'ionic_force_magnitude': 14.914957998361531, 'motion_vector': [2.0974998474121094, 3.643840789794922, -4.29998779296875], 'cosine_ionic_motion': 0.19709987365095533, 'ionic_motion_component': 2.9397363369863636, 'ionic_force_x': -4.891388177871704, 'ionic_force_y': -6.8576348423957825, 'ionic_force_z': -12.308661103248596, 'radial_force': 8.423350517357312, 'axial_force': -12.308661103248596, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 130, 'contributions': [{'ion': 1313, 'force': [-3.5466692447662354, -5.008401393890381, -7.102478504180908], 'magnitude': 9.386594772338867, 'distance': 5.947234153747559, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.0859452850752351, 'motion_component': 0.8067335028722198}, {'ion': 1387, 'force': [-0.37983453273773193, -0.5484148859977722, -1.9710179567337036], 'magnitude': 2.0808520317077637, 'distance': 12.631312370300293, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.45391548181313884, 'motion_component': 0.9445309271792581}, {'ion': 1460, 'force': [-0.9648844003677368, -1.3008185625076294, -3.2351646423339844], 'magnitude': 3.6179304122924805, 'distance': 9.579413414001465, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.32849483507551613, 'motion_component': 1.1884714828583895}]}, 3205: {'frame': 3205, 'ionic_force': [-0.6016021221876144, 0.16618561744689941, -6.180601716041565], 'ionic_force_magnitude': 6.21203512105355, 'motion_vector': [-2.4292831420898438, -0.1877899169921875, 1.3914337158203125], 'cosine_ionic_motion': -0.41133902842181963, 'ionic_motion_component': -2.555252491216388, 'ionic_force_x': -0.6016021221876144, 'ionic_force_y': 0.16618561744689941, 'ionic_force_z': -6.180601716041565, 'radial_force': 0.6241336177989842, 'axial_force': -6.180601716041565, 'before_closest_residue': 1105, 'closest_residue': 130, 'next_closest_residue': 1105, 'contributions': [{'ion': 1313, 'force': [-0.47208482027053833, 0.13534782826900482, -4.1929497718811035], 'magnitude': 4.221612453460693, 'distance': 8.868085861206055, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.39786613493239775, 'motion_component': -1.679636592081345}, {'ion': 1460, 'force': [-0.1295173019170761, 0.030837789177894592, -1.9876519441604614], 'magnitude': 1.9921059608459473, 'distance': 12.909601211547852, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.43954280105675997, 'motion_component': -0.8756158111541572}]}, 3206: {'frame': 3206, 'ionic_force': [-2.3814292550086975, -0.07051205262541771, -6.440298318862915], 'ionic_force_magnitude': 6.866849327175107, 'motion_vector': [4.136890411376953, -0.5502357482910156, -0.2530059814453125], 'cosine_ionic_motion': -0.2850374206019799, 'ionic_motion_component': -1.9573090198804335, 'ionic_force_x': -2.3814292550086975, 'ionic_force_y': -0.07051205262541771, 'ionic_force_z': -6.440298318862915, 'radial_force': 2.3824729266408737, 'axial_force': -6.440298318862915, 'before_closest_residue': 130, 'closest_residue': 1105, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [-1.8158272504806519, -0.09443157911300659, -4.377440452575684], 'magnitude': 4.740056037902832, 'distance': 8.369071960449219, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3205352276549729, 'motion_component': -1.5193549276856588}, {'ion': 1460, 'force': [-0.5656020045280457, 0.023919526487588882, -2.0628578662872314], 'magnitude': 2.1391260623931885, 'distance': 12.458072662353516, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.20473505796635882, 'motion_component': -0.4379541001504612}]}, 3207: {'frame': 3207, 'ionic_force': [0.5504616945981979, -0.20011846721172333, -6.7197370529174805], 'ionic_force_magnitude': 6.7452147140392205, 'motion_vector': [-0.4560203552246094, -0.9889564514160156, 2.2855987548828125], 'cosine_ionic_motion': -0.9024609612745147, 'ionic_motion_component': -6.087292954834836, 'ionic_force_x': 0.5504616945981979, 'ionic_force_y': -0.20011846721172333, 'ionic_force_z': -6.7197370529174805, 'radial_force': 0.5857093802724089, 'axial_force': -6.7197370529174805, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [0.4108598530292511, -0.13039463758468628, -4.540388107299805], 'magnitude': 4.5608038902282715, 'distance': 8.531950950622559, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9037776946529549, 'motion_component': -4.1219528871178355}, {'ion': 1460, 'force': [0.13960184156894684, -0.06972382962703705, -2.179348945617676], 'magnitude': 2.1849284172058105, 'distance': 12.326803207397461, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8994986514893245, 'motion_component': -1.9653401082788329}]}, 3208: {'frame': 3208, 'ionic_force': [0.6337229162454605, -2.9306737780570984, -10.785738706588745], 'ionic_force_magnitude': 11.194758281212362, 'motion_vector': [0.30518341064453125, 1.3927268981933594, -1.3763351440429688], 'cosine_ionic_motion': 0.49388111416975305, 'ionic_motion_component': 5.528879692786231, 'ionic_force_x': 0.6337229162454605, 'ionic_force_y': -2.9306737780570984, 'ionic_force_z': -10.785738706588745, 'radial_force': 2.998408499181877, 'axial_force': -10.785738706588745, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1313, 'force': [0.44283202290534973, -2.438164234161377, -7.620040416717529], 'magnitude': 8.012849807739258, 'distance': 6.436882019042969, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.45513940674212605, 'motion_component': 3.6469636778250076}, {'ion': 1460, 'force': [0.19089089334011078, -0.49250954389572144, -3.165698289871216], 'magnitude': 3.2094626426696777, 'distance': 10.170747756958008, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5863647716762116, 'motion_component': 1.8819158471922193}]}, 3209: {'frame': 3209, 'ionic_force': [0.43650949746370316, -0.5205679461359978, -6.388556241989136], 'ionic_force_magnitude': 6.424576436231311, 'motion_vector': [-2.8515777587890625, -0.7392349243164062, -1.9197006225585938], 'cosine_ionic_motion': 0.5048408404249863, 'ionic_motion_component': 3.2433885674415786, 'ionic_force_x': 0.43650949746370316, 'ionic_force_y': -0.5205679461359978, 'ionic_force_z': -6.388556241989136, 'radial_force': 0.6793611174627716, 'axial_force': -6.388556241989136, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 1105, 'contributions': [{'ion': 1313, 'force': [0.33712059259414673, -0.4496636390686035, -4.658642292022705], 'magnitude': 4.692419052124023, 'distance': 8.411445617675781, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5039206562836169, 'motion_component': 2.3646068414033508}, {'ion': 1460, 'force': [0.09938890486955643, -0.07090430706739426, -1.7299139499664307], 'magnitude': 1.7342168092727661, 'distance': 13.836216926574707, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5067312342068669, 'motion_component': 0.8787818106888905}]}, 3210: {'frame': 3210, 'ionic_force': [-1.0865365266799927, -0.441194579005</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{3320: {'frame': 3320, 'ionic_force': [4.8733450174331665, 3.184350647032261, -8.640591382980347], 'ionic_force_magnitude': 10.418704341223512, 'motion_vector': [-0.18167495727539062, 0.760711669921875, 0.7443389892578125], 'cosine_ionic_motion': -0.4351086894470255, 'ionic_motion_component': -4.533268791645797, 'ionic_force_x': 4.8733450174331665, 'ionic_force_y': 3.184350647032261, 'ionic_force_z': -8.640591382980347, 'radial_force': 5.821475818226461, 'axial_force': -8.640591382980347, 'contributions': [{'ion': 1387, 'force': [0.3318135738372803, -0.0069795772433280945, -1.9514002799987793], 'magnitude': 1.9794220924377441, 'distance': 12.950896263122559, 'cosine_with_motion': -0.7103326722280674, 'motion_component': -1.4060482193826478}, {'ion': 1460, 'force': [1.624815821647644, -0.2846843898296356, -5.312528133392334], 'magnitude': 5.562735557556152, 'distance': 7.725468635559082, 'cosine_with_motion': -0.7435987748913293, 'motion_component': -4.1364433416914}, {'ion': 2433, 'force': [2.916715621948242, 3.4760146141052246, -1.3766629695892334], 'magnitude': 4.741846561431885, 'distance': 8.367491722106934, 'cosine_with_motion': 0.21283327257076928, 'motion_component': 1.0092227157837357}]}, 3321: {'frame': 3321, 'ionic_force': [4.962071061134338, 4.828094765543938, -10.522126078605652], 'ionic_force_magnitude': 12.595546256311902, 'motion_vector': [3.44659423828125, 0.5642127990722656, -0.29720306396484375], 'cosine_ionic_motion': 0.5199156061735278, 'ionic_motion_component': 6.548621066937112, 'ionic_force_x': 4.962071061134338, 'ionic_force_y': 4.828094765543938, 'ionic_force_z': -10.522126078605652, 'radial_force': 6.9233408323452945, 'axial_force': -10.522126078605652, 'contributions': [{'ion': 1387, 'force': [0.4181758165359497, 0.16234956681728363, -2.319929599761963], 'magnitude': 2.362901210784912, 'distance': 11.853490829467773, 'cosine_with_motion': 0.26833152479280165, 'motion_component': 0.6340408627544847}, {'ion': 1460, 'force': [2.362652540206909, 0.5963982939720154, -7.155970096588135], 'magnitude': 7.559479236602783, 'distance': 6.62709379196167, 'cosine_with_motion': 0.40029079586086974, 'motion_component': 3.0259899505259265}, {'ion': 2433, 'force': [2.1812427043914795, 4.069346904754639, -1.0462263822555542], 'magnitude': 4.734130859375, 'distance': 8.374307632446289, 'cosine_with_motion': 0.6101627710360925, 'motion_component': 2.8885903144106857}]}, 3322: {'frame': 3322, 'ionic_force': [5.101867258548737, 2.400673806667328, -5.333805024623871], 'ionic_force_magnitude': 7.761556563639349, 'motion_vector': [-1.1910209655761719, 1.1273345947265625, 1.091339111328125], 'cosine_ionic_motion': -0.6011411421058467, 'ionic_motion_component': -4.665790977185289, 'ionic_force_x': 5.101867258548737, 'ionic_force_y': 2.400673806667328, 'ionic_force_z': -5.333805024623871, 'radial_force': 5.638464706803635, 'axial_force': -5.333805024623871, 'contributions': [{'ion': 1387, 'force': [0.8166144490242004, 0.16744935512542725, -1.7120360136032104], 'magnitude': 1.904196858406067, 'distance': 13.204231262207031, 'cosine_with_motion': -0.7070687055580778, 'motion_component': -1.3463980228761798}, {'ion': 1460, 'force': [2.6996209621429443, 0.5092499852180481, -3.1144349575042725], 'magnitude': 4.152949810028076, 'distance': 8.941094398498535, 'cosine_with_motion': -0.7383261436332469, 'motion_component': -3.066231583865708}, {'ion': 2433, 'force': [1.5856318473815918, 1.7239744663238525, -0.5073340535163879], 'magnitude': 2.3966026306152344, 'distance': 11.769852638244629, 'cosine_with_motion': -0.10563347096891086, 'motion_component': -0.2531614541572438}]}, 3323: {'frame': 3323, 'ionic_force': [5.707005620002747, 4.04939991235733, -7.091884225606918], 'ionic_force_magnitude': 9.963050469929113, 'motion_vector': [-0.09119033813476562, -1.4596443176269531, 0.58355712890625], 'cosine_ionic_motion': -0.6737404389098686, 'ionic_motion_component': -6.712509996491213, 'ionic_force_x': 5.707005620002747, 'ionic_force_y': 4.04939991235733, 'ionic_force_z': -7.091884225606918, 'radial_force': 6.997681958830545, 'axial_force': -7.091884225606918, 'contributions': [{'ion': 1387, 'force': [0.8393199443817139, 0.3989105820655823, -2.18998122215271], 'magnitude': 2.3789925575256348, 'distance': 11.813334465026855, 'cosine_with_motion': -0.5170273796606956, 'motion_component': -1.2300042650106304}, {'ion': 1460, 'force': [3.4794766902923584, 1.5985596179962158, -4.6523637771606445], 'magnitude': 6.02549934387207, 'distance': 7.422881603240967, 'cosine_with_motion': -0.5655173853401619, 'motion_component': -3.4075245058578427}, {'ion': 2433, 'force': [1.3882089853286743, 2.0519297122955322, -0.24953922629356384], 'magnitude': 2.4899415969848633, 'distance': 11.547141075134277, 'cosine_with_motion': -0.8333453521952254, 'motion_component': -2.0749813240573336}]}, 3324: {'frame': 3324, 'ionic_force': [9.42669403553009, 3.5997143760323524, -10.327790841460228], 'ionic_force_magnitude': 14.438966988447003, 'motion_vector': [1.4581718444824219, 0.5040359497070312, -1.6050872802734375], 'cosine_ionic_motion': 0.9997192109901553, 'ionic_motion_component': 14.434912685203136, 'ionic_force_x': 9.42669403553009, 'ionic_force_y': 3.5997143760323524, 'ionic_force_z': -10.327790841460228, 'radial_force': 10.090614650679738, 'axial_force': -10.327790841460228, 'contributions': [{'ion': 1316, 'force': [0.5152910947799683, 0.09902171045541763, -1.5304564237594604], 'magnitude': 1.617908239364624, 'distance': 14.32491683959961, 'cosine_with_motion': 0.9044381588025899, 'motion_component': 1.4632979506664054}, {'ion': 1387, 'force': [1.6848300695419312, 0.3395357131958008, -3.116074562072754], 'magnitude': 3.558631420135498, 'distance': 9.658897399902344, 'cosine_with_motion': 0.9629840296835332, 'motion_component': 3.4269052191387033}, {'ion': 1460, 'force': [5.295093536376953, 0.8498631119728088, -5.482320308685303], 'magnitude': 7.6691670417785645, 'distance': 6.579531192779541, 'cosine_with_motion': 0.9926726186717297, 'motion_component': 7.612971853423932}, {'ion': 2433, 'force': [1.9314793348312378, 2.311293840408325, -0.19893954694271088], 'magnitude': 3.018653392791748, 'distance': 10.487269401550293, 'cosine_with_motion': 0.6399335650787177, 'motion_component': 1.9317376565473425}]}, 3325: {'frame': 3325, 'ionic_force': [6.025220155715942, 3.329250246286392, -5.533735513687134], 'ionic_force_magnitude': 8.832293805274247, 'motion_vector': [-1.0484428405761719, -1.0520210266113281, -0.158599853515625], 'cosine_ionic_motion': -0.6777865381816526, 'ionic_motion_component': -5.986409842480087, 'ionic_force_x': 6.025220155715942, 'ionic_force_y': 3.329250246286392, 'ionic_force_z': -5.533735513687134, 'radial_force': 6.883835059561178, 'axial_force': -5.533735513687134, 'contributions': [{'ion': 1387, 'force': [1.0765461921691895, 0.23434945940971375, -2.0206117630004883], 'magnitude': 2.3014655113220215, 'distance': 12.010658264160156, 'cosine_with_motion': -0.3068244551499629, 'motion_component': -0.7061458862244105}, {'ion': 1460, 'force': [2.5632970333099365, 0.5630773901939392, -3.0066704750061035], 'magnitude': 3.9909415245056152, 'distance': 9.120766639709473, 'cosine_with_motion': -0.47019937350483226, 'motion_component': -1.8765382588053043}, {'ion': 2433, 'force': [2.3853769302368164, 2.5318233966827393, -0.506453275680542], 'magnitude': 3.515202283859253, 'distance': 9.718379974365234, 'cosine_with_motion': -0.9682872249034437, 'motion_component': -3.403725551910478}]}, 3326: {'frame': 3326, 'ionic_force': [5.521149039268494, 2.2750196903944016, -6.492782413959503], 'ionic_force_magnitude': 8.821282490688043, 'motion_vector': [0.80645751953125, 0.5555877685546875, -0.410614013671875], 'cosine_ionic_motion': 0.8948647231467417, 'ionic_motion_component': 7.893854513828756, 'ionic_force_x': 5.521149039268494, 'ionic_force_y': 2.2750196903944016, 'ionic_force_z': -6.492782413959503, 'radial_force': 5.971499083605192, 'axial_force': -6.492782413959503, 'contributions': [{'ion': 1387, 'force': [0.7306075096130371, 0.05163702368736267, -1.8644970655441284], 'magnitude': 2.0031981468200684, 'distance': 12.873809814453125, 'cosine_with_motion': 0.6503710687869672, 'motion_component': 1.3028221533939597}, {'ion': 1460, 'force': [2.9076755046844482, 0.214521124958992, -4.017284393310547], 'magnitude': 4.963785648345947, 'distance': 8.178290367126465, 'cosine_with_motion': 0.7804168984028671, 'motion_component': 3.873822364127798}, {'ion': 2433, 'force': [1.8828660249710083, 2.008861541748047, -0.6110009551048279], 'magnitude': 2.820289134979248, 'distance': 10.849812507629395, 'cosine_with_motion': 0.9634508776201375, 'motion_component': 2.7172101317688018}]}, 3327: {'frame': 3327, 'ionic_force': [4.962403953075409, 2.0606805086135864, -5.490831732749939], 'ionic_force_magnitude': 7.682518484810309, 'motion_vector': [-0.40179443359375, 0.5124359130859375, 0.6054840087890625], 'cosine_ionic_motion': -0.6239824605969704, 'ionic_motion_component': -4.7937567877336456, 'ionic_force_x': 4.962403953075409, 'ionic_force_y': 2.0606805086135864, 'ionic_force_z': -5.490831732749939, 'radial_force': 5.373253870056615, 'axial_force': -5.490831732749939, 'contributions': [{'ion': 1387, 'force': [0.7123898863792419, 0.10276107490062714, -1.644201397895813], 'magnitude': 1.7948418855667114, 'distance': 13.600533485412598, 'cosine_with_motion': -0.7701518053219849, 'motion_component': -1.382300725170892}, {'ion': 1460, 'force': [2.544466972351074, 0.2279723435640335, -3.2194597721099854], 'magnitude': 4.109890937805176, 'distance': 8.987810134887695, 'cosine_with_motion': -0.7812058518484315, 'motion_component': -3.2106709714302584}, {'ion': 2433, 'force': [1.7055470943450928, 1.7299470901489258, -0.6271705627441406], 'magnitude': 2.508974075317383, 'distance': 11.503260612487793, 'cosine_with_motion': -0.0800267830802497, 'motion_component': -0.20078512136664983}]}, 3328: {'frame': 3328, 'ionic_force': [5.662827789783478, 2.698476254940033, -6.413617879152298], 'ionic_force_magnitude': 8.971281233748122, 'motion_vector': [-1.1094818115234375, 0.8973617553710938, 1.1634902954101562], 'cosine_ionic_motion': -0.6855367750310243, 'ionic_motion_component': -6.150143204880036, 'ionic_force_x': 5.662827789783478, 'ionic_force_y': 2.698476254940033, 'ionic_force_z': -6.413617879152298, 'radial_force': 6.272909426671105, 'axial_force': -6.413617879152298, 'contributions': [{'ion': 1387, 'force': [0.7809037566184998, 0.18411484360694885, -1.7854108810424805], 'magnitude': 1.9573965072631836, 'distance': 13.023557662963867, 'cosine_with_motion': -0.7709661628922033, 'motion_component': -1.5090864508773922}, {'ion': 1460, 'force': [3.093663454055786, 0.4853256046772003, -4.167239665985107], 'magnitude': 5.21269416809082, 'distance': 7.9806437492370605, 'cosine_with_motion': -0.8174437983446711, 'motion_component': -4.261084555910353}, {'ion': 2433, 'force': [1.788260579109192, 2.029035806655884, -0.4609673321247101], 'magnitude': 2.7436022758483887, 'distance': 11.000399589538574, 'cosine_with_motion': -0.1384938768402133, 'motion_component': -0.3799721065212349}]}, 3329: {'frame': 3329, 'ionic_force': [6.12342631816864, 5.340087965130806, -8.698342144489288], 'ionic_force_magnitude': 11.90269067950494, 'motion_vector': [0.8754844665527344, -1.0129776000976562, 0.6521530151367188], 'cosine_ionic_motion': -0.3227464606590609, 'ionic_motion_component': -3.8415512891298116, 'ionic_force_x': 6.12342631816864, 'ionic_force_y': 5.340087965130806, 'ionic_force_z': -8.698342144489288, 'radial_force': 8.12483165052515, 'axial_force': -8.698342144489288, 'contributions': [{'ion': 1316, 'force': [0.37819957733154297, 0.24994249641895294, -1.4104505777359009], 'magnitude': 1.4815117120742798, 'distance': 14.969817161560059, 'cosine_with_motion': -0.38158253503441575, 'motion_component': -0.5653190013484792}, {'ion': 1387, 'force': [0.9713860750198364, 0.7008095979690552, -2.4578428268432617], 'magnitude': 2.734175682067871, 'distance': 11.019346237182617, 'cosine_with_motion': -0.35913446296586105, 'motion_component': -0.9819366955576072}, {'ion': 1460, 'force': [3.2983713150024414, 2.064893960952759, -4.52915096282959], 'magnitude': 5.971285343170166, 'distance': 7.456501483917236, 'cosine_with_motion': -0.2426363541558891, 'motion_component': -1.4488509092765014}, {'ion': 2433, 'force': [1.4754693508148193, 2.324441909790039, -0.3008977770805359], 'magnitude': 2.7695810794830322, 'distance': 10.948685646057129, 'cosine_with_motion': -0.3052609156370647, 'motion_component': -0.8454448625147428}]}, 3330: {'frame': 3330, 'ionic_force': [8.562611877918243, 3.4708504751324654, -9.022035978734493], 'ionic_force_magnitude': 12.913646208339978, 'motion_vector': [1.0237197875976562, -1.2902107238769531, 0.8571853637695312], 'cosine_ionic_motion': -0.14371961245459278, 'ionic_motion_component': -1.8559442284383432, 'ionic_force_x': 8.562611877918243, 'ionic_force_y': 3.4708504751324654, 'ionic_force_z': -9.022035978734493, 'radial_force': 9.239324931649165, 'axial_force': -9.022035978734493, 'contributions': [{'ion': 1316, 'force': [0.5562570691108704, 0.11473546177148819, -1.4796452522277832], 'magnitude': 1.5849088430404663, 'distance': 14.47327709197998, 'cosine_with_motion': -0.28779764622325893, 'motion_component': -0.4561330512855037}, {'ion': 1387, 'force': [1.3070932626724243, 0.29501739144325256, -2.6750640869140625], 'magnitude': 2.9919052124023438, 'distance': 10.53404426574707, 'cosine_with_motion': -0.24041965554896735, 'motion_component': -0.7193127855523347}, {'ion': 1460, 'force': [4.905503273010254, 1.0822356939315796, -4.953392505645752], 'magnitude': 7.054877281188965, 'distance': 6.8600029945373535, 'cosine_with_motion': -0.04736466428845592, 'motion_component': -0.33415189509761234}, {'ion': 2433, 'force': [1.7937582731246948, 1.978861927986145, 0.0860658660531044], 'magnitude': 2.672240734100342, 'distance': 11.146313667297363, 'cosine_with_motion': -0.12960900139424755, 'motion_component': -0.3463464546020445}]}, 3331: {'frame': 3331, 'ionic_force': [12.735351324081421, 2.3743116538971663, -6.971976637840271], 'ionic_force_magnitude': 14.711729586156919, 'motion_vector': [-1.5520782470703125, 0.7276382446289062, -2.8383560180664062], 'cosine_ionic_motion': 0.035881050304702455, 'ionic_motion_component': 0.5278723093500758, 'ionic_force_x': 12.735351324081421, 'ionic_force_y': 2.3743116538971663, 'ionic_force_z': -6.971976637840271, 'radial_force': 12.954787886245544, 'axial_force': -6.971976637840271, 'contributions': [{'ion': 1316, 'force': [0.7236177921295166, -0.01991807110607624, -1.514197587966919], 'magnitude': 1.6783366203308105, 'distance': 14.064668655395508, 'cosine_with_motion': 0.5678690160279444, 'motion_component': 0.9530753588752279}, {'ion': 1387, 'force': [2.3421452045440674, -0.13869722187519073, -2.969356060028076], 'magnitude': 3.784435987472534, 'distance': 9.366308212280273, 'cosine_with_motion': 0.3739069185928592, 'motion_component': 1.4150268355639988}, {'ion': 1460, 'force': [6.530500888824463, -0.4096313416957855, -3.7830898761749268], 'magnitude': 7.558241367340088, 'distance': 6.627636432647705, 'cosine_with_motion': 0.01212381215447484, 'motion_component': 0.09163469545941672}, {'ion': 2433, 'force': [3.139087438583374, 2.9425582885742188, 1.2946668863296509], 'magnitude': 4.4931817054748535, 'distance': 8.595913887023926, 'cosine_with_motion': -0.42995467800748755, 'motion_component': -1.931864480817218}]}, 3332: {'frame': 3332, 'ionic_force': [5.920918166637421, 3.972064346075058, -6.426218777894974], 'ionic_force_magnitude': 9.598481905319595, 'motion_vector': [0.7343177795410156, 1.0062751770019531, 2.0959930419921875], 'cosine_ionic_motion': -0.21896350382145063, 'ionic_motion_component': -2.1017172293555717, 'ionic_force_x': 5.920918166637421, 'ionic_force_y': 3.972064346075058, 'ionic_force_z': -6.426218777894974, 'radial_force': 7.12983640102476, 'axial_force': -6.426218777894974, 'contributions': [{'ion': 1387, 'force': [0.6480094790458679, 0.07161861658096313, -1.956294298171997], 'magnitude': 2.06207013130188, 'distance': 12.688705444335938, 'cosine_with_motion': -0.7065626176169941, 'motion_component': -1.4569816124307788}, {'ion': 1460, 'force': [2.506962299346924, 0.3197813332080841, -4.0640716552734375], 'magnitude': 4.785791397094727, 'distance': 8.328987121582031, 'cosine_with_motion': -0.5446592892584318, 'motion_component': -2.606625695022325}, {'ion': 2433, 'force': [2.765946388244629, 3.5806643962860107, -0.4058528244495392], 'magnitude': 4.542723178863525, 'distance': 8.54891300201416, 'cosine_with_motion': 0.43187531744995167, 'motion_component': 1.9618899948423572}]}, 3333: {'frame': 3333, 'ionic_force': [11.138619840145111, 7.894609674811363, -10.194625984877348], 'ionic_force_magnitude': 17.038899988920527, 'motion_vector': [-0.58197021484375, -0.06623077392578125, -0.9650726318359375], 'cosine_ionic_motion': 0.1472983279094927, 'ionic_motion_component': 2.5098014777850675, 'ionic_force_x': 11.138619840145111, 'ionic_force_y': 7.894609674811363, 'ionic_force_z': -10.194625984877348, 'radial_force': 13.652608317127518, 'axial_force': -10.194625984877348, 'contributions': [{'ion': 1316, 'force': [0.6237956881523132, 0.15656648576259613, -1.627447485923767], 'magnitude': 1.7499197721481323, 'distance': 13.773996353149414, 'cosine_with_motion': 0.6060249544382219, 'motion_component': 1.06049509096636}, {'ion': 1387, 'force': [1.9665889739990234, 0.6323477029800415, -3.3439724445343018], 'magnitude': 3.9305837154388428, 'distance': 9.190528869628906, 'cosine_with_motion': 0.4599211400015446, 'motion_component': 1.8077584950588932}, {'ion': 1460, 'force': [5.7677435874938965, 2.1759836673736572, -5.206416130065918], 'magnitude': 8.068985939025879, 'distance': 6.414451599121094, 'cosine_with_motion': 0.16728169529424516, 'motion_component': 1.3497937077936975}, {'ion': 2433, 'force': [2.780491590499878, 4.929711818695068, -0.01678992435336113], 'magnitude': 5.659811973571777, 'distance': 7.658928871154785, 'cosine_with_motion': -0.30182028666503474, 'motion_component': -1.7082461370083915}]}, 3334: {'frame': 3334, 'ionic_force': [8.556934595108032, 6.820997595787048, -7.33417646586895], 'ionic_force_magnitude': 13.173355013025168, 'motion_vector': [0.17787933349609375, -0.084075927734375, 0.6251068115234375], 'cosine_ionic_motion': -0.42117706074107514, 'ionic_motion_component': -5.548314944484647, 'ionic_force_x': 8.556934595108032, 'ionic_force_y': 6.820997595787048, 'ionic_force_z': -7.33417646586895, 'radial_force': 10.942903539129336, 'axial_force': -7.33417646586895, 'contributions': [{'ion': 1387, 'force': [1.4384901523590088, 0.4807847738265991, -2.7401866912841797], 'magnitude': 3.131937265396118, 'distance': 10.295857429504395, 'cosine_with_motion': -0.7295832994848833, 'motion_component': -2.2850091222240625}, {'ion': 1460, 'force': [4.045209884643555, 1.0065531730651855, -4.721059799194336], 'magnitude': 6.298037528991699, 'distance': 7.260498046875, 'cosine_with_motion': -0.5611922266405833, 'motion_component': -3.534409758359267}, {'ion': 2433, 'force': [3.0732345581054688, 5.333659648895264, 0.12707002460956573], 'magnitude': 6.157015800476074, 'distance': 7.343175411224365, 'cosine_with_motion': 0.04403173563774378, 'motion_component': 0.2711040889088734}]}, 3335: {'frame': 3335, 'ionic_force': [10.957434237003326, 7.65510667860508, -10.461147874593735], 'ionic_force_magnitude': 16.973557027717963, 'motion_vector': [0.046604156494140625, 0.275848388671875, -0.0363616943359375], 'cosine_ionic_motion': 0.627074144131308, 'ionic_motion_component': 10.64367874602019, 'ionic_force_x': 10.957434237003326, 'ionic_force_y': 7.65510667860508, 'ionic_force_z': -10.461147874593735, 'radial_force': 13.366601038374593, 'axial_force': -10.461147874593735, 'contributions': [{'ion': 1316, 'force': [0.5002949833869934, 0.06886790692806244, -1.5100455284118652], 'magnitude': 1.5922547578811646, 'distance': 14.439852714538574, 'cosine_with_motion': 0.21643463805504745, 'motion_component': 0.344619091924816}, {'ion': 1387, 'force': [1.7298309803009033, 0.3097245991230011, -3.301562786102295], 'magnitude': 3.740128517150879, 'distance': 9.421624183654785, 'cosine_with_motion': 0.27115584312548485, 'motion_component': 1.0141577034043774}, {'ion': 1460, 'force': [5.743025779724121, 1.7341681718826294, -5.573688983917236], 'magnitude': 8.188754081726074, 'distance': 6.36737060546875, 'cosine_with_motion': 0.41066215110078985, 'motion_component': 3.3628113618595847}, {'ion': 2433, 'force': [2.9842824935913086, 5.542346000671387, -0.07585057616233826], 'magnitude': 6.295180320739746, 'distance': 7.262145519256592, 'cosine_with_motion': 0.9407340673341933, 'motion_component': 5.922090530346958}]}, 3336: {'frame': 3336, 'ionic_force': [9.11018654704094, 6.392471864819527, -9.55652368068695], 'ionic_force_magnitude': 14.669231074733448, 'motion_vector': [-4.241512298583984, -1.3926010131835938, -0.917877197265625], 'cosine_ionic_motion': -0.5799124377910689, 'ionic_motion_component': -8.506869553069176, 'ionic_force_x': 9.11018654704094, 'ionic_force_y': 6.392471864819527, 'ionic_force_z': -9.55652368068695, 'radial_force': 11.129204619576143, 'axial_force': -9.55652368068695, 'contributions': [{'ion': 1316, 'force': [0.46599122881889343, 0.17207498848438263, -1.45326566696167], 'magnitude': 1.5358186960220337, 'distance': 14.702767372131348, 'cosine_with_motion': -0.12603612829488975, 'motion_component': -0.19356862820591123}, {'ion': 1387, 'force': [1.0968544483184814, 0.3437471389770508, -2.457841634750366], 'magnitude': 2.7133443355560303, 'distance': 11.061565399169922, 'cosine_with_motion': -0.2324851428875588, 'motion_component': -0.6308122367540214}, {'ion': 1460, 'force': [5.049988269805908, 1.1790555715560913, -5.30512809753418], 'magnitude': 7.4186882972717285, 'distance': 6.6896820068359375, 'cosine_with_motion': -0.538038635350998, 'motion_component': -3.991540987216098}, {'ion': 2433, 'force': [2.4973526000976562, 4.697594165802002, -0.34028828144073486], 'magnitude': 5.3310370445251465, 'distance': 7.891565799713135, 'cosine_with_motion': -0.6923507626904895, 'motion_component': -3.6909476351492234}]}, 3337: {'frame': 3337, 'ionic_force': [-1.0386495990678668, 10.650418624281883, -13.788317680358887], 'ionic_force_magnitude': 17.45359316348905, 'motion_vector': [0.44036865234375, 2.80010986328125, -1.7934036254882812], 'cosine_ionic_motion': 0.9239821916649363, 'ionic_motion_component': 16.12680926362876, 'ionic_force_x': -1.0386495990678668, 'ionic_force_y': 10.650418624281883, 'ionic_force_z': -13.788317680358887, 'radial_force': 10.70094434440691, 'axial_force': -13.788317680358887, 'contributions': [{'ion': 1387, 'force': [-0.007922927848994732, 0.10124565660953522, -2.5693626403808594], 'magnitude': 2.571368932723999, 'distance': 11.362838745117188, 'cosine_with_motion': 0.5667177533058034, 'motion_component': 1.4572403853948068}, {'ion': 1460, 'force': [0.24486219882965088, 0.3454366624355316, -9.121464729309082], 'magnitude': 9.13128662109375, 'distance': 6.029801845550537, 'cosine_with_motion': 0.5691957685666009, 'motion_component': 5.197489938044287}, {'ion': 2433, 'force': [-1.275588870048523, 10.203736305236816, -2.0974903106689453], 'magnitude': 10.494894981384277, 'distance': 5.624449253082275, 'cosine_with_motion': 0.9025415453681213, 'motion_component': 9.472079013835085}]}, 3338: {'frame': 3338, 'ionic_force': [0.4838514244183898, 6.611688911914825, -7.909306526184082], 'ionic_force_magnitude': 10.320158535312686, 'motion_vector': [0.3501434326171875, -1.3354682922363281, -0.2438507080078125], 'cosine_ionic_motion': -0.4652546041033829, 'ionic_motion_component': -4.801501273631051, 'ionic_force_x': 0.4838514244183898, 'ionic_force_y': 6.611688911914825, 'ionic_force_z': -7.909306526184082, 'radial_force': 6.629369688654355, 'axial_force': -7.909306526184082, 'contributions': [{'ion': 1387, 'force': [0.04897297918796539, 0.46202152967453003, -1.8418389558792114], 'magnitude': 1.8995349407196045, 'distance': 13.22042465209961, 'cosine_with_motion': -0.056600802095017826, 'motion_component': -0.10751520117704749}, {'ion': 1460, 'force': [0.4208226501941681, 1.4192343950271606, -4.18621301651001], 'magnitude': 4.4402360916137695, 'distance': 8.647010803222656, 'cosine_with_motion': -0.1168145613509119, 'motion_component': -0.5186842424025317}, {'ion': 2433, 'force': [0.014055795036256313, 4.730432987213135, -1.8812545537948608], 'magnitude': 5.09080696105957, 'distance': 8.075617790222168, 'cosine_with_motion': -0.8201650955329496, 'motion_component': -4.175301935356039}]}, 3339: {'frame': 3339, 'ionic_force': [1.6150415539741516, 6.130378037691116, -9.246256113052368], 'ionic_force_magnitude': 11.21084948673503, 'motion_vector': [3.524639129638672, 0.14524078369140625, 2.0793838500976562], 'cosine_ionic_motion': -0.27541953448901435, 'ionic_motion_component': -3.0876869468629677, 'ionic_force_x': 1.6150415539741516, 'ionic_force_y': 6.130378037691116, 'ionic_force_z': -9.246256113052368, 'radial_force': 6.339549992394478, 'axial_force': -9.246256113052368, 'contributions': [{'ion': 1387, 'force': [0.22951126098632812, 0.4398341476917267, -2.3072080612182617], 'magnitude': 2.3599445819854736, 'distance': 11.860913276672363, 'cosine_with_motion': -0.4061335554517213, 'motion_component': -0.9584526927085806}, {'ion': 1460, 'force': [0.8212767243385315, 1.1787450313568115, -4.737607955932617], 'magnitude': 4.950643062591553, 'distance': 8.189139366149902, 'cosine_with_motion': -0.3347133815773649, 'motion_component': -1.6570464033133092}, {'ion': 2433, 'force': [0.564253568649292, 4.511798858642578, -2.2014400959014893], 'magnitude': 5.051836013793945, 'distance': 8.106705665588379, 'cosine_with_motion': -0.09346860421670186, 'motion_component': -0.47218808329276385}]}, 3340: {'frame': 3340, 'ionic_force': [7.662343084812164, 5.0752958953380585, -9.21539893746376], 'ionic_force_magnitude': 13.01513378921678, 'motion_vector': [-0.8464088439941406, -2.9289093017578125, 0.38051605224609375], 'cosine_ionic_motion': -0.6216180445886148, 'ionic_motion_component': -8.090442016112144, 'ionic_force_x': 7.662343084812164, 'ionic_force_y': 5.0752958953380585, 'ionic_force_z': -9.21539893746376, 'radial_force': 9.19076329662581, 'axial_force': -9.21539893746376, 'contributions': [{'ion': 1316, 'force': [0.6508142352104187, 0.245817631483078, -1.7105921506881714], 'magnitude': 1.8466485738754272, 'distance': 13.408398628234863, 'cosine_with_motion': -0.338712414616134, 'motion_component': -0.6254827999084984}, {'ion': 1387, 'force': [1.4326162338256836, 0.5672101974487305, -2.7843194007873535], 'magnitude': 3.1822242736816406, 'distance': 10.214183807373047, 'cosine_with_motion': -0.4023037665843089, 'motion_component': -1.2802208037761034}, {'ion': 1460, 'force': [4.253185749053955, 1.8484575748443604, -4.438457012176514], 'magnitude': 6.4192118644714355, 'distance': 7.191643714904785, 'cosine_with_motion': -0.5426708286919631, 'motion_component': -3.483519195765453}, {'ion': 2433, 'force': [1.325726866722107, 2.4138104915618896, -0.2820303738117218], 'magnitude': 2.7683160305023193, 'distance': 10.951187133789062, 'cosine_with_motion': -0.9757626049800445, 'motion_component': -2.701219314438271}]}, 3341: {'frame': 3341, 'ionic_force': [14.888546645641327, 3.9325586408376694, -6.769061803817749], 'ionic_force_magnitude': 16.821237659190512, 'motion_vector': [0.7330703735351562, 1.167449951171875, -0.67529296875], 'cosine_ionic_motion': 0.7775177842387024, 'ionic_motion_component': 13.078811432926425, 'ionic_force_x': 14.888546645641327, 'ionic_force_y': 3.9325586408376694, 'ionic_force_z': -6.769061803817749, 'radial_force': 15.399150583167392, 'axial_force': -6.769061803817749, 'contributions': [{'ion': 1316, 'force': [0.40359848737716675, -0.08952778577804565, -1.4260478019714355], 'magnitude': 1.4847623109817505, 'distance': 14.953420639038086, 'cosine_with_motion': 0.5064765055924272, 'motion_component': 0.751997257062042}, {'ion': 1387, 'force': [0.9169735908508301, -0.240996316075325, -2.4629430770874023], 'magnitude': 2.639130115509033, 'distance': 11.216015815734863, 'cosine_with_motion': 0.507029090482631, 'motion_component': 1.338115802175614}, {'ion': 1460, 'force': [4.683155536651611, -1.4487550258636475, -5.592735767364502], 'magnitude': 7.437037944793701, 'distance': 6.681424140930176, 'cosine_with_motion': 0.4833909417143953, 'motion_component': 3.5949966741954995}, {'ion': 2433, 'force': [8.884819030761719, 5.7118377685546875, 2.712664842605591], 'magnitude': 10.90521240234375, 'distance': 5.517622470855713, 'cosine_with_motion': 0.6779970679963836, 'motion_component': 7.393701814322099}]}, 3342: {'frame': 3342, 'ionic_force': [9.231768727302551, 6.486842645332217, -8.162149548530579], 'ionic_force_magnitude': 13.925708836259645, 'motion_vector': [-1.4764938354492188, 1.4851150512695312, 0.42453765869140625], 'cosine_ionic_motion': -0.2507741042712223, 'ionic_motion_component': -3.4922071597548583, 'ionic_force_x': 9.231768727302551, 'ionic_force_y': 6.486842645332217, 'ionic_force_z': -8.162149548530579, 'radial_force': 11.282937620128104, 'axial_force': -8.162149548530579, 'contributions': [{'ion': 1387, 'force': [0.796237587928772, 0.016238732263445854, -1.9542186260223389], 'magnitude': 2.110267400741577, 'distance': 12.542967796325684, 'cosine_with_motion': -0.4393621985204794, 'motion_component': -0.9271717172143745}, {'ion': 1460, 'force': [3.3354697227478027, 0.10465142130851746, -4.341390609741211], 'magnitude': 5.475763320922852, 'distance': 7.786579132080078, 'cosine_with_motion': -0.5651434645811022, 'motion_component': -3.094591785827248}, {'ion': 2433, 'force': [5.100061416625977, 6.365952491760254, -1.8665403127670288], 'magnitude': 8.367792129516602, 'distance': 6.29888391494751, 'cosine_with_motion': 0.06328509364338056, 'motion_component': 0.5295565281574355}]}, 3343: {'frame': 3343, 'ionic_force': [6.78049048781395, 6.935463041067123, -10.414144240319729], 'ionic_force_magnitude': 14.231307006298756, 'motion_vector': [-1.2784309387207031, -1.8371505737304688, -1.54437255859375], 'cosine_ionic_motion': -0.13764005680158262, 'ionic_motion_component': -1.9587979047077215, 'ionic_force_x': 6.78049048781395, 'ionic_force_y': 6.935463041067123, 'ionic_force_z': -10.414144240319729, 'radial_force': 9.699262799272091, 'axial_force': -10.414144240319729, 'contributions': [{'ion': 1316, 'force': [0.30228039622306824, 0.15748772025108337, -1.4446684122085571], 'magnitude': 1.4843324422836304, 'distance': 14.955586433410645, 'cosine_with_motion': 0.3853319596324988, 'motion_component': 0.5719607082213471}, {'ion': 1387, 'force': [0.6677933931350708, 0.4127635955810547, -2.39450740814209], 'magnitude': 2.519918203353882, 'distance': 11.478253364562988, 'cosine_with_motion': 0.30441458706669083, 'motion_component': 0.7670998458948546}, {'ion': 1460, 'force': [3.6871559619903564, 1.7069761753082275, -6.695205211639404], 'magnitude': 7.831644535064697, 'distance': 6.510922908782959, 'cosine_with_motion': 0.11692689494059591, 'motion_component': 0.91572990354382}, {'ion': 2433, 'force': [2.123260736465454, 4.658235549926758, 0.12023679167032242], 'magnitude': 5.1207275390625, 'distance': 8.051989555358887, 'cosine_with_motion': -0.8228495518087805, 'motion_component': -4.21358843681035}]}, 3344: {'frame': 3344, 'ionic_force': [4.965911656618118, 8.838596478104591, -13.473165035247803], 'ionic_force_magnitude': 16.861412821917458, 'motion_vector': [3.2638702392578125, 0.03415679931640625, 2.7843475341796875], 'cosine_ionic_motion': -0.29034934299537596, 'ionic_motion_component': -4.895700134817542, 'ionic_force_x': 4.965911656618118, 'ionic_force_y': 8.838596478104591, 'ionic_force_z': -13.473165035247803, 'radial_force': 10.138099737332366, 'axial_force': -13.473165035247803, 'contributions': [{'ion': 1387, 'force': [0.446129709482193, -0.06396286189556122, -2.735747814178467], 'magnitude': 2.772623062133789, 'distance': 10.94267749786377, 'cosine_with_motion': -0.5181302545307397, 'motion_component': -1.4365799324708046}, {'ion': 1460, 'force': [1.9232772588729858, -0.41003602743148804, -6.321849346160889], 'magnitude': 6.620642185211182, 'distance': 7.081397533416748, 'cosine_with_motion': -0.3991940414069441, 'motion_component': -2.642920945873833}, {'ion': 2433, 'force': [2.5965046882629395, 9.31259536743164, -4.415567874908447], 'magnitude': 10.628429412841797, 'distance': 5.589004993438721, 'cosine_with_motion': -0.07679394585184894, 'motion_component': -0.8161990217935475}]}, 3345: {'frame': 3345, 'ionic_force': [11.459057569503784, 4.5299258679151535, -9.10696730017662], 'ionic_force_magnitude': 15.</t>
+          <t>{3320: {'frame': 3320, 'ionic_force': [4.8733450174331665, 3.184350647032261, -8.640591382980347], 'ionic_force_magnitude': 10.418704341223512, 'motion_vector': [-0.18167495727539062, 0.760711669921875, 0.7443389892578125], 'cosine_ionic_motion': -0.4351086894470255, 'ionic_motion_component': -4.533268791645797, 'ionic_force_x': 4.8733450174331665, 'ionic_force_y': 3.184350647032261, 'ionic_force_z': -8.640591382980347, 'radial_force': 5.821475818226461, 'axial_force': -8.640591382980347, 'before_closest_residue': None, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1387, 'force': [0.3318135738372803, -0.0069795772433280945, -1.9514002799987793], 'magnitude': 1.9794220924377441, 'distance': 12.950896263122559, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7103326722280674, 'motion_component': -1.4060482193826478}, {'ion': 1460, 'force': [1.624815821647644, -0.2846843898296356, -5.312528133392334], 'magnitude': 5.562735557556152, 'distance': 7.725468635559082, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7435987748913293, 'motion_component': -4.1364433416914}, {'ion': 2433, 'force': [2.916715621948242, 3.4760146141052246, -1.3766629695892334], 'magnitude': 4.741846561431885, 'distance': 8.367491722106934, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 1073, 'cosine_with_motion': 0.21283327257076928, 'motion_component': 1.0092227157837357}]}, 3321: {'frame': 3321, 'ionic_force': [4.962071061134338, 4.828094765543938, -10.522126078605652], 'ionic_force_magnitude': 12.595546256311902, 'motion_vector': [3.44659423828125, 0.5642127990722656, -0.29720306396484375], 'cosine_ionic_motion': 0.5199156061735278, 'ionic_motion_component': 6.548621066937112, 'ionic_force_x': 4.962071061134338, 'ionic_force_y': 4.828094765543938, 'ionic_force_z': -10.522126078605652, 'radial_force': 6.9233408323452945, 'axial_force': -10.522126078605652, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.4181758165359497, 0.16234956681728363, -2.319929599761963], 'magnitude': 2.362901210784912, 'distance': 11.853490829467773, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.26833152479280165, 'motion_component': 0.6340408627544847}, {'ion': 1460, 'force': [2.362652540206909, 0.5963982939720154, -7.155970096588135], 'magnitude': 7.559479236602783, 'distance': 6.62709379196167, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.40029079586086974, 'motion_component': 3.0259899505259265}, {'ion': 2433, 'force': [2.1812427043914795, 4.069346904754639, -1.0462263822555542], 'magnitude': 4.734130859375, 'distance': 8.374307632446289, 'before_closest_residue': 1105, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.6101627710360925, 'motion_component': 2.8885903144106857}]}, 3322: {'frame': 3322, 'ionic_force': [5.101867258548737, 2.400673806667328, -5.333805024623871], 'ionic_force_magnitude': 7.761556563639349, 'motion_vector': [-1.1910209655761719, 1.1273345947265625, 1.091339111328125], 'cosine_ionic_motion': -0.6011411421058467, 'ionic_motion_component': -4.665790977185289, 'ionic_force_x': 5.101867258548737, 'ionic_force_y': 2.400673806667328, 'ionic_force_z': -5.333805024623871, 'radial_force': 5.638464706803635, 'axial_force': -5.333805024623871, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.8166144490242004, 0.16744935512542725, -1.7120360136032104], 'magnitude': 1.904196858406067, 'distance': 13.204231262207031, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7070687055580778, 'motion_component': -1.3463980228761798}, {'ion': 1460, 'force': [2.6996209621429443, 0.5092499852180481, -3.1144349575042725], 'magnitude': 4.152949810028076, 'distance': 8.941094398498535, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7383261436332469, 'motion_component': -3.066231583865708}, {'ion': 2433, 'force': [1.5856318473815918, 1.7239744663238525, -0.5073340535163879], 'magnitude': 2.3966026306152344, 'distance': 11.769852638244629, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.10563347096891086, 'motion_component': -0.2531614541572438}]}, 3323: {'frame': 3323, 'ionic_force': [5.707005620002747, 4.04939991235733, -7.091884225606918], 'ionic_force_magnitude': 9.963050469929113, 'motion_vector': [-0.09119033813476562, -1.4596443176269531, 0.58355712890625], 'cosine_ionic_motion': -0.6737404389098686, 'ionic_motion_component': -6.712509996491213, 'ionic_force_x': 5.707005620002747, 'ionic_force_y': 4.04939991235733, 'ionic_force_z': -7.091884225606918, 'radial_force': 6.997681958830545, 'axial_force': -7.091884225606918, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.8393199443817139, 0.3989105820655823, -2.18998122215271], 'magnitude': 2.3789925575256348, 'distance': 11.813334465026855, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5170273796606956, 'motion_component': -1.2300042650106304}, {'ion': 1460, 'force': [3.4794766902923584, 1.5985596179962158, -4.6523637771606445], 'magnitude': 6.02549934387207, 'distance': 7.422881603240967, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5655173853401619, 'motion_component': -3.4075245058578427}, {'ion': 2433, 'force': [1.3882089853286743, 2.0519297122955322, -0.24953922629356384], 'magnitude': 2.4899415969848633, 'distance': 11.547141075134277, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.8333453521952254, 'motion_component': -2.0749813240573336}]}, 3324: {'frame': 3324, 'ionic_force': [9.42669403553009, 3.5997143760323524, -10.327790841460228], 'ionic_force_magnitude': 14.438966988447003, 'motion_vector': [1.4581718444824219, 0.5040359497070312, -1.6050872802734375], 'cosine_ionic_motion': 0.9997192109901553, 'ionic_motion_component': 14.434912685203136, 'ionic_force_x': 9.42669403553009, 'ionic_force_y': 3.5997143760323524, 'ionic_force_z': -10.327790841460228, 'radial_force': 10.090614650679738, 'axial_force': -10.327790841460228, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1316, 'force': [0.5152910947799683, 0.09902171045541763, -1.5304564237594604], 'magnitude': 1.617908239364624, 'distance': 14.32491683959961, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9044381588025899, 'motion_component': 1.4632979506664054}, {'ion': 1387, 'force': [1.6848300695419312, 0.3395357131958008, -3.116074562072754], 'magnitude': 3.558631420135498, 'distance': 9.658897399902344, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9629840296835332, 'motion_component': 3.4269052191387033}, {'ion': 1460, 'force': [5.295093536376953, 0.8498631119728088, -5.482320308685303], 'magnitude': 7.6691670417785645, 'distance': 6.579531192779541, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9926726186717297, 'motion_component': 7.612971853423932}, {'ion': 2433, 'force': [1.9314793348312378, 2.311293840408325, -0.19893954694271088], 'magnitude': 3.018653392791748, 'distance': 10.487269401550293, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 780, 'cosine_with_motion': 0.6399335650787177, 'motion_component': 1.9317376565473425}]}, 3325: {'frame': 3325, 'ionic_force': [6.025220155715942, 3.329250246286392, -5.533735513687134], 'ionic_force_magnitude': 8.832293805274247, 'motion_vector': [-1.0484428405761719, -1.0520210266113281, -0.158599853515625], 'cosine_ionic_motion': -0.6777865381816526, 'ionic_motion_component': -5.986409842480087, 'ionic_force_x': 6.025220155715942, 'ionic_force_y': 3.329250246286392, 'ionic_force_z': -5.533735513687134, 'radial_force': 6.883835059561178, 'axial_force': -5.533735513687134, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [1.0765461921691895, 0.23434945940971375, -2.0206117630004883], 'magnitude': 2.3014655113220215, 'distance': 12.010658264160156, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3068244551499629, 'motion_component': -0.7061458862244105}, {'ion': 1460, 'force': [2.5632970333099365, 0.5630773901939392, -3.0066704750061035], 'magnitude': 3.9909415245056152, 'distance': 9.120766639709473, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.47019937350483226, 'motion_component': -1.8765382588053043}, {'ion': 2433, 'force': [2.3853769302368164, 2.5318233966827393, -0.506453275680542], 'magnitude': 3.515202283859253, 'distance': 9.718379974365234, 'before_closest_residue': 1073, 'closest_residue': 780, 'next_closest_residue': 1073, 'cosine_with_motion': -0.9682872249034437, 'motion_component': -3.403725551910478}]}, 3326: {'frame': 3326, 'ionic_force': [5.521149039268494, 2.2750196903944016, -6.492782413959503], 'ionic_force_magnitude': 8.821282490688043, 'motion_vector': [0.80645751953125, 0.5555877685546875, -0.410614013671875], 'cosine_ionic_motion': 0.8948647231467417, 'ionic_motion_component': 7.893854513828756, 'ionic_force_x': 5.521149039268494, 'ionic_force_y': 2.2750196903944016, 'ionic_force_z': -6.492782413959503, 'radial_force': 5.971499083605192, 'axial_force': -6.492782413959503, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.7306075096130371, 0.05163702368736267, -1.8644970655441284], 'magnitude': 2.0031981468200684, 'distance': 12.873809814453125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6503710687869672, 'motion_component': 1.3028221533939597}, {'ion': 1460, 'force': [2.9076755046844482, 0.214521124958992, -4.017284393310547], 'magnitude': 4.963785648345947, 'distance': 8.178290367126465, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7804168984028671, 'motion_component': 3.873822364127798}, {'ion': 2433, 'force': [1.8828660249710083, 2.008861541748047, -0.6110009551048279], 'magnitude': 2.820289134979248, 'distance': 10.849812507629395, 'before_closest_residue': 780, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.9634508776201375, 'motion_component': 2.7172101317688018}]}, 3327: {'frame': 3327, 'ionic_force': [4.962403953075409, 2.0606805086135864, -5.490831732749939], 'ionic_force_magnitude': 7.682518484810309, 'motion_vector': [-0.40179443359375, 0.5124359130859375, 0.6054840087890625], 'cosine_ionic_motion': -0.6239824605969704, 'ionic_motion_component': -4.7937567877336456, 'ionic_force_x': 4.962403953075409, 'ionic_force_y': 2.0606805086135864, 'ionic_force_z': -5.490831732749939, 'radial_force': 5.373253870056615, 'axial_force': -5.490831732749939, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.7123898863792419, 0.10276107490062714, -1.644201397895813], 'magnitude': 1.7948418855667114, 'distance': 13.600533485412598, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7701518053219849, 'motion_component': -1.382300725170892}, {'ion': 1460, 'force': [2.544466972351074, 0.2279723435640335, -3.2194597721099854], 'magnitude': 4.109890937805176, 'distance': 8.987810134887695, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7812058518484315, 'motion_component': -3.2106709714302584}, {'ion': 2433, 'force': [1.7055470943450928, 1.7299470901489258, -0.6271705627441406], 'magnitude': 2.508974075317383, 'distance': 11.503260612487793, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.0800267830802497, 'motion_component': -0.20078512136664983}]}, 3328: {'frame': 3328, 'ionic_force': [5.662827789783478, 2.698476254940033, -6.413617879152298], 'ionic_force_magnitude': 8.971281233748122, 'motion_vector': [-1.1094818115234375, 0.8973617553710938, 1.1634902954101562], 'cosine_ionic_motion': -0.6855367750310243, 'ionic_motion_component': -6.150143204880036, 'ionic_force_x': 5.662827789783478, 'ionic_force_y': 2.698476254940033, 'ionic_force_z': -6.413617879152298, 'radial_force': 6.272909426671105, 'axial_force': -6.413617879152298, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.7809037566184998, 0.18411484360694885, -1.7854108810424805], 'magnitude': 1.9573965072631836, 'distance': 13.023557662963867, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7709661628922033, 'motion_component': -1.5090864508773922}, {'ion': 1460, 'force': [3.093663454055786, 0.4853256046772003, -4.167239665985107], 'magnitude': 5.21269416809082, 'distance': 7.9806437492370605, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8174437983446711, 'motion_component': -4.261084555910353}, {'ion': 2433, 'force': [1.788260579109192, 2.029035806655884, -0.4609673321247101], 'magnitude': 2.7436022758483887, 'distance': 11.000399589538574, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.1384938768402133, 'motion_component': -0.3799721065212349}]}, 3329: {'frame': 3329, 'ionic_force': [6.12342631816864, 5.340087965130806, -8.698342144489288], 'ionic_force_magnitude': 11.90269067950494, 'motion_vector': [0.8754844665527344, -1.0129776000976562, 0.6521530151367188], 'cosine_ionic_motion': -0.3227464606590609, 'ionic_motion_component': -3.8415512891298116, 'ionic_force_x': 6.12342631816864, 'ionic_force_y': 5.340087965130806, 'ionic_force_z': -8.698342144489288, 'radial_force': 8.12483165052515, 'axial_force': -8.698342144489288, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1316, 'force': [0.37819957733154297, 0.24994249641895294, -1.4104505777359009], 'magnitude': 1.4815117120742798, 'distance': 14.969817161560059, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.38158253503441575, 'motion_component': -0.5653190013484792}, {'ion': 1387, 'force': [0.9713860750198364, 0.7008095979690552, -2.4578428268432617], 'magnitude': 2.734175682067871, 'distance': 11.019346237182617, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.35913446296586105, 'motion_component': -0.9819366955576072}, {'ion': 1460, 'force': [3.2983713150024414, 2.064893960952759, -4.52915096282959], 'magnitude': 5.971285343170166, 'distance': 7.456501483917236, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2426363541558891, 'motion_component': -1.4488509092765014}, {'ion': 2433, 'force': [1.4754693508148193, 2.324441909790039, -0.3008977770805359], 'magnitude': 2.7695810794830322, 'distance': 10.948685646057129, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1105, 'cosine_with_motion': -0.3052609156370647, 'motion_component': -0.8454448625147428}]}, 3330: {'frame': 3330, 'ionic_force': [8.562611877918243, 3.4708504751324654, -9.022035978734493], 'ionic_force_magnitude': 12.913646208339978, 'motion_vector': [1.0237197875976562, -1.2902107238769531, 0.8571853637695312], 'cosine_ionic_motion': -0.14371961245459278, 'ionic_motion_component': -1.8559442284383432, 'ionic_force_x': 8.562611877918243, 'ionic_force_y': 3.4708504751324654, 'ionic_force_z': -9.022035978734493, 'radial_force': 9.239324931649165, 'axial_force': -9.022035978734493, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 780, 'contributions': [{'ion': 1316, 'force': [0.5562570691108704, 0.11473546177148819, -1.4796452522277832], 'magnitude': 1.5849088430404663, 'distance': 14.47327709197998, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.28779764622325893, 'motion_component': -0.4561330512855037}, {'ion': 1387, 'force': [1.3070932626724243, 0.29501739144325256, -2.6750640869140625], 'magnitude': 2.9919052124023438, 'distance': 10.53404426574707, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.24041965554896735, 'motion_component': -0.7193127855523347}, {'ion': 1460, 'force': [4.905503273010254, 1.0822356939315796, -4.953392505645752], 'magnitude': 7.054877281188965, 'distance': 6.8600029945373535, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.04736466428845592, 'motion_component': -0.33415189509761234}, {'ion': 2433, 'force': [1.7937582731246948, 1.978861927986145, 0.0860658660531044], 'magnitude': 2.672240734100342, 'distance': 11.146313667297363, 'before_closest_residue': 1073, 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': -0.12960900139424755, 'motion_component': -0.3463464546020445}]}, 3331: {'frame': 3331, 'ionic_force': [12.735351324081421, 2.3743116538971663, -6.971976637840271], 'ionic_force_magnitude': 14.711729586156919, 'motion_vector': [-1.5520782470703125, 0.7276382446289062, -2.8383560180664062], 'cosine_ionic_motion': 0.035881050304702455, 'ionic_motion_component': 0.5278723093500758, 'ionic_force_x': 12.735351324081421, 'ionic_force_y': 2.3743116538971663, 'ionic_force_z': -6.971976637840271, 'radial_force': 12.954787886245544, 'axial_force': -6.971976637840271, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1316, 'force': [0.7236177921295166, -0.01991807110607624, -1.514197587966919], 'magnitude': 1.6783366203308105, 'distance': 14.064668655395508, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5678690160279444, 'motion_component': 0.9530753588752279}, {'ion': 1387, 'force': [2.3421452045440674, -0.13869722187519073, -2.969356060028076], 'magnitude': 3.784435987472534, 'distance': 9.366308212280273, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3739069185928592, 'motion_component': 1.4150268355639988}, {'ion': 1460, 'force': [6.530500888824463, -0.4096313416957855, -3.7830898761749268], 'magnitude': 7.558241367340088, 'distance': 6.627636432647705, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.01212381215447484, 'motion_component': 0.09163469545941672}, {'ion': 2433, 'force': [3.139087438583374, 2.9425582885742188, 1.2946668863296509], 'magnitude': 4.4931817054748535, 'distance': 8.595913887023926, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.42995467800748755, 'motion_component': -1.931864480817218}]}, 3332: {'frame': 3332, 'ionic_force': [5.920918166637421, 3.972064346075058, -6.426218777894974], 'ionic_force_magnitude': 9.598481905319595, 'motion_vector': [0.7343177795410156, 1.0062751770019531, 2.0959930419921875], 'cosine_ionic_motion': -0.21896350382145063, 'ionic_motion_component': -2.1017172293555717, 'ionic_force_x': 5.920918166637421, 'ionic_force_y': 3.972064346075058, 'ionic_force_z': -6.426218777894974, 'radial_force': 7.12983640102476, 'axial_force': -6.426218777894974, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.6480094790458679, 0.07161861658096313, -1.956294298171997], 'magnitude': 2.06207013130188, 'distance': 12.688705444335938, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7065626176169941, 'motion_component': -1.4569816124307788}, {'ion': 1460, 'force': [2.506962299346924, 0.3197813332080841, -4.0640716552734375], 'magnitude': 4.785791397094727, 'distance': 8.328987121582031, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5446592892584318, 'motion_component': -2.606625695022325}, {'ion': 2433, 'force': [2.765946388244629, 3.5806643962860107, -0.4058528244495392], 'magnitude': 4.542723178863525, 'distance': 8.54891300201416, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.43187531744995167, 'motion_component': 1.9618899948423572}]}, 3333: {'frame': 3333, 'ionic_force': [11.138619840145111, 7.894609674811363, -10.194625984877348], 'ionic_force_magnitude': 17.038899988920527, 'motion_vector': [-0.58197021484375, -0.06623077392578125, -0.9650726318359375], 'cosine_ionic_motion': 0.1472983279094927, 'ionic_motion_component': 2.5098014777850675, 'ionic_force_x': 11.138619840145111, 'ionic_force_y': 7.894609674811363, 'ionic_force_z': -10.194625984877348, 'radial_force': 13.652608317127518, 'axial_force': -10.194625984877348, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1316, 'force': [0.6237956881523132, 0.15656648576259613, -1.627447485923767], 'magnitude': 1.7499197721481323, 'distance': 13.773996353149414, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6060249544382219, 'motion_component': 1.06049509096636}, {'ion': 1387, 'force': [1.9665889739990234, 0.6323477029800415, -3.3439724445343018], 'magnitude': 3.9305837154388428, 'distance': 9.190528869628906, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4599211400015446, 'motion_component': 1.8077584950588932}, {'ion': 1460, 'force': [5.7677435874938965, 2.1759836673736572, -5.206416130065918], 'magnitude': 8.068985939025879, 'distance': 6.414451599121094, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.16728169529424516, 'motion_component': 1.3497937077936975}, {'ion': 2433, 'force': [2.780491590499878, 4.929711818695068, -0.01678992435336113], 'magnitude': 5.659811973571777, 'distance': 7.658928871154785, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.30182028666503474, 'motion_component': -1.7082461370083915}]}, 3334: {'frame': 3334, 'ionic_force': [8.556934595108032, 6.820997595787048, -7.33417646586895], 'ionic_force_magnitude': 13.173355013025168, 'motion_vector': [0.17787933349609375, -0.084075927734375, 0.6251068115234375], 'cosine_ionic_motion': -0.42117706074107514, 'ionic_motion_component': -5.548314944484647, 'ionic_force_x': 8.556934595108032, 'ionic_force_y': 6.820997595787048, 'ionic_force_z': -7.33417646586895, 'radial_force': 10.942903539129336, 'axial_force': -7.33417646586895, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [1.4384901523590088, 0.4807847738265991, -2.7401866912841797], 'magnitude': 3.131937265396118, 'distance': 10.295857429504395, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7295832994848833, 'motion_component': -2.2850091222240625}, {'ion': 1460, 'force': [4.045209884643555, 1.0065531730651855, -4.721059799194336], 'magnitude': 6.298037528991699, 'distance': 7.260498046875, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5611922266405833, 'motion_component': -3.534409758359267}, {'ion': 2433, 'force': [3.0732345581054688, 5.333659648895264, 0.12707002460956573], 'magnitude': 6.157015800476074, 'distance': 7.343175411224365, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.04403173563774378, 'motion_component': 0.2711040889088734}]}, 3335: {'frame': 3335, 'ionic_force': [10.957434237003326, 7.65510667860508, -10.461147874593735], 'ionic_force_magnitude': 16.973557027717963, 'motion_vector': [0.046604156494140625, 0.275848388671875, -0.0363616943359375], 'cosine_ionic_motion': 0.627074144131308, 'ionic_motion_component': 10.64367874602019, 'ionic_force_x': 10.957434237003326, 'ionic_force_y': 7.65510667860508, 'ionic_force_z': -10.461147874593735, 'radial_force': 13.366601038374593, 'axial_force': -10.461147874593735, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1316, 'force': [0.5002949833869934, 0.06886790692806244, -1.5100455284118652], 'magnitude': 1.5922547578811646, 'distance': 14.439852714538574, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.21643463805504745, 'motion_component': 0.344619091924816}, {'ion': 1387, 'force': [1.7298309803009033, 0.3097245991230011, -3.301562786102295], 'magnitude': 3.740128517150879, 'distance': 9.421624183654785, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.27115584312548485, 'motion_component': 1.0141577034043774}, {'ion': 1460, 'force': [5.743025779724121, 1.7341681718826294, -5.573688983917236], 'magnitude': 8.188754081726074, 'distance': 6.36737060546875, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.41066215110078985, 'motion_component': 3.3628113618595847}, {'ion': 2433, 'force': [2.9842824935913086, 5.542346000671387, -0.07585057616233826], 'magnitude': 6.295180320739746, 'distance': 7.262145519256592, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.9407340673341933, 'motion_component': 5.922090530346958}]}, 3336: {'frame': 3336, 'ionic_force': [9.11018654704094, 6.392471864819527, -9.55652368068695], 'ionic_force_magnitude': 14.669231074733448, 'motion_vector': [-4.241512298583984, -1.3926010131835938, -0.917877197265625], 'cosine_ionic_motion': -0.5799124377910689, 'ionic_motion_component': -8.506869553069176, 'ionic_force_x': 9.11018654704094, 'ionic_force_y': 6.392471864819527, 'ionic_force_z': -9.55652368068695, 'radial_force': 11.129204619576143, 'axial_force': -9.55652368068695, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 780, 'contributions': [{'ion': 1316, 'force': [0.46599122881889343, 0.17207498848438263, -1.45326566696167], 'magnitude': 1.5358186960220337, 'distance': 14.702767372131348, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.12603612829488975, 'motion_component': -0.19356862820591123}, {'ion': 1387, 'force': [1.0968544483184814, 0.3437471389770508, -2.457841634750366], 'magnitude': 2.7133443355560303, 'distance': 11.061565399169922, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2324851428875588, 'motion_component': -0.6308122367540214}, {'ion': 1460, 'force': [5.049988269805908, 1.1790555715560913, -5.30512809753418], 'magnitude': 7.4186882972717285, 'distance': 6.6896820068359375, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.538038635350998, 'motion_component': -3.991540987216098}, {'ion': 2433, 'force': [2.4973526000976562, 4.697594165802002, -0.34028828144073486], 'magnitude': 5.3310370445251465, 'distance': 7.891565799713135, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.6923507626904895, 'motion_component': -3.6909476351492234}]}, 3337: {'frame': 3337, 'ionic_force': [-1.0386495990678668, 10.650418624281883, -13.788317680358887], 'ionic_force_magnitude': 17.45359316348905, 'motion_vector': [0.44036865234375, 2.80010986328125, -1.7934036254882812], 'cosine_ionic_motion': 0.9239821916649363, 'ionic_motion_component': 16.12680926362876, 'ionic_force_x': -1.0386495990678668, 'ionic_force_y': 10.650418624281883, 'ionic_force_z': -13.788317680358887, 'radial_force': 10.70094434440691, 'axial_force': -13.788317680358887, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [-0.007922927848994732, 0.10124565660953522, -2.5693626403808594], 'magnitude': 2.571368932723999, 'distance': 11.362838745117188, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5667177533058034, 'motion_component': 1.4572403853948068}, {'ion': 1460, 'force': [0.24486219882965088, 0.3454366624355316, -9.121464729309082], 'magnitude': 9.13128662109375, 'distance': 6.029801845550537, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5691957685666009, 'motion_component': 5.197489938044287}, {'ion': 2433, 'force': [-1.275588870048523, 10.203736305236816, -2.0974903106689453], 'magnitude': 10.494894981384277, 'distance': 5.624449253082275, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.9025415453681213, 'motion_component': 9.472079013835085}]}, 3338: {'frame': 3338, 'ionic_force': [0.4838514244183898, 6.611688911914825, -7.909306526184082], 'ionic_force_magnitude': 10.320158535312686, 'motion_vector': [0.3501434326171875, -1.3354682922363281, -0.2438507080078125], 'cosine_ionic_motion': -0.4652546041033829, 'ionic_motion_component': -4.801501273631051, 'ionic_force_x': 0.4838514244183898, 'ionic_force_y': 6.611688911914825, 'ionic_force_z': -7.909306526184082, 'radial_force': 6.629369688654355, 'axial_force': -7.909306526184082, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 780, 'contributions': [{'ion': 1387, 'force': [0.04897297918796539, 0.46202152967453003, -1.8418389558792114], 'magnitude': 1.8995349407196045, 'distance': 13.22042465209961, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.056600802095017826, 'motion_component': -0.10751520117704749}, {'ion': 1460, 'force': [0.4208226501941681, 1.4192343950271606, -4.18621301651001], 'magnitude': 4.4402360916137695, 'distance': 8.647010803222656, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.1168145613509119, 'motion_component': -0.5186842424025317}, {'ion': 2433, 'force': [0.014055795036256313, 4.730432987213135, -1.8812545537948608], 'magnitude': 5.09080696105957, 'distance': 8.075617790222168, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.8201650955329496, 'motion_component': -4.175301935356039}]}, 3339: {'frame': 3339, 'ionic_force': [1.6150415539741516, 6.130378037691116, -9.246256113052368], 'ionic_force_magnitude': 11.21084948673503, 'motion_vector': [3.524639129638672, 0.14524078369140625, 2.0793838500976562], 'cosine_ionic_motion': -0.27541953448901435, 'ionic_motion_component': -3.0876869468629677, 'ionic_force_x': 1.6150415539741516, 'ionic_force_y': 6.130378037691116, 'ionic_force_z': -9.246256113052368, 'radial_force': 6.339549992394478, 'axial_force': -9.246256113052368, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1387, 'force': [0.22951126098632812, 0.4398341476917267, -2.3072080612182617], 'magnitude': 2.3599445819854736, 'distance': 11.860913276672363, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.4061335554517213, 'motion_component': -0.9584526927085806}, {'ion': 1460, 'force': [0.821276724338</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{4333: {'frame': 4333, 'ionic_force': [5.670064628124237, -0.11623673886060715, -16.053759455680847], 'ionic_force_magnitude': 17.02604876439125, 'motion_vector': [-1.0914764404296875, 2.8184471130371094, 0.5848388671875], 'cosine_ionic_motion': -0.30345207696552395, 'ionic_motion_component': -5.166589860070817, 'ionic_force_x': 5.670064628124237, 'ionic_force_y': -0.11623673886060715, 'ionic_force_z': -16.053759455680847, 'radial_force': 5.671255933791614, 'axial_force': -16.053759455680847, 'contributions': [{'ion': 1308, 'force': [0.17358297109603882, -0.07655664533376694, -1.6345635652542114], 'magnitude': 1.6455363035202026, 'distance': 14.20415210723877, 'cosine_with_motion': -0.2687048108516073, 'motion_component': -0.4421635449013345}, {'ion': 1316, 'force': [0.8972761631011963, -0.14553450047969818, -3.8930156230926514], 'magnitude': 3.9977312088012695, 'distance': 9.113018035888672, 'cosine_with_motion': -0.2979077327293967, 'motion_component': -1.190955063856654}, {'ion': 1387, 'force': [4.599205493927002, 0.10585440695285797, -10.526180267333984], 'magnitude': 11.487574577331543, 'distance': 5.375945568084717, 'cosine_with_motion': -0.30759072151122985, 'motion_component': -3.5334713216154103}]}, 4334: {'frame': 4334, 'ionic_force': [3.895419254899025, 7.656647235155106, -16.01752197742462], 'ionic_force_magnitude': 18.175795673156294, 'motion_vector': [0.5448684692382812, -2.2713394165039062, -1.4224014282226562], 'cosine_ionic_motion': 0.15118571210621812, 'ionic_motion_component': 2.747920611943252, 'ionic_force_x': 3.895419254899025, 'ionic_force_y': 7.656647235155106, 'ionic_force_z': -16.01752197742462, 'radial_force': 8.59060754865722, 'axial_force': -16.01752197742462, 'contributions': [{'ion': 1308, 'force': [0.18028856813907623, 0.2747263014316559, -1.6901415586471558], 'magnitude': 1.721789002418518, 'distance': 13.886061668395996, 'cosine_with_motion': 0.39889620431807066, 'motion_component': 0.6868150546000797}, {'ion': 1316, 'force': [0.8013342618942261, 1.1461530923843384, -3.9313461780548096], 'magnitude': 4.172683238983154, 'distance': 8.919927597045898, 'cosine_with_motion': 0.3001616454276057, 'motion_component': 1.2524794981272755}, {'ion': 1387, 'force': [2.9137964248657227, 6.235767841339111, -10.396034240722656], 'magnitude': 12.468061447143555, 'distance': 5.160236358642578, 'cosine_with_motion': 0.06485580436767582, 'motion_component': 0.8086261068832242}]}, 4335: {'frame': 4335, 'ionic_force': [7.201493963599205, 1.6286407187581062, -22.629054307937622], 'ionic_force_magnitude': 23.803110821280125, 'motion_vector': [-2.4897499084472656, -1.9592094421386719, -2.6416397094726562], 'cosine_ionic_motion': 0.3937050990196898, 'ionic_motion_component': 9.371406102868741, 'ionic_force_x': 7.201493963599205, 'ionic_force_y': 1.6286407187581062, 'ionic_force_z': -22.629054307937622, 'radial_force': 7.383358713929096, 'axial_force': -22.629054307937622, 'contributions': [{'ion': 1308, 'force': [0.17067889869213104, -0.07447502017021179, -1.5542986392974854], 'magnitude': 1.565414309501648, 'distance': 14.563118934631348, 'cosine_with_motion': 0.5926381165473805, 'motion_component': 0.9277242097333298}, {'ion': 1316, 'force': [0.7298926711082458, 0.04116610437631607, -3.5585622787475586], 'magnitude': 3.632878065109253, 'distance': 9.559685707092285, 'cosine_with_motion': 0.5006490876675077, 'motion_component': 1.8187971175178699}, {'ion': 1387, 'force': [6.300922393798828, 1.661949634552002, -17.516193389892578], 'magnitude': 18.68905258178711, 'distance': 4.214784622192383, 'cosine_with_motion': 0.3544794253429433, 'motion_component': 6.624885037317597}]}, 4336: {'frame': 4336, 'ionic_force': [-0.5388405174016953, -1.7428620159626007, -9.03514313697815], 'ionic_force_magnitude': 9.217468666372689, 'motion_vector': [0.6896553039550781, 0.1011199951171875, 0.940399169921875], 'cosine_ionic_motion': -0.8382634653281991, 'ionic_motion_component': -7.726667225827664, 'ionic_force_x': -0.5388405174016953, 'ionic_force_y': -1.7428620159626007, 'ionic_force_z': -9.03514313697815, 'radial_force': 1.8242579614404721, 'axial_force': -9.03514313697815, 'contributions': [{'ion': 1316, 'force': [-0.19560758769512177, -0.3452792465686798, -2.427891969680786], 'magnitude': 2.4601097106933594, 'distance': 11.616941452026367, 'cosine_with_motion': -0.8518276766603495, 'motion_component': -2.0955894897212177}, {'ion': 1387, 'force': [-0.3432329297065735, -1.397582769393921, -6.607251167297363], 'magnitude': 6.762160301208496, 'distance': 7.006906032562256, 'cosine_with_motion': -0.8327335038641387, 'motion_component': -5.631077594624198}]}, 4337: {'frame': 4337, 'ionic_force': [-0.16387367993593216, -1.5002783238887787, -8.31986379623413], 'ionic_force_magnitude': 8.455638545964089, 'motion_vector': [-1.2149238586425781, 0.8994140625, 1.17535400390625], 'cosine_ionic_motion': -0.6750159695501066, 'ionic_motion_component': -5.707691051269203, 'ionic_force_x': -0.16387367993593216, 'ionic_force_y': -1.5002783238887787, 'ionic_force_z': -8.31986379623413, 'radial_force': 1.509201653890648, 'axial_force': -8.31986379623413, 'contributions': [{'ion': 1316, 'force': [-0.0917414203286171, -0.38027724623680115, -2.686659812927246], 'magnitude': 2.714989423751831, 'distance': 11.058213233947754, 'cosine_with_motion': -0.6517738113728772, 'motion_component': -1.7695590827597387}, {'ion': 1387, 'force': [-0.07213225960731506, -1.1200010776519775, -5.633203983306885], 'magnitude': 5.743917942047119, 'distance': 7.602648735046387, 'cosine_with_motion': -0.6856177321457585, 'motion_component': -3.9381319494534495}]}, 4338: {'frame': 4338, 'ionic_force': [-2.4280003905296326, -1.0742815136909485, -10.110801935195923], 'ionic_force_magnitude': 10.453591843946834, 'motion_vector': [1.5186386108398438, 5.265224456787109, -0.11255645751953125], 'cosine_ionic_motion': -0.1432126280334982, 'ionic_motion_component': -1.4970863603611686, 'ionic_force_x': -2.4280003905296326, 'ionic_force_y': -1.0742815136909485, 'ionic_force_z': -10.110801935195923, 'radial_force': 2.655045511299225, 'axial_force': -10.110801935195923, 'contributions': [{'ion': 1316, 'force': [-0.5445583462715149, -0.3111899495124817, -2.85630202293396], 'magnitude': 2.92435359954834, 'distance': 10.65501594543457, 'cosine_with_motion': -0.13376092719612437, 'motion_component': -0.39116425460121373}, {'ion': 1387, 'force': [-1.8834420442581177, -0.7630915641784668, -7.254499912261963], 'magnitude': 7.533752918243408, 'distance': 6.638399124145508, 'cosine_with_motion': -0.14679564559442262, 'motion_component': -1.10592210987212}]}, 4339: {'frame': 4339, 'ionic_force': [-0.01052268361672759, 7.317051321268082, -8.848112106323242], 'ionic_force_magnitude': 11.48165661440044, 'motion_vector': [-0.3119239807128906, 0.11574172973632812, 2.2965164184570312], 'cosine_ionic_motion': -0.7307586444093754, 'ionic_motion_component': -8.390319823113206, 'ionic_force_x': -0.01052268361672759, 'ionic_force_y': 7.317051321268082, 'ionic_force_z': -8.848112106323242, 'radial_force': 7.317058887622914, 'axial_force': -8.848112106323242, 'contributions': [{'ion': 1308, 'force': [0.015117759816348553, 0.40834537148475647, -1.4295883178710938], 'magnitude': 1.4868414402008057, 'distance': 14.942962646484375, 'cosine_with_motion': -0.9392277961859843, 'motion_component': -1.3964827394725436}, {'ion': 1316, 'force': [-0.007704783696681261, 1.2880055904388428, -2.648350715637207], 'magnitude': 2.944958209991455, 'distance': 10.61767578125, 'cosine_with_motion': -0.8678253609626467, 'motion_component': -2.5557094833582963}, {'ion': 1387, 'force': [-0.017935659736394882, 5.620700359344482, -4.770173072814941], 'magnitude': 7.37205171585083, 'distance': 6.710808753967285, 'cosine_with_motion': -0.6020206998732269, 'motion_component': -4.438127686965383}]}, 4340: {'frame': 4340, 'ionic_force': [-0.6614977717399597, 11.020213901996613, -11.043931484222412], 'ionic_force_magnitude': 15.615732975943697, 'motion_vector': [0.09852218627929688, -2.540813446044922, -1.569000244140625], 'cosine_ionic_motion': -0.23013628428245336, 'ionic_motion_component': -3.59374676343066, 'ionic_force_x': -0.6614977717399597, 'ionic_force_y': 11.020213901996613, 'ionic_force_z': -11.043931484222412, 'radial_force': 11.040049535567144, 'axial_force': -11.043931484222412, 'contributions': [{'ion': 1308, 'force': [-0.11230937391519547, 0.5389495491981506, -1.9288716316223145], 'magnitude': 2.0058977603912354, 'distance': 12.865143775939941, 'cosine_with_motion': 0.27463385257681466, 'motion_component': 0.5508874269489278}, {'ion': 1316, 'force': [-0.09320607036352158, 2.1498072147369385, -3.7819480895996094], 'magnitude': 4.351263046264648, 'distance': 8.734969139099121, 'cosine_with_motion': 0.03556952269342487, 'motion_component': 0.15477234838873555}, {'ion': 1387, 'force': [-0.4559823274612427, 8.331457138061523, -5.333111763000488], 'magnitude': 9.902685165405273, 'distance': 5.790186405181885, 'cosine_with_motion': -0.43416573845546347, 'motion_component': -4.299406738489893}]}, 4341: {'frame': 4341, 'ionic_force': [-1.1659248024225235, 9.977354973554611, -17.802505493164062], 'ionic_force_magnitude': 20.441041919318973, 'motion_vector': [-0.7720985412597656, -0.6841316223144531, -3.7374649047851562], 'cosine_ionic_motion': 0.7647606975638053, 'ionic_motion_component': 15.632505477149364, 'ionic_force_x': -1.1659248024225235, 'ionic_force_y': 9.977354973554611, 'ionic_force_z': -17.802505493164062, 'radial_force': 10.045247279844283, 'axial_force': -17.802505493164062, 'contributions': [{'ion': 1308, 'force': [-0.09177793562412262, 0.24030449986457825, -1.6979613304138184], 'magnitude': 1.717335820198059, 'distance': 13.904053688049316, 'cosine_with_motion': 0.9390324383797626, 'motion_component': 1.6126339887252703}, {'ion': 1316, 'force': [-0.13407957553863525, 0.977773129940033, -3.8091092109680176], 'magnitude': 3.9348864555358887, 'distance': 9.185503005981445, 'cosine_with_motion': 0.8960829730796381, 'motion_component': 3.5259846615014645}, {'ion': 1387, 'force': [-0.9400672912597656, 8.75927734375, -12.295434951782227], 'magnitude': 15.125685691833496, 'distance': 4.685020446777344, 'cosine_with_motion': 0.6937792513859733, 'motion_component': 10.493887334066017}]}, 4342: {'frame': 4342, 'ionic_force': [-1.3840811252593994, 1.351293995976448, -7.411204814910889], 'ionic_force_magnitude': 7.659479932307392, 'motion_vector': [-2.657154083251953, -1.6822662353515625, 5.648590087890625], 'cosine_ionic_motion': -0.8170268253809583, 'ionic_motion_component': -6.258000573162266, 'ionic_force_x': -1.3840811252593994, 'ionic_force_y': 1.351293995976448, 'ionic_force_z': -7.411204814910889, 'radial_force': 1.9343412379570781, 'axial_force': -7.411204814910889, 'contributions': [{'ion': 1316, 'force': [-0.2974294424057007, 0.23622436821460724, -2.1497864723205566], 'magnitude': 2.183082342147827, 'distance': 12.332013130187988, 'cosine_with_motion': -0.832544475446919, 'motion_component': -1.8175130650926032}, {'ion': 1387, 'force': [-1.0866516828536987, 1.1150696277618408, -5.261418342590332], 'magnitude': 5.4869585037231445, 'distance': 7.778631687164307, 'cosine_with_motion': -0.8092803195561473, 'motion_component': -4.440487642549986}]}, 4343: {'frame': 4343, 'ionic_force': [-16.709574282169342, -0.8938723057508469, -13.62956953048706], 'ionic_force_magnitude': 21.58179895135493, 'motion_vector': [2.1892776489257812, 5.375339508056641, -3.4262237548828125], 'cosine_ionic_motion': 0.036513285370066664, 'ionic_motion_component': 0.788022383910228, 'ionic_force_x': -16.709574282169342, 'ionic_force_y': -0.8938723057508469, 'ionic_force_z': -13.62956953048706, 'radial_force': 16.733465880992004, 'axial_force': -13.62956953048706, 'contributions': [{'ion': 1308, 'force': [-0.6828966736793518, -0.1254197210073471, -2.168544292449951], 'magnitude': 2.2769854068756104, 'distance': 12.07504940032959, 'cosine_with_motion': 0.34279108699768035, 'motion_component': 0.7805302860302322}, {'ion': 1316, 'force': [-2.210134983062744, -0.2589053511619568, -4.237045764923096], 'magnitude': 4.785842418670654, 'distance': 8.32894229888916, 'cosine_with_motion': 0.2569054433894155, 'motion_component': 1.2295089090269506}, {'ion': 1387, 'force': [-13.816542625427246, -0.509547233581543, -7.223979473114014], 'magnitude': 15.599434852600098, 'distance': 4.613330841064453, 'cosine_with_motion': -0.07833721866182479, 'motion_component': -1.2220163395787154}]}, 4344: {'frame': 4344, 'ionic_force': [-1.153914988040924, 3.170382857322693, -5.203489422798157], 'ionic_force_magnitude': 6.201544116976302, 'motion_vector': [1.4634857177734375, -1.2306327819824219, 0.8022537231445312], 'cosine_ionic_motion': -0.7593428919930103, 'ionic_motion_component': -4.709098444607024, 'ionic_force_x': -1.153914988040924, 'ionic_force_y': 3.170382857322693, 'ionic_force_z': -5.203489422798157, 'radial_force': 3.373847545700767, 'axial_force': -5.203489422798157, 'contributions': [{'ion': 1316, 'force': [-0.2957773804664612, 0.846617579460144, -1.985202670097351], 'magnitude': 2.1783652305603027, 'distance': 12.345357894897461, 'cosine_with_motion': -0.6790620152713646, 'motion_component': -1.4792451065752275}, {'ion': 1387, 'force': [-0.8581376075744629, 2.323765277862549, -3.2182867527008057], 'magnitude': 4.061237812042236, 'distance': 9.041485786437988, 'cosine_with_motion': -0.7952878508257138, 'motion_component': -3.2298533141553847}]}, 4345: {'frame': 4345, 'ionic_force': [0.08994757011532784, 5.610477715730667, -9.722934126853943], 'ionic_force_magnitude': 11.225907482213682, 'motion_vector': [-1.1395187377929688, 0.0416717529296875, -1.0085220336914062], 'cosine_ionic_motion': 0.5814891324386149, 'ionic_motion_component': 6.5277432026685895, 'ionic_force_x': 0.08994757011532784, 'ionic_force_y': 5.610477715730667, 'ionic_force_z': -9.722934126853943, 'radial_force': 5.611198692265321, 'axial_force': -9.722934126853943, 'contributions': [{'ion': 1308, 'force': [-0.04955724999308586, 0.3378300964832306, -1.4625250101089478], 'magnitude': 1.5018537044525146, 'distance': 14.868091583251953, 'cosine_with_motion': 0.6760140450308809, 'motion_component': 1.0152741867035733}, {'ion': 1316, 'force': [-0.044318169355392456, 1.0932285785675049, -2.809373140335083], 'magnitude': 3.014911413192749, 'distance': 10.493775367736816, 'cosine_with_motion': 0.6382689866249723, 'motion_component': 1.9243243929068639}, {'ion': 1387, 'force': [0.18382298946380615, 4.179419040679932, -5.451035976409912], 'magnitude': 6.871326446533203, 'distance': 6.951023101806641, 'cosine_with_motion': 0.5221909782986967, 'motion_component': 3.5881446979568086}]}, 4346: {'frame': 4346, 'ionic_force': [-0.9703720510005951, 4.194342374801636, -6.858072519302368], 'ionic_force_magnitude': 8.097363061789316, 'motion_vector': [-4.582515716552734, 0.4224891662597656, 2.309173583984375], 'cosine_ionic_motion': -0.23068510028921504, 'ionic_motion_component': -1.867941009987054, 'ionic_force_x': -0.9703720510005951, 'ionic_force_y': 4.194342374801636, 'ionic_force_z': -6.858072519302368, 'radial_force': 4.305128322642628, 'axial_force': -6.858072519302368, 'contributions': [{'ion': 1316, 'force': [-0.26130351424217224, 0.9197101593017578, -2.4406163692474365], 'magnitude': 2.6212124824523926, 'distance': 11.25428581237793, 'cosine_with_motion': -0.30007228847047807, 'motion_component': -0.7865532102811734}, {'ion': 1387, 'force': [-0.7090685367584229, 3.274632215499878, -4.417456150054932], 'magnitude': 5.544358730316162, 'distance': 7.7382612228393555, 'cosine_with_motion': -0.1950429042251414, 'motion_component': -1.0813878190443305}]}, 4347: {'frame': 4347, 'ionic_force': [-5.324795186519623, 4.4520832896232605, -5.531670093536377], 'ionic_force_magnitude': 8.87546412419373, 'motion_vector': [-0.36487579345703125, -0.39484405517578125, 1.3642425537109375], 'cosine_ionic_motion': -0.5656374441017312, 'ionic_motion_component': -5.020294842425552, 'ionic_force_x': -5.324795186519623, 'ionic_force_y': 4.4520832896232605, 'ionic_force_z': -5.531670093536377, 'radial_force': 6.940784494286306, 'axial_force': -5.531670093536377, 'contributions': [{'ion': 1308, 'force': [-0.5734414458274841, 0.4193485379219055, -1.335965633392334], 'magnitude': 1.5131069421768188, 'distance': 14.812700271606445, 'cosine_with_motion': -0.8017682373028415, 'motion_component': -1.213161044334834}, {'ion': 1316, 'force': [-1.3264715671539307, 1.0629514455795288, -2.074846029281616], 'magnitude': 2.6822338104248047, 'distance': 11.125530242919922, 'cosine_with_motion': -0.7033365199731868, 'motion_component': -1.8865130497748017}, {'ion': 1387, 'force': [-3.424882173538208, 2.969783306121826, -2.1208584308624268], 'magnitude': 5.004745006561279, 'distance': 8.144756317138672, 'cosine_with_motion': -0.3837599886865634, 'motion_component': -1.9206208369105298}]}, 4348: {'frame': 4348, 'ionic_force': [-4.811583518981934, 3.2644795179367065, -4.231451034545898], 'ionic_force_magnitude': 7.191198811111148, 'motion_vector': [1.2287940979003906, -3.6073760986328125, -4.4157257080078125], 'cosine_ionic_motion': 0.023752005658367503, 'ionic_motion_component': 0.17080539485195764, 'ionic_force_x': -4.811583518981934, 'ionic_force_y': 3.2644795179367065, 'ionic_force_z': -4.231451034545898, 'radial_force': 5.8144786940160715, 'axial_force': -4.231451034545898, 'contributions': [{'ion': 1316, 'force': [-1.6572506427764893, 1.0221670866012573, -2.0923280715942383], 'magnitude': 2.858170986175537, 'distance': 10.777670860290527, 'cosine_with_motion': 0.2108659991227886, 'motion_component': 0.602691103493072}, {'ion': 1387, 'force': [-3.1543328762054443, 2.242312431335449, -2.13912296295166], 'magnitude': 4.421948432922363, 'distance': 8.664873123168945, 'cosine_with_motion': -0.09766865255972287, 'motion_component': -0.43188574558306664}]}, 4349: {'frame': 4349, 'ionic_force': [-2.8148942589759827, 0.3423163443803787, -5.1887286901474], 'ionic_force_magnitude': 5.913012395455015, 'motion_vector': [3.6558074951171875, 0.5428085327148438, 1.3375320434570312], 'cosine_ionic_motion': -0.7334051060764676, 'ionic_motion_component': -4.336633483120153, 'ionic_force_x': -2.8148942589759827, 'ionic_force_y': 0.3423163443803787, 'ionic_force_z': -5.1887286901474, 'radial_force': 2.835632234413675, 'axial_force': -5.1887286901474, 'contributions': [{'ion': 1316, 'force': [-0.7681282162666321, 0.059397414326667786, -1.9104300737380981], 'magnitude': 2.0599253177642822, 'distance': 12.69530963897705, 'cosine_with_motion': -0.658453806185171, 'motion_component': -1.356365627793785}, {'ion': 1387, 'force': [-2.0467660427093506, 0.28291893005371094, -3.2782986164093018], 'magnitude': 3.875117540359497, 'distance': 9.25606918334961, 'cosine_with_motion': -0.769078047461971, 'motion_component': -2.9802678535875486}]}, 4350: {'frame': 4350, 'ionic_force': [-1.14635768532753, 1.0225782543420792, -9.443222522735596], 'ionic_force_magnitude': 9.567353544364483, 'motion_vector': [-3.0155258178710938, -3.347362518310547, 1.5890350341796875], 'cosine_ionic_motion': -0.3275592344848105, 'ionic_motion_component': -3.1338750030375686, 'ionic_force_x': -1.14635768532753, 'ionic_force_y': 1.0225782543420792, 'ionic_force_z': -9.443222522735596, 'radial_force': 1.536164779235218, 'axial_force': -9.443222522735596, 'contributions': [{'ion': 1316, 'force': [-0.2180737555027008, 0.12293900549411774, -2.9367432594299316], 'magnitude': 2.9473938941955566, 'distance': 10.613287925720215, 'cosine_with_motion': -0.31393846865149616, 'motion_component': -0.9253003451579868}, {'ion': 1387, 'force': [-0.9282839298248291, 0.8996392488479614, -6.506479263305664], 'magnitude': 6.6336517333984375, 'distance': 7.074450492858887, 'cosine_with_motion': -0.33293495212071195, 'motion_component': -2.2085744950483175}]}, 4351: {'frame': 4351, 'ionic_force': [-5.821552753448486, -2.9807128310203552, -7.226513624191284], 'ionic_force_magnitude': 9.746672488742774, 'motion_vector': [0.9067535400390625, 2.27435302734375, -1.0322418212890625], 'cosine_ionic_motion': -0.17755595543049107, 'ionic_motion_component': -1.7305797460068055, 'ionic_force_x': -5.821552753448486, 'ionic_force_y': -2.9807128310203552, 'ionic_force_z': -7.226513624191284, 'radial_force': 6.540269523665904, 'axial_force': -7.226513624191284, 'contributions': [{'ion': 1316, 'force': [-1.437971591949463, -0.7615723013877869, -2.7652251720428467], 'magnitude': 3.2084615230560303, 'distance': 10.172334671020508, 'cosine_with_motion': -0.021299930527719835, 'motion_component': -0.06834000613675784}, {'ion': 1387, 'force': [-4.383581161499023, -2.2191405296325684, -4.4612884521484375], 'magnitude': 6.6365251541137695, 'distance': 7.07291841506958, 'cosine_with_motion': -0.2504684154112141, 'motion_component': -1.6622398829874785}]}, 4352: {'frame': 4352, 'ionic_force': [-3.8882360458374023, 0.07716289162635803, -8.414870738983154], 'ionic_force_magnitude': 9.270080000398504, 'motion_vector': [-1.1390266418457031, -0.5661506652832031, -1.0862197875976562], 'cosine_ionic_motion': 0.8722952131855376, 'ionic_motion_component': 8.086246410194603, 'ionic_force_x': -3.8882360458374023, 'ionic_force_y': 0.07716289162635803, 'ionic_force_z': -8.414870738983154, 'radial_force': 3.889001627666594, 'axial_force': -8.414870738983154, 'contributions': [{'ion': 1316, 'force': [-0.9431006908416748, -0.052728161215782166, -2.691154956817627], 'magnitude': 2.8521103858947754, 'distance': 10.789115905761719, 'cosine_with_motion': 0.8441814635731749, 'motion_component': 2.4076987968412804}, {'ion': 1387, 'force': [-2.9451353549957275, 0.1298910528421402, -5.723715782165527], 'magnitude': 6.438292980194092, 'distance': 7.180979251861572, 'cosine_with_motion': 0.8819958134782798, 'motion_component': 5.678547440850384}]}, 4353: {'frame': 4353, 'ionic_force': [-6.081224143505096, -0.8584663271903992, -9.448819756507874], 'ionic_force_magnitude': 11.269358735502326, 'motion_vector': [1.2044410705566406, -1.20880126953125, 0.8453292846679688], 'cosine_ionic_motion': -0.6651334853126875, 'ionic_motion_component': -7.495627852983643, 'ionic_force_x': -6.081224143505096, 'ionic_force_y': -0.8584663271903992, 'ionic_force_z': -9.448819756507874, 'radial_force': 6.141518665482428, 'axial_force': -9.448819756507874, 'contributions': [{'ion': 1308, 'force': [-0.4175664782524109, -0.13317164778709412, -1.4587963819503784], 'magnitude': 1.5232148170471191, 'distance': 14.763470649719238, 'cosine_with_motion': -0.5430137956490898, 'motion_component': -0.827126651667454}, {'ion': 1316, 'force': [-1.1213693618774414, -0.22113272547721863, -2.5067636966705322], 'magnitude': 2.755037784576416, 'distance': 10.977545738220215, 'cosine_with_motion': -0.6103808725777308, 'motion_component': -1.6816223630058307}, {'ion': 1387, 'force': [-4.542288303375244, -0.5041619539260864, -5.483259677886963], 'magnitude': 7.138115882873535, 'distance': 6.819888114929199, 'cosine_with_motion': -0.6986267543476838, 'motion_component': -4.986878762952777}]}, 4354: {'frame': 4354, 'ionic_force': [-3.467491030693054, -1.7887528538703918, -8.15508508682251], 'ionic_force_magnitude': 9.040384040154553, 'motion_vector': [-1.2567825317382812, 0.8124618530273438, 0.4911346435546875], 'cosine_ionic_motion': -0.077297958681048, 'ionic_motion_component': -0.6988032319966724, 'ionic_force_x': -3.467491030693054, 'ionic_force_y': -1.7887528538703918, 'ionic_force_z': -8.15508508682251, 'radial_force': 3.901683075310737, 'axial_force': -8.15508508682251, 'contributions': [{'ion': 1316, 'force': [-0.8548189401626587, -0.5112813115119934, -2.679126739501953], 'magnitude': 2.8582937717437744, 'distance': 10.777440071105957, 'cosine_with_motion': -0.14591067328640753, 'motion_component': -0.4170555891222918}, {'ion': 1387, 'force': [-2.6126720905303955, -1.2774715423583984, -5.475958347320557], 'magnitude': 6.200331687927246, 'distance': 7.317480564117432, 'cosine_with_motion': -0.045440745930926375, 'motion_component': -0.2817476814382047}]}, 4355: {'frame': 4355, 'ionic_force': [-4.742857813835144, -1.030191957950592, -6.752213716506958], 'ionic_force_magnitude': 8.315550840796288, 'motion_vector': [-0.8599281311035156, 1.072509765625, 0.5235366821289062], 'cosine_ionic_motion': -0.04589578220628883, 'ionic_motion_component': -0.38164871031450837, 'ionic_force_x': -4.742857813835144, 'ionic_force_y': -1.030191957950592, 'ionic_force_z': -6.752213716506958, 'radial_force': 4.853451937794703, 'axial_force': -6.752213716506958, 'contributions': [{'ion': 1316, 'force': [-1.2849539518356323, -0.36015647649765015, -2.5392329692840576], 'magnitude': 2.8685402870178223, 'distance': 10.758173942565918, 'cosine_with_motion': -0.14472490427713985, 'motion_component': -0.4151492194617141}, {'ion': 1387, 'force': [-3.4579038619995117, -0.6700354814529419, -4.2129807472229], 'magnitude': 5.491379737854004, 'distance': 7.77549934387207, 'cosine_with_motion': 0.006100551507003937, 'motion_component': 0.033500446055334976}]}, 4356: {'frame': 4356, 'ionic_force': [-8.145591795444489, 0.5536623261868954, -8.388230919837952], 'ionic_force_magnitude': 11.705538246231, 'motion_vector': [-0.17728042602539062, -5.445198059082031, 0.5759963989257812], 'cosine_ionic_motion': -0.09983658107924243, 'ionic_motion_component': -1.1686409181960145, 'ionic_force_x': -8.145591795444489, 'ionic_force_y': 0.5536623261868954, 'ionic_force_z': -8.388230919837952, 'radial_force': 8.164386545812935, 'axial_force': -8.388230919837952, 'contributions': [{'ion': 1308, 'force': [-0.6154080033302307, -0.04097851738333702, -1.5266047716140747], 'magnitude': 1.6464896202087402, 'distance': 14.20003890991211, 'cosine_with_motion': -0.06065081615029968, 'motion_component': -0.09986094493453779}, {'ion': 1316, 'force': [-1.5749125480651855, -0.061273880302906036, -2.6270933151245117], 'magnitude': 3.063612699508667, 'distance': 10.410033226013184, 'cosine_with_motion': -0.05364366311720108, 'motion_component': -0.16434341226880056}, {'ion': 1387, 'force': [-5.955271244049072, 0.6559147238731384, -4.234532833099365], 'magnitude': 7.336671352386475, 'distance': 6.726970195770264, 'cosine_with_motion': -0.12327614605629073, 'motion_component': -0.904436581779466}]}, 4357: {'frame': 4357, 'ionic_force': [-5.270969092845917, -5.013264775276184, -4.879510402679443], 'ionic_force_magnitude': 8.759312795797326, 'motion_vector': [0.0101470947265625, 0.001705169677734375, 0.09522247314453125], 'cosine_ionic_motion': -0.6277842758580351, 'ionic_motion_component': -5.498958840523645, 'ionic_force_x': -5.270969092845917, 'ionic_force_y': -5.013264775276184, 'ionic_force_z': -4.879510402679443, 'radial_force': 7.274334257151088, 'axial_force': -4.879510402679443, 'contributions': [{'ion': 1308, 'force': [-0.6041297316551208, -0.6097363233566284, -1.3066514730453491], 'magnitude': 1.5633583068847656, 'distance': 14.572691917419434, 'cosine_with_motion': -0.8788449065300563, 'motion_component': -1.3739494831185086}, {'ion': 1316, 'force': [-1.375537633895874, -1.3294124603271484, -1.9107221364974976], 'magnitude': 2.703756809234619, 'distance': 11.081160545349121, 'cosine_with_motion': -0.7652552232236913, 'motion_component': -2.069063945781279}, {'ion': 1387, 'force': [-3.291301727294922, -3.0741159915924072, -1.6621367931365967], 'magnitude': 4.800578594207764, 'distance': 8.31614875793457, 'cosine_with_motion': -0.4282703242108116, 'motion_component': -2.055945354053961}]}, 4358: {'frame': 4358, 'ionic_force': [-4.603870153427124, -3.909831404685974, -3.866476058959961], 'ionic_force_magnitude': 7.171613424969053, 'motion_vector': [1.1465644836425781, -0.06743621826171875, 0.3713531494140625], 'cosine_ionic_motion': -0.7451740365570843, 'ionic_motion_component': -5.344100124511165, 'ionic_force_x': -4.603870153427124, 'ionic_force_y': -3.909831404685974, 'ionic_force_z': -3.866476058959961, 'radial_force': 6.040066390585934, 'axial_force': -3.866476058959961, 'contributions': [{'ion': 1316, 'force': [-1.2709743976593018, -1.2347279787063599, -1.9208208322525024], 'magnitude': 2.613327741622925, 'distance': 11.27125072479248, 'cosine_with_motion': -0.6616836431521577, 'motion_component': -1.7291962063176305}, {'ion': 1387, 'force': [-3.3328957557678223, -2.6751034259796143, -1.9456552267074585], 'magnitude': 4.695737361907959, 'distance': 8.408473014831543, 'cosine_with_motion': -0.7698267254974382, 'motion_component': -3.6149038997023144}]}, 4359: {'frame': 4359, 'ionic_force': [-6.097867250442505, -7.210108399391174, -5.836791396141052], 'ionic_force_magnitude': 11.101251368069125, 'motion_vector': [-1.8090705871582031, 0.6514205932617188, -0.31896209716796875], 'cosine_ionic_motion': 0.3788134547827392, 'ionic_motion_component': 4.205303383149875, 'ionic_force_x': -6.097867250442505, 'ionic_force_y': -7.210108399391174, 'ionic_force_z': -5.836791396141052, 'radial_force': 9.442968184580016, 'axial_force': -5.836791396141052, 'contributions': [{'ion': 1308, 'force': [-0.5732018947601318, -0.8108179569244385, -1.6454930305480957], 'magnitude': 1.9218828678131104, 'distance': 13.143335342407227, 'cosine_with_motion': 0.2759391664501587, 'motion_component': 0.5303227369907617}, {'ion': 1316, 'force': [-1.4675121307373047, -1.8761595487594604, -2.2478926181793213], 'magnitude': 3.275146961212158, 'distance': 10.068242073059082, 'cosine_with_motion': 0.33675482397552703, 'motion_component': 1.1029215441539115}, {'ion': 1387, 'force': [-4.057153224945068, -4.523130893707275, -1.9434057474136353], 'magnitude': 6.379344463348389, 'distance': 7.214081287384033, 'cosine_with_motion': 0.4031854911937974, 'motion_component': 2.572058988408134}]}, 4360: {'frame': 4360, 'ionic_force': [-5.140026926994324, -3.9340438842773438, -3.686625123023987], 'ionic_force_magnitude': 7.449012209102514, 'motion_vector': [-0.8460655212402344, 0.20500564575195312, 0.1761016845703125], 'cosine_ionic_motion': 0.4372801521611261, 'ionic_motion_component': 3.257305192246433, 'ionic_force_x': -5.140026926994324, 'ionic_force_y': -3.9340438842773438, 'ionic_force_z': -3.686625123023987, 'radial_force': 6.472756607014254, 'axial_force': -3.686625123023987, 'contributions': [{'ion': 1316, 'force': [-1.4018090963363647, -1.172297477722168, -1.9389605522155762], 'magnitude': 2.664379358291626, 'distance': 11.162744522094727, 'cosine_with_motion': 0.25533607786550655, 'motion_component': 0.6803122125233402}, {'ion': 1387, 'force': [-3.738217830657959, -2.761746406555176, -1.7476645708084106], 'magnitude': 4.965465545654297, 'distance': 8.17690658569336, 'cosine_with_motion': 0.518983195660116, 'motion_component': 2.576993131386971}]}, 4361: {'frame': 4361, 'ionic_force': [-5.4141963720321655, -3.7038130164146423, -4.313818573951721], 'ionic_force_magnitude': 7.851164493529584, 'motion_vector': [1.1817245483398438, -0.8403396606445312, -0.4484710693359375], 'cosine_ionic_motion': -0.11337134838642916, 'ionic_motion_component': -0.8900971050351052, 'ionic_force_x': -5.4141963720321655, 'ionic_force_y': -3.7038130164146423, 'ionic_force_z': -4.313818573951721, 'radial_force': 6.559859237475206, 'axial_force': -4.313818573951721, 'contributions': [{'ion': 1308, 'force': [-0.7086317539215088, -0.5181094408035278, -1.3205690383911133], 'magnitude': 1.5857172012329102, 'distance': 14.469588279724121, 'cosine_with_motion': 0.07903236422258367, 'motion_component': 0.1253229768646662}, {'ion': 1316, 'force': [-1.3960002660751343, -0.9637919068336487, -1.544816255569458], 'magnitude': 2.294377565383911, 'distance': 12.029195785522461, 'cosine_with_motion': -0.04220302413094465, 'motion_component': -0.09682967574426726}, {'ion': 1387, 'force': [-3.3095643520355225, -2.221911668777466, -1.44843327999115], 'magnitude': 4.241234302520752, 'distance': 8.84754753112793, 'cosine_with_motion': -0.21658561481700964, 'motion_component': -0.9185902935916275}]}, 4362: {'frame': 4362, 'ionic_force': [-4.9034892320632935, -4.803059756755829, -4.693336129188538], 'ionic_force_magnitude': 8.315106355151116, 'motion_vector': [0.7227058410644531, -0.5454826354980469, 0.70068359375], 'cosine_ionic_motion': -0.4424713221093263, 'ionic_motion_component': -3.6791961024433757, 'ionic_force_x': -4.9034892320632935, 'ionic_force_y': -4.803059756755829, 'ionic_force_z': -4.693336129188538, 'radial_force': 6.863933979572358, 'axial_force': -4.693336129188538, 'contributions': [{'ion': 1308, 'force': [-0.5720486640930176, -0.5742262005805969, -1.2654268741607666], 'magnitude': 1.5027576684951782, 'distance': 14.863618850708008, 'cosine_with_motion': -0.573580941371845, 'motion_component': -0.8619531518802396}, {'ion': 1316, 'force': [-1.2409831285476685, -1.17379891872406, -1.7205088138580322], 'magnitude': 2.424457311630249, 'distance': 11.702045440</t>
+          <t>{4333: {'frame': 4333, 'ionic_force': [5.670064628124237, -0.11623673886060715, -16.053759455680847], 'ionic_force_magnitude': 17.02604876439125, 'motion_vector': [-1.0914764404296875, 2.8184471130371094, 0.5848388671875], 'cosine_ionic_motion': -0.30345207696552395, 'ionic_motion_component': -5.166589860070817, 'ionic_force_x': 5.670064628124237, 'ionic_force_y': -0.11623673886060715, 'ionic_force_z': -16.053759455680847, 'radial_force': 5.671255933791614, 'axial_force': -16.053759455680847, 'before_closest_residue': None, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.17358297109603882, -0.07655664533376694, -1.6345635652542114], 'magnitude': 1.6455363035202026, 'distance': 14.20415210723877, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2687048108516073, 'motion_component': -0.4421635449013345}, {'ion': 1316, 'force': [0.8972761631011963, -0.14553450047969818, -3.8930156230926514], 'magnitude': 3.9977312088012695, 'distance': 9.113018035888672, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2979077327293967, 'motion_component': -1.190955063856654}, {'ion': 1387, 'force': [4.599205493927002, 0.10585440695285797, -10.526180267333984], 'magnitude': 11.487574577331543, 'distance': 5.375945568084717, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.30759072151122985, 'motion_component': -3.5334713216154103}]}, 4334: {'frame': 4334, 'ionic_force': [3.895419254899025, 7.656647235155106, -16.01752197742462], 'ionic_force_magnitude': 18.175795673156294, 'motion_vector': [0.5448684692382812, -2.2713394165039062, -1.4224014282226562], 'cosine_ionic_motion': 0.15118571210621812, 'ionic_motion_component': 2.747920611943252, 'ionic_force_x': 3.895419254899025, 'ionic_force_y': 7.656647235155106, 'ionic_force_z': -16.01752197742462, 'radial_force': 8.59060754865722, 'axial_force': -16.01752197742462, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 780, 'contributions': [{'ion': 1308, 'force': [0.18028856813907623, 0.2747263014316559, -1.6901415586471558], 'magnitude': 1.721789002418518, 'distance': 13.886061668395996, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.39889620431807066, 'motion_component': 0.6868150546000797}, {'ion': 1316, 'force': [0.8013342618942261, 1.1461530923843384, -3.9313461780548096], 'magnitude': 4.172683238983154, 'distance': 8.919927597045898, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3001616454276057, 'motion_component': 1.2524794981272755}, {'ion': 1387, 'force': [2.9137964248657227, 6.235767841339111, -10.396034240722656], 'magnitude': 12.468061447143555, 'distance': 5.160236358642578, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.06485580436767582, 'motion_component': 0.8086261068832242}]}, 4335: {'frame': 4335, 'ionic_force': [7.201493963599205, 1.6286407187581062, -22.629054307937622], 'ionic_force_magnitude': 23.803110821280125, 'motion_vector': [-2.4897499084472656, -1.9592094421386719, -2.6416397094726562], 'cosine_ionic_motion': 0.3937050990196898, 'ionic_motion_component': 9.371406102868741, 'ionic_force_x': 7.201493963599205, 'ionic_force_y': 1.6286407187581062, 'ionic_force_z': -22.629054307937622, 'radial_force': 7.383358713929096, 'axial_force': -22.629054307937622, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 1105, 'contributions': [{'ion': 1308, 'force': [0.17067889869213104, -0.07447502017021179, -1.5542986392974854], 'magnitude': 1.565414309501648, 'distance': 14.563118934631348, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5926381165473805, 'motion_component': 0.9277242097333298}, {'ion': 1316, 'force': [0.7298926711082458, 0.04116610437631607, -3.5585622787475586], 'magnitude': 3.632878065109253, 'distance': 9.559685707092285, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5006490876675077, 'motion_component': 1.8187971175178699}, {'ion': 1387, 'force': [6.300922393798828, 1.661949634552002, -17.516193389892578], 'magnitude': 18.68905258178711, 'distance': 4.214784622192383, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3544794253429433, 'motion_component': 6.624885037317597}]}, 4336: {'frame': 4336, 'ionic_force': [-0.5388405174016953, -1.7428620159626007, -9.03514313697815], 'ionic_force_magnitude': 9.217468666372689, 'motion_vector': [0.6896553039550781, 0.1011199951171875, 0.940399169921875], 'cosine_ionic_motion': -0.8382634653281991, 'ionic_motion_component': -7.726667225827664, 'ionic_force_x': -0.5388405174016953, 'ionic_force_y': -1.7428620159626007, 'ionic_force_z': -9.03514313697815, 'radial_force': 1.8242579614404721, 'axial_force': -9.03514313697815, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-0.19560758769512177, -0.3452792465686798, -2.427891969680786], 'magnitude': 2.4601097106933594, 'distance': 11.616941452026367, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8518276766603495, 'motion_component': -2.0955894897212177}, {'ion': 1387, 'force': [-0.3432329297065735, -1.397582769393921, -6.607251167297363], 'magnitude': 6.762160301208496, 'distance': 7.006906032562256, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8327335038641387, 'motion_component': -5.631077594624198}]}, 4337: {'frame': 4337, 'ionic_force': [-0.16387367993593216, -1.5002783238887787, -8.31986379623413], 'ionic_force_magnitude': 8.455638545964089, 'motion_vector': [-1.2149238586425781, 0.8994140625, 1.17535400390625], 'cosine_ionic_motion': -0.6750159695501066, 'ionic_motion_component': -5.707691051269203, 'ionic_force_x': -0.16387367993593216, 'ionic_force_y': -1.5002783238887787, 'ionic_force_z': -8.31986379623413, 'radial_force': 1.509201653890648, 'axial_force': -8.31986379623413, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 780, 'contributions': [{'ion': 1316, 'force': [-0.0917414203286171, -0.38027724623680115, -2.686659812927246], 'magnitude': 2.714989423751831, 'distance': 11.058213233947754, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6517738113728772, 'motion_component': -1.7695590827597387}, {'ion': 1387, 'force': [-0.07213225960731506, -1.1200010776519775, -5.633203983306885], 'magnitude': 5.743917942047119, 'distance': 7.602648735046387, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6856177321457585, 'motion_component': -3.9381319494534495}]}, 4338: {'frame': 4338, 'ionic_force': [-2.4280003905296326, -1.0742815136909485, -10.110801935195923], 'ionic_force_magnitude': 10.453591843946834, 'motion_vector': [1.5186386108398438, 5.265224456787109, -0.11255645751953125], 'cosine_ionic_motion': -0.1432126280334982, 'ionic_motion_component': -1.4970863603611686, 'ionic_force_x': -2.4280003905296326, 'ionic_force_y': -1.0742815136909485, 'ionic_force_z': -10.110801935195923, 'radial_force': 2.655045511299225, 'axial_force': -10.110801935195923, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 130, 'contributions': [{'ion': 1316, 'force': [-0.5445583462715149, -0.3111899495124817, -2.85630202293396], 'magnitude': 2.92435359954834, 'distance': 10.65501594543457, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.13376092719612437, 'motion_component': -0.39116425460121373}, {'ion': 1387, 'force': [-1.8834420442581177, -0.7630915641784668, -7.254499912261963], 'magnitude': 7.533752918243408, 'distance': 6.638399124145508, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.14679564559442262, 'motion_component': -1.10592210987212}]}, 4339: {'frame': 4339, 'ionic_force': [-0.01052268361672759, 7.317051321268082, -8.848112106323242], 'ionic_force_magnitude': 11.48165661440044, 'motion_vector': [-0.3119239807128906, 0.11574172973632812, 2.2965164184570312], 'cosine_ionic_motion': -0.7307586444093754, 'ionic_motion_component': -8.390319823113206, 'ionic_force_x': -0.01052268361672759, 'ionic_force_y': 7.317051321268082, 'ionic_force_z': -8.848112106323242, 'radial_force': 7.317058887622914, 'axial_force': -8.848112106323242, 'before_closest_residue': 780, 'closest_residue': 130, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.015117759816348553, 0.40834537148475647, -1.4295883178710938], 'magnitude': 1.4868414402008057, 'distance': 14.942962646484375, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9392277961859843, 'motion_component': -1.3964827394725436}, {'ion': 1316, 'force': [-0.007704783696681261, 1.2880055904388428, -2.648350715637207], 'magnitude': 2.944958209991455, 'distance': 10.61767578125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8678253609626467, 'motion_component': -2.5557094833582963}, {'ion': 1387, 'force': [-0.017935659736394882, 5.620700359344482, -4.770173072814941], 'magnitude': 7.37205171585083, 'distance': 6.710808753967285, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6020206998732269, 'motion_component': -4.438127686965383}]}, 4340: {'frame': 4340, 'ionic_force': [-0.6614977717399597, 11.020213901996613, -11.043931484222412], 'ionic_force_magnitude': 15.615732975943697, 'motion_vector': [0.09852218627929688, -2.540813446044922, -1.569000244140625], 'cosine_ionic_motion': -0.23013628428245336, 'ionic_motion_component': -3.59374676343066, 'ionic_force_x': -0.6614977717399597, 'ionic_force_y': 11.020213901996613, 'ionic_force_z': -11.043931484222412, 'radial_force': 11.040049535567144, 'axial_force': -11.043931484222412, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.11230937391519547, 0.5389495491981506, -1.9288716316223145], 'magnitude': 2.0058977603912354, 'distance': 12.865143775939941, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.27463385257681466, 'motion_component': 0.5508874269489278}, {'ion': 1316, 'force': [-0.09320607036352158, 2.1498072147369385, -3.7819480895996094], 'magnitude': 4.351263046264648, 'distance': 8.734969139099121, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.03556952269342487, 'motion_component': 0.15477234838873555}, {'ion': 1387, 'force': [-0.4559823274612427, 8.331457138061523, -5.333111763000488], 'magnitude': 9.902685165405273, 'distance': 5.790186405181885, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.43416573845546347, 'motion_component': -4.299406738489893}]}, 4341: {'frame': 4341, 'ionic_force': [-1.1659248024225235, 9.977354973554611, -17.802505493164062], 'ionic_force_magnitude': 20.441041919318973, 'motion_vector': [-0.7720985412597656, -0.6841316223144531, -3.7374649047851562], 'cosine_ionic_motion': 0.7647606975638053, 'ionic_motion_component': 15.632505477149364, 'ionic_force_x': -1.1659248024225235, 'ionic_force_y': 9.977354973554611, 'ionic_force_z': -17.802505493164062, 'radial_force': 10.045247279844283, 'axial_force': -17.802505493164062, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.09177793562412262, 0.24030449986457825, -1.6979613304138184], 'magnitude': 1.717335820198059, 'distance': 13.904053688049316, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9390324383797626, 'motion_component': 1.6126339887252703}, {'ion': 1316, 'force': [-0.13407957553863525, 0.977773129940033, -3.8091092109680176], 'magnitude': 3.9348864555358887, 'distance': 9.185503005981445, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8960829730796381, 'motion_component': 3.5259846615014645}, {'ion': 1387, 'force': [-0.9400672912597656, 8.75927734375, -12.295434951782227], 'magnitude': 15.125685691833496, 'distance': 4.685020446777344, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6937792513859733, 'motion_component': 10.493887334066017}]}, 4342: {'frame': 4342, 'ionic_force': [-1.3840811252593994, 1.351293995976448, -7.411204814910889], 'ionic_force_magnitude': 7.659479932307392, 'motion_vector': [-2.657154083251953, -1.6822662353515625, 5.648590087890625], 'cosine_ionic_motion': -0.8170268253809583, 'ionic_motion_component': -6.258000573162266, 'ionic_force_x': -1.3840811252593994, 'ionic_force_y': 1.351293995976448, 'ionic_force_z': -7.411204814910889, 'radial_force': 1.9343412379570781, 'axial_force': -7.411204814910889, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1316, 'force': [-0.2974294424057007, 0.23622436821460724, -2.1497864723205566], 'magnitude': 2.183082342147827, 'distance': 12.332013130187988, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.832544475446919, 'motion_component': -1.8175130650926032}, {'ion': 1387, 'force': [-1.0866516828536987, 1.1150696277618408, -5.261418342590332], 'magnitude': 5.4869585037231445, 'distance': 7.778631687164307, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8092803195561473, 'motion_component': -4.440487642549986}]}, 4343: {'frame': 4343, 'ionic_force': [-16.709574282169342, -0.8938723057508469, -13.62956953048706], 'ionic_force_magnitude': 21.58179895135493, 'motion_vector': [2.1892776489257812, 5.375339508056641, -3.4262237548828125], 'cosine_ionic_motion': 0.036513285370066664, 'ionic_motion_component': 0.788022383910228, 'ionic_force_x': -16.709574282169342, 'ionic_force_y': -0.8938723057508469, 'ionic_force_z': -13.62956953048706, 'radial_force': 16.733465880992004, 'axial_force': -13.62956953048706, 'before_closest_residue': 130, 'closest_residue': 'SF', 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.6828966736793518, -0.1254197210073471, -2.168544292449951], 'magnitude': 2.2769854068756104, 'distance': 12.07504940032959, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.34279108699768035, 'motion_component': 0.7805302860302322}, {'ion': 1316, 'force': [-2.210134983062744, -0.2589053511619568, -4.237045764923096], 'magnitude': 4.785842418670654, 'distance': 8.32894229888916, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2569054433894155, 'motion_component': 1.2295089090269506}, {'ion': 1387, 'force': [-13.816542625427246, -0.509547233581543, -7.223979473114014], 'magnitude': 15.599434852600098, 'distance': 4.613330841064453, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.07833721866182479, 'motion_component': -1.2220163395787154}]}, 4344: {'frame': 4344, 'ionic_force': [-1.153914988040924, 3.170382857322693, -5.203489422798157], 'ionic_force_magnitude': 6.201544116976302, 'motion_vector': [1.4634857177734375, -1.2306327819824219, 0.8022537231445312], 'cosine_ionic_motion': -0.7593428919930103, 'ionic_motion_component': -4.709098444607024, 'ionic_force_x': -1.153914988040924, 'ionic_force_y': 3.170382857322693, 'ionic_force_z': -5.203489422798157, 'radial_force': 3.373847545700767, 'axial_force': -5.203489422798157, 'before_closest_residue': 'SF', 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1316, 'force': [-0.2957773804664612, 0.846617579460144, -1.985202670097351], 'magnitude': 2.1783652305603027, 'distance': 12.345357894897461, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6790620152713646, 'motion_component': -1.4792451065752275}, {'ion': 1387, 'force': [-0.8581376075744629, 2.323765277862549, -3.2182867527008057], 'magnitude': 4.061237812042236, 'distance': 9.041485786437988, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7952878508257138, 'motion_component': -3.2298533141553847}]}, 4345: {'frame': 4345, 'ionic_force': [0.08994757011532784, 5.610477715730667, -9.722934126853943], 'ionic_force_magnitude': 11.225907482213682, 'motion_vector': [-1.1395187377929688, 0.0416717529296875, -1.0085220336914062], 'cosine_ionic_motion': 0.5814891324386149, 'ionic_motion_component': 6.5277432026685895, 'ionic_force_x': 0.08994757011532784, 'ionic_force_y': 5.610477715730667, 'ionic_force_z': -9.722934126853943, 'radial_force': 5.611198692265321, 'axial_force': -9.722934126853943, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.04955724999308586, 0.3378300964832306, -1.4625250101089478], 'magnitude': 1.5018537044525146, 'distance': 14.868091583251953, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6760140450308809, 'motion_component': 1.0152741867035733}, {'ion': 1316, 'force': [-0.044318169355392456, 1.0932285785675049, -2.809373140335083], 'magnitude': 3.014911413192749, 'distance': 10.493775367736816, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6382689866249723, 'motion_component': 1.9243243929068639}, {'ion': 1387, 'force': [0.18382298946380615, 4.179419040679932, -5.451035976409912], 'magnitude': 6.871326446533203, 'distance': 6.951023101806641, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5221909782986967, 'motion_component': 3.5881446979568086}]}, 4346: {'frame': 4346, 'ionic_force': [-0.9703720510005951, 4.194342374801636, -6.858072519302368], 'ionic_force_magnitude': 8.097363061789316, 'motion_vector': [-4.582515716552734, 0.4224891662597656, 2.309173583984375], 'cosine_ionic_motion': -0.23068510028921504, 'ionic_motion_component': -1.867941009987054, 'ionic_force_x': -0.9703720510005951, 'ionic_force_y': 4.194342374801636, 'ionic_force_z': -6.858072519302368, 'radial_force': 4.305128322642628, 'axial_force': -6.858072519302368, 'before_closest_residue': 455, 'closest_residue': 130, 'next_closest_residue': 98, 'contributions': [{'ion': 1316, 'force': [-0.26130351424217224, 0.9197101593017578, -2.4406163692474365], 'magnitude': 2.6212124824523926, 'distance': 11.25428581237793, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.30007228847047807, 'motion_component': -0.7865532102811734}, {'ion': 1387, 'force': [-0.7090685367584229, 3.274632215499878, -4.417456150054932], 'magnitude': 5.544358730316162, 'distance': 7.7382612228393555, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.1950429042251414, 'motion_component': -1.0813878190443305}]}, 4347: {'frame': 4347, 'ionic_force': [-5.324795186519623, 4.4520832896232605, -5.531670093536377], 'ionic_force_magnitude': 8.87546412419373, 'motion_vector': [-0.36487579345703125, -0.39484405517578125, 1.3642425537109375], 'cosine_ionic_motion': -0.5656374441017312, 'ionic_motion_component': -5.020294842425552, 'ionic_force_x': -5.324795186519623, 'ionic_force_y': 4.4520832896232605, 'ionic_force_z': -5.531670093536377, 'radial_force': 6.940784494286306, 'axial_force': -5.531670093536377, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.5734414458274841, 0.4193485379219055, -1.335965633392334], 'magnitude': 1.5131069421768188, 'distance': 14.812700271606445, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8017682373028415, 'motion_component': -1.213161044334834}, {'ion': 1316, 'force': [-1.3264715671539307, 1.0629514455795288, -2.074846029281616], 'magnitude': 2.6822338104248047, 'distance': 11.125530242919922, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7033365199731868, 'motion_component': -1.8865130497748017}, {'ion': 1387, 'force': [-3.424882173538208, 2.969783306121826, -2.1208584308624268], 'magnitude': 5.004745006561279, 'distance': 8.144756317138672, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3837599886865634, 'motion_component': -1.9206208369105298}]}, 4348: {'frame': 4348, 'ionic_force': [-4.811583518981934, 3.2644795179367065, -4.231451034545898], 'ionic_force_magnitude': 7.191198811111148, 'motion_vector': [1.2287940979003906, -3.6073760986328125, -4.4157257080078125], 'cosine_ionic_motion': 0.023752005658367503, 'ionic_motion_component': 0.17080539485195764, 'ionic_force_x': -4.811583518981934, 'ionic_force_y': 3.2644795179367065, 'ionic_force_z': -4.231451034545898, 'radial_force': 5.8144786940160715, 'axial_force': -4.231451034545898, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-1.6572506427764893, 1.0221670866012573, -2.0923280715942383], 'magnitude': 2.858170986175537, 'distance': 10.777670860290527, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2108659991227886, 'motion_component': 0.602691103493072}, {'ion': 1387, 'force': [-3.1543328762054443, 2.242312431335449, -2.13912296295166], 'magnitude': 4.421948432922363, 'distance': 8.664873123168945, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.09766865255972287, 'motion_component': -0.43188574558306664}]}, 4349: {'frame': 4349, 'ionic_force': [-2.8148942589759827, 0.3423163443803787, -5.1887286901474], 'ionic_force_magnitude': 5.913012395455015, 'motion_vector': [3.6558074951171875, 0.5428085327148438, 1.3375320434570312], 'cosine_ionic_motion': -0.7334051060764676, 'ionic_motion_component': -4.336633483120153, 'ionic_force_x': -2.8148942589759827, 'ionic_force_y': 0.3423163443803787, 'ionic_force_z': -5.1887286901474, 'radial_force': 2.835632234413675, 'axial_force': -5.1887286901474, 'before_closest_residue': 98, 'closest_residue': 1105, 'next_closest_residue': 130, 'contributions': [{'ion': 1316, 'force': [-0.7681282162666321, 0.059397414326667786, -1.9104300737380981], 'magnitude': 2.0599253177642822, 'distance': 12.69530963897705, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.658453806185171, 'motion_component': -1.356365627793785}, {'ion': 1387, 'force': [-2.0467660427093506, 0.28291893005371094, -3.2782986164093018], 'magnitude': 3.875117540359497, 'distance': 9.25606918334961, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.769078047461971, 'motion_component': -2.9802678535875486}]}, 4350: {'frame': 4350, 'ionic_force': [-1.14635768532753, 1.0225782543420792, -9.443222522735596], 'ionic_force_magnitude': 9.567353544364483, 'motion_vector': [-3.0155258178710938, -3.347362518310547, 1.5890350341796875], 'cosine_ionic_motion': -0.3275592344848105, 'ionic_motion_component': -3.1338750030375686, 'ionic_force_x': -1.14635768532753, 'ionic_force_y': 1.0225782543420792, 'ionic_force_z': -9.443222522735596, 'radial_force': 1.536164779235218, 'axial_force': -9.443222522735596, 'before_closest_residue': 1105, 'closest_residue': 130, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-0.2180737555027008, 0.12293900549411774, -2.9367432594299316], 'magnitude': 2.9473938941955566, 'distance': 10.613287925720215, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.31393846865149616, 'motion_component': -0.9253003451579868}, {'ion': 1387, 'force': [-0.9282839298248291, 0.8996392488479614, -6.506479263305664], 'magnitude': 6.6336517333984375, 'distance': 7.074450492858887, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.33293495212071195, 'motion_component': -2.2085744950483175}]}, 4351: {'frame': 4351, 'ionic_force': [-5.821552753448486, -2.9807128310203552, -7.226513624191284], 'ionic_force_magnitude': 9.746672488742774, 'motion_vector': [0.9067535400390625, 2.27435302734375, -1.0322418212890625], 'cosine_ionic_motion': -0.17755595543049107, 'ionic_motion_component': -1.7305797460068055, 'ionic_force_x': -5.821552753448486, 'ionic_force_y': -2.9807128310203552, 'ionic_force_z': -7.226513624191284, 'radial_force': 6.540269523665904, 'axial_force': -7.226513624191284, 'before_closest_residue': 130, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-1.437971591949463, -0.7615723013877869, -2.7652251720428467], 'magnitude': 3.2084615230560303, 'distance': 10.172334671020508, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.021299930527719835, 'motion_component': -0.06834000613675784}, {'ion': 1387, 'force': [-4.383581161499023, -2.2191405296325684, -4.4612884521484375], 'magnitude': 6.6365251541137695, 'distance': 7.07291841506958, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2504684154112141, 'motion_component': -1.6622398829874785}]}, 4352: {'frame': 4352, 'ionic_force': [-3.8882360458374023, 0.07716289162635803, -8.414870738983154], 'ionic_force_magnitude': 9.270080000398504, 'motion_vector': [-1.1390266418457031, -0.5661506652832031, -1.0862197875976562], 'cosine_ionic_motion': 0.8722952131855376, 'ionic_motion_component': 8.086246410194603, 'ionic_force_x': -3.8882360458374023, 'ionic_force_y': 0.07716289162635803, 'ionic_force_z': -8.414870738983154, 'radial_force': 3.889001627666594, 'axial_force': -8.414870738983154, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-0.9431006908416748, -0.052728161215782166, -2.691154956817627], 'magnitude': 2.8521103858947754, 'distance': 10.789115905761719, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8441814635731749, 'motion_component': 2.4076987968412804}, {'ion': 1387, 'force': [-2.9451353549957275, 0.1298910528421402, -5.723715782165527], 'magnitude': 6.438292980194092, 'distance': 7.180979251861572, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8819958134782798, 'motion_component': 5.678547440850384}]}, 4353: {'frame': 4353, 'ionic_force': [-6.081224143505096, -0.8584663271903992, -9.448819756507874], 'ionic_force_magnitude': 11.269358735502326, 'motion_vector': [1.2044410705566406, -1.20880126953125, 0.8453292846679688], 'cosine_ionic_motion': -0.6651334853126875, 'ionic_motion_component': -7.495627852983643, 'ionic_force_x': -6.081224143505096, 'ionic_force_y': -0.8584663271903992, 'ionic_force_z': -9.448819756507874, 'radial_force': 6.141518665482428, 'axial_force': -9.448819756507874, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1308, 'force': [-0.4175664782524109, -0.13317164778709412, -1.4587963819503784], 'magnitude': 1.5232148170471191, 'distance': 14.763470649719238, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5430137956490898, 'motion_component': -0.827126651667454}, {'ion': 1316, 'force': [-1.1213693618774414, -0.22113272547721863, -2.5067636966705322], 'magnitude': 2.755037784576416, 'distance': 10.977545738220215, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6103808725777308, 'motion_component': -1.6816223630058307}, {'ion': 1387, 'force': [-4.542288303375244, -0.5041619539260864, -5.483259677886963], 'magnitude': 7.138115882873535, 'distance': 6.819888114929199, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6986267543476838, 'motion_component': -4.986878762952777}]}, 4354: {'frame': 4354, 'ionic_force': [-3.467491030693054, -1.7887528538703918, -8.15508508682251], 'ionic_force_magnitude': 9.040384040154553, 'motion_vector': [-1.2567825317382812, 0.8124618530273438, 0.4911346435546875], 'cosine_ionic_motion': -0.077297958681048, 'ionic_motion_component': -0.6988032319966724, 'ionic_force_x': -3.467491030693054, 'ionic_force_y': -1.7887528538703918, 'ionic_force_z': -8.15508508682251, 'radial_force': 3.901683075310737, 'axial_force': -8.15508508682251, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-0.8548189401626587, -0.5112813115119934, -2.679126739501953], 'magnitude': 2.8582937717437744, 'distance': 10.777440071105957, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.14591067328640753, 'motion_component': -0.4170555891222918}, {'ion': 1387, 'force': [-2.6126720905303955, -1.2774715423583984, -5.475958347320557], 'magnitude': 6.200331687927246, 'distance': 7.317480564117432, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.045440745930926375, 'motion_component': -0.2817476814382047}]}, 4355: {'frame': 4355, 'ionic_force': [-4.742857813835144, -1.030191957950592, -6.752213716506958], 'ionic_force_magnitude': 8.315550840796288, 'motion_vector': [-0.8599281311035156, 1.072509765625, 0.5235366821289062], 'cosine_ionic_motion': -0.04589578220628883, 'ionic_motion_component': -0.38164871031450837, 'ionic_force_x': -4.742857813835144, 'ionic_force_y': -1.030191957950592, 'ionic_force_z': -6.752213716506958, 'radial_force': 4.853451937794703, 'axial_force': -6.752213716506958, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1316, 'force': [-1.2849539518356323, -0.36015647649765015, -2.5392329692840576], 'magnitude': 2.8685402870178223, 'distance': 10.758173942565918, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.14472490427713985, 'motion_component': -0.4151492194617141}, {'ion': 1387, 'force': [-3.4579038619995117, -0.6700354814529419, -4.2129807472229], 'magnitude': 5.491379737854004, 'distance': 7.77549934387207, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.006100551507003937, 'motion_component': 0.033500446055334976}]}, 4356: {'frame': 4356, 'ionic_force': [-8.145591795444489, 0.5536623261868954, -8.388230919837952], 'ionic_force_magnitude': 11.705538246231, 'motion_vector': [-0.17728042602539062, -5.445198059082031, 0.5759963989257812], 'cosine_ionic_motion': -0.09983658107924243, 'ionic_motion_component': -1.1686409181960145, 'ionic_force_x': -8.145591795444489, 'ionic_force_y': 0.5536623261868954, 'ionic_force_z': -8.388230919837952, 'radial_force': 8.164386545812935, 'axial_force': -8.388230919837952, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1073, 'contributions': [{'ion': 1308, 'force': [-0.6154080033302307, -0.04097851738333702, -1.5266047716140747], 'magnitude': 1.6464896202087402, 'distance': 14.20003890991211, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.06065081615029968, 'motion_component': -0.09986094493453779}, {'i</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{4408: {'frame': 4408, 'ionic_force': [9.28405300155282, -3.821890950202942, -9.041797399520874], 'ionic_force_magnitude': 13.51127643062888, 'motion_vector': [0.9472541809082031, 6.171745300292969, -2.0280227661132812], 'cosine_ionic_motion': 0.03994897088398283, 'ionic_motion_component': 0.5397615887326366, 'ionic_force_x': 9.28405300155282, 'ionic_force_y': -3.821890950202942, 'ionic_force_z': -9.041797399520874, 'radial_force': 10.039944749394046, 'axial_force': -9.041797399520874, 'contributions': [{'ion': 1308, 'force': [0.0392477847635746, -0.5659531354904175, -1.739326000213623], 'magnitude': 1.8295077085494995, 'distance': 13.471064567565918, 'cosine_with_motion': 0.00596555141577959, 'motion_component': 0.010914022006728752}, {'ion': 1316, 'force': [0.1305760145187378, -2.5276927947998047, -4.4630842208862305], 'magnitude': 5.130828380584717, 'distance': 8.044059753417969, 'cosine_with_motion': -0.190751381479075, 'motion_component': -0.9787126361579297}, {'ion': 1460, 'force': [9.114229202270508, -0.7282450199127197, -2.8393871784210205], 'magnitude': 9.574007987976074, 'distance': 5.888736724853516, 'cosine_with_motion': 0.157463841084995, 'motion_component': 1.5075601164077739}]}, 4409: {'frame': 4409, 'ionic_force': [2.3813661485910416, 3.48429112136364, -6.0583014488220215], 'ionic_force_magnitude': 7.383373605396644, 'motion_vector': [1.2028884887695312, 0.22224044799804688, -0.367950439453125], 'cosine_ionic_motion': 0.6221774438388844, 'ionic_motion_component': 4.593768516713172, 'ionic_force_x': 2.3813661485910416, 'ionic_force_y': 3.48429112136364, 'ionic_force_z': -6.0583014488220215, 'radial_force': 4.220330479010953, 'axial_force': -6.0583014488220215, 'contributions': [{'ion': 1308, 'force': [0.11879675090312958, 0.2119782418012619, -1.456363558769226], 'magnitude': 1.4764965772628784, 'distance': 14.995219230651855, 'cosine_with_motion': 0.38486557312870256, 'motion_component': 0.5682527165054461}, {'ion': 1316, 'force': [0.3882765471935272, 1.0418009757995605, -3.5045788288116455], 'magnitude': 3.6767079830169678, 'distance': 9.502534866333008, 'cosine_with_motion': 0.4233068597611323, 'motion_component': 1.5563756601938152}, {'ion': 1460, 'force': [1.8742928504943848, 2.2305119037628174, -1.09735906124115], 'magnitude': 3.1132545471191406, 'distance': 10.326704025268555, 'cosine_with_motion': 0.7931057531386033, 'motion_component': 2.469140102033048}]}, 4410: {'frame': 4410, 'ionic_force': [2.7379980981349945, 3.005010947585106, -6.075490713119507], 'ionic_force_magnitude': 7.310151283366067, 'motion_vector': [-0.20865249633789062, -4.049587249755859, 2.408935546875], 'cosine_ionic_motion': -0.7939953037108676, 'ionic_motion_component': -5.804225788408629, 'ionic_force_x': 2.7379980981349945, 'ionic_force_y': 3.005010947585106, 'ionic_force_z': -6.075490713119507, 'radial_force': 4.065307415251297, 'axial_force': -6.075490713119507, 'contributions': [{'ion': 1308, 'force': [0.2570955455303192, 0.21237300336360931, -1.531499981880188], 'magnitude': 1.5673840045928955, 'distance': 14.55396556854248, 'cosine_with_motion': -0.6226418300254172, 'motion_component': -0.9759188427346958}, {'ion': 1316, 'force': [1.0977156162261963, 1.1136078834533691, -3.712677240371704], 'magnitude': 4.0285325050354, 'distance': 9.078113555908203, 'cosine_with_motion': -0.7200942571398282, 'motion_component': -2.900923142959339}, {'ion': 1460, 'force': [1.383186936378479, 1.6790300607681274, -0.8313134908676147], 'magnitude': 2.3288259506225586, 'distance': 11.939895629882812, 'cosine_with_motion': -0.8276203568856679, 'motion_component': -1.9273837390999855}]}, 4411: {'frame': 4411, 'ionic_force': [6.368192136287689, 0.6474573612213135, -10.474817991256714], 'ionic_force_magnitude': 12.275784458405555, 'motion_vector': [-2.447307586669922, -1.137054443359375, 2.16204833984375], 'cosine_ionic_motion': -0.918028029918748, 'ionic_motion_component': -11.269514222057236, 'ionic_force_x': 6.368192136287689, 'ionic_force_y': 0.6474573612213135, 'ionic_force_z': -10.474817991256714, 'radial_force': 6.401021177849362, 'axial_force': -10.474817991256714, 'contributions': [{'ion': 1308, 'force': [0.3361741900444031, -0.34610939025878906, -2.0818889141082764], 'magnitude': 2.1370694637298584, 'distance': 12.464065551757812, 'cosine_with_motion': -0.6671931374770188, 'motion_component': -1.4258381357650443}, {'ion': 1316, 'force': [2.108905553817749, -1.8903121948242188, -7.310626983642578], 'magnitude': 7.840027332305908, 'distance': 6.50744104385376, 'cosine_with_motion': -0.6941344152193054, 'motion_component': -5.442032838588133}, {'ion': 1460, 'force': [3.923112392425537, 2.8838789463043213, -1.0823020935058594], 'magnitude': 4.987879753112793, 'distance': 8.158514022827148, 'cosine_with_motion': -0.8824677491173122, 'motion_component': -4.401643196460441}]}, 4412: {'frame': 4412, 'ionic_force': [6.665052300319076, -3.4289957880973816, -16.710674703121185], 'ionic_force_magnitude': 18.314682178905333, 'motion_vector': [-1.1050071716308594, 3.6569137573242188, -0.751708984375], 'cosine_ionic_motion': -0.10297495998403897, 'ionic_motion_component': -1.8859536644931683, 'ionic_force_x': 6.665052300319076, 'ionic_force_y': -3.4289957880973816, 'ionic_force_z': -16.710674703121185, 'radial_force': 7.495394204495064, 'axial_force': -16.710674703121185, 'contributions': [{'ion': 1308, 'force': [0.019204726442694664, -0.8384458422660828, -2.92292857170105], 'magnitude': 3.0408670902252197, 'distance': 10.448894500732422, 'cosine_with_motion': -0.07518488886952328, 'motion_component': -0.2286272422142609}, {'ion': 1316, 'force': [0.2137768417596817, -8.213178634643555, -14.422178268432617], 'magnitude': 16.598230361938477, 'distance': 4.472374439239502, 'cosine_with_motion': -0.3006561911623409, 'motion_component': -4.990360527573039}, {'ion': 1460, 'force': [6.432070732116699, 5.622628688812256, 0.6344321370124817], 'magnitude': 8.566679000854492, 'distance': 6.225336074829102, 'cosine_with_motion': 0.38906957811169834, 'motion_component': 3.3330342370915735}]}, 4413: {'frame': 4413, 'ionic_force': [-2.547465205192566, 7.662760257720947, -13.662325963377953], 'ionic_force_magnitude': 15.870306376014476, 'motion_vector': [-0.39898681640625, 0.20450210571289062, -7.287322998046875], 'cosine_ionic_motion': 0.8815448570321193, 'ionic_motion_component': 13.990386965299612, 'ionic_force_x': -2.547465205192566, 'ionic_force_y': 7.662760257720947, 'ionic_force_z': -13.662325963377953, 'radial_force': 8.075114472190124, 'axial_force': -13.662325963377953, 'contributions': [{'ion': 1308, 'force': [-0.4219435453414917, 0.12968969345092773, -2.742938280105591], 'magnitude': 2.778230667114258, 'distance': 10.931629180908203, 'cosine_with_motion': 0.9950406445494476, 'motion_component': 2.764452530560943}, {'ion': 1316, 'force': [-4.159623622894287, 3.1517434120178223, -10.773609161376953], 'magnitude': 11.971074104309082, 'distance': 5.266262531280518, 'cosine_with_motion': 0.9246346516533765, 'motion_component': 11.068869716949145}, {'ion': 1460, 'force': [2.034101963043213, 4.381327152252197, -0.14577852189540863], 'magnitude': 4.832685470581055, 'distance': 8.288477897644043, 'cosine_with_motion': 0.032500516046732666, 'motion_component': 0.1570647748159848}]}, 4414: {'frame': 4414, 'ionic_force': [0.45747989416122437, 1.9616330564022064, -3.9405404329299927], 'ionic_force_magnitude': 4.425511383454767, 'motion_vector': [-0.04938507080078125, -0.9767036437988281, 0.471405029296875], 'cosine_ionic_motion': -0.7901159574218629, 'ionic_motion_component': -3.496667163819716, 'ionic_force_x': 0.45747989416122437, 'ionic_force_y': 1.9616330564022064, 'ionic_force_z': -3.9405404329299927, 'radial_force': 2.0142721021579053, 'axial_force': -3.9405404329299927, 'contributions': [{'ion': 1316, 'force': [-0.3398584723472595, 0.2946309745311737, -2.221829891204834], 'magnitude': 2.2669007778167725, 'distance': 12.10187816619873, 'cosine_with_motion': -0.5356952746826692, 'motion_component': -1.2143680491908284}, {'ion': 1460, 'force': [0.7973383665084839, 1.6670020818710327, -1.7187105417251587], 'magnitude': 2.5236105918884277, 'distance': 11.469853401184082, 'cosine_with_motion': -0.9043784954636804, 'motion_component': -2.2822991356094935}]}, 4415: {'frame': 4415, 'ionic_force': [0.11436110734939575, 1.6295432336628437, -4.317601203918457], 'ionic_force_magnitude': 4.6162939431245755, 'motion_vector': [-1.1576690673828125, 0.13907241821289062, -4.969749450683594], 'cosine_ionic_motion': 0.9145691038902696, 'ionic_motion_component': 4.2219198148575225, 'ionic_force_x': 0.11436110734939575, 'ionic_force_y': 1.6295432336628437, 'ionic_force_z': -4.317601203918457, 'radial_force': 1.6335512276174682, 'axial_force': -4.317601203918457, 'contributions': [{'ion': 1316, 'force': [-0.3461155891418457, 0.052372146397829056, -2.328737497329712], 'magnitude': 2.35490083694458, 'distance': 11.873608589172363, 'cosine_with_motion': 0.9966853552791446, 'motion_component': 2.3470950127604313}, {'ion': 1460, 'force': [0.46047669649124146, 1.5771710872650146, -1.9888637065887451], 'magnitude': 2.5797455310821533, 'distance': 11.344376564025879, 'cosine_with_motion': 0.7267480067537534, 'motion_component': 1.874824819083032}]}}</t>
+          <t>{4408: {'frame': 4408, 'ionic_force': [9.28405300155282, -3.821890950202942, -9.041797399520874], 'ionic_force_magnitude': 13.51127643062888, 'motion_vector': [0.9472541809082031, 6.171745300292969, -2.0280227661132812], 'cosine_ionic_motion': 0.03994897088398283, 'ionic_motion_component': 0.5397615887326366, 'ionic_force_x': 9.28405300155282, 'ionic_force_y': -3.821890950202942, 'ionic_force_z': -9.041797399520874, 'radial_force': 10.039944749394046, 'axial_force': -9.041797399520874, 'before_closest_residue': None, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.0392477847635746, -0.5659531354904175, -1.739326000213623], 'magnitude': 1.8295077085494995, 'distance': 13.471064567565918, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.00596555141577959, 'motion_component': 0.010914022006728752}, {'ion': 1316, 'force': [0.1305760145187378, -2.5276927947998047, -4.4630842208862305], 'magnitude': 5.130828380584717, 'distance': 8.044059753417969, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.190751381479075, 'motion_component': -0.9787126361579297}, {'ion': 1460, 'force': [9.114229202270508, -0.7282450199127197, -2.8393871784210205], 'magnitude': 9.574007987976074, 'distance': 5.888736724853516, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.157463841084995, 'motion_component': 1.5075601164077739}]}, 4409: {'frame': 4409, 'ionic_force': [2.3813661485910416, 3.48429112136364, -6.0583014488220215], 'ionic_force_magnitude': 7.383373605396644, 'motion_vector': [1.2028884887695312, 0.22224044799804688, -0.367950439453125], 'cosine_ionic_motion': 0.6221774438388844, 'ionic_motion_component': 4.593768516713172, 'ionic_force_x': 2.3813661485910416, 'ionic_force_y': 3.48429112136364, 'ionic_force_z': -6.0583014488220215, 'radial_force': 4.220330479010953, 'axial_force': -6.0583014488220215, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.11879675090312958, 0.2119782418012619, -1.456363558769226], 'magnitude': 1.4764965772628784, 'distance': 14.995219230651855, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.38486557312870256, 'motion_component': 0.5682527165054461}, {'ion': 1316, 'force': [0.3882765471935272, 1.0418009757995605, -3.5045788288116455], 'magnitude': 3.6767079830169678, 'distance': 9.502534866333008, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4233068597611323, 'motion_component': 1.5563756601938152}, {'ion': 1460, 'force': [1.8742928504943848, 2.2305119037628174, -1.09735906124115], 'magnitude': 3.1132545471191406, 'distance': 10.326704025268555, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.7931057531386033, 'motion_component': 2.469140102033048}]}, 4410: {'frame': 4410, 'ionic_force': [2.7379980981349945, 3.005010947585106, -6.075490713119507], 'ionic_force_magnitude': 7.310151283366067, 'motion_vector': [-0.20865249633789062, -4.049587249755859, 2.408935546875], 'cosine_ionic_motion': -0.7939953037108676, 'ionic_motion_component': -5.804225788408629, 'ionic_force_x': 2.7379980981349945, 'ionic_force_y': 3.005010947585106, 'ionic_force_z': -6.075490713119507, 'radial_force': 4.065307415251297, 'axial_force': -6.075490713119507, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 780, 'contributions': [{'ion': 1308, 'force': [0.2570955455303192, 0.21237300336360931, -1.531499981880188], 'magnitude': 1.5673840045928955, 'distance': 14.55396556854248, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6226418300254172, 'motion_component': -0.9759188427346958}, {'ion': 1316, 'force': [1.0977156162261963, 1.1136078834533691, -3.712677240371704], 'magnitude': 4.0285325050354, 'distance': 9.078113555908203, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7200942571398282, 'motion_component': -2.900923142959339}, {'ion': 1460, 'force': [1.383186936378479, 1.6790300607681274, -0.8313134908676147], 'magnitude': 2.3288259506225586, 'distance': 11.939895629882812, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.8276203568856679, 'motion_component': -1.9273837390999855}]}, 4411: {'frame': 4411, 'ionic_force': [6.368192136287689, 0.6474573612213135, -10.474817991256714], 'ionic_force_magnitude': 12.275784458405555, 'motion_vector': [-2.447307586669922, -1.137054443359375, 2.16204833984375], 'cosine_ionic_motion': -0.918028029918748, 'ionic_motion_component': -11.269514222057236, 'ionic_force_x': 6.368192136287689, 'ionic_force_y': 0.6474573612213135, 'ionic_force_z': -10.474817991256714, 'radial_force': 6.401021177849362, 'axial_force': -10.474817991256714, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1308, 'force': [0.3361741900444031, -0.34610939025878906, -2.0818889141082764], 'magnitude': 2.1370694637298584, 'distance': 12.464065551757812, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6671931374770188, 'motion_component': -1.4258381357650443}, {'ion': 1316, 'force': [2.108905553817749, -1.8903121948242188, -7.310626983642578], 'magnitude': 7.840027332305908, 'distance': 6.50744104385376, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6941344152193054, 'motion_component': -5.442032838588133}, {'ion': 1460, 'force': [3.923112392425537, 2.8838789463043213, -1.0823020935058594], 'magnitude': 4.987879753112793, 'distance': 8.158514022827148, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.8824677491173122, 'motion_component': -4.401643196460441}]}, 4412: {'frame': 4412, 'ionic_force': [6.665052300319076, -3.4289957880973816, -16.710674703121185], 'ionic_force_magnitude': 18.314682178905333, 'motion_vector': [-1.1050071716308594, 3.6569137573242188, -0.751708984375], 'cosine_ionic_motion': -0.10297495998403897, 'ionic_motion_component': -1.8859536644931683, 'ionic_force_x': 6.665052300319076, 'ionic_force_y': -3.4289957880973816, 'ionic_force_z': -16.710674703121185, 'radial_force': 7.495394204495064, 'axial_force': -16.710674703121185, 'before_closest_residue': 780, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1308, 'force': [0.019204726442694664, -0.8384458422660828, -2.92292857170105], 'magnitude': 3.0408670902252197, 'distance': 10.448894500732422, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.07518488886952328, 'motion_component': -0.2286272422142609}, {'ion': 1316, 'force': [0.2137768417596817, -8.213178634643555, -14.422178268432617], 'magnitude': 16.598230361938477, 'distance': 4.472374439239502, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3006561911623409, 'motion_component': -4.990360527573039}, {'ion': 1460, 'force': [6.432070732116699, 5.622628688812256, 0.6344321370124817], 'magnitude': 8.566679000854492, 'distance': 6.225336074829102, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.38906957811169834, 'motion_component': 3.3330342370915735}]}, 4413: {'frame': 4413, 'ionic_force': [-2.547465205192566, 7.662760257720947, -13.662325963377953], 'ionic_force_magnitude': 15.870306376014476, 'motion_vector': [-0.39898681640625, 0.20450210571289062, -7.287322998046875], 'cosine_ionic_motion': 0.8815448570321193, 'ionic_motion_component': 13.990386965299612, 'ionic_force_x': -2.547465205192566, 'ionic_force_y': 7.662760257720947, 'ionic_force_z': -13.662325963377953, 'radial_force': 8.075114472190124, 'axial_force': -13.662325963377953, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.4219435453414917, 0.12968969345092773, -2.742938280105591], 'magnitude': 2.778230667114258, 'distance': 10.931629180908203, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9950406445494476, 'motion_component': 2.764452530560943}, {'ion': 1316, 'force': [-4.159623622894287, 3.1517434120178223, -10.773609161376953], 'magnitude': 11.971074104309082, 'distance': 5.266262531280518, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9246346516533765, 'motion_component': 11.068869716949145}, {'ion': 1460, 'force': [2.034101963043213, 4.381327152252197, -0.14577852189540863], 'magnitude': 4.832685470581055, 'distance': 8.288477897644043, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.032500516046732666, 'motion_component': 0.1570647748159848}]}, 4414: {'frame': 4414, 'ionic_force': [0.45747989416122437, 1.9616330564022064, -3.9405404329299927], 'ionic_force_magnitude': 4.425511383454767, 'motion_vector': [-0.04938507080078125, -0.9767036437988281, 0.471405029296875], 'cosine_ionic_motion': -0.7901159574218629, 'ionic_motion_component': -3.496667163819716, 'ionic_force_x': 0.45747989416122437, 'ionic_force_y': 1.9616330564022064, 'ionic_force_z': -3.9405404329299927, 'radial_force': 2.0142721021579053, 'axial_force': -3.9405404329299927, 'before_closest_residue': 'SF', 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1316, 'force': [-0.3398584723472595, 0.2946309745311737, -2.221829891204834], 'magnitude': 2.2669007778167725, 'distance': 12.10187816619873, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5356952746826692, 'motion_component': -1.2143680491908284}, {'ion': 1460, 'force': [0.7973383665084839, 1.6670020818710327, -1.7187105417251587], 'magnitude': 2.5236105918884277, 'distance': 11.469853401184082, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.9043784954636804, 'motion_component': -2.2822991356094935}]}, 4415: {'frame': 4415, 'ionic_force': [0.11436110734939575, 1.6295432336628437, -4.317601203918457], 'ionic_force_magnitude': 4.6162939431245755, 'motion_vector': [-1.1576690673828125, 0.13907241821289062, -4.969749450683594], 'cosine_ionic_motion': 0.9145691038902696, 'ionic_motion_component': 4.2219198148575225, 'ionic_force_x': 0.11436110734939575, 'ionic_force_y': 1.6295432336628437, 'ionic_force_z': -4.317601203918457, 'radial_force': 1.6335512276174682, 'axial_force': -4.317601203918457, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': None, 'contributions': [{'ion': 1316, 'force': [-0.3461155891418457, 0.052372146397829056, -2.328737497329712], 'magnitude': 2.35490083694458, 'distance': 11.873608589172363, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9966853552791446, 'motion_component': 2.3470950127604313}, {'ion': 1460, 'force': [0.46047669649124146, 1.5771710872650146, -1.9888637065887451], 'magnitude': 2.5797455310821533, 'distance': 11.344376564025879, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.7267480067537534, 'motion_component': 1.874824819083032}]}}</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{4857: {'frame': 4857, 'ionic_force': [-23.60623151063919, 0.16038507223129272, 2.653203248977661], 'ionic_force_magnitude': 23.755407320980098, 'motion_vector': [0.9804725646972656, -0.3909263610839844, 0.2857513427734375], 'cosine_ionic_motion': -0.8642116533491877, 'ionic_motion_component': -20.52969983684761, 'ionic_force_x': -23.60623151063919, 'ionic_force_y': 0.16038507223129272, 'ionic_force_z': 2.653203248977661, 'radial_force': 23.606776347169667, 'axial_force': 2.653203248977661, 'contributions': [{'ion': 1308, 'force': [-1.2521235942840576, 1.593077540397644, -2.4381844997406006], 'magnitude': 3.1702449321746826, 'distance': 10.233463287353516, 'cosine_with_motion': -0.7347405368026476, 'motion_component': -2.329307494535591}, {'ion': 1320, 'force': [-0.6172628998756409, 0.6778424382209778, -1.6455979347229004], 'magnitude': 1.8837400674819946, 'distance': 13.275734901428223, 'cosine_with_motion': -0.6507174342681865, 'motion_component': -1.2257824654629097}, {'ion': 1460, 'force': [-21.736845016479492, -2.110534906387329, 6.736985683441162], 'magnitude': 22.854578018188477, 'distance': 3.8113815784454346, 'cosine_with_motion': -0.7427224759895918, 'motion_component': -16.9746092376122}]}, 4858: {'frame': 4858, 'ionic_force': [-8.50262776017189, 3.199307382106781, 3.651916027069092], 'ionic_force_magnitude': 9.791156071782979, 'motion_vector': [-0.14766693115234375, 1.5113677978515625, -0.5906982421875], 'cosine_ionic_motion': 0.24656918258421606, 'ionic_motion_component': 2.414197349174013, 'ionic_force_x': -8.50262776017189, 'ionic_force_y': 3.199307382106781, 'ionic_force_z': 3.651916027069092, 'radial_force': 9.084615927668523, 'axial_force': 3.651916027069092, 'contributions': [{'ion': 1308, 'force': [-1.0608267784118652, 1.5705699920654297, -2.8913075923919678], 'magnitude': 3.4571235179901123, 'distance': 9.799673080444336, 'cosine_with_motion': 0.7523887522231089, 'motion_component': 2.6011008640142848}, {'ion': 1320, 'force': [-0.4662999212741852, 0.6704815030097961, -1.7270715236663818], 'magnitude': 1.9104337692260742, 'distance': 13.182660102844238, 'cosine_with_motion': 0.6753826513946052, 'motion_component': 1.2902738108900658}, {'ion': 1460, 'force': [-6.97550106048584, 0.9582558870315552, 8.270295143127441], 'magnitude': 10.861567497253418, 'distance': 5.5286970138549805, 'cosine_with_motion': -0.1360003780017847, 'motion_component': -1.4771773018897036}]}, 4859: {'frame': 4859, 'ionic_force': [-9.53341594338417, 13.158035159111023, 4.4725987911224365], 'ionic_force_magnitude': 16.85301304646511, 'motion_vector': [-0.5728759765625, -0.2980232238769531, -0.14586639404296875], 'cosine_ionic_motion': 0.07955984094930431, 'ionic_motion_component': 1.3408230374933148, 'ionic_force_x': -9.53341594338417, 'ionic_force_y': 13.158035159111023, 'ionic_force_z': 4.4725987911224365, 'radial_force': 16.248689448628568, 'axial_force': 4.4725987911224365, 'contributions': [{'ion': 1308, 'force': [-0.8318650126457214, 1.5506973266601562, -2.159569263458252], 'magnitude': 2.785749673843384, 'distance': 10.916866302490234, 'cosine_with_motion': 0.1786205972552863, 'motion_component': 0.49759226274005286}, {'ion': 1320, 'force': [-0.4241594970226288, 0.7252730131149292, -1.4648845195770264], 'magnitude': 1.6887328624725342, 'distance': 14.021308898925781, 'cosine_with_motion': 0.2151362361665056, 'motion_component': 0.36330764449495057}, {'ion': 1460, 'force': [-8.27739143371582, 10.882064819335938, 8.097052574157715], 'magnitude': 15.890148162841797, 'distance': 4.570935249328613, 'cosine_with_motion': 0.030202565824339556, 'motion_component': 0.47992324150436616}]}, 4860: {'frame': 4860, 'ionic_force': [-2.976147174835205, 6.678335726261139, -2.335963726043701], 'ionic_force_magnitude': 7.675568161923092, 'motion_vector': [0.6911888122558594, -0.11594009399414062, 0.5926361083984375], 'cosine_ionic_motion': -0.598417063639624, 'ionic_motion_component': -4.593190961223803, 'ionic_force_x': -2.976147174835205, 'ionic_force_y': 6.678335726261139, 'ionic_force_z': -2.335963726043701, 'radial_force': 7.311471813454215, 'axial_force': -2.335963726043701, 'contributions': [{'ion': 1308, 'force': [-0.9280287027359009, 1.4536443948745728, -2.190319776535034], 'magnitude': 2.7877984046936035, 'distance': 10.912854194641113, 'cosine_with_motion': -0.8238689283199169, 'motion_component': -2.2967804955902}, {'ion': 1320, 'force': [-0.4511340856552124, 0.7071818709373474, -1.4634768962860107], 'magnitude': 1.6868292093276978, 'distance': 14.029218673706055, 'cosine_with_motion': -0.8145641030190202, 'motion_component': -1.3740305233741053}, {'ion': 1460, 'force': [-1.5969843864440918, 4.517509460449219, 1.3178329467773438], 'magnitude': 4.969399929046631, 'distance': 8.173669815063477, 'cosine_with_motion': -0.18561192477866056, 'motion_component': -0.9223798648451975}]}, 4861: {'frame': 4861, 'ionic_force': [-2.949042022228241, 8.77355444431305, -2.55695903301239], 'ionic_force_magnitude': 9.60261141214706, 'motion_vector': [0.4648017883300781, 0.24734878540039062, -0.2841033935546875], 'cosine_ionic_motion': 0.2655944164048997, 'ionic_motion_component': 2.5503999739722283, 'ionic_force_x': -2.949042022228241, 'ionic_force_y': 8.77355444431305, 'ionic_force_z': -2.55695903301239, 'radial_force': 9.255922776049577, 'axial_force': -2.55695903301239, 'contributions': [{'ion': 1308, 'force': [-0.8082016706466675, 1.8407821655273438, -2.506990909576416], 'magnitude': 3.2135140895843506, 'distance': 10.164334297180176, 'cosine_with_motion': 0.41189868486252534, 'motion_component': 1.3236421976845847}, {'ion': 1320, 'force': [-0.4184555411338806, 0.7065335512161255, -1.485287070274353], 'magnitude': 1.6971659660339355, 'distance': 13.986430168151855, 'cosine_with_motion': 0.39614474603532723, 'motion_component': 0.672323388035597}, {'ion': 1460, 'force': [-1.7223848104476929, 6.22623872756958, 1.435318946838379], 'magnitude': 6.617612838745117, 'distance': 7.0830183029174805, 'cosine_with_motion': 0.0837816523417639, 'motion_component': 0.554434531374163}]}, 4862: {'frame': 4862, 'ionic_force': [-2.821112185716629, 16.71923440694809, -1.5727373361587524], 'ionic_force_magnitude': 17.02835799034726, 'motion_vector': [-0.7869873046875, 0.3434638977050781, -0.23621368408203125], 'cosine_ionic_motion': 0.5495663586687077, 'ionic_motion_component': 9.358212694862338, 'ionic_force_x': -2.821112185716629, 'ionic_force_y': 16.71923440694809, 'ionic_force_z': -1.5727373361587524, 'radial_force': 16.955573511942195, 'axial_force': -1.5727373361587524, 'contributions': [{'ion': 1308, 'force': [-0.5865727663040161, 1.652468204498291, -2.294264078140259], 'magnitude': 2.8876230716705322, 'distance': 10.722567558288574, 'cosine_with_motion': 0.6109457566715136, 'motion_component': 1.7641810025489164}, {'ion': 1320, 'force': [-0.32260993123054504, 0.7156185507774353, -1.465861201286316], 'magnitude': 1.6628097295761108, 'distance': 14.130182266235352, 'cosine_with_motion': 0.5712511650610931, 'motion_component': 0.9498819854370506}, {'ion': 1460, 'force': [-1.9119294881820679, 14.351147651672363, 2.1873879432678223], 'magnitude': 14.642252922058105, 'distance': 4.761733531951904, 'cosine_with_motion': 0.45376553288560995, 'motion_component': 6.644149834145949}]}, 4863: {'frame': 4863, 'ionic_force': [-3.69932222366333, 9.218546092510223, -2.963527649641037], 'ionic_force_magnitude': 10.36576447274449, 'motion_vector': [1.4510307312011719, -0.018299102783203125, -1.9164810180664062], 'cosine_ionic_motion': 0.005739696896891008, 'ionic_motion_component': 0.059496346178114605, 'ionic_force_x': -3.69932222366333, 'ionic_force_y': 9.218546092510223, 'ionic_force_z': -2.963527649641037, 'radial_force': 9.93310510234463, 'axial_force': -2.963527649641037, 'contributions': [{'ion': 1308, 'force': [-0.7104681134223938, 1.5558724403381348, -1.9979960918426514], 'magnitude': 2.630112648010254, 'distance': 11.235227584838867, 'cosine_with_motion': 0.4380751251609181, 'motion_component': 1.1521869135222806}, {'ion': 1320, 'force': [-0.3768095374107361, 0.7196657061576843, -1.397373080253601], 'magnitude': 1.6163402795791626, 'distance': 14.331863403320312, 'cosine_with_motion': 0.5451289495529077, 'motion_component': 0.8811138419875748}, {'ion': 1460, 'force': [-2.6120445728302, 6.943007946014404, 0.43184152245521545], 'magnitude': 7.430654048919678, 'distance': 6.684293746948242, 'cosine_with_motion': -0.2656299511950648, 'motion_component': -1.9738043384000463}]}, 4864: {'frame': 4864, 'ionic_force': [-3.9271629452705383, 6.102272391319275, -2.3661776781082153], 'ionic_force_magnitude': 7.63276712214784, 'motion_vector': [-1.0789031982421875, -0.15365219116210938, 2.0991592407226562], 'cosine_ionic_motion': -0.09237188980147616, 'ionic_motion_component': -0.7050531234873706, 'ionic_force_x': -3.9271629452705383, 'ionic_force_y': 6.102272391319275, 'ionic_force_z': -2.3661776781082153, 'radial_force': 7.256744251836593, 'axial_force': -2.3661776781082153, 'contributions': [{'ion': 1308, 'force': [-0.32004624605178833, 1.0951236486434937, -1.809603214263916], 'magnitude': 2.139249563217163, 'distance': 12.457712173461914, 'cosine_with_motion': -0.7157728839742278, 'motion_component': -1.5312169138518108}, {'ion': 1460, 'force': [-3.60711669921875, 5.007148742675781, -0.5565744638442993], 'magnitude': 6.196176528930664, 'distance': 7.319933891296387, 'cosine_with_motion': 0.13333443679738946, 'motion_component': 0.8261637182101396}]}, 4865: {'frame': 4865, 'ionic_force': [-3.168602854013443, 5.503656804561615, -3.0944536328315735], 'ionic_force_magnitude': 7.064412612142925, 'motion_vector': [3.705402374267578, -1.9471969604492188, -2.8583602905273438], 'cosine_ionic_motion': -0.3801608278025133, 'ionic_motion_component': -2.6856129465707697, 'ionic_force_x': -3.168602854013443, 'ionic_force_y': 5.503656804561615, 'ionic_force_z': -3.0944536328315735, 'radial_force': 6.350612747511811, 'axial_force': -3.0944536328315735, 'contributions': [{'ion': 1308, 'force': [-0.8212441205978394, 1.7357362508773804, -2.2392847537994385], 'magnitude': 2.949850559234619, 'distance': 10.608867645263672, 'cosine_with_motion': -0.0014832429453785205, 'motion_component': -0.004375345063333924}, {'ion': 1320, 'force': [-0.41535165905952454, 0.8550887703895569, -1.5833065509796143], 'magnitude': 1.8467683792114258, 'distance': 13.407963752746582, 'cosine_with_motion': 0.14118443913662393, 'motion_component': 0.26073495759911935}, {'ion': 1460, 'force': [-1.932007074356079, 2.9128317832946777, 0.7281376719474792], 'magnitude': 3.5703535079956055, 'distance': 9.643028259277344, 'cosine_with_motion': -0.8240002960827033, 'motion_component': -2.9419724204515667}]}, 4866: {'frame': 4866, 'ionic_force': [-7.758470341563225, 11.393471777439117, -3.07043993473053], 'ionic_force_magnitude': 14.122062971712237, 'motion_vector': [-0.006435394287109375, 0.24068450927734375, 0.5570297241210938], 'cosine_ionic_motion': 0.12623792979283582, 'ionic_motion_component': 1.782739993953016, 'ionic_force_x': -7.758470341563225, 'ionic_force_y': 11.393471777439117, 'ionic_force_z': -3.07043993473053, 'radial_force': 13.784232339315013, 'axial_force': -3.07043993473053, 'contributions': [{'ion': 1308, 'force': [0.049068644642829895, 0.7890864014625549, -2.0871825218200684], 'magnitude': 2.2319042682647705, 'distance': 12.196389198303223, 'cosine_with_motion': -0.7184098472140821, 'motion_component': -1.603421891308001}, {'ion': 1460, 'force': [-7.807538986206055, 10.604385375976562, -0.9832574129104614], 'magnitude': 13.205204963684082, 'distance': 5.0141401290893555, 'cosine_with_motion': 0.25642628453809563, 'motion_component': 3.386161754441588}]}, 4867: {'frame': 4867, 'ionic_force': [0.12337589636445045, 4.056435167789459, -4.2135396003723145], 'ionic_force_magnitude': 5.850111438783753, 'motion_vector': [-0.9177093505859375, 0.6418495178222656, 2.0229339599609375], 'cosine_ionic_motion': -0.44602597766328916, 'ionic_motion_component': -2.609301673922715, 'ionic_force_x': 0.12337589636445045, 'ionic_force_y': 4.056435167789459, 'ionic_force_z': -4.2135396003723145, 'radial_force': 4.058310964216866, 'axial_force': -4.2135396003723145, 'contributions': [{'ion': 1308, 'force': [0.09774009138345718, 0.9288542866706848, -2.069882869720459], 'magnitude': 2.270845413208008, 'distance': 12.091362953186035, 'cosine_with_motion': -0.7009982594382919, 'motion_component': -1.5918586226891804}, {'ion': 1460, 'force': [0.02563580498099327, 3.1275808811187744, -2.1436567306518555], 'magnitude': 3.7917916774749756, 'distance': 9.357219696044922, 'cosine_with_motion': -0.2683278059184076, 'motion_component': -1.0174431206508086}]}, 4868: {'frame': 4868, 'ionic_force': [-1.2063874416053295, 6.333217084407806, -5.534350037574768], 'ionic_force_magnitude': 8.496707576226324, 'motion_vector': [0.3851051330566406, 2.4810562133789062, 0.2808074951171875], 'cosine_ionic_motion': 0.6379499331499946, 'ionic_motion_component': 5.420474030248636, 'ionic_force_x': -1.2063874416053295, 'ionic_force_y': 6.333217084407806, 'ionic_force_z': -5.534350037574768, 'radial_force': 6.447093088943107, 'axial_force': -5.534350037574768, 'contributions': [{'ion': 1308, 'force': [-0.13308840990066528, 1.483996033668518, -2.676917314529419], 'magnitude': 3.0636322498321533, 'distance': 10.40999984741211, 'cosine_with_motion': 0.37195321146052107, 'motion_component': 1.1395278843755534}, {'ion': 1320, 'force': [-0.05506179854273796, 0.6272523999214172, -1.598051905632019], 'magnitude': 1.7176283597946167, 'distance': 13.90286922454834, 'cosine_with_motion': 0.25033097015726313, 'motion_component': 0.4299755799140038}, {'ion': 1460, 'force': [-1.0182372331619263, 4.221968650817871, -1.25938081741333], 'magnitude': 4.5219316482543945, 'distance': 8.568544387817383, 'cosine_with_motion': 0.851620709199047, 'motion_component': 3.8509706902766823}]}, 4869: {'frame': 4869, 'ionic_force': [0.0542104747146368, 5.165193021297455, -3.881076753139496], 'ionic_force_magnitude': 6.461030450832787, 'motion_vector': [-0.0664825439453125, -0.035305023193359375, -0.05754852294921875], 'cosine_ionic_motion': 0.06107260201521054, 'ionic_motion_component': 0.39459194133186715, 'ionic_force_x': 0.0542104747146368, 'ionic_force_y': 5.165193021297455, 'ionic_force_z': -3.881076753139496, 'radial_force': 5.165477492239098, 'axial_force': -3.881076753139496, 'contributions': [{'ion': 1308, 'force': [-0.011133236810564995, 1.6809277534484863, -1.8282040357589722], 'magnitude': 2.4835402965545654, 'distance': 11.562012672424316, 'cosine_with_motion': 0.19804797994433204, 'motion_component': 0.49186012500856546}, {'ion': 1320, 'force': [0.029794860631227493, 0.8571366667747498, -1.3412694931030273], 'magnitude': 1.5920348167419434, 'distance': 14.440850257873535, 'cosine_with_motion': 0.2979502960962926, 'motion_component': 0.47434724454418253}, {'ion': 1460, 'force': [0.035548850893974304, 2.6271286010742188, -0.7116032242774963], 'magnitude': 2.7220301628112793, 'distance': 11.043903350830078, 'cosine_with_motion': -0.20999599232849375, 'motion_component': -0.5716154000736449}]}, 4870: {'frame': 4870, 'ionic_force': [-0.09000088274478912, 4.857101559638977, -3.782764494419098], 'ionic_force_magnitude': 6.157015749515344, 'motion_vector': [-0.150634765625, -2.8217086791992188, -4.534019470214844], 'cosine_ionic_motion': 0.10516778943237615, 'ionic_motion_component': 0.6475197358768533, 'ionic_force_x': -0.09000088274478912, 'ionic_force_y': 4.857101559638977, 'ionic_force_z': -3.782764494419098, 'radial_force': 4.85793533505153, 'axial_force': -3.782764494419098, 'contributions': [{'ion': 1308, 'force': [-0.0317416787147522, 1.5285658836364746, -1.7929517030715942], 'magnitude': 2.3563101291656494, 'distance': 11.870057106018066, 'cosine_with_motion': 0.30352157353261566, 'motion_component': 0.7151909310539509}, {'ion': 1320, 'force': [-0.024010654538869858, 0.8109053373336792, -1.3013789653778076], 'magnitude': 1.5335354804992676, 'distance': 14.71370792388916, 'cosine_with_motion': 0.44135347987078855, 'motion_component': 0.6768312379802743}, {'ion': 1460, 'force': [-0.03424854949116707, 2.5176303386688232, -0.688433825969696], 'magnitude': 2.6102828979492188, 'distance': 11.277822494506836, 'cosine_with_motion': -0.28521913588366826, 'motion_component': -0.7445026222250654}]}, 4871: {'frame': 4871, 'ionic_force': [-1.4377694465219975, 2.7718199491500854, -5.007754564285278], 'ionic_force_magnitude': 5.901505959327551, 'motion_vector': [-0.12489700317382812, -0.5373611450195312, 0.7347412109375], 'cosine_ionic_motion': -0.9201397059694539, 'ionic_motion_component': -5.430209958192633, 'ionic_force_x': -1.4377694465219975, 'ionic_force_y': 2.7718199491500854, 'ionic_force_z': -5.007754564285278, 'radial_force': 3.122525710359893, 'axial_force': -5.007754564285278, 'contributions': [{'ion': 1308, 'force': [-0.03414252772927284, 0.5607947111129761, -1.570929765701294], 'magnitude': 1.6683754920959473, 'distance': 14.106593132019043, 'cosine_with_motion': -0.9467690197126633, 'motion_component': -1.579566219617024}, {'ion': 1460, 'force': [-1.4036269187927246, 2.2110252380371094, -3.4368247985839844], 'magnitude': 4.3209452629089355, 'distance': 8.765560150146484, 'cosine_with_motion': -0.8911577797428331, 'motion_component': -3.8506437663609603}]}, 4872: {'frame': 4872, 'ionic_force': [-1.5672330230518128, 3.253392219543457, -6.297172904014587], 'ionic_force_magnitude': 7.259143673036479, 'motion_vector': [1.6905479431152344, -0.46477508544921875, 1.652435302734375], 'cosine_ionic_motion': -0.8329315936526057, 'ionic_motion_component': -6.046370108135505, 'ionic_force_x': -1.5672330230518128, 'ionic_force_y': 3.253392219543457, 'ionic_force_z': -6.297172904014587, 'radial_force': 3.6112020550960624, 'axial_force': -6.297172904014587, 'contributions': [{'ion': 1308, 'force': [2.390443842159584e-05, 0.5934185981750488, -1.8552712202072144], 'magnitude': 1.9478647708892822, 'distance': 13.055383682250977, 'cosine_with_motion': -0.7120286142675283, 'motion_component': -1.3869354112101064}, {'ion': 1460, 'force': [-1.5672569274902344, 2.659973621368408, -4.441901683807373], 'magnitude': 5.409458637237549, 'distance': 7.8341546058654785, 'cosine_with_motion': -0.861349512827743, 'motion_component': -4.659434702269067}]}, 4873: {'frame': 4873, 'ionic_force': [-1.6994890123605728, 6.724162369966507, -11.125696539878845], 'ionic_force_magnitude': 13.110444156407517, 'motion_vector': [-1.8945083618164062, 4.309528350830078, 0.9468460083007812], 'cosine_ionic_motion': 0.34411208913073765, 'ionic_motion_component': 4.511462328093263, 'ionic_force_x': -1.6994890123605728, 'ionic_force_y': 6.724162369966507, 'ionic_force_z': -11.125696539878845, 'radial_force': 6.935605415593358, 'axial_force': -11.125696539878845, 'contributions': [{'ion': 1308, 'force': [0.2984895706176758, 0.8108097314834595, -2.3136789798736572], 'magnitude': 2.469740629196167, 'distance': 11.594268798828125, 'cosine_with_motion': 0.06223117700292426, 'motion_component': 0.153694867391323}, {'ion': 1320, 'force': [0.10234962403774261, 0.38926997780799866, -1.4215017557144165], 'magnitude': 1.477387547492981, 'distance': 14.990696907043457, 'cosine_with_motion': 0.019413726224842758, 'motion_component': 0.028681596305214274}, {'ion': 1460, 'force': [-2.100328207015991, 5.524082660675049, -7.3905158042907715], 'magnitude': 9.462905883789062, 'distance': 5.923205375671387, 'cosine_with_motion': 0.4574795577949567, 'motion_component': 4.329086093616461}]}, 4874: {'frame': 4874, 'ionic_force': [-1.8247650638222694, 5.6435387134552, -3.796484112739563], 'ionic_force_magnitude': 7.0422005343995835, 'motion_vector': [1.5041236877441406, -3.0937538146972656, -1.0170440673828125], 'cosine_ionic_motion': -0.6469517009967339, 'ionic_motion_component': -4.55596361448992, 'ionic_force_x': -1.8247650638222694, 'ionic_force_y': 5.6435387134552, 'ionic_force_z': -3.796484112739563, 'radial_force': 5.931213766878907, 'axial_force': -3.796484112739563, 'contributions': [{'ion': 1308, 'force': [-0.06882379204034805, 1.2181742191314697, -1.544019103050232], 'magnitude': 1.9679126739501953, 'distance': 12.988713264465332, 'cosine_with_motion': -0.3260818599535824, 'motion_component': -0.641700611758041}, {'ion': 1460, 'force': [-1.7559412717819214, 4.4253644943237305, -2.252465009689331], 'magnitude': 5.266951560974121, 'distance': 7.939431190490723, 'cosine_with_motion': -0.7431742677572718, 'motion_component': -3.9142629071584913}]}, 4875: {'frame': 4875, 'ionic_force': [-1.1494073271751404, 5.382365703582764, -6.437063932418823], 'ionic_force_magnitude': 8.469167009860838, 'motion_vector': [-4.102687835693359, -0.4046134948730469, 2.7181549072265625], 'cosine_ionic_motion': -0.35769251277853253, 'ionic_motion_component': -3.029357628898174, 'ionic_force_x': -1.1494073271751404, 'ionic_force_y': 5.382365703582764, 'ionic_force_z': -6.437063932418823, 'radial_force': 5.5037258081110725, 'axial_force': -6.437063932418823, 'contributions': [{'ion': 1308, 'force': [0.1549651026725769, 0.9382805824279785, -2.0105345249176025], 'magnitude': 2.2241029739379883, 'distance': 12.21776008605957, 'cosine_with_motion': -0.5900523524559439, 'motion_component': -1.3123371483160682}, {'ion': 1460, 'force': [-1.3043724298477173, 4.444085121154785, -4.426529407501221], 'magnitude': 6.406671524047852, 'distance': 7.198678970336914, 'cosine_with_motion': -0.26800505197085495, 'motion_component': -1.7170203886894198}]}, 4876: {'frame': 4876, 'ionic_force': [-5.890000581741333, 6.048319339752197, -6.3055113554000854], 'ionic_force_magnitude': 10.537255199605498, 'motion_vector': [5.018623352050781, -2.8053436279296875, -2.0750503540039062], 'cosine_ionic_motion': -0.519231764832483, 'ionic_motion_component': -5.471277613781421, 'ionic_force_x': -5.890000581741333, 'ionic_force_y': 6.048319339752197, 'ionic_force_z': -6.3055113554000854, 'radial_force': 8.442409234841302, 'axial_force': -6.3055113554000854, 'contributions': [{'ion': 1308, 'force': [-1.146353840827942, 1.7300130128860474, -2.72662091255188], 'magnitude': 3.4265921115875244, 'distance': 9.84323501586914, 'cosine_with_motion': -0.23626317181720632, 'motion_component': -0.8095775295885126}, {'ion': 1320, 'force': [-0.5717068910598755, 0.7419012784957886, -1.8075217008590698], 'magnitude': 2.035780191421509, 'distance': 12.770373344421387, 'cosine_with_motion': -0.09641626228940431, 'motion_component': -0.19628231660630036}, {'ion': 1460, 'force': [-4.171939849853516, 3.5764050483703613, -1.7713687419891357], 'magnitude': 5.773517608642578, 'distance': 7.58313512802124, 'cosine_with_motion': -0.7734311038664372, 'motion_component': -4.465417884486193}]}, 4877: {'frame': 4877, 'ionic_force': [-1.2858441323041916, 6.905015721917152, -19.02397847175598], 'ionic_force_magnitude': 20.27916157404786, 'motion_vector': [-1.6677970886230469, 2.3718338012695312, 1.7540283203125], 'cosine_ionic_motion': -0.2160392511374309, 'ionic_motion_component': -4.381094880152263, 'ionic_force_x': -1.2858441323041916, 'ionic_force_y': 6.905015721917152, 'ionic_force_z': -19.02397847175598, 'radial_force': 7.023719616592349, 'axial_force': -19.02397847175598, 'contributions': [{'ion': 1308, 'force': [0.548943817615509, 0.45097389817237854, -2.8554723262786865], 'magnitude': 2.9425225257873535, 'distance': 10.622069358825684, 'cosine_with_motion': -0.48683309000334857, 'motion_component': -1.4325173471264652}, {'ion': 1320, 'force': [0.22946275770664215, 0.1839812844991684, -1.6267189979553223], 'magnitude': 1.6530932188034058, 'distance': 14.171648979187012, 'cosine_with_motion': -0.49976073485214356, 'motion_component': -0.826151048322767}, {'ion': 1460, 'force': [-2.0642507076263428, 6.2700605392456055, -14.541787147521973], 'magnitude': 15.96992015838623, 'distance': 4.559504508972168, 'cosine_with_motion': -0.13290148720347839, 'motion_component': -2.122426196693901}]}, 4878: {'frame': 4878, 'ionic_force': [-4.718822101131082, 12.355452835559845, -11.77543318271637], 'ionic_force_magnitude': 17.70834050481537, 'motion_vector': [3.3215065002441406, -4.6515045166015625, -1.365631103515625], 'cosine_ionic_motion': -0.5483564622691216, 'ionic_motion_component': -9.710482951877548, 'ionic_force_x': -4.718822101131082, 'ionic_force_y': 12.355452835559845, 'ionic_force_z': -11.77543318271637, 'radial_force': 13.225902494494164, 'axial_force': -11.77543318271637, 'contributions': [{'ion': 1308, 'force': [0.08313600718975067, 1.643194556236267, -3.1667728424072266], 'magnitude': 3.568676233291626, 'distance': 9.645294189453125, 'cosine_with_motion': -0.14508000757337663, 'motion_component': -0.5177435774466472}, {'ion': 1320, 'force': [-0.023140454664826393, 0.592434823513031, -1.7460500001907349], 'magnitude': 1.8439644575119019, 'distance': 13.418153762817383, 'cosine_with_motion': -0.04135362622311115, 'motion_component': -0.07625461900061781}, {'ion': 1460, 'force': [-4.778817653656006, 10.119823455810547, -6.862610340118408], 'magnitude': 13.127961158752441, 'distance': 5.028870105743408, 'cosine_with_motion': -0.6944326580126445, 'motion_component': -9.11648447082684}]}, 4879: {'frame': 4879, 'ionic_force': [16.751477003097534, -3.802208073437214, -9.315209746360779], 'ionic_force_magnitude': 19.540775333586726, 'motion_vector': [1.0792694091796875, 2.2563400268554688, 0.31360626220703125], 'cosine_ionic_motion': 0.13356250676512846, 'ionic_motion_component': 2.6099149376880324, 'ionic_force_x': 16.751477003097534, 'ionic_force_y': -3.802208073437214, 'ionic_force_z': -9.315209746360779, 'radial_force': 17.177565835094814, 'axial_force': -9.315209746360779, 'contributions': [{'ion': 1308, 'force': [0.9992598295211792, -0.08213885873556137, -2.9084274768829346], 'magnitude': 3.0763967037200928, 'distance': 10.388381004333496, 'cosine_with_motion': -0.0024453919914148078, 'motion_component': -0.007522996143335624}, {'ion': 1320, 'force': [0.36823737621307373, -0.04548029601573944, -1.686635136604309], 'magnitude': 1.7269641160964966, 'distance': 13.865239143371582, 'cosine_with_motion': -0.05378284459316496, 'motion_component': -0.09288104654053786}, {'ion': 1460, 'force': [15.383979797363281, -3.674588918685913, -4.720147132873535], 'magnitude': 16.50603675842285, 'distance': 4.484847068786621, 'cosine_with_motion': 0.16420168966862303, 'motion_component': 2.7103190141106452}]}, 4880: {'frame': 4880, 'ionic_force': [11.858177244663239, 6.56685571372509, -19.13987958431244], 'ionic_force_magnitude': 23.453676727385687, 'motion_vector': [-0.8839454650878906, 1.5736312866210938, 0.37496185302734375], 'cosine_ionic_motion': -0.169418778362439, 'ionic_motion_component': -3.9734932592612493, 'ionic_force_x': 11.858177244663239, 'ionic_force_y': 6.56685571372509, 'ionic_force_z': -19.13987958431244, 'radial_force': 13.555071432151617, 'axial_force': -19.13987958431244, 'contributions': [{'ion': 1308, 'force': [1.1822991371154785, 0.5047712326049805, -2.458538770675659], 'magnitude': 2.7743537425994873, 'distance': 10.939264297485352, 'cosine_with_motion': -0.22928060965663458, 'motion_component': -0.6361054945617823}, {'ion': 1320, 'force': [0.4902520775794983, 0.22216300666332245, -1.5701862573623657], 'magnitude': 1.6598759889602661, 'distance': 14.142663955688477, 'cosine_with_motion': -0.2197840868520927, 'motion_component': -0.36481433416091846}, {'ion': 1460, 'force': [10.185626029968262, 5.839921474456787, -15.111154556274414], 'magnitude': 19.13631820678711, 'distance': 4.165238380432129, 'cosine_with_motion': -0.15533675314471485, 'motion_component': -2.972573447942579}]}, 4881: {'frame': 4881, 'ionic_force': [3.114603340625763, 12.471758097410202, -14.59370231628418], 'ionic_force_magnitude': 19.447921516349048, 'motion_vector': [0.3200035095214844, -2.01806640625, -2.126708984375], 'cosine_ionic_motion': 0.11968036629602533, 'ionic_motion_component': 2.3275343707730065, 'ionic_force_x': 3.114603340625763, 'ionic_force_y': 12.471758097410202, 'ionic_force_z': -14.59370231628418, 'radial_force': 12.854785257239971, 'axial_force': -14.59370231628418, 'contributions': [{'ion': 1308, 'force': [1.0287961959838867, 0.8844953179359436, -2.4416749477386475], 'magnitude': 2.7933008670806885, 'distance': 10.902100563049316, 'cosine_with_motion': 0.45362420374227375, 'motion_component': 1.2671089138537504}, {'ion': 1320, 'force': [0.4618956446647644, 0.41249433159828186, -1.5808985233306885], 'magnitude': 1.6978631019592285, 'distance': 13.983558654785156, 'cosine_with_motion': 0.53470770419971, 'motion_component': 0.9078605109345066}, {'ion': 1460, 'force': [1.6239114999771118, 11.174768447875977, -10.571128845214844], 'magnitude': 15.468073844909668, 'distance': 4.63287878036499, 'cosine_with_motion': 0.009863212837963545, 'motion_component': 0.15256490293600677}]}, 4882: {'frame': 4882, 'ionic_force': [2.9245057702064514, 1.4519258439540863, -13.961868047714233], 'ionic_force_magnitude': 14.33856973474329, 'motion_vector': [-5.703945159912109, -0.015411376953125, -1.0719757080078125], 'cosine_ionic_motion': -0.02087051426507955, 'ionic_motion_component': -0.2992533241897977, 'ionic_force_x': 2.9245057702064514, 'ionic_force_y': 1.4519258439540863, 'ionic_force_z': -13.961868047714233, 'radial_force': 3.2650915234205327, 'axial_force': -13.961868047714233, 'contributions': [{'ion': 1308, 'force': [0.6743703484535217, 0.30599769949913025, -2.060572385787964], 'magnitude': 2.1896045207977295, 'distance': 12.31363296508789, 'cosine_with_motion': -0.12924092607834214, 'motion_component': -0.28298653249725403}, {'ion': 1460, 'force': [2.2501354217529297, 1.145928144454956, -11.90129566192627], 'magnitude': 12.166228294372559, 'distance': 5.2238545417785645, 'cosine_with_motion': -0.0013370432807549883, 'motion_component': -0.016266773147486813}]}, 4883: {'frame': 4883, 'ionic_force': [-3.27836936712265, 0.9993527233600616, -6.624387979507446], 'ionic_force_magnitude': 7.458480252438702, 'motion_vector': [1.4264259338378906, 0.6671638488769531, 5.739585876464844], 'cosine_ionic_motion': -0.9468419034633856, 'ionic_motion_component': -7.062001639163133, 'ionic_force_x': -3.27836936712265, 'ionic_force_y': 0.9993527233600616, 'ionic_force_z': -6.624387979507446, 'radial_force': 3.4273038343536655, 'axial_force': -6.624387979507446, 'contributions': [{'ion': 1308, 'force': [-0.274458110332489, 0.2523268163204193, -2.2293708324432373], 'magnitude': 2.2603297233581543, 'distance': 12.11945629119873, 'cosine_with_motion': -0.9677411690240902, 'motion_component': -2.18741411319553}, {'ion': 1460, 'force': [-3.003911256790161, 0.7470259070396423, -4.395017147064209], 'magnitude': 5.3756585121154785, 'distance': 7.858745098114014, 'cosine_with_motion': -0.9067888945866973, 'motion_component': -4.874587594102056}]}, 4884: {'frame': 4884, 'ionic_force': [-6.833262346684933, 17.534541964530945, -3.9410240650177], 'ionic_force_magnitude': 19.227202263604745, 'motion_vector': [0.24680328369140625, -1.6334991455078125, 0.6660842895507812], 'cosine_ionic_motion': -0.9622021441283682, 'ionic_motion_component': -18.500455243630302, 'ionic_force_x': -6.833262346684933, 'ionic_force_y': 17.534541964530945, 'ionic_force_z': -3.9410240650177, 'radial_force': 18.818970115405325, 'axial_force': -3.9410240650177, 'contributions': [{'ion': 1308, 'force': [-0.2761423885822296, 2.3214807510375977, -6.306930065155029], 'magnitude': 6.726283550262451, 'distance': 7.025568008422852, 'cosine_with_motion': -0.6728191096191648, 'motion_component': -4.525572306611302}, {'ion': 1320, 'force': [-0.03301822394132614, 0.6696442365646362, -2.9598124027252197], 'magnitude': 3.0347986221313477, 'distance': 10.459335327148438, 'cosine_with_motion': -0.5685579212934188, 'motion_component': -1.7254588325924702}, {'ion': 1460, 'force': [-6.524101734161377, 14.543416976928711, 5.325718402862549], 'magnitude': 16.805896759033203, 'distance': 4.4446563720703125, 'cosine_with_motion': -0.7288765819072703, 'motion_component': -12.24942439985157}]}, 4885: {'frame': 4885, 'ionic_force': [8.870568364858627, 13.079958885908127, -2.2769949436187744], 'ionic_force_magnitude': 15.967373407857131, 'motion_vector': [-0.5143928527832031, -0.7691268920898438, 0.460906982421875], 'cosine_ionic_motion': -0.9495140680693623, 'ionic_motion_component': -15.161245680876982, 'ionic_force_x': 8.870568364858627, 'ionic_force_y': 13.079958885908127, 'ionic_force_z': -2.2769949436187744, 'radial_force': 15.804186393885566, 'axial_force': -2.2769949436187744, 'contributions': [{'ion': 1308, 'force': [-0.0231691375374794, 0.9201945662498474, -9.202110290527344], 'magnitude': 9.24803352355957, 'distance': 5.991621017456055, 'cosine_with_motion': -0.5164409343596666, 'motion_component': -4.776063202192125}, {'io</t>
+          <t>{4857: {'frame': 4857, 'ionic_force': [-23.60623151063919, 0.16038507223129272, 2.653203248977661], 'ionic_force_magnitude': 23.755407320980098, 'motion_vector': [0.9804725646972656, -0.3909263610839844, 0.2857513427734375], 'cosine_ionic_motion': -0.8642116533491877, 'ionic_motion_component': -20.52969983684761, 'ionic_force_x': -23.60623151063919, 'ionic_force_y': 0.16038507223129272, 'ionic_force_z': 2.653203248977661, 'radial_force': 23.606776347169667, 'axial_force': 2.653203248977661, 'before_closest_residue': None, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-1.2521235942840576, 1.593077540397644, -2.4381844997406006], 'magnitude': 3.1702449321746826, 'distance': 10.233463287353516, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7347405368026476, 'motion_component': -2.329307494535591}, {'ion': 1320, 'force': [-0.6172628998756409, 0.6778424382209778, -1.6455979347229004], 'magnitude': 1.8837400674819946, 'distance': 13.275734901428223, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6507174342681865, 'motion_component': -1.2257824654629097}, {'ion': 1460, 'force': [-21.736845016479492, -2.110534906387329, 6.736985683441162], 'magnitude': 22.854578018188477, 'distance': 3.8113815784454346, 'before_closest_residue': 455, 'closest_residue': 130, 'next_closest_residue': 130, 'cosine_with_motion': -0.7427224759895918, 'motion_component': -16.9746092376122}]}, 4858: {'frame': 4858, 'ionic_force': [-8.50262776017189, 3.199307382106781, 3.651916027069092], 'ionic_force_magnitude': 9.791156071782979, 'motion_vector': [-0.14766693115234375, 1.5113677978515625, -0.5906982421875], 'cosine_ionic_motion': 0.24656918258421606, 'ionic_motion_component': 2.414197349174013, 'ionic_force_x': -8.50262776017189, 'ionic_force_y': 3.199307382106781, 'ionic_force_z': 3.651916027069092, 'radial_force': 9.084615927668523, 'axial_force': 3.651916027069092, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-1.0608267784118652, 1.5705699920654297, -2.8913075923919678], 'magnitude': 3.4571235179901123, 'distance': 9.799673080444336, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7523887522231089, 'motion_component': 2.6011008640142848}, {'ion': 1320, 'force': [-0.4662999212741852, 0.6704815030097961, -1.7270715236663818], 'magnitude': 1.9104337692260742, 'distance': 13.182660102844238, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6753826513946052, 'motion_component': 1.2902738108900658}, {'ion': 1460, 'force': [-6.97550106048584, 0.9582558870315552, 8.270295143127441], 'magnitude': 10.861567497253418, 'distance': 5.5286970138549805, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 130, 'cosine_with_motion': -0.1360003780017847, 'motion_component': -1.4771773018897036}]}, 4859: {'frame': 4859, 'ionic_force': [-9.53341594338417, 13.158035159111023, 4.4725987911224365], 'ionic_force_magnitude': 16.85301304646511, 'motion_vector': [-0.5728759765625, -0.2980232238769531, -0.14586639404296875], 'cosine_ionic_motion': 0.07955984094930431, 'ionic_motion_component': 1.3408230374933148, 'ionic_force_x': -9.53341594338417, 'ionic_force_y': 13.158035159111023, 'ionic_force_z': 4.4725987911224365, 'radial_force': 16.248689448628568, 'axial_force': 4.4725987911224365, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.8318650126457214, 1.5506973266601562, -2.159569263458252], 'magnitude': 2.785749673843384, 'distance': 10.916866302490234, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.1786205972552863, 'motion_component': 0.49759226274005286}, {'ion': 1320, 'force': [-0.4241594970226288, 0.7252730131149292, -1.4648845195770264], 'magnitude': 1.6887328624725342, 'distance': 14.021308898925781, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2151362361665056, 'motion_component': 0.36330764449495057}, {'ion': 1460, 'force': [-8.27739143371582, 10.882064819335938, 8.097052574157715], 'magnitude': 15.890148162841797, 'distance': 4.570935249328613, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 1105, 'cosine_with_motion': 0.030202565824339556, 'motion_component': 0.47992324150436616}]}, 4860: {'frame': 4860, 'ionic_force': [-2.976147174835205, 6.678335726261139, -2.335963726043701], 'ionic_force_magnitude': 7.675568161923092, 'motion_vector': [0.6911888122558594, -0.11594009399414062, 0.5926361083984375], 'cosine_ionic_motion': -0.598417063639624, 'ionic_motion_component': -4.593190961223803, 'ionic_force_x': -2.976147174835205, 'ionic_force_y': 6.678335726261139, 'ionic_force_z': -2.335963726043701, 'radial_force': 7.311471813454215, 'axial_force': -2.335963726043701, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.9280287027359009, 1.4536443948745728, -2.190319776535034], 'magnitude': 2.7877984046936035, 'distance': 10.912854194641113, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8238689283199169, 'motion_component': -2.2967804955902}, {'ion': 1320, 'force': [-0.4511340856552124, 0.7071818709373474, -1.4634768962860107], 'magnitude': 1.6868292093276978, 'distance': 14.029218673706055, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8145641030190202, 'motion_component': -1.3740305233741053}, {'ion': 1460, 'force': [-1.5969843864440918, 4.517509460449219, 1.3178329467773438], 'magnitude': 4.969399929046631, 'distance': 8.173669815063477, 'before_closest_residue': 130, 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': -0.18561192477866056, 'motion_component': -0.9223798648451975}]}, 4861: {'frame': 4861, 'ionic_force': [-2.949042022228241, 8.77355444431305, -2.55695903301239], 'ionic_force_magnitude': 9.60261141214706, 'motion_vector': [0.4648017883300781, 0.24734878540039062, -0.2841033935546875], 'cosine_ionic_motion': 0.2655944164048997, 'ionic_motion_component': 2.5503999739722283, 'ionic_force_x': -2.949042022228241, 'ionic_force_y': 8.77355444431305, 'ionic_force_z': -2.55695903301239, 'radial_force': 9.255922776049577, 'axial_force': -2.55695903301239, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.8082016706466675, 1.8407821655273438, -2.506990909576416], 'magnitude': 3.2135140895843506, 'distance': 10.164334297180176, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.41189868486252534, 'motion_component': 1.3236421976845847}, {'ion': 1320, 'force': [-0.4184555411338806, 0.7065335512161255, -1.485287070274353], 'magnitude': 1.6971659660339355, 'distance': 13.986430168151855, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.39614474603532723, 'motion_component': 0.672323388035597}, {'ion': 1460, 'force': [-1.7223848104476929, 6.22623872756958, 1.435318946838379], 'magnitude': 6.617612838745117, 'distance': 7.0830183029174805, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 1105, 'cosine_with_motion': 0.0837816523417639, 'motion_component': 0.554434531374163}]}, 4862: {'frame': 4862, 'ionic_force': [-2.821112185716629, 16.71923440694809, -1.5727373361587524], 'ionic_force_magnitude': 17.02835799034726, 'motion_vector': [-0.7869873046875, 0.3434638977050781, -0.23621368408203125], 'cosine_ionic_motion': 0.5495663586687077, 'ionic_motion_component': 9.358212694862338, 'ionic_force_x': -2.821112185716629, 'ionic_force_y': 16.71923440694809, 'ionic_force_z': -1.5727373361587524, 'radial_force': 16.955573511942195, 'axial_force': -1.5727373361587524, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.5865727663040161, 1.652468204498291, -2.294264078140259], 'magnitude': 2.8876230716705322, 'distance': 10.722567558288574, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6109457566715136, 'motion_component': 1.7641810025489164}, {'ion': 1320, 'force': [-0.32260993123054504, 0.7156185507774353, -1.465861201286316], 'magnitude': 1.6628097295761108, 'distance': 14.130182266235352, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5712511650610931, 'motion_component': 0.9498819854370506}, {'ion': 1460, 'force': [-1.9119294881820679, 14.351147651672363, 2.1873879432678223], 'magnitude': 14.642252922058105, 'distance': 4.761733531951904, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': 0.45376553288560995, 'motion_component': 6.644149834145949}]}, 4863: {'frame': 4863, 'ionic_force': [-3.69932222366333, 9.218546092510223, -2.963527649641037], 'ionic_force_magnitude': 10.36576447274449, 'motion_vector': [1.4510307312011719, -0.018299102783203125, -1.9164810180664062], 'cosine_ionic_motion': 0.005739696896891008, 'ionic_motion_component': 0.059496346178114605, 'ionic_force_x': -3.69932222366333, 'ionic_force_y': 9.218546092510223, 'ionic_force_z': -2.963527649641037, 'radial_force': 9.93310510234463, 'axial_force': -2.963527649641037, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.7104681134223938, 1.5558724403381348, -1.9979960918426514], 'magnitude': 2.630112648010254, 'distance': 11.235227584838867, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4380751251609181, 'motion_component': 1.1521869135222806}, {'ion': 1320, 'force': [-0.3768095374107361, 0.7196657061576843, -1.397373080253601], 'magnitude': 1.6163402795791626, 'distance': 14.331863403320312, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5451289495529077, 'motion_component': 0.8811138419875748}, {'ion': 1460, 'force': [-2.6120445728302, 6.943007946014404, 0.43184152245521545], 'magnitude': 7.430654048919678, 'distance': 6.684293746948242, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 455, 'cosine_with_motion': -0.2656299511950648, 'motion_component': -1.9738043384000463}]}, 4864: {'frame': 4864, 'ionic_force': [-3.9271629452705383, 6.102272391319275, -2.3661776781082153], 'ionic_force_magnitude': 7.63276712214784, 'motion_vector': [-1.0789031982421875, -0.15365219116210938, 2.0991592407226562], 'cosine_ionic_motion': -0.09237188980147616, 'ionic_motion_component': -0.7050531234873706, 'ionic_force_x': -3.9271629452705383, 'ionic_force_y': 6.102272391319275, 'ionic_force_z': -2.3661776781082153, 'radial_force': 7.256744251836593, 'axial_force': -2.3661776781082153, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.32004624605178833, 1.0951236486434937, -1.809603214263916], 'magnitude': 2.139249563217163, 'distance': 12.457712173461914, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7157728839742278, 'motion_component': -1.5312169138518108}, {'ion': 1460, 'force': [-3.60711669921875, 5.007148742675781, -0.5565744638442993], 'magnitude': 6.196176528930664, 'distance': 7.319933891296387, 'before_closest_residue': 1105, 'closest_residue': 455, 'next_closest_residue': 780, 'cosine_with_motion': 0.13333443679738946, 'motion_component': 0.8261637182101396}]}, 4865: {'frame': 4865, 'ionic_force': [-3.168602854013443, 5.503656804561615, -3.0944536328315735], 'ionic_force_magnitude': 7.064412612142925, 'motion_vector': [3.705402374267578, -1.9471969604492188, -2.8583602905273438], 'cosine_ionic_motion': -0.3801608278025133, 'ionic_motion_component': -2.6856129465707697, 'ionic_force_x': -3.168602854013443, 'ionic_force_y': 5.503656804561615, 'ionic_force_z': -3.0944536328315735, 'radial_force': 6.350612747511811, 'axial_force': -3.0944536328315735, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [-0.8212441205978394, 1.7357362508773804, -2.2392847537994385], 'magnitude': 2.949850559234619, 'distance': 10.608867645263672, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.0014832429453785205, 'motion_component': -0.004375345063333924}, {'ion': 1320, 'force': [-0.41535165905952454, 0.8550887703895569, -1.5833065509796143], 'magnitude': 1.8467683792114258, 'distance': 13.407963752746582, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.14118443913662393, 'motion_component': 0.26073495759911935}, {'ion': 1460, 'force': [-1.932007074356079, 2.9128317832946777, 0.7281376719474792], 'magnitude': 3.5703535079956055, 'distance': 9.643028259277344, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 455, 'cosine_with_motion': -0.8240002960827033, 'motion_component': -2.9419724204515667}]}, 4866: {'frame': 4866, 'ionic_force': [-7.758470341563225, 11.393471777439117, -3.07043993473053], 'ionic_force_magnitude': 14.122062971712237, 'motion_vector': [-0.006435394287109375, 0.24068450927734375, 0.5570297241210938], 'cosine_ionic_motion': 0.12623792979283582, 'ionic_motion_component': 1.782739993953016, 'ionic_force_x': -7.758470341563225, 'ionic_force_y': 11.393471777439117, 'ionic_force_z': -3.07043993473053, 'radial_force': 13.784232339315013, 'axial_force': -3.07043993473053, 'before_closest_residue': 98, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.049068644642829895, 0.7890864014625549, -2.0871825218200684], 'magnitude': 2.2319042682647705, 'distance': 12.196389198303223, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7184098472140821, 'motion_component': -1.603421891308001}, {'ion': 1460, 'force': [-7.807538986206055, 10.604385375976562, -0.9832574129104614], 'magnitude': 13.205204963684082, 'distance': 5.0141401290893555, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 'SF', 'cosine_with_motion': 0.25642628453809563, 'motion_component': 3.386161754441588}]}, 4867: {'frame': 4867, 'ionic_force': [0.12337589636445045, 4.056435167789459, -4.2135396003723145], 'ionic_force_magnitude': 5.850111438783753, 'motion_vector': [-0.9177093505859375, 0.6418495178222656, 2.0229339599609375], 'cosine_ionic_motion': -0.44602597766328916, 'ionic_motion_component': -2.609301673922715, 'ionic_force_x': 0.12337589636445045, 'ionic_force_y': 4.056435167789459, 'ionic_force_z': -4.2135396003723145, 'radial_force': 4.058310964216866, 'axial_force': -4.2135396003723145, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.09774009138345718, 0.9288542866706848, -2.069882869720459], 'magnitude': 2.270845413208008, 'distance': 12.091362953186035, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7009982594382919, 'motion_component': -1.5918586226891804}, {'ion': 1460, 'force': [0.02563580498099327, 3.1275808811187744, -2.1436567306518555], 'magnitude': 3.7917916774749756, 'distance': 9.357219696044922, 'before_closest_residue': 455, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.2683278059184076, 'motion_component': -1.0174431206508086}]}, 4868: {'frame': 4868, 'ionic_force': [-1.2063874416053295, 6.333217084407806, -5.534350037574768], 'ionic_force_magnitude': 8.496707576226324, 'motion_vector': [0.3851051330566406, 2.4810562133789062, 0.2808074951171875], 'cosine_ionic_motion': 0.6379499331499946, 'ionic_motion_component': 5.420474030248636, 'ionic_force_x': -1.2063874416053295, 'ionic_force_y': 6.333217084407806, 'ionic_force_z': -5.534350037574768, 'radial_force': 6.447093088943107, 'axial_force': -5.534350037574768, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.13308840990066528, 1.483996033668518, -2.676917314529419], 'magnitude': 3.0636322498321533, 'distance': 10.40999984741211, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.37195321146052107, 'motion_component': 1.1395278843755534}, {'ion': 1320, 'force': [-0.05506179854273796, 0.6272523999214172, -1.598051905632019], 'magnitude': 1.7176283597946167, 'distance': 13.90286922454834, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.25033097015726313, 'motion_component': 0.4299755799140038}, {'ion': 1460, 'force': [-1.0182372331619263, 4.221968650817871, -1.25938081741333], 'magnitude': 4.5219316482543945, 'distance': 8.568544387817383, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': 0.851620709199047, 'motion_component': 3.8509706902766823}]}, 4869: {'frame': 4869, 'ionic_force': [0.0542104747146368, 5.165193021297455, -3.881076753139496], 'ionic_force_magnitude': 6.461030450832787, 'motion_vector': [-0.0664825439453125, -0.035305023193359375, -0.05754852294921875], 'cosine_ionic_motion': 0.06107260201521054, 'ionic_motion_component': 0.39459194133186715, 'ionic_force_x': 0.0542104747146368, 'ionic_force_y': 5.165193021297455, 'ionic_force_z': -3.881076753139496, 'radial_force': 5.165477492239098, 'axial_force': -3.881076753139496, 'before_closest_residue': 455, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-0.011133236810564995, 1.6809277534484863, -1.8282040357589722], 'magnitude': 2.4835402965545654, 'distance': 11.562012672424316, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.19804797994433204, 'motion_component': 0.49186012500856546}, {'ion': 1320, 'force': [0.029794860631227493, 0.8571366667747498, -1.3412694931030273], 'magnitude': 1.5920348167419434, 'distance': 14.440850257873535, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2979502960962926, 'motion_component': 0.47434724454418253}, {'ion': 1460, 'force': [0.035548850893974304, 2.6271286010742188, -0.7116032242774963], 'magnitude': 2.7220301628112793, 'distance': 11.043903350830078, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.20999599232849375, 'motion_component': -0.5716154000736449}]}, 4870: {'frame': 4870, 'ionic_force': [-0.09000088274478912, 4.857101559638977, -3.782764494419098], 'ionic_force_magnitude': 6.157015749515344, 'motion_vector': [-0.150634765625, -2.8217086791992188, -4.534019470214844], 'cosine_ionic_motion': 0.10516778943237615, 'ionic_motion_component': 0.6475197358768533, 'ionic_force_x': -0.09000088274478912, 'ionic_force_y': 4.857101559638977, 'ionic_force_z': -3.782764494419098, 'radial_force': 4.85793533505153, 'axial_force': -3.782764494419098, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.0317416787147522, 1.5285658836364746, -1.7929517030715942], 'magnitude': 2.3563101291656494, 'distance': 11.870057106018066, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.30352157353261566, 'motion_component': 0.7151909310539509}, {'ion': 1320, 'force': [-0.024010654538869858, 0.8109053373336792, -1.3013789653778076], 'magnitude': 1.5335354804992676, 'distance': 14.71370792388916, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.44135347987078855, 'motion_component': 0.6768312379802743}, {'ion': 1460, 'force': [-0.03424854949116707, 2.5176303386688232, -0.688433825969696], 'magnitude': 2.6102828979492188, 'distance': 11.277822494506836, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.28521913588366826, 'motion_component': -0.7445026222250654}]}, 4871: {'frame': 4871, 'ionic_force': [-1.4377694465219975, 2.7718199491500854, -5.007754564285278], 'ionic_force_magnitude': 5.901505959327551, 'motion_vector': [-0.12489700317382812, -0.5373611450195312, 0.7347412109375], 'cosine_ionic_motion': -0.9201397059694539, 'ionic_motion_component': -5.430209958192633, 'ionic_force_x': -1.4377694465219975, 'ionic_force_y': 2.7718199491500854, 'ionic_force_z': -5.007754564285278, 'radial_force': 3.122525710359893, 'axial_force': -5.007754564285278, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.03414252772927284, 0.5607947111129761, -1.570929765701294], 'magnitude': 1.6683754920959473, 'distance': 14.106593132019043, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9467690197126633, 'motion_component': -1.579566219617024}, {'ion': 1460, 'force': [-1.4036269187927246, 2.2110252380371094, -3.4368247985839844], 'magnitude': 4.3209452629089355, 'distance': 8.765560150146484, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.8911577797428331, 'motion_component': -3.8506437663609603}]}, 4872: {'frame': 4872, 'ionic_force': [-1.5672330230518128, 3.253392219543457, -6.297172904014587], 'ionic_force_magnitude': 7.259143673036479, 'motion_vector': [1.6905479431152344, -0.46477508544921875, 1.652435302734375], 'cosine_ionic_motion': -0.8329315936526057, 'ionic_motion_component': -6.046370108135505, 'ionic_force_x': -1.5672330230518128, 'ionic_force_y': 3.253392219543457, 'ionic_force_z': -6.297172904014587, 'radial_force': 3.6112020550960624, 'axial_force': -6.297172904014587, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [2.390443842159584e-05, 0.5934185981750488, -1.8552712202072144], 'magnitude': 1.9478647708892822, 'distance': 13.055383682250977, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7120286142675283, 'motion_component': -1.3869354112101064}, {'ion': 1460, 'force': [-1.5672569274902344, 2.659973621368408, -4.441901683807373], 'magnitude': 5.409458637237549, 'distance': 7.8341546058654785, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.861349512827743, 'motion_component': -4.659434702269067}]}, 4873: {'frame': 4873, 'ionic_force': [-1.6994890123605728, 6.724162369966507, -11.125696539878845], 'ionic_force_magnitude': 13.110444156407517, 'motion_vector': [-1.8945083618164062, 4.309528350830078, 0.9468460083007812], 'cosine_ionic_motion': 0.34411208913073765, 'ionic_motion_component': 4.511462328093263, 'ionic_force_x': -1.6994890123605728, 'ionic_force_y': 6.724162369966507, 'ionic_force_z': -11.125696539878845, 'radial_force': 6.935605415593358, 'axial_force': -11.125696539878845, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [0.2984895706176758, 0.8108097314834595, -2.3136789798736572], 'magnitude': 2.469740629196167, 'distance': 11.594268798828125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.06223117700292426, 'motion_component': 0.153694867391323}, {'ion': 1320, 'force': [0.10234962403774261, 0.38926997780799866, -1.4215017557144165], 'magnitude': 1.477387547492981, 'distance': 14.990696907043457, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.019413726224842758, 'motion_component': 0.028681596305214274}, {'ion': 1460, 'force': [-2.100328207015991, 5.524082660675049, -7.3905158042907715], 'magnitude': 9.462905883789062, 'distance': 5.923205375671387, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': 0.4574795577949567, 'motion_component': 4.329086093616461}]}, 4874: {'frame': 4874, 'ionic_force': [-1.8247650638222694, 5.6435387134552, -3.796484112739563], 'ionic_force_magnitude': 7.0422005343995835, 'motion_vector': [1.5041236877441406, -3.0937538146972656, -1.0170440673828125], 'cosine_ionic_motion': -0.6469517009967339, 'ionic_motion_component': -4.55596361448992, 'ionic_force_x': -1.8247650638222694, 'ionic_force_y': 5.6435387134552, 'ionic_force_z': -3.796484112739563, 'radial_force': 5.931213766878907, 'axial_force': -3.796484112739563, 'before_closest_residue': 455, 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [-0.06882379204034805, 1.2181742191314697, -1.544019103050232], 'magnitude': 1.9679126739501953, 'distance': 12.988713264465332, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3260818599535824, 'motion_component': -0.641700611758041}, {'ion': 1460, 'force': [-1.7559412717819214, 4.4253644943237305, -2.252465009689331], 'magnitude': 5.266951560974121, 'distance': 7.939431190490723, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.7431742677572718, 'motion_component': -3.9142629071584913}]}, 4875: {'frame': 4875, 'ionic_force': [-1.1494073271751404, 5.382365703582764, -6.437063932418823], 'ionic_force_magnitude': 8.469167009860838, 'motion_vector': [-4.102687835693359, -0.4046134948730469, 2.7181549072265625], 'cosine_ionic_motion': -0.35769251277853253, 'ionic_motion_component': -3.029357628898174, 'ionic_force_x': -1.1494073271751404, 'ionic_force_y': 5.382365703582764, 'ionic_force_z': -6.437063932418823, 'radial_force': 5.5037258081110725, 'axial_force': -6.437063932418823, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.1549651026725769, 0.9382805824279785, -2.0105345249176025], 'magnitude': 2.2241029739379883, 'distance': 12.21776008605957, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5900523524559439, 'motion_component': -1.3123371483160682}, {'ion': 1460, 'force': [-1.3043724298477173, 4.444085121154785, -4.426529407501221], 'magnitude': 6.406671524047852, 'distance': 7.198678970336914, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.26800505197085495, 'motion_component': -1.7170203886894198}]}, 4876: {'frame': 4876, 'ionic_force': [-5.890000581741333, 6.048319339752197, -6.3055113554000854], 'ionic_force_magnitude': 10.537255199605498, 'motion_vector': [5.018623352050781, -2.8053436279296875, -2.0750503540039062], 'cosine_ionic_motion': -0.519231764832483, 'ionic_motion_component': -5.471277613781421, 'ionic_force_x': -5.890000581741333, 'ionic_force_y': 6.048319339752197, 'ionic_force_z': -6.3055113554000854, 'radial_force': 8.442409234841302, 'axial_force': -6.3055113554000854, 'before_closest_residue': 455, 'closest_residue': 98, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [-1.146353840827942, 1.7300130128860474, -2.72662091255188], 'magnitude': 3.4265921115875244, 'distance': 9.84323501586914, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.23626317181720632, 'motion_component': -0.8095775295885126}, {'ion': 1320, 'force': [-0.5717068910598755, 0.7419012784957886, -1.8075217008590698], 'magnitude': 2.035780191421509, 'distance': 12.770373344421387, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.09641626228940431, 'motion_component': -0.19628231660630036}, {'ion': 1460, 'force': [-4.171939849853516, 3.5764050483703613, -1.7713687419891357], 'magnitude': 5.773517608642578, 'distance': 7.58313512802124, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.7734311038664372, 'motion_component': -4.465417884486193}]}, 4877: {'frame': 4877, 'ionic_force': [-1.2858441323041916, 6.905015721917152, -19.02397847175598], 'ionic_force_magnitude': 20.27916157404786, 'motion_vector': [-1.6677970886230469, 2.3718338012695312, 1.7540283203125], 'cosine_ionic_motion': -0.2160392511374309, 'ionic_motion_component': -4.381094880152263, 'ionic_force_x': -1.2858441323041916, 'ionic_force_y': 6.905015721917152, 'ionic_force_z': -19.02397847175598, 'radial_force': 7.023719616592349, 'axial_force': -19.02397847175598, 'before_closest_residue': 98, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.548943817615509, 0.45097389817237854, -2.8554723262786865], 'magnitude': 2.9425225257873535, 'distance': 10.622069358825684, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.48683309000334857, 'motion_component': -1.4325173471264652}, {'ion': 1320, 'force': [0.22946275770664215, 0.1839812844991684, -1.6267189979553223], 'magnitude': 1.6530932188034058, 'distance': 14.171648979187012, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.49976073485214356, 'motion_component': -0.826151048322767}, {'ion': 1460, 'force': [-2.0642507076263428, 6.2700605392456055, -14.541787147521973], 'magnitude': 15.96992015838623, 'distance': 4.559504508972168, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.13290148720347839, 'motion_component': -2.122426196693901}]}, 4878: {'frame': 4878, 'ionic_force': [-4.718822101131082, 12.355452835559845, -11.77543318271637], 'ionic_force_magnitude': 17.70834050481537, 'motion_vector': [3.3215065002441406, -4.6515045166015625, -1.365631103515625], 'cosine_ionic_motion': -0.5483564622691216, 'ionic_motion_component': -9.710482951877548, 'ionic_force_x': -4.718822101131082, 'ionic_force_y': 12.355452835559845, 'ionic_force_z': -11.77543318271637, 'radial_force': 13.225902494494164, 'axial_force': -11.77543318271637, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.08313600718975067, 1.643194556236267, -3.1667728424072266], 'magnitude': 3.568676233291626, 'distance': 9.645294189453125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.14508000757337663, 'motion_component': -0.5177435774466472}, {'ion': 1320, 'force': [-0.023140454664826393, 0.592434823513031, -1.7460500001907349], 'magnitude': 1.8439644575119019, 'distance': 13.418153762817383, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.04135362622311115, 'motion_component': -0.07625461900061781}, {'ion': 1460, 'force': [-4.778817653656006, 10.119823455810547, -6.862610340118408], 'magnitude': 13.127961158752441, 'distance': 5.028870105743408, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.6944326580126445, 'motion_component': -9.11648447082684}]}, 4879: {'frame': 4879, 'ionic_force': [16.751477003097534, -3.802208073437214, -9.315209746360779], 'ionic_force_magnitude': 19.540775333586726, 'motion_vector': [1.0792694091796875, 2.2563400268554688, 0.31360626220703125], 'cosine_ionic_motion': 0.13356250676512846, 'ionic_motion_component': 2.6099149376880324, 'ionic_force_x': 16.751477003097534, 'ionic_force_y': -3.802208073437214, 'ionic_force_z': -9.315209746360779, 'radial_force': 17.177565835094814, 'axial_force': -9.315209746360779, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.9992598295211792, -0.08213885873556137, -2.90842</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{4992: {'frame': 4992, 'ionic_force': [-9.90977567434311, -3.2852199375629425, -0.025440236553549767], 'ionic_force_magnitude': 10.440161452755383, 'motion_vector': [1.30914306640625, -2.567424774169922, 0.49839019775390625], 'cosine_ionic_motion': -0.14905922879596165, 'ionic_motion_component': -1.556202414653044, 'ionic_force_x': -9.90977567434311, 'ionic_force_y': -3.2852199375629425, 'ionic_force_z': -0.025440236553549767, 'radial_force': 10.440130456750216, 'axial_force': -0.025440236553549767, 'contributions': [{'ion': 1309, 'force': [-0.8666126132011414, -0.2845568358898163, -1.5572242736816406], 'magnitude': 1.8046987056732178, 'distance': 13.56334114074707, 'cosine_with_motion': -0.2235692216062886, 'motion_component': -0.4034750869979291}, {'ion': 1316, 'force': [-3.8274505138397217, -1.5964282751083374, 4.4594645500183105], 'magnitude': 6.089727878570557, 'distance': 7.383633136749268, 'cosine_with_motion': 0.073584092113622, 'motion_component': 0.44810709179433417}, {'ion': 1320, 'force': [-3.069931983947754, -1.0022555589675903, -2.9554810523986816], 'magnitude': 4.377655506134033, 'distance': 8.708598136901855, 'cosine_with_motion': -0.22796719378171773, 'motion_component': -0.9979618179615599}, {'ion': 1460, 'force': [-2.145780563354492, -0.4019792675971985, 0.027800539508461952], 'magnitude': 2.1832852363586426, 'distance': 12.331439971923828, 'cosine_with_motion': -0.27613096677313564, 'motion_component': -0.602872663331882}]}, 4993: {'frame': 4993, 'ionic_force': [-6.721731662750244, -7.0382163524627686, 0.02508533000946045], 'ionic_force_magnitude': 9.732358154315692, 'motion_vector': [-1.2147407531738281, 0.47171783447265625, 0.3584442138671875], 'cosine_ionic_motion': 0.3690367022768285, 'ionic_motion_component': 3.5915973586456644, 'ionic_force_x': -6.721731662750244, 'ionic_force_y': -7.0382163524627686, 'ionic_force_z': 0.02508533000946045, 'radial_force': 9.732325825315009, 'axial_force': 0.02508533000946045, 'contributions': [{'ion': 1309, 'force': [-0.767593502998352, -0.664334774017334, -1.574743628501892], 'magnitude': 1.873594880104065, 'distance': 13.311628341674805, 'cosine_with_motion': 0.02155868336146814, 'motion_component': 0.040392239910257643}, {'ion': 1316, 'force': [-0.9619420766830444, -1.5705485343933105, 2.251835346221924], 'magnitude': 2.9090750217437744, 'distance': 10.68295955657959, 'cosine_with_motion': 0.31406873477619174, 'motion_component': 0.9136495223597336}, {'ion': 1320, 'force': [-2.390256643295288, -2.211256742477417, -2.6654586791992188], 'magnitude': 4.2080464363098145, 'distance': 8.882369041442871, 'cosine_with_motion': 0.15913419023094658, 'motion_component': 0.6696440311311278}, {'ion': 1460, 'force': [-2.6019394397735596, -2.592076301574707, 2.0134522914886475], 'magnitude': 4.18842887878418, 'distance': 8.903144836425781, 'cosine_with_motion': 0.46984474326150344, 'motion_component': 1.9679114067019796}]}, 4994: {'frame': 4994, 'ionic_force': [-8.510059118270874, -4.980317711830139, -0.8486621975898743], 'ionic_force_magnitude': 9.89671148578417, 'motion_vector': [0.4574928283691406, 1.3063774108886719, 0.06430816650390625], 'cosine_ionic_motion': -0.762318113348161, 'ionic_motion_component': -7.544442428194064, 'ionic_force_x': -8.510059118270874, 'ionic_force_y': -4.980317711830139, 'ionic_force_z': -0.8486621975898743, 'radial_force': 9.860257131902506, 'axial_force': -0.8486621975898743, 'contributions': [{'ion': 1309, 'force': [-0.9202994108200073, -0.567900538444519, -1.5354427099227905], 'magnitude': 1.8780431747436523, 'distance': 13.295854568481445, 'cosine_with_motion': -0.4848207257917492, 'motion_component': -0.9105142778132502}, {'ion': 1316, 'force': [-1.8541682958602905, -1.3925756216049194, 2.6088037490844727], 'magnitude': 3.490424633026123, 'distance': 9.752813339233398, 'cosine_with_motion': -0.5168421163071228, 'motion_component': -1.8039984403479077}, {'ion': 1320, 'force': [-2.610811948776245, -1.7711108922958374, -2.3384480476379395], 'magnitude': 3.927023410797119, 'distance': 9.194694519042969, 'cosine_with_motion': -0.6723389238516795, 'motion_component': -2.640290627803788}, {'ion': 1460, 'force': [-3.124779462814331, -1.2487306594848633, 0.41642481088638306], 'magnitude': 3.3907203674316406, 'distance': 9.89516544342041, 'cosine_with_motion': -0.6457740657600884, 'motion_component': -2.189639274119873}]}, 4995: {'frame': 4995, 'ionic_force': [-7.9496631026268005, -3.4401994943618774, -2.7620067689567804], 'ionic_force_magnitude': 9.091798358852705, 'motion_vector': [0.29911041259765625, -1.0097732543945312, -0.8112640380859375], 'cosine_ionic_motion': 0.2760697449015972, 'ionic_motion_component': 2.5099704536252263, 'ionic_force_x': -7.9496631026268005, 'ionic_force_y': -3.4401994943618774, 'ionic_force_z': -2.7620067689567804, 'radial_force': 8.662108057873308, 'axial_force': -2.7620067689567804, 'contributions': [{'ion': 1309, 'force': [-0.9697037935256958, -0.4882330298423767, -1.6673376560211182], 'magnitude': 1.989651083946228, 'distance': 12.917562484741211, 'cosine_with_motion': 0.5881295353879933, 'motion_component': 1.1701726210799208}, {'ion': 1316, 'force': [-0.7669690251350403, -0.3876888155937195, 1.759548544883728], 'magnitude': 1.9582020044326782, 'distance': 13.020878791809082, 'cosine_with_motion': -0.48608984963177254, 'motion_component': -0.9518621296608849}, {'ion': 1320, 'force': [-3.7609140872955322, -1.9077779054641724, -2.8672845363616943], 'magnitude': 5.099550247192383, 'distance': 8.06869125366211, 'cosine_with_motion': 0.461351578304799, 'motion_component': 2.3526855188822395}, {'ion': 1460, 'force': [-2.4520761966705322, -0.6564997434616089, 0.013066878542304039], 'magnitude': 2.5384721755981445, 'distance': 11.43622875213623, 'cosine_with_motion': -0.02404027018762123, 'motion_component': -0.061025553861092874}]}, 4996: {'frame': 4996, 'ionic_force': [-5.756140172481537, -3.3770331740379333, -4.165502771735191], 'ionic_force_magnitude': 7.866950875983785, 'motion_vector': [-0.20244598388671875, 1.0721435546875, 1.0912857055664062], 'cosine_ionic_motion': -0.5766948765207079, 'ionic_motion_component': -4.536830264019944, 'ionic_force_x': -5.756140172481537, 'ionic_force_y': -3.3770331740379333, 'ionic_force_z': -4.165502771735191, 'radial_force': 6.673642389565723, 'axial_force': -4.165502771735191, 'contributions': [{'ion': 1309, 'force': [-0.8596774935722351, -0.5392806529998779, -1.5933207273483276], 'magnitude': 1.889057993888855, 'distance': 13.257035255432129, 'cosine_with_motion': -0.7350984190555, 'motion_component': -1.3886435159335724}, {'ion': 1320, 'force': [-2.712550401687622, -1.9728121757507324, -2.712400197982788], 'magnitude': 4.313587188720703, 'distance': 8.773033142089844, 'cosine_with_motion': -0.6799253774807416, 'motion_component': -2.9329172369528784}, {'ion': 1460, 'force': [-2.1839122772216797, -0.864940345287323, 0.14021815359592438], 'magnitude': 2.353137493133545, 'distance': 11.878056526184082, 'cosine_with_motion': -0.09148190274176744, 'motion_component': -0.21526948954107716}]}, 4997: {'frame': 4997, 'ionic_force': [-6.240003228187561, -2.746828645467758, -4.2932528257369995], 'ionic_force_magnitude': 8.056967650490607, 'motion_vector': [-0.3025016784667969, -0.6528167724609375, -0.76025390625], 'cosine_ionic_motion': 0.8234675078649084, 'ionic_motion_component': 6.634651072097687, 'ionic_force_x': -6.240003228187561, 'ionic_force_y': -2.746828645467758, 'ionic_force_z': -4.2932528257369995, 'radial_force': 6.817822811965226, 'axial_force': -4.2932528257369995, 'contributions': [{'ion': 1309, 'force': [-1.0400985479354858, -0.5203492045402527, -1.7408907413482666], 'magnitude': 2.093625783920288, 'distance': 12.592719078063965, 'cosine_with_motion': 0.9025147840163484, 'motion_component': 1.889528208024867}, {'ion': 1320, 'force': [-3.253243923187256, -1.7816591262817383, -2.824697256088257], 'magnitude': 4.662276268005371, 'distance': 8.438592910766602, 'cosine_with_motion': 0.8800268431847608, 'motion_component': 4.102928252537652}, {'ion': 1460, 'force': [-1.9466607570648193, -0.4448203146457672, 0.2723351716995239], 'magnitude': 2.0153212547302246, 'distance': 12.835030555725098, 'cosine_with_motion': 0.31865627031193433, 'motion_component': 0.6421947467171396}]}, 4998: {'frame': 4998, 'ionic_force': [-5.917741358280182, -2.6335960030555725, -4.115299761295319], 'ionic_force_magnitude': 7.67405908343996, 'motion_vector': [1.2956390380859375, -1.7068977355957031, 0.36876678466796875], 'cosine_ionic_motion': -0.28103523912743056, 'ionic_motion_component': -2.15668102959258, 'ionic_force_x': -5.917741358280182, 'ionic_force_y': -2.6335960030555725, 'ionic_force_z': -4.115299761295319, 'radial_force': 6.477305820386286, 'axial_force': -4.115299761295319, 'contributions': [{'ion': 1309, 'force': [-0.8881041407585144, -0.46092355251312256, -1.5887774229049683], 'magnitude': 1.8776030540466309, 'distance': 13.297412872314453, 'cosine_with_motion': -0.23263898336225206, 'motion_component': -0.4368036629911547}, {'ion': 1320, 'force': [-3.2808942794799805, -1.594046950340271, -2.6922800540924072], 'magnitude': 4.533610820770264, 'distance': 8.557500839233398, 'cosine_with_motion': -0.2559131491847294, 'motion_component': -1.160210559338669}, {'ion': 1460, 'force': [-1.748742938041687, -0.578625500202179, 0.16575771570205688], 'magnitude': 1.8494282960891724, 'distance': 13.39831829071045, 'cosine_with_motion': -0.3026160485951843, 'motion_component': -0.5596666774590444}]}, 4999: {'frame': 4999, 'ionic_force': [-11.94784277677536, -6.789508700370789, -1.4325785636901855], 'ionic_force_magnitude': 13.816680381050233, 'motion_vector': [-0.551971435546875, 1.3257789611816406, 0.19469451904296875], 'cosine_ionic_motion': -0.13411382016327142, 'ionic_motion_component': -1.8530077878775715, 'ionic_force_x': -11.94784277677536, 'ionic_force_y': -6.789508700370789, 'ionic_force_z': -1.4325785636901855, 'radial_force': 13.742211445431693, 'axial_force': -1.4325785636901855, 'contributions': [{'ion': 1309, 'force': [-0.7131099104881287, -0.7815901041030884, -1.624629020690918], 'magnitude': 1.938769817352295, 'distance': 13.085969924926758, 'cosine_with_motion': -0.34128113473276755, 'motion_component': -0.6616655531706854}, {'ion': 1320, 'force': [-2.2887518405914307, -2.6869468688964844, -2.5399811267852783], 'magnitude': 4.348513603210449, 'distance': 8.737730026245117, 'cosine_with_motion': -0.44327089905166983, 'motion_component': -1.9275696379600227}, {'ion': 1460, 'force': [-8.9459810256958, -3.320971727371216, 2.7320315837860107], 'magnitude': 9.925896644592285, 'distance': 5.783412456512451, 'cosine_with_motion': 0.07417239319387016, 'motion_component': 0.7362275165773262}]}, 5000: {'frame': 5000, 'ionic_force': [-9.01192718744278, -4.783424496650696, -3.6936601996421814], 'ionic_force_magnitude': 10.850765282566433, 'motion_vector': [-0.7812538146972656, 0.4613761901855469, -0.36583709716796875], 'cosine_ionic_motion': 0.5826446516183137, 'ionic_motion_component': 6.322140357853013, 'ionic_force_x': -9.01192718744278, 'ionic_force_y': -4.783424496650696, 'ionic_force_z': -3.6936601996421814, 'radial_force': 10.202743824429206, 'axial_force': -3.6936601996421814, 'contributions': [{'ion': 1309, 'force': [-0.9397225975990295, -0.6545020341873169, -1.707296371459961], 'magnitude': 2.055799722671509, 'distance': 12.70804214477539, 'cosine_with_motion': 0.525454039767896, 'motion_component': 1.080228253059616}, {'ion': 1320, 'force': [-3.7437233924865723, -2.7520456314086914, -2.9792110919952393], 'magnitude': 5.519503593444824, 'distance': 7.755664825439453, 'cosine_with_motion': 0.5083565310182332, 'motion_component': 2.805875644879151}, {'ion': 1460, 'force': [-4.328481197357178, -1.3768768310546875, 0.9928472638130188], 'magnitude': 4.649439334869385, 'distance': 8.450234413146973, 'cosine_with_motion': 0.523942040511297, 'motion_component': 2.436036667233086}]}, 5001: {'frame': 5001, 'ionic_force': [-6.330652832984924, -3.146571785211563, -2.4073009490966797], 'ionic_force_magnitude': 7.468144157070839, 'motion_vector': [-0.016719818115234375, -0.3343772888183594, 0.31487274169921875], 'cosine_ionic_motion': 0.11653666175395425, 'ionic_motion_component': 0.870312589562334, 'ionic_force_x': -6.330652832984924, 'ionic_force_y': -3.146571785211563, 'ionic_force_z': -2.4073009490966797, 'radial_force': 7.06951761376047, 'axial_force': -2.4073009490966797, 'contributions': [{'ion': 1309, 'force': [-0.9957014322280884, -0.4937232434749603, -1.515923261642456], 'magnitude': 1.8796827793121338, 'distance': 13.290054321289062, 'cosine_with_motion': -0.3421508167823267, 'motion_component': -0.6431349952876526}, {'ion': 1320, 'force': [-2.770164966583252, -1.6772152185440063, -2.3731327056884766], 'magnitude': 4.014800548553467, 'distance': 9.09362506866455, 'cosine_with_motion': -0.07592411220123893, 'motion_component': -0.3048201694466055}, {'ion': 1460, 'force': [-2.564786434173584, -0.9756333231925964, 1.481755018234253], 'magnitude': 3.1185874938964844, 'distance': 10.317870140075684, 'cosine_with_motion': 0.5830420678716011, 'motion_component': 1.8182676836329943}]}, 5002: {'frame': 5002, 'ionic_force': [-7.864047288894653, -3.612726092338562, -1.8392441272735596], 'ionic_force_magnitude': 8.847476958994891, 'motion_vector': [1.8620643615722656, -2.09149169921875, 0.0738525390625], 'cosine_ionic_motion': -0.2914451320352368, 'ionic_motion_component': -2.5785540904929816, 'ionic_force_x': -7.864047288894653, 'ionic_force_y': -3.612726092338562, 'ionic_force_z': -1.8392441272735596, 'radial_force': 8.654191445781356, 'axial_force': -1.8392441272735596, 'contributions': [{'ion': 1309, 'force': [-1.0093481540679932, -0.5549268126487732, -1.643075942993164], 'magnitude': 2.0065956115722656, 'distance': 12.862906455993652, 'cosine_with_motion': -0.14947363285212528, 'motion_component': -0.299933138318341}, {'ion': 1320, 'force': [-3.4694180488586426, -2.0770719051361084, -2.471514940261841], 'magnitude': 4.739142894744873, 'distance': 8.369877815246582, 'cosine_with_motion': -0.17314703360432673, 'motion_component': -0.8205685344170597}, {'ion': 1460, 'force': [-3.3852810859680176, -0.9807273745536804, 2.2753467559814453], 'magnitude': 4.195135116577148, 'distance': 8.896026611328125, 'cosine_with_motion': -0.34755786630106694, 'motion_component': -1.4580521448367174}]}, 5003: {'frame': 5003, 'ionic_force': [-5.132673859596252, -6.734123051166534, -1.4360578060150146], 'ionic_force_magnitude': 8.58807407044512, 'motion_vector': [-0.707275390625, -0.40502166748046875, -0.429779052734375], 'cosine_ionic_motion': 0.8814315808209459, 'ionic_motion_component': 7.569799704119818, 'ionic_force_x': -5.132673859596252, 'ionic_force_y': -6.734123051166534, 'ionic_force_z': -1.4360578060150146, 'radial_force': 8.467157387059435, 'axial_force': -1.4360578060150146, 'contributions': [{'ion': 1309, 'force': [-0.6637636423110962, -0.8726678490638733, -1.511733055114746], 'magnitude': 1.8674763441085815, 'distance': 13.333417892456055, 'cosine_with_motion': 0.8558256065889733, 'motion_component': 1.5982341395508683}, {'ion': 1320, 'force': [-2.242825746536255, -3.0832972526550293, -2.36020565032959], 'magnitude': 4.484145164489746, 'distance': 8.604570388793945, 'cosine_with_motion': 0.9316849689159826, 'motion_component': 4.17781086980186}, {'ion': 1460, 'force': [-2.2260844707489014, -2.778157949447632, 2.4358808994293213], 'magnitude': 4.313598155975342, 'distance': 8.773021697998047, 'cosine_with_motion': 0.41583722061378225, 'motion_component': 1.793754685761428}]}, 5004: {'frame': 5004, 'ionic_force': [-4.717077851295471, -4.595800518989563, -2.3284347653388977], 'ionic_force_magnitude': 6.985256925981022, 'motion_vector': [-0.6747245788574219, 2.4837417602539062, -0.2197113037109375], 'cosine_ionic_motion': -0.42787515374866464, 'ionic_motion_component': -2.9888178811780546, 'ionic_force_x': -4.717077851295471, 'ionic_force_y': -4.595800518989563, 'ionic_force_z': -2.3284347653388977, 'radial_force': 6.585757804955102, 'axial_force': -2.3284347653388977, 'contributions': [{'ion': 1309, 'force': [-0.6875178813934326, -0.8340977430343628, -1.441748857498169], 'magnitude': 1.8019543886184692, 'distance': 13.573665618896484, 'cosine_with_motion': -0.27736274933035654, 'motion_component': -0.4997950258276198}, {'ion': 1320, 'force': [-2.1348366737365723, -2.760021209716797, -1.877365231513977], 'magnitude': 3.9622902870178223, 'distance': 9.15368366241455, 'cosine_with_motion': -0.48873895636195097, 'motion_component': -1.936525656408099}, {'ion': 1460, 'force': [-1.8947232961654663, -1.0016815662384033, 0.9906793236732483], 'magnitude': 2.3610990047454834, 'distance': 11.858014106750488, 'cosine_with_motion': -0.23399998864807015, 'motion_component': -0.552497107667592}]}, 5005: {'frame': 5005, 'ionic_force': [-5.8636956214904785, -3.0404764115810394, -2.9966933727264404], 'ionic_force_magnitude': 7.253109286437775, 'motion_vector': [1.9760818481445312, -2.551136016845703, 1.67626953125], 'cosine_ionic_motion': -0.33568837728081463, 'ionic_motion_component': -2.434784486604704, 'ionic_force_x': -5.8636956214904785, 'ionic_force_y': -3.0404764115810394, 'ionic_force_z': -2.9966933727264404, 'radial_force': 6.605105839490183, 'axial_force': -2.9966933727264404, 'contributions': [{'ion': 1309, 'force': [-0.8727691173553467, -0.5728297829627991, -1.483247995376587], 'magnitude': 1.8138039112091064, 'distance': 13.529254913330078, 'cosine_with_motion': -0.4168848729684455, 'motion_component': -0.7561473993155872}, {'ion': 1320, 'force': [-3.1719272136688232, -2.036134958267212, -2.4662981033325195], 'magnitude': 4.504396915435791, 'distance': 8.585206031799316, 'cosine_with_motion': -0.31793913100847976, 'motion_component': -1.4321241320576232}, {'ion': 1460, 'force': [-1.8189992904663086, -0.43151167035102844, 0.952852725982666], 'magnitude': 2.098306179046631, 'distance': 12.578666687011719, 'cosine_with_motion': -0.11748188627750467, 'motion_component': -0.24651297452992438}]}, 5006: {'frame': 5006, 'ionic_force': [-4.633662641048431, -6.107035517692566, -2.5804152488708496], 'ionic_force_magnitude': 8.088587957240227, 'motion_vector': [-2.692249298095703, 2.7754745483398438, -1.560882568359375], 'cosine_ionic_motion': -0.013259507049575554, 'ionic_motion_component': -0.10725068904013872, 'ionic_force_x': -4.633662641048431, 'ionic_force_y': -6.107035517692566, 'ionic_force_z': -2.5804152488708496, 'radial_force': 7.665944970152501, 'axial_force': -2.5804152488708496, 'contributions': [{'ion': 1309, 'force': [-0.7836499810218811, -1.1199933290481567, -1.7357754707336426], 'magnitude': 2.2093911170959473, 'distance': 12.258370399475098, 'cosine_with_motion': 0.18567602863252866, 'motion_component': 0.41023095682033883}, {'ion': 1320, 'force': [-2.376492977142334, -4.063398838043213, -2.111187219619751], 'magnitude': 5.159073352813721, 'distance': 8.02200984954834, 'cosine_with_motion': -0.07365114574792865, 'motion_component': -0.3799716820196793}, {'ion': 1460, 'force': [-1.4735196828842163, -0.9236433506011963, 1.266547441482544], 'magnitude': 2.151399612426758, 'distance': 12.422486305236816, 'cosine_with_motion': -0.06391642443920177, 'motion_component': -0.1375097622119199}]}, 5007: {'frame': 5007, 'ionic_force': [-5.718433976173401, -2.855208694934845, -3.147172212600708], 'ionic_force_magnitude': 7.124422556758681, 'motion_vector': [0.5759010314941406, -0.5521697998046875, 0.14435577392578125], 'cosine_ionic_motion': -0.37583636937022347, 'ionic_motion_component': -2.6776171075915074, 'ionic_force_x': -5.718433976173401, 'ionic_force_y': -2.855208694934845, 'ionic_force_z': -3.147172212600708, 'radial_force': 6.391611990060556, 'axial_force': -3.147172212600708, 'contributions': [{'ion': 1309, 'force': [-0.9638186693191528, -0.5711681842803955, -1.511455774307251], 'magnitude': 1.8814032077789307, 'distance': 13.283976554870605, 'cosine_with_motion': -0.3001565084066107, 'motion_component': -0.5647154217011554}, {'ion': 1320, 'force': [-3.205503225326538, -1.8640981912612915, -2.3779666423797607], 'magnitude': 4.405092239379883, 'distance': 8.681435585021973, 'cosine_with_motion': -0.32478865433870185, 'motion_component': -1.4307240068059563}, {'ion': 1460, 'force': [-1.54911208152771, -0.41994231939315796, 0.7422502040863037], 'magnitude': 1.7683424949645996, 'distance': 13.702059745788574, 'cosine_with_motion': -0.38577229909063343, 'motion_component': -0.682177547541098}]}, 5008: {'frame': 5008, 'ionic_force': [-5.75127911567688, -3.5837172269821167, -3.116843521595001], 'ionic_force_magnitude': 7.45888424414122, 'motion_vector': [0.1088409423828125, -0.9409523010253906, -0.1216583251953125], 'cosine_ionic_motion': 0.4387472499987256, 'ionic_motion_component': 3.2725649501757834, 'ionic_force_x': -5.75127911567688, 'ionic_force_y': -3.5837172269821167, 'ionic_force_z': -3.116843521595001, 'radial_force': 6.776447493295394, 'axial_force': -3.116843521595001, 'contributions': [{'ion': 1309, 'force': [-0.929062008857727, -0.6301071643829346, -1.557762622833252], 'magnitude': 1.9201081991195679, 'distance': 13.149407386779785, 'cosine_with_motion': 0.37153807724211496, 'motion_component': 0.7133933226855955}, {'ion': 1320, 'force': [-3.084425449371338, -2.398221731185913, -2.444641351699829], 'magnitude': 4.608841419219971, 'distance': 8.487370491027832, 'cosine_with_motion': 0.5039926709766444, 'motion_component': 2.3228222934584686}, {'ion': 1460, 'force': [-1.737791657447815, -0.555388331413269, 0.8855604529380798], 'magnitude': 2.0279529094696045, 'distance': 12.794994354248047, 'cosine_with_motion': 0.11654576116051595, 'motion_component': 0.23634932566563815}]}, 5009: {'frame': 5009, 'ionic_force': [-4.791661620140076, -3.3943287134170532, -3.0958730578422546], 'ionic_force_magnitude': 6.638216514013718, 'motion_vector': [-0.2537117004394531, 1.1904716491699219, 0.37801361083984375], 'cosine_ionic_motion': -0.4722309263117984, 'ionic_motion_component': -3.1347711334709754, 'ionic_force_x': -4.791661620140076, 'ionic_force_y': -3.3943287134170532, 'ionic_force_z': -3.0958730578422546, 'radial_force': 5.87209404698621, 'axial_force': -3.0958730578422546, 'contributions': [{'ion': 1309, 'force': [-0.8100695610046387, -0.6891690492630005, -1.492370843887329], 'magnitude': 1.8325767517089844, 'distance': 13.459779739379883, 'cosine_with_motion': -0.5047908100773542, 'motion_component': -0.9250678833166076}, {'ion': 1320, 'force': [-2.5722618103027344, -2.1343741416931152, -2.2908530235290527], 'magnitude': 4.052171230316162, 'distance': 9.051595687866211, 'cosine_with_motion': -0.5332870526809247, 'motion_component': -2.1609704321776206}, {'ion': 1460, 'force': [-1.4093302488327026, -0.5707855224609375, 0.6873508095741272], 'magnitude': 1.6686698198318481, 'distance': 14.10534954071045, 'cosine_with_motion': -0.02920451360238688, 'motion_component': -0.048732690720088456}]}, 5010: {'frame': 5010, 'ionic_force': [-6.056791543960571, -3.679370939731598, -3.146594524383545], 'ionic_force_magnitude': 7.753937800886345, 'motion_vector': [0.18355178833007812, 0.16788864135742188, -0.24420166015625], 'cosine_ionic_motion': -0.3555627191622645, 'ionic_motion_component': -2.7570112086982186, 'ionic_force_x': -6.056791543960571, 'ionic_force_y': -3.679370939731598, 'ionic_force_z': -3.146594524383545, 'radial_force': 7.086783072673642, 'axial_force': -3.146594524383545, 'contributions': [{'ion': 1309, 'force': [-1.0071114301681519, -0.6563244462013245, -1.6691867113113403], 'magnitude': 2.056992769241333, 'distance': 12.70435619354248, 'cosine_with_motion': 0.15699508780823138, 'motion_component': 0.3229377694326381}, {'ion': 1320, 'force': [-3.5231919288635254, -2.5213658809661865, -2.321716070175171], 'magnitude': 4.915336608886719, 'distance': 8.218497276306152, 'cosine_with_motion': -0.2935827208285289, 'motion_component': -1.4430578597423107}, {'ion': 1460, 'force': [-1.526488184928894, -0.5016806125640869, 0.8443082571029663], 'magnitude': 1.81513249874115, 'distance': 13.52430248260498, 'cosine_with_motion': -0.9018025914210851, 'motion_component': -1.6368912062349423}]}, 5011: {'frame': 5011, 'ionic_force': [-5.516871929168701, -3.2253422141075134, -3.525465488433838], 'ionic_force_magnitude': 7.2984666328682755, 'motion_vector': [0.9372367858886719, -0.7911605834960938, -0.0274505615234375], 'cosine_ionic_motion': -0.2816719609338294, 'ionic_motion_component': -2.0557734082901304, 'ionic_force_x': -5.516871929168701, 'ionic_force_y': -3.2253422141075134, 'ionic_force_z': -3.525465488433838, 'radial_force': 6.390517058967415, 'axial_force': -3.525465488433838, 'contributions': [{'ion': 1309, 'force': [-0.9378553628921509, -0.546708881855011, -1.6660550832748413], 'magnitude': 1.9885177612304688, 'distance': 12.921243667602539, 'cosine_with_motion': -0.16426040768421035, 'motion_component': -0.3266347355442112}, {'ion': 1320, 'force': [-3.1024675369262695, -2.091669797897339, -2.5550997257232666], 'magnitude': 4.530885696411133, 'distance': 8.560073852539062, 'cosine_with_motion': -0.21278014597992131, 'motion_component': -0.9640824441874996}, {'ion': 1460, 'force': [-1.4765490293502808, -0.5869635343551636, 0.69568932056427], 'magnitude': 1.7345623970031738, 'distance': 13.834837913513184, 'cosine_with_motion': -0.44106586930846237, 'motion_component': -0.7650562903700497}]}, 5012: {'frame': 5012, 'ionic_force': [-5.650092005729675, -4.366848289966583, -3.620231330394745], 'ionic_force_magnitude': 8.006183769210281, 'motion_vector': [-0.8405380249023438, -0.2687263488769531, 0.18675994873046875], 'cosine_ionic_motion': 0.7265048948557896, 'ionic_motion_component': 5.816531697446245, 'ionic_force_x': -5.650092005729675, 'ionic_force_y': -4.366848289966583, 'ionic_force_z': -3.620231330394745, 'radial_force': 7.140931568135523, 'axial_force': -3.620231330394745, 'contributions': [{'ion': 1309, 'force': [-0.7837142944335938, -0.6856822371482849, -1.6732805967330933], 'magnitude': 1.9708465337753296, 'distance': 12.979042053222656, 'cosine_with_motion': 0.2984203489596868, 'motion_component': 0.5881407195424284}, {'ion': 1320, 'force': [-3.166684865951538, -2.999635934829712, -2.8368637561798096], 'magnitude': 5.203220844268799, 'distance': 7.987905502319336, 'cosine_with_motion': 0.625998048098166, 'motion_component': 3.257205947883776}, {'ion': 1460, 'force': [-1.6996928453445435, -0.6815301179885864, 0.889913022518158], 'magnitude': 2.0360217094421387, 'distance': 12.76961612701416, 'cosine_with_motion': 0.9681552541475777, 'motion_component': 1.9711850814531946}]}, 5013: {'frame': 5013, 'ionic_force': [-5.9465718269348145, -4.000038325786591, -3.3016263842582703], 'ionic_force_magnitude': 7.8906755022549735, 'motion_vector': [-0.21096038818359375, 1.4655113220214844, 0.278533935546875], 'cosine_ionic_motion': -0.4649415414172259, 'ionic_motion_component': -3.6687028308415703, 'ionic_force_x': -5.9465718269348145, 'ionic_force_y': -4.000038325786591, 'ionic_force_z': -3.3016263842582703, 'radial_force': 7.166730293561803, 'axial_force': -3.3016263842582703, 'contributions': [{'ion': 1309, 'force': [-0.7687656879425049, -0.6304101347923279, -1.5830514430999756], 'magnitude': 1.8693499565124512, 'distance': 13.326733589172363, 'cosine_with_motion': -0.4270177269430876, 'motion_component': -0.7982455958570078}, {'ion': 1320, 'force': [-2.5553226470947266, -2.115832567214966, -2.6662724018096924], 'magnitude': 4.256222248077393, 'distance': 8.831955909729004, 'cosine_with_motion': -0.5153085487858513, 'motion_component': -2.193267829759243}, {'ion': 1460, 'force': [-2.622483491897583, -1.2537956237792969, 0.9476974606513977], 'magnitude': 3.0573768615722656, 'distance': 10.42064380645752, 'cosine_with_motion': -0.22149356868241477, 'motion_component': -0.6771893240015832}]}, 5014: {'frame': 5014, 'ionic_force': [-6.269465744495392, -3.210474908351898, -4.206337511539459], 'ionic_force_magnitude': 8.204061501448063, 'motion_vector': [-0.07615280151367188, 0.12347412109375, -0.5725250244140625], 'cosine_ionic_motion': 0.5137294905108934, 'ionic_motion_component': 4.214668335258949, 'ionic_force_x': -6.269465744495392, 'ionic_force_y': -3.210474908351898, 'ionic_force_z': -4.206337511539459, 'radial_force': 7.043674457167814, 'axial_force': -4.206337511539459, 'contributions': [{'ion': 1309, 'force': [-0.9814146161079407, -0.5977436304092407, -1.782705545425415], 'magnitude': 2.120969533920288, 'distance': 12.511282920837402, 'cosine_with_motion': 0.8155094870457856, 'motion_component': 1.7296706601974083}, {'ion': 1320, 'force': [-3.2142367362976074, -2.007704019546509, -2.7193706035614014], 'magnitude': 4.664458274841309, 'distance': 8.43661880493164, 'cosine_with_motion': 0.5640035191898288, 'motion_component': 2.6307708040646354}, {'ion': 1460, 'force': [-2.0738143920898438, -0.6050272583961487, 0.2957386374473572], 'magnitude': 2.1804184913635254, 'distance': 12.339544296264648, 'cosine_with_motion': -0.06685550885342192, 'motion_component': -0.14577299787865972}]}, 5015: {'frame': 5015, 'ionic_force': [-6.003054678440094, -2.8174749612808228, -4.174112513661385], 'ionic_force_magnitude': 7.8356905188049915, 'motion_vector': [-0.7897682189941406, -0.2777671813964844, 0.30731964111328125], 'cosine_ionic_motion': 0.6068754930825757, 'ionic_motion_component': 4.755288547242243, 'ionic_force_x': -6.003054678440094, 'ionic_force_y': -2.8174749612808228, 'ionic_force_z': -4.174112513661385, 'radial_force': 6.631352096653131, 'axial_force': -4.174112513661385, 'contributions': [{'ion': 1309, 'force': [-0.8658602833747864, -0.46252405643463135, -1.602197527885437], 'magnitude': 1.8790102005004883, 'distance': 13.29243278503418, 'cosine_with_motion': 0.19091160358013518, 'motion_component': 0.35872485650961394}, {'ion': 1320, 'force': [-3.3091530799865723, -1.7206918001174927, -2.800626277923584], 'magnitude': 4.6642022132873535, 'distance': 8.436850547790527, 'cosine_with_motion': 0.5362836659961173, 'motion_component': 2.5013354411892053}, {'ion': 1460, 'force': [-1.8280413150787354, -0.6342591047286987, 0.2287112921476364], 'magnitude': 1.9484169483184814, 'distance': 13.053533554077148, 'cosine_with_motion': 0.9727015971388674, 'motion_component': 1.8952282556125608}]}, 5016: {'frame': 5016, 'ionic_force': [-4.904240369796753, -2.443116396665573, -3.3296403288841248], 'ionic_force_magnitude': 6.411465983075317, 'motion_vector': [1.1025390625, 0.10252761840820312, 0.24944305419921875], 'cosine_ionic_motion': -0.8915613515141652, 'ionic_motion_component': -5.716215277057725, 'ionic_force_x': -4.904240369796753, 'ionic_force_y': -2.443116396665573, 'ionic_force_z': -3.3296403288841248, 'radial_force': 5.479086724299988, 'axial_force': -3.3296403288841248, 'contributions': [{'ion': 1309, 'force': [-1.0098766088485718, -0.4893936812877655, -1.7097877264022827], 'magnitude': 2.045172691345215, 'distance': 12.741015434265137, 'cosine_with_motion': -0.6849855578015981, 'motion_component': -1.4009137019063496}, {'ion': 1320, 'force': [-2.484668016433716, -1.4379808902740479, -2.1973519325256348], 'magnitude': 3.615206718444824, 'distance': 9.583022117614746, 'cosine_with_motion': -0.8371041514779677, 'motion_component': -3.0263045629930083}, {'ion': 1460, 'force': [-1.4096957445144653, -0.5157418251037598, 0.5774993300437927], 'magnitude': 1.608333706855774, 'distance': 14.367491722106934, 'cosine_with_motion': -0.8014488515229483, 'motion_component': -1.288997173785691}]}, 5017: {'frame': 5017, 'ionic_force': [-5.9368895292282104, -3.2834761142730713, -4.590190887451172], 'ionic_force_magnitude': 8.191320104751195, 'motion_vector': [0.5471343994140625, -1.6718521118164062, -0.3502349853515625], 'cosine_ionic_motion': 0.2619658768360037, 'ionic_motion_component': 2.1458463536855326, 'ionic_force_x': -5.9368895292282104, 'ionic_force_y': -3.2834761142730713, 'ionic_force_z': -4.590190887451172, 'radial_force': 6.784384472836232, 'axial_force': -4.590190887451172, 'contributions': [{'ion': 1309, 'force': [-0.9971057176589966, -0.5652839541435242, -2.227571964263916], 'magnitude': 2.5051631927490234, 'distance': 11.512006759643555, 'cosine_with_motion': 0.2625429580884971, 'motion_component': 0.6577129548394858}, {'ion': 1320, 'force': [-3.1286773681640625, -1.8227983713150024, -2.7695655822753906], 'magnitude': 4.558696269989014, 'distance': 8.533923149108887, 'cosine_with_motion': 0.2819798713288931, 'motion_component': 1.2854605198777804}, {'ion': 1460, 'force': [-1.8111064434051514, -0.8953937888145447, 0.40694665908813477], 'magnitude': 2.0609323978424072, 'distance': 12.692207336425781, 'cosine_with_motion': 0.09834044099433077, 'motion_component': 0.20267299659885296}]}, 5018: {'frame': 5018, 'ionic_force': [-5.11282</t>
+          <t>{4992: {'frame': 4992, 'ionic_force': [-9.90977567434311, -3.2852199375629425, -0.025440236553549767], 'ionic_force_magnitude': 10.440161452755383, 'motion_vector': [1.30914306640625, -2.567424774169922, 0.49839019775390625], 'cosine_ionic_motion': -0.14905922879596165, 'ionic_motion_component': -1.556202414653044, 'ionic_force_x': -9.90977567434311, 'ionic_force_y': -3.2852199375629425, 'ionic_force_z': -0.025440236553549767, 'radial_force': 10.440130456750216, 'axial_force': -0.025440236553549767, 'before_closest_residue': None, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.8666126132011414, -0.2845568358898163, -1.5572242736816406], 'magnitude': 1.8046987056732178, 'distance': 13.56334114074707, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2235692216062886, 'motion_component': -0.4034750869979291}, {'ion': 1316, 'force': [-3.8274505138397217, -1.5964282751083374, 4.4594645500183105], 'magnitude': 6.089727878570557, 'distance': 7.383633136749268, 'before_closest_residue': 780, 'closest_residue': 130, 'next_closest_residue': 130, 'cosine_with_motion': 0.073584092113622, 'motion_component': 0.44810709179433417}, {'ion': 1320, 'force': [-3.069931983947754, -1.0022555589675903, -2.9554810523986816], 'magnitude': 4.377655506134033, 'distance': 8.708598136901855, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.22796719378171773, 'motion_component': -0.9979618179615599}, {'ion': 1460, 'force': [-2.145780563354492, -0.4019792675971985, 0.027800539508461952], 'magnitude': 2.1832852363586426, 'distance': 12.331439971923828, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 130, 'cosine_with_motion': -0.27613096677313564, 'motion_component': -0.602872663331882}]}, 4993: {'frame': 4993, 'ionic_force': [-6.721731662750244, -7.0382163524627686, 0.02508533000946045], 'ionic_force_magnitude': 9.732358154315692, 'motion_vector': [-1.2147407531738281, 0.47171783447265625, 0.3584442138671875], 'cosine_ionic_motion': 0.3690367022768285, 'ionic_motion_component': 3.5915973586456644, 'ionic_force_x': -6.721731662750244, 'ionic_force_y': -7.0382163524627686, 'ionic_force_z': 0.02508533000946045, 'radial_force': 9.732325825315009, 'axial_force': 0.02508533000946045, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.767593502998352, -0.664334774017334, -1.574743628501892], 'magnitude': 1.873594880104065, 'distance': 13.311628341674805, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.02155868336146814, 'motion_component': 0.040392239910257643}, {'ion': 1316, 'force': [-0.9619420766830444, -1.5705485343933105, 2.251835346221924], 'magnitude': 2.9090750217437744, 'distance': 10.68295955657959, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 1105, 'cosine_with_motion': 0.31406873477619174, 'motion_component': 0.9136495223597336}, {'ion': 1320, 'force': [-2.390256643295288, -2.211256742477417, -2.6654586791992188], 'magnitude': 4.2080464363098145, 'distance': 8.882369041442871, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.15913419023094658, 'motion_component': 0.6696440311311278}, {'ion': 1460, 'force': [-2.6019394397735596, -2.592076301574707, 2.0134522914886475], 'magnitude': 4.18842887878418, 'distance': 8.903144836425781, 'before_closest_residue': 423, 'closest_residue': 130, 'next_closest_residue': 780, 'cosine_with_motion': 0.46984474326150344, 'motion_component': 1.9679114067019796}]}, 4994: {'frame': 4994, 'ionic_force': [-8.510059118270874, -4.980317711830139, -0.8486621975898743], 'ionic_force_magnitude': 9.89671148578417, 'motion_vector': [0.4574928283691406, 1.3063774108886719, 0.06430816650390625], 'cosine_ionic_motion': -0.762318113348161, 'ionic_motion_component': -7.544442428194064, 'ionic_force_x': -8.510059118270874, 'ionic_force_y': -4.980317711830139, 'ionic_force_z': -0.8486621975898743, 'radial_force': 9.860257131902506, 'axial_force': -0.8486621975898743, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.9202994108200073, -0.567900538444519, -1.5354427099227905], 'magnitude': 1.8780431747436523, 'distance': 13.295854568481445, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.4848207257917492, 'motion_component': -0.9105142778132502}, {'ion': 1316, 'force': [-1.8541682958602905, -1.3925756216049194, 2.6088037490844727], 'magnitude': 3.490424633026123, 'distance': 9.752813339233398, 'before_closest_residue': 130, 'closest_residue': 1105, 'next_closest_residue': None, 'cosine_with_motion': -0.5168421163071228, 'motion_component': -1.8039984403479077}, {'ion': 1320, 'force': [-2.610811948776245, -1.7711108922958374, -2.3384480476379395], 'magnitude': 3.927023410797119, 'distance': 9.194694519042969, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6723389238516795, 'motion_component': -2.640290627803788}, {'ion': 1460, 'force': [-3.124779462814331, -1.2487306594848633, 0.41642481088638306], 'magnitude': 3.3907203674316406, 'distance': 9.89516544342041, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 423, 'cosine_with_motion': -0.6457740657600884, 'motion_component': -2.189639274119873}]}, 4995: {'frame': 4995, 'ionic_force': [-7.9496631026268005, -3.4401994943618774, -2.7620067689567804], 'ionic_force_magnitude': 9.091798358852705, 'motion_vector': [0.29911041259765625, -1.0097732543945312, -0.8112640380859375], 'cosine_ionic_motion': 0.2760697449015972, 'ionic_motion_component': 2.5099704536252263, 'ionic_force_x': -7.9496631026268005, 'ionic_force_y': -3.4401994943618774, 'ionic_force_z': -2.7620067689567804, 'radial_force': 8.662108057873308, 'axial_force': -2.7620067689567804, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.9697037935256958, -0.4882330298423767, -1.6673376560211182], 'magnitude': 1.989651083946228, 'distance': 12.917562484741211, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5881295353879933, 'motion_component': 1.1701726210799208}, {'ion': 1316, 'force': [-0.7669690251350403, -0.3876888155937195, 1.759548544883728], 'magnitude': 1.9582020044326782, 'distance': 13.020878791809082, 'before_closest_residue': 1105, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.48608984963177254, 'motion_component': -0.9518621296608849}, {'ion': 1320, 'force': [-3.7609140872955322, -1.9077779054641724, -2.8672845363616943], 'magnitude': 5.099550247192383, 'distance': 8.06869125366211, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.461351578304799, 'motion_component': 2.3526855188822395}, {'ion': 1460, 'force': [-2.4520761966705322, -0.6564997434616089, 0.013066878542304039], 'magnitude': 2.5384721755981445, 'distance': 11.43622875213623, 'before_closest_residue': 780, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.02404027018762123, 'motion_component': -0.061025553861092874}]}, 4996: {'frame': 4996, 'ionic_force': [-5.756140172481537, -3.3770331740379333, -4.165502771735191], 'ionic_force_magnitude': 7.866950875983785, 'motion_vector': [-0.20244598388671875, 1.0721435546875, 1.0912857055664062], 'cosine_ionic_motion': -0.5766948765207079, 'ionic_motion_component': -4.536830264019944, 'ionic_force_x': -5.756140172481537, 'ionic_force_y': -3.3770331740379333, 'ionic_force_z': -4.165502771735191, 'radial_force': 6.673642389565723, 'axial_force': -4.165502771735191, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.8596774935722351, -0.5392806529998779, -1.5933207273483276], 'magnitude': 1.889057993888855, 'distance': 13.257035255432129, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7350984190555, 'motion_component': -1.3886435159335724}, {'ion': 1320, 'force': [-2.712550401687622, -1.9728121757507324, -2.712400197982788], 'magnitude': 4.313587188720703, 'distance': 8.773033142089844, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6799253774807416, 'motion_component': -2.9329172369528784}, {'ion': 1460, 'force': [-2.1839122772216797, -0.864940345287323, 0.14021815359592438], 'magnitude': 2.353137493133545, 'distance': 11.878056526184082, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 780, 'cosine_with_motion': -0.09148190274176744, 'motion_component': -0.21526948954107716}]}, 4997: {'frame': 4997, 'ionic_force': [-6.240003228187561, -2.746828645467758, -4.2932528257369995], 'ionic_force_magnitude': 8.056967650490607, 'motion_vector': [-0.3025016784667969, -0.6528167724609375, -0.76025390625], 'cosine_ionic_motion': 0.8234675078649084, 'ionic_motion_component': 6.634651072097687, 'ionic_force_x': -6.240003228187561, 'ionic_force_y': -2.746828645467758, 'ionic_force_z': -4.2932528257369995, 'radial_force': 6.817822811965226, 'axial_force': -4.2932528257369995, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.0400985479354858, -0.5203492045402527, -1.7408907413482666], 'magnitude': 2.093625783920288, 'distance': 12.592719078063965, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9025147840163484, 'motion_component': 1.889528208024867}, {'ion': 1320, 'force': [-3.253243923187256, -1.7816591262817383, -2.824697256088257], 'magnitude': 4.662276268005371, 'distance': 8.438592910766602, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8800268431847608, 'motion_component': 4.102928252537652}, {'ion': 1460, 'force': [-1.9466607570648193, -0.4448203146457672, 0.2723351716995239], 'magnitude': 2.0153212547302246, 'distance': 12.835030555725098, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 455, 'cosine_with_motion': 0.31865627031193433, 'motion_component': 0.6421947467171396}]}, 4998: {'frame': 4998, 'ionic_force': [-5.917741358280182, -2.6335960030555725, -4.115299761295319], 'ionic_force_magnitude': 7.67405908343996, 'motion_vector': [1.2956390380859375, -1.7068977355957031, 0.36876678466796875], 'cosine_ionic_motion': -0.28103523912743056, 'ionic_motion_component': -2.15668102959258, 'ionic_force_x': -5.917741358280182, 'ionic_force_y': -2.6335960030555725, 'ionic_force_z': -4.115299761295319, 'radial_force': 6.477305820386286, 'axial_force': -4.115299761295319, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.8881041407585144, -0.46092355251312256, -1.5887774229049683], 'magnitude': 1.8776030540466309, 'distance': 13.297412872314453, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.23263898336225206, 'motion_component': -0.4368036629911547}, {'ion': 1320, 'force': [-3.2808942794799805, -1.594046950340271, -2.6922800540924072], 'magnitude': 4.533610820770264, 'distance': 8.557500839233398, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2559131491847294, 'motion_component': -1.160210559338669}, {'ion': 1460, 'force': [-1.748742938041687, -0.578625500202179, 0.16575771570205688], 'magnitude': 1.8494282960891724, 'distance': 13.39831829071045, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 780, 'cosine_with_motion': -0.3026160485951843, 'motion_component': -0.5596666774590444}]}, 4999: {'frame': 4999, 'ionic_force': [-11.94784277677536, -6.789508700370789, -1.4325785636901855], 'ionic_force_magnitude': 13.816680381050233, 'motion_vector': [-0.551971435546875, 1.3257789611816406, 0.19469451904296875], 'cosine_ionic_motion': -0.13411382016327142, 'ionic_motion_component': -1.8530077878775715, 'ionic_force_x': -11.94784277677536, 'ionic_force_y': -6.789508700370789, 'ionic_force_z': -1.4325785636901855, 'radial_force': 13.742211445431693, 'axial_force': -1.4325785636901855, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.7131099104881287, -0.7815901041030884, -1.624629020690918], 'magnitude': 1.938769817352295, 'distance': 13.085969924926758, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.34128113473276755, 'motion_component': -0.6616655531706854}, {'ion': 1320, 'force': [-2.2887518405914307, -2.6869468688964844, -2.5399811267852783], 'magnitude': 4.348513603210449, 'distance': 8.737730026245117, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.44327089905166983, 'motion_component': -1.9275696379600227}, {'ion': 1460, 'force': [-8.9459810256958, -3.320971727371216, 2.7320315837860107], 'magnitude': 9.925896644592285, 'distance': 5.783412456512451, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.07417239319387016, 'motion_component': 0.7362275165773262}]}, 5000: {'frame': 5000, 'ionic_force': [-9.01192718744278, -4.783424496650696, -3.6936601996421814], 'ionic_force_magnitude': 10.850765282566433, 'motion_vector': [-0.7812538146972656, 0.4613761901855469, -0.36583709716796875], 'cosine_ionic_motion': 0.5826446516183137, 'ionic_motion_component': 6.322140357853013, 'ionic_force_x': -9.01192718744278, 'ionic_force_y': -4.783424496650696, 'ionic_force_z': -3.6936601996421814, 'radial_force': 10.202743824429206, 'axial_force': -3.6936601996421814, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.9397225975990295, -0.6545020341873169, -1.707296371459961], 'magnitude': 2.055799722671509, 'distance': 12.70804214477539, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.525454039767896, 'motion_component': 1.080228253059616}, {'ion': 1320, 'force': [-3.7437233924865723, -2.7520456314086914, -2.9792110919952393], 'magnitude': 5.519503593444824, 'distance': 7.755664825439453, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5083565310182332, 'motion_component': 2.805875644879151}, {'ion': 1460, 'force': [-4.328481197357178, -1.3768768310546875, 0.9928472638130188], 'magnitude': 4.649439334869385, 'distance': 8.450234413146973, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.523942040511297, 'motion_component': 2.436036667233086}]}, 5001: {'frame': 5001, 'ionic_force': [-6.330652832984924, -3.146571785211563, -2.4073009490966797], 'ionic_force_magnitude': 7.468144157070839, 'motion_vector': [-0.016719818115234375, -0.3343772888183594, 0.31487274169921875], 'cosine_ionic_motion': 0.11653666175395425, 'ionic_motion_component': 0.870312589562334, 'ionic_force_x': -6.330652832984924, 'ionic_force_y': -3.146571785211563, 'ionic_force_z': -2.4073009490966797, 'radial_force': 7.06951761376047, 'axial_force': -2.4073009490966797, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.9957014322280884, -0.4937232434749603, -1.515923261642456], 'magnitude': 1.8796827793121338, 'distance': 13.290054321289062, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3421508167823267, 'motion_component': -0.6431349952876526}, {'ion': 1320, 'force': [-2.770164966583252, -1.6772152185440063, -2.3731327056884766], 'magnitude': 4.014800548553467, 'distance': 9.09362506866455, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.07592411220123893, 'motion_component': -0.3048201694466055}, {'ion': 1460, 'force': [-2.564786434173584, -0.9756333231925964, 1.481755018234253], 'magnitude': 3.1185874938964844, 'distance': 10.317870140075684, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.5830420678716011, 'motion_component': 1.8182676836329943}]}, 5002: {'frame': 5002, 'ionic_force': [-7.864047288894653, -3.612726092338562, -1.8392441272735596], 'ionic_force_magnitude': 8.847476958994891, 'motion_vector': [1.8620643615722656, -2.09149169921875, 0.0738525390625], 'cosine_ionic_motion': -0.2914451320352368, 'ionic_motion_component': -2.5785540904929816, 'ionic_force_x': -7.864047288894653, 'ionic_force_y': -3.612726092338562, 'ionic_force_z': -1.8392441272735596, 'radial_force': 8.654191445781356, 'axial_force': -1.8392441272735596, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.0093481540679932, -0.5549268126487732, -1.643075942993164], 'magnitude': 2.0065956115722656, 'distance': 12.862906455993652, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.14947363285212528, 'motion_component': -0.299933138318341}, {'ion': 1320, 'force': [-3.4694180488586426, -2.0770719051361084, -2.471514940261841], 'magnitude': 4.739142894744873, 'distance': 8.369877815246582, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.17314703360432673, 'motion_component': -0.8205685344170597}, {'ion': 1460, 'force': [-3.3852810859680176, -0.9807273745536804, 2.2753467559814453], 'magnitude': 4.195135116577148, 'distance': 8.896026611328125, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 1105, 'cosine_with_motion': -0.34755786630106694, 'motion_component': -1.4580521448367174}]}, 5003: {'frame': 5003, 'ionic_force': [-5.132673859596252, -6.734123051166534, -1.4360578060150146], 'ionic_force_magnitude': 8.58807407044512, 'motion_vector': [-0.707275390625, -0.40502166748046875, -0.429779052734375], 'cosine_ionic_motion': 0.8814315808209459, 'ionic_motion_component': 7.569799704119818, 'ionic_force_x': -5.132673859596252, 'ionic_force_y': -6.734123051166534, 'ionic_force_z': -1.4360578060150146, 'radial_force': 8.467157387059435, 'axial_force': -1.4360578060150146, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.6637636423110962, -0.8726678490638733, -1.511733055114746], 'magnitude': 1.8674763441085815, 'distance': 13.333417892456055, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8558256065889733, 'motion_component': 1.5982341395508683}, {'ion': 1320, 'force': [-2.242825746536255, -3.0832972526550293, -2.36020565032959], 'magnitude': 4.484145164489746, 'distance': 8.604570388793945, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9316849689159826, 'motion_component': 4.17781086980186}, {'ion': 1460, 'force': [-2.2260844707489014, -2.778157949447632, 2.4358808994293213], 'magnitude': 4.313598155975342, 'distance': 8.773021697998047, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': 0.41583722061378225, 'motion_component': 1.793754685761428}]}, 5004: {'frame': 5004, 'ionic_force': [-4.717077851295471, -4.595800518989563, -2.3284347653388977], 'ionic_force_magnitude': 6.985256925981022, 'motion_vector': [-0.6747245788574219, 2.4837417602539062, -0.2197113037109375], 'cosine_ionic_motion': -0.42787515374866464, 'ionic_motion_component': -2.9888178811780546, 'ionic_force_x': -4.717077851295471, 'ionic_force_y': -4.595800518989563, 'ionic_force_z': -2.3284347653388977, 'radial_force': 6.585757804955102, 'axial_force': -2.3284347653388977, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.6875178813934326, -0.8340977430343628, -1.441748857498169], 'magnitude': 1.8019543886184692, 'distance': 13.573665618896484, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.27736274933035654, 'motion_component': -0.4997950258276198}, {'ion': 1320, 'force': [-2.1348366737365723, -2.760021209716797, -1.877365231513977], 'magnitude': 3.9622902870178223, 'distance': 9.15368366241455, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.48873895636195097, 'motion_component': -1.936525656408099}, {'ion': 1460, 'force': [-1.8947232961654663, -1.0016815662384033, 0.9906793236732483], 'magnitude': 2.3610990047454834, 'distance': 11.858014106750488, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.23399998864807015, 'motion_component': -0.552497107667592}]}, 5005: {'frame': 5005, 'ionic_force': [-5.8636956214904785, -3.0404764115810394, -2.9966933727264404], 'ionic_force_magnitude': 7.253109286437775, 'motion_vector': [1.9760818481445312, -2.551136016845703, 1.67626953125], 'cosine_ionic_motion': -0.33568837728081463, 'ionic_motion_component': -2.434784486604704, 'ionic_force_x': -5.8636956214904785, 'ionic_force_y': -3.0404764115810394, 'ionic_force_z': -2.9966933727264404, 'radial_force': 6.605105839490183, 'axial_force': -2.9966933727264404, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.8727691173553467, -0.5728297829627991, -1.483247995376587], 'magnitude': 1.8138039112091064, 'distance': 13.529254913330078, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.4168848729684455, 'motion_component': -0.7561473993155872}, {'ion': 1320, 'force': [-3.1719272136688232, -2.036134958267212, -2.4662981033325195], 'magnitude': 4.504396915435791, 'distance': 8.585206031799316, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.31793913100847976, 'motion_component': -1.4321241320576232}, {'ion': 1460, 'force': [-1.8189992904663086, -0.43151167035102844, 0.952852725982666], 'magnitude': 2.098306179046631, 'distance': 12.578666687011719, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.11748188627750467, 'motion_component': -0.24651297452992438}]}, 5006: {'frame': 5006, 'ionic_force': [-4.633662641048431, -6.107035517692566, -2.5804152488708496], 'ionic_force_magnitude': 8.088587957240227, 'motion_vector': [-2.692249298095703, 2.7754745483398438, -1.560882568359375], 'cosine_ionic_motion': -0.013259507049575554, 'ionic_motion_component': -0.10725068904013872, 'ionic_force_x': -4.633662641048431, 'ionic_force_y': -6.107035517692566, 'ionic_force_z': -2.5804152488708496, 'radial_force': 7.665944970152501, 'axial_force': -2.5804152488708496, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.7836499810218811, -1.1199933290481567, -1.7357754707336426], 'magnitude': 2.2093911170959473, 'distance': 12.258370399475098, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.18567602863252866, 'motion_component': 0.41023095682033883}, {'ion': 1320, 'force': [-2.376492977142334, -4.063398838043213, -2.111187219619751], 'magnitude': 5.159073352813721, 'distance': 8.02200984954834, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.07365114574792865, 'motion_component': -0.3799716820196793}, {'ion': 1460, 'force': [-1.4735196828842163, -0.9236433506011963, 1.266547441482544], 'magnitude': 2.151399612426758, 'distance': 12.422486305236816, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.06391642443920177, 'motion_component': -0.1375097622119199}]}, 5007: {'frame': 5007, 'ionic_force': [-5.718433976173401, -2.855208694934845, -3.147172212600708], 'ionic_force_magnitude': 7.124422556758681, 'motion_vector': [0.5759010314941406, -0.5521697998046875, 0.14435577392578125], 'cosine_ionic_motion': -0.37583636937022347, 'ionic_motion_component': -2.6776171075915074, 'ionic_force_x': -5.718433976173401, 'ionic_force_y': -2.855208694934845, 'ionic_force_z': -3.147172212600708, 'radial_force': 6.391611990060556, 'axial_force': -3.147172212600708, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.9638186693191528, -0.5711681842803955, -1.511455774307251], 'magnitude': 1.8814032077789307, 'distance': 13.283976554870605, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3001565084066107, 'motion_component': -0.5647154217011554}, {'ion': 1320, 'force': [-3.205503225326538, -1.8640981912612915, -2.3779666423797607], 'magnitude': 4.405092239379883, 'distance': 8.681435585021973, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.32478865433870185, 'motion_component': -1.4307240068059563}, {'ion': 1460, 'force': [-1.54911208152771, -0.41994231939315796, 0.7422502040863037], 'magnitude': 1.7683424949645996, 'distance': 13.702059745788574, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.38577229909063343, 'motion_component': -0.682177547541098}]}, 5008: {'frame': 5008, 'ionic_force': [-5.75127911567688, -3.5837172269821167, -3.116843521595001], 'ionic_force_magnitude': 7.45888424414122, 'motion_vector': [0.1088409423828125, -0.9409523010253906, -0.1216583251953125], 'cosine_ionic_motion': 0.4387472499987256, 'ionic_motion_component': 3.2725649501757834, 'ionic_force_x': -5.75127911567688, 'ionic_force_y': -3.5837172269821167, 'ionic_force_z': -3.116843521595001, 'radial_force': 6.776447493295394, 'axial_force': -3.116843521595001, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.929062008857727, -0.6301071643829346, -1.557762622833252], 'magnitude': 1.9201081991195679, 'distance': 13.149407386779785, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.37153807724211496, 'motion_component': 0.7133933226855955}, {'ion': 1320, 'force': [-3.084425449371338, -2.398221731185913, -2.444641351699829], 'magnitude': 4.608841419219971, 'distance': 8.487370491027832, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5039926709766444, 'motion_component': 2.3228222934584686}, {'ion': 1460, 'force': [-1.737791657447815, -0.555388331413269, 0.8855604529380798], 'magnitude': 2.0279529094696045, 'distance': 12.794994354248047, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.11654576116051595, 'motion_component': 0.23634932566563815}]}, 5009: {'frame': 5009, 'ionic_force': [-4.791661620140076, -3.3943287134170532, -3.0958730578422546], 'ionic_force_magnitude': 6.638216514013718, 'motion_vector': [-0.2537117004394531, 1.1904716491699219, 0.37801361083984375], 'cosine_ionic_motion': -0.4722309263117984, 'ionic_motion_component': -3.1347711334709754, 'ionic_force_x': -4.791661620140076, 'ionic_force_y': -3.3943287134170532, 'ionic_force_z': -3.0958730578422546, 'radial_force': 5.87209404698621, 'axial_force': -3.0958730578422546, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.8100695610046387, -0.6891690492630005, -1.492370843887329], 'magnitude': 1.8325767517089844, 'distance': 13.459779739379883, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5047908100773542, 'motion_component': -0.9250678833166076}, {'ion': 1320, 'force': [-2.5722618103027344, -2.1343741416931152, -2.2908530235290527], 'magnitude': 4.052171230316162, 'distance': 9.051595687866211, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5332870526809247, 'motion_component': -2.1609704321776206}, {'ion': 1460, 'force': [-1.4093302488327026, -0.5707855224609375, 0.6873508095741272], 'magnitude': 1.6686698198318481, 'distance': 14.10534954071045, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.02920451360238688, 'motion_component': -0.048732690720088456}]}, 5010: {'frame': 5010, 'ionic_force': [-6.056791543960571, -3.679370939731598, -3.146594524383545], 'ionic_force_magnitude': 7.753937800886345, 'motion_vector': [0.18355178833007812, 0.16788864135742188, -0.24420166015625], 'cosine_ionic_motion': -0.3555627191622645, 'ionic_motion_component': -2.7570112086982186, 'ionic_force_x': -6.056791543960571, 'ionic_force_y': -3.679370939731598, 'ionic_force_z': -3.146594524383545, 'radial_force': 7.086783072673642, 'axial_force': -3.146594524383545, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.0071114301681519, -0.6563244462013245, -1.6691867113113403], 'magnitude': 2.056992769241333, 'distance': 12.70435619354248, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.15699508780823138, 'motion_component': 0.3229377694326381}, {'ion': 1320, 'force': [-3.5231919288635254, -2.5213658809661865, -2.321716070175171], 'magnitude': 4.915336608886719, 'distance': 8.218497276306152, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2935827208285289, 'motion_component': -1.4430578597423107}, {'ion': 1460, 'force': [-1.526488184928894, -0.5016806125640869, 0.8443082571029663], 'magnitude': 1.81513249874115, 'distance': 13.52430248260498, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 455, 'cosine_with_motion': -0.9018025914210851, 'motion_component': -1.6368912062349423}]}, 5011: {'frame': 5011, 'ionic_force': [-5.516871929168701, -3.2253422141075134, -3.525465488433838], 'ionic_force_magnitude': 7.2984666328682755, 'motion_vector': [0.9372367858886719, -0.7911605834960938, -0.0274505615234375], 'cosine_ionic_motion': -0.2816719609338294, 'ionic_motion_component': -2.0557734082901304, 'ionic_force_x': -5.516871929168701, 'ionic_force_y': -3.2253422141075134, 'ionic_force_z': -3.525465488433838, 'radial_force': 6.390517058967415, 'axial_force': -3.525465488433838, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-0.9378553628921509, -0.546708881855011, -1.6660550832748413], 'magnitude': 1.9885177612304688, 'distance': 12.921243667602539, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.16426040768421035, 'motion_component': -0.3266347355442112}, {'ion': 1320, 'force': [-3.1024675369262695, -2.091669797897339, -2.5550997257232666], 'magnitude': 4.530885696411133, 'distance': 8.560073852539062, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.21278014597992131, 'motion_component': -0.9640824441874996}, {'ion': 1460, 'force': [-1.4765490293502808, -0.5869635343551636, 0.69568932056427], 'magnitude': 1.7345623970031738, 'distance': 13.834837913513184, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 780, 'cosine_with_motion': -0.44106586930846237, 'motion_component': -0.7650562903700497}]}, 5012: {'frame': 5012, 'ionic_force': [-5.650092005729675, -4.366848289966583, -3.620231330394745], 'ionic_force_magnitude': 8.0</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{5173: {'frame': 5173, 'ionic_force': [0.15724579244852066, 4.5542712807655334, -5.197363078594208], 'ionic_force_magnitude': 6.912213546237034, 'motion_vector': [-0.32863616943359375, 0.4364585876464844, -0.3377685546875], 'cosine_ionic_motion': 0.8314539168547679, 'ionic_motion_component': 5.747187027155367, 'ionic_force_x': 0.15724579244852066, 'ionic_force_y': 4.5542712807655334, 'ionic_force_z': -5.197363078594208, 'radial_force': 4.5569850930246085, 'axial_force': -5.197363078594208, 'contributions': [{'ion': 1308, 'force': [0.7354629039764404, 2.4643869400024414, -0.565873920917511], 'magnitude': 2.633310079574585, 'distance': 11.22840404510498, 'cosine_with_motion': 0.6060114431838383, 'motion_component': 1.5958160407950677}, {'ion': 1309, 'force': [-0.48083266615867615, 1.5299593210220337, -3.0795645713806152], 'magnitude': 3.4721310138702393, 'distance': 9.778471946716309, 'cosine_with_motion': 0.8366618689570267, 'motion_component': 2.904999593045128}, {'ion': 1403, 'force': [-0.09738444536924362, 0.5599250197410583, -1.5519245862960815], 'magnitude': 1.652715802192688, 'distance': 14.173266410827637, 'cosine_with_motion': 0.7541353633832589, 'motion_component': 1.246371467798952}]}, 5174: {'frame': 5174, 'ionic_force': [-0.5605248957872391, 5.194657146930695, -6.168241083621979], 'ionic_force_magnitude': 8.083677943772715, 'motion_vector': [-2.1065216064453125, -0.9170722961425781, 2.1868057250976562], 'cosine_ionic_motion': -0.6658256553908883, 'ionic_motion_component': -5.382320164881336, 'ionic_force_x': -0.5605248957872391, 'ionic_force_y': 5.194657146930695, 'ionic_force_z': -6.168241083621979, 'radial_force': 5.224811100217446, 'axial_force': -6.168241083621979, 'contributions': [{'ion': 1308, 'force': [0.4955497980117798, 2.235003709793091, -0.6512793898582458], 'magnitude': 2.3801209926605225, 'distance': 11.81053352355957, 'cosine_with_motion': -0.5984301635066598, 'motion_component': -1.4243362059982232}, {'ion': 1309, 'force': [-0.8381993174552917, 2.3942766189575195, -3.879767417907715], 'magnitude': 4.635486602783203, 'distance': 8.462942123413086, 'cosine_with_motion': -0.6062927398856023, 'motion_component': -2.8104617289922547}, {'ion': 1403, 'force': [-0.2178753763437271, 0.5653768181800842, -1.637194275856018], 'magnitude': 1.7457164525985718, 'distance': 13.790569305419922, 'cosine_with_motion': -0.6573360244306076, 'motion_component': -1.147522273230206}]}, 5175: {'frame': 5175, 'ionic_force': [-3.0609599202871323, 6.934767544269562, -6.165554910898209], 'ionic_force_magnitude': 9.771107607940857, 'motion_vector': [0.8205947875976562, 1.4489250183105469, -0.349456787109375], 'cosine_ionic_motion': 0.5829055047166817, 'ionic_motion_component': 5.6956324118477735, 'ionic_force_x': -3.0609599202871323, 'ionic_force_y': 6.934767544269562, 'ionic_force_z': -6.165554910898209, 'radial_force': 7.580268895405934, 'axial_force': -6.165554910898209, 'contributions': [{'ion': 1308, 'force': [0.23377586901187897, 3.548218250274658, -0.4093410074710846], 'magnitude': 3.5793943405151367, 'distance': 9.630842208862305, 'cosine_with_motion': 0.8991608912132001, 'motion_component': 3.218451420795778}, {'ion': 1309, 'force': [-2.680544376373291, 2.8133533000946045, -3.845205307006836], 'magnitude': 5.466797828674316, 'distance': 7.792961597442627, 'cosine_with_motion': 0.34623075238245715, 'motion_component': 1.892773534790706}, {'ion': 1403, 'force': [-0.6141914129257202, 0.5731959939002991, -1.911008596420288], 'magnitude': 2.087519645690918, 'distance': 12.611123085021973, 'cosine_with_motion': 0.2799529169991263, 'motion_component': 0.5844072358015922}]}, 5176: {'frame': 5176, 'ionic_force': [-0.9744367897510529, 5.9303571581840515, -4.997504740953445], 'ionic_force_magnitude': 7.816246971321807, 'motion_vector': [-0.2884254455566406, 1.5469932556152344, -1.362060546875], 'cosine_ionic_motion': 0.9996707091622106, 'ionic_motion_component': 7.813673152808251, 'ionic_force_x': -0.9744367897510529, 'ionic_force_y': 5.9303571581840515, 'ionic_force_z': -4.997504740953445, 'radial_force': 6.0098804547881945, 'axial_force': -4.997504740953445, 'contributions': [{'ion': 1308, 'force': [0.5721141695976257, 2.9097232818603516, -0.24224546551704407], 'magnitude': 2.9753129482269287, 'distance': 10.563375473022461, 'cosine_with_motion': 0.7535516993446264, 'motion_component': 2.242052118813529}, {'ion': 1309, 'force': [-1.1644694805145264, 2.285262107849121, -3.060650587081909], 'magnitude': 3.99324369430542, 'distance': 9.11813735961914, 'cosine_with_motion': 0.9673941460377422, 'motion_component': 3.863040438722315}, {'ion': 1403, 'force': [-0.3820814788341522, 0.7353717684745789, -1.6946086883544922], 'magnitude': 1.8863871097564697, 'distance': 13.266416549682617, 'cosine_with_motion': 0.905742166955266, 'motion_component': 1.708580390070872}]}, 5177: {'frame': 5177, 'ionic_force': [-0.9265254437923431, 5.745557546615601, -3.907246023416519], 'ionic_force_magnitude': 7.0097398244849485, 'motion_vector': [1.0473556518554688, -0.16293716430664062, -0.0436553955078125], 'cosine_ionic_motion': -0.23344863634489804, 'ionic_motion_component': -1.6364142031585363, 'ionic_force_x': -0.9265254437923431, 'ionic_force_y': 5.745557546615601, 'ionic_force_z': -3.907246023416519, 'radial_force': 5.819783580122724, 'axial_force': -3.907246023416519, 'contributions': [{'ion': 1308, 'force': [0.689740777015686, 2.4730772972106934, -0.39926019310951233], 'magnitude': 2.5983190536499023, 'distance': 11.303756713867188, 'cosine_with_motion': 0.12221501182130788, 'motion_component': 0.3175536045510019}, {'ion': 1309, 'force': [-1.2035044431686401, 2.5528600215911865, -2.146219491958618], 'magnitude': 3.5456700325012207, 'distance': 9.676535606384277, 'cosine_with_motion': -0.42078615680419346, 'motion_component': -1.4919688284648274}, {'ion': 1403, 'force': [-0.41276177763938904, 0.7196202278137207, -1.3617663383483887], 'magnitude': 1.594563603401184, 'distance': 14.429394721984863, 'cosine_with_motion': -0.2897338193037402, 'motion_component': -0.46199900587296655}]}, 5178: {'frame': 5178, 'ionic_force': [-0.6896159946918488, 5.541051208972931, -4.2868136167526245], 'ionic_force_magnitude': 7.039573119541477, 'motion_vector': [-0.499969482421875, -1.2579994201660156, 0.6877059936523438], 'cosine_ionic_motion': -0.8957020063259677, 'ionic_motion_component': -6.305359766851653, 'ionic_force_x': -0.6896159946918488, 'ionic_force_y': 5.541051208972931, 'ionic_force_z': -4.2868136167526245, 'radial_force': 5.583799666946801, 'axial_force': -4.2868136167526245, 'contributions': [{'ion': 1308, 'force': [0.52821284532547, 2.203639030456543, -0.34880292415618896], 'magnitude': 2.2927489280700684, 'distance': 12.033468246459961, 'cosine_with_motion': -0.9410791659335338, 'motion_component': -2.1576581707824296}, {'ion': 1309, 'force': [-0.9532740116119385, 2.5756494998931885, -2.5336785316467285], 'magnitude': 3.7366065979003906, 'distance': 9.426063537597656, 'cosine_with_motion': -0.794204453800667, 'motion_component': -2.9676295725849258}, {'ion': 1403, 'force': [-0.26455482840538025, 0.7617626786231995, -1.404332160949707], 'magnitude': 1.6193888187408447, 'distance': 14.318366050720215, 'cosine_with_motion': -0.7287143440952004, 'motion_component': -1.1800719301357088}]}, 5179: {'frame': 5179, 'ionic_force': [-2.030127376317978, 6.3477553725242615, -5.428711324930191], 'ionic_force_magnitude': 8.595715332822024, 'motion_vector': [0.006259918212890625, 2.1265487670898438, -1.1589584350585938], 'cosine_ionic_motion': 0.9500465456928359, 'ionic_motion_component': 8.16632965970651, 'ionic_force_x': -2.030127376317978, 'ionic_force_y': 6.3477553725242615, 'ionic_force_z': -5.428711324930191, 'radial_force': 6.66448913522157, 'axial_force': -5.428711324930191, 'contributions': [{'ion': 1308, 'force': [0.29383471608161926, 2.3622288703918457, -0.319489985704422], 'magnitude': 2.401777982711792, 'distance': 11.75716495513916, 'cosine_with_motion': 0.9275760945020237, 'motion_component': 2.2278319278088166}, {'ion': 1309, 'force': [-1.8343040943145752, 3.2689404487609863, -3.492114543914795], 'magnitude': 5.123036861419678, 'distance': 8.050174713134766, 'cosine_with_motion': 0.885550252509541, 'motion_component': 4.53670662706779}, {'ion': 1403, 'force': [-0.489657998085022, 0.7165860533714294, -1.6171067953109741], 'magnitude': 1.8352915048599243, 'distance': 13.449821472167969, 'cosine_with_motion': 0.7637974619760005, 'motion_component': 1.4017909947725329}]}, 5180: {'frame': 5180, 'ionic_force': [-0.47080206871032715, 4.05627167224884, -2.3710789382457733], 'ionic_force_magnitude': 4.721970965432023, 'motion_vector': [0.3277015686035156, -0.06797409057617188, 1.3685455322265625], 'cosine_ionic_motion': -0.552400466844324, 'ionic_motion_component': -2.6084189657299928, 'ionic_force_x': -0.47080206871032715, 'ionic_force_y': 4.05627167224884, 'ionic_force_z': -2.3710789382457733, 'radial_force': 4.083502720335855, 'axial_force': -2.3710789382457733, 'contributions': [{'ion': 1308, 'force': [0.32464051246643066, 1.7187424898147583, -0.2759523093700409], 'magnitude': 1.770767331123352, 'distance': 13.69267463684082, 'cosine_with_motion': -0.15556355057782062, 'motion_component': -0.27546685084777156}, {'ion': 1309, 'force': [-0.7954425811767578, 2.337529182434082, -2.0951266288757324], 'magnitude': 3.238259792327881, 'distance': 10.125423431396484, 'cosine_with_motion': -0.7204338815501123, 'motion_component': -2.332952148085589}]}, 5181: {'frame': 5181, 'ionic_force': [-0.6866850852966309, 5.2680962681770325, -3.737524628639221], 'ionic_force_magnitude': 6.4956497016722174, 'motion_vector': [-0.3796195983886719, -1.8383750915527344, -0.54205322265625], 'cosine_ionic_motion': -0.5829162005149764, 'ionic_motion_component': -3.7864194439750087, 'ionic_force_x': -0.6866850852966309, 'ionic_force_y': 5.2680962681770325, 'ionic_force_z': -3.737524628639221, 'radial_force': 5.312661733740406, 'axial_force': -3.737524628639221, 'contributions': [{'ion': 1308, 'force': [0.3693566620349884, 1.7314714193344116, -0.16969358921051025], 'magnitude': 1.7785425186157227, 'distance': 13.662712097167969, 'cosine_with_motion': -0.9298734282283851, 'motion_component': -1.6538194403953677}, {'ion': 1309, 'force': [-0.789997935295105, 2.699798583984375, -2.170147180557251], 'magnitude': 3.5528225898742676, 'distance': 9.666790008544922, 'cosine_with_motion': -0.5023273269637426, 'motion_component': -1.7846798437849252}, {'ion': 1403, 'force': [-0.2660438120365143, 0.8368262648582458, -1.39768385887146], 'magnitude': 1.6506295204162598, 'distance': 14.182221412658691, 'cosine_with_motion': -0.21078027551344006, 'motion_component': -0.3479201363469171}]}, 5182: {'frame': 5182, 'ionic_force': [-1.5095845460891724, 5.511749029159546, -4.918577492237091], 'ionic_force_magnitude': 7.53993550432454, 'motion_vector': [3.399822235107422, 1.0570564270019531, -0.6069412231445312], 'cosine_ionic_motion': 0.1351049295348629, 'ionic_motion_component': 1.018682455009178, 'ionic_force_x': -1.5095845460891724, 'ionic_force_y': 5.511749029159546, 'ionic_force_z': -4.918577492237091, 'radial_force': 5.714737339741211, 'axial_force': -4.918577492237091, 'contributions': [{'ion': 1308, 'force': [0.24988240003585815, 2.1664843559265137, -0.3289939761161804], 'magnitude': 2.2055232524871826, 'distance': 12.26911449432373, 'cosine_with_motion': 0.4192119235928302, 'motion_component': 0.9245816354512906}, {'ion': 1309, 'force': [-1.407989263534546, 2.6396069526672363, -3.090088129043579], 'magnitude': 4.301000118255615, 'distance': 8.785860061645508, 'cosine_with_motion': -0.00780209540420473, 'motion_component': -0.033556814397886825}, {'ion': 1403, 'force': [-0.3514776825904846, 0.7056577205657959, -1.4994953870773315], 'magnitude': 1.694100260734558, 'distance': 13.999079704284668, 'cosine_with_motion': 0.07535424101003572, 'motion_component': 0.12765764161992088}]}, 5183: {'frame': 5183, 'ionic_force': [0.906077116727829, 3.351901054382324, -2.439151182770729], 'ionic_force_magnitude': 4.243309429235511, 'motion_vector': [-0.3704338073730469, 0.2990570068359375, 0.07714080810546875], 'cosine_ionic_motion': 0.23386514195069716, 'ionic_motion_component': 0.9923621620088946, 'ionic_force_x': 0.906077116727829, 'ionic_force_y': 3.351901054382324, 'ionic_force_z': -2.439151182770729, 'radial_force': 3.472206275529602, 'axial_force': -2.439151182770729, 'contributions': [{'ion': 1308, 'force': [0.6261655688285828, 1.4340345859527588, -0.20961131155490875], 'magnitude': 1.5787575244903564, 'distance': 14.501446723937988, 'cosine_with_motion': 0.23736511913737168, 'motion_component': 0.37474197496300743}, {'ion': 1309, 'force': [0.2799115478992462, 1.9178664684295654, -2.2295398712158203], 'magnitude': 2.954219102859497, 'distance': 10.601020812988281, 'cosine_with_motion': 0.20906377391369516, 'motion_component': 0.6176201873585594}]}, 5184: {'frame': 5184, 'ionic_force': [0.7254925360903144, 4.958870887756348, -4.047217309474945], 'ionic_force_magnitude': 6.441793838013896, 'motion_vector': [-0.18041229248046875, 0.4036216735839844, 0.16362762451171875], 'cosine_ionic_motion': 0.3979180144561937, 'ionic_motion_component': 2.563305813558633, 'ionic_force_x': 0.7254925360903144, 'ionic_force_y': 4.958870887756348, 'ionic_force_z': -4.047217309474945, 'radial_force': 5.011660393657992, 'axial_force': -4.047217309474945, 'contributions': [{'ion': 1308, 'force': [0.5973078608512878, 1.5048673152923584, -0.26393312215805054], 'magnitude': 1.6404459476470947, 'distance': 14.22617244720459, 'cosine_with_motion': 0.5902359183247087, 'motion_component': 0.9682501389175825}, {'ion': 1309, 'force': [0.1381777822971344, 2.6733298301696777, -2.3793797492980957], 'magnitude': 3.581512689590454, 'distance': 9.6279935836792, 'cosine_with_motion': 0.3937215782895846, 'motion_component': 1.410118846732325}, {'ion': 1403, 'force': [-0.009993107058107853, 0.7806737422943115, -1.4039044380187988], 'magnitude': 1.6063930988311768, 'distance': 14.376167297363281, 'cosine_with_motion': 0.1151254858041788, 'motion_component': 0.18493679439559696}]}, 5185: {'frame': 5185, 'ionic_force': [0.7339238412678242, 5.119778215885162, -3.856375366449356], 'ionic_force_magnitude': 6.45154277298004, 'motion_vector': [-0.11819076538085938, -0.16250991821289062, 0.146270751953125], 'cosine_ionic_motion': -0.924755423083406, 'ionic_motion_component': -5.966099166567847, 'ionic_force_x': 0.7339238412678242, 'ionic_force_y': 5.119778215885162, 'ionic_force_z': -3.856375366449356, 'radial_force': 5.172114962433992, 'axial_force': -3.856375366449356, 'contributions': [{'ion': 1308, 'force': [0.8244546055793762, 1.679525375366211, -0.2533508837223053], 'magnitude': 1.8880459070205688, 'distance': 13.260587692260742, 'cosine_with_motion': -0.8682598275267359, 'motion_component': -1.6393144610569834}, {'ion': 1309, 'force': [-0.028522875159978867, 2.627678871154785, -2.242663860321045], 'magnitude': 3.454714298248291, 'distance': 9.803089141845703, 'cosine_with_motion': -0.8754357746797629, 'motion_component': -3.024380502198848}, {'ion': 1403, 'force': [-0.06200788915157318, 0.8125739693641663, -1.3603606224060059], 'magnitude': 1.5857813358306885, 'distance': 14.469295501708984, 'cosine_with_motion': -0.8213012027582747, 'motion_component': -1.302404121518519}]}, 5186: {'frame': 5186, 'ionic_force': [0.6085753031075001, 5.361973226070404, -3.9645311534404755], 'ionic_force_magnitude': 6.696165174429937, 'motion_vector': [0.29323577880859375, 0.5634040832519531, 0.6587371826171875], 'cosine_ionic_motion': 0.09593404861098064, 'ionic_motion_component': 0.6423902353509172, 'ionic_force_x': 0.6085753031075001, 'ionic_force_y': 5.361973226070404, 'ionic_force_z': -3.9645311534404755, 'radial_force': 5.396398871159196, 'axial_force': -3.9645311534404755, 'contributions': [{'ion': 1308, 'force': [0.7067315578460693, 1.7726627588272095, -0.21329709887504578], 'magnitude': 1.920233964920044, 'distance': 13.148977279663086, 'cosine_with_motion': 0.6063586115181139, 'motion_component': 1.1643503887190967}, {'ion': 1309, 'force': [-0.05736168473958969, 2.774033784866333, -2.3771002292633057], 'magnitude': 3.6536500453948975, 'distance': 9.532472610473633, 'cosine_with_motion': -0.005923090307569401, 'motion_component': -0.021640899696546034}, {'ion': 1403, 'force': [-0.04079456999897957, 0.8152766823768616, -1.374133825302124], 'magnitude': 1.598306655883789, 'distance': 14.41248893737793, 'cosine_with_motion': -0.31303085430443395, 'motion_component': -0.5003192851393142}]}, 5187: {'frame': 5187, 'ionic_force': [0.44809454679489136, 5.63523006439209, -3.661033511161804], 'ionic_force_magnitude': 6.7349664417386315, 'motion_vector': [-0.44336700439453125, -0.58660888671875, -0.7073516845703125], 'cosine_ionic_motion': -0.1331114322693107, 'ionic_motion_component': -0.8965010293455722, 'ionic_force_x': 0.44809454679489136, 'ionic_force_y': 5.63523006439209, 'ionic_force_z': -3.661033511161804, 'radial_force': 5.653017477550887, 'axial_force': -3.661033511161804, 'contributions': [{'ion': 1308, 'force': [0.5526303648948669, 1.42279052734375, -0.1382688283920288], 'magnitude': 1.5325963497161865, 'distance': 14.718214988708496, 'cosine_with_motion': -0.6278833176374604, 'motion_component': -0.962291660716259}, {'ion': 1309, 'force': [-0.0501912422478199, 3.1493821144104004, -2.052255630493164], 'magnitude': 3.7593722343444824, 'distance': 9.397479057312012, 'cosine_with_motion': -0.09738347942390585, 'motion_component': -0.36610075432767797}, {'ion': 1403, 'force': [-0.054344575852155685, 1.0630574226379395, -1.4705090522766113], 'magnitude': 1.8153350353240967, 'distance': 13.523548126220703, 'cosine_with_motion': 0.23791276105627682, 'motion_component': 0.43189137043733694}]}, 5188: {'frame': 5188, 'ionic_force': [0.6004464058205485, 5.34605211019516, -4.232802301645279], 'ionic_force_magnitude': 6.845248306380018, 'motion_vector': [0.09778976440429688, 0.3133354187011719, -0.27387237548828125], 'cosine_ionic_motion': 0.9886528166637947, 'ionic_motion_component': 6.767574018865675, 'ionic_force_x': 0.6004464058205485, 'ionic_force_y': 5.34605211019516, 'ionic_force_z': -4.232802301645279, 'radial_force': 5.37966625834586, 'axial_force': -4.232802301645279, 'contributions': [{'ion': 1308, 'force': [0.7558067440986633, 2.0558364391326904, -0.4618763029575348], 'magnitude': 2.238534450531006, 'distance': 12.178313255310059, 'cosine_with_motion': 0.8825643705961469, 'motion_component': 1.975650853246151}, {'ion': 1309, 'force': [-0.012659800238907337, 2.442432165145874, -2.3873846530914307], 'magnitude': 3.4154415130615234, 'distance': 9.859289169311523, 'cosine_with_motion': 0.9711197726701742, 'motion_component': 3.3168027721633653}, {'ion': 1403, 'force': [-0.14270053803920746, 0.8477835059165955, -1.3835413455963135], 'magnitude': 1.6288913488388062, 'distance': 14.276540756225586, 'cosine_with_motion': 0.9055977262933529, 'motion_component': 1.4751202866299886}]}, 5189: {'frame': 5189, 'ionic_force': [0.32750216871500015, 4.727729856967926, -3.834524780511856], 'ionic_force_magnitude': 6.096086249663672, 'motion_vector': [-0.000904083251953125, -0.1085205078125, 0.5684127807617188], 'cosine_ionic_motion': -0.7633747994882957, 'ionic_motion_component': -4.653598618500362, 'ionic_force_x': 0.32750216871500015, 'ionic_force_y': 4.727729856967926, 'ionic_force_z': -3.834524780511856, 'radial_force': 4.739059745453627, 'axial_force': -3.834524780511856, 'contributions': [{'ion': 1308, 'force': [0.5216655135154724, 1.448395848274231, -0.2568974792957306], 'magnitude': 1.5607632398605347, 'distance': 14.58480167388916, 'cosine_with_motion': -0.33622893755916217, 'motion_component': -0.5247737514062334}, {'ion': 1309, 'force': [-0.11025428026914597, 2.4549198150634766, -2.214020013809204], 'magnitude': 3.307668685913086, 'distance': 10.018623352050781, 'cosine_with_motion': -0.7966152203201085, 'motion_component': -2.6349391937450988}, {'ion': 1403, 'force': [-0.0839090645313263, 0.8244141936302185, -1.3636072874069214], 'magnitude': 1.5956579446792603, 'distance': 14.424446105957031, 'cosine_with_motion': -0.9362191895719004, 'motion_component': -1.4938856029452705}]}, 5190: {'frame': 5190, 'ionic_force': [0.34706735610961914, 4.918230354785919, -3.804109513759613], 'ionic_force_magnitude': 6.227414773811919, 'motion_vector': [0.3770256042480469, -0.35123443603515625, -0.49456024169921875], 'cosine_ionic_motion': 0.06402448857565023, 'ionic_motion_component': 0.39870704604175666, 'ionic_force_x': 0.34706735610961914, 'ionic_force_y': 4.918230354785919, 'ionic_force_z': -3.804109513759613, 'radial_force': 4.930460989848165, 'axial_force': -3.804109513759613, 'contributions': [{'ion': 1308, 'force': [0.5309812426567078, 1.4431406259536743, -0.21502536535263062], 'magnitude': 1.5526853799819946, 'distance': 14.62269115447998, 'cosine_with_motion': -0.1806608335869741, 'motion_component': -0.28050943300189246}, {'ion': 1309, 'force': [-0.07559871673583984, 2.564948797225952, -2.245485782623291], 'magnitude': 3.4098215103149414, 'distance': 9.867410659790039, 'cosine_with_motion': 0.07437417935511147, 'motion_component': 0.25360268929463814}, {'ion': 1403, 'force': [-0.10831516981124878, 0.9101409316062927, -1.3435983657836914], 'magnitude': 1.6264517307281494, 'distance': 14.287243843078613, 'cosine_with_motion': 0.26168234308413185, 'motion_component': 0.42561370202601617}]}, 5191: {'frame': 5191, 'ionic_force': [0.657955770380795, 5.201777338981628, -4.198868662118912], 'ionic_force_magnitude': 6.717283031244436, 'motion_vector': [-0.9679679870605469, 0.518524169921875, 1.3073348999023438], 'cosine_ionic_motion': -0.2989874499026258, 'ionic_motion_component': -2.0083833237859543, 'ionic_force_x': 0.657955770380795, 'ionic_force_y': 5.201777338981628, 'ionic_force_z': -4.198868662118912, 'radial_force': 5.243223558090975, 'axial_force': -4.198868662118912, 'contributions': [{'ion': 1308, 'force': [0.6094868183135986, 1.5151386260986328, -0.26498427987098694], 'magnitude': 1.6544896364212036, 'distance': 14.165666580200195, 'cosine_with_motion': -0.05336790472600894, 'motion_component': -0.08829664447299024}, {'ion': 1309, 'force': [0.05508818104863167, 2.8828670978546143, -2.548942804336548], 'magnitude': 3.8485147953033447, 'distance': 9.288005828857422, 'cosine_with_motion': -0.2877654872420616, 'motion_component': -1.1074697614626865}, {'ion': 1403, 'force': [-0.006619228981435299, 0.8037716150283813, -1.384941577911377], 'magnitude': 1.601298213005066, 'distance': 14.399020195007324, 'cosine_with_motion': -0.5074739143486897, 'motion_component': -0.8126170453461972}]}, 5192: {'frame': 5192, 'ionic_force': [0.1945376694202423, 5.99289608001709, -3.5691631473600864], 'ionic_force_magnitude': 6.977934787828059, 'motion_vector': [-2.582378387451172, -1.3664169311523438, 0.01790618896484375], 'cosine_ionic_motion': -0.4294408475329646, 'ionic_motion_component': -2.996610229314639, 'ionic_force_x': 0.1945376694202423, 'ionic_force_y': 5.99289608001709, 'ionic_force_z': -3.5691631473600864, 'radial_force': 5.996052729146706, 'axial_force': -3.5691631473600864, 'contributions': [{'ion': 1308, 'force': [0.6152461171150208, 1.7376521825790405, -0.03967398777604103], 'magnitude': 1.8437833786010742, 'distance': 13.41881275177002, 'cosine_with_motion': -0.7358333946801904, 'motion_component': -1.356717336705017}, {'ion': 1309, 'force': [-0.2750970125198364, 3.165602922439575, -1.957560658454895], 'magnitude': 3.732125997543335, 'distance': 9.431719779968262, 'cosine_with_motion': -0.3347561495557672, 'motion_component': -1.2493521061189088}, {'ion': 1403, 'force': [-0.14561143517494202, 1.0896409749984741, -1.5719285011291504], 'magnitude': 1.9181969165802002, 'distance': 13.155957221984863, 'cosine_with_motion': -0.20359788913885363, 'motion_component': -0.39054084032030834}]}, 5193: {'frame': 5193, 'ionic_force': [-1.93711456656456, 6.59854257106781, -4.372821029275656], 'ionic_force_magnitude': 8.149523952984381, 'motion_vector': [0.4185295104980469, 1.0166091918945312, -0.2987213134765625], 'cosine_ionic_motion': 0.7758910631739562, 'ionic_motion_component': 6.323142804242674, 'ionic_force_x': -1.93711456656456, 'ionic_force_y': 6.59854257106781, 'ionic_force_z': -4.372821029275656, 'radial_force': 6.877003483072463, 'axial_force': -4.372821029275656, 'contributions': [{'ion': 1308, 'force': [0.4174995720386505, 2.2765603065490723, -0.059432800859212875], 'magnitude': 2.3152894973754883, 'distance': 11.974748611450195, 'cosine_with_motion': 0.9503974281845952, 'motion_component': 2.2004450859416735}, {'ion': 1309, 'force': [-1.7871077060699463, 3.376755714416504, -2.6929991245269775], 'magnitude': 4.674235820770264, 'distance': 8.427790641784668, 'cosine_with_motion': 0.655258731336676, 'motion_component': 3.062833615510769}, {'ion': 1403, 'force': [-0.5675064325332642, 0.9452265501022339, -1.6203891038894653], 'magnitude': 1.9598922729492188, 'distance': 13.015262603759766, 'cosine_with_motion': 0.540776768071992, 'motion_component': 1.0598641965006337}]}, 5194: {'frame': 5194, 'ionic_force': [-0.9560555219650269, 5.772682011127472, -3.487354025244713], 'ionic_force_magnitude': 6.811720624046837, 'motion_vector': [-0.6451492309570312, -1.4054031372070312, -0.01318359375], 'cosine_ionic_motion': -0.7072447724738669, 'ionic_motion_component': -4.8175538029095515, 'ionic_force_x': -0.9560555219650269, 'ionic_force_y': 5.772682011127472, 'ionic_force_z': -3.487354025244713, 'radial_force': 5.8513160709941605, 'axial_force': -3.487354025244713, 'contributions': [{'ion': 1308, 'force': [0.6240898370742798, 2.3083484172821045, -0.197579488158226], 'magnitude': 2.3993747234344482, 'distance': 11.763051986694336, 'cosine_with_motion': -0.9821161896001479, 'motion_component': -2.3564645829506077}, {'ion': 1309, 'force': [-1.1822179555892944, 2.5775022506713867, -1.9253954887390137], 'magnitude': 3.4275801181793213, 'distance': 9.841815948486328, 'cosine_with_motion': -0.5347176855163869, 'motion_component': -1.8327876662373213}, {'ion': 1403, 'force': [-0.3979274034500122, 0.8868313431739807, -1.3643790483474731], 'magnitude': 1.675215244293213, 'distance': 14.077766418457031, 'cosine_with_motion': -0.3750572757112363, 'motion_component': -0.6283016794686191}]}, 5195: {'frame': 5195, 'ionic_force': [-2.697285771369934, 7.435713529586792, -4.3827709555625916], 'ionic_force_magnitude': 9.042890438097643, 'motion_vector': [0.4557342529296875, 0.3656768798828125, 0.8678741455078125], 'cosine_ionic_motion': -0.24456839884992476, 'ionic_motion_component': -2.2116052354208353, 'ionic_force_x': -2.697285771369934, 'ionic_force_y': 7.435713529586792, 'ionic_force_z': -4.3827709555625916, 'radial_force': 7.90981581495516, 'axial_force': -4.3827709555625916, 'contributions': [{'ion': 1308, 'force': [-0.6983073353767395, 3.93900203704834, -0.37639325857162476], 'magnitude': 4.018089294433594, 'distance': 9.089902877807617, 'cosine_with_motion': 0.18922900283928057, 'motion_component': 0.760339042032788}, {'ion': 1309, 'force': [-1.4922806024551392, 2.734032154083252, -2.6263973712921143], 'magnitude': 4.074284553527832, 'distance': 9.026997566223145, 'cosine_with_motion': -0.4597326047091931, 'motion_component': -1.8730815485615615}, {'ion': 1403, 'force': [-0.5066978335380554, 0.7626793384552002, -1.3799803256988525], 'magnitude': 1.6561305522918701, 'distance': 14.158647537231445, 'cosine_with_motion': -0.6635122356815232, 'motion_component': -1.0988628374351261}]}, 5196: {'frame': 5196, 'ionic_force': [-2.689316511154175, 6.572674095630646, -2.8800116777420044], 'ionic_force_magnitude': 7.66335013740537, 'motion_vector': [0.2856636047363281, 0.22528839111328125, 0.144744873046875], 'cosine_ionic_motion': 0.09852816387166814, 'ionic_motion_component': 0.7550558181442468, 'ionic_force_x': -2.689316511154175, 'ionic_force_y': 6.572674095630646, 'ionic_force_z': -2.8800116777420044, 'radial_force': 7.101582081799843, 'axial_force': -2.8800116777420044, 'contributions': [{'ion': 1308, 'force': [-0.6410857439041138, 2.2917823791503906, 1.5949033498764038], 'magnitude': 2.864781618118286, 'distance': 10.765229225158691, 'cosine_with_motion': 0.5028366061858794, 'motion_component': 1.4405170996993453}, {'ion': 1309, 'force': [-1.6070647239685059, 3.372495651245117, -2.893615961074829], 'magnitude': 4.725399017333984, 'distance': 8.382040977478027, 'cosine_with_motion': -0.06384747410201075, 'motion_component': -0.30170480085153173}, {'ion': 1403, 'force': [-0.4411660432815552, 0.9083960652351379, -1.581299066543579], 'magnitude': 1.876250982284546, 'distance': 13.302203178405762, 'cosine_with_motion': -0.20453358387588322, 'motion_component': -0.3837563310297796}]}, 5197: {'frame': 5197, 'ionic_force': [-2.394786536693573, 9.815348863601685, -3.377447187900543], 'ionic_force_magnitude': 10.652850575202534, 'motion_vector': [-0.7711677551269531, -0.23419952392578125, -1.1207962036132812], 'cosine_ionic_motion': 0.22667240517304837, 'ionic_motion_component': 2.4147072618302503, 'ionic_force_x': -2.394786536693573, 'ionic_force_y': 9.815348863601685, 'ionic_force_z': -3.377447187900543, 'radial_force': 10.10327055316919, 'axial_force': -3.377447187900543, 'contributions': [{'ion': 1308, 'force': [-0.5111057162284851, 5.275302886962891, 0.6245482563972473], 'magnitude': 5.336676120758057, 'distance': 7.88739538192749, 'cosine_with_motion': -0.2092136235456392, 'motion_component': -1.1165053118480337}, {'ion': 1309, 'force': [-1.4601268768310547, 3.5319414138793945, -2.432771682739258], 'magnitude': 4.530447959899902, 'distance': 8.560486793518066, 'cosine_with_motion': 0.48374883718600237, 'motion_component': 2.191598932025954}, {'ion': 1403, 'force': [-0.4235539436340332, 1.0081045627593994, -1.5692237615585327], 'magnitude': 1.9126254320144653, 'distance': 13.175105094909668, 'cosine_with_motion': 0.7004055536376355, 'motion_component': 1.3396134605632426}]}, 5198: {'frame': 5198, 'ionic_force': [-2.4582442939281464, 7.281810879707336, -3.801115170121193], 'ionic_force_magnitude': 8.574159505921259, 'motion_vector': [1.0001983642578125, 2.0919723510742188, -0.8253173828125], 'cosine_ionic_motion': 0.7539895480987615, 'ionic_motion_component': 6.46482665119627, 'ionic_force_x': -2.4582442939281464, 'ionic_force_y': 7.281810879707336, 'ionic_force_z': -3.801115170121193, 'radial_force': 7.685553636300668, 'axial_force': -3.801115170121193, 'contributions': [{'ion': 1308, 'force': [-0.5375314950942993, 3.8752388954162598, -0.03662027418613434], 'magnitude': 3.912513017654419, 'distance': 9.211729049682617, 'cosine_with_motion': 0.7891637841625229, 'motion_component': 3.087613531795399}, {'ion': 1309, 'force': [-1.4404795169830322, 2.623394727706909, -2.3200292587280273], 'magnitude': 3.7867817878723145, 'distance': 9.363407135009766, 'cosine_with_motion': 0.6396840948812568, 'motion_component': 2.4223441302027737}, {'ion': 1403, 'force': [-0.4802332818508148, 0.7831772565841675, -1.4444656372070312], 'magnitude': 1.7118620872497559, 'distance': 13.926264762878418, 'cosine_with_motion': 0.5577956065243156, 'motion_component': 0.954869117280472}]}, 5199: {'frame': 5199, 'ionic_force': [-1.14464071393013, 4.792068958282471, -1.1551509499549866], 'ionic_force_magnitude': 5.060484263596008, 'motion_vector': [0.4618873596191406, -1.79718017578125, 1.5188522338867188], 'cosine_ionic_motion': -0.8978699993094448, 'ionic_motion_component': -4.543657002260404, 'ionic_force_x': -1.14464071393013, 'ionic_force_y': 4.792068958282471, 'ionic_force_z': -1.1551509499549866, 'radial_force': 4.926878044453802, 'axial_force': -1.1551509499549866, 'contributions': [{'ion': 1308, 'force': [-0.3644380271434784, 2.3148305416107178, 0.5557435154914856], 'magnitude': 2.4083409309387207, 'distance': 11.741133689880371, 'cosine_with_motion': -0.6033545233363018, 'motion_component': -1.4530834354263635}, {'ion': 1309, 'force': [-0.7802026867866516, 2.477238416671753, -1.7108944654464722], 'magnitude': 3.1100780963897705, 'distance': 10.331975936889648, 'cosine_with_motion': -0.9937286248646539, 'motion_component': -3.0905737117048435}]}, 5200: {'frame': 5200, 'ionic_force': [-1.6555381119251251, 7.148874580860138, -3.147367298603058], 'ionic_force_magnitude': 7.984556038078806, 'motion_vector': [-1.8232803344726562, -0.8938713073730469, -0.5885772705078125], 'cosine_ionic_motion': -0.08999526784902638, 'ionic_motion_component': -0.718572259302463, 'ionic_force_x': -1.6555381119251251, 'ionic_force_y': 7.148874580860138, 'ionic_force_z': -3.147367298603058, 'radial_force': 7.338066108512844, 'axial_force': -3.147367298603058, 'contributions': [{'ion': 1308, 'force': [-0.19619184732437134, 2.808659076690674, 0.9512656331062317]</t>
+          <t>{5173: {'frame': 5173, 'ionic_force': [0.15724579244852066, 4.5542712807655334, -5.197363078594208], 'ionic_force_magnitude': 6.912213546237034, 'motion_vector': [-0.32863616943359375, 0.4364585876464844, -0.3377685546875], 'cosine_ionic_motion': 0.8314539168547679, 'ionic_motion_component': 5.747187027155367, 'ionic_force_x': 0.15724579244852066, 'ionic_force_y': 4.5542712807655334, 'ionic_force_z': -5.197363078594208, 'radial_force': 4.5569850930246085, 'axial_force': -5.197363078594208, 'before_closest_residue': None, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [0.7354629039764404, 2.4643869400024414, -0.565873920917511], 'magnitude': 2.633310079574585, 'distance': 11.22840404510498, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.6060114431838383, 'motion_component': 1.5958160407950677}, {'ion': 1309, 'force': [-0.48083266615867615, 1.5299593210220337, -3.0795645713806152], 'magnitude': 3.4721310138702393, 'distance': 9.778471946716309, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8366618689570267, 'motion_component': 2.904999593045128}, {'ion': 1403, 'force': [-0.09738444536924362, 0.5599250197410583, -1.5519245862960815], 'magnitude': 1.652715802192688, 'distance': 14.173266410827637, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7541353633832589, 'motion_component': 1.246371467798952}]}, 5174: {'frame': 5174, 'ionic_force': [-0.5605248957872391, 5.194657146930695, -6.168241083621979], 'ionic_force_magnitude': 8.083677943772715, 'motion_vector': [-2.1065216064453125, -0.9170722961425781, 2.1868057250976562], 'cosine_ionic_motion': -0.6658256553908883, 'ionic_motion_component': -5.382320164881336, 'ionic_force_x': -0.5605248957872391, 'ionic_force_y': 5.194657146930695, 'ionic_force_z': -6.168241083621979, 'radial_force': 5.224811100217446, 'axial_force': -6.168241083621979, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.4955497980117798, 2.235003709793091, -0.6512793898582458], 'magnitude': 2.3801209926605225, 'distance': 11.81053352355957, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.5984301635066598, 'motion_component': -1.4243362059982232}, {'ion': 1309, 'force': [-0.8381993174552917, 2.3942766189575195, -3.879767417907715], 'magnitude': 4.635486602783203, 'distance': 8.462942123413086, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6062927398856023, 'motion_component': -2.8104617289922547}, {'ion': 1403, 'force': [-0.2178753763437271, 0.5653768181800842, -1.637194275856018], 'magnitude': 1.7457164525985718, 'distance': 13.790569305419922, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6573360244306076, 'motion_component': -1.147522273230206}]}, 5175: {'frame': 5175, 'ionic_force': [-3.0609599202871323, 6.934767544269562, -6.165554910898209], 'ionic_force_magnitude': 9.771107607940857, 'motion_vector': [0.8205947875976562, 1.4489250183105469, -0.349456787109375], 'cosine_ionic_motion': 0.5829055047166817, 'ionic_motion_component': 5.6956324118477735, 'ionic_force_x': -3.0609599202871323, 'ionic_force_y': 6.934767544269562, 'ionic_force_z': -6.165554910898209, 'radial_force': 7.580268895405934, 'axial_force': -6.165554910898209, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.23377586901187897, 3.548218250274658, -0.4093410074710846], 'magnitude': 3.5793943405151367, 'distance': 9.630842208862305, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.8991608912132001, 'motion_component': 3.218451420795778}, {'ion': 1309, 'force': [-2.680544376373291, 2.8133533000946045, -3.845205307006836], 'magnitude': 5.466797828674316, 'distance': 7.792961597442627, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.34623075238245715, 'motion_component': 1.892773534790706}, {'ion': 1403, 'force': [-0.6141914129257202, 0.5731959939002991, -1.911008596420288], 'magnitude': 2.087519645690918, 'distance': 12.611123085021973, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2799529169991263, 'motion_component': 0.5844072358015922}]}, 5176: {'frame': 5176, 'ionic_force': [-0.9744367897510529, 5.9303571581840515, -4.997504740953445], 'ionic_force_magnitude': 7.816246971321807, 'motion_vector': [-0.2884254455566406, 1.5469932556152344, -1.362060546875], 'cosine_ionic_motion': 0.9996707091622106, 'ionic_motion_component': 7.813673152808251, 'ionic_force_x': -0.9744367897510529, 'ionic_force_y': 5.9303571581840515, 'ionic_force_z': -4.997504740953445, 'radial_force': 6.0098804547881945, 'axial_force': -4.997504740953445, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.5721141695976257, 2.9097232818603516, -0.24224546551704407], 'magnitude': 2.9753129482269287, 'distance': 10.563375473022461, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.7535516993446264, 'motion_component': 2.242052118813529}, {'ion': 1309, 'force': [-1.1644694805145264, 2.285262107849121, -3.060650587081909], 'magnitude': 3.99324369430542, 'distance': 9.11813735961914, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9673941460377422, 'motion_component': 3.863040438722315}, {'ion': 1403, 'force': [-0.3820814788341522, 0.7353717684745789, -1.6946086883544922], 'magnitude': 1.8863871097564697, 'distance': 13.266416549682617, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.905742166955266, 'motion_component': 1.708580390070872}]}, 5177: {'frame': 5177, 'ionic_force': [-0.9265254437923431, 5.745557546615601, -3.907246023416519], 'ionic_force_magnitude': 7.0097398244849485, 'motion_vector': [1.0473556518554688, -0.16293716430664062, -0.0436553955078125], 'cosine_ionic_motion': -0.23344863634489804, 'ionic_motion_component': -1.6364142031585363, 'ionic_force_x': -0.9265254437923431, 'ionic_force_y': 5.745557546615601, 'ionic_force_z': -3.907246023416519, 'radial_force': 5.819783580122724, 'axial_force': -3.907246023416519, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.689740777015686, 2.4730772972106934, -0.39926019310951233], 'magnitude': 2.5983190536499023, 'distance': 11.303756713867188, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.12221501182130788, 'motion_component': 0.3175536045510019}, {'ion': 1309, 'force': [-1.2035044431686401, 2.5528600215911865, -2.146219491958618], 'magnitude': 3.5456700325012207, 'distance': 9.676535606384277, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.42078615680419346, 'motion_component': -1.4919688284648274}, {'ion': 1403, 'force': [-0.41276177763938904, 0.7196202278137207, -1.3617663383483887], 'magnitude': 1.594563603401184, 'distance': 14.429394721984863, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2897338193037402, 'motion_component': -0.46199900587296655}]}, 5178: {'frame': 5178, 'ionic_force': [-0.6896159946918488, 5.541051208972931, -4.2868136167526245], 'ionic_force_magnitude': 7.039573119541477, 'motion_vector': [-0.499969482421875, -1.2579994201660156, 0.6877059936523438], 'cosine_ionic_motion': -0.8957020063259677, 'ionic_motion_component': -6.305359766851653, 'ionic_force_x': -0.6896159946918488, 'ionic_force_y': 5.541051208972931, 'ionic_force_z': -4.2868136167526245, 'radial_force': 5.583799666946801, 'axial_force': -4.2868136167526245, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.52821284532547, 2.203639030456543, -0.34880292415618896], 'magnitude': 2.2927489280700684, 'distance': 12.033468246459961, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.9410791659335338, 'motion_component': -2.1576581707824296}, {'ion': 1309, 'force': [-0.9532740116119385, 2.5756494998931885, -2.5336785316467285], 'magnitude': 3.7366065979003906, 'distance': 9.426063537597656, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.794204453800667, 'motion_component': -2.9676295725849258}, {'ion': 1403, 'force': [-0.26455482840538025, 0.7617626786231995, -1.404332160949707], 'magnitude': 1.6193888187408447, 'distance': 14.318366050720215, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7287143440952004, 'motion_component': -1.1800719301357088}]}, 5179: {'frame': 5179, 'ionic_force': [-2.030127376317978, 6.3477553725242615, -5.428711324930191], 'ionic_force_magnitude': 8.595715332822024, 'motion_vector': [0.006259918212890625, 2.1265487670898438, -1.1589584350585938], 'cosine_ionic_motion': 0.9500465456928359, 'ionic_motion_component': 8.16632965970651, 'ionic_force_x': -2.030127376317978, 'ionic_force_y': 6.3477553725242615, 'ionic_force_z': -5.428711324930191, 'radial_force': 6.66448913522157, 'axial_force': -5.428711324930191, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.29383471608161926, 2.3622288703918457, -0.319489985704422], 'magnitude': 2.401777982711792, 'distance': 11.75716495513916, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.9275760945020237, 'motion_component': 2.2278319278088166}, {'ion': 1309, 'force': [-1.8343040943145752, 3.2689404487609863, -3.492114543914795], 'magnitude': 5.123036861419678, 'distance': 8.050174713134766, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.885550252509541, 'motion_component': 4.53670662706779}, {'ion': 1403, 'force': [-0.489657998085022, 0.7165860533714294, -1.6171067953109741], 'magnitude': 1.8352915048599243, 'distance': 13.449821472167969, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7637974619760005, 'motion_component': 1.4017909947725329}]}, 5180: {'frame': 5180, 'ionic_force': [-0.47080206871032715, 4.05627167224884, -2.3710789382457733], 'ionic_force_magnitude': 4.721970965432023, 'motion_vector': [0.3277015686035156, -0.06797409057617188, 1.3685455322265625], 'cosine_ionic_motion': -0.552400466844324, 'ionic_motion_component': -2.6084189657299928, 'ionic_force_x': -0.47080206871032715, 'ionic_force_y': 4.05627167224884, 'ionic_force_z': -2.3710789382457733, 'radial_force': 4.083502720335855, 'axial_force': -2.3710789382457733, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.32464051246643066, 1.7187424898147583, -0.2759523093700409], 'magnitude': 1.770767331123352, 'distance': 13.69267463684082, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.15556355057782062, 'motion_component': -0.27546685084777156}, {'ion': 1309, 'force': [-0.7954425811767578, 2.337529182434082, -2.0951266288757324], 'magnitude': 3.238259792327881, 'distance': 10.125423431396484, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7204338815501123, 'motion_component': -2.332952148085589}]}, 5181: {'frame': 5181, 'ionic_force': [-0.6866850852966309, 5.2680962681770325, -3.737524628639221], 'ionic_force_magnitude': 6.4956497016722174, 'motion_vector': [-0.3796195983886719, -1.8383750915527344, -0.54205322265625], 'cosine_ionic_motion': -0.5829162005149764, 'ionic_motion_component': -3.7864194439750087, 'ionic_force_x': -0.6866850852966309, 'ionic_force_y': 5.2680962681770325, 'ionic_force_z': -3.737524628639221, 'radial_force': 5.312661733740406, 'axial_force': -3.737524628639221, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.3693566620349884, 1.7314714193344116, -0.16969358921051025], 'magnitude': 1.7785425186157227, 'distance': 13.662712097167969, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.9298734282283851, 'motion_component': -1.6538194403953677}, {'ion': 1309, 'force': [-0.789997935295105, 2.699798583984375, -2.170147180557251], 'magnitude': 3.5528225898742676, 'distance': 9.666790008544922, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5023273269637426, 'motion_component': -1.7846798437849252}, {'ion': 1403, 'force': [-0.2660438120365143, 0.8368262648582458, -1.39768385887146], 'magnitude': 1.6506295204162598, 'distance': 14.182221412658691, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.21078027551344006, 'motion_component': -0.3479201363469171}]}, 5182: {'frame': 5182, 'ionic_force': [-1.5095845460891724, 5.511749029159546, -4.918577492237091], 'ionic_force_magnitude': 7.53993550432454, 'motion_vector': [3.399822235107422, 1.0570564270019531, -0.6069412231445312], 'cosine_ionic_motion': 0.1351049295348629, 'ionic_motion_component': 1.018682455009178, 'ionic_force_x': -1.5095845460891724, 'ionic_force_y': 5.511749029159546, 'ionic_force_z': -4.918577492237091, 'radial_force': 5.714737339741211, 'axial_force': -4.918577492237091, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.24988240003585815, 2.1664843559265137, -0.3289939761161804], 'magnitude': 2.2055232524871826, 'distance': 12.26911449432373, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.4192119235928302, 'motion_component': 0.9245816354512906}, {'ion': 1309, 'force': [-1.407989263534546, 2.6396069526672363, -3.090088129043579], 'magnitude': 4.301000118255615, 'distance': 8.785860061645508, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.00780209540420473, 'motion_component': -0.033556814397886825}, {'ion': 1403, 'force': [-0.3514776825904846, 0.7056577205657959, -1.4994953870773315], 'magnitude': 1.694100260734558, 'distance': 13.999079704284668, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.07535424101003572, 'motion_component': 0.12765764161992088}]}, 5183: {'frame': 5183, 'ionic_force': [0.906077116727829, 3.351901054382324, -2.439151182770729], 'ionic_force_magnitude': 4.243309429235511, 'motion_vector': [-0.3704338073730469, 0.2990570068359375, 0.07714080810546875], 'cosine_ionic_motion': 0.23386514195069716, 'ionic_motion_component': 0.9923621620088946, 'ionic_force_x': 0.906077116727829, 'ionic_force_y': 3.351901054382324, 'ionic_force_z': -2.439151182770729, 'radial_force': 3.472206275529602, 'axial_force': -2.439151182770729, 'before_closest_residue': 98, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.6261655688285828, 1.4340345859527588, -0.20961131155490875], 'magnitude': 1.5787575244903564, 'distance': 14.501446723937988, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.23736511913737168, 'motion_component': 0.37474197496300743}, {'ion': 1309, 'force': [0.2799115478992462, 1.9178664684295654, -2.2295398712158203], 'magnitude': 2.954219102859497, 'distance': 10.601020812988281, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.20906377391369516, 'motion_component': 0.6176201873585594}]}, 5184: {'frame': 5184, 'ionic_force': [0.7254925360903144, 4.958870887756348, -4.047217309474945], 'ionic_force_magnitude': 6.441793838013896, 'motion_vector': [-0.18041229248046875, 0.4036216735839844, 0.16362762451171875], 'cosine_ionic_motion': 0.3979180144561937, 'ionic_motion_component': 2.563305813558633, 'ionic_force_x': 0.7254925360903144, 'ionic_force_y': 4.958870887756348, 'ionic_force_z': -4.047217309474945, 'radial_force': 5.011660393657992, 'axial_force': -4.047217309474945, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.5973078608512878, 1.5048673152923584, -0.26393312215805054], 'magnitude': 1.6404459476470947, 'distance': 14.22617244720459, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.5902359183247087, 'motion_component': 0.9682501389175825}, {'ion': 1309, 'force': [0.1381777822971344, 2.6733298301696777, -2.3793797492980957], 'magnitude': 3.581512689590454, 'distance': 9.6279935836792, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3937215782895846, 'motion_component': 1.410118846732325}, {'ion': 1403, 'force': [-0.009993107058107853, 0.7806737422943115, -1.4039044380187988], 'magnitude': 1.6063930988311768, 'distance': 14.376167297363281, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.1151254858041788, 'motion_component': 0.18493679439559696}]}, 5185: {'frame': 5185, 'ionic_force': [0.7339238412678242, 5.119778215885162, -3.856375366449356], 'ionic_force_magnitude': 6.45154277298004, 'motion_vector': [-0.11819076538085938, -0.16250991821289062, 0.146270751953125], 'cosine_ionic_motion': -0.924755423083406, 'ionic_motion_component': -5.966099166567847, 'ionic_force_x': 0.7339238412678242, 'ionic_force_y': 5.119778215885162, 'ionic_force_z': -3.856375366449356, 'radial_force': 5.172114962433992, 'axial_force': -3.856375366449356, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.8244546055793762, 1.679525375366211, -0.2533508837223053], 'magnitude': 1.8880459070205688, 'distance': 13.260587692260742, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.8682598275267359, 'motion_component': -1.6393144610569834}, {'ion': 1309, 'force': [-0.028522875159978867, 2.627678871154785, -2.242663860321045], 'magnitude': 3.454714298248291, 'distance': 9.803089141845703, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8754357746797629, 'motion_component': -3.024380502198848}, {'ion': 1403, 'force': [-0.06200788915157318, 0.8125739693641663, -1.3603606224060059], 'magnitude': 1.5857813358306885, 'distance': 14.469295501708984, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8213012027582747, 'motion_component': -1.302404121518519}]}, 5186: {'frame': 5186, 'ionic_force': [0.6085753031075001, 5.361973226070404, -3.9645311534404755], 'ionic_force_magnitude': 6.696165174429937, 'motion_vector': [0.29323577880859375, 0.5634040832519531, 0.6587371826171875], 'cosine_ionic_motion': 0.09593404861098064, 'ionic_motion_component': 0.6423902353509172, 'ionic_force_x': 0.6085753031075001, 'ionic_force_y': 5.361973226070404, 'ionic_force_z': -3.9645311534404755, 'radial_force': 5.396398871159196, 'axial_force': -3.9645311534404755, 'before_closest_residue': 455, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.7067315578460693, 1.7726627588272095, -0.21329709887504578], 'magnitude': 1.920233964920044, 'distance': 13.148977279663086, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.6063586115181139, 'motion_component': 1.1643503887190967}, {'ion': 1309, 'force': [-0.05736168473958969, 2.774033784866333, -2.3771002292633057], 'magnitude': 3.6536500453948975, 'distance': 9.532472610473633, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.005923090307569401, 'motion_component': -0.021640899696546034}, {'ion': 1403, 'force': [-0.04079456999897957, 0.8152766823768616, -1.374133825302124], 'magnitude': 1.598306655883789, 'distance': 14.41248893737793, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.31303085430443395, 'motion_component': -0.5003192851393142}]}, 5187: {'frame': 5187, 'ionic_force': [0.44809454679489136, 5.63523006439209, -3.661033511161804], 'ionic_force_magnitude': 6.7349664417386315, 'motion_vector': [-0.44336700439453125, -0.58660888671875, -0.7073516845703125], 'cosine_ionic_motion': -0.1331114322693107, 'ionic_motion_component': -0.8965010293455722, 'ionic_force_x': 0.44809454679489136, 'ionic_force_y': 5.63523006439209, 'ionic_force_z': -3.661033511161804, 'radial_force': 5.653017477550887, 'axial_force': -3.661033511161804, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [0.5526303648948669, 1.42279052734375, -0.1382688283920288], 'magnitude': 1.5325963497161865, 'distance': 14.718214988708496, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.6278833176374604, 'motion_component': -0.962291660716259}, {'ion': 1309, 'force': [-0.0501912422478199, 3.1493821144104004, -2.052255630493164], 'magnitude': 3.7593722343444824, 'distance': 9.397479057312012, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.09738347942390585, 'motion_component': -0.36610075432767797}, {'ion': 1403, 'force': [-0.054344575852155685, 1.0630574226379395, -1.4705090522766113], 'magnitude': 1.8153350353240967, 'distance': 13.523548126220703, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.23791276105627682, 'motion_component': 0.43189137043733694}]}, 5188: {'frame': 5188, 'ionic_force': [0.6004464058205485, 5.34605211019516, -4.232802301645279], 'ionic_force_magnitude': 6.845248306380018, 'motion_vector': [0.09778976440429688, 0.3133354187011719, -0.27387237548828125], 'cosine_ionic_motion': 0.9886528166637947, 'ionic_motion_component': 6.767574018865675, 'ionic_force_x': 0.6004464058205485, 'ionic_force_y': 5.34605211019516, 'ionic_force_z': -4.232802301645279, 'radial_force': 5.37966625834586, 'axial_force': -4.232802301645279, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.7558067440986633, 2.0558364391326904, -0.4618763029575348], 'magnitude': 2.238534450531006, 'distance': 12.178313255310059, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.8825643705961469, 'motion_component': 1.975650853246151}, {'ion': 1309, 'force': [-0.012659800238907337, 2.442432165145874, -2.3873846530914307], 'magnitude': 3.4154415130615234, 'distance': 9.859289169311523, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9711197726701742, 'motion_component': 3.3168027721633653}, {'ion': 1403, 'force': [-0.14270053803920746, 0.8477835059165955, -1.3835413455963135], 'magnitude': 1.6288913488388062, 'distance': 14.276540756225586, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9055977262933529, 'motion_component': 1.4751202866299886}]}, 5189: {'frame': 5189, 'ionic_force': [0.32750216871500015, 4.727729856967926, -3.834524780511856], 'ionic_force_magnitude': 6.096086249663672, 'motion_vector': [-0.000904083251953125, -0.1085205078125, 0.5684127807617188], 'cosine_ionic_motion': -0.7633747994882957, 'ionic_motion_component': -4.653598618500362, 'ionic_force_x': 0.32750216871500015, 'ionic_force_y': 4.727729856967926, 'ionic_force_z': -3.834524780511856, 'radial_force': 4.739059745453627, 'axial_force': -3.834524780511856, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [0.5216655135154724, 1.448395848274231, -0.2568974792957306], 'magnitude': 1.5607632398605347, 'distance': 14.58480167388916, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.33622893755916217, 'motion_component': -0.5247737514062334}, {'ion': 1309, 'force': [-0.11025428026914597, 2.4549198150634766, -2.214020013809204], 'magnitude': 3.307668685913086, 'distance': 10.018623352050781, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7966152203201085, 'motion_component': -2.6349391937450988}, {'ion': 1403, 'force': [-0.0839090645313263, 0.8244141936302185, -1.3636072874069214], 'magnitude': 1.5956579446792603, 'distance': 14.424446105957031, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9362191895719004, 'motion_component': -1.4938856029452705}]}, 5190: {'frame': 5190, 'ionic_force': [0.34706735610961914, 4.918230354785919, -3.804109513759613], 'ionic_force_magnitude': 6.227414773811919, 'motion_vector': [0.3770256042480469, -0.35123443603515625, -0.49456024169921875], 'cosine_ionic_motion': 0.06402448857565023, 'ionic_motion_component': 0.39870704604175666, 'ionic_force_x': 0.34706735610961914, 'ionic_force_y': 4.918230354785919, 'ionic_force_z': -3.804109513759613, 'radial_force': 4.930460989848165, 'axial_force': -3.804109513759613, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1308, 'force': [0.5309812426567078, 1.4431406259536743, -0.21502536535263062], 'magnitude': 1.5526853799819946, 'distance': 14.62269115447998, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.1806608335869741, 'motion_component': -0.28050943300189246}, {'ion': 1309, 'force': [-0.07559871673583984, 2.564948797225952, -2.245485782623291], 'magnitude': 3.4098215103149414, 'distance': 9.867410659790039, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.07437417935511147, 'motion_component': 0.25360268929463814}, {'ion': 1403, 'force': [-0.10831516981124878, 0.9101409316062927, -1.3435983657836914], 'magnitude': 1.6264517307281494, 'distance': 14.287243843078613, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.26168234308413185, 'motion_component': 0.42561370202601617}]}, 5191: {'frame': 5191, 'ionic_force': [0.657955770380795, 5.201777338981628, -4.198868662118912], 'ionic_force_magnitude': 6.717283031244436, 'motion_vector': [-0.9679679870605469, 0.518524169921875, 1.3073348999023438], 'cosine_ionic_motion': -0.2989874499026258, 'ionic_motion_component': -2.0083833237859543, 'ionic_force_x': 0.657955770380795, 'ionic_force_y': 5.201777338981628, 'ionic_force_z': -4.198868662118912, 'radial_force': 5.243223558090975, 'axial_force': -4.198868662118912, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.6094868183135986, 1.5151386260986328, -0.26498427987098694], 'magnitude': 1.6544896364212036, 'distance': 14.165666580200195, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.05336790472600894, 'motion_component': -0.08829664447299024}, {'ion': 1309, 'force': [0.05508818104863167, 2.8828670978546143, -2.548942804336548], 'magnitude': 3.8485147953033447, 'distance': 9.288005828857422, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2877654872420616, 'motion_component': -1.1074697614626865}, {'ion': 1403, 'force': [-0.006619228981435299, 0.8037716150283813, -1.384941577911377], 'magnitude': 1.601298213005066, 'distance': 14.399020195007324, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5074739143486897, 'motion_component': -0.8126170453461972}]}, 5192: {'frame': 5192, 'ionic_force': [0.1945376694202423, 5.99289608001709, -3.5691631473600864], 'ionic_force_magnitude': 6.977934787828059, 'motion_vector': [-2.582378387451172, -1.3664169311523438, 0.01790618896484375], 'cosine_ionic_motion': -0.4294408475329646, 'ionic_motion_component': -2.996610229314639, 'ionic_force_x': 0.1945376694202423, 'ionic_force_y': 5.99289608001709, 'ionic_force_z': -3.5691631473600864, 'radial_force': 5.996052729146706, 'axial_force': -3.5691631473600864, 'before_closest_residue': 455, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.6152461171150208, 1.7376521825790405, -0.03967398777604103], 'magnitude': 1.8437833786010742, 'distance': 13.41881275177002, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.7358333946801904, 'motion_component': -1.356717336705017}, {'ion': 1309, 'force': [-0.2750970125198364, 3.165602922439575, -1.957560658454895], 'magnitude': 3.732125997543335, 'distance': 9.431719779968262, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3347561495557672, 'motion_component': -1.2493521061189088}, {'ion': 1403, 'force': [-0.14561143517494202, 1.0896409749984741, -1.5719285011291504], 'magnitude': 1.9181969165802002, 'distance': 13.155957221984863, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.20359788913885363, 'motion_component': -0.39054084032030834}]}, 5193: {'frame': 5193, 'ionic_force': [-1.93711456656456, 6.59854257106781, -4.372821029275656], 'ionic_force_magnitude': 8.149523952984381, 'motion_vector': [0.4185295104980469, 1.0166091918945312, -0.2987213134765625], 'cosine_ionic_motion': 0.7758910631739562, 'ionic_motion_component': 6.323142804242674, 'ionic_force_x': -1.93711456656456, 'ionic_force_y': 6.59854257106781, 'ionic_force_z': -4.372821029275656, 'radial_force': 6.877003483072463, 'axial_force': -4.372821029275656, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.4174995720386505, 2.2765603065490723, -0.059432800859212875], 'magnitude': 2.3152894973754883, 'distance': 11.974748611450195, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.9503974281845952, 'motion_component': 2.2004450859416735}, {'ion': 1309, 'force': [-1.7871077060699463, 3.376755714416504, -2.6929991245269775], 'magnitude': 4.674235820770264, 'distance': 8.427790641784668, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.655258731336676, 'motion_component': 3.062833615510769}, {'ion': 1403, 'force': [-0.5675064325332642, 0.9452265501022339, -1.6203891038894653], 'magnitude': 1.9598922729492188, 'distance': 13.015262603759766, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.540776768071992, 'motion_component': 1.0598641965006337}]}, 5194: {'frame': 5194, 'ionic_force': [-0.9560555219650269, 5.772682011127472, -3.487354025244713], 'ionic_force_magnitude': 6.811720624046837, 'motion_vector': [-0.6451492309570312, -1.4054031372070312, -0.01318359375], 'cosine_ionic_motion': -0.7072447724738669, 'ionic_motion_component': -4.8175538029095515, 'ionic_force_x': -0.9560555219650269, 'ionic_force_y': 5.772682011127472, 'ionic_force_z': -3.487354025244713, 'radial_force': 5.8513160709941605, 'axial_force': -3.487354025244713, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [0.624089837</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>{5213: {'frame': 5213, 'ionic_force': [9.059208557009697, 6.910908341407776, -17.690110206604004], 'ionic_force_magnitude': 21.042098586037763, 'motion_vector': [-0.08104324340820312, -3.535572052001953, 0.40856170654296875], 'cosine_ionic_motion': -0.43245966970827554, 'ionic_motion_component': -9.099859004486863, 'ionic_force_x': 9.059208557009697, 'ionic_force_y': 6.910908341407776, 'ionic_force_z': -17.690110206604004, 'radial_force': 11.394293035670852, 'axial_force': -17.690110206604004, 'contributions': [{'ion': 1308, 'force': [4.778199672698975, 9.435524940490723, -10.170702934265137], 'magnitude': 14.673224449157715, 'distance': 4.756705284118652, 'cosine_with_motion': -0.7255885946159099, 'motion_component': -10.646724441459995}, {'ion': 1320, 'force': [4.232130527496338, -3.0712902545928955, -4.9525957107543945], 'magnitude': 7.202219009399414, 'distance': 6.789470195770264, 'cosine_with_motion': 0.33121377374106037, 'motion_component': 2.3854740970482444}, {'ion': 1403, 'force': [0.04887835681438446, 0.5466736555099487, -2.5668115615844727], 'magnitude': 2.624835729598999, 'distance': 11.246515274047852, 'cosine_with_motion': -0.31949001303026325, 'motion_component': -0.8386088114752297}]}, 5214: {'frame': 5214, 'ionic_force': [0.876273438334465, -7.065377295017242, -7.964790105819702], 'ionic_force_magnitude': 10.682944017893153, 'motion_vector': [-2.800647735595703, -0.17963790893554688, 2.6386032104492188], 'cosine_ionic_motion': -0.5394970021714701, 'ionic_motion_component': -5.763416272018996, 'ionic_force_x': 0.876273438334465, 'ionic_force_y': -7.065377295017242, 'ionic_force_z': -7.964790105819702, 'radial_force': 7.119509214803761, 'axial_force': -7.964790105819702, 'contributions': [{'ion': 1308, 'force': [-1.3250770568847656, -3.1238503456115723, -2.5353305339813232], 'magnitude': 4.2358198165893555, 'distance': 8.85319995880127, 'cosine_with_motion': -0.14816259756217112, 'motion_component': -0.6275900945759094}, {'ion': 1320, 'force': [2.0835518836975098, -3.640300989151001, -2.173349618911743], 'magnitude': 4.724026679992676, 'distance': 8.383258819580078, 'cosine_with_motion': -0.5998743875613214, 'motion_component': -2.8338226264943356}, {'ion': 1403, 'force': [0.11779861152172089, -0.3012259602546692, -3.2561099529266357], 'magnitude': 3.272134780883789, 'distance': 10.072875022888184, 'cosine_with_motion': -0.7035172793829035, 'motion_component': -2.302003315099296}]}, 5215: {'frame': 5215, 'ionic_force': [-3.1574587523937225, -9.676621198654175, -7.118128061294556], 'ionic_force_magnitude': 12.42072021632804, 'motion_vector': [0.9844284057617188, -0.2884941101074219, -5.571617126464844], 'cosine_ionic_motion': 0.5591117071431897, 'ionic_motion_component': 6.944570084099098, 'ionic_force_x': -3.1574587523937225, 'ionic_force_y': -9.676621198654175, 'ionic_force_z': -7.118128061294556, 'radial_force': 10.178729959838362, 'axial_force': -7.118128061294556, 'contributions': [{'ion': 1308, 'force': [-2.1365599632263184, -3.032615900039673, -0.8023586273193359], 'magnitude': 3.7954483032226562, 'distance': 9.352710723876953, 'cosine_with_motion': 0.15077678582865442, 'motion_component': 0.5722654804066467}, {'ion': 1320, 'force': [0.5601136684417725, -6.005922317504883, -0.8906189203262329], 'magnitude': 6.097379207611084, 'distance': 7.378998756408691, 'cosine_with_motion': 0.20977316123691703, 'motion_component': 1.2790664955624322}, {'ion': 1403, 'force': [-1.2336101531982422, -0.5227363109588623, -3.747150182723999], 'magnitude': 3.9794700145721436, 'distance': 9.133903503417969, 'cosine_with_motion': 0.8788779690915066, 'motion_component': 3.4974685416808162}, {'ion': 1469, 'force': [-0.34740230441093445, -0.11534667015075684, -1.6780003309249878], 'magnitude': 1.7174626588821411, 'distance': 13.903539657592773, 'cosine_with_motion': 0.9291435751757805, 'motion_component': 1.5957694874407418}]}, 5216: {'frame': 5216, 'ionic_force': [0.3360389769077301, -3.4986054599285126, -5.366488456726074], 'ionic_force_magnitude': 6.415010577888161, 'motion_vector': [0.49591064453125, 1.3578147888183594, -0.21898651123046875], 'cosine_ionic_motion': -0.3634329471769188, 'ionic_motion_component': -2.3314262004930035, 'ionic_force_x': 0.3360389769077301, 'ionic_force_y': -3.4986054599285126, 'ionic_force_z': -5.366488456726074, 'radial_force': 3.51470658209797, 'axial_force': -5.366488456726074, 'contributions': [{'ion': 1308, 'force': [-0.5920225381851196, -1.5384231805801392, -1.2295265197753906], 'magnitude': 2.0564465522766113, 'distance': 12.706043243408203, 'cosine_with_motion': -0.7028663925785696, 'motion_component': -1.4454071028631574}, {'ion': 1320, 'force': [1.186414122581482, -1.7023833990097046, -2.2223496437072754], 'magnitude': 3.0404810905456543, 'distance': 10.449557304382324, 'cosine_with_motion': -0.2781600982653527, 'motion_component': -0.8457405365038682}, {'ion': 1403, 'force': [-0.2583526074886322, -0.2577988803386688, -1.9146122932434082], 'magnitude': 1.9490886926651, 'distance': 13.051283836364746, 'cosine_with_motion': -0.020665348923662074, 'motion_component': -0.04027859703741399}]}, 5217: {'frame': 5217, 'ionic_force': [-0.5696889609098434, -2.4908271618187428, -6.695563793182373], 'ionic_force_magnitude': 7.166543097673472, 'motion_vector': [1.0223388671875, -0.4985237121582031, 2.0433120727539062], 'cosine_ionic_motion': -0.7769881557830077, 'ionic_motion_component': -5.5683191048007545, 'ionic_force_x': -0.5696889609098434, 'ionic_force_y': -2.4908271618187428, 'ionic_force_z': -6.695563793182373, 'radial_force': 2.555144900438437, 'axial_force': -6.695563793182373, 'contributions': [{'ion': 1308, 'force': [-1.6062496900558472, -1.6342322826385498, -2.415165901184082], 'magnitude': 3.329231023788452, 'distance': 9.986126899719238, 'cosine_with_motion': -0.7401330330015188, 'motion_component': -2.4640738930936728}, {'ion': 1320, 'force': [1.2217909097671509, -0.8660487532615662, -2.349320888519287], 'magnitude': 2.7860584259033203, 'distance': 10.916261672973633, 'cosine_with_motion': -0.47880292106144073, 'motion_component': -1.333972960252149}, {'ion': 1403, 'force': [-0.18523018062114716, 0.009453874081373215, -1.931077003479004], 'magnitude': 1.939963459968567, 'distance': 13.08194351196289, 'cosine_with_motion': -0.912528632425414, 'motion_component': -1.7702721473163905}]}, 5218: {'frame': 5218, 'ionic_force': [4.206250421702862, -4.269712045788765, -7.6996800899505615], 'ionic_force_magnitude': 9.757461609025693, 'motion_vector': [-0.7376747131347656, 0.12036895751953125, 5.263938903808594], 'cosine_ionic_motion': -0.8509877619478586, 'ionic_motion_component': -8.303480416956926, 'ionic_force_x': 4.206250421702862, 'ionic_force_y': -4.269712045788765, 'ionic_force_z': -7.6996800899505615, 'radial_force': 5.993578527393228, 'axial_force': -7.6996800899505615, 'contributions': [{'ion': 1308, 'force': [-1.0178943872451782, -2.646784543991089, -2.161548376083374], 'magnitude': 3.5656511783599854, 'distance': 9.649384498596191, 'cosine_with_motion': -0.5773913926795388, 'motion_component': -2.0587763371135157}, {'ion': 1320, 'force': [5.3220672607421875, -1.4583486318588257, -2.8955790996551514], 'magnitude': 6.231818199157715, 'distance': 7.298971652984619, 'cosine_with_motion': -0.5838190835985204, 'motion_component': -3.6382544330410886}, {'ion': 1403, 'force': [-0.09792245179414749, -0.1645788699388504, -2.642552614212036], 'magnitude': 2.6494827270507812, 'distance': 11.194082260131836, 'cosine_with_motion': -0.9837579542078188, 'motion_component': -2.606449820321628}]}, 5219: {'frame': 5219, 'ionic_force': [-0.8370766043663025, 7.505206935107708, 4.665254652500153], 'ionic_force_magnitude': 8.876566304210236, 'motion_vector': [-1.3892173767089844, -0.5494041442871094, 1.6649017333984375], 'cosine_ionic_motion': 0.24207837425350287, 'ionic_motion_component': 2.1488247398766385, 'ionic_force_x': -0.8370766043663025, 'ionic_force_y': 7.505206935107708, 'ionic_force_z': 4.665254652500153, 'radial_force': 7.551743400061091, 'axial_force': 4.665254652500153, 'contributions': [{'ion': 1308, 'force': [-1.2311298847198486, -4.110632419586182, -0.6271311640739441], 'magnitude': 4.336619853973389, 'distance': 8.749703407287598, 'cosine_with_motion': 0.30148794664863837, 'motion_component': 1.3074386645678937}, {'ion': 1320, 'force': [1.5758368968963623, 11.999844551086426, 15.897293090820312], 'magnitude': 19.98007583618164, 'distance': 4.076340675354004, 'cosine_with_motion': 0.3957087251708299, 'motion_component': 7.906290618905373}, {'ion': 1403, 'force': [-1.0520174503326416, -0.32890668511390686, -8.382981300354004], 'magnitude': 8.455134391784668, 'distance': 6.266265392303467, 'cosine_with_motion': -0.6511147850343424, 'motion_component': -5.505262943493138}, {'ion': 1469, 'force': [-0.12976616621017456, -0.0550985112786293, -2.221925973892212], 'magnitude': 2.226393938064575, 'distance': 12.211472511291504, 'cosine_with_motion': -0.7005236558494705, 'motion_component': -1.5596416475744035}]}, 5220: {'frame': 5220, 'ionic_force': [-7.989065766334534, -10.187750428915024, -5.366817504167557], 'ionic_force_magnitude': 14.01492635527265, 'motion_vector': [-0.5346794128417969, -1.1390304565429688, -0.756134033203125], 'cosine_ionic_motion': 0.9688891272673253, 'ionic_motion_component': 13.578909765075954, 'ionic_force_x': -7.989065766334534, 'ionic_force_y': -10.187750428915024, 'ionic_force_z': -5.366817504167557, 'radial_force': 12.946637811442654, 'axial_force': -5.366817504167557, 'contributions': [{'ion': 1308, 'force': [-1.290416955947876, -3.383082866668701, 0.44074055552482605], 'magnitude': 3.6475577354431152, 'distance': 9.540430068969727, 'cosine_with_motion': 0.7862651912087649, 'motion_component': 2.867947724152115}, {'ion': 1320, 'force': [-1.2900820970535278, -3.8637619018554688, 8.199496269226074], 'magnitude': 9.155583381652832, 'distance': 6.021795749664307, 'cosine_with_motion': -0.0825272300641764, 'motion_component': -0.7555849354875583}, {'ion': 1403, 'force': [-4.87747859954834, -2.6918888092041016, -11.338939666748047], 'magnitude': 12.633590698242188, 'distance': 5.126319408416748, 'cosine_with_motion': 0.7682381903521565, 'motion_component': 9.705606906917723}, {'ion': 1469, 'force': [-0.53108811378479, -0.24901685118675232, -2.66811466217041], 'magnitude': 2.7318308353424072, 'distance': 11.02407455444336, 'cosine_with_motion': 0.6446005870361542, 'motion_component': 1.7609397736349202}]}, 5221: {'frame': 5221, 'ionic_force': [-10.496177196502686, -8.205937772989273, 0.1122767822816968], 'ionic_force_magnitude': 13.32365402396785, 'motion_vector': [0.09583663940429688, 4.582389831542969, -4.5017547607421875], 'cosine_ionic_motion': -0.4569579844587636, 'ionic_motion_component': -6.0883500884182435, 'ionic_force_x': -10.496177196502686, 'ionic_force_y': -8.205937772989273, 'ionic_force_z': 0.1122767822816968, 'radial_force': 13.32318094429987, 'axial_force': 0.1122767822816968, 'contributions': [{'ion': 1308, 'force': [-0.9717339277267456, -2.528850793838501, 0.010465134866535664], 'magnitude': 2.709144353866577, 'distance': 11.070137023925781, 'cosine_with_motion': -0.6738649628328864, 'motion_component': -1.825597403703803}, {'ion': 1320, 'force': [-6.512366771697998, -3.0620293617248535, 8.233292579650879], 'magnitude': 10.934991836547852, 'distance': 5.510104179382324, 'cosine_with_motion': -0.7362136948005549, 'motion_component': -8.050490911518978}, {'ion': 1403, 'force': [-2.5566587448120117, -2.16740083694458, -6.0023908615112305], 'magnitude': 6.874796390533447, 'distance': 6.9492692947387695, 'cosine_with_motion': 0.3813827954446882, 'motion_component': 2.6219290923979797}, {'ion': 1469, 'force': [-0.4554177522659302, -0.4476567804813385, -2.1290900707244873], 'magnitude': 2.22279691696167, 'distance': 12.221348762512207, 'cosine_with_motion': 0.5244785240319814, 'motion_component': 1.1658092836760383}]}, 5222: {'frame': 5222, 'ionic_force': [-10.679179668426514, 1.4521918892860413, -9.871692180633545], 'ionic_force_magnitude': 14.615199149618997, 'motion_vector': [-3.9730682373046875, -1.5599021911621094, 2.0731430053710938], 'cosine_ionic_motion': 0.2840376600251383, 'ionic_motion_component': 4.151266967259171, 'ionic_force_x': -10.679179668426514, 'ionic_force_y': 1.4521918892860413, 'ionic_force_z': -9.871692180633545, 'radial_force': 10.777464436213297, 'axial_force': -9.871692180633545, 'contributions': [{'ion': 1308, 'force': [-2.3145053386688232, -2.909573793411255, -2.4544501304626465], 'magnitude': 4.454983711242676, 'distance': 8.632686614990234, 'cosine_with_motion': 0.4089915671206331, 'motion_component': 1.822050778624856}, {'ion': 1320, 'force': [-7.233617305755615, 3.4570906162261963, -3.964205026626587], 'magnitude': 8.943802833557129, 'distance': 6.0926737785339355, 'cosine_with_motion': 0.356471846835402, 'motion_component': 3.1882140577431386}, {'ion': 1403, 'force': [-1.1310570240020752, 0.9046750664710999, -3.4530370235443115], 'magnitude': 3.74448823928833, 'distance': 9.4161376953125, 'cosine_with_motion': -0.22940328619630437, 'motion_component': -0.8589978912641101}]}, 5223: {'frame': 5223, 'ionic_force': [-9.0616614818573, -0.7365338355302811, -3.7814049124717712], 'ionic_force_magnitude': 9.846583875371337, 'motion_vector': [1.1881523132324219, 0.9744796752929688, 2.5615386962890625], 'cosine_ionic_motion': -0.7197750582208821, 'ionic_motion_component': -7.0873254821722025, 'ionic_force_x': -9.0616614818573, 'ionic_force_y': -0.7365338355302811, 'ionic_force_z': -3.7814049124717712, 'radial_force': 9.09154502285817, 'axial_force': -3.7814049124717712, 'contributions': [{'ion': 1308, 'force': [-2.0935752391815186, -1.8744561672210693, -0.5705388188362122], 'magnitude': 2.8674304485321045, 'distance': 10.760255813598633, 'cosine_with_motion': -0.6742965102789934, 'motion_component': -1.933498388602409}, {'ion': 1320, 'force': [-4.028995990753174, 0.7997772693634033, 0.7936450242996216], 'magnitude': 4.183578014373779, 'distance': 8.908306121826172, 'cosine_with_motion': -0.15801994549859863, 'motion_component': -0.6610887659741991}, {'ion': 1403, 'force': [-2.2542738914489746, 0.2554945647716522, -2.6964259147644043], 'magnitude': 3.523881435394287, 'distance': 9.706404685974121, 'cosine_with_motion': -0.886971707792664, 'motion_component': -3.125583209489937}, {'ion': 1469, 'force': [-0.6848163604736328, 0.08265049755573273, -1.3080852031707764], 'magnitude': 1.4788141250610352, 'distance': 14.983464241027832, 'cosine_with_motion': -0.9244940953963866, 'motion_component': -1.367155000136628}]}, 5224: {'frame': 5224, 'ionic_force': [-11.852895140647888, 1.5224820375442505, -2.5712924543768167], 'ionic_force_magnitude': 12.223772725953896, 'motion_vector': [0.0398406982421875, 2.6087303161621094, -0.5442276000976562], 'cosine_ionic_motion': 0.1503708447138321, 'ionic_motion_component': 1.8380990303915896, 'ionic_force_x': -11.852895140647888, 'ionic_force_y': 1.5224820375442505, 'ionic_force_z': -2.5712924543768167, 'radial_force': 11.950275091806015, 'axial_force': -2.5712924543768167, 'contributions': [{'ion': 1308, 'force': [-3.0808727741241455, -2.469778537750244, 0.02193385921418667], 'magnitude': 3.948678731918335, 'distance': 9.16944694519043, 'cosine_with_motion': -0.6250168030414615, 'motion_component': -2.4679905922540377}, {'ion': 1320, 'force': [-3.7092082500457764, 2.256039619445801, 2.863736867904663], 'magnitude': 5.2008585929870605, 'distance': 7.989719390869141, 'cosine_with_motion': 0.3014942239922375, 'motion_component': 1.5680288067766102}, {'ion': 1403, 'force': [-4.130849361419678, 1.4701601266860962, -3.665073871612549], 'magnitude': 5.714722633361816, 'distance': 7.622044086456299, 'cosine_with_motion': 0.3719633106605391, 'motion_component': 2.125667116136732}, {'ion': 1469, 'force': [-0.9319647550582886, 0.26606082916259766, -1.7918893098831177], 'magnitude': 2.0372073650360107, 'distance': 12.765899658203125, 'cosine_with_motion': 0.3006044973620889, 'motion_component': 0.6123937048573254}]}, 5225: {'frame': 5225, 'ionic_force': [-12.727189838886261, 4.494718790054321, -5.815616488456726], 'ionic_force_magnitude': 14.697117177784452, 'motion_vector': [1.9323806762695312, 0.8050422668457031, -0.5858154296875], 'cosine_ionic_motion': -0.5498999726922859, 'ionic_motion_component': -8.081944334718996, 'ionic_force_x': -12.727189838886261, 'ionic_force_y': 4.494718790054321, 'ionic_force_z': -5.815616488456726, 'radial_force': 13.49755008128205, 'axial_force': -5.815616488456726, 'contributions': [{'ion': 1308, 'force': [-5.498988151550293, -1.1754382848739624, 0.6942658424377441], 'magnitude': 5.665909767150879, 'distance': 7.654806613922119, 'cosine_with_motion': -0.9726077449400174, 'motion_component': -5.510707500471813}, {'ion': 1320, 'force': [-4.546165466308594, 3.720468282699585, -2.5248541831970215], 'magnitude': 6.394090175628662, 'distance': 7.2057576179504395, 'cosine_with_motion': -0.3101345317109207, 'motion_component': -1.983028263270576}, {'ion': 1403, 'force': [-2.0169267654418945, 1.4461729526519775, -2.5027101039886475], 'magnitude': 3.524623155593872, 'distance': 9.70538330078125, 'cosine_with_motion': -0.16538079293163058, 'motion_component': -0.5829049549384706}, {'ion': 1469, 'force': [-0.6651094555854797, 0.5035158395767212, -1.4823180437088013], 'magnitude': 1.7009308338165283, 'distance': 13.970943450927734, 'cosine_with_motion': -0.0031178895486980596, 'motion_component': -0.005303314350566524}]}, 5226: {'frame': 5226, 'ionic_force': [-8.63455793261528, 10.306835412979126, -8.068451166152954], 'ionic_force_magnitude': 15.680763729567671, 'motion_vector': [-0.0262298583984375, 0.5780372619628906, 0.1553192138671875], 'cosine_ionic_motion': 0.5248802706088915, 'ionic_motion_component': 8.23052350972957, 'ionic_force_x': -8.63455793261528, 'ionic_force_y': 10.306835412979126, 'ionic_force_z': -8.068451166152954, 'radial_force': 13.445685067036564, 'axial_force': -8.068451166152954, 'contributions': [{'ion': 1308, 'force': [-3.372286558151245, 1.1184394359588623, 0.5709807872772217], 'magnitude': 3.5985054969787598, 'distance': 9.605234146118164, 'cosine_with_motion': 0.382035810311084, 'motion_component': 1.374757997942818}, {'ion': 1320, 'force': [-3.445181369781494, 6.423120021820068, -3.7658469676971436], 'magnitude': 8.204105377197266, 'distance': 6.361410617828369, 'cosine_with_motion': 0.6547561796468672, 'motion_component': 5.371688847001148}, {'ion': 1403, 'force': [-1.4268732070922852, 2.1184980869293213, -3.1947760581970215], 'magnitude': 4.090305328369141, 'distance': 9.009303092956543, 'cosine_with_motion': 0.31249432221731166, 'motion_component': 1.278197102482256}, {'ion': 1469, 'force': [-0.39021679759025574, 0.646777868270874, -1.6788089275360107], 'magnitude': 1.8409210443496704, 'distance': 13.429241180419922, 'cosine_with_motion': 0.11183524775394986, 'motion_component': 0.20587985755624938}]}, 5227: {'frame': 5227, 'ionic_force': [-7.94691988825798, 10.216525435447693, -6.894068896770477], 'ionic_force_magnitude': 14.66489391836702, 'motion_vector': [-1.3651809692382812, -0.9860496520996094, 0.14288330078125], 'cosine_ionic_motion': -0.008475451243119256, 'ionic_motion_component': -0.12429159339063578, 'ionic_force_x': -7.94691988825798, 'ionic_force_y': 10.216525435447693, 'ionic_force_z': -6.894068896770477, 'radial_force': 12.94337389105097, 'axial_force': -6.894068896770477, 'contributions': [{'ion': 1308, 'force': [-3.113513946533203, 1.471713900566101, 0.5079912543296814], 'magnitude': 3.4810869693756104, 'distance': 9.765885353088379, 'cosine_with_motion': 0.4881399211648226, 'motion_component': 1.6992574855999774}, {'ion': 1320, 'force': [-3.006080389022827, 5.83809232711792, -2.921882152557373], 'magnitude': 7.1872968673706055, 'distance': 6.796514511108398, 'cosine_with_motion': -0.17043338293533036, 'motion_component': -1.2249553237593886}, {'ion': 1403, 'force': [-1.393346905708313, 2.2208824157714844, -2.820758104324341], 'magnitude': 3.851027250289917, 'distance': 9.284975051879883, 'cosine_with_motion': -0.10613156239445612, 'motion_component': -0.40871553483142975}, {'ion': 1469, 'force': [-0.4339786469936371, 0.6858367919921875, -1.6594198942184448], 'magnitude': 1.8472638130187988, 'distance': 13.40616512298584, 'cosine_with_motion': -0.10278906205083915, 'motion_component': -0.1898785247648629}]}, 5228: {'frame': 5228, 'ionic_force': [-9.87448799610138, 7.389701664447784, -6.990283265709877], 'ionic_force_magnitude': 14.176645019522642, 'motion_vector': [0.7691383361816406, -0.3768424987792969, -0.10305023193359375], 'cosine_ionic_motion': -0.789812787166785, 'ionic_motion_component': -11.1968955155433, 'ionic_force_x': -9.87448799610138, 'ionic_force_y': 7.389701664447784, 'ionic_force_z': -6.990283265709877, 'radial_force': 12.333418174808337, 'axial_force': -6.990283265709877, 'contributions': [{'ion': 1308, 'force': [-2.4451513290405273, 0.9452031254768372, 0.08026061952114105], 'magnitude': 2.622711658477783, 'distance': 11.251069068908691, 'cosine_with_motion': -0.9923019662020579, 'motion_component': -2.6025218019028573}, {'ion': 1320, 'force': [-5.125226974487305, 4.3977861404418945, -2.9678163528442383], 'magnitude': 7.3767476081848145, 'distance': 6.708672046661377, 'cosine_with_motion': -0.8318170866945936, 'motion_component': -6.136104879864973}, {'ion': 1403, 'force': [-1.7134193181991577, 1.530916690826416, -2.4926624298095703], 'magnitude': 3.3901147842407227, 'distance': 9.896049499511719, 'cosine_with_motion': -0.560051014426819, 'motion_component': -1.8986371754413724}, {'ion': 1469, 'force': [-0.5906903743743896, 0.5157957077026367, -1.6100651025772095], 'magnitude': 1.790885329246521, 'distance': 13.615549087524414, 'cosine_with_motion': -0.3124889054191626, 'motion_component': -0.5596317703114053}]}, 5229: {'frame': 5229, 'ionic_force': [-9.413652211427689, 7.915450572967529, -7.1453061401844025], 'ionic_force_magnitude': 14.224155706676102, 'motion_vector': [-2.0034332275390625, -4.632930755615234, 0.2904510498046875], 'cosine_ionic_motion': -0.2765377108802912, 'ionic_motion_component': -3.9335154583290404, 'ionic_force_x': -9.413652211427689, 'ionic_force_y': 7.915450572967529, 'ionic_force_z': -7.1453061401844025, 'radial_force': 12.299235981588833, 'axial_force': -7.1453061401844025, 'contributions': [{'ion': 1308, 'force': [-3.0030407905578613, 0.9390349388122559, 0.19887909293174744], 'magnitude': 3.152712106704712, 'distance': 10.261878967285156, 'cosine_with_motion': 0.10813634399926765, 'motion_component': 0.3409227587045228}, {'ion': 1320, 'force': [-4.218984603881836, 4.771722316741943, -2.8418822288513184], 'magnitude': 6.974629878997803, 'distance': 6.899354457855225, 'cosine_with_motion': -0.41062905962600516, 'motion_component': -2.8639856380834434}, {'ion': 1403, 'force': [-1.7074979543685913, 1.6937834024429321, -2.7924537658691406], 'magnitude': 3.685410261154175, 'distance': 9.49130916595459, 'cosine_with_motion': -0.28108048830992605, 'motion_component': -1.0358969432865663}, {'ion': 1469, 'force': [-0.4841288626194, 0.510909914970398, -1.709849238395691], 'magnitude': 1.8490521907806396, 'distance': 13.399681091308594, 'cosine_with_motion': -0.20256639275756702, 'motion_component': -0.37455583836772854}]}, 5230: {'frame': 5230, 'ionic_force': [-13.472239375114441, -2.136018753051758, -5.8683589696884155], 'ionic_force_magnitude': 14.849291124188225, 'motion_vector': [5.115959167480469, 0.8695487976074219, -4.300270080566406], 'cosine_ionic_motion': -0.4551001034999545, 'ionic_motion_component': -6.7579139275190165, 'ionic_force_x': -13.472239375114441, 'ionic_force_y': -2.136018753051758, 'ionic_force_z': -5.8683589696884155, 'radial_force': 13.64052088058857, 'axial_force': -5.8683589696884155, 'contributions': [{'ion': 1308, 'force': [-3.4431419372558594, -1.4593416452407837, 1.5944634675979614], 'magnitude': 4.065368175506592, 'distance': 9.03689193725586, 'cosine_with_motion': -0.9394801019205968, 'motion_component': -3.819332482993259}, {'ion': 1320, 'force': [-6.761546611785889, -0.46857988834381104, -2.9621737003326416], 'magnitude': 7.396793365478516, 'distance': 6.699575424194336, 'cosine_with_motion': -0.44655252950108015, 'motion_component': -3.3030568067030313}, {'ion': 1403, 'force': [-2.4797613620758057, -0.12971417605876923, -2.8303792476654053], 'magnitude': 3.7652475833892822, 'distance': 9.390144348144531, 'cosine_with_motion': -0.024738096463148694, 'motion_component': -0.0931450562886138}, {'ion': 1469, 'force': [-0.7877894639968872, -0.07838304340839386, -1.67026948928833], 'magnitude': 1.8483929634094238, 'distance': 13.402070045471191, 'cosine_with_motion': 0.2475774303234592, 'motion_component': 0.4576203640856893}]}, 5231: {'frame': 5231, 'ionic_force': [-4.702645644545555, -10.708216772880405, -12.202762365341187], 'ionic_force_magnitude': 16.902313210272368, 'motion_vector': [-1.9342155456542969, 1.1726150512695312, 1.3013763427734375], 'cosine_ionic_motion': -0.43849772857207303, 'ionic_motion_component': -7.411625950318177, 'ionic_force_x': -4.702645644545555, 'ionic_force_y': -10.708216772880405, 'ionic_force_z': -12.202762365341187, 'radial_force': 11.695331654688571, 'axial_force': -12.202762365341187, 'contributions': [{'ion': 1308, 'force': [-4.075906753540039, -10.616989135742188, -3.460934638977051], 'magnitude': 11.887453079223633, 'distance': 5.284752368927002, 'cosine_with_motion': -0.29238051464697856, 'motion_component': -3.475659674190411}, {'ion': 1320, 'force': [-0.42284056544303894, -0.09886391460895538, -6.389946937561035], 'magnitude': 6.404685020446777, 'distance': 7.199795246124268, 'cosine_with_motion': -0.4555500386801142, 'motion_component': -2.9176545042145263}, {'ion': 1403, 'force': [-0.2038983255624771, 0.007636277470737696, -2.3518807888031006], 'magnitude': 2.36071515083313, 'distance': 11.858977317810059, 'cosine_with_motion': -0.43135733794867037, 'motion_component': -1.0183118087160872}]}, 5232: {'frame': 5232, 'ionic_force': [-15.006769359111786, -7.3863255977630615, -12.328855037689209], 'ionic_force_magnitude': 20.778873862028732, 'motion_vector': [-2.0798912048339844, 0.45478057861328125, 1.3255767822265625], 'cosine_ionic_motion': 0.2208754185682539, 'ionic_motion_component': 4.589542461652547, 'ionic_force_x': -15.006769359111786, 'ionic_force_y': -7.3863255977630615, 'ionic_force_z': -12.328855037689209, 'radial_force': 16.726055495356526, 'axial_force': -12.328855037689209, 'contributions': [{'ion': 1308, 'force': [-10.581357955932617, -10.495577812194824, -2.068549871444702], 'magnitude': 15.04663372039795, 'distance': 4.6973114013671875, 'cosine_with_motion': 0.38405388094854503, 'motion_component': 5.778718101797736}, {'ion': 1320, 'force': [-3.4290311336517334, 2.5227065086364746, -7.157139778137207], 'magnitude': 8.327482223510742, 'distance': 6.31411075592041, 'cosine_with_motion': -0.057842646264237296, 'motion_component': -0.48168358166323344}, {'ion': 1403, 'force': [-0.9963802695274353, 0.5865457057952881, -3.1031653881073], 'magnitude': 3.3115622997283936, 'distance': 10.012731552124023, 'cosine_with_motion': -0.21364315361773834, 'motion_component': -0.7074926152914962}]}, 5233: {'frame': 5233, 'ionic_force': [-14.879006922245026, 1.6513826549053192, -8.93515632301569], 'ionic_force_magnitude': 17.434131185174234, 'motion_vector': [-1.1857566833496094, -2.693035125732422, 0.8188629150390625], 'cosine_ionic_motion': 0.11040390686238014, 'ionic_motion_component': 1.9247961955944932, 'ionic_force_x': -14.879006922245026, 'ionic_force_y': 1.6513826549053192, 'ionic_force_z': -8.93515632301569, 'radial_force': 14.970367786568824, 'axial_force': -8.93515632301569, 'contributions': [{'ion': 1308, 'force': [-8.045933723449707, -1.5553702116012573, 0.07402922958135605], 'magnitude': 8.19522476196289, 'distance': 6.364856243133545, 'cosine_with_motion': 0.5509090435760458, 'motion_component': 4.514823348282454}, {'ion': 1320, 'force': [-4.9024658203125, 2.3702609539031982, -4.955585479736328], 'magnitude': 7.362753391265869, 'distance': 6.715044975280762, 'cosine_with_motion': -0.20579584488781474, 'motion_component': -1.5152240276781868}, {'ion': 1403, 'force': [-1.4236538410186768, 0.6275284290313721, -2.5825090408325195], 'magnitude': 3.0149519443511963, 'distance': 10.493704795837402, 'cosine_with_motion': -0.22984487928672453, 'motion_component': -0.6929712621797393}, {'ion': 1469, 'force': [-0.5069535374641418, 0.20896348357200623, -1.4710910320281982], 'magnitude': 1.569960594177246, 'distance': 14.542016983032227, 'cosine_with_motion': -0.24321109813377306, 'motion_component': -0.3818318543778467}]}, 5234: {'frame': 5234, 'ionic_force': [-12.36766916513443, -6.169648960232735, -5.632678389549255], 'ionic_force_magnitude': 14.924840860485348, 'motion_vector': [-0.7371978759765625, 0.9959373474121094, -1.500885009765625], 'cosine_ionic_motion': 0.39337879102866113, 'ionic_motion_component': 5.8711158539928885, 'ionic_force_x': -12.36766916513443, 'ionic_force_y': -6.169648960232735, 'ionic_force_z': -5.632678389549255, 'radial_force': 13.82113630895513, 'axial_force': -5.632678389549255, 'contributions': [{'ion': 1308, 'force': [-4.263079643249512, -5.226989269256592, 1.3957465887069702], 'magnitude': 6.887914657592773, 'distance': 6.942647933959961, 'cosine_with_motion': -0.3101546325173943, 'motion_component': -2.1363187537023762}, {'ion': 1320, 'force': [-5.668378829956055, -0.6114987134933472, -3.2219982147216797], 'magnitude': 6.54871940612793, 'distance': 7.12017822265625, 'cosine_with_motion': 0.6594842117417947, 'motion_component': 4.318776847613336}, {'ion': 1403, 'force': [-1.7518445253372192, -0.24626709520816803, -2.2820186614990234], 'magnitude': 2.8874237537384033, 'distance': 10.72293758392334, 'cosine_with_motion': 0.7956310726232749, 'motion_component': 2.2973240529196257}, {'ion': 1469, 'force': [-0.6843661665916443, -0.08489388227462769, -1.5244081020355225], 'magnitude': 1.6731359958648682, 'distance': 14.086509704589844, 'cosine_with_motion': 0.8315723490625314, 'motion_component': 1.3913336358783646}]}, 5235: {'frame': 5235, 'ionic_force': [-9.108755230903625, -5.003531493246555, -4.880807518959045], 'ionic_force_magnitude': 11.481595328940635, 'motion_vector': [0.478057861328125, 0.5345573425292969, -0.0841217041015625], 'cosine_ionic_motion': -0.7983481136190297, 'ionic_motion_component': -9.166309972196819, 'ionic_force_x': -9.108755230903625, 'ionic_force_y': -5.003531493246555, 'ionic_force_z': -4.880807518959045, 'radial_force': 10.39253334179998, 'axial_force': -4.880807518959045, 'contributions': [{'ion': 1308, 'force': [-4.102746486663818, -5.535513401031494, -1.0437307357788086], 'magnitude': 6.968774318695068, 'distance': 6.902252674102783, 'cosine_with_motion': -0.960400735912664, 'motion_component': -6.692815687143749}, {'ion': 1320, 'force': [-3.311994791030884, 0.44610047340393066, -1.7596060037612915], 'magnitude': 3.776841163635254, 'distance': 9.375720977783203, 'cosine_with_motion': -0.4388687590021384, 'motion_component': -1.6575375503540872}, {'ion': 1403, 'force': [-1.6940139532089233, 0.08588143438100815, -2.0774707794189453], 'magnitude': 2.681966543197632, 'distance': 11.12608528137207, 'cosine_with_motion': -0.30423817852102863, 'motion_component': -0.8159565702947376}]}, 5236: {'frame': 5236, 'ionic_force': [-8.572914719581604, -3.368498131632805, -3.489031046628952], 'ionic_force_magnitude': 9.849618474660495, 'motion_vector': [-1.1881294250488281, -1.5159759521484375, -0.36592864990234375], 'cosine_ionic_motion': 0.8580266738193267, 'ionic_motion_component': 8.451235378202336, 'ionic_force_x': -8.572914719581604, 'ionic_force_y': -3.368498131632805, 'ionic_force_z': -3.489031046628952, 'radial_force': 9.210952526858046, 'axial_force': -3.489031046628952, 'contributions': [{'ion': 1308, 'force': [-4.18311882019043, -3.761627435684204, -0.9836950898170471], 'magnitude': 5.711040496826172, 'distance': 7.6245012283325195, 'cosine_with_motion': 0.9853378826804866, 'motion_component': 5.62730424929216}, {'ion': 1320, 'force': [-2.6477365493774414, 0.20306988060474396, -0.23778191208839417], 'magnitude': 2.6661369800567627, 'distance': 11.159065246582031, 'cosine_with_motion': 0.5595886122897646, 'motion_component': 1.4919398983652878}, {'ion': 1403, 'force': [-1.742059350013733, 0.19005942344665527, -2.2675540447235107], 'magnitude': 2.8657801151275635, 'distance': 10.763354301452637, 'cosine_with_motion': 0.4647919112995481, 'motion_component': 1.3319913392970584}]}, 5237: {'frame': 5237, 'ionic_force': [-6.391249179840088, -5.777417056262493, -3.9080119132995605], 'ionic_force_magnitude': 9.460400151964539, 'motion_vector': [0.7070693969726562, -0.0630950927734375, -0.1740264</t>
+          <t>{5213: {'frame': 5213, 'ionic_force': [9.059208557009697, 6.910908341407776, -17.690110206604004], 'ionic_force_magnitude': 21.042098586037763, 'motion_vector': [-0.08104324340820312, -3.535572052001953, 0.40856170654296875], 'cosine_ionic_motion': -0.43245966970827554, 'ionic_motion_component': -9.099859004486863, 'ionic_force_x': 9.059208557009697, 'ionic_force_y': 6.910908341407776, 'ionic_force_z': -17.690110206604004, 'radial_force': 11.394293035670852, 'axial_force': -17.690110206604004, 'before_closest_residue': None, 'closest_residue': 130, 'next_closest_residue': 780, 'contributions': [{'ion': 1308, 'force': [4.778199672698975, 9.435524940490723, -10.170702934265137], 'magnitude': 14.673224449157715, 'distance': 4.756705284118652, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 423, 'cosine_with_motion': -0.7255885946159099, 'motion_component': -10.646724441459995}, {'ion': 1320, 'force': [4.232130527496338, -3.0712902545928955, -4.9525957107543945], 'magnitude': 7.202219009399414, 'distance': 6.789470195770264, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.33121377374106037, 'motion_component': 2.3854740970482444}, {'ion': 1403, 'force': [0.04887835681438446, 0.5466736555099487, -2.5668115615844727], 'magnitude': 2.624835729598999, 'distance': 11.246515274047852, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.31949001303026325, 'motion_component': -0.8386088114752297}]}, 5214: {'frame': 5214, 'ionic_force': [0.876273438334465, -7.065377295017242, -7.964790105819702], 'ionic_force_magnitude': 10.682944017893153, 'motion_vector': [-2.800647735595703, -0.17963790893554688, 2.6386032104492188], 'cosine_ionic_motion': -0.5394970021714701, 'ionic_motion_component': -5.763416272018996, 'ionic_force_x': 0.876273438334465, 'ionic_force_y': -7.065377295017242, 'ionic_force_z': -7.964790105819702, 'radial_force': 7.119509214803761, 'axial_force': -7.964790105819702, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 1105, 'contributions': [{'ion': 1308, 'force': [-1.3250770568847656, -3.1238503456115723, -2.5353305339813232], 'magnitude': 4.2358198165893555, 'distance': 8.85319995880127, 'before_closest_residue': 1105, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.14816259756217112, 'motion_component': -0.6275900945759094}, {'ion': 1320, 'force': [2.0835518836975098, -3.640300989151001, -2.173349618911743], 'magnitude': 4.724026679992676, 'distance': 8.383258819580078, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.5998743875613214, 'motion_component': -2.8338226264943356}, {'ion': 1403, 'force': [0.11779861152172089, -0.3012259602546692, -3.2561099529266357], 'magnitude': 3.272134780883789, 'distance': 10.072875022888184, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7035172793829035, 'motion_component': -2.302003315099296}]}, 5215: {'frame': 5215, 'ionic_force': [-3.1574587523937225, -9.676621198654175, -7.118128061294556], 'ionic_force_magnitude': 12.42072021632804, 'motion_vector': [0.9844284057617188, -0.2884941101074219, -5.571617126464844], 'cosine_ionic_motion': 0.5591117071431897, 'ionic_motion_component': 6.944570084099098, 'ionic_force_x': -3.1574587523937225, 'ionic_force_y': -9.676621198654175, 'ionic_force_z': -7.118128061294556, 'radial_force': 10.178729959838362, 'axial_force': -7.118128061294556, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1308, 'force': [-2.1365599632263184, -3.032615900039673, -0.8023586273193359], 'magnitude': 3.7954483032226562, 'distance': 9.352710723876953, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.15077678582865442, 'motion_component': 0.5722654804066467}, {'ion': 1320, 'force': [0.5601136684417725, -6.005922317504883, -0.8906189203262329], 'magnitude': 6.097379207611084, 'distance': 7.378998756408691, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.20977316123691703, 'motion_component': 1.2790664955624322}, {'ion': 1403, 'force': [-1.2336101531982422, -0.5227363109588623, -3.747150182723999], 'magnitude': 3.9794700145721436, 'distance': 9.133903503417969, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8788779690915066, 'motion_component': 3.4974685416808162}, {'ion': 1469, 'force': [-0.34740230441093445, -0.11534667015075684, -1.6780003309249878], 'magnitude': 1.7174626588821411, 'distance': 13.903539657592773, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9291435751757805, 'motion_component': 1.5957694874407418}]}, 5216: {'frame': 5216, 'ionic_force': [0.3360389769077301, -3.4986054599285126, -5.366488456726074], 'ionic_force_magnitude': 6.415010577888161, 'motion_vector': [0.49591064453125, 1.3578147888183594, -0.21898651123046875], 'cosine_ionic_motion': -0.3634329471769188, 'ionic_motion_component': -2.3314262004930035, 'ionic_force_x': 0.3360389769077301, 'ionic_force_y': -3.4986054599285126, 'ionic_force_z': -5.366488456726074, 'radial_force': 3.51470658209797, 'axial_force': -5.366488456726074, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.5920225381851196, -1.5384231805801392, -1.2295265197753906], 'magnitude': 2.0564465522766113, 'distance': 12.706043243408203, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.7028663925785696, 'motion_component': -1.4454071028631574}, {'ion': 1320, 'force': [1.186414122581482, -1.7023833990097046, -2.2223496437072754], 'magnitude': 3.0404810905456543, 'distance': 10.449557304382324, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.2781600982653527, 'motion_component': -0.8457405365038682}, {'ion': 1403, 'force': [-0.2583526074886322, -0.2577988803386688, -1.9146122932434082], 'magnitude': 1.9490886926651, 'distance': 13.051283836364746, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.020665348923662074, 'motion_component': -0.04027859703741399}]}, 5217: {'frame': 5217, 'ionic_force': [-0.5696889609098434, -2.4908271618187428, -6.695563793182373], 'ionic_force_magnitude': 7.166543097673472, 'motion_vector': [1.0223388671875, -0.4985237121582031, 2.0433120727539062], 'cosine_ionic_motion': -0.7769881557830077, 'ionic_motion_component': -5.5683191048007545, 'ionic_force_x': -0.5696889609098434, 'ionic_force_y': -2.4908271618187428, 'ionic_force_z': -6.695563793182373, 'radial_force': 2.555144900438437, 'axial_force': -6.695563793182373, 'before_closest_residue': 1105, 'closest_residue': 130, 'next_closest_residue': 780, 'contributions': [{'ion': 1308, 'force': [-1.6062496900558472, -1.6342322826385498, -2.415165901184082], 'magnitude': 3.329231023788452, 'distance': 9.986126899719238, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.7401330330015188, 'motion_component': -2.4640738930936728}, {'ion': 1320, 'force': [1.2217909097671509, -0.8660487532615662, -2.349320888519287], 'magnitude': 2.7860584259033203, 'distance': 10.916261672973633, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 1105, 'cosine_with_motion': -0.47880292106144073, 'motion_component': -1.333972960252149}, {'ion': 1403, 'force': [-0.18523018062114716, 0.009453874081373215, -1.931077003479004], 'magnitude': 1.939963459968567, 'distance': 13.08194351196289, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.912528632425414, 'motion_component': -1.7702721473163905}]}, 5218: {'frame': 5218, 'ionic_force': [4.206250421702862, -4.269712045788765, -7.6996800899505615], 'ionic_force_magnitude': 9.757461609025693, 'motion_vector': [-0.7376747131347656, 0.12036895751953125, 5.263938903808594], 'cosine_ionic_motion': -0.8509877619478586, 'ionic_motion_component': -8.303480416956926, 'ionic_force_x': 4.206250421702862, 'ionic_force_y': -4.269712045788765, 'ionic_force_z': -7.6996800899505615, 'radial_force': 5.993578527393228, 'axial_force': -7.6996800899505615, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1308, 'force': [-1.0178943872451782, -2.646784543991089, -2.161548376083374], 'magnitude': 3.5656511783599854, 'distance': 9.649384498596191, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.5773913926795388, 'motion_component': -2.0587763371135157}, {'ion': 1320, 'force': [5.3220672607421875, -1.4583486318588257, -2.8955790996551514], 'magnitude': 6.231818199157715, 'distance': 7.298971652984619, 'before_closest_residue': 98, 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': -0.5838190835985204, 'motion_component': -3.6382544330410886}, {'ion': 1403, 'force': [-0.09792245179414749, -0.1645788699388504, -2.642552614212036], 'magnitude': 2.6494827270507812, 'distance': 11.194082260131836, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9837579542078188, 'motion_component': -2.606449820321628}]}, 5219: {'frame': 5219, 'ionic_force': [-0.8370766043663025, 7.505206935107708, 4.665254652500153], 'ionic_force_magnitude': 8.876566304210236, 'motion_vector': [-1.3892173767089844, -0.5494041442871094, 1.6649017333984375], 'cosine_ionic_motion': 0.24207837425350287, 'ionic_motion_component': 2.1488247398766385, 'ionic_force_x': -0.8370766043663025, 'ionic_force_y': 7.505206935107708, 'ionic_force_z': 4.665254652500153, 'radial_force': 7.551743400061091, 'axial_force': 4.665254652500153, 'before_closest_residue': 780, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1308, 'force': [-1.2311298847198486, -4.110632419586182, -0.6271311640739441], 'magnitude': 4.336619853973389, 'distance': 8.749703407287598, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.30148794664863837, 'motion_component': 1.3074386645678937}, {'ion': 1320, 'force': [1.5758368968963623, 11.999844551086426, 15.897293090820312], 'magnitude': 19.98007583618164, 'distance': 4.076340675354004, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 130, 'cosine_with_motion': 0.3957087251708299, 'motion_component': 7.906290618905373}, {'ion': 1403, 'force': [-1.0520174503326416, -0.32890668511390686, -8.382981300354004], 'magnitude': 8.455134391784668, 'distance': 6.266265392303467, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6511147850343424, 'motion_component': -5.505262943493138}, {'ion': 1469, 'force': [-0.12976616621017456, -0.0550985112786293, -2.221925973892212], 'magnitude': 2.226393938064575, 'distance': 12.211472511291504, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7005236558494705, 'motion_component': -1.5596416475744035}]}, 5220: {'frame': 5220, 'ionic_force': [-7.989065766334534, -10.187750428915024, -5.366817504167557], 'ionic_force_magnitude': 14.01492635527265, 'motion_vector': [-0.5346794128417969, -1.1390304565429688, -0.756134033203125], 'cosine_ionic_motion': 0.9688891272673253, 'ionic_motion_component': 13.578909765075954, 'ionic_force_x': -7.989065766334534, 'ionic_force_y': -10.187750428915024, 'ionic_force_z': -5.366817504167557, 'radial_force': 12.946637811442654, 'axial_force': -5.366817504167557, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 1073, 'contributions': [{'ion': 1308, 'force': [-1.290416955947876, -3.383082866668701, 0.44074055552482605], 'magnitude': 3.6475577354431152, 'distance': 9.540430068969727, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.7862651912087649, 'motion_component': 2.867947724152115}, {'ion': 1320, 'force': [-1.2900820970535278, -3.8637619018554688, 8.199496269226074], 'magnitude': 9.155583381652832, 'distance': 6.021795749664307, 'before_closest_residue': 780, 'closest_residue': 130, 'next_closest_residue': 780, 'cosine_with_motion': -0.0825272300641764, 'motion_component': -0.7555849354875583}, {'ion': 1403, 'force': [-4.87747859954834, -2.6918888092041016, -11.338939666748047], 'magnitude': 12.633590698242188, 'distance': 5.126319408416748, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7682381903521565, 'motion_component': 9.705606906917723}, {'ion': 1469, 'force': [-0.53108811378479, -0.24901685118675232, -2.66811466217041], 'magnitude': 2.7318308353424072, 'distance': 11.02407455444336, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6446005870361542, 'motion_component': 1.7609397736349202}]}, 5221: {'frame': 5221, 'ionic_force': [-10.496177196502686, -8.205937772989273, 0.1122767822816968], 'ionic_force_magnitude': 13.32365402396785, 'motion_vector': [0.09583663940429688, 4.582389831542969, -4.5017547607421875], 'cosine_ionic_motion': -0.4569579844587636, 'ionic_motion_component': -6.0883500884182435, 'ionic_force_x': -10.496177196502686, 'ionic_force_y': -8.205937772989273, 'ionic_force_z': 0.1122767822816968, 'radial_force': 13.32318094429987, 'axial_force': 0.1122767822816968, 'before_closest_residue': 'SF', 'closest_residue': 1073, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-0.9717339277267456, -2.528850793838501, 0.010465134866535664], 'magnitude': 2.709144353866577, 'distance': 11.070137023925781, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.6738649628328864, 'motion_component': -1.825597403703803}, {'ion': 1320, 'force': [-6.512366771697998, -3.0620293617248535, 8.233292579650879], 'magnitude': 10.934991836547852, 'distance': 5.510104179382324, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.7362136948005549, 'motion_component': -8.050490911518978}, {'ion': 1403, 'force': [-2.5566587448120117, -2.16740083694458, -6.0023908615112305], 'magnitude': 6.874796390533447, 'distance': 6.9492692947387695, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3813827954446882, 'motion_component': 2.6219290923979797}, {'ion': 1469, 'force': [-0.4554177522659302, -0.4476567804813385, -2.1290900707244873], 'magnitude': 2.22279691696167, 'distance': 12.221348762512207, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5244785240319814, 'motion_component': 1.1658092836760383}]}, 5222: {'frame': 5222, 'ionic_force': [-10.679179668426514, 1.4521918892860413, -9.871692180633545], 'ionic_force_magnitude': 14.615199149618997, 'motion_vector': [-3.9730682373046875, -1.5599021911621094, 2.0731430053710938], 'cosine_ionic_motion': 0.2840376600251383, 'ionic_motion_component': 4.151266967259171, 'ionic_force_x': -10.679179668426514, 'ionic_force_y': 1.4521918892860413, 'ionic_force_z': -9.871692180633545, 'radial_force': 10.777464436213297, 'axial_force': -9.871692180633545, 'before_closest_residue': 1073, 'closest_residue': 130, 'next_closest_residue': 1105, 'contributions': [{'ion': 1308, 'force': [-2.3145053386688232, -2.909573793411255, -2.4544501304626465], 'magnitude': 4.454983711242676, 'distance': 8.632686614990234, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.4089915671206331, 'motion_component': 1.822050778624856}, {'ion': 1320, 'force': [-7.233617305755615, 3.4570906162261963, -3.964205026626587], 'magnitude': 8.943802833557129, 'distance': 6.0926737785339355, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.356471846835402, 'motion_component': 3.1882140577431386}, {'ion': 1403, 'force': [-1.1310570240020752, 0.9046750664710999, -3.4530370235443115], 'magnitude': 3.74448823928833, 'distance': 9.4161376953125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.22940328619630437, 'motion_component': -0.8589978912641101}]}, 5223: {'frame': 5223, 'ionic_force': [-9.0616614818573, -0.7365338355302811, -3.7814049124717712], 'ionic_force_magnitude': 9.846583875371337, 'motion_vector': [1.1881523132324219, 0.9744796752929688, 2.5615386962890625], 'cosine_ionic_motion': -0.7197750582208821, 'ionic_motion_component': -7.0873254821722025, 'ionic_force_x': -9.0616614818573, 'ionic_force_y': -0.7365338355302811, 'ionic_force_z': -3.7814049124717712, 'radial_force': 9.09154502285817, 'axial_force': -3.7814049124717712, 'before_closest_residue': 130, 'closest_residue': 1105, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-2.0935752391815186, -1.8744561672210693, -0.5705388188362122], 'magnitude': 2.8674304485321045, 'distance': 10.760255813598633, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.6742965102789934, 'motion_component': -1.933498388602409}, {'ion': 1320, 'force': [-4.028995990753174, 0.7997772693634033, 0.7936450242996216], 'magnitude': 4.183578014373779, 'distance': 8.908306121826172, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': -0.15801994549859863, 'motion_component': -0.6610887659741991}, {'ion': 1403, 'force': [-2.2542738914489746, 0.2554945647716522, -2.6964259147644043], 'magnitude': 3.523881435394287, 'distance': 9.706404685974121, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.886971707792664, 'motion_component': -3.125583209489937}, {'ion': 1469, 'force': [-0.6848163604736328, 0.08265049755573273, -1.3080852031707764], 'magnitude': 1.4788141250610352, 'distance': 14.983464241027832, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9244940953963866, 'motion_component': -1.367155000136628}]}, 5224: {'frame': 5224, 'ionic_force': [-11.852895140647888, 1.5224820375442505, -2.5712924543768167], 'ionic_force_magnitude': 12.223772725953896, 'motion_vector': [0.0398406982421875, 2.6087303161621094, -0.5442276000976562], 'cosine_ionic_motion': 0.1503708447138321, 'ionic_motion_component': 1.8380990303915896, 'ionic_force_x': -11.852895140647888, 'ionic_force_y': 1.5224820375442505, 'ionic_force_z': -2.5712924543768167, 'radial_force': 11.950275091806015, 'axial_force': -2.5712924543768167, 'before_closest_residue': 1105, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-3.0808727741241455, -2.469778537750244, 0.02193385921418667], 'magnitude': 3.948678731918335, 'distance': 9.16944694519043, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.6250168030414615, 'motion_component': -2.4679905922540377}, {'ion': 1320, 'force': [-3.7092082500457764, 2.256039619445801, 2.863736867904663], 'magnitude': 5.2008585929870605, 'distance': 7.989719390869141, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 'SF', 'cosine_with_motion': 0.3014942239922375, 'motion_component': 1.5680288067766102}, {'ion': 1403, 'force': [-4.130849361419678, 1.4701601266860962, -3.665073871612549], 'magnitude': 5.714722633361816, 'distance': 7.622044086456299, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3719633106605391, 'motion_component': 2.125667116136732}, {'ion': 1469, 'force': [-0.9319647550582886, 0.26606082916259766, -1.7918893098831177], 'magnitude': 2.0372073650360107, 'distance': 12.765899658203125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3006044973620889, 'motion_component': 0.6123937048573254}]}, 5225: {'frame': 5225, 'ionic_force': [-12.727189838886261, 4.494718790054321, -5.815616488456726], 'ionic_force_magnitude': 14.697117177784452, 'motion_vector': [1.9323806762695312, 0.8050422668457031, -0.5858154296875], 'cosine_ionic_motion': -0.5498999726922859, 'ionic_motion_component': -8.081944334718996, 'ionic_force_x': -12.727189838886261, 'ionic_force_y': 4.494718790054321, 'ionic_force_z': -5.815616488456726, 'radial_force': 13.49755008128205, 'axial_force': -5.815616488456726, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-5.498988151550293, -1.1754382848739624, 0.6942658424377441], 'magnitude': 5.665909767150879, 'distance': 7.654806613922119, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.9726077449400174, 'motion_component': -5.510707500471813}, {'ion': 1320, 'force': [-4.546165466308594, 3.720468282699585, -2.5248541831970215], 'magnitude': 6.394090175628662, 'distance': 7.2057576179504395, 'before_closest_residue': 780, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.3101345317109207, 'motion_component': -1.983028263270576}, {'ion': 1403, 'force': [-2.0169267654418945, 1.4461729526519775, -2.5027101039886475], 'magnitude': 3.524623155593872, 'distance': 9.70538330078125, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.16538079293163058, 'motion_component': -0.5829049549384706}, {'ion': 1469, 'force': [-0.6651094555854797, 0.5035158395767212, -1.4823180437088013], 'magnitude': 1.7009308338165283, 'distance': 13.970943450927734, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.0031178895486980596, 'motion_component': -0.005303314350566524}]}, 5226: {'frame': 5226, 'ionic_force': [-8.63455793261528, 10.306835412979126, -8.068451166152954], 'ionic_force_magnitude': 15.680763729567671, 'motion_vector': [-0.0262298583984375, 0.5780372619628906, 0.1553192138671875], 'cosine_ionic_motion': 0.5248802706088915, 'ionic_motion_component': 8.23052350972957, 'ionic_force_x': -8.63455793261528, 'ionic_force_y': 10.306835412979126, 'ionic_force_z': -8.068451166152954, 'radial_force': 13.445685067036564, 'axial_force': -8.068451166152954, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-3.372286558151245, 1.1184394359588623, 0.5709807872772217], 'magnitude': 3.5985054969787598, 'distance': 9.605234146118164, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': 0.382035810311084, 'motion_component': 1.374757997942818}, {'ion': 1320, 'force': [-3.445181369781494, 6.423120021820068, -3.7658469676971436], 'magnitude': 8.204105377197266, 'distance': 6.361410617828369, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': 0.6547561796468672, 'motion_component': 5.371688847001148}, {'ion': 1403, 'force': [-1.4268732070922852, 2.1184980869293213, -3.1947760581970215], 'magnitude': 4.090305328369141, 'distance': 9.009303092956543, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.31249432221731166, 'motion_component': 1.278197102482256}, {'ion': 1469, 'force': [-0.39021679759025574, 0.646777868270874, -1.6788089275360107], 'magnitude': 1.8409210443496704, 'distance': 13.429241180419922, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.11183524775394986, 'motion_component': 0.20587985755624938}]}, 5227: {'frame': 5227, 'ionic_force': [-7.94691988825798, 10.216525435447693, -6.894068896770477], 'ionic_force_magnitude': 14.66489391836702, 'motion_vector': [-1.3651809692382812, -0.9860496520996094, 0.14288330078125], 'cosine_ionic_motion': -0.008475451243119256, 'ionic_motion_component': -0.12429159339063578, 'ionic_force_x': -7.94691988825798, 'ionic_force_y': 10.216525435447693, 'ionic_force_z': -6.894068896770477, 'radial_force': 12.94337389105097, 'axial_force': -6.894068896770477, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-3.113513946533203, 1.471713900566101, 0.5079912543296814], 'magnitude': 3.4810869693756104, 'distance': 9.765885353088379, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': 0.4881399211648226, 'motion_component': 1.6992574855999774}, {'ion': 1320, 'force': [-3.006080389022827, 5.83809232711792, -2.921882152557373], 'magnitude': 7.1872968673706055, 'distance': 6.796514511108398, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.17043338293533036, 'motion_component': -1.2249553237593886}, {'ion': 1403, 'force': [-1.393346905708313, 2.2208824157714844, -2.820758104324341], 'magnitude': 3.851027250289917, 'distance': 9.284975051879883, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.10613156239445612, 'motion_component': -0.40871553483142975}, {'ion': 1469, 'force': [-0.4339786469936371, 0.6858367919921875, -1.6594198942184448], 'magnitude': 1.8472638130187988, 'distance': 13.40616512298584, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.10278906205083915, 'motion_component': -0.1898785247648629}]}, 5228: {'frame': 5228, 'ionic_force': [-9.87448799610138, 7.389701664447784, -6.990283265709877], 'ionic_force_magnitude': 14.176645019522642, 'motion_vector': [0.7691383361816406, -0.3768424987792969, -0.10305023193359375], 'cosine_ionic_motion': -0.789812787166785, 'ionic_motion_component': -11.1968955155433, 'ionic_force_x': -9.87448799610138, 'ionic_force_y': 7.389701664447784, 'ionic_force_z': -6.990283265709877, 'radial_force': 12.333418174808337, 'axial_force': -6.990283265709877, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1308, 'force': [-2.4451513290405273, 0.9452031254768372, 0.08026061952114105], 'magnitude': 2.622711658477783, 'distance': 11.251069068908691, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.9923019662020579, 'motion_component': -2.6025218019028573}, {'ion': 1320, 'force': [-5.125226974487305, 4.3977861404418945, -2.9678163528442383], 'magnitude': 7.3767476081848145, 'distance': 6.708672046661377, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.8318170866945936, 'motion_component': -6.136104879864973}, {'ion': 1403, 'force': [-1.7134193181991577, 1.530916690826416, -2.4926624298095703], 'magnitude': 3.3901147842407227, 'distance': 9.896049499511719, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.560051014426819, 'motion_component': -1.8986371754413724}, {'ion': 1469, 'force': [-0.5906903743743896, 0.5157957077026367, -1.6100651025772095], 'magnitude': 1.790885329246521, 'distance': 13.615549087524414, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3124889054191626, 'motion_component': -0.5596317703114053}]}, 5229: {'frame': 5229, 'ionic_force': [-9.413652211427689, 7.915450572967529, -7.1453061401844025], 'ionic_force_magnitude': 14.224155706676102, 'motion_vector': [-2.0034332275390625, -4.632930755615234, 0.2904510498046875], 'cosine_ionic_motion': -0.2765377108802912, 'ionic_motion_component': -3.9335154583290404, 'ionic_force_x': -9.413652211427689, 'ionic_force_y': 7.915450572967529, 'ionic_force_z': -7.1453061401844025, 'radial_force': 12.299235981588833, 'axial_force': -7.1453061401844025, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 1105, 'contributions': [{'ion': 1308, 'force': [-3.0030407905578613, 0.9390349388122559, 0.19887909293174744], 'magnitude': 3.152712106704712, 'distance': 10.261878967285156, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': 0.10813634399926765, 'motion_component': 0.3409227587045228}, {'ion': 1320, 'force': [-4.218984603881836, 4.771722316741943, -2.8418822288513184], 'magnitude': 6.974629878997803, 'distance': 6.899354457855225, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.41062905962600516, 'motion_component': -2.8639856380834434}, {'ion': 1403, 'force': [-1.7074979543685913, 1.6937834024429321, -2.7924537658691406], 'magnitude': 3.685410261154175, 'distance': 9.49130916595459, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.28108048830992605, 'motion_component': -1.0358969432865663}, {'ion': 1469, 'force': [-0.4841288626194, 0.510909914970398, -1.709849238395691], 'magnitude': 1.8490521907806396, 'distance': 13.399681091308594, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.20256639275756702, 'motion_component': -0.37455583836772854}]}, 5230: {'frame': 5230, 'ionic_force': [-13.472239375114441, -2.136018753051758, -5.8683589696884155], 'ionic_force_magnitude': 14.849291124188225, 'motion_vector': [5.115959167480469, 0.8695487976074219, -4.300270080566406], 'cosine_ionic_motion': -0.4551001034999545, 'ionic_motion_component': -6.7579139275190165, 'ionic_force_x': -13.472239375114441, 'ionic_force_y': -2.136018753051758, 'ionic_force_z': -5.8683589696884155, 'radial_force': 13.64052088058857, 'axial_force': -5.8683589696884155, 'before_closest_residue': 98, 'closest_residue': 1105, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-3.4431419372558594, -1.4593416452407837, 1.5944634675979614], 'magnitude': 4.065368175506592, 'distance': 9.03689193725586, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.9394801019205968, 'motion_component': -3.819332482993259}, {'ion': 1320, 'force': [-6.761546611785889, -0.46857988834381104, -2.9621737003326416], 'magnitude': 7.396793365478516, 'distance': 6.699575424194336, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'cosine_with_motion': -0.44655252950108015, 'motion_component': -3.3030568067030313}, {'ion': 1403, 'force': [-2.4797613620758057, -0.12971417605876923, -2.8303792476654053], 'magnitude': 3.7652475833892822, 'distance': 9.390144348144531, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.024738096463148694, 'motion_component': -0.0931450562886138}, {'ion': 1469, 'force': [-0.7877894639968872, -0.07838304340839386, -1.67026948928833], 'magnitude': 1.8483929634094238, 'distance': 13.402070045471191, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2475774303234592, 'motion_component': 0.4576203640856893}]}, 5231: {'frame': 5231, 'ionic_force': [-4.702645644545555, -10.708216772880405, -12.202762365341187], 'ionic_force_magnitude': 16.902313210272368, 'motion_vector': [-1.9342155456542969, 1.1726150512695312, 1.3013763427734375], 'cosine_ionic_motion': -0.43849772857207303, 'ionic_motion_component': -7.411625950318177, 'ionic_force_x': -4.702645644545555, 'ionic_force_y': -10.708216772880405, 'ionic_force_z': -12.202762365341187, 'radial_force': 11.695331654688571, 'axial_force': -12.202762365341187, 'before_closest_residue': 1105, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1308, 'force': [-4.075906753540039, -10.616989135742188, -3.460934638977051], 'magnitude': 11.887453079223633, 'distance': 5.284752368927002, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_mot</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{5293: {'frame': 5293, 'ionic_force': [-4.439165145158768, -11.485485851764679, -5.509422957897186], 'ionic_force_magnitude': 13.489859664432528, 'motion_vector': [3.6029815673828125, -0.9414405822753906, -2.305633544921875], 'cosine_ionic_motion': 0.12729862041329584, 'ionic_motion_component': 1.7172405248512268, 'ionic_force_x': -4.439165145158768, 'ionic_force_y': -11.485485851764679, 'ionic_force_z': -5.509422957897186, 'radial_force': 12.31351178328421, 'axial_force': -5.509422957897186, 'contributions': [{'ion': 1309, 'force': [-0.4600997269153595, -6.4237165451049805, -1.8560487031936646], 'magnitude': 6.702293872833252, 'distance': 7.038130283355713, 'cosine_with_motion': 0.2953168585098998, 'motion_component': 1.9793003634343174}, {'ion': 1320, 'force': [-2.2913060188293457, -4.553028583526611, 0.9146720767021179], 'magnitude': 5.178492069244385, 'distance': 8.00695514678955, 'cosine_with_motion': -0.26797402199208176, 'motion_component': -1.387701281697467}, {'ion': 1469, 'force': [-1.280375599861145, -0.43071743845939636, -2.963862419128418], 'magnitude': 3.2572009563446045, 'distance': 10.095939636230469, 'cosine_with_motion': 0.18406364306654752, 'motion_component': 0.5995323182463634}, {'ion': 2436, 'force': [-0.4073837995529175, -0.0780232846736908, -1.6041839122772217], 'magnitude': 1.656941533088684, 'distance': 14.155181884765625, 'cosine_with_motion': 0.3175182671968274, 'motion_component': 0.5261092018864266}]}, 5294: {'frame': 5294, 'ionic_force': [0.1658477745950222, -6.8131378293037415, -5.872682213783264], 'ionic_force_magnitude': 8.99637421128724, 'motion_vector': [-1.1986160278320312, 0.10608673095703125, 0.8895950317382812], 'cosine_ionic_motion': -0.4565192458823854, 'ionic_motion_component': -4.10701797061259, 'ionic_force_x': 0.1658477745950222, 'ionic_force_y': -6.8131378293037415, 'ionic_force_z': -5.872682213783264, 'radial_force': 6.815156092521126, 'axial_force': -5.872682213783264, 'contributions': [{'ion': 1309, 'force': [1.4283074140548706, -3.2946081161499023, -1.909952163696289], 'magnitude': 4.067237377166748, 'distance': 9.034814834594727, 'cosine_with_motion': -0.6178726576783165, 'motion_component': -2.5130349266499294}, {'ion': 1320, 'force': [-1.2332184314727783, -2.8408944606781006, -1.2032557725906372], 'magnitude': 3.3225491046905518, 'distance': 9.996163368225098, 'cosine_with_motion': 0.021392684254919057, 'motion_component': 0.0710782469366329}, {'ion': 1469, 'force': [-0.029241207987070084, -0.6776352524757385, -2.759474277496338], 'magnitude': 2.841609239578247, 'distance': 10.809033393859863, 'cosine_with_motion': -0.585957106898025, 'motion_component': -1.665061108476534}]}, 5295: {'frame': 5295, 'ionic_force': [-0.8948521912097931, -8.003737807273865, -7.197145462036133], 'ionic_force_magnitude': 10.800901912961034, 'motion_vector': [1.4610366821289062, 0.4837226867675781, -0.33788299560546875], 'cosine_ionic_motion': -0.16142186763286107, 'ionic_motion_component': -1.7435017589095119, 'ionic_force_x': -0.8948521912097931, 'ionic_force_y': -8.003737807273865, 'ionic_force_z': -7.197145462036133, 'radial_force': 8.053606603981724, 'axial_force': -7.197145462036133, 'contributions': [{'ion': 1309, 'force': [1.2909294366836548, -4.2322163581848145, -2.066220760345459], 'magnitude': 4.883382320404053, 'distance': 8.245342254638672, 'cosine_with_motion': 0.06979078553032043, 'motion_component': 0.340815084300246}, {'ion': 1320, 'force': [-1.8195945024490356, -3.148383855819702, -1.8783209323883057], 'magnitude': 4.09283971786499, 'distance': 9.006513595581055, 'cosine_with_motion': -0.5499726823402922, 'motion_component': -2.2509498785102373}, {'ion': 1469, 'force': [-0.36618712544441223, -0.6231375932693481, -3.252603769302368], 'magnitude': 3.331940174102783, 'distance': 9.98206615447998, 'cosine_with_motion': 0.05001077294285725, 'motion_component': 0.16663289920801638}]}, 5296: {'frame': 5296, 'ionic_force': [0.31867482099914923, -8.267817586660385, -7.231484055519104], 'ionic_force_magnitude': 10.988754384963595, 'motion_vector': [-0.4652824401855469, 0.103912353515625, -2.422882080078125], 'cosine_ionic_motion': 0.6085736128030453, 'ionic_motion_component': 6.687465956262602, 'ionic_force_x': 0.31867482099914923, 'ionic_force_y': -8.267817586660385, 'ionic_force_z': -7.231484055519104, 'radial_force': 8.273956809642506, 'axial_force': -7.231484055519104, 'contributions': [{'ion': 1309, 'force': [2.060899019241333, -4.070521354675293, -2.4136157035827637], 'magnitude': 5.161587715148926, 'distance': 8.020055770874023, 'cosine_with_motion': 0.350394413188984, 'motion_component': 1.808591562717023}, {'ion': 1320, 'force': [-1.741642713546753, -3.7549068927764893, -1.5699185132980347], 'magnitude': 4.426882743835449, 'distance': 8.660042762756348, 'cosine_with_motion': 0.3863979687561965, 'motion_component': 1.7105384314382377}, {'ion': 1469, 'force': [-0.000581484695430845, -0.4423893392086029, -3.2479498386383057], 'magnitude': 3.2779393196105957, 'distance': 10.063952445983887, 'cosine_with_motion': 0.9665632598820196, 'motion_component': 3.1683358083492243}]}, 5297: {'frame': 5297, 'ionic_force': [2.0586469620466232, -4.025961697101593, -6.761675596237183], 'ionic_force_magnitude': 8.134288645580657, 'motion_vector': [0.11940383911132812, -0.8824501037597656, 1.4705276489257812], 'cosine_ionic_motion': -0.439411799823159, 'ionic_motion_component': -3.5743024140356825, 'ionic_force_x': 2.0586469620466232, 'ionic_force_y': -4.025961697101593, 'ionic_force_z': -6.761675596237183, 'radial_force': 4.521769001272945, 'axial_force': -6.761675596237183, 'contributions': [{'ion': 1309, 'force': [2.703697919845581, -1.9296005964279175, -3.2435293197631836], 'magnitude': 4.642609596252441, 'distance': 8.45644760131836, 'cosine_with_motion': -0.34381617958818117, 'motion_component': -1.5962042757614867}, {'ion': 1320, 'force': [-0.5463349223136902, -1.8209863901138306, -1.1804895401000977], 'magnitude': 2.2378625869750977, 'distance': 12.18014144897461, 'cosine_with_motion': -0.050490734426634716, 'motion_component': -0.1129913241681777}, {'ion': 1469, 'force': [-0.09871603548526764, -0.27537471055984497, -2.3376567363739014], 'magnitude': 2.3558895587921143, 'distance': 11.871116638183594, 'cosine_with_motion': -0.7916784499341073, 'motion_component': -1.8651069085584862}]}, 5298: {'frame': 5298, 'ionic_force': [2.64043165743351, -8.706450581550598, -7.226660072803497], 'ionic_force_magnitude': 11.618897403558226, 'motion_vector': [-0.8501853942871094, 0.7801551818847656, 2.5111923217773438], 'cosine_ionic_motion': -0.8466110490409935, 'ionic_motion_component': -9.836686919526105, 'ionic_force_x': 2.64043165743351, 'ionic_force_y': -8.706450581550598, 'ionic_force_z': -7.226660072803497, 'radial_force': 9.098030614729751, 'axial_force': -7.226660072803497, 'contributions': [{'ion': 1309, 'force': [3.2287416458129883, -6.1072096824646, -3.8306076526641846], 'magnitude': 7.899135589599609, 'distance': 6.483048439025879, 'cosine_with_motion': -0.7846489917489425, 'motion_component': -6.19804851018975}, {'ion': 1320, 'force': [-0.4978197515010834, -2.0856738090515137, -0.9577496647834778], 'magnitude': 2.3484344482421875, 'distance': 11.889945030212402, 'cosine_with_motion': -0.5560732892391631, 'motion_component': -1.3059016451634013}, {'ion': 1469, 'force': [-0.09049023687839508, -0.5135670900344849, -2.438302755355835], 'magnitude': 2.493443489074707, 'distance': 11.539029121398926, 'cosine_with_motion': -0.9355482454164143, 'motion_component': -2.3327365935457256}]}, 5299: {'frame': 5299, 'ionic_force': [8.148396573960781, -5.8599869310855865, -10.365723192691803], 'ionic_force_magnitude': 14.428583813615887, 'motion_vector': [-0.3539390563964844, 2.2585983276367188, 2.1390380859375], 'cosine_ionic_motion': -0.84767086277239, 'ionic_motion_component': -12.230690089871521, 'ionic_force_x': 8.148396573960781, 'ionic_force_y': -5.8599869310855865, 'ionic_force_z': -10.365723192691803, 'radial_force': 10.036723248103918, 'axial_force': -10.365723192691803, 'contributions': [{'ion': 1309, 'force': [9.771367073059082, -2.351778030395508, -4.5568013191223145], 'magnitude': 11.03516674041748, 'distance': 5.485037326812744, 'cosine_with_motion': -0.5359722734248957, 'motion_component': -5.914543591356164}, {'ion': 1320, 'force': [-1.1783761978149414, -2.824215888977051, -0.5681673884391785], 'magnitude': 3.11248779296875, 'distance': 10.32797622680664, 'cosine_with_motion': -0.7365107631581589, 'motion_component': -2.2923807326295993}, {'ion': 1469, 'force': [-0.3746396005153656, -0.5283625721931458, -3.711301326751709], 'magnitude': 3.767396926879883, 'distance': 9.387465476989746, 'cosine_with_motion': -0.7629798072189766, 'motion_component': -2.8744477578251457}, {'ion': 2436, 'force': [-0.06995470076799393, -0.1556304395198822, -1.529453158378601], 'magnitude': 1.5389416217803955, 'distance': 14.687841415405273, 'cosine_with_motion': -0.7468235204612907, 'motion_component': -1.1493178342881796}]}, 5300: {'frame': 5300, 'ionic_force': [11.58044770359993, 2.511912077665329, -5.298129674047232], 'ionic_force_magnitude': 12.98024072753482, 'motion_vector': [2.946308135986328, -2.5934295654296875, 0.6218948364257812], 'cosine_ionic_motion': 0.47126898983142484, 'ionic_motion_component': 6.117184935434054, 'ionic_force_x': 11.58044770359993, 'ionic_force_y': 2.511912077665329, 'ionic_force_z': -5.298129674047232, 'radial_force': 11.849745621815426, 'axial_force': -5.298129674047232, 'contributions': [{'ion': 1309, 'force': [15.33890438079834, 5.875173568725586, 3.291243076324463], 'magnitude': 16.752071380615234, 'distance': 4.451791286468506, 'cosine_with_motion': 0.48071337114347773, 'motion_component': 8.052945245231506}, {'ion': 1320, 'force': [-2.06095027923584, -3.7897627353668213, -0.05836188420653343], 'magnitude': 4.314304351806641, 'distance': 8.772303581237793, 'cosine_with_motion': 0.21696714822175778, 'motion_component': 0.9360623548549916}, {'ion': 1469, 'force': [-1.4913935661315918, 0.3887030780315399, -6.317618370056152], 'magnitude': 6.502894878387451, 'distance': 7.145220756530762, 'cosine_with_motion': -0.36106680502471306, 'motion_component': -2.347979613803373}, {'ion': 2436, 'force': [-0.2061128318309784, 0.037798166275024414, -2.213392496109009], 'magnitude': 2.223289728164673, 'distance': 12.21999454498291, 'cosine_with_motion': -0.23561603955225588, 'motion_component': -0.5238427378697725}]}, 5301: {'frame': 5301, 'ionic_force': [11.182874098420143, -8.029923260211945, -7.2750024273991585], 'ionic_force_magnitude': 15.571191379745887, 'motion_vector': [-1.3564949035644531, -1.4149208068847656, -1.5110244750976562], 'cosine_ionic_motion': 0.18643873805724717, 'ionic_motion_component': 2.9030732708877087, 'ionic_force_x': 11.182874098420143, 'ionic_force_y': -8.029923260211945, 'ionic_force_z': -7.2750024273991585, 'radial_force': 13.767219787088784, 'axial_force': -7.2750024273991585, 'contributions': [{'ion': 1309, 'force': [8.657218933105469, -1.525900959968567, 3.219957113265991], 'magnitude': 9.361833572387695, 'distance': 5.9550933837890625, 'cosine_with_motion': -0.6236493685107676, 'motion_component': -5.838501907603841}, {'ion': 1320, 'force': [-0.21056003868579865, -2.90226411819458, -0.06113452464342117], 'magnitude': 2.910534143447876, 'distance': 10.680280685424805, 'cosine_with_motion': 0.6225524357419339, 'motion_component': 1.811960224222066}, {'ion': 1469, 'force': [2.363967180252075, -3.182705879211426, -7.91904354095459], 'magnitude': 8.856026649475098, 'distance': 6.122793197631836, 'cosine_with_motion': 0.6050922614910305, 'motion_component': 5.3587131976036195}, {'ion': 2436, 'force': [0.3722480237483978, -0.4190523028373718, -2.5147814750671387], 'magnitude': 2.5764896869659424, 'distance': 11.351541519165039, 'cosine_with_motion': 0.6097060384339743, 'motion_component': 1.570901341876704}]}, 5302: {'frame': 5302, 'ionic_force': [9.384686825796962, -10.808709025382996, -6.232582181692123], 'ionic_force_magnitude': 15.612354667545477, 'motion_vector': [-1.703094482421875, 1.6502799987792969, -1.0469818115234375], 'cosine_ionic_motion': -0.6744132230711771, 'ionic_motion_component': -10.529178431069681, 'ionic_force_x': 9.384686825796962, 'ionic_force_y': -10.808709025382996, 'ionic_force_z': -6.232582181692123, 'radial_force': 14.314347264674101, 'axial_force': -6.232582181692123, 'contributions': [{'ion': 1309, 'force': [9.655634880065918, -6.011810302734375, 0.029120855033397675], 'magnitude': 11.374268531799316, 'distance': 5.402655601501465, 'cosine_with_motion': -0.8952160799916463, 'motion_component': -10.182428538158979}, {'ion': 1320, 'force': [-0.391956627368927, -2.144749641418457, -0.11846282333135605], 'magnitude': 2.1834867000579834, 'distance': 12.33087158203125, 'cosine_with_motion': -0.4854638859897166, 'motion_component': -1.0600039710206126}, {'ion': 1469, 'force': [0.1119040995836258, -2.1314122676849365, -4.249485492706299], 'magnitude': 4.755372524261475, 'distance': 8.355583190917969, 'cosine_with_motion': 0.06011979097258749, 'motion_component': 0.2858920014635995}, {'ion': 2436, 'force': [0.009104473516345024, -0.520736813545227, -1.8937547206878662], 'magnitude': 1.9640663862228394, 'distance': 13.001425743103027, 'cosine_with_motion': 0.21759044093186494, 'motion_component': 0.42736206507377106}]}, 5303: {'frame': 5303, 'ionic_force': [4.634013906121254, -7.393165856599808, -18.30676108598709], 'ionic_force_magnitude': 20.279804923241485, 'motion_vector': [2.9986648559570312, -0.3383674621582031, -0.0259552001953125], 'cosine_ionic_motion': 0.2756939581042625, 'ionic_motion_component': 5.591019688870754, 'ionic_force_x': 4.634013906121254, 'ionic_force_y': -7.393165856599808, 'ionic_force_z': -18.30676108598709, 'radial_force': 8.725421838817784, 'axial_force': -18.30676108598709, 'contributions': [{'ion': 1309, 'force': [6.351526737213135, -4.161134243011475, -12.593794822692871], 'magnitude': 14.705801963806152, 'distance': 4.751433849334717, 'cosine_with_motion': 0.46825843997322103, 'motion_component': 6.886115674686596}, {'ion': 1320, 'force': [-0.7893285751342773, -2.2547266483306885, -0.49746209383010864], 'magnitude': 2.440143585205078, 'distance': 11.664371490478516, 'cosine_with_motion': -0.21606729356545698, 'motion_component': -0.5272352060481691}, {'ion': 1469, 'force': [-0.7389268279075623, -0.7736309766769409, -3.6220219135284424], 'magnitude': 3.7767128944396973, 'distance': 9.375880241394043, 'cosine_with_motion': -0.16319631554447808, 'motion_component': -0.6163456335657835}, {'ion': 2436, 'force': [-0.1892574280500412, -0.20367398858070374, -1.593482255935669], 'magnitude': 1.6175559759140015, 'distance': 14.326476097106934, 'cosine_with_motion': -0.093669258529189, 'motion_component': -0.15151526404247218}]}, 5304: {'frame': 5304, 'ionic_force': [11.509692594408989, -10.579159915447235, -10.748389482498169], 'ionic_force_magnitude': 18.971545129532174, 'motion_vector': [-1.4822731018066406, 2.659027099609375, -2.7203369140625], 'cosine_ionic_motion': -0.20594956949000837, 'ionic_motion_component': -3.9071815519874162, 'ionic_force_x': 11.509692594408989, 'ionic_force_y': -10.579159915447235, 'ionic_force_z': -10.748389482498169, 'radial_force': 15.633030676564243, 'axial_force': -10.748389482498169, 'contributions': [{'ion': 1309, 'force': [10.475059509277344, -6.060859680175781, -4.418924331665039], 'magnitude': 12.883625030517578, 'distance': 5.076332092285156, 'cosine_with_motion': -0.3730478564218393, 'motion_component': -4.806208557360378}, {'ion': 1320, 'force': [-0.10482928156852722, -3.094301462173462, -0.409082293510437], 'magnitude': 3.122985601425171, 'distance': 10.310602188110352, 'cosine_with_motion': -0.5458528017668542, 'motion_component': -1.7046904380766525}, {'ion': 1469, 'force': [0.9543324708938599, -1.1745716333389282, -4.332919597625732], 'magnitude': 4.589614391326904, 'distance': 8.50512981414795, 'cosine_with_motion': 0.3868788436129706, 'motion_component': 1.7756247490290527}, {'ion': 2436, 'force': [0.18512989580631256, -0.24942713975906372, -1.5874632596969604], 'magnitude': 1.6175681352615356, 'distance': 14.326422691345215, 'cosine_with_motion': 0.5119368498997857, 'motion_component': 0.8280927206379406}]}, 5305: {'frame': 5305, 'ionic_force': [-7.564083315432072, 10.154234908521175, -16.6937335729599], 'ionic_force_magnitude': 20.952436220764316, 'motion_vector': [3.7210350036621094, 0.5313720703125, 4.7978057861328125], 'cosine_ionic_motion': -0.80534045139699, 'ionic_motion_component': -16.873844443896978, 'ionic_force_x': -7.564083315432072, 'ionic_force_y': 10.154234908521175, 'ionic_force_z': -16.6937335729599, 'radial_force': 12.66190518761801, 'axial_force': -16.6937335729599, 'contributions': [{'ion': 1309, 'force': [-6.675297737121582, 13.578149795532227, -11.790082931518555], 'magnitude': 19.181549072265625, 'distance': 4.160324573516846, 'cosine_with_motion': -0.6346004901054394, 'motion_component': -12.17262015225235}, {'ion': 1320, 'force': [-0.9775453209877014, -3.548858880996704, -1.993395209312439], 'magnitude': 4.186121940612793, 'distance': 8.905597686767578, 'cosine_with_motion': -0.5913323316384337, 'motion_component': -2.4753893727261147}, {'ion': 1469, 'force': [0.08875974267721176, 0.12494399398565292, -2.9102554321289062], 'magnitude': 2.91428804397583, 'distance': 10.673399925231934, 'cosine_with_motion': -0.7637664263245683, 'motion_component': -2.2258355180118463}]}, 5306: {'frame': 5306, 'ionic_force': [17.47581458091736, -4.5736775398254395, -4.979289084672928], 'ionic_force_magnitude': 18.738087983933962, 'motion_vector': [-1.9650535583496094, -1.8321075439453125, -0.7120208740234375], 'cosine_ionic_motion': -0.4304121236027933, 'ionic_motion_component': -8.065100241421, 'ionic_force_x': 17.47581458091736, 'ionic_force_y': -4.5736775398254395, 'ionic_force_z': -4.979289084672928, 'radial_force': 18.064402052238194, 'axial_force': -4.979289084672928, 'contributions': [{'ion': 1309, 'force': [4.468284606933594, 4.662998676300049, 3.70725679397583], 'magnitude': 7.44666862487793, 'distance': 6.677102088928223, 'cosine_with_motion': -0.9645342433791801, 'motion_component': -7.182567102252463}, {'ion': 1320, 'force': [7.873488903045654, -10.533976554870605, 0.34959670901298523], 'magnitude': 13.155938148498535, 'distance': 5.023519992828369, 'cosine_with_motion': 0.09786899057282514, 'motion_component': 1.2875583823797827}, {'ion': 1469, 'force': [4.469884872436523, 1.055068850517273, -6.895050525665283], 'magnitude': 8.2846097946167, 'distance': 6.330427169799805, 'cosine_with_motion': -0.25219732116268007, 'motion_component': -2.0893564481400375}, {'ion': 2436, 'force': [0.6641561985015869, 0.24223148822784424, -2.14109206199646], 'magnitude': 2.2547848224639893, 'distance': 12.13434886932373, 'cosine_with_motion': -0.03580609982653162, 'motion_component': -0.08073505180798435}]}, 5307: {'frame': 5307, 'ionic_force': [6.0052439123392105, 2.971535697579384, -1.2920927703380585], 'ionic_force_magnitude': 6.823670755233991, 'motion_vector': [-1.8429718017578125, 0.5340690612792969, 3.6442413330078125], 'cosine_ionic_motion': -0.5048908635908108, 'ionic_motion_component': -3.44520902046945, 'ionic_force_x': 6.0052439123392105, 'ionic_force_y': 2.971535697579384, 'ionic_force_z': -1.2920927703380585, 'radial_force': 6.700222298452175, 'axial_force': -1.2920927703380585, 'contributions': [{'ion': 1309, 'force': [5.069587707519531, 8.484151840209961, 7.271227836608887], 'magnitude': 12.269975662231445, 'distance': 5.201722621917725, 'cosine_with_motion': 0.4291373195283767, 'motion_component': 5.265504527085966}, {'ion': 1320, 'force': [-0.18250830471515656, -4.807651519775391, -0.49011465907096863], 'magnitude': 4.836014270782471, 'distance': 8.285624504089355, 'cosine_with_motion': -0.2017022843551575, 'motion_component': -0.975435141621853}, {'ion': 1469, 'force': [0.850151538848877, -0.5294232368469238, -5.994930744171143], 'magnitude': 6.078012943267822, 'distance': 7.390745162963867, 'cosine_with_motion': -0.9466319012710269, 'motion_component': -5.753640939993872}, {'ion': 2436, 'force': [0.26801297068595886, -0.17554138600826263, -2.078275203704834], 'magnitude': 2.102825164794922, 'distance': 12.565143585205078, 'cosine_with_motion': -0.942369072941603, 'motion_component': -1.9816373740599276}]}, 5308: {'frame': 5308, 'ionic_force': [-3.9245860427618027, -5.353306509554386, -11.027286529541016], 'ionic_force_magnitude': 12.870948465318119, 'motion_vector': [-0.12729644775390625, 0.5117263793945312, -0.26439666748046875], 'cosine_ionic_motion': 0.08900058775676298, 'ionic_motion_component': 1.145521978400319, 'ionic_force_x': -3.9245860427618027, 'ionic_force_y': -5.353306509554386, 'ionic_force_z': -11.027286529541016, 'radial_force': 6.637790761411368, 'axial_force': -11.027286529541016, 'contributions': [{'ion': 1309, 'force': [0.1623639464378357, 0.4300653338432312, 3.4034218788146973], 'magnitude': 3.434326410293579, 'distance': 9.832144737243652, 'cosine_with_motion': -0.3457480673528202, 'motion_component': -1.1874117610608668}, {'ion': 1320, 'force': [-3.1859545707702637, -5.096459865570068, 2.4922938346862793], 'magnitude': 6.506591796875, 'distance': 7.143190860748291, 'cosine_with_motion': -0.7455033842480661, 'motion_component': -4.850686286735993}, {'ion': 1469, 'force': [-1.04063880443573, -0.7825348973274231, -12.82127857208252], 'magnitude': 12.887221336364746, 'distance': 5.075623512268066, 'cosine_with_motion': 0.4106676150977118, 'motion_component': 5.292364458409139}, {'ion': 2436, 'force': [0.13964338600635529, 0.09562291949987411, -4.101723670959473], 'magnitude': 4.1052141189575195, 'distance': 8.992928504943848, 'cosine_with_motion': 0.4606960465227934, 'motion_component': 1.891255809716336}]}, 5309: {'frame': 5309, 'ionic_force': [-6.100982252508402, -3.1015712544322014, -15.906369686126709], 'ionic_force_magnitude': 17.31630229822387, 'motion_vector': [0.6568450927734375, -0.14005661010742188, -0.313629150390625], 'cosine_ionic_motion': 0.11029630434347097, 'ionic_motion_component': 1.909924148388446, 'ionic_force_x': -6.100982252508402, 'ionic_force_y': -3.1015712544322014, 'ionic_force_z': -15.906369686126709, 'radial_force': 6.844101744695401, 'axial_force': -15.906369686126709, 'contributions': [{'ion': 1309, 'force': [0.20207388699054718, 0.08543962985277176, 2.6796698570251465], 'magnitude': 2.688636302947998, 'distance': 11.112276077270508, 'cosine_with_motion': -0.3611103386395704, 'motion_component': -0.970894309377176}, {'ion': 1320, 'force': [-3.724456787109375, -3.0685253143310547, 2.46171236038208], 'magnitude': 5.417328834533691, 'distance': 7.828461647033691, 'cosine_with_motion': -0.6944816395866571, 'motion_component': -3.7622355398655856}, {'ion': 1469, 'force': [-2.5375022888183594, -0.4666903018951416, -17.041349411010742], 'magnitude': 17.235553741455078, 'distance': 4.388907432556152, 'cosine_with_motion': 0.29300374354212066, 'motion_component': 5.050081723024142}, {'ion': 2436, 'force': [-0.041097063571214676, 0.34820473194122314, -4.006402492523193], 'magnitude': 4.0217156410217285, 'distance': 9.085803985595703, 'cosine_with_motion': 0.39609276644881936, 'motion_component': 1.59297246126204}]}, 5310: {'frame': 5310, 'ionic_force': [-2.138845317065716, -6.399635553359985, -14.446752071380615], 'ionic_force_magnitude': 15.944862492919254, 'motion_vector': [-0.4894981384277344, 0.20468902587890625, 0.37158966064453125], 'cosine_ionic_motion': -0.5452217807443366, 'ionic_motion_component': -8.693486322113017, 'ionic_force_x': -2.138845317065716, 'ionic_force_y': -6.399635553359985, 'ionic_force_z': -14.446752071380615, 'radial_force': 6.747591756038824, 'axial_force': -14.446752071380615, 'contributions': [{'ion': 1309, 'force': [-0.425532728433609, 0.4280744194984436, 4.451706409454346], 'magnitude': 4.4924397468566895, 'distance': 8.596623420715332, 'cosine_with_motion': 0.6701482337154809, 'motion_component': 3.0106006276943322}, {'ion': 1320, 'force': [-2.6733267307281494, -4.865641117095947, 5.675074100494385], 'magnitude': 7.938992977142334, 'distance': 6.466753959655762, 'cosine_with_motion': 0.4708679390348454, 'motion_component': 3.7382171379287144}, {'ion': 1469, 'force': [0.8352939486503601, -1.7298543453216553, -20.9677677154541], 'magnitude': 21.055578231811523, 'distance': 3.970867872238159, 'cosine_with_motion': -0.6272065415358462, 'motion_component': -13.206196705608171}, {'ion': 2436, 'force': [0.12472019344568253, -0.23221451044082642, -3.605764865875244], 'magnitude': 3.615386486053467, 'distance': 9.582783699035645, 'cosine_with_motion': -0.6184975575539667, 'motion_component': -2.2361076710314904}]}, 5311: {'frame': 5311, 'ionic_force': [-1.5457566678524017, -3.735124170780182, -10.29975938796997], 'ionic_force_magnitude': 11.064608429466993, 'motion_vector': [0.5821189880371094, -0.71893310546875, 0.33875274658203125], 'cosine_ionic_motion': -0.15629080861675848, 'ionic_motion_component': -1.7292965984691986, 'ionic_force_x': -1.5457566678524017, 'ionic_force_y': -3.735124170780182, 'ionic_force_z': -10.29975938796997, 'radial_force': 4.042340441793158, 'axial_force': -10.29975938796997, 'contributions': [{'ion': 1309, 'force': [0.2618166506290436, 0.38895392417907715, 3.28230881690979], 'magnitude': 3.315627336502075, 'distance': 10.006591796875, 'cosine_with_motion': 0.30146056067917015, 'motion_component': 0.9995308598941133}, {'ion': 1320, 'force': [-0.6014491319656372, -3.967463493347168, 2.3787336349487305], 'magnitude': 4.66485595703125, 'distance': 8.436259269714355, 'cosine_with_motion': 0.71984257043354, 'motion_component': 3.3579619209873}, {'ion': 1469, 'force': [-1.1576669216156006, -0.06768996268510818, -12.637163162231445], 'magnitude': 12.690258979797363, 'distance': 5.114860534667969, 'cosine_with_motion': -0.3924399710702723, 'motion_component': -4.980164781043792}, {'ion': 2436, 'force': [-0.04845726490020752, -0.08892463892698288, -3.323638677597046], 'magnitude': 3.325181007385254, 'distance': 9.992206573486328, 'cosine_with_motion': -0.33280123710707715, 'motion_component': -1.1066244041700855}]}, 5312: {'frame': 5312, 'ionic_force': [-0.6932454779744148, -6.2057766020298, -20.55894696712494], 'ionic_force_magnitude': 21.486334096911186, 'motion_vector': [-0.3184471130371094, 0.7150497436523438, -0.7793121337890625], 'cosine_ionic_motion': 0.49742079003617534, 'ionic_motion_component': 10.687749281466774, 'ionic_force_x': -0.6932454779744148, 'ionic_force_y': -6.2057766020298, 'ionic_force_z': -20.55894696712494, 'radial_force': 6.244377673318016, 'axial_force': -20.55894696712494, 'contributions': [{'ion': 1309, 'force': [0.08076175302267075, 0.06683516502380371, 2.8113584518432617], 'magnitude': 2.81331205368042, 'distance': 10.86325740814209, 'cosine_with_motion': -0.6979538305612016, 'motion_component': -1.9635620526184647}, {'ion': 1320, 'force': [-0.7783627510070801, -3.133505344390869, 1.1805278062820435], 'magnitude': 3.4377827644348145, 'distance': 9.827200889587402, 'cosine_with_motion': -0.7670759051133565, 'motion_component': -2.6370403123848902}, {'ion': 1469, 'force': [-0.06458400189876556, -2.735037326812744, -20.452817916870117], 'magnitude': 20.634979248046875, 'distance': 4.011132717132568, 'cosine_with_motion': 0.6144162662202742, 'motion_component': 12.678466790651052}, {'ion': 2436, 'force': [0.06893952190876007, -0.40406909584999084, -4.098015308380127], 'magnitude': 4.118464946746826, 'distance': 8.978449821472168, 'cosine_with_motion': 0.6337033185455325, 'motion_component': 2.6098849380748117}]}, 5313: {'frame': 5313, 'ionic_force': [-6.034946657717228, -5.350842729210854, -16.52107262611389], 'ionic_force_magnitude': 18.384720280482124, 'motion_vector': [-0.3755340576171875, -0.5339927673339844, 0.46227264404296875], 'cosine_ionic_motion': -0.17092017347635274, 'ionic_motion_component': -3.142319579654225, 'ionic_force_x': -6.034946657717228, 'ionic_force_y': -5.350842729210854, 'ionic_force_z': -16.52107262611389, 'radial_force': 8.065488148540112, 'axial_force': -16.52107262611389, 'contributions': [{'ion': 1309, 'force': [-0.11181335151195526, -3.108283758163452, 3.290030002593994], 'magnitude': 4.527496814727783, 'distance': 8.563276290893555, 'cosine_with_motion': 0.8898428749727498, 'motion_component': 4.028760797518868}, {'ion': 1320, 'force': [-4.065372467041016, -4.175497531890869, 2.469059705734253], 'magnitude': 6.329161643981934, 'distance': 7.242623805999756, 'cosine_with_motion': 0.9673964643253833, 'motion_component': 6.1228087225875925}, {'ion': 1469, 'force': [-1.8919004201889038, 1.7885223627090454, -18.668319702148438], 'magnitude': 18.84898567199707, 'distance': 4.196865558624268, 'cosine_with_motion': -0.5885820179472476, 'motion_component': -11.094174008723336}, {'ion': 2436, 'force': [0.03413958102464676, 0.1444161981344223, -3.611842632293701], 'magnitude': 3.6148898601531982, 'distance': 9.583441734313965, 'cosine_with_motion': -0.6085152255557099, 'motion_component': -2.1997155227084764}]}, 5314: {'frame': 5314, 'ionic_force': [-5.211430847644806, -8.442669451236725, -17.771475553512573], 'ionic_force_magnitude': 20.35345234331819, 'motion_vector': [-0.15516281127929688, 0.3010063171386719, -0.0225677490234375], 'cosine_ionic_motion': -0.19276747009609363, 'ionic_motion_component': -3.9234835159428556, 'ionic_force_x': -5.211430847644806, 'ionic_force_y': -8.442669451236725, 'ionic_force_z': -17.771475553512573, 'radial_force': 9.921576434349014, 'axial_force': -17.771475553512573, 'contributions': [{'ion': 1309, 'force': [-0.48251619935035706, -3.664240598678589, 1.9041845798492432], 'magnitude': 4.157571315765381, 'distance': 8.936123847961426, 'cosine_with_motion': -0.759047802567711, 'motion_component': -3.155795436619493}, {'ion': 1320, 'force': [-3.720808982849121, -2.3928604125976562, 4.966029167175293], 'magnitude': 6.6506876945495605, 'distance': 7.0653839111328125, 'cosine_with_motion': -0.11297411757773741, 'motion_component': -0.7513555677998909}, {'ion': 1469, 'force': [-1.2004474401474, -2.1353933811187744, -20.877975463867188], 'magnitude': 21.02120018005371, 'distance': 3.974113702774048, 'cosine_with_motion': 0.002055755984253285, 'motion_component': 0.04321445715726568}, {'ion': 2436, 'force': [0.19234177470207214, -0.2501750588417053, -3.763713836669922], 'magnitude': 3.7769198417663574, 'distance': 9.37562370300293, 'cosine_with_motion': -0.015766023567895776, 'motion_component': -0.059547009893312186}]}, 5315: {'frame': 5315, 'ionic_force': [-4.354976288974285, -2.9413586780428886, -13.101229906082153], 'ionic_force_magnitude': 14.115935477411613, 'motion_vector': [0.5261955261230469, -0.461700439453125, -0.2435302734375], 'cosine_ionic_motion': 0.21572260525693082, 'ionic_motion_component': 3.0451263768259706, 'ionic_force_x': -4.354976288974285, 'ionic_force_y': -2.9413586780428886, 'ionic_force_z': -13.101229906082153, 'radial_force': 5.2552268600343455, 'axial_force': -13.101229906082153, 'contributions': [{'ion': 1309, 'force': [-1.3679094314575195, -3.2166194915771484, 1.7919011116027832], 'magnitude': 3.9279417991638184, 'distance': 9.193619728088379, 'cosine_with_motion': 0.11298760627771773, 'motion_component': 0.44380874123271497}, {'ion': 1320, 'force': [-0.15094943344593048, 0.24601347744464874, 6.12855863571167], 'magnitude': 6.135351657867432, 'distance': 7.356128692626953, 'cosine_with_motion': -0.37064926599663733, 'motion_component': -2.2740635689315685}, {'ion': 1469, 'force': [-2.7265963554382324, 0.12713120877742767, -17.374311447143555], 'magnitude': 17.58741569519043, 'distance': 4.34478235244751, 'cosine_with_motion': 0.21002214050115225, 'motion_component': 3.6937466750015853}, {'ion': 2436, 'force': [-0.10952106863260269, -0.09788387268781662, -3.6473782062530518], 'magnitude': 3.6503348350524902, 'distance': 9.536800384521484, 'cosine_with_motion': 0.32370584867965324, 'motion_component': 1.1816347130642422}]}, 5316: {'frame': 5316, 'ionic_force': [1.7553037405014038, -11.83569049090147, -15.618502497673035], 'ionic_force_magnitude': 19.6749150160211, 'motion_vector': [-0.0081329345703125, -0.06674957275390625, -0.1145172119140625], 'cosine_ionic_motion': 0.9814416458058247, 'ionic_motion_component': 19.30978097441348, 'ionic_force_x': 1.7553037405014038, 'ionic_force_y': -11.83569049090147, 'ionic_force_z': -15.618502497673035, 'radial_force': 11.965143568626067, 'axial_force': -15.618502497673035, 'contributions': [{'ion': 1309, 'force': [-1.1511693000793457, -4.0106306076049805, 0.9726828336715698], 'magnitude': 4.2844438552856445, 'distance': 8.80281925201416, 'cosine_with_motion': 0.29119307062612976, 'motion_component': 1.2476004088355062}, {'ion': 13</t>
+          <t>{5293: {'frame': 5293, 'ionic_force': [-4.439165145158768, -11.485485851764679, -5.509422957897186], 'ionic_force_magnitude': 13.489859664432528, 'motion_vector': [3.6029815673828125, -0.9414405822753906, -2.305633544921875], 'cosine_ionic_motion': 0.12729862041329584, 'ionic_motion_component': 1.7172405248512268, 'ionic_force_x': -4.439165145158768, 'ionic_force_y': -11.485485851764679, 'ionic_force_z': -5.509422957897186, 'radial_force': 12.31351178328421, 'axial_force': -5.509422957897186, 'before_closest_residue': None, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [-0.4600997269153595, -6.4237165451049805, -1.8560487031936646], 'magnitude': 6.702293872833252, 'distance': 7.038130283355713, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.2953168585098998, 'motion_component': 1.9793003634343174}, {'ion': 1320, 'force': [-2.2913060188293457, -4.553028583526611, 0.9146720767021179], 'magnitude': 5.178492069244385, 'distance': 8.00695514678955, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 423, 'cosine_with_motion': -0.26797402199208176, 'motion_component': -1.387701281697467}, {'ion': 1469, 'force': [-1.280375599861145, -0.43071743845939636, -2.963862419128418], 'magnitude': 3.2572009563446045, 'distance': 10.095939636230469, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.18406364306654752, 'motion_component': 0.5995323182463634}, {'ion': 2436, 'force': [-0.4073837995529175, -0.0780232846736908, -1.6041839122772217], 'magnitude': 1.656941533088684, 'distance': 14.155181884765625, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3175182671968274, 'motion_component': 0.5261092018864266}]}, 5294: {'frame': 5294, 'ionic_force': [0.1658477745950222, -6.8131378293037415, -5.872682213783264], 'ionic_force_magnitude': 8.99637421128724, 'motion_vector': [-1.1986160278320312, 0.10608673095703125, 0.8895950317382812], 'cosine_ionic_motion': -0.4565192458823854, 'ionic_motion_component': -4.10701797061259, 'ionic_force_x': 0.1658477745950222, 'ionic_force_y': -6.8131378293037415, 'ionic_force_z': -5.872682213783264, 'radial_force': 6.815156092521126, 'axial_force': -5.872682213783264, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [1.4283074140548706, -3.2946081161499023, -1.909952163696289], 'magnitude': 4.067237377166748, 'distance': 9.034814834594727, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.6178726576783165, 'motion_component': -2.5130349266499294}, {'ion': 1320, 'force': [-1.2332184314727783, -2.8408944606781006, -1.2032557725906372], 'magnitude': 3.3225491046905518, 'distance': 9.996163368225098, 'before_closest_residue': 130, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.021392684254919057, 'motion_component': 0.0710782469366329}, {'ion': 1469, 'force': [-0.029241207987070084, -0.6776352524757385, -2.759474277496338], 'magnitude': 2.841609239578247, 'distance': 10.809033393859863, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.585957106898025, 'motion_component': -1.665061108476534}]}, 5295: {'frame': 5295, 'ionic_force': [-0.8948521912097931, -8.003737807273865, -7.197145462036133], 'ionic_force_magnitude': 10.800901912961034, 'motion_vector': [1.4610366821289062, 0.4837226867675781, -0.33788299560546875], 'cosine_ionic_motion': -0.16142186763286107, 'ionic_motion_component': -1.7435017589095119, 'ionic_force_x': -0.8948521912097931, 'ionic_force_y': -8.003737807273865, 'ionic_force_z': -7.197145462036133, 'radial_force': 8.053606603981724, 'axial_force': -7.197145462036133, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [1.2909294366836548, -4.2322163581848145, -2.066220760345459], 'magnitude': 4.883382320404053, 'distance': 8.245342254638672, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.06979078553032043, 'motion_component': 0.340815084300246}, {'ion': 1320, 'force': [-1.8195945024490356, -3.148383855819702, -1.8783209323883057], 'magnitude': 4.09283971786499, 'distance': 9.006513595581055, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.5499726823402922, 'motion_component': -2.2509498785102373}, {'ion': 1469, 'force': [-0.36618712544441223, -0.6231375932693481, -3.252603769302368], 'magnitude': 3.331940174102783, 'distance': 9.98206615447998, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.05001077294285725, 'motion_component': 0.16663289920801638}]}, 5296: {'frame': 5296, 'ionic_force': [0.31867482099914923, -8.267817586660385, -7.231484055519104], 'ionic_force_magnitude': 10.988754384963595, 'motion_vector': [-0.4652824401855469, 0.103912353515625, -2.422882080078125], 'cosine_ionic_motion': 0.6085736128030453, 'ionic_motion_component': 6.687465956262602, 'ionic_force_x': 0.31867482099914923, 'ionic_force_y': -8.267817586660385, 'ionic_force_z': -7.231484055519104, 'radial_force': 8.273956809642506, 'axial_force': -7.231484055519104, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [2.060899019241333, -4.070521354675293, -2.4136157035827637], 'magnitude': 5.161587715148926, 'distance': 8.020055770874023, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.350394413188984, 'motion_component': 1.808591562717023}, {'ion': 1320, 'force': [-1.741642713546753, -3.7549068927764893, -1.5699185132980347], 'magnitude': 4.426882743835449, 'distance': 8.660042762756348, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 423, 'cosine_with_motion': 0.3863979687561965, 'motion_component': 1.7105384314382377}, {'ion': 1469, 'force': [-0.000581484695430845, -0.4423893392086029, -3.2479498386383057], 'magnitude': 3.2779393196105957, 'distance': 10.063952445983887, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.9665632598820196, 'motion_component': 3.1683358083492243}]}, 5297: {'frame': 5297, 'ionic_force': [2.0586469620466232, -4.025961697101593, -6.761675596237183], 'ionic_force_magnitude': 8.134288645580657, 'motion_vector': [0.11940383911132812, -0.8824501037597656, 1.4705276489257812], 'cosine_ionic_motion': -0.439411799823159, 'ionic_motion_component': -3.5743024140356825, 'ionic_force_x': 2.0586469620466232, 'ionic_force_y': -4.025961697101593, 'ionic_force_z': -6.761675596237183, 'radial_force': 4.521769001272945, 'axial_force': -6.761675596237183, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [2.703697919845581, -1.9296005964279175, -3.2435293197631836], 'magnitude': 4.642609596252441, 'distance': 8.45644760131836, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 1105, 'cosine_with_motion': -0.34381617958818117, 'motion_component': -1.5962042757614867}, {'ion': 1320, 'force': [-0.5463349223136902, -1.8209863901138306, -1.1804895401000977], 'magnitude': 2.2378625869750977, 'distance': 12.18014144897461, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.050490734426634716, 'motion_component': -0.1129913241681777}, {'ion': 1469, 'force': [-0.09871603548526764, -0.27537471055984497, -2.3376567363739014], 'magnitude': 2.3558895587921143, 'distance': 11.871116638183594, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7916784499341073, 'motion_component': -1.8651069085584862}]}, 5298: {'frame': 5298, 'ionic_force': [2.64043165743351, -8.706450581550598, -7.226660072803497], 'ionic_force_magnitude': 11.618897403558226, 'motion_vector': [-0.8501853942871094, 0.7801551818847656, 2.5111923217773438], 'cosine_ionic_motion': -0.8466110490409935, 'ionic_motion_component': -9.836686919526105, 'ionic_force_x': 2.64043165743351, 'ionic_force_y': -8.706450581550598, 'ionic_force_z': -7.226660072803497, 'radial_force': 9.098030614729751, 'axial_force': -7.226660072803497, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [3.2287416458129883, -6.1072096824646, -3.8306076526641846], 'magnitude': 7.899135589599609, 'distance': 6.483048439025879, 'before_closest_residue': 98, 'closest_residue': 1105, 'next_closest_residue': 1073, 'cosine_with_motion': -0.7846489917489425, 'motion_component': -6.19804851018975}, {'ion': 1320, 'force': [-0.4978197515010834, -2.0856738090515137, -0.9577496647834778], 'magnitude': 2.3484344482421875, 'distance': 11.889945030212402, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.5560732892391631, 'motion_component': -1.3059016451634013}, {'ion': 1469, 'force': [-0.09049023687839508, -0.5135670900344849, -2.438302755355835], 'magnitude': 2.493443489074707, 'distance': 11.539029121398926, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9355482454164143, 'motion_component': -2.3327365935457256}]}, 5299: {'frame': 5299, 'ionic_force': [8.148396573960781, -5.8599869310855865, -10.365723192691803], 'ionic_force_magnitude': 14.428583813615887, 'motion_vector': [-0.3539390563964844, 2.2585983276367188, 2.1390380859375], 'cosine_ionic_motion': -0.84767086277239, 'ionic_motion_component': -12.230690089871521, 'ionic_force_x': 8.148396573960781, 'ionic_force_y': -5.8599869310855865, 'ionic_force_z': -10.365723192691803, 'radial_force': 10.036723248103918, 'axial_force': -10.365723192691803, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [9.771367073059082, -2.351778030395508, -4.5568013191223145], 'magnitude': 11.03516674041748, 'distance': 5.485037326812744, 'before_closest_residue': 1105, 'closest_residue': 1073, 'next_closest_residue': 1105, 'cosine_with_motion': -0.5359722734248957, 'motion_component': -5.914543591356164}, {'ion': 1320, 'force': [-1.1783761978149414, -2.824215888977051, -0.5681673884391785], 'magnitude': 3.11248779296875, 'distance': 10.32797622680664, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.7365107631581589, 'motion_component': -2.2923807326295993}, {'ion': 1469, 'force': [-0.3746396005153656, -0.5283625721931458, -3.711301326751709], 'magnitude': 3.767396926879883, 'distance': 9.387465476989746, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7629798072189766, 'motion_component': -2.8744477578251457}, {'ion': 2436, 'force': [-0.06995470076799393, -0.1556304395198822, -1.529453158378601], 'magnitude': 1.5389416217803955, 'distance': 14.687841415405273, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7468235204612907, 'motion_component': -1.1493178342881796}]}, 5300: {'frame': 5300, 'ionic_force': [11.58044770359993, 2.511912077665329, -5.298129674047232], 'ionic_force_magnitude': 12.98024072753482, 'motion_vector': [2.946308135986328, -2.5934295654296875, 0.6218948364257812], 'cosine_ionic_motion': 0.47126898983142484, 'ionic_motion_component': 6.117184935434054, 'ionic_force_x': 11.58044770359993, 'ionic_force_y': 2.511912077665329, 'ionic_force_z': -5.298129674047232, 'radial_force': 11.849745621815426, 'axial_force': -5.298129674047232, 'before_closest_residue': 1105, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [15.33890438079834, 5.875173568725586, 3.291243076324463], 'magnitude': 16.752071380615234, 'distance': 4.451791286468506, 'before_closest_residue': 1073, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': 0.48071337114347773, 'motion_component': 8.052945245231506}, {'ion': 1320, 'force': [-2.06095027923584, -3.7897627353668213, -0.05836188420653343], 'magnitude': 4.314304351806641, 'distance': 8.772303581237793, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 423, 'cosine_with_motion': 0.21696714822175778, 'motion_component': 0.9360623548549916}, {'ion': 1469, 'force': [-1.4913935661315918, 0.3887030780315399, -6.317618370056152], 'magnitude': 6.502894878387451, 'distance': 7.145220756530762, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.36106680502471306, 'motion_component': -2.347979613803373}, {'ion': 2436, 'force': [-0.2061128318309784, 0.037798166275024414, -2.213392496109009], 'magnitude': 2.223289728164673, 'distance': 12.21999454498291, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.23561603955225588, 'motion_component': -0.5238427378697725}]}, 5301: {'frame': 5301, 'ionic_force': [11.182874098420143, -8.029923260211945, -7.2750024273991585], 'ionic_force_magnitude': 15.571191379745887, 'motion_vector': [-1.3564949035644531, -1.4149208068847656, -1.5110244750976562], 'cosine_ionic_motion': 0.18643873805724717, 'ionic_motion_component': 2.9030732708877087, 'ionic_force_x': 11.182874098420143, 'ionic_force_y': -8.029923260211945, 'ionic_force_z': -7.2750024273991585, 'radial_force': 13.767219787088784, 'axial_force': -7.2750024273991585, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [8.657218933105469, -1.525900959968567, 3.219957113265991], 'magnitude': 9.361833572387695, 'distance': 5.9550933837890625, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': -0.6236493685107676, 'motion_component': -5.838501907603841}, {'ion': 1320, 'force': [-0.21056003868579865, -2.90226411819458, -0.06113452464342117], 'magnitude': 2.910534143447876, 'distance': 10.680280685424805, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': 0.6225524357419339, 'motion_component': 1.811960224222066}, {'ion': 1469, 'force': [2.363967180252075, -3.182705879211426, -7.91904354095459], 'magnitude': 8.856026649475098, 'distance': 6.122793197631836, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6050922614910305, 'motion_component': 5.3587131976036195}, {'ion': 2436, 'force': [0.3722480237483978, -0.4190523028373718, -2.5147814750671387], 'magnitude': 2.5764896869659424, 'distance': 11.351541519165039, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6097060384339743, 'motion_component': 1.570901341876704}]}, 5302: {'frame': 5302, 'ionic_force': [9.384686825796962, -10.808709025382996, -6.232582181692123], 'ionic_force_magnitude': 15.612354667545477, 'motion_vector': [-1.703094482421875, 1.6502799987792969, -1.0469818115234375], 'cosine_ionic_motion': -0.6744132230711771, 'ionic_motion_component': -10.529178431069681, 'ionic_force_x': 9.384686825796962, 'ionic_force_y': -10.808709025382996, 'ionic_force_z': -6.232582181692123, 'radial_force': 14.314347264674101, 'axial_force': -6.232582181692123, 'before_closest_residue': 'SF', 'closest_residue': 1105, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [9.655634880065918, -6.011810302734375, 0.029120855033397675], 'magnitude': 11.374268531799316, 'distance': 5.402655601501465, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 'SF', 'cosine_with_motion': -0.8952160799916463, 'motion_component': -10.182428538158979}, {'ion': 1320, 'force': [-0.391956627368927, -2.144749641418457, -0.11846282333135605], 'magnitude': 2.1834867000579834, 'distance': 12.33087158203125, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.4854638859897166, 'motion_component': -1.0600039710206126}, {'ion': 1469, 'force': [0.1119040995836258, -2.1314122676849365, -4.249485492706299], 'magnitude': 4.755372524261475, 'distance': 8.355583190917969, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.06011979097258749, 'motion_component': 0.2858920014635995}, {'ion': 2436, 'force': [0.009104473516345024, -0.520736813545227, -1.8937547206878662], 'magnitude': 1.9640663862228394, 'distance': 13.001425743103027, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.21759044093186494, 'motion_component': 0.42736206507377106}]}, 5303: {'frame': 5303, 'ionic_force': [4.634013906121254, -7.393165856599808, -18.30676108598709], 'ionic_force_magnitude': 20.279804923241485, 'motion_vector': [2.9986648559570312, -0.3383674621582031, -0.0259552001953125], 'cosine_ionic_motion': 0.2756939581042625, 'ionic_motion_component': 5.591019688870754, 'ionic_force_x': 4.634013906121254, 'ionic_force_y': -7.393165856599808, 'ionic_force_z': -18.30676108598709, 'radial_force': 8.725421838817784, 'axial_force': -18.30676108598709, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [6.351526737213135, -4.161134243011475, -12.593794822692871], 'magnitude': 14.705801963806152, 'distance': 4.751433849334717, 'before_closest_residue': 1105, 'closest_residue': 'SF', 'next_closest_residue': 1105, 'cosine_with_motion': 0.46825843997322103, 'motion_component': 6.886115674686596}, {'ion': 1320, 'force': [-0.7893285751342773, -2.2547266483306885, -0.49746209383010864], 'magnitude': 2.440143585205078, 'distance': 11.664371490478516, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.21606729356545698, 'motion_component': -0.5272352060481691}, {'ion': 1469, 'force': [-0.7389268279075623, -0.7736309766769409, -3.6220219135284424], 'magnitude': 3.7767128944396973, 'distance': 9.375880241394043, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.16319631554447808, 'motion_component': -0.6163456335657835}, {'ion': 2436, 'force': [-0.1892574280500412, -0.20367398858070374, -1.593482255935669], 'magnitude': 1.6175559759140015, 'distance': 14.326476097106934, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.093669258529189, 'motion_component': -0.15151526404247218}]}, 5304: {'frame': 5304, 'ionic_force': [11.509692594408989, -10.579159915447235, -10.748389482498169], 'ionic_force_magnitude': 18.971545129532174, 'motion_vector': [-1.4822731018066406, 2.659027099609375, -2.7203369140625], 'cosine_ionic_motion': -0.20594956949000837, 'ionic_motion_component': -3.9071815519874162, 'ionic_force_x': 11.509692594408989, 'ionic_force_y': -10.579159915447235, 'ionic_force_z': -10.748389482498169, 'radial_force': 15.633030676564243, 'axial_force': -10.748389482498169, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [10.475059509277344, -6.060859680175781, -4.418924331665039], 'magnitude': 12.883625030517578, 'distance': 5.076332092285156, 'before_closest_residue': 'SF', 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': -0.3730478564218393, 'motion_component': -4.806208557360378}, {'ion': 1320, 'force': [-0.10482928156852722, -3.094301462173462, -0.409082293510437], 'magnitude': 3.122985601425171, 'distance': 10.310602188110352, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.5458528017668542, 'motion_component': -1.7046904380766525}, {'ion': 1469, 'force': [0.9543324708938599, -1.1745716333389282, -4.332919597625732], 'magnitude': 4.589614391326904, 'distance': 8.50512981414795, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3868788436129706, 'motion_component': 1.7756247490290527}, {'ion': 2436, 'force': [0.18512989580631256, -0.24942713975906372, -1.5874632596969604], 'magnitude': 1.6175681352615356, 'distance': 14.326422691345215, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5119368498997857, 'motion_component': 0.8280927206379406}]}, 5305: {'frame': 5305, 'ionic_force': [-7.564083315432072, 10.154234908521175, -16.6937335729599], 'ionic_force_magnitude': 20.952436220764316, 'motion_vector': [3.7210350036621094, 0.5313720703125, 4.7978057861328125], 'cosine_ionic_motion': -0.80534045139699, 'ionic_motion_component': -16.873844443896978, 'ionic_force_x': -7.564083315432072, 'ionic_force_y': 10.154234908521175, 'ionic_force_z': -16.6937335729599, 'radial_force': 12.66190518761801, 'axial_force': -16.6937335729599, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 423, 'contributions': [{'ion': 1309, 'force': [-6.675297737121582, 13.578149795532227, -11.790082931518555], 'magnitude': 19.181549072265625, 'distance': 4.160324573516846, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 1105, 'cosine_with_motion': -0.6346004901054394, 'motion_component': -12.17262015225235}, {'ion': 1320, 'force': [-0.9775453209877014, -3.548858880996704, -1.993395209312439], 'magnitude': 4.186121940612793, 'distance': 8.905597686767578, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 98, 'cosine_with_motion': -0.5913323316384337, 'motion_component': -2.4753893727261147}, {'ion': 1469, 'force': [0.08875974267721176, 0.12494399398565292, -2.9102554321289062], 'magnitude': 2.91428804397583, 'distance': 10.673399925231934, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7637664263245683, 'motion_component': -2.2258355180118463}]}, 5306: {'frame': 5306, 'ionic_force': [17.47581458091736, -4.5736775398254395, -4.979289084672928], 'ionic_force_magnitude': 18.738087983933962, 'motion_vector': [-1.9650535583496094, -1.8321075439453125, -0.7120208740234375], 'cosine_ionic_motion': -0.4304121236027933, 'ionic_motion_component': -8.065100241421, 'ionic_force_x': 17.47581458091736, 'ionic_force_y': -4.5736775398254395, 'ionic_force_z': -4.979289084672928, 'radial_force': 18.064402052238194, 'axial_force': -4.979289084672928, 'before_closest_residue': 780, 'closest_residue': 423, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [4.468284606933594, 4.662998676300049, 3.70725679397583], 'magnitude': 7.44666862487793, 'distance': 6.677102088928223, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': -0.9645342433791801, 'motion_component': -7.182567102252463}, {'ion': 1320, 'force': [7.873488903045654, -10.533976554870605, 0.34959670901298523], 'magnitude': 13.155938148498535, 'distance': 5.023519992828369, 'before_closest_residue': 455, 'closest_residue': 98, 'next_closest_residue': 455, 'cosine_with_motion': 0.09786899057282514, 'motion_component': 1.2875583823797827}, {'ion': 1469, 'force': [4.469884872436523, 1.055068850517273, -6.895050525665283], 'magnitude': 8.2846097946167, 'distance': 6.330427169799805, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.25219732116268007, 'motion_component': -2.0893564481400375}, {'ion': 2436, 'force': [0.6641561985015869, 0.24223148822784424, -2.14109206199646], 'magnitude': 2.2547848224639893, 'distance': 12.13434886932373, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.03580609982653162, 'motion_component': -0.08073505180798435}]}, 5307: {'frame': 5307, 'ionic_force': [6.0052439123392105, 2.971535697579384, -1.2920927703380585], 'ionic_force_magnitude': 6.823670755233991, 'motion_vector': [-1.8429718017578125, 0.5340690612792969, 3.6442413330078125], 'cosine_ionic_motion': -0.5048908635908108, 'ionic_motion_component': -3.44520902046945, 'ionic_force_x': 6.0052439123392105, 'ionic_force_y': 2.971535697579384, 'ionic_force_z': -1.2920927703380585, 'radial_force': 6.700222298452175, 'axial_force': -1.2920927703380585, 'before_closest_residue': 423, 'closest_residue': 780, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [5.069587707519531, 8.484151840209961, 7.271227836608887], 'magnitude': 12.269975662231445, 'distance': 5.201722621917725, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': 0.4291373195283767, 'motion_component': 5.265504527085966}, {'ion': 1320, 'force': [-0.18250830471515656, -4.807651519775391, -0.49011465907096863], 'magnitude': 4.836014270782471, 'distance': 8.285624504089355, 'before_closest_residue': 98, 'closest_residue': 455, 'next_closest_residue': 423, 'cosine_with_motion': -0.2017022843551575, 'motion_component': -0.975435141621853}, {'ion': 1469, 'force': [0.850151538848877, -0.5294232368469238, -5.994930744171143], 'magnitude': 6.078012943267822, 'distance': 7.390745162963867, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9466319012710269, 'motion_component': -5.753640939993872}, {'ion': 2436, 'force': [0.26801297068595886, -0.17554138600826263, -2.078275203704834], 'magnitude': 2.102825164794922, 'distance': 12.565143585205078, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.942369072941603, 'motion_component': -1.9816373740599276}]}, 5308: {'frame': 5308, 'ionic_force': [-3.9245860427618027, -5.353306509554386, -11.027286529541016], 'ionic_force_magnitude': 12.870948465318119, 'motion_vector': [-0.12729644775390625, 0.5117263793945312, -0.26439666748046875], 'cosine_ionic_motion': 0.08900058775676298, 'ionic_motion_component': 1.145521978400319, 'ionic_force_x': -3.9245860427618027, 'ionic_force_y': -5.353306509554386, 'ionic_force_z': -11.027286529541016, 'radial_force': 6.637790761411368, 'axial_force': -11.027286529541016, 'before_closest_residue': 780, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [0.1623639464378357, 0.4300653338432312, 3.4034218788146973], 'magnitude': 3.434326410293579, 'distance': 9.832144737243652, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': -0.3457480673528202, 'motion_component': -1.1874117610608668}, {'ion': 1320, 'force': [-3.1859545707702637, -5.096459865570068, 2.4922938346862793], 'magnitude': 6.506591796875, 'distance': 7.143190860748291, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.7455033842480661, 'motion_component': -4.850686286735993}, {'ion': 1469, 'force': [-1.04063880443573, -0.7825348973274231, -12.82127857208252], 'magnitude': 12.887221336364746, 'distance': 5.075623512268066, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4106676150977118, 'motion_component': 5.292364458409139}, {'ion': 2436, 'force': [0.13964338600635529, 0.09562291949987411, -4.101723670959473], 'magnitude': 4.1052141189575195, 'distance': 8.992928504943848, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4606960465227934, 'motion_component': 1.891255809716336}]}, 5309: {'frame': 5309, 'ionic_force': [-6.100982252508402, -3.1015712544322014, -15.906369686126709], 'ionic_force_magnitude': 17.31630229822387, 'motion_vector': [0.6568450927734375, -0.14005661010742188, -0.313629150390625], 'cosine_ionic_motion': 0.11029630434347097, 'ionic_motion_component': 1.909924148388446, 'ionic_force_x': -6.100982252508402, 'ionic_force_y': -3.1015712544322014, 'ionic_force_z': -15.906369686126709, 'radial_force': 6.844101744695401, 'axial_force': -15.906369686126709, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [0.20207388699054718, 0.08543962985277176, 2.6796698570251465], 'magnitude': 2.688636302947998, 'distance': 11.112276077270508, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': -0.3611103386395704, 'motion_component': -0.970894309377176}, {'ion': 1320, 'force': [-3.724456787109375, -3.0685253143310547, 2.46171236038208], 'magnitude': 5.417328834533691, 'distance': 7.828461647033691, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.6944816395866571, 'motion_component': -3.7622355398655856}, {'ion': 1469, 'force': [-2.5375022888183594, -0.4666903018951416, -17.041349411010742], 'magnitude': 17.235553741455078, 'distance': 4.388907432556152, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.29300374354212066, 'motion_component': 5.050081723024142}, {'ion': 2436, 'force': [-0.041097063571214676, 0.34820473194122314, -4.006402492523193], 'magnitude': 4.0217156410217285, 'distance': 9.085803985595703, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.39609276644881936, 'motion_component': 1.59297246126204}]}, 5310: {'frame': 5310, 'ionic_force': [-2.138845317065716, -6.399635553359985, -14.446752071380615], 'ionic_force_magnitude': 15.944862492919254, 'motion_vector': [-0.4894981384277344, 0.20468902587890625, 0.37158966064453125], 'cosine_ionic_motion': -0.5452217807443366, 'ionic_motion_component': -8.693486322113017, 'ionic_force_x': -2.138845317065716, 'ionic_force_y': -6.399635553359985, 'ionic_force_z': -14.446752071380615, 'radial_force': 6.747591756038824, 'axial_force': -14.446752071380615, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [-0.425532728433609, 0.4280744194984436, 4.451706409454346], 'magnitude': 4.4924397468566895, 'distance': 8.596623420715332, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 1105, 'cosine_with_motion': 0.6701482337154809, 'motion_component': 3.0106006276943322}, {'ion': 1320, 'force': [-2.6733267307281494, -4.865641117095947, 5.675074100494385], 'magnitude': 7.938992977142334, 'distance': 6.466753959655762, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 130, 'cosine_with_motion': 0.4708679390348454, 'motion_component': 3.7382171379287144}, {'ion': 1469, 'force': [0.8352939486503601, -1.7298543453216553, -20.9677677154541], 'magnitude': 21.055578231811523, 'distance': 3.970867872238159, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6272065415358462, 'motion_component': -13.206196705608171}, {'ion': 2436, 'force': [0.12472019344568253, -0.23221451044082642, -3.605764865875244], 'magnitude': 3.615386486053467, 'distance': 9.582783699035645, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6184975575539667, 'motion_component': -2.2361076710314904}]}, 5311: {'frame': 5311, 'ionic_force': [-1.5457566678524017, -3.735124170780182, -10.29975938796997], 'ionic_force_magnitude': 11.064608429466993, 'motion_vector': [0.5821189880371094, -0.71893310546875, 0.33875274658203125], 'cosine_ionic_motion': -0.15629080861675848, 'ionic_motion_component': -1.7292965984691986, 'ionic_force_x': -1.5457566678524017, 'ionic_force_y': -3.735124170780182, 'ionic_force_z': -10.29975938796997, 'radial_force': 4.042340441793158, 'axial_force': -10.29975938796997, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [0.2618166506290436, 0.38895392417907715, 3.28230881690979], 'magnitude': 3.315627336502075, 'distance': 10.006591796875, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 11</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>{5347: {'frame': 5347, 'ionic_force': [0.6853100061416626, -9.129887342453003, -11.733562916517258], 'ionic_force_magnitude': 14.88290937304499, 'motion_vector': [3.316211700439453, -1.65020751953125, -0.9902801513671875], 'cosine_ionic_motion': 0.5074709139954511, 'ionic_motion_component': 7.552643622450607, 'ionic_force_x': 0.6853100061416626, 'ionic_force_y': -9.129887342453003, 'ionic_force_z': -11.733562916517258, 'radial_force': 9.15557167469085, 'axial_force': -11.733562916517258, 'contributions': [{'ion': 1309, 'force': [-3.900376081466675, -0.4288240671157837, -0.44240328669548035], 'magnitude': 3.948739528656006, 'distance': 9.169376373291016, 'cosine_with_motion': -0.7786338398051467, 'motion_component': -3.0746222669723364}, {'ion': 1320, 'force': [5.2017621994018555, -9.052448272705078, -8.116565704345703], 'magnitude': 13.224363327026367, 'distance': 5.010506629943848, 'cosine_with_motion': 0.793340665917229, 'motion_component': 10.491425302286757}, {'ion': 2436, 'force': [-0.6160761117935181, 0.3513849973678589, -3.174593925476074], 'magnitude': 3.2528553009033203, 'distance': 10.102682113647461, 'cosine_with_motion': 0.04176044234126463, 'motion_component': 0.13584067736087846}]}, 5348: {'frame': 5348, 'ionic_force': [-2.9597952365875244, -4.185118928551674, -6.418415784835815], 'ionic_force_magnitude': 8.21411404082493, 'motion_vector': [1.4751319885253906, 0.6213607788085938, -1.0232925415039062], 'cosine_ionic_motion': -0.02554542998862456, 'ionic_motion_component': -0.20983307514847122, 'ionic_force_x': -2.9597952365875244, 'ionic_force_y': -4.185118928551674, 'ionic_force_z': -6.418415784835815, 'radial_force': 5.125973886848011, 'axial_force': -6.418415784835815, 'contributions': [{'ion': 1309, 'force': [-6.009511947631836, -2.5683140754699707, -1.4689178466796875], 'magnitude': 6.6983723640441895, 'distance': 7.04019021987915, 'cosine_with_motion': -0.7039018768949364, 'motion_component': -4.714996792595642}, {'ion': 1320, 'force': [2.708761215209961, -1.4557560682296753, -2.3566243648529053], 'magnitude': 3.874311685562134, 'distance': 9.25703239440918, 'cosine_with_motion': 0.7476143142621089, 'motion_component': 2.8964909137275363}, {'ion': 2436, 'force': [0.3409554958343506, -0.1610487848520279, -2.5928735733032227], 'magnitude': 2.6201491355895996, 'distance': 11.256568908691406, 'cosine_with_motion': 0.6139624104715719, 'motion_component': 1.6086729895284697}]}, 5349: {'frame': 5349, 'ionic_force': [-7.378105878829956, -6.646641850471497, -10.801924467086792], 'ionic_force_magnitude': 14.672963791964886, 'motion_vector': [-0.10723876953125, -1.5981407165527344, 3.5609359741210938], 'cosine_ionic_motion': -0.47216925748123195, 'ionic_motion_component': -6.9281224187010615, 'ionic_force_x': -7.378105878829956, 'ionic_force_y': -6.646641850471497, 'ionic_force_z': -10.801924467086792, 'radial_force': 9.93047301228216, 'axial_force': -10.801924467086792, 'contributions': [{'ion': 1309, 'force': [-10.252406120300293, -4.798220634460449, -6.5559773445129395], 'magnitude': 13.08111572265625, 'distance': 5.037866592407227, 'cosine_with_motion': -0.28541032674556904, 'motion_component': -3.733485544288841}, {'ion': 1320, 'force': [2.3740317821502686, -1.7368981838226318, -2.094464063644409], 'magnitude': 3.61104154586792, 'distance': 9.588546752929688, 'cosine_with_motion': -0.35015323973539414, 'motion_component': -1.2644179383602139}, {'ion': 2436, 'force': [0.5002684593200684, -0.11152303218841553, -2.1514830589294434], 'magnitude': 2.2116928100585938, 'distance': 12.25199031829834, 'cosine_with_motion': -0.872733684797831, 'motion_component': -1.9302188522429757}]}, 5350: {'frame': 5350, 'ionic_force': [-0.14506256580352783, -16.753881365060806, -3.0993531867861748], 'ionic_force_magnitude': 17.038766801590157, 'motion_vector': [2.5827255249023438, 0.7509269714355469, 2.464935302734375], 'cosine_ionic_motion': -0.33131159151419914, 'ionic_motion_component': -5.645140946474135, 'ionic_force_x': -0.14506256580352783, 'ionic_force_y': -16.753881365060806, 'ionic_force_z': -3.0993531867861748, 'radial_force': 16.754509361438465, 'axial_force': -3.0993531867861748, 'contributions': [{'ion': 1309, 'force': [-7.1796159744262695, -10.836474418640137, 3.318307876586914], 'magnitude': 13.415931701660156, 'distance': 4.974605083465576, 'cosine_with_motion': -0.3779898179059257, 'motion_component': -5.07108568105761}, {'ion': 1320, 'force': [5.264742851257324, -4.707367897033691, -0.06457030028104782], 'magnitude': 7.062648296356201, 'distance': 6.856228351593018, 'cosine_with_motion': 0.3843443305678448, 'motion_component': 2.714488781801923}, {'ion': 2434, 'force': [0.3296545743942261, -0.23305991291999817, -1.7742886543273926], 'magnitude': 1.8196399211883545, 'distance': 13.50754165649414, 'cosine_with_motion': -0.5569081574761272, 'motion_component': -1.0133722924457365}, {'ion': 2436, 'force': [1.4401559829711914, -0.97697913646698, -4.578802108764648], 'magnitude': 4.8983635902404785, 'distance': 8.232723236083984, 'cosine_with_motion': -0.4644758616720765, 'motion_component': -2.2751716672537476}]}, 5351: {'frame': 5351, 'ionic_force': [6.5781702399253845, -10.670942857861519, 6.412924081087112], 'ionic_force_magnitude': 14.080729400530808, 'motion_vector': [-4.924442291259766, -0.13016128540039062, 1.0756683349609375], 'cosine_ionic_motion': -0.3395388214293875, 'ionic_motion_component': -4.7809542655223565, 'ionic_force_x': 6.5781702399253845, 'ionic_force_y': -10.670942857861519, 'ionic_force_z': 6.412924081087112, 'radial_force': 12.535603104006832, 'axial_force': 6.412924081087112, 'contributions': [{'ion': 1309, 'force': [-0.7276131510734558, -8.576908111572266, 12.734542846679688], 'magnitude': 15.370795249938965, 'distance': 4.647515773773193, 'cosine_with_motion': 0.23737887367365, 'motion_component': 3.648702129922416}, {'ion': 1320, 'force': [2.105349540710449, -1.2945811748504639, 0.18129947781562805], 'magnitude': 2.478165864944458, 'distance': 11.574542999267578, 'cosine_with_motion': -0.8006204730018646, 'motion_component': -1.984070416350552}, {'ion': 2434, 'force': [1.0735446214675903, -0.11892910301685333, -2.175081729888916], 'magnitude': 2.428502082824707, 'distance': 11.692296028137207, 'cosine_with_motion': -0.6215390624157976, 'motion_component': -1.5094089525808843}, {'ion': 2436, 'force': [4.126889228820801, -0.680524468421936, -4.327836513519287], 'magnitude': 6.018678665161133, 'distance': 7.427085876464844, 'cosine_with_motion': -0.8201429451411554, 'motion_component': -4.93617713739299}]}, 5352: {'frame': 5352, 'ionic_force': [9.924710154533386, -10.801763534545898, -9.8836290538311], 'ionic_force_magnitude': 17.687964562986828, 'motion_vector': [1.6225547790527344, 0.3573951721191406, -0.7139053344726562], 'cosine_ionic_motion': 0.6033578075989015, 'ionic_motion_component': 10.672171519610794, 'ionic_force_x': 9.924710154533386, 'ionic_force_y': -10.801763534545898, 'ionic_force_z': -9.8836290538311, 'radial_force': 14.668945671306565, 'axial_force': -9.8836290538311, 'contributions': [{'ion': 1309, 'force': [5.455544471740723, -4.775212287902832, 4.03164005279541], 'magnitude': 8.295766830444336, 'distance': 6.326169013977051, 'cosine_with_motion': 0.28444257656282923, 'motion_component': 2.359669156171975}, {'ion': 1320, 'force': [3.4328699111938477, -2.7567880153656006, 0.24743130803108215], 'magnitude': 4.409727573394775, 'distance': 8.676871299743652, 'cosine_with_motion': 0.5527925122176478, 'motion_component': 2.4376644442580866}, {'ion': 2434, 'force': [0.07548081874847412, -0.4966468811035156, -2.923949956893921], 'magnitude': 2.9667892456054688, 'distance': 10.57853889465332, 'cosine_with_motion': 0.37882856508898916, 'motion_component': 1.1239045384416073}, {'ion': 2436, 'force': [0.9608149528503418, -2.77311635017395, -11.238750457763672], 'magnitude': 11.615629196166992, 'distance': 5.346230506896973, 'cosine_with_motion': 0.4090121636963402, 'motion_component': 4.750933804418082}]}, 5353: {'frame': 5353, 'ionic_force': [11.046917110681534, -10.955666691064835, -16.785257935523987], 'ionic_force_magnitude': 22.88680611745656, 'motion_vector': [-1.0786094665527344, -0.3579292297363281, -0.06634521484375], 'cosine_ionic_motion': -0.2640805144456472, 'ionic_motion_component': -6.043959533515713, 'ionic_force_x': 11.046917110681534, 'ionic_force_y': -10.955666691064835, 'ionic_force_z': -16.785257935523987, 'radial_force': 15.558310007708934, 'axial_force': -16.785257935523987, 'contributions': [{'ion': 1309, 'force': [0.8205000758171082, -5.329401016235352, 1.1785228252410889], 'magnitude': 5.519479274749756, 'distance': 7.755681991577148, 'cosine_with_motion': 0.15029737672327664, 'motion_component': 0.8295632579359236}, {'ion': 1320, 'force': [3.7472195625305176, -2.678145170211792, 0.29563629627227783], 'magnitude': 4.615356922149658, 'distance': 8.481377601623535, 'cosine_with_motion': -0.5905579328226201, 'motion_component': -2.7256354706602135}, {'ion': 2434, 'force': [0.39906546473503113, -0.3938721716403961, -2.652449131011963], 'magnitude': 2.7110652923583984, 'distance': 11.066213607788086, 'cosine_with_motion': -0.0367698516531741, 'motion_component': -0.09968546798404}, {'ion': 2436, 'force': [6.080132007598877, -2.554248332977295, -15.60696792602539], 'magnitude': 16.943130493164062, 'distance': 4.426620006561279, 'cosine_with_motion': -0.23892883827431421, 'motion_component': -4.0482022507508475}]}, 5354: {'frame': 5354, 'ionic_force': [-0.8884754180908203, -10.587919175624847, -4.579100914299488], 'ionic_force_magnitude': 11.569856793472182, 'motion_vector': [-1.3265037536621094, 1.3291473388671875, 1.2285842895507812], 'cosine_ionic_motion': -0.7133261353379372, 'ionic_motion_component': -8.25308123290089, 'ionic_force_x': -0.8884754180908203, 'ionic_force_y': -10.587919175624847, 'ionic_force_z': -4.579100914299488, 'radial_force': 10.62513157744957, 'axial_force': -4.579100914299488, 'contributions': [{'ion': 1309, 'force': [-6.627227306365967, -5.314355373382568, 7.1092095375061035], 'magnitude': 11.077156066894531, 'distance': 5.4746317863464355, 'cosine_with_motion': 0.4208694645766861, 'motion_component': 4.662036524869421}, {'ion': 1320, 'force': [3.325421094894409, -3.054407835006714, 0.12004440277814865], 'magnitude': 4.5168843269348145, 'distance': 8.573330879211426, 'cosine_with_motion': -0.8211762565733415, 'motion_component': -3.709158100849936}, {'ion': 2434, 'force': [0.26523327827453613, -0.28264373540878296, -2.6325316429138184], 'magnitude': 2.6609132289886475, 'distance': 11.170013427734375, 'cosine_with_motion': -0.6634877643934309, 'motion_component': -1.7654833460838617}, {'ion': 2436, 'force': [2.148097515106201, -1.9365122318267822, -9.175823211669922], 'magnitude': 9.620818138122559, 'distance': 5.874393939971924, 'cosine_with_motion': -0.773372547498979, 'motion_component': -7.440476332000287}]}, 5355: {'frame': 5355, 'ionic_force': [-1.0782689899206161, -3.377299338579178, -19.434728145599365], 'ionic_force_magnitude': 19.755441603020266, 'motion_vector': [-0.3754844665527344, 2.017047882080078, -2.8304595947265625], 'cosine_ionic_motion': 0.7037424023399148, 'ionic_motion_component': 13.90274193299538, 'ionic_force_x': -1.0782689899206161, 'ionic_force_y': -3.377299338579178, 'ionic_force_z': -19.434728145599365, 'radial_force': 3.5452524362859945, 'axial_force': -19.434728145599365, 'contributions': [{'ion': 1309, 'force': [-4.155211925506592, -0.5779337286949158, 3.243894577026367], 'magnitude': 5.303078651428223, 'distance': 7.912341117858887, 'cosine_with_motion': -0.4739911959579365, 'motion_component': -2.5136126988026177}, {'ion': 1320, 'force': [5.40611457824707, -3.8656556606292725, 1.663935661315918], 'magnitude': 6.851134777069092, 'distance': 6.961258888244629, 'cosine_with_motion': -0.6069518120289323, 'motion_component': -4.15830878571586}, {'ion': 2434, 'force': [-0.2116548866033554, 0.1417645514011383, -3.8158822059631348], 'magnitude': 3.824375867843628, 'distance': 9.31727123260498, 'cosine_with_motion': 0.835196737960166, 'motion_component': 3.1941063817137327}, {'ion': 2436, 'force': [-2.1175167560577393, 0.9245254993438721, -20.526676177978516], 'magnitude': 20.656307220458984, 'distance': 4.009061336517334, 'cosine_with_motion': 0.8414164330538239, 'motion_component': 17.380556983894365}]}, 5356: {'frame': 5356, 'ionic_force': [9.193988606333733, -9.341656267642975, -8.68997049331665], 'ionic_force_magnitude': 15.726142422441105, 'motion_vector': [-5.566600799560547, -5.137775421142578, 0.14322662353515625], 'cosine_ionic_motion': -0.03716797145292092, 'ionic_motion_component': -0.5845088126218596, 'ionic_force_x': 9.193988606333733, 'ionic_force_y': -9.341656267642975, 'ionic_force_z': -8.68997049331665, 'radial_force': 13.107096105399846, 'axial_force': -8.68997049331665, 'contributions': [{'ion': 1309, 'force': [-5.083637714385986, 1.7815605401992798, 4.272593021392822], 'magnitude': 6.875491142272949, 'distance': 6.948917865753174, 'cosine_with_motion': 0.37927224489761086, 'motion_component': 2.6076830443856958}, {'ion': 1320, 'force': [15.738530158996582, -14.13753890991211, -3.5142836570739746], 'magnitude': 21.44577980041504, 'distance': 3.934577465057373, 'cosine_with_motion': -0.09525757946206342, 'motion_component': -2.042873198654397}, {'ion': 2434, 'force': [-0.2095593959093094, 0.4638260006904602, -2.334017753601074], 'magnitude': 2.3888676166534424, 'distance': 11.788891792297363, 'cosine_with_motion': -0.08568202920856213, 'motion_component': -0.20468302640401867}, {'ion': 2436, 'force': [-1.2513444423675537, 2.5504961013793945, -7.114262104034424], 'magnitude': 7.660523414611816, 'distance': 6.583241939544678, 'cosine_with_motion': -0.12331218202884321, 'motion_component': -0.9446358543236686}]}, 5357: {'frame': 5357, 'ionic_force': [-6.36072164773941, -7.776129573583603, -3.584123432636261], 'ionic_force_magnitude': 10.666438571779926, 'motion_vector': [1.0815353393554688, -1.1651802062988281, 1.2048263549804688], 'cosine_ionic_motion': -0.10043836085855601, 'ionic_motion_component': -1.071319606348053, 'ionic_force_x': -6.36072164773941, 'ionic_force_y': -7.776129573583603, 'ionic_force_z': -3.584123432636261, 'radial_force': 10.046241636810368, 'axial_force': -3.584123432636261, 'contributions': [{'ion': 1309, 'force': [-1.7606245279312134, -0.44900551438331604, 1.1280972957611084], 'magnitude': 2.13869309425354, 'distance': 12.459333419799805, 'cosine_with_motion': -0.005120338601344486, 'motion_component': -0.010950832851939651}, {'ion': 1320, 'force': [-1.3347965478897095, -6.032811641693115, -0.6402768492698669], 'magnitude': 6.211799621582031, 'distance': 7.310723304748535, 'cosine_with_motion': 0.38853205719115985, 'motion_component': 2.4134832243306086}, {'ion': 2434, 'force': [-0.9485629200935364, -0.36116552352905273, -1.7239831686019897], 'magnitude': 2.000582456588745, 'distance': 12.882223129272461, 'cosine_with_motion': -0.6721193525377495, 'motion_component': -1.344630176815933}, {'ion': 2436, 'force': [-2.316737651824951, -0.9331468939781189, -2.3479607105255127], 'magnitude': 3.427966594696045, 'distance': 9.84126091003418, 'cosine_with_motion': -0.6211325241080135, 'motion_component': -2.129221633842434}]}, 5358: {'frame': 5358, 'ionic_force': [-8.373949587345123, -10.114233255386353, -2.16071218252182], 'ionic_force_magnitude': 13.307494999866014, 'motion_vector': [-0.13986587524414062, 0.56707763671875, 0.13983154296875], 'cosine_ionic_motion': -0.6089035342787845, 'ionic_motion_component': -8.102980737815669, 'ionic_force_x': -8.373949587345123, 'ionic_force_y': -10.114233255386353, 'ionic_force_z': -2.16071218252182, 'radial_force': 13.130908043077628, 'axial_force': -2.16071218252182, 'contributions': [{'ion': 1309, 'force': [-2.585419178009033, -2.5263538360595703, 2.679021120071411], 'magnitude': 4.499334335327148, 'distance': 8.590034484863281, 'cosine_with_motion': -0.2577219996351968, 'motion_component': -1.1595774628844175}, {'ion': 1320, 'force': [-1.769490361213684, -4.937245845794678, 0.018840014934539795], 'magnitude': 5.244792461395264, 'distance': 7.956185340881348, 'cosine_with_motion': -0.8094466141356852, 'motion_component': -4.245379473738665}, {'ion': 2434, 'force': [-0.9104146361351013, -0.6412608623504639, -1.7891393899917603], 'magnitude': 2.107389450073242, 'distance': 12.551528930664062, 'cosine_with_motion': -0.3843774113266263, 'motion_component': -0.8100328801187882}, {'ion': 2436, 'force': [-3.1086254119873047, -2.0093727111816406, -3.0694339275360107], 'magnitude': 4.808591842651367, 'distance': 8.309216499328613, 'cosine_with_motion': -0.39262866442624267, 'motion_component': -1.887990983593486}]}, 5359: {'frame': 5359, 'ionic_force': [-7.488657891750336, -9.668851613998413, -3.8453208655118942], 'ionic_force_magnitude': 12.82003046454787, 'motion_vector': [-0.3754844665527344, 0.34723663330078125, 0.0055084228515625], 'cosine_ionic_motion': -0.08642539269380385, 'ionic_motion_component': -1.1079761672450783, 'ionic_force_x': -7.488657891750336, 'ionic_force_y': -9.668851613998413, 'ionic_force_z': -3.8453208655118942, 'radial_force': 12.229746054321582, 'axial_force': -3.8453208655118942, 'contributions': [{'ion': 1309, 'force': [-3.55322265625, -1.968692660331726, 0.8038131594657898], 'magnitude': 4.140924453735352, 'distance': 8.95406723022461, 'cosine_with_motion': 0.3092681448214228, 'motion_component': 1.2806561095230804}, {'ion': 1320, 'force': [-0.5556600689888, -5.521777629852295, -0.23913930356502533], 'magnitude': 5.554815292358398, 'distance': 7.730974197387695, 'cosine_with_motion': -0.6018995063443169, 'motion_component': -3.3434406354042325}, {'ion': 2434, 'force': [-0.9361525774002075, -0.5566215515136719, -1.8760818243026733], 'magnitude': 2.169306993484497, 'distance': 12.37110710144043, 'cosine_with_motion': 0.133298819524226, 'motion_component': 0.2891660423462572}, {'ion': 2436, 'force': [-2.443622589111328, -1.6217597723007202, -2.5339128971099854], 'magnitude': 3.8758368492126465, 'distance': 9.255210876464844, 'cosine_with_motion': 0.1717416192223846, 'motion_component': 0.6656424831540266}]}, 5360: {'frame': 5360, 'ionic_force': [-5.99063166975975, -12.09947857260704, -4.111779734492302], 'ionic_force_magnitude': 14.113531879607137, 'motion_vector': [0.4962959289550781, -1.1936683654785156, -0.0410003662109375], 'cosine_ionic_motion': 0.637564935265345, 'ionic_motion_component': 8.998293039187107, 'ionic_force_x': -5.99063166975975, 'ionic_force_y': -12.09947857260704, 'ionic_force_z': -4.111779734492302, 'radial_force': 13.50129806839718, 'axial_force': -4.111779734492302, 'contributions': [{'ion': 1309, 'force': [-1.7648735046386719, -0.8681292533874512, 0.4014160633087158], 'magnitude': 2.0073769092559814, 'distance': 12.860404014587402, 'cosine_with_motion': 0.05542519617332915, 'motion_component': 0.11125925468247111}, {'ion': 1320, 'force': [-0.222377210855484, -9.145050048828125, 0.049248531460762024], 'magnitude': 9.147886276245117, 'distance': 6.024328708648682, 'cosine_with_motion': 0.9131206022804962, 'motion_component': 8.35312313240585}, {'ion': 2434, 'force': [-0.8280560374259949, -0.4974512755870819, -1.6552377939224243], 'magnitude': 1.91649329662323, 'distance': 13.161803245544434, 'cosine_with_motion': 0.10113794630997673, 'motion_component': 0.1938302006527346}, {'ion': 2436, 'force': [-3.1753249168395996, -1.5888479948043823, -2.9072065353393555], 'magnitude': 4.589005947113037, 'distance': 8.505693435668945, 'cosine_with_motion': 0.074107570812104, 'motion_component': 0.340080087499274}]}, 5361: {'frame': 5361, 'ionic_force': [-5.120174393057823, -19.02680516242981, -0.25727808475494385], 'ionic_force_magnitude': 19.705372174036345, 'motion_vector': [-0.574737548828125, 0.9560508728027344, -0.38732147216796875], 'cosine_ionic_motion': -0.6510080193920725, 'ionic_motion_component': -12.82835531040306, 'ionic_force_x': -5.120174393057823, 'ionic_force_y': -19.02680516242981, 'ionic_force_z': -0.25727808475494385, 'radial_force': 19.703692560136812, 'axial_force': -0.25727808475494385, 'contributions': [{'ion': 1309, 'force': [-1.4405096769332886, -0.9803712368011475, 0.35021817684173584], 'magnitude': 1.7773150205612183, 'distance': 13.667428970336914, 'cosine_with_motion': -0.1167459297738805, 'motion_component': -0.2074942939315676}, {'ion': 1320, 'force': [0.1950037032365799, -15.115640640258789, 4.1602349281311035], 'magnitude': 15.678908348083496, 'distance': 4.601624011993408, 'cosine_with_motion': -0.8736388570428829, 'motion_component': -13.69770373827267}, {'ion': 2434, 'force': [-0.9663851857185364, -0.6437287330627441, -2.0172598361968994], 'magnitude': 2.3275790214538574, 'distance': 11.943093299865723, 'cosine_with_motion': 0.2624381036375999, 'motion_component': 0.6108454331708925}, {'ion': 2436, 'force': [-2.908283233642578, -2.287064552307129, -2.750471353530884], 'magnitude': 4.610191822052002, 'distance': 8.486127853393555, 'cosine_with_motion': 0.10107972759484486, 'motion_component': 0.4659969298493891}]}, 5362: {'frame': 5362, 'ionic_force': [-2.3333985209465027, -17.115698158740997, 4.077326849102974], 'ionic_force_magnitude': 17.748703230182798, 'motion_vector': [0.4037361145019531, -0.2184600830078125, -0.226226806640625], 'cosine_ionic_motion': 0.2063827837405274, 'ionic_motion_component': 3.6630267804296164, 'ionic_force_x': -2.3333985209465027, 'ionic_force_y': -17.115698158740997, 'ionic_force_z': 4.077326849102974, 'radial_force': 17.274023043827555, 'axial_force': 4.077326849102974, 'contributions': [{'ion': 1309, 'force': [-1.5750622749328613, -0.9575368165969849, 0.24507339298725128], 'magnitude': 1.8595050573349, 'distance': 13.361966133117676, 'cosine_with_motion': -0.5066735521869951, 'motion_component': -0.9421620101963059}, {'ion': 1320, 'force': [3.2834606170654297, -13.994690895080566, 8.046475410461426], 'magnitude': 16.473562240600586, 'distance': 4.489265441894531, 'cosine_with_motion': 0.3039632998783835, 'motion_component': 5.007358344099799}, {'ion': 2434, 'force': [-0.9333657622337341, -0.5060002207756042, -1.6682040691375732], 'magnitude': 1.977400541305542, 'distance': 12.957514762878418, 'cosine_with_motion': 0.1097857354681624, 'motion_component': 0.2170903667758015}, {'ion': 2436, 'force': [-3.108431100845337, -1.6574702262878418, -2.54601788520813], 'magnitude': 4.346465110778809, 'distance': 8.739789009094238, 'cosine_with_motion': -0.14247442357158616, 'motion_component': -0.6192601042226045}]}, 5363: {'frame': 5363, 'ionic_force': [-4.615044325590134, -13.802704691886902, 2.612096294760704], 'ionic_force_magnitude': 14.786356481287097, 'motion_vector': [-0.16725540161132812, -0.3708457946777344, 0.30941009521484375], 'cosine_ionic_motion': 0.8863761547181133, 'ionic_motion_component': 13.106273800174508, 'ionic_force_x': -4.615044325590134, 'ionic_force_y': -13.802704691886902, 'ionic_force_z': 2.612096294760704, 'radial_force': 14.553806750764501, 'axial_force': 2.612096294760704, 'contributions': [{'ion': 1309, 'force': [-1.4222971200942993, -1.290872573852539, 0.12278829514980316], 'magnitude': 1.924670934677124, 'distance': 13.133811950683594, 'cosine_with_motion': 0.7670795510974251, 'motion_component': 1.476375688362606}, {'ion': 1320, 'force': [0.3337534964084625, -10.261008262634277, 7.174679279327393], 'magnitude': 12.525003433227539, 'distance': 5.148492813110352, 'cosine_with_motion': 0.9324657304241323, 'motion_component': 11.679136241201018}, {'ion': 2434, 'force': [-0.8723053932189941, -0.5652945041656494, -1.9188066720962524], 'magnitude': 2.182267904281616, 'distance': 12.334314346313477, 'cosine_with_motion': -0.2135258965253157, 'motion_component': -0.4659707309890351}, {'ion': 2436, 'force': [-2.6541953086853027, -1.685529351234436, -2.7665646076202393], 'magnitude': 4.188035488128662, 'distance': 8.903563499450684, 'cosine_with_motion': 0.09950545026923256, 'motion_component': 0.41673236184657725}]}, 5364: {'frame': 5364, 'ionic_force': [-5.364780865609646, -11.734835743904114, 1.9194905273616314], 'ionic_force_magnitude': 13.044987066189526, 'motion_vector': [0.7199592590332031, 0.047824859619140625, -0.00384521484375], 'cosine_ionic_motion': -0.47074968515216353, 'ionic_motion_component': -6.1409235542227645, 'ionic_force_x': -5.364780865609646, 'ionic_force_y': -11.734835743904114, 'ionic_force_z': 1.9194905273616314, 'radial_force': 12.90299359344261, 'axial_force': 1.9194905273616314, 'contributions': [{'ion': 1309, 'force': [-1.2786661386489868, -1.378605604171753, 0.06221873685717583], 'magnitude': 1.8813323974609375, 'distance': 13.284226417541504, 'cosine_with_motion': -0.7269007740173844, 'motion_component': -1.3675419927947812}, {'ion': 1320, 'force': [-0.05913498252630234, -7.958459854125977, 6.173501968383789], 'magnitude': 10.072373390197754, 'distance': 5.741206169128418, 'cosine_with_motion': -0.061494054302821094, 'motion_component': -0.6193910793836221}, {'ion': 2434, 'force': [-0.9266603589057922, -0.606224775314331, -1.7449246644973755], 'magnitude': 2.0666325092315674, 'distance': 12.674692153930664, 'cosine_with_motion': -0.462342170077388, 'motion_component': -0.9554913652822146}, {'ion': 2436, 'force': [-3.1003193855285645, -1.7915455102920532, -2.571305513381958], 'magnitude': 4.408313274383545, 'distance': 8.678262710571289, 'cosine_with_motion': -0.7255607242424008, 'motion_component': -3.198499114070995}]}, 5365: {'frame': 5365, 'ionic_force': [-4.773198127746582, -14.88428270816803, 1.0287406668066978], 'ionic_force_magnitude': 15.664724685194285, 'motion_vector': [-0.7137031555175781, 0.053272247314453125, -0.5380477905273438], 'cosine_ionic_motion': 0.14688671051438024, 'ionic_motion_component': 2.3009398801215992, 'ionic_force_x': -4.773198127746582, 'ionic_force_y': -14.88428270816803, 'ionic_force_z': 1.0287406668066978, 'radial_force': 15.630908230278665, 'axial_force': 1.0287406668066978, 'contributions': [{'ion': 1309, 'force': [-0.9053996205329895, -1.410875916481018, 0.084062360227108], 'magnitude': 1.6785070896148682, 'distance': 14.06395435333252, 'cosine_with_motion': 0.3498541792620414, 'motion_component': 0.5872326946989048}, {'ion': 1320, 'force': [0.3944142460823059, -10.42065715789795, 5.925753593444824], 'magnitude': 11.994174003601074, 'distance': 5.261188507080078, 'cosine_with_motion': -0.37478686319241056, 'motion_component': -4.495258911100009}, {'ion': 2434, 'force': [-0.8353512287139893, -0.7200510501861572, -1.9241082668304443], 'magnitude': 2.217764139175415, 'distance': 12.235208511352539, 'cosine_with_motion': 0.8022675846631492, 'motion_component': 1.7792402857389131}, {'ion': 2436, 'force': [-3.426861524581909, -2.3326985836029053, -3.05696702003479], 'magnitude': 5.150719165802002, 'distance': 8.028512954711914, 'cosine_with_motion': 0.8600207886859776, 'motion_component': 4.429725728516766}]}, 5366: {'frame': 5366, 'ionic_force': [-7.155528903007507, -14.01739877462387, 7.555211916565895], 'ionic_force_magnitude': 17.457671362264268, 'motion_vector': [0.0323638916015625, -0.11964035034179688, 0.4410858154296875], 'cosine_ionic_motion': 0.5973538208346165, 'ionic_motion_component': 10.428406691123625, 'ionic_force_x': -7.155528903007507, 'ionic_force_y': -14.01739877462387, 'ionic_force_z': 7.555211916565895, 'radial_force': 15.738140369452886, 'axial_force': 7.555211916565895, 'contributions': [{'ion': 1309, 'force': [-1.2609608173370361, -1.393578290939331, -0.11961029469966888], 'magnitude': 1.8831859827041626, 'distance': 13.277687072753906, 'cosine_with_motion': 0.08479238949629006, 'motion_component': 0.15967983512905182}, {'ion': 1320, 'force': [-2.2902896404266357, -10.353372573852539, 11.880364418029785], 'magnitude': 15.924220085144043, 'distance': 4.566042423248291, 'cosine_with_motion': 0.8778571958683916, 'motion_component': 13.97919184290714}, {'ion': 2434, 'force': [-0.7939726114273071, -0.5141727328300476, -1.6001249551773071], 'magnitude': 1.8588076829910278, 'distance': 13.364472389221191, 'cosine_with_motion': -0.7866795238692053, 'motion_component': -1.462285938092987}, {'ion': 2436, 'force': [-2.8103058338165283, -1.7562751770019531, -2.605417251586914], 'magnitude': 4.215509414672852, 'distance': 8.874502182006836, 'cosine_with_motion': -0.5333112914507774, 'motion_component': -2.248178821084748}]}, 5367: {'frame': 5367, 'ionic_force': [-10.474521219730377, -7.64684385061264, -1.9239774346351624], 'ionic_force_magnitude': 13.110740056427767, 'motion_vector': [0.06612777709960938, -0.14238357543945312, 0.14096832275390625], 'cosine_ionic_motion': 0.045153985928468254, 'ionic_motion_component': 0.5920021720197445, 'ionic_force_x': -10.474521219730377, 'ionic_force_y': -7.64684385061264, 'ionic_force_z': -1.9239774346351624, 'radial_force': 12.968801627684583, 'axial_force': -1.9239774346351624, 'contributions': [{'ion': 1309, 'force': [-2.1570794582366943, -3.1891884803771973, 1.5716099739074707], 'magnitude': 4.158590316772461, 'distance': 8.935029029846191, 'cosine_with_motion': 0.6074449589642145, 'motion_component': 2.5261146834102273}, {'ion': 1320, 'force': [-4.7571210861206055, -2.028890371322632, 0.9322972893714905], 'magnitude': 5.255071640014648, 'distance': 7.948400020599365, 'cosine_with_motion': 0.09535427561499123, 'motion_component': 0.5010935265026362}, {'ion': 2434, 'force': [-0.8019500374794006, -0.6224215626716614, -1.7185429334640503], 'magnitude': 1.9959765672683716, 'distance': 12.897078514099121, 'cosine_with_motion': -0.4907397782220592, 'motion_component': -0.9795050759979063}, {'ion': 2436, 'force': [-2.7583706378936768, -1.80634343624115, -2.7093417644500732], 'magnitude': 4.267553806304932, 'distance': 8.820221900939941, 'cosine_with_motion': -0.34110894490204924, 'motion_component': -1.4557008757963885}]}, 5368: {'frame': 5368, 'ionic_force': [-7.8661617040634155, -5.908215522766113, -2.403372425585985], 'ionic_force_magnitude': 10.127176784968029, 'motion_vector': [-0.2716789245605469, 1.168243408203125, -0.486358642578125], 'cosine_ionic_motion': -0.27436994724357705, 'ionic_motion_component': -2.7785929602180564, 'ionic_force_x': -7.8661617040634155, 'ionic_force_y': -5.908215522766113, 'ionic_force_z': -2.403372425585985, 'radial_force': 9.837861079418042, 'axial_force': -2.403372425585985, 'contributions': [{'ion': 1309, 'force': [-1.2717992067337036, -1.4661600589752197, -0.025815505534410477], 'magnitude': 1.9410731792449951, 'distance': 13.078203201293945, 'cosine_with_motion': -0.5392528651463202, 'motion_component': -1.0467292586320212}, {'ion': 1320, 'force': [-2.6795947551727295, -1.736313819885254, 2.1068739891052246], 'magnitude': 3.825432300567627, 'distance': 9.315985679626465, 'cosine_with_motion': -0.4696160162881312, 'motion_component': -1.7964842439859154}, {'ion': 2434, 'force': [-0.9058058261871338, -0.6099779605865479, -1.7394031286239624], 'magnitude': 2.0537965297698975, 'distance': 12.714237213134766, 'cosine_with_motion': 0.14275172396010247, 'motion_component': 0.29318300798421504}, {'ion': 2436, 'force': [-3.0089619159698486, -2.095763683319092, -2.745027780532837], 'magnitude': 4.580530166625977, 'distance': 8.513559341430664, 'cosine_with_motion': -0.049898693700076234, 'motion_component': -0.22856246161882865}]}, 5369: {'frame': 5369, 'ionic_force': [-6.711408376693726, -4.462401032447815, -3.780743934214115], 'ionic_force_magnitude': 8.90224971955083, 'motion_vector': [0.5668296813964844, -0.4966011047363281, 0.5632095336914062], 'cosine_ionic_motion': -0.4438709940897048, 'ionic_motion_component': -3.951450432651823, 'ionic_force_x': -6.711408376693726, 'ionic_force_y': -4.462401032447815, 'ionic_force_z': -3.780743934214115, 'radial_force': 8.059530096298793, 'axial_force': -3.780743934214115, 'contributions': [{'ion': 1309, 'force': [-1.5613667964935303, -1.5342515707015991, -0.11372516304254532], 'magnitude': 2.1919689178466797, 'distance': 12.306989669799805, 'cosine_with_motion': -0.09076123179609208, 'motion_component': -0.19894579554980885}, {'ion': 1320, 'force': [-2.044916868209839, -1.249974012374878, 0.6413288116455078], 'magnitude': 2.4810123443603516, 'distance': 11.567900657653809, 'cosine_with_motion': -0.07590719605042631, 'motion_component': -0.18832669687147074}, {'ion': 2434, 'force': [-0.7636282444000244, -0.5087323188781738, -1.6250380277633667], 'magnitude': 1.8661953210830688, 'distance': 13.337992668151855, 'cosine_with_motion': -0.623928444178269, 'motion_component': -1.1643723905510441}, {'ion': 2436, 'force': [-2.341496467590332, -1.169443130493164, -2.683309555053711], 'magnitude': 3.748379945755005, 'distance': 9.411248207092285, 'cosine_with_motion': -0.6402247461472825, 'motion_component': -2.3998056755567063}]}, 5370: {'frame': 5370, 'ionic_force'</t>
+          <t>{5347: {'frame': 5347, 'ionic_force': [0.6853100061416626, -9.129887342453003, -11.733562916517258], 'ionic_force_magnitude': 14.88290937304499, 'motion_vector': [3.316211700439453, -1.65020751953125, -0.9902801513671875], 'cosine_ionic_motion': 0.5074709139954511, 'ionic_motion_component': 7.552643622450607, 'ionic_force_x': 0.6853100061416626, 'ionic_force_y': -9.129887342453003, 'ionic_force_z': -11.733562916517258, 'radial_force': 9.15557167469085, 'axial_force': -11.733562916517258, 'before_closest_residue': None, 'closest_residue': 130, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [-3.900376081466675, -0.4288240671157837, -0.44240328669548035], 'magnitude': 3.948739528656006, 'distance': 9.169376373291016, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.7786338398051467, 'motion_component': -3.0746222669723364}, {'ion': 1320, 'force': [5.2017621994018555, -9.052448272705078, -8.116565704345703], 'magnitude': 13.224363327026367, 'distance': 5.010506629943848, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.793340665917229, 'motion_component': 10.491425302286757}, {'ion': 2436, 'force': [-0.6160761117935181, 0.3513849973678589, -3.174593925476074], 'magnitude': 3.2528553009033203, 'distance': 10.102682113647461, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.04176044234126463, 'motion_component': 0.13584067736087846}]}, 5348: {'frame': 5348, 'ionic_force': [-2.9597952365875244, -4.185118928551674, -6.418415784835815], 'ionic_force_magnitude': 8.21411404082493, 'motion_vector': [1.4751319885253906, 0.6213607788085938, -1.0232925415039062], 'cosine_ionic_motion': -0.02554542998862456, 'ionic_motion_component': -0.20983307514847122, 'ionic_force_x': -2.9597952365875244, 'ionic_force_y': -4.185118928551674, 'ionic_force_z': -6.418415784835815, 'radial_force': 5.125973886848011, 'axial_force': -6.418415784835815, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [-6.009511947631836, -2.5683140754699707, -1.4689178466796875], 'magnitude': 6.6983723640441895, 'distance': 7.04019021987915, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.7039018768949364, 'motion_component': -4.714996792595642}, {'ion': 1320, 'force': [2.708761215209961, -1.4557560682296753, -2.3566243648529053], 'magnitude': 3.874311685562134, 'distance': 9.25703239440918, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.7476143142621089, 'motion_component': 2.8964909137275363}, {'ion': 2436, 'force': [0.3409554958343506, -0.1610487848520279, -2.5928735733032227], 'magnitude': 2.6201491355895996, 'distance': 11.256568908691406, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6139624104715719, 'motion_component': 1.6086729895284697}]}, 5349: {'frame': 5349, 'ionic_force': [-7.378105878829956, -6.646641850471497, -10.801924467086792], 'ionic_force_magnitude': 14.672963791964886, 'motion_vector': [-0.10723876953125, -1.5981407165527344, 3.5609359741210938], 'cosine_ionic_motion': -0.47216925748123195, 'ionic_motion_component': -6.9281224187010615, 'ionic_force_x': -7.378105878829956, 'ionic_force_y': -6.646641850471497, 'ionic_force_z': -10.801924467086792, 'radial_force': 9.93047301228216, 'axial_force': -10.801924467086792, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [-10.252406120300293, -4.798220634460449, -6.5559773445129395], 'magnitude': 13.08111572265625, 'distance': 5.037866592407227, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.28541032674556904, 'motion_component': -3.733485544288841}, {'ion': 1320, 'force': [2.3740317821502686, -1.7368981838226318, -2.094464063644409], 'magnitude': 3.61104154586792, 'distance': 9.588546752929688, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 130, 'cosine_with_motion': -0.35015323973539414, 'motion_component': -1.2644179383602139}, {'ion': 2436, 'force': [0.5002684593200684, -0.11152303218841553, -2.1514830589294434], 'magnitude': 2.2116928100585938, 'distance': 12.25199031829834, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.872733684797831, 'motion_component': -1.9302188522429757}]}, 5350: {'frame': 5350, 'ionic_force': [-0.14506256580352783, -16.753881365060806, -3.0993531867861748], 'ionic_force_magnitude': 17.038766801590157, 'motion_vector': [2.5827255249023438, 0.7509269714355469, 2.464935302734375], 'cosine_ionic_motion': -0.33131159151419914, 'ionic_motion_component': -5.645140946474135, 'ionic_force_x': -0.14506256580352783, 'ionic_force_y': -16.753881365060806, 'ionic_force_z': -3.0993531867861748, 'radial_force': 16.754509361438465, 'axial_force': -3.0993531867861748, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 748, 'contributions': [{'ion': 1309, 'force': [-7.1796159744262695, -10.836474418640137, 3.318307876586914], 'magnitude': 13.415931701660156, 'distance': 4.974605083465576, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.3779898179059257, 'motion_component': -5.07108568105761}, {'ion': 1320, 'force': [5.264742851257324, -4.707367897033691, -0.06457030028104782], 'magnitude': 7.062648296356201, 'distance': 6.856228351593018, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 98, 'cosine_with_motion': 0.3843443305678448, 'motion_component': 2.714488781801923}, {'ion': 2434, 'force': [0.3296545743942261, -0.23305991291999817, -1.7742886543273926], 'magnitude': 1.8196399211883545, 'distance': 13.50754165649414, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5569081574761272, 'motion_component': -1.0133722924457365}, {'ion': 2436, 'force': [1.4401559829711914, -0.97697913646698, -4.578802108764648], 'magnitude': 4.8983635902404785, 'distance': 8.232723236083984, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.4644758616720765, 'motion_component': -2.2751716672537476}]}, 5351: {'frame': 5351, 'ionic_force': [6.5781702399253845, -10.670942857861519, 6.412924081087112], 'ionic_force_magnitude': 14.080729400530808, 'motion_vector': [-4.924442291259766, -0.13016128540039062, 1.0756683349609375], 'cosine_ionic_motion': -0.3395388214293875, 'ionic_motion_component': -4.7809542655223565, 'ionic_force_x': 6.5781702399253845, 'ionic_force_y': -10.670942857861519, 'ionic_force_z': 6.412924081087112, 'radial_force': 12.535603104006832, 'axial_force': 6.412924081087112, 'before_closest_residue': 780, 'closest_residue': 748, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [-0.7276131510734558, -8.576908111572266, 12.734542846679688], 'magnitude': 15.370795249938965, 'distance': 4.647515773773193, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 130, 'cosine_with_motion': 0.23737887367365, 'motion_component': 3.648702129922416}, {'ion': 1320, 'force': [2.105349540710449, -1.2945811748504639, 0.18129947781562805], 'magnitude': 2.478165864944458, 'distance': 11.574542999267578, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.8006204730018646, 'motion_component': -1.984070416350552}, {'ion': 2434, 'force': [1.0735446214675903, -0.11892910301685333, -2.175081729888916], 'magnitude': 2.428502082824707, 'distance': 11.692296028137207, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6215390624157976, 'motion_component': -1.5094089525808843}, {'ion': 2436, 'force': [4.126889228820801, -0.680524468421936, -4.327836513519287], 'magnitude': 6.018678665161133, 'distance': 7.427085876464844, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8201429451411554, 'motion_component': -4.93617713739299}]}, 5352: {'frame': 5352, 'ionic_force': [9.924710154533386, -10.801763534545898, -9.8836290538311], 'ionic_force_magnitude': 17.687964562986828, 'motion_vector': [1.6225547790527344, 0.3573951721191406, -0.7139053344726562], 'cosine_ionic_motion': 0.6033578075989015, 'ionic_motion_component': 10.672171519610794, 'ionic_force_x': 9.924710154533386, 'ionic_force_y': -10.801763534545898, 'ionic_force_z': -9.8836290538311, 'radial_force': 14.668945671306565, 'axial_force': -9.8836290538311, 'before_closest_residue': 748, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [5.455544471740723, -4.775212287902832, 4.03164005279541], 'magnitude': 8.295766830444336, 'distance': 6.326169013977051, 'before_closest_residue': 455, 'closest_residue': 130, 'next_closest_residue': 98, 'cosine_with_motion': 0.28444257656282923, 'motion_component': 2.359669156171975}, {'ion': 1320, 'force': [3.4328699111938477, -2.7567880153656006, 0.24743130803108215], 'magnitude': 4.409727573394775, 'distance': 8.676871299743652, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.5527925122176478, 'motion_component': 2.4376644442580866}, {'ion': 2434, 'force': [0.07548081874847412, -0.4966468811035156, -2.923949956893921], 'magnitude': 2.9667892456054688, 'distance': 10.57853889465332, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.37882856508898916, 'motion_component': 1.1239045384416073}, {'ion': 2436, 'force': [0.9608149528503418, -2.77311635017395, -11.238750457763672], 'magnitude': 11.615629196166992, 'distance': 5.346230506896973, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4090121636963402, 'motion_component': 4.750933804418082}]}, 5353: {'frame': 5353, 'ionic_force': [11.046917110681534, -10.955666691064835, -16.785257935523987], 'ionic_force_magnitude': 22.88680611745656, 'motion_vector': [-1.0786094665527344, -0.3579292297363281, -0.06634521484375], 'cosine_ionic_motion': -0.2640805144456472, 'ionic_motion_component': -6.043959533515713, 'ionic_force_x': 11.046917110681534, 'ionic_force_y': -10.955666691064835, 'ionic_force_z': -16.785257935523987, 'radial_force': 15.558310007708934, 'axial_force': -16.785257935523987, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [0.8205000758171082, -5.329401016235352, 1.1785228252410889], 'magnitude': 5.519479274749756, 'distance': 7.755681991577148, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 455, 'cosine_with_motion': 0.15029737672327664, 'motion_component': 0.8295632579359236}, {'ion': 1320, 'force': [3.7472195625305176, -2.678145170211792, 0.29563629627227783], 'magnitude': 4.615356922149658, 'distance': 8.481377601623535, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.5905579328226201, 'motion_component': -2.7256354706602135}, {'ion': 2434, 'force': [0.39906546473503113, -0.3938721716403961, -2.652449131011963], 'magnitude': 2.7110652923583984, 'distance': 11.066213607788086, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.0367698516531741, 'motion_component': -0.09968546798404}, {'ion': 2436, 'force': [6.080132007598877, -2.554248332977295, -15.60696792602539], 'magnitude': 16.943130493164062, 'distance': 4.426620006561279, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.23892883827431421, 'motion_component': -4.0482022507508475}]}, 5354: {'frame': 5354, 'ionic_force': [-0.8884754180908203, -10.587919175624847, -4.579100914299488], 'ionic_force_magnitude': 11.569856793472182, 'motion_vector': [-1.3265037536621094, 1.3291473388671875, 1.2285842895507812], 'cosine_ionic_motion': -0.7133261353379372, 'ionic_motion_component': -8.25308123290089, 'ionic_force_x': -0.8884754180908203, 'ionic_force_y': -10.587919175624847, 'ionic_force_z': -4.579100914299488, 'radial_force': 10.62513157744957, 'axial_force': -4.579100914299488, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [-6.627227306365967, -5.314355373382568, 7.1092095375061035], 'magnitude': 11.077156066894531, 'distance': 5.4746317863464355, 'before_closest_residue': 98, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': 0.4208694645766861, 'motion_component': 4.662036524869421}, {'ion': 1320, 'force': [3.325421094894409, -3.054407835006714, 0.12004440277814865], 'magnitude': 4.5168843269348145, 'distance': 8.573330879211426, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.8211762565733415, 'motion_component': -3.709158100849936}, {'ion': 2434, 'force': [0.26523327827453613, -0.28264373540878296, -2.6325316429138184], 'magnitude': 2.6609132289886475, 'distance': 11.170013427734375, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6634877643934309, 'motion_component': -1.7654833460838617}, {'ion': 2436, 'force': [2.148097515106201, -1.9365122318267822, -9.175823211669922], 'magnitude': 9.620818138122559, 'distance': 5.874393939971924, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.773372547498979, 'motion_component': -7.440476332000287}]}, 5355: {'frame': 5355, 'ionic_force': [-1.0782689899206161, -3.377299338579178, -19.434728145599365], 'ionic_force_magnitude': 19.755441603020266, 'motion_vector': [-0.3754844665527344, 2.017047882080078, -2.8304595947265625], 'cosine_ionic_motion': 0.7037424023399148, 'ionic_motion_component': 13.90274193299538, 'ionic_force_x': -1.0782689899206161, 'ionic_force_y': -3.377299338579178, 'ionic_force_z': -19.434728145599365, 'radial_force': 3.5452524362859945, 'axial_force': -19.434728145599365, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [-4.155211925506592, -0.5779337286949158, 3.243894577026367], 'magnitude': 5.303078651428223, 'distance': 7.912341117858887, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 780, 'cosine_with_motion': -0.4739911959579365, 'motion_component': -2.5136126988026177}, {'ion': 1320, 'force': [5.40611457824707, -3.8656556606292725, 1.663935661315918], 'magnitude': 6.851134777069092, 'distance': 6.961258888244629, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.6069518120289323, 'motion_component': -4.15830878571586}, {'ion': 2434, 'force': [-0.2116548866033554, 0.1417645514011383, -3.8158822059631348], 'magnitude': 3.824375867843628, 'distance': 9.31727123260498, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.835196737960166, 'motion_component': 3.1941063817137327}, {'ion': 2436, 'force': [-2.1175167560577393, 0.9245254993438721, -20.526676177978516], 'magnitude': 20.656307220458984, 'distance': 4.009061336517334, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8414164330538239, 'motion_component': 17.380556983894365}]}, 5356: {'frame': 5356, 'ionic_force': [9.193988606333733, -9.341656267642975, -8.68997049331665], 'ionic_force_magnitude': 15.726142422441105, 'motion_vector': [-5.566600799560547, -5.137775421142578, 0.14322662353515625], 'cosine_ionic_motion': -0.03716797145292092, 'ionic_motion_component': -0.5845088126218596, 'ionic_force_x': 9.193988606333733, 'ionic_force_y': -9.341656267642975, 'ionic_force_z': -8.68997049331665, 'radial_force': 13.107096105399846, 'axial_force': -8.68997049331665, 'before_closest_residue': 'SF', 'closest_residue': 130, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-5.083637714385986, 1.7815605401992798, 4.272593021392822], 'magnitude': 6.875491142272949, 'distance': 6.948917865753174, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.37927224489761086, 'motion_component': 2.6076830443856958}, {'ion': 1320, 'force': [15.738530158996582, -14.13753890991211, -3.5142836570739746], 'magnitude': 21.44577980041504, 'distance': 3.934577465057373, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.09525757946206342, 'motion_component': -2.042873198654397}, {'ion': 2434, 'force': [-0.2095593959093094, 0.4638260006904602, -2.334017753601074], 'magnitude': 2.3888676166534424, 'distance': 11.788891792297363, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.08568202920856213, 'motion_component': -0.20468302640401867}, {'ion': 2436, 'force': [-1.2513444423675537, 2.5504961013793945, -7.114262104034424], 'magnitude': 7.660523414611816, 'distance': 6.583241939544678, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.12331218202884321, 'motion_component': -0.9446358543236686}]}, 5357: {'frame': 5357, 'ionic_force': [-6.36072164773941, -7.776129573583603, -3.584123432636261], 'ionic_force_magnitude': 10.666438571779926, 'motion_vector': [1.0815353393554688, -1.1651802062988281, 1.2048263549804688], 'cosine_ionic_motion': -0.10043836085855601, 'ionic_motion_component': -1.071319606348053, 'ionic_force_x': -6.36072164773941, 'ionic_force_y': -7.776129573583603, 'ionic_force_z': -3.584123432636261, 'radial_force': 10.046241636810368, 'axial_force': -3.584123432636261, 'before_closest_residue': 130, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.7606245279312134, -0.44900551438331604, 1.1280972957611084], 'magnitude': 2.13869309425354, 'distance': 12.459333419799805, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 1105, 'cosine_with_motion': -0.005120338601344486, 'motion_component': -0.010950832851939651}, {'ion': 1320, 'force': [-1.3347965478897095, -6.032811641693115, -0.6402768492698669], 'magnitude': 6.211799621582031, 'distance': 7.310723304748535, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.38853205719115985, 'motion_component': 2.4134832243306086}, {'ion': 2434, 'force': [-0.9485629200935364, -0.36116552352905273, -1.7239831686019897], 'magnitude': 2.000582456588745, 'distance': 12.882223129272461, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6721193525377495, 'motion_component': -1.344630176815933}, {'ion': 2436, 'force': [-2.316737651824951, -0.9331468939781189, -2.3479607105255127], 'magnitude': 3.427966594696045, 'distance': 9.84126091003418, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6211325241080135, 'motion_component': -2.129221633842434}]}, 5358: {'frame': 5358, 'ionic_force': [-8.373949587345123, -10.114233255386353, -2.16071218252182], 'ionic_force_magnitude': 13.307494999866014, 'motion_vector': [-0.13986587524414062, 0.56707763671875, 0.13983154296875], 'cosine_ionic_motion': -0.6089035342787845, 'ionic_motion_component': -8.102980737815669, 'ionic_force_x': -8.373949587345123, 'ionic_force_y': -10.114233255386353, 'ionic_force_z': -2.16071218252182, 'radial_force': 13.130908043077628, 'axial_force': -2.16071218252182, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-2.585419178009033, -2.5263538360595703, 2.679021120071411], 'magnitude': 4.499334335327148, 'distance': 8.590034484863281, 'before_closest_residue': 780, 'closest_residue': 1105, 'next_closest_residue': 780, 'cosine_with_motion': -0.2577219996351968, 'motion_component': -1.1595774628844175}, {'ion': 1320, 'force': [-1.769490361213684, -4.937245845794678, 0.018840014934539795], 'magnitude': 5.244792461395264, 'distance': 7.956185340881348, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.8094466141356852, 'motion_component': -4.245379473738665}, {'ion': 2434, 'force': [-0.9104146361351013, -0.6412608623504639, -1.7891393899917603], 'magnitude': 2.107389450073242, 'distance': 12.551528930664062, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3843774113266263, 'motion_component': -0.8100328801187882}, {'ion': 2436, 'force': [-3.1086254119873047, -2.0093727111816406, -3.0694339275360107], 'magnitude': 4.808591842651367, 'distance': 8.309216499328613, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.39262866442624267, 'motion_component': -1.887990983593486}]}, 5359: {'frame': 5359, 'ionic_force': [-7.488657891750336, -9.668851613998413, -3.8453208655118942], 'ionic_force_magnitude': 12.82003046454787, 'motion_vector': [-0.3754844665527344, 0.34723663330078125, 0.0055084228515625], 'cosine_ionic_motion': -0.08642539269380385, 'ionic_motion_component': -1.1079761672450783, 'ionic_force_x': -7.488657891750336, 'ionic_force_y': -9.668851613998413, 'ionic_force_z': -3.8453208655118942, 'radial_force': 12.229746054321582, 'axial_force': -3.8453208655118942, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-3.55322265625, -1.968692660331726, 0.8038131594657898], 'magnitude': 4.140924453735352, 'distance': 8.95406723022461, 'before_closest_residue': 1105, 'closest_residue': 780, 'next_closest_residue': 455, 'cosine_with_motion': 0.3092681448214228, 'motion_component': 1.2806561095230804}, {'ion': 1320, 'force': [-0.5556600689888, -5.521777629852295, -0.23913930356502533], 'magnitude': 5.554815292358398, 'distance': 7.730974197387695, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.6018995063443169, 'motion_component': -3.3434406354042325}, {'ion': 2434, 'force': [-0.9361525774002075, -0.5566215515136719, -1.8760818243026733], 'magnitude': 2.169306993484497, 'distance': 12.37110710144043, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.133298819524226, 'motion_component': 0.2891660423462572}, {'ion': 2436, 'force': [-2.443622589111328, -1.6217597723007202, -2.5339128971099854], 'magnitude': 3.8758368492126465, 'distance': 9.255210876464844, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.1717416192223846, 'motion_component': 0.6656424831540266}]}, 5360: {'frame': 5360, 'ionic_force': [-5.99063166975975, -12.09947857260704, -4.111779734492302], 'ionic_force_magnitude': 14.113531879607137, 'motion_vector': [0.4962959289550781, -1.1936683654785156, -0.0410003662109375], 'cosine_ionic_motion': 0.637564935265345, 'ionic_motion_component': 8.998293039187107, 'ionic_force_x': -5.99063166975975, 'ionic_force_y': -12.09947857260704, 'ionic_force_z': -4.111779734492302, 'radial_force': 13.50129806839718, 'axial_force': -4.111779734492302, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.7648735046386719, -0.8681292533874512, 0.4014160633087158], 'magnitude': 2.0073769092559814, 'distance': 12.860404014587402, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': 0.05542519617332915, 'motion_component': 0.11125925468247111}, {'ion': 1320, 'force': [-0.222377210855484, -9.145050048828125, 0.049248531460762024], 'magnitude': 9.147886276245117, 'distance': 6.024328708648682, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 1105, 'cosine_with_motion': 0.9131206022804962, 'motion_component': 8.35312313240585}, {'ion': 2434, 'force': [-0.8280560374259949, -0.4974512755870819, -1.6552377939224243], 'magnitude': 1.91649329662323, 'distance': 13.161803245544434, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.10113794630997673, 'motion_component': 0.1938302006527346}, {'ion': 2436, 'force': [-3.1753249168395996, -1.5888479948043823, -2.9072065353393555], 'magnitude': 4.589005947113037, 'distance': 8.505693435668945, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.074107570812104, 'motion_component': 0.340080087499274}]}, 5361: {'frame': 5361, 'ionic_force': [-5.120174393057823, -19.02680516242981, -0.25727808475494385], 'ionic_force_magnitude': 19.705372174036345, 'motion_vector': [-0.574737548828125, 0.9560508728027344, -0.38732147216796875], 'cosine_ionic_motion': -0.6510080193920725, 'ionic_motion_component': -12.82835531040306, 'ionic_force_x': -5.120174393057823, 'ionic_force_y': -19.02680516242981, 'ionic_force_z': -0.25727808475494385, 'radial_force': 19.703692560136812, 'axial_force': -0.25727808475494385, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.4405096769332886, -0.9803712368011475, 0.35021817684173584], 'magnitude': 1.7773150205612183, 'distance': 13.667428970336914, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 455, 'cosine_with_motion': -0.1167459297738805, 'motion_component': -0.2074942939315676}, {'ion': 1320, 'force': [0.1950037032365799, -15.115640640258789, 4.1602349281311035], 'magnitude': 15.678908348083496, 'distance': 4.601624011993408, 'before_closest_residue': 98, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': -0.8736388570428829, 'motion_component': -13.69770373827267}, {'ion': 2434, 'force': [-0.9663851857185364, -0.6437287330627441, -2.0172598361968994], 'magnitude': 2.3275790214538574, 'distance': 11.943093299865723, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.2624381036375999, 'motion_component': 0.6108454331708925}, {'ion': 2436, 'force': [-2.908283233642578, -2.287064552307129, -2.750471353530884], 'magnitude': 4.610191822052002, 'distance': 8.486127853393555, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.10107972759484486, 'motion_component': 0.4659969298493891}]}, 5362: {'frame': 5362, 'ionic_force': [-2.3333985209465027, -17.115698158740997, 4.077326849102974], 'ionic_force_magnitude': 17.748703230182798, 'motion_vector': [0.4037361145019531, -0.2184600830078125, -0.226226806640625], 'cosine_ionic_motion': 0.2063827837405274, 'ionic_motion_component': 3.6630267804296164, 'ionic_force_x': -2.3333985209465027, 'ionic_force_y': -17.115698158740997, 'ionic_force_z': 4.077326849102974, 'radial_force': 17.274023043827555, 'axial_force': 4.077326849102974, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.5750622749328613, -0.9575368165969849, 0.24507339298725128], 'magnitude': 1.8595050573349, 'distance': 13.361966133117676, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 423, 'cosine_with_motion': -0.5066735521869951, 'motion_component': -0.9421620101963059}, {'ion': 1320, 'force': [3.2834606170654297, -13.994690895080566, 8.046475410461426], 'magnitude': 16.473562240600586, 'distance': 4.489265441894531, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': 0.3039632998783835, 'motion_component': 5.007358344099799}, {'ion': 2434, 'force': [-0.9333657622337341, -0.5060002207756042, -1.6682040691375732], 'magnitude': 1.977400541305542, 'distance': 12.957514762878418, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.1097857354681624, 'motion_component': 0.2170903667758015}, {'ion': 2436, 'force': [-3.108431100845337, -1.6574702262878418, -2.54601788520813], 'magnitude': 4.346465110778809, 'distance': 8.739789009094238, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.14247442357158616, 'motion_component': -0.6192601042226045}]}, 5363: {'frame': 5363, 'ionic_force': [-4.615044325590134, -13.802704691886902, 2.612096294760704], 'ionic_force_magnitude': 14.786356481287097, 'motion_vector': [-0.16725540161132812, -0.3708457946777344, 0.30941009521484375], 'cosine_ionic_motion': 0.8863761547181133, 'ionic_motion_component': 13.106273800174508, 'ionic_force_x': -4.615044325590134, 'ionic_force_y': -13.802704691886902, 'ionic_force_z': 2.612096294760704, 'radial_force': 14.553806750764501, 'axial_force': 2.612096294760704, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.4222971200942993, -1.290872573852539, 0.12278829514980316], 'magnitude': 1.924670934677124, 'distance': 13.133811950683594, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.7670795510974251, 'motion_component': 1.476375688362606}, {'ion': 1320, 'force': [0.3337534964084625, -10.261008262634277, 7.174679279327393], 'magnitude': 12.525003433227539, 'distance': 5.148492813110352, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': 0.9324657304241323, 'motion_component': 11.679136241201018}, {'ion': 2434, 'force': [-0.8723053932189941, -0.5652945041656494, -1.9188066720962524], 'magnitude': 2.182267904281616, 'distance': 12.334314346313477, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.2135258965253157, 'motion_component': -0.4659707309890351}, {'ion': 2436, 'force': [-2.6541953086853027, -1.685529351234436, -2.7665646076202393], 'magnitude': 4.188035488128662, 'distance': 8.903563499450684, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.09950545026923256, 'motion_component': 0.41673236184657725}]}, 5364: {'frame': 5364, 'ionic_force': [-5.364780865609646, -11.734835743904114, 1.9194905273616314], 'ionic_force_magnitude': 13.044987066189526, 'motion_vector': [0.7199592590332031, 0.047824859619140625, -0.00384521484375], 'cosine_ionic_motion': -0.47074968515216353, 'ionic_motion_component': -6.1409235542227645, 'ionic_force_x': -5.364780865609646, 'ionic_force_y': -11.734835743904114, 'ionic_force_z': 1.9194905273616314, 'radial_force': 12.90299359344261, 'axial_force': 1.9194905273616314, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'contributions': [{'ion': 1309, 'force': [-1.2786661386489868, -1.378605604171753, 0.06221873685717583], 'magnitude': 1.8813323974609375, 'distance': 13.284226417541504, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.7269007740173844, 'motion_component': -1.3675419927947812}, {'ion': 1320, 'force': [-0.05913498252630234, -7.958459854125977, 6.173501968383789], 'magnitude': 10.072373390197754, 'distance': 5.741206169128418, 'before_closest_residue': 1105, 'closest_residue': 1105, 'next_closest_residue': 1105, 'cosine_with_motion': -0.061494054302821094, 'motion_component': -0.6193910793836221}, {'ion': 2434, 'force': [-0.9266603589057922, -0.606224775314331, -1.7449246644973755], 'magnitude': 2.0666325092315674, 'distance': 12.674692153930664, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.462342170077388, 'motion_component': -0.9554913652822146}, {'ion': 2436, 'force': [-3.1003193855285645, -1.7915455102920532, -2.571305513381958], 'magnitude': 4.408313274383545, 'distance': 8.678262710571289, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{5415: {'frame': 5415, 'ionic_force': [-0.86297807097435, 12.021617323160172, -7.310816407203674], 'ionic_force_magnitude': 14.096526194609996, 'motion_vector': [-0.3487205505371094, 3.4752159118652344, 0.6145477294921875], 'cosine_ionic_motion': 0.7518541705699963, 'ionic_motion_component': 10.598532009966725, 'ionic_force_x': -0.86297807097435, 'ionic_force_y': 12.021617323160172, 'ionic_force_z': -7.310816407203674, 'radial_force': 12.05255218679792, 'axial_force': -7.310816407203674, 'contributions': [{'ion': 1309, 'force': [-1.2417367696762085, 2.2549033164978027, 3.7121427059173584], 'magnitude': 4.517355442047119, 'distance': 8.572882652282715, 'cosine_with_motion': 0.6585883074501265, 'motion_component': 2.9750776534110397}, {'ion': 1469, 'force': [3.919631004333496, 7.311126232147217, -1.3659437894821167], 'magnitude': 8.407251358032227, 'distance': 6.284084796905518, 'cosine_with_motion': 0.7781850453014673, 'motion_component': 6.542397326645556}, {'ion': 2434, 'force': [-3.1615939140319824, 2.1154823303222656, -7.686925411224365], 'magnitude': 8.576698303222656, 'distance': 6.221698760986328, 'cosine_with_motion': 0.12264335860419856, 'motion_component': 1.0518751575718213}, {'ion': 2444, 'force': [-0.37927839159965515, 0.34010544419288635, -1.9700899124145508], 'magnitude': 2.0348901748657227, 'distance': 12.773165702819824, 'cosine_with_motion': 0.014340683672517583, 'motion_component': 0.0291817164848438}]}, 5416: {'frame': 5416, 'ionic_force': [-2.890625089406967, 9.539554595947266, -3.3671732246875763], 'ionic_force_magnitude': 10.52124853910507, 'motion_vector': [-2.1743736267089844, -0.24370956420898438, 0.42597198486328125], 'cosine_ionic_motion': 0.10771079835192808, 'ionic_motion_component': 1.1332520798060641, 'ionic_force_x': -2.890625089406967, 'ionic_force_y': 9.539554595947266, 'ionic_force_z': -3.3671732246875763, 'radial_force': 9.967889209685652, 'axial_force': -3.3671732246875763, 'contributions': [{'ion': 1309, 'force': [-1.7372729778289795, 1.9497443437576294, 1.9252551794052124], 'magnitude': 3.244414806365967, 'distance': 10.115814208984375, 'cosine_with_motion': 0.57002217966702, 'motion_component': 1.849388441445887}, {'ion': 1469, 'force': [1.0098694562911987, 3.874903678894043, -0.12357929348945618], 'magnitude': 4.0062432289123535, 'distance': 9.103331565856934, 'cosine_with_motion': -0.35753160520772975, 'motion_component': -1.432358656018975}, {'ion': 2434, 'force': [-1.7631807327270508, 3.0347986221313477, -3.503937005996704], 'magnitude': 4.959474086761475, 'distance': 8.181844711303711, 'cosine_with_motion': 0.14487779028910183, 'motion_component': 0.7185176510370184}, {'ion': 2444, 'force': [-0.4000408351421356, 0.6801079511642456, -1.6649121046066284], 'magnitude': 1.8424201011657715, 'distance': 13.423776626586914, 'cosine_with_motion': -0.0012458317985159255, 'motion_component': -0.00229534554213906}]}, 5417: {'frame': 5417, 'ionic_force': [-4.601493835449219, 9.4010049700737, -1.1370874345302582], 'ionic_force_magnitude': 10.528324073602322, 'motion_vector': [0.7505950927734375, 1.0793838500976562, -1.4337081909179688], 'cosine_ionic_motion': 0.4064264224237802, 'ionic_motion_component': 4.278989087352351, 'ionic_force_x': -4.601493835449219, 'ionic_force_y': 9.4010049700737, 'ionic_force_z': -1.1370874345302582, 'radial_force': 10.46673970083462, 'axial_force': -1.1370874345302582, 'contributions': [{'ion': 1309, 'force': [-1.6386932134628296, 1.689590573310852, 3.3819234371185303], 'magnitude': 4.120368480682373, 'distance': 8.976375579833984, 'cosine_with_motion': -0.5308672048478624, 'motion_component': -2.187368593057652}, {'ion': 1469, 'force': [0.2765955328941345, 4.555323600769043, -0.1436668336391449], 'magnitude': 4.56597375869751, 'distance': 8.527118682861328, 'cosine_with_motion': 0.6001537030888063, 'motion_component': 2.7402861903056674}, {'ion': 2434, 'force': [-2.509505271911621, 2.4902234077453613, -2.8283956050872803], 'magnitude': 4.527543544769287, 'distance': 8.563232421875, 'cosine_with_motion': 0.5517515902465349, 'motion_component': 2.4980793799438032}, {'ion': 2444, 'force': [-0.7298908829689026, 0.6658673882484436, -1.5469484329223633], 'magnitude': 1.8355298042297363, 'distance': 13.448948860168457, 'cosine_with_motion': 0.669012387353238, 'motion_component': 1.227992153000633}]}, 5418: {'frame': 5418, 'ionic_force': [-1.8272255063056946, 7.148484110832214, -0.753704845905304], 'ionic_force_magnitude': 7.416714173301805, 'motion_vector': [0.6279106140136719, 0.4439239501953125, -0.27136993408203125], 'cosine_ionic_motion': 0.3688091800561364, 'ionic_motion_component': 2.735352272966164, 'ionic_force_x': -1.8272255063056946, 'ionic_force_y': 7.148484110832214, 'ionic_force_z': -0.753704845905304, 'radial_force': 7.378318110092214, 'axial_force': -0.753704845905304, 'contributions': [{'ion': 1309, 'force': [-1.2601678371429443, 2.125608205795288, 2.1942358016967773], 'magnitude': 3.3046791553497314, 'distance': 10.023154258728027, 'cosine_with_motion': -0.1644300780964941, 'motion_component': -0.5433886430388242}, {'ion': 1469, 'force': [0.4336826205253601, 3.54756498336792, -0.8087297081947327], 'magnitude': 3.6643335819244385, 'distance': 9.518566131591797, 'cosine_with_motion': 0.6916117806805393, 'motion_component': 2.5342963743771456}, {'ion': 2434, 'force': [-1.0007402896881104, 1.4753109216690063, -2.1392109394073486], 'magnitude': 2.784644842147827, 'distance': 10.919032096862793, 'cosine_with_motion': 0.26733916725288576, 'motion_component': 0.7444446326850809}]}, 5419: {'frame': 5419, 'ionic_force': [-2.556093394756317, 7.023166179656982, -1.4966426491737366], 'ionic_force_magnitude': 7.622231684298261, 'motion_vector': [-0.07321548461914062, -1.4095268249511719, 1.3923492431640625], 'cosine_ionic_motion': -0.7805771866631694, 'ionic_motion_component': -5.949740164224408, 'ionic_force_x': -2.556093394756317, 'ionic_force_y': 7.023166179656982, 'ionic_force_z': -1.4966426491737366, 'radial_force': 7.473852863804219, 'axial_force': -1.4966426491737366, 'contributions': [{'ion': 1309, 'force': [-2.2032456398010254, 2.115774631500244, 1.356068730354309], 'magnitude': 3.3421125411987305, 'distance': 9.966863632202148, 'cosine_with_motion': -0.14077735077576017, 'motion_component': -0.4704937454166113}, {'ion': 1469, 'force': [0.5705264210700989, 3.1289117336273193, -0.7028989195823669], 'magnitude': 3.257246732711792, 'distance': 10.095869064331055, 'cosine_with_motion': -0.8409491019474874, 'motion_component': -2.7391786691732083}, {'ion': 2434, 'force': [-0.9233741760253906, 1.778479814529419, -2.1498124599456787], 'magnitude': 2.9389290809631348, 'distance': 10.628561973571777, 'cosine_with_motion': -0.9323354010550714, 'motion_component': -2.7400675900062055}]}, 5420: {'frame': 5420, 'ionic_force': [-4.017000198364258, 7.976373076438904, -4.721324697136879], 'ionic_force_magnitude': 10.101966389965497, 'motion_vector': [1.37384033203125, 0.6198310852050781, 1.271148681640625], 'cosine_ionic_motion': -0.33017035763647795, 'ionic_motion_component': -3.3353698558065883, 'ionic_force_x': -4.017000198364258, 'ionic_force_y': 7.976373076438904, 'ionic_force_z': -4.721324697136879, 'radial_force': 8.930779252013673, 'axial_force': -4.721324697136879, 'contributions': [{'ion': 1309, 'force': [-2.296131134033203, 1.0717114210128784, 0.202259823679924], 'magnitude': 2.5419859886169434, 'distance': 11.428321838378906, 'cosine_with_motion': -0.44556351398937477, 'motion_component': -1.132616194223882}, {'ion': 1469, 'force': [0.5067126154899597, 4.24498176574707, -0.2817506194114685], 'magnitude': 4.2843918800354, 'distance': 8.802873611450195, 'cosine_with_motion': 0.3514901901202061, 'motion_component': 1.505921613751351}, {'ion': 2434, 'force': [-1.693018913269043, 2.0171566009521484, -2.944333791732788], 'magnitude': 3.9502322673797607, 'distance': 9.167643547058105, 'cosine_with_motion': -0.6186448965736641, 'motion_component': -2.4437910563266314}, {'ion': 2444, 'force': [-0.5345627665519714, 0.6425232887268066, -1.6975001096725464], 'magnitude': 1.8921153545379639, 'distance': 13.246319770812988, 'cosine_with_motion': -0.6685027957609565, 'motion_component': -1.2648843400024923}]}, 5421: {'frame': 5421, 'ionic_force': [-4.36628919839859, 9.376880168914795, -2.967519700527191], 'ionic_force_magnitude': 10.76087990079142, 'motion_vector': [-0.43817138671875, 0.11849594116210938, -1.432342529296875], 'cosine_ionic_motion': 0.44993154895126, 'ionic_motion_component': 4.841659361841564, 'ionic_force_x': -4.36628919839859, 'ionic_force_y': 9.376880168914795, 'ionic_force_z': -2.967519700527191, 'radial_force': 10.343614603524232, 'axial_force': -2.967519700527191, 'contributions': [{'ion': 1309, 'force': [-3.586841344833374, 1.4117411375045776, 1.6100742816925049], 'magnitude': 4.177413463592529, 'distance': 8.914875984191895, 'cosine_with_motion': -0.09037177139810013, 'motion_component': -0.377520252610303}, {'ion': 1469, 'force': [1.202595829963684, 3.48968505859375, 0.13294559717178345], 'magnitude': 3.6934826374053955, 'distance': 9.480932235717773, 'cosine_with_motion': -0.05475204072792799, 'motion_component': -0.2022257049529017}, {'ion': 2434, 'force': [-1.507516622543335, 3.459397077560425, -2.9776651859283447], 'magnitude': 4.806924819946289, 'distance': 8.310657501220703, 'cosine_with_motion': 0.7387225120534889, 'motion_component': 3.550983443186361}, {'ion': 2444, 'force': [-0.4745270609855652, 1.0160568952560425, -1.7328743934631348], 'magnitude': 2.0640740394592285, 'distance': 12.682544708251953, 'cosine_with_motion': 0.906179644664221, 'motion_component': 1.8704217850621294}]}, 5422: {'frame': 5422, 'ionic_force': [-3.337195932865143, 8.502465009689331, -4.2525006383657455], 'ionic_force_magnitude': 10.075343647470499, 'motion_vector': [0.1480560302734375, -0.8996047973632812, 0.5749053955078125], 'cosine_ionic_motion': -0.9749704271170396, 'ionic_motion_component': -9.823162099325264, 'ionic_force_x': -3.337195932865143, 'ionic_force_y': 8.502465009689331, 'ionic_force_z': -4.2525006383657455, 'radial_force': 9.133936059296838, 'axial_force': -4.2525006383657455, 'contributions': [{'ion': 1309, 'force': [-2.566864252090454, 1.8449293375015259, 0.5315044522285461], 'magnitude': 3.205472469329834, 'distance': 10.17707633972168, 'cosine_with_motion': -0.501938957417652, 'motion_component': -1.6089514764139317}, {'ion': 1469, 'force': [1.0937838554382324, 3.111398458480835, -0.23599140346050262], 'magnitude': 3.3064868450164795, 'distance': 10.020413398742676, 'cosine_with_motion': -0.7780253814588048, 'motion_component': -2.572530709600221}, {'ion': 2434, 'force': [-1.3929810523986816, 2.763676643371582, -2.991767168045044], 'magnitude': 4.304529666900635, 'distance': 8.782258033752441, 'cosine_with_motion': -0.9510453856970562, 'motion_component': -4.093803070234479}, {'ion': 2444, 'force': [-0.4711344838142395, 0.7824605703353882, -1.5562465190887451], 'magnitude': 1.8044710159301758, 'distance': 13.564197540283203, 'cosine_with_motion': -0.8578010229664738, 'motion_component': -1.5478770422136625}]}, 5423: {'frame': 5423, 'ionic_force': [-7.194524526596069, 10.885988421738148, -3.873266875743866], 'ionic_force_magnitude': 13.611323351266917, 'motion_vector': [-0.2519950866699219, 0.5466041564941406, 0.0637054443359375], 'cosine_ionic_motion': 0.9123871441683606, 'ionic_motion_component': 12.418796440814543, 'ionic_force_x': -7.194524526596069, 'ionic_force_y': 10.885988421738148, 'ionic_force_z': -3.873266875743866, 'radial_force': 13.048598663535078, 'axial_force': -3.873266875743866, 'contributions': [{'ion': 1309, 'force': [-7.53367280960083, -0.03545748442411423, 1.090088963508606], 'magnitude': 7.612212181091309, 'distance': 6.604099273681641, 'cosine_with_motion': 0.4229142947215601, 'motion_component': 3.219313426221046}, {'ion': 1469, 'force': [3.078547954559326, 6.243687152862549, 0.9668325781822205], 'magnitude': 7.0282182693481445, 'distance': 6.873001575469971, 'cosine_with_motion': 0.6343949704708078, 'motion_component': 4.45866631981975}, {'ion': 2434, 'force': [-2.2350199222564697, 3.7992143630981445, -4.083253383636475], 'magnitude': 6.008519172668457, 'distance': 7.4333624839782715, 'cosine_with_motion': 0.654372414694982, 'motion_component': 3.931809165797851}, {'ion': 2444, 'force': [-0.5043797492980957, 0.8785443902015686, -1.8469350337982178], 'magnitude': 2.106515645980835, 'distance': 12.554132461547852, 'cosine_with_motion': 0.3840500646571, 'motion_component': 0.8090074727170524}]}, 5424: {'frame': 5424, 'ionic_force': [-9.829724729061127, 8.064699590206146, -3.82029065862298], 'ionic_force_magnitude': 13.276200075539274, 'motion_vector': [-1.8115425109863281, -1.1403274536132812, 0.10491180419921875], 'cosine_ionic_motion': 0.2885408107742469, 'ionic_motion_component': 3.8307255337972204, 'ionic_force_x': -9.829724729061127, 'ionic_force_y': 8.064699590206146, 'ionic_force_z': -3.82029065862298, 'radial_force': 12.71467135750614, 'axial_force': -3.82029065862298, 'contributions': [{'ion': 1309, 'force': [-8.29712200164795, 0.1777876615524292, 0.9536499381065369], 'magnitude': 8.353639602661133, 'distance': 6.30421781539917, 'cosine_with_motion': 0.8338212823493995, 'motion_component': 6.965442263992603}, {'ion': 1469, 'force': [0.7835202217102051, 3.773498058319092, -0.03277162089943886], 'magnitude': 3.854123115539551, 'distance': 9.281245231628418, 'cosine_with_motion': -0.6932081742710833, 'motion_component': -2.671709695405911}, {'ion': 2434, 'force': [-1.8014920949935913, 3.1987240314483643, -3.0620651245117188], 'magnitude': 4.7805280685424805, 'distance': 8.33357048034668, 'cosine_with_motion': -0.06884699269022612, 'motion_component': -0.3291250055472901}, {'ion': 2444, 'force': [-0.5146308541297913, 0.914689838886261, -1.6791038513183594], 'magnitude': 1.9801243543624878, 'distance': 12.948599815368652, 'cosine_with_motion': -0.06761305818944655, 'motion_component': -0.13388225810879462}]}, 5425: {'frame': 5425, 'ionic_force': [-7.359991593286395, 3.306031584739685, -5.195836968719959], 'ionic_force_magnitude': 9.59666832281182, 'motion_vector': [0.7701644897460938, 1.122161865234375, -0.6427230834960938], 'cosine_ionic_motion': 0.09560626418969688, 'ionic_motion_component': 0.9175016070116421, 'ionic_force_x': -7.359991593286395, 'ionic_force_y': 3.306031584739685, 'ionic_force_z': -5.195836968719959, 'radial_force': 8.068415029765314, 'axial_force': -5.195836968719959, 'contributions': [{'ion': 1309, 'force': [-4.172080993652344, -2.511462926864624, -0.10490787774324417], 'magnitude': 4.87080192565918, 'distance': 8.255983352661133, 'cosine_with_motion': -0.8135006963141567, 'motion_component': -3.9624007676868804}, {'ion': 1469, 'force': [0.024452881887555122, 2.9648444652557373, -0.17231887578964233], 'magnitude': 2.9699485301971436, 'distance': 10.572911262512207, 'cosine_with_motion': 0.77325275445924, 'motion_component': 2.2965209036455843}, {'ion': 2434, 'force': [-2.4676637649536133, 2.1257126331329346, -3.127074718475342], 'magnitude': 4.515153884887695, 'distance': 8.574973106384277, 'cosine_with_motion': 0.36708742493103036, 'motion_component': 1.6574562268455113}, {'ion': 2444, 'force': [-0.7446997165679932, 0.7269374132156372, -1.791535496711731], 'magnitude': 2.0718626976013184, 'distance': 12.658683776855469, 'cosine_with_motion': 0.4469046351630615, 'motion_component': 0.9259250504055956}]}, 5426: {'frame': 5426, 'ionic_force': [-5.71360582113266, 4.7653467655181885, -4.617043234407902], 'ionic_force_magnitude': 8.756192637402826, 'motion_vector': [0.9683570861816406, -1.1876640319824219, -1.7886962890625], 'cosine_ionic_motion': -0.14225960241465066, 'ionic_motion_component': -1.2456524832630174, 'ionic_force_x': -5.71360582113266, 'ionic_force_y': 4.7653467655181885, 'ionic_force_z': -4.617043234407902, 'radial_force': 7.440014870611193, 'axial_force': -4.617043234407902, 'contributions': [{'ion': 1309, 'force': [-3.82336688041687, -1.281545877456665, 0.038811035454273224], 'magnitude': 4.032617092132568, 'distance': 9.073514938354492, 'cosine_with_motion': -0.23686059447804464, 'motion_component': -0.9551680765469284}, {'ion': 1469, 'force': [0.3030494451522827, 3.1069347858428955, -0.22176901996135712], 'magnitude': 3.129547119140625, 'distance': 10.299788475036621, 'cosine_with_motion': -0.40697035549176575, 'motion_component': -1.2736328422891834}, {'ion': 2434, 'force': [-1.6431152820587158, 2.2570924758911133, -2.791811227798462], 'magnitude': 3.948227882385254, 'distance': 9.169970512390137, 'cosine_with_motion': 0.07762936310697147, 'motion_component': 0.306498423729046}, {'ion': 2444, 'force': [-0.5501731038093567, 0.6828653812408447, -1.642274022102356], 'magnitude': 1.8617355823516846, 'distance': 13.353959083557129, 'cosine_with_motion': 0.3634511718692843, 'motion_component': 0.6766499945516973}]}, 5427: {'frame': 5427, 'ionic_force': [-8.04122668504715, 2.214553475379944, -8.471194505691528], 'ionic_force_magnitude': 11.888091101976386, 'motion_vector': [1.9277992248535156, -0.47090911865234375, 1.2962722778320312], 'cosine_ionic_motion': -0.9768244492629804, 'ionic_motion_component': -11.612578043476221, 'ionic_force_x': -8.04122668504715, 'ionic_force_y': 2.214553475379944, 'ionic_force_z': -8.471194505691528, 'radial_force': 8.340597921949707, 'axial_force': -8.471194505691528, 'contributions': [{'ion': 1309, 'force': [-7.151926517486572, -4.424306392669678, -2.266660690307617], 'magnitude': 8.709896087646484, 'distance': 6.1739420890808105, 'cosine_with_motion': -0.7092263629987502, 'motion_component': -6.17728795671141}, {'ion': 1469, 'force': [1.0913169384002686, 4.217013835906982, -1.362021803855896], 'magnitude': 4.563910484313965, 'distance': 8.529046058654785, 'cosine_with_motion': -0.1522963508158204, 'motion_component': -0.6950669595563213}, {'ion': 2434, 'force': [-1.582262396812439, 1.9491033554077148, -3.3685457706451416], 'magnitude': 4.2011494636535645, 'distance': 8.889656066894531, 'cosine_with_motion': -0.8369729709418179, 'motion_component': -3.516248744739322}, {'ion': 2444, 'force': [-0.398354709148407, 0.4727426767349243, -1.4739662408828735], 'magnitude': 1.5983580350875854, 'distance': 14.412257194519043, 'cosine_with_motion': -0.7657695663854323, 'motion_component': -1.2239739834485697}]}, 5428: {'frame': 5428, 'ionic_force': [-4.013658359646797, 2.036353588104248, -10.628021240234375], 'ionic_force_magnitude': 11.541708055856407, 'motion_vector': [0.24727249145507812, -2.330799102783203, -4.778404235839844], 'cosine_ionic_motion': 0.733311095968307, 'ionic_motion_component': 8.4636625837863, 'ionic_force_x': -4.013658359646797, 'ionic_force_y': 2.036353588104248, 'ionic_force_z': -10.628021240234375, 'radial_force': 4.5006876545421, 'axial_force': -10.628021240234375, 'contributions': [{'ion': 1309, 'force': [-4.697807788848877, -6.503828525543213, -1.5563700199127197], 'magnitude': 8.172605514526367, 'distance': 6.373658657073975, 'cosine_with_motion': 0.49277885349233314, 'motion_component': 4.027286881652531}, {'ion': 1469, 'force': [2.3175904750823975, 4.2220258712768555, -0.8517012596130371], 'magnitude': 4.891024589538574, 'distance': 8.238897323608398, 'cosine_with_motion': -0.19967505294610755, 'motion_component': -0.9766156258850804}, {'ion': 2434, 'force': [-1.4328304529190063, 3.6519341468811035, -6.213566780090332], 'magnitude': 7.3483357429504395, 'distance': 6.7216291427612305, 'cosine_with_motion': 0.5324640438268261, 'motion_component': 3.91272456724384}, {'ion': 2444, 'force': [-0.20061059296131134, 0.666222095489502, -2.006383180618286], 'magnitude': 2.123598337173462, 'distance': 12.503536224365234, 'cosine_with_motion': 0.7064737784360602, 'motion_component': 1.5002665511818145}]}, 5429: {'frame': 5429, 'ionic_force': [-0.07442072033882141, -0.02468770742416382, -7.9879608154296875], 'ionic_force_magnitude': 7.9883456306893565, 'motion_vector': [3.7690887451171875, -2.5068588256835938, -3.2027816772460938], 'cosine_ionic_motion': 0.572624250980996, 'ionic_motion_component': 4.574320433350805, 'ionic_force_x': -0.07442072033882141, 'ionic_force_y': -0.02468770742416382, 'ionic_force_z': -7.9879608154296875, 'radial_force': 0.0784087145259389, 'axial_force': -7.9879608154296875, 'contributions': [{'ion': 1309, 'force': [-1.8123735189437866, -2.4131195545196533, -2.5620484352111816], 'magnitude': 3.9587795734405518, 'distance': 9.15774154663086, 'cosine_with_motion': 0.3381963958982721, 'motion_component': 1.3388449937113478}, {'ion': 1469, 'force': [1.9238256216049194, 2.0180952548980713, -2.4386179447174072], 'magnitude': 3.7041423320770264, 'distance': 9.467279434204102, 'cosine_with_motion': 0.4869727291469073, 'motion_component': 1.803816336372222}, {'ion': 2434, 'force': [-0.18587282299995422, 0.3703365921974182, -2.9872944355010986], 'magnitude': 3.0158956050872803, 'distance': 10.492063522338867, 'cosine_with_motion': 0.4747044569942231, 'motion_component': 1.431659057345513}]}, 5430: {'frame': 5430, 'ionic_force': [2.4746485874056816, -1.7678358405828476, -3.220875859260559], 'ionic_force_magnitude': 4.429804791541682, 'motion_vector': [-0.60418701171875, 0.23330307006835938, 2.4262313842773438], 'cosine_ionic_motion': -0.8739764423926943, 'ionic_motion_component': -3.87154503220571, 'ionic_force_x': 2.4746485874056816, 'ionic_force_y': -1.7678358405828476, 'ionic_force_z': -3.220875859260559, 'radial_force': 3.0412381015629473, 'axial_force': -3.220875859260559, 'contributions': [{'ion': 1309, 'force': [0.12402363866567612, -1.6623444557189941, -1.531604528427124], 'magnitude': 2.26375412940979, 'distance': 12.110285758972168, 'cosine_with_motion': -0.7350923070401219, 'motion_component': -1.6640683471142113}, {'ion': 1320, 'force': [0.5745420455932617, -0.34557026624679565, 1.4239434003829956], 'magnitude': 1.5738908052444458, 'distance': 14.523849487304688, 'cosine_with_motion': 0.7658917483680011, 'motion_component': 1.20542995909179}, {'ion': 1469, 'force': [1.4435352087020874, 0.3784688711166382, -1.497428059577942], 'magnitude': 2.11407732963562, 'distance': 12.531660079956055, 'cosine_with_motion': -0.832002319477491, 'motion_component': -1.7589173250676327}, {'ion': 2434, 'force': [0.33254769444465637, -0.13838998973369598, -1.6157866716384888], 'magnitude': 1.6554474830627441, 'distance': 14.161567687988281, 'cosine_with_motion': -0.9991191765221671, 'motion_component': -1.6539893131995007}]}, 5431: {'frame': 5431, 'ionic_force': [3.104661077260971, -1.3943484723567963, -5.393718481063843], 'ionic_force_magnitude': 6.377721154142177, 'motion_vector': [-2.8593292236328125, 1.6220474243164062, -1.3614044189453125], 'cosine_ionic_motion': -0.1672747077358023, 'ionic_motion_component': -1.0668314420795766, 'ionic_force_x': 3.104661077260971, 'ionic_force_y': -1.3943484723567963, 'ionic_force_z': -5.393718481063843, 'radial_force': 3.4033994868400304, 'axial_force': -5.393718481063843, 'contributions': [{'ion': 1309, 'force': [0.6289064884185791, -2.2084546089172363, -1.3620975017547607], 'magnitude': 2.669851064682007, 'distance': 11.151300430297852, 'cosine_with_motion': -0.3711823052455934, 'motion_component': -0.9910014747644809}, {'ion': 1469, 'force': [2.067415952682495, 1.0044293403625488, -1.9814109802246094], 'magnitude': 3.0346460342407227, 'distance': 10.459598541259766, 'cosine_with_motion': -0.14676256689893674, 'motion_component': -0.44537244017870137}, {'ion': 2434, 'force': [0.40833863615989685, -0.19032320380210876, -2.0502099990844727], 'magnitude': 2.0991246700286865, 'distance': 12.576213836669922, 'cosine_with_motion': 0.17604603464467547, 'motion_component': 0.3695425753775714}]}, 5432: {'frame': 5432, 'ionic_force': [1.1073409914970398, -2.299594771116972, -5.362725257873535], 'ionic_force_magnitude': 5.939121346986686, 'motion_vector': [-2.0052490234375, -1.7602043151855469, -0.211578369140625], 'cosine_ionic_motion': 0.18632320852044088, 'ionic_motion_component': 1.106596145162802, 'ionic_force_x': 1.1073409914970398, 'ionic_force_y': -2.299594771116972, 'ionic_force_z': -5.362725257873535, 'radial_force': 2.5523205485985034, 'axial_force': -5.362725257873535, 'contributions': [{'ion': 1309, 'force': [-0.5481927990913391, -3.5546693801879883, -2.8332223892211914], 'magnitude': 4.578573703765869, 'distance': 8.51537799835205, 'cosine_with_motion': 0.6491793774627083, 'motion_component': 2.972315746727638}, {'ion': 1320, 'force': [0.22608864307403564, -0.023177023977041245, 1.754052996635437], 'magnitude': 1.7687156200408936, 'distance': 13.700613975524902, 'cosine_with_motion': -0.1655403146509752, 'motion_component': -0.29279375053671397}, {'ion': 1469, 'force': [1.5149571895599365, 1.144568681716919, -2.3458662033081055], 'magnitude': 3.0179829597473145, 'distance': 10.488433837890625, 'cosine_with_motion': -0.5640343802705116, 'motion_component': -1.7022461345254385}, {'ion': 2434, 'force': [-0.08551204204559326, 0.1336829513311386, -1.9376896619796753], 'magnitude': 1.9441771507263184, 'distance': 13.06775951385498, 'cosine_with_motion': 0.06651673609911267, 'motion_component': 0.12932031630161678}]}, 5433: {'frame': 5433, 'ionic_force': [-0.44162964820861816, -0.36573115549981594, -4.841521263122559], 'ionic_force_magnitude': 4.875358875564747, 'motion_vector': [1.0330657958984375, 1.6155204772949219, -5.069999694824219], 'cosine_ionic_motion': 0.889221364727531, 'ionic_motion_component': 4.335273272866165, 'ionic_force_x': -0.44162964820861816, 'ionic_force_y': -0.36573115549981594, 'ionic_force_z': -4.841521263122559, 'radial_force': 0.5734073807338883, 'axial_force': -4.841521263122559, 'contributions': [{'ion': 1309, 'force': [-0.640687882900238, -1.2333738803863525, -1.1129107475280762], 'magnitude': 1.7805230617523193, 'distance': 13.655111312866211, 'cosine_with_motion': 0.30959821103666846, 'motion_component': 0.551246759031236}, {'ion': 1320, 'force': [-0.537470281124115, 0.01673593558371067, 1.5264745950698853], 'magnitude': 1.6184186935424805, 'distance': 14.322657585144043, 'cosine_with_motion': -0.9424075972696683, 'motion_component': -1.525210077137657}, {'ion': 1469, 'force': [1.1431920528411865, 1.02493155002594, -3.420396089553833], 'magnitude': 3.749197483062744, 'distance': 9.410222053527832, 'cosine_with_motion': 0.9928946105038673, 'motion_component': 3.722558026865098}, {'ion': 2434, 'force': [-0.40666353702545166, -0.174024760723114, -1.8346890211105347], 'magnitude': 1.8872582912445068, 'distance': 13.263354301452637, 'cosine_with_motion': 0.8407321155935801, 'motion_component': 1.586678610431468}]}}</t>
+          <t>{5415: {'frame': 5415, 'ionic_force': [-0.86297807097435, 12.021617323160172, -7.310816407203674], 'ionic_force_magnitude': 14.096526194609996, 'motion_vector': [-0.3487205505371094, 3.4752159118652344, 0.6145477294921875], 'cosine_ionic_motion': 0.7518541705699963, 'ionic_motion_component': 10.598532009966725, 'ionic_force_x': -0.86297807097435, 'ionic_force_y': 12.021617323160172, 'ionic_force_z': -7.310816407203674, 'radial_force': 12.05255218679792, 'axial_force': -7.310816407203674, 'before_closest_residue': None, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-1.2417367696762085, 2.2549033164978027, 3.7121427059173584], 'magnitude': 4.517355442047119, 'distance': 8.572882652282715, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 780, 'cosine_with_motion': 0.6585883074501265, 'motion_component': 2.9750776534110397}, {'ion': 1469, 'force': [3.919631004333496, 7.311126232147217, -1.3659437894821167], 'magnitude': 8.407251358032227, 'distance': 6.284084796905518, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.7781850453014673, 'motion_component': 6.542397326645556}, {'ion': 2434, 'force': [-3.1615939140319824, 2.1154823303222656, -7.686925411224365], 'magnitude': 8.576698303222656, 'distance': 6.221698760986328, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.12264335860419856, 'motion_component': 1.0518751575718213}, {'ion': 2444, 'force': [-0.37927839159965515, 0.34010544419288635, -1.9700899124145508], 'magnitude': 2.0348901748657227, 'distance': 12.773165702819824, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.014340683672517583, 'motion_component': 0.0291817164848438}]}, 5416: {'frame': 5416, 'ionic_force': [-2.890625089406967, 9.539554595947266, -3.3671732246875763], 'ionic_force_magnitude': 10.52124853910507, 'motion_vector': [-2.1743736267089844, -0.24370956420898438, 0.42597198486328125], 'cosine_ionic_motion': 0.10771079835192808, 'ionic_motion_component': 1.1332520798060641, 'ionic_force_x': -2.890625089406967, 'ionic_force_y': 9.539554595947266, 'ionic_force_z': -3.3671732246875763, 'radial_force': 9.967889209685652, 'axial_force': -3.3671732246875763, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-1.7372729778289795, 1.9497443437576294, 1.9252551794052124], 'magnitude': 3.244414806365967, 'distance': 10.115814208984375, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 130, 'cosine_with_motion': 0.57002217966702, 'motion_component': 1.849388441445887}, {'ion': 1469, 'force': [1.0098694562911987, 3.874903678894043, -0.12357929348945618], 'magnitude': 4.0062432289123535, 'distance': 9.103331565856934, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.35753160520772975, 'motion_component': -1.432358656018975}, {'ion': 2434, 'force': [-1.7631807327270508, 3.0347986221313477, -3.503937005996704], 'magnitude': 4.959474086761475, 'distance': 8.181844711303711, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.14487779028910183, 'motion_component': 0.7185176510370184}, {'ion': 2444, 'force': [-0.4000408351421356, 0.6801079511642456, -1.6649121046066284], 'magnitude': 1.8424201011657715, 'distance': 13.423776626586914, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.0012458317985159255, 'motion_component': -0.00229534554213906}]}, 5417: {'frame': 5417, 'ionic_force': [-4.601493835449219, 9.4010049700737, -1.1370874345302582], 'ionic_force_magnitude': 10.528324073602322, 'motion_vector': [0.7505950927734375, 1.0793838500976562, -1.4337081909179688], 'cosine_ionic_motion': 0.4064264224237802, 'ionic_motion_component': 4.278989087352351, 'ionic_force_x': -4.601493835449219, 'ionic_force_y': 9.4010049700737, 'ionic_force_z': -1.1370874345302582, 'radial_force': 10.46673970083462, 'axial_force': -1.1370874345302582, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-1.6386932134628296, 1.689590573310852, 3.3819234371185303], 'magnitude': 4.120368480682373, 'distance': 8.976375579833984, 'before_closest_residue': 780, 'closest_residue': 130, 'next_closest_residue': 130, 'cosine_with_motion': -0.5308672048478624, 'motion_component': -2.187368593057652}, {'ion': 1469, 'force': [0.2765955328941345, 4.555323600769043, -0.1436668336391449], 'magnitude': 4.56597375869751, 'distance': 8.527118682861328, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.6001537030888063, 'motion_component': 2.7402861903056674}, {'ion': 2434, 'force': [-2.509505271911621, 2.4902234077453613, -2.8283956050872803], 'magnitude': 4.527543544769287, 'distance': 8.563232421875, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5517515902465349, 'motion_component': 2.4980793799438032}, {'ion': 2444, 'force': [-0.7298908829689026, 0.6658673882484436, -1.5469484329223633], 'magnitude': 1.8355298042297363, 'distance': 13.448948860168457, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.669012387353238, 'motion_component': 1.227992153000633}]}, 5418: {'frame': 5418, 'ionic_force': [-1.8272255063056946, 7.148484110832214, -0.753704845905304], 'ionic_force_magnitude': 7.416714173301805, 'motion_vector': [0.6279106140136719, 0.4439239501953125, -0.27136993408203125], 'cosine_ionic_motion': 0.3688091800561364, 'ionic_motion_component': 2.735352272966164, 'ionic_force_x': -1.8272255063056946, 'ionic_force_y': 7.148484110832214, 'ionic_force_z': -0.753704845905304, 'radial_force': 7.378318110092214, 'axial_force': -0.753704845905304, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-1.2601678371429443, 2.125608205795288, 2.1942358016967773], 'magnitude': 3.3046791553497314, 'distance': 10.023154258728027, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 780, 'cosine_with_motion': -0.1644300780964941, 'motion_component': -0.5433886430388242}, {'ion': 1469, 'force': [0.4336826205253601, 3.54756498336792, -0.8087297081947327], 'magnitude': 3.6643335819244385, 'distance': 9.518566131591797, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.6916117806805393, 'motion_component': 2.5342963743771456}, {'ion': 2434, 'force': [-1.0007402896881104, 1.4753109216690063, -2.1392109394073486], 'magnitude': 2.784644842147827, 'distance': 10.919032096862793, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.26733916725288576, 'motion_component': 0.7444446326850809}]}, 5419: {'frame': 5419, 'ionic_force': [-2.556093394756317, 7.023166179656982, -1.4966426491737366], 'ionic_force_magnitude': 7.622231684298261, 'motion_vector': [-0.07321548461914062, -1.4095268249511719, 1.3923492431640625], 'cosine_ionic_motion': -0.7805771866631694, 'ionic_motion_component': -5.949740164224408, 'ionic_force_x': -2.556093394756317, 'ionic_force_y': 7.023166179656982, 'ionic_force_z': -1.4966426491737366, 'radial_force': 7.473852863804219, 'axial_force': -1.4966426491737366, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-2.2032456398010254, 2.115774631500244, 1.356068730354309], 'magnitude': 3.3421125411987305, 'distance': 9.966863632202148, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 423, 'cosine_with_motion': -0.14077735077576017, 'motion_component': -0.4704937454166113}, {'ion': 1469, 'force': [0.5705264210700989, 3.1289117336273193, -0.7028989195823669], 'magnitude': 3.257246732711792, 'distance': 10.095869064331055, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.8409491019474874, 'motion_component': -2.7391786691732083}, {'ion': 2434, 'force': [-0.9233741760253906, 1.778479814529419, -2.1498124599456787], 'magnitude': 2.9389290809631348, 'distance': 10.628561973571777, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9323354010550714, 'motion_component': -2.7400675900062055}]}, 5420: {'frame': 5420, 'ionic_force': [-4.017000198364258, 7.976373076438904, -4.721324697136879], 'ionic_force_magnitude': 10.101966389965497, 'motion_vector': [1.37384033203125, 0.6198310852050781, 1.271148681640625], 'cosine_ionic_motion': -0.33017035763647795, 'ionic_motion_component': -3.3353698558065883, 'ionic_force_x': -4.017000198364258, 'ionic_force_y': 7.976373076438904, 'ionic_force_z': -4.721324697136879, 'radial_force': 8.930779252013673, 'axial_force': -4.721324697136879, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-2.296131134033203, 1.0717114210128784, 0.202259823679924], 'magnitude': 2.5419859886169434, 'distance': 11.428321838378906, 'before_closest_residue': 780, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.44556351398937477, 'motion_component': -1.132616194223882}, {'ion': 1469, 'force': [0.5067126154899597, 4.24498176574707, -0.2817506194114685], 'magnitude': 4.2843918800354, 'distance': 8.802873611450195, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.3514901901202061, 'motion_component': 1.505921613751351}, {'ion': 2434, 'force': [-1.693018913269043, 2.0171566009521484, -2.944333791732788], 'magnitude': 3.9502322673797607, 'distance': 9.167643547058105, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6186448965736641, 'motion_component': -2.4437910563266314}, {'ion': 2444, 'force': [-0.5345627665519714, 0.6425232887268066, -1.6975001096725464], 'magnitude': 1.8921153545379639, 'distance': 13.246319770812988, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6685027957609565, 'motion_component': -1.2648843400024923}]}, 5421: {'frame': 5421, 'ionic_force': [-4.36628919839859, 9.376880168914795, -2.967519700527191], 'ionic_force_magnitude': 10.76087990079142, 'motion_vector': [-0.43817138671875, 0.11849594116210938, -1.432342529296875], 'cosine_ionic_motion': 0.44993154895126, 'ionic_motion_component': 4.841659361841564, 'ionic_force_x': -4.36628919839859, 'ionic_force_y': 9.376880168914795, 'ionic_force_z': -2.967519700527191, 'radial_force': 10.343614603524232, 'axial_force': -2.967519700527191, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-3.586841344833374, 1.4117411375045776, 1.6100742816925049], 'magnitude': 4.177413463592529, 'distance': 8.914875984191895, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 780, 'cosine_with_motion': -0.09037177139810013, 'motion_component': -0.377520252610303}, {'ion': 1469, 'force': [1.202595829963684, 3.48968505859375, 0.13294559717178345], 'magnitude': 3.6934826374053955, 'distance': 9.480932235717773, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.05475204072792799, 'motion_component': -0.2022257049529017}, {'ion': 2434, 'force': [-1.507516622543335, 3.459397077560425, -2.9776651859283447], 'magnitude': 4.806924819946289, 'distance': 8.310657501220703, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7387225120534889, 'motion_component': 3.550983443186361}, {'ion': 2444, 'force': [-0.4745270609855652, 1.0160568952560425, -1.7328743934631348], 'magnitude': 2.0640740394592285, 'distance': 12.682544708251953, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.906179644664221, 'motion_component': 1.8704217850621294}]}, 5422: {'frame': 5422, 'ionic_force': [-3.337195932865143, 8.502465009689331, -4.2525006383657455], 'ionic_force_magnitude': 10.075343647470499, 'motion_vector': [0.1480560302734375, -0.8996047973632812, 0.5749053955078125], 'cosine_ionic_motion': -0.9749704271170396, 'ionic_motion_component': -9.823162099325264, 'ionic_force_x': -3.337195932865143, 'ionic_force_y': 8.502465009689331, 'ionic_force_z': -4.2525006383657455, 'radial_force': 9.133936059296838, 'axial_force': -4.2525006383657455, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-2.566864252090454, 1.8449293375015259, 0.5315044522285461], 'magnitude': 3.205472469329834, 'distance': 10.17707633972168, 'before_closest_residue': 455, 'closest_residue': 780, 'next_closest_residue': 423, 'cosine_with_motion': -0.501938957417652, 'motion_component': -1.6089514764139317}, {'ion': 1469, 'force': [1.0937838554382324, 3.111398458480835, -0.23599140346050262], 'magnitude': 3.3064868450164795, 'distance': 10.020413398742676, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1105, 'cosine_with_motion': -0.7780253814588048, 'motion_component': -2.572530709600221}, {'ion': 2434, 'force': [-1.3929810523986816, 2.763676643371582, -2.991767168045044], 'magnitude': 4.304529666900635, 'distance': 8.782258033752441, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9510453856970562, 'motion_component': -4.093803070234479}, {'ion': 2444, 'force': [-0.4711344838142395, 0.7824605703353882, -1.5562465190887451], 'magnitude': 1.8044710159301758, 'distance': 13.564197540283203, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8578010229664738, 'motion_component': -1.5478770422136625}]}, 5423: {'frame': 5423, 'ionic_force': [-7.194524526596069, 10.885988421738148, -3.873266875743866], 'ionic_force_magnitude': 13.611323351266917, 'motion_vector': [-0.2519950866699219, 0.5466041564941406, 0.0637054443359375], 'cosine_ionic_motion': 0.9123871441683606, 'ionic_motion_component': 12.418796440814543, 'ionic_force_x': -7.194524526596069, 'ionic_force_y': 10.885988421738148, 'ionic_force_z': -3.873266875743866, 'radial_force': 13.048598663535078, 'axial_force': -3.873266875743866, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-7.53367280960083, -0.03545748442411423, 1.090088963508606], 'magnitude': 7.612212181091309, 'distance': 6.604099273681641, 'before_closest_residue': 780, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.4229142947215601, 'motion_component': 3.219313426221046}, {'ion': 1469, 'force': [3.078547954559326, 6.243687152862549, 0.9668325781822205], 'magnitude': 7.0282182693481445, 'distance': 6.873001575469971, 'before_closest_residue': 1073, 'closest_residue': 1105, 'next_closest_residue': 1073, 'cosine_with_motion': 0.6343949704708078, 'motion_component': 4.45866631981975}, {'ion': 2434, 'force': [-2.2350199222564697, 3.7992143630981445, -4.083253383636475], 'magnitude': 6.008519172668457, 'distance': 7.4333624839782715, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.654372414694982, 'motion_component': 3.931809165797851}, {'ion': 2444, 'force': [-0.5043797492980957, 0.8785443902015686, -1.8469350337982178], 'magnitude': 2.106515645980835, 'distance': 12.554132461547852, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3840500646571, 'motion_component': 0.8090074727170524}]}, 5424: {'frame': 5424, 'ionic_force': [-9.829724729061127, 8.064699590206146, -3.82029065862298], 'ionic_force_magnitude': 13.276200075539274, 'motion_vector': [-1.8115425109863281, -1.1403274536132812, 0.10491180419921875], 'cosine_ionic_motion': 0.2885408107742469, 'ionic_motion_component': 3.8307255337972204, 'ionic_force_x': -9.829724729061127, 'ionic_force_y': 8.064699590206146, 'ionic_force_z': -3.82029065862298, 'radial_force': 12.71467135750614, 'axial_force': -3.82029065862298, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-8.29712200164795, 0.1777876615524292, 0.9536499381065369], 'magnitude': 8.353639602661133, 'distance': 6.30421781539917, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.8338212823493995, 'motion_component': 6.965442263992603}, {'ion': 1469, 'force': [0.7835202217102051, 3.773498058319092, -0.03277162089943886], 'magnitude': 3.854123115539551, 'distance': 9.281245231628418, 'before_closest_residue': 1105, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.6932081742710833, 'motion_component': -2.671709695405911}, {'ion': 2434, 'force': [-1.8014920949935913, 3.1987240314483643, -3.0620651245117188], 'magnitude': 4.7805280685424805, 'distance': 8.33357048034668, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.06884699269022612, 'motion_component': -0.3291250055472901}, {'ion': 2444, 'force': [-0.5146308541297913, 0.914689838886261, -1.6791038513183594], 'magnitude': 1.9801243543624878, 'distance': 12.948599815368652, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.06761305818944655, 'motion_component': -0.13388225810879462}]}, 5425: {'frame': 5425, 'ionic_force': [-7.359991593286395, 3.306031584739685, -5.195836968719959], 'ionic_force_magnitude': 9.59666832281182, 'motion_vector': [0.7701644897460938, 1.122161865234375, -0.6427230834960938], 'cosine_ionic_motion': 0.09560626418969688, 'ionic_motion_component': 0.9175016070116421, 'ionic_force_x': -7.359991593286395, 'ionic_force_y': 3.306031584739685, 'ionic_force_z': -5.195836968719959, 'radial_force': 8.068415029765314, 'axial_force': -5.195836968719959, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-4.172080993652344, -2.511462926864624, -0.10490787774324417], 'magnitude': 4.87080192565918, 'distance': 8.255983352661133, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': -0.8135006963141567, 'motion_component': -3.9624007676868804}, {'ion': 1469, 'force': [0.024452881887555122, 2.9648444652557373, -0.17231887578964233], 'magnitude': 2.9699485301971436, 'distance': 10.572911262512207, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.77325275445924, 'motion_component': 2.2965209036455843}, {'ion': 2434, 'force': [-2.4676637649536133, 2.1257126331329346, -3.127074718475342], 'magnitude': 4.515153884887695, 'distance': 8.574973106384277, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.36708742493103036, 'motion_component': 1.6574562268455113}, {'ion': 2444, 'force': [-0.7446997165679932, 0.7269374132156372, -1.791535496711731], 'magnitude': 2.0718626976013184, 'distance': 12.658683776855469, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4469046351630615, 'motion_component': 0.9259250504055956}]}, 5426: {'frame': 5426, 'ionic_force': [-5.71360582113266, 4.7653467655181885, -4.617043234407902], 'ionic_force_magnitude': 8.756192637402826, 'motion_vector': [0.9683570861816406, -1.1876640319824219, -1.7886962890625], 'cosine_ionic_motion': -0.14225960241465066, 'ionic_motion_component': -1.2456524832630174, 'ionic_force_x': -5.71360582113266, 'ionic_force_y': 4.7653467655181885, 'ionic_force_z': -4.617043234407902, 'radial_force': 7.440014870611193, 'axial_force': -4.617043234407902, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [-3.82336688041687, -1.281545877456665, 0.038811035454273224], 'magnitude': 4.032617092132568, 'distance': 9.073514938354492, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': -0.23686059447804464, 'motion_component': -0.9551680765469284}, {'ion': 1469, 'force': [0.3030494451522827, 3.1069347858428955, -0.22176901996135712], 'magnitude': 3.129547119140625, 'distance': 10.299788475036621, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.40697035549176575, 'motion_component': -1.2736328422891834}, {'ion': 2434, 'force': [-1.6431152820587158, 2.2570924758911133, -2.791811227798462], 'magnitude': 3.948227882385254, 'distance': 9.169970512390137, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.07762936310697147, 'motion_component': 0.306498423729046}, {'ion': 2444, 'force': [-0.5501731038093567, 0.6828653812408447, -1.642274022102356], 'magnitude': 1.8617355823516846, 'distance': 13.353959083557129, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.3634511718692843, 'motion_component': 0.6766499945516973}]}, 5427: {'frame': 5427, 'ionic_force': [-8.04122668504715, 2.214553475379944, -8.471194505691528], 'ionic_force_magnitude': 11.888091101976386, 'motion_vector': [1.9277992248535156, -0.47090911865234375, 1.2962722778320312], 'cosine_ionic_motion': -0.9768244492629804, 'ionic_motion_component': -11.612578043476221, 'ionic_force_x': -8.04122668504715, 'ionic_force_y': 2.214553475379944, 'ionic_force_z': -8.471194505691528, 'radial_force': 8.340597921949707, 'axial_force': -8.471194505691528, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 98, 'contributions': [{'ion': 1309, 'force': [-7.151926517486572, -4.424306392669678, -2.266660690307617], 'magnitude': 8.709896087646484, 'distance': 6.1739420890808105, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 423, 'cosine_with_motion': -0.7092263629987502, 'motion_component': -6.17728795671141}, {'ion': 1469, 'force': [1.0913169384002686, 4.217013835906982, -1.362021803855896], 'magnitude': 4.563910484313965, 'distance': 8.529046058654785, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.1522963508158204, 'motion_component': -0.6950669595563213}, {'ion': 2434, 'force': [-1.582262396812439, 1.9491033554077148, -3.3685457706451416], 'magnitude': 4.2011494636535645, 'distance': 8.889656066894531, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.8369729709418179, 'motion_component': -3.516248744739322}, {'ion': 2444, 'force': [-0.398354709148407, 0.4727426767349243, -1.4739662408828735], 'magnitude': 1.5983580350875854, 'distance': 14.412257194519043, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7657695663854323, 'motion_component': -1.2239739834485697}]}, 5428: {'frame': 5428, 'ionic_force': [-4.013658359646797, 2.036353588104248, -10.628021240234375], 'ionic_force_magnitude': 11.541708055856407, 'motion_vector': [0.24727249145507812, -2.330799102783203, -4.778404235839844], 'cosine_ionic_motion': 0.733311095968307, 'ionic_motion_component': 8.4636625837863, 'ionic_force_x': -4.013658359646797, 'ionic_force_y': 2.036353588104248, 'ionic_force_z': -10.628021240234375, 'radial_force': 4.5006876545421, 'axial_force': -10.628021240234375, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [-4.697807788848877, -6.503828525543213, -1.5563700199127197], 'magnitude': 8.172605514526367, 'distance': 6.373658657073975, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 423, 'cosine_with_motion': 0.49277885349233314, 'motion_component': 4.027286881652531}, {'ion': 1469, 'force': [2.3175904750823975, 4.2220258712768555, -0.8517012596130371], 'magnitude': 4.891024589538574, 'distance': 8.238897323608398, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.19967505294610755, 'motion_component': -0.9766156258850804}, {'ion': 2434, 'force': [-1.4328304529190063, 3.6519341468811035, -6.213566780090332], 'magnitude': 7.3483357429504395, 'distance': 6.7216291427612305, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.5324640438268261, 'motion_component': 3.91272456724384}, {'ion': 2444, 'force': [-0.20061059296131134, 0.666222095489502, -2.006383180618286], 'magnitude': 2.123598337173462, 'distance': 12.503536224365234, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7064737784360602, 'motion_component': 1.5002665511818145}]}, 5429: {'frame': 5429, 'ionic_force': [-0.07442072033882141, -0.02468770742416382, -7.9879608154296875], 'ionic_force_magnitude': 7.9883456306893565, 'motion_vector': [3.7690887451171875, -2.5068588256835938, -3.2027816772460938], 'cosine_ionic_motion': 0.572624250980996, 'ionic_motion_component': 4.574320433350805, 'ionic_force_x': -0.07442072033882141, 'ionic_force_y': -0.02468770742416382, 'ionic_force_z': -7.9879608154296875, 'radial_force': 0.0784087145259389, 'axial_force': -7.9879608154296875, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [-1.8123735189437866, -2.4131195545196533, -2.5620484352111816], 'magnitude': 3.9587795734405518, 'distance': 9.15774154663086, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 455, 'cosine_with_motion': 0.3381963958982721, 'motion_component': 1.3388449937113478}, {'ion': 1469, 'force': [1.9238256216049194, 2.0180952548980713, -2.4386179447174072], 'magnitude': 3.7041423320770264, 'distance': 9.467279434204102, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.4869727291469073, 'motion_component': 1.803816336372222}, {'ion': 2434, 'force': [-0.18587282299995422, 0.3703365921974182, -2.9872944355010986], 'magnitude': 3.0158956050872803, 'distance': 10.492063522338867, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.4747044569942231, 'motion_component': 1.431659057345513}]}, 5430: {'frame': 5430, 'ionic_force': [2.4746485874056816, -1.7678358405828476, -3.220875859260559], 'ionic_force_magnitude': 4.429804791541682, 'motion_vector': [-0.60418701171875, 0.23330307006835938, 2.4262313842773438], 'cosine_ionic_motion': -0.8739764423926943, 'ionic_motion_component': -3.87154503220571, 'ionic_force_x': 2.4746485874056816, 'ionic_force_y': -1.7678358405828476, 'ionic_force_z': -3.220875859260559, 'radial_force': 3.0412381015629473, 'axial_force': -3.220875859260559, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [0.12402363866567612, -1.6623444557189941, -1.531604528427124], 'magnitude': 2.26375412940979, 'distance': 12.110285758972168, 'before_closest_residue': 423, 'closest_residue': 455, 'next_closest_residue': 98, 'cosine_with_motion': -0.7350923070401219, 'motion_component': -1.6640683471142113}, {'ion': 1320, 'force': [0.5745420455932617, -0.34557026624679565, 1.4239434003829956], 'magnitude': 1.5738908052444458, 'distance': 14.523849487304688, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7658917483680011, 'motion_component': 1.20542995909179}, {'ion': 1469, 'force': [1.4435352087020874, 0.3784688711166382, -1.497428059577942], 'magnitude': 2.11407732963562, 'distance': 12.531660079956055, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.832002319477491, 'motion_component': -1.7589173250676327}, {'ion': 2434, 'force': [0.33254769444465637, -0.13838998973369598, -1.6157866716384888], 'magnitude': 1.6554474830627441, 'distance': 14.161567687988281, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.9991191765221671, 'motion_component': -1.6539893131995007}]}, 5431: {'frame': 5431, 'ionic_force': [3.104661077260971, -1.3943484723567963, -5.393718481063843], 'ionic_force_magnitude': 6.377721154142177, 'motion_vector': [-2.8593292236328125, 1.6220474243164062, -1.3614044189453125], 'cosine_ionic_motion': -0.1672747077358023, 'ionic_motion_component': -1.0668314420795766, 'ionic_force_x': 3.104661077260971, 'ionic_force_y': -1.3943484723567963, 'ionic_force_z': -5.393718481063843, 'radial_force': 3.4033994868400304, 'axial_force': -5.393718481063843, 'before_closest_residue': 780, 'closest_residue': 780, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [0.6289064884185791, -2.2084546089172363, -1.3620975017547607], 'magnitude': 2.669851064682007, 'distance': 11.151300430297852, 'before_closest_residue': 455, 'closest_residue': 98, 'next_closest_residue': 455, 'cosine_with_motion': -0.3711823052455934, 'motion_component': -0.9910014747644809}, {'ion': 1469, 'force': [2.067415952682495, 1.0044293403625488, -1.9814109802246094], 'magnitude': 3.0346460342407227, 'distance': 10.459598541259766, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.14676256689893674, 'motion_component': -0.44537244017870137}, {'ion': 2434, 'force': [0.40833863615989685, -0.19032320380210876, -2.0502099990844727], 'magnitude': 2.0991246700286865, 'distance': 12.576213836669922, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.17604603464467547, 'motion_component': 0.3695425753775714}]}, 5432: {'frame': 5432, 'ionic_force': [1.1073409914970398, -2.299594771116972, -5.362725257873535], 'ionic_force_magnitude': 5.939121346986686, 'motion_vector': [-2.0052490234375, -1.7602043151855469, -0.211578369140625], 'cosine_ionic_motion': 0.18632320852044088, 'ionic_motion_component': 1.106596145162802, 'ionic_force_x': 1.1073409914970398, 'ionic_force_y': -2.299594771116972, 'ionic_force_z': -5.362725257873535, 'radial_force': 2.5523205485985034, 'axial_force': -5.362725257873535, 'before_closest_residue': 780, 'closest_residue': 130, 'next_closest_residue': 1105, 'contributions': [{'ion': 1309, 'force': [-0.5481927990913391, -3.5546693801879883, -2.8332223892211914], 'magnitude': 4.578573703765869, 'distance': 8.51537799835205, 'before_closest_residue': 98, 'closest_residue': 455, 'next_closest_residue': 423, 'cosine_with_motion': 0.6491793774627083, 'motion_component': 2.972315746727638}, {'ion': 1320, 'force': [0.22608864307403564, -0.023177023977041245, 1.754052996635437], 'magnitude': 1.7687156200408936, 'distance': 13.700613975524902, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.1655403146509752, 'motion_component': -0.29279375053671397}, {'ion': 1469, 'force': [1.5149571895599365, 1.144568681716919, -2.3458662033081055], 'magnitude': 3.0179829597473145, 'distance': 10.488433837890625, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.5640343802705116, 'motion_component': -1.7022461345254385}, {'ion': 2434, 'force': [-0.08551204204559326, 0.1336829513311386, -1.9376896619796753], 'magnitude': 1.9441771507263184, 'distance': 13.06775951385498, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.06651673609911267, 'motion_component': 0.12932031630161678}]}, 5433: {'frame': 5433, 'ionic_force': [-0.44162964820861816, -0.36573115549981594, -4.841521263122559], 'ionic_force_magnitude': 4.875358875564747, 'motion_vector': [1.0330657958984375, 1.6155204772949219, -5.069999694824219], 'cosine_ionic_motion': 0.889221364727531, 'ionic_motion_component': 4.3352</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{5477: {'frame': 5477, 'ionic_force': [1.4224569201469421, -4.641303360462189, -9.415545463562012], 'ionic_force_magnitude': 10.59327980136061, 'motion_vector': [-0.5623664855957031, 0.9072761535644531, 0.3484649658203125], 'cosine_ionic_motion': -0.6970970980387372, 'ionic_motion_component': -7.384544608240852, 'ionic_force_x': 1.4224569201469421, 'ionic_force_y': -4.641303360462189, 'ionic_force_z': -9.415545463562012, 'radial_force': 4.854387765054573, 'axial_force': -9.415545463562012, 'contributions': [{'ion': 1309, 'force': [-0.14590446650981903, -7.744018077850342, -4.193130970001221], 'magnitude': 8.807579040527344, 'distance': 6.1396098136901855, 'cosine_with_motion': -0.8498765392041681, 'motion_component': -7.485354932675172}, {'ion': 1469, 'force': [1.5043941736221313, 2.458629608154297, -1.5455207824707031], 'magnitude': 3.270580291748047, 'distance': 10.075268745422363, 'cosine_with_motion': 0.23038555492130164, 'motion_component': 0.753494470362682}, {'ion': 2444, 'force': [0.06396721303462982, 0.6440851092338562, -3.676893711090088], 'magnitude': 3.7334280014038086, 'distance': 9.430074691772461, 'cosine_with_motion': -0.174821671211077, 'motion_component': -0.6526841261401124}]}, 5478: {'frame': 5478, 'ionic_force': [3.782637048512697, -4.220937579870224, -11.806665897369385], 'ionic_force_magnitude': 13.096641428474966, 'motion_vector': [5.6822967529296875, -1.4546623229980469, 1.581939697265625], 'cosine_ionic_motion': 0.112572399553655, 'ionic_motion_component': 1.4743203516972347, 'ionic_force_x': 3.782637048512697, 'ionic_force_y': -4.220937579870224, 'ionic_force_z': -11.806665897369385, 'radial_force': 5.667861774420893, 'axial_force': -11.806665897369385, 'contributions': [{'ion': 1309, 'force': [2.848625421524048, -7.680440902709961, -5.491806507110596], 'magnitude': 9.862239837646484, 'distance': 5.802047252655029, 'cosine_with_motion': 0.311636488808021, 'motion_component': 3.073433847690566}, {'ion': 1469, 'force': [1.1187093257904053, 2.1294939517974854, -1.1434855461120605], 'magnitude': 2.663421392440796, 'distance': 11.164752006530762, 'cosine_with_motion': 0.08962698302468124, 'motion_component': 0.23871443615680477}, {'ion': 2443, 'force': [-0.03920864686369896, 0.29816392064094543, -1.4478132724761963], 'magnitude': 1.478716492652893, 'distance': 14.983959197998047, 'cosine_with_motion': -0.3280365163349735, 'motion_component': -0.48507299002336723}, {'ion': 2444, 'force': [-0.14548905193805695, 1.0318454504013062, -3.7235605716705322], 'magnitude': 3.8666231632232666, 'distance': 9.266230583190918, 'cosine_with_motion': -0.34985431505545295, 'motion_component': -1.3527548319276432}]}, 5479: {'frame': 5479, 'ionic_force': [7.66579008102417, -0.03574265539646149, -6.5100264847278595], 'ionic_force_magnitude': 10.057139749232956, 'motion_vector': [-0.8315162658691406, 0.4536933898925781, 0.4904327392578125], 'cosine_ionic_motion': -0.8933169575861272, 'ionic_motion_component': -8.98421348280329, 'ionic_force_x': 7.66579008102417, 'ionic_force_y': -0.03574265539646149, 'ionic_force_z': -6.5100264847278595, 'radial_force': 7.665873407756179, 'axial_force': -6.5100264847278595, 'contributions': [{'ion': 1309, 'force': [2.8427734375, -2.1192972660064697, -0.8717526197433472], 'magnitude': 3.6514017581939697, 'distance': 9.535407066345215, 'cosine_with_motion': -0.963547918868339, 'motion_component': -3.518300505546865}, {'ion': 1469, 'force': [1.5580865144729614, 1.1739774942398071, -0.4098491966724396], 'magnitude': 1.9934475421905518, 'distance': 12.905256271362305, 'cosine_with_motion': -0.4533369941770629, 'motion_component': -0.9037035172938319}, {'ion': 2443, 'force': [0.5962351560592651, 0.1816510409116745, -1.6120604276657104], 'magnitude': 1.7283612489700317, 'distance': 13.859634399414062, 'cosine_with_motion': -0.6530594455283119, 'motion_component': -1.1287225779949241}, {'ion': 2444, 'force': [2.6686949729919434, 0.7279260754585266, -3.6163642406463623], 'magnitude': 4.553009986877441, 'distance': 8.539250373840332, 'cosine_with_motion': -0.7541136132982074, 'motion_component': -3.433486780340937}]}, 5480: {'frame': 5480, 'ionic_force': [8.63328468799591, 0.006521552801132202, -5.980384021997452], 'ionic_force_magnitude': 10.502315939124951, 'motion_vector': [-2.4467201232910156, 2.9426307678222656, 1.0514373779296875], 'cosine_ionic_motion': -0.6571806221442732, 'ionic_motion_component': -6.9019185228298525, 'ionic_force_x': 8.63328468799591, 'ionic_force_y': 0.006521552801132202, 'ionic_force_z': -5.980384021997452, 'radial_force': 8.633287151174551, 'axial_force': -5.980384021997452, 'contributions': [{'ion': 1309, 'force': [4.6044087409973145, -2.470323085784912, -0.8643374443054199], 'magnitude': 5.296239852905273, 'distance': 7.917448043823242, 'cosine_with_motion': -0.9250340582306482, 'motion_component': -4.899202125768213}, {'ion': 1469, 'force': [1.6390438079833984, 1.4995357990264893, -0.4266315996646881], 'magnitude': 2.2620978355407715, 'distance': 12.11471939086914, 'cosine_with_motion': -0.005154729957164885, 'motion_component': -0.011660503617133777}, {'ion': 2443, 'force': [0.6318773031234741, 0.20215561985969543, -1.57472562789917], 'magnitude': 1.708770513534546, 'distance': 13.938857078552246, 'cosine_with_motion': -0.38439987659516817, 'motion_component': -0.6568511695921728}, {'ion': 2444, 'force': [1.7579548358917236, 0.7751532196998596, -3.114689350128174], 'magnitude': 3.6595845222473145, 'distance': 9.524741172790527, 'cosine_with_motion': -0.36457819253244267, 'motion_component': -1.334204640375063}]}, 5481: {'frame': 5481, 'ionic_force': [10.722378462553024, 3.6098837852478027, -5.247070275247097], 'ionic_force_magnitude': 12.471263260415826, 'motion_vector': [1.9404220581054688, -4.451213836669922, 0.8924026489257812], 'cosine_ionic_motion': 0.0008944936529652115, 'ionic_motion_component': 0.011155465830900187, 'ionic_force_x': 10.722378462553024, 'ionic_force_y': 3.6098837852478027, 'ionic_force_z': -5.247070275247097, 'radial_force': 11.313737704101856, 'axial_force': -5.247070275247097, 'contributions': [{'ion': 1309, 'force': [8.690352439880371, -0.589633584022522, -0.05870877951383591], 'magnitude': 8.710530281066895, 'distance': 6.173717498779297, 'cosine_with_motion': 0.45193035456920416, 'motion_component': 3.9365530964176982}, {'ion': 1469, 'force': [0.9652875065803528, 1.5830146074295044, -0.20551034808158875], 'magnitude': 1.865462303161621, 'distance': 13.34061336517334, 'cosine_with_motion': -0.5816164448618182, 'motion_component': -1.0849835709259943}, {'ion': 2443, 'force': [0.3752489387989044, 0.6354923248291016, -1.8373764753341675], 'magnitude': 1.9800541400909424, 'distance': 12.948829650878906, 'cosine_with_motion': -0.3826061510855403, 'motion_component': -0.757580910428099}, {'ion': 2444, 'force': [0.691489577293396, 1.9810104370117188, -3.145474672317505], 'magnitude': 3.781080722808838, 'distance': 9.370463371276855, 'cosine_with_motion': -0.5508565617056489, 'motion_component': -2.0828331023756945}]}, 5482: {'frame': 5482, 'ionic_force': [10.771212220191956, -0.8395132049918175, -7.971047785133123], 'ionic_force_magnitude': 13.426146055612676, 'motion_vector': [-3.371776580810547, 2.4830093383789062, -2.777191162109375], 'cosine_ionic_motion': -0.24110797819383406, 'ionic_motion_component': -3.2371509304038923, 'ionic_force_x': 10.771212220191956, 'ionic_force_y': -0.8395132049918175, 'ionic_force_z': -7.971047785133123, 'radial_force': 10.803878706916704, 'axial_force': -7.971047785133123, 'contributions': [{'ion': 1309, 'force': [2.8360345363616943, -2.8020989894866943, 0.3442707359790802], 'magnitude': 4.001671314239502, 'distance': 9.10853099822998, 'cosine_with_motion': -0.8691628231816363, 'motion_component': -3.4781039011742347}, {'ion': 1469, 'force': [2.137364387512207, 1.547278881072998, -0.054249223321676254], 'magnitude': 2.639193296432495, 'distance': 11.215882301330566, 'cosine_with_motion': -0.24237600744025303, 'motion_component': -0.6396771424608481}, {'ion': 2443, 'force': [0.930376410484314, 0.07820767909288406, -2.1504712104797363], 'magnitude': 2.344406843185425, 'distance': 11.900153160095215, 'cosine_with_motion': 0.25717236860653303, 'motion_component': 0.6029166436709448}, {'ion': 2444, 'force': [4.86743688583374, 0.33709922432899475, -6.110598087310791], 'magnitude': 7.819525718688965, 'distance': 6.515966415405273, 'cosine_with_motion': 0.035515385916932506, 'motion_component': 0.2777134832245567}]}, 5483: {'frame': 5483, 'ionic_force': [14.705014813691378, -4.830581963062286, -13.659503698348999], 'ionic_force_magnitude': 20.64349834834095, 'motion_vector': [-1.0512886047363281, -1.1198539733886719, -3.1050186157226562], 'cosine_ionic_motion': 0.45255552467683335, 'ionic_motion_component': 9.342329226198782, 'ionic_force_x': 14.705014813691378, 'ionic_force_y': -4.830581963062286, 'ionic_force_z': -13.659503698348999, 'radial_force': 15.478113023645536, 'axial_force': -13.659503698348999, 'contributions': [{'ion': 1309, 'force': [12.95172119140625, -9.656329154968262, -6.279929161071777], 'magnitude': 17.332895278930664, 'distance': 4.376565933227539, 'cosine_with_motion': 0.27807920582061574, 'motion_component': 4.819917962997209}, {'ion': 1469, 'force': [1.47786545753479, 2.6548736095428467, -0.7496045827865601], 'magnitude': 3.129592180252075, 'distance': 10.299714088439941, 'cosine_with_motion': -0.20285152649453522, 'motion_component': -0.6348425513631568}, {'ion': 2443, 'force': [0.023254413157701492, 0.36658936738967896, -1.7489255666732788], 'magnitude': 1.7870839834213257, 'distance': 13.630022048950195, 'cosine_with_motion': 0.8069254149980343, 'motion_component': 1.4420434863079719}, {'ion': 2444, 'force': [0.2521737515926361, 1.8042842149734497, -4.881044387817383], 'magnitude': 5.209954738616943, 'distance': 7.982741832733154, 'cosine_with_motion': 0.7130983805644391, 'motion_component': 3.7152102230572357}]}, 5484: {'frame': 5484, 'ionic_force': [3.3583530709147453, -1.8520203530788422, -9.582316398620605], 'ionic_force_magnitude': 10.32130332372875, 'motion_vector': [-1.2701416015625, -1.1113739013671875, -2.5788192749023438], 'cosine_ionic_motion': 0.7074375045446344, 'ionic_motion_component': 7.301677066986908, 'ionic_force_x': 3.3583530709147453, 'ionic_force_y': -1.8520203530788422, 'ionic_force_z': -9.582316398620605, 'radial_force': 3.8351681497870183, 'axial_force': -9.582316398620605, 'contributions': [{'ion': 1309, 'force': [2.1952145099639893, -4.486453056335449, -5.257387638092041], 'magnitude': 7.251713752746582, 'distance': 6.766260623931885, 'cosine_with_motion': 0.7049620782123642, 'motion_component': 5.112183207305485}, {'ion': 1469, 'force': [1.2880535125732422, 2.27970814704895, -1.8271305561065674], 'magnitude': 3.1928915977478027, 'distance': 10.19710636138916, 'cosine_with_motion': 0.05510102667779303, 'motion_component': 0.17593160856745982}, {'ion': 2444, 'force': [-0.12491495162248611, 0.35472455620765686, -2.497798204421997], 'magnitude': 2.5259511470794678, 'distance': 11.46453857421875, 'cosine_with_motion': 0.7971501673219711, 'motion_component': 2.0135623682589534}]}, 5485: {'frame': 5485, 'ionic_force': [1.483163833618164, -0.4733795076608658, -5.7409727573394775], 'ionic_force_magnitude': 5.948330128375544, 'motion_vector': [4.385654449462891, -1.0877685546875, 2.3917007446289062], 'cosine_ionic_motion': -0.22068268473215408, 'ionic_motion_component': -1.312693462403074, 'ionic_force_x': 1.483163833618164, 'ionic_force_y': -0.4733795076608658, 'ionic_force_z': -5.7409727573394775, 'radial_force': 1.5568760758731481, 'axial_force': -5.7409727573394775, 'contributions': [{'ion': 1309, 'force': [0.5064878463745117, -2.087893009185791, -3.4851157665252686], 'magnitude': 4.094125270843506, 'distance': 9.005099296569824, 'cosine_with_motion': -0.18359875780452614, 'motion_component': -0.7516762541344804}, {'ion': 1469, 'force': [0.7889192700386047, 1.6113115549087524, -1.897242546081543], 'magnitude': 2.611177444458008, 'distance': 11.275890350341797, 'cosine_with_motion': -0.21202473408075306, 'motion_component': -0.5536342103565328}, {'ion': 2436, 'force': [0.3979494571685791, -0.12599879503250122, 1.4812759160995483], 'magnitude': 1.538966417312622, 'distance': 14.687723159790039, 'cosine_with_motion': 0.6895196838728914, 'motion_component': 1.0611476762695622}, {'ion': 2444, 'force': [-0.2101927399635315, 0.129200741648674, -1.8398903608322144], 'magnitude': 1.8563593626022339, 'distance': 13.373282432556152, 'cosine_with_motion': -0.5756054760786232, 'motion_component': -1.0685306575260782}]}, 5486: {'frame': 5486, 'ionic_force': [4.225400745868683, -1.113166643306613, -5.5725942850112915], 'ionic_force_magnitude': 7.081451722937793, 'motion_vector': [-1.728607177734375, 5.325992584228516, 4.6172027587890625], 'cosine_ionic_motion': -0.7581095044957695, 'ionic_motion_component': -5.368515856787083, 'ionic_force_x': 4.225400745868683, 'ionic_force_y': -1.113166643306613, 'ionic_force_z': -5.5725942850112915, 'radial_force': 4.369571081806329, 'axial_force': -5.5725942850112915, 'contributions': [{'ion': 1309, 'force': [2.1206986904144287, -2.4510836601257324, -1.6197460889816284], 'magnitude': 3.623361825942993, 'distance': 9.57223129272461, 'cosine_with_motion': -0.9202215468575357, 'motion_component': -3.334295689758271}, {'ion': 1469, 'force': [1.5200526714324951, 1.3517338037490845, -1.3707325458526611], 'magnitude': 2.4528865814208984, 'distance': 11.634034156799316, 'cosine_with_motion': -0.098707559429281, 'motion_component': -0.24211843857373339}, {'ion': 2444, 'force': [0.584649384021759, -0.01381678692996502, -2.582115650177002], 'magnitude': 2.6475133895874023, 'distance': 11.19824504852295, 'cosine_with_motion': -0.6769000204594124, 'motion_component': -1.7921018533477944}]}, 5487: {'frame': 5487, 'ionic_force': [15.482393935322762, 3.9336164593696594, -6.411904938519001], 'ionic_force_magnitude': 17.213087618395118, 'motion_vector': [0.3015022277832031, -3.9131088256835938, 0.8899307250976562], 'cosine_ionic_motion': -0.23719556888232954, 'ionic_motion_component': -4.082868109866613, 'ionic_force_x': 15.482393935322762, 'ionic_force_y': 3.9336164593696594, 'ionic_force_z': -6.411904938519001, 'radial_force': 15.974287477629257, 'axial_force': -6.411904938519001, 'contributions': [{'ion': 1309, 'force': [13.761055946350098, -2.1138620376586914, -0.08146259933710098], 'magnitude': 13.922704696655273, 'distance': 4.883230686187744, 'cosine_with_motion': 0.22038793154140668, 'motion_component': 3.068396117715446}, {'ion': 1469, 'force': [0.9084755182266235, 1.9054216146469116, -0.2553384602069855], 'magnitude': 2.1263012886047363, 'distance': 12.495586395263672, 'cosine_with_motion': -0.8658976507435727, 'motion_component': -1.8411592612795076}, {'ion': 2443, 'force': [0.1551320105791092, 0.6592459082603455, -1.8346444368362427], 'magnitude': 1.9556562900543213, 'distance': 13.029350280761719, 'cosine_with_motion': -0.5292905712008917, 'motion_component': -1.0351104068303}, {'ion': 2444, 'force': [0.6577304601669312, 3.4828109741210938, -4.240459442138672], 'magnitude': 5.526669979095459, 'distance': 7.750635147094727, 'cosine_with_motion': -0.7735209358664246, 'motion_component': -4.274994714874654}]}, 5488: {'frame': 5488, 'ionic_force': [10.131879150867462, -2.3410739302635193, 1.1676548570394516], 'ionic_force_magnitude': 10.464177948597303, 'motion_vector': [0.2902336120605469, 0.38472747802734375, 0.097137451171875], 'cosine_ionic_motion': 0.41858651573256284, 'ionic_motion_component': 4.380163787508862, 'ionic_force_x': 10.131879150867462, 'ionic_force_y': -2.3410739302635193, 'ionic_force_z': 1.1676548570394516, 'radial_force': 10.398826966285295, 'axial_force': 1.1676548570394516, 'contributions': [{'ion': 1309, 'force': [5.3689775466918945, -8.8337984085083, 14.100717544555664], 'magnitude': 17.484054565429688, 'distance': 4.357605934143066, 'cosine_with_motion': -0.054754537935703916, 'motion_component': -0.9573313061794977}, {'ion': 1469, 'force': [2.2769510746002197, 3.038987398147583, 0.0664893239736557], 'magnitude': 3.797943115234375, 'distance': 9.349638938903809, 'cosine_with_motion': 0.9835887182888736, 'motion_component': 3.735613939452394}, {'ion': 2443, 'force': [0.3027248978614807, 0.33519941568374634, -2.6992714405059814], 'magnitude': 2.7367987632751465, 'distance': 11.014063835144043, 'cosine_with_motion': -0.03372762061171953, 'motion_component': -0.09230570945979721}, {'ion': 2444, 'force': [2.183225631713867, 3.118537664413452, -10.300280570983887], 'magnitude': 10.98123550415039, 'distance': 5.498489856719971, 'cosine_with_motion': 0.15428015145398466, 'motion_component': 1.694186662448928}]}, 5489: {'frame': 5489, 'ionic_force': [11.221921682357788, -2.8993600010871887, -5.796612232923508], 'ionic_force_magnitude': 12.959109847507065, 'motion_vector': [-0.5663490295410156, 0.11797332763671875, -0.6750717163085938], 'cosine_ionic_motion': -0.24168081898249347, 'ionic_motion_component': -3.1319682812296037, 'ionic_force_x': 11.221921682357788, 'ionic_force_y': -2.8993600010871887, 'ionic_force_z': -5.796612232923508, 'radial_force': 11.590419089095793, 'axial_force': -5.796612232923508, 'contributions': [{'ion': 1309, 'force': [6.7409892082214355, -7.9767279624938965, 4.073198318481445], 'magnitude': 11.209820747375488, 'distance': 5.442140102386475, 'cosine_with_motion': -0.7534133565420311, 'motion_component': -8.44562826709155}, {'ion': 1469, 'force': [2.320533037185669, 3.024193286895752, -0.05600830912590027], 'magnitude': 3.8123161792755127, 'distance': 9.33199691772461, 'cosine_with_motion': -0.27133866911752824, 'motion_component': -1.0344288301227174}, {'ion': 2443, 'force': [0.43547987937927246, 0.21962839365005493, -2.5775437355041504], 'magnitude': 2.6232824325561523, 'distance': 11.249844551086426, 'cosine_with_motion': 0.6514462620569944, 'motion_component': 1.7089275777366293}, {'ion': 2444, 'force': [1.7249195575714111, 1.8335462808609009, -7.236258506774902], 'magnitude': 7.661636829376221, 'distance': 6.582763671875, 'cosine_with_motion': 0.6055053157498032, 'motion_component': 4.639161737269472}]}, 5490: {'frame': 5490, 'ionic_force': [4.6175917610526085, -3.9973922222852707, -10.50867223739624], 'ionic_force_magnitude': 12.154566649763792, 'motion_vector': [0.1108245849609375, -3.2973403930664062, -3.8913345336914062], 'cosine_ionic_motion': 0.8802824710280489, 'ionic_motion_component': 10.699451964729185, 'ionic_force_x': 4.6175917610526085, 'ionic_force_y': -3.9973922222852707, 'ionic_force_z': -10.50867223739624, 'radial_force': 6.107478878434842, 'axial_force': -10.50867223739624, 'contributions': [{'ion': 1309, 'force': [1.3767764568328857, -9.229324340820312, 0.24545180797576904], 'magnitude': 9.334676742553711, 'distance': 5.963749885559082, 'cosine_with_motion': 0.6221765749990734, 'motion_component': 5.807817134494535}, {'ion': 1469, 'force': [2.126258611679077, 3.1915740966796875, -0.6759365797042847], 'magnitude': 3.894099473953247, 'distance': 9.233482360839844, 'cosine_with_motion': -0.38546180551476794, 'motion_component': -1.5010266361122788}, {'ion': 2443, 'force': [0.12220724672079086, 0.23922725021839142, -2.3671770095825195], 'magnitude': 2.382370948791504, 'distance': 11.80495548248291, 'cosine_with_motion': 0.6941030928097753, 'motion_component': 1.6536110358295508}, {'ion': 2444, 'force': [0.9923494458198547, 1.801130771636963, -7.711010456085205], 'magnitude': 7.980508327484131, 'distance': 6.449911594390869, 'cosine_with_motion': 0.5938281486675583, 'motion_component': 4.7390504322573275}]}, 5491: {'frame': 5491, 'ionic_force': [3.531671144068241, -3.3812859058380127, -9.039488315582275], 'ionic_force_magnitude': 10.277068864925035, 'motion_vector': [0.054042816162109375, 6.2353515625, 0.45986175537109375], 'cosine_ionic_motion': -0.3898304601081398, 'ionic_motion_component': -4.006314484176764, 'ionic_force_x': 3.531671144068241, 'ionic_force_y': -3.3812859058380127, 'ionic_force_z': -9.039488315582275, 'radial_force': 4.8893553201688125, 'axial_force': -9.039488315582275, 'contributions': [{'ion': 1309, 'force': [0.08836428076028824, -4.612890720367432, -2.9233412742614746], 'magnitude': 5.461913108825684, 'distance': 7.796445369720459, 'cosine_with_motion': -0.8814617600389186, 'motion_component': -4.814467416335644}, {'ion': 1469, 'force': [3.120267152786255, 1.8323882818222046, -2.4592511653900146], 'magnitude': 4.375114917755127, 'distance': 8.711126327514648, 'cosine_with_motion': 0.3824934866218572, 'motion_component': 1.6734529448831683}, {'ion': 2444, 'force': [0.323039710521698, -0.6007834672927856, -3.656895875930786], 'magnitude': 3.719970941543579, 'distance': 9.44711685180664, 'cosine_with_motion': -0.23260932244380778, 'motion_component': -0.865299891166011}]}, 5492: {'frame': 5492, 'ionic_force': [7.392548680305481, -1.4014756679534912, -11.69499546289444], 'ionic_force_magnitude': 13.906359297662114, 'motion_vector': [2.7979888916015625, 1.0762748718261719, 3.96209716796875], 'cosine_ionic_motion': -0.39310618776822775, 'ionic_motion_component': -5.466675889239203, 'ionic_force_x': 7.392548680305481, 'ionic_force_y': -1.4014756679534912, 'ionic_force_z': -11.69499546289444, 'radial_force': 7.524221556981957, 'axial_force': -11.69499546289444, 'contributions': [{'ion': 1309, 'force': [6.099052906036377, -4.69687557220459, -7.9687724113464355], 'magnitude': 11.079730033874512, 'distance': 5.473995685577393, 'cosine_with_motion': -0.3553767598406582, 'motion_component': -3.9374786012320016}, {'ion': 1469, 'force': [1.0042378902435303, 1.8420790433883667, -0.7561507821083069], 'magnitude': 2.230137586593628, 'distance': 12.20121955871582, 'cosine_with_motion': 0.16213359381764256, 'motion_component': 0.36158019590189205}, {'ion': 2444, 'force': [0.28925788402557373, 1.453320860862732, -2.9700722694396973], 'magnitude': 3.3192079067230225, 'distance': 10.001193046569824, 'cosine_with_motion': -0.5696472702968612, 'motion_component': -1.8907777069422327}]}, 5493: {'frame': 5493, 'ionic_force': [10.50127774477005, 5.519231498241425, -3.8027787916362286], 'ionic_force_magnitude': 12.457924271005234, 'motion_vector': [-1.495269775390625, 1.0756874084472656, 0.23244476318359375], 'cosine_ionic_motion': -0.4604190596535929, 'ionic_motion_component': -5.7358657780919025, 'ionic_force_x': 10.50127774477005, 'ionic_force_y': 5.519231498241425, 'ionic_force_z': -3.8027787916362286, 'radial_force': 11.863336402715007, 'axial_force': -3.8027787916362286, 'contributions': [{'ion': 1309, 'force': [7.177574157714844, 0.5480061769485474, 0.4017539322376251], 'magnitude': 7.2096662521362305, 'distance': 6.7859625816345215, 'cosine_with_motion': -0.7507798160511517, 'motion_component': -5.412871918936274}, {'ion': 1469, 'force': [0.9419129490852356, 1.280834674835205, -0.03194640204310417], 'magnitude': 1.5902068614959717, 'distance': 14.44914722442627, 'cosine_with_motion': -0.012891961460507317, 'motion_component': -0.02050088629485819}, {'ion': 2443, 'force': [0.5624699592590332, 0.8197107911109924, -1.5806218385696411], 'magnitude': 1.8672609329223633, 'distance': 13.334186553955078, 'cosine_with_motion': -0.09423761570225872, 'motion_component': -0.17596622429598163}, {'ion': 2444, 'force': [1.8193206787109375, 2.8706798553466797, -2.5919644832611084], 'magnitude': 4.274226188659668, 'distance': 8.813335418701172, 'cosine_with_motion': -0.02960224101162135, 'motion_component': -0.1265266770110891}]}, 5494: {'frame': 5494, 'ionic_force': [7.604774683713913, 7.194220662117004, -4.560827128589153], 'ionic_force_magnitude': 11.418868289903429, 'motion_vector': [0.6881828308105469, 0.4589118957519531, 0.434112548828125], 'cosine_ionic_motion': 0.6145182648430363, 'ionic_motion_component': 7.017103127982624, 'ionic_force_x': 7.604774683713913, 'ionic_force_y': 7.194220662117004, 'ionic_force_z': -4.560827128589153, 'radial_force': 10.468496020216431, 'axial_force': -4.560827128589153, 'contributions': [{'ion': 1309, 'force': [5.270052433013916, 1.1801180839538574, -0.09136883914470673], 'magnitude': 5.401340484619141, 'distance': 7.8400397300720215, 'cosine_with_motion': 0.8182541697057424, 'motion_component': 4.419669416924913}, {'ion': 1469, 'force': [0.786957323551178, 1.485055923461914, -0.08958549052476883], 'magnitude': 1.6830681562423706, 'distance': 14.04488468170166, 'cosine_with_motion': 0.7531818377095537, 'motion_component': 1.2676563817786788}, {'ion': 2443, 'force': [0.3067300617694855, 1.0199345350265503, -1.5694105625152588], 'magnitude': 1.8966810703277588, 'distance': 13.230366706848145, 'cosine_with_motion': -0.0012159144470626063, 'motion_component': -0.0023062019846715742}, {'ion': 2444, 'force': [1.2410348653793335, 3.5091121196746826, -2.810462236404419], 'magnitude': 4.663982391357422, 'distance': 8.43704891204834, 'cosine_with_motion': 0.2856107534826452, 'motion_component': 1.332083575267653}]}, 5495: {'frame': 5495, 'ionic_force': [7.7076713144779205, 6.843995451927185, -3.1370171401649714], 'ionic_force_magnitude': 10.774476663658175, 'motion_vector': [0.6293601989746094, -1.066162109375, -0.34174346923828125], 'cosine_ionic_motion': -0.09927879076110027, 'ionic_motion_component': -1.0696770142516778, 'ionic_force_x': 7.7076713144779205, 'ionic_force_y': 6.843995451927185, 'ionic_force_z': -3.1370171401649714, 'radial_force': 10.307689888526225, 'axial_force': -3.1370171401649714, 'contributions': [{'ion': 1309, 'force': [4.939149856567383, 1.1103832721710205, 0.3859111964702606], 'magnitude': 5.077113151550293, 'distance': 8.08650016784668, 'cosine_with_motion': 0.2749294025598821, 'motion_component': 1.3958477346173073}, {'ion': 1469, 'force': [1.0719969272613525, 1.4649080038070679, 0.0071951355785131454], 'magnitude': 1.815264344215393, 'distance': 13.523811340332031, 'cosine_with_motion': -0.3815711058689474, 'motion_component': -0.6926524235055304}, {'ion': 2443, 'force': [0.3923477232456207, 1.103355884552002, -1.5097792148590088], 'magnitude': 1.910697340965271, 'distance': 13.181750297546387, 'cosine_with_motion': -0.16848680323152304, 'motion_component': -0.3219272821939594}, {'ion': 2444, 'force': [1.3041768074035645, 3.1653482913970947, -2.0203442573547363], 'magnitude': 3.9751853942871094, 'distance': 9.138824462890625, 'cosine_with_motion': -0.36500061517302956, 'motion_component': -1.4509450661405054}]}, 5496: {'frame': 5496, 'ionic_force': [8.74626049399376, 6.5846357345581055, -4.182012894656509], 'ionic_force_magnitude': 11.71937422547334, 'motion_vector': [0.7211837768554688, -0.30852508544921875, -0.23809051513671875], 'cosine_ionic_motion': 0.5487553892618503, 'ionic_motion_component': 6.431069765004918, 'ionic_force_x': 8.74626049399376, 'ionic_force_y': 6.5846357345581055, 'ionic_force_z': -4.182012894656509, 'radial_force': 10.947808017389395, 'axial_force': -4.182012894656509, 'contributions': [{'ion': 1309, 'force': [5.159459590911865, 1.0115982294082642, -0.0068298703990876675], 'magnitude': 5.257699489593506, 'distance': 7.946413516998291, 'cosine_with_motion': 0.7912912796099127, 'motion_component': 4.160371529084642}, {'ion': 1469, 'force': [1.318227767944336, 1.3875240087509155, 0.040635738521814346], 'magnitude': 1.9143141508102417, 'distance': 13.169292449951172, 'cosine_with_motion': 0.3268593891850779, 'motion_component': 0.6257115470666249}, {'ion': 2443, 'force': [0.47910425066947937, 1.0934357643127441, -1.6458216905593872], 'magnitude': 2.0331923961639404, 'distance': 12.778497695922852, 'cosine_with_motion': 0.2400100975735285, 'motion_component': 0.48798672728567816}, {'ion': 2444, 'force': [1.7894688844680786, 3.0920777320861816, -2.5699970722198486], 'magnitude': 4.400912284851074, 'distance': 8.68555736541748, 'cosine_with_motion': 0.26290005160501845, 'motion_component': 1.1570000549089627}]}, 5497: {'frame': 5497, 'ionic_force': [6.961087644100189, 5.41208153963089, -4.26440330222249], 'ionic_force_magnitude': 9.794513939163284, 'motion_vector': [-1.509521484375, 1.9396095275878906, 0.17327117919921875], 'cosine_ionic_motion': -0.031056908057381913, 'ionic_motion_component': -0.3041873188753397, 'ionic_force_x': 6.961087644100189, 'ionic_force_y': 5.41208153963089, 'ionic_force_z': -4.26440330222249, 'radial_force': 8.81744678353421, 'axial_force': -4.26440330222249, 'contributions': [{'ion': 1309, 'force': [3.2068612575531006, 0.40660589933395386, -0.12844008207321167], 'magnitude': 3.235086441040039, 'distance': 10.130388259887695, 'cosine_with_motion': -0.5111621811598831, 'motion_component': -1.6536538458867085}, {'ion': 1469, 'force': [1.2073882818222046, 1.2977768182754517, -0.038394588977098465], 'magnitude': 1.772987723350525, 'distance': 13.684098243713379, 'cosine_with_motion': 0.15748131430486484, 'motion_component': 0.27921242850128447}, {'ion': 2443, 'force': [0.6200312972068787, 1.031477451324463, -1.5388377904891968], 'magnitude': 1.9535624980926514, 'distance': 13.036331176757812, 'cosine_with_motion': 0.16580428864796673, 'motion_component': 0.32390903411250704}, {'ion': 2444, 'force': [1.9268068075180054, 2.6762213706970215, -2.5587308406829834], 'magnitude': 4.173948764801025, 'distance': 8.918575286865234, 'cosine_with_motion': 0.1788103758969193, 'motion_component': 0.7463453587972211}]}, 5498: {'frame': 5498, 'ionic_force': [4.10741001367569, 5.098243832588196, -3.6214068830013275], 'ionic_force_magnitude': 7.481810944498417, 'motion_vector': [-0.3549995422363281, 0.2932014465332031, 0.5114364624023438], 'cosine_ionic_motion': -0.352603884698631, 'ionic_motion_component': -2.6381156036108755, 'ionic_force_x': 4.10741001367569, 'ionic_force_y': 5.098243832588196, 'ionic_force_z': -3.6214068830013275, 'radial_force': 6.54697695100318, 'axial_force': -3.6214068830013275, 'contributions': [{'ion': 1309, 'force': [2.7465009689331055, 1.1063706874847412, -0.25553974509239197], 'magnitude': 2.971973180770874, 'distance': 10.56930923461914, 'cosine_with_motion': -0.38202445241844485, 'motion_component': -1.1353664041428075}, {'ion': 2443, 'force': [0.3203471302986145, 1.1662036180496216, -1.4032648801803589], 'magnitude': 1.852513313293457, 'distance': 13.387157440185547, 'cosine_with_motion': -0.3839537031283095, 'motion_component': -0.71127933747524}, {'ion': 2444, 'force': [1.0405619144439697, 2.825669527053833, -1.9626022577285767], 'magnitude': 3.594299077987671, 'distance': 9.61085319519043, 'cosine_with_motion': -0.22020147314330785, 'motion_component': -0.791469925361028}]}, 5499: {'frame': 5499, 'ionic_force': [4.963673681020737, 6.609779596328735, -3.376120550557971], 'ionic_force_magnitude': 8.9289099388224, 'motion_vector': [0.3253974914550781, -0.08216476440429688, -0.2378997802734375], 'cosine_ionic_motion': 0.5105307809870959, 'ionic_motion_component': 4.558483364430443, 'ionic_force_x': 4.963673681020737, 'ionic_force_y': 6.609779596328735, 'ionic_force_z': -3.376120550557971, 'radial_force': 8.266029441255434, 'axial_force': -3.376120550557971, 'contributions': [{'ion': 1309, 'force': [3.1469173431396484, 1.3124815225601196, -0.09989611059427261], 'magnitude': 3.4111106395721436, 'distance': 9.865546226501465, 'cosine_with_motion': 0.6698188633880374, 'motion_component': 2.2848262464939917}, {'ion': 1469, 'force': [0.7330875396728516, 1.2971830368041992, -0.008259242400527], 'magnitude': 1.4900232553482056, 'distance': 14.92699909210205, 'cosine_with_motion': 0.21849183202341296, 'motion_component': 0.3255579170800985}, {'ion': 2443, 'force': [0.2510865032672882, 1.1263843774795532, -1.4073807001113892], 'magnitude': 1.8200292587280273, 'distance': 13.506096839904785, 'cosine_with_motion': 0.4326988603405221, 'motion_component': 0.787524601535635}, {'ion': 2444, 'force': [0.8325822949409485, 2.8737306594848633, -1.8605844974517822], 'magnitude': 3.5232508182525635, 'distance': 9.707273483276367, 'cosine_with_motion': 0.3294044407574017, 'motion_component': 1.1605744432274108}]}, 5500: {'frame': 5500, 'ionic_force': [5.459194302558899, 5.718991637229919, -2.9895115792751312], 'ionic_force_magnitude': 8.45262369104513, 'motion_vector': [2.9813499450683594, -5.0980072021484375, -0.931304931640625], 'cosine_ionic_motion': -0.19976887581490052, 'ionic_motion_component': -1.6885711324464805, 'ionic_force_x': 5.459194302558899, 'ionic_force_y': 5.718991637229919, 'ionic_force_z': -2.9895115792751312, 'radial_force': 7.906305570859079, 'axial_force': -2.9895115792751312, 'contributions': [{'ion': 1309, 'force': [4.1073384284973145, 2.204691171646118, 0.19625237584114075], 'magnitude': 4.665769577026367, 'distance': 8.435433387756348, 'cosine_with_motion': 0.029506956898164696, 'motion_component': 0.1376726661623504}, {'ion': 2443, 'force': [0.4238545298576355, 0.9974464178085327, -1.34289908409</t>
+          <t>{5477: {'frame': 5477, 'ionic_force': [1.4224569201469421, -4.641303360462189, -9.415545463562012], 'ionic_force_magnitude': 10.59327980136061, 'motion_vector': [-0.5623664855957031, 0.9072761535644531, 0.3484649658203125], 'cosine_ionic_motion': -0.6970970980387372, 'ionic_motion_component': -7.384544608240852, 'ionic_force_x': 1.4224569201469421, 'ionic_force_y': -4.641303360462189, 'ionic_force_z': -9.415545463562012, 'radial_force': 4.854387765054573, 'axial_force': -9.415545463562012, 'before_closest_residue': None, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [-0.14590446650981903, -7.744018077850342, -4.193130970001221], 'magnitude': 8.807579040527344, 'distance': 6.1396098136901855, 'before_closest_residue': 423, 'closest_residue': 130, 'next_closest_residue': 98, 'cosine_with_motion': -0.8498765392041681, 'motion_component': -7.485354932675172}, {'ion': 1469, 'force': [1.5043941736221313, 2.458629608154297, -1.5455207824707031], 'magnitude': 3.270580291748047, 'distance': 10.075268745422363, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.23038555492130164, 'motion_component': 0.753494470362682}, {'ion': 2444, 'force': [0.06396721303462982, 0.6440851092338562, -3.676893711090088], 'magnitude': 3.7334280014038086, 'distance': 9.430074691772461, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.174821671211077, 'motion_component': -0.6526841261401124}]}, 5478: {'frame': 5478, 'ionic_force': [3.782637048512697, -4.220937579870224, -11.806665897369385], 'ionic_force_magnitude': 13.096641428474966, 'motion_vector': [5.6822967529296875, -1.4546623229980469, 1.581939697265625], 'cosine_ionic_motion': 0.112572399553655, 'ionic_motion_component': 1.4743203516972347, 'ionic_force_x': 3.782637048512697, 'ionic_force_y': -4.220937579870224, 'ionic_force_z': -11.806665897369385, 'radial_force': 5.667861774420893, 'axial_force': -11.806665897369385, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 455, 'contributions': [{'ion': 1309, 'force': [2.848625421524048, -7.680440902709961, -5.491806507110596], 'magnitude': 9.862239837646484, 'distance': 5.802047252655029, 'before_closest_residue': 130, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.311636488808021, 'motion_component': 3.073433847690566}, {'ion': 1469, 'force': [1.1187093257904053, 2.1294939517974854, -1.1434855461120605], 'magnitude': 2.663421392440796, 'distance': 11.164752006530762, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.08962698302468124, 'motion_component': 0.23871443615680477}, {'ion': 2443, 'force': [-0.03920864686369896, 0.29816392064094543, -1.4478132724761963], 'magnitude': 1.478716492652893, 'distance': 14.983959197998047, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3280365163349735, 'motion_component': -0.48507299002336723}, {'ion': 2444, 'force': [-0.14548905193805695, 1.0318454504013062, -3.7235605716705322], 'magnitude': 3.8666231632232666, 'distance': 9.266230583190918, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.34985431505545295, 'motion_component': -1.3527548319276432}]}, 5479: {'frame': 5479, 'ionic_force': [7.66579008102417, -0.03574265539646149, -6.5100264847278595], 'ionic_force_magnitude': 10.057139749232956, 'motion_vector': [-0.8315162658691406, 0.4536933898925781, 0.4904327392578125], 'cosine_ionic_motion': -0.8933169575861272, 'ionic_motion_component': -8.98421348280329, 'ionic_force_x': 7.66579008102417, 'ionic_force_y': -0.03574265539646149, 'ionic_force_z': -6.5100264847278595, 'radial_force': 7.665873407756179, 'axial_force': -6.5100264847278595, 'before_closest_residue': 130, 'closest_residue': 455, 'next_closest_residue': 455, 'contributions': [{'ion': 1309, 'force': [2.8427734375, -2.1192972660064697, -0.8717526197433472], 'magnitude': 3.6514017581939697, 'distance': 9.535407066345215, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.963547918868339, 'motion_component': -3.518300505546865}, {'ion': 1469, 'force': [1.5580865144729614, 1.1739774942398071, -0.4098491966724396], 'magnitude': 1.9934475421905518, 'distance': 12.905256271362305, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.4533369941770629, 'motion_component': -0.9037035172938319}, {'ion': 2443, 'force': [0.5962351560592651, 0.1816510409116745, -1.6120604276657104], 'magnitude': 1.7283612489700317, 'distance': 13.859634399414062, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6530594455283119, 'motion_component': -1.1287225779949241}, {'ion': 2444, 'force': [2.6686949729919434, 0.7279260754585266, -3.6163642406463623], 'magnitude': 4.553009986877441, 'distance': 8.539250373840332, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7541136132982074, 'motion_component': -3.433486780340937}]}, 5480: {'frame': 5480, 'ionic_force': [8.63328468799591, 0.006521552801132202, -5.980384021997452], 'ionic_force_magnitude': 10.502315939124951, 'motion_vector': [-2.4467201232910156, 2.9426307678222656, 1.0514373779296875], 'cosine_ionic_motion': -0.6571806221442732, 'ionic_motion_component': -6.9019185228298525, 'ionic_force_x': 8.63328468799591, 'ionic_force_y': 0.006521552801132202, 'ionic_force_z': -5.980384021997452, 'radial_force': 8.633287151174551, 'axial_force': -5.980384021997452, 'before_closest_residue': 455, 'closest_residue': 455, 'next_closest_residue': 423, 'contributions': [{'ion': 1309, 'force': [4.6044087409973145, -2.470323085784912, -0.8643374443054199], 'magnitude': 5.296239852905273, 'distance': 7.917448043823242, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.9250340582306482, 'motion_component': -4.899202125768213}, {'ion': 1469, 'force': [1.6390438079833984, 1.4995357990264893, -0.4266315996646881], 'magnitude': 2.2620978355407715, 'distance': 12.11471939086914, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.005154729957164885, 'motion_component': -0.011660503617133777}, {'ion': 2443, 'force': [0.6318773031234741, 0.20215561985969543, -1.57472562789917], 'magnitude': 1.708770513534546, 'distance': 13.938857078552246, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.38439987659516817, 'motion_component': -0.6568511695921728}, {'ion': 2444, 'force': [1.7579548358917236, 0.7751532196998596, -3.114689350128174], 'magnitude': 3.6595845222473145, 'distance': 9.524741172790527, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.36457819253244267, 'motion_component': -1.334204640375063}]}, 5481: {'frame': 5481, 'ionic_force': [10.722378462553024, 3.6098837852478027, -5.247070275247097], 'ionic_force_magnitude': 12.471263260415826, 'motion_vector': [1.9404220581054688, -4.451213836669922, 0.8924026489257812], 'cosine_ionic_motion': 0.0008944936529652115, 'ionic_motion_component': 0.011155465830900187, 'ionic_force_x': 10.722378462553024, 'ionic_force_y': 3.6098837852478027, 'ionic_force_z': -5.247070275247097, 'radial_force': 11.313737704101856, 'axial_force': -5.247070275247097, 'before_closest_residue': 455, 'closest_residue': 423, 'next_closest_residue': 423, 'contributions': [{'ion': 1309, 'force': [8.690352439880371, -0.589633584022522, -0.05870877951383591], 'magnitude': 8.710530281066895, 'distance': 6.173717498779297, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.45193035456920416, 'motion_component': 3.9365530964176982}, {'ion': 1469, 'force': [0.9652875065803528, 1.5830146074295044, -0.20551034808158875], 'magnitude': 1.865462303161621, 'distance': 13.34061336517334, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.5816164448618182, 'motion_component': -1.0849835709259943}, {'ion': 2443, 'force': [0.3752489387989044, 0.6354923248291016, -1.8373764753341675], 'magnitude': 1.9800541400909424, 'distance': 12.948829650878906, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.3826061510855403, 'motion_component': -0.757580910428099}, {'ion': 2444, 'force': [0.691489577293396, 1.9810104370117188, -3.145474672317505], 'magnitude': 3.781080722808838, 'distance': 9.370463371276855, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5508565617056489, 'motion_component': -2.0828331023756945}]}, 5482: {'frame': 5482, 'ionic_force': [10.771212220191956, -0.8395132049918175, -7.971047785133123], 'ionic_force_magnitude': 13.426146055612676, 'motion_vector': [-3.371776580810547, 2.4830093383789062, -2.777191162109375], 'cosine_ionic_motion': -0.24110797819383406, 'ionic_motion_component': -3.2371509304038923, 'ionic_force_x': 10.771212220191956, 'ionic_force_y': -0.8395132049918175, 'ionic_force_z': -7.971047785133123, 'radial_force': 10.803878706916704, 'axial_force': -7.971047785133123, 'before_closest_residue': 423, 'closest_residue': 423, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [2.8360345363616943, -2.8020989894866943, 0.3442707359790802], 'magnitude': 4.001671314239502, 'distance': 9.10853099822998, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.8691628231816363, 'motion_component': -3.4781039011742347}, {'ion': 1469, 'force': [2.137364387512207, 1.547278881072998, -0.054249223321676254], 'magnitude': 2.639193296432495, 'distance': 11.215882301330566, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.24237600744025303, 'motion_component': -0.6396771424608481}, {'ion': 2443, 'force': [0.930376410484314, 0.07820767909288406, -2.1504712104797363], 'magnitude': 2.344406843185425, 'distance': 11.900153160095215, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.25717236860653303, 'motion_component': 0.6029166436709448}, {'ion': 2444, 'force': [4.86743688583374, 0.33709922432899475, -6.110598087310791], 'magnitude': 7.819525718688965, 'distance': 6.515966415405273, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.035515385916932506, 'motion_component': 0.2777134832245567}]}, 5483: {'frame': 5483, 'ionic_force': [14.705014813691378, -4.830581963062286, -13.659503698348999], 'ionic_force_magnitude': 20.64349834834095, 'motion_vector': [-1.0512886047363281, -1.1198539733886719, -3.1050186157226562], 'cosine_ionic_motion': 0.45255552467683335, 'ionic_motion_component': 9.342329226198782, 'ionic_force_x': 14.705014813691378, 'ionic_force_y': -4.830581963062286, 'ionic_force_z': -13.659503698348999, 'radial_force': 15.478113023645536, 'axial_force': -13.659503698348999, 'before_closest_residue': 423, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [12.95172119140625, -9.656329154968262, -6.279929161071777], 'magnitude': 17.332895278930664, 'distance': 4.376565933227539, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.27807920582061574, 'motion_component': 4.819917962997209}, {'ion': 1469, 'force': [1.47786545753479, 2.6548736095428467, -0.7496045827865601], 'magnitude': 3.129592180252075, 'distance': 10.299714088439941, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.20285152649453522, 'motion_component': -0.6348425513631568}, {'ion': 2443, 'force': [0.023254413157701492, 0.36658936738967896, -1.7489255666732788], 'magnitude': 1.7870839834213257, 'distance': 13.630022048950195, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.8069254149980343, 'motion_component': 1.4420434863079719}, {'ion': 2444, 'force': [0.2521737515926361, 1.8042842149734497, -4.881044387817383], 'magnitude': 5.209954738616943, 'distance': 7.982741832733154, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7130983805644391, 'motion_component': 3.7152102230572357}]}, 5484: {'frame': 5484, 'ionic_force': [3.3583530709147453, -1.8520203530788422, -9.582316398620605], 'ionic_force_magnitude': 10.32130332372875, 'motion_vector': [-1.2701416015625, -1.1113739013671875, -2.5788192749023438], 'cosine_ionic_motion': 0.7074375045446344, 'ionic_motion_component': 7.301677066986908, 'ionic_force_x': 3.3583530709147453, 'ionic_force_y': -1.8520203530788422, 'ionic_force_z': -9.582316398620605, 'radial_force': 3.8351681497870183, 'axial_force': -9.582316398620605, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 130, 'contributions': [{'ion': 1309, 'force': [2.1952145099639893, -4.486453056335449, -5.257387638092041], 'magnitude': 7.251713752746582, 'distance': 6.766260623931885, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': 0.7049620782123642, 'motion_component': 5.112183207305485}, {'ion': 1469, 'force': [1.2880535125732422, 2.27970814704895, -1.8271305561065674], 'magnitude': 3.1928915977478027, 'distance': 10.19710636138916, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.05510102667779303, 'motion_component': 0.17593160856745982}, {'ion': 2444, 'force': [-0.12491495162248611, 0.35472455620765686, -2.497798204421997], 'magnitude': 2.5259511470794678, 'distance': 11.46453857421875, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.7971501673219711, 'motion_component': 2.0135623682589534}]}, 5485: {'frame': 5485, 'ionic_force': [1.483163833618164, -0.4733795076608658, -5.7409727573394775], 'ionic_force_magnitude': 5.948330128375544, 'motion_vector': [4.385654449462891, -1.0877685546875, 2.3917007446289062], 'cosine_ionic_motion': -0.22068268473215408, 'ionic_motion_component': -1.312693462403074, 'ionic_force_x': 1.483163833618164, 'ionic_force_y': -0.4733795076608658, 'ionic_force_z': -5.7409727573394775, 'radial_force': 1.5568760758731481, 'axial_force': -5.7409727573394775, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [0.5064878463745117, -2.087893009185791, -3.4851157665252686], 'magnitude': 4.094125270843506, 'distance': 9.005099296569824, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.18359875780452614, 'motion_component': -0.7516762541344804}, {'ion': 1469, 'force': [0.7889192700386047, 1.6113115549087524, -1.897242546081543], 'magnitude': 2.611177444458008, 'distance': 11.275890350341797, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.21202473408075306, 'motion_component': -0.5536342103565328}, {'ion': 2436, 'force': [0.3979494571685791, -0.12599879503250122, 1.4812759160995483], 'magnitude': 1.538966417312622, 'distance': 14.687723159790039, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6895196838728914, 'motion_component': 1.0611476762695622}, {'ion': 2444, 'force': [-0.2101927399635315, 0.129200741648674, -1.8398903608322144], 'magnitude': 1.8563593626022339, 'distance': 13.373282432556152, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5756054760786232, 'motion_component': -1.0685306575260782}]}, 5486: {'frame': 5486, 'ionic_force': [4.225400745868683, -1.113166643306613, -5.5725942850112915], 'ionic_force_magnitude': 7.081451722937793, 'motion_vector': [-1.728607177734375, 5.325992584228516, 4.6172027587890625], 'cosine_ionic_motion': -0.7581095044957695, 'ionic_motion_component': -5.368515856787083, 'ionic_force_x': 4.225400745868683, 'ionic_force_y': -1.113166643306613, 'ionic_force_z': -5.5725942850112915, 'radial_force': 4.369571081806329, 'axial_force': -5.5725942850112915, 'before_closest_residue': 130, 'closest_residue': 780, 'next_closest_residue': 455, 'contributions': [{'ion': 1309, 'force': [2.1206986904144287, -2.4510836601257324, -1.6197460889816284], 'magnitude': 3.623361825942993, 'distance': 9.57223129272461, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 98, 'cosine_with_motion': -0.9202215468575357, 'motion_component': -3.334295689758271}, {'ion': 1469, 'force': [1.5200526714324951, 1.3517338037490845, -1.3707325458526611], 'magnitude': 2.4528865814208984, 'distance': 11.634034156799316, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1105, 'cosine_with_motion': -0.098707559429281, 'motion_component': -0.24211843857373339}, {'ion': 2444, 'force': [0.584649384021759, -0.01381678692996502, -2.582115650177002], 'magnitude': 2.6475133895874023, 'distance': 11.19824504852295, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.6769000204594124, 'motion_component': -1.7921018533477944}]}, 5487: {'frame': 5487, 'ionic_force': [15.482393935322762, 3.9336164593696594, -6.411904938519001], 'ionic_force_magnitude': 17.213087618395118, 'motion_vector': [0.3015022277832031, -3.9131088256835938, 0.8899307250976562], 'cosine_ionic_motion': -0.23719556888232954, 'ionic_motion_component': -4.082868109866613, 'ionic_force_x': 15.482393935322762, 'ionic_force_y': 3.9336164593696594, 'ionic_force_z': -6.411904938519001, 'radial_force': 15.974287477629257, 'axial_force': -6.411904938519001, 'before_closest_residue': 780, 'closest_residue': 455, 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [13.761055946350098, -2.1138620376586914, -0.08146259933710098], 'magnitude': 13.922704696655273, 'distance': 4.883230686187744, 'before_closest_residue': 98, 'closest_residue': 98, 'next_closest_residue': 130, 'cosine_with_motion': 0.22038793154140668, 'motion_component': 3.068396117715446}, {'ion': 1469, 'force': [0.9084755182266235, 1.9054216146469116, -0.2553384602069855], 'magnitude': 2.1263012886047363, 'distance': 12.495586395263672, 'before_closest_residue': 1073, 'closest_residue': 1105, 'next_closest_residue': 1073, 'cosine_with_motion': -0.8658976507435727, 'motion_component': -1.8411592612795076}, {'ion': 2443, 'force': [0.1551320105791092, 0.6592459082603455, -1.8346444368362427], 'magnitude': 1.9556562900543213, 'distance': 13.029350280761719, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.5292905712008917, 'motion_component': -1.0351104068303}, {'ion': 2444, 'force': [0.6577304601669312, 3.4828109741210938, -4.240459442138672], 'magnitude': 5.526669979095459, 'distance': 7.750635147094727, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.7735209358664246, 'motion_component': -4.274994714874654}]}, 5488: {'frame': 5488, 'ionic_force': [10.131879150867462, -2.3410739302635193, 1.1676548570394516], 'ionic_force_magnitude': 10.464177948597303, 'motion_vector': [0.2902336120605469, 0.38472747802734375, 0.097137451171875], 'cosine_ionic_motion': 0.41858651573256284, 'ionic_motion_component': 4.380163787508862, 'ionic_force_x': 10.131879150867462, 'ionic_force_y': -2.3410739302635193, 'ionic_force_z': 1.1676548570394516, 'radial_force': 10.398826966285295, 'axial_force': 1.1676548570394516, 'before_closest_residue': 455, 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [5.3689775466918945, -8.8337984085083, 14.100717544555664], 'magnitude': 17.484054565429688, 'distance': 4.357605934143066, 'before_closest_residue': 98, 'closest_residue': 130, 'next_closest_residue': 130, 'cosine_with_motion': -0.054754537935703916, 'motion_component': -0.9573313061794977}, {'ion': 1469, 'force': [2.2769510746002197, 3.038987398147583, 0.0664893239736557], 'magnitude': 3.797943115234375, 'distance': 9.349638938903809, 'before_closest_residue': 1105, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': 0.9835887182888736, 'motion_component': 3.735613939452394}, {'ion': 2443, 'force': [0.3027248978614807, 0.33519941568374634, -2.6992714405059814], 'magnitude': 2.7367987632751465, 'distance': 11.014063835144043, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': -0.03372762061171953, 'motion_component': -0.09230570945979721}, {'ion': 2444, 'force': [2.183225631713867, 3.118537664413452, -10.300280570983887], 'magnitude': 10.98123550415039, 'distance': 5.498489856719971, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.15428015145398466, 'motion_component': 1.694186662448928}]}, 5489: {'frame': 5489, 'ionic_force': [11.221921682357788, -2.8993600010871887, -5.796612232923508], 'ionic_force_magnitude': 12.959109847507065, 'motion_vector': [-0.5663490295410156, 0.11797332763671875, -0.6750717163085938], 'cosine_ionic_motion': -0.24168081898249347, 'ionic_motion_component': -3.1319682812296037, 'ionic_force_x': 11.221921682357788, 'ionic_force_y': -2.8993600010871887, 'ionic_force_z': -5.796612232923508, 'radial_force': 11.590419089095793, 'axial_force': -5.796612232923508, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 'SF', 'contributions': [{'ion': 1309, 'force': [6.7409892082214355, -7.9767279624938965, 4.073198318481445], 'magnitude': 11.209820747375488, 'distance': 5.442140102386475, 'before_closest_residue': 130, 'closest_residue': 130, 'next_closest_residue': 98, 'cosine_with_motion': -0.7534133565420311, 'motion_component': -8.44562826709155}, {'ion': 1469, 'force': [2.320533037185669, 3.024193286895752, -0.05600830912590027], 'magnitude': 3.8123161792755127, 'distance': 9.33199691772461, 'before_closest_residue': 1073, 'closest_residue': 1073, 'next_closest_residue': 1073, 'cosine_with_motion': -0.27133866911752824, 'motion_component': -1.0344288301227174}, {'ion': 2443, 'force': [0.43547987937927246, 0.21962839365005493, -2.5775437355041504], 'magnitude': 2.6232824325561523, 'distance': 11.249844551086426, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6514462620569944, 'motion_component': 1.7089275777366293}, {'ion': 2444, 'force': [1.7249195575714111, 1.8335462808609009, -7.236258506774902], 'magnitude': 7.661636829376221, 'distance': 6.582763671875, 'before_closest_residue': None, 'closest_residue': None, 'next_closest_residue': None, 'cosine_with_motion': 0.6055053157498032, 'motion_component': 4.639161737269472}]}, 5490: {'frame': 5490, 'ionic_force': [4.6175917610526085, -3.9973922222852707, -10.50867223739624], 'ionic_force_magnitude': 12.154566649763792, 'motion_vector': [0.1108245849609375, -3.2973403930664062, -3.8913345336914062], 'cosine_ionic_motion': 0.8802824710280489, 'ionic_motion_component': 10.699451964729185, 'ionic_force_x': 4.6175917610526085, 'ionic_force_y': -3.9973922222852707, 'ionic_force_z': -10.50867223739624, 'radial_force': 6.107478878434842, 'axial_force': -10.50867223739624, 'before_closest_residue': 'SF', 'closest_residue': 'SF', 'next_closest_residue': 780, 'contributions': [{'ion': 1309, 'force': [1.3767764568328857, -9.22932434082031